<commit_message>
Altrações 13/03/20 - Marcos
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257FC933-3F77-44C6-89B1-1658B280413F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3865B9-AA83-4AE2-974C-49AAC09878E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="615" windowWidth="20460" windowHeight="10905" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2813" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2830" uniqueCount="724">
   <si>
     <t>Prioridade</t>
   </si>
@@ -2315,6 +2315,31 @@
   </si>
   <si>
     <t>Solicito geração do arquivo REINF: Gerado integração do faturamento da Balsa Nova, calculado percentual, agregado ao faturamento da BK, apurado as retenções, conciliado, acompanhamento da transmissão e fechamento do período.</t>
+  </si>
+  <si>
+    <t>Gestao</t>
+  </si>
+  <si>
+    <t>Solicito o ajustes nos lançamentos de GASTOS GERAIS no contrato 350.000.536, seguindo a orientação abaixo:
+- SERV.DE INFORMATICA ISS 2,90% - valor 3214,80 lançar na competência nov/2019
+- SERV.DE INFORMATICA ISS 2,90% - valor 4.500,00 lançar na competência dez/2019
+- SERV.DE INFORMATICA ISS 2,90% - valor 4.500,00 lançar na competência jan/2020
+- alterar o lançamento em CONSERTO, RESTAURACAO, MANUTENCAO para SERV.DE INFORMATICA ISS 2,90% - valor 4.500,00 lançar na competência fev/2020: Informado ao usuário que esta demanda deve ser feita junto ao Depto Fiscal</t>
+  </si>
+  <si>
+    <t>12/03/20</t>
+  </si>
+  <si>
+    <t>Solicito a localização dos lançamentos com os titulos listados:
+Forn: 000084-01-BK CONSULTORIA LF -305593LPM-
+R$ 13.165,12 - Emissão 27/12/2019.
+Forn: 000084-01-BK CONSULTORIA LF -305614LPM-
+R$ 3.809,81 - Emissão 27/12/2019.
+Forn: 000084-01-BK CONSULTORIA LF -305618LPM-
+R$ 2.818,16 - Emissão 27/12/2019.
+Forn: 000084-01-BK CONSULTORIA LF -305624LPM-
+R$ 30.543,98 - Emissão 27/12/2019. 
+Foi orientado ao usuário processar o off-line deste período</t>
   </si>
 </sst>
 </file>
@@ -3018,8 +3043,8 @@
   <dimension ref="A1:J452"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A431" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A438" sqref="A438"/>
+      <pane ySplit="1" topLeftCell="A438" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I436" sqref="I436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15014,9 +15039,15 @@
       <c r="F435" s="20" t="s">
         <v>528</v>
       </c>
-      <c r="G435" s="27"/>
-      <c r="H435" s="49"/>
-      <c r="I435" s="21"/>
+      <c r="G435" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H435" s="49" t="s">
+        <v>722</v>
+      </c>
+      <c r="I435" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J435" s="21"/>
     </row>
     <row r="436" spans="1:10" x14ac:dyDescent="0.25">
@@ -15077,28 +15108,64 @@
       </c>
       <c r="J437" s="21"/>
     </row>
-    <row r="438" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A438" s="27"/>
-      <c r="B438" s="25"/>
-      <c r="C438" s="19"/>
-      <c r="D438" s="20"/>
-      <c r="E438" s="19"/>
-      <c r="F438" s="20"/>
-      <c r="G438" s="27"/>
-      <c r="H438" s="49"/>
-      <c r="I438" s="21"/>
+    <row r="438" spans="1:10" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A438" s="27">
+        <v>43902</v>
+      </c>
+      <c r="B438" s="25" t="s">
+        <v>451</v>
+      </c>
+      <c r="C438" s="19" t="s">
+        <v>720</v>
+      </c>
+      <c r="D438" s="20">
+        <v>320998</v>
+      </c>
+      <c r="E438" s="19" t="s">
+        <v>721</v>
+      </c>
+      <c r="F438" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G438" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H438" s="49" t="s">
+        <v>722</v>
+      </c>
+      <c r="I438" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J438" s="21"/>
     </row>
-    <row r="439" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A439" s="27"/>
-      <c r="B439" s="25"/>
-      <c r="C439" s="19"/>
-      <c r="D439" s="20"/>
-      <c r="E439" s="19"/>
-      <c r="F439" s="20"/>
-      <c r="G439" s="27"/>
-      <c r="H439" s="49"/>
-      <c r="I439" s="21"/>
+    <row r="439" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A439" s="27">
+        <v>43902</v>
+      </c>
+      <c r="B439" s="25" t="s">
+        <v>607</v>
+      </c>
+      <c r="C439" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D439" s="20">
+        <v>3200002</v>
+      </c>
+      <c r="E439" s="19" t="s">
+        <v>723</v>
+      </c>
+      <c r="F439" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G439" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H439" s="49" t="s">
+        <v>722</v>
+      </c>
+      <c r="I439" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J439" s="21"/>
     </row>
     <row r="440" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Inclusão de filtro  AND CN9_SITUAC <> '09'
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C29EEF-2FDF-4ADF-8477-17DCF066000E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AEE6CE-B96A-4BD5-8C98-3B271A8F0909}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="0" windowWidth="19170" windowHeight="10320" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_FilterDatabase_0" localSheetId="0">Plan1!$A$1:$I$53</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$J$437</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$J$438</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Planilha1!$A$1:$I$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2865" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2923" uniqueCount="747">
   <si>
     <t>Prioridade</t>
   </si>
@@ -2373,6 +2373,50 @@
   </si>
   <si>
     <t>BKFINR26</t>
+  </si>
+  <si>
+    <t>20/03/20</t>
+  </si>
+  <si>
+    <t>Criar campo para gravar qual usuário aprovou o pedido de compras e incluir no relatório de Pedidos e Faturamento</t>
+  </si>
+  <si>
+    <t>21/03/20</t>
+  </si>
+  <si>
+    <t>Conforme falamos, por favor tente incluir o previsto de faturamento do mês naquele relatório pedido de faturamento vs faturamento.</t>
+  </si>
+  <si>
+    <t>Relatorio de Pedidos e Faturamento: Duplicou um registro.
+A coluna saldo renomear para saldo a receber.
+Ocultar a coluna Imp. Retidos. Não preciso desta informação.
+Tem como adicionar uma coluna “nome emissor da fatura”? gostaria de saber quem da minha área emitiu a nota.</t>
+  </si>
+  <si>
+    <t>Erro ao acessar algumas empresas</t>
+  </si>
+  <si>
+    <t>13/03/20</t>
+  </si>
+  <si>
+    <t>Reindex tabela XX6 e XX7</t>
+  </si>
+  <si>
+    <t>João Pedro</t>
+  </si>
+  <si>
+    <t>Erro ao tentar aprovar a medição 041501</t>
+  </si>
+  <si>
+    <t>06/09/20</t>
+  </si>
+  <si>
+    <t>Alterações relatório Pedidos e Faturamento:
+A primeira coluna DT Emissão é a data de emissão do pedido aprovada pelo gestor? Se sim tem como colocar no cabeçalho da coluna “data emissão pedido”?
+A segunda coluna DT Emissão é a data de emissão da fatura? Se sim tem como colocar no cabeçalho da coluna “data emissão fatura”?
+Tem como adicionar uma coluna “nome emissor da fatura”? gostaria de saber quem da minha área emitiu a nota.
+Precisa por favor incluir uma coluna com o valor líquido da nota
+A coluna saldo precisa refletir o saldo liquido a receber do cliente</t>
   </si>
 </sst>
 </file>
@@ -3073,11 +3117,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J455"/>
+  <dimension ref="A1:J459"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A439" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A445" sqref="A445"/>
+      <pane ySplit="1" topLeftCell="A448" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A451" sqref="A451"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14935,21 +14979,21 @@
       </c>
       <c r="J430" s="21"/>
     </row>
-    <row r="431" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A431" s="27">
-        <v>43899</v>
+        <v>43896</v>
       </c>
       <c r="B431" s="25" t="s">
-        <v>451</v>
+        <v>743</v>
       </c>
       <c r="C431" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D431" s="20">
-        <v>320976</v>
+      <c r="D431" s="20" t="s">
+        <v>684</v>
       </c>
       <c r="E431" s="19" t="s">
-        <v>711</v>
+        <v>744</v>
       </c>
       <c r="F431" s="20" t="s">
         <v>106</v>
@@ -14958,31 +15002,31 @@
         <v>126</v>
       </c>
       <c r="H431" s="49" t="s">
-        <v>712</v>
+        <v>745</v>
       </c>
       <c r="I431" s="21" t="s">
         <v>17</v>
       </c>
       <c r="J431" s="21"/>
     </row>
-    <row r="432" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A432" s="27">
-        <v>43900</v>
+        <v>43899</v>
       </c>
       <c r="B432" s="25" t="s">
-        <v>540</v>
+        <v>451</v>
       </c>
       <c r="C432" s="19" t="s">
-        <v>98</v>
+        <v>21</v>
       </c>
       <c r="D432" s="20">
-        <v>320986</v>
+        <v>320976</v>
       </c>
       <c r="E432" s="19" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="F432" s="20" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
       <c r="G432" s="27" t="s">
         <v>126</v>
@@ -15000,19 +15044,19 @@
         <v>43900</v>
       </c>
       <c r="B433" s="25" t="s">
-        <v>526</v>
+        <v>540</v>
       </c>
       <c r="C433" s="19" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="D433" s="20">
-        <v>320988</v>
+        <v>320986</v>
       </c>
       <c r="E433" s="19" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F433" s="20" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="G433" s="27" t="s">
         <v>126</v>
@@ -15030,19 +15074,19 @@
         <v>43900</v>
       </c>
       <c r="B434" s="25" t="s">
-        <v>716</v>
+        <v>526</v>
       </c>
       <c r="C434" s="19" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D434" s="20">
-        <v>320992</v>
+        <v>320988</v>
       </c>
       <c r="E434" s="19" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="F434" s="20" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G434" s="27" t="s">
         <v>126</v>
@@ -15055,28 +15099,30 @@
       </c>
       <c r="J434" s="21"/>
     </row>
-    <row r="435" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A435" s="27">
         <v>43900</v>
       </c>
       <c r="B435" s="25" t="s">
-        <v>17</v>
+        <v>716</v>
       </c>
       <c r="C435" s="19" t="s">
-        <v>703</v>
-      </c>
-      <c r="D435" s="20"/>
+        <v>29</v>
+      </c>
+      <c r="D435" s="20">
+        <v>320992</v>
+      </c>
       <c r="E435" s="19" t="s">
-        <v>704</v>
+        <v>715</v>
       </c>
       <c r="F435" s="20" t="s">
-        <v>528</v>
+        <v>110</v>
       </c>
       <c r="G435" s="27" t="s">
         <v>126</v>
       </c>
       <c r="H435" s="49" t="s">
-        <v>722</v>
+        <v>712</v>
       </c>
       <c r="I435" s="21" t="s">
         <v>17</v>
@@ -15085,7 +15131,7 @@
     </row>
     <row r="436" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A436" s="27">
-        <v>43901</v>
+        <v>43900</v>
       </c>
       <c r="B436" s="25" t="s">
         <v>17</v>
@@ -15095,40 +15141,38 @@
       </c>
       <c r="D436" s="20"/>
       <c r="E436" s="19" t="s">
-        <v>717</v>
+        <v>704</v>
       </c>
       <c r="F436" s="20" t="s">
-        <v>86</v>
+        <v>528</v>
       </c>
       <c r="G436" s="27" t="s">
         <v>126</v>
       </c>
       <c r="H436" s="49" t="s">
-        <v>718</v>
+        <v>722</v>
       </c>
       <c r="I436" s="21" t="s">
         <v>17</v>
       </c>
       <c r="J436" s="21"/>
     </row>
-    <row r="437" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A437" s="27">
         <v>43901</v>
       </c>
       <c r="B437" s="25" t="s">
-        <v>540</v>
+        <v>17</v>
       </c>
       <c r="C437" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D437" s="20">
-        <v>320995</v>
-      </c>
+        <v>703</v>
+      </c>
+      <c r="D437" s="20"/>
       <c r="E437" s="19" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="F437" s="20" t="s">
-        <v>501</v>
+        <v>86</v>
       </c>
       <c r="G437" s="27" t="s">
         <v>126</v>
@@ -15137,55 +15181,55 @@
         <v>718</v>
       </c>
       <c r="I437" s="21" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J437" s="21"/>
     </row>
-    <row r="438" spans="1:10" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A438" s="27">
-        <v>43902</v>
+        <v>43901</v>
       </c>
       <c r="B438" s="25" t="s">
-        <v>451</v>
+        <v>540</v>
       </c>
       <c r="C438" s="19" t="s">
-        <v>720</v>
+        <v>98</v>
       </c>
       <c r="D438" s="20">
-        <v>320998</v>
+        <v>320995</v>
       </c>
       <c r="E438" s="19" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="F438" s="20" t="s">
-        <v>106</v>
+        <v>501</v>
       </c>
       <c r="G438" s="27" t="s">
         <v>126</v>
       </c>
       <c r="H438" s="49" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="I438" s="21" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J438" s="21"/>
     </row>
-    <row r="439" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:10" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A439" s="27">
         <v>43902</v>
       </c>
       <c r="B439" s="25" t="s">
-        <v>607</v>
+        <v>451</v>
       </c>
       <c r="C439" s="19" t="s">
-        <v>90</v>
+        <v>720</v>
       </c>
       <c r="D439" s="20">
-        <v>3200002</v>
+        <v>320998</v>
       </c>
       <c r="E439" s="19" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="F439" s="20" t="s">
         <v>106</v>
@@ -15201,33 +15245,37 @@
       </c>
       <c r="J439" s="21"/>
     </row>
-    <row r="440" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A440" s="27">
-        <v>43903</v>
+        <v>43902</v>
       </c>
       <c r="B440" s="25" t="s">
-        <v>435</v>
+        <v>607</v>
       </c>
       <c r="C440" s="19" t="s">
-        <v>613</v>
+        <v>90</v>
       </c>
       <c r="D440" s="20">
-        <v>320005</v>
+        <v>3200002</v>
       </c>
       <c r="E440" s="19" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="F440" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="G440" s="27"/>
-      <c r="H440" s="49"/>
-      <c r="I440" s="21"/>
-      <c r="J440" s="21" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="441" spans="1:10" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="G440" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H440" s="49" t="s">
+        <v>722</v>
+      </c>
+      <c r="I440" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J440" s="21"/>
+    </row>
+    <row r="441" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A441" s="27">
         <v>43903</v>
       </c>
@@ -15238,186 +15286,310 @@
         <v>613</v>
       </c>
       <c r="D441" s="20">
+        <v>320005</v>
+      </c>
+      <c r="E441" s="19" t="s">
+        <v>726</v>
+      </c>
+      <c r="F441" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G441" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H441" s="49" t="s">
+        <v>735</v>
+      </c>
+      <c r="I441" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J441" s="21" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="442" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A442" s="27">
+        <v>43903</v>
+      </c>
+      <c r="B442" s="25" t="s">
+        <v>435</v>
+      </c>
+      <c r="C442" s="19" t="s">
+        <v>613</v>
+      </c>
+      <c r="D442" s="20">
         <v>320009</v>
       </c>
-      <c r="E441" s="19" t="s">
+      <c r="E442" s="19" t="s">
         <v>727</v>
       </c>
-      <c r="F441" s="20" t="s">
+      <c r="F442" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="G441" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="H441" s="49" t="s">
+      <c r="G442" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H442" s="49" t="s">
         <v>728</v>
       </c>
-      <c r="I441" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J441" s="21"/>
-    </row>
-    <row r="442" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A442" s="27">
-        <v>43904</v>
-      </c>
-      <c r="B442" s="25" t="s">
-        <v>638</v>
-      </c>
-      <c r="C442" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D442" s="20"/>
-      <c r="E442" s="19" t="s">
-        <v>724</v>
-      </c>
-      <c r="F442" s="20" t="s">
-        <v>541</v>
-      </c>
-      <c r="G442" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="H442" s="49" t="s">
-        <v>725</v>
-      </c>
       <c r="I442" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J442" s="21" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="443" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J442" s="21"/>
+    </row>
+    <row r="443" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A443" s="27">
-        <v>43907</v>
+        <v>43903</v>
       </c>
       <c r="B443" s="25" t="s">
-        <v>638</v>
+        <v>244</v>
       </c>
       <c r="C443" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D443" s="20"/>
+      <c r="D443" s="20" t="s">
+        <v>684</v>
+      </c>
       <c r="E443" s="19" t="s">
-        <v>731</v>
+        <v>740</v>
       </c>
       <c r="F443" s="20" t="s">
-        <v>548</v>
+        <v>106</v>
       </c>
       <c r="G443" s="27" t="s">
         <v>126</v>
       </c>
       <c r="H443" s="49" t="s">
-        <v>732</v>
+        <v>741</v>
       </c>
       <c r="I443" s="21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J443" s="21" t="s">
-        <v>733</v>
+        <v>742</v>
       </c>
     </row>
     <row r="444" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A444" s="27">
+        <v>43904</v>
+      </c>
+      <c r="B444" s="25" t="s">
+        <v>638</v>
+      </c>
+      <c r="C444" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D444" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="E444" s="19" t="s">
+        <v>724</v>
+      </c>
+      <c r="F444" s="20" t="s">
+        <v>541</v>
+      </c>
+      <c r="G444" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H444" s="49" t="s">
+        <v>725</v>
+      </c>
+      <c r="I444" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J444" s="21" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="445" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A445" s="27">
+        <v>43907</v>
+      </c>
+      <c r="B445" s="25" t="s">
+        <v>638</v>
+      </c>
+      <c r="C445" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D445" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="E445" s="19" t="s">
+        <v>731</v>
+      </c>
+      <c r="F445" s="20" t="s">
+        <v>548</v>
+      </c>
+      <c r="G445" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H445" s="49" t="s">
+        <v>732</v>
+      </c>
+      <c r="I445" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J445" s="21" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="446" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A446" s="27">
+        <v>43907</v>
+      </c>
+      <c r="B446" s="25" t="s">
+        <v>638</v>
+      </c>
+      <c r="C446" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D446" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="E446" s="19" t="s">
+        <v>739</v>
+      </c>
+      <c r="F446" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G446" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H446" s="49" t="s">
+        <v>725</v>
+      </c>
+      <c r="I446" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J446" s="21" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="447" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A447" s="27">
+        <v>43907</v>
+      </c>
+      <c r="B447" s="25" t="s">
+        <v>638</v>
+      </c>
+      <c r="C447" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D447" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="E447" s="19" t="s">
+        <v>746</v>
+      </c>
+      <c r="F447" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G447" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H447" s="49" t="s">
+        <v>735</v>
+      </c>
+      <c r="I447" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J447" s="21" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="448" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A448" s="27">
         <v>43908</v>
       </c>
-      <c r="B444" s="25" t="s">
+      <c r="B448" s="25" t="s">
         <v>540</v>
       </c>
-      <c r="C444" s="19" t="s">
+      <c r="C448" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D444" s="20">
+      <c r="D448" s="20">
         <v>320034</v>
       </c>
-      <c r="E444" s="19" t="s">
+      <c r="E448" s="19" t="s">
         <v>730</v>
       </c>
-      <c r="F444" s="20" t="s">
+      <c r="F448" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="G444" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="H444" s="49" t="s">
+      <c r="G448" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H448" s="49" t="s">
         <v>728</v>
       </c>
-      <c r="I444" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J444" s="21"/>
-    </row>
-    <row r="445" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A445" s="27"/>
-      <c r="B445" s="25"/>
-      <c r="C445" s="19"/>
-      <c r="D445" s="20"/>
-      <c r="E445" s="19"/>
-      <c r="F445" s="20"/>
-      <c r="G445" s="27"/>
-      <c r="H445" s="49"/>
-      <c r="I445" s="21"/>
-      <c r="J445" s="21"/>
-    </row>
-    <row r="446" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A446" s="27"/>
-      <c r="B446" s="25"/>
-      <c r="C446" s="19"/>
-      <c r="D446" s="20"/>
-      <c r="E446" s="19"/>
-      <c r="F446" s="20"/>
-      <c r="G446" s="27"/>
-      <c r="H446" s="49"/>
-      <c r="I446" s="21"/>
-      <c r="J446" s="21"/>
-    </row>
-    <row r="447" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A447" s="27"/>
-      <c r="B447" s="25"/>
-      <c r="C447" s="19"/>
-      <c r="D447" s="20"/>
-      <c r="E447" s="19"/>
-      <c r="F447" s="20"/>
-      <c r="G447" s="27"/>
-      <c r="H447" s="49"/>
-      <c r="I447" s="21"/>
-      <c r="J447" s="21"/>
-    </row>
-    <row r="448" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A448" s="27"/>
-      <c r="B448" s="25"/>
-      <c r="C448" s="19"/>
-      <c r="D448" s="20"/>
-      <c r="E448" s="19"/>
-      <c r="F448" s="20"/>
-      <c r="G448" s="27"/>
-      <c r="H448" s="49"/>
-      <c r="I448" s="21"/>
+      <c r="I448" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J448" s="21"/>
     </row>
-    <row r="449" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A449" s="27"/>
-      <c r="B449" s="25"/>
-      <c r="C449" s="19"/>
-      <c r="D449" s="20"/>
-      <c r="E449" s="19"/>
-      <c r="F449" s="20"/>
-      <c r="G449" s="27"/>
-      <c r="H449" s="49"/>
-      <c r="I449" s="21"/>
-      <c r="J449" s="21"/>
-    </row>
-    <row r="450" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A450" s="27"/>
-      <c r="B450" s="25"/>
-      <c r="C450" s="19"/>
-      <c r="D450" s="20"/>
-      <c r="E450" s="19"/>
-      <c r="F450" s="20"/>
-      <c r="G450" s="27"/>
-      <c r="H450" s="49"/>
-      <c r="I450" s="21"/>
-      <c r="J450" s="21"/>
+    <row r="449" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A449" s="27">
+        <v>43909</v>
+      </c>
+      <c r="B449" s="25" t="s">
+        <v>638</v>
+      </c>
+      <c r="C449" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D449" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="E449" s="19" t="s">
+        <v>736</v>
+      </c>
+      <c r="F449" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G449" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H449" s="49" t="s">
+        <v>737</v>
+      </c>
+      <c r="I449" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J449" s="21" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="450" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A450" s="27">
+        <v>43909</v>
+      </c>
+      <c r="B450" s="25" t="s">
+        <v>638</v>
+      </c>
+      <c r="C450" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D450" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="E450" s="19" t="s">
+        <v>738</v>
+      </c>
+      <c r="F450" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="G450" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H450" s="49" t="s">
+        <v>732</v>
+      </c>
+      <c r="I450" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J450" s="21" t="s">
+        <v>734</v>
+      </c>
     </row>
     <row r="451" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A451" s="27"/>
@@ -15479,8 +15651,56 @@
       <c r="I455" s="21"/>
       <c r="J455" s="21"/>
     </row>
+    <row r="456" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A456" s="27"/>
+      <c r="B456" s="25"/>
+      <c r="C456" s="19"/>
+      <c r="D456" s="20"/>
+      <c r="E456" s="19"/>
+      <c r="F456" s="20"/>
+      <c r="G456" s="27"/>
+      <c r="H456" s="49"/>
+      <c r="I456" s="21"/>
+      <c r="J456" s="21"/>
+    </row>
+    <row r="457" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A457" s="27"/>
+      <c r="B457" s="25"/>
+      <c r="C457" s="19"/>
+      <c r="D457" s="20"/>
+      <c r="E457" s="19"/>
+      <c r="F457" s="20"/>
+      <c r="G457" s="27"/>
+      <c r="H457" s="49"/>
+      <c r="I457" s="21"/>
+      <c r="J457" s="21"/>
+    </row>
+    <row r="458" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A458" s="27"/>
+      <c r="B458" s="25"/>
+      <c r="C458" s="19"/>
+      <c r="D458" s="20"/>
+      <c r="E458" s="19"/>
+      <c r="F458" s="20"/>
+      <c r="G458" s="27"/>
+      <c r="H458" s="49"/>
+      <c r="I458" s="21"/>
+      <c r="J458" s="21"/>
+    </row>
+    <row r="459" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A459" s="27"/>
+      <c r="B459" s="25"/>
+      <c r="C459" s="19"/>
+      <c r="D459" s="20"/>
+      <c r="E459" s="19"/>
+      <c r="F459" s="20"/>
+      <c r="G459" s="27"/>
+      <c r="H459" s="49"/>
+      <c r="I459" s="21"/>
+      <c r="J459" s="21"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J437" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J438" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="79" firstPageNumber="0" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Gravar data e usuário que liberou ped de venda
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AEE6CE-B96A-4BD5-8C98-3B271A8F0909}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A41C763-89D5-4407-A9A2-C4BA9F47E9BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="0" windowWidth="19170" windowHeight="10320" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_FilterDatabase_0" localSheetId="0">Plan1!$A$1:$I$53</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$J$438</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$J$439</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Planilha1!$A$1:$I$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2923" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2947" uniqueCount="750">
   <si>
     <t>Prioridade</t>
   </si>
@@ -2378,9 +2378,6 @@
     <t>20/03/20</t>
   </si>
   <si>
-    <t>Criar campo para gravar qual usuário aprovou o pedido de compras e incluir no relatório de Pedidos e Faturamento</t>
-  </si>
-  <si>
     <t>21/03/20</t>
   </si>
   <si>
@@ -2417,6 +2414,18 @@
 Tem como adicionar uma coluna “nome emissor da fatura”? gostaria de saber quem da minha área emitiu a nota.
 Precisa por favor incluir uma coluna com o valor líquido da nota
 A coluna saldo precisa refletir o saldo liquido a receber do cliente</t>
+  </si>
+  <si>
+    <t>Criar campos para gravar data e qual usuário aprovou o pedido de compras e incluir no relatório de Pedidos e Faturamento</t>
+  </si>
+  <si>
+    <t>Criar filtro com código de Produto no relatório de Contas a Pagar com Hist. De Compras</t>
+  </si>
+  <si>
+    <t>Incluir no Relatório Diário de Contas a Pagar o portador e a forma de pgto</t>
+  </si>
+  <si>
+    <t>Verificar diferença entre Valor previsto no relatorio de Pedidos e Faturamento</t>
   </si>
 </sst>
 </file>
@@ -3117,11 +3126,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J459"/>
+  <dimension ref="A1:J461"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A448" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A451" sqref="A451"/>
+      <pane ySplit="1" topLeftCell="A451" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E454" sqref="E454"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14859,54 +14868,44 @@
       </c>
       <c r="J426" s="21"/>
     </row>
-    <row r="427" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A427" s="27">
+        <v>43889</v>
+      </c>
+      <c r="B427" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C427" s="19" t="s">
+        <v>582</v>
+      </c>
+      <c r="D427" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="E427" s="19"/>
+      <c r="F427" s="20"/>
+      <c r="G427" s="27"/>
+      <c r="H427" s="49"/>
+      <c r="I427" s="21"/>
+      <c r="J427" s="21"/>
+    </row>
+    <row r="428" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A428" s="27">
         <v>43893</v>
       </c>
-      <c r="B427" s="25" t="s">
+      <c r="B428" s="25" t="s">
         <v>623</v>
       </c>
-      <c r="C427" s="19" t="s">
+      <c r="C428" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D427" s="20">
+      <c r="D428" s="20">
         <v>320944</v>
       </c>
-      <c r="E427" s="19" t="s">
+      <c r="E428" s="19" t="s">
         <v>705</v>
       </c>
-      <c r="F427" s="20" t="s">
+      <c r="F428" s="20" t="s">
         <v>106</v>
-      </c>
-      <c r="G427" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="H427" s="49" t="s">
-        <v>706</v>
-      </c>
-      <c r="I427" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="J427" s="21"/>
-    </row>
-    <row r="428" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A428" s="27">
-        <v>43894</v>
-      </c>
-      <c r="B428" s="25" t="s">
-        <v>607</v>
-      </c>
-      <c r="C428" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="D428" s="20">
-        <v>320947</v>
-      </c>
-      <c r="E428" s="19" t="s">
-        <v>707</v>
-      </c>
-      <c r="F428" s="20" t="s">
-        <v>86</v>
       </c>
       <c r="G428" s="27" t="s">
         <v>126</v>
@@ -14919,51 +14918,51 @@
       </c>
       <c r="J428" s="21"/>
     </row>
-    <row r="429" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A429" s="27">
-        <v>43896</v>
+        <v>43894</v>
       </c>
       <c r="B429" s="25" t="s">
-        <v>62</v>
+        <v>607</v>
       </c>
       <c r="C429" s="19" t="s">
-        <v>582</v>
+        <v>90</v>
       </c>
       <c r="D429" s="20">
-        <v>320965</v>
+        <v>320947</v>
       </c>
       <c r="E429" s="19" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="F429" s="20" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="G429" s="27" t="s">
         <v>126</v>
       </c>
       <c r="H429" s="49" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="I429" s="21" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J429" s="21"/>
     </row>
-    <row r="430" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A430" s="27">
         <v>43896</v>
       </c>
       <c r="B430" s="25" t="s">
-        <v>483</v>
+        <v>62</v>
       </c>
       <c r="C430" s="19" t="s">
-        <v>90</v>
+        <v>582</v>
       </c>
       <c r="D430" s="20">
-        <v>320966</v>
+        <v>320965</v>
       </c>
       <c r="E430" s="19" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="F430" s="20" t="s">
         <v>61</v>
@@ -14984,46 +14983,46 @@
         <v>43896</v>
       </c>
       <c r="B431" s="25" t="s">
-        <v>743</v>
+        <v>483</v>
       </c>
       <c r="C431" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D431" s="20" t="s">
-        <v>684</v>
+        <v>90</v>
+      </c>
+      <c r="D431" s="20">
+        <v>320966</v>
       </c>
       <c r="E431" s="19" t="s">
-        <v>744</v>
+        <v>710</v>
       </c>
       <c r="F431" s="20" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="G431" s="27" t="s">
         <v>126</v>
       </c>
       <c r="H431" s="49" t="s">
-        <v>745</v>
+        <v>709</v>
       </c>
       <c r="I431" s="21" t="s">
         <v>17</v>
       </c>
       <c r="J431" s="21"/>
     </row>
-    <row r="432" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A432" s="27">
-        <v>43899</v>
+        <v>43896</v>
       </c>
       <c r="B432" s="25" t="s">
-        <v>451</v>
+        <v>742</v>
       </c>
       <c r="C432" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D432" s="20">
-        <v>320976</v>
+      <c r="D432" s="20" t="s">
+        <v>684</v>
       </c>
       <c r="E432" s="19" t="s">
-        <v>711</v>
+        <v>743</v>
       </c>
       <c r="F432" s="20" t="s">
         <v>106</v>
@@ -15032,31 +15031,31 @@
         <v>126</v>
       </c>
       <c r="H432" s="49" t="s">
-        <v>712</v>
+        <v>744</v>
       </c>
       <c r="I432" s="21" t="s">
         <v>17</v>
       </c>
       <c r="J432" s="21"/>
     </row>
-    <row r="433" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A433" s="27">
-        <v>43900</v>
+        <v>43899</v>
       </c>
       <c r="B433" s="25" t="s">
-        <v>540</v>
+        <v>451</v>
       </c>
       <c r="C433" s="19" t="s">
-        <v>98</v>
+        <v>21</v>
       </c>
       <c r="D433" s="20">
-        <v>320986</v>
+        <v>320976</v>
       </c>
       <c r="E433" s="19" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="F433" s="20" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
       <c r="G433" s="27" t="s">
         <v>126</v>
@@ -15074,19 +15073,19 @@
         <v>43900</v>
       </c>
       <c r="B434" s="25" t="s">
-        <v>526</v>
+        <v>540</v>
       </c>
       <c r="C434" s="19" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="D434" s="20">
-        <v>320988</v>
+        <v>320986</v>
       </c>
       <c r="E434" s="19" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F434" s="20" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="G434" s="27" t="s">
         <v>126</v>
@@ -15104,19 +15103,19 @@
         <v>43900</v>
       </c>
       <c r="B435" s="25" t="s">
-        <v>716</v>
+        <v>526</v>
       </c>
       <c r="C435" s="19" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D435" s="20">
-        <v>320992</v>
+        <v>320988</v>
       </c>
       <c r="E435" s="19" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="F435" s="20" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G435" s="27" t="s">
         <v>126</v>
@@ -15129,28 +15128,30 @@
       </c>
       <c r="J435" s="21"/>
     </row>
-    <row r="436" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A436" s="27">
         <v>43900</v>
       </c>
       <c r="B436" s="25" t="s">
-        <v>17</v>
+        <v>716</v>
       </c>
       <c r="C436" s="19" t="s">
-        <v>703</v>
-      </c>
-      <c r="D436" s="20"/>
+        <v>29</v>
+      </c>
+      <c r="D436" s="20">
+        <v>320992</v>
+      </c>
       <c r="E436" s="19" t="s">
-        <v>704</v>
+        <v>715</v>
       </c>
       <c r="F436" s="20" t="s">
-        <v>528</v>
+        <v>110</v>
       </c>
       <c r="G436" s="27" t="s">
         <v>126</v>
       </c>
       <c r="H436" s="49" t="s">
-        <v>722</v>
+        <v>712</v>
       </c>
       <c r="I436" s="21" t="s">
         <v>17</v>
@@ -15159,7 +15160,7 @@
     </row>
     <row r="437" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A437" s="27">
-        <v>43901</v>
+        <v>43900</v>
       </c>
       <c r="B437" s="25" t="s">
         <v>17</v>
@@ -15169,40 +15170,38 @@
       </c>
       <c r="D437" s="20"/>
       <c r="E437" s="19" t="s">
-        <v>717</v>
+        <v>704</v>
       </c>
       <c r="F437" s="20" t="s">
-        <v>86</v>
+        <v>528</v>
       </c>
       <c r="G437" s="27" t="s">
         <v>126</v>
       </c>
       <c r="H437" s="49" t="s">
-        <v>718</v>
+        <v>722</v>
       </c>
       <c r="I437" s="21" t="s">
         <v>17</v>
       </c>
       <c r="J437" s="21"/>
     </row>
-    <row r="438" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A438" s="27">
         <v>43901</v>
       </c>
       <c r="B438" s="25" t="s">
-        <v>540</v>
+        <v>17</v>
       </c>
       <c r="C438" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D438" s="20">
-        <v>320995</v>
-      </c>
+        <v>703</v>
+      </c>
+      <c r="D438" s="20"/>
       <c r="E438" s="19" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="F438" s="20" t="s">
-        <v>501</v>
+        <v>86</v>
       </c>
       <c r="G438" s="27" t="s">
         <v>126</v>
@@ -15211,55 +15210,55 @@
         <v>718</v>
       </c>
       <c r="I438" s="21" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J438" s="21"/>
     </row>
-    <row r="439" spans="1:10" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A439" s="27">
-        <v>43902</v>
+        <v>43901</v>
       </c>
       <c r="B439" s="25" t="s">
-        <v>451</v>
+        <v>540</v>
       </c>
       <c r="C439" s="19" t="s">
-        <v>720</v>
+        <v>98</v>
       </c>
       <c r="D439" s="20">
-        <v>320998</v>
+        <v>320995</v>
       </c>
       <c r="E439" s="19" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="F439" s="20" t="s">
-        <v>106</v>
+        <v>501</v>
       </c>
       <c r="G439" s="27" t="s">
         <v>126</v>
       </c>
       <c r="H439" s="49" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="I439" s="21" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J439" s="21"/>
     </row>
-    <row r="440" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:10" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A440" s="27">
         <v>43902</v>
       </c>
       <c r="B440" s="25" t="s">
-        <v>607</v>
+        <v>451</v>
       </c>
       <c r="C440" s="19" t="s">
-        <v>90</v>
+        <v>720</v>
       </c>
       <c r="D440" s="20">
-        <v>3200002</v>
+        <v>320998</v>
       </c>
       <c r="E440" s="19" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="F440" s="20" t="s">
         <v>106</v>
@@ -15275,39 +15274,37 @@
       </c>
       <c r="J440" s="21"/>
     </row>
-    <row r="441" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A441" s="27">
-        <v>43903</v>
+        <v>43902</v>
       </c>
       <c r="B441" s="25" t="s">
-        <v>435</v>
+        <v>607</v>
       </c>
       <c r="C441" s="19" t="s">
-        <v>613</v>
+        <v>90</v>
       </c>
       <c r="D441" s="20">
-        <v>320005</v>
+        <v>3200002</v>
       </c>
       <c r="E441" s="19" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="F441" s="20" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
       <c r="G441" s="27" t="s">
         <v>126</v>
       </c>
       <c r="H441" s="49" t="s">
-        <v>735</v>
+        <v>722</v>
       </c>
       <c r="I441" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J441" s="21" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="442" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J441" s="21"/>
+    </row>
+    <row r="442" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A442" s="27">
         <v>43903</v>
       </c>
@@ -15318,40 +15315,42 @@
         <v>613</v>
       </c>
       <c r="D442" s="20">
-        <v>320009</v>
+        <v>320005</v>
       </c>
       <c r="E442" s="19" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="F442" s="20" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="G442" s="27" t="s">
         <v>126</v>
       </c>
       <c r="H442" s="49" t="s">
-        <v>728</v>
+        <v>735</v>
       </c>
       <c r="I442" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J442" s="21"/>
+      <c r="J442" s="21" t="s">
+        <v>729</v>
+      </c>
     </row>
     <row r="443" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A443" s="27">
         <v>43903</v>
       </c>
       <c r="B443" s="25" t="s">
-        <v>244</v>
+        <v>435</v>
       </c>
       <c r="C443" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D443" s="20" t="s">
-        <v>684</v>
+        <v>613</v>
+      </c>
+      <c r="D443" s="20">
+        <v>320009</v>
       </c>
       <c r="E443" s="19" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
       <c r="F443" s="20" t="s">
         <v>106</v>
@@ -15360,21 +15359,19 @@
         <v>126</v>
       </c>
       <c r="H443" s="49" t="s">
-        <v>741</v>
+        <v>728</v>
       </c>
       <c r="I443" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J443" s="21" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="444" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J443" s="21"/>
+    </row>
+    <row r="444" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A444" s="27">
-        <v>43904</v>
+        <v>43903</v>
       </c>
       <c r="B444" s="25" t="s">
-        <v>638</v>
+        <v>244</v>
       </c>
       <c r="C444" s="19" t="s">
         <v>10</v>
@@ -15383,27 +15380,27 @@
         <v>684</v>
       </c>
       <c r="E444" s="19" t="s">
-        <v>724</v>
+        <v>739</v>
       </c>
       <c r="F444" s="20" t="s">
-        <v>541</v>
+        <v>106</v>
       </c>
       <c r="G444" s="27" t="s">
         <v>126</v>
       </c>
       <c r="H444" s="49" t="s">
-        <v>725</v>
+        <v>740</v>
       </c>
       <c r="I444" s="21" t="s">
         <v>17</v>
       </c>
       <c r="J444" s="21" t="s">
-        <v>734</v>
+        <v>741</v>
       </c>
     </row>
     <row r="445" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A445" s="27">
-        <v>43907</v>
+        <v>43904</v>
       </c>
       <c r="B445" s="25" t="s">
         <v>638</v>
@@ -15415,25 +15412,25 @@
         <v>684</v>
       </c>
       <c r="E445" s="19" t="s">
-        <v>731</v>
+        <v>724</v>
       </c>
       <c r="F445" s="20" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="G445" s="27" t="s">
         <v>126</v>
       </c>
       <c r="H445" s="49" t="s">
-        <v>732</v>
+        <v>725</v>
       </c>
       <c r="I445" s="21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J445" s="21" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="446" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="446" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A446" s="27">
         <v>43907</v>
       </c>
@@ -15447,25 +15444,25 @@
         <v>684</v>
       </c>
       <c r="E446" s="19" t="s">
-        <v>739</v>
+        <v>731</v>
       </c>
       <c r="F446" s="20" t="s">
-        <v>110</v>
+        <v>548</v>
       </c>
       <c r="G446" s="27" t="s">
         <v>126</v>
       </c>
       <c r="H446" s="49" t="s">
-        <v>725</v>
+        <v>732</v>
       </c>
       <c r="I446" s="21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J446" s="21" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="447" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A447" s="27">
         <v>43907</v>
       </c>
@@ -15479,85 +15476,85 @@
         <v>684</v>
       </c>
       <c r="E447" s="19" t="s">
-        <v>746</v>
+        <v>738</v>
       </c>
       <c r="F447" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G447" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H447" s="49" t="s">
+        <v>725</v>
+      </c>
+      <c r="I447" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J447" s="21" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="448" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A448" s="27">
+        <v>43907</v>
+      </c>
+      <c r="B448" s="25" t="s">
+        <v>638</v>
+      </c>
+      <c r="C448" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D448" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="E448" s="19" t="s">
+        <v>745</v>
+      </c>
+      <c r="F448" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="G447" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="H447" s="49" t="s">
+      <c r="G448" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H448" s="49" t="s">
         <v>735</v>
       </c>
-      <c r="I447" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J447" s="21" t="s">
+      <c r="I448" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J448" s="21" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="448" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A448" s="27">
+    <row r="449" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A449" s="27">
         <v>43908</v>
       </c>
-      <c r="B448" s="25" t="s">
+      <c r="B449" s="25" t="s">
         <v>540</v>
       </c>
-      <c r="C448" s="19" t="s">
+      <c r="C449" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="D448" s="20">
+      <c r="D449" s="20">
         <v>320034</v>
       </c>
-      <c r="E448" s="19" t="s">
+      <c r="E449" s="19" t="s">
         <v>730</v>
       </c>
-      <c r="F448" s="20" t="s">
+      <c r="F449" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="G448" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="H448" s="49" t="s">
+      <c r="G449" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H449" s="49" t="s">
         <v>728</v>
       </c>
-      <c r="I448" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J448" s="21"/>
-    </row>
-    <row r="449" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A449" s="27">
-        <v>43909</v>
-      </c>
-      <c r="B449" s="25" t="s">
-        <v>638</v>
-      </c>
-      <c r="C449" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D449" s="20" t="s">
-        <v>684</v>
-      </c>
-      <c r="E449" s="19" t="s">
-        <v>736</v>
-      </c>
-      <c r="F449" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="G449" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="H449" s="49" t="s">
-        <v>737</v>
-      </c>
       <c r="I449" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J449" s="21" t="s">
-        <v>734</v>
-      </c>
+      <c r="J449" s="21"/>
     </row>
     <row r="450" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A450" s="27">
@@ -15573,10 +15570,10 @@
         <v>684</v>
       </c>
       <c r="E450" s="19" t="s">
-        <v>738</v>
+        <v>747</v>
       </c>
       <c r="F450" s="20" t="s">
-        <v>241</v>
+        <v>110</v>
       </c>
       <c r="G450" s="27" t="s">
         <v>126</v>
@@ -15587,53 +15584,121 @@
       <c r="I450" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J450" s="21" t="s">
+      <c r="J450" s="21"/>
+    </row>
+    <row r="451" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A451" s="27">
+        <v>43909</v>
+      </c>
+      <c r="B451" s="25" t="s">
+        <v>638</v>
+      </c>
+      <c r="C451" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D451" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="E451" s="19" t="s">
+        <v>746</v>
+      </c>
+      <c r="F451" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G451" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H451" s="49" t="s">
+        <v>736</v>
+      </c>
+      <c r="I451" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J451" s="21" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="451" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A451" s="27"/>
-      <c r="B451" s="25"/>
-      <c r="C451" s="19"/>
-      <c r="D451" s="20"/>
-      <c r="E451" s="19"/>
-      <c r="F451" s="20"/>
-      <c r="G451" s="27"/>
-      <c r="H451" s="49"/>
-      <c r="I451" s="21"/>
-      <c r="J451" s="21"/>
-    </row>
-    <row r="452" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A452" s="27"/>
-      <c r="B452" s="25"/>
-      <c r="C452" s="19"/>
-      <c r="D452" s="20"/>
-      <c r="E452" s="19"/>
-      <c r="F452" s="20"/>
-      <c r="G452" s="27"/>
-      <c r="H452" s="49"/>
-      <c r="I452" s="21"/>
-      <c r="J452" s="21"/>
+    <row r="452" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A452" s="27">
+        <v>43909</v>
+      </c>
+      <c r="B452" s="25" t="s">
+        <v>638</v>
+      </c>
+      <c r="C452" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D452" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="E452" s="19" t="s">
+        <v>737</v>
+      </c>
+      <c r="F452" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="G452" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H452" s="49" t="s">
+        <v>732</v>
+      </c>
+      <c r="I452" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J452" s="21" t="s">
+        <v>734</v>
+      </c>
     </row>
     <row r="453" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A453" s="27"/>
-      <c r="B453" s="25"/>
-      <c r="C453" s="19"/>
-      <c r="D453" s="20"/>
-      <c r="E453" s="19"/>
-      <c r="F453" s="20"/>
-      <c r="G453" s="27"/>
-      <c r="H453" s="49"/>
-      <c r="I453" s="21"/>
+      <c r="A453" s="27">
+        <v>43910</v>
+      </c>
+      <c r="B453" s="25" t="s">
+        <v>638</v>
+      </c>
+      <c r="C453" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D453" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="E453" s="19" t="s">
+        <v>748</v>
+      </c>
+      <c r="F453" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G453" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H453" s="49" t="s">
+        <v>735</v>
+      </c>
+      <c r="I453" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J453" s="21"/>
     </row>
     <row r="454" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A454" s="27"/>
-      <c r="B454" s="25"/>
-      <c r="C454" s="19"/>
-      <c r="D454" s="20"/>
-      <c r="E454" s="19"/>
-      <c r="F454" s="20"/>
+      <c r="A454" s="27">
+        <v>43910</v>
+      </c>
+      <c r="B454" s="25" t="s">
+        <v>638</v>
+      </c>
+      <c r="C454" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D454" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="E454" s="19" t="s">
+        <v>749</v>
+      </c>
+      <c r="F454" s="20" t="s">
+        <v>86</v>
+      </c>
       <c r="G454" s="27"/>
       <c r="H454" s="49"/>
       <c r="I454" s="21"/>
@@ -15699,8 +15764,32 @@
       <c r="I459" s="21"/>
       <c r="J459" s="21"/>
     </row>
+    <row r="460" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A460" s="27"/>
+      <c r="B460" s="25"/>
+      <c r="C460" s="19"/>
+      <c r="D460" s="20"/>
+      <c r="E460" s="19"/>
+      <c r="F460" s="20"/>
+      <c r="G460" s="27"/>
+      <c r="H460" s="49"/>
+      <c r="I460" s="21"/>
+      <c r="J460" s="21"/>
+    </row>
+    <row r="461" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A461" s="27"/>
+      <c r="B461" s="25"/>
+      <c r="C461" s="19"/>
+      <c r="D461" s="20"/>
+      <c r="E461" s="19"/>
+      <c r="F461" s="20"/>
+      <c r="G461" s="27"/>
+      <c r="H461" s="49"/>
+      <c r="I461" s="21"/>
+      <c r="J461" s="21"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J438" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J439" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="79" firstPageNumber="0" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Alterações 26/03/20 NFs e e-mail Diego Oliveria
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1DE5BA-DE10-45E2-805C-8E289D9E6C23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83074CE-318A-439B-8A8D-F9769DDDCC99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2958" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2987" uniqueCount="762">
   <si>
     <t>Prioridade</t>
   </si>
@@ -2435,6 +2435,33 @@
   </si>
   <si>
     <t>23/03/20</t>
+  </si>
+  <si>
+    <t>WhatsApp</t>
+  </si>
+  <si>
+    <t>Considerar codigo 30 no arquivo de envio ao banco dos liquidos de folha para certos colaboradores tipo PJ</t>
+  </si>
+  <si>
+    <t>25/03/20</t>
+  </si>
+  <si>
+    <t>EFD 01/2020</t>
+  </si>
+  <si>
+    <t>Diego Oliveira</t>
+  </si>
+  <si>
+    <t>Retirar o e-mail do Diego Oliveira de todas as notificações de compras</t>
+  </si>
+  <si>
+    <t>26/03/20</t>
+  </si>
+  <si>
+    <t>Arquivo de envio de NFs a Prefeitura de SP com problemas de duplicidade e cod. De município ncorreto.</t>
+  </si>
+  <si>
+    <t>26/06/20</t>
   </si>
 </sst>
 </file>
@@ -3139,7 +3166,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A451" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E455" sqref="E455"/>
+      <selection pane="bottomLeft" activeCell="I459" sqref="I459"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15749,52 +15776,118 @@
       </c>
       <c r="J455" s="21"/>
     </row>
-    <row r="456" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A456" s="27"/>
-      <c r="B456" s="25"/>
-      <c r="C456" s="19"/>
-      <c r="D456" s="20"/>
-      <c r="E456" s="19"/>
-      <c r="F456" s="20"/>
-      <c r="G456" s="27"/>
-      <c r="H456" s="49"/>
-      <c r="I456" s="21"/>
+    <row r="456" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A456" s="27">
+        <v>43915</v>
+      </c>
+      <c r="B456" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C456" s="19" t="s">
+        <v>575</v>
+      </c>
+      <c r="D456" s="20" t="s">
+        <v>753</v>
+      </c>
+      <c r="E456" s="19" t="s">
+        <v>754</v>
+      </c>
+      <c r="F456" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G456" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H456" s="49" t="s">
+        <v>755</v>
+      </c>
+      <c r="I456" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J456" s="21"/>
     </row>
     <row r="457" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A457" s="27"/>
-      <c r="B457" s="25"/>
-      <c r="C457" s="19"/>
-      <c r="D457" s="20"/>
-      <c r="E457" s="19"/>
-      <c r="F457" s="20"/>
+      <c r="A457" s="27">
+        <v>43916</v>
+      </c>
+      <c r="B457" s="25" t="s">
+        <v>540</v>
+      </c>
+      <c r="C457" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D457" s="20" t="s">
+        <v>753</v>
+      </c>
+      <c r="E457" s="19" t="s">
+        <v>756</v>
+      </c>
+      <c r="F457" s="20" t="s">
+        <v>163</v>
+      </c>
       <c r="G457" s="27"/>
       <c r="H457" s="49"/>
       <c r="I457" s="21"/>
       <c r="J457" s="21"/>
     </row>
     <row r="458" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A458" s="27"/>
-      <c r="B458" s="25"/>
-      <c r="C458" s="19"/>
-      <c r="D458" s="20"/>
-      <c r="E458" s="19"/>
-      <c r="F458" s="20"/>
-      <c r="G458" s="27"/>
-      <c r="H458" s="49"/>
-      <c r="I458" s="21"/>
+      <c r="A458" s="27">
+        <v>43916</v>
+      </c>
+      <c r="B458" s="25" t="s">
+        <v>757</v>
+      </c>
+      <c r="C458" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D458" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="E458" s="19" t="s">
+        <v>758</v>
+      </c>
+      <c r="F458" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G458" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H458" s="49" t="s">
+        <v>759</v>
+      </c>
+      <c r="I458" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J458" s="21"/>
     </row>
-    <row r="459" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A459" s="27"/>
-      <c r="B459" s="25"/>
-      <c r="C459" s="19"/>
-      <c r="D459" s="20"/>
-      <c r="E459" s="19"/>
-      <c r="F459" s="20"/>
-      <c r="G459" s="27"/>
-      <c r="H459" s="49"/>
-      <c r="I459" s="21"/>
+    <row r="459" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A459" s="27">
+        <v>43916</v>
+      </c>
+      <c r="B459" s="25" t="s">
+        <v>623</v>
+      </c>
+      <c r="C459" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D459" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="E459" s="19" t="s">
+        <v>760</v>
+      </c>
+      <c r="F459" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G459" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H459" s="49" t="s">
+        <v>761</v>
+      </c>
+      <c r="I459" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J459" s="21"/>
     </row>
     <row r="460" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Alteração CriaTrab e BKFINR26 (N. Gestor Ped Av.)
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5263619A-2FC9-49AF-BBCF-E2B414868187}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFFE642-1403-4763-BBFB-446F03D7CFC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="750" windowWidth="19170" windowHeight="10320" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3009" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3017" uniqueCount="769">
   <si>
     <t>Prioridade</t>
   </si>
@@ -2477,6 +2477,12 @@
   </si>
   <si>
     <t>Verificar contrato 455-DRH Ambiência</t>
+  </si>
+  <si>
+    <t>Por favor verifique porque estes pedidos de faturamento filtrados não aparecem o relatório de medição nem os gestores responsáveis? Porque são pedidos avulsos, não oriundos da Gestão de Contratos, mas consigo informar o nome do Gestor do Contrato da última revisão</t>
+  </si>
+  <si>
+    <t>02/04/20</t>
   </si>
 </sst>
 </file>
@@ -3181,7 +3187,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A455" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A462" sqref="A462"/>
+      <selection pane="bottomLeft" activeCell="E463" sqref="E463"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15989,16 +15995,34 @@
       <c r="I462" s="21"/>
       <c r="J462" s="21"/>
     </row>
-    <row r="463" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A463" s="27"/>
-      <c r="B463" s="25"/>
-      <c r="C463" s="19"/>
-      <c r="D463" s="20"/>
-      <c r="E463" s="19"/>
-      <c r="F463" s="20"/>
-      <c r="G463" s="27"/>
-      <c r="H463" s="49"/>
-      <c r="I463" s="21"/>
+    <row r="463" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+      <c r="A463" s="27">
+        <v>43922</v>
+      </c>
+      <c r="B463" s="25" t="s">
+        <v>638</v>
+      </c>
+      <c r="C463" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D463" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="E463" s="19" t="s">
+        <v>767</v>
+      </c>
+      <c r="F463" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G463" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H463" s="49" t="s">
+        <v>768</v>
+      </c>
+      <c r="I463" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J463" s="21"/>
     </row>
     <row r="464" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Acertos NFs de Saída
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E93DF2F-E449-4552-804E-D28C4DA17B91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E08B99B-95A6-4A02-BF29-D68C07C207DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="630" yWindow="75" windowWidth="19170" windowHeight="10320" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3270,7 +3270,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A471" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A476" sqref="A476"/>
+      <selection pane="bottomLeft" activeCell="C477" sqref="C477"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Acerto variavel não existe aFormat
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3209DF07-AC6F-401F-BF00-5C68276CE431}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316BB33B-2908-468E-91D8-FAA46D380C01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="165" windowWidth="19170" windowHeight="10320" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="450" yWindow="510" windowWidth="19170" windowHeight="10320" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3155" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3169" uniqueCount="807">
   <si>
     <t>Prioridade</t>
   </si>
@@ -2584,6 +2584,18 @@
   </si>
   <si>
     <t>1 hjora</t>
+  </si>
+  <si>
+    <t>Alterar o lay out do Excel para as Rentabilidades</t>
+  </si>
+  <si>
+    <t>09/04//2020</t>
+  </si>
+  <si>
+    <t>Alterar o ISS da NF 000002227 da BK TER pois a alíquota foi alterada pela Prefeitura para 2%</t>
+  </si>
+  <si>
+    <t>09/04/20</t>
   </si>
 </sst>
 </file>
@@ -3287,8 +3299,8 @@
   <dimension ref="A1:J491"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A471" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E477" sqref="E477"/>
+      <pane ySplit="1" topLeftCell="A475" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A482" sqref="A482"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16633,27 +16645,57 @@
       <c r="J479" s="21"/>
     </row>
     <row r="480" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A480" s="27"/>
-      <c r="B480" s="25"/>
-      <c r="C480" s="19"/>
-      <c r="D480" s="20"/>
-      <c r="E480" s="19"/>
-      <c r="F480" s="20"/>
+      <c r="A480" s="27">
+        <v>43929</v>
+      </c>
+      <c r="B480" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C480" s="19" t="s">
+        <v>581</v>
+      </c>
+      <c r="D480" s="20" t="s">
+        <v>683</v>
+      </c>
+      <c r="E480" s="19" t="s">
+        <v>803</v>
+      </c>
+      <c r="F480" s="20" t="s">
+        <v>501</v>
+      </c>
       <c r="G480" s="27"/>
       <c r="H480" s="49"/>
       <c r="I480" s="21"/>
       <c r="J480" s="21"/>
     </row>
-    <row r="481" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A481" s="27"/>
-      <c r="B481" s="25"/>
-      <c r="C481" s="19"/>
-      <c r="D481" s="20"/>
-      <c r="E481" s="19"/>
-      <c r="F481" s="20"/>
-      <c r="G481" s="27"/>
-      <c r="H481" s="49"/>
-      <c r="I481" s="21"/>
+    <row r="481" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A481" s="27" t="s">
+        <v>804</v>
+      </c>
+      <c r="B481" s="25" t="s">
+        <v>540</v>
+      </c>
+      <c r="C481" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D481" s="20" t="s">
+        <v>683</v>
+      </c>
+      <c r="E481" s="19" t="s">
+        <v>805</v>
+      </c>
+      <c r="F481" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G481" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H481" s="49" t="s">
+        <v>806</v>
+      </c>
+      <c r="I481" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J481" s="21"/>
     </row>
     <row r="482" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Acertos diversos Rentabilidade, GeraCSV e GeraXlsx
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316BB33B-2908-468E-91D8-FAA46D380C01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D147C211-C7E0-4CE7-9967-D80D1F7016C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="510" windowWidth="19170" windowHeight="10320" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3169" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3182" uniqueCount="809">
   <si>
     <t>Prioridade</t>
   </si>
@@ -2592,10 +2592,16 @@
     <t>09/04//2020</t>
   </si>
   <si>
-    <t>Alterar o ISS da NF 000002227 da BK TER pois a alíquota foi alterada pela Prefeitura para 2%</t>
-  </si>
-  <si>
     <t>09/04/20</t>
+  </si>
+  <si>
+    <t>Problema com medição não baixada no cronograma de 12/19 do contrato 281035455</t>
+  </si>
+  <si>
+    <t>Ajuste no valor do ISS do titulo 000002227 - BKTER para R$ 193,28 para R$77,31, o mesmo esta calculando 5% sobre a nota sendo que alíquota de São Paulo para esse serviço mudou para 2%</t>
+  </si>
+  <si>
+    <t>Foram criados novos centros de custo para o Consórcio Osasco: 197.001.292, 198.001.293 e 199.001.294, assim como os centros de custo anteriores, torna-se necessária a conversão dos valores referentes a faturamento e custos de 50% para 100% em todos os relatórios.</t>
   </si>
 </sst>
 </file>
@@ -3296,11 +3302,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J491"/>
+  <dimension ref="A1:J492"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A475" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A482" sqref="A482"/>
+      <pane ySplit="1" topLeftCell="A477" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A484" sqref="A484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16668,58 +16674,88 @@
       <c r="I480" s="21"/>
       <c r="J480" s="21"/>
     </row>
-    <row r="481" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A481" s="27" t="s">
-        <v>804</v>
+    <row r="481" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+      <c r="A481" s="27">
+        <v>43929</v>
       </c>
       <c r="B481" s="25" t="s">
-        <v>540</v>
+        <v>62</v>
       </c>
       <c r="C481" s="19" t="s">
-        <v>98</v>
+        <v>581</v>
       </c>
       <c r="D481" s="20" t="s">
         <v>683</v>
       </c>
       <c r="E481" s="19" t="s">
+        <v>808</v>
+      </c>
+      <c r="F481" s="20"/>
+      <c r="G481" s="27"/>
+      <c r="H481" s="49"/>
+      <c r="I481" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J481" s="21"/>
+    </row>
+    <row r="482" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A482" s="27" t="s">
+        <v>804</v>
+      </c>
+      <c r="B482" s="25" t="s">
+        <v>540</v>
+      </c>
+      <c r="C482" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D482" s="20" t="s">
+        <v>683</v>
+      </c>
+      <c r="E482" s="19" t="s">
+        <v>807</v>
+      </c>
+      <c r="F482" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G482" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H482" s="49" t="s">
         <v>805</v>
       </c>
-      <c r="F481" s="20" t="s">
+      <c r="I482" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J482" s="21"/>
+    </row>
+    <row r="483" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A483" s="27">
+        <v>43930</v>
+      </c>
+      <c r="B483" s="25" t="s">
+        <v>422</v>
+      </c>
+      <c r="C483" s="19" t="s">
+        <v>775</v>
+      </c>
+      <c r="D483" s="20" t="s">
+        <v>683</v>
+      </c>
+      <c r="E483" s="19" t="s">
+        <v>806</v>
+      </c>
+      <c r="F483" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="G481" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="H481" s="49" t="s">
-        <v>806</v>
-      </c>
-      <c r="I481" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J481" s="21"/>
-    </row>
-    <row r="482" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A482" s="27"/>
-      <c r="B482" s="25"/>
-      <c r="C482" s="19"/>
-      <c r="D482" s="20"/>
-      <c r="E482" s="19"/>
-      <c r="F482" s="20"/>
-      <c r="G482" s="27"/>
-      <c r="H482" s="49"/>
-      <c r="I482" s="21"/>
-      <c r="J482" s="21"/>
-    </row>
-    <row r="483" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A483" s="27"/>
-      <c r="B483" s="25"/>
-      <c r="C483" s="19"/>
-      <c r="D483" s="20"/>
-      <c r="E483" s="19"/>
-      <c r="F483" s="20"/>
-      <c r="G483" s="27"/>
-      <c r="H483" s="49"/>
-      <c r="I483" s="21"/>
+      <c r="G483" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H483" s="49" t="s">
+        <v>805</v>
+      </c>
+      <c r="I483" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J483" s="21"/>
     </row>
     <row r="484" spans="1:10" x14ac:dyDescent="0.25">
@@ -16806,7 +16842,7 @@
       <c r="I490" s="21"/>
       <c r="J490" s="21"/>
     </row>
-    <row r="491" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A491" s="27"/>
       <c r="B491" s="25"/>
       <c r="C491" s="19"/>
@@ -16817,6 +16853,18 @@
       <c r="H491" s="49"/>
       <c r="I491" s="21"/>
       <c r="J491" s="21"/>
+    </row>
+    <row r="492" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A492" s="27"/>
+      <c r="B492" s="25"/>
+      <c r="C492" s="19"/>
+      <c r="D492" s="20"/>
+      <c r="E492" s="19"/>
+      <c r="F492" s="20"/>
+      <c r="G492" s="27"/>
+      <c r="H492" s="49"/>
+      <c r="I492" s="21"/>
+      <c r="J492" s="21"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J476" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Aleração nos rel de rent 19x00129x e Parame.Plan.
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D147C211-C7E0-4CE7-9967-D80D1F7016C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0021B2A-1477-4FEF-A4CB-A548009D7218}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_FilterDatabase_0" localSheetId="0">Plan1!$A$1:$I$53</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$J$476</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$J$485</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Planilha1!$A$1:$I$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3182" uniqueCount="809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3212" uniqueCount="816">
   <si>
     <t>Prioridade</t>
   </si>
@@ -2602,6 +2602,27 @@
   </si>
   <si>
     <t>Foram criados novos centros de custo para o Consórcio Osasco: 197.001.292, 198.001.293 e 199.001.294, assim como os centros de custo anteriores, torna-se necessária a conversão dos valores referentes a faturamento e custos de 50% para 100% em todos os relatórios.</t>
+  </si>
+  <si>
+    <t>Solicitação de emissão do relatório de contas a receber com database em 31/03/20</t>
+  </si>
+  <si>
+    <t>13/04/20</t>
+  </si>
+  <si>
+    <t>12/04/20</t>
+  </si>
+  <si>
+    <t>Opção não disponível na versão 12.1.25</t>
+  </si>
+  <si>
+    <t>Enviar passo-a-passo para cadastro de bancos</t>
+  </si>
+  <si>
+    <t>13/042020</t>
+  </si>
+  <si>
+    <t>Verificação de IR Retido em dez/2019 para o cliente Bradesco Saude na empresa BK Corretora - Valor abaixo de R$ 10,00 foi devidamente retido porque a soma dos Irs retido do período ultrapassaram R$ 10,00</t>
   </si>
 </sst>
 </file>
@@ -3302,11 +3323,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J492"/>
+  <dimension ref="A1:J493"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A477" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A484" sqref="A484"/>
+      <pane ySplit="1" topLeftCell="A478" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A487" sqref="A487"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14809,14 +14830,20 @@
         <v>684</v>
       </c>
       <c r="F418" s="20" t="s">
-        <v>528</v>
-      </c>
-      <c r="G418" s="27"/>
+        <v>86</v>
+      </c>
+      <c r="G418" s="27" t="s">
+        <v>126</v>
+      </c>
       <c r="H418" s="49" t="s">
-        <v>764</v>
-      </c>
-      <c r="I418" s="21"/>
-      <c r="J418" s="21"/>
+        <v>810</v>
+      </c>
+      <c r="I418" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J418" s="21" t="s">
+        <v>812</v>
+      </c>
     </row>
     <row r="419" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A419" s="27">
@@ -16652,29 +16679,35 @@
     </row>
     <row r="480" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A480" s="27">
-        <v>43929</v>
+        <v>43928</v>
       </c>
       <c r="B480" s="25" t="s">
-        <v>62</v>
+        <v>483</v>
       </c>
       <c r="C480" s="19" t="s">
-        <v>581</v>
-      </c>
-      <c r="D480" s="20" t="s">
-        <v>683</v>
+        <v>90</v>
+      </c>
+      <c r="D480" s="20">
+        <v>420344</v>
       </c>
       <c r="E480" s="19" t="s">
-        <v>803</v>
+        <v>813</v>
       </c>
       <c r="F480" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="G480" s="27"/>
-      <c r="H480" s="49"/>
-      <c r="I480" s="21"/>
+        <v>106</v>
+      </c>
+      <c r="G480" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H480" s="49" t="s">
+        <v>810</v>
+      </c>
+      <c r="I480" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J480" s="21"/>
     </row>
-    <row r="481" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A481" s="27">
         <v>43929</v>
       </c>
@@ -16688,61 +16721,61 @@
         <v>683</v>
       </c>
       <c r="E481" s="19" t="s">
-        <v>808</v>
-      </c>
-      <c r="F481" s="20"/>
-      <c r="G481" s="27"/>
-      <c r="H481" s="49"/>
+        <v>803</v>
+      </c>
+      <c r="F481" s="20" t="s">
+        <v>501</v>
+      </c>
+      <c r="G481" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H481" s="49" t="s">
+        <v>811</v>
+      </c>
       <c r="I481" s="21" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J481" s="21"/>
     </row>
-    <row r="482" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A482" s="27" t="s">
-        <v>804</v>
+    <row r="482" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+      <c r="A482" s="27">
+        <v>43929</v>
       </c>
       <c r="B482" s="25" t="s">
-        <v>540</v>
+        <v>62</v>
       </c>
       <c r="C482" s="19" t="s">
-        <v>98</v>
+        <v>581</v>
       </c>
       <c r="D482" s="20" t="s">
         <v>683</v>
       </c>
       <c r="E482" s="19" t="s">
-        <v>807</v>
-      </c>
-      <c r="F482" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="G482" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="H482" s="49" t="s">
-        <v>805</v>
-      </c>
+        <v>808</v>
+      </c>
+      <c r="F482" s="20"/>
+      <c r="G482" s="27"/>
+      <c r="H482" s="49"/>
       <c r="I482" s="21" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J482" s="21"/>
     </row>
-    <row r="483" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A483" s="27">
-        <v>43930</v>
+    <row r="483" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A483" s="27" t="s">
+        <v>804</v>
       </c>
       <c r="B483" s="25" t="s">
-        <v>422</v>
+        <v>540</v>
       </c>
       <c r="C483" s="19" t="s">
-        <v>775</v>
+        <v>98</v>
       </c>
       <c r="D483" s="20" t="s">
         <v>683</v>
       </c>
       <c r="E483" s="19" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="F483" s="20" t="s">
         <v>106</v>
@@ -16758,40 +16791,94 @@
       </c>
       <c r="J483" s="21"/>
     </row>
-    <row r="484" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A484" s="27"/>
-      <c r="B484" s="25"/>
-      <c r="C484" s="19"/>
-      <c r="D484" s="20"/>
-      <c r="E484" s="19"/>
-      <c r="F484" s="20"/>
-      <c r="G484" s="27"/>
-      <c r="H484" s="49"/>
-      <c r="I484" s="21"/>
+    <row r="484" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A484" s="27">
+        <v>43930</v>
+      </c>
+      <c r="B484" s="25" t="s">
+        <v>422</v>
+      </c>
+      <c r="C484" s="19" t="s">
+        <v>775</v>
+      </c>
+      <c r="D484" s="20" t="s">
+        <v>683</v>
+      </c>
+      <c r="E484" s="19" t="s">
+        <v>806</v>
+      </c>
+      <c r="F484" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G484" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H484" s="49" t="s">
+        <v>805</v>
+      </c>
+      <c r="I484" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J484" s="21"/>
     </row>
     <row r="485" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A485" s="27"/>
-      <c r="B485" s="25"/>
-      <c r="C485" s="19"/>
-      <c r="D485" s="20"/>
-      <c r="E485" s="19"/>
-      <c r="F485" s="20"/>
-      <c r="G485" s="27"/>
-      <c r="H485" s="49"/>
-      <c r="I485" s="21"/>
+      <c r="A485" s="27" t="s">
+        <v>814</v>
+      </c>
+      <c r="B485" s="25" t="s">
+        <v>637</v>
+      </c>
+      <c r="C485" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D485" s="20" t="s">
+        <v>752</v>
+      </c>
+      <c r="E485" s="19" t="s">
+        <v>809</v>
+      </c>
+      <c r="F485" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G485" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H485" s="49" t="s">
+        <v>810</v>
+      </c>
+      <c r="I485" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J485" s="21"/>
     </row>
-    <row r="486" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A486" s="27"/>
-      <c r="B486" s="25"/>
-      <c r="C486" s="19"/>
-      <c r="D486" s="20"/>
-      <c r="E486" s="19"/>
-      <c r="F486" s="20"/>
-      <c r="G486" s="27"/>
-      <c r="H486" s="49"/>
-      <c r="I486" s="21"/>
+    <row r="486" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A486" s="27">
+        <v>43934</v>
+      </c>
+      <c r="B486" s="25" t="s">
+        <v>540</v>
+      </c>
+      <c r="C486" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D486" s="20" t="s">
+        <v>752</v>
+      </c>
+      <c r="E486" s="19" t="s">
+        <v>815</v>
+      </c>
+      <c r="F486" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G486" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H486" s="49" t="s">
+        <v>810</v>
+      </c>
+      <c r="I486" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J486" s="21"/>
     </row>
     <row r="487" spans="1:10" x14ac:dyDescent="0.25">
@@ -16854,7 +16941,7 @@
       <c r="I491" s="21"/>
       <c r="J491" s="21"/>
     </row>
-    <row r="492" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A492" s="27"/>
       <c r="B492" s="25"/>
       <c r="C492" s="19"/>
@@ -16866,8 +16953,20 @@
       <c r="I492" s="21"/>
       <c r="J492" s="21"/>
     </row>
+    <row r="493" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A493" s="27"/>
+      <c r="B493" s="25"/>
+      <c r="C493" s="19"/>
+      <c r="D493" s="20"/>
+      <c r="E493" s="19"/>
+      <c r="F493" s="20"/>
+      <c r="G493" s="27"/>
+      <c r="H493" s="49"/>
+      <c r="I493" s="21"/>
+      <c r="J493" s="21"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J476" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J485" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="79" firstPageNumber="0" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Comparar para criar Graficos em Xlsx
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7714B7AC-8C65-420B-8450-E0174B2A8FF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFFD8DE-5A04-4667-AF86-B159BF6947CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3270" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3286" uniqueCount="832">
   <si>
     <t>Prioridade</t>
   </si>
@@ -2659,6 +2659,18 @@
   </si>
   <si>
     <t>Incluir colunas de bancos de recebimento das baixas mais outras diversas alterações solicitadas nos dia 1,16 e 17/04/20</t>
+  </si>
+  <si>
+    <t>Telefone</t>
+  </si>
+  <si>
+    <t>Inclusão do campo "Cliente não Reteve" no mapa de INSS Retido</t>
+  </si>
+  <si>
+    <t>20/04/20</t>
+  </si>
+  <si>
+    <t>Inclusão de mais um banco no Relatório de Pedidos e Faturamento</t>
   </si>
 </sst>
 </file>
@@ -3363,7 +3375,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A485" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A494" sqref="A494"/>
+      <selection pane="bottomLeft" activeCell="A496" sqref="A496"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17132,27 +17144,63 @@
       <c r="J493" s="21"/>
     </row>
     <row r="494" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A494" s="27"/>
-      <c r="B494" s="25"/>
-      <c r="C494" s="19"/>
-      <c r="D494" s="20"/>
-      <c r="E494" s="19"/>
-      <c r="F494" s="20"/>
-      <c r="G494" s="27"/>
-      <c r="H494" s="49"/>
-      <c r="I494" s="21"/>
+      <c r="A494" s="27">
+        <v>43938</v>
+      </c>
+      <c r="B494" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C494" s="19" t="s">
+        <v>581</v>
+      </c>
+      <c r="D494" s="20" t="s">
+        <v>828</v>
+      </c>
+      <c r="E494" s="19" t="s">
+        <v>829</v>
+      </c>
+      <c r="F494" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G494" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H494" s="49" t="s">
+        <v>830</v>
+      </c>
+      <c r="I494" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J494" s="21"/>
     </row>
     <row r="495" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A495" s="27"/>
-      <c r="B495" s="25"/>
-      <c r="C495" s="19"/>
-      <c r="D495" s="20"/>
-      <c r="E495" s="19"/>
-      <c r="F495" s="20"/>
-      <c r="G495" s="27"/>
-      <c r="H495" s="49"/>
-      <c r="I495" s="21"/>
+      <c r="A495" s="27">
+        <v>43941</v>
+      </c>
+      <c r="B495" s="25" t="s">
+        <v>637</v>
+      </c>
+      <c r="C495" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D495" s="20" t="s">
+        <v>683</v>
+      </c>
+      <c r="E495" s="19" t="s">
+        <v>831</v>
+      </c>
+      <c r="F495" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G495" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H495" s="49" t="s">
+        <v>830</v>
+      </c>
+      <c r="I495" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="J495" s="21"/>
     </row>
     <row r="496" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tela para visualizar ND no GCT
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48BEF07-091E-4779-8E8E-FA68C7B61358}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26C34F1-0F33-42EC-BC29-9AE7700C4992}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3331" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3346" uniqueCount="782">
   <si>
     <t>Prioridade</t>
   </si>
@@ -2457,7 +2457,61 @@
     <t>Acima</t>
   </si>
   <si>
-    <t>Relação de filiais a sere criadas:
+    <t>Alteração na validação do campo "Valor Licitado" na solicitação de compras, para não validar quando for digitado pelo almoxarifado, neste caso, gravando valor zero.</t>
+  </si>
+  <si>
+    <t>Acerto na planilha do contrato DAESP Presidente Prudente - Solicitado pelos Sr. João da Gestão e verificação das planilhas de SJ do R Preto e Sorocaba</t>
+  </si>
+  <si>
+    <t>Verificação de Problema com Nota Fiscal devido a medição ter sido feita em moeda 4</t>
+  </si>
+  <si>
+    <t>Verificação de problemas com o cliente Fundação Parque Zoologico: Foi verificado falta de preenchimento de alguns campos. Alterado o dicionário de dados para tornar os campos de retenção de impostos do cadastro de clientes obrigatorios em todas as empresas.</t>
+  </si>
+  <si>
+    <t>Alterado o dicionário de todas as empreas</t>
+  </si>
+  <si>
+    <t>Manipulação em base de dados</t>
+  </si>
+  <si>
+    <t>Ponto de Entrada/MT110LOK.prw</t>
+  </si>
+  <si>
+    <t>Problema com importação de arquivo VT: usuario estava utilizando arquivo incorreto</t>
+  </si>
+  <si>
+    <t>Reabertura de periodo fiscal dese de janeiro/20</t>
+  </si>
+  <si>
+    <t>Configurar livros fiscais e EFD para Empresa BKTER</t>
+  </si>
+  <si>
+    <t>Acertar valor do ISS para a NF 2229 da BKTER, pois estava configurado 5% mas a prefeitura alterou para 2%.</t>
+  </si>
+  <si>
+    <t>BK</t>
+  </si>
+  <si>
+    <t>Geração dos dados REINF empresa BK Março e Balsa Nova e consolidação dos DADOS para envio e fechamento do período do REINF</t>
+  </si>
+  <si>
+    <t>Continuação geração dos dados REINF empresa BK Março e Balsa Nova e consolidação dos DADOS para envio e fechamento do período do REINF. Reinstalação do Integrador do REINF ao governo, devido ao erro de acesso na maquina VMSIGA12, foi transferido para outra maquina</t>
+  </si>
+  <si>
+    <t>Atualização e implementação do TSS para emissão do REINF conforme documentação Totvs</t>
+  </si>
+  <si>
+    <t>Emitir razão contabil em Excel os relatórios razão das contas do grupo 1.1.1.02 (bancos), de 01/01/2015 a 31/12/2019</t>
+  </si>
+  <si>
+    <t>Gerar medição zerada para os contratos 258000430, 258000432 e 227000494 - mês 04/2020</t>
+  </si>
+  <si>
+    <t>Integração Rubi-Microsiga de titulo Pensão Rescisão</t>
+  </si>
+  <si>
+    <t>Relação de filiais a serem criadas:
 03.022.122/0005-09 – Brasília - DF
 03.022.122/0006-81 – Rio de janeiro - RJ
 03.022.122/0007-62 – Salvador - BA
@@ -2473,58 +2527,16 @@
 03.022.122/0017-34 - RIO DAS OSTRAS - RJ</t>
   </si>
   <si>
-    <t>Alteração na validação do campo "Valor Licitado" na solicitação de compras, para não validar quando for digitado pelo almoxarifado, neste caso, gravando valor zero.</t>
-  </si>
-  <si>
-    <t>Acerto na planilha do contrato DAESP Presidente Prudente - Solicitado pelos Sr. João da Gestão e verificação das planilhas de SJ do R Preto e Sorocaba</t>
-  </si>
-  <si>
-    <t>Verificação de Problema com Nota Fiscal devido a medição ter sido feita em moeda 4</t>
-  </si>
-  <si>
-    <t>Verificação de problemas com o cliente Fundação Parque Zoologico: Foi verificado falta de preenchimento de alguns campos. Alterado o dicionário de dados para tornar os campos de retenção de impostos do cadastro de clientes obrigatorios em todas as empresas.</t>
-  </si>
-  <si>
-    <t>Alterado o dicionário de todas as empreas</t>
-  </si>
-  <si>
-    <t>Manipulação em base de dados</t>
-  </si>
-  <si>
-    <t>Ponto de Entrada/MT110LOK.prw</t>
-  </si>
-  <si>
-    <t>Problema com importação de arquivo VT: usuario estava utilizando arquivo incorreto</t>
-  </si>
-  <si>
-    <t>Reabertura de periodo fiscal dese de janeiro/20</t>
-  </si>
-  <si>
-    <t>Configurar livros fiscais e EFD para Empresa BKTER</t>
-  </si>
-  <si>
-    <t>Acertar valor do ISS para a NF 2229 da BKTER, pois estava configurado 5% mas a prefeitura alterou para 2%.</t>
-  </si>
-  <si>
-    <t>BK</t>
-  </si>
-  <si>
-    <t>Geração dos dados REINF empresa BK Março e Balsa Nova e consolidação dos DADOS para envio e fechamento do período do REINF</t>
-  </si>
-  <si>
-    <t>Continuação geração dos dados REINF empresa BK Março e Balsa Nova e consolidação dos DADOS para envio e fechamento do período do REINF. Reinstalação do Integrador do REINF ao governo, devido ao erro de acesso na maquina VMSIGA12, foi transferido para outra maquina</t>
-  </si>
-  <si>
-    <t>Atualização e implementação do TSS para emissão do REINF conforme documentação Totvs</t>
-  </si>
-  <si>
-    <t>Emitir razão contabil em Excel os relatórios razão das contas do grupo 1.1.1.02 (bancos), de 01/01/2015 a 31/12/2019</t>
-  </si>
-  <si>
-    <t>Gerar medição zerada para os contratos 258000430, 258000432 e 227000494 - mês 04/2020</t>
-  </si>
-  <si>
-    <t>Integração Rubi-Microsiga de titulo Pensão Rescisão</t>
+    <t>Acerto de erro na rotina de impressão de dados de usuários</t>
+  </si>
+  <si>
+    <t>AcessoUser</t>
+  </si>
+  <si>
+    <t>Bruno</t>
+  </si>
+  <si>
+    <t>Acerto na tela de cadastramento de Notas de Débito</t>
   </si>
 </sst>
 </file>
@@ -3234,11 +3246,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J530"/>
+  <dimension ref="A1:J531"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A522" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E523" sqref="E523"/>
+      <pane ySplit="1" topLeftCell="A521" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A529" sqref="A529"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15377,7 +15389,7 @@
         <v>645</v>
       </c>
       <c r="D437" s="19" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E437" s="18" t="s">
         <v>656</v>
@@ -16752,7 +16764,7 @@
         <v>630</v>
       </c>
       <c r="E482" s="18" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="F482" s="19" t="s">
         <v>498</v>
@@ -16899,7 +16911,7 @@
         <v>645</v>
       </c>
       <c r="D487" s="19" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E487" s="18" t="s">
         <v>727</v>
@@ -17022,7 +17034,7 @@
         <v>630</v>
       </c>
       <c r="E491" s="18" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="F491" s="19" t="s">
         <v>498</v>
@@ -17322,7 +17334,7 @@
         <v>711</v>
       </c>
       <c r="E501" s="18" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="F501" s="19" t="s">
         <v>61</v>
@@ -17720,7 +17732,7 @@
         <v>755</v>
       </c>
       <c r="E515" s="56" t="s">
-        <v>759</v>
+        <v>777</v>
       </c>
       <c r="F515" s="19" t="s">
         <v>758</v>
@@ -17746,7 +17758,7 @@
         <v>755</v>
       </c>
       <c r="E516" s="18" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="F516" s="19" t="s">
         <v>110</v>
@@ -17776,7 +17788,7 @@
         <v>755</v>
       </c>
       <c r="E517" s="18" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="F517" s="19" t="s">
         <v>86</v>
@@ -17791,7 +17803,7 @@
         <v>17</v>
       </c>
       <c r="J517" s="20" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="518" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -17808,7 +17820,7 @@
         <v>755</v>
       </c>
       <c r="E518" s="18" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="F518" s="19" t="s">
         <v>86</v>
@@ -17823,7 +17835,7 @@
         <v>17</v>
       </c>
       <c r="J518" s="20" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="519" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -17840,7 +17852,7 @@
         <v>681</v>
       </c>
       <c r="E519" s="18" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="F519" s="19" t="s">
         <v>106</v>
@@ -17855,7 +17867,7 @@
         <v>17</v>
       </c>
       <c r="J519" s="20" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="520" spans="1:10" x14ac:dyDescent="0.25">
@@ -17872,7 +17884,7 @@
         <v>755</v>
       </c>
       <c r="E520" s="18" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F520" s="19" t="s">
         <v>106</v>
@@ -17904,7 +17916,7 @@
         <v>755</v>
       </c>
       <c r="E521" s="18" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="F521" s="19" t="s">
         <v>106</v>
@@ -17934,7 +17946,7 @@
         <v>755</v>
       </c>
       <c r="E522" s="18" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="F522" s="19" t="s">
         <v>110</v>
@@ -17949,7 +17961,7 @@
         <v>17</v>
       </c>
       <c r="J522" s="20" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="523" spans="1:10" x14ac:dyDescent="0.25">
@@ -17966,7 +17978,7 @@
         <v>681</v>
       </c>
       <c r="E523" s="18" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="F523" s="19" t="s">
         <v>61</v>
@@ -17990,7 +18002,7 @@
         <v>755</v>
       </c>
       <c r="E524" s="18" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="F524" s="19" t="s">
         <v>106</v>
@@ -18020,7 +18032,7 @@
         <v>630</v>
       </c>
       <c r="E525" s="18" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="F525" s="19" t="s">
         <v>110</v>
@@ -18050,7 +18062,7 @@
         <v>681</v>
       </c>
       <c r="E526" s="18" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="F526" s="19" t="s">
         <v>86</v>
@@ -18067,28 +18079,66 @@
       <c r="J526" s="20"/>
     </row>
     <row r="527" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A527" s="26"/>
-      <c r="B527" s="24"/>
-      <c r="C527" s="18"/>
-      <c r="D527" s="19"/>
-      <c r="E527" s="18"/>
-      <c r="F527" s="19"/>
-      <c r="G527" s="26"/>
-      <c r="H527" s="6"/>
-      <c r="I527" s="20"/>
+      <c r="A527" s="26">
+        <v>43958</v>
+      </c>
+      <c r="B527" s="24" t="s">
+        <v>780</v>
+      </c>
+      <c r="C527" s="18" t="s">
+        <v>696</v>
+      </c>
+      <c r="D527" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="E527" s="18" t="s">
+        <v>781</v>
+      </c>
+      <c r="F527" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G527" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H527" s="6">
+        <v>43958</v>
+      </c>
+      <c r="I527" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J527" s="20"/>
     </row>
     <row r="528" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A528" s="26"/>
-      <c r="B528" s="24"/>
-      <c r="C528" s="18"/>
-      <c r="D528" s="19"/>
-      <c r="E528" s="18"/>
-      <c r="F528" s="19"/>
-      <c r="G528" s="26"/>
-      <c r="H528" s="6"/>
-      <c r="I528" s="20"/>
-      <c r="J528" s="20"/>
+      <c r="A528" s="26">
+        <v>43959</v>
+      </c>
+      <c r="B528" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C528" s="18" t="s">
+        <v>645</v>
+      </c>
+      <c r="D528" s="19" t="s">
+        <v>770</v>
+      </c>
+      <c r="E528" s="18" t="s">
+        <v>778</v>
+      </c>
+      <c r="F528" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G528" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H528" s="6">
+        <v>43959</v>
+      </c>
+      <c r="I528" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J528" s="20" t="s">
+        <v>779</v>
+      </c>
     </row>
     <row r="529" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A529" s="26"/>
@@ -18113,6 +18163,18 @@
       <c r="H530" s="6"/>
       <c r="I530" s="20"/>
       <c r="J530" s="20"/>
+    </row>
+    <row r="531" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A531" s="26"/>
+      <c r="B531" s="24"/>
+      <c r="C531" s="18"/>
+      <c r="D531" s="19"/>
+      <c r="E531" s="18"/>
+      <c r="F531" s="19"/>
+      <c r="G531" s="26"/>
+      <c r="H531" s="6"/>
+      <c r="I531" s="20"/>
+      <c r="J531" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J524" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Adequação de relatórios para as novas filiais
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2260553-5441-448D-B4C0-5E46176EB1C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA85DF7E-FCFB-448C-AF0E-6BD79F22336D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3354" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3361" uniqueCount="785">
   <si>
     <t>Prioridade</t>
   </si>
@@ -2543,6 +2543,9 @@
   </si>
   <si>
     <t>BKGCTA21</t>
+  </si>
+  <si>
+    <t>Aplicação de patch de atualização 20-04-30_ATUALIZACAO_12.1.25_GCT_EXPEDICAO_CONTINUA_TTTP12_LG - Gestão de Contratos</t>
   </si>
 </sst>
 </file>
@@ -3252,11 +3255,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J531"/>
+  <dimension ref="A1:J537"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A521" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J530" sqref="J530"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A523" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A530" sqref="A530"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18178,16 +18181,34 @@
         <v>783</v>
       </c>
     </row>
-    <row r="530" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A530" s="26"/>
-      <c r="B530" s="24"/>
-      <c r="C530" s="18"/>
-      <c r="D530" s="19"/>
-      <c r="E530" s="18"/>
-      <c r="F530" s="19"/>
-      <c r="G530" s="26"/>
-      <c r="H530" s="6"/>
-      <c r="I530" s="20"/>
+    <row r="530" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A530" s="26">
+        <v>43966</v>
+      </c>
+      <c r="B530" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C530" s="18" t="s">
+        <v>645</v>
+      </c>
+      <c r="D530" s="19" t="s">
+        <v>711</v>
+      </c>
+      <c r="E530" s="18" t="s">
+        <v>784</v>
+      </c>
+      <c r="F530" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G530" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H530" s="6">
+        <v>43966</v>
+      </c>
+      <c r="I530" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J530" s="20"/>
     </row>
     <row r="531" spans="1:10" x14ac:dyDescent="0.25">
@@ -18201,6 +18222,78 @@
       <c r="H531" s="6"/>
       <c r="I531" s="20"/>
       <c r="J531" s="20"/>
+    </row>
+    <row r="532" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A532" s="26"/>
+      <c r="B532" s="24"/>
+      <c r="C532" s="18"/>
+      <c r="D532" s="19"/>
+      <c r="E532" s="18"/>
+      <c r="F532" s="19"/>
+      <c r="G532" s="26"/>
+      <c r="H532" s="6"/>
+      <c r="I532" s="20"/>
+      <c r="J532" s="20"/>
+    </row>
+    <row r="533" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A533" s="26"/>
+      <c r="B533" s="24"/>
+      <c r="C533" s="18"/>
+      <c r="D533" s="19"/>
+      <c r="E533" s="18"/>
+      <c r="F533" s="19"/>
+      <c r="G533" s="26"/>
+      <c r="H533" s="6"/>
+      <c r="I533" s="20"/>
+      <c r="J533" s="20"/>
+    </row>
+    <row r="534" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A534" s="26"/>
+      <c r="B534" s="24"/>
+      <c r="C534" s="18"/>
+      <c r="D534" s="19"/>
+      <c r="E534" s="18"/>
+      <c r="F534" s="19"/>
+      <c r="G534" s="26"/>
+      <c r="H534" s="6"/>
+      <c r="I534" s="20"/>
+      <c r="J534" s="20"/>
+    </row>
+    <row r="535" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A535" s="26"/>
+      <c r="B535" s="24"/>
+      <c r="C535" s="18"/>
+      <c r="D535" s="19"/>
+      <c r="E535" s="18"/>
+      <c r="F535" s="19"/>
+      <c r="G535" s="26"/>
+      <c r="H535" s="6"/>
+      <c r="I535" s="20"/>
+      <c r="J535" s="20"/>
+    </row>
+    <row r="536" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A536" s="26"/>
+      <c r="B536" s="24"/>
+      <c r="C536" s="18"/>
+      <c r="D536" s="19"/>
+      <c r="E536" s="18"/>
+      <c r="F536" s="19"/>
+      <c r="G536" s="26"/>
+      <c r="H536" s="6"/>
+      <c r="I536" s="20"/>
+      <c r="J536" s="20"/>
+    </row>
+    <row r="537" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A537" s="26"/>
+      <c r="B537" s="24"/>
+      <c r="C537" s="18"/>
+      <c r="D537" s="19"/>
+      <c r="E537" s="18"/>
+      <c r="F537" s="19"/>
+      <c r="G537" s="26"/>
+      <c r="H537" s="6"/>
+      <c r="I537" s="20"/>
+      <c r="J537" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J524" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Ponte de entrada para alterar campos de venc SE2
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA85DF7E-FCFB-448C-AF0E-6BD79F22336D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20EEA48-66D1-4143-8ADD-A91BD6AEF5C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3361" uniqueCount="785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3371" uniqueCount="786">
   <si>
     <t>Prioridade</t>
   </si>
@@ -2546,6 +2546,9 @@
   </si>
   <si>
     <t>Aplicação de patch de atualização 20-04-30_ATUALIZACAO_12.1.25_GCT_EXPEDICAO_CONTINUA_TTTP12_LG - Gestão de Contratos</t>
+  </si>
+  <si>
+    <t>Auxilio para emissão de razonete contas a receber de alguns clientes, referente a janeiro/2020</t>
   </si>
 </sst>
 </file>
@@ -3259,7 +3262,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A523" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A530" sqref="A530"/>
+      <selection pane="bottomLeft" activeCell="A533" sqref="A533"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18038,7 +18041,7 @@
         <v>549</v>
       </c>
       <c r="D525" s="19" t="s">
-        <v>630</v>
+        <v>755</v>
       </c>
       <c r="E525" s="18" t="s">
         <v>776</v>
@@ -18211,23 +18214,49 @@
       </c>
       <c r="J530" s="20"/>
     </row>
-    <row r="531" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A531" s="26"/>
-      <c r="B531" s="24"/>
-      <c r="C531" s="18"/>
-      <c r="D531" s="19"/>
-      <c r="E531" s="18"/>
-      <c r="F531" s="19"/>
-      <c r="G531" s="26"/>
-      <c r="H531" s="6"/>
-      <c r="I531" s="20"/>
+    <row r="531" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A531" s="26">
+        <v>43968</v>
+      </c>
+      <c r="B531" s="24" t="s">
+        <v>482</v>
+      </c>
+      <c r="C531" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D531" s="19" t="s">
+        <v>755</v>
+      </c>
+      <c r="E531" s="18" t="s">
+        <v>785</v>
+      </c>
+      <c r="F531" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G531" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H531" s="6">
+        <v>43969</v>
+      </c>
+      <c r="I531" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J531" s="20"/>
     </row>
     <row r="532" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A532" s="26"/>
-      <c r="B532" s="24"/>
-      <c r="C532" s="18"/>
-      <c r="D532" s="19"/>
+      <c r="A532" s="26">
+        <v>43968</v>
+      </c>
+      <c r="B532" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C532" s="18" t="s">
+        <v>552</v>
+      </c>
+      <c r="D532" s="19" t="s">
+        <v>755</v>
+      </c>
       <c r="E532" s="18"/>
       <c r="F532" s="19"/>
       <c r="G532" s="26"/>

</xml_diff>

<commit_message>
Inclusão ND BKFINR26 - Ini. Grafico Excel
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20EEA48-66D1-4143-8ADD-A91BD6AEF5C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACE9AA6-E9E7-4749-8C01-31730E341040}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3371" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3403" uniqueCount="791">
   <si>
     <t>Prioridade</t>
   </si>
@@ -2549,6 +2549,21 @@
   </si>
   <si>
     <t>Auxilio para emissão de razonete contas a receber de alguns clientes, referente a janeiro/2020</t>
+  </si>
+  <si>
+    <t>Alteração na integração de liquidos BK para não gerar mais Pas para Despesas de Viagem e tipos CX. Alterada também a configuração de contabilização para estes casos.</t>
+  </si>
+  <si>
+    <t>Verificação de algumas NFs da CMOG que não estavam nos livros de março/20 (foram incluídas depois do fechamento)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTERAR  títulos do Microsiga que estão lançado para o dia 20 e 21/5, PARA O DIA 19/05/20,devido o feriado </t>
+  </si>
+  <si>
+    <t>Alterar as datas dos feriados cadastrados de todas as empresas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificação e exclusão de titulo CPX 000062161 </t>
   </si>
 </sst>
 </file>
@@ -3258,11 +3273,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J537"/>
+  <dimension ref="A1:J544"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A523" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A533" sqref="A533"/>
+      <pane ySplit="1" topLeftCell="A528" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E531" sqref="E531"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18214,21 +18229,21 @@
       </c>
       <c r="J530" s="20"/>
     </row>
-    <row r="531" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A531" s="26">
-        <v>43968</v>
+        <v>43966</v>
       </c>
       <c r="B531" s="24" t="s">
-        <v>482</v>
+        <v>23</v>
       </c>
       <c r="C531" s="18" t="s">
-        <v>90</v>
+        <v>552</v>
       </c>
       <c r="D531" s="19" t="s">
         <v>755</v>
       </c>
       <c r="E531" s="18" t="s">
-        <v>785</v>
+        <v>790</v>
       </c>
       <c r="F531" s="19" t="s">
         <v>106</v>
@@ -18237,79 +18252,161 @@
         <v>126</v>
       </c>
       <c r="H531" s="6">
-        <v>43969</v>
+        <v>43966</v>
       </c>
       <c r="I531" s="20" t="s">
         <v>17</v>
       </c>
       <c r="J531" s="20"/>
     </row>
-    <row r="532" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A532" s="26">
         <v>43968</v>
       </c>
       <c r="B532" s="24" t="s">
-        <v>23</v>
+        <v>482</v>
       </c>
       <c r="C532" s="18" t="s">
-        <v>552</v>
+        <v>90</v>
       </c>
       <c r="D532" s="19" t="s">
         <v>755</v>
       </c>
-      <c r="E532" s="18"/>
-      <c r="F532" s="19"/>
-      <c r="G532" s="26"/>
-      <c r="H532" s="6"/>
-      <c r="I532" s="20"/>
+      <c r="E532" s="18" t="s">
+        <v>785</v>
+      </c>
+      <c r="F532" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G532" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H532" s="6">
+        <v>43969</v>
+      </c>
+      <c r="I532" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J532" s="20"/>
     </row>
-    <row r="533" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A533" s="26"/>
-      <c r="B533" s="24"/>
-      <c r="C533" s="18"/>
-      <c r="D533" s="19"/>
-      <c r="E533" s="18"/>
-      <c r="F533" s="19"/>
-      <c r="G533" s="26"/>
-      <c r="H533" s="6"/>
-      <c r="I533" s="20"/>
+    <row r="533" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A533" s="26">
+        <v>43969</v>
+      </c>
+      <c r="B533" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C533" s="18" t="s">
+        <v>552</v>
+      </c>
+      <c r="D533" s="19" t="s">
+        <v>755</v>
+      </c>
+      <c r="E533" s="18" t="s">
+        <v>786</v>
+      </c>
+      <c r="F533" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G533" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H533" s="6">
+        <v>43969</v>
+      </c>
+      <c r="I533" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J533" s="20"/>
     </row>
-    <row r="534" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A534" s="26"/>
-      <c r="B534" s="24"/>
-      <c r="C534" s="18"/>
-      <c r="D534" s="19"/>
-      <c r="E534" s="18"/>
-      <c r="F534" s="19"/>
-      <c r="G534" s="26"/>
-      <c r="H534" s="6"/>
-      <c r="I534" s="20"/>
+    <row r="534" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A534" s="26">
+        <v>43969</v>
+      </c>
+      <c r="B534" s="24" t="s">
+        <v>522</v>
+      </c>
+      <c r="C534" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D534" s="19" t="s">
+        <v>755</v>
+      </c>
+      <c r="E534" s="18" t="s">
+        <v>787</v>
+      </c>
+      <c r="F534" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G534" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H534" s="6">
+        <v>43969</v>
+      </c>
+      <c r="I534" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J534" s="20"/>
     </row>
-    <row r="535" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A535" s="26"/>
-      <c r="B535" s="24"/>
-      <c r="C535" s="18"/>
-      <c r="D535" s="19"/>
-      <c r="E535" s="18"/>
-      <c r="F535" s="19"/>
-      <c r="G535" s="26"/>
-      <c r="H535" s="6"/>
-      <c r="I535" s="20"/>
+    <row r="535" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A535" s="26">
+        <v>43970</v>
+      </c>
+      <c r="B535" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C535" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D535" s="19" t="s">
+        <v>755</v>
+      </c>
+      <c r="E535" s="18" t="s">
+        <v>788</v>
+      </c>
+      <c r="F535" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G535" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H535" s="6">
+        <v>43970</v>
+      </c>
+      <c r="I535" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J535" s="20"/>
     </row>
     <row r="536" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A536" s="26"/>
-      <c r="B536" s="24"/>
-      <c r="C536" s="18"/>
-      <c r="D536" s="19"/>
-      <c r="E536" s="18"/>
-      <c r="F536" s="19"/>
-      <c r="G536" s="26"/>
-      <c r="H536" s="6"/>
-      <c r="I536" s="20"/>
+      <c r="A536" s="26">
+        <v>43970</v>
+      </c>
+      <c r="B536" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C536" s="18" t="s">
+        <v>645</v>
+      </c>
+      <c r="D536" s="19" t="s">
+        <v>770</v>
+      </c>
+      <c r="E536" s="18" t="s">
+        <v>789</v>
+      </c>
+      <c r="F536" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G536" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H536" s="6">
+        <v>43970</v>
+      </c>
+      <c r="I536" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J536" s="20"/>
     </row>
     <row r="537" spans="1:10" x14ac:dyDescent="0.25">
@@ -18323,6 +18420,90 @@
       <c r="H537" s="6"/>
       <c r="I537" s="20"/>
       <c r="J537" s="20"/>
+    </row>
+    <row r="538" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A538" s="26"/>
+      <c r="B538" s="24"/>
+      <c r="C538" s="18"/>
+      <c r="D538" s="19"/>
+      <c r="E538" s="18"/>
+      <c r="F538" s="19"/>
+      <c r="G538" s="26"/>
+      <c r="H538" s="6"/>
+      <c r="I538" s="20"/>
+      <c r="J538" s="20"/>
+    </row>
+    <row r="539" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A539" s="26"/>
+      <c r="B539" s="24"/>
+      <c r="C539" s="18"/>
+      <c r="D539" s="19"/>
+      <c r="E539" s="18"/>
+      <c r="F539" s="19"/>
+      <c r="G539" s="26"/>
+      <c r="H539" s="6"/>
+      <c r="I539" s="20"/>
+      <c r="J539" s="20"/>
+    </row>
+    <row r="540" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A540" s="26"/>
+      <c r="B540" s="24"/>
+      <c r="C540" s="18"/>
+      <c r="D540" s="19"/>
+      <c r="E540" s="18"/>
+      <c r="F540" s="19"/>
+      <c r="G540" s="26"/>
+      <c r="H540" s="6"/>
+      <c r="I540" s="20"/>
+      <c r="J540" s="20"/>
+    </row>
+    <row r="541" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A541" s="26"/>
+      <c r="B541" s="24"/>
+      <c r="C541" s="18"/>
+      <c r="D541" s="19"/>
+      <c r="E541" s="18"/>
+      <c r="F541" s="19"/>
+      <c r="G541" s="26"/>
+      <c r="H541" s="6"/>
+      <c r="I541" s="20"/>
+      <c r="J541" s="20"/>
+    </row>
+    <row r="542" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A542" s="26"/>
+      <c r="B542" s="24"/>
+      <c r="C542" s="18"/>
+      <c r="D542" s="19"/>
+      <c r="E542" s="18"/>
+      <c r="F542" s="19"/>
+      <c r="G542" s="26"/>
+      <c r="H542" s="6"/>
+      <c r="I542" s="20"/>
+      <c r="J542" s="20"/>
+    </row>
+    <row r="543" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A543" s="26"/>
+      <c r="B543" s="24"/>
+      <c r="C543" s="18"/>
+      <c r="D543" s="19"/>
+      <c r="E543" s="18"/>
+      <c r="F543" s="19"/>
+      <c r="G543" s="26"/>
+      <c r="H543" s="6"/>
+      <c r="I543" s="20"/>
+      <c r="J543" s="20"/>
+    </row>
+    <row r="544" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A544" s="26"/>
+      <c r="B544" s="24"/>
+      <c r="C544" s="18"/>
+      <c r="D544" s="19"/>
+      <c r="E544" s="18"/>
+      <c r="F544" s="19"/>
+      <c r="G544" s="26"/>
+      <c r="H544" s="6"/>
+      <c r="I544" s="20"/>
+      <c r="J544" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J524" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Alterações - Implantação de Filiais
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACE9AA6-E9E7-4749-8C01-31730E341040}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0903410-8427-47E5-BDC5-E59F01793B57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_FilterDatabase_0" localSheetId="0">Plan1!$A$1:$I$53</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$J$524</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$J$536</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Planilha1!$A$1:$I$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3403" uniqueCount="791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3433" uniqueCount="796">
   <si>
     <t>Prioridade</t>
   </si>
@@ -2564,6 +2564,22 @@
   </si>
   <si>
     <t xml:space="preserve">Verificação e exclusão de titulo CPX 000062161 </t>
+  </si>
+  <si>
+    <t>Em conversa com o pessoal da ARAUCÁRIA NITROGENADOS descobri que temos 2 contratos ativos com eles, e destes, 1 tem retenção de INSS e o outro não.
+Teríamos como fazer essa divisão no Microsiga para que os próximos pedidos lançados pela Chris respeitem essa regra?</t>
+  </si>
+  <si>
+    <t>Aguardando numeros de contrato para testes</t>
+  </si>
+  <si>
+    <t>Solicita auxlio para emissão de relatório com saldos de contas contábeis me a mês: foi indicado o relatorio comparativo Contas 12 Meses</t>
+  </si>
+  <si>
+    <t>Solicitou execução de contabilização off-line financeiro para a NF 002018320 - CATHO FORN: 000023 - CATHO ON LINE  -  VALOR R$ 4,49 - Abril/2020</t>
+  </si>
+  <si>
+    <t>Solicitou execução de contabilização off-line de compras para a NF 002018320 FORN: 000023 - CATHO ON LINE  -  VALOR R$ 299,03 - Fevereiro/2020</t>
   </si>
 </sst>
 </file>
@@ -3276,8 +3292,8 @@
   <dimension ref="A1:J544"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A528" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E531" sqref="E531"/>
+      <pane ySplit="1" topLeftCell="A534" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A541" sqref="A541"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11707,7 +11723,7 @@
       <c r="G305" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="H305" s="54">
+      <c r="H305" s="23">
         <v>43748</v>
       </c>
       <c r="I305" s="20" t="s">
@@ -11735,7 +11751,7 @@
       <c r="G306" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="H306" s="54">
+      <c r="H306" s="23">
         <v>43753</v>
       </c>
       <c r="I306" s="20" t="s">
@@ -11791,7 +11807,7 @@
       <c r="G308" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="H308" s="54">
+      <c r="H308" s="23">
         <v>43719</v>
       </c>
       <c r="I308" s="20" t="s">
@@ -12160,9 +12176,15 @@
       <c r="F323" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G323" s="20"/>
-      <c r="H323" s="6"/>
-      <c r="I323" s="20"/>
+      <c r="G323" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H323" s="6">
+        <v>43755</v>
+      </c>
+      <c r="I323" s="20" t="s">
+        <v>12</v>
+      </c>
       <c r="J323" s="20"/>
     </row>
     <row r="324" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -18409,52 +18431,122 @@
       </c>
       <c r="J536" s="20"/>
     </row>
-    <row r="537" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A537" s="26"/>
-      <c r="B537" s="24"/>
-      <c r="C537" s="18"/>
-      <c r="D537" s="19"/>
-      <c r="E537" s="18"/>
-      <c r="F537" s="19"/>
+    <row r="537" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+      <c r="A537" s="26">
+        <v>43971</v>
+      </c>
+      <c r="B537" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C537" s="18" t="s">
+        <v>552</v>
+      </c>
+      <c r="D537" s="19" t="s">
+        <v>755</v>
+      </c>
+      <c r="E537" s="18" t="s">
+        <v>791</v>
+      </c>
+      <c r="F537" s="19" t="s">
+        <v>86</v>
+      </c>
       <c r="G537" s="26"/>
       <c r="H537" s="6"/>
-      <c r="I537" s="20"/>
-      <c r="J537" s="20"/>
-    </row>
-    <row r="538" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A538" s="26"/>
-      <c r="B538" s="24"/>
-      <c r="C538" s="18"/>
-      <c r="D538" s="19"/>
-      <c r="E538" s="18"/>
-      <c r="F538" s="19"/>
-      <c r="G538" s="26"/>
-      <c r="H538" s="6"/>
-      <c r="I538" s="20"/>
+      <c r="I537" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J537" s="20" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="538" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A538" s="26">
+        <v>43976</v>
+      </c>
+      <c r="B538" s="24" t="s">
+        <v>482</v>
+      </c>
+      <c r="C538" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D538" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="E538" s="18" t="s">
+        <v>793</v>
+      </c>
+      <c r="F538" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G538" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H538" s="6">
+        <v>43976</v>
+      </c>
+      <c r="I538" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J538" s="20"/>
     </row>
-    <row r="539" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A539" s="26"/>
-      <c r="B539" s="24"/>
-      <c r="C539" s="18"/>
-      <c r="D539" s="19"/>
-      <c r="E539" s="18"/>
-      <c r="F539" s="19"/>
-      <c r="G539" s="26"/>
-      <c r="H539" s="6"/>
-      <c r="I539" s="20"/>
+    <row r="539" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A539" s="26">
+        <v>43976</v>
+      </c>
+      <c r="B539" s="24" t="s">
+        <v>571</v>
+      </c>
+      <c r="C539" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D539" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="E539" s="18" t="s">
+        <v>795</v>
+      </c>
+      <c r="F539" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G539" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H539" s="6">
+        <v>43976</v>
+      </c>
+      <c r="I539" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J539" s="20"/>
     </row>
-    <row r="540" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A540" s="26"/>
-      <c r="B540" s="24"/>
-      <c r="C540" s="18"/>
-      <c r="D540" s="19"/>
-      <c r="E540" s="18"/>
-      <c r="F540" s="19"/>
-      <c r="G540" s="26"/>
-      <c r="H540" s="6"/>
-      <c r="I540" s="20"/>
+    <row r="540" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A540" s="26">
+        <v>43976</v>
+      </c>
+      <c r="B540" s="24" t="s">
+        <v>571</v>
+      </c>
+      <c r="C540" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D540" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="E540" s="18" t="s">
+        <v>794</v>
+      </c>
+      <c r="F540" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G540" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H540" s="6">
+        <v>43976</v>
+      </c>
+      <c r="I540" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J540" s="20"/>
     </row>
     <row r="541" spans="1:10" x14ac:dyDescent="0.25">
@@ -18506,7 +18598,7 @@
       <c r="J544" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J524" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J536" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="10" firstPageNumber="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Acerto Rentabilidade / Avaliação Fornec. Anderson
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E106E58-5602-49C5-BADF-A95CBD437D9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E27BE1E-9CEC-41F4-B9B5-101E734B850E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4075" uniqueCount="904">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4098" uniqueCount="910">
   <si>
     <t>Prioridade</t>
   </si>
@@ -2895,9 +2895,6 @@
     <t xml:space="preserve">Nova planilha com lançamentos do off-line gerado dia 20/07/20 </t>
   </si>
   <si>
-    <t>Reabilitar a empresa ESA</t>
-  </si>
-  <si>
     <t>Alterar Lançamento padronizado "Desconto Juros Antecipados de conta débito 11101002 para 34301004</t>
   </si>
   <si>
@@ -2912,6 +2909,28 @@
   </si>
   <si>
     <t>Cria a empresa BHG Poupatempo (empresa 15)</t>
+  </si>
+  <si>
+    <t>Titulos solicitados pelo Edson</t>
+  </si>
+  <si>
+    <t>Acertar acessos as empresas de todos usuários</t>
+  </si>
+  <si>
+    <t>Atualizar módulo fiscal</t>
+  </si>
+  <si>
+    <t>Parâmetros já estavam ok</t>
+  </si>
+  <si>
+    <t>Dúvidas relatório contas a pagar BHG Osasco</t>
+  </si>
+  <si>
+    <t>os valores previstos do Contrato 132.000.464 no Relatório Comparativo (BKGCTR14). Os valores de previsão estão aparecendo quadruplicados, conforme mostrado no anexo.
+Observo que esse contrato tem 4 planilhas e que não tinha esse problema até antes desse último faturamento. Não sei se na hora da medição ficou alguma coisa em aberto.</t>
+  </si>
+  <si>
+    <t>Treinamento para emissão de NFs - Barueri</t>
   </si>
 </sst>
 </file>
@@ -3621,11 +3640,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J638"/>
+  <dimension ref="A1:J641"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A620" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E626" sqref="E626"/>
+      <pane ySplit="1" topLeftCell="A627" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F634" sqref="F634"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21132,8 +21151,12 @@
       <c r="F614" s="19" t="s">
         <v>884</v>
       </c>
-      <c r="G614" s="26"/>
-      <c r="H614" s="6"/>
+      <c r="G614" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H614" s="6">
+        <v>44035</v>
+      </c>
       <c r="I614" s="20" t="s">
         <v>17</v>
       </c>
@@ -21299,7 +21322,7 @@
         <v>751</v>
       </c>
       <c r="E620" s="18" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="F620" s="19" t="s">
         <v>86</v>
@@ -21308,7 +21331,7 @@
       <c r="H620" s="6"/>
       <c r="I620" s="20"/>
       <c r="J620" s="20" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="621" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -21348,16 +21371,16 @@
         <v>44033</v>
       </c>
       <c r="B622" s="24" t="s">
-        <v>51</v>
+        <v>548</v>
       </c>
       <c r="C622" s="18" t="s">
-        <v>10</v>
+        <v>549</v>
       </c>
       <c r="D622" s="19" t="s">
         <v>751</v>
       </c>
       <c r="E622" s="18" t="s">
-        <v>898</v>
+        <v>903</v>
       </c>
       <c r="F622" s="19" t="s">
         <v>163</v>
@@ -21381,13 +21404,23 @@
         <v>751</v>
       </c>
       <c r="E623" s="18" t="s">
-        <v>901</v>
-      </c>
-      <c r="F623" s="19"/>
-      <c r="G623" s="26"/>
-      <c r="H623" s="6"/>
-      <c r="I623" s="20"/>
-      <c r="J623" s="20"/>
+        <v>900</v>
+      </c>
+      <c r="F623" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G623" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H623" s="6">
+        <v>44039</v>
+      </c>
+      <c r="I623" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J623" s="20" t="s">
+        <v>906</v>
+      </c>
     </row>
     <row r="624" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A624" s="26">
@@ -21403,7 +21436,7 @@
         <v>751</v>
       </c>
       <c r="E624" s="18" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F624" s="19" t="s">
         <v>106</v>
@@ -21433,7 +21466,7 @@
         <v>751</v>
       </c>
       <c r="E625" s="18" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="F625" s="19" t="s">
         <v>61</v>
@@ -21602,23 +21635,51 @@
       <c r="J630" s="20"/>
     </row>
     <row r="631" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A631" s="26"/>
-      <c r="B631" s="24"/>
-      <c r="C631" s="18"/>
-      <c r="D631" s="19"/>
-      <c r="E631" s="18"/>
-      <c r="F631" s="19"/>
-      <c r="G631" s="26"/>
-      <c r="H631" s="6"/>
-      <c r="I631" s="20"/>
+      <c r="A631" s="26">
+        <v>44034</v>
+      </c>
+      <c r="B631" s="24" t="s">
+        <v>571</v>
+      </c>
+      <c r="C631" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D631" s="19" t="s">
+        <v>751</v>
+      </c>
+      <c r="E631" s="18" t="s">
+        <v>907</v>
+      </c>
+      <c r="F631" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G631" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H631" s="6">
+        <v>44035</v>
+      </c>
+      <c r="I631" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J631" s="20"/>
     </row>
-    <row r="632" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A632" s="26"/>
-      <c r="B632" s="24"/>
-      <c r="C632" s="18"/>
-      <c r="D632" s="19"/>
-      <c r="E632" s="18"/>
+    <row r="632" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A632" s="26">
+        <v>44035</v>
+      </c>
+      <c r="B632" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C632" s="18" t="s">
+        <v>552</v>
+      </c>
+      <c r="D632" s="19" t="s">
+        <v>751</v>
+      </c>
+      <c r="E632" s="18" t="s">
+        <v>908</v>
+      </c>
       <c r="F632" s="19"/>
       <c r="G632" s="26"/>
       <c r="H632" s="6"/>
@@ -21626,12 +21687,24 @@
       <c r="J632" s="20"/>
     </row>
     <row r="633" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A633" s="26"/>
-      <c r="B633" s="24"/>
-      <c r="C633" s="18"/>
-      <c r="D633" s="19"/>
-      <c r="E633" s="18"/>
-      <c r="F633" s="19"/>
+      <c r="A633" s="26">
+        <v>44035</v>
+      </c>
+      <c r="B633" s="24" t="s">
+        <v>518</v>
+      </c>
+      <c r="C633" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D633" s="19" t="s">
+        <v>751</v>
+      </c>
+      <c r="E633" s="18" t="s">
+        <v>909</v>
+      </c>
+      <c r="F633" s="19" t="s">
+        <v>61</v>
+      </c>
       <c r="G633" s="26"/>
       <c r="H633" s="6"/>
       <c r="I633" s="20"/>
@@ -21642,7 +21715,9 @@
       <c r="B634" s="24"/>
       <c r="C634" s="18"/>
       <c r="D634" s="19"/>
-      <c r="E634" s="18"/>
+      <c r="E634" s="18" t="s">
+        <v>904</v>
+      </c>
       <c r="F634" s="19"/>
       <c r="G634" s="26"/>
       <c r="H634" s="6"/>
@@ -21654,7 +21729,9 @@
       <c r="B635" s="24"/>
       <c r="C635" s="18"/>
       <c r="D635" s="19"/>
-      <c r="E635" s="18"/>
+      <c r="E635" s="18" t="s">
+        <v>905</v>
+      </c>
       <c r="F635" s="19"/>
       <c r="G635" s="26"/>
       <c r="H635" s="6"/>
@@ -21696,6 +21773,42 @@
       <c r="H638" s="6"/>
       <c r="I638" s="20"/>
       <c r="J638" s="20"/>
+    </row>
+    <row r="639" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A639" s="26"/>
+      <c r="B639" s="24"/>
+      <c r="C639" s="18"/>
+      <c r="D639" s="19"/>
+      <c r="E639" s="18"/>
+      <c r="F639" s="19"/>
+      <c r="G639" s="26"/>
+      <c r="H639" s="6"/>
+      <c r="I639" s="20"/>
+      <c r="J639" s="20"/>
+    </row>
+    <row r="640" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A640" s="26"/>
+      <c r="B640" s="24"/>
+      <c r="C640" s="18"/>
+      <c r="D640" s="19"/>
+      <c r="E640" s="18"/>
+      <c r="F640" s="19"/>
+      <c r="G640" s="26"/>
+      <c r="H640" s="6"/>
+      <c r="I640" s="20"/>
+      <c r="J640" s="20"/>
+    </row>
+    <row r="641" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A641" s="26"/>
+      <c r="B641" s="24"/>
+      <c r="C641" s="18"/>
+      <c r="D641" s="19"/>
+      <c r="E641" s="18"/>
+      <c r="F641" s="19"/>
+      <c r="G641" s="26"/>
+      <c r="H641" s="6"/>
+      <c r="I641" s="20"/>
+      <c r="J641" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J619" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Descrição do Serviço na NFS
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E27BE1E-9CEC-41F4-B9B5-101E734B850E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B598FB53-DCA3-4762-927E-CAC962B1AAFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4098" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4133" uniqueCount="917">
   <si>
     <t>Prioridade</t>
   </si>
@@ -2914,9 +2914,6 @@
     <t>Titulos solicitados pelo Edson</t>
   </si>
   <si>
-    <t>Acertar acessos as empresas de todos usuários</t>
-  </si>
-  <si>
     <t>Atualizar módulo fiscal</t>
   </si>
   <si>
@@ -2931,6 +2928,30 @@
   </si>
   <si>
     <t>Treinamento para emissão de NFs - Barueri</t>
+  </si>
+  <si>
+    <t>Presencial</t>
+  </si>
+  <si>
+    <t>Alterar a formatação do texto do corpo da NF para 13 linhas no máximo e bloquear se estiver com mais linhas</t>
+  </si>
+  <si>
+    <t>Incrementar o numero de remessa da NF de Barueri automaticamente</t>
+  </si>
+  <si>
+    <t>mtdescrnfe.prw</t>
+  </si>
+  <si>
+    <t>nfebarue.ini e mtdescrnfe.prw</t>
+  </si>
+  <si>
+    <t>Inclusão do usuário Anderson para avaliação de fornecedores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificar alguma forma de quando o Anderson aprovar pagamentos de férias e rescisões eu receber e-mail automático com os valores/datas. </t>
+  </si>
+  <si>
+    <t>Reconfigurar envio de e-mail pelo protheus (aguardar migração)</t>
   </si>
 </sst>
 </file>
@@ -3640,11 +3661,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J641"/>
+  <dimension ref="A1:J645"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A627" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F634" sqref="F634"/>
+      <pane ySplit="1" topLeftCell="A629" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A639" sqref="A639"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21383,11 +21404,17 @@
         <v>903</v>
       </c>
       <c r="F622" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="G622" s="26"/>
-      <c r="H622" s="6"/>
-      <c r="I622" s="20"/>
+        <v>86</v>
+      </c>
+      <c r="G622" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H622" s="6">
+        <v>44039</v>
+      </c>
+      <c r="I622" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J622" s="20"/>
     </row>
     <row r="623" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -21419,7 +21446,7 @@
         <v>17</v>
       </c>
       <c r="J623" s="20" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="624" spans="1:10" x14ac:dyDescent="0.25">
@@ -21648,7 +21675,7 @@
         <v>751</v>
       </c>
       <c r="E631" s="18" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="F631" s="19" t="s">
         <v>106</v>
@@ -21678,7 +21705,7 @@
         <v>751</v>
       </c>
       <c r="E632" s="18" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="F632" s="19"/>
       <c r="G632" s="26"/>
@@ -21700,62 +21727,132 @@
         <v>751</v>
       </c>
       <c r="E633" s="18" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="F633" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G633" s="26"/>
-      <c r="H633" s="6"/>
-      <c r="I633" s="20"/>
+      <c r="G633" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H633" s="6">
+        <v>44036</v>
+      </c>
+      <c r="I633" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J633" s="20"/>
     </row>
     <row r="634" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A634" s="26"/>
-      <c r="B634" s="24"/>
-      <c r="C634" s="18"/>
-      <c r="D634" s="19"/>
+      <c r="A634" s="26">
+        <v>44036</v>
+      </c>
+      <c r="B634" s="24" t="s">
+        <v>434</v>
+      </c>
+      <c r="C634" s="18" t="s">
+        <v>577</v>
+      </c>
+      <c r="D634" s="19" t="s">
+        <v>751</v>
+      </c>
       <c r="E634" s="18" t="s">
-        <v>904</v>
-      </c>
-      <c r="F634" s="19"/>
-      <c r="G634" s="26"/>
-      <c r="H634" s="6"/>
-      <c r="I634" s="20"/>
+        <v>914</v>
+      </c>
+      <c r="F634" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G634" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H634" s="6">
+        <v>44036</v>
+      </c>
+      <c r="I634" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J634" s="20"/>
     </row>
-    <row r="635" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A635" s="26"/>
-      <c r="B635" s="24"/>
-      <c r="C635" s="18"/>
-      <c r="D635" s="19"/>
+    <row r="635" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A635" s="26">
+        <v>44036</v>
+      </c>
+      <c r="B635" s="24" t="s">
+        <v>635</v>
+      </c>
+      <c r="C635" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D635" s="19" t="s">
+        <v>909</v>
+      </c>
       <c r="E635" s="18" t="s">
-        <v>905</v>
-      </c>
-      <c r="F635" s="19"/>
-      <c r="G635" s="26"/>
-      <c r="H635" s="6"/>
-      <c r="I635" s="20"/>
-      <c r="J635" s="20"/>
-    </row>
-    <row r="636" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A636" s="26"/>
-      <c r="B636" s="24"/>
-      <c r="C636" s="18"/>
-      <c r="D636" s="19"/>
-      <c r="E636" s="18"/>
-      <c r="F636" s="19"/>
-      <c r="G636" s="26"/>
-      <c r="H636" s="6"/>
-      <c r="I636" s="20"/>
-      <c r="J636" s="20"/>
-    </row>
-    <row r="637" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A637" s="26"/>
-      <c r="B637" s="24"/>
-      <c r="C637" s="18"/>
-      <c r="D637" s="19"/>
-      <c r="E637" s="18"/>
+        <v>910</v>
+      </c>
+      <c r="F635" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G635" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H635" s="6">
+        <v>44038</v>
+      </c>
+      <c r="I635" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J635" s="20" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="636" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A636" s="26">
+        <v>44036</v>
+      </c>
+      <c r="B636" s="24" t="s">
+        <v>635</v>
+      </c>
+      <c r="C636" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D636" s="19" t="s">
+        <v>909</v>
+      </c>
+      <c r="E636" s="18" t="s">
+        <v>911</v>
+      </c>
+      <c r="F636" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G636" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H636" s="6">
+        <v>44038</v>
+      </c>
+      <c r="I636" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J636" s="20" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="637" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A637" s="26">
+        <v>44036</v>
+      </c>
+      <c r="B637" s="24" t="s">
+        <v>597</v>
+      </c>
+      <c r="C637" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D637" s="19" t="s">
+        <v>751</v>
+      </c>
+      <c r="E637" s="18" t="s">
+        <v>915</v>
+      </c>
       <c r="F637" s="19"/>
       <c r="G637" s="26"/>
       <c r="H637" s="6"/>
@@ -21763,12 +21860,24 @@
       <c r="J637" s="20"/>
     </row>
     <row r="638" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A638" s="26"/>
-      <c r="B638" s="24"/>
-      <c r="C638" s="18"/>
-      <c r="D638" s="19"/>
-      <c r="E638" s="18"/>
-      <c r="F638" s="19"/>
+      <c r="A638" s="26">
+        <v>44039</v>
+      </c>
+      <c r="B638" s="24" t="s">
+        <v>817</v>
+      </c>
+      <c r="C638" s="18" t="s">
+        <v>818</v>
+      </c>
+      <c r="D638" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="E638" s="18" t="s">
+        <v>916</v>
+      </c>
+      <c r="F638" s="19" t="s">
+        <v>86</v>
+      </c>
       <c r="G638" s="26"/>
       <c r="H638" s="6"/>
       <c r="I638" s="20"/>
@@ -21779,7 +21888,9 @@
       <c r="B639" s="24"/>
       <c r="C639" s="18"/>
       <c r="D639" s="19"/>
-      <c r="E639" s="18"/>
+      <c r="E639" s="18" t="s">
+        <v>904</v>
+      </c>
       <c r="F639" s="19"/>
       <c r="G639" s="26"/>
       <c r="H639" s="6"/>
@@ -21809,6 +21920,54 @@
       <c r="H641" s="6"/>
       <c r="I641" s="20"/>
       <c r="J641" s="20"/>
+    </row>
+    <row r="642" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A642" s="26"/>
+      <c r="B642" s="24"/>
+      <c r="C642" s="18"/>
+      <c r="D642" s="19"/>
+      <c r="E642" s="18"/>
+      <c r="F642" s="19"/>
+      <c r="G642" s="26"/>
+      <c r="H642" s="6"/>
+      <c r="I642" s="20"/>
+      <c r="J642" s="20"/>
+    </row>
+    <row r="643" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A643" s="26"/>
+      <c r="B643" s="24"/>
+      <c r="C643" s="18"/>
+      <c r="D643" s="19"/>
+      <c r="E643" s="18"/>
+      <c r="F643" s="19"/>
+      <c r="G643" s="26"/>
+      <c r="H643" s="6"/>
+      <c r="I643" s="20"/>
+      <c r="J643" s="20"/>
+    </row>
+    <row r="644" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A644" s="26"/>
+      <c r="B644" s="24"/>
+      <c r="C644" s="18"/>
+      <c r="D644" s="19"/>
+      <c r="E644" s="18"/>
+      <c r="F644" s="19"/>
+      <c r="G644" s="26"/>
+      <c r="H644" s="6"/>
+      <c r="I644" s="20"/>
+      <c r="J644" s="20"/>
+    </row>
+    <row r="645" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A645" s="26"/>
+      <c r="B645" s="24"/>
+      <c r="C645" s="18"/>
+      <c r="D645" s="19"/>
+      <c r="E645" s="18"/>
+      <c r="F645" s="19"/>
+      <c r="G645" s="26"/>
+      <c r="H645" s="6"/>
+      <c r="I645" s="20"/>
+      <c r="J645" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J619" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Inclusão contas a Receber BKFINR29
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmsiga12\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D9431A-3B49-4B23-94CF-EBEB01076DF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0DA593-F575-4C42-857A-9F8189929617}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4220" uniqueCount="933">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4238" uniqueCount="936">
   <si>
     <t>Prioridade</t>
   </si>
@@ -3001,6 +3001,16 @@
   </si>
   <si>
     <t>Acerto no dicionário de dados referente campos CNC_NOME e CNC_NOMECL que estavam com tamanhos diferentes do cadastro de clientes</t>
+  </si>
+  <si>
+    <t>Por gentileza verificar o motivo de não conseguir abrir a planilha para medição,
+Contrato 076.000.490 – Competência 07/2020</t>
+  </si>
+  <si>
+    <t>BKFINR29</t>
+  </si>
+  <si>
+    <t>Melhoria no relatorio de Previsões de Pagamentos, incluir contas a receber</t>
   </si>
 </sst>
 </file>
@@ -3710,11 +3720,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J653"/>
+  <dimension ref="A1:J656"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A645" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A650" sqref="A650"/>
+      <pane ySplit="1" topLeftCell="A642" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A652" sqref="A652"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22227,10 +22237,18 @@
       <c r="F647" s="19" t="s">
         <v>528</v>
       </c>
-      <c r="G647" s="26"/>
-      <c r="H647" s="6"/>
-      <c r="I647" s="20"/>
-      <c r="J647" s="20"/>
+      <c r="G647" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H647" s="6">
+        <v>44046</v>
+      </c>
+      <c r="I647" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J647" s="20" t="s">
+        <v>934</v>
+      </c>
     </row>
     <row r="648" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A648" s="26">
@@ -22283,43 +22301,79 @@
       <c r="F649" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="G649" s="26"/>
-      <c r="H649" s="6"/>
-      <c r="I649" s="20"/>
+      <c r="G649" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H649" s="6">
+        <v>44043</v>
+      </c>
+      <c r="I649" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J649" s="20"/>
     </row>
-    <row r="650" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A650" s="26"/>
-      <c r="B650" s="24"/>
-      <c r="C650" s="18"/>
-      <c r="D650" s="19"/>
-      <c r="E650" s="18"/>
-      <c r="F650" s="19"/>
-      <c r="G650" s="26"/>
-      <c r="H650" s="6"/>
-      <c r="I650" s="20"/>
+    <row r="650" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A650" s="26">
+        <v>44043</v>
+      </c>
+      <c r="B650" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="C650" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D650" s="19" t="s">
+        <v>751</v>
+      </c>
+      <c r="E650" s="18" t="s">
+        <v>933</v>
+      </c>
+      <c r="F650" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G650" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H650" s="6">
+        <v>44043</v>
+      </c>
+      <c r="I650" s="20" t="s">
+        <v>12</v>
+      </c>
       <c r="J650" s="20"/>
     </row>
     <row r="651" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A651" s="26"/>
-      <c r="B651" s="24"/>
-      <c r="C651" s="18"/>
-      <c r="D651" s="19"/>
-      <c r="E651" s="18"/>
-      <c r="F651" s="19"/>
+      <c r="A651" s="26">
+        <v>44046</v>
+      </c>
+      <c r="B651" s="24" t="s">
+        <v>597</v>
+      </c>
+      <c r="C651" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D651" s="19" t="s">
+        <v>751</v>
+      </c>
+      <c r="E651" s="18" t="s">
+        <v>935</v>
+      </c>
+      <c r="F651" s="19" t="s">
+        <v>498</v>
+      </c>
       <c r="G651" s="26"/>
       <c r="H651" s="6"/>
       <c r="I651" s="20"/>
-      <c r="J651" s="20"/>
+      <c r="J651" s="20" t="s">
+        <v>934</v>
+      </c>
     </row>
     <row r="652" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A652" s="26"/>
       <c r="B652" s="24"/>
       <c r="C652" s="18"/>
       <c r="D652" s="19"/>
-      <c r="E652" s="18" t="s">
-        <v>918</v>
-      </c>
+      <c r="E652" s="18"/>
       <c r="F652" s="19"/>
       <c r="G652" s="26"/>
       <c r="H652" s="6"/>
@@ -22337,6 +22391,44 @@
       <c r="H653" s="6"/>
       <c r="I653" s="20"/>
       <c r="J653" s="20"/>
+    </row>
+    <row r="654" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A654" s="26"/>
+      <c r="B654" s="24"/>
+      <c r="C654" s="18"/>
+      <c r="D654" s="19"/>
+      <c r="E654" s="18"/>
+      <c r="F654" s="19"/>
+      <c r="G654" s="26"/>
+      <c r="H654" s="6"/>
+      <c r="I654" s="20"/>
+      <c r="J654" s="20"/>
+    </row>
+    <row r="655" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A655" s="26"/>
+      <c r="B655" s="24"/>
+      <c r="C655" s="18"/>
+      <c r="D655" s="19"/>
+      <c r="E655" s="18" t="s">
+        <v>918</v>
+      </c>
+      <c r="F655" s="19"/>
+      <c r="G655" s="26"/>
+      <c r="H655" s="6"/>
+      <c r="I655" s="20"/>
+      <c r="J655" s="20"/>
+    </row>
+    <row r="656" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A656" s="26"/>
+      <c r="B656" s="24"/>
+      <c r="C656" s="18"/>
+      <c r="D656" s="19"/>
+      <c r="E656" s="18"/>
+      <c r="F656" s="19"/>
+      <c r="G656" s="26"/>
+      <c r="H656" s="6"/>
+      <c r="I656" s="20"/>
+      <c r="J656" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J644" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Alteração de pasta do xxLog de alguns prw
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.30.55\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA45E582-1DA8-44FB-996D-8215C2EDD3E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B45942-056E-474F-9925-94E727903929}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11160" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_FilterDatabase_0" localSheetId="0">Plan1!$A$1:$I$53</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$J$673</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$J$693</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Planilha1!$A$1:$I$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4462" uniqueCount="983">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4530" uniqueCount="996">
   <si>
     <t>Prioridade</t>
   </si>
@@ -3176,6 +3176,46 @@
 E-mail do gestor
 Tels do Gestor
 Gestor BK</t>
+  </si>
+  <si>
+    <t>Edson aprovou vários pagamentos e não aparece no financeiro para integrar</t>
+  </si>
+  <si>
+    <t>Gerar o diário auxilio contas a receber da balsa nova mês a mês de janeiro a julho - Balsa Nova</t>
+  </si>
+  <si>
+    <t>Por gentileza verificar o motivo de alguns lançamentos não estarem visível para a Vanderleia,
+Possivelmente a NF já foi aprovada pelo Nelson, porem antes da aprovação não estava visível, tendo também outros casos, como em BKDAHER TABOAO,</t>
+  </si>
+  <si>
+    <t>Gerar o diário auxilio contas a receber / pagar julho/2020 BK</t>
+  </si>
+  <si>
+    <t>Não há problemas com o sistema</t>
+  </si>
+  <si>
+    <t>Aplicação de patch de atualização Gestão de Contratos: 20-08-06_ATUALIZACAO_12.1.25_GCT_EXPEDICAO_CONTINUA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificação da parada de Envio de e-mails pelo sistema </t>
+  </si>
+  <si>
+    <t>Rafael acertou regra no firewall</t>
+  </si>
+  <si>
+    <t>Dividir em 6 parcelas os pagamentos de rescição de funcionários das empresas BHG OSASCO, BHG CAMPINAS, BKDAHER TABOAO e BKDAHER LIMEIRA na integração Rubi-Microsiga</t>
+  </si>
+  <si>
+    <t>Não procede</t>
+  </si>
+  <si>
+    <t>Alterar pedidos de vendas em aberto na virada da emsissão de NFs para Barueri</t>
+  </si>
+  <si>
+    <t>Queryes criadas</t>
+  </si>
+  <si>
+    <t>Criação de mais instâncias de slaves de servidores Protheus para otimizar o uso de memória do VMSIGA12</t>
   </si>
 </sst>
 </file>
@@ -3885,11 +3925,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J689"/>
+  <dimension ref="A1:J697"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A679" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F674" sqref="F674"/>
+      <pane ySplit="1" topLeftCell="A685" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G693" sqref="G693"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23383,44 +23423,54 @@
     </row>
     <row r="681" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A681" s="26">
-        <v>44056</v>
+        <v>44055</v>
       </c>
       <c r="B681" s="24" t="s">
         <v>518</v>
       </c>
       <c r="C681" s="18" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="D681" s="19" t="s">
-        <v>681</v>
+        <v>826</v>
       </c>
       <c r="E681" s="18" t="s">
-        <v>975</v>
-      </c>
-      <c r="F681" s="19"/>
-      <c r="G681" s="26"/>
-      <c r="H681" s="6"/>
-      <c r="I681" s="20"/>
-      <c r="J681" s="20"/>
-    </row>
-    <row r="682" spans="1:10" ht="140.25" x14ac:dyDescent="0.25">
+        <v>993</v>
+      </c>
+      <c r="F681" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G681" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H681" s="6">
+        <v>44060</v>
+      </c>
+      <c r="I681" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J681" s="20" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="682" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A682" s="26">
         <v>44056</v>
       </c>
       <c r="B682" s="24" t="s">
-        <v>23</v>
+        <v>518</v>
       </c>
       <c r="C682" s="18" t="s">
-        <v>976</v>
+        <v>90</v>
       </c>
       <c r="D682" s="19" t="s">
         <v>681</v>
       </c>
       <c r="E682" s="18" t="s">
-        <v>982</v>
+        <v>975</v>
       </c>
       <c r="F682" s="19" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G682" s="26" t="s">
         <v>126</v>
@@ -23431,28 +23481,28 @@
       <c r="I682" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J682" s="24" t="s">
-        <v>981</v>
-      </c>
-    </row>
-    <row r="683" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+      <c r="J682" s="20" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="683" spans="1:10" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A683" s="26">
         <v>44056</v>
       </c>
       <c r="B683" s="24" t="s">
-        <v>571</v>
+        <v>23</v>
       </c>
       <c r="C683" s="18" t="s">
-        <v>90</v>
+        <v>976</v>
       </c>
       <c r="D683" s="19" t="s">
-        <v>630</v>
+        <v>681</v>
       </c>
       <c r="E683" s="18" t="s">
-        <v>977</v>
+        <v>982</v>
       </c>
       <c r="F683" s="19" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G683" s="26" t="s">
         <v>126</v>
@@ -23463,25 +23513,25 @@
       <c r="I683" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J683" s="20" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="684" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="J683" s="24" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="684" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A684" s="26">
         <v>44056</v>
       </c>
       <c r="B684" s="24" t="s">
-        <v>979</v>
+        <v>571</v>
       </c>
       <c r="C684" s="18" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D684" s="19" t="s">
         <v>630</v>
       </c>
       <c r="E684" s="18" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="F684" s="19" t="s">
         <v>106</v>
@@ -23495,72 +23545,330 @@
       <c r="I684" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J684" s="20"/>
-    </row>
-    <row r="685" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A685" s="26"/>
-      <c r="B685" s="24"/>
-      <c r="C685" s="18"/>
-      <c r="D685" s="19"/>
-      <c r="E685" s="18"/>
-      <c r="F685" s="19"/>
-      <c r="G685" s="26"/>
-      <c r="H685" s="6"/>
-      <c r="I685" s="20"/>
+      <c r="J684" s="20" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="685" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A685" s="26">
+        <v>44056</v>
+      </c>
+      <c r="B685" s="24" t="s">
+        <v>979</v>
+      </c>
+      <c r="C685" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D685" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="E685" s="18" t="s">
+        <v>980</v>
+      </c>
+      <c r="F685" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G685" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H685" s="6">
+        <v>44056</v>
+      </c>
+      <c r="I685" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J685" s="20"/>
     </row>
     <row r="686" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A686" s="26"/>
-      <c r="B686" s="24"/>
-      <c r="C686" s="18"/>
-      <c r="D686" s="19"/>
-      <c r="E686" s="18"/>
-      <c r="F686" s="19"/>
-      <c r="G686" s="26"/>
-      <c r="H686" s="6"/>
-      <c r="I686" s="20"/>
+      <c r="A686" s="26">
+        <v>44057</v>
+      </c>
+      <c r="B686" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C686" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D686" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="E686" s="18" t="s">
+        <v>983</v>
+      </c>
+      <c r="F686" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G686" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H686" s="6">
+        <v>44057</v>
+      </c>
+      <c r="I686" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J686" s="20"/>
     </row>
-    <row r="687" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A687" s="26"/>
-      <c r="B687" s="24"/>
-      <c r="C687" s="18"/>
-      <c r="D687" s="19"/>
-      <c r="E687" s="18"/>
-      <c r="F687" s="19"/>
-      <c r="G687" s="26"/>
-      <c r="H687" s="6"/>
-      <c r="I687" s="20"/>
+    <row r="687" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A687" s="26">
+        <v>44057</v>
+      </c>
+      <c r="B687" s="24" t="s">
+        <v>597</v>
+      </c>
+      <c r="C687" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D687" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="E687" s="18" t="s">
+        <v>984</v>
+      </c>
+      <c r="F687" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G687" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H687" s="6">
+        <v>44057</v>
+      </c>
+      <c r="I687" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J687" s="20"/>
     </row>
     <row r="688" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A688" s="26"/>
-      <c r="B688" s="24"/>
-      <c r="C688" s="18"/>
-      <c r="D688" s="19"/>
+      <c r="A688" s="26">
+        <v>44057</v>
+      </c>
+      <c r="B688" s="24" t="s">
+        <v>597</v>
+      </c>
+      <c r="C688" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D688" s="19" t="s">
+        <v>630</v>
+      </c>
       <c r="E688" s="18" t="s">
+        <v>986</v>
+      </c>
+      <c r="F688" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G688" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H688" s="6">
+        <v>44057</v>
+      </c>
+      <c r="I688" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J688" s="20"/>
+    </row>
+    <row r="689" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A689" s="26">
+        <v>44059</v>
+      </c>
+      <c r="B689" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C689" s="18" t="s">
+        <v>645</v>
+      </c>
+      <c r="D689" s="19" t="s">
+        <v>710</v>
+      </c>
+      <c r="E689" s="18" t="s">
+        <v>988</v>
+      </c>
+      <c r="F689" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G689" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H689" s="6">
+        <v>44059</v>
+      </c>
+      <c r="I689" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J689" s="20"/>
+    </row>
+    <row r="690" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A690" s="26">
+        <v>44059</v>
+      </c>
+      <c r="B690" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C690" s="18" t="s">
+        <v>645</v>
+      </c>
+      <c r="D690" s="19" t="s">
+        <v>765</v>
+      </c>
+      <c r="E690" s="18" t="s">
+        <v>995</v>
+      </c>
+      <c r="F690" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G690" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H690" s="6">
+        <v>44059</v>
+      </c>
+      <c r="I690" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J690" s="20"/>
+    </row>
+    <row r="691" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+      <c r="A691" s="26">
+        <v>44060</v>
+      </c>
+      <c r="B691" s="24" t="s">
+        <v>691</v>
+      </c>
+      <c r="C691" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D691" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="E691" s="18" t="s">
+        <v>985</v>
+      </c>
+      <c r="F691" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G691" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H691" s="6">
+        <v>44060</v>
+      </c>
+      <c r="I691" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J691" s="20" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="692" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A692" s="26">
+        <v>44060</v>
+      </c>
+      <c r="B692" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C692" s="18" t="s">
+        <v>645</v>
+      </c>
+      <c r="D692" s="19" t="s">
+        <v>765</v>
+      </c>
+      <c r="E692" s="18" t="s">
+        <v>989</v>
+      </c>
+      <c r="F692" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G692" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H692" s="6">
+        <v>44060</v>
+      </c>
+      <c r="I692" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J692" s="20" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="693" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A693" s="26">
+        <v>44060</v>
+      </c>
+      <c r="B693" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C693" s="18" t="s">
+        <v>552</v>
+      </c>
+      <c r="D693" s="19" t="s">
+        <v>735</v>
+      </c>
+      <c r="E693" s="18" t="s">
+        <v>991</v>
+      </c>
+      <c r="F693" s="19" t="s">
+        <v>528</v>
+      </c>
+      <c r="G693" s="26"/>
+      <c r="H693" s="6"/>
+      <c r="I693" s="20"/>
+      <c r="J693" s="20"/>
+    </row>
+    <row r="694" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A694" s="26"/>
+      <c r="B694" s="24"/>
+      <c r="C694" s="18"/>
+      <c r="D694" s="19"/>
+      <c r="E694" s="18"/>
+      <c r="F694" s="19"/>
+      <c r="G694" s="26"/>
+      <c r="H694" s="6"/>
+      <c r="I694" s="20"/>
+      <c r="J694" s="20"/>
+    </row>
+    <row r="695" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A695" s="26"/>
+      <c r="B695" s="24"/>
+      <c r="C695" s="18"/>
+      <c r="D695" s="19"/>
+      <c r="E695" s="18"/>
+      <c r="F695" s="19"/>
+      <c r="G695" s="26"/>
+      <c r="H695" s="6"/>
+      <c r="I695" s="20"/>
+      <c r="J695" s="20"/>
+    </row>
+    <row r="696" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A696" s="26"/>
+      <c r="B696" s="24"/>
+      <c r="C696" s="18"/>
+      <c r="D696" s="19"/>
+      <c r="E696" s="18" t="s">
         <v>918</v>
       </c>
-      <c r="F688" s="19"/>
-      <c r="G688" s="26"/>
-      <c r="H688" s="6"/>
-      <c r="I688" s="20"/>
-      <c r="J688" s="20"/>
-    </row>
-    <row r="689" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A689" s="26"/>
-      <c r="B689" s="24"/>
-      <c r="C689" s="18"/>
-      <c r="D689" s="19"/>
-      <c r="E689" s="18"/>
-      <c r="F689" s="19"/>
-      <c r="G689" s="26"/>
-      <c r="H689" s="6"/>
-      <c r="I689" s="20"/>
-      <c r="J689" s="20"/>
+      <c r="F696" s="19"/>
+      <c r="G696" s="26"/>
+      <c r="H696" s="6"/>
+      <c r="I696" s="20"/>
+      <c r="J696" s="20"/>
+    </row>
+    <row r="697" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A697" s="26"/>
+      <c r="B697" s="24"/>
+      <c r="C697" s="18"/>
+      <c r="D697" s="19"/>
+      <c r="E697" s="18"/>
+      <c r="F697" s="19"/>
+      <c r="G697" s="26"/>
+      <c r="H697" s="6"/>
+      <c r="I697" s="20"/>
+      <c r="J697" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J673" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J693" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="10" firstPageNumber="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Alt Tipo NF e Rel Ped n Fat/Lib
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17203E3-B105-4039-9F08-0866DF81BE0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AA6D0D-3968-49AE-8ABA-B513FC1F0148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4697" uniqueCount="1028">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4719" uniqueCount="1033">
   <si>
     <t>Prioridade</t>
   </si>
@@ -3321,6 +3321,21 @@
   </si>
   <si>
     <t>Bloqueio de contas contabeis via conta sintética</t>
+  </si>
+  <si>
+    <t>Adequação do FINR07</t>
+  </si>
+  <si>
+    <t>Registro bloqueado para classificação de NF</t>
+  </si>
+  <si>
+    <t>0 hora</t>
+  </si>
+  <si>
+    <t>Outro usuário com a NF aberta</t>
+  </si>
+  <si>
+    <t>Emissão de relatorio de contas a pagar de julho/2020</t>
   </si>
 </sst>
 </file>
@@ -4033,8 +4048,8 @@
   <dimension ref="A1:J726"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A711" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E714" sqref="E714"/>
+      <pane ySplit="1" topLeftCell="A713" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A716" sqref="A716"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24376,10 +24391,18 @@
       <c r="E708" s="18" t="s">
         <v>1025</v>
       </c>
-      <c r="F708" s="19"/>
-      <c r="G708" s="26"/>
-      <c r="H708" s="6"/>
-      <c r="I708" s="20"/>
+      <c r="F708" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G708" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H708" s="6">
+        <v>44068</v>
+      </c>
+      <c r="I708" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J708" s="20"/>
     </row>
     <row r="709" spans="1:10" ht="51" x14ac:dyDescent="0.25">
@@ -24492,11 +24515,21 @@
       <c r="E712" s="18" t="s">
         <v>1020</v>
       </c>
-      <c r="F712" s="19"/>
-      <c r="G712" s="26"/>
-      <c r="H712" s="6"/>
-      <c r="I712" s="20"/>
-      <c r="J712" s="20"/>
+      <c r="F712" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G712" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H712" s="6">
+        <v>44068</v>
+      </c>
+      <c r="I712" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J712" s="20" t="s">
+        <v>1028</v>
+      </c>
     </row>
     <row r="713" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A713" s="26">
@@ -24682,28 +24715,66 @@
       <c r="I721" s="20"/>
       <c r="J721" s="20"/>
     </row>
-    <row r="722" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A722" s="26"/>
-      <c r="B722" s="24"/>
-      <c r="C722" s="18"/>
-      <c r="D722" s="19"/>
-      <c r="E722" s="18"/>
-      <c r="F722" s="19"/>
-      <c r="G722" s="26"/>
-      <c r="H722" s="6"/>
-      <c r="I722" s="20"/>
-      <c r="J722" s="20"/>
+    <row r="722" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A722" s="26">
+        <v>43976</v>
+      </c>
+      <c r="B722" s="24" t="s">
+        <v>496</v>
+      </c>
+      <c r="C722" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D722" s="19" t="s">
+        <v>735</v>
+      </c>
+      <c r="E722" s="18" t="s">
+        <v>1029</v>
+      </c>
+      <c r="F722" s="19" t="s">
+        <v>1030</v>
+      </c>
+      <c r="G722" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H722" s="6">
+        <v>44068</v>
+      </c>
+      <c r="I722" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J722" s="20" t="s">
+        <v>1031</v>
+      </c>
     </row>
     <row r="723" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A723" s="26"/>
-      <c r="B723" s="24"/>
-      <c r="C723" s="18"/>
-      <c r="D723" s="19"/>
-      <c r="E723" s="18"/>
-      <c r="F723" s="19"/>
-      <c r="G723" s="26"/>
-      <c r="H723" s="6"/>
-      <c r="I723" s="20"/>
+      <c r="A723" s="26">
+        <v>44068</v>
+      </c>
+      <c r="B723" s="24" t="s">
+        <v>597</v>
+      </c>
+      <c r="C723" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D723" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="E723" s="18" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F723" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G723" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H723" s="6">
+        <v>44069</v>
+      </c>
+      <c r="I723" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J723" s="20"/>
     </row>
     <row r="724" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Acertos Rentabilidade (mes s/ fat)
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AA6D0D-3968-49AE-8ABA-B513FC1F0148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1DC55F-1D00-4688-A93F-BF762E6A9E28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4719" uniqueCount="1033">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4752" uniqueCount="1041">
   <si>
     <t>Prioridade</t>
   </si>
@@ -3336,6 +3336,30 @@
   </si>
   <si>
     <t>Emissão de relatorio de contas a pagar de julho/2020</t>
+  </si>
+  <si>
+    <t>Incluir pedidos não faturados no relatorio de pedidos não liberados</t>
+  </si>
+  <si>
+    <t>Ficaram pendências não resolvidas com a Christiane</t>
+  </si>
+  <si>
+    <t>Somente funcionou após a manutenção do servidor VMSIGA12</t>
+  </si>
+  <si>
+    <t>Erro encontrado na Rentabilidade onde o sistema não considerava despesas para competências sem cronograma</t>
+  </si>
+  <si>
+    <t>BKGCTR11 e BKGCTR14</t>
+  </si>
+  <si>
+    <t>Copiar TES da BK para a empresa 15 - BHG Interior</t>
+  </si>
+  <si>
+    <t>Exceto 108</t>
+  </si>
+  <si>
+    <t>Criar relatório com relação de NFs semelhante al Mapa de Inss Retido por Contrato</t>
   </si>
 </sst>
 </file>
@@ -4045,11 +4069,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J726"/>
+  <dimension ref="A1:J731"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A713" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A716" sqref="A716"/>
+      <pane ySplit="1" topLeftCell="A714" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A727" sqref="A727"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23424,12 +23448,20 @@
         <v>969</v>
       </c>
       <c r="F675" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="G675" s="26"/>
-      <c r="H675" s="6"/>
-      <c r="I675" s="20"/>
-      <c r="J675" s="20"/>
+        <v>498</v>
+      </c>
+      <c r="G675" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H675" s="6">
+        <v>44066</v>
+      </c>
+      <c r="I675" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J675" s="20" t="s">
+        <v>1035</v>
+      </c>
     </row>
     <row r="676" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A676" s="26">
@@ -24585,7 +24617,7 @@
       <c r="I714" s="20"/>
       <c r="J714" s="20"/>
     </row>
-    <row r="715" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="715" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A715" s="26">
         <v>44064</v>
       </c>
@@ -24613,7 +24645,9 @@
       <c r="I715" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J715" s="20"/>
+      <c r="J715" s="20" t="s">
+        <v>1034</v>
+      </c>
     </row>
     <row r="716" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A716" s="26"/>
@@ -24778,42 +24812,174 @@
       <c r="J723" s="20"/>
     </row>
     <row r="724" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A724" s="26"/>
-      <c r="B724" s="24"/>
-      <c r="C724" s="18"/>
-      <c r="D724" s="19"/>
-      <c r="E724" s="18"/>
-      <c r="F724" s="19"/>
-      <c r="G724" s="26"/>
-      <c r="H724" s="6"/>
-      <c r="I724" s="20"/>
-      <c r="J724" s="20"/>
-    </row>
-    <row r="725" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A725" s="26"/>
-      <c r="B725" s="24"/>
-      <c r="C725" s="18"/>
-      <c r="D725" s="19"/>
+      <c r="A724" s="26">
+        <v>44069</v>
+      </c>
+      <c r="B724" s="24" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C724" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D724" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="E724" s="18" t="s">
+        <v>1033</v>
+      </c>
+      <c r="F724" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G724" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H724" s="6">
+        <v>44070</v>
+      </c>
+      <c r="I724" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J724" s="20" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="725" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A725" s="26">
+        <v>44070</v>
+      </c>
+      <c r="B725" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="C725" s="18" t="s">
+        <v>552</v>
+      </c>
+      <c r="D725" s="19" t="s">
+        <v>681</v>
+      </c>
       <c r="E725" s="18" t="s">
+        <v>1036</v>
+      </c>
+      <c r="F725" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="G725" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H725" s="6">
+        <v>44070</v>
+      </c>
+      <c r="I725" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J725" s="20" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="726" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A726" s="26">
+        <v>44070</v>
+      </c>
+      <c r="B726" s="24" t="s">
+        <v>522</v>
+      </c>
+      <c r="C726" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D726" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="E726" s="18" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F726" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G726" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H726" s="6">
+        <v>44070</v>
+      </c>
+      <c r="I726" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J726" s="20" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="727" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A727" s="26">
+        <v>44070</v>
+      </c>
+      <c r="B727" s="24" t="s">
+        <v>775</v>
+      </c>
+      <c r="C727" s="18" t="s">
+        <v>552</v>
+      </c>
+      <c r="D727" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="E727" s="18" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F727" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G727" s="26"/>
+      <c r="H727" s="6"/>
+      <c r="I727" s="20"/>
+      <c r="J727" s="20"/>
+    </row>
+    <row r="728" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A728" s="26"/>
+      <c r="B728" s="24"/>
+      <c r="C728" s="18"/>
+      <c r="D728" s="19"/>
+      <c r="E728" s="18"/>
+      <c r="F728" s="19"/>
+      <c r="G728" s="26"/>
+      <c r="H728" s="6"/>
+      <c r="I728" s="20"/>
+      <c r="J728" s="20"/>
+    </row>
+    <row r="729" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A729" s="26"/>
+      <c r="B729" s="24"/>
+      <c r="C729" s="18"/>
+      <c r="D729" s="19"/>
+      <c r="E729" s="18"/>
+      <c r="F729" s="19"/>
+      <c r="G729" s="26"/>
+      <c r="H729" s="6"/>
+      <c r="I729" s="20"/>
+      <c r="J729" s="20"/>
+    </row>
+    <row r="730" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A730" s="26"/>
+      <c r="B730" s="24"/>
+      <c r="C730" s="18"/>
+      <c r="D730" s="19"/>
+      <c r="E730" s="18" t="s">
         <v>918</v>
       </c>
-      <c r="F725" s="19"/>
-      <c r="G725" s="26"/>
-      <c r="H725" s="6"/>
-      <c r="I725" s="20"/>
-      <c r="J725" s="20"/>
-    </row>
-    <row r="726" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A726" s="26"/>
-      <c r="B726" s="24"/>
-      <c r="C726" s="18"/>
-      <c r="D726" s="19"/>
-      <c r="E726" s="18"/>
-      <c r="F726" s="19"/>
-      <c r="G726" s="26"/>
-      <c r="H726" s="6"/>
-      <c r="I726" s="20"/>
-      <c r="J726" s="20"/>
+      <c r="F730" s="19"/>
+      <c r="G730" s="26"/>
+      <c r="H730" s="6"/>
+      <c r="I730" s="20"/>
+      <c r="J730" s="20"/>
+    </row>
+    <row r="731" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A731" s="26"/>
+      <c r="B731" s="24"/>
+      <c r="C731" s="18"/>
+      <c r="D731" s="19"/>
+      <c r="E731" s="18"/>
+      <c r="F731" s="19"/>
+      <c r="G731" s="26"/>
+      <c r="H731" s="6"/>
+      <c r="I731" s="20"/>
+      <c r="J731" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J715" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Melhorias BKFINR10 e Acerto Tela XXRM
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1DC55F-1D00-4688-A93F-BF762E6A9E28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBF2C85-E412-4C1E-8DE0-08F5E07218AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4200" yWindow="-16320" windowWidth="29040" windowHeight="15990" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_FilterDatabase_0" localSheetId="0">Plan1!$A$1:$I$53</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$J$715</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$J$727</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Planilha1!$A$1:$I$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4752" uniqueCount="1041">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4798" uniqueCount="1053">
   <si>
     <t>Prioridade</t>
   </si>
@@ -3359,7 +3359,43 @@
     <t>Exceto 108</t>
   </si>
   <si>
-    <t>Criar relatório com relação de NFs semelhante al Mapa de Inss Retido por Contrato</t>
+    <t>Criar relatório com relação de NFs semelhante ao Mapa de Inss Retido por Contrato</t>
+  </si>
+  <si>
+    <t>Joao Vitor</t>
+  </si>
+  <si>
+    <t>Problema com cadastro de armazéns na inclusão de pré-nota</t>
+  </si>
+  <si>
+    <t>Despesas Furnas Atualizadas - necessário revisar BKFINR10 - lentidão para emitir longos períodos</t>
+  </si>
+  <si>
+    <t>Pedidos em aberto sem liberação e sem faturamento</t>
+  </si>
+  <si>
+    <t>BKFATR04</t>
+  </si>
+  <si>
+    <t>Alterar o relatório de "Faturamento por Contrato": Filtro por prefixo,sufixo e contratos e incluir informações da planilha</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Relação de Despesas por CC readequado</t>
+  </si>
+  <si>
+    <t>Copiada a tabela NNR</t>
+  </si>
+  <si>
+    <t>Revisadas diversas queries do BKFINR10</t>
+  </si>
+  <si>
+    <t>Juliana</t>
+  </si>
+  <si>
+    <t>Criação de conta Bancária - BHG Interior 3 - BB 5704-5</t>
+  </si>
+  <si>
+    <t>Criação da conta bancária CXB - Fundo Fixo Barueri</t>
   </si>
 </sst>
 </file>
@@ -4069,11 +4105,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J731"/>
+  <dimension ref="A1:J735"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A714" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A727" sqref="A727"/>
+      <pane ySplit="1" topLeftCell="A712" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E724" sqref="E724"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24435,7 +24471,9 @@
       <c r="I708" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J708" s="20"/>
+      <c r="J708" s="20" t="s">
+        <v>1047</v>
+      </c>
     </row>
     <row r="709" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A709" s="26">
@@ -24650,98 +24688,166 @@
       </c>
     </row>
     <row r="716" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A716" s="26"/>
-      <c r="B716" s="24"/>
-      <c r="C716" s="18"/>
-      <c r="D716" s="19"/>
-      <c r="E716" s="18"/>
-      <c r="F716" s="19"/>
-      <c r="G716" s="26"/>
-      <c r="H716" s="6"/>
-      <c r="I716" s="20"/>
+      <c r="A716" s="26">
+        <v>44065</v>
+      </c>
+      <c r="B716" s="24" t="s">
+        <v>817</v>
+      </c>
+      <c r="C716" s="18" t="s">
+        <v>818</v>
+      </c>
+      <c r="D716" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="E716" s="18" t="s">
+        <v>1024</v>
+      </c>
+      <c r="F716" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G716" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H716" s="6">
+        <v>44065</v>
+      </c>
+      <c r="I716" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J716" s="20"/>
     </row>
     <row r="717" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A717" s="26"/>
-      <c r="B717" s="24"/>
-      <c r="C717" s="18"/>
-      <c r="D717" s="19"/>
-      <c r="E717" s="18"/>
+      <c r="A717" s="26">
+        <v>44068</v>
+      </c>
+      <c r="B717" s="24" t="s">
+        <v>482</v>
+      </c>
+      <c r="C717" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D717" s="19" t="s">
+        <v>735</v>
+      </c>
+      <c r="E717" s="18" t="s">
+        <v>1027</v>
+      </c>
       <c r="F717" s="19"/>
       <c r="G717" s="26"/>
       <c r="H717" s="6"/>
       <c r="I717" s="20"/>
       <c r="J717" s="20"/>
     </row>
-    <row r="718" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A718" s="26"/>
-      <c r="B718" s="24"/>
-      <c r="C718" s="18"/>
-      <c r="D718" s="19"/>
-      <c r="E718" s="18"/>
-      <c r="F718" s="19"/>
-      <c r="G718" s="26"/>
-      <c r="H718" s="6"/>
-      <c r="I718" s="20"/>
-      <c r="J718" s="20"/>
+    <row r="718" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A718" s="26">
+        <v>43976</v>
+      </c>
+      <c r="B718" s="24" t="s">
+        <v>496</v>
+      </c>
+      <c r="C718" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D718" s="19" t="s">
+        <v>735</v>
+      </c>
+      <c r="E718" s="18" t="s">
+        <v>1029</v>
+      </c>
+      <c r="F718" s="19" t="s">
+        <v>1030</v>
+      </c>
+      <c r="G718" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H718" s="6">
+        <v>44068</v>
+      </c>
+      <c r="I718" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J718" s="20" t="s">
+        <v>1031</v>
+      </c>
     </row>
     <row r="719" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A719" s="26"/>
-      <c r="B719" s="24"/>
-      <c r="C719" s="18"/>
-      <c r="D719" s="19"/>
-      <c r="E719" s="18"/>
-      <c r="F719" s="19"/>
-      <c r="G719" s="26"/>
-      <c r="H719" s="6"/>
-      <c r="I719" s="20"/>
+      <c r="A719" s="26">
+        <v>44068</v>
+      </c>
+      <c r="B719" s="24" t="s">
+        <v>597</v>
+      </c>
+      <c r="C719" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D719" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="E719" s="18" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F719" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G719" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H719" s="6">
+        <v>44069</v>
+      </c>
+      <c r="I719" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J719" s="20"/>
     </row>
     <row r="720" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A720" s="26">
-        <v>44065</v>
+        <v>44069</v>
       </c>
       <c r="B720" s="24" t="s">
-        <v>817</v>
+        <v>1002</v>
       </c>
       <c r="C720" s="18" t="s">
-        <v>818</v>
+        <v>21</v>
       </c>
       <c r="D720" s="19" t="s">
         <v>681</v>
       </c>
       <c r="E720" s="18" t="s">
-        <v>1024</v>
+        <v>1033</v>
       </c>
       <c r="F720" s="19" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="G720" s="26" t="s">
         <v>126</v>
       </c>
       <c r="H720" s="6">
-        <v>44065</v>
+        <v>44070</v>
       </c>
       <c r="I720" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J720" s="20"/>
+      <c r="J720" s="20" t="s">
+        <v>1005</v>
+      </c>
     </row>
     <row r="721" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A721" s="26">
-        <v>44068</v>
+        <v>44069</v>
       </c>
       <c r="B721" s="24" t="s">
-        <v>482</v>
+        <v>421</v>
       </c>
       <c r="C721" s="18" t="s">
-        <v>90</v>
+        <v>552</v>
       </c>
       <c r="D721" s="19" t="s">
-        <v>735</v>
+        <v>630</v>
       </c>
       <c r="E721" s="18" t="s">
-        <v>1027</v>
+        <v>1044</v>
       </c>
       <c r="F721" s="19"/>
       <c r="G721" s="26"/>
@@ -24751,51 +24857,51 @@
     </row>
     <row r="722" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A722" s="26">
-        <v>43976</v>
+        <v>44070</v>
       </c>
       <c r="B722" s="24" t="s">
-        <v>496</v>
+        <v>421</v>
       </c>
       <c r="C722" s="18" t="s">
-        <v>21</v>
+        <v>552</v>
       </c>
       <c r="D722" s="19" t="s">
-        <v>735</v>
+        <v>681</v>
       </c>
       <c r="E722" s="18" t="s">
-        <v>1029</v>
+        <v>1036</v>
       </c>
       <c r="F722" s="19" t="s">
-        <v>1030</v>
+        <v>159</v>
       </c>
       <c r="G722" s="26" t="s">
         <v>126</v>
       </c>
       <c r="H722" s="6">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="I722" s="20" t="s">
         <v>17</v>
       </c>
       <c r="J722" s="20" t="s">
-        <v>1031</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="723" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A723" s="26">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="B723" s="24" t="s">
-        <v>597</v>
+        <v>522</v>
       </c>
       <c r="C723" s="18" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="D723" s="19" t="s">
         <v>681</v>
       </c>
       <c r="E723" s="18" t="s">
-        <v>1032</v>
+        <v>1038</v>
       </c>
       <c r="F723" s="19" t="s">
         <v>106</v>
@@ -24804,112 +24910,114 @@
         <v>126</v>
       </c>
       <c r="H723" s="6">
-        <v>44069</v>
+        <v>44070</v>
       </c>
       <c r="I723" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J723" s="20"/>
+      <c r="J723" s="20" t="s">
+        <v>1039</v>
+      </c>
     </row>
     <row r="724" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A724" s="26">
-        <v>44069</v>
+        <v>44070</v>
       </c>
       <c r="B724" s="24" t="s">
-        <v>1002</v>
+        <v>775</v>
       </c>
       <c r="C724" s="18" t="s">
-        <v>21</v>
+        <v>552</v>
       </c>
       <c r="D724" s="19" t="s">
         <v>681</v>
       </c>
       <c r="E724" s="18" t="s">
-        <v>1033</v>
+        <v>1040</v>
       </c>
       <c r="F724" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G724" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H724" s="6">
+        <v>44071</v>
+      </c>
+      <c r="I724" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J724" s="20" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="725" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A725" s="26">
+        <v>44071</v>
+      </c>
+      <c r="B725" s="24" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C725" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D725" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="E725" s="18" t="s">
+        <v>1042</v>
+      </c>
+      <c r="F725" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G725" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H725" s="6">
+        <v>44071</v>
+      </c>
+      <c r="I725" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J725" s="20" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="726" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A726" s="26">
+        <v>44071</v>
+      </c>
+      <c r="B726" s="24" t="s">
+        <v>597</v>
+      </c>
+      <c r="C726" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D726" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="E726" s="18" t="s">
+        <v>1043</v>
+      </c>
+      <c r="F726" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="G724" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="H724" s="6">
-        <v>44070</v>
-      </c>
-      <c r="I724" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="J724" s="20" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="725" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A725" s="26">
-        <v>44070</v>
-      </c>
-      <c r="B725" s="24" t="s">
-        <v>421</v>
-      </c>
-      <c r="C725" s="18" t="s">
-        <v>552</v>
-      </c>
-      <c r="D725" s="19" t="s">
-        <v>681</v>
-      </c>
-      <c r="E725" s="18" t="s">
-        <v>1036</v>
-      </c>
-      <c r="F725" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="G725" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="H725" s="6">
-        <v>44070</v>
-      </c>
-      <c r="I725" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="J725" s="20" t="s">
-        <v>1037</v>
-      </c>
-    </row>
-    <row r="726" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A726" s="26">
-        <v>44070</v>
-      </c>
-      <c r="B726" s="24" t="s">
-        <v>522</v>
-      </c>
-      <c r="C726" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="D726" s="19" t="s">
-        <v>681</v>
-      </c>
-      <c r="E726" s="18" t="s">
-        <v>1038</v>
-      </c>
-      <c r="F726" s="19" t="s">
-        <v>106</v>
-      </c>
       <c r="G726" s="26" t="s">
         <v>126</v>
       </c>
       <c r="H726" s="6">
-        <v>44070</v>
+        <v>44074</v>
       </c>
       <c r="I726" s="20" t="s">
         <v>17</v>
       </c>
       <c r="J726" s="20" t="s">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="727" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="727" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A727" s="26">
-        <v>44070</v>
+        <v>44071</v>
       </c>
       <c r="B727" s="24" t="s">
         <v>775</v>
@@ -24921,38 +25029,82 @@
         <v>681</v>
       </c>
       <c r="E727" s="18" t="s">
-        <v>1040</v>
+        <v>1046</v>
       </c>
       <c r="F727" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G727" s="26"/>
-      <c r="H727" s="6"/>
-      <c r="I727" s="20"/>
-      <c r="J727" s="20"/>
+      <c r="G727" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H727" s="6">
+        <v>44071</v>
+      </c>
+      <c r="I727" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J727" s="20" t="s">
+        <v>1045</v>
+      </c>
     </row>
     <row r="728" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A728" s="26"/>
-      <c r="B728" s="24"/>
-      <c r="C728" s="18"/>
-      <c r="D728" s="19"/>
-      <c r="E728" s="18"/>
-      <c r="F728" s="19"/>
-      <c r="G728" s="26"/>
-      <c r="H728" s="6"/>
-      <c r="I728" s="20"/>
+      <c r="A728" s="26">
+        <v>44074</v>
+      </c>
+      <c r="B728" s="24" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C728" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D728" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="E728" s="18" t="s">
+        <v>1051</v>
+      </c>
+      <c r="F728" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G728" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H728" s="6">
+        <v>44074</v>
+      </c>
+      <c r="I728" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J728" s="20"/>
     </row>
     <row r="729" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A729" s="26"/>
-      <c r="B729" s="24"/>
-      <c r="C729" s="18"/>
-      <c r="D729" s="19"/>
-      <c r="E729" s="18"/>
-      <c r="F729" s="19"/>
-      <c r="G729" s="26"/>
-      <c r="H729" s="6"/>
-      <c r="I729" s="20"/>
+      <c r="A729" s="26">
+        <v>44074</v>
+      </c>
+      <c r="B729" s="24" t="s">
+        <v>482</v>
+      </c>
+      <c r="C729" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D729" s="19" t="s">
+        <v>735</v>
+      </c>
+      <c r="E729" s="18" t="s">
+        <v>1052</v>
+      </c>
+      <c r="F729" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G729" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H729" s="6">
+        <v>44074</v>
+      </c>
+      <c r="I729" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J729" s="20"/>
     </row>
     <row r="730" spans="1:10" x14ac:dyDescent="0.25">
@@ -24960,9 +25112,7 @@
       <c r="B730" s="24"/>
       <c r="C730" s="18"/>
       <c r="D730" s="19"/>
-      <c r="E730" s="18" t="s">
-        <v>918</v>
-      </c>
+      <c r="E730" s="18"/>
       <c r="F730" s="19"/>
       <c r="G730" s="26"/>
       <c r="H730" s="6"/>
@@ -24981,8 +25131,58 @@
       <c r="I731" s="20"/>
       <c r="J731" s="20"/>
     </row>
+    <row r="732" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A732" s="26"/>
+      <c r="B732" s="24"/>
+      <c r="C732" s="18"/>
+      <c r="D732" s="19"/>
+      <c r="E732" s="18"/>
+      <c r="F732" s="19"/>
+      <c r="G732" s="26"/>
+      <c r="H732" s="6"/>
+      <c r="I732" s="20"/>
+      <c r="J732" s="20"/>
+    </row>
+    <row r="733" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A733" s="26"/>
+      <c r="B733" s="24"/>
+      <c r="C733" s="18"/>
+      <c r="D733" s="19"/>
+      <c r="E733" s="18"/>
+      <c r="F733" s="19"/>
+      <c r="G733" s="26"/>
+      <c r="H733" s="6"/>
+      <c r="I733" s="20"/>
+      <c r="J733" s="20"/>
+    </row>
+    <row r="734" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A734" s="26"/>
+      <c r="B734" s="24"/>
+      <c r="C734" s="18"/>
+      <c r="D734" s="19"/>
+      <c r="E734" s="18" t="s">
+        <v>918</v>
+      </c>
+      <c r="F734" s="19"/>
+      <c r="G734" s="26"/>
+      <c r="H734" s="6"/>
+      <c r="I734" s="20"/>
+      <c r="J734" s="20"/>
+    </row>
+    <row r="735" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A735" s="26"/>
+      <c r="B735" s="24"/>
+      <c r="C735" s="18"/>
+      <c r="D735" s="19"/>
+      <c r="E735" s="18"/>
+      <c r="F735" s="19"/>
+      <c r="G735" s="26"/>
+      <c r="H735" s="6"/>
+      <c r="I735" s="20"/>
+      <c r="J735" s="20"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J715" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J727" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="10" firstPageNumber="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Natureza no CNA e ND Rentabilidade
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59743C94-1AB3-42FB-9A4D-EDEF150B10FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733B368F-AB13-4C4B-845C-CD4627C585DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5330" uniqueCount="1170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5354" uniqueCount="1176">
   <si>
     <t>Prioridade</t>
   </si>
@@ -3750,6 +3750,24 @@
   </si>
   <si>
     <t>Conferência NFs de setembro</t>
+  </si>
+  <si>
+    <t>Alterar dia de vencimento do ISS Barueri para dia 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MV_DIAISS </t>
+  </si>
+  <si>
+    <t>Alterar o superior dos usuários da TI para Rafael e remover o Rafael do staf do Anderson</t>
+  </si>
+  <si>
+    <t>MV_XXUSERS 000011/000016/000076/000093/000194/000056/000103/000165/ (falta ver nas outras empresas)</t>
+  </si>
+  <si>
+    <t>Atualizações: 20-10-09-MONITOR_ELECTRON_0.2.8_WINDOWS-X64.SETUP, 20-08-31_ATUALIZACAO_12.1.25_CTB_EXPEDICAO_CONTINUA, 20-10-05_ATUALIZACAO_12.1.25_FAT_EXPEDICAO_CONTINUA</t>
+  </si>
+  <si>
+    <t>UPDDISTR executado para FATe CTB.</t>
   </si>
 </sst>
 </file>
@@ -4745,8 +4763,8 @@
   <dimension ref="A1:J811"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A793" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E802" sqref="E802"/>
+      <pane ySplit="1" topLeftCell="A802" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E804" sqref="E804"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27915,40 +27933,100 @@
       <c r="J801" s="20"/>
     </row>
     <row r="802" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A802" s="26"/>
-      <c r="B802" s="24"/>
-      <c r="C802" s="18"/>
-      <c r="D802" s="19"/>
-      <c r="E802" s="18"/>
-      <c r="F802" s="19"/>
-      <c r="G802" s="26"/>
-      <c r="H802" s="6"/>
-      <c r="I802" s="20"/>
-      <c r="J802" s="20"/>
-    </row>
-    <row r="803" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A803" s="26"/>
-      <c r="B803" s="24"/>
-      <c r="C803" s="18"/>
-      <c r="D803" s="19"/>
-      <c r="E803" s="18"/>
-      <c r="F803" s="19"/>
-      <c r="G803" s="26"/>
-      <c r="H803" s="6"/>
-      <c r="I803" s="20"/>
-      <c r="J803" s="20"/>
-    </row>
-    <row r="804" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A804" s="26"/>
-      <c r="B804" s="24"/>
-      <c r="C804" s="18"/>
-      <c r="D804" s="19"/>
-      <c r="E804" s="18"/>
-      <c r="F804" s="19"/>
-      <c r="G804" s="26"/>
-      <c r="H804" s="6"/>
-      <c r="I804" s="20"/>
-      <c r="J804" s="20"/>
+      <c r="A802" s="26">
+        <v>44112</v>
+      </c>
+      <c r="B802" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C802" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D802" s="19" t="s">
+        <v>906</v>
+      </c>
+      <c r="E802" s="18" t="s">
+        <v>1170</v>
+      </c>
+      <c r="F802" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G802" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H802" s="6">
+        <v>44113</v>
+      </c>
+      <c r="I802" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J802" s="20" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="803" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A803" s="26">
+        <v>44113</v>
+      </c>
+      <c r="B803" s="24" t="s">
+        <v>817</v>
+      </c>
+      <c r="C803" s="18" t="s">
+        <v>818</v>
+      </c>
+      <c r="D803" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="E803" s="18" t="s">
+        <v>1172</v>
+      </c>
+      <c r="F803" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G803" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H803" s="6">
+        <v>44113</v>
+      </c>
+      <c r="I803" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J803" s="20" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="804" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A804" s="26">
+        <v>44115</v>
+      </c>
+      <c r="B804" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C804" s="18" t="s">
+        <v>645</v>
+      </c>
+      <c r="D804" s="19" t="s">
+        <v>710</v>
+      </c>
+      <c r="E804" s="18" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F804" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G804" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H804" s="6">
+        <v>44115</v>
+      </c>
+      <c r="I804" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J804" s="20" t="s">
+        <v>1175</v>
+      </c>
     </row>
     <row r="805" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A805" s="26"/>

</xml_diff>

<commit_message>
Consulta pedido - marcação Doc Saida
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C987CDD5-6DFE-4CF3-8DE0-78E066ADADAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8892360-50B2-462F-AC45-CB74E3FD723C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7890" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="221" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5363" uniqueCount="1178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5460" uniqueCount="1192">
   <si>
     <t>Prioridade</t>
   </si>
@@ -2958,9 +2958,6 @@
     <t>Ainda continua saindo o valor diferenciado da pensão das rescisões, segue dois casos</t>
   </si>
   <si>
-    <t>Atualizar modulo fiscal</t>
-  </si>
-  <si>
     <t>Adiantamento a empregados da BHG Osasco referente o mês 03/2020 que não consta os títulos do financeiro, é o mesmo caso de indenizações a pagar</t>
   </si>
   <si>
@@ -3770,11 +3767,56 @@
     <t>UPDDISTR executado para FATe CTB.</t>
   </si>
   <si>
-    <t>Criei o campo CNA_XXNAT na tabela de planilhas do contrato, pois tive uma situação onde a retenção de IRRF era só para um contrato do cliente, então alterei o sistema para considerar a Natureza do pedido de vendas (MV_1DUPNAT), então no momento do encerramento da medição eu gravo a Natureza do pedido ou da Planilha (se informado) ou do cliente.</t>
-  </si>
-  <si>
     <t>MV_1DUPNAT = 
 SC5-&gt;C5_NATUREZ</t>
+  </si>
+  <si>
+    <t>Solicita alterar os centros de custos dos Docs de Entrada: 000048320, 000048543, 000048699, 000048226, 000048544 e 000048715 para 302000508 - Balsa Nova</t>
+  </si>
+  <si>
+    <t>Alterar a NF 551 para reter ISS e parametrizar o cliente 000331 para reter ISS.</t>
+  </si>
+  <si>
+    <t>Solicita acerto na integração de alguns título de pensão alimentícia - Interior 3</t>
+  </si>
+  <si>
+    <t>Criei o campo CNA_XXNAT na tabela de planilhas do contrato, pois tive uma situação onde a retenção de IRRF era só para um contrato do cliente, então alterei o sistema para considerar a Natureza do pedido de vendas (MV_1DUPNAT), então no momento do encerramento da medição eu gravo a Natureza do pedido ou da Planilha (se informado) ou do cliente. (ticket Totvs 9983158).</t>
+  </si>
+  <si>
+    <t>Preciso gerar borderô do titulo LF 063893 VT = INTERIOR 3 = R$ 1.452,00 e o Microsiga não deixa gerar borderô (devido ser TIPO CLA)</t>
+  </si>
+  <si>
+    <t>Problemas com dizimas na integração Rubi-Microsiga</t>
+  </si>
+  <si>
+    <t>Controladora</t>
+  </si>
+  <si>
+    <t>Corrigir o produto do contrato 334000521</t>
+  </si>
+  <si>
+    <t>Informo que o contrato  ( CT 013/2015 ) DAESP precisa ser alterado o polo de recolhimento do ISS em 2% retido para o município de São Paulo</t>
+  </si>
+  <si>
+    <t>Acertos conforme planilha fornecida - EFD BK Setembro 2020</t>
+  </si>
+  <si>
+    <t>Suportes e treinamento para a BK Corretora, referente a titulos de adiantamento do contas a receber e compensações</t>
+  </si>
+  <si>
+    <t>Desenvolvimento de consulta a pedidos de Venda contendo informações similares ao RM da Petrobrás, mas para uso geral de qualquer pedido, contendo impostos retidos, município de prestação etc.</t>
+  </si>
+  <si>
+    <t>Criar opção para consultar os pedidos marcados na preparação do doc de saída</t>
+  </si>
+  <si>
+    <t>Corrigir as NFs 21, 119 e 275 que foram bitributadas pelo cliente em São Paulo 5%</t>
+  </si>
+  <si>
+    <t>Correção da retenção contratual conforme planilha fornecida pela Fábia</t>
+  </si>
+  <si>
+    <t>Inclusão do campo retenção contratual no Mapa de Inss Retido e no Mapa de Medições</t>
   </si>
 </sst>
 </file>
@@ -4767,11 +4809,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J812"/>
+  <dimension ref="A1:J821"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A802" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E805" sqref="E805"/>
+      <pane ySplit="1" topLeftCell="A814" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E819" sqref="E819"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20141,10 +20183,10 @@
         <v>735</v>
       </c>
       <c r="E543" s="18" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F543" s="19" t="s">
         <v>1029</v>
-      </c>
-      <c r="F543" s="19" t="s">
-        <v>1030</v>
       </c>
       <c r="G543" s="26" t="s">
         <v>126</v>
@@ -20156,7 +20198,7 @@
         <v>17</v>
       </c>
       <c r="J543" s="20" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="544" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -22390,7 +22432,7 @@
         <v>17</v>
       </c>
       <c r="J617" s="20" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="618" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -23051,7 +23093,7 @@
         <v>751</v>
       </c>
       <c r="E639" s="18" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F639" s="19" t="s">
         <v>106</v>
@@ -23066,7 +23108,7 @@
         <v>17</v>
       </c>
       <c r="J639" s="20" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="640" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -23098,7 +23140,7 @@
         <v>17</v>
       </c>
       <c r="J640" s="20" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="641" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -23190,7 +23232,7 @@
         <v>17</v>
       </c>
       <c r="J643" s="20" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="644" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -23207,7 +23249,7 @@
         <v>765</v>
       </c>
       <c r="E644" s="18" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="F644" s="19" t="s">
         <v>110</v>
@@ -23222,7 +23264,7 @@
         <v>17</v>
       </c>
       <c r="J644" s="20" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="645" spans="1:10" x14ac:dyDescent="0.25">
@@ -23239,7 +23281,7 @@
         <v>751</v>
       </c>
       <c r="E645" s="18" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F645" s="19" t="s">
         <v>106</v>
@@ -23263,13 +23305,13 @@
         <v>518</v>
       </c>
       <c r="C646" s="18" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D646" s="19" t="s">
         <v>751</v>
       </c>
       <c r="E646" s="18" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F646" s="19" t="s">
         <v>61</v>
@@ -23299,7 +23341,7 @@
         <v>751</v>
       </c>
       <c r="E647" s="18" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F647" s="19" t="s">
         <v>106</v>
@@ -23329,7 +23371,7 @@
         <v>751</v>
       </c>
       <c r="E648" s="18" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="F648" s="19" t="s">
         <v>106</v>
@@ -23344,7 +23386,7 @@
         <v>17</v>
       </c>
       <c r="J648" s="20" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="649" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -23361,7 +23403,7 @@
         <v>765</v>
       </c>
       <c r="E649" s="18" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="F649" s="19" t="s">
         <v>86</v>
@@ -23391,7 +23433,7 @@
         <v>751</v>
       </c>
       <c r="E650" s="18" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="F650" s="19" t="s">
         <v>86</v>
@@ -23421,7 +23463,7 @@
         <v>681</v>
       </c>
       <c r="E651" s="18" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F651" s="19" t="s">
         <v>528</v>
@@ -23436,7 +23478,7 @@
         <v>17</v>
       </c>
       <c r="J651" s="20" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="652" spans="1:10" x14ac:dyDescent="0.25">
@@ -23453,7 +23495,7 @@
         <v>751</v>
       </c>
       <c r="E652" s="18" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="F652" s="19" t="s">
         <v>498</v>
@@ -23468,7 +23510,7 @@
         <v>17</v>
       </c>
       <c r="J652" s="20" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="653" spans="1:10" x14ac:dyDescent="0.25">
@@ -23485,7 +23527,7 @@
         <v>751</v>
       </c>
       <c r="E653" s="18" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="F653" s="19" t="s">
         <v>86</v>
@@ -23500,7 +23542,7 @@
         <v>17</v>
       </c>
       <c r="J653" s="20" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="654" spans="1:10" x14ac:dyDescent="0.25">
@@ -23517,7 +23559,7 @@
         <v>751</v>
       </c>
       <c r="E654" s="18" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="F654" s="19" t="s">
         <v>106</v>
@@ -23547,7 +23589,7 @@
         <v>751</v>
       </c>
       <c r="E655" s="18" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="F655" s="19" t="s">
         <v>106</v>
@@ -23568,7 +23610,7 @@
         <v>44047</v>
       </c>
       <c r="B656" s="24" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="C656" s="18" t="s">
         <v>29</v>
@@ -23577,7 +23619,7 @@
         <v>751</v>
       </c>
       <c r="E656" s="18" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F656" s="19" t="s">
         <v>61</v>
@@ -23592,7 +23634,7 @@
         <v>17</v>
       </c>
       <c r="J656" s="20" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="657" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -23609,7 +23651,7 @@
         <v>751</v>
       </c>
       <c r="E657" s="18" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="F657" s="19" t="s">
         <v>110</v>
@@ -23633,7 +23675,7 @@
         <v>751</v>
       </c>
       <c r="E658" s="18" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="F658" s="19" t="s">
         <v>61</v>
@@ -23663,7 +23705,7 @@
         <v>751</v>
       </c>
       <c r="E659" s="18" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="F659" s="19" t="s">
         <v>106</v>
@@ -23678,7 +23720,7 @@
         <v>12</v>
       </c>
       <c r="J659" s="20" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="660" spans="1:10" x14ac:dyDescent="0.25">
@@ -23695,7 +23737,7 @@
         <v>751</v>
       </c>
       <c r="E660" s="18" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="F660" s="19" t="s">
         <v>61</v>
@@ -23725,7 +23767,7 @@
         <v>751</v>
       </c>
       <c r="E661" s="18" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="F661" s="19" t="s">
         <v>110</v>
@@ -23740,7 +23782,7 @@
         <v>17</v>
       </c>
       <c r="J661" s="20" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="662" spans="1:10" x14ac:dyDescent="0.25">
@@ -23757,7 +23799,7 @@
         <v>681</v>
       </c>
       <c r="E662" s="18" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="F662" s="19" t="s">
         <v>86</v>
@@ -23787,7 +23829,7 @@
         <v>751</v>
       </c>
       <c r="E663" s="18" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F663" s="19" t="s">
         <v>110</v>
@@ -23817,7 +23859,7 @@
         <v>751</v>
       </c>
       <c r="E664" s="18" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="F664" s="19" t="s">
         <v>106</v>
@@ -23847,7 +23889,7 @@
         <v>681</v>
       </c>
       <c r="E665" s="18" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="F665" s="19" t="s">
         <v>110</v>
@@ -23862,7 +23904,7 @@
         <v>17</v>
       </c>
       <c r="J665" s="20" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="666" spans="1:10" x14ac:dyDescent="0.25">
@@ -23879,7 +23921,7 @@
         <v>681</v>
       </c>
       <c r="E666" s="18" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F666" s="19" t="s">
         <v>86</v>
@@ -23909,7 +23951,7 @@
         <v>681</v>
       </c>
       <c r="E667" s="18" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="F667" s="19" t="s">
         <v>106</v>
@@ -23939,7 +23981,7 @@
         <v>681</v>
       </c>
       <c r="E668" s="18" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="F668" s="19" t="s">
         <v>106</v>
@@ -23969,7 +24011,7 @@
         <v>681</v>
       </c>
       <c r="E669" s="18" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="F669" s="19" t="s">
         <v>86</v>
@@ -23999,7 +24041,7 @@
         <v>681</v>
       </c>
       <c r="E670" s="18" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="F670" s="19" t="s">
         <v>240</v>
@@ -24029,7 +24071,7 @@
         <v>681</v>
       </c>
       <c r="E671" s="18" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="F671" s="19" t="s">
         <v>110</v>
@@ -24044,7 +24086,7 @@
         <v>17</v>
       </c>
       <c r="J671" s="20" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="672" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -24061,7 +24103,7 @@
         <v>630</v>
       </c>
       <c r="E672" s="18" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F672" s="19" t="s">
         <v>106</v>
@@ -24091,7 +24133,7 @@
         <v>630</v>
       </c>
       <c r="E673" s="18" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="F673" s="19" t="s">
         <v>86</v>
@@ -24121,7 +24163,7 @@
         <v>765</v>
       </c>
       <c r="E674" s="18" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="F674" s="19" t="s">
         <v>106</v>
@@ -24151,7 +24193,7 @@
         <v>630</v>
       </c>
       <c r="E675" s="18" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="F675" s="19" t="s">
         <v>110</v>
@@ -24160,7 +24202,7 @@
       <c r="H675" s="6"/>
       <c r="I675" s="20"/>
       <c r="J675" s="20" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="676" spans="1:10" x14ac:dyDescent="0.25">
@@ -24177,7 +24219,7 @@
         <v>826</v>
       </c>
       <c r="E676" s="18" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="F676" s="19" t="s">
         <v>86</v>
@@ -24192,7 +24234,7 @@
         <v>17</v>
       </c>
       <c r="J676" s="20" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="677" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -24200,7 +24242,7 @@
         <v>44055</v>
       </c>
       <c r="B677" s="24" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C677" s="18" t="s">
         <v>552</v>
@@ -24209,7 +24251,7 @@
         <v>630</v>
       </c>
       <c r="E677" s="18" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="F677" s="19" t="s">
         <v>498</v>
@@ -24224,7 +24266,7 @@
         <v>17</v>
       </c>
       <c r="J677" s="20" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="678" spans="1:10" x14ac:dyDescent="0.25">
@@ -24232,7 +24274,7 @@
         <v>44055</v>
       </c>
       <c r="B678" s="24" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C678" s="18" t="s">
         <v>552</v>
@@ -24241,7 +24283,7 @@
         <v>630</v>
       </c>
       <c r="E678" s="18" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="F678" s="19"/>
       <c r="G678" s="26"/>
@@ -24254,7 +24296,7 @@
         <v>44055</v>
       </c>
       <c r="B679" s="24" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C679" s="18" t="s">
         <v>552</v>
@@ -24263,7 +24305,7 @@
         <v>630</v>
       </c>
       <c r="E679" s="18" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="F679" s="19"/>
       <c r="G679" s="26"/>
@@ -24276,7 +24318,7 @@
         <v>44055</v>
       </c>
       <c r="B680" s="24" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C680" s="18" t="s">
         <v>552</v>
@@ -24285,7 +24327,7 @@
         <v>630</v>
       </c>
       <c r="E680" s="18" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="F680" s="19"/>
       <c r="G680" s="26"/>
@@ -24307,7 +24349,7 @@
         <v>630</v>
       </c>
       <c r="E681" s="18" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="F681" s="19"/>
       <c r="G681" s="26"/>
@@ -24329,7 +24371,7 @@
         <v>630</v>
       </c>
       <c r="E682" s="18" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="F682" s="19"/>
       <c r="G682" s="26"/>
@@ -24351,7 +24393,7 @@
         <v>681</v>
       </c>
       <c r="E683" s="18" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="F683" s="19" t="s">
         <v>106</v>
@@ -24366,7 +24408,7 @@
         <v>17</v>
       </c>
       <c r="J683" s="20" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="684" spans="1:10" ht="140.25" x14ac:dyDescent="0.25">
@@ -24377,13 +24419,13 @@
         <v>23</v>
       </c>
       <c r="C684" s="18" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="D684" s="19" t="s">
         <v>681</v>
       </c>
       <c r="E684" s="18" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="F684" s="19" t="s">
         <v>110</v>
@@ -24398,7 +24440,7 @@
         <v>17</v>
       </c>
       <c r="J684" s="24" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="685" spans="1:10" ht="51" x14ac:dyDescent="0.25">
@@ -24415,7 +24457,7 @@
         <v>630</v>
       </c>
       <c r="E685" s="18" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="F685" s="19" t="s">
         <v>106</v>
@@ -24430,7 +24472,7 @@
         <v>17</v>
       </c>
       <c r="J685" s="20" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="686" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -24438,7 +24480,7 @@
         <v>44056</v>
       </c>
       <c r="B686" s="24" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C686" s="18" t="s">
         <v>10</v>
@@ -24447,7 +24489,7 @@
         <v>630</v>
       </c>
       <c r="E686" s="18" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="F686" s="19" t="s">
         <v>106</v>
@@ -24477,7 +24519,7 @@
         <v>681</v>
       </c>
       <c r="E687" s="18" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="F687" s="19" t="s">
         <v>86</v>
@@ -24492,7 +24534,7 @@
         <v>17</v>
       </c>
       <c r="J687" s="20" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="688" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -24509,7 +24551,7 @@
         <v>681</v>
       </c>
       <c r="E688" s="18" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="F688" s="19" t="s">
         <v>86</v>
@@ -24524,7 +24566,7 @@
         <v>17</v>
       </c>
       <c r="J688" s="20" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="689" spans="1:10" x14ac:dyDescent="0.25">
@@ -24541,7 +24583,7 @@
         <v>630</v>
       </c>
       <c r="E689" s="18" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="F689" s="19" t="s">
         <v>110</v>
@@ -24571,7 +24613,7 @@
         <v>630</v>
       </c>
       <c r="E690" s="18" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="F690" s="19" t="s">
         <v>106</v>
@@ -24601,7 +24643,7 @@
         <v>630</v>
       </c>
       <c r="E691" s="18" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="F691" s="19" t="s">
         <v>106</v>
@@ -24631,7 +24673,7 @@
         <v>710</v>
       </c>
       <c r="E692" s="18" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="F692" s="19" t="s">
         <v>106</v>
@@ -24661,7 +24703,7 @@
         <v>765</v>
       </c>
       <c r="E693" s="18" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="F693" s="19" t="s">
         <v>110</v>
@@ -24691,7 +24733,7 @@
         <v>630</v>
       </c>
       <c r="E694" s="18" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F694" s="19" t="s">
         <v>106</v>
@@ -24706,7 +24748,7 @@
         <v>17</v>
       </c>
       <c r="J694" s="20" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="695" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -24723,7 +24765,7 @@
         <v>765</v>
       </c>
       <c r="E695" s="18" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="F695" s="19" t="s">
         <v>106</v>
@@ -24738,7 +24780,7 @@
         <v>17</v>
       </c>
       <c r="J695" s="20" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="696" spans="1:10" x14ac:dyDescent="0.25">
@@ -24755,7 +24797,7 @@
         <v>681</v>
       </c>
       <c r="E696" s="18" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="F696" s="19" t="s">
         <v>703</v>
@@ -24785,7 +24827,7 @@
         <v>735</v>
       </c>
       <c r="E697" s="18" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="F697" s="19" t="s">
         <v>528</v>
@@ -24815,7 +24857,7 @@
         <v>630</v>
       </c>
       <c r="E698" s="18" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="F698" s="19" t="s">
         <v>110</v>
@@ -24845,7 +24887,7 @@
         <v>681</v>
       </c>
       <c r="E699" s="18" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="F699" s="19" t="s">
         <v>703</v>
@@ -24875,7 +24917,7 @@
         <v>630</v>
       </c>
       <c r="E700" s="18" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="F700" s="19" t="s">
         <v>703</v>
@@ -24905,7 +24947,7 @@
         <v>765</v>
       </c>
       <c r="E701" s="18" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="F701" s="19" t="s">
         <v>86</v>
@@ -24935,7 +24977,7 @@
         <v>630</v>
       </c>
       <c r="E702" s="18" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="F702" s="19" t="s">
         <v>61</v>
@@ -24950,7 +24992,7 @@
         <v>17</v>
       </c>
       <c r="J702" s="20" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="703" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -24967,7 +25009,7 @@
         <v>630</v>
       </c>
       <c r="E703" s="18" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="F703" s="19" t="s">
         <v>86</v>
@@ -24982,7 +25024,7 @@
         <v>12</v>
       </c>
       <c r="J703" s="20" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="704" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -24999,7 +25041,7 @@
         <v>630</v>
       </c>
       <c r="E704" s="18" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="F704" s="19" t="s">
         <v>86</v>
@@ -25029,7 +25071,7 @@
         <v>630</v>
       </c>
       <c r="E705" s="18" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="F705" s="19" t="s">
         <v>86</v>
@@ -25041,7 +25083,7 @@
         <v>44062</v>
       </c>
       <c r="I705" s="20" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="J705" s="20"/>
     </row>
@@ -25059,7 +25101,7 @@
         <v>681</v>
       </c>
       <c r="E706" s="18" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="F706" s="19" t="s">
         <v>61</v>
@@ -25080,7 +25122,7 @@
         <v>44062</v>
       </c>
       <c r="B707" s="24" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C707" s="18" t="s">
         <v>552</v>
@@ -25089,7 +25131,7 @@
         <v>630</v>
       </c>
       <c r="E707" s="18" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="F707" s="19" t="s">
         <v>86</v>
@@ -25104,7 +25146,7 @@
         <v>17</v>
       </c>
       <c r="J707" s="20" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="708" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -25121,7 +25163,7 @@
         <v>630</v>
       </c>
       <c r="E708" s="18" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="F708" s="19" t="s">
         <v>86</v>
@@ -25136,7 +25178,7 @@
         <v>12</v>
       </c>
       <c r="J708" s="20" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="709" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -25153,7 +25195,7 @@
         <v>681</v>
       </c>
       <c r="E709" s="18" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="F709" s="19" t="s">
         <v>110</v>
@@ -25168,7 +25210,7 @@
         <v>17</v>
       </c>
       <c r="J709" s="20" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="710" spans="1:10" ht="51" x14ac:dyDescent="0.25">
@@ -25185,7 +25227,7 @@
         <v>630</v>
       </c>
       <c r="E710" s="18" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="F710" s="19" t="s">
         <v>240</v>
@@ -25200,7 +25242,7 @@
         <v>17</v>
       </c>
       <c r="J710" s="20" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="711" spans="1:10" x14ac:dyDescent="0.25">
@@ -25208,7 +25250,7 @@
         <v>44063</v>
       </c>
       <c r="B711" s="24" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C711" s="18" t="s">
         <v>21</v>
@@ -25217,7 +25259,7 @@
         <v>735</v>
       </c>
       <c r="E711" s="18" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="F711" s="19" t="s">
         <v>86</v>
@@ -25232,7 +25274,7 @@
         <v>17</v>
       </c>
       <c r="J711" s="20" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="712" spans="1:10" x14ac:dyDescent="0.25">
@@ -25240,7 +25282,7 @@
         <v>44063</v>
       </c>
       <c r="B712" s="24" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C712" s="18" t="s">
         <v>21</v>
@@ -25249,7 +25291,7 @@
         <v>735</v>
       </c>
       <c r="E712" s="18" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="F712" s="19" t="s">
         <v>110</v>
@@ -25279,7 +25321,7 @@
         <v>751</v>
       </c>
       <c r="E713" s="18" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="F713" s="19" t="s">
         <v>110</v>
@@ -25294,7 +25336,7 @@
         <v>17</v>
       </c>
       <c r="J713" s="20" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="714" spans="1:10" x14ac:dyDescent="0.25">
@@ -25302,7 +25344,7 @@
         <v>44064</v>
       </c>
       <c r="B714" s="24" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C714" s="18" t="s">
         <v>21</v>
@@ -25311,7 +25353,7 @@
         <v>751</v>
       </c>
       <c r="E714" s="18" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="F714" s="19" t="s">
         <v>106</v>
@@ -25332,7 +25374,7 @@
         <v>44064</v>
       </c>
       <c r="B715" s="24" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C715" s="18" t="s">
         <v>21</v>
@@ -25341,7 +25383,7 @@
         <v>751</v>
       </c>
       <c r="E715" s="18" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F715" s="19" t="s">
         <v>86</v>
@@ -25356,7 +25398,7 @@
         <v>17</v>
       </c>
       <c r="J715" s="20" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="716" spans="1:10" ht="51" x14ac:dyDescent="0.25">
@@ -25373,7 +25415,7 @@
         <v>751</v>
       </c>
       <c r="E716" s="18" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="F716" s="19" t="s">
         <v>61</v>
@@ -25403,7 +25445,7 @@
         <v>681</v>
       </c>
       <c r="E717" s="18" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F717" s="19" t="s">
         <v>61</v>
@@ -25433,7 +25475,7 @@
         <v>681</v>
       </c>
       <c r="E718" s="18" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="F718" s="19" t="s">
         <v>106</v>
@@ -25463,7 +25505,7 @@
         <v>735</v>
       </c>
       <c r="E719" s="18" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="F719" s="19"/>
       <c r="G719" s="26" t="s">
@@ -25487,7 +25529,7 @@
         <v>630</v>
       </c>
       <c r="E720" s="18" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="F720" s="19" t="s">
         <v>110</v>
@@ -25502,7 +25544,7 @@
         <v>17</v>
       </c>
       <c r="J720" s="20" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="721" spans="1:10" x14ac:dyDescent="0.25">
@@ -25510,7 +25552,7 @@
         <v>44069</v>
       </c>
       <c r="B721" s="24" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C721" s="18" t="s">
         <v>21</v>
@@ -25519,7 +25561,7 @@
         <v>681</v>
       </c>
       <c r="E721" s="18" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="F721" s="19" t="s">
         <v>86</v>
@@ -25534,7 +25576,7 @@
         <v>17</v>
       </c>
       <c r="J721" s="20" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="722" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -25551,7 +25593,7 @@
         <v>681</v>
       </c>
       <c r="E722" s="18" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="F722" s="19" t="s">
         <v>159</v>
@@ -25566,7 +25608,7 @@
         <v>17</v>
       </c>
       <c r="J722" s="20" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="723" spans="1:10" x14ac:dyDescent="0.25">
@@ -25583,7 +25625,7 @@
         <v>681</v>
       </c>
       <c r="E723" s="18" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="F723" s="19" t="s">
         <v>106</v>
@@ -25598,7 +25640,7 @@
         <v>17</v>
       </c>
       <c r="J723" s="20" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="724" spans="1:10" x14ac:dyDescent="0.25">
@@ -25615,7 +25657,7 @@
         <v>681</v>
       </c>
       <c r="E724" s="18" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="F724" s="19" t="s">
         <v>61</v>
@@ -25630,7 +25672,7 @@
         <v>17</v>
       </c>
       <c r="J724" s="20" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="725" spans="1:10" x14ac:dyDescent="0.25">
@@ -25638,7 +25680,7 @@
         <v>44071</v>
       </c>
       <c r="B725" s="24" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="C725" s="18" t="s">
         <v>21</v>
@@ -25647,7 +25689,7 @@
         <v>630</v>
       </c>
       <c r="E725" s="18" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="F725" s="19" t="s">
         <v>106</v>
@@ -25662,7 +25704,7 @@
         <v>17</v>
       </c>
       <c r="J725" s="20" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="726" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -25679,7 +25721,7 @@
         <v>681</v>
       </c>
       <c r="E726" s="18" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="F726" s="19" t="s">
         <v>61</v>
@@ -25694,7 +25736,7 @@
         <v>17</v>
       </c>
       <c r="J726" s="20" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="727" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -25711,7 +25753,7 @@
         <v>630</v>
       </c>
       <c r="E727" s="18" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F727" s="19" t="s">
         <v>110</v>
@@ -25741,7 +25783,7 @@
         <v>630</v>
       </c>
       <c r="E728" s="18" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="F728" s="19" t="s">
         <v>86</v>
@@ -25756,7 +25798,7 @@
         <v>17</v>
       </c>
       <c r="J728" s="20" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="729" spans="1:10" x14ac:dyDescent="0.25">
@@ -25764,7 +25806,7 @@
         <v>44074</v>
       </c>
       <c r="B729" s="24" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="C729" s="18" t="s">
         <v>10</v>
@@ -25773,7 +25815,7 @@
         <v>681</v>
       </c>
       <c r="E729" s="18" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="F729" s="19" t="s">
         <v>106</v>
@@ -25803,7 +25845,7 @@
         <v>735</v>
       </c>
       <c r="E730" s="18" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="F730" s="19" t="s">
         <v>106</v>
@@ -25833,7 +25875,7 @@
         <v>681</v>
       </c>
       <c r="E731" s="18" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="F731" s="19" t="s">
         <v>516</v>
@@ -25854,16 +25896,16 @@
         <v>44076</v>
       </c>
       <c r="B732" s="24" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C732" s="18" t="s">
         <v>1072</v>
-      </c>
-      <c r="C732" s="18" t="s">
-        <v>1073</v>
       </c>
       <c r="D732" s="19" t="s">
         <v>751</v>
       </c>
       <c r="E732" s="18" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="F732" s="19" t="s">
         <v>61</v>
@@ -25893,7 +25935,7 @@
         <v>751</v>
       </c>
       <c r="E733" s="18" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="F733" s="19" t="s">
         <v>86</v>
@@ -25923,7 +25965,7 @@
         <v>751</v>
       </c>
       <c r="E734" s="18" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="F734" s="19" t="s">
         <v>106</v>
@@ -25953,10 +25995,10 @@
         <v>751</v>
       </c>
       <c r="E735" s="18" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="F735" s="19" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="G735" s="26" t="s">
         <v>126</v>
@@ -25983,7 +26025,7 @@
         <v>751</v>
       </c>
       <c r="E736" s="18" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="F736" s="19" t="s">
         <v>106</v>
@@ -26013,7 +26055,7 @@
         <v>751</v>
       </c>
       <c r="E737" s="18" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="F737" s="19" t="s">
         <v>110</v>
@@ -26043,7 +26085,7 @@
         <v>751</v>
       </c>
       <c r="E738" s="18" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="F738" s="19" t="s">
         <v>106</v>
@@ -26058,7 +26100,7 @@
         <v>17</v>
       </c>
       <c r="J738" s="20" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="739" spans="1:10" x14ac:dyDescent="0.25">
@@ -26075,7 +26117,7 @@
         <v>751</v>
       </c>
       <c r="E739" s="18" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="F739" s="19" t="s">
         <v>110</v>
@@ -26105,7 +26147,7 @@
         <v>751</v>
       </c>
       <c r="E740" s="18" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="F740" s="19" t="s">
         <v>498</v>
@@ -26135,7 +26177,7 @@
         <v>735</v>
       </c>
       <c r="E741" s="18" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="F741" s="19" t="s">
         <v>106</v>
@@ -26150,7 +26192,7 @@
         <v>17</v>
       </c>
       <c r="J741" s="20" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="742" spans="1:10" x14ac:dyDescent="0.25">
@@ -26167,7 +26209,7 @@
         <v>906</v>
       </c>
       <c r="E742" s="18" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="F742" s="19" t="s">
         <v>106</v>
@@ -26197,7 +26239,7 @@
         <v>751</v>
       </c>
       <c r="E743" s="18" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="F743" s="19" t="s">
         <v>86</v>
@@ -26212,7 +26254,7 @@
         <v>17</v>
       </c>
       <c r="J743" s="20" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="744" spans="1:10" x14ac:dyDescent="0.25">
@@ -26229,7 +26271,7 @@
         <v>906</v>
       </c>
       <c r="E744" s="18" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="F744" s="19" t="s">
         <v>86</v>
@@ -26244,7 +26286,7 @@
         <v>17</v>
       </c>
       <c r="J744" s="20" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="745" spans="1:10" x14ac:dyDescent="0.25">
@@ -26261,7 +26303,7 @@
         <v>906</v>
       </c>
       <c r="E745" s="18" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="F745" s="19"/>
       <c r="G745" s="26"/>
@@ -26283,7 +26325,7 @@
         <v>751</v>
       </c>
       <c r="E746" s="18" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="F746" s="19" t="s">
         <v>106</v>
@@ -26298,7 +26340,7 @@
         <v>17</v>
       </c>
       <c r="J746" s="20" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="747" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -26306,7 +26348,7 @@
         <v>44084</v>
       </c>
       <c r="B747" s="24" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C747" s="18" t="s">
         <v>552</v>
@@ -26315,7 +26357,7 @@
         <v>906</v>
       </c>
       <c r="E747" s="18" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="F747" s="19" t="s">
         <v>61</v>
@@ -26330,7 +26372,7 @@
         <v>17</v>
       </c>
       <c r="J747" s="20" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="748" spans="1:10" x14ac:dyDescent="0.25">
@@ -26347,7 +26389,7 @@
         <v>751</v>
       </c>
       <c r="E748" s="18" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="F748" s="19"/>
       <c r="G748" s="26"/>
@@ -26369,7 +26411,7 @@
         <v>765</v>
       </c>
       <c r="E749" s="18" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="F749" s="19" t="s">
         <v>86</v>
@@ -26399,7 +26441,7 @@
         <v>751</v>
       </c>
       <c r="E750" s="18" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="F750" s="19" t="s">
         <v>106</v>
@@ -26414,7 +26456,7 @@
         <v>17</v>
       </c>
       <c r="J750" s="20" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="751" spans="1:10" x14ac:dyDescent="0.25">
@@ -26431,7 +26473,7 @@
         <v>906</v>
       </c>
       <c r="E751" s="18" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="F751" s="19" t="s">
         <v>106</v>
@@ -26446,7 +26488,7 @@
         <v>17</v>
       </c>
       <c r="J751" s="20" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="752" spans="1:10" x14ac:dyDescent="0.25">
@@ -26463,7 +26505,7 @@
         <v>751</v>
       </c>
       <c r="E752" s="18" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="F752" s="19" t="s">
         <v>106</v>
@@ -26484,7 +26526,7 @@
         <v>44085</v>
       </c>
       <c r="B753" s="24" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C753" s="18" t="s">
         <v>552</v>
@@ -26493,7 +26535,7 @@
         <v>751</v>
       </c>
       <c r="E753" s="18" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="F753" s="19" t="s">
         <v>86</v>
@@ -26508,7 +26550,7 @@
         <v>17</v>
       </c>
       <c r="J753" s="20" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="754" spans="1:10" x14ac:dyDescent="0.25">
@@ -26525,10 +26567,10 @@
         <v>751</v>
       </c>
       <c r="E754" s="18" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F754" s="19" t="s">
         <v>1125</v>
-      </c>
-      <c r="F754" s="19" t="s">
-        <v>1126</v>
       </c>
       <c r="G754" s="26" t="s">
         <v>126</v>
@@ -26555,7 +26597,7 @@
         <v>751</v>
       </c>
       <c r="E755" s="18" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F755" s="19" t="s">
         <v>163</v>
@@ -26576,7 +26618,7 @@
         <v>44088</v>
       </c>
       <c r="B756" s="24" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C756" s="18" t="s">
         <v>90</v>
@@ -26585,7 +26627,7 @@
         <v>751</v>
       </c>
       <c r="E756" s="18" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F756" s="19" t="s">
         <v>106</v>
@@ -26615,7 +26657,7 @@
         <v>630</v>
       </c>
       <c r="E757" s="18" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F757" s="19" t="s">
         <v>703</v>
@@ -26630,7 +26672,7 @@
         <v>17</v>
       </c>
       <c r="J757" s="20" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="758" spans="1:10" x14ac:dyDescent="0.25">
@@ -26641,13 +26683,13 @@
         <v>23</v>
       </c>
       <c r="C758" s="18" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="D758" s="19" t="s">
         <v>751</v>
       </c>
       <c r="E758" s="18" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="F758" s="19"/>
       <c r="G758" s="26"/>
@@ -26660,7 +26702,7 @@
         <v>44089</v>
       </c>
       <c r="B759" s="24" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C759" s="18" t="s">
         <v>21</v>
@@ -26669,7 +26711,7 @@
         <v>751</v>
       </c>
       <c r="E759" s="18" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="F759" s="19" t="s">
         <v>106</v>
@@ -26684,7 +26726,7 @@
         <v>12</v>
       </c>
       <c r="J759" s="20" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="760" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -26701,7 +26743,7 @@
         <v>630</v>
       </c>
       <c r="E760" s="18" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="F760" s="19" t="s">
         <v>110</v>
@@ -26731,7 +26773,7 @@
         <v>906</v>
       </c>
       <c r="E761" s="18" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="F761" s="19" t="s">
         <v>106</v>
@@ -26746,7 +26788,7 @@
         <v>17</v>
       </c>
       <c r="J761" s="20" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="762" spans="1:10" x14ac:dyDescent="0.25">
@@ -26763,7 +26805,7 @@
         <v>751</v>
       </c>
       <c r="E762" s="18" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="F762" s="19" t="s">
         <v>86</v>
@@ -26793,7 +26835,7 @@
         <v>751</v>
       </c>
       <c r="E763" s="18" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="F763" s="19" t="s">
         <v>106</v>
@@ -26823,7 +26865,7 @@
         <v>751</v>
       </c>
       <c r="E764" s="18" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="F764" s="19" t="s">
         <v>106</v>
@@ -26838,7 +26880,7 @@
         <v>17</v>
       </c>
       <c r="J764" s="20" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="765" spans="1:10" x14ac:dyDescent="0.25">
@@ -26855,7 +26897,7 @@
         <v>751</v>
       </c>
       <c r="E765" s="18" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="F765" s="19" t="s">
         <v>86</v>
@@ -26876,7 +26918,7 @@
         <v>44096</v>
       </c>
       <c r="B766" s="24" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C766" s="18" t="s">
         <v>552</v>
@@ -26885,7 +26927,7 @@
         <v>751</v>
       </c>
       <c r="E766" s="18" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="F766" s="19" t="s">
         <v>106</v>
@@ -26900,7 +26942,7 @@
         <v>12</v>
       </c>
       <c r="J766" s="18" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="767" spans="1:10" x14ac:dyDescent="0.25">
@@ -26911,13 +26953,13 @@
         <v>23</v>
       </c>
       <c r="C767" s="18" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="D767" s="19" t="s">
         <v>735</v>
       </c>
       <c r="E767" s="18" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="F767" s="19" t="s">
         <v>110</v>
@@ -26947,7 +26989,7 @@
         <v>681</v>
       </c>
       <c r="E768" s="18" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="F768" s="19" t="s">
         <v>110</v>
@@ -26977,7 +27019,7 @@
         <v>751</v>
       </c>
       <c r="E769" s="18" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="F769" s="19" t="s">
         <v>106</v>
@@ -27007,7 +27049,7 @@
         <v>751</v>
       </c>
       <c r="E770" s="18" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="F770" s="19" t="s">
         <v>86</v>
@@ -27037,7 +27079,7 @@
         <v>751</v>
       </c>
       <c r="E771" s="18" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="F771" s="19" t="s">
         <v>106</v>
@@ -27058,7 +27100,7 @@
         <v>44098</v>
       </c>
       <c r="B772" s="24" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C772" s="18" t="s">
         <v>552</v>
@@ -27067,7 +27109,7 @@
         <v>751</v>
       </c>
       <c r="E772" s="18" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="F772" s="19" t="s">
         <v>106</v>
@@ -27097,7 +27139,7 @@
         <v>751</v>
       </c>
       <c r="E773" s="18" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="F773" s="19"/>
       <c r="G773" s="26"/>
@@ -27119,7 +27161,7 @@
         <v>765</v>
       </c>
       <c r="E774" s="18" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="F774" s="19" t="s">
         <v>106</v>
@@ -27134,7 +27176,7 @@
         <v>17</v>
       </c>
       <c r="J774" s="20" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="775" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -27151,7 +27193,7 @@
         <v>630</v>
       </c>
       <c r="E775" s="18" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="F775" s="19" t="s">
         <v>498</v>
@@ -27166,7 +27208,7 @@
         <v>17</v>
       </c>
       <c r="J775" s="20" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="776" spans="1:10" x14ac:dyDescent="0.25">
@@ -27174,7 +27216,7 @@
         <v>44102</v>
       </c>
       <c r="B776" s="24" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C776" s="18" t="s">
         <v>552</v>
@@ -27183,7 +27225,7 @@
         <v>906</v>
       </c>
       <c r="E776" s="18" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="F776" s="19" t="s">
         <v>106</v>
@@ -27198,7 +27240,7 @@
         <v>17</v>
       </c>
       <c r="J776" s="20" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="777" spans="1:10" x14ac:dyDescent="0.25">
@@ -27215,7 +27257,7 @@
         <v>681</v>
       </c>
       <c r="E777" s="18" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="F777" s="19" t="s">
         <v>106</v>
@@ -27245,7 +27287,7 @@
         <v>906</v>
       </c>
       <c r="E778" s="18" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="F778" s="19" t="s">
         <v>106</v>
@@ -27275,7 +27317,7 @@
         <v>906</v>
       </c>
       <c r="E779" s="18" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="F779" s="19" t="s">
         <v>106</v>
@@ -27290,7 +27332,7 @@
         <v>17</v>
       </c>
       <c r="J779" s="20" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="780" spans="1:10" ht="51" x14ac:dyDescent="0.25">
@@ -27298,7 +27340,7 @@
         <v>44103</v>
       </c>
       <c r="B780" s="24" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C780" s="18" t="s">
         <v>90</v>
@@ -27307,7 +27349,7 @@
         <v>630</v>
       </c>
       <c r="E780" s="18" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="F780" s="19" t="s">
         <v>106</v>
@@ -27322,7 +27364,7 @@
         <v>12</v>
       </c>
       <c r="J780" s="20" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="781" spans="1:10" x14ac:dyDescent="0.25">
@@ -27339,7 +27381,7 @@
         <v>630</v>
       </c>
       <c r="E781" s="18" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="F781" s="19" t="s">
         <v>106</v>
@@ -27360,7 +27402,7 @@
         <v>44104</v>
       </c>
       <c r="B782" s="24" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="C782" s="18" t="s">
         <v>21</v>
@@ -27369,7 +27411,7 @@
         <v>630</v>
       </c>
       <c r="E782" s="18" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F782" s="19" t="s">
         <v>106</v>
@@ -27390,7 +27432,7 @@
         <v>44104</v>
       </c>
       <c r="B783" s="24" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="C783" s="18" t="s">
         <v>549</v>
@@ -27399,7 +27441,7 @@
         <v>630</v>
       </c>
       <c r="E783" s="18" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="F783" s="19" t="s">
         <v>106</v>
@@ -27420,16 +27462,16 @@
         <v>44105</v>
       </c>
       <c r="B784" s="24" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C784" s="18" t="s">
         <v>1072</v>
-      </c>
-      <c r="C784" s="18" t="s">
-        <v>1073</v>
       </c>
       <c r="D784" s="19" t="s">
         <v>906</v>
       </c>
       <c r="E784" s="18" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="F784" s="19" t="s">
         <v>86</v>
@@ -27459,7 +27501,7 @@
         <v>630</v>
       </c>
       <c r="E785" s="18" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="F785" s="19" t="s">
         <v>61</v>
@@ -27480,7 +27522,7 @@
         <v>44105</v>
       </c>
       <c r="B786" s="24" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="C786" s="18" t="s">
         <v>552</v>
@@ -27489,7 +27531,7 @@
         <v>906</v>
       </c>
       <c r="E786" s="18" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="F786" s="19" t="s">
         <v>523</v>
@@ -27504,7 +27546,7 @@
         <v>17</v>
       </c>
       <c r="J786" s="20" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="787" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -27512,7 +27554,7 @@
         <v>44106</v>
       </c>
       <c r="B787" s="24" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="C787" s="18" t="s">
         <v>21</v>
@@ -27521,7 +27563,7 @@
         <v>630</v>
       </c>
       <c r="E787" s="18" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="F787" s="19" t="s">
         <v>106</v>
@@ -27536,7 +27578,7 @@
         <v>12</v>
       </c>
       <c r="J787" s="20" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="788" spans="1:10" x14ac:dyDescent="0.25">
@@ -27553,7 +27595,7 @@
         <v>630</v>
       </c>
       <c r="E788" s="18" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="F788" s="19" t="s">
         <v>110</v>
@@ -27583,7 +27625,7 @@
         <v>630</v>
       </c>
       <c r="E789" s="18" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F789" s="19"/>
       <c r="G789" s="26"/>
@@ -27605,7 +27647,7 @@
         <v>630</v>
       </c>
       <c r="E790" s="18" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F790" s="19"/>
       <c r="G790" s="26"/>
@@ -27627,7 +27669,7 @@
         <v>906</v>
       </c>
       <c r="E791" s="18" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F791" s="19" t="s">
         <v>86</v>
@@ -27648,19 +27690,19 @@
         <v>44109</v>
       </c>
       <c r="B792" s="24" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C792" s="18" t="s">
         <v>1155</v>
-      </c>
-      <c r="C792" s="18" t="s">
-        <v>1156</v>
       </c>
       <c r="D792" s="19" t="s">
         <v>630</v>
       </c>
       <c r="E792" s="18" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F792" s="19" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="G792" s="26" t="s">
         <v>126</v>
@@ -27672,7 +27714,7 @@
         <v>17</v>
       </c>
       <c r="J792" s="20" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="793" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -27680,16 +27722,16 @@
         <v>44109</v>
       </c>
       <c r="B793" s="24" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="C793" s="18" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="D793" s="19" t="s">
         <v>630</v>
       </c>
       <c r="E793" s="18" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="F793" s="19" t="s">
         <v>106</v>
@@ -27704,7 +27746,7 @@
         <v>17</v>
       </c>
       <c r="J793" s="20" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="794" spans="1:10" x14ac:dyDescent="0.25">
@@ -27721,7 +27763,7 @@
         <v>630</v>
       </c>
       <c r="E794" s="18" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="F794" s="19" t="s">
         <v>106</v>
@@ -27751,7 +27793,7 @@
         <v>630</v>
       </c>
       <c r="E795" s="18" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="F795" s="19" t="s">
         <v>86</v>
@@ -27781,7 +27823,7 @@
         <v>630</v>
       </c>
       <c r="E796" s="18" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="F796" s="19" t="s">
         <v>86</v>
@@ -27811,7 +27853,7 @@
         <v>630</v>
       </c>
       <c r="E797" s="18" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="F797" s="19" t="s">
         <v>61</v>
@@ -27841,7 +27883,7 @@
         <v>630</v>
       </c>
       <c r="E798" s="18" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="F798" s="19" t="s">
         <v>106</v>
@@ -27871,7 +27913,7 @@
         <v>630</v>
       </c>
       <c r="E799" s="18" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="F799" s="19" t="s">
         <v>554</v>
@@ -27901,7 +27943,7 @@
         <v>906</v>
       </c>
       <c r="E800" s="18" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="F800" s="19" t="s">
         <v>86</v>
@@ -27916,7 +27958,7 @@
         <v>17</v>
       </c>
       <c r="J800" s="20" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="801" spans="1:10" x14ac:dyDescent="0.25">
@@ -27933,12 +27975,20 @@
         <v>906</v>
       </c>
       <c r="E801" s="18" t="s">
-        <v>1169</v>
-      </c>
-      <c r="F801" s="19"/>
-      <c r="G801" s="26"/>
-      <c r="H801" s="6"/>
-      <c r="I801" s="20"/>
+        <v>1168</v>
+      </c>
+      <c r="F801" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G801" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H801" s="6">
+        <v>44112</v>
+      </c>
+      <c r="I801" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J801" s="20"/>
     </row>
     <row r="802" spans="1:10" x14ac:dyDescent="0.25">
@@ -27955,7 +28005,7 @@
         <v>906</v>
       </c>
       <c r="E802" s="18" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="F802" s="19" t="s">
         <v>106</v>
@@ -27970,190 +28020,540 @@
         <v>17</v>
       </c>
       <c r="J802" s="20" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="803" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A803" s="26">
+        <v>44112</v>
+      </c>
+      <c r="B803" s="24" t="s">
+        <v>684</v>
+      </c>
+      <c r="C803" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D803" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="E803" s="18" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F803" s="19"/>
+      <c r="G803" s="26"/>
+      <c r="H803" s="6"/>
+      <c r="I803" s="20"/>
+      <c r="J803" s="20"/>
+    </row>
+    <row r="804" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A804" s="26">
+        <v>44112</v>
+      </c>
+      <c r="B804" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="C804" s="18" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D804" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="E804" s="18" t="s">
+        <v>1183</v>
+      </c>
+      <c r="F804" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G804" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H804" s="6">
+        <v>44112</v>
+      </c>
+      <c r="I804" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J804" s="20"/>
+    </row>
+    <row r="805" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A805" s="26">
+        <v>44113</v>
+      </c>
+      <c r="B805" s="24" t="s">
+        <v>522</v>
+      </c>
+      <c r="C805" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D805" s="19" t="s">
+        <v>751</v>
+      </c>
+      <c r="E805" s="18" t="s">
+        <v>1184</v>
+      </c>
+      <c r="F805" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G805" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H805" s="6">
+        <v>44113</v>
+      </c>
+      <c r="I805" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J805" s="20"/>
+    </row>
+    <row r="806" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A806" s="26">
+        <v>44113</v>
+      </c>
+      <c r="B806" s="24" t="s">
+        <v>817</v>
+      </c>
+      <c r="C806" s="18" t="s">
+        <v>818</v>
+      </c>
+      <c r="D806" s="19" t="s">
+        <v>681</v>
+      </c>
+      <c r="E806" s="18" t="s">
         <v>1171</v>
       </c>
-    </row>
-    <row r="803" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A803" s="26">
+      <c r="F806" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G806" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H806" s="6">
         <v>44113</v>
       </c>
-      <c r="B803" s="24" t="s">
-        <v>817</v>
-      </c>
-      <c r="C803" s="18" t="s">
-        <v>818</v>
-      </c>
-      <c r="D803" s="19" t="s">
+      <c r="I806" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J806" s="20" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="807" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A807" s="26">
+        <v>44113</v>
+      </c>
+      <c r="B807" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C807" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D807" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="E807" s="18" t="s">
+        <v>1180</v>
+      </c>
+      <c r="F807" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G807" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H807" s="6">
+        <v>44113</v>
+      </c>
+      <c r="I807" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J807" s="20"/>
+    </row>
+    <row r="808" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A808" s="26">
+        <v>44114</v>
+      </c>
+      <c r="B808" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C808" s="18" t="s">
+        <v>645</v>
+      </c>
+      <c r="D808" s="19" t="s">
+        <v>765</v>
+      </c>
+      <c r="E808" s="18" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F808" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G808" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H808" s="6">
+        <v>44114</v>
+      </c>
+      <c r="I808" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J808" s="20" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="809" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A809" s="26">
+        <v>44115</v>
+      </c>
+      <c r="B809" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C809" s="18" t="s">
+        <v>645</v>
+      </c>
+      <c r="D809" s="19" t="s">
+        <v>710</v>
+      </c>
+      <c r="E809" s="18" t="s">
+        <v>1173</v>
+      </c>
+      <c r="F809" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G809" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H809" s="6">
+        <v>44115</v>
+      </c>
+      <c r="I809" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J809" s="20" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="810" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A810" s="26">
+        <v>44117</v>
+      </c>
+      <c r="B810" s="24" t="s">
+        <v>522</v>
+      </c>
+      <c r="C810" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D810" s="19" t="s">
+        <v>751</v>
+      </c>
+      <c r="E810" s="18" t="s">
+        <v>1185</v>
+      </c>
+      <c r="F810" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G810" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H810" s="6">
+        <v>44117</v>
+      </c>
+      <c r="I810" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J810" s="20"/>
+    </row>
+    <row r="811" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A811" s="26">
+        <v>44117</v>
+      </c>
+      <c r="B811" s="24" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C811" s="18" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D811" s="19" t="s">
+        <v>906</v>
+      </c>
+      <c r="E811" s="18" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F811" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G811" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H811" s="6">
+        <v>44117</v>
+      </c>
+      <c r="I811" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J811" s="20"/>
+    </row>
+    <row r="812" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A812" s="26">
+        <v>44118</v>
+      </c>
+      <c r="B812" s="24" t="s">
+        <v>967</v>
+      </c>
+      <c r="C812" s="18" t="s">
+        <v>552</v>
+      </c>
+      <c r="D812" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="E812" s="18" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F812" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G812" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H812" s="6">
+        <v>44119</v>
+      </c>
+      <c r="I812" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J812" s="20"/>
+    </row>
+    <row r="813" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A813" s="26">
+        <v>44118</v>
+      </c>
+      <c r="B813" s="24" t="s">
+        <v>522</v>
+      </c>
+      <c r="C813" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D813" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="E813" s="18" t="s">
+        <v>1177</v>
+      </c>
+      <c r="F813" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G813" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H813" s="6">
+        <v>44118</v>
+      </c>
+      <c r="I813" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J813" s="20"/>
+    </row>
+    <row r="814" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A814" s="26">
+        <v>44118</v>
+      </c>
+      <c r="B814" s="24" t="s">
+        <v>548</v>
+      </c>
+      <c r="C814" s="18" t="s">
+        <v>549</v>
+      </c>
+      <c r="D814" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="E814" s="18" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F814" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G814" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H814" s="6">
+        <v>44118</v>
+      </c>
+      <c r="I814" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J814" s="20"/>
+    </row>
+    <row r="815" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A815" s="26">
+        <v>44118</v>
+      </c>
+      <c r="B815" s="24" t="s">
+        <v>518</v>
+      </c>
+      <c r="C815" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D815" s="19" t="s">
+        <v>826</v>
+      </c>
+      <c r="E815" s="18" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F815" s="19" t="s">
+        <v>498</v>
+      </c>
+      <c r="G815" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H815" s="6">
+        <v>44118</v>
+      </c>
+      <c r="I815" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J815" s="20"/>
+    </row>
+    <row r="816" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A816" s="26">
+        <v>44119</v>
+      </c>
+      <c r="B816" s="24" t="s">
+        <v>635</v>
+      </c>
+      <c r="C816" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D816" s="19" t="s">
         <v>681</v>
       </c>
-      <c r="E803" s="18" t="s">
-        <v>1172</v>
-      </c>
-      <c r="F803" s="19" t="s">
+      <c r="E816" s="18" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F816" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G816" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H816" s="6">
+        <v>44119</v>
+      </c>
+      <c r="I816" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J816" s="20"/>
+    </row>
+    <row r="817" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A817" s="26">
+        <v>44119</v>
+      </c>
+      <c r="B817" s="24" t="s">
+        <v>619</v>
+      </c>
+      <c r="C817" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D817" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="E817" s="18" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F817" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="G803" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="H803" s="6">
-        <v>44113</v>
-      </c>
-      <c r="I803" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="J803" s="20" t="s">
-        <v>1173</v>
-      </c>
-    </row>
-    <row r="804" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A804" s="26">
-        <v>44114</v>
-      </c>
-      <c r="B804" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C804" s="18" t="s">
-        <v>645</v>
-      </c>
-      <c r="D804" s="19" t="s">
-        <v>765</v>
-      </c>
-      <c r="E804" s="18" t="s">
-        <v>1176</v>
-      </c>
-      <c r="F804" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="G804" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="H804" s="6">
-        <v>44114</v>
-      </c>
-      <c r="I804" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="J804" s="20" t="s">
-        <v>1177</v>
-      </c>
-    </row>
-    <row r="805" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A805" s="26">
-        <v>44115</v>
-      </c>
-      <c r="B805" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C805" s="18" t="s">
-        <v>645</v>
-      </c>
-      <c r="D805" s="19" t="s">
-        <v>710</v>
-      </c>
-      <c r="E805" s="18" t="s">
-        <v>1174</v>
-      </c>
-      <c r="F805" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="G805" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="H805" s="6">
-        <v>44115</v>
-      </c>
-      <c r="I805" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="J805" s="20" t="s">
-        <v>1175</v>
-      </c>
-    </row>
-    <row r="806" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A806" s="26"/>
-      <c r="B806" s="24"/>
-      <c r="C806" s="18"/>
-      <c r="D806" s="19"/>
-      <c r="E806" s="18"/>
-      <c r="F806" s="19"/>
-      <c r="G806" s="26"/>
-      <c r="H806" s="6"/>
-      <c r="I806" s="20"/>
-      <c r="J806" s="20"/>
-    </row>
-    <row r="807" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A807" s="26"/>
-      <c r="B807" s="24"/>
-      <c r="C807" s="18"/>
-      <c r="D807" s="19"/>
-      <c r="E807" s="18"/>
-      <c r="F807" s="19"/>
-      <c r="G807" s="26"/>
-      <c r="H807" s="6"/>
-      <c r="I807" s="20"/>
-      <c r="J807" s="20"/>
-    </row>
-    <row r="808" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A808" s="26"/>
-      <c r="B808" s="24"/>
-      <c r="C808" s="18"/>
-      <c r="D808" s="19"/>
-      <c r="E808" s="18"/>
-      <c r="F808" s="19"/>
-      <c r="G808" s="26"/>
-      <c r="H808" s="6"/>
-      <c r="I808" s="20"/>
-      <c r="J808" s="20"/>
-    </row>
-    <row r="809" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A809" s="26"/>
-      <c r="B809" s="24"/>
-      <c r="C809" s="18"/>
-      <c r="D809" s="19"/>
-      <c r="E809" s="18"/>
-      <c r="F809" s="19"/>
-      <c r="G809" s="26"/>
-      <c r="H809" s="6"/>
-      <c r="I809" s="20"/>
-      <c r="J809" s="20"/>
-    </row>
-    <row r="810" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A810" s="26"/>
-      <c r="B810" s="24"/>
-      <c r="C810" s="18"/>
-      <c r="D810" s="19"/>
-      <c r="E810" s="18"/>
-      <c r="F810" s="19"/>
-      <c r="G810" s="26"/>
-      <c r="H810" s="6"/>
-      <c r="I810" s="20"/>
-      <c r="J810" s="20"/>
-    </row>
-    <row r="811" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A811" s="26"/>
-      <c r="B811" s="24"/>
-      <c r="C811" s="18"/>
-      <c r="D811" s="19"/>
-      <c r="E811" s="18" t="s">
-        <v>918</v>
-      </c>
-      <c r="F811" s="19"/>
-      <c r="G811" s="26"/>
-      <c r="H811" s="6"/>
-      <c r="I811" s="20"/>
-      <c r="J811" s="20"/>
-    </row>
-    <row r="812" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A812" s="26"/>
-      <c r="B812" s="24"/>
-      <c r="C812" s="18"/>
-      <c r="D812" s="19"/>
-      <c r="E812" s="18"/>
-      <c r="F812" s="19"/>
-      <c r="G812" s="26"/>
-      <c r="H812" s="6"/>
-      <c r="I812" s="20"/>
-      <c r="J812" s="20"/>
+      <c r="G817" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H817" s="6">
+        <v>44119</v>
+      </c>
+      <c r="I817" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J817" s="20"/>
+    </row>
+    <row r="818" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A818" s="26">
+        <v>44119</v>
+      </c>
+      <c r="B818" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="C818" s="18" t="s">
+        <v>552</v>
+      </c>
+      <c r="D818" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="E818" s="18" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F818" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G818" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H818" s="6">
+        <v>44119</v>
+      </c>
+      <c r="I818" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J818" s="20"/>
+    </row>
+    <row r="819" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A819" s="26">
+        <v>44119</v>
+      </c>
+      <c r="B819" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="C819" s="18" t="s">
+        <v>552</v>
+      </c>
+      <c r="D819" s="19" t="s">
+        <v>630</v>
+      </c>
+      <c r="E819" s="18" t="s">
+        <v>1191</v>
+      </c>
+      <c r="F819" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G819" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H819" s="6">
+        <v>44119</v>
+      </c>
+      <c r="I819" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J819" s="20"/>
+    </row>
+    <row r="820" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A820" s="26"/>
+      <c r="B820" s="24"/>
+      <c r="C820" s="18"/>
+      <c r="D820" s="19"/>
+      <c r="E820" s="18"/>
+      <c r="F820" s="19"/>
+      <c r="G820" s="26"/>
+      <c r="H820" s="6"/>
+      <c r="I820" s="20"/>
+      <c r="J820" s="20"/>
+    </row>
+    <row r="821" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A821" s="26"/>
+      <c r="B821" s="24"/>
+      <c r="C821" s="18"/>
+      <c r="D821" s="19"/>
+      <c r="E821" s="18"/>
+      <c r="F821" s="19"/>
+      <c r="G821" s="26"/>
+      <c r="H821" s="6"/>
+      <c r="I821" s="20"/>
+      <c r="J821" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J788" xr:uid="{00000000-0009-0000-0000-000000000000}">
@@ -28764,25 +29164,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B1" s="57" t="s">
         <v>1114</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="C1" s="57" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E1" s="57" t="s">
         <v>1115</v>
       </c>
-      <c r="C1" s="57" t="s">
-        <v>1119</v>
-      </c>
-      <c r="D1" s="57" t="s">
-        <v>1120</v>
-      </c>
-      <c r="E1" s="57" t="s">
+      <c r="F1" s="57" t="s">
         <v>1116</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="G1" s="58" t="s">
         <v>1117</v>
-      </c>
-      <c r="G1" s="58" t="s">
-        <v>1118</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -28793,10 +29193,10 @@
         <v>47689</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="E2" s="42">
         <v>281</v>
@@ -28805,7 +29205,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="60" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -28813,13 +29213,13 @@
         <v>43957</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C3" s="42">
         <v>281046510</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="E3" s="42">
         <v>281</v>
@@ -28828,7 +29228,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="60" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -28839,10 +29239,10 @@
         <v>47982</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="E4" s="42">
         <v>281</v>
@@ -28851,7 +29251,7 @@
         <v>19</v>
       </c>
       <c r="G4" s="60" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -28859,13 +29259,13 @@
         <v>44170</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C5" s="42">
         <v>345000529</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="E5" s="42">
         <v>345</v>
@@ -28888,7 +29288,7 @@
         <v>289000550</v>
       </c>
       <c r="D6" s="62" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="E6" s="62">
         <v>289</v>

</xml_diff>

<commit_message>
Campos CXN,  Parc. Rentab, Lib NFE Fiscal
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AEC5B3-15A6-4266-97EF-05F77A85FBB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C54E4BC-4C30-4D38-A3D0-CB689736EB6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7021" uniqueCount="1465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7098" uniqueCount="1482">
   <si>
     <t>Prioridade</t>
   </si>
@@ -4015,9 +4015,6 @@
     <t>Obrigar anexar pelo menos um documento na Pré-Nota</t>
   </si>
   <si>
-    <t>Atualizar SIGAFIN</t>
-  </si>
-  <si>
     <t>Problemas com a baixa da NF EG0000058/9</t>
   </si>
   <si>
@@ -4664,6 +4661,66 @@
   </si>
   <si>
     <t>Acerto cheque da PA 340352LDV com valor divergente (cheque SEF x PA SE2)</t>
+  </si>
+  <si>
+    <t>Pontos de Entrada:
+CN120CPO -&gt; CN120VCPO
+CN120PED -&gt; CN120PED
+CN130INC -&gt; MVC-MODELPOS
+CN130PGRV -&gt; MVC-FORMCOMMITTTSPOS
+CTA120MNU -&gt; CNT121BT (ok)</t>
+  </si>
+  <si>
+    <t>Rentabilidade com problemas em titulos parcelados - Balsa Nova</t>
+  </si>
+  <si>
+    <t>Nova Medição - inclusão da descrição do contrato na tela de seleção do contrato/planilha</t>
+  </si>
+  <si>
+    <t>Acerto nas Notas Fiscais: 1253 (045762 07/12/20), 1254 (045763 07/12/20), 1285 (045745 08/12/20), 1286  045751 08/12/20 1288  (045756 08/12/20 336000521-002), 1289  (045805 08/12/20) e 1292  (045773 08/12/20).</t>
+  </si>
+  <si>
+    <t>Impressão de ND (dúvida no uso da Taxa)</t>
+  </si>
+  <si>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>Está ocorrendo o error log abaixo quando da classificação do Doc de Entrada, erro ocorreu após aplicação do patch 20-11-30_ATUALIZACAO_12.1.25_COM_EXPEDICAO_CONTINUA.</t>
+  </si>
+  <si>
+    <t>Solicitação Totvs: #10517769 
+Marcar como usado: "D1_SERIE" , "D1_FORNECE" e "D1_LOJA"</t>
+  </si>
+  <si>
+    <t>Reclamou do sistema lento</t>
+  </si>
+  <si>
+    <t>Internet do usuário estava apenas com 1,25 mb</t>
+  </si>
+  <si>
+    <t>Bárbara Santos</t>
+  </si>
+  <si>
+    <t>Não está conseguindo incluir fornecedores na geração da cotação</t>
+  </si>
+  <si>
+    <t>Não estava conseguindo classificar documento que ele próprio implantou</t>
+  </si>
+  <si>
+    <t>Problema no dicionário dos campos C8_FORNECE e C8_LOJA na empresa Balsa Nova</t>
+  </si>
+  <si>
+    <t>Alterado fonte MT103INC</t>
+  </si>
+  <si>
+    <t>NF 1036 pedido 045510 - Nf saiu sem retenção de impostos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O cliente estaca com o campo  "Modo de abatimento de impostos: 3-Não efetua retenção" </t>
+  </si>
+  <si>
+    <t>Auxilio para exclusão do Doc de Entrada 000004543 fornecedor 004393</t>
   </si>
 </sst>
 </file>
@@ -5390,11 +5447,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1059"/>
+  <dimension ref="A1:J1072"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1027" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1036" sqref="A1036"/>
+      <pane ySplit="1" topLeftCell="A1043" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1047" sqref="E1047"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24843,9 +24900,15 @@
       <c r="F676" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="G676" s="26"/>
-      <c r="H676" s="6"/>
-      <c r="I676" s="20"/>
+      <c r="G676" s="26" t="s">
+        <v>882</v>
+      </c>
+      <c r="H676" s="6">
+        <v>44054</v>
+      </c>
+      <c r="I676" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J676" s="20" t="s">
         <v>965</v>
       </c>
@@ -27070,10 +27133,18 @@
       <c r="E750" s="18" t="s">
         <v>1063</v>
       </c>
-      <c r="F750" s="19"/>
-      <c r="G750" s="26"/>
-      <c r="H750" s="6"/>
-      <c r="I750" s="20"/>
+      <c r="F750" s="19" t="s">
+        <v>702</v>
+      </c>
+      <c r="G750" s="26" t="s">
+        <v>882</v>
+      </c>
+      <c r="H750" s="6">
+        <v>44084</v>
+      </c>
+      <c r="I750" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J750" s="20"/>
     </row>
     <row r="751" spans="1:10" x14ac:dyDescent="0.25">
@@ -29907,7 +29978,7 @@
         <v>17</v>
       </c>
       <c r="J843" s="20" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="844" spans="1:10" x14ac:dyDescent="0.25">
@@ -30698,7 +30769,7 @@
         <v>680</v>
       </c>
       <c r="E870" s="18" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="F870" s="19" t="s">
         <v>106</v>
@@ -30758,7 +30829,7 @@
         <v>750</v>
       </c>
       <c r="E872" s="18" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="F872" s="19" t="s">
         <v>106</v>
@@ -30773,7 +30844,7 @@
         <v>17</v>
       </c>
       <c r="J872" s="20" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="873" spans="1:10" x14ac:dyDescent="0.25">
@@ -30790,7 +30861,7 @@
         <v>680</v>
       </c>
       <c r="E873" s="18" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="F873" s="19" t="s">
         <v>86</v>
@@ -30805,7 +30876,7 @@
         <v>17</v>
       </c>
       <c r="J873" s="20" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="874" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -30822,7 +30893,7 @@
         <v>750</v>
       </c>
       <c r="E874" s="18" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="F874" s="19" t="s">
         <v>86</v>
@@ -30837,7 +30908,7 @@
         <v>17</v>
       </c>
       <c r="J874" s="20" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="875" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -30854,7 +30925,7 @@
         <v>750</v>
       </c>
       <c r="E875" s="18" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="F875" s="19" t="s">
         <v>106</v>
@@ -30869,7 +30940,7 @@
         <v>17</v>
       </c>
       <c r="J875" s="20" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="876" spans="1:10" x14ac:dyDescent="0.25">
@@ -30886,7 +30957,7 @@
         <v>764</v>
       </c>
       <c r="E876" s="18" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="F876" s="19" t="s">
         <v>106</v>
@@ -30901,7 +30972,7 @@
         <v>17</v>
       </c>
       <c r="J876" s="20" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="877" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -30918,7 +30989,7 @@
         <v>630</v>
       </c>
       <c r="E877" s="18" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="F877" s="19" t="s">
         <v>106</v>
@@ -30948,7 +31019,7 @@
         <v>630</v>
       </c>
       <c r="E878" s="18" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="F878" s="19" t="s">
         <v>106</v>
@@ -30978,7 +31049,7 @@
         <v>630</v>
       </c>
       <c r="E879" s="18" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="F879" s="19" t="s">
         <v>86</v>
@@ -31008,7 +31079,7 @@
         <v>630</v>
       </c>
       <c r="E880" s="18" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="F880" s="19" t="s">
         <v>61</v>
@@ -31038,7 +31109,7 @@
         <v>630</v>
       </c>
       <c r="E881" s="18" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="F881" s="19" t="s">
         <v>61</v>
@@ -31068,7 +31139,7 @@
         <v>630</v>
       </c>
       <c r="E882" s="18" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="F882" s="19" t="s">
         <v>106</v>
@@ -31098,7 +31169,7 @@
         <v>630</v>
       </c>
       <c r="E883" s="18" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="F883" s="19" t="s">
         <v>106</v>
@@ -31128,7 +31199,7 @@
         <v>764</v>
       </c>
       <c r="E884" s="18" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="F884" s="19" t="s">
         <v>61</v>
@@ -31158,7 +31229,7 @@
         <v>630</v>
       </c>
       <c r="E885" s="18" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="F885" s="19" t="s">
         <v>106</v>
@@ -31188,7 +31259,7 @@
         <v>630</v>
       </c>
       <c r="E886" s="18" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="F886" s="19" t="s">
         <v>106</v>
@@ -31218,7 +31289,7 @@
         <v>734</v>
       </c>
       <c r="E887" s="18" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="F887" s="19" t="s">
         <v>86</v>
@@ -31248,7 +31319,7 @@
         <v>630</v>
       </c>
       <c r="E888" s="18" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="F888" s="19" t="s">
         <v>110</v>
@@ -31278,7 +31349,7 @@
         <v>764</v>
       </c>
       <c r="E889" s="18" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="F889" s="19" t="s">
         <v>61</v>
@@ -31308,7 +31379,7 @@
         <v>709</v>
       </c>
       <c r="E890" s="18" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="F890" s="19" t="s">
         <v>110</v>
@@ -31323,7 +31394,7 @@
         <v>17</v>
       </c>
       <c r="J890" s="20" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="891" spans="1:10" ht="51" x14ac:dyDescent="0.25">
@@ -31331,7 +31402,7 @@
         <v>44144</v>
       </c>
       <c r="B891" s="24" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="C891" s="18" t="s">
         <v>10</v>
@@ -31340,7 +31411,7 @@
         <v>630</v>
       </c>
       <c r="E891" s="18" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="F891" s="19" t="s">
         <v>106</v>
@@ -31355,7 +31426,7 @@
         <v>17</v>
       </c>
       <c r="J891" s="20" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="892" spans="1:10" x14ac:dyDescent="0.25">
@@ -31372,7 +31443,7 @@
         <v>630</v>
       </c>
       <c r="E892" s="18" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="F892" s="19" t="s">
         <v>110</v>
@@ -31402,7 +31473,7 @@
         <v>750</v>
       </c>
       <c r="E893" s="18" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F893" s="19" t="s">
         <v>106</v>
@@ -31417,7 +31488,7 @@
         <v>17</v>
       </c>
       <c r="J893" s="20" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="894" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -31434,7 +31505,7 @@
         <v>680</v>
       </c>
       <c r="E894" s="18" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="F894" s="19" t="s">
         <v>110</v>
@@ -31449,7 +31520,7 @@
         <v>17</v>
       </c>
       <c r="J894" s="20" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="895" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -31466,7 +31537,7 @@
         <v>630</v>
       </c>
       <c r="E895" s="18" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="F895" s="19" t="s">
         <v>61</v>
@@ -31496,7 +31567,7 @@
         <v>630</v>
       </c>
       <c r="E896" s="18" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="F896" s="19" t="s">
         <v>61</v>
@@ -31511,7 +31582,7 @@
         <v>17</v>
       </c>
       <c r="J896" s="20" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="897" spans="1:10" x14ac:dyDescent="0.25">
@@ -31528,7 +31599,7 @@
         <v>630</v>
       </c>
       <c r="E897" s="18" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F897" s="19" t="s">
         <v>106</v>
@@ -31558,7 +31629,7 @@
         <v>630</v>
       </c>
       <c r="E898" s="18" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="F898" s="19" t="s">
         <v>106</v>
@@ -31588,7 +31659,7 @@
         <v>630</v>
       </c>
       <c r="E899" s="18" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="F899" s="19" t="s">
         <v>106</v>
@@ -31603,7 +31674,7 @@
         <v>17</v>
       </c>
       <c r="J899" s="20" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="900" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -31620,7 +31691,7 @@
         <v>630</v>
       </c>
       <c r="E900" s="18" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="F900" s="19" t="s">
         <v>106</v>
@@ -31635,7 +31706,7 @@
         <v>17</v>
       </c>
       <c r="J900" s="20" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="901" spans="1:10" x14ac:dyDescent="0.25">
@@ -31643,7 +31714,7 @@
         <v>44146</v>
       </c>
       <c r="B901" s="24" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="C901" s="18" t="s">
         <v>552</v>
@@ -31652,7 +31723,7 @@
         <v>630</v>
       </c>
       <c r="E901" s="18" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="F901" s="19" t="s">
         <v>106</v>
@@ -31682,7 +31753,7 @@
         <v>630</v>
       </c>
       <c r="E902" s="18" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="F902" s="19" t="s">
         <v>106</v>
@@ -31712,7 +31783,7 @@
         <v>630</v>
       </c>
       <c r="E903" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="F903" s="19" t="s">
         <v>106</v>
@@ -31727,7 +31798,7 @@
         <v>17</v>
       </c>
       <c r="J903" s="20" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="904" spans="1:10" x14ac:dyDescent="0.25">
@@ -31744,7 +31815,7 @@
         <v>734</v>
       </c>
       <c r="E904" s="18" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="F904" s="19" t="s">
         <v>106</v>
@@ -31759,7 +31830,7 @@
         <v>17</v>
       </c>
       <c r="J904" s="20" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="905" spans="1:10" x14ac:dyDescent="0.25">
@@ -31776,7 +31847,7 @@
         <v>734</v>
       </c>
       <c r="E905" s="18" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="F905" s="19" t="s">
         <v>86</v>
@@ -31806,7 +31877,7 @@
         <v>680</v>
       </c>
       <c r="E906" s="18" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="F906" s="19" t="s">
         <v>106</v>
@@ -31836,7 +31907,7 @@
         <v>680</v>
       </c>
       <c r="E907" s="18" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="F907" s="19" t="s">
         <v>554</v>
@@ -31866,7 +31937,7 @@
         <v>750</v>
       </c>
       <c r="E908" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="F908" s="19" t="s">
         <v>110</v>
@@ -31881,7 +31952,7 @@
         <v>17</v>
       </c>
       <c r="J908" s="20" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="909" spans="1:10" x14ac:dyDescent="0.25">
@@ -31898,7 +31969,7 @@
         <v>680</v>
       </c>
       <c r="E909" s="18" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="F909" s="19" t="s">
         <v>106</v>
@@ -31928,7 +31999,7 @@
         <v>630</v>
       </c>
       <c r="E910" s="18" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="F910" s="19" t="s">
         <v>106</v>
@@ -31943,7 +32014,7 @@
         <v>17</v>
       </c>
       <c r="J910" s="20" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="911" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -31960,7 +32031,7 @@
         <v>630</v>
       </c>
       <c r="E911" s="18" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="F911" s="19" t="s">
         <v>106</v>
@@ -31990,7 +32061,7 @@
         <v>750</v>
       </c>
       <c r="E912" s="18" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="F912" s="19" t="s">
         <v>1028</v>
@@ -32005,7 +32076,7 @@
         <v>17</v>
       </c>
       <c r="J912" s="20" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="913" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -32022,7 +32093,7 @@
         <v>750</v>
       </c>
       <c r="E913" s="18" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="F913" s="19" t="s">
         <v>106</v>
@@ -32052,7 +32123,7 @@
         <v>750</v>
       </c>
       <c r="E914" s="18" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="F914" s="19" t="s">
         <v>86</v>
@@ -32084,7 +32155,7 @@
         <v>630</v>
       </c>
       <c r="E915" s="18" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="F915" s="19" t="s">
         <v>61</v>
@@ -32114,7 +32185,7 @@
         <v>734</v>
       </c>
       <c r="E916" s="18" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="F916" s="19" t="s">
         <v>110</v>
@@ -32129,7 +32200,7 @@
         <v>17</v>
       </c>
       <c r="J916" s="20" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="917" spans="1:10" x14ac:dyDescent="0.25">
@@ -32146,7 +32217,7 @@
         <v>630</v>
       </c>
       <c r="E917" s="18" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="F917" s="19" t="s">
         <v>106</v>
@@ -32176,7 +32247,7 @@
         <v>734</v>
       </c>
       <c r="E918" s="18" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="F918" s="19" t="s">
         <v>106</v>
@@ -32191,7 +32262,7 @@
         <v>17</v>
       </c>
       <c r="J918" s="20" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="919" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -32208,7 +32279,7 @@
         <v>680</v>
       </c>
       <c r="E919" s="18" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="F919" s="19" t="s">
         <v>110</v>
@@ -32223,7 +32294,7 @@
         <v>17</v>
       </c>
       <c r="J919" s="20" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="920" spans="1:10" x14ac:dyDescent="0.25">
@@ -32240,7 +32311,7 @@
         <v>680</v>
       </c>
       <c r="E920" s="18" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="F920" s="19" t="s">
         <v>110</v>
@@ -32270,7 +32341,7 @@
         <v>630</v>
       </c>
       <c r="E921" s="18" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="F921" s="19" t="s">
         <v>702</v>
@@ -32285,7 +32356,7 @@
         <v>17</v>
       </c>
       <c r="J921" s="20" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="922" spans="1:10" x14ac:dyDescent="0.25">
@@ -32302,7 +32373,7 @@
         <v>630</v>
       </c>
       <c r="E922" s="18" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="F922" s="19" t="s">
         <v>106</v>
@@ -32332,7 +32403,7 @@
         <v>630</v>
       </c>
       <c r="E923" s="18" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="F923" s="19" t="s">
         <v>106</v>
@@ -32362,7 +32433,7 @@
         <v>630</v>
       </c>
       <c r="E924" s="18" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="F924" s="19" t="s">
         <v>106</v>
@@ -32392,7 +32463,7 @@
         <v>630</v>
       </c>
       <c r="E925" s="18" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="F925" s="19" t="s">
         <v>106</v>
@@ -32422,7 +32493,7 @@
         <v>680</v>
       </c>
       <c r="E926" s="18" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="F926" s="19" t="s">
         <v>106</v>
@@ -32452,7 +32523,7 @@
         <v>630</v>
       </c>
       <c r="E927" s="18" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="F927" s="19" t="s">
         <v>106</v>
@@ -32482,7 +32553,7 @@
         <v>630</v>
       </c>
       <c r="E928" s="18" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="F928" s="19" t="s">
         <v>106</v>
@@ -32497,7 +32568,7 @@
         <v>17</v>
       </c>
       <c r="J928" s="20" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="929" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -32514,7 +32585,7 @@
         <v>680</v>
       </c>
       <c r="E929" s="18" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="F929" s="19" t="s">
         <v>106</v>
@@ -32544,7 +32615,7 @@
         <v>630</v>
       </c>
       <c r="E930" s="18" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="F930" s="19" t="s">
         <v>106</v>
@@ -32574,7 +32645,7 @@
         <v>764</v>
       </c>
       <c r="E931" s="18" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="F931" s="19" t="s">
         <v>106</v>
@@ -32606,7 +32677,7 @@
         <v>680</v>
       </c>
       <c r="E932" s="18" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="F932" s="19" t="s">
         <v>86</v>
@@ -32636,7 +32707,7 @@
         <v>680</v>
       </c>
       <c r="E933" s="18" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="F933" s="19" t="s">
         <v>110</v>
@@ -32666,7 +32737,7 @@
         <v>680</v>
       </c>
       <c r="E934" s="18" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="F934" s="19" t="s">
         <v>106</v>
@@ -32696,7 +32767,7 @@
         <v>680</v>
       </c>
       <c r="E935" s="18" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="F935" s="19" t="s">
         <v>106</v>
@@ -32711,7 +32782,7 @@
         <v>17</v>
       </c>
       <c r="J935" s="20" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="936" spans="1:10" x14ac:dyDescent="0.25">
@@ -32728,7 +32799,7 @@
         <v>905</v>
       </c>
       <c r="E936" s="18" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="F936" s="19" t="s">
         <v>498</v>
@@ -32758,7 +32829,7 @@
         <v>750</v>
       </c>
       <c r="E937" s="18" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="F937" s="19" t="s">
         <v>106</v>
@@ -32773,7 +32844,7 @@
         <v>17</v>
       </c>
       <c r="J937" s="20" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="938" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -32790,7 +32861,7 @@
         <v>764</v>
       </c>
       <c r="E938" s="18" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="F938" s="19" t="s">
         <v>106</v>
@@ -32820,7 +32891,7 @@
         <v>750</v>
       </c>
       <c r="E939" s="18" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="F939" s="19" t="s">
         <v>106</v>
@@ -32850,7 +32921,7 @@
         <v>750</v>
       </c>
       <c r="E940" s="18" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="F940" s="19" t="s">
         <v>106</v>
@@ -32880,7 +32951,7 @@
         <v>680</v>
       </c>
       <c r="E941" s="18" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="F941" s="19" t="s">
         <v>106</v>
@@ -32910,7 +32981,7 @@
         <v>750</v>
       </c>
       <c r="E942" s="18" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="F942" s="19" t="s">
         <v>106</v>
@@ -32940,7 +33011,7 @@
         <v>750</v>
       </c>
       <c r="E943" s="18" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="F943" s="19" t="s">
         <v>106</v>
@@ -32955,7 +33026,7 @@
         <v>17</v>
       </c>
       <c r="J943" s="20" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="944" spans="1:10" x14ac:dyDescent="0.25">
@@ -32972,7 +33043,7 @@
         <v>750</v>
       </c>
       <c r="E944" s="18" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="F944" s="19" t="s">
         <v>106</v>
@@ -33002,7 +33073,7 @@
         <v>750</v>
       </c>
       <c r="E945" s="18" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="F945" s="19" t="s">
         <v>106</v>
@@ -33017,7 +33088,7 @@
         <v>17</v>
       </c>
       <c r="J945" s="20" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="946" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -33034,7 +33105,7 @@
         <v>680</v>
       </c>
       <c r="E946" s="18" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="F946" s="19" t="s">
         <v>516</v>
@@ -33064,7 +33135,7 @@
         <v>750</v>
       </c>
       <c r="E947" s="18" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="F947" s="19" t="s">
         <v>106</v>
@@ -33079,7 +33150,7 @@
         <v>17</v>
       </c>
       <c r="J947" s="20" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="948" spans="1:10" x14ac:dyDescent="0.25">
@@ -33096,7 +33167,7 @@
         <v>750</v>
       </c>
       <c r="E948" s="18" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="F948" s="19" t="s">
         <v>106</v>
@@ -33126,7 +33197,7 @@
         <v>750</v>
       </c>
       <c r="E949" s="18" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="F949" s="19" t="s">
         <v>106</v>
@@ -33141,7 +33212,7 @@
         <v>12</v>
       </c>
       <c r="J949" s="20" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="950" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -33158,7 +33229,7 @@
         <v>750</v>
       </c>
       <c r="E950" s="18" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="F950" s="19" t="s">
         <v>86</v>
@@ -33188,7 +33259,7 @@
         <v>750</v>
       </c>
       <c r="E951" s="18" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="F951" s="19" t="s">
         <v>86</v>
@@ -33203,7 +33274,7 @@
         <v>17</v>
       </c>
       <c r="J951" s="20" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="952" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -33220,7 +33291,7 @@
         <v>680</v>
       </c>
       <c r="E952" s="18" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="F952" s="19" t="s">
         <v>106</v>
@@ -33241,7 +33312,7 @@
         <v>44165</v>
       </c>
       <c r="B953" s="24" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="C953" s="18" t="s">
         <v>34</v>
@@ -33250,7 +33321,7 @@
         <v>750</v>
       </c>
       <c r="E953" s="18" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="F953" s="19" t="s">
         <v>106</v>
@@ -33280,7 +33351,7 @@
         <v>750</v>
       </c>
       <c r="E954" s="18" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="F954" s="19" t="s">
         <v>106</v>
@@ -33295,7 +33366,7 @@
         <v>17</v>
       </c>
       <c r="J954" s="20" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="955" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -33312,7 +33383,7 @@
         <v>750</v>
       </c>
       <c r="E955" s="18" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="F955" s="19" t="s">
         <v>86</v>
@@ -33342,7 +33413,7 @@
         <v>750</v>
       </c>
       <c r="E956" s="18" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="F956" s="19" t="s">
         <v>1028</v>
@@ -33372,7 +33443,7 @@
         <v>680</v>
       </c>
       <c r="E957" s="18" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="F957" s="19" t="s">
         <v>106</v>
@@ -33402,7 +33473,7 @@
         <v>680</v>
       </c>
       <c r="E958" s="18" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="F958" s="19" t="s">
         <v>106</v>
@@ -33417,7 +33488,7 @@
         <v>17</v>
       </c>
       <c r="J958" s="20" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="959" spans="1:10" x14ac:dyDescent="0.25">
@@ -33434,7 +33505,7 @@
         <v>905</v>
       </c>
       <c r="E959" s="18" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F959" s="19" t="s">
         <v>106</v>
@@ -33464,7 +33535,7 @@
         <v>680</v>
       </c>
       <c r="E960" s="18" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="F960" s="19" t="s">
         <v>106</v>
@@ -33485,7 +33556,7 @@
         <v>44166</v>
       </c>
       <c r="B961" s="24" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="C961" s="18" t="s">
         <v>10</v>
@@ -33494,7 +33565,7 @@
         <v>905</v>
       </c>
       <c r="E961" s="18" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="F961" s="19" t="s">
         <v>106</v>
@@ -33524,7 +33595,7 @@
         <v>905</v>
       </c>
       <c r="E962" s="18" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="F962" s="19" t="s">
         <v>106</v>
@@ -33545,7 +33616,7 @@
         <v>44166</v>
       </c>
       <c r="B963" s="24" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="C963" s="18" t="s">
         <v>10</v>
@@ -33554,7 +33625,7 @@
         <v>905</v>
       </c>
       <c r="E963" s="18" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="F963" s="19" t="s">
         <v>106</v>
@@ -33584,7 +33655,7 @@
         <v>750</v>
       </c>
       <c r="E964" s="18" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="F964" s="19" t="s">
         <v>106</v>
@@ -33614,7 +33685,7 @@
         <v>905</v>
       </c>
       <c r="E965" s="18" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="F965" s="19" t="s">
         <v>110</v>
@@ -33644,7 +33715,7 @@
         <v>905</v>
       </c>
       <c r="E966" s="18" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="F966" s="19" t="s">
         <v>86</v>
@@ -33674,7 +33745,7 @@
         <v>750</v>
       </c>
       <c r="E967" s="18" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="F967" s="19" t="s">
         <v>106</v>
@@ -33704,7 +33775,7 @@
         <v>680</v>
       </c>
       <c r="E968" s="18" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="F968" s="19" t="s">
         <v>1028</v>
@@ -33734,7 +33805,7 @@
         <v>680</v>
       </c>
       <c r="E969" s="18" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="F969" s="19" t="s">
         <v>106</v>
@@ -33766,7 +33837,7 @@
         <v>750</v>
       </c>
       <c r="E970" s="18" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="F970" s="19" t="s">
         <v>106</v>
@@ -33796,7 +33867,7 @@
         <v>680</v>
       </c>
       <c r="E971" s="18" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="F971" s="19" t="s">
         <v>106</v>
@@ -33826,7 +33897,7 @@
         <v>750</v>
       </c>
       <c r="E972" s="18" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="F972" s="19" t="s">
         <v>110</v>
@@ -33841,7 +33912,7 @@
         <v>17</v>
       </c>
       <c r="J972" s="20" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="973" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -33858,7 +33929,7 @@
         <v>750</v>
       </c>
       <c r="E973" s="18" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="F973" s="19" t="s">
         <v>1028</v>
@@ -33888,7 +33959,7 @@
         <v>750</v>
       </c>
       <c r="E974" s="18" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="F974" s="19" t="s">
         <v>86</v>
@@ -33903,7 +33974,7 @@
         <v>17</v>
       </c>
       <c r="J974" s="20" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="975" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -33920,7 +33991,7 @@
         <v>905</v>
       </c>
       <c r="E975" s="18" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="F975" s="19" t="s">
         <v>86</v>
@@ -33950,7 +34021,7 @@
         <v>905</v>
       </c>
       <c r="E976" s="18" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="F976" s="19" t="s">
         <v>86</v>
@@ -33980,7 +34051,7 @@
         <v>630</v>
       </c>
       <c r="E977" s="18" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="F977" s="19" t="s">
         <v>106</v>
@@ -34001,7 +34072,7 @@
         <v>44168</v>
       </c>
       <c r="B978" s="24" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="C978" s="18" t="s">
         <v>552</v>
@@ -34010,7 +34081,7 @@
         <v>630</v>
       </c>
       <c r="E978" s="18" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="F978" s="19" t="s">
         <v>1028</v>
@@ -34040,7 +34111,7 @@
         <v>905</v>
       </c>
       <c r="E979" s="18" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="F979" s="19" t="s">
         <v>106</v>
@@ -34061,7 +34132,7 @@
         <v>44168</v>
       </c>
       <c r="B980" s="24" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="C980" s="18" t="s">
         <v>98</v>
@@ -34070,7 +34141,7 @@
         <v>630</v>
       </c>
       <c r="E980" s="18" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="F980" s="19"/>
       <c r="G980" s="26"/>
@@ -34083,7 +34154,7 @@
         <v>44169</v>
       </c>
       <c r="B981" s="24" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="C981" s="18" t="s">
         <v>552</v>
@@ -34092,7 +34163,7 @@
         <v>630</v>
       </c>
       <c r="E981" s="18" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="F981" s="19" t="s">
         <v>110</v>
@@ -34107,7 +34178,7 @@
         <v>17</v>
       </c>
       <c r="J981" s="20" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="982" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -34124,7 +34195,7 @@
         <v>630</v>
       </c>
       <c r="E982" s="18" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="F982" s="19" t="s">
         <v>106</v>
@@ -34145,7 +34216,7 @@
         <v>44169</v>
       </c>
       <c r="B983" s="24" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="C983" s="18" t="s">
         <v>21</v>
@@ -34154,7 +34225,7 @@
         <v>734</v>
       </c>
       <c r="E983" s="18" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="F983" s="19" t="s">
         <v>110</v>
@@ -34169,7 +34240,7 @@
         <v>17</v>
       </c>
       <c r="J983" s="20" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="984" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -34186,7 +34257,7 @@
         <v>630</v>
       </c>
       <c r="E984" s="18" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="F984" s="19" t="s">
         <v>106</v>
@@ -34201,7 +34272,7 @@
         <v>17</v>
       </c>
       <c r="J984" s="20" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="985" spans="1:10" x14ac:dyDescent="0.25">
@@ -34218,7 +34289,7 @@
         <v>680</v>
       </c>
       <c r="E985" s="18" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="F985" s="19" t="s">
         <v>106</v>
@@ -34239,7 +34310,7 @@
         <v>44172</v>
       </c>
       <c r="B986" s="24" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="C986" s="18" t="s">
         <v>10</v>
@@ -34248,7 +34319,7 @@
         <v>680</v>
       </c>
       <c r="E986" s="18" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="F986" s="19" t="s">
         <v>106</v>
@@ -34278,7 +34349,7 @@
         <v>680</v>
       </c>
       <c r="E987" s="18" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="F987" s="19" t="s">
         <v>106</v>
@@ -34308,7 +34379,7 @@
         <v>630</v>
       </c>
       <c r="E988" s="18" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="F988" s="19" t="s">
         <v>106</v>
@@ -34338,7 +34409,7 @@
         <v>734</v>
       </c>
       <c r="E989" s="18" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="F989" s="19" t="s">
         <v>106</v>
@@ -34368,7 +34439,7 @@
         <v>630</v>
       </c>
       <c r="E990" s="18" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="F990" s="19" t="s">
         <v>106</v>
@@ -34398,7 +34469,7 @@
         <v>734</v>
       </c>
       <c r="E991" s="18" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="F991" s="19" t="s">
         <v>1028</v>
@@ -34428,7 +34499,7 @@
         <v>630</v>
       </c>
       <c r="E992" s="18" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="F992" s="19" t="s">
         <v>106</v>
@@ -34458,7 +34529,7 @@
         <v>750</v>
       </c>
       <c r="E993" s="18" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="F993" s="19" t="s">
         <v>106</v>
@@ -34488,7 +34559,7 @@
         <v>905</v>
       </c>
       <c r="E994" s="18" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="F994" s="19" t="s">
         <v>110</v>
@@ -34518,7 +34589,7 @@
         <v>905</v>
       </c>
       <c r="E995" s="18" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="F995" s="19" t="s">
         <v>110</v>
@@ -34548,7 +34619,7 @@
         <v>905</v>
       </c>
       <c r="E996" s="18" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="F996" s="19" t="s">
         <v>86</v>
@@ -34578,7 +34649,7 @@
         <v>734</v>
       </c>
       <c r="E997" s="18" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="F997" s="19" t="s">
         <v>86</v>
@@ -34593,7 +34664,7 @@
         <v>17</v>
       </c>
       <c r="J997" s="20" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="998" spans="1:10" x14ac:dyDescent="0.25">
@@ -34610,7 +34681,7 @@
         <v>734</v>
       </c>
       <c r="E998" s="18" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="F998" s="19" t="s">
         <v>163</v>
@@ -34637,10 +34708,10 @@
         <v>552</v>
       </c>
       <c r="D999" s="19" t="s">
+        <v>1420</v>
+      </c>
+      <c r="E999" s="18" t="s">
         <v>1421</v>
-      </c>
-      <c r="E999" s="18" t="s">
-        <v>1422</v>
       </c>
       <c r="F999" s="19" t="s">
         <v>106</v>
@@ -34670,7 +34741,7 @@
         <v>764</v>
       </c>
       <c r="E1000" s="18" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="F1000" s="19" t="s">
         <v>106</v>
@@ -34700,7 +34771,7 @@
         <v>905</v>
       </c>
       <c r="E1001" s="18" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="F1001" s="19" t="s">
         <v>86</v>
@@ -34730,7 +34801,7 @@
         <v>905</v>
       </c>
       <c r="E1002" s="18" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="F1002" s="19" t="s">
         <v>106</v>
@@ -34760,7 +34831,7 @@
         <v>680</v>
       </c>
       <c r="E1003" s="18" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="F1003" s="19" t="s">
         <v>106</v>
@@ -34790,7 +34861,7 @@
         <v>630</v>
       </c>
       <c r="E1004" s="18" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="F1004" s="19" t="s">
         <v>86</v>
@@ -34820,7 +34891,7 @@
         <v>630</v>
       </c>
       <c r="E1005" s="18" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="F1005" s="19" t="s">
         <v>106</v>
@@ -34835,7 +34906,7 @@
         <v>17</v>
       </c>
       <c r="J1005" s="20" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="1006" spans="1:10" x14ac:dyDescent="0.25">
@@ -34852,7 +34923,7 @@
         <v>750</v>
       </c>
       <c r="E1006" s="18" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="F1006" s="19" t="s">
         <v>106</v>
@@ -34867,7 +34938,7 @@
         <v>17</v>
       </c>
       <c r="J1006" s="20" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="1007" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -34884,7 +34955,7 @@
         <v>680</v>
       </c>
       <c r="E1007" s="18" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="F1007" s="19"/>
       <c r="G1007" s="26"/>
@@ -34903,10 +34974,10 @@
         <v>644</v>
       </c>
       <c r="D1008" s="19" t="s">
+        <v>1433</v>
+      </c>
+      <c r="E1008" s="18" t="s">
         <v>1434</v>
-      </c>
-      <c r="E1008" s="18" t="s">
-        <v>1435</v>
       </c>
       <c r="F1008" s="19"/>
       <c r="G1008" s="26"/>
@@ -34928,7 +34999,7 @@
         <v>750</v>
       </c>
       <c r="E1009" s="18" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="F1009" s="19" t="s">
         <v>106</v>
@@ -34955,10 +35026,10 @@
         <v>98</v>
       </c>
       <c r="D1010" s="19" t="s">
+        <v>1436</v>
+      </c>
+      <c r="E1010" s="18" t="s">
         <v>1437</v>
-      </c>
-      <c r="E1010" s="18" t="s">
-        <v>1438</v>
       </c>
       <c r="F1010" s="19" t="s">
         <v>106</v>
@@ -34988,7 +35059,7 @@
         <v>734</v>
       </c>
       <c r="E1011" s="18" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="F1011" s="19" t="s">
         <v>159</v>
@@ -35018,7 +35089,7 @@
         <v>680</v>
       </c>
       <c r="E1012" s="18" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="F1012" s="19" t="s">
         <v>61</v>
@@ -35048,7 +35119,7 @@
         <v>750</v>
       </c>
       <c r="E1013" s="18" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="F1013" s="19" t="s">
         <v>86</v>
@@ -35078,7 +35149,7 @@
         <v>905</v>
       </c>
       <c r="E1014" s="18" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="F1014" s="19" t="s">
         <v>106</v>
@@ -35108,7 +35179,7 @@
         <v>750</v>
       </c>
       <c r="E1015" s="18" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="F1015" s="19" t="s">
         <v>106</v>
@@ -35138,7 +35209,7 @@
         <v>630</v>
       </c>
       <c r="E1016" s="18" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="F1016" s="19" t="s">
         <v>106</v>
@@ -35168,7 +35239,7 @@
         <v>630</v>
       </c>
       <c r="E1017" s="18" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="F1017" s="19" t="s">
         <v>106</v>
@@ -35198,7 +35269,7 @@
         <v>630</v>
       </c>
       <c r="E1018" s="18" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="F1018" s="19" t="s">
         <v>106</v>
@@ -35228,7 +35299,7 @@
         <v>680</v>
       </c>
       <c r="E1019" s="18" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="F1019" s="19" t="s">
         <v>1028</v>
@@ -35258,7 +35329,7 @@
         <v>680</v>
       </c>
       <c r="E1020" s="18" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="F1020" s="19" t="s">
         <v>106</v>
@@ -35288,7 +35359,7 @@
         <v>680</v>
       </c>
       <c r="E1021" s="18" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F1021" s="19" t="s">
         <v>110</v>
@@ -35318,7 +35389,7 @@
         <v>630</v>
       </c>
       <c r="E1022" s="18" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="F1022" s="19" t="s">
         <v>163</v>
@@ -35333,7 +35404,7 @@
         <v>17</v>
       </c>
       <c r="J1022" s="20" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="1023" spans="1:10" x14ac:dyDescent="0.25">
@@ -35350,7 +35421,7 @@
         <v>680</v>
       </c>
       <c r="E1023" s="18" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="F1023" s="19" t="s">
         <v>106</v>
@@ -35380,7 +35451,7 @@
         <v>680</v>
       </c>
       <c r="E1024" s="18" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="F1024" s="19" t="s">
         <v>1028</v>
@@ -35410,7 +35481,7 @@
         <v>680</v>
       </c>
       <c r="E1025" s="18" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="F1025" s="19" t="s">
         <v>106</v>
@@ -35440,7 +35511,7 @@
         <v>764</v>
       </c>
       <c r="E1026" s="18" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="F1026" s="19" t="s">
         <v>86</v>
@@ -35470,7 +35541,7 @@
         <v>709</v>
       </c>
       <c r="E1027" s="18" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="F1027" s="19" t="s">
         <v>86</v>
@@ -35500,7 +35571,7 @@
         <v>709</v>
       </c>
       <c r="E1028" s="18" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="F1028" s="19" t="s">
         <v>86</v>
@@ -35530,7 +35601,7 @@
         <v>709</v>
       </c>
       <c r="E1029" s="18" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="F1029" s="19" t="s">
         <v>106</v>
@@ -35560,7 +35631,7 @@
         <v>709</v>
       </c>
       <c r="E1030" s="18" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="F1030" s="19" t="s">
         <v>61</v>
@@ -35590,7 +35661,7 @@
         <v>709</v>
       </c>
       <c r="E1031" s="18" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="F1031" s="19" t="s">
         <v>86</v>
@@ -35620,7 +35691,7 @@
         <v>709</v>
       </c>
       <c r="E1032" s="18" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="F1032" s="19" t="s">
         <v>86</v>
@@ -35650,7 +35721,7 @@
         <v>709</v>
       </c>
       <c r="E1033" s="18" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="F1033" s="19" t="s">
         <v>86</v>
@@ -35680,7 +35751,7 @@
         <v>764</v>
       </c>
       <c r="E1034" s="18" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="F1034" s="19" t="s">
         <v>86</v>
@@ -35710,7 +35781,7 @@
         <v>764</v>
       </c>
       <c r="E1035" s="18" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="F1035" s="19" t="s">
         <v>106</v>
@@ -35727,147 +35798,313 @@
       <c r="J1035" s="20"/>
     </row>
     <row r="1036" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1036" s="26"/>
-      <c r="B1036" s="24"/>
-      <c r="C1036" s="18"/>
-      <c r="D1036" s="19"/>
-      <c r="E1036" s="18"/>
-      <c r="F1036" s="19"/>
-      <c r="G1036" s="26"/>
-      <c r="H1036" s="6"/>
-      <c r="I1036" s="20"/>
+      <c r="A1036" s="26">
+        <v>44187</v>
+      </c>
+      <c r="B1036" s="24" t="s">
+        <v>966</v>
+      </c>
+      <c r="C1036" s="18" t="s">
+        <v>552</v>
+      </c>
+      <c r="D1036" s="19" t="s">
+        <v>750</v>
+      </c>
+      <c r="E1036" s="18" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F1036" s="19" t="s">
+        <v>498</v>
+      </c>
+      <c r="G1036" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1036" s="6">
+        <v>44187</v>
+      </c>
+      <c r="I1036" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J1036" s="20"/>
     </row>
-    <row r="1037" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1037" s="26"/>
-      <c r="B1037" s="24"/>
-      <c r="C1037" s="18"/>
-      <c r="D1037" s="19"/>
-      <c r="E1037" s="18"/>
-      <c r="F1037" s="19"/>
-      <c r="G1037" s="26"/>
-      <c r="H1037" s="6"/>
-      <c r="I1037" s="20"/>
+    <row r="1037" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1037" s="26">
+        <v>44187</v>
+      </c>
+      <c r="B1037" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1037" s="18" t="s">
+        <v>644</v>
+      </c>
+      <c r="D1037" s="19" t="s">
+        <v>764</v>
+      </c>
+      <c r="E1037" s="18" t="s">
+        <v>1466</v>
+      </c>
+      <c r="F1037" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1037" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1037" s="6">
+        <v>44188</v>
+      </c>
+      <c r="I1037" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J1037" s="20"/>
     </row>
-    <row r="1038" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1038" s="26"/>
-      <c r="B1038" s="24"/>
-      <c r="C1038" s="18"/>
-      <c r="D1038" s="19"/>
-      <c r="E1038" s="18"/>
-      <c r="F1038" s="19"/>
-      <c r="G1038" s="26"/>
-      <c r="H1038" s="6"/>
-      <c r="I1038" s="20"/>
+    <row r="1038" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A1038" s="26">
+        <v>44188</v>
+      </c>
+      <c r="B1038" s="24" t="s">
+        <v>522</v>
+      </c>
+      <c r="C1038" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1038" s="19" t="s">
+        <v>734</v>
+      </c>
+      <c r="E1038" s="18" t="s">
+        <v>1467</v>
+      </c>
+      <c r="F1038" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1038" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1038" s="6">
+        <v>44188</v>
+      </c>
+      <c r="I1038" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J1038" s="20"/>
     </row>
     <row r="1039" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1039" s="26"/>
+      <c r="A1039" s="26">
+        <v>44188</v>
+      </c>
       <c r="B1039" s="24" t="s">
-        <v>17</v>
+        <v>1039</v>
       </c>
       <c r="C1039" s="18" t="s">
-        <v>644</v>
+        <v>21</v>
       </c>
       <c r="D1039" s="19" t="s">
-        <v>709</v>
+        <v>680</v>
       </c>
       <c r="E1039" s="18" t="s">
-        <v>1243</v>
-      </c>
-      <c r="F1039" s="19"/>
-      <c r="G1039" s="26"/>
-      <c r="H1039" s="6"/>
-      <c r="I1039" s="20"/>
+        <v>1468</v>
+      </c>
+      <c r="F1039" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1039" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1039" s="6">
+        <v>44188</v>
+      </c>
+      <c r="I1039" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J1039" s="20"/>
     </row>
-    <row r="1040" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1040" s="26"/>
+    <row r="1040" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A1040" s="26">
+        <v>44188</v>
+      </c>
       <c r="B1040" s="24" t="s">
-        <v>17</v>
+        <v>1469</v>
       </c>
       <c r="C1040" s="18" t="s">
-        <v>644</v>
+        <v>98</v>
       </c>
       <c r="D1040" s="19" t="s">
-        <v>709</v>
+        <v>680</v>
       </c>
       <c r="E1040" s="18" t="s">
-        <v>1251</v>
-      </c>
-      <c r="F1040" s="19"/>
-      <c r="G1040" s="26"/>
-      <c r="H1040" s="6"/>
-      <c r="I1040" s="20"/>
-      <c r="J1040" s="20"/>
-    </row>
-    <row r="1041" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1041" s="26"/>
+        <v>1470</v>
+      </c>
+      <c r="F1040" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1040" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1040" s="6">
+        <v>44188</v>
+      </c>
+      <c r="I1040" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1040" s="20" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1041" s="26">
+        <v>44193</v>
+      </c>
       <c r="B1041" s="24" t="s">
-        <v>17</v>
+        <v>522</v>
       </c>
       <c r="C1041" s="18" t="s">
-        <v>644</v>
+        <v>98</v>
       </c>
       <c r="D1041" s="19" t="s">
-        <v>709</v>
+        <v>750</v>
       </c>
       <c r="E1041" s="18" t="s">
-        <v>1420</v>
-      </c>
-      <c r="F1041" s="19"/>
-      <c r="G1041" s="26"/>
-      <c r="H1041" s="6"/>
-      <c r="I1041" s="20"/>
-      <c r="J1041" s="20"/>
+        <v>1479</v>
+      </c>
+      <c r="F1041" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1041" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1041" s="6">
+        <v>44193</v>
+      </c>
+      <c r="I1041" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1041" s="18" t="s">
+        <v>1480</v>
+      </c>
     </row>
     <row r="1042" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1042" s="26"/>
-      <c r="B1042" s="24"/>
-      <c r="C1042" s="18"/>
-      <c r="D1042" s="19"/>
-      <c r="E1042" s="18"/>
-      <c r="F1042" s="19"/>
-      <c r="G1042" s="26"/>
-      <c r="H1042" s="6"/>
-      <c r="I1042" s="20"/>
-      <c r="J1042" s="20"/>
-    </row>
-    <row r="1043" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1043" s="26"/>
-      <c r="B1043" s="24"/>
-      <c r="C1043" s="18"/>
-      <c r="D1043" s="19"/>
-      <c r="E1043" s="18"/>
-      <c r="F1043" s="19"/>
-      <c r="G1043" s="26"/>
-      <c r="H1043" s="6"/>
-      <c r="I1043" s="20"/>
-      <c r="J1043" s="20"/>
+      <c r="A1042" s="26">
+        <v>44193</v>
+      </c>
+      <c r="B1042" s="24" t="s">
+        <v>683</v>
+      </c>
+      <c r="C1042" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1042" s="19" t="s">
+        <v>680</v>
+      </c>
+      <c r="E1042" s="18" t="s">
+        <v>1472</v>
+      </c>
+      <c r="F1042" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1042" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1042" s="6">
+        <v>44193</v>
+      </c>
+      <c r="I1042" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1042" s="20" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1043" s="26">
+        <v>44193</v>
+      </c>
+      <c r="B1043" s="24" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C1043" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1043" s="19" t="s">
+        <v>680</v>
+      </c>
+      <c r="E1043" s="18" t="s">
+        <v>1475</v>
+      </c>
+      <c r="F1043" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1043" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1043" s="6">
+        <v>44193</v>
+      </c>
+      <c r="I1043" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1043" s="20" t="s">
+        <v>1477</v>
+      </c>
     </row>
     <row r="1044" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1044" s="26"/>
-      <c r="B1044" s="24"/>
-      <c r="C1044" s="18"/>
-      <c r="D1044" s="19"/>
-      <c r="E1044" s="18"/>
-      <c r="F1044" s="19"/>
-      <c r="G1044" s="26"/>
-      <c r="H1044" s="6"/>
-      <c r="I1044" s="20"/>
-      <c r="J1044" s="20"/>
+      <c r="A1044" s="26">
+        <v>44193</v>
+      </c>
+      <c r="B1044" s="24" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C1044" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1044" s="19" t="s">
+        <v>680</v>
+      </c>
+      <c r="E1044" s="18" t="s">
+        <v>1476</v>
+      </c>
+      <c r="F1044" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1044" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1044" s="6">
+        <v>44193</v>
+      </c>
+      <c r="I1044" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1044" s="20" t="s">
+        <v>1478</v>
+      </c>
     </row>
     <row r="1045" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1045" s="26"/>
-      <c r="B1045" s="24"/>
-      <c r="C1045" s="18"/>
-      <c r="D1045" s="19"/>
-      <c r="E1045" s="18"/>
-      <c r="F1045" s="19"/>
-      <c r="G1045" s="26"/>
-      <c r="H1045" s="6"/>
-      <c r="I1045" s="20"/>
+      <c r="A1045" s="26">
+        <v>44193</v>
+      </c>
+      <c r="B1045" s="24" t="s">
+        <v>522</v>
+      </c>
+      <c r="C1045" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1045" s="19" t="s">
+        <v>680</v>
+      </c>
+      <c r="E1045" s="18" t="s">
+        <v>1481</v>
+      </c>
+      <c r="F1045" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1045" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1045" s="6">
+        <v>44193</v>
+      </c>
+      <c r="I1045" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="J1045" s="20"/>
     </row>
     <row r="1046" spans="1:10" x14ac:dyDescent="0.25">
@@ -35954,24 +36191,42 @@
       <c r="I1052" s="20"/>
       <c r="J1052" s="20"/>
     </row>
-    <row r="1053" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1053" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A1053" s="26"/>
-      <c r="B1053" s="24"/>
-      <c r="C1053" s="18"/>
-      <c r="D1053" s="19"/>
-      <c r="E1053" s="18"/>
+      <c r="B1053" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1053" s="18" t="s">
+        <v>644</v>
+      </c>
+      <c r="D1053" s="19" t="s">
+        <v>709</v>
+      </c>
+      <c r="E1053" s="18" t="s">
+        <v>1243</v>
+      </c>
       <c r="F1053" s="19"/>
       <c r="G1053" s="26"/>
       <c r="H1053" s="6"/>
       <c r="I1053" s="20"/>
-      <c r="J1053" s="20"/>
+      <c r="J1053" s="20" t="s">
+        <v>1464</v>
+      </c>
     </row>
     <row r="1054" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1054" s="26"/>
-      <c r="B1054" s="24"/>
-      <c r="C1054" s="18"/>
-      <c r="D1054" s="19"/>
-      <c r="E1054" s="18"/>
+      <c r="B1054" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1054" s="18" t="s">
+        <v>644</v>
+      </c>
+      <c r="D1054" s="19" t="s">
+        <v>709</v>
+      </c>
+      <c r="E1054" s="18" t="s">
+        <v>1419</v>
+      </c>
       <c r="F1054" s="19"/>
       <c r="G1054" s="26"/>
       <c r="H1054" s="6"/>
@@ -36037,6 +36292,162 @@
       <c r="H1059" s="6"/>
       <c r="I1059" s="20"/>
       <c r="J1059" s="20"/>
+    </row>
+    <row r="1060" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1060" s="26"/>
+      <c r="B1060" s="24"/>
+      <c r="C1060" s="18"/>
+      <c r="D1060" s="19"/>
+      <c r="E1060" s="18"/>
+      <c r="F1060" s="19"/>
+      <c r="G1060" s="26"/>
+      <c r="H1060" s="6"/>
+      <c r="I1060" s="20"/>
+      <c r="J1060" s="20"/>
+    </row>
+    <row r="1061" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1061" s="26"/>
+      <c r="B1061" s="24"/>
+      <c r="C1061" s="18"/>
+      <c r="D1061" s="19"/>
+      <c r="E1061" s="18"/>
+      <c r="F1061" s="19"/>
+      <c r="G1061" s="26"/>
+      <c r="H1061" s="6"/>
+      <c r="I1061" s="20"/>
+      <c r="J1061" s="20"/>
+    </row>
+    <row r="1062" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1062" s="26"/>
+      <c r="B1062" s="24"/>
+      <c r="C1062" s="18"/>
+      <c r="D1062" s="19"/>
+      <c r="E1062" s="18"/>
+      <c r="F1062" s="19"/>
+      <c r="G1062" s="26"/>
+      <c r="H1062" s="6"/>
+      <c r="I1062" s="20"/>
+      <c r="J1062" s="20"/>
+    </row>
+    <row r="1063" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1063" s="26"/>
+      <c r="B1063" s="24"/>
+      <c r="C1063" s="18"/>
+      <c r="D1063" s="19"/>
+      <c r="E1063" s="18"/>
+      <c r="F1063" s="19"/>
+      <c r="G1063" s="26"/>
+      <c r="H1063" s="6"/>
+      <c r="I1063" s="20"/>
+      <c r="J1063" s="20"/>
+    </row>
+    <row r="1064" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1064" s="26"/>
+      <c r="B1064" s="24"/>
+      <c r="C1064" s="18"/>
+      <c r="D1064" s="19"/>
+      <c r="E1064" s="18"/>
+      <c r="F1064" s="19"/>
+      <c r="G1064" s="26"/>
+      <c r="H1064" s="6"/>
+      <c r="I1064" s="20"/>
+      <c r="J1064" s="20"/>
+    </row>
+    <row r="1065" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1065" s="26"/>
+      <c r="B1065" s="24"/>
+      <c r="C1065" s="18"/>
+      <c r="D1065" s="19"/>
+      <c r="E1065" s="18"/>
+      <c r="F1065" s="19"/>
+      <c r="G1065" s="26"/>
+      <c r="H1065" s="6"/>
+      <c r="I1065" s="20"/>
+      <c r="J1065" s="20"/>
+    </row>
+    <row r="1066" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1066" s="26"/>
+      <c r="B1066" s="24"/>
+      <c r="C1066" s="18"/>
+      <c r="D1066" s="19"/>
+      <c r="E1066" s="18"/>
+      <c r="F1066" s="19"/>
+      <c r="G1066" s="26"/>
+      <c r="H1066" s="6"/>
+      <c r="I1066" s="20"/>
+      <c r="J1066" s="20"/>
+    </row>
+    <row r="1067" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1067" s="26"/>
+      <c r="B1067" s="24"/>
+      <c r="C1067" s="18"/>
+      <c r="D1067" s="19"/>
+      <c r="E1067" s="18"/>
+      <c r="F1067" s="19"/>
+      <c r="G1067" s="26"/>
+      <c r="H1067" s="6"/>
+      <c r="I1067" s="20"/>
+      <c r="J1067" s="20"/>
+    </row>
+    <row r="1068" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1068" s="26"/>
+      <c r="B1068" s="24"/>
+      <c r="C1068" s="18"/>
+      <c r="D1068" s="19"/>
+      <c r="E1068" s="18"/>
+      <c r="F1068" s="19"/>
+      <c r="G1068" s="26"/>
+      <c r="H1068" s="6"/>
+      <c r="I1068" s="20"/>
+      <c r="J1068" s="20"/>
+    </row>
+    <row r="1069" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1069" s="26"/>
+      <c r="B1069" s="24"/>
+      <c r="C1069" s="18"/>
+      <c r="D1069" s="19"/>
+      <c r="E1069" s="18"/>
+      <c r="F1069" s="19"/>
+      <c r="G1069" s="26"/>
+      <c r="H1069" s="6"/>
+      <c r="I1069" s="20"/>
+      <c r="J1069" s="20"/>
+    </row>
+    <row r="1070" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1070" s="26"/>
+      <c r="B1070" s="24"/>
+      <c r="C1070" s="18"/>
+      <c r="D1070" s="19"/>
+      <c r="E1070" s="18"/>
+      <c r="F1070" s="19"/>
+      <c r="G1070" s="26"/>
+      <c r="H1070" s="6"/>
+      <c r="I1070" s="20"/>
+      <c r="J1070" s="20"/>
+    </row>
+    <row r="1071" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1071" s="26"/>
+      <c r="B1071" s="24"/>
+      <c r="C1071" s="18"/>
+      <c r="D1071" s="19"/>
+      <c r="E1071" s="18"/>
+      <c r="F1071" s="19"/>
+      <c r="G1071" s="26"/>
+      <c r="H1071" s="6"/>
+      <c r="I1071" s="20"/>
+      <c r="J1071" s="20"/>
+    </row>
+    <row r="1072" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1072" s="26"/>
+      <c r="B1072" s="24"/>
+      <c r="C1072" s="18"/>
+      <c r="D1072" s="19"/>
+      <c r="E1072" s="18"/>
+      <c r="F1072" s="19"/>
+      <c r="G1072" s="26"/>
+      <c r="H1072" s="6"/>
+      <c r="I1072" s="20"/>
+      <c r="J1072" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1035" xr:uid="{00000000-0009-0000-0000-000000000000}">

</xml_diff>

<commit_message>
Acerto corpo nota pic red inss
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE7C740-F695-4616-AAA9-940164C6C5EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9F1E7E-2DB9-43CF-8260-06372B32BFD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7270" uniqueCount="1525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7324" uniqueCount="1533">
   <si>
     <t>Data</t>
   </si>
@@ -4851,6 +4851,31 @@
   </si>
   <si>
     <t>Relação de usuários</t>
+  </si>
+  <si>
+    <t>Lançamento contabil padrão de faturamento incorreto</t>
+  </si>
+  <si>
+    <t>Contas cadastradas no cliente 221 e produto 221000562-002 estão incorretas</t>
+  </si>
+  <si>
+    <t>Atualização dos módulos Estoque, Contabilidade e Gestão de Contratos</t>
+  </si>
+  <si>
+    <t>Reemitir a nf 1544 pedido 046180, Depto Fiscal reconfigurou os impostos</t>
+  </si>
+  <si>
+    <t>Numero do RPS 1609 divergente do numero da NF no site da Pref. De Barueri 1609</t>
+  </si>
+  <si>
+    <t>Eliminar resíduos dos pedidos 5984/5988/5990/5993/5996/6004/6014</t>
+  </si>
+  <si>
+    <t>Quanto a esse titulo abaixo, gentileza ajustar para cair em um único dia.
+É que se  aprovarmos ele sairá parcelado, por favor verifica</t>
+  </si>
+  <si>
+    <t>Fui extrair um relatório de rentabilidade do contrato  305.000.554, e o resultado está saindo diferente do relatório Comparativos</t>
   </si>
 </sst>
 </file>
@@ -5533,11 +5558,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1112"/>
+  <dimension ref="A1:J1118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1079" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1088" sqref="A1088"/>
+      <pane ySplit="1" topLeftCell="A1084" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1095" sqref="F1095"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37500,113 +37525,233 @@
       <c r="J1087" s="19"/>
     </row>
     <row r="1088" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1088" s="24"/>
-      <c r="B1088" s="22"/>
-      <c r="C1088" s="17"/>
-      <c r="D1088" s="18"/>
-      <c r="E1088" s="17"/>
-      <c r="F1088" s="18"/>
-      <c r="G1088" s="24"/>
-      <c r="H1088" s="6"/>
-      <c r="I1088" s="19"/>
+      <c r="A1088" s="24">
+        <v>44213</v>
+      </c>
+      <c r="B1088" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1088" s="17" t="s">
+        <v>629</v>
+      </c>
+      <c r="D1088" s="18" t="s">
+        <v>694</v>
+      </c>
+      <c r="E1088" s="17" t="s">
+        <v>1527</v>
+      </c>
+      <c r="F1088" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1088" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1088" s="6">
+        <v>44213</v>
+      </c>
+      <c r="I1088" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="J1088" s="19"/>
     </row>
-    <row r="1089" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1089" s="24"/>
-      <c r="B1089" s="22"/>
-      <c r="C1089" s="17"/>
-      <c r="D1089" s="18"/>
-      <c r="E1089" s="17"/>
-      <c r="F1089" s="18"/>
-      <c r="G1089" s="24"/>
-      <c r="H1089" s="6"/>
-      <c r="I1089" s="19"/>
-      <c r="J1089" s="19"/>
+    <row r="1089" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1089" s="24">
+        <v>44214</v>
+      </c>
+      <c r="B1089" s="22" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C1089" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1089" s="18" t="s">
+        <v>615</v>
+      </c>
+      <c r="E1089" s="17" t="s">
+        <v>1525</v>
+      </c>
+      <c r="F1089" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1089" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1089" s="6">
+        <v>44214</v>
+      </c>
+      <c r="I1089" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1089" s="19" t="s">
+        <v>1526</v>
+      </c>
     </row>
     <row r="1090" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1090" s="24"/>
-      <c r="B1090" s="22"/>
-      <c r="C1090" s="17"/>
-      <c r="D1090" s="18"/>
-      <c r="E1090" s="17"/>
-      <c r="F1090" s="18"/>
-      <c r="G1090" s="24"/>
-      <c r="H1090" s="6"/>
-      <c r="I1090" s="19"/>
+      <c r="A1090" s="24">
+        <v>44214</v>
+      </c>
+      <c r="B1090" s="22" t="s">
+        <v>503</v>
+      </c>
+      <c r="C1090" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1090" s="18" t="s">
+        <v>719</v>
+      </c>
+      <c r="E1090" s="17" t="s">
+        <v>1514</v>
+      </c>
+      <c r="F1090" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1090" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1090" s="6">
+        <v>44214</v>
+      </c>
+      <c r="I1090" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="J1090" s="19"/>
     </row>
     <row r="1091" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1091" s="24"/>
-      <c r="B1091" s="22"/>
-      <c r="C1091" s="17"/>
-      <c r="D1091" s="18"/>
-      <c r="E1091" s="17"/>
-      <c r="F1091" s="18"/>
-      <c r="G1091" s="24"/>
-      <c r="H1091" s="6"/>
-      <c r="I1091" s="19"/>
+      <c r="A1091" s="24">
+        <v>44214</v>
+      </c>
+      <c r="B1091" s="22" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C1091" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1091" s="18" t="s">
+        <v>615</v>
+      </c>
+      <c r="E1091" s="17" t="s">
+        <v>1528</v>
+      </c>
+      <c r="F1091" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1091" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1091" s="6">
+        <v>44214</v>
+      </c>
+      <c r="I1091" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="J1091" s="19"/>
     </row>
     <row r="1092" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1092" s="24"/>
-      <c r="B1092" s="22"/>
-      <c r="C1092" s="17"/>
-      <c r="D1092" s="18"/>
-      <c r="E1092" s="17"/>
-      <c r="F1092" s="18"/>
-      <c r="G1092" s="24"/>
-      <c r="H1092" s="6"/>
-      <c r="I1092" s="19"/>
+      <c r="A1092" s="24">
+        <v>44214</v>
+      </c>
+      <c r="B1092" s="22" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C1092" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1092" s="18" t="s">
+        <v>665</v>
+      </c>
+      <c r="E1092" s="17" t="s">
+        <v>1529</v>
+      </c>
+      <c r="F1092" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1092" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1092" s="6">
+        <v>44214</v>
+      </c>
+      <c r="I1092" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="J1092" s="19"/>
     </row>
-    <row r="1093" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A1093" s="24"/>
+    <row r="1093" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1093" s="24">
+        <v>44215</v>
+      </c>
       <c r="B1093" s="22" t="s">
-        <v>16</v>
+        <v>533</v>
       </c>
       <c r="C1093" s="17" t="s">
-        <v>629</v>
+        <v>534</v>
       </c>
       <c r="D1093" s="18" t="s">
-        <v>694</v>
+        <v>735</v>
       </c>
       <c r="E1093" s="17" t="s">
-        <v>1228</v>
-      </c>
-      <c r="F1093" s="18"/>
-      <c r="G1093" s="24"/>
-      <c r="H1093" s="6"/>
-      <c r="I1093" s="19"/>
-      <c r="J1093" s="19" t="s">
-        <v>1449</v>
-      </c>
+        <v>1531</v>
+      </c>
+      <c r="F1093" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1093" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1093" s="6">
+        <v>44215</v>
+      </c>
+      <c r="I1093" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1093" s="19"/>
     </row>
     <row r="1094" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1094" s="24"/>
+      <c r="A1094" s="24">
+        <v>44215</v>
+      </c>
       <c r="B1094" s="22" t="s">
-        <v>16</v>
+        <v>313</v>
       </c>
       <c r="C1094" s="17" t="s">
-        <v>629</v>
+        <v>28</v>
       </c>
       <c r="D1094" s="18" t="s">
-        <v>694</v>
+        <v>665</v>
       </c>
       <c r="E1094" s="17" t="s">
-        <v>1404</v>
-      </c>
-      <c r="F1094" s="18"/>
-      <c r="G1094" s="24"/>
-      <c r="H1094" s="6"/>
-      <c r="I1094" s="19"/>
+        <v>1530</v>
+      </c>
+      <c r="F1094" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1094" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1094" s="6">
+        <v>44215</v>
+      </c>
+      <c r="I1094" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="J1094" s="19"/>
     </row>
-    <row r="1095" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1095" s="24"/>
-      <c r="B1095" s="22"/>
-      <c r="C1095" s="17"/>
-      <c r="D1095" s="18"/>
-      <c r="E1095" s="17"/>
+    <row r="1095" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1095" s="24">
+        <v>44215</v>
+      </c>
+      <c r="B1095" s="22" t="s">
+        <v>951</v>
+      </c>
+      <c r="C1095" s="17" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1095" s="18" t="s">
+        <v>735</v>
+      </c>
+      <c r="E1095" s="17" t="s">
+        <v>1532</v>
+      </c>
       <c r="F1095" s="18"/>
       <c r="G1095" s="24"/>
       <c r="H1095" s="6"/>
@@ -37649,24 +37794,42 @@
       <c r="I1098" s="19"/>
       <c r="J1098" s="19"/>
     </row>
-    <row r="1099" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1099" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A1099" s="24"/>
-      <c r="B1099" s="22"/>
-      <c r="C1099" s="17"/>
-      <c r="D1099" s="18"/>
-      <c r="E1099" s="17"/>
+      <c r="B1099" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1099" s="17" t="s">
+        <v>629</v>
+      </c>
+      <c r="D1099" s="18" t="s">
+        <v>694</v>
+      </c>
+      <c r="E1099" s="17" t="s">
+        <v>1228</v>
+      </c>
       <c r="F1099" s="18"/>
       <c r="G1099" s="24"/>
       <c r="H1099" s="6"/>
       <c r="I1099" s="19"/>
-      <c r="J1099" s="19"/>
+      <c r="J1099" s="19" t="s">
+        <v>1449</v>
+      </c>
     </row>
     <row r="1100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1100" s="24"/>
-      <c r="B1100" s="22"/>
-      <c r="C1100" s="17"/>
-      <c r="D1100" s="18"/>
-      <c r="E1100" s="17"/>
+      <c r="B1100" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1100" s="17" t="s">
+        <v>629</v>
+      </c>
+      <c r="D1100" s="18" t="s">
+        <v>694</v>
+      </c>
+      <c r="E1100" s="17" t="s">
+        <v>1404</v>
+      </c>
       <c r="F1100" s="18"/>
       <c r="G1100" s="24"/>
       <c r="H1100" s="6"/>
@@ -37816,6 +37979,78 @@
       <c r="H1112" s="6"/>
       <c r="I1112" s="19"/>
       <c r="J1112" s="19"/>
+    </row>
+    <row r="1113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1113" s="24"/>
+      <c r="B1113" s="22"/>
+      <c r="C1113" s="17"/>
+      <c r="D1113" s="18"/>
+      <c r="E1113" s="17"/>
+      <c r="F1113" s="18"/>
+      <c r="G1113" s="24"/>
+      <c r="H1113" s="6"/>
+      <c r="I1113" s="19"/>
+      <c r="J1113" s="19"/>
+    </row>
+    <row r="1114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1114" s="24"/>
+      <c r="B1114" s="22"/>
+      <c r="C1114" s="17"/>
+      <c r="D1114" s="18"/>
+      <c r="E1114" s="17"/>
+      <c r="F1114" s="18"/>
+      <c r="G1114" s="24"/>
+      <c r="H1114" s="6"/>
+      <c r="I1114" s="19"/>
+      <c r="J1114" s="19"/>
+    </row>
+    <row r="1115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1115" s="24"/>
+      <c r="B1115" s="22"/>
+      <c r="C1115" s="17"/>
+      <c r="D1115" s="18"/>
+      <c r="E1115" s="17"/>
+      <c r="F1115" s="18"/>
+      <c r="G1115" s="24"/>
+      <c r="H1115" s="6"/>
+      <c r="I1115" s="19"/>
+      <c r="J1115" s="19"/>
+    </row>
+    <row r="1116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1116" s="24"/>
+      <c r="B1116" s="22"/>
+      <c r="C1116" s="17"/>
+      <c r="D1116" s="18"/>
+      <c r="E1116" s="17"/>
+      <c r="F1116" s="18"/>
+      <c r="G1116" s="24"/>
+      <c r="H1116" s="6"/>
+      <c r="I1116" s="19"/>
+      <c r="J1116" s="19"/>
+    </row>
+    <row r="1117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1117" s="24"/>
+      <c r="B1117" s="22"/>
+      <c r="C1117" s="17"/>
+      <c r="D1117" s="18"/>
+      <c r="E1117" s="17"/>
+      <c r="F1117" s="18"/>
+      <c r="G1117" s="24"/>
+      <c r="H1117" s="6"/>
+      <c r="I1117" s="19"/>
+      <c r="J1117" s="19"/>
+    </row>
+    <row r="1118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1118" s="24"/>
+      <c r="B1118" s="22"/>
+      <c r="C1118" s="17"/>
+      <c r="D1118" s="18"/>
+      <c r="E1118" s="17"/>
+      <c r="F1118" s="18"/>
+      <c r="G1118" s="24"/>
+      <c r="H1118" s="6"/>
+      <c r="I1118" s="19"/>
+      <c r="J1118" s="19"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1065" xr:uid="{00000000-0009-0000-0000-000000000000}">

</xml_diff>

<commit_message>
Gravar outro dados SF1 Doc Ent
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9F1E7E-2DB9-43CF-8260-06372B32BFD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAF939F-E0D9-4A41-A733-093FDDA5A649}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha1" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_FilterDatabase_0" localSheetId="0">'Demandas BK - Protheus'!$A$1:$I$53</definedName>
@@ -53,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7324" uniqueCount="1533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7372" uniqueCount="1542">
   <si>
     <t>Data</t>
   </si>
@@ -4876,6 +4875,34 @@
   </si>
   <si>
     <t>Fui extrair um relatório de rentabilidade do contrato  305.000.554, e o resultado está saindo diferente do relatório Comparativos</t>
+  </si>
+  <si>
+    <t>Ajustes EFD BK de dezembro/2020</t>
+  </si>
+  <si>
+    <t>Conforme nos falamos via fone, segue abaixo o modelo de titulo LPM, utilizado para pagamento de PESSOA JURIDICA. Conforme você pode ver no e-mail abaixo, foi criada uma função para títulos LPM (CLT) e, agora teremos que colocar uma condição para os LPM de PESSOA JURIDICA. O que consegui observar de diferente, entre eles,  é o NR do CHQ que tem as siglas PJ. Podemos utilizar para fazer uma nova condição e direcionar esses títulos PJ para a conta 2.1.1.01.001 (fornecedor)?</t>
+  </si>
+  <si>
+    <t>Alterado o fonte LP530BX.PRW</t>
+  </si>
+  <si>
+    <t>Estou tentando gerar o Arquivo de Folha pelo Consorcio BHG INTERIOR conta 6559-5, não esta deixando, quando eu gero mais de 1 arquivo ele sobrepõe o outro ou seja, so aparece o arquivo Nº 1</t>
+  </si>
+  <si>
+    <t>Acerto NF que não aparecia para aprovar</t>
+  </si>
+  <si>
+    <t>Estava como superior o Roger (verificar depois)</t>
+  </si>
+  <si>
+    <t>Ajustes EFD Balsa e HBG de dezembro/2020</t>
+  </si>
+  <si>
+    <t>Ajustes EFD Balsa e BK de dezembro/2020 (diversas planilhas
+Ajuste TES 118 BK</t>
+  </si>
+  <si>
+    <t>Gravar dados adicionais da mesma forma que na pré-nota de entrada no documento de entrada</t>
   </si>
 </sst>
 </file>
@@ -5558,11 +5585,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1118"/>
+  <dimension ref="A1:J1126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1084" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1095" sqref="F1095"/>
+      <pane ySplit="1" topLeftCell="A1100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1103" sqref="A1103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37759,105 +37786,209 @@
       <c r="J1095" s="19"/>
     </row>
     <row r="1096" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1096" s="24"/>
-      <c r="B1096" s="22"/>
-      <c r="C1096" s="17"/>
-      <c r="D1096" s="18"/>
-      <c r="E1096" s="17"/>
-      <c r="F1096" s="18"/>
-      <c r="G1096" s="24"/>
-      <c r="H1096" s="6"/>
-      <c r="I1096" s="19"/>
+      <c r="A1096" s="24">
+        <v>44216</v>
+      </c>
+      <c r="B1096" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="C1096" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1096" s="18" t="s">
+        <v>735</v>
+      </c>
+      <c r="E1096" s="17" t="s">
+        <v>1533</v>
+      </c>
+      <c r="F1096" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1096" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1096" s="6">
+        <v>44216</v>
+      </c>
+      <c r="I1096" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="J1096" s="19"/>
     </row>
-    <row r="1097" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1097" s="24"/>
-      <c r="B1097" s="22"/>
-      <c r="C1097" s="17"/>
-      <c r="D1097" s="18"/>
-      <c r="E1097" s="17"/>
-      <c r="F1097" s="18"/>
-      <c r="G1097" s="24"/>
-      <c r="H1097" s="6"/>
-      <c r="I1097" s="19"/>
-      <c r="J1097" s="19"/>
-    </row>
-    <row r="1098" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1098" s="24"/>
-      <c r="B1098" s="22"/>
-      <c r="C1098" s="17"/>
-      <c r="D1098" s="18"/>
-      <c r="E1098" s="17"/>
+    <row r="1097" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1097" s="24">
+        <v>44216</v>
+      </c>
+      <c r="B1097" s="22" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C1097" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1097" s="18" t="s">
+        <v>735</v>
+      </c>
+      <c r="E1097" s="17" t="s">
+        <v>1534</v>
+      </c>
+      <c r="F1097" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1097" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1097" s="6">
+        <v>44216</v>
+      </c>
+      <c r="I1097" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1097" s="19" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A1098" s="24">
+        <v>44216</v>
+      </c>
+      <c r="B1098" s="22" t="s">
+        <v>668</v>
+      </c>
+      <c r="C1098" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1098" s="18" t="s">
+        <v>665</v>
+      </c>
+      <c r="E1098" s="17" t="s">
+        <v>1536</v>
+      </c>
       <c r="F1098" s="18"/>
       <c r="G1098" s="24"/>
       <c r="H1098" s="6"/>
       <c r="I1098" s="19"/>
       <c r="J1098" s="19"/>
     </row>
-    <row r="1099" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A1099" s="24"/>
+    <row r="1099" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1099" s="24">
+        <v>44216</v>
+      </c>
       <c r="B1099" s="22" t="s">
-        <v>16</v>
+        <v>481</v>
       </c>
       <c r="C1099" s="17" t="s">
-        <v>629</v>
+        <v>20</v>
       </c>
       <c r="D1099" s="18" t="s">
-        <v>694</v>
+        <v>665</v>
       </c>
       <c r="E1099" s="17" t="s">
-        <v>1228</v>
-      </c>
-      <c r="F1099" s="18"/>
-      <c r="G1099" s="24"/>
-      <c r="H1099" s="6"/>
-      <c r="I1099" s="19"/>
+        <v>1537</v>
+      </c>
+      <c r="F1099" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1099" s="24" t="s">
+        <v>1171</v>
+      </c>
+      <c r="H1099" s="6">
+        <v>44216</v>
+      </c>
+      <c r="I1099" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="J1099" s="19" t="s">
-        <v>1449</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="1100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1100" s="24"/>
+      <c r="A1100" s="24">
+        <v>44216</v>
+      </c>
       <c r="B1100" s="22" t="s">
-        <v>16</v>
+        <v>507</v>
       </c>
       <c r="C1100" s="17" t="s">
-        <v>629</v>
+        <v>97</v>
       </c>
       <c r="D1100" s="18" t="s">
-        <v>694</v>
+        <v>735</v>
       </c>
       <c r="E1100" s="17" t="s">
-        <v>1404</v>
-      </c>
-      <c r="F1100" s="18"/>
-      <c r="G1100" s="24"/>
-      <c r="H1100" s="6"/>
-      <c r="I1100" s="19"/>
+        <v>1539</v>
+      </c>
+      <c r="F1100" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1100" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1100" s="6">
+        <v>44216</v>
+      </c>
+      <c r="I1100" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="J1100" s="19"/>
     </row>
-    <row r="1101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1101" s="24"/>
-      <c r="B1101" s="22"/>
-      <c r="C1101" s="17"/>
-      <c r="D1101" s="18"/>
-      <c r="E1101" s="17"/>
-      <c r="F1101" s="18"/>
-      <c r="G1101" s="24"/>
-      <c r="H1101" s="6"/>
-      <c r="I1101" s="19"/>
+    <row r="1101" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1101" s="24">
+        <v>44217</v>
+      </c>
+      <c r="B1101" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="C1101" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1101" s="18" t="s">
+        <v>735</v>
+      </c>
+      <c r="E1101" s="17" t="s">
+        <v>1540</v>
+      </c>
+      <c r="F1101" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1101" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1101" s="6">
+        <v>44217</v>
+      </c>
+      <c r="I1101" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="J1101" s="19"/>
     </row>
-    <row r="1102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1102" s="24"/>
-      <c r="B1102" s="22"/>
-      <c r="C1102" s="17"/>
-      <c r="D1102" s="18"/>
-      <c r="E1102" s="17"/>
-      <c r="F1102" s="18"/>
-      <c r="G1102" s="24"/>
-      <c r="H1102" s="6"/>
-      <c r="I1102" s="19"/>
+    <row r="1102" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1102" s="24">
+        <v>44217</v>
+      </c>
+      <c r="B1102" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="C1102" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1102" s="18" t="s">
+        <v>665</v>
+      </c>
+      <c r="E1102" s="17" t="s">
+        <v>1541</v>
+      </c>
+      <c r="F1102" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1102" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1102" s="6">
+        <v>44217</v>
+      </c>
+      <c r="I1102" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="J1102" s="19"/>
     </row>
     <row r="1103" spans="1:10" x14ac:dyDescent="0.25">
@@ -37908,24 +38039,42 @@
       <c r="I1106" s="19"/>
       <c r="J1106" s="19"/>
     </row>
-    <row r="1107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1107" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A1107" s="24"/>
-      <c r="B1107" s="22"/>
-      <c r="C1107" s="17"/>
-      <c r="D1107" s="18"/>
-      <c r="E1107" s="17"/>
+      <c r="B1107" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1107" s="17" t="s">
+        <v>629</v>
+      </c>
+      <c r="D1107" s="18" t="s">
+        <v>694</v>
+      </c>
+      <c r="E1107" s="17" t="s">
+        <v>1228</v>
+      </c>
       <c r="F1107" s="18"/>
       <c r="G1107" s="24"/>
       <c r="H1107" s="6"/>
       <c r="I1107" s="19"/>
-      <c r="J1107" s="19"/>
+      <c r="J1107" s="19" t="s">
+        <v>1449</v>
+      </c>
     </row>
     <row r="1108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1108" s="24"/>
-      <c r="B1108" s="22"/>
-      <c r="C1108" s="17"/>
-      <c r="D1108" s="18"/>
-      <c r="E1108" s="17"/>
+      <c r="B1108" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1108" s="17" t="s">
+        <v>629</v>
+      </c>
+      <c r="D1108" s="18" t="s">
+        <v>694</v>
+      </c>
+      <c r="E1108" s="17" t="s">
+        <v>1404</v>
+      </c>
       <c r="F1108" s="18"/>
       <c r="G1108" s="24"/>
       <c r="H1108" s="6"/>
@@ -38052,6 +38201,102 @@
       <c r="I1118" s="19"/>
       <c r="J1118" s="19"/>
     </row>
+    <row r="1119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1119" s="24"/>
+      <c r="B1119" s="22"/>
+      <c r="C1119" s="17"/>
+      <c r="D1119" s="18"/>
+      <c r="E1119" s="17"/>
+      <c r="F1119" s="18"/>
+      <c r="G1119" s="24"/>
+      <c r="H1119" s="6"/>
+      <c r="I1119" s="19"/>
+      <c r="J1119" s="19"/>
+    </row>
+    <row r="1120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1120" s="24"/>
+      <c r="B1120" s="22"/>
+      <c r="C1120" s="17"/>
+      <c r="D1120" s="18"/>
+      <c r="E1120" s="17"/>
+      <c r="F1120" s="18"/>
+      <c r="G1120" s="24"/>
+      <c r="H1120" s="6"/>
+      <c r="I1120" s="19"/>
+      <c r="J1120" s="19"/>
+    </row>
+    <row r="1121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1121" s="24"/>
+      <c r="B1121" s="22"/>
+      <c r="C1121" s="17"/>
+      <c r="D1121" s="18"/>
+      <c r="E1121" s="17"/>
+      <c r="F1121" s="18"/>
+      <c r="G1121" s="24"/>
+      <c r="H1121" s="6"/>
+      <c r="I1121" s="19"/>
+      <c r="J1121" s="19"/>
+    </row>
+    <row r="1122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1122" s="24"/>
+      <c r="B1122" s="22"/>
+      <c r="C1122" s="17"/>
+      <c r="D1122" s="18"/>
+      <c r="E1122" s="17"/>
+      <c r="F1122" s="18"/>
+      <c r="G1122" s="24"/>
+      <c r="H1122" s="6"/>
+      <c r="I1122" s="19"/>
+      <c r="J1122" s="19"/>
+    </row>
+    <row r="1123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1123" s="24"/>
+      <c r="B1123" s="22"/>
+      <c r="C1123" s="17"/>
+      <c r="D1123" s="18"/>
+      <c r="E1123" s="17"/>
+      <c r="F1123" s="18"/>
+      <c r="G1123" s="24"/>
+      <c r="H1123" s="6"/>
+      <c r="I1123" s="19"/>
+      <c r="J1123" s="19"/>
+    </row>
+    <row r="1124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1124" s="24"/>
+      <c r="B1124" s="22"/>
+      <c r="C1124" s="17"/>
+      <c r="D1124" s="18"/>
+      <c r="E1124" s="17"/>
+      <c r="F1124" s="18"/>
+      <c r="G1124" s="24"/>
+      <c r="H1124" s="6"/>
+      <c r="I1124" s="19"/>
+      <c r="J1124" s="19"/>
+    </row>
+    <row r="1125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1125" s="24"/>
+      <c r="B1125" s="22"/>
+      <c r="C1125" s="17"/>
+      <c r="D1125" s="18"/>
+      <c r="E1125" s="17"/>
+      <c r="F1125" s="18"/>
+      <c r="G1125" s="24"/>
+      <c r="H1125" s="6"/>
+      <c r="I1125" s="19"/>
+      <c r="J1125" s="19"/>
+    </row>
+    <row r="1126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1126" s="24"/>
+      <c r="B1126" s="22"/>
+      <c r="C1126" s="17"/>
+      <c r="D1126" s="18"/>
+      <c r="E1126" s="17"/>
+      <c r="F1126" s="18"/>
+      <c r="G1126" s="24"/>
+      <c r="H1126" s="6"/>
+      <c r="I1126" s="19"/>
+      <c r="J1126" s="19"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1065" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J1058">
@@ -38063,98 +38308,4 @@
   <pageSetup paperSize="9" scale="10" firstPageNumber="0" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BE47A0-52AD-4DE9-9016-8618E23C11F7}">
-  <dimension ref="D3:J15"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="J3">
-        <v>321.14999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D4">
-        <v>6.75123622</v>
-      </c>
-      <c r="J4">
-        <v>204.23</v>
-      </c>
-    </row>
-    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D5">
-        <v>58447.05</v>
-      </c>
-      <c r="J5">
-        <v>115.68</v>
-      </c>
-    </row>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D6">
-        <v>6.5965221600000001</v>
-      </c>
-      <c r="J6">
-        <f>SUM(J3:J5)</f>
-        <v>641.05999999999995</v>
-      </c>
-    </row>
-    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D7">
-        <f>+D4-D6</f>
-        <v>0.15471405999999988</v>
-      </c>
-    </row>
-    <row r="8" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D8">
-        <f>+D7*D5</f>
-        <v>9042.5804005229929</v>
-      </c>
-    </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="G9">
-        <v>60836.34</v>
-      </c>
-    </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="G10">
-        <v>49577.79</v>
-      </c>
-    </row>
-    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="G11">
-        <f>+G9-G10</f>
-        <v>11258.549999999996</v>
-      </c>
-    </row>
-    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="G12">
-        <f>+G11/G9</f>
-        <v>0.18506290812366419</v>
-      </c>
-    </row>
-    <row r="14" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="G14">
-        <f>1-G12</f>
-        <v>0.81493709187633578</v>
-      </c>
-    </row>
-    <row r="15" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="G15">
-        <f>+G14*G9</f>
-        <v>49577.79</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Substituir M0_NOME por FWEmpName(cEmpAnt)
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E1B384-3DDA-4333-84C5-167B25689EF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABEB0CD-CAB1-4663-A453-9734783C41A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7372" uniqueCount="1542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7396" uniqueCount="1546">
   <si>
     <t>Data</t>
   </si>
@@ -4903,6 +4903,18 @@
   </si>
   <si>
     <t>Gravar dados adicionais da mesma forma que na pré-nota de entrada no documento de entrada</t>
+  </si>
+  <si>
+    <t>Espelho do pedido de venda não sai obs de pedido avulos</t>
+  </si>
+  <si>
+    <t>Fabio Quirino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segue o que está ocorrendo quando realizo a aprovação (tela de erro). </t>
+  </si>
+  <si>
+    <t>Retirar bitributação de alguns produtos</t>
   </si>
 </sst>
 </file>
@@ -5588,8 +5600,8 @@
   <dimension ref="A1:J1131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1094" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1102" sqref="A1102"/>
+      <pane ySplit="1" topLeftCell="A1097" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1105" sqref="A1105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37515,10 +37527,18 @@
       <c r="E1086" s="17" t="s">
         <v>1523</v>
       </c>
-      <c r="F1086" s="18"/>
-      <c r="G1086" s="24"/>
-      <c r="H1086" s="6"/>
-      <c r="I1086" s="19"/>
+      <c r="F1086" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1086" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1086" s="6">
+        <v>44217</v>
+      </c>
+      <c r="I1086" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="J1086" s="19"/>
     </row>
     <row r="1087" spans="1:10" x14ac:dyDescent="0.25">
@@ -37992,39 +38012,93 @@
       <c r="J1102" s="19"/>
     </row>
     <row r="1103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1103" s="24"/>
-      <c r="B1103" s="22"/>
-      <c r="C1103" s="17"/>
-      <c r="D1103" s="18"/>
-      <c r="E1103" s="17"/>
-      <c r="F1103" s="18"/>
-      <c r="G1103" s="24"/>
-      <c r="H1103" s="6"/>
-      <c r="I1103" s="19"/>
+      <c r="A1103" s="24">
+        <v>44218</v>
+      </c>
+      <c r="B1103" s="22" t="s">
+        <v>420</v>
+      </c>
+      <c r="C1103" s="17" t="s">
+        <v>680</v>
+      </c>
+      <c r="D1103" s="18" t="s">
+        <v>615</v>
+      </c>
+      <c r="E1103" s="17" t="s">
+        <v>1542</v>
+      </c>
+      <c r="F1103" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1103" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1103" s="6">
+        <v>44218</v>
+      </c>
+      <c r="I1103" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="J1103" s="19"/>
     </row>
     <row r="1104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1104" s="24"/>
-      <c r="B1104" s="22"/>
-      <c r="C1104" s="17"/>
-      <c r="D1104" s="18"/>
-      <c r="E1104" s="17"/>
-      <c r="F1104" s="18"/>
-      <c r="G1104" s="24"/>
-      <c r="H1104" s="6"/>
-      <c r="I1104" s="19"/>
+      <c r="A1104" s="24">
+        <v>44221</v>
+      </c>
+      <c r="B1104" s="22" t="s">
+        <v>1543</v>
+      </c>
+      <c r="C1104" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1104" s="18" t="s">
+        <v>615</v>
+      </c>
+      <c r="E1104" s="17" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F1104" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1104" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1104" s="6">
+        <v>44221</v>
+      </c>
+      <c r="I1104" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="J1104" s="19"/>
     </row>
     <row r="1105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1105" s="24"/>
-      <c r="B1105" s="22"/>
-      <c r="C1105" s="17"/>
-      <c r="D1105" s="18"/>
-      <c r="E1105" s="17"/>
-      <c r="F1105" s="18"/>
-      <c r="G1105" s="24"/>
-      <c r="H1105" s="6"/>
-      <c r="I1105" s="19"/>
+      <c r="A1105" s="24">
+        <v>44221</v>
+      </c>
+      <c r="B1105" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="C1105" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1105" s="18" t="s">
+        <v>615</v>
+      </c>
+      <c r="E1105" s="17" t="s">
+        <v>1545</v>
+      </c>
+      <c r="F1105" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1105" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1105" s="6">
+        <v>44221</v>
+      </c>
+      <c r="I1105" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="J1105" s="19"/>
     </row>
     <row r="1106" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Alteração na chamada da func GeraCsv
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F201CE1-EEA7-496F-A767-E20D75BFCD6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B029E925-891B-4284-B054-927B7A522490}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7626" uniqueCount="1590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7718" uniqueCount="1610">
   <si>
     <t>Responsável</t>
   </si>
@@ -4938,9 +4938,6 @@
     <t>Google Meet</t>
   </si>
   <si>
-    <t>Por favor pode verificar a condição de pagamento ainda não abre para colocar mais datas no vencimento (Pré nota).</t>
-  </si>
-  <si>
     <t>Refazimento da NF 758 que estava sem INSS retido</t>
   </si>
   <si>
@@ -5032,9 +5029,6 @@
     <t>Desentendimento estre as áreas Fiscal, Financeiro e Gestão</t>
   </si>
   <si>
-    <t>Camado aberto na Totvs, realizado os procedimentos solicitados , sem sucesso</t>
-  </si>
-  <si>
     <t>Executado Backup/Restore das tabelas CT2010 e CTK010</t>
   </si>
   <si>
@@ -5048,6 +5042,75 @@
   </si>
   <si>
     <t>Favor excluir os pagamentos da colaboradora Raquel Azevedo Nogueira</t>
+  </si>
+  <si>
+    <t>Em desenvolvimento</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
+  </si>
+  <si>
+    <t>Camado aberto na Totvs, realizado os procedimentos solicitados , sem sucesso - em andamento</t>
+  </si>
+  <si>
+    <t>Jose Mário: Visualizo os 2 documentos mas não consigo classificar p pagamento:</t>
+  </si>
+  <si>
+    <t>Atualização dos pacotes: 21-02-04_ATUALIZACAO_12.1.25_GCT_EXPEDICAO_CONTINUA (execução do cmpatibilizador UPDDISTR) e do pacote 10567712_drhgch-23055_12.1.25 (DIRF 2021)</t>
+  </si>
+  <si>
+    <t>Por favor pode verificar a condição de pagamento ainda não abre para colocar mais datas no vencimento (Pré nota) quando tem mais de 1 vencimento</t>
+  </si>
+  <si>
+    <t>Reunião - Digitação de Documentos de Entrada</t>
+  </si>
+  <si>
+    <t>Atualização dos Binários:
+20-11-13-DBACCESS_WINDOWS_X64_BUILD-20200606
+21-01-11-P12-SMARTCLIENT_BUILD-19.3.1.2_WINDOWS_X64
+21-01-21-P12_APPSERVER_BUILD-19.3.1.5_WINDOWS_X64</t>
+  </si>
+  <si>
+    <t>Necessário atualizar manualmente todas as pastas locais de acesso ao Protheus</t>
+  </si>
+  <si>
+    <t>Ediane: Estou tentando fazer umas baixas só do Balsa nova e não está permitindo</t>
+  </si>
+  <si>
+    <t>Contabilidade não havia criado o calendário contábil para 2021 nesta empresa</t>
+  </si>
+  <si>
+    <t>Auxilio Fernando da Contabilidade emitir realtório de Despesas por CC</t>
+  </si>
+  <si>
+    <t>Alinhamento da base teste com a base oficial</t>
+  </si>
+  <si>
+    <t>Solicita bloqueio de lançamentos contábeis Off-Line</t>
+  </si>
+  <si>
+    <t>Solicita a possibilidade de deixar abertura e bloqueio de períodos contábeis somente para ele e o Xavier</t>
+  </si>
+  <si>
+    <t>Solicita alteração dos pedidos 044137 e 044878 que sairão pela filial e não pela matriz (alterar retençao de ISS)</t>
+  </si>
+  <si>
+    <t>Sr. José Mário solicitou emissão de pedidos emitidos no mês de janeiro/2021</t>
+  </si>
+  <si>
+    <t>Emitido o relatório e demonstrado onde emitir</t>
+  </si>
+  <si>
+    <t>Pedidos referentes a contrato finalizado</t>
+  </si>
+  <si>
+    <t>Ediane: Estou tentando fazer umas baixas só do Balsa nova e não está permitindo (BKTER)</t>
+  </si>
+  <si>
+    <t>Esclarecimentos a respeitos de titulos a pagar não baixados na empresa Balsa Nova</t>
+  </si>
+  <si>
+    <t>Financeiro não está baixando os títulos a pagar na Balsa Nova</t>
   </si>
 </sst>
 </file>
@@ -5702,11 +5765,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1154"/>
+  <dimension ref="A1:J1167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1092" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1099" sqref="A1099"/>
+      <pane ySplit="1" topLeftCell="A1118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1126" sqref="D1126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -37942,7 +38005,7 @@
         <v>687</v>
       </c>
       <c r="F1091" s="10" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="G1091" s="11" t="s">
         <v>83</v>
@@ -37954,7 +38017,7 @@
         <v>14</v>
       </c>
       <c r="J1091" s="13" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="1092" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -38033,7 +38096,7 @@
         <v>1048</v>
       </c>
       <c r="E1094" s="11" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="F1094" s="10" t="s">
         <v>1551</v>
@@ -38068,7 +38131,7 @@
         <v>728</v>
       </c>
       <c r="F1095" s="10" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="G1095" s="11" t="s">
         <v>103</v>
@@ -38095,10 +38158,10 @@
         <v>673</v>
       </c>
       <c r="E1096" s="11" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="F1096" s="10" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="G1096" s="11" t="s">
         <v>83</v>
@@ -38125,10 +38188,10 @@
         <v>531</v>
       </c>
       <c r="E1097" s="11" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="F1097" s="10" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="G1097" s="11" t="s">
         <v>83</v>
@@ -38155,10 +38218,10 @@
         <v>1048</v>
       </c>
       <c r="E1098" s="11" t="s">
+        <v>1556</v>
+      </c>
+      <c r="F1098" s="10" t="s">
         <v>1557</v>
-      </c>
-      <c r="F1098" s="10" t="s">
-        <v>1558</v>
       </c>
       <c r="G1098" s="11" t="s">
         <v>103</v>
@@ -38188,7 +38251,7 @@
         <v>728</v>
       </c>
       <c r="F1099" s="10" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="G1099" s="11" t="s">
         <v>103</v>
@@ -38218,7 +38281,7 @@
         <v>687</v>
       </c>
       <c r="F1100" s="10" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="G1100" s="11" t="s">
         <v>103</v>
@@ -38230,7 +38293,7 @@
         <v>14</v>
       </c>
       <c r="J1100" s="13" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="1101" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -38250,7 +38313,7 @@
         <v>687</v>
       </c>
       <c r="F1101" s="10" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="G1101" s="11" t="s">
         <v>103</v>
@@ -38262,7 +38325,7 @@
         <v>14</v>
       </c>
       <c r="J1101" s="13" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="1102" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -38282,7 +38345,7 @@
         <v>687</v>
       </c>
       <c r="F1102" s="10" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="G1102" s="11" t="s">
         <v>103</v>
@@ -38294,7 +38357,7 @@
         <v>14</v>
       </c>
       <c r="J1102" s="13" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="1103" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -38314,7 +38377,7 @@
         <v>687</v>
       </c>
       <c r="F1103" s="10" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="G1103" s="11" t="s">
         <v>103</v>
@@ -38326,7 +38389,7 @@
         <v>14</v>
       </c>
       <c r="J1103" s="13" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="1104" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -38346,7 +38409,7 @@
         <v>687</v>
       </c>
       <c r="F1104" s="10" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="G1104" s="11" t="s">
         <v>103</v>
@@ -38358,7 +38421,7 @@
         <v>14</v>
       </c>
       <c r="J1104" s="13" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="1105" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -38378,7 +38441,7 @@
         <v>687</v>
       </c>
       <c r="F1105" s="10" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="G1105" s="11" t="s">
         <v>103</v>
@@ -38390,7 +38453,7 @@
         <v>14</v>
       </c>
       <c r="J1105" s="13" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="1106" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -38410,7 +38473,7 @@
         <v>687</v>
       </c>
       <c r="F1106" s="10" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="G1106" s="11" t="s">
         <v>103</v>
@@ -38422,7 +38485,7 @@
         <v>14</v>
       </c>
       <c r="J1106" s="13" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="1107" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -38454,7 +38517,7 @@
         <v>14</v>
       </c>
       <c r="J1107" s="10" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="1108" spans="1:10" x14ac:dyDescent="0.2">
@@ -38465,7 +38528,7 @@
         <v>44228</v>
       </c>
       <c r="C1108" s="14" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="D1108" s="10" t="s">
         <v>18</v>
@@ -38474,7 +38537,7 @@
         <v>712</v>
       </c>
       <c r="F1108" s="10" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="G1108" s="11" t="s">
         <v>103</v>
@@ -38504,7 +38567,7 @@
         <v>608</v>
       </c>
       <c r="F1109" s="10" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="G1109" s="11" t="s">
         <v>103</v>
@@ -38534,7 +38597,7 @@
         <v>658</v>
       </c>
       <c r="F1110" s="10" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="G1110" s="11" t="s">
         <v>107</v>
@@ -38546,7 +38609,7 @@
         <v>14</v>
       </c>
       <c r="J1110" s="13" t="s">
-        <v>1584</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="1111" spans="1:10" x14ac:dyDescent="0.2">
@@ -38566,7 +38629,7 @@
         <v>658</v>
       </c>
       <c r="F1111" s="10" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="G1111" s="11" t="s">
         <v>103</v>
@@ -38596,7 +38659,7 @@
         <v>658</v>
       </c>
       <c r="F1112" s="10" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="G1112" s="11" t="s">
         <v>83</v>
@@ -38626,7 +38689,7 @@
         <v>658</v>
       </c>
       <c r="F1113" s="10" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="G1113" s="11" t="s">
         <v>107</v>
@@ -38638,7 +38701,7 @@
         <v>14</v>
       </c>
       <c r="J1113" s="13" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="1114" spans="1:10" x14ac:dyDescent="0.2">
@@ -38658,7 +38721,7 @@
         <v>658</v>
       </c>
       <c r="F1114" s="10" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="G1114" s="11" t="s">
         <v>107</v>
@@ -38670,7 +38733,7 @@
         <v>14</v>
       </c>
       <c r="J1114" s="13" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="1115" spans="1:10" x14ac:dyDescent="0.2">
@@ -38690,7 +38753,7 @@
         <v>658</v>
       </c>
       <c r="F1115" s="10" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="G1115" s="11" t="s">
         <v>103</v>
@@ -38720,10 +38783,10 @@
         <v>712</v>
       </c>
       <c r="F1116" s="10" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="G1116" s="11" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
       <c r="H1116" s="12" t="s">
         <v>123</v>
@@ -38733,97 +38796,237 @@
       </c>
       <c r="J1116" s="13"/>
     </row>
-    <row r="1117" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1117" s="12"/>
-      <c r="B1117" s="9"/>
-      <c r="C1117" s="14"/>
-      <c r="D1117" s="10"/>
-      <c r="E1117" s="11"/>
-      <c r="F1117" s="10"/>
-      <c r="G1117" s="11"/>
-      <c r="H1117" s="12"/>
-      <c r="I1117" s="13"/>
-      <c r="J1117" s="13"/>
+    <row r="1117" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1117" s="12">
+        <v>44235</v>
+      </c>
+      <c r="B1117" s="9">
+        <v>44235</v>
+      </c>
+      <c r="C1117" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1117" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="E1117" s="11" t="s">
+        <v>687</v>
+      </c>
+      <c r="F1117" s="10" t="s">
+        <v>1595</v>
+      </c>
+      <c r="G1117" s="11" t="s">
+        <v>495</v>
+      </c>
+      <c r="H1117" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1117" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1117" s="13" t="s">
+        <v>1596</v>
+      </c>
     </row>
     <row r="1118" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1118" s="12"/>
-      <c r="B1118" s="9"/>
-      <c r="C1118" s="14"/>
-      <c r="D1118" s="10"/>
-      <c r="E1118" s="11"/>
-      <c r="F1118" s="10"/>
-      <c r="G1118" s="11"/>
-      <c r="H1118" s="12"/>
-      <c r="I1118" s="13"/>
+      <c r="A1118" s="12">
+        <v>44235</v>
+      </c>
+      <c r="B1118" s="9">
+        <v>44235</v>
+      </c>
+      <c r="C1118" s="14" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D1118" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1118" s="11" t="s">
+        <v>658</v>
+      </c>
+      <c r="F1118" s="10" t="s">
+        <v>1599</v>
+      </c>
+      <c r="G1118" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1118" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1118" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="J1118" s="13"/>
     </row>
-    <row r="1119" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1119" s="12"/>
-      <c r="B1119" s="9"/>
-      <c r="C1119" s="14"/>
-      <c r="D1119" s="10"/>
+    <row r="1119" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1119" s="12">
+        <v>44235</v>
+      </c>
+      <c r="B1119" s="9">
+        <v>44235</v>
+      </c>
+      <c r="C1119" s="14" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D1119" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="E1119" s="11"/>
-      <c r="F1119" s="10"/>
-      <c r="G1119" s="11"/>
-      <c r="H1119" s="12"/>
-      <c r="I1119" s="13"/>
-      <c r="J1119" s="13"/>
+      <c r="F1119" s="10" t="s">
+        <v>1597</v>
+      </c>
+      <c r="G1119" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1119" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1119" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1119" s="13" t="s">
+        <v>1598</v>
+      </c>
     </row>
     <row r="1120" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1120" s="12"/>
-      <c r="B1120" s="9"/>
-      <c r="C1120" s="14"/>
-      <c r="D1120" s="10"/>
-      <c r="E1120" s="11"/>
-      <c r="F1120" s="10"/>
-      <c r="G1120" s="11"/>
-      <c r="H1120" s="12"/>
-      <c r="I1120" s="13"/>
+      <c r="A1120" s="12">
+        <v>44236</v>
+      </c>
+      <c r="B1120" s="9">
+        <v>44237</v>
+      </c>
+      <c r="C1120" s="14" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1120" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1120" s="11" t="s">
+        <v>728</v>
+      </c>
+      <c r="F1120" s="10" t="s">
+        <v>1591</v>
+      </c>
+      <c r="G1120" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1120" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1120" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="J1120" s="13"/>
     </row>
     <row r="1121" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1121" s="12"/>
-      <c r="B1121" s="9"/>
-      <c r="C1121" s="14"/>
-      <c r="D1121" s="10"/>
-      <c r="E1121" s="11"/>
-      <c r="F1121" s="10"/>
-      <c r="G1121" s="11"/>
-      <c r="H1121" s="12"/>
-      <c r="I1121" s="13"/>
+      <c r="A1121" s="12">
+        <v>44236</v>
+      </c>
+      <c r="B1121" s="9">
+        <v>44236</v>
+      </c>
+      <c r="C1121" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="D1121" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1121" s="11" t="s">
+        <v>728</v>
+      </c>
+      <c r="F1121" s="10" t="s">
+        <v>1594</v>
+      </c>
+      <c r="G1121" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1121" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1121" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="J1121" s="13"/>
     </row>
-    <row r="1122" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1122" s="36"/>
-      <c r="B1122" s="37"/>
-      <c r="C1122" s="38"/>
-      <c r="D1122" s="39"/>
-      <c r="E1122" s="40"/>
-      <c r="F1122" s="39"/>
-      <c r="G1122" s="40"/>
-      <c r="H1122" s="36"/>
-      <c r="I1122" s="41"/>
-      <c r="J1122" s="41"/>
+    <row r="1122" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1122" s="12">
+        <v>44237</v>
+      </c>
+      <c r="B1122" s="9">
+        <v>44237</v>
+      </c>
+      <c r="C1122" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1122" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="E1122" s="11" t="s">
+        <v>687</v>
+      </c>
+      <c r="F1122" s="10" t="s">
+        <v>1592</v>
+      </c>
+      <c r="G1122" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1122" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1122" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1122" s="13"/>
     </row>
     <row r="1123" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1123" s="12"/>
-      <c r="B1123" s="9"/>
-      <c r="C1123" s="14"/>
-      <c r="D1123" s="10"/>
-      <c r="E1123" s="11"/>
-      <c r="F1123" s="10"/>
-      <c r="G1123" s="11"/>
-      <c r="H1123" s="12"/>
-      <c r="I1123" s="13"/>
+      <c r="A1123" s="12">
+        <v>44237</v>
+      </c>
+      <c r="B1123" s="9">
+        <v>44237</v>
+      </c>
+      <c r="C1123" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1123" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="E1123" s="11" t="s">
+        <v>742</v>
+      </c>
+      <c r="F1123" s="10" t="s">
+        <v>1600</v>
+      </c>
+      <c r="G1123" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1123" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1123" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="J1123" s="13"/>
     </row>
     <row r="1124" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1124" s="12"/>
-      <c r="B1124" s="9"/>
-      <c r="C1124" s="14"/>
-      <c r="D1124" s="10"/>
-      <c r="E1124" s="11"/>
-      <c r="F1124" s="10"/>
+      <c r="A1124" s="12">
+        <v>44237</v>
+      </c>
+      <c r="B1124" s="9">
+        <v>44237</v>
+      </c>
+      <c r="C1124" s="14" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D1124" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1124" s="11" t="s">
+        <v>712</v>
+      </c>
+      <c r="F1124" s="10" t="s">
+        <v>1601</v>
+      </c>
       <c r="G1124" s="11"/>
       <c r="H1124" s="12"/>
       <c r="I1124" s="13"/>
@@ -38831,581 +39034,833 @@
     </row>
     <row r="1125" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1125" s="12">
-        <v>44222</v>
-      </c>
-      <c r="B1125" s="9"/>
+        <v>44237</v>
+      </c>
+      <c r="B1125" s="9">
+        <v>44237</v>
+      </c>
       <c r="C1125" s="14" t="s">
-        <v>1530</v>
+        <v>1104</v>
       </c>
       <c r="D1125" s="10" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="E1125" s="11" t="s">
-        <v>608</v>
+        <v>712</v>
       </c>
       <c r="F1125" s="10" t="s">
-        <v>1553</v>
+        <v>1602</v>
       </c>
       <c r="G1125" s="11"/>
       <c r="H1125" s="12"/>
       <c r="I1125" s="13"/>
       <c r="J1125" s="13"/>
     </row>
-    <row r="1126" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1126" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1126" s="12">
-        <v>44176</v>
-      </c>
-      <c r="B1126" s="9"/>
+        <v>44237</v>
+      </c>
+      <c r="B1126" s="9">
+        <v>44237</v>
+      </c>
       <c r="C1126" s="14" t="s">
-        <v>9</v>
+        <v>613</v>
       </c>
       <c r="D1126" s="10" t="s">
-        <v>622</v>
+        <v>117</v>
       </c>
       <c r="E1126" s="11" t="s">
-        <v>1405</v>
+        <v>658</v>
       </c>
       <c r="F1126" s="10" t="s">
-        <v>1406</v>
-      </c>
-      <c r="G1126" s="11"/>
-      <c r="H1126" s="12"/>
-      <c r="I1126" s="13"/>
-      <c r="J1126" s="13"/>
-    </row>
-    <row r="1127" spans="1:10" ht="72" x14ac:dyDescent="0.2">
+        <v>1603</v>
+      </c>
+      <c r="G1126" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1126" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1126" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1126" s="13" t="s">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1127" s="12">
-        <v>43864</v>
-      </c>
-      <c r="B1127" s="9"/>
+        <v>44236</v>
+      </c>
+      <c r="B1127" s="9">
+        <v>44237</v>
+      </c>
       <c r="C1127" s="14" t="s">
-        <v>20</v>
+        <v>977</v>
       </c>
       <c r="D1127" s="10" t="s">
-        <v>571</v>
-      </c>
-      <c r="E1127" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="E1127" s="11" t="s">
+        <v>658</v>
+      </c>
       <c r="F1127" s="10" t="s">
-        <v>572</v>
-      </c>
-      <c r="G1127" s="11"/>
-      <c r="H1127" s="12"/>
-      <c r="I1127" s="13"/>
+        <v>1604</v>
+      </c>
+      <c r="G1127" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1127" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1127" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="J1127" s="13" t="s">
-        <v>1436</v>
-      </c>
-    </row>
-    <row r="1128" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1128" s="12"/>
-      <c r="B1128" s="9"/>
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1128" s="12">
+        <v>44238</v>
+      </c>
+      <c r="B1128" s="9">
+        <v>44238</v>
+      </c>
       <c r="C1128" s="14" t="s">
-        <v>14</v>
+        <v>1208</v>
       </c>
       <c r="D1128" s="10" t="s">
-        <v>622</v>
+        <v>7</v>
       </c>
       <c r="E1128" s="11" t="s">
-        <v>687</v>
+        <v>658</v>
       </c>
       <c r="F1128" s="10" t="s">
-        <v>1391</v>
-      </c>
-      <c r="G1128" s="11"/>
-      <c r="H1128" s="12"/>
-      <c r="I1128" s="13"/>
-      <c r="J1128" s="13"/>
-    </row>
-    <row r="1129" spans="1:10" ht="84" x14ac:dyDescent="0.2">
+        <v>1607</v>
+      </c>
+      <c r="G1128" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1128" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1128" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1128" s="13" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1129" s="12">
-        <v>44168</v>
-      </c>
-      <c r="B1129" s="9"/>
+        <v>44238</v>
+      </c>
+      <c r="B1129" s="9">
+        <v>44238</v>
+      </c>
       <c r="C1129" s="14" t="s">
-        <v>1365</v>
+        <v>497</v>
       </c>
       <c r="D1129" s="10" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E1129" s="11" t="s">
-        <v>608</v>
+        <v>712</v>
       </c>
       <c r="F1129" s="10" t="s">
-        <v>1364</v>
-      </c>
-      <c r="G1129" s="11"/>
-      <c r="H1129" s="12"/>
-      <c r="I1129" s="13"/>
-      <c r="J1129" s="13"/>
-    </row>
-    <row r="1130" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1130" s="12">
-        <v>44131</v>
-      </c>
+        <v>1608</v>
+      </c>
+      <c r="G1129" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1129" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1129" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1129" s="13" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1130" s="12"/>
       <c r="B1130" s="9"/>
-      <c r="C1130" s="14" t="s">
-        <v>1179</v>
-      </c>
-      <c r="D1130" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1130" s="11" t="s">
-        <v>728</v>
-      </c>
-      <c r="F1130" s="10" t="s">
-        <v>1213</v>
-      </c>
+      <c r="C1130" s="14"/>
+      <c r="D1130" s="10"/>
+      <c r="E1130" s="11"/>
+      <c r="F1130" s="10"/>
       <c r="G1130" s="11"/>
       <c r="H1130" s="12"/>
       <c r="I1130" s="13"/>
       <c r="J1130" s="13"/>
     </row>
     <row r="1131" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1131" s="12">
-        <v>44112</v>
-      </c>
+      <c r="A1131" s="12"/>
       <c r="B1131" s="9"/>
-      <c r="C1131" s="14" t="s">
-        <v>661</v>
-      </c>
-      <c r="D1131" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1131" s="11" t="s">
-        <v>608</v>
-      </c>
-      <c r="F1131" s="10" t="s">
-        <v>1145</v>
-      </c>
+      <c r="C1131" s="14"/>
+      <c r="D1131" s="10"/>
+      <c r="E1131" s="11"/>
+      <c r="F1131" s="10"/>
       <c r="G1131" s="11"/>
       <c r="H1131" s="12"/>
       <c r="I1131" s="13"/>
       <c r="J1131" s="13"/>
     </row>
     <row r="1132" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1132" s="12">
-        <v>44088</v>
-      </c>
+      <c r="A1132" s="12"/>
       <c r="B1132" s="9"/>
-      <c r="C1132" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1132" s="10" t="s">
-        <v>951</v>
-      </c>
-      <c r="E1132" s="11" t="s">
-        <v>728</v>
-      </c>
-      <c r="F1132" s="10" t="s">
-        <v>1058</v>
-      </c>
+      <c r="C1132" s="14"/>
+      <c r="D1132" s="10"/>
+      <c r="E1132" s="11"/>
+      <c r="F1132" s="10"/>
       <c r="G1132" s="11"/>
       <c r="H1132" s="12"/>
       <c r="I1132" s="13"/>
       <c r="J1132" s="13"/>
     </row>
     <row r="1133" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1133" s="12">
-        <v>44083</v>
-      </c>
+      <c r="A1133" s="12"/>
       <c r="B1133" s="9"/>
-      <c r="C1133" s="14" t="s">
-        <v>501</v>
-      </c>
-      <c r="D1133" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1133" s="11" t="s">
-        <v>882</v>
-      </c>
-      <c r="F1133" s="10" t="s">
-        <v>1035</v>
-      </c>
+      <c r="C1133" s="14"/>
+      <c r="D1133" s="10"/>
+      <c r="E1133" s="11"/>
+      <c r="F1133" s="10"/>
       <c r="G1133" s="11"/>
       <c r="H1133" s="12"/>
       <c r="I1133" s="13"/>
       <c r="J1133" s="13"/>
     </row>
     <row r="1134" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1134" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1134" s="12"/>
       <c r="B1134" s="9"/>
-      <c r="C1134" s="14" t="s">
-        <v>661</v>
-      </c>
-      <c r="D1134" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1134" s="11" t="s">
-        <v>608</v>
-      </c>
-      <c r="F1134" s="10" t="s">
-        <v>948</v>
-      </c>
+      <c r="C1134" s="14"/>
+      <c r="D1134" s="10"/>
+      <c r="E1134" s="11"/>
+      <c r="F1134" s="10"/>
       <c r="G1134" s="11"/>
       <c r="H1134" s="12"/>
       <c r="I1134" s="13"/>
       <c r="J1134" s="13"/>
     </row>
     <row r="1135" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1135" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1135" s="9"/>
-      <c r="C1135" s="14" t="s">
-        <v>661</v>
-      </c>
-      <c r="D1135" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1135" s="11" t="s">
-        <v>608</v>
-      </c>
-      <c r="F1135" s="10" t="s">
-        <v>947</v>
-      </c>
-      <c r="G1135" s="11"/>
-      <c r="H1135" s="12"/>
-      <c r="I1135" s="13"/>
-      <c r="J1135" s="13"/>
+      <c r="A1135" s="36"/>
+      <c r="B1135" s="37"/>
+      <c r="C1135" s="38"/>
+      <c r="D1135" s="39"/>
+      <c r="E1135" s="40"/>
+      <c r="F1135" s="39"/>
+      <c r="G1135" s="40"/>
+      <c r="H1135" s="36"/>
+      <c r="I1135" s="41"/>
+      <c r="J1135" s="41"/>
     </row>
     <row r="1136" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1136" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1136" s="12"/>
       <c r="B1136" s="9"/>
-      <c r="C1136" s="14" t="s">
-        <v>943</v>
-      </c>
-      <c r="D1136" s="10" t="s">
-        <v>531</v>
-      </c>
-      <c r="E1136" s="11" t="s">
-        <v>608</v>
-      </c>
-      <c r="F1136" s="10" t="s">
-        <v>945</v>
-      </c>
+      <c r="C1136" s="14"/>
+      <c r="D1136" s="10"/>
+      <c r="E1136" s="11"/>
+      <c r="F1136" s="10"/>
       <c r="G1136" s="11"/>
       <c r="H1136" s="12"/>
       <c r="I1136" s="13"/>
       <c r="J1136" s="13"/>
     </row>
-    <row r="1137" spans="1:10" ht="108" x14ac:dyDescent="0.2">
-      <c r="A1137" s="12">
-        <v>44055</v>
-      </c>
+    <row r="1137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1137" s="12"/>
       <c r="B1137" s="9"/>
-      <c r="C1137" s="14" t="s">
-        <v>943</v>
-      </c>
-      <c r="D1137" s="10" t="s">
-        <v>531</v>
-      </c>
-      <c r="E1137" s="11" t="s">
-        <v>608</v>
-      </c>
-      <c r="F1137" s="10" t="s">
-        <v>946</v>
-      </c>
+      <c r="C1137" s="14"/>
+      <c r="D1137" s="10"/>
+      <c r="E1137" s="11"/>
+      <c r="F1137" s="10"/>
       <c r="G1137" s="11"/>
       <c r="H1137" s="12"/>
       <c r="I1137" s="13"/>
       <c r="J1137" s="13"/>
     </row>
-    <row r="1138" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1138" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1138" s="12">
-        <v>44055</v>
+        <v>44222</v>
       </c>
       <c r="B1138" s="9"/>
       <c r="C1138" s="14" t="s">
-        <v>943</v>
+        <v>1530</v>
       </c>
       <c r="D1138" s="10" t="s">
-        <v>531</v>
+        <v>39</v>
       </c>
       <c r="E1138" s="11" t="s">
         <v>608</v>
       </c>
       <c r="F1138" s="10" t="s">
-        <v>949</v>
+        <v>1593</v>
       </c>
       <c r="G1138" s="11"/>
       <c r="H1138" s="12"/>
       <c r="I1138" s="13"/>
       <c r="J1138" s="13"/>
     </row>
-    <row r="1139" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="1139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1139" s="12">
-        <v>44047</v>
+        <v>44176</v>
       </c>
       <c r="B1139" s="9"/>
       <c r="C1139" s="14" t="s">
-        <v>575</v>
+        <v>9</v>
       </c>
       <c r="D1139" s="10" t="s">
-        <v>7</v>
+        <v>622</v>
       </c>
       <c r="E1139" s="11" t="s">
-        <v>728</v>
+        <v>1405</v>
       </c>
       <c r="F1139" s="10" t="s">
-        <v>918</v>
-      </c>
-      <c r="G1139" s="11" t="s">
-        <v>107</v>
-      </c>
+        <v>1406</v>
+      </c>
+      <c r="G1139" s="11"/>
       <c r="H1139" s="12"/>
       <c r="I1139" s="13"/>
       <c r="J1139" s="13"/>
     </row>
-    <row r="1140" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1140" spans="1:10" ht="72" x14ac:dyDescent="0.2">
       <c r="A1140" s="12">
-        <v>43949</v>
+        <v>43864</v>
       </c>
       <c r="B1140" s="9"/>
       <c r="C1140" s="14" t="s">
-        <v>501</v>
+        <v>20</v>
       </c>
       <c r="D1140" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1140" s="11" t="s">
-        <v>728</v>
-      </c>
+        <v>571</v>
+      </c>
+      <c r="E1140" s="11"/>
       <c r="F1140" s="10" t="s">
-        <v>729</v>
-      </c>
-      <c r="G1140" s="11" t="s">
-        <v>730</v>
-      </c>
+        <v>572</v>
+      </c>
+      <c r="G1140" s="11"/>
       <c r="H1140" s="12"/>
-      <c r="I1140" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="J1140" s="13"/>
-    </row>
-    <row r="1141" spans="1:10" ht="168" x14ac:dyDescent="0.2">
-      <c r="A1141" s="12">
-        <v>43949</v>
-      </c>
+      <c r="I1140" s="13"/>
+      <c r="J1140" s="13" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1141" s="12"/>
       <c r="B1141" s="9"/>
       <c r="C1141" s="14" t="s">
-        <v>501</v>
+        <v>14</v>
       </c>
       <c r="D1141" s="10" t="s">
-        <v>95</v>
+        <v>622</v>
       </c>
       <c r="E1141" s="11" t="s">
-        <v>728</v>
+        <v>687</v>
       </c>
       <c r="F1141" s="10" t="s">
-        <v>749</v>
-      </c>
-      <c r="G1141" s="11" t="s">
-        <v>731</v>
-      </c>
+        <v>1391</v>
+      </c>
+      <c r="G1141" s="11"/>
       <c r="H1141" s="12"/>
-      <c r="I1141" s="13" t="s">
-        <v>304</v>
-      </c>
+      <c r="I1141" s="13"/>
       <c r="J1141" s="13"/>
     </row>
-    <row r="1142" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="1142" spans="1:10" ht="84" x14ac:dyDescent="0.2">
       <c r="A1142" s="12">
-        <v>43838</v>
+        <v>44168</v>
       </c>
       <c r="B1142" s="9"/>
       <c r="C1142" s="14" t="s">
-        <v>113</v>
+        <v>1365</v>
       </c>
       <c r="D1142" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="E1142" s="11"/>
+        <v>95</v>
+      </c>
+      <c r="E1142" s="11" t="s">
+        <v>608</v>
+      </c>
       <c r="F1142" s="10" t="s">
-        <v>518</v>
-      </c>
-      <c r="G1142" s="11" t="s">
-        <v>685</v>
-      </c>
+        <v>1364</v>
+      </c>
+      <c r="G1142" s="11"/>
       <c r="H1142" s="12"/>
       <c r="I1142" s="13"/>
       <c r="J1142" s="13"/>
     </row>
-    <row r="1143" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1143" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1143" s="12">
-        <v>43816</v>
+        <v>44131</v>
       </c>
       <c r="B1143" s="9"/>
       <c r="C1143" s="14" t="s">
-        <v>511</v>
+        <v>1179</v>
       </c>
       <c r="D1143" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1143" s="11"/>
+        <v>95</v>
+      </c>
+      <c r="E1143" s="11" t="s">
+        <v>728</v>
+      </c>
       <c r="F1143" s="10" t="s">
-        <v>510</v>
-      </c>
-      <c r="G1143" s="11" t="s">
-        <v>500</v>
-      </c>
+        <v>1213</v>
+      </c>
+      <c r="G1143" s="11"/>
       <c r="H1143" s="12"/>
       <c r="I1143" s="13"/>
       <c r="J1143" s="13"/>
     </row>
-    <row r="1144" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="1144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1144" s="12">
-        <v>43762</v>
+        <v>44112</v>
       </c>
       <c r="B1144" s="9"/>
       <c r="C1144" s="14" t="s">
-        <v>475</v>
+        <v>661</v>
       </c>
       <c r="D1144" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1144" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="E1144" s="11" t="s">
+        <v>608</v>
+      </c>
       <c r="F1144" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="G1144" s="11" t="s">
-        <v>477</v>
-      </c>
+        <v>1145</v>
+      </c>
+      <c r="G1144" s="11"/>
       <c r="H1144" s="12"/>
       <c r="I1144" s="13"/>
       <c r="J1144" s="13"/>
     </row>
     <row r="1145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1145" s="12">
-        <v>44222</v>
+        <v>44088</v>
       </c>
       <c r="B1145" s="9"/>
       <c r="C1145" s="14" t="s">
-        <v>1548</v>
+        <v>20</v>
       </c>
       <c r="D1145" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1145" s="11"/>
+        <v>951</v>
+      </c>
+      <c r="E1145" s="11" t="s">
+        <v>728</v>
+      </c>
       <c r="F1145" s="10" t="s">
-        <v>1547</v>
-      </c>
-      <c r="G1145" s="11" t="s">
-        <v>107</v>
-      </c>
+        <v>1058</v>
+      </c>
+      <c r="G1145" s="11"/>
       <c r="H1145" s="12"/>
       <c r="I1145" s="13"/>
       <c r="J1145" s="13"/>
     </row>
     <row r="1146" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1146" s="12"/>
+      <c r="A1146" s="12">
+        <v>44083</v>
+      </c>
       <c r="B1146" s="9"/>
-      <c r="C1146" s="14"/>
-      <c r="D1146" s="10"/>
-      <c r="E1146" s="11"/>
-      <c r="F1146" s="10"/>
+      <c r="C1146" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="D1146" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1146" s="11" t="s">
+        <v>882</v>
+      </c>
+      <c r="F1146" s="10" t="s">
+        <v>1035</v>
+      </c>
       <c r="G1146" s="11"/>
       <c r="H1146" s="12"/>
       <c r="I1146" s="13"/>
       <c r="J1146" s="13"/>
     </row>
     <row r="1147" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1147" s="12"/>
+      <c r="A1147" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1147" s="9"/>
-      <c r="C1147" s="14"/>
-      <c r="D1147" s="10"/>
-      <c r="E1147" s="11"/>
-      <c r="F1147" s="10"/>
+      <c r="C1147" s="14" t="s">
+        <v>661</v>
+      </c>
+      <c r="D1147" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1147" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="F1147" s="10" t="s">
+        <v>948</v>
+      </c>
       <c r="G1147" s="11"/>
       <c r="H1147" s="12"/>
       <c r="I1147" s="13"/>
       <c r="J1147" s="13"/>
     </row>
     <row r="1148" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1148" s="12"/>
+      <c r="A1148" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1148" s="9"/>
-      <c r="C1148" s="14"/>
-      <c r="D1148" s="10"/>
-      <c r="E1148" s="11"/>
-      <c r="F1148" s="10"/>
+      <c r="C1148" s="14" t="s">
+        <v>661</v>
+      </c>
+      <c r="D1148" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1148" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="F1148" s="10" t="s">
+        <v>947</v>
+      </c>
       <c r="G1148" s="11"/>
       <c r="H1148" s="12"/>
       <c r="I1148" s="13"/>
       <c r="J1148" s="13"/>
     </row>
     <row r="1149" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1149" s="12"/>
+      <c r="A1149" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1149" s="9"/>
-      <c r="C1149" s="14"/>
-      <c r="D1149" s="10"/>
-      <c r="E1149" s="11"/>
-      <c r="F1149" s="10"/>
+      <c r="C1149" s="14" t="s">
+        <v>943</v>
+      </c>
+      <c r="D1149" s="10" t="s">
+        <v>531</v>
+      </c>
+      <c r="E1149" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="F1149" s="10" t="s">
+        <v>945</v>
+      </c>
       <c r="G1149" s="11"/>
       <c r="H1149" s="12"/>
       <c r="I1149" s="13"/>
       <c r="J1149" s="13"/>
     </row>
-    <row r="1150" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1150" s="12"/>
+    <row r="1150" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A1150" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1150" s="9"/>
-      <c r="C1150" s="14"/>
-      <c r="D1150" s="10"/>
-      <c r="E1150" s="11"/>
-      <c r="F1150" s="10"/>
+      <c r="C1150" s="14" t="s">
+        <v>943</v>
+      </c>
+      <c r="D1150" s="10" t="s">
+        <v>531</v>
+      </c>
+      <c r="E1150" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="F1150" s="10" t="s">
+        <v>946</v>
+      </c>
       <c r="G1150" s="11"/>
       <c r="H1150" s="12"/>
       <c r="I1150" s="13"/>
       <c r="J1150" s="13"/>
     </row>
-    <row r="1151" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1151" s="12"/>
+    <row r="1151" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1151" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1151" s="9"/>
-      <c r="C1151" s="14"/>
-      <c r="D1151" s="10"/>
-      <c r="E1151" s="11"/>
-      <c r="F1151" s="10"/>
+      <c r="C1151" s="14" t="s">
+        <v>943</v>
+      </c>
+      <c r="D1151" s="10" t="s">
+        <v>531</v>
+      </c>
+      <c r="E1151" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="F1151" s="10" t="s">
+        <v>949</v>
+      </c>
       <c r="G1151" s="11"/>
       <c r="H1151" s="12"/>
       <c r="I1151" s="13"/>
-      <c r="J1151" s="13"/>
-    </row>
-    <row r="1152" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1152" s="12"/>
+      <c r="J1151" s="13" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1152" s="12">
+        <v>44047</v>
+      </c>
       <c r="B1152" s="9"/>
-      <c r="C1152" s="14"/>
-      <c r="D1152" s="10"/>
-      <c r="E1152" s="11"/>
-      <c r="F1152" s="10"/>
-      <c r="G1152" s="11"/>
+      <c r="C1152" s="14" t="s">
+        <v>575</v>
+      </c>
+      <c r="D1152" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1152" s="11" t="s">
+        <v>728</v>
+      </c>
+      <c r="F1152" s="10" t="s">
+        <v>918</v>
+      </c>
+      <c r="G1152" s="11" t="s">
+        <v>107</v>
+      </c>
       <c r="H1152" s="12"/>
       <c r="I1152" s="13"/>
       <c r="J1152" s="13"/>
     </row>
-    <row r="1153" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1153" s="12"/>
+    <row r="1153" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1153" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1153" s="9"/>
-      <c r="C1153" s="14"/>
-      <c r="D1153" s="10"/>
-      <c r="E1153" s="11"/>
-      <c r="F1153" s="10"/>
-      <c r="G1153" s="11"/>
+      <c r="C1153" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="D1153" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1153" s="11" t="s">
+        <v>728</v>
+      </c>
+      <c r="F1153" s="10" t="s">
+        <v>729</v>
+      </c>
+      <c r="G1153" s="11" t="s">
+        <v>730</v>
+      </c>
       <c r="H1153" s="12"/>
-      <c r="I1153" s="13"/>
+      <c r="I1153" s="13" t="s">
+        <v>304</v>
+      </c>
       <c r="J1153" s="13"/>
     </row>
-    <row r="1154" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1154" s="12"/>
+    <row r="1154" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1154" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1154" s="9"/>
-      <c r="C1154" s="14"/>
-      <c r="D1154" s="10"/>
-      <c r="E1154" s="11"/>
-      <c r="F1154" s="10"/>
-      <c r="G1154" s="11"/>
+      <c r="C1154" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="D1154" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1154" s="11" t="s">
+        <v>728</v>
+      </c>
+      <c r="F1154" s="10" t="s">
+        <v>749</v>
+      </c>
+      <c r="G1154" s="11" t="s">
+        <v>731</v>
+      </c>
       <c r="H1154" s="12"/>
-      <c r="I1154" s="13"/>
+      <c r="I1154" s="13" t="s">
+        <v>304</v>
+      </c>
       <c r="J1154" s="13"/>
+    </row>
+    <row r="1155" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1155" s="12">
+        <v>43838</v>
+      </c>
+      <c r="B1155" s="9"/>
+      <c r="C1155" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1155" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="E1155" s="11"/>
+      <c r="F1155" s="10" t="s">
+        <v>518</v>
+      </c>
+      <c r="G1155" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="H1155" s="12"/>
+      <c r="I1155" s="13"/>
+      <c r="J1155" s="13" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1156" s="12">
+        <v>43816</v>
+      </c>
+      <c r="B1156" s="9"/>
+      <c r="C1156" s="14" t="s">
+        <v>511</v>
+      </c>
+      <c r="D1156" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1156" s="11"/>
+      <c r="F1156" s="10" t="s">
+        <v>510</v>
+      </c>
+      <c r="G1156" s="11" t="s">
+        <v>500</v>
+      </c>
+      <c r="H1156" s="12"/>
+      <c r="I1156" s="13"/>
+      <c r="J1156" s="13"/>
+    </row>
+    <row r="1157" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1157" s="12">
+        <v>43762</v>
+      </c>
+      <c r="B1157" s="9"/>
+      <c r="C1157" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1157" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1157" s="11"/>
+      <c r="F1157" s="10" t="s">
+        <v>476</v>
+      </c>
+      <c r="G1157" s="11" t="s">
+        <v>477</v>
+      </c>
+      <c r="H1157" s="12"/>
+      <c r="I1157" s="13"/>
+      <c r="J1157" s="13"/>
+    </row>
+    <row r="1158" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1158" s="12">
+        <v>44222</v>
+      </c>
+      <c r="B1158" s="9"/>
+      <c r="C1158" s="14" t="s">
+        <v>1548</v>
+      </c>
+      <c r="D1158" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1158" s="11"/>
+      <c r="F1158" s="10" t="s">
+        <v>1547</v>
+      </c>
+      <c r="G1158" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1158" s="12"/>
+      <c r="I1158" s="13"/>
+      <c r="J1158" s="13"/>
+    </row>
+    <row r="1159" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1159" s="12"/>
+      <c r="B1159" s="9"/>
+      <c r="C1159" s="14"/>
+      <c r="D1159" s="10"/>
+      <c r="E1159" s="11"/>
+      <c r="F1159" s="10"/>
+      <c r="G1159" s="11"/>
+      <c r="H1159" s="12"/>
+      <c r="I1159" s="13"/>
+      <c r="J1159" s="13"/>
+    </row>
+    <row r="1160" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1160" s="12"/>
+      <c r="B1160" s="9"/>
+      <c r="C1160" s="14"/>
+      <c r="D1160" s="10"/>
+      <c r="E1160" s="11"/>
+      <c r="F1160" s="10"/>
+      <c r="G1160" s="11"/>
+      <c r="H1160" s="12"/>
+      <c r="I1160" s="13"/>
+      <c r="J1160" s="13"/>
+    </row>
+    <row r="1161" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1161" s="12"/>
+      <c r="B1161" s="9"/>
+      <c r="C1161" s="14"/>
+      <c r="D1161" s="10"/>
+      <c r="E1161" s="11"/>
+      <c r="F1161" s="10"/>
+      <c r="G1161" s="11"/>
+      <c r="H1161" s="12"/>
+      <c r="I1161" s="13"/>
+      <c r="J1161" s="13"/>
+    </row>
+    <row r="1162" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1162" s="12"/>
+      <c r="B1162" s="9"/>
+      <c r="C1162" s="14"/>
+      <c r="D1162" s="10"/>
+      <c r="E1162" s="11"/>
+      <c r="F1162" s="10"/>
+      <c r="G1162" s="11"/>
+      <c r="H1162" s="12"/>
+      <c r="I1162" s="13"/>
+      <c r="J1162" s="13"/>
+    </row>
+    <row r="1163" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1163" s="12"/>
+      <c r="B1163" s="9"/>
+      <c r="C1163" s="14"/>
+      <c r="D1163" s="10"/>
+      <c r="E1163" s="11"/>
+      <c r="F1163" s="10"/>
+      <c r="G1163" s="11"/>
+      <c r="H1163" s="12"/>
+      <c r="I1163" s="13"/>
+      <c r="J1163" s="13"/>
+    </row>
+    <row r="1164" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1164" s="12"/>
+      <c r="B1164" s="9"/>
+      <c r="C1164" s="14"/>
+      <c r="D1164" s="10"/>
+      <c r="E1164" s="11"/>
+      <c r="F1164" s="10"/>
+      <c r="G1164" s="11"/>
+      <c r="H1164" s="12"/>
+      <c r="I1164" s="13"/>
+      <c r="J1164" s="13"/>
+    </row>
+    <row r="1165" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1165" s="12"/>
+      <c r="B1165" s="9"/>
+      <c r="C1165" s="14"/>
+      <c r="D1165" s="10"/>
+      <c r="E1165" s="11"/>
+      <c r="F1165" s="10"/>
+      <c r="G1165" s="11"/>
+      <c r="H1165" s="12"/>
+      <c r="I1165" s="13"/>
+      <c r="J1165" s="13"/>
+    </row>
+    <row r="1166" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1166" s="12"/>
+      <c r="B1166" s="9"/>
+      <c r="C1166" s="14"/>
+      <c r="D1166" s="10"/>
+      <c r="E1166" s="11"/>
+      <c r="F1166" s="10"/>
+      <c r="G1166" s="11"/>
+      <c r="H1166" s="12"/>
+      <c r="I1166" s="13"/>
+      <c r="J1166" s="13"/>
+    </row>
+    <row r="1167" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1167" s="12"/>
+      <c r="B1167" s="9"/>
+      <c r="C1167" s="14"/>
+      <c r="D1167" s="10"/>
+      <c r="E1167" s="11"/>
+      <c r="F1167" s="10"/>
+      <c r="G1167" s="11"/>
+      <c r="H1167" s="12"/>
+      <c r="I1167" s="13"/>
+      <c r="J1167" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1089" xr:uid="{00000000-0009-0000-0000-000000000000}">

</xml_diff>

<commit_message>
Novas siglas - lib prev maior que fat
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B87AD57-4C40-4CBE-BAFF-BFF09F047171}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACADAE8C-6E1B-469A-B829-1825336ECA56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9127" uniqueCount="1910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9172" uniqueCount="1919">
   <si>
     <t>Responsável</t>
   </si>
@@ -6091,12 +6091,42 @@
   <si>
     <t>Remover configuração de bitributação para os pedidios 046906 e 046845</t>
   </si>
+  <si>
+    <t>21-04-05_ATUALIZACAO_12.1.25_FAT_EXPEDICAO_CONTINUA</t>
+  </si>
+  <si>
+    <t>21-04-08-LIB_LABEL_05042021_P12_LOBO</t>
+  </si>
+  <si>
+    <t>Reunião saída Jadair</t>
+  </si>
+  <si>
+    <t>Favor verificar os casos abaixo,  pois a conta de CREDITO deveria ser 31103001(receita) e está vindo a própria conta do cliente.</t>
+  </si>
+  <si>
+    <t>A fórmula do LP 610-001 é a seguinte: 
+Débito: Conta cadastrada no Cliente
+Crédito: Se for série = 2, a conta será 31103002, outras séries: utiliza a conta cadastrada no Produto</t>
+  </si>
+  <si>
+    <t>Refazer e reconfigura impostos NFs 2082,2085,1486,1487,1853 e 1854</t>
+  </si>
+  <si>
+    <t>Configurar sistema para gerar tituloa a pagar na bitributação e não abatimanto para o cliente 000367</t>
+  </si>
+  <si>
+    <t>Efetuados testes em ambiente de homologação e não foi possível
+Aberto ticket na Totvs</t>
+  </si>
+  <si>
+    <t>Refazimento de 22 notas da Petrobras sem a bitributação</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -6196,13 +6226,6 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -6355,9 +6378,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6464,8 +6487,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6860,11 +6882,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1338"/>
+  <dimension ref="A1:J1346"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1282" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1290" sqref="A1290"/>
+      <pane ySplit="1" topLeftCell="A1290" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1297" sqref="A1297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -44911,7 +44933,7 @@
       <c r="I1281" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1281" s="41" t="s">
+      <c r="J1281" s="40" t="s">
         <v>1898</v>
       </c>
     </row>
@@ -45160,134 +45182,212 @@
       <c r="J1289" s="13"/>
     </row>
     <row r="1290" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1290" s="12"/>
-      <c r="B1290" s="12"/>
-      <c r="C1290" s="14"/>
-      <c r="D1290" s="10"/>
-      <c r="E1290" s="11"/>
-      <c r="F1290" s="10"/>
-      <c r="G1290" s="11"/>
-      <c r="H1290" s="12"/>
-      <c r="I1290" s="13"/>
+      <c r="A1290" s="12">
+        <v>44309</v>
+      </c>
+      <c r="B1290" s="12">
+        <v>44309</v>
+      </c>
+      <c r="C1290" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1290" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1290" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1290" s="10" t="s">
+        <v>1910</v>
+      </c>
+      <c r="G1290" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1290" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1290" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1290" s="13"/>
     </row>
     <row r="1291" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1291" s="12"/>
-      <c r="B1291" s="12"/>
-      <c r="C1291" s="14"/>
-      <c r="D1291" s="10"/>
-      <c r="E1291" s="11"/>
-      <c r="F1291" s="10"/>
-      <c r="G1291" s="11"/>
-      <c r="H1291" s="12"/>
-      <c r="I1291" s="13"/>
+      <c r="A1291" s="12">
+        <v>44309</v>
+      </c>
+      <c r="B1291" s="12">
+        <v>44309</v>
+      </c>
+      <c r="C1291" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1291" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1291" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1291" s="10" t="s">
+        <v>1911</v>
+      </c>
+      <c r="G1291" s="11" t="s">
+        <v>1625</v>
+      </c>
+      <c r="H1291" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1291" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1291" s="13"/>
     </row>
     <row r="1292" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1292" s="12"/>
-      <c r="B1292" s="12"/>
-      <c r="C1292" s="14"/>
-      <c r="D1292" s="10"/>
-      <c r="E1292" s="11"/>
-      <c r="F1292" s="10"/>
+      <c r="A1292" s="12">
+        <v>44312</v>
+      </c>
+      <c r="B1292" s="12">
+        <v>44312</v>
+      </c>
+      <c r="C1292" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="D1292" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1292" s="11" t="s">
+        <v>759</v>
+      </c>
+      <c r="F1292" s="10" t="s">
+        <v>1912</v>
+      </c>
       <c r="G1292" s="11"/>
       <c r="H1292" s="12"/>
       <c r="I1292" s="13"/>
       <c r="J1292" s="13"/>
     </row>
-    <row r="1293" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1293" s="12"/>
-      <c r="B1293" s="9"/>
-      <c r="C1293" s="14"/>
-      <c r="D1293" s="10"/>
-      <c r="E1293" s="11"/>
-      <c r="F1293" s="10"/>
-      <c r="G1293" s="11"/>
-      <c r="H1293" s="12"/>
-      <c r="I1293" s="13"/>
-      <c r="J1293" s="13"/>
+    <row r="1293" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1293" s="12">
+        <v>44314</v>
+      </c>
+      <c r="B1293" s="12">
+        <v>44314</v>
+      </c>
+      <c r="C1293" s="14" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D1293" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1293" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1293" s="10" t="s">
+        <v>1913</v>
+      </c>
+      <c r="G1293" s="11" t="s">
+        <v>1625</v>
+      </c>
+      <c r="H1293" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1293" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1293" s="13" t="s">
+        <v>1914</v>
+      </c>
     </row>
     <row r="1294" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1294" s="1" t="s">
-        <v>1481</v>
-      </c>
-      <c r="B1294" s="2" t="s">
-        <v>1482</v>
-      </c>
-      <c r="C1294" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1294" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1294" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1294" s="4" t="s">
-        <v>1583</v>
-      </c>
-      <c r="G1294" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1294" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1294" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1294" s="36"/>
-    </row>
-    <row r="1295" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1295" s="12"/>
-      <c r="B1295" s="9"/>
-      <c r="C1295" s="14"/>
-      <c r="D1295" s="10"/>
-      <c r="E1295" s="11"/>
-      <c r="F1295" s="10"/>
+      <c r="A1294" s="12">
+        <v>44314</v>
+      </c>
+      <c r="B1294" s="12">
+        <v>44314</v>
+      </c>
+      <c r="C1294" s="14" t="s">
+        <v>559</v>
+      </c>
+      <c r="D1294" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1294" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1294" s="10" t="s">
+        <v>1915</v>
+      </c>
+      <c r="G1294" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1294" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1294" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1294" s="13"/>
+    </row>
+    <row r="1295" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1295" s="12">
+        <v>44315</v>
+      </c>
+      <c r="B1295" s="12"/>
+      <c r="C1295" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="D1295" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1295" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1295" s="10" t="s">
+        <v>1916</v>
+      </c>
       <c r="G1295" s="11"/>
       <c r="H1295" s="12"/>
       <c r="I1295" s="13"/>
-      <c r="J1295" s="13"/>
+      <c r="J1295" s="13" t="s">
+        <v>1917</v>
+      </c>
     </row>
     <row r="1296" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1296" s="12"/>
-      <c r="B1296" s="9">
-        <v>44255</v>
+      <c r="A1296" s="12">
+        <v>44315</v>
+      </c>
+      <c r="B1296" s="12">
+        <v>44315</v>
       </c>
       <c r="C1296" s="14" t="s">
-        <v>13</v>
+        <v>462</v>
       </c>
       <c r="D1296" s="10" t="s">
-        <v>584</v>
+        <v>107</v>
       </c>
       <c r="E1296" s="11" t="s">
-        <v>647</v>
+        <v>620</v>
       </c>
       <c r="F1296" s="10" t="s">
-        <v>1618</v>
-      </c>
-      <c r="G1296" s="11"/>
-      <c r="H1296" s="12"/>
-      <c r="I1296" s="13"/>
+        <v>1918</v>
+      </c>
+      <c r="G1296" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1296" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1296" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1296" s="13"/>
     </row>
     <row r="1297" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1297" s="12"/>
-      <c r="B1297" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1297" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1297" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1297" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1297" s="10" t="s">
-        <v>1610</v>
-      </c>
+      <c r="B1297" s="12"/>
+      <c r="C1297" s="14"/>
+      <c r="D1297" s="10"/>
+      <c r="E1297" s="11"/>
+      <c r="F1297" s="10"/>
       <c r="G1297" s="11"/>
       <c r="H1297" s="12"/>
       <c r="I1297" s="13"/>
@@ -45295,21 +45395,11 @@
     </row>
     <row r="1298" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1298" s="12"/>
-      <c r="B1298" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1298" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1298" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1298" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1298" s="10" t="s">
-        <v>1615</v>
-      </c>
+      <c r="B1298" s="12"/>
+      <c r="C1298" s="14"/>
+      <c r="D1298" s="10"/>
+      <c r="E1298" s="11"/>
+      <c r="F1298" s="10"/>
       <c r="G1298" s="11"/>
       <c r="H1298" s="12"/>
       <c r="I1298" s="13"/>
@@ -45317,43 +45407,23 @@
     </row>
     <row r="1299" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1299" s="12"/>
-      <c r="B1299" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1299" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1299" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1299" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1299" s="10" t="s">
-        <v>1611</v>
-      </c>
+      <c r="B1299" s="12"/>
+      <c r="C1299" s="14"/>
+      <c r="D1299" s="10"/>
+      <c r="E1299" s="11"/>
+      <c r="F1299" s="10"/>
       <c r="G1299" s="11"/>
       <c r="H1299" s="12"/>
       <c r="I1299" s="13"/>
       <c r="J1299" s="13"/>
     </row>
     <row r="1300" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1300" s="12">
-        <v>44159</v>
-      </c>
-      <c r="B1300" s="9"/>
-      <c r="C1300" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1300" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1300" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1300" s="10" t="s">
-        <v>1619</v>
-      </c>
+      <c r="A1300" s="12"/>
+      <c r="B1300" s="12"/>
+      <c r="C1300" s="14"/>
+      <c r="D1300" s="10"/>
+      <c r="E1300" s="11"/>
+      <c r="F1300" s="10"/>
       <c r="G1300" s="11"/>
       <c r="H1300" s="12"/>
       <c r="I1300" s="13"/>
@@ -45361,65 +45431,53 @@
     </row>
     <row r="1301" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1301" s="12"/>
-      <c r="B1301" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1301" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1301" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1301" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1301" s="10" t="s">
-        <v>1612</v>
-      </c>
+      <c r="B1301" s="9"/>
+      <c r="C1301" s="14"/>
+      <c r="D1301" s="10"/>
+      <c r="E1301" s="11"/>
+      <c r="F1301" s="10"/>
       <c r="G1301" s="11"/>
       <c r="H1301" s="12"/>
       <c r="I1301" s="13"/>
       <c r="J1301" s="13"/>
     </row>
     <row r="1302" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1302" s="12">
-        <v>44239</v>
-      </c>
-      <c r="B1302" s="9"/>
-      <c r="C1302" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1302" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1302" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1302" s="10" t="s">
-        <v>1609</v>
-      </c>
-      <c r="G1302" s="11"/>
-      <c r="H1302" s="12"/>
-      <c r="I1302" s="13"/>
-      <c r="J1302" s="13"/>
+      <c r="A1302" s="1" t="s">
+        <v>1481</v>
+      </c>
+      <c r="B1302" s="2" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C1302" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1302" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1302" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1302" s="4" t="s">
+        <v>1583</v>
+      </c>
+      <c r="G1302" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1302" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1302" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1302" s="36"/>
     </row>
     <row r="1303" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1303" s="12"/>
-      <c r="B1303" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1303" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1303" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1303" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1303" s="10" t="s">
-        <v>1608</v>
-      </c>
+      <c r="B1303" s="9"/>
+      <c r="C1303" s="14"/>
+      <c r="D1303" s="10"/>
+      <c r="E1303" s="11"/>
+      <c r="F1303" s="10"/>
       <c r="G1303" s="11"/>
       <c r="H1303" s="12"/>
       <c r="I1303" s="13"/>
@@ -45440,7 +45498,7 @@
         <v>647</v>
       </c>
       <c r="F1304" s="10" t="s">
-        <v>1613</v>
+        <v>1618</v>
       </c>
       <c r="G1304" s="11"/>
       <c r="H1304" s="12"/>
@@ -45450,7 +45508,7 @@
     <row r="1305" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1305" s="12"/>
       <c r="B1305" s="9">
-        <v>44291</v>
+        <v>44255</v>
       </c>
       <c r="C1305" s="14" t="s">
         <v>13</v>
@@ -45462,7 +45520,7 @@
         <v>647</v>
       </c>
       <c r="F1305" s="10" t="s">
-        <v>1616</v>
+        <v>1610</v>
       </c>
       <c r="G1305" s="11"/>
       <c r="H1305" s="12"/>
@@ -45472,7 +45530,7 @@
     <row r="1306" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1306" s="12"/>
       <c r="B1306" s="9">
-        <v>44235</v>
+        <v>44255</v>
       </c>
       <c r="C1306" s="14" t="s">
         <v>13</v>
@@ -45484,7 +45542,7 @@
         <v>647</v>
       </c>
       <c r="F1306" s="10" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
       <c r="G1306" s="11"/>
       <c r="H1306" s="12"/>
@@ -45492,10 +45550,10 @@
       <c r="J1306" s="13"/>
     </row>
     <row r="1307" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1307" s="12">
-        <v>44245</v>
-      </c>
-      <c r="B1307" s="9"/>
+      <c r="A1307" s="12"/>
+      <c r="B1307" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1307" s="14" t="s">
         <v>13</v>
       </c>
@@ -45506,7 +45564,7 @@
         <v>647</v>
       </c>
       <c r="F1307" s="10" t="s">
-        <v>1614</v>
+        <v>1611</v>
       </c>
       <c r="G1307" s="11"/>
       <c r="H1307" s="12"/>
@@ -45514,7 +45572,9 @@
       <c r="J1307" s="13"/>
     </row>
     <row r="1308" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1308" s="12"/>
+      <c r="A1308" s="12">
+        <v>44159</v>
+      </c>
       <c r="B1308" s="9"/>
       <c r="C1308" s="14" t="s">
         <v>13</v>
@@ -45526,7 +45586,7 @@
         <v>647</v>
       </c>
       <c r="F1308" s="10" t="s">
-        <v>1585</v>
+        <v>1619</v>
       </c>
       <c r="G1308" s="11"/>
       <c r="H1308" s="12"/>
@@ -45534,21 +45594,21 @@
       <c r="J1308" s="13"/>
     </row>
     <row r="1309" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1309" s="12">
-        <v>44176</v>
-      </c>
-      <c r="B1309" s="9"/>
+      <c r="A1309" s="12"/>
+      <c r="B1309" s="12">
+        <v>44309</v>
+      </c>
       <c r="C1309" s="14" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D1309" s="10" t="s">
         <v>584</v>
       </c>
       <c r="E1309" s="11" t="s">
-        <v>1355</v>
+        <v>647</v>
       </c>
       <c r="F1309" s="10" t="s">
-        <v>1356</v>
+        <v>1612</v>
       </c>
       <c r="G1309" s="11"/>
       <c r="H1309" s="12"/>
@@ -45556,103 +45616,109 @@
       <c r="J1309" s="13"/>
     </row>
     <row r="1310" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1310" s="12"/>
+      <c r="A1310" s="12">
+        <v>44239</v>
+      </c>
       <c r="B1310" s="9"/>
-      <c r="C1310" s="14"/>
-      <c r="D1310" s="10"/>
-      <c r="E1310" s="11"/>
-      <c r="F1310" s="10"/>
+      <c r="C1310" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1310" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1310" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1310" s="10" t="s">
+        <v>1609</v>
+      </c>
       <c r="G1310" s="11"/>
       <c r="H1310" s="12"/>
       <c r="I1310" s="13"/>
       <c r="J1310" s="13"/>
     </row>
-    <row r="1311" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1311" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1311" s="9"/>
+    <row r="1311" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1311" s="12"/>
+      <c r="B1311" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1311" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1311" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1311" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1311" s="10" t="s">
-        <v>1663</v>
+        <v>1608</v>
       </c>
       <c r="G1311" s="11"/>
       <c r="H1311" s="12"/>
       <c r="I1311" s="13"/>
-      <c r="J1311" s="13" t="s">
-        <v>1686</v>
-      </c>
-    </row>
-    <row r="1312" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1312" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1312" s="9"/>
+      <c r="J1311" s="13"/>
+    </row>
+    <row r="1312" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1312" s="12"/>
+      <c r="B1312" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1312" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1312" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1312" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1312" s="10" t="s">
-        <v>1662</v>
+        <v>1613</v>
       </c>
       <c r="G1312" s="11"/>
       <c r="H1312" s="12"/>
       <c r="I1312" s="13"/>
       <c r="J1312" s="13"/>
     </row>
-    <row r="1313" spans="1:10" ht="84" x14ac:dyDescent="0.2">
-      <c r="A1313" s="12">
-        <v>43864</v>
-      </c>
-      <c r="B1313" s="9"/>
+    <row r="1313" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1313" s="12"/>
+      <c r="B1313" s="12">
+        <v>44309</v>
+      </c>
       <c r="C1313" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1313" s="10" t="s">
-        <v>533</v>
+        <v>584</v>
       </c>
       <c r="E1313" s="11" t="s">
-        <v>1582</v>
+        <v>647</v>
       </c>
       <c r="F1313" s="10" t="s">
-        <v>534</v>
+        <v>1616</v>
       </c>
       <c r="G1313" s="11"/>
       <c r="H1313" s="12"/>
       <c r="I1313" s="13"/>
-      <c r="J1313" s="13" t="s">
-        <v>1709</v>
-      </c>
-    </row>
-    <row r="1314" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1314" s="12">
-        <v>44131</v>
-      </c>
-      <c r="B1314" s="9"/>
+      <c r="J1313" s="13"/>
+    </row>
+    <row r="1314" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1314" s="12"/>
+      <c r="B1314" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1314" s="14" t="s">
-        <v>1132</v>
+        <v>13</v>
       </c>
       <c r="D1314" s="10" t="s">
-        <v>89</v>
+        <v>584</v>
       </c>
       <c r="E1314" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1314" s="10" t="s">
-        <v>1165</v>
+        <v>1617</v>
       </c>
       <c r="G1314" s="11"/>
       <c r="H1314" s="12"/>
@@ -45661,20 +45727,20 @@
     </row>
     <row r="1315" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1315" s="12">
-        <v>44112</v>
+        <v>44245</v>
       </c>
       <c r="B1315" s="9"/>
       <c r="C1315" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1315" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1315" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1315" s="10" t="s">
-        <v>1098</v>
+        <v>1614</v>
       </c>
       <c r="G1315" s="11"/>
       <c r="H1315" s="12"/>
@@ -45682,21 +45748,19 @@
       <c r="J1315" s="13"/>
     </row>
     <row r="1316" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1316" s="12">
-        <v>44088</v>
-      </c>
+      <c r="A1316" s="12"/>
       <c r="B1316" s="9"/>
       <c r="C1316" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1316" s="10" t="s">
-        <v>906</v>
+        <v>584</v>
       </c>
       <c r="E1316" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1316" s="10" t="s">
-        <v>1012</v>
+        <v>1585</v>
       </c>
       <c r="G1316" s="11"/>
       <c r="H1316" s="12"/>
@@ -45705,20 +45769,20 @@
     </row>
     <row r="1317" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1317" s="12">
-        <v>44083</v>
+        <v>44176</v>
       </c>
       <c r="B1317" s="9"/>
       <c r="C1317" s="14" t="s">
-        <v>468</v>
+        <v>8</v>
       </c>
       <c r="D1317" s="10" t="s">
-        <v>89</v>
+        <v>584</v>
       </c>
       <c r="E1317" s="11" t="s">
-        <v>837</v>
+        <v>1355</v>
       </c>
       <c r="F1317" s="10" t="s">
-        <v>989</v>
+        <v>1356</v>
       </c>
       <c r="G1317" s="11"/>
       <c r="H1317" s="12"/>
@@ -45726,52 +45790,44 @@
       <c r="J1317" s="13"/>
     </row>
     <row r="1318" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1318" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1318" s="12"/>
       <c r="B1318" s="9"/>
-      <c r="C1318" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="D1318" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1318" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1318" s="10" t="s">
-        <v>903</v>
-      </c>
+      <c r="C1318" s="14"/>
+      <c r="D1318" s="10"/>
+      <c r="E1318" s="11"/>
+      <c r="F1318" s="10"/>
       <c r="G1318" s="11"/>
       <c r="H1318" s="12"/>
       <c r="I1318" s="13"/>
       <c r="J1318" s="13"/>
     </row>
-    <row r="1319" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1319" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1319" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1319" s="9"/>
       <c r="C1319" s="14" t="s">
-        <v>623</v>
+        <v>898</v>
       </c>
       <c r="D1319" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1319" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1319" s="10" t="s">
-        <v>902</v>
+        <v>1663</v>
       </c>
       <c r="G1319" s="11"/>
       <c r="H1319" s="12"/>
       <c r="I1319" s="13"/>
-      <c r="J1319" s="13"/>
-    </row>
-    <row r="1320" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1319" s="13" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1320" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1320" s="9"/>
       <c r="C1320" s="14" t="s">
@@ -45781,115 +45837,109 @@
         <v>494</v>
       </c>
       <c r="E1320" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1320" s="10" t="s">
-        <v>900</v>
+        <v>1662</v>
       </c>
       <c r="G1320" s="11"/>
       <c r="H1320" s="12"/>
       <c r="I1320" s="13"/>
       <c r="J1320" s="13"/>
     </row>
-    <row r="1321" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="1321" spans="1:10" ht="84" x14ac:dyDescent="0.2">
       <c r="A1321" s="12">
-        <v>44055</v>
+        <v>43864</v>
       </c>
       <c r="B1321" s="9"/>
       <c r="C1321" s="14" t="s">
-        <v>898</v>
+        <v>19</v>
       </c>
       <c r="D1321" s="10" t="s">
-        <v>494</v>
+        <v>533</v>
       </c>
       <c r="E1321" s="11" t="s">
-        <v>570</v>
+        <v>1582</v>
       </c>
       <c r="F1321" s="10" t="s">
-        <v>901</v>
+        <v>534</v>
       </c>
       <c r="G1321" s="11"/>
       <c r="H1321" s="12"/>
       <c r="I1321" s="13"/>
-      <c r="J1321" s="13"/>
-    </row>
-    <row r="1322" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="J1321" s="13" t="s">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1322" s="12">
-        <v>44055</v>
+        <v>44131</v>
       </c>
       <c r="B1322" s="9"/>
       <c r="C1322" s="14" t="s">
-        <v>898</v>
+        <v>1132</v>
       </c>
       <c r="D1322" s="10" t="s">
-        <v>494</v>
+        <v>89</v>
       </c>
       <c r="E1322" s="11" t="s">
-        <v>570</v>
+        <v>685</v>
       </c>
       <c r="F1322" s="10" t="s">
-        <v>904</v>
+        <v>1165</v>
       </c>
       <c r="G1322" s="11"/>
       <c r="H1322" s="12"/>
       <c r="I1322" s="13"/>
-      <c r="J1322" s="13" t="s">
-        <v>1592</v>
-      </c>
-    </row>
-    <row r="1323" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1322" s="13"/>
+    </row>
+    <row r="1323" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1323" s="12">
-        <v>44047</v>
+        <v>44112</v>
       </c>
       <c r="B1323" s="9"/>
       <c r="C1323" s="14" t="s">
-        <v>537</v>
+        <v>623</v>
       </c>
       <c r="D1323" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E1323" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1323" s="10" t="s">
-        <v>873</v>
-      </c>
-      <c r="G1323" s="11" t="s">
-        <v>1628</v>
-      </c>
+        <v>1098</v>
+      </c>
+      <c r="G1323" s="11"/>
       <c r="H1323" s="12"/>
       <c r="I1323" s="13"/>
       <c r="J1323" s="13"/>
     </row>
-    <row r="1324" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1324" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1324" s="12">
-        <v>43949</v>
+        <v>44088</v>
       </c>
       <c r="B1324" s="9"/>
       <c r="C1324" s="14" t="s">
-        <v>468</v>
+        <v>19</v>
       </c>
       <c r="D1324" s="10" t="s">
-        <v>89</v>
+        <v>906</v>
       </c>
       <c r="E1324" s="11" t="s">
         <v>685</v>
       </c>
       <c r="F1324" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1324" s="11" t="s">
-        <v>1643</v>
-      </c>
+        <v>1012</v>
+      </c>
+      <c r="G1324" s="11"/>
       <c r="H1324" s="12"/>
-      <c r="I1324" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1324" s="13"/>
       <c r="J1324" s="13"/>
     </row>
-    <row r="1325" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1325" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1325" s="12">
-        <v>43949</v>
+        <v>44083</v>
       </c>
       <c r="B1325" s="9"/>
       <c r="C1325" s="14" t="s">
@@ -45899,261 +45949,445 @@
         <v>89</v>
       </c>
       <c r="E1325" s="11" t="s">
-        <v>685</v>
+        <v>837</v>
       </c>
       <c r="F1325" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1325" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>989</v>
+      </c>
+      <c r="G1325" s="11"/>
       <c r="H1325" s="12"/>
-      <c r="I1325" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1325" s="13" t="s">
-        <v>1571</v>
-      </c>
-    </row>
-    <row r="1326" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1325" s="13"/>
+      <c r="J1325" s="13"/>
+    </row>
+    <row r="1326" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1326" s="12">
-        <v>43838</v>
+        <v>44055</v>
       </c>
       <c r="B1326" s="9"/>
       <c r="C1326" s="14" t="s">
-        <v>103</v>
+        <v>623</v>
       </c>
       <c r="D1326" s="10" t="s">
-        <v>460</v>
+        <v>6</v>
       </c>
       <c r="E1326" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1326" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G1326" s="11" t="s">
-        <v>1644</v>
-      </c>
+        <v>903</v>
+      </c>
+      <c r="G1326" s="11"/>
       <c r="H1326" s="12"/>
       <c r="I1326" s="13"/>
-      <c r="J1326" s="13" t="s">
-        <v>1536</v>
-      </c>
+      <c r="J1326" s="13"/>
     </row>
     <row r="1327" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1327" s="12">
-        <v>43816</v>
+        <v>44055</v>
       </c>
       <c r="B1327" s="9"/>
       <c r="C1327" s="14" t="s">
-        <v>475</v>
+        <v>623</v>
       </c>
       <c r="D1327" s="10" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="E1327" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1327" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="G1327" s="11" t="s">
-        <v>1636</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="G1327" s="11"/>
       <c r="H1327" s="12"/>
       <c r="I1327" s="13"/>
-      <c r="J1327" s="13" t="s">
-        <v>1572</v>
-      </c>
-    </row>
-    <row r="1328" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1327" s="13"/>
+    </row>
+    <row r="1328" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1328" s="12">
-        <v>43762</v>
+        <v>44055</v>
       </c>
       <c r="B1328" s="9"/>
       <c r="C1328" s="14" t="s">
-        <v>446</v>
+        <v>898</v>
       </c>
       <c r="D1328" s="10" t="s">
-        <v>17</v>
+        <v>494</v>
       </c>
       <c r="E1328" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1328" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G1328" s="11" t="s">
-        <v>1633</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="G1328" s="11"/>
       <c r="H1328" s="12"/>
       <c r="I1328" s="13"/>
       <c r="J1328" s="13"/>
     </row>
-    <row r="1329" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1329" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A1329" s="12">
-        <v>44222</v>
+        <v>44055</v>
       </c>
       <c r="B1329" s="9"/>
       <c r="C1329" s="14" t="s">
-        <v>1497</v>
+        <v>898</v>
       </c>
       <c r="D1329" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1329" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1329" s="10" t="s">
-        <v>1496</v>
-      </c>
-      <c r="G1329" s="11" t="s">
-        <v>309</v>
-      </c>
+        <v>901</v>
+      </c>
+      <c r="G1329" s="11"/>
       <c r="H1329" s="12"/>
       <c r="I1329" s="13"/>
       <c r="J1329" s="13"/>
     </row>
     <row r="1330" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1330" s="12">
-        <v>44266</v>
+        <v>44055</v>
       </c>
       <c r="B1330" s="9"/>
       <c r="C1330" s="14" t="s">
-        <v>537</v>
+        <v>898</v>
       </c>
       <c r="D1330" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1330" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1330" s="10" t="s">
-        <v>1717</v>
+        <v>904</v>
       </c>
       <c r="G1330" s="11"/>
       <c r="H1330" s="12"/>
       <c r="I1330" s="13"/>
       <c r="J1330" s="13" t="s">
-        <v>1718</v>
-      </c>
-    </row>
-    <row r="1331" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1331" s="12">
-        <v>44279</v>
+        <v>44047</v>
       </c>
       <c r="B1331" s="9"/>
       <c r="C1331" s="14" t="s">
-        <v>1390</v>
+        <v>537</v>
       </c>
       <c r="D1331" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1331" s="11" t="s">
-        <v>1582</v>
+        <v>685</v>
       </c>
       <c r="F1331" s="10" t="s">
-        <v>1734</v>
-      </c>
-      <c r="G1331" s="11"/>
+        <v>873</v>
+      </c>
+      <c r="G1331" s="11" t="s">
+        <v>1628</v>
+      </c>
       <c r="H1331" s="12"/>
       <c r="I1331" s="13"/>
       <c r="J1331" s="13"/>
     </row>
-    <row r="1332" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="1332" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A1332" s="12">
-        <v>44286</v>
+        <v>43949</v>
       </c>
       <c r="B1332" s="9"/>
       <c r="C1332" s="14" t="s">
-        <v>288</v>
+        <v>468</v>
       </c>
       <c r="D1332" s="10" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="E1332" s="11" t="s">
-        <v>1582</v>
+        <v>685</v>
       </c>
       <c r="F1332" s="10" t="s">
-        <v>1843</v>
-      </c>
-      <c r="G1332" s="11"/>
+        <v>686</v>
+      </c>
+      <c r="G1332" s="11" t="s">
+        <v>1643</v>
+      </c>
       <c r="H1332" s="12"/>
-      <c r="I1332" s="13"/>
+      <c r="I1332" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1332" s="13"/>
     </row>
-    <row r="1333" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1333" s="12"/>
+    <row r="1333" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1333" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1333" s="9"/>
-      <c r="C1333" s="14"/>
-      <c r="D1333" s="10"/>
-      <c r="E1333" s="11"/>
-      <c r="F1333" s="10"/>
-      <c r="G1333" s="11"/>
+      <c r="C1333" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1333" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1333" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1333" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="G1333" s="11" t="s">
+        <v>687</v>
+      </c>
       <c r="H1333" s="12"/>
-      <c r="I1333" s="13"/>
-      <c r="J1333" s="13"/>
-    </row>
-    <row r="1334" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1334" s="12"/>
+      <c r="I1333" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1333" s="13" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1334" s="12">
+        <v>43838</v>
+      </c>
       <c r="B1334" s="9"/>
-      <c r="C1334" s="14"/>
-      <c r="D1334" s="10"/>
-      <c r="E1334" s="11"/>
-      <c r="F1334" s="10"/>
-      <c r="G1334" s="11"/>
+      <c r="C1334" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1334" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1334" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1334" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G1334" s="11" t="s">
+        <v>1644</v>
+      </c>
       <c r="H1334" s="12"/>
       <c r="I1334" s="13"/>
-      <c r="J1334" s="13"/>
+      <c r="J1334" s="13" t="s">
+        <v>1536</v>
+      </c>
     </row>
     <row r="1335" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1335" s="12"/>
+      <c r="A1335" s="12">
+        <v>43816</v>
+      </c>
       <c r="B1335" s="9"/>
-      <c r="C1335" s="14"/>
-      <c r="D1335" s="10"/>
-      <c r="E1335" s="11"/>
-      <c r="F1335" s="10"/>
-      <c r="G1335" s="11"/>
+      <c r="C1335" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1335" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1335" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1335" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G1335" s="11" t="s">
+        <v>1636</v>
+      </c>
       <c r="H1335" s="12"/>
       <c r="I1335" s="13"/>
-      <c r="J1335" s="13"/>
-    </row>
-    <row r="1336" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1336" s="12"/>
+      <c r="J1335" s="13" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1336" s="12">
+        <v>43762</v>
+      </c>
       <c r="B1336" s="9"/>
-      <c r="C1336" s="14"/>
-      <c r="D1336" s="10"/>
-      <c r="E1336" s="11"/>
-      <c r="F1336" s="10"/>
-      <c r="G1336" s="11"/>
+      <c r="C1336" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1336" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1336" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1336" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1336" s="11" t="s">
+        <v>1633</v>
+      </c>
       <c r="H1336" s="12"/>
       <c r="I1336" s="13"/>
       <c r="J1336" s="13"/>
     </row>
     <row r="1337" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1337" s="12"/>
+      <c r="A1337" s="12">
+        <v>44222</v>
+      </c>
       <c r="B1337" s="9"/>
-      <c r="C1337" s="14"/>
-      <c r="D1337" s="10"/>
-      <c r="E1337" s="11"/>
-      <c r="F1337" s="10"/>
-      <c r="G1337" s="11"/>
+      <c r="C1337" s="14" t="s">
+        <v>1497</v>
+      </c>
+      <c r="D1337" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1337" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1337" s="10" t="s">
+        <v>1496</v>
+      </c>
+      <c r="G1337" s="11" t="s">
+        <v>309</v>
+      </c>
       <c r="H1337" s="12"/>
       <c r="I1337" s="13"/>
       <c r="J1337" s="13"/>
     </row>
-    <row r="1338" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1338" s="12"/>
+    <row r="1338" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1338" s="12">
+        <v>44266</v>
+      </c>
       <c r="B1338" s="9"/>
-      <c r="C1338" s="14"/>
-      <c r="D1338" s="10"/>
-      <c r="E1338" s="11"/>
-      <c r="F1338" s="10"/>
+      <c r="C1338" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1338" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1338" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1338" s="10" t="s">
+        <v>1717</v>
+      </c>
       <c r="G1338" s="11"/>
       <c r="H1338" s="12"/>
       <c r="I1338" s="13"/>
-      <c r="J1338" s="13"/>
+      <c r="J1338" s="13" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1339" s="12">
+        <v>44279</v>
+      </c>
+      <c r="B1339" s="9"/>
+      <c r="C1339" s="14" t="s">
+        <v>1390</v>
+      </c>
+      <c r="D1339" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1339" s="11" t="s">
+        <v>1582</v>
+      </c>
+      <c r="F1339" s="10" t="s">
+        <v>1734</v>
+      </c>
+      <c r="G1339" s="11"/>
+      <c r="H1339" s="12"/>
+      <c r="I1339" s="13"/>
+      <c r="J1339" s="13"/>
+    </row>
+    <row r="1340" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1340" s="12">
+        <v>44286</v>
+      </c>
+      <c r="B1340" s="9"/>
+      <c r="C1340" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1340" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1340" s="11" t="s">
+        <v>1582</v>
+      </c>
+      <c r="F1340" s="10" t="s">
+        <v>1843</v>
+      </c>
+      <c r="G1340" s="11"/>
+      <c r="H1340" s="12"/>
+      <c r="I1340" s="13"/>
+      <c r="J1340" s="13"/>
+    </row>
+    <row r="1341" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1341" s="12"/>
+      <c r="B1341" s="9"/>
+      <c r="C1341" s="14"/>
+      <c r="D1341" s="10"/>
+      <c r="E1341" s="11"/>
+      <c r="F1341" s="10"/>
+      <c r="G1341" s="11"/>
+      <c r="H1341" s="12"/>
+      <c r="I1341" s="13"/>
+      <c r="J1341" s="13"/>
+    </row>
+    <row r="1342" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1342" s="12"/>
+      <c r="B1342" s="9"/>
+      <c r="C1342" s="14"/>
+      <c r="D1342" s="10"/>
+      <c r="E1342" s="11"/>
+      <c r="F1342" s="10"/>
+      <c r="G1342" s="11"/>
+      <c r="H1342" s="12"/>
+      <c r="I1342" s="13"/>
+      <c r="J1342" s="13"/>
+    </row>
+    <row r="1343" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1343" s="12"/>
+      <c r="B1343" s="9"/>
+      <c r="C1343" s="14"/>
+      <c r="D1343" s="10"/>
+      <c r="E1343" s="11"/>
+      <c r="F1343" s="10"/>
+      <c r="G1343" s="11"/>
+      <c r="H1343" s="12"/>
+      <c r="I1343" s="13"/>
+      <c r="J1343" s="13"/>
+    </row>
+    <row r="1344" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1344" s="12"/>
+      <c r="B1344" s="9"/>
+      <c r="C1344" s="14"/>
+      <c r="D1344" s="10"/>
+      <c r="E1344" s="11"/>
+      <c r="F1344" s="10"/>
+      <c r="G1344" s="11"/>
+      <c r="H1344" s="12"/>
+      <c r="I1344" s="13"/>
+      <c r="J1344" s="13"/>
+    </row>
+    <row r="1345" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1345" s="12"/>
+      <c r="B1345" s="9"/>
+      <c r="C1345" s="14"/>
+      <c r="D1345" s="10"/>
+      <c r="E1345" s="11"/>
+      <c r="F1345" s="10"/>
+      <c r="G1345" s="11"/>
+      <c r="H1345" s="12"/>
+      <c r="I1345" s="13"/>
+      <c r="J1345" s="13"/>
+    </row>
+    <row r="1346" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1346" s="12"/>
+      <c r="B1346" s="9"/>
+      <c r="C1346" s="14"/>
+      <c r="D1346" s="10"/>
+      <c r="E1346" s="11"/>
+      <c r="F1346" s="10"/>
+      <c r="G1346" s="11"/>
+      <c r="H1346" s="12"/>
+      <c r="I1346" s="13"/>
+      <c r="J1346" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1172" xr:uid="{00000000-0009-0000-0000-000000000000}">
@@ -46161,8 +46395,8 @@
       <sortCondition ref="A1:A1023"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1297:F1307">
-    <sortCondition ref="F1297:F1307"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1305:F1315">
+    <sortCondition ref="F1305:F1315"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -46179,7 +46413,7 @@
   <dimension ref="B1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46194,14 +46428,14 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="41" t="s">
         <v>1742</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="43"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -46224,7 +46458,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="37" t="s">
         <v>1748</v>
       </c>
       <c r="C5" t="s">
@@ -46244,7 +46478,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="37" t="s">
         <v>1751</v>
       </c>
       <c r="C6" t="s">

</xml_diff>

<commit_message>
Alteração inversão multa e Bonificação
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC1C210-8C1F-4BEA-8F3F-044DCFC69937}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DA5117-4553-4CB6-A4E3-01AC39083B0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="347" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9384" uniqueCount="1945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9428" uniqueCount="1951">
   <si>
     <t>Responsável</t>
   </si>
@@ -6200,6 +6200,24 @@
   </si>
   <si>
     <t>BKGCTR08, BKGCTR10, BKGCTR12 e BKGCTR13</t>
+  </si>
+  <si>
+    <t>Edivaldo</t>
+  </si>
+  <si>
+    <t>EFD abril/2021</t>
+  </si>
+  <si>
+    <t>Adilson Marinho</t>
+  </si>
+  <si>
+    <t>Relação de Nfs liberadas por Adilson Marinho em 12/05/2021</t>
+  </si>
+  <si>
+    <t>Relação de Contas Contabeis x Plano Referencial</t>
+  </si>
+  <si>
+    <t>Acerto de dados dos clientes 370 e 371</t>
   </si>
 </sst>
 </file>
@@ -6965,11 +6983,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1371"/>
+  <dimension ref="A1:J1378"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1308" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1323" sqref="A1323"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1314" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1329" sqref="A1329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -46275,112 +46293,192 @@
       </c>
     </row>
     <row r="1323" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1323" s="12"/>
-      <c r="B1323" s="12"/>
-      <c r="C1323" s="14"/>
-      <c r="D1323" s="10"/>
-      <c r="E1323" s="11"/>
-      <c r="F1323" s="10"/>
-      <c r="G1323" s="11"/>
-      <c r="H1323" s="12"/>
-      <c r="I1323" s="13"/>
+      <c r="A1323" s="12">
+        <v>44268</v>
+      </c>
+      <c r="B1323" s="12">
+        <v>44268</v>
+      </c>
+      <c r="C1323" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1323" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1323" s="11" t="s">
+        <v>1836</v>
+      </c>
+      <c r="F1323" s="10" t="s">
+        <v>1804</v>
+      </c>
+      <c r="G1323" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1323" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1323" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1323" s="13"/>
     </row>
     <row r="1324" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1324" s="12"/>
-      <c r="B1324" s="12"/>
-      <c r="C1324" s="14"/>
-      <c r="D1324" s="10"/>
-      <c r="E1324" s="11"/>
-      <c r="F1324" s="10"/>
-      <c r="G1324" s="11"/>
-      <c r="H1324" s="12"/>
-      <c r="I1324" s="13"/>
+      <c r="A1324" s="12">
+        <v>44268</v>
+      </c>
+      <c r="B1324" s="12">
+        <v>44268</v>
+      </c>
+      <c r="C1324" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1324" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1324" s="11" t="s">
+        <v>1836</v>
+      </c>
+      <c r="F1324" s="10" t="s">
+        <v>1776</v>
+      </c>
+      <c r="G1324" s="11" t="s">
+        <v>1628</v>
+      </c>
+      <c r="H1324" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1324" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1324" s="13"/>
     </row>
     <row r="1325" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1325" s="12"/>
-      <c r="B1325" s="12"/>
-      <c r="C1325" s="14"/>
-      <c r="D1325" s="10"/>
-      <c r="E1325" s="11"/>
-      <c r="F1325" s="10"/>
-      <c r="G1325" s="11"/>
-      <c r="H1325" s="12"/>
-      <c r="I1325" s="13"/>
+      <c r="A1325" s="12">
+        <v>44268</v>
+      </c>
+      <c r="B1325" s="12">
+        <v>44268</v>
+      </c>
+      <c r="C1325" s="14" t="s">
+        <v>1945</v>
+      </c>
+      <c r="D1325" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1325" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1325" s="10" t="s">
+        <v>1946</v>
+      </c>
+      <c r="G1325" s="11" t="s">
+        <v>1651</v>
+      </c>
+      <c r="H1325" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1325" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1325" s="13"/>
     </row>
     <row r="1326" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1326" s="12"/>
-      <c r="B1326" s="9"/>
-      <c r="C1326" s="14"/>
-      <c r="D1326" s="10"/>
-      <c r="E1326" s="11"/>
-      <c r="F1326" s="10"/>
-      <c r="G1326" s="11"/>
-      <c r="H1326" s="12"/>
-      <c r="I1326" s="13"/>
+      <c r="A1326" s="12">
+        <v>44268</v>
+      </c>
+      <c r="B1326" s="12">
+        <v>44268</v>
+      </c>
+      <c r="C1326" s="14" t="s">
+        <v>1947</v>
+      </c>
+      <c r="D1326" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1326" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1326" s="10" t="s">
+        <v>1948</v>
+      </c>
+      <c r="G1326" s="11" t="s">
+        <v>1650</v>
+      </c>
+      <c r="H1326" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1326" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1326" s="13"/>
     </row>
     <row r="1327" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1327" s="1" t="s">
-        <v>1481</v>
-      </c>
-      <c r="B1327" s="2" t="s">
-        <v>1482</v>
-      </c>
-      <c r="C1327" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1327" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1327" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1327" s="4" t="s">
-        <v>1583</v>
-      </c>
-      <c r="G1327" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1327" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1327" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1327" s="36"/>
+      <c r="A1327" s="12">
+        <v>44268</v>
+      </c>
+      <c r="B1327" s="12">
+        <v>44268</v>
+      </c>
+      <c r="C1327" s="14" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D1327" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1327" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1327" s="10" t="s">
+        <v>1949</v>
+      </c>
+      <c r="G1327" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1327" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1327" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1327" s="13"/>
     </row>
     <row r="1328" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1328" s="12"/>
-      <c r="B1328" s="9"/>
-      <c r="C1328" s="14"/>
-      <c r="D1328" s="10"/>
-      <c r="E1328" s="11"/>
-      <c r="F1328" s="10"/>
-      <c r="G1328" s="11"/>
-      <c r="H1328" s="12"/>
-      <c r="I1328" s="13"/>
+      <c r="A1328" s="12">
+        <v>44268</v>
+      </c>
+      <c r="B1328" s="12">
+        <v>44268</v>
+      </c>
+      <c r="C1328" s="14" t="s">
+        <v>559</v>
+      </c>
+      <c r="D1328" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1328" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1328" s="10" t="s">
+        <v>1950</v>
+      </c>
+      <c r="G1328" s="11" t="s">
+        <v>1650</v>
+      </c>
+      <c r="H1328" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1328" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1328" s="13"/>
     </row>
     <row r="1329" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1329" s="12"/>
-      <c r="B1329" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1329" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1329" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1329" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1329" s="10" t="s">
-        <v>1618</v>
-      </c>
+      <c r="B1329" s="12"/>
+      <c r="C1329" s="14"/>
+      <c r="D1329" s="10"/>
+      <c r="E1329" s="11"/>
+      <c r="F1329" s="10"/>
       <c r="G1329" s="11"/>
       <c r="H1329" s="12"/>
       <c r="I1329" s="13"/>
@@ -46388,21 +46486,11 @@
     </row>
     <row r="1330" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1330" s="12"/>
-      <c r="B1330" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1330" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1330" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1330" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1330" s="10" t="s">
-        <v>1610</v>
-      </c>
+      <c r="B1330" s="12"/>
+      <c r="C1330" s="14"/>
+      <c r="D1330" s="10"/>
+      <c r="E1330" s="11"/>
+      <c r="F1330" s="10"/>
       <c r="G1330" s="11"/>
       <c r="H1330" s="12"/>
       <c r="I1330" s="13"/>
@@ -46410,21 +46498,11 @@
     </row>
     <row r="1331" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1331" s="12"/>
-      <c r="B1331" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1331" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1331" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1331" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1331" s="10" t="s">
-        <v>1615</v>
-      </c>
+      <c r="B1331" s="12"/>
+      <c r="C1331" s="14"/>
+      <c r="D1331" s="10"/>
+      <c r="E1331" s="11"/>
+      <c r="F1331" s="10"/>
       <c r="G1331" s="11"/>
       <c r="H1331" s="12"/>
       <c r="I1331" s="13"/>
@@ -46432,87 +46510,65 @@
     </row>
     <row r="1332" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1332" s="12"/>
-      <c r="B1332" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1332" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1332" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1332" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1332" s="10" t="s">
-        <v>1611</v>
-      </c>
+      <c r="B1332" s="12"/>
+      <c r="C1332" s="14"/>
+      <c r="D1332" s="10"/>
+      <c r="E1332" s="11"/>
+      <c r="F1332" s="10"/>
       <c r="G1332" s="11"/>
       <c r="H1332" s="12"/>
       <c r="I1332" s="13"/>
       <c r="J1332" s="13"/>
     </row>
     <row r="1333" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1333" s="12">
-        <v>44159</v>
-      </c>
+      <c r="A1333" s="12"/>
       <c r="B1333" s="9"/>
-      <c r="C1333" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1333" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1333" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1333" s="10" t="s">
-        <v>1619</v>
-      </c>
+      <c r="C1333" s="14"/>
+      <c r="D1333" s="10"/>
+      <c r="E1333" s="11"/>
+      <c r="F1333" s="10"/>
       <c r="G1333" s="11"/>
       <c r="H1333" s="12"/>
       <c r="I1333" s="13"/>
       <c r="J1333" s="13"/>
     </row>
     <row r="1334" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1334" s="12"/>
-      <c r="B1334" s="12">
-        <v>44309</v>
-      </c>
-      <c r="C1334" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1334" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1334" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1334" s="10" t="s">
-        <v>1612</v>
-      </c>
-      <c r="G1334" s="11"/>
-      <c r="H1334" s="12"/>
-      <c r="I1334" s="13"/>
-      <c r="J1334" s="13"/>
+      <c r="A1334" s="1" t="s">
+        <v>1481</v>
+      </c>
+      <c r="B1334" s="2" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C1334" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1334" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1334" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1334" s="4" t="s">
+        <v>1583</v>
+      </c>
+      <c r="G1334" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1334" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1334" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1334" s="36"/>
     </row>
     <row r="1335" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1335" s="12">
-        <v>44239</v>
-      </c>
+      <c r="A1335" s="12"/>
       <c r="B1335" s="9"/>
-      <c r="C1335" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1335" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1335" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1335" s="10" t="s">
-        <v>1609</v>
-      </c>
+      <c r="C1335" s="14"/>
+      <c r="D1335" s="10"/>
+      <c r="E1335" s="11"/>
+      <c r="F1335" s="10"/>
       <c r="G1335" s="11"/>
       <c r="H1335" s="12"/>
       <c r="I1335" s="13"/>
@@ -46533,7 +46589,7 @@
         <v>647</v>
       </c>
       <c r="F1336" s="10" t="s">
-        <v>1608</v>
+        <v>1618</v>
       </c>
       <c r="G1336" s="11"/>
       <c r="H1336" s="12"/>
@@ -46555,7 +46611,7 @@
         <v>647</v>
       </c>
       <c r="F1337" s="10" t="s">
-        <v>1613</v>
+        <v>1610</v>
       </c>
       <c r="G1337" s="11"/>
       <c r="H1337" s="12"/>
@@ -46564,8 +46620,8 @@
     </row>
     <row r="1338" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1338" s="12"/>
-      <c r="B1338" s="12">
-        <v>44309</v>
+      <c r="B1338" s="9">
+        <v>44255</v>
       </c>
       <c r="C1338" s="14" t="s">
         <v>13</v>
@@ -46577,7 +46633,7 @@
         <v>647</v>
       </c>
       <c r="F1338" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="G1338" s="11"/>
       <c r="H1338" s="12"/>
@@ -46587,7 +46643,7 @@
     <row r="1339" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1339" s="12"/>
       <c r="B1339" s="9">
-        <v>44235</v>
+        <v>44255</v>
       </c>
       <c r="C1339" s="14" t="s">
         <v>13</v>
@@ -46599,7 +46655,7 @@
         <v>647</v>
       </c>
       <c r="F1339" s="10" t="s">
-        <v>1617</v>
+        <v>1611</v>
       </c>
       <c r="G1339" s="11"/>
       <c r="H1339" s="12"/>
@@ -46608,7 +46664,7 @@
     </row>
     <row r="1340" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1340" s="12">
-        <v>44245</v>
+        <v>44159</v>
       </c>
       <c r="B1340" s="9"/>
       <c r="C1340" s="14" t="s">
@@ -46621,7 +46677,7 @@
         <v>647</v>
       </c>
       <c r="F1340" s="10" t="s">
-        <v>1614</v>
+        <v>1619</v>
       </c>
       <c r="G1340" s="11"/>
       <c r="H1340" s="12"/>
@@ -46630,7 +46686,9 @@
     </row>
     <row r="1341" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1341" s="12"/>
-      <c r="B1341" s="9"/>
+      <c r="B1341" s="12">
+        <v>44309</v>
+      </c>
       <c r="C1341" s="14" t="s">
         <v>13</v>
       </c>
@@ -46641,7 +46699,7 @@
         <v>647</v>
       </c>
       <c r="F1341" s="10" t="s">
-        <v>1585</v>
+        <v>1612</v>
       </c>
       <c r="G1341" s="11"/>
       <c r="H1341" s="12"/>
@@ -46650,20 +46708,20 @@
     </row>
     <row r="1342" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1342" s="12">
-        <v>44176</v>
+        <v>44239</v>
       </c>
       <c r="B1342" s="9"/>
       <c r="C1342" s="14" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D1342" s="10" t="s">
         <v>584</v>
       </c>
       <c r="E1342" s="11" t="s">
-        <v>1355</v>
+        <v>647</v>
       </c>
       <c r="F1342" s="10" t="s">
-        <v>1356</v>
+        <v>1609</v>
       </c>
       <c r="G1342" s="11"/>
       <c r="H1342" s="12"/>
@@ -46672,102 +46730,108 @@
     </row>
     <row r="1343" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1343" s="12"/>
-      <c r="B1343" s="9"/>
-      <c r="C1343" s="14"/>
-      <c r="D1343" s="10"/>
-      <c r="E1343" s="11"/>
-      <c r="F1343" s="10"/>
+      <c r="B1343" s="9">
+        <v>44255</v>
+      </c>
+      <c r="C1343" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1343" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1343" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1343" s="10" t="s">
+        <v>1608</v>
+      </c>
       <c r="G1343" s="11"/>
       <c r="H1343" s="12"/>
       <c r="I1343" s="13"/>
       <c r="J1343" s="13"/>
     </row>
-    <row r="1344" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1344" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1344" s="9"/>
+    <row r="1344" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1344" s="12"/>
+      <c r="B1344" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1344" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1344" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1344" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1344" s="10" t="s">
-        <v>1663</v>
+        <v>1613</v>
       </c>
       <c r="G1344" s="11"/>
       <c r="H1344" s="12"/>
       <c r="I1344" s="13"/>
-      <c r="J1344" s="13" t="s">
-        <v>1686</v>
-      </c>
-    </row>
-    <row r="1345" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1345" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1345" s="9"/>
+      <c r="J1344" s="13"/>
+    </row>
+    <row r="1345" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1345" s="12"/>
+      <c r="B1345" s="12">
+        <v>44309</v>
+      </c>
       <c r="C1345" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1345" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1345" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1345" s="10" t="s">
-        <v>1662</v>
+        <v>1616</v>
       </c>
       <c r="G1345" s="11"/>
       <c r="H1345" s="12"/>
       <c r="I1345" s="13"/>
       <c r="J1345" s="13"/>
     </row>
-    <row r="1346" spans="1:10" ht="84" x14ac:dyDescent="0.2">
-      <c r="A1346" s="12">
-        <v>43864</v>
-      </c>
-      <c r="B1346" s="9"/>
+    <row r="1346" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1346" s="12"/>
+      <c r="B1346" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1346" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1346" s="10" t="s">
-        <v>533</v>
+        <v>584</v>
       </c>
       <c r="E1346" s="11" t="s">
-        <v>1582</v>
+        <v>647</v>
       </c>
       <c r="F1346" s="10" t="s">
-        <v>534</v>
+        <v>1617</v>
       </c>
       <c r="G1346" s="11"/>
       <c r="H1346" s="12"/>
       <c r="I1346" s="13"/>
-      <c r="J1346" s="13" t="s">
-        <v>1709</v>
-      </c>
-    </row>
-    <row r="1347" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1346" s="13"/>
+    </row>
+    <row r="1347" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1347" s="12">
-        <v>44131</v>
+        <v>44245</v>
       </c>
       <c r="B1347" s="9"/>
       <c r="C1347" s="14" t="s">
-        <v>1132</v>
+        <v>13</v>
       </c>
       <c r="D1347" s="10" t="s">
-        <v>89</v>
+        <v>584</v>
       </c>
       <c r="E1347" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1347" s="10" t="s">
-        <v>1165</v>
+        <v>1614</v>
       </c>
       <c r="G1347" s="11"/>
       <c r="H1347" s="12"/>
@@ -46775,21 +46839,19 @@
       <c r="J1347" s="13"/>
     </row>
     <row r="1348" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1348" s="12">
-        <v>44112</v>
-      </c>
+      <c r="A1348" s="12"/>
       <c r="B1348" s="9"/>
       <c r="C1348" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1348" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1348" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1348" s="10" t="s">
-        <v>1098</v>
+        <v>1585</v>
       </c>
       <c r="G1348" s="11"/>
       <c r="H1348" s="12"/>
@@ -46798,20 +46860,20 @@
     </row>
     <row r="1349" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1349" s="12">
-        <v>44088</v>
+        <v>44176</v>
       </c>
       <c r="B1349" s="9"/>
       <c r="C1349" s="14" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D1349" s="10" t="s">
-        <v>906</v>
+        <v>584</v>
       </c>
       <c r="E1349" s="11" t="s">
-        <v>685</v>
+        <v>1355</v>
       </c>
       <c r="F1349" s="10" t="s">
-        <v>1012</v>
+        <v>1356</v>
       </c>
       <c r="G1349" s="11"/>
       <c r="H1349" s="12"/>
@@ -46819,166 +46881,156 @@
       <c r="J1349" s="13"/>
     </row>
     <row r="1350" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1350" s="12">
-        <v>44083</v>
-      </c>
+      <c r="A1350" s="12"/>
       <c r="B1350" s="9"/>
-      <c r="C1350" s="14" t="s">
-        <v>468</v>
-      </c>
-      <c r="D1350" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1350" s="11" t="s">
-        <v>837</v>
-      </c>
-      <c r="F1350" s="10" t="s">
-        <v>989</v>
-      </c>
+      <c r="C1350" s="14"/>
+      <c r="D1350" s="10"/>
+      <c r="E1350" s="11"/>
+      <c r="F1350" s="10"/>
       <c r="G1350" s="11"/>
       <c r="H1350" s="12"/>
       <c r="I1350" s="13"/>
       <c r="J1350" s="13"/>
     </row>
-    <row r="1351" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1351" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1351" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1351" s="9"/>
       <c r="C1351" s="14" t="s">
-        <v>623</v>
+        <v>898</v>
       </c>
       <c r="D1351" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1351" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1351" s="10" t="s">
-        <v>903</v>
+        <v>1663</v>
       </c>
       <c r="G1351" s="11"/>
       <c r="H1351" s="12"/>
       <c r="I1351" s="13"/>
-      <c r="J1351" s="13"/>
-    </row>
-    <row r="1352" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1351" s="13" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1352" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1352" s="9"/>
       <c r="C1352" s="14" t="s">
-        <v>623</v>
+        <v>898</v>
       </c>
       <c r="D1352" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1352" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1352" s="10" t="s">
-        <v>902</v>
+        <v>1662</v>
       </c>
       <c r="G1352" s="11"/>
       <c r="H1352" s="12"/>
       <c r="I1352" s="13"/>
       <c r="J1352" s="13"/>
     </row>
-    <row r="1353" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1353" spans="1:10" ht="84" x14ac:dyDescent="0.2">
       <c r="A1353" s="12">
-        <v>44055</v>
+        <v>43864</v>
       </c>
       <c r="B1353" s="9"/>
       <c r="C1353" s="14" t="s">
-        <v>898</v>
+        <v>19</v>
       </c>
       <c r="D1353" s="10" t="s">
-        <v>494</v>
+        <v>533</v>
       </c>
       <c r="E1353" s="11" t="s">
-        <v>570</v>
+        <v>1582</v>
       </c>
       <c r="F1353" s="10" t="s">
-        <v>900</v>
+        <v>534</v>
       </c>
       <c r="G1353" s="11"/>
       <c r="H1353" s="12"/>
       <c r="I1353" s="13"/>
-      <c r="J1353" s="13"/>
-    </row>
-    <row r="1354" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="J1353" s="13" t="s">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1354" s="12">
-        <v>44055</v>
+        <v>44131</v>
       </c>
       <c r="B1354" s="9"/>
       <c r="C1354" s="14" t="s">
-        <v>898</v>
+        <v>1132</v>
       </c>
       <c r="D1354" s="10" t="s">
-        <v>494</v>
+        <v>89</v>
       </c>
       <c r="E1354" s="11" t="s">
-        <v>570</v>
+        <v>685</v>
       </c>
       <c r="F1354" s="10" t="s">
-        <v>901</v>
+        <v>1165</v>
       </c>
       <c r="G1354" s="11"/>
       <c r="H1354" s="12"/>
       <c r="I1354" s="13"/>
       <c r="J1354" s="13"/>
     </row>
-    <row r="1355" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1355" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1355" s="12">
-        <v>44055</v>
+        <v>44112</v>
       </c>
       <c r="B1355" s="9"/>
       <c r="C1355" s="14" t="s">
-        <v>898</v>
+        <v>623</v>
       </c>
       <c r="D1355" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1355" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1355" s="10" t="s">
-        <v>904</v>
+        <v>1098</v>
       </c>
       <c r="G1355" s="11"/>
       <c r="H1355" s="12"/>
       <c r="I1355" s="13"/>
-      <c r="J1355" s="13" t="s">
-        <v>1592</v>
-      </c>
-    </row>
-    <row r="1356" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1355" s="13"/>
+    </row>
+    <row r="1356" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1356" s="12">
-        <v>44047</v>
+        <v>44088</v>
       </c>
       <c r="B1356" s="9"/>
       <c r="C1356" s="14" t="s">
-        <v>537</v>
+        <v>19</v>
       </c>
       <c r="D1356" s="10" t="s">
-        <v>6</v>
+        <v>906</v>
       </c>
       <c r="E1356" s="11" t="s">
         <v>685</v>
       </c>
       <c r="F1356" s="10" t="s">
-        <v>873</v>
-      </c>
-      <c r="G1356" s="11" t="s">
-        <v>1628</v>
-      </c>
+        <v>1012</v>
+      </c>
+      <c r="G1356" s="11"/>
       <c r="H1356" s="12"/>
       <c r="I1356" s="13"/>
       <c r="J1356" s="13"/>
     </row>
-    <row r="1357" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1357" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1357" s="12">
-        <v>43949</v>
+        <v>44083</v>
       </c>
       <c r="B1357" s="9"/>
       <c r="C1357" s="14" t="s">
@@ -46988,151 +47040,131 @@
         <v>89</v>
       </c>
       <c r="E1357" s="11" t="s">
-        <v>685</v>
+        <v>837</v>
       </c>
       <c r="F1357" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1357" s="11" t="s">
-        <v>1643</v>
-      </c>
+        <v>989</v>
+      </c>
+      <c r="G1357" s="11"/>
       <c r="H1357" s="12"/>
-      <c r="I1357" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1357" s="13"/>
       <c r="J1357" s="13"/>
     </row>
-    <row r="1358" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1358" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1358" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1358" s="9"/>
       <c r="C1358" s="14" t="s">
-        <v>468</v>
+        <v>623</v>
       </c>
       <c r="D1358" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1358" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1358" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1358" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>903</v>
+      </c>
+      <c r="G1358" s="11"/>
       <c r="H1358" s="12"/>
-      <c r="I1358" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1358" s="13" t="s">
-        <v>1571</v>
-      </c>
-    </row>
-    <row r="1359" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1358" s="13"/>
+      <c r="J1358" s="13"/>
+    </row>
+    <row r="1359" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1359" s="12">
-        <v>43838</v>
+        <v>44055</v>
       </c>
       <c r="B1359" s="9"/>
       <c r="C1359" s="14" t="s">
-        <v>103</v>
+        <v>623</v>
       </c>
       <c r="D1359" s="10" t="s">
-        <v>460</v>
+        <v>6</v>
       </c>
       <c r="E1359" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1359" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G1359" s="11" t="s">
-        <v>1644</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="G1359" s="11"/>
       <c r="H1359" s="12"/>
       <c r="I1359" s="13"/>
-      <c r="J1359" s="13" t="s">
-        <v>1536</v>
-      </c>
+      <c r="J1359" s="13"/>
     </row>
     <row r="1360" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1360" s="12">
-        <v>43816</v>
+        <v>44055</v>
       </c>
       <c r="B1360" s="9"/>
       <c r="C1360" s="14" t="s">
-        <v>475</v>
+        <v>898</v>
       </c>
       <c r="D1360" s="10" t="s">
-        <v>38</v>
+        <v>494</v>
       </c>
       <c r="E1360" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1360" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="G1360" s="11" t="s">
-        <v>1636</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="G1360" s="11"/>
       <c r="H1360" s="12"/>
       <c r="I1360" s="13"/>
-      <c r="J1360" s="13" t="s">
-        <v>1572</v>
-      </c>
-    </row>
-    <row r="1361" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1360" s="13"/>
+    </row>
+    <row r="1361" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A1361" s="12">
-        <v>43762</v>
+        <v>44055</v>
       </c>
       <c r="B1361" s="9"/>
       <c r="C1361" s="14" t="s">
-        <v>446</v>
+        <v>898</v>
       </c>
       <c r="D1361" s="10" t="s">
-        <v>17</v>
+        <v>494</v>
       </c>
       <c r="E1361" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1361" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G1361" s="11" t="s">
-        <v>1633</v>
-      </c>
+        <v>901</v>
+      </c>
+      <c r="G1361" s="11"/>
       <c r="H1361" s="12"/>
       <c r="I1361" s="13"/>
       <c r="J1361" s="13"/>
     </row>
-    <row r="1362" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1362" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1362" s="12">
-        <v>44222</v>
+        <v>44055</v>
       </c>
       <c r="B1362" s="9"/>
       <c r="C1362" s="14" t="s">
-        <v>1497</v>
+        <v>898</v>
       </c>
       <c r="D1362" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1362" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1362" s="10" t="s">
-        <v>1496</v>
-      </c>
-      <c r="G1362" s="11" t="s">
-        <v>309</v>
-      </c>
+        <v>904</v>
+      </c>
+      <c r="G1362" s="11"/>
       <c r="H1362" s="12"/>
       <c r="I1362" s="13"/>
-      <c r="J1362" s="13"/>
-    </row>
-    <row r="1363" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="J1362" s="13" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1363" s="12">
-        <v>44266</v>
+        <v>44047</v>
       </c>
       <c r="B1363" s="9"/>
       <c r="C1363" s="14" t="s">
@@ -47142,133 +47174,311 @@
         <v>6</v>
       </c>
       <c r="E1363" s="11" t="s">
-        <v>570</v>
+        <v>685</v>
       </c>
       <c r="F1363" s="10" t="s">
-        <v>1717</v>
-      </c>
-      <c r="G1363" s="11"/>
+        <v>873</v>
+      </c>
+      <c r="G1363" s="11" t="s">
+        <v>1628</v>
+      </c>
       <c r="H1363" s="12"/>
       <c r="I1363" s="13"/>
-      <c r="J1363" s="13" t="s">
-        <v>1718</v>
-      </c>
-    </row>
-    <row r="1364" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1363" s="13"/>
+    </row>
+    <row r="1364" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A1364" s="12">
-        <v>44279</v>
+        <v>43949</v>
       </c>
       <c r="B1364" s="9"/>
       <c r="C1364" s="14" t="s">
-        <v>1390</v>
+        <v>468</v>
       </c>
       <c r="D1364" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E1364" s="11" t="s">
-        <v>1582</v>
+        <v>685</v>
       </c>
       <c r="F1364" s="10" t="s">
-        <v>1734</v>
-      </c>
-      <c r="G1364" s="11"/>
+        <v>686</v>
+      </c>
+      <c r="G1364" s="11" t="s">
+        <v>1643</v>
+      </c>
       <c r="H1364" s="12"/>
-      <c r="I1364" s="13"/>
+      <c r="I1364" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1364" s="13"/>
     </row>
-    <row r="1365" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="1365" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A1365" s="12">
-        <v>44286</v>
+        <v>43949</v>
       </c>
       <c r="B1365" s="9"/>
       <c r="C1365" s="14" t="s">
-        <v>288</v>
+        <v>468</v>
       </c>
       <c r="D1365" s="10" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="E1365" s="11" t="s">
-        <v>1582</v>
+        <v>685</v>
       </c>
       <c r="F1365" s="10" t="s">
-        <v>1842</v>
-      </c>
-      <c r="G1365" s="11"/>
+        <v>705</v>
+      </c>
+      <c r="G1365" s="11" t="s">
+        <v>687</v>
+      </c>
       <c r="H1365" s="12"/>
-      <c r="I1365" s="13"/>
-      <c r="J1365" s="13"/>
-    </row>
-    <row r="1366" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1366" s="12"/>
+      <c r="I1365" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1365" s="13" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1366" s="12">
+        <v>43838</v>
+      </c>
       <c r="B1366" s="9"/>
-      <c r="C1366" s="14"/>
-      <c r="D1366" s="10"/>
-      <c r="E1366" s="11"/>
-      <c r="F1366" s="10"/>
-      <c r="G1366" s="11"/>
+      <c r="C1366" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1366" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1366" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1366" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G1366" s="11" t="s">
+        <v>1644</v>
+      </c>
       <c r="H1366" s="12"/>
       <c r="I1366" s="13"/>
-      <c r="J1366" s="13"/>
+      <c r="J1366" s="13" t="s">
+        <v>1536</v>
+      </c>
     </row>
     <row r="1367" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1367" s="12"/>
+      <c r="A1367" s="12">
+        <v>43816</v>
+      </c>
       <c r="B1367" s="9"/>
-      <c r="C1367" s="14"/>
-      <c r="D1367" s="10"/>
-      <c r="E1367" s="11"/>
-      <c r="F1367" s="10"/>
-      <c r="G1367" s="11"/>
+      <c r="C1367" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1367" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1367" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1367" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G1367" s="11" t="s">
+        <v>1636</v>
+      </c>
       <c r="H1367" s="12"/>
       <c r="I1367" s="13"/>
-      <c r="J1367" s="13"/>
-    </row>
-    <row r="1368" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1368" s="12"/>
+      <c r="J1367" s="13" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1368" s="12">
+        <v>43762</v>
+      </c>
       <c r="B1368" s="9"/>
-      <c r="C1368" s="14"/>
-      <c r="D1368" s="10"/>
-      <c r="E1368" s="11"/>
-      <c r="F1368" s="10"/>
-      <c r="G1368" s="11"/>
+      <c r="C1368" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1368" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1368" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1368" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1368" s="11" t="s">
+        <v>1633</v>
+      </c>
       <c r="H1368" s="12"/>
       <c r="I1368" s="13"/>
       <c r="J1368" s="13"/>
     </row>
     <row r="1369" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1369" s="12"/>
+      <c r="A1369" s="12">
+        <v>44222</v>
+      </c>
       <c r="B1369" s="9"/>
-      <c r="C1369" s="14"/>
-      <c r="D1369" s="10"/>
-      <c r="E1369" s="11"/>
-      <c r="F1369" s="10"/>
-      <c r="G1369" s="11"/>
+      <c r="C1369" s="14" t="s">
+        <v>1497</v>
+      </c>
+      <c r="D1369" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1369" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1369" s="10" t="s">
+        <v>1496</v>
+      </c>
+      <c r="G1369" s="11" t="s">
+        <v>309</v>
+      </c>
       <c r="H1369" s="12"/>
       <c r="I1369" s="13"/>
       <c r="J1369" s="13"/>
     </row>
-    <row r="1370" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1370" s="12"/>
+    <row r="1370" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1370" s="12">
+        <v>44266</v>
+      </c>
       <c r="B1370" s="9"/>
-      <c r="C1370" s="14"/>
-      <c r="D1370" s="10"/>
-      <c r="E1370" s="11"/>
-      <c r="F1370" s="10"/>
+      <c r="C1370" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1370" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1370" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1370" s="10" t="s">
+        <v>1717</v>
+      </c>
       <c r="G1370" s="11"/>
       <c r="H1370" s="12"/>
       <c r="I1370" s="13"/>
-      <c r="J1370" s="13"/>
+      <c r="J1370" s="13" t="s">
+        <v>1718</v>
+      </c>
     </row>
     <row r="1371" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1371" s="12"/>
+      <c r="A1371" s="12">
+        <v>44279</v>
+      </c>
       <c r="B1371" s="9"/>
-      <c r="C1371" s="14"/>
-      <c r="D1371" s="10"/>
-      <c r="E1371" s="11"/>
-      <c r="F1371" s="10"/>
+      <c r="C1371" s="14" t="s">
+        <v>1390</v>
+      </c>
+      <c r="D1371" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1371" s="11" t="s">
+        <v>1582</v>
+      </c>
+      <c r="F1371" s="10" t="s">
+        <v>1734</v>
+      </c>
       <c r="G1371" s="11"/>
       <c r="H1371" s="12"/>
       <c r="I1371" s="13"/>
       <c r="J1371" s="13"/>
+    </row>
+    <row r="1372" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1372" s="12">
+        <v>44286</v>
+      </c>
+      <c r="B1372" s="9"/>
+      <c r="C1372" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1372" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1372" s="11" t="s">
+        <v>1582</v>
+      </c>
+      <c r="F1372" s="10" t="s">
+        <v>1842</v>
+      </c>
+      <c r="G1372" s="11"/>
+      <c r="H1372" s="12"/>
+      <c r="I1372" s="13"/>
+      <c r="J1372" s="13"/>
+    </row>
+    <row r="1373" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1373" s="12"/>
+      <c r="B1373" s="9"/>
+      <c r="C1373" s="14"/>
+      <c r="D1373" s="10"/>
+      <c r="E1373" s="11"/>
+      <c r="F1373" s="10"/>
+      <c r="G1373" s="11"/>
+      <c r="H1373" s="12"/>
+      <c r="I1373" s="13"/>
+      <c r="J1373" s="13"/>
+    </row>
+    <row r="1374" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1374" s="12"/>
+      <c r="B1374" s="9"/>
+      <c r="C1374" s="14"/>
+      <c r="D1374" s="10"/>
+      <c r="E1374" s="11"/>
+      <c r="F1374" s="10"/>
+      <c r="G1374" s="11"/>
+      <c r="H1374" s="12"/>
+      <c r="I1374" s="13"/>
+      <c r="J1374" s="13"/>
+    </row>
+    <row r="1375" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1375" s="12"/>
+      <c r="B1375" s="9"/>
+      <c r="C1375" s="14"/>
+      <c r="D1375" s="10"/>
+      <c r="E1375" s="11"/>
+      <c r="F1375" s="10"/>
+      <c r="G1375" s="11"/>
+      <c r="H1375" s="12"/>
+      <c r="I1375" s="13"/>
+      <c r="J1375" s="13"/>
+    </row>
+    <row r="1376" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1376" s="12"/>
+      <c r="B1376" s="9"/>
+      <c r="C1376" s="14"/>
+      <c r="D1376" s="10"/>
+      <c r="E1376" s="11"/>
+      <c r="F1376" s="10"/>
+      <c r="G1376" s="11"/>
+      <c r="H1376" s="12"/>
+      <c r="I1376" s="13"/>
+      <c r="J1376" s="13"/>
+    </row>
+    <row r="1377" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1377" s="12"/>
+      <c r="B1377" s="9"/>
+      <c r="C1377" s="14"/>
+      <c r="D1377" s="10"/>
+      <c r="E1377" s="11"/>
+      <c r="F1377" s="10"/>
+      <c r="G1377" s="11"/>
+      <c r="H1377" s="12"/>
+      <c r="I1377" s="13"/>
+      <c r="J1377" s="13"/>
+    </row>
+    <row r="1378" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1378" s="12"/>
+      <c r="B1378" s="9"/>
+      <c r="C1378" s="14"/>
+      <c r="D1378" s="10"/>
+      <c r="E1378" s="11"/>
+      <c r="F1378" s="10"/>
+      <c r="G1378" s="11"/>
+      <c r="H1378" s="12"/>
+      <c r="I1378" s="13"/>
+      <c r="J1378" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1172" xr:uid="{00000000-0009-0000-0000-000000000000}">
@@ -47276,8 +47486,8 @@
       <sortCondition ref="A1:A1023"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1330:F1340">
-    <sortCondition ref="F1330:F1340"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1337:F1347">
+    <sortCondition ref="F1337:F1347"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -47293,8 +47503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE13D4C-C1F0-4B00-8A02-71F13D132F72}">
   <dimension ref="B1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47776,7 +47986,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="B27" s="37" t="s">
         <v>1803</v>
       </c>
       <c r="C27" t="s">
@@ -47787,6 +47997,9 @@
       </c>
       <c r="E27" t="s">
         <v>1749</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1779</v>
       </c>
       <c r="G27" t="s">
         <v>1761</v>
@@ -47810,7 +48023,7 @@
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="B29" s="37" t="s">
         <v>1775</v>
       </c>
       <c r="C29" t="s">
@@ -47821,6 +48034,9 @@
       </c>
       <c r="E29" t="s">
         <v>1749</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1779</v>
       </c>
       <c r="G29" t="s">
         <v>1754</v>

</xml_diff>

<commit_message>
Alteração de data fiscal
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3B5243-C416-4D20-9258-5BCBAE3F8253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42948D7B-C0A9-4052-95EE-B7992B5F8CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9683" uniqueCount="2001">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9726" uniqueCount="2009">
   <si>
     <t>Responsável</t>
   </si>
@@ -6370,6 +6370,30 @@
   </si>
   <si>
     <t>Problemas nos relatorios de mapa de inss retido e outros com NFs duplicadas</t>
+  </si>
+  <si>
+    <t>Marcelo Soares</t>
+  </si>
+  <si>
+    <t>Solicita aumento do campo de endereço no ped de compras</t>
+  </si>
+  <si>
+    <t>C1_XXENDEN (de 40 para 60)</t>
+  </si>
+  <si>
+    <t>Pedido 047733 - Departamento Hidroviário com divergência de 0,01 com a medição</t>
+  </si>
+  <si>
+    <t>Problemas ao emitir a NF 3010 (a NF já existia no sistema)</t>
+  </si>
+  <si>
+    <t>Problemas com o lote enviado a Barueri devido a Ediane ter enviado a NF 3010 por engano</t>
+  </si>
+  <si>
+    <t>Fechamento das datas fiscais de todas as empresas</t>
+  </si>
+  <si>
+    <t>Revisar o contrato 302000483 para deixar apenas 1 item</t>
   </si>
 </sst>
 </file>
@@ -7135,11 +7159,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1410"/>
+  <dimension ref="A1:J1415"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1350" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1363" sqref="A1363"/>
+      <pane ySplit="1" topLeftCell="A1356" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1369" sqref="A1369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -47705,122 +47729,194 @@
       <c r="J1363" s="13"/>
     </row>
     <row r="1364" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1364" s="12"/>
-      <c r="B1364" s="12"/>
-      <c r="C1364" s="14"/>
-      <c r="D1364" s="10"/>
-      <c r="E1364" s="11"/>
-      <c r="F1364" s="10"/>
-      <c r="G1364" s="11"/>
-      <c r="H1364" s="12"/>
-      <c r="I1364" s="13"/>
-      <c r="J1364" s="13"/>
+      <c r="A1364" s="12">
+        <v>44347</v>
+      </c>
+      <c r="B1364" s="12">
+        <v>44351</v>
+      </c>
+      <c r="C1364" s="14" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D1364" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1364" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1364" s="10" t="s">
+        <v>2002</v>
+      </c>
+      <c r="G1364" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1364" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1364" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1364" s="13" t="s">
+        <v>2003</v>
+      </c>
     </row>
     <row r="1365" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1365" s="12"/>
-      <c r="B1365" s="12"/>
-      <c r="C1365" s="14"/>
-      <c r="D1365" s="10"/>
-      <c r="E1365" s="11"/>
-      <c r="F1365" s="10"/>
-      <c r="G1365" s="11"/>
-      <c r="H1365" s="12"/>
-      <c r="I1365" s="13"/>
+      <c r="A1365" s="12">
+        <v>44354</v>
+      </c>
+      <c r="B1365" s="12">
+        <v>44354</v>
+      </c>
+      <c r="C1365" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1365" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1365" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1365" s="10" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G1365" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1365" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1365" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1365" s="13"/>
     </row>
     <row r="1366" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1366" s="12"/>
-      <c r="B1366" s="9"/>
-      <c r="C1366" s="14"/>
-      <c r="D1366" s="10"/>
-      <c r="E1366" s="11"/>
-      <c r="F1366" s="10"/>
-      <c r="G1366" s="11"/>
-      <c r="H1366" s="12"/>
-      <c r="I1366" s="13"/>
+      <c r="A1366" s="12">
+        <v>44354</v>
+      </c>
+      <c r="B1366" s="12">
+        <v>44354</v>
+      </c>
+      <c r="C1366" s="14" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D1366" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1366" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1366" s="10" t="s">
+        <v>2005</v>
+      </c>
+      <c r="G1366" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1366" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1366" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1366" s="13"/>
     </row>
-    <row r="1367" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1367" s="1" t="s">
-        <v>1480</v>
-      </c>
-      <c r="B1367" s="2" t="s">
-        <v>1481</v>
-      </c>
-      <c r="C1367" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1367" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1367" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1367" s="4" t="s">
-        <v>1582</v>
-      </c>
-      <c r="G1367" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1367" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1367" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1367" s="36"/>
+    <row r="1367" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1367" s="12">
+        <v>44354</v>
+      </c>
+      <c r="B1367" s="12">
+        <v>44354</v>
+      </c>
+      <c r="C1367" s="14" t="s">
+        <v>559</v>
+      </c>
+      <c r="D1367" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1367" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1367" s="10" t="s">
+        <v>2006</v>
+      </c>
+      <c r="G1367" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1367" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1367" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1367" s="13"/>
     </row>
     <row r="1368" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1368" s="12"/>
-      <c r="B1368" s="9"/>
-      <c r="C1368" s="14"/>
-      <c r="D1368" s="10"/>
-      <c r="E1368" s="11"/>
-      <c r="F1368" s="10"/>
-      <c r="G1368" s="11"/>
-      <c r="H1368" s="12"/>
-      <c r="I1368" s="13"/>
+      <c r="A1368" s="12">
+        <v>44354</v>
+      </c>
+      <c r="B1368" s="12">
+        <v>44354</v>
+      </c>
+      <c r="C1368" s="14" t="s">
+        <v>1995</v>
+      </c>
+      <c r="D1368" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1368" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1368" s="10" t="s">
+        <v>2007</v>
+      </c>
+      <c r="G1368" s="11" t="s">
+        <v>1649</v>
+      </c>
+      <c r="H1368" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1368" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1368" s="13"/>
     </row>
     <row r="1369" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1369" s="12"/>
-      <c r="B1369" s="9">
-        <v>44255</v>
+      <c r="A1369" s="12">
+        <v>44355</v>
+      </c>
+      <c r="B1369" s="12">
+        <v>44355</v>
       </c>
       <c r="C1369" s="14" t="s">
-        <v>13</v>
+        <v>387</v>
       </c>
       <c r="D1369" s="10" t="s">
-        <v>584</v>
+        <v>494</v>
       </c>
       <c r="E1369" s="11" t="s">
-        <v>647</v>
+        <v>620</v>
       </c>
       <c r="F1369" s="10" t="s">
-        <v>1617</v>
-      </c>
-      <c r="G1369" s="11"/>
-      <c r="H1369" s="12"/>
-      <c r="I1369" s="13"/>
+        <v>2008</v>
+      </c>
+      <c r="G1369" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1369" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1369" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1369" s="13"/>
     </row>
     <row r="1370" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1370" s="12"/>
-      <c r="B1370" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1370" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1370" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1370" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1370" s="10" t="s">
-        <v>1609</v>
-      </c>
+      <c r="B1370" s="12"/>
+      <c r="C1370" s="14"/>
+      <c r="D1370" s="10"/>
+      <c r="E1370" s="11"/>
+      <c r="F1370" s="10"/>
       <c r="G1370" s="11"/>
       <c r="H1370" s="12"/>
       <c r="I1370" s="13"/>
@@ -47828,65 +47924,53 @@
     </row>
     <row r="1371" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1371" s="12"/>
-      <c r="B1371" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1371" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1371" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1371" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1371" s="10" t="s">
-        <v>1614</v>
-      </c>
+      <c r="B1371" s="9"/>
+      <c r="C1371" s="14"/>
+      <c r="D1371" s="10"/>
+      <c r="E1371" s="11"/>
+      <c r="F1371" s="10"/>
       <c r="G1371" s="11"/>
       <c r="H1371" s="12"/>
       <c r="I1371" s="13"/>
       <c r="J1371" s="13"/>
     </row>
     <row r="1372" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1372" s="12"/>
-      <c r="B1372" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1372" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1372" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1372" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1372" s="10" t="s">
-        <v>1610</v>
-      </c>
-      <c r="G1372" s="11"/>
-      <c r="H1372" s="12"/>
-      <c r="I1372" s="13"/>
-      <c r="J1372" s="13"/>
+      <c r="A1372" s="1" t="s">
+        <v>1480</v>
+      </c>
+      <c r="B1372" s="2" t="s">
+        <v>1481</v>
+      </c>
+      <c r="C1372" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1372" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1372" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1372" s="4" t="s">
+        <v>1582</v>
+      </c>
+      <c r="G1372" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1372" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1372" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1372" s="36"/>
     </row>
     <row r="1373" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1373" s="12">
-        <v>44159</v>
-      </c>
+      <c r="A1373" s="12"/>
       <c r="B1373" s="9"/>
-      <c r="C1373" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1373" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1373" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1373" s="10" t="s">
-        <v>1618</v>
-      </c>
+      <c r="C1373" s="14"/>
+      <c r="D1373" s="10"/>
+      <c r="E1373" s="11"/>
+      <c r="F1373" s="10"/>
       <c r="G1373" s="11"/>
       <c r="H1373" s="12"/>
       <c r="I1373" s="13"/>
@@ -47894,8 +47978,8 @@
     </row>
     <row r="1374" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1374" s="12"/>
-      <c r="B1374" s="12">
-        <v>44309</v>
+      <c r="B1374" s="9">
+        <v>44255</v>
       </c>
       <c r="C1374" s="14" t="s">
         <v>13</v>
@@ -47907,7 +47991,7 @@
         <v>647</v>
       </c>
       <c r="F1374" s="10" t="s">
-        <v>1611</v>
+        <v>1617</v>
       </c>
       <c r="G1374" s="11"/>
       <c r="H1374" s="12"/>
@@ -47915,10 +47999,10 @@
       <c r="J1374" s="13"/>
     </row>
     <row r="1375" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1375" s="12">
-        <v>44239</v>
-      </c>
-      <c r="B1375" s="9"/>
+      <c r="A1375" s="12"/>
+      <c r="B1375" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1375" s="14" t="s">
         <v>13</v>
       </c>
@@ -47929,7 +48013,7 @@
         <v>647</v>
       </c>
       <c r="F1375" s="10" t="s">
-        <v>1608</v>
+        <v>1609</v>
       </c>
       <c r="G1375" s="11"/>
       <c r="H1375" s="12"/>
@@ -47951,7 +48035,7 @@
         <v>647</v>
       </c>
       <c r="F1376" s="10" t="s">
-        <v>1607</v>
+        <v>1614</v>
       </c>
       <c r="G1376" s="11"/>
       <c r="H1376" s="12"/>
@@ -47973,7 +48057,7 @@
         <v>647</v>
       </c>
       <c r="F1377" s="10" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="G1377" s="11"/>
       <c r="H1377" s="12"/>
@@ -47981,10 +48065,10 @@
       <c r="J1377" s="13"/>
     </row>
     <row r="1378" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1378" s="12"/>
-      <c r="B1378" s="12">
-        <v>44309</v>
-      </c>
+      <c r="A1378" s="12">
+        <v>44159</v>
+      </c>
+      <c r="B1378" s="9"/>
       <c r="C1378" s="14" t="s">
         <v>13</v>
       </c>
@@ -47995,7 +48079,7 @@
         <v>647</v>
       </c>
       <c r="F1378" s="10" t="s">
-        <v>1615</v>
+        <v>1618</v>
       </c>
       <c r="G1378" s="11"/>
       <c r="H1378" s="12"/>
@@ -48004,8 +48088,8 @@
     </row>
     <row r="1379" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1379" s="12"/>
-      <c r="B1379" s="9">
-        <v>44235</v>
+      <c r="B1379" s="12">
+        <v>44309</v>
       </c>
       <c r="C1379" s="14" t="s">
         <v>13</v>
@@ -48017,7 +48101,7 @@
         <v>647</v>
       </c>
       <c r="F1379" s="10" t="s">
-        <v>1616</v>
+        <v>1611</v>
       </c>
       <c r="G1379" s="11"/>
       <c r="H1379" s="12"/>
@@ -48026,7 +48110,7 @@
     </row>
     <row r="1380" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1380" s="12">
-        <v>44245</v>
+        <v>44239</v>
       </c>
       <c r="B1380" s="9"/>
       <c r="C1380" s="14" t="s">
@@ -48039,7 +48123,7 @@
         <v>647</v>
       </c>
       <c r="F1380" s="10" t="s">
-        <v>1613</v>
+        <v>1608</v>
       </c>
       <c r="G1380" s="11"/>
       <c r="H1380" s="12"/>
@@ -48048,7 +48132,9 @@
     </row>
     <row r="1381" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1381" s="12"/>
-      <c r="B1381" s="9"/>
+      <c r="B1381" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1381" s="14" t="s">
         <v>13</v>
       </c>
@@ -48059,7 +48145,7 @@
         <v>647</v>
       </c>
       <c r="F1381" s="10" t="s">
-        <v>1584</v>
+        <v>1607</v>
       </c>
       <c r="G1381" s="11"/>
       <c r="H1381" s="12"/>
@@ -48067,21 +48153,21 @@
       <c r="J1381" s="13"/>
     </row>
     <row r="1382" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1382" s="12">
-        <v>44176</v>
-      </c>
-      <c r="B1382" s="9"/>
+      <c r="A1382" s="12"/>
+      <c r="B1382" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1382" s="14" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D1382" s="10" t="s">
         <v>584</v>
       </c>
       <c r="E1382" s="11" t="s">
-        <v>1354</v>
+        <v>647</v>
       </c>
       <c r="F1382" s="10" t="s">
-        <v>1355</v>
+        <v>1612</v>
       </c>
       <c r="G1382" s="11"/>
       <c r="H1382" s="12"/>
@@ -48090,102 +48176,106 @@
     </row>
     <row r="1383" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1383" s="12"/>
-      <c r="B1383" s="9"/>
-      <c r="C1383" s="14"/>
-      <c r="D1383" s="10"/>
-      <c r="E1383" s="11"/>
-      <c r="F1383" s="10"/>
+      <c r="B1383" s="12">
+        <v>44309</v>
+      </c>
+      <c r="C1383" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1383" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1383" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1383" s="10" t="s">
+        <v>1615</v>
+      </c>
       <c r="G1383" s="11"/>
       <c r="H1383" s="12"/>
       <c r="I1383" s="13"/>
       <c r="J1383" s="13"/>
     </row>
-    <row r="1384" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1384" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1384" s="9"/>
+    <row r="1384" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1384" s="12"/>
+      <c r="B1384" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1384" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1384" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1384" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1384" s="10" t="s">
-        <v>1662</v>
+        <v>1616</v>
       </c>
       <c r="G1384" s="11"/>
       <c r="H1384" s="12"/>
       <c r="I1384" s="13"/>
-      <c r="J1384" s="13" t="s">
-        <v>1685</v>
-      </c>
-    </row>
-    <row r="1385" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1384" s="13"/>
+    </row>
+    <row r="1385" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1385" s="12">
-        <v>44252</v>
+        <v>44245</v>
       </c>
       <c r="B1385" s="9"/>
       <c r="C1385" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1385" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1385" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1385" s="10" t="s">
-        <v>1661</v>
+        <v>1613</v>
       </c>
       <c r="G1385" s="11"/>
       <c r="H1385" s="12"/>
       <c r="I1385" s="13"/>
       <c r="J1385" s="13"/>
     </row>
-    <row r="1386" spans="1:10" ht="84" x14ac:dyDescent="0.2">
-      <c r="A1386" s="12">
-        <v>43864</v>
-      </c>
+    <row r="1386" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1386" s="12"/>
       <c r="B1386" s="9"/>
       <c r="C1386" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1386" s="10" t="s">
-        <v>533</v>
+        <v>584</v>
       </c>
       <c r="E1386" s="11" t="s">
-        <v>1581</v>
+        <v>647</v>
       </c>
       <c r="F1386" s="10" t="s">
-        <v>534</v>
+        <v>1584</v>
       </c>
       <c r="G1386" s="11"/>
       <c r="H1386" s="12"/>
       <c r="I1386" s="13"/>
-      <c r="J1386" s="13" t="s">
-        <v>1708</v>
-      </c>
-    </row>
-    <row r="1387" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1386" s="13"/>
+    </row>
+    <row r="1387" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1387" s="12">
-        <v>44131</v>
+        <v>44176</v>
       </c>
       <c r="B1387" s="9"/>
       <c r="C1387" s="14" t="s">
-        <v>1131</v>
+        <v>8</v>
       </c>
       <c r="D1387" s="10" t="s">
-        <v>89</v>
+        <v>584</v>
       </c>
       <c r="E1387" s="11" t="s">
-        <v>685</v>
+        <v>1354</v>
       </c>
       <c r="F1387" s="10" t="s">
-        <v>1164</v>
+        <v>1355</v>
       </c>
       <c r="G1387" s="11"/>
       <c r="H1387" s="12"/>
@@ -48193,462 +48283,506 @@
       <c r="J1387" s="13"/>
     </row>
     <row r="1388" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1388" s="12">
-        <v>44112</v>
-      </c>
+      <c r="A1388" s="12"/>
       <c r="B1388" s="9"/>
-      <c r="C1388" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="D1388" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1388" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1388" s="10" t="s">
-        <v>1097</v>
-      </c>
+      <c r="C1388" s="14"/>
+      <c r="D1388" s="10"/>
+      <c r="E1388" s="11"/>
+      <c r="F1388" s="10"/>
       <c r="G1388" s="11"/>
       <c r="H1388" s="12"/>
       <c r="I1388" s="13"/>
       <c r="J1388" s="13"/>
     </row>
-    <row r="1389" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1389" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1389" s="12">
-        <v>44088</v>
+        <v>44252</v>
       </c>
       <c r="B1389" s="9"/>
       <c r="C1389" s="14" t="s">
-        <v>19</v>
+        <v>898</v>
       </c>
       <c r="D1389" s="10" t="s">
-        <v>906</v>
+        <v>494</v>
       </c>
       <c r="E1389" s="11" t="s">
-        <v>685</v>
+        <v>759</v>
       </c>
       <c r="F1389" s="10" t="s">
-        <v>1011</v>
+        <v>1662</v>
       </c>
       <c r="G1389" s="11"/>
       <c r="H1389" s="12"/>
       <c r="I1389" s="13"/>
-      <c r="J1389" s="13"/>
-    </row>
-    <row r="1390" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1389" s="13" t="s">
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1390" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1390" s="9"/>
       <c r="C1390" s="14" t="s">
-        <v>623</v>
+        <v>898</v>
       </c>
       <c r="D1390" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1390" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1390" s="10" t="s">
-        <v>903</v>
+        <v>1661</v>
       </c>
       <c r="G1390" s="11"/>
       <c r="H1390" s="12"/>
       <c r="I1390" s="13"/>
       <c r="J1390" s="13"/>
     </row>
-    <row r="1391" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1391" spans="1:10" ht="84" x14ac:dyDescent="0.2">
       <c r="A1391" s="12">
-        <v>44055</v>
+        <v>43864</v>
       </c>
       <c r="B1391" s="9"/>
       <c r="C1391" s="14" t="s">
-        <v>623</v>
+        <v>19</v>
       </c>
       <c r="D1391" s="10" t="s">
-        <v>6</v>
+        <v>533</v>
       </c>
       <c r="E1391" s="11" t="s">
-        <v>570</v>
+        <v>1581</v>
       </c>
       <c r="F1391" s="10" t="s">
-        <v>902</v>
+        <v>534</v>
       </c>
       <c r="G1391" s="11"/>
       <c r="H1391" s="12"/>
       <c r="I1391" s="13"/>
-      <c r="J1391" s="13"/>
-    </row>
-    <row r="1392" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1391" s="13" t="s">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1392" s="12">
-        <v>44055</v>
+        <v>44131</v>
       </c>
       <c r="B1392" s="9"/>
       <c r="C1392" s="14" t="s">
-        <v>898</v>
+        <v>1131</v>
       </c>
       <c r="D1392" s="10" t="s">
-        <v>494</v>
+        <v>89</v>
       </c>
       <c r="E1392" s="11" t="s">
-        <v>570</v>
+        <v>685</v>
       </c>
       <c r="F1392" s="10" t="s">
-        <v>900</v>
+        <v>1164</v>
       </c>
       <c r="G1392" s="11"/>
       <c r="H1392" s="12"/>
       <c r="I1392" s="13"/>
       <c r="J1392" s="13"/>
     </row>
-    <row r="1393" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="1393" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1393" s="12">
-        <v>44055</v>
+        <v>44112</v>
       </c>
       <c r="B1393" s="9"/>
       <c r="C1393" s="14" t="s">
-        <v>898</v>
+        <v>623</v>
       </c>
       <c r="D1393" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1393" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1393" s="10" t="s">
-        <v>901</v>
+        <v>1097</v>
       </c>
       <c r="G1393" s="11"/>
       <c r="H1393" s="12"/>
       <c r="I1393" s="13"/>
       <c r="J1393" s="13"/>
     </row>
-    <row r="1394" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1394" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1394" s="12">
-        <v>44055</v>
+        <v>44088</v>
       </c>
       <c r="B1394" s="9"/>
       <c r="C1394" s="14" t="s">
-        <v>898</v>
+        <v>19</v>
       </c>
       <c r="D1394" s="10" t="s">
-        <v>494</v>
+        <v>906</v>
       </c>
       <c r="E1394" s="11" t="s">
-        <v>570</v>
+        <v>685</v>
       </c>
       <c r="F1394" s="10" t="s">
-        <v>904</v>
+        <v>1011</v>
       </c>
       <c r="G1394" s="11"/>
       <c r="H1394" s="12"/>
       <c r="I1394" s="13"/>
-      <c r="J1394" s="13" t="s">
-        <v>1591</v>
-      </c>
-    </row>
-    <row r="1395" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1394" s="13"/>
+    </row>
+    <row r="1395" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1395" s="12">
-        <v>44047</v>
+        <v>44055</v>
       </c>
       <c r="B1395" s="9"/>
       <c r="C1395" s="14" t="s">
-        <v>537</v>
+        <v>623</v>
       </c>
       <c r="D1395" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E1395" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1395" s="10" t="s">
-        <v>873</v>
-      </c>
-      <c r="G1395" s="11" t="s">
-        <v>1627</v>
-      </c>
+        <v>903</v>
+      </c>
+      <c r="G1395" s="11"/>
       <c r="H1395" s="12"/>
       <c r="I1395" s="13"/>
       <c r="J1395" s="13"/>
     </row>
-    <row r="1396" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1396" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1396" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1396" s="9"/>
       <c r="C1396" s="14" t="s">
-        <v>468</v>
+        <v>623</v>
       </c>
       <c r="D1396" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1396" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1396" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1396" s="11" t="s">
-        <v>1642</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="G1396" s="11"/>
       <c r="H1396" s="12"/>
-      <c r="I1396" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1396" s="13"/>
       <c r="J1396" s="13"/>
     </row>
-    <row r="1397" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1397" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1397" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1397" s="9"/>
       <c r="C1397" s="14" t="s">
-        <v>468</v>
+        <v>898</v>
       </c>
       <c r="D1397" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1397" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1397" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1397" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="G1397" s="11"/>
       <c r="H1397" s="12"/>
-      <c r="I1397" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1397" s="13" t="s">
-        <v>1570</v>
-      </c>
-    </row>
-    <row r="1398" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1397" s="13"/>
+      <c r="J1397" s="13"/>
+    </row>
+    <row r="1398" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A1398" s="12">
-        <v>43838</v>
+        <v>44055</v>
       </c>
       <c r="B1398" s="9"/>
       <c r="C1398" s="14" t="s">
-        <v>103</v>
+        <v>898</v>
       </c>
       <c r="D1398" s="10" t="s">
-        <v>460</v>
+        <v>494</v>
       </c>
       <c r="E1398" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1398" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G1398" s="11" t="s">
-        <v>1643</v>
-      </c>
+        <v>901</v>
+      </c>
+      <c r="G1398" s="11"/>
       <c r="H1398" s="12"/>
       <c r="I1398" s="13"/>
-      <c r="J1398" s="13" t="s">
-        <v>1535</v>
-      </c>
-    </row>
-    <row r="1399" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1398" s="13"/>
+    </row>
+    <row r="1399" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1399" s="12">
-        <v>43816</v>
+        <v>44055</v>
       </c>
       <c r="B1399" s="9"/>
       <c r="C1399" s="14" t="s">
-        <v>475</v>
+        <v>898</v>
       </c>
       <c r="D1399" s="10" t="s">
-        <v>38</v>
+        <v>494</v>
       </c>
       <c r="E1399" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1399" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="G1399" s="11" t="s">
-        <v>1635</v>
-      </c>
+        <v>904</v>
+      </c>
+      <c r="G1399" s="11"/>
       <c r="H1399" s="12"/>
       <c r="I1399" s="13"/>
       <c r="J1399" s="13" t="s">
-        <v>1571</v>
-      </c>
-    </row>
-    <row r="1400" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1400" s="12">
-        <v>43762</v>
+        <v>44047</v>
       </c>
       <c r="B1400" s="9"/>
       <c r="C1400" s="14" t="s">
-        <v>446</v>
+        <v>537</v>
       </c>
       <c r="D1400" s="10" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E1400" s="11" t="s">
-        <v>837</v>
+        <v>685</v>
       </c>
       <c r="F1400" s="10" t="s">
-        <v>447</v>
+        <v>873</v>
       </c>
       <c r="G1400" s="11" t="s">
-        <v>1632</v>
+        <v>1627</v>
       </c>
       <c r="H1400" s="12"/>
       <c r="I1400" s="13"/>
       <c r="J1400" s="13"/>
     </row>
-    <row r="1401" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1401" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A1401" s="12">
-        <v>44222</v>
+        <v>43949</v>
       </c>
       <c r="B1401" s="9"/>
       <c r="C1401" s="14" t="s">
-        <v>1496</v>
+        <v>468</v>
       </c>
       <c r="D1401" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E1401" s="11" t="s">
-        <v>837</v>
+        <v>685</v>
       </c>
       <c r="F1401" s="10" t="s">
-        <v>1495</v>
+        <v>686</v>
       </c>
       <c r="G1401" s="11" t="s">
-        <v>309</v>
+        <v>1642</v>
       </c>
       <c r="H1401" s="12"/>
-      <c r="I1401" s="13"/>
+      <c r="I1401" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1401" s="13"/>
     </row>
-    <row r="1402" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1402" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A1402" s="12">
-        <v>44266</v>
+        <v>43949</v>
       </c>
       <c r="B1402" s="9"/>
       <c r="C1402" s="14" t="s">
-        <v>537</v>
+        <v>468</v>
       </c>
       <c r="D1402" s="10" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="E1402" s="11" t="s">
-        <v>570</v>
+        <v>685</v>
       </c>
       <c r="F1402" s="10" t="s">
-        <v>1716</v>
-      </c>
-      <c r="G1402" s="11"/>
+        <v>705</v>
+      </c>
+      <c r="G1402" s="11" t="s">
+        <v>687</v>
+      </c>
       <c r="H1402" s="12"/>
-      <c r="I1402" s="13"/>
+      <c r="I1402" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1402" s="13" t="s">
-        <v>1717</v>
-      </c>
-    </row>
-    <row r="1403" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1403" s="12">
-        <v>44279</v>
+        <v>43838</v>
       </c>
       <c r="B1403" s="9"/>
       <c r="C1403" s="14" t="s">
-        <v>1389</v>
+        <v>103</v>
       </c>
       <c r="D1403" s="10" t="s">
-        <v>89</v>
+        <v>460</v>
       </c>
       <c r="E1403" s="11" t="s">
-        <v>1581</v>
+        <v>647</v>
       </c>
       <c r="F1403" s="10" t="s">
-        <v>1733</v>
-      </c>
-      <c r="G1403" s="11"/>
+        <v>481</v>
+      </c>
+      <c r="G1403" s="11" t="s">
+        <v>1643</v>
+      </c>
       <c r="H1403" s="12"/>
       <c r="I1403" s="13"/>
-      <c r="J1403" s="13"/>
-    </row>
-    <row r="1404" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1403" s="13" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1404" s="12">
-        <v>44286</v>
+        <v>43816</v>
       </c>
       <c r="B1404" s="9"/>
       <c r="C1404" s="14" t="s">
-        <v>288</v>
+        <v>475</v>
       </c>
       <c r="D1404" s="10" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="E1404" s="11" t="s">
-        <v>1581</v>
+        <v>570</v>
       </c>
       <c r="F1404" s="10" t="s">
-        <v>1841</v>
-      </c>
-      <c r="G1404" s="11"/>
+        <v>474</v>
+      </c>
+      <c r="G1404" s="11" t="s">
+        <v>1635</v>
+      </c>
       <c r="H1404" s="12"/>
       <c r="I1404" s="13"/>
-      <c r="J1404" s="13"/>
-    </row>
-    <row r="1405" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1405" s="12"/>
+      <c r="J1404" s="13" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1405" s="12">
+        <v>43762</v>
+      </c>
       <c r="B1405" s="9"/>
-      <c r="C1405" s="14"/>
-      <c r="D1405" s="10"/>
-      <c r="E1405" s="11"/>
-      <c r="F1405" s="10"/>
-      <c r="G1405" s="11"/>
+      <c r="C1405" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1405" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1405" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1405" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1405" s="11" t="s">
+        <v>1632</v>
+      </c>
       <c r="H1405" s="12"/>
       <c r="I1405" s="13"/>
       <c r="J1405" s="13"/>
     </row>
     <row r="1406" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1406" s="12"/>
+      <c r="A1406" s="12">
+        <v>44222</v>
+      </c>
       <c r="B1406" s="9"/>
-      <c r="C1406" s="14"/>
-      <c r="D1406" s="10"/>
-      <c r="E1406" s="11"/>
-      <c r="F1406" s="10"/>
-      <c r="G1406" s="11"/>
+      <c r="C1406" s="14" t="s">
+        <v>1496</v>
+      </c>
+      <c r="D1406" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1406" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1406" s="10" t="s">
+        <v>1495</v>
+      </c>
+      <c r="G1406" s="11" t="s">
+        <v>309</v>
+      </c>
       <c r="H1406" s="12"/>
       <c r="I1406" s="13"/>
       <c r="J1406" s="13"/>
     </row>
-    <row r="1407" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1407" s="12"/>
+    <row r="1407" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1407" s="12">
+        <v>44266</v>
+      </c>
       <c r="B1407" s="9"/>
-      <c r="C1407" s="14"/>
-      <c r="D1407" s="10"/>
-      <c r="E1407" s="11"/>
-      <c r="F1407" s="10"/>
+      <c r="C1407" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1407" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1407" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1407" s="10" t="s">
+        <v>1716</v>
+      </c>
       <c r="G1407" s="11"/>
       <c r="H1407" s="12"/>
       <c r="I1407" s="13"/>
-      <c r="J1407" s="13"/>
+      <c r="J1407" s="13" t="s">
+        <v>1717</v>
+      </c>
     </row>
     <row r="1408" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1408" s="12"/>
+      <c r="A1408" s="12">
+        <v>44279</v>
+      </c>
       <c r="B1408" s="9"/>
-      <c r="C1408" s="14"/>
-      <c r="D1408" s="10"/>
-      <c r="E1408" s="11"/>
-      <c r="F1408" s="10"/>
+      <c r="C1408" s="14" t="s">
+        <v>1389</v>
+      </c>
+      <c r="D1408" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1408" s="11" t="s">
+        <v>1581</v>
+      </c>
+      <c r="F1408" s="10" t="s">
+        <v>1733</v>
+      </c>
       <c r="G1408" s="11"/>
       <c r="H1408" s="12"/>
       <c r="I1408" s="13"/>
       <c r="J1408" s="13"/>
     </row>
-    <row r="1409" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1409" s="12"/>
+    <row r="1409" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1409" s="12">
+        <v>44286</v>
+      </c>
       <c r="B1409" s="9"/>
-      <c r="C1409" s="14"/>
-      <c r="D1409" s="10"/>
-      <c r="E1409" s="11"/>
-      <c r="F1409" s="10"/>
+      <c r="C1409" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1409" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1409" s="11" t="s">
+        <v>1581</v>
+      </c>
+      <c r="F1409" s="10" t="s">
+        <v>1841</v>
+      </c>
       <c r="G1409" s="11"/>
       <c r="H1409" s="12"/>
       <c r="I1409" s="13"/>
@@ -48666,14 +48800,74 @@
       <c r="I1410" s="13"/>
       <c r="J1410" s="13"/>
     </row>
+    <row r="1411" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1411" s="12"/>
+      <c r="B1411" s="9"/>
+      <c r="C1411" s="14"/>
+      <c r="D1411" s="10"/>
+      <c r="E1411" s="11"/>
+      <c r="F1411" s="10"/>
+      <c r="G1411" s="11"/>
+      <c r="H1411" s="12"/>
+      <c r="I1411" s="13"/>
+      <c r="J1411" s="13"/>
+    </row>
+    <row r="1412" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1412" s="12"/>
+      <c r="B1412" s="9"/>
+      <c r="C1412" s="14"/>
+      <c r="D1412" s="10"/>
+      <c r="E1412" s="11"/>
+      <c r="F1412" s="10"/>
+      <c r="G1412" s="11"/>
+      <c r="H1412" s="12"/>
+      <c r="I1412" s="13"/>
+      <c r="J1412" s="13"/>
+    </row>
+    <row r="1413" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1413" s="12"/>
+      <c r="B1413" s="9"/>
+      <c r="C1413" s="14"/>
+      <c r="D1413" s="10"/>
+      <c r="E1413" s="11"/>
+      <c r="F1413" s="10"/>
+      <c r="G1413" s="11"/>
+      <c r="H1413" s="12"/>
+      <c r="I1413" s="13"/>
+      <c r="J1413" s="13"/>
+    </row>
+    <row r="1414" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1414" s="12"/>
+      <c r="B1414" s="9"/>
+      <c r="C1414" s="14"/>
+      <c r="D1414" s="10"/>
+      <c r="E1414" s="11"/>
+      <c r="F1414" s="10"/>
+      <c r="G1414" s="11"/>
+      <c r="H1414" s="12"/>
+      <c r="I1414" s="13"/>
+      <c r="J1414" s="13"/>
+    </row>
+    <row r="1415" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1415" s="12"/>
+      <c r="B1415" s="9"/>
+      <c r="C1415" s="14"/>
+      <c r="D1415" s="10"/>
+      <c r="E1415" s="11"/>
+      <c r="F1415" s="10"/>
+      <c r="G1415" s="11"/>
+      <c r="H1415" s="12"/>
+      <c r="I1415" s="13"/>
+      <c r="J1415" s="13"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1331" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J1039">
       <sortCondition ref="A1:A1023"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1370:F1380">
-    <sortCondition ref="F1370:F1380"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1375:F1385">
+    <sortCondition ref="F1375:F1385"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Filtro Compensação a Pagar
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04EF4B9-285D-49FD-A422-A3AF4D3F7DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BFF792-4FCC-4357-BF24-59A92BF1119F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9836" uniqueCount="2027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9840" uniqueCount="2028">
   <si>
     <t>Responsável</t>
   </si>
@@ -6449,6 +6449,9 @@
   </si>
   <si>
     <t>Testes nova medição</t>
+  </si>
+  <si>
+    <t>Criar lançamento contabil para acrescimo de titulo no financeiro</t>
   </si>
 </sst>
 </file>
@@ -7214,11 +7217,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1430"/>
+  <dimension ref="A1:J1435"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1368" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1386" sqref="A1386"/>
+      <pane ySplit="1" topLeftCell="A1374" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1387" sqref="A1387"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -48458,12 +48461,24 @@
       <c r="J1385" s="13"/>
     </row>
     <row r="1386" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1386" s="12"/>
-      <c r="B1386" s="9"/>
-      <c r="C1386" s="14"/>
-      <c r="D1386" s="10"/>
-      <c r="E1386" s="11"/>
-      <c r="F1386" s="10"/>
+      <c r="A1386" s="12">
+        <v>44364</v>
+      </c>
+      <c r="B1386" s="12">
+        <v>44364</v>
+      </c>
+      <c r="C1386" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1386" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1386" s="11" t="s">
+        <v>669</v>
+      </c>
+      <c r="F1386" s="10" t="s">
+        <v>2027</v>
+      </c>
       <c r="G1386" s="11"/>
       <c r="H1386" s="12"/>
       <c r="I1386" s="13"/>
@@ -48483,7 +48498,7 @@
     </row>
     <row r="1388" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1388" s="12"/>
-      <c r="B1388" s="9"/>
+      <c r="B1388" s="12"/>
       <c r="C1388" s="14"/>
       <c r="D1388" s="10"/>
       <c r="E1388" s="11"/>
@@ -48494,38 +48509,20 @@
       <c r="J1388" s="13"/>
     </row>
     <row r="1389" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1389" s="1" t="s">
-        <v>1479</v>
-      </c>
-      <c r="B1389" s="2" t="s">
-        <v>1480</v>
-      </c>
-      <c r="C1389" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1389" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1389" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1389" s="4" t="s">
-        <v>1581</v>
-      </c>
-      <c r="G1389" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1389" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1389" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1389" s="36"/>
+      <c r="A1389" s="12"/>
+      <c r="B1389" s="12"/>
+      <c r="C1389" s="14"/>
+      <c r="D1389" s="10"/>
+      <c r="E1389" s="11"/>
+      <c r="F1389" s="10"/>
+      <c r="G1389" s="11"/>
+      <c r="H1389" s="12"/>
+      <c r="I1389" s="13"/>
+      <c r="J1389" s="13"/>
     </row>
     <row r="1390" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1390" s="12"/>
-      <c r="B1390" s="9"/>
+      <c r="B1390" s="12"/>
       <c r="C1390" s="14"/>
       <c r="D1390" s="10"/>
       <c r="E1390" s="11"/>
@@ -48537,21 +48534,11 @@
     </row>
     <row r="1391" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1391" s="12"/>
-      <c r="B1391" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1391" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1391" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1391" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1391" s="10" t="s">
-        <v>1616</v>
-      </c>
+      <c r="B1391" s="9"/>
+      <c r="C1391" s="14"/>
+      <c r="D1391" s="10"/>
+      <c r="E1391" s="11"/>
+      <c r="F1391" s="10"/>
       <c r="G1391" s="11"/>
       <c r="H1391" s="12"/>
       <c r="I1391" s="13"/>
@@ -48559,21 +48546,11 @@
     </row>
     <row r="1392" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1392" s="12"/>
-      <c r="B1392" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1392" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1392" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1392" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1392" s="10" t="s">
-        <v>1608</v>
-      </c>
+      <c r="B1392" s="12"/>
+      <c r="C1392" s="14"/>
+      <c r="D1392" s="10"/>
+      <c r="E1392" s="11"/>
+      <c r="F1392" s="10"/>
       <c r="G1392" s="11"/>
       <c r="H1392" s="12"/>
       <c r="I1392" s="13"/>
@@ -48581,65 +48558,53 @@
     </row>
     <row r="1393" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1393" s="12"/>
-      <c r="B1393" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1393" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1393" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1393" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1393" s="10" t="s">
-        <v>1613</v>
-      </c>
+      <c r="B1393" s="9"/>
+      <c r="C1393" s="14"/>
+      <c r="D1393" s="10"/>
+      <c r="E1393" s="11"/>
+      <c r="F1393" s="10"/>
       <c r="G1393" s="11"/>
       <c r="H1393" s="12"/>
       <c r="I1393" s="13"/>
       <c r="J1393" s="13"/>
     </row>
     <row r="1394" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1394" s="12"/>
-      <c r="B1394" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1394" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1394" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1394" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1394" s="10" t="s">
-        <v>1609</v>
-      </c>
-      <c r="G1394" s="11"/>
-      <c r="H1394" s="12"/>
-      <c r="I1394" s="13"/>
-      <c r="J1394" s="13"/>
+      <c r="A1394" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B1394" s="2" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C1394" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1394" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1394" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1394" s="4" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G1394" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1394" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1394" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1394" s="36"/>
     </row>
     <row r="1395" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1395" s="12">
-        <v>44159</v>
-      </c>
+      <c r="A1395" s="12"/>
       <c r="B1395" s="9"/>
-      <c r="C1395" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1395" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1395" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1395" s="10" t="s">
-        <v>1617</v>
-      </c>
+      <c r="C1395" s="14"/>
+      <c r="D1395" s="10"/>
+      <c r="E1395" s="11"/>
+      <c r="F1395" s="10"/>
       <c r="G1395" s="11"/>
       <c r="H1395" s="12"/>
       <c r="I1395" s="13"/>
@@ -48647,8 +48612,8 @@
     </row>
     <row r="1396" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1396" s="12"/>
-      <c r="B1396" s="12">
-        <v>44309</v>
+      <c r="B1396" s="9">
+        <v>44255</v>
       </c>
       <c r="C1396" s="14" t="s">
         <v>13</v>
@@ -48660,7 +48625,7 @@
         <v>647</v>
       </c>
       <c r="F1396" s="10" t="s">
-        <v>1610</v>
+        <v>1616</v>
       </c>
       <c r="G1396" s="11"/>
       <c r="H1396" s="12"/>
@@ -48668,10 +48633,10 @@
       <c r="J1396" s="13"/>
     </row>
     <row r="1397" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1397" s="12">
-        <v>44239</v>
-      </c>
-      <c r="B1397" s="9"/>
+      <c r="A1397" s="12"/>
+      <c r="B1397" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1397" s="14" t="s">
         <v>13</v>
       </c>
@@ -48682,7 +48647,7 @@
         <v>647</v>
       </c>
       <c r="F1397" s="10" t="s">
-        <v>1607</v>
+        <v>1608</v>
       </c>
       <c r="G1397" s="11"/>
       <c r="H1397" s="12"/>
@@ -48704,7 +48669,7 @@
         <v>647</v>
       </c>
       <c r="F1398" s="10" t="s">
-        <v>1606</v>
+        <v>1613</v>
       </c>
       <c r="G1398" s="11"/>
       <c r="H1398" s="12"/>
@@ -48726,7 +48691,7 @@
         <v>647</v>
       </c>
       <c r="F1399" s="10" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="G1399" s="11"/>
       <c r="H1399" s="12"/>
@@ -48734,10 +48699,10 @@
       <c r="J1399" s="13"/>
     </row>
     <row r="1400" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1400" s="12"/>
-      <c r="B1400" s="12">
-        <v>44309</v>
-      </c>
+      <c r="A1400" s="12">
+        <v>44159</v>
+      </c>
+      <c r="B1400" s="9"/>
       <c r="C1400" s="14" t="s">
         <v>13</v>
       </c>
@@ -48748,7 +48713,7 @@
         <v>647</v>
       </c>
       <c r="F1400" s="10" t="s">
-        <v>1614</v>
+        <v>1617</v>
       </c>
       <c r="G1400" s="11"/>
       <c r="H1400" s="12"/>
@@ -48757,8 +48722,8 @@
     </row>
     <row r="1401" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1401" s="12"/>
-      <c r="B1401" s="9">
-        <v>44235</v>
+      <c r="B1401" s="12">
+        <v>44309</v>
       </c>
       <c r="C1401" s="14" t="s">
         <v>13</v>
@@ -48770,7 +48735,7 @@
         <v>647</v>
       </c>
       <c r="F1401" s="10" t="s">
-        <v>1615</v>
+        <v>1610</v>
       </c>
       <c r="G1401" s="11"/>
       <c r="H1401" s="12"/>
@@ -48779,7 +48744,7 @@
     </row>
     <row r="1402" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1402" s="12">
-        <v>44245</v>
+        <v>44239</v>
       </c>
       <c r="B1402" s="9"/>
       <c r="C1402" s="14" t="s">
@@ -48792,7 +48757,7 @@
         <v>647</v>
       </c>
       <c r="F1402" s="10" t="s">
-        <v>1612</v>
+        <v>1607</v>
       </c>
       <c r="G1402" s="11"/>
       <c r="H1402" s="12"/>
@@ -48801,7 +48766,9 @@
     </row>
     <row r="1403" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1403" s="12"/>
-      <c r="B1403" s="9"/>
+      <c r="B1403" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1403" s="14" t="s">
         <v>13</v>
       </c>
@@ -48812,7 +48779,7 @@
         <v>647</v>
       </c>
       <c r="F1403" s="10" t="s">
-        <v>1583</v>
+        <v>1606</v>
       </c>
       <c r="G1403" s="11"/>
       <c r="H1403" s="12"/>
@@ -48821,125 +48788,119 @@
     </row>
     <row r="1404" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1404" s="12"/>
-      <c r="B1404" s="9"/>
-      <c r="C1404" s="14"/>
-      <c r="D1404" s="10"/>
-      <c r="E1404" s="11"/>
-      <c r="F1404" s="10"/>
+      <c r="B1404" s="9">
+        <v>44255</v>
+      </c>
+      <c r="C1404" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1404" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1404" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1404" s="10" t="s">
+        <v>1611</v>
+      </c>
       <c r="G1404" s="11"/>
       <c r="H1404" s="12"/>
       <c r="I1404" s="13"/>
       <c r="J1404" s="13"/>
     </row>
     <row r="1405" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1405" s="12">
-        <v>44176</v>
-      </c>
-      <c r="B1405" s="9"/>
+      <c r="A1405" s="12"/>
+      <c r="B1405" s="12">
+        <v>44309</v>
+      </c>
       <c r="C1405" s="14" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D1405" s="10" t="s">
         <v>584</v>
       </c>
       <c r="E1405" s="11" t="s">
-        <v>1353</v>
+        <v>647</v>
       </c>
       <c r="F1405" s="10" t="s">
-        <v>1354</v>
+        <v>1614</v>
       </c>
       <c r="G1405" s="11"/>
       <c r="H1405" s="12"/>
       <c r="I1405" s="13"/>
       <c r="J1405" s="13"/>
     </row>
-    <row r="1406" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1406" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1406" s="9"/>
+    <row r="1406" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1406" s="12"/>
+      <c r="B1406" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1406" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1406" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1406" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1406" s="10" t="s">
-        <v>1661</v>
+        <v>1615</v>
       </c>
       <c r="G1406" s="11"/>
       <c r="H1406" s="12"/>
       <c r="I1406" s="13"/>
-      <c r="J1406" s="13" t="s">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="1407" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1406" s="13"/>
+    </row>
+    <row r="1407" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1407" s="12">
-        <v>44252</v>
+        <v>44245</v>
       </c>
       <c r="B1407" s="9"/>
       <c r="C1407" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1407" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1407" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1407" s="10" t="s">
-        <v>1660</v>
+        <v>1612</v>
       </c>
       <c r="G1407" s="11"/>
       <c r="H1407" s="12"/>
       <c r="I1407" s="13"/>
       <c r="J1407" s="13"/>
     </row>
-    <row r="1408" spans="1:10" ht="84" x14ac:dyDescent="0.2">
-      <c r="A1408" s="12">
-        <v>43864</v>
-      </c>
+    <row r="1408" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1408" s="12"/>
       <c r="B1408" s="9"/>
       <c r="C1408" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1408" s="10" t="s">
-        <v>533</v>
+        <v>584</v>
       </c>
       <c r="E1408" s="11" t="s">
-        <v>1580</v>
+        <v>647</v>
       </c>
       <c r="F1408" s="10" t="s">
-        <v>534</v>
+        <v>1583</v>
       </c>
       <c r="G1408" s="11"/>
       <c r="H1408" s="12"/>
       <c r="I1408" s="13"/>
-      <c r="J1408" s="13" t="s">
-        <v>1707</v>
-      </c>
+      <c r="J1408" s="13"/>
     </row>
     <row r="1409" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1409" s="12">
-        <v>44112</v>
-      </c>
+      <c r="A1409" s="12"/>
       <c r="B1409" s="9"/>
-      <c r="C1409" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="D1409" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1409" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1409" s="10" t="s">
-        <v>1097</v>
-      </c>
+      <c r="C1409" s="14"/>
+      <c r="D1409" s="10"/>
+      <c r="E1409" s="11"/>
+      <c r="F1409" s="10"/>
       <c r="G1409" s="11"/>
       <c r="H1409" s="12"/>
       <c r="I1409" s="13"/>
@@ -48947,417 +48908,471 @@
     </row>
     <row r="1410" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1410" s="12">
-        <v>44088</v>
+        <v>44176</v>
       </c>
       <c r="B1410" s="9"/>
       <c r="C1410" s="14" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D1410" s="10" t="s">
-        <v>906</v>
+        <v>584</v>
       </c>
       <c r="E1410" s="11" t="s">
-        <v>685</v>
+        <v>1353</v>
       </c>
       <c r="F1410" s="10" t="s">
-        <v>1011</v>
+        <v>1354</v>
       </c>
       <c r="G1410" s="11"/>
       <c r="H1410" s="12"/>
       <c r="I1410" s="13"/>
       <c r="J1410" s="13"/>
     </row>
-    <row r="1411" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1411" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1411" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1411" s="9"/>
       <c r="C1411" s="14" t="s">
-        <v>623</v>
+        <v>898</v>
       </c>
       <c r="D1411" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1411" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1411" s="10" t="s">
-        <v>903</v>
+        <v>1661</v>
       </c>
       <c r="G1411" s="11"/>
       <c r="H1411" s="12"/>
       <c r="I1411" s="13"/>
-      <c r="J1411" s="13"/>
-    </row>
-    <row r="1412" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1411" s="13" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1412" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1412" s="9"/>
       <c r="C1412" s="14" t="s">
-        <v>623</v>
+        <v>898</v>
       </c>
       <c r="D1412" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1412" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1412" s="10" t="s">
-        <v>902</v>
+        <v>1660</v>
       </c>
       <c r="G1412" s="11"/>
       <c r="H1412" s="12"/>
       <c r="I1412" s="13"/>
       <c r="J1412" s="13"/>
     </row>
-    <row r="1413" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1413" spans="1:10" ht="84" x14ac:dyDescent="0.2">
       <c r="A1413" s="12">
-        <v>44055</v>
+        <v>43864</v>
       </c>
       <c r="B1413" s="9"/>
       <c r="C1413" s="14" t="s">
-        <v>898</v>
+        <v>19</v>
       </c>
       <c r="D1413" s="10" t="s">
-        <v>494</v>
+        <v>533</v>
       </c>
       <c r="E1413" s="11" t="s">
-        <v>570</v>
+        <v>1580</v>
       </c>
       <c r="F1413" s="10" t="s">
-        <v>900</v>
+        <v>534</v>
       </c>
       <c r="G1413" s="11"/>
       <c r="H1413" s="12"/>
       <c r="I1413" s="13"/>
-      <c r="J1413" s="13"/>
-    </row>
-    <row r="1414" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="J1413" s="13" t="s">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1414" s="12">
-        <v>44055</v>
+        <v>44112</v>
       </c>
       <c r="B1414" s="9"/>
       <c r="C1414" s="14" t="s">
-        <v>898</v>
+        <v>623</v>
       </c>
       <c r="D1414" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1414" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1414" s="10" t="s">
-        <v>901</v>
+        <v>1097</v>
       </c>
       <c r="G1414" s="11"/>
       <c r="H1414" s="12"/>
       <c r="I1414" s="13"/>
       <c r="J1414" s="13"/>
     </row>
-    <row r="1415" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1415" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1415" s="12">
-        <v>44055</v>
+        <v>44088</v>
       </c>
       <c r="B1415" s="9"/>
       <c r="C1415" s="14" t="s">
-        <v>898</v>
+        <v>19</v>
       </c>
       <c r="D1415" s="10" t="s">
-        <v>494</v>
+        <v>906</v>
       </c>
       <c r="E1415" s="11" t="s">
-        <v>570</v>
+        <v>685</v>
       </c>
       <c r="F1415" s="10" t="s">
-        <v>904</v>
+        <v>1011</v>
       </c>
       <c r="G1415" s="11"/>
       <c r="H1415" s="12"/>
       <c r="I1415" s="13"/>
-      <c r="J1415" s="13" t="s">
-        <v>1590</v>
-      </c>
-    </row>
-    <row r="1416" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1415" s="13"/>
+    </row>
+    <row r="1416" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1416" s="12">
-        <v>44047</v>
+        <v>44055</v>
       </c>
       <c r="B1416" s="9"/>
       <c r="C1416" s="14" t="s">
-        <v>537</v>
+        <v>623</v>
       </c>
       <c r="D1416" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E1416" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1416" s="10" t="s">
-        <v>873</v>
-      </c>
-      <c r="G1416" s="11" t="s">
-        <v>1626</v>
-      </c>
+        <v>903</v>
+      </c>
+      <c r="G1416" s="11"/>
       <c r="H1416" s="12"/>
       <c r="I1416" s="13"/>
       <c r="J1416" s="13"/>
     </row>
-    <row r="1417" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1417" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1417" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1417" s="9"/>
       <c r="C1417" s="14" t="s">
-        <v>468</v>
+        <v>623</v>
       </c>
       <c r="D1417" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1417" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1417" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1417" s="11" t="s">
-        <v>1641</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="G1417" s="11"/>
       <c r="H1417" s="12"/>
-      <c r="I1417" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1417" s="13"/>
       <c r="J1417" s="13"/>
     </row>
-    <row r="1418" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1418" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1418" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1418" s="9"/>
       <c r="C1418" s="14" t="s">
-        <v>468</v>
+        <v>898</v>
       </c>
       <c r="D1418" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1418" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1418" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1418" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="G1418" s="11"/>
       <c r="H1418" s="12"/>
-      <c r="I1418" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1418" s="13" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="1419" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1418" s="13"/>
+      <c r="J1418" s="13"/>
+    </row>
+    <row r="1419" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A1419" s="12">
-        <v>43838</v>
+        <v>44055</v>
       </c>
       <c r="B1419" s="9"/>
       <c r="C1419" s="14" t="s">
-        <v>103</v>
+        <v>898</v>
       </c>
       <c r="D1419" s="10" t="s">
-        <v>460</v>
+        <v>494</v>
       </c>
       <c r="E1419" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1419" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G1419" s="11" t="s">
-        <v>1642</v>
-      </c>
+        <v>901</v>
+      </c>
+      <c r="G1419" s="11"/>
       <c r="H1419" s="12"/>
       <c r="I1419" s="13"/>
-      <c r="J1419" s="13" t="s">
-        <v>1534</v>
-      </c>
-    </row>
-    <row r="1420" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1419" s="13"/>
+    </row>
+    <row r="1420" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1420" s="12">
-        <v>43816</v>
+        <v>44055</v>
       </c>
       <c r="B1420" s="9"/>
       <c r="C1420" s="14" t="s">
-        <v>475</v>
+        <v>898</v>
       </c>
       <c r="D1420" s="10" t="s">
-        <v>38</v>
+        <v>494</v>
       </c>
       <c r="E1420" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1420" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="G1420" s="11" t="s">
-        <v>1634</v>
-      </c>
+        <v>904</v>
+      </c>
+      <c r="G1420" s="11"/>
       <c r="H1420" s="12"/>
       <c r="I1420" s="13"/>
       <c r="J1420" s="13" t="s">
-        <v>1570</v>
-      </c>
-    </row>
-    <row r="1421" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1421" s="12">
-        <v>43762</v>
+        <v>44047</v>
       </c>
       <c r="B1421" s="9"/>
       <c r="C1421" s="14" t="s">
-        <v>446</v>
+        <v>537</v>
       </c>
       <c r="D1421" s="10" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E1421" s="11" t="s">
-        <v>837</v>
+        <v>685</v>
       </c>
       <c r="F1421" s="10" t="s">
-        <v>447</v>
+        <v>873</v>
       </c>
       <c r="G1421" s="11" t="s">
-        <v>1631</v>
+        <v>1626</v>
       </c>
       <c r="H1421" s="12"/>
       <c r="I1421" s="13"/>
       <c r="J1421" s="13"/>
     </row>
-    <row r="1422" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1422" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A1422" s="12">
-        <v>44222</v>
+        <v>43949</v>
       </c>
       <c r="B1422" s="9"/>
       <c r="C1422" s="14" t="s">
-        <v>1495</v>
+        <v>468</v>
       </c>
       <c r="D1422" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E1422" s="11" t="s">
-        <v>837</v>
+        <v>685</v>
       </c>
       <c r="F1422" s="10" t="s">
-        <v>1494</v>
+        <v>686</v>
       </c>
       <c r="G1422" s="11" t="s">
-        <v>309</v>
+        <v>1641</v>
       </c>
       <c r="H1422" s="12"/>
-      <c r="I1422" s="13"/>
+      <c r="I1422" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1422" s="13"/>
     </row>
-    <row r="1423" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1423" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A1423" s="12">
-        <v>44266</v>
+        <v>43949</v>
       </c>
       <c r="B1423" s="9"/>
       <c r="C1423" s="14" t="s">
-        <v>537</v>
+        <v>468</v>
       </c>
       <c r="D1423" s="10" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="E1423" s="11" t="s">
-        <v>570</v>
+        <v>685</v>
       </c>
       <c r="F1423" s="10" t="s">
-        <v>1715</v>
-      </c>
-      <c r="G1423" s="11"/>
+        <v>705</v>
+      </c>
+      <c r="G1423" s="11" t="s">
+        <v>687</v>
+      </c>
       <c r="H1423" s="12"/>
-      <c r="I1423" s="13"/>
+      <c r="I1423" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1423" s="13" t="s">
-        <v>1716</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="1424" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1424" s="12">
-        <v>44286</v>
+        <v>43838</v>
       </c>
       <c r="B1424" s="9"/>
       <c r="C1424" s="14" t="s">
-        <v>288</v>
+        <v>103</v>
       </c>
       <c r="D1424" s="10" t="s">
-        <v>25</v>
+        <v>460</v>
       </c>
       <c r="E1424" s="11" t="s">
-        <v>1580</v>
+        <v>647</v>
       </c>
       <c r="F1424" s="10" t="s">
-        <v>1840</v>
-      </c>
-      <c r="G1424" s="11"/>
+        <v>481</v>
+      </c>
+      <c r="G1424" s="11" t="s">
+        <v>1642</v>
+      </c>
       <c r="H1424" s="12"/>
       <c r="I1424" s="13"/>
-      <c r="J1424" s="13"/>
+      <c r="J1424" s="13" t="s">
+        <v>1534</v>
+      </c>
     </row>
     <row r="1425" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1425" s="12"/>
+      <c r="A1425" s="12">
+        <v>43816</v>
+      </c>
       <c r="B1425" s="9"/>
-      <c r="C1425" s="14"/>
-      <c r="D1425" s="10"/>
-      <c r="E1425" s="11"/>
-      <c r="F1425" s="10"/>
-      <c r="G1425" s="11"/>
+      <c r="C1425" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1425" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1425" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1425" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G1425" s="11" t="s">
+        <v>1634</v>
+      </c>
       <c r="H1425" s="12"/>
       <c r="I1425" s="13"/>
-      <c r="J1425" s="13"/>
-    </row>
-    <row r="1426" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1426" s="12"/>
+      <c r="J1425" s="13" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1426" s="12">
+        <v>43762</v>
+      </c>
       <c r="B1426" s="9"/>
-      <c r="C1426" s="14"/>
-      <c r="D1426" s="10"/>
-      <c r="E1426" s="11"/>
-      <c r="F1426" s="10"/>
-      <c r="G1426" s="11"/>
+      <c r="C1426" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1426" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1426" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1426" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1426" s="11" t="s">
+        <v>1631</v>
+      </c>
       <c r="H1426" s="12"/>
       <c r="I1426" s="13"/>
       <c r="J1426" s="13"/>
     </row>
     <row r="1427" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1427" s="12"/>
+      <c r="A1427" s="12">
+        <v>44222</v>
+      </c>
       <c r="B1427" s="9"/>
-      <c r="C1427" s="14"/>
-      <c r="D1427" s="10"/>
-      <c r="E1427" s="11"/>
-      <c r="F1427" s="10"/>
-      <c r="G1427" s="11"/>
+      <c r="C1427" s="14" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D1427" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1427" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1427" s="10" t="s">
+        <v>1494</v>
+      </c>
+      <c r="G1427" s="11" t="s">
+        <v>309</v>
+      </c>
       <c r="H1427" s="12"/>
       <c r="I1427" s="13"/>
       <c r="J1427" s="13"/>
     </row>
-    <row r="1428" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1428" s="12"/>
+    <row r="1428" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1428" s="12">
+        <v>44266</v>
+      </c>
       <c r="B1428" s="9"/>
-      <c r="C1428" s="14"/>
-      <c r="D1428" s="10"/>
-      <c r="E1428" s="11"/>
-      <c r="F1428" s="10"/>
+      <c r="C1428" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1428" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1428" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1428" s="10" t="s">
+        <v>1715</v>
+      </c>
       <c r="G1428" s="11"/>
       <c r="H1428" s="12"/>
       <c r="I1428" s="13"/>
-      <c r="J1428" s="13"/>
-    </row>
-    <row r="1429" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1429" s="12"/>
+      <c r="J1428" s="13" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1429" s="12">
+        <v>44286</v>
+      </c>
       <c r="B1429" s="9"/>
-      <c r="C1429" s="14"/>
-      <c r="D1429" s="10"/>
-      <c r="E1429" s="11"/>
-      <c r="F1429" s="10"/>
+      <c r="C1429" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1429" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1429" s="11" t="s">
+        <v>1580</v>
+      </c>
+      <c r="F1429" s="10" t="s">
+        <v>1840</v>
+      </c>
       <c r="G1429" s="11"/>
       <c r="H1429" s="12"/>
       <c r="I1429" s="13"/>
@@ -49375,10 +49390,70 @@
       <c r="I1430" s="13"/>
       <c r="J1430" s="13"/>
     </row>
+    <row r="1431" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1431" s="12"/>
+      <c r="B1431" s="9"/>
+      <c r="C1431" s="14"/>
+      <c r="D1431" s="10"/>
+      <c r="E1431" s="11"/>
+      <c r="F1431" s="10"/>
+      <c r="G1431" s="11"/>
+      <c r="H1431" s="12"/>
+      <c r="I1431" s="13"/>
+      <c r="J1431" s="13"/>
+    </row>
+    <row r="1432" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1432" s="12"/>
+      <c r="B1432" s="9"/>
+      <c r="C1432" s="14"/>
+      <c r="D1432" s="10"/>
+      <c r="E1432" s="11"/>
+      <c r="F1432" s="10"/>
+      <c r="G1432" s="11"/>
+      <c r="H1432" s="12"/>
+      <c r="I1432" s="13"/>
+      <c r="J1432" s="13"/>
+    </row>
+    <row r="1433" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1433" s="12"/>
+      <c r="B1433" s="9"/>
+      <c r="C1433" s="14"/>
+      <c r="D1433" s="10"/>
+      <c r="E1433" s="11"/>
+      <c r="F1433" s="10"/>
+      <c r="G1433" s="11"/>
+      <c r="H1433" s="12"/>
+      <c r="I1433" s="13"/>
+      <c r="J1433" s="13"/>
+    </row>
+    <row r="1434" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1434" s="12"/>
+      <c r="B1434" s="9"/>
+      <c r="C1434" s="14"/>
+      <c r="D1434" s="10"/>
+      <c r="E1434" s="11"/>
+      <c r="F1434" s="10"/>
+      <c r="G1434" s="11"/>
+      <c r="H1434" s="12"/>
+      <c r="I1434" s="13"/>
+      <c r="J1434" s="13"/>
+    </row>
+    <row r="1435" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1435" s="12"/>
+      <c r="B1435" s="9"/>
+      <c r="C1435" s="14"/>
+      <c r="D1435" s="10"/>
+      <c r="E1435" s="11"/>
+      <c r="F1435" s="10"/>
+      <c r="G1435" s="11"/>
+      <c r="H1435" s="12"/>
+      <c r="I1435" s="13"/>
+      <c r="J1435" s="13"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1378" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1392:F1402">
-    <sortCondition ref="F1392:F1402"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1397:F1407">
+    <sortCondition ref="F1397:F1407"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Despesas p/ CC com impostos
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BFF792-4FCC-4357-BF24-59A92BF1119F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0594C500-150B-46BE-8954-372960B845A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9840" uniqueCount="2028">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9882" uniqueCount="2035">
   <si>
     <t>Responsável</t>
   </si>
@@ -6452,6 +6452,27 @@
   </si>
   <si>
     <t>Criar lançamento contabil para acrescimo de titulo no financeiro</t>
+  </si>
+  <si>
+    <t>Criar filtro na tela de compensação de conas a pagar com opção para exportar para o excel e acerto titulos com problemas na compensação</t>
+  </si>
+  <si>
+    <t>Alterar campos do Browse dos Tipos de Entrada e Saída (TES)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consulta pedido na tela da nova medição </t>
+  </si>
+  <si>
+    <t>Informar todos os CNPJ’s ativos dos clientes da BK</t>
+  </si>
+  <si>
+    <t>Sergio Oliveira</t>
+  </si>
+  <si>
+    <t>Informar todos os CNPJ’s ativos dos clientes da BK por centro de custo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incluir coluna ISS Apurado na Mapa de Inss retido </t>
   </si>
 </sst>
 </file>
@@ -7217,11 +7238,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1435"/>
+  <dimension ref="A1:J1441"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1374" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1387" sqref="A1387"/>
+      <pane ySplit="1" topLeftCell="A1383" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1393" sqref="A1393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -48484,81 +48505,189 @@
       <c r="I1386" s="13"/>
       <c r="J1386" s="13"/>
     </row>
-    <row r="1387" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1387" s="12"/>
-      <c r="B1387" s="12"/>
-      <c r="C1387" s="14"/>
-      <c r="D1387" s="10"/>
-      <c r="E1387" s="11"/>
-      <c r="F1387" s="10"/>
-      <c r="G1387" s="11"/>
-      <c r="H1387" s="12"/>
-      <c r="I1387" s="13"/>
+    <row r="1387" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1387" s="12">
+        <v>44365</v>
+      </c>
+      <c r="B1387" s="12">
+        <v>44365</v>
+      </c>
+      <c r="C1387" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1387" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1387" s="11" t="s">
+        <v>669</v>
+      </c>
+      <c r="F1387" s="10" t="s">
+        <v>2028</v>
+      </c>
+      <c r="G1387" s="11" t="s">
+        <v>1627</v>
+      </c>
+      <c r="H1387" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1387" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1387" s="13"/>
     </row>
     <row r="1388" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1388" s="12"/>
-      <c r="B1388" s="12"/>
-      <c r="C1388" s="14"/>
-      <c r="D1388" s="10"/>
-      <c r="E1388" s="11"/>
-      <c r="F1388" s="10"/>
-      <c r="G1388" s="11"/>
-      <c r="H1388" s="12"/>
-      <c r="I1388" s="13"/>
+      <c r="A1388" s="12">
+        <v>44365</v>
+      </c>
+      <c r="B1388" s="12">
+        <v>44367</v>
+      </c>
+      <c r="C1388" s="14" t="s">
+        <v>2021</v>
+      </c>
+      <c r="D1388" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1388" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1388" s="10" t="s">
+        <v>2029</v>
+      </c>
+      <c r="G1388" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1388" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1388" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1388" s="13"/>
     </row>
     <row r="1389" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1389" s="12"/>
-      <c r="B1389" s="12"/>
-      <c r="C1389" s="14"/>
-      <c r="D1389" s="10"/>
-      <c r="E1389" s="11"/>
-      <c r="F1389" s="10"/>
-      <c r="G1389" s="11"/>
-      <c r="H1389" s="12"/>
-      <c r="I1389" s="13"/>
+      <c r="A1389" s="12">
+        <v>44367</v>
+      </c>
+      <c r="B1389" s="12">
+        <v>44367</v>
+      </c>
+      <c r="C1389" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1389" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1389" s="11" t="s">
+        <v>1834</v>
+      </c>
+      <c r="F1389" s="10" t="s">
+        <v>2030</v>
+      </c>
+      <c r="G1389" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1389" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1389" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1389" s="13"/>
     </row>
     <row r="1390" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1390" s="12"/>
-      <c r="B1390" s="12"/>
-      <c r="C1390" s="14"/>
-      <c r="D1390" s="10"/>
-      <c r="E1390" s="11"/>
-      <c r="F1390" s="10"/>
-      <c r="G1390" s="11"/>
-      <c r="H1390" s="12"/>
-      <c r="I1390" s="13"/>
+      <c r="A1390" s="12">
+        <v>44369</v>
+      </c>
+      <c r="B1390" s="12">
+        <v>44369</v>
+      </c>
+      <c r="C1390" s="14" t="s">
+        <v>575</v>
+      </c>
+      <c r="D1390" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1390" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1390" s="10" t="s">
+        <v>2031</v>
+      </c>
+      <c r="G1390" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1390" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1390" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1390" s="13"/>
     </row>
     <row r="1391" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1391" s="12"/>
-      <c r="B1391" s="9"/>
-      <c r="C1391" s="14"/>
-      <c r="D1391" s="10"/>
-      <c r="E1391" s="11"/>
-      <c r="F1391" s="10"/>
-      <c r="G1391" s="11"/>
-      <c r="H1391" s="12"/>
-      <c r="I1391" s="13"/>
+      <c r="A1391" s="12">
+        <v>44369</v>
+      </c>
+      <c r="B1391" s="12">
+        <v>44369</v>
+      </c>
+      <c r="C1391" s="14" t="s">
+        <v>2032</v>
+      </c>
+      <c r="D1391" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="E1391" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1391" s="10" t="s">
+        <v>2033</v>
+      </c>
+      <c r="G1391" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1391" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1391" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1391" s="13"/>
     </row>
     <row r="1392" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1392" s="12"/>
-      <c r="B1392" s="12"/>
-      <c r="C1392" s="14"/>
-      <c r="D1392" s="10"/>
-      <c r="E1392" s="11"/>
-      <c r="F1392" s="10"/>
-      <c r="G1392" s="11"/>
-      <c r="H1392" s="12"/>
-      <c r="I1392" s="13"/>
+      <c r="A1392" s="12">
+        <v>44370</v>
+      </c>
+      <c r="B1392" s="12">
+        <v>44370</v>
+      </c>
+      <c r="C1392" s="14" t="s">
+        <v>1994</v>
+      </c>
+      <c r="D1392" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1392" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1392" s="10" t="s">
+        <v>2034</v>
+      </c>
+      <c r="G1392" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1392" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1392" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1392" s="13"/>
     </row>
     <row r="1393" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1393" s="12"/>
-      <c r="B1393" s="9"/>
+      <c r="B1393" s="12"/>
       <c r="C1393" s="14"/>
       <c r="D1393" s="10"/>
       <c r="E1393" s="11"/>
@@ -48569,38 +48698,20 @@
       <c r="J1393" s="13"/>
     </row>
     <row r="1394" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1394" s="1" t="s">
-        <v>1479</v>
-      </c>
-      <c r="B1394" s="2" t="s">
-        <v>1480</v>
-      </c>
-      <c r="C1394" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1394" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1394" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1394" s="4" t="s">
-        <v>1581</v>
-      </c>
-      <c r="G1394" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1394" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1394" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1394" s="36"/>
+      <c r="A1394" s="12"/>
+      <c r="B1394" s="12"/>
+      <c r="C1394" s="14"/>
+      <c r="D1394" s="10"/>
+      <c r="E1394" s="11"/>
+      <c r="F1394" s="10"/>
+      <c r="G1394" s="11"/>
+      <c r="H1394" s="12"/>
+      <c r="I1394" s="13"/>
+      <c r="J1394" s="13"/>
     </row>
     <row r="1395" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1395" s="12"/>
-      <c r="B1395" s="9"/>
+      <c r="B1395" s="12"/>
       <c r="C1395" s="14"/>
       <c r="D1395" s="10"/>
       <c r="E1395" s="11"/>
@@ -48612,21 +48723,11 @@
     </row>
     <row r="1396" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1396" s="12"/>
-      <c r="B1396" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1396" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1396" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1396" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1396" s="10" t="s">
-        <v>1616</v>
-      </c>
+      <c r="B1396" s="12"/>
+      <c r="C1396" s="14"/>
+      <c r="D1396" s="10"/>
+      <c r="E1396" s="11"/>
+      <c r="F1396" s="10"/>
       <c r="G1396" s="11"/>
       <c r="H1396" s="12"/>
       <c r="I1396" s="13"/>
@@ -48634,21 +48735,11 @@
     </row>
     <row r="1397" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1397" s="12"/>
-      <c r="B1397" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1397" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1397" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1397" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1397" s="10" t="s">
-        <v>1608</v>
-      </c>
+      <c r="B1397" s="12"/>
+      <c r="C1397" s="14"/>
+      <c r="D1397" s="10"/>
+      <c r="E1397" s="11"/>
+      <c r="F1397" s="10"/>
       <c r="G1397" s="11"/>
       <c r="H1397" s="12"/>
       <c r="I1397" s="13"/>
@@ -48656,21 +48747,11 @@
     </row>
     <row r="1398" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1398" s="12"/>
-      <c r="B1398" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1398" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1398" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1398" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1398" s="10" t="s">
-        <v>1613</v>
-      </c>
+      <c r="B1398" s="12"/>
+      <c r="C1398" s="14"/>
+      <c r="D1398" s="10"/>
+      <c r="E1398" s="11"/>
+      <c r="F1398" s="10"/>
       <c r="G1398" s="11"/>
       <c r="H1398" s="12"/>
       <c r="I1398" s="13"/>
@@ -48678,75 +48759,63 @@
     </row>
     <row r="1399" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1399" s="12"/>
-      <c r="B1399" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1399" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1399" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1399" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1399" s="10" t="s">
-        <v>1609</v>
-      </c>
+      <c r="B1399" s="9"/>
+      <c r="C1399" s="14"/>
+      <c r="D1399" s="10"/>
+      <c r="E1399" s="11"/>
+      <c r="F1399" s="10"/>
       <c r="G1399" s="11"/>
       <c r="H1399" s="12"/>
       <c r="I1399" s="13"/>
       <c r="J1399" s="13"/>
     </row>
     <row r="1400" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1400" s="12">
-        <v>44159</v>
-      </c>
-      <c r="B1400" s="9"/>
-      <c r="C1400" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1400" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1400" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1400" s="10" t="s">
-        <v>1617</v>
-      </c>
-      <c r="G1400" s="11"/>
-      <c r="H1400" s="12"/>
-      <c r="I1400" s="13"/>
-      <c r="J1400" s="13"/>
+      <c r="A1400" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B1400" s="2" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C1400" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1400" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1400" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1400" s="4" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G1400" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1400" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1400" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1400" s="36"/>
     </row>
     <row r="1401" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1401" s="12"/>
-      <c r="B1401" s="12">
-        <v>44309</v>
-      </c>
-      <c r="C1401" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1401" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1401" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1401" s="10" t="s">
-        <v>1610</v>
-      </c>
+      <c r="B1401" s="9"/>
+      <c r="C1401" s="14"/>
+      <c r="D1401" s="10"/>
+      <c r="E1401" s="11"/>
+      <c r="F1401" s="10"/>
       <c r="G1401" s="11"/>
       <c r="H1401" s="12"/>
       <c r="I1401" s="13"/>
       <c r="J1401" s="13"/>
     </row>
     <row r="1402" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1402" s="12">
-        <v>44239</v>
-      </c>
-      <c r="B1402" s="9"/>
+      <c r="A1402" s="12"/>
+      <c r="B1402" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1402" s="14" t="s">
         <v>13</v>
       </c>
@@ -48757,7 +48826,7 @@
         <v>647</v>
       </c>
       <c r="F1402" s="10" t="s">
-        <v>1607</v>
+        <v>1616</v>
       </c>
       <c r="G1402" s="11"/>
       <c r="H1402" s="12"/>
@@ -48779,7 +48848,7 @@
         <v>647</v>
       </c>
       <c r="F1403" s="10" t="s">
-        <v>1606</v>
+        <v>1608</v>
       </c>
       <c r="G1403" s="11"/>
       <c r="H1403" s="12"/>
@@ -48801,7 +48870,7 @@
         <v>647</v>
       </c>
       <c r="F1404" s="10" t="s">
-        <v>1611</v>
+        <v>1613</v>
       </c>
       <c r="G1404" s="11"/>
       <c r="H1404" s="12"/>
@@ -48810,8 +48879,8 @@
     </row>
     <row r="1405" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1405" s="12"/>
-      <c r="B1405" s="12">
-        <v>44309</v>
+      <c r="B1405" s="9">
+        <v>44255</v>
       </c>
       <c r="C1405" s="14" t="s">
         <v>13</v>
@@ -48823,7 +48892,7 @@
         <v>647</v>
       </c>
       <c r="F1405" s="10" t="s">
-        <v>1614</v>
+        <v>1609</v>
       </c>
       <c r="G1405" s="11"/>
       <c r="H1405" s="12"/>
@@ -48831,10 +48900,10 @@
       <c r="J1405" s="13"/>
     </row>
     <row r="1406" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1406" s="12"/>
-      <c r="B1406" s="9">
-        <v>44235</v>
-      </c>
+      <c r="A1406" s="12">
+        <v>44159</v>
+      </c>
+      <c r="B1406" s="9"/>
       <c r="C1406" s="14" t="s">
         <v>13</v>
       </c>
@@ -48845,7 +48914,7 @@
         <v>647</v>
       </c>
       <c r="F1406" s="10" t="s">
-        <v>1615</v>
+        <v>1617</v>
       </c>
       <c r="G1406" s="11"/>
       <c r="H1406" s="12"/>
@@ -48853,10 +48922,10 @@
       <c r="J1406" s="13"/>
     </row>
     <row r="1407" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1407" s="12">
-        <v>44245</v>
-      </c>
-      <c r="B1407" s="9"/>
+      <c r="A1407" s="12"/>
+      <c r="B1407" s="12">
+        <v>44309</v>
+      </c>
       <c r="C1407" s="14" t="s">
         <v>13</v>
       </c>
@@ -48867,7 +48936,7 @@
         <v>647</v>
       </c>
       <c r="F1407" s="10" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="G1407" s="11"/>
       <c r="H1407" s="12"/>
@@ -48875,7 +48944,9 @@
       <c r="J1407" s="13"/>
     </row>
     <row r="1408" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1408" s="12"/>
+      <c r="A1408" s="12">
+        <v>44239</v>
+      </c>
       <c r="B1408" s="9"/>
       <c r="C1408" s="14" t="s">
         <v>13</v>
@@ -48887,7 +48958,7 @@
         <v>647</v>
       </c>
       <c r="F1408" s="10" t="s">
-        <v>1583</v>
+        <v>1607</v>
       </c>
       <c r="G1408" s="11"/>
       <c r="H1408" s="12"/>
@@ -48896,124 +48967,128 @@
     </row>
     <row r="1409" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1409" s="12"/>
-      <c r="B1409" s="9"/>
-      <c r="C1409" s="14"/>
-      <c r="D1409" s="10"/>
-      <c r="E1409" s="11"/>
-      <c r="F1409" s="10"/>
+      <c r="B1409" s="9">
+        <v>44255</v>
+      </c>
+      <c r="C1409" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1409" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1409" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1409" s="10" t="s">
+        <v>1606</v>
+      </c>
       <c r="G1409" s="11"/>
       <c r="H1409" s="12"/>
       <c r="I1409" s="13"/>
       <c r="J1409" s="13"/>
     </row>
     <row r="1410" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1410" s="12">
-        <v>44176</v>
-      </c>
-      <c r="B1410" s="9"/>
+      <c r="A1410" s="12"/>
+      <c r="B1410" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1410" s="14" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D1410" s="10" t="s">
         <v>584</v>
       </c>
       <c r="E1410" s="11" t="s">
-        <v>1353</v>
+        <v>647</v>
       </c>
       <c r="F1410" s="10" t="s">
-        <v>1354</v>
+        <v>1611</v>
       </c>
       <c r="G1410" s="11"/>
       <c r="H1410" s="12"/>
       <c r="I1410" s="13"/>
       <c r="J1410" s="13"/>
     </row>
-    <row r="1411" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1411" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1411" s="9"/>
+    <row r="1411" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1411" s="12"/>
+      <c r="B1411" s="12">
+        <v>44309</v>
+      </c>
       <c r="C1411" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1411" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1411" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1411" s="10" t="s">
-        <v>1661</v>
+        <v>1614</v>
       </c>
       <c r="G1411" s="11"/>
       <c r="H1411" s="12"/>
       <c r="I1411" s="13"/>
-      <c r="J1411" s="13" t="s">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="1412" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1412" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1412" s="9"/>
+      <c r="J1411" s="13"/>
+    </row>
+    <row r="1412" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1412" s="12"/>
+      <c r="B1412" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1412" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1412" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1412" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1412" s="10" t="s">
-        <v>1660</v>
+        <v>1615</v>
       </c>
       <c r="G1412" s="11"/>
       <c r="H1412" s="12"/>
       <c r="I1412" s="13"/>
       <c r="J1412" s="13"/>
     </row>
-    <row r="1413" spans="1:10" ht="84" x14ac:dyDescent="0.2">
+    <row r="1413" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1413" s="12">
-        <v>43864</v>
+        <v>44245</v>
       </c>
       <c r="B1413" s="9"/>
       <c r="C1413" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1413" s="10" t="s">
-        <v>533</v>
+        <v>584</v>
       </c>
       <c r="E1413" s="11" t="s">
-        <v>1580</v>
+        <v>647</v>
       </c>
       <c r="F1413" s="10" t="s">
-        <v>534</v>
+        <v>1612</v>
       </c>
       <c r="G1413" s="11"/>
       <c r="H1413" s="12"/>
       <c r="I1413" s="13"/>
-      <c r="J1413" s="13" t="s">
-        <v>1707</v>
-      </c>
+      <c r="J1413" s="13"/>
     </row>
     <row r="1414" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1414" s="12">
-        <v>44112</v>
-      </c>
+      <c r="A1414" s="12"/>
       <c r="B1414" s="9"/>
       <c r="C1414" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1414" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1414" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1414" s="10" t="s">
-        <v>1097</v>
+        <v>1583</v>
       </c>
       <c r="G1414" s="11"/>
       <c r="H1414" s="12"/>
@@ -49021,22 +49096,12 @@
       <c r="J1414" s="13"/>
     </row>
     <row r="1415" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1415" s="12">
-        <v>44088</v>
-      </c>
+      <c r="A1415" s="12"/>
       <c r="B1415" s="9"/>
-      <c r="C1415" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1415" s="10" t="s">
-        <v>906</v>
-      </c>
-      <c r="E1415" s="11" t="s">
-        <v>685</v>
-      </c>
-      <c r="F1415" s="10" t="s">
-        <v>1011</v>
-      </c>
+      <c r="C1415" s="14"/>
+      <c r="D1415" s="10"/>
+      <c r="E1415" s="11"/>
+      <c r="F1415" s="10"/>
       <c r="G1415" s="11"/>
       <c r="H1415" s="12"/>
       <c r="I1415" s="13"/>
@@ -49044,51 +49109,53 @@
     </row>
     <row r="1416" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1416" s="12">
-        <v>44055</v>
+        <v>44176</v>
       </c>
       <c r="B1416" s="9"/>
       <c r="C1416" s="14" t="s">
-        <v>623</v>
+        <v>8</v>
       </c>
       <c r="D1416" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1416" s="11" t="s">
-        <v>570</v>
+        <v>1353</v>
       </c>
       <c r="F1416" s="10" t="s">
-        <v>903</v>
+        <v>1354</v>
       </c>
       <c r="G1416" s="11"/>
       <c r="H1416" s="12"/>
       <c r="I1416" s="13"/>
       <c r="J1416" s="13"/>
     </row>
-    <row r="1417" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1417" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1417" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1417" s="9"/>
       <c r="C1417" s="14" t="s">
-        <v>623</v>
+        <v>898</v>
       </c>
       <c r="D1417" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1417" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1417" s="10" t="s">
-        <v>902</v>
+        <v>1661</v>
       </c>
       <c r="G1417" s="11"/>
       <c r="H1417" s="12"/>
       <c r="I1417" s="13"/>
-      <c r="J1417" s="13"/>
-    </row>
-    <row r="1418" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1417" s="13" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1418" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1418" s="9"/>
       <c r="C1418" s="14" t="s">
@@ -49098,362 +49165,496 @@
         <v>494</v>
       </c>
       <c r="E1418" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1418" s="10" t="s">
-        <v>900</v>
+        <v>1660</v>
       </c>
       <c r="G1418" s="11"/>
       <c r="H1418" s="12"/>
       <c r="I1418" s="13"/>
       <c r="J1418" s="13"/>
     </row>
-    <row r="1419" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="1419" spans="1:10" ht="84" x14ac:dyDescent="0.2">
       <c r="A1419" s="12">
-        <v>44055</v>
+        <v>43864</v>
       </c>
       <c r="B1419" s="9"/>
       <c r="C1419" s="14" t="s">
-        <v>898</v>
+        <v>19</v>
       </c>
       <c r="D1419" s="10" t="s">
-        <v>494</v>
+        <v>533</v>
       </c>
       <c r="E1419" s="11" t="s">
-        <v>570</v>
+        <v>1580</v>
       </c>
       <c r="F1419" s="10" t="s">
-        <v>901</v>
+        <v>534</v>
       </c>
       <c r="G1419" s="11"/>
       <c r="H1419" s="12"/>
       <c r="I1419" s="13"/>
-      <c r="J1419" s="13"/>
-    </row>
-    <row r="1420" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="J1419" s="13" t="s">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1420" s="12">
-        <v>44055</v>
+        <v>44112</v>
       </c>
       <c r="B1420" s="9"/>
       <c r="C1420" s="14" t="s">
-        <v>898</v>
+        <v>623</v>
       </c>
       <c r="D1420" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1420" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1420" s="10" t="s">
-        <v>904</v>
+        <v>1097</v>
       </c>
       <c r="G1420" s="11"/>
       <c r="H1420" s="12"/>
       <c r="I1420" s="13"/>
-      <c r="J1420" s="13" t="s">
-        <v>1590</v>
-      </c>
-    </row>
-    <row r="1421" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1420" s="13"/>
+    </row>
+    <row r="1421" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1421" s="12">
-        <v>44047</v>
+        <v>44088</v>
       </c>
       <c r="B1421" s="9"/>
       <c r="C1421" s="14" t="s">
-        <v>537</v>
+        <v>19</v>
       </c>
       <c r="D1421" s="10" t="s">
-        <v>6</v>
+        <v>906</v>
       </c>
       <c r="E1421" s="11" t="s">
         <v>685</v>
       </c>
       <c r="F1421" s="10" t="s">
-        <v>873</v>
-      </c>
-      <c r="G1421" s="11" t="s">
-        <v>1626</v>
-      </c>
+        <v>1011</v>
+      </c>
+      <c r="G1421" s="11"/>
       <c r="H1421" s="12"/>
       <c r="I1421" s="13"/>
       <c r="J1421" s="13"/>
     </row>
-    <row r="1422" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1422" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1422" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1422" s="9"/>
       <c r="C1422" s="14" t="s">
-        <v>468</v>
+        <v>623</v>
       </c>
       <c r="D1422" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1422" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1422" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1422" s="11" t="s">
-        <v>1641</v>
-      </c>
+        <v>903</v>
+      </c>
+      <c r="G1422" s="11"/>
       <c r="H1422" s="12"/>
-      <c r="I1422" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1422" s="13"/>
       <c r="J1422" s="13"/>
     </row>
-    <row r="1423" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1423" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1423" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1423" s="9"/>
       <c r="C1423" s="14" t="s">
-        <v>468</v>
+        <v>623</v>
       </c>
       <c r="D1423" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1423" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1423" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1423" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="G1423" s="11"/>
       <c r="H1423" s="12"/>
-      <c r="I1423" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1423" s="13" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="1424" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1423" s="13"/>
+      <c r="J1423" s="13"/>
+    </row>
+    <row r="1424" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1424" s="12">
-        <v>43838</v>
+        <v>44055</v>
       </c>
       <c r="B1424" s="9"/>
       <c r="C1424" s="14" t="s">
-        <v>103</v>
+        <v>898</v>
       </c>
       <c r="D1424" s="10" t="s">
-        <v>460</v>
+        <v>494</v>
       </c>
       <c r="E1424" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1424" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G1424" s="11" t="s">
-        <v>1642</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="G1424" s="11"/>
       <c r="H1424" s="12"/>
       <c r="I1424" s="13"/>
-      <c r="J1424" s="13" t="s">
-        <v>1534</v>
-      </c>
-    </row>
-    <row r="1425" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1424" s="13"/>
+    </row>
+    <row r="1425" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A1425" s="12">
-        <v>43816</v>
+        <v>44055</v>
       </c>
       <c r="B1425" s="9"/>
       <c r="C1425" s="14" t="s">
-        <v>475</v>
+        <v>898</v>
       </c>
       <c r="D1425" s="10" t="s">
-        <v>38</v>
+        <v>494</v>
       </c>
       <c r="E1425" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1425" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="G1425" s="11" t="s">
-        <v>1634</v>
-      </c>
+        <v>901</v>
+      </c>
+      <c r="G1425" s="11"/>
       <c r="H1425" s="12"/>
       <c r="I1425" s="13"/>
-      <c r="J1425" s="13" t="s">
-        <v>1570</v>
-      </c>
-    </row>
-    <row r="1426" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1425" s="13"/>
+    </row>
+    <row r="1426" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1426" s="12">
-        <v>43762</v>
+        <v>44055</v>
       </c>
       <c r="B1426" s="9"/>
       <c r="C1426" s="14" t="s">
-        <v>446</v>
+        <v>898</v>
       </c>
       <c r="D1426" s="10" t="s">
-        <v>17</v>
+        <v>494</v>
       </c>
       <c r="E1426" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1426" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G1426" s="11" t="s">
-        <v>1631</v>
-      </c>
+        <v>904</v>
+      </c>
+      <c r="G1426" s="11"/>
       <c r="H1426" s="12"/>
       <c r="I1426" s="13"/>
-      <c r="J1426" s="13"/>
-    </row>
-    <row r="1427" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1426" s="13" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1427" s="12">
-        <v>44222</v>
+        <v>44047</v>
       </c>
       <c r="B1427" s="9"/>
       <c r="C1427" s="14" t="s">
-        <v>1495</v>
+        <v>537</v>
       </c>
       <c r="D1427" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1427" s="11" t="s">
-        <v>837</v>
+        <v>685</v>
       </c>
       <c r="F1427" s="10" t="s">
-        <v>1494</v>
+        <v>873</v>
       </c>
       <c r="G1427" s="11" t="s">
-        <v>309</v>
+        <v>1626</v>
       </c>
       <c r="H1427" s="12"/>
       <c r="I1427" s="13"/>
       <c r="J1427" s="13"/>
     </row>
-    <row r="1428" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1428" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A1428" s="12">
-        <v>44266</v>
+        <v>43949</v>
       </c>
       <c r="B1428" s="9"/>
       <c r="C1428" s="14" t="s">
-        <v>537</v>
+        <v>468</v>
       </c>
       <c r="D1428" s="10" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="E1428" s="11" t="s">
-        <v>570</v>
+        <v>685</v>
       </c>
       <c r="F1428" s="10" t="s">
-        <v>1715</v>
-      </c>
-      <c r="G1428" s="11"/>
+        <v>686</v>
+      </c>
+      <c r="G1428" s="11" t="s">
+        <v>1641</v>
+      </c>
       <c r="H1428" s="12"/>
-      <c r="I1428" s="13"/>
-      <c r="J1428" s="13" t="s">
-        <v>1716</v>
-      </c>
-    </row>
-    <row r="1429" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1428" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1428" s="13"/>
+    </row>
+    <row r="1429" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A1429" s="12">
-        <v>44286</v>
+        <v>43949</v>
       </c>
       <c r="B1429" s="9"/>
       <c r="C1429" s="14" t="s">
-        <v>288</v>
+        <v>468</v>
       </c>
       <c r="D1429" s="10" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="E1429" s="11" t="s">
-        <v>1580</v>
+        <v>685</v>
       </c>
       <c r="F1429" s="10" t="s">
-        <v>1840</v>
-      </c>
-      <c r="G1429" s="11"/>
+        <v>705</v>
+      </c>
+      <c r="G1429" s="11" t="s">
+        <v>687</v>
+      </c>
       <c r="H1429" s="12"/>
-      <c r="I1429" s="13"/>
-      <c r="J1429" s="13"/>
-    </row>
-    <row r="1430" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1430" s="12"/>
+      <c r="I1429" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1429" s="13" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1430" s="12">
+        <v>43838</v>
+      </c>
       <c r="B1430" s="9"/>
-      <c r="C1430" s="14"/>
-      <c r="D1430" s="10"/>
-      <c r="E1430" s="11"/>
-      <c r="F1430" s="10"/>
-      <c r="G1430" s="11"/>
+      <c r="C1430" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1430" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1430" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1430" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G1430" s="11" t="s">
+        <v>1642</v>
+      </c>
       <c r="H1430" s="12"/>
       <c r="I1430" s="13"/>
-      <c r="J1430" s="13"/>
+      <c r="J1430" s="13" t="s">
+        <v>1534</v>
+      </c>
     </row>
     <row r="1431" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1431" s="12"/>
+      <c r="A1431" s="12">
+        <v>43816</v>
+      </c>
       <c r="B1431" s="9"/>
-      <c r="C1431" s="14"/>
-      <c r="D1431" s="10"/>
-      <c r="E1431" s="11"/>
-      <c r="F1431" s="10"/>
-      <c r="G1431" s="11"/>
+      <c r="C1431" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1431" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1431" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1431" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G1431" s="11" t="s">
+        <v>1634</v>
+      </c>
       <c r="H1431" s="12"/>
       <c r="I1431" s="13"/>
-      <c r="J1431" s="13"/>
-    </row>
-    <row r="1432" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1432" s="12"/>
+      <c r="J1431" s="13" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1432" s="12">
+        <v>43762</v>
+      </c>
       <c r="B1432" s="9"/>
-      <c r="C1432" s="14"/>
-      <c r="D1432" s="10"/>
-      <c r="E1432" s="11"/>
-      <c r="F1432" s="10"/>
-      <c r="G1432" s="11"/>
+      <c r="C1432" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1432" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1432" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1432" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1432" s="11" t="s">
+        <v>1631</v>
+      </c>
       <c r="H1432" s="12"/>
       <c r="I1432" s="13"/>
       <c r="J1432" s="13"/>
     </row>
     <row r="1433" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1433" s="12"/>
+      <c r="A1433" s="12">
+        <v>44222</v>
+      </c>
       <c r="B1433" s="9"/>
-      <c r="C1433" s="14"/>
-      <c r="D1433" s="10"/>
-      <c r="E1433" s="11"/>
-      <c r="F1433" s="10"/>
-      <c r="G1433" s="11"/>
+      <c r="C1433" s="14" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D1433" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1433" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1433" s="10" t="s">
+        <v>1494</v>
+      </c>
+      <c r="G1433" s="11" t="s">
+        <v>309</v>
+      </c>
       <c r="H1433" s="12"/>
       <c r="I1433" s="13"/>
       <c r="J1433" s="13"/>
     </row>
-    <row r="1434" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1434" s="12"/>
+    <row r="1434" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1434" s="12">
+        <v>44266</v>
+      </c>
       <c r="B1434" s="9"/>
-      <c r="C1434" s="14"/>
-      <c r="D1434" s="10"/>
-      <c r="E1434" s="11"/>
-      <c r="F1434" s="10"/>
+      <c r="C1434" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1434" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1434" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1434" s="10" t="s">
+        <v>1715</v>
+      </c>
       <c r="G1434" s="11"/>
       <c r="H1434" s="12"/>
       <c r="I1434" s="13"/>
-      <c r="J1434" s="13"/>
-    </row>
-    <row r="1435" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1435" s="12"/>
+      <c r="J1434" s="13" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1435" s="12">
+        <v>44286</v>
+      </c>
       <c r="B1435" s="9"/>
-      <c r="C1435" s="14"/>
-      <c r="D1435" s="10"/>
-      <c r="E1435" s="11"/>
-      <c r="F1435" s="10"/>
+      <c r="C1435" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1435" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1435" s="11" t="s">
+        <v>1580</v>
+      </c>
+      <c r="F1435" s="10" t="s">
+        <v>1840</v>
+      </c>
       <c r="G1435" s="11"/>
       <c r="H1435" s="12"/>
       <c r="I1435" s="13"/>
       <c r="J1435" s="13"/>
     </row>
+    <row r="1436" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1436" s="12"/>
+      <c r="B1436" s="9"/>
+      <c r="C1436" s="14"/>
+      <c r="D1436" s="10"/>
+      <c r="E1436" s="11"/>
+      <c r="F1436" s="10"/>
+      <c r="G1436" s="11"/>
+      <c r="H1436" s="12"/>
+      <c r="I1436" s="13"/>
+      <c r="J1436" s="13"/>
+    </row>
+    <row r="1437" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1437" s="12"/>
+      <c r="B1437" s="9"/>
+      <c r="C1437" s="14"/>
+      <c r="D1437" s="10"/>
+      <c r="E1437" s="11"/>
+      <c r="F1437" s="10"/>
+      <c r="G1437" s="11"/>
+      <c r="H1437" s="12"/>
+      <c r="I1437" s="13"/>
+      <c r="J1437" s="13"/>
+    </row>
+    <row r="1438" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1438" s="12"/>
+      <c r="B1438" s="9"/>
+      <c r="C1438" s="14"/>
+      <c r="D1438" s="10"/>
+      <c r="E1438" s="11"/>
+      <c r="F1438" s="10"/>
+      <c r="G1438" s="11"/>
+      <c r="H1438" s="12"/>
+      <c r="I1438" s="13"/>
+      <c r="J1438" s="13"/>
+    </row>
+    <row r="1439" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1439" s="12"/>
+      <c r="B1439" s="9"/>
+      <c r="C1439" s="14"/>
+      <c r="D1439" s="10"/>
+      <c r="E1439" s="11"/>
+      <c r="F1439" s="10"/>
+      <c r="G1439" s="11"/>
+      <c r="H1439" s="12"/>
+      <c r="I1439" s="13"/>
+      <c r="J1439" s="13"/>
+    </row>
+    <row r="1440" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1440" s="12"/>
+      <c r="B1440" s="9"/>
+      <c r="C1440" s="14"/>
+      <c r="D1440" s="10"/>
+      <c r="E1440" s="11"/>
+      <c r="F1440" s="10"/>
+      <c r="G1440" s="11"/>
+      <c r="H1440" s="12"/>
+      <c r="I1440" s="13"/>
+      <c r="J1440" s="13"/>
+    </row>
+    <row r="1441" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1441" s="12"/>
+      <c r="B1441" s="9"/>
+      <c r="C1441" s="14"/>
+      <c r="D1441" s="10"/>
+      <c r="E1441" s="11"/>
+      <c r="F1441" s="10"/>
+      <c r="G1441" s="11"/>
+      <c r="H1441" s="12"/>
+      <c r="I1441" s="13"/>
+      <c r="J1441" s="13"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1378" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1397:F1407">
-    <sortCondition ref="F1397:F1407"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1403:F1413">
+    <sortCondition ref="F1403:F1413"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
bkfinr26 - Considerar Ret. Contratual
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FA3E1C-80F9-405D-B1D8-25CECE491BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AAF51A-2AA9-403B-8E62-C3BF7293EB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_FilterDatabase_0" localSheetId="0">'Demandas BK - Protheus'!$A$1:$I$53</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Demandas BK - Protheus'!$A$1:$J$1378</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Demandas BK - Protheus'!$A$1:$J$1395</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9903" uniqueCount="2039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9915" uniqueCount="2041">
   <si>
     <t>Responsável</t>
   </si>
@@ -6485,6 +6485,12 @@
   </si>
   <si>
     <t>Refazimento da rotina que gera relatórios em excel da BK utilizando novas fuções do Protheus</t>
+  </si>
+  <si>
+    <t>Não é possível</t>
+  </si>
+  <si>
+    <t>No calculo do liq da NF e do Saldo a receber, considerar a retenção contratual</t>
   </si>
 </sst>
 </file>
@@ -7254,7 +7260,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1377" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1395" sqref="A1395"/>
+      <selection pane="bottomLeft" activeCell="A1397" sqref="A1397"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -48512,10 +48518,18 @@
       <c r="F1386" s="10" t="s">
         <v>2027</v>
       </c>
-      <c r="G1386" s="11"/>
-      <c r="H1386" s="12"/>
-      <c r="I1386" s="13"/>
-      <c r="J1386" s="13"/>
+      <c r="G1386" s="11" t="s">
+        <v>1625</v>
+      </c>
+      <c r="H1386" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1386" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1386" s="13" t="s">
+        <v>2039</v>
+      </c>
     </row>
     <row r="1387" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1387" s="12">
@@ -48788,16 +48802,36 @@
       <c r="J1395" s="13"/>
     </row>
     <row r="1396" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1396" s="12"/>
-      <c r="B1396" s="12"/>
-      <c r="C1396" s="14"/>
-      <c r="D1396" s="10"/>
-      <c r="E1396" s="11"/>
-      <c r="F1396" s="10"/>
-      <c r="G1396" s="11"/>
-      <c r="H1396" s="12"/>
-      <c r="I1396" s="13"/>
-      <c r="J1396" s="13"/>
+      <c r="A1396" s="12">
+        <v>44376</v>
+      </c>
+      <c r="B1396" s="12">
+        <v>44376</v>
+      </c>
+      <c r="C1396" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1396" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1396" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1396" s="10" t="s">
+        <v>2040</v>
+      </c>
+      <c r="G1396" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1396" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1396" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1396" s="13" t="s">
+        <v>607</v>
+      </c>
     </row>
     <row r="1397" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1397" s="12"/>
@@ -49742,7 +49776,7 @@
       <c r="J1443" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1378" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J1395" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1405:F1415">
     <sortCondition ref="F1405:F1415"/>
   </sortState>

</xml_diff>

<commit_message>
Acerto aviso de pedidos não entregues
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AAF51A-2AA9-403B-8E62-C3BF7293EB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B2D0C1-FA15-4C22-AF63-3B0148CFF5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_FilterDatabase_0" localSheetId="0">'Demandas BK - Protheus'!$A$1:$I$53</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Demandas BK - Protheus'!$A$1:$J$1395</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Demandas BK - Protheus'!$A$1:$J$1402</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9915" uniqueCount="2041">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10025" uniqueCount="2061">
   <si>
     <t>Responsável</t>
   </si>
@@ -6491,6 +6491,66 @@
   </si>
   <si>
     <t>No calculo do liq da NF e do Saldo a receber, considerar a retenção contratual</t>
+  </si>
+  <si>
+    <t>Google Meets</t>
+  </si>
+  <si>
+    <t>Suporte emissão de relatorio de despesas</t>
+  </si>
+  <si>
+    <t>Alterar e-mails do cliente Correios</t>
+  </si>
+  <si>
+    <t>Alterar datas de vencimentos dos titulos do dia 09/07 para o dia 08/07</t>
+  </si>
+  <si>
+    <t>Correção no titulo do financeiro de pensão, "029840-GUILHERME RODRIGUES PEREIRA DOS SANTOS"</t>
+  </si>
+  <si>
+    <t>Iniciado a geração do REINF empresa BK Maio/2020 e Balsa Nova/Bk e consolidação dos DADOS para envio e fechamento do período do REINF.</t>
+  </si>
+  <si>
+    <t>Gerado o titulo de pensão no financeiro, "Pensionista: NOEMY DE SOUZA FARIA – R$ 279,06 Pensionista: MARIA JULIA PEREIRA FARIA – R$ 232,55", conforme solicitado pelo RH.</t>
+  </si>
+  <si>
+    <t>Finalizado analise dos dados REINF empresa BK Maio/2020 e Balsa Nova/Bk e consolidação dos DADOS para envio e fechamento do período do REINF.</t>
+  </si>
+  <si>
+    <t>Ajustado lançamentos, conforme solicitado pelo RH. "Não consegui lançar para esse ex-funcionário abaixo esses 03 títulos como Forma (CLA), no formato normal (CLT) eu consegui, você poderia alterá-lo por gentileza."</t>
+  </si>
+  <si>
+    <t>Gerado o arquivo ECF da Bk base 2020,  enviado para conferencia e envio da contabilidade</t>
+  </si>
+  <si>
+    <t>Programado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instalado novo certificado A1 no serviço de integração do REINF, testes de geração e serviço normalizado. Atualizado as contas referenciais ECD do lucro presumido, teste de geração. </t>
+  </si>
+  <si>
+    <t>Criado rotina para considerar 1 real de saldo ou não na baixa Petrobras quando lançado juros, conforme solicitado pelo financeiro</t>
+  </si>
+  <si>
+    <t>Restaurado e Gerado o arquivo para retificar a DIRF, conforme solicitado pelo RH</t>
+  </si>
+  <si>
+    <t>Analise nas pendências da geração do ECD das demais empresas.</t>
+  </si>
+  <si>
+    <t>Questões fiscais a respeito da NF 18 de Campos dos Goytacazes (foi necessário refazer a NF com retenção de ISS, mesmo isso sendo indevido, devido ao entendimento da Petrobras)</t>
+  </si>
+  <si>
+    <t>Iss de muitas notas emitidas na filial do RJ estão com alíquota errada de ISS</t>
+  </si>
+  <si>
+    <t>Michele Moraes</t>
+  </si>
+  <si>
+    <t>No meu relatorio de pedido de compras não entregue tem que aparecer so os pedidos pendentes e esta entrando no relatório os pedidos "em recebimento - Pre nota ", ele vem o aviso por email Origem: V10BKGct06 01/07/21 21:55:51 - BK</t>
+  </si>
+  <si>
+    <t>BKGCT06</t>
   </si>
 </sst>
 </file>
@@ -7256,11 +7316,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1443"/>
+  <dimension ref="A1:J1461"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1377" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1397" sqref="A1397"/>
+      <pane ySplit="1" topLeftCell="A1405" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1414" sqref="B1414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -47829,89 +47889,87 @@
       </c>
       <c r="J1363" s="13"/>
     </row>
-    <row r="1364" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1364" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1364" s="12">
-        <v>44347</v>
+        <v>44349</v>
       </c>
       <c r="B1364" s="12">
-        <v>44351</v>
+        <v>44349</v>
       </c>
       <c r="C1364" s="14" t="s">
-        <v>2000</v>
+        <v>490</v>
       </c>
       <c r="D1364" s="10" t="s">
-        <v>17</v>
+        <v>491</v>
       </c>
       <c r="E1364" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1364" s="10" t="s">
-        <v>2001</v>
+        <v>2045</v>
       </c>
       <c r="G1364" s="11" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="H1364" s="12" t="s">
         <v>112</v>
       </c>
       <c r="I1364" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1364" s="13" t="s">
-        <v>2002</v>
-      </c>
-    </row>
-    <row r="1365" spans="1:10" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="J1364" s="13"/>
+    </row>
+    <row r="1365" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1365" s="12">
-        <v>44354</v>
+        <v>44349</v>
       </c>
       <c r="B1365" s="12">
-        <v>44354</v>
+        <v>44349</v>
       </c>
       <c r="C1365" s="14" t="s">
-        <v>387</v>
+        <v>2036</v>
       </c>
       <c r="D1365" s="10" t="s">
-        <v>494</v>
+        <v>83</v>
       </c>
       <c r="E1365" s="11" t="s">
-        <v>570</v>
+        <v>620</v>
       </c>
       <c r="F1365" s="10" t="s">
-        <v>2003</v>
+        <v>2046</v>
       </c>
       <c r="G1365" s="11" t="s">
-        <v>309</v>
+        <v>1627</v>
       </c>
       <c r="H1365" s="12" t="s">
         <v>112</v>
       </c>
       <c r="I1365" s="13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J1365" s="13"/>
     </row>
     <row r="1366" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1366" s="12">
-        <v>44354</v>
+        <v>44347</v>
       </c>
       <c r="B1366" s="12">
-        <v>44354</v>
+        <v>44351</v>
       </c>
       <c r="C1366" s="14" t="s">
-        <v>1159</v>
+        <v>2000</v>
       </c>
       <c r="D1366" s="10" t="s">
-        <v>107</v>
+        <v>17</v>
       </c>
       <c r="E1366" s="11" t="s">
-        <v>620</v>
+        <v>570</v>
       </c>
       <c r="F1366" s="10" t="s">
-        <v>2004</v>
+        <v>2001</v>
       </c>
       <c r="G1366" s="11" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="H1366" s="12" t="s">
         <v>112</v>
@@ -47919,9 +47977,11 @@
       <c r="I1366" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1366" s="13"/>
-    </row>
-    <row r="1367" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1366" s="13" t="s">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1367" s="12">
         <v>44354</v>
       </c>
@@ -47929,19 +47989,19 @@
         <v>44354</v>
       </c>
       <c r="C1367" s="14" t="s">
-        <v>559</v>
+        <v>387</v>
       </c>
       <c r="D1367" s="10" t="s">
-        <v>107</v>
+        <v>494</v>
       </c>
       <c r="E1367" s="11" t="s">
-        <v>620</v>
+        <v>570</v>
       </c>
       <c r="F1367" s="10" t="s">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="G1367" s="11" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="H1367" s="12" t="s">
         <v>112</v>
@@ -47959,19 +48019,19 @@
         <v>44354</v>
       </c>
       <c r="C1368" s="14" t="s">
-        <v>1994</v>
+        <v>1159</v>
       </c>
       <c r="D1368" s="10" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="E1368" s="11" t="s">
         <v>620</v>
       </c>
       <c r="F1368" s="10" t="s">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="G1368" s="11" t="s">
-        <v>1648</v>
+        <v>295</v>
       </c>
       <c r="H1368" s="12" t="s">
         <v>112</v>
@@ -47981,24 +48041,24 @@
       </c>
       <c r="J1368" s="13"/>
     </row>
-    <row r="1369" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1369" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1369" s="12">
-        <v>44355</v>
+        <v>44354</v>
       </c>
       <c r="B1369" s="12">
-        <v>44355</v>
+        <v>44354</v>
       </c>
       <c r="C1369" s="14" t="s">
-        <v>387</v>
+        <v>559</v>
       </c>
       <c r="D1369" s="10" t="s">
-        <v>494</v>
+        <v>107</v>
       </c>
       <c r="E1369" s="11" t="s">
         <v>620</v>
       </c>
       <c r="F1369" s="10" t="s">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="G1369" s="11" t="s">
         <v>295</v>
@@ -48013,10 +48073,10 @@
     </row>
     <row r="1370" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1370" s="12">
-        <v>44355</v>
+        <v>44354</v>
       </c>
       <c r="B1370" s="12">
-        <v>44355</v>
+        <v>44354</v>
       </c>
       <c r="C1370" s="14" t="s">
         <v>1994</v>
@@ -48028,10 +48088,10 @@
         <v>620</v>
       </c>
       <c r="F1370" s="10" t="s">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="G1370" s="11" t="s">
-        <v>295</v>
+        <v>1648</v>
       </c>
       <c r="H1370" s="12" t="s">
         <v>112</v>
@@ -48049,19 +48109,19 @@
         <v>44355</v>
       </c>
       <c r="C1371" s="14" t="s">
-        <v>66</v>
+        <v>387</v>
       </c>
       <c r="D1371" s="10" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="E1371" s="11" t="s">
         <v>620</v>
       </c>
       <c r="F1371" s="10" t="s">
-        <v>2014</v>
+        <v>2007</v>
       </c>
       <c r="G1371" s="11" t="s">
-        <v>1626</v>
+        <v>295</v>
       </c>
       <c r="H1371" s="12" t="s">
         <v>112</v>
@@ -48073,22 +48133,22 @@
     </row>
     <row r="1372" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1372" s="12">
-        <v>44357</v>
+        <v>44355</v>
       </c>
       <c r="B1372" s="12">
-        <v>44357</v>
+        <v>44355</v>
       </c>
       <c r="C1372" s="14" t="s">
-        <v>387</v>
+        <v>1994</v>
       </c>
       <c r="D1372" s="10" t="s">
-        <v>494</v>
+        <v>89</v>
       </c>
       <c r="E1372" s="11" t="s">
-        <v>685</v>
+        <v>620</v>
       </c>
       <c r="F1372" s="10" t="s">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="G1372" s="11" t="s">
         <v>295</v>
@@ -48101,27 +48161,27 @@
       </c>
       <c r="J1372" s="13"/>
     </row>
-    <row r="1373" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="1373" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1373" s="12">
-        <v>44357</v>
+        <v>44355</v>
       </c>
       <c r="B1373" s="12">
-        <v>44357</v>
+        <v>44355</v>
       </c>
       <c r="C1373" s="14" t="s">
-        <v>2000</v>
+        <v>66</v>
       </c>
       <c r="D1373" s="10" t="s">
-        <v>17</v>
+        <v>491</v>
       </c>
       <c r="E1373" s="11" t="s">
-        <v>669</v>
+        <v>620</v>
       </c>
       <c r="F1373" s="10" t="s">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="G1373" s="11" t="s">
-        <v>309</v>
+        <v>1626</v>
       </c>
       <c r="H1373" s="12" t="s">
         <v>112</v>
@@ -48131,86 +48191,78 @@
       </c>
       <c r="J1373" s="13"/>
     </row>
-    <row r="1374" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="1374" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1374" s="12">
-        <v>44357</v>
+        <v>44356</v>
       </c>
       <c r="B1374" s="12">
-        <v>44357</v>
+        <v>44356</v>
       </c>
       <c r="C1374" s="14" t="s">
-        <v>46</v>
+        <v>490</v>
       </c>
       <c r="D1374" s="10" t="s">
-        <v>2013</v>
+        <v>491</v>
       </c>
       <c r="E1374" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1374" s="10" t="s">
+        <v>2047</v>
+      </c>
+      <c r="G1374" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1374" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1374" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1374" s="13"/>
+    </row>
+    <row r="1375" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1375" s="12">
+        <v>44356</v>
+      </c>
+      <c r="B1375" s="12">
+        <v>44356</v>
+      </c>
+      <c r="C1375" s="14" t="s">
+        <v>2036</v>
+      </c>
+      <c r="D1375" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1375" s="11" t="s">
         <v>620</v>
       </c>
-      <c r="F1374" s="10" t="s">
-        <v>2012</v>
-      </c>
-      <c r="G1374" s="11" t="s">
-        <v>1668</v>
-      </c>
-      <c r="H1374" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1374" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1374" s="13"/>
-    </row>
-    <row r="1375" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1375" s="12">
-        <v>44358</v>
-      </c>
-      <c r="B1375" s="12">
-        <v>44358</v>
-      </c>
-      <c r="C1375" s="14" t="s">
-        <v>1159</v>
-      </c>
-      <c r="D1375" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1375" s="11" t="s">
-        <v>685</v>
-      </c>
       <c r="F1375" s="10" t="s">
-        <v>2009</v>
-      </c>
-      <c r="G1375" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="H1375" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1375" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1375" s="13" t="s">
-        <v>2010</v>
-      </c>
+        <v>2048</v>
+      </c>
+      <c r="G1375" s="11"/>
+      <c r="H1375" s="12"/>
+      <c r="I1375" s="13"/>
+      <c r="J1375" s="13"/>
     </row>
     <row r="1376" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1376" s="12">
-        <v>44279</v>
-      </c>
-      <c r="B1376" s="9">
-        <v>44361</v>
+        <v>44357</v>
+      </c>
+      <c r="B1376" s="12">
+        <v>44357</v>
       </c>
       <c r="C1376" s="14" t="s">
-        <v>1388</v>
+        <v>387</v>
       </c>
       <c r="D1376" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1376" s="11" t="s">
-        <v>620</v>
+        <v>685</v>
       </c>
       <c r="F1376" s="10" t="s">
-        <v>1732</v>
+        <v>2011</v>
       </c>
       <c r="G1376" s="11" t="s">
         <v>295</v>
@@ -48223,24 +48275,24 @@
       </c>
       <c r="J1376" s="13"/>
     </row>
-    <row r="1377" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1377" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1377" s="12">
-        <v>44361</v>
-      </c>
-      <c r="B1377" s="9">
-        <v>44361</v>
+        <v>44357</v>
+      </c>
+      <c r="B1377" s="12">
+        <v>44357</v>
       </c>
       <c r="C1377" s="14" t="s">
-        <v>527</v>
+        <v>2000</v>
       </c>
       <c r="D1377" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E1377" s="11" t="s">
-        <v>837</v>
+        <v>669</v>
       </c>
       <c r="F1377" s="10" t="s">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="G1377" s="11" t="s">
         <v>309</v>
@@ -48251,31 +48303,29 @@
       <c r="I1377" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1377" s="13" t="s">
-        <v>2016</v>
-      </c>
+      <c r="J1377" s="13"/>
     </row>
     <row r="1378" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1378" s="12">
-        <v>44361</v>
-      </c>
-      <c r="B1378" s="9">
-        <v>44361</v>
+        <v>44357</v>
+      </c>
+      <c r="B1378" s="12">
+        <v>44357</v>
       </c>
       <c r="C1378" s="14" t="s">
-        <v>898</v>
+        <v>46</v>
       </c>
       <c r="D1378" s="10" t="s">
-        <v>1834</v>
+        <v>2013</v>
       </c>
       <c r="E1378" s="11" t="s">
-        <v>570</v>
+        <v>620</v>
       </c>
       <c r="F1378" s="10" t="s">
-        <v>1961</v>
+        <v>2012</v>
       </c>
       <c r="G1378" s="11" t="s">
-        <v>1648</v>
+        <v>1668</v>
       </c>
       <c r="H1378" s="12" t="s">
         <v>112</v>
@@ -48283,31 +48333,29 @@
       <c r="I1378" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1378" s="13" t="s">
-        <v>2022</v>
-      </c>
+      <c r="J1378" s="13"/>
     </row>
     <row r="1379" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1379" s="12">
-        <v>44361</v>
-      </c>
-      <c r="B1379" s="9">
-        <v>44361</v>
+        <v>44358</v>
+      </c>
+      <c r="B1379" s="12">
+        <v>44358</v>
       </c>
       <c r="C1379" s="14" t="s">
-        <v>932</v>
+        <v>1159</v>
       </c>
       <c r="D1379" s="10" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="E1379" s="11" t="s">
-        <v>620</v>
+        <v>685</v>
       </c>
       <c r="F1379" s="10" t="s">
-        <v>2017</v>
+        <v>2009</v>
       </c>
       <c r="G1379" s="11" t="s">
-        <v>1648</v>
+        <v>295</v>
       </c>
       <c r="H1379" s="12" t="s">
         <v>112</v>
@@ -48316,30 +48364,30 @@
         <v>13</v>
       </c>
       <c r="J1379" s="13" t="s">
-        <v>2018</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="1380" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1380" s="12">
-        <v>44361</v>
+        <v>44279</v>
       </c>
       <c r="B1380" s="9">
         <v>44361</v>
       </c>
       <c r="C1380" s="14" t="s">
-        <v>1198</v>
+        <v>1388</v>
       </c>
       <c r="D1380" s="10" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="E1380" s="11" t="s">
-        <v>837</v>
+        <v>620</v>
       </c>
       <c r="F1380" s="10" t="s">
-        <v>2019</v>
+        <v>1732</v>
       </c>
       <c r="G1380" s="11" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="H1380" s="12" t="s">
         <v>112</v>
@@ -48357,19 +48405,19 @@
         <v>44361</v>
       </c>
       <c r="C1381" s="14" t="s">
-        <v>1283</v>
+        <v>527</v>
       </c>
       <c r="D1381" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E1381" s="11" t="s">
-        <v>620</v>
+        <v>837</v>
       </c>
       <c r="F1381" s="10" t="s">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="G1381" s="11" t="s">
-        <v>1623</v>
+        <v>309</v>
       </c>
       <c r="H1381" s="12" t="s">
         <v>112</v>
@@ -48377,9 +48425,11 @@
       <c r="I1381" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1381" s="13"/>
-    </row>
-    <row r="1382" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1381" s="13" t="s">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1382" s="12">
         <v>44361</v>
       </c>
@@ -48387,19 +48437,19 @@
         <v>44361</v>
       </c>
       <c r="C1382" s="14" t="s">
-        <v>2021</v>
+        <v>898</v>
       </c>
       <c r="D1382" s="10" t="s">
-        <v>89</v>
+        <v>1834</v>
       </c>
       <c r="E1382" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1382" s="10" t="s">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="G1382" s="11" t="s">
-        <v>308</v>
+        <v>1648</v>
       </c>
       <c r="H1382" s="12" t="s">
         <v>112</v>
@@ -48407,29 +48457,31 @@
       <c r="I1382" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1382" s="13"/>
+      <c r="J1382" s="13" t="s">
+        <v>2022</v>
+      </c>
     </row>
     <row r="1383" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1383" s="12">
-        <v>44362</v>
-      </c>
-      <c r="B1383" s="12">
-        <v>44362</v>
+        <v>44361</v>
+      </c>
+      <c r="B1383" s="9">
+        <v>44361</v>
       </c>
       <c r="C1383" s="14" t="s">
-        <v>1056</v>
+        <v>932</v>
       </c>
       <c r="D1383" s="10" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="E1383" s="11" t="s">
         <v>620</v>
       </c>
       <c r="F1383" s="10" t="s">
-        <v>2024</v>
+        <v>2017</v>
       </c>
       <c r="G1383" s="11" t="s">
-        <v>295</v>
+        <v>1648</v>
       </c>
       <c r="H1383" s="12" t="s">
         <v>112</v>
@@ -48437,26 +48489,28 @@
       <c r="I1383" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1383" s="13"/>
+      <c r="J1383" s="13" t="s">
+        <v>2018</v>
+      </c>
     </row>
     <row r="1384" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1384" s="12">
-        <v>44362</v>
-      </c>
-      <c r="B1384" s="12">
-        <v>44362</v>
+        <v>44361</v>
+      </c>
+      <c r="B1384" s="9">
+        <v>44361</v>
       </c>
       <c r="C1384" s="14" t="s">
-        <v>13</v>
+        <v>1198</v>
       </c>
       <c r="D1384" s="10" t="s">
-        <v>584</v>
+        <v>6</v>
       </c>
       <c r="E1384" s="11" t="s">
-        <v>698</v>
+        <v>837</v>
       </c>
       <c r="F1384" s="10" t="s">
-        <v>2025</v>
+        <v>2019</v>
       </c>
       <c r="G1384" s="11" t="s">
         <v>309</v>
@@ -48471,25 +48525,25 @@
     </row>
     <row r="1385" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1385" s="12">
-        <v>44362</v>
-      </c>
-      <c r="B1385" s="12">
-        <v>44362</v>
+        <v>44361</v>
+      </c>
+      <c r="B1385" s="9">
+        <v>44361</v>
       </c>
       <c r="C1385" s="14" t="s">
-        <v>13</v>
+        <v>1283</v>
       </c>
       <c r="D1385" s="10" t="s">
-        <v>584</v>
+        <v>17</v>
       </c>
       <c r="E1385" s="11" t="s">
-        <v>698</v>
+        <v>620</v>
       </c>
       <c r="F1385" s="10" t="s">
-        <v>2026</v>
+        <v>2020</v>
       </c>
       <c r="G1385" s="11" t="s">
-        <v>1627</v>
+        <v>1623</v>
       </c>
       <c r="H1385" s="12" t="s">
         <v>112</v>
@@ -48501,25 +48555,25 @@
     </row>
     <row r="1386" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1386" s="12">
-        <v>44364</v>
-      </c>
-      <c r="B1386" s="12">
-        <v>44364</v>
+        <v>44361</v>
+      </c>
+      <c r="B1386" s="9">
+        <v>44361</v>
       </c>
       <c r="C1386" s="14" t="s">
-        <v>19</v>
+        <v>2021</v>
       </c>
       <c r="D1386" s="10" t="s">
-        <v>494</v>
+        <v>89</v>
       </c>
       <c r="E1386" s="11" t="s">
-        <v>669</v>
+        <v>837</v>
       </c>
       <c r="F1386" s="10" t="s">
-        <v>2027</v>
+        <v>2023</v>
       </c>
       <c r="G1386" s="11" t="s">
-        <v>1625</v>
+        <v>308</v>
       </c>
       <c r="H1386" s="12" t="s">
         <v>112</v>
@@ -48527,31 +48581,29 @@
       <c r="I1386" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1386" s="13" t="s">
-        <v>2039</v>
-      </c>
-    </row>
-    <row r="1387" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1386" s="13"/>
+    </row>
+    <row r="1387" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1387" s="12">
-        <v>44365</v>
+        <v>44362</v>
       </c>
       <c r="B1387" s="12">
-        <v>44365</v>
+        <v>44362</v>
       </c>
       <c r="C1387" s="14" t="s">
-        <v>19</v>
+        <v>1056</v>
       </c>
       <c r="D1387" s="10" t="s">
-        <v>494</v>
+        <v>83</v>
       </c>
       <c r="E1387" s="11" t="s">
-        <v>669</v>
+        <v>620</v>
       </c>
       <c r="F1387" s="10" t="s">
-        <v>2028</v>
+        <v>2024</v>
       </c>
       <c r="G1387" s="11" t="s">
-        <v>1627</v>
+        <v>295</v>
       </c>
       <c r="H1387" s="12" t="s">
         <v>112</v>
@@ -48563,22 +48615,22 @@
     </row>
     <row r="1388" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1388" s="12">
-        <v>44365</v>
+        <v>44362</v>
       </c>
       <c r="B1388" s="12">
-        <v>44367</v>
+        <v>44362</v>
       </c>
       <c r="C1388" s="14" t="s">
-        <v>2021</v>
+        <v>13</v>
       </c>
       <c r="D1388" s="10" t="s">
-        <v>89</v>
+        <v>584</v>
       </c>
       <c r="E1388" s="11" t="s">
-        <v>620</v>
+        <v>698</v>
       </c>
       <c r="F1388" s="10" t="s">
-        <v>2029</v>
+        <v>2025</v>
       </c>
       <c r="G1388" s="11" t="s">
         <v>309</v>
@@ -48593,25 +48645,25 @@
     </row>
     <row r="1389" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1389" s="12">
-        <v>44367</v>
+        <v>44362</v>
       </c>
       <c r="B1389" s="12">
-        <v>44367</v>
+        <v>44362</v>
       </c>
       <c r="C1389" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1389" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1389" s="11" t="s">
-        <v>1834</v>
+        <v>698</v>
       </c>
       <c r="F1389" s="10" t="s">
-        <v>2030</v>
+        <v>2026</v>
       </c>
       <c r="G1389" s="11" t="s">
-        <v>309</v>
+        <v>1627</v>
       </c>
       <c r="H1389" s="12" t="s">
         <v>112</v>
@@ -48621,24 +48673,24 @@
       </c>
       <c r="J1389" s="13"/>
     </row>
-    <row r="1390" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1390" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1390" s="12">
-        <v>44369</v>
+        <v>44363</v>
       </c>
       <c r="B1390" s="12">
-        <v>44369</v>
+        <v>44363</v>
       </c>
       <c r="C1390" s="14" t="s">
-        <v>575</v>
+        <v>490</v>
       </c>
       <c r="D1390" s="10" t="s">
-        <v>107</v>
+        <v>491</v>
       </c>
       <c r="E1390" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1390" s="10" t="s">
-        <v>2031</v>
+        <v>2049</v>
       </c>
       <c r="G1390" s="11" t="s">
         <v>295</v>
@@ -48647,61 +48699,61 @@
         <v>112</v>
       </c>
       <c r="I1390" s="13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J1390" s="13"/>
     </row>
-    <row r="1391" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1391" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1391" s="12">
-        <v>44369</v>
+        <v>44363</v>
       </c>
       <c r="B1391" s="12">
-        <v>44369</v>
+        <v>44363</v>
       </c>
       <c r="C1391" s="14" t="s">
-        <v>2032</v>
+        <v>2036</v>
       </c>
       <c r="D1391" s="10" t="s">
-        <v>491</v>
+        <v>83</v>
       </c>
       <c r="E1391" s="11" t="s">
-        <v>570</v>
+        <v>2051</v>
       </c>
       <c r="F1391" s="10" t="s">
-        <v>2033</v>
+        <v>2050</v>
       </c>
       <c r="G1391" s="11" t="s">
-        <v>295</v>
+        <v>1627</v>
       </c>
       <c r="H1391" s="12" t="s">
         <v>112</v>
       </c>
       <c r="I1391" s="13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J1391" s="13"/>
     </row>
     <row r="1392" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1392" s="12">
-        <v>44370</v>
+        <v>44364</v>
       </c>
       <c r="B1392" s="12">
-        <v>44370</v>
+        <v>44364</v>
       </c>
       <c r="C1392" s="14" t="s">
-        <v>1994</v>
+        <v>19</v>
       </c>
       <c r="D1392" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1392" s="11" t="s">
-        <v>837</v>
+        <v>669</v>
       </c>
       <c r="F1392" s="10" t="s">
-        <v>2034</v>
+        <v>2027</v>
       </c>
       <c r="G1392" s="11" t="s">
-        <v>295</v>
+        <v>1625</v>
       </c>
       <c r="H1392" s="12" t="s">
         <v>112</v>
@@ -48709,29 +48761,31 @@
       <c r="I1392" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1392" s="13"/>
+      <c r="J1392" s="13" t="s">
+        <v>2039</v>
+      </c>
     </row>
     <row r="1393" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1393" s="12">
-        <v>44372</v>
+        <v>44365</v>
       </c>
       <c r="B1393" s="12">
-        <v>44372</v>
+        <v>44365</v>
       </c>
       <c r="C1393" s="14" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D1393" s="10" t="s">
-        <v>584</v>
+        <v>494</v>
       </c>
       <c r="E1393" s="11" t="s">
-        <v>698</v>
+        <v>669</v>
       </c>
       <c r="F1393" s="10" t="s">
-        <v>2038</v>
+        <v>2028</v>
       </c>
       <c r="G1393" s="11" t="s">
-        <v>1631</v>
+        <v>1627</v>
       </c>
       <c r="H1393" s="12" t="s">
         <v>112</v>
@@ -48743,25 +48797,25 @@
     </row>
     <row r="1394" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1394" s="12">
-        <v>44375</v>
+        <v>44365</v>
       </c>
       <c r="B1394" s="12">
-        <v>44375</v>
+        <v>44367</v>
       </c>
       <c r="C1394" s="14" t="s">
-        <v>2036</v>
+        <v>2021</v>
       </c>
       <c r="D1394" s="10" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E1394" s="11" t="s">
-        <v>837</v>
+        <v>620</v>
       </c>
       <c r="F1394" s="10" t="s">
-        <v>2037</v>
+        <v>2029</v>
       </c>
       <c r="G1394" s="11" t="s">
-        <v>1631</v>
+        <v>309</v>
       </c>
       <c r="H1394" s="12" t="s">
         <v>112</v>
@@ -48773,22 +48827,22 @@
     </row>
     <row r="1395" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1395" s="12">
-        <v>44376</v>
+        <v>44367</v>
       </c>
       <c r="B1395" s="12">
-        <v>44376</v>
+        <v>44367</v>
       </c>
       <c r="C1395" s="14" t="s">
-        <v>1159</v>
+        <v>898</v>
       </c>
       <c r="D1395" s="10" t="s">
-        <v>107</v>
+        <v>494</v>
       </c>
       <c r="E1395" s="11" t="s">
-        <v>620</v>
+        <v>1834</v>
       </c>
       <c r="F1395" s="10" t="s">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="G1395" s="11" t="s">
         <v>309</v>
@@ -48803,353 +48857,525 @@
     </row>
     <row r="1396" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1396" s="12">
+        <v>44369</v>
+      </c>
+      <c r="B1396" s="12">
+        <v>44369</v>
+      </c>
+      <c r="C1396" s="14" t="s">
+        <v>575</v>
+      </c>
+      <c r="D1396" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1396" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1396" s="10" t="s">
+        <v>2031</v>
+      </c>
+      <c r="G1396" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1396" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1396" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1396" s="13"/>
+    </row>
+    <row r="1397" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1397" s="12">
+        <v>44369</v>
+      </c>
+      <c r="B1397" s="12">
+        <v>44369</v>
+      </c>
+      <c r="C1397" s="14" t="s">
+        <v>2032</v>
+      </c>
+      <c r="D1397" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="E1397" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1397" s="10" t="s">
+        <v>2033</v>
+      </c>
+      <c r="G1397" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1397" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1397" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1397" s="13"/>
+    </row>
+    <row r="1398" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1398" s="12">
+        <v>44370</v>
+      </c>
+      <c r="B1398" s="12">
+        <v>44370</v>
+      </c>
+      <c r="C1398" s="14" t="s">
+        <v>2036</v>
+      </c>
+      <c r="D1398" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1398" s="11" t="s">
+        <v>2051</v>
+      </c>
+      <c r="F1398" s="10" t="s">
+        <v>2052</v>
+      </c>
+      <c r="G1398" s="11" t="s">
+        <v>1631</v>
+      </c>
+      <c r="H1398" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1398" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1398" s="13"/>
+    </row>
+    <row r="1399" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1399" s="12">
+        <v>44370</v>
+      </c>
+      <c r="B1399" s="12">
+        <v>44370</v>
+      </c>
+      <c r="C1399" s="14" t="s">
+        <v>1994</v>
+      </c>
+      <c r="D1399" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1399" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1399" s="10" t="s">
+        <v>2034</v>
+      </c>
+      <c r="G1399" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1399" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1399" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1399" s="13"/>
+    </row>
+    <row r="1400" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1400" s="12">
+        <v>44372</v>
+      </c>
+      <c r="B1400" s="12">
+        <v>44372</v>
+      </c>
+      <c r="C1400" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1400" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1400" s="11" t="s">
+        <v>698</v>
+      </c>
+      <c r="F1400" s="10" t="s">
+        <v>2038</v>
+      </c>
+      <c r="G1400" s="11" t="s">
+        <v>1631</v>
+      </c>
+      <c r="H1400" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1400" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1400" s="13"/>
+    </row>
+    <row r="1401" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1401" s="12">
+        <v>44375</v>
+      </c>
+      <c r="B1401" s="12">
+        <v>44375</v>
+      </c>
+      <c r="C1401" s="14" t="s">
+        <v>2036</v>
+      </c>
+      <c r="D1401" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1401" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1401" s="10" t="s">
+        <v>2037</v>
+      </c>
+      <c r="G1401" s="11" t="s">
+        <v>1631</v>
+      </c>
+      <c r="H1401" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1401" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1401" s="13"/>
+    </row>
+    <row r="1402" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1402" s="12">
         <v>44376</v>
       </c>
-      <c r="B1396" s="12">
+      <c r="B1402" s="12">
         <v>44376</v>
       </c>
-      <c r="C1396" s="14" t="s">
+      <c r="C1402" s="14" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D1402" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1402" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1402" s="10" t="s">
+        <v>2035</v>
+      </c>
+      <c r="G1402" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1402" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1402" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1402" s="13"/>
+    </row>
+    <row r="1403" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1403" s="12">
+        <v>44376</v>
+      </c>
+      <c r="B1403" s="12">
+        <v>44376</v>
+      </c>
+      <c r="C1403" s="14" t="s">
         <v>537</v>
       </c>
-      <c r="D1396" s="10" t="s">
+      <c r="D1403" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E1396" s="11" t="s">
+      <c r="E1403" s="11" t="s">
         <v>620</v>
       </c>
-      <c r="F1396" s="10" t="s">
+      <c r="F1403" s="10" t="s">
         <v>2040</v>
       </c>
-      <c r="G1396" s="11" t="s">
+      <c r="G1403" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="H1396" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1396" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1396" s="13" t="s">
+      <c r="H1403" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1403" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1403" s="13" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="1397" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1397" s="12"/>
-      <c r="B1397" s="12"/>
-      <c r="C1397" s="14"/>
-      <c r="D1397" s="10"/>
-      <c r="E1397" s="11"/>
-      <c r="F1397" s="10"/>
-      <c r="G1397" s="11"/>
-      <c r="H1397" s="12"/>
-      <c r="I1397" s="13"/>
-      <c r="J1397" s="13"/>
-    </row>
-    <row r="1398" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1398" s="12"/>
-      <c r="B1398" s="12"/>
-      <c r="C1398" s="14"/>
-      <c r="D1398" s="10"/>
-      <c r="E1398" s="11"/>
-      <c r="F1398" s="10"/>
-      <c r="G1398" s="11"/>
-      <c r="H1398" s="12"/>
-      <c r="I1398" s="13"/>
-      <c r="J1398" s="13"/>
-    </row>
-    <row r="1399" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1399" s="12"/>
-      <c r="B1399" s="12"/>
-      <c r="C1399" s="14"/>
-      <c r="D1399" s="10"/>
-      <c r="E1399" s="11"/>
-      <c r="F1399" s="10"/>
-      <c r="G1399" s="11"/>
-      <c r="H1399" s="12"/>
-      <c r="I1399" s="13"/>
-      <c r="J1399" s="13"/>
-    </row>
-    <row r="1400" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1400" s="12"/>
-      <c r="B1400" s="12"/>
-      <c r="C1400" s="14"/>
-      <c r="D1400" s="10"/>
-      <c r="E1400" s="11"/>
-      <c r="F1400" s="10"/>
-      <c r="G1400" s="11"/>
-      <c r="H1400" s="12"/>
-      <c r="I1400" s="13"/>
-      <c r="J1400" s="13"/>
-    </row>
-    <row r="1401" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1401" s="12"/>
-      <c r="B1401" s="9"/>
-      <c r="C1401" s="14"/>
-      <c r="D1401" s="10"/>
-      <c r="E1401" s="11"/>
-      <c r="F1401" s="10"/>
-      <c r="G1401" s="11"/>
-      <c r="H1401" s="12"/>
-      <c r="I1401" s="13"/>
-      <c r="J1401" s="13"/>
-    </row>
-    <row r="1402" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1402" s="1" t="s">
-        <v>1479</v>
-      </c>
-      <c r="B1402" s="2" t="s">
-        <v>1480</v>
-      </c>
-      <c r="C1402" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1402" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1402" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1402" s="4" t="s">
-        <v>1581</v>
-      </c>
-      <c r="G1402" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1402" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1402" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1402" s="36"/>
-    </row>
-    <row r="1403" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1403" s="12"/>
-      <c r="B1403" s="9"/>
-      <c r="C1403" s="14"/>
-      <c r="D1403" s="10"/>
-      <c r="E1403" s="11"/>
-      <c r="F1403" s="10"/>
-      <c r="G1403" s="11"/>
-      <c r="H1403" s="12"/>
-      <c r="I1403" s="13"/>
-      <c r="J1403" s="13"/>
-    </row>
-    <row r="1404" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1404" s="12"/>
-      <c r="B1404" s="9">
-        <v>44255</v>
+    <row r="1404" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1404" s="12">
+        <v>44377</v>
+      </c>
+      <c r="B1404" s="12">
+        <v>44377</v>
       </c>
       <c r="C1404" s="14" t="s">
-        <v>13</v>
+        <v>387</v>
       </c>
       <c r="D1404" s="10" t="s">
-        <v>584</v>
+        <v>494</v>
       </c>
       <c r="E1404" s="11" t="s">
-        <v>647</v>
+        <v>2041</v>
       </c>
       <c r="F1404" s="10" t="s">
-        <v>1616</v>
-      </c>
-      <c r="G1404" s="11"/>
-      <c r="H1404" s="12"/>
-      <c r="I1404" s="13"/>
+        <v>2056</v>
+      </c>
+      <c r="G1404" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1404" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1404" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1404" s="13"/>
     </row>
-    <row r="1405" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1405" s="12"/>
-      <c r="B1405" s="9">
-        <v>44255</v>
+    <row r="1405" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1405" s="12">
+        <v>44377</v>
+      </c>
+      <c r="B1405" s="12">
+        <v>44377</v>
       </c>
       <c r="C1405" s="14" t="s">
-        <v>13</v>
+        <v>559</v>
       </c>
       <c r="D1405" s="10" t="s">
-        <v>584</v>
+        <v>6</v>
       </c>
       <c r="E1405" s="11" t="s">
-        <v>647</v>
+        <v>685</v>
       </c>
       <c r="F1405" s="10" t="s">
-        <v>1608</v>
-      </c>
-      <c r="G1405" s="11"/>
-      <c r="H1405" s="12"/>
-      <c r="I1405" s="13"/>
+        <v>2053</v>
+      </c>
+      <c r="G1405" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H1405" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1405" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="J1405" s="13"/>
     </row>
     <row r="1406" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1406" s="12"/>
-      <c r="B1406" s="9">
-        <v>44255</v>
+      <c r="A1406" s="12">
+        <v>44377</v>
+      </c>
+      <c r="B1406" s="12">
+        <v>44377</v>
       </c>
       <c r="C1406" s="14" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="D1406" s="10" t="s">
-        <v>584</v>
+        <v>491</v>
       </c>
       <c r="E1406" s="11" t="s">
-        <v>647</v>
+        <v>620</v>
       </c>
       <c r="F1406" s="10" t="s">
-        <v>1613</v>
-      </c>
-      <c r="G1406" s="11"/>
-      <c r="H1406" s="12"/>
-      <c r="I1406" s="13"/>
+        <v>2054</v>
+      </c>
+      <c r="G1406" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1406" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1406" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="J1406" s="13"/>
     </row>
     <row r="1407" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1407" s="12"/>
-      <c r="B1407" s="9">
-        <v>44255</v>
+      <c r="A1407" s="12">
+        <v>44377</v>
+      </c>
+      <c r="B1407" s="12">
+        <v>44377</v>
       </c>
       <c r="C1407" s="14" t="s">
-        <v>13</v>
+        <v>2036</v>
       </c>
       <c r="D1407" s="10" t="s">
-        <v>584</v>
+        <v>83</v>
       </c>
       <c r="E1407" s="11" t="s">
-        <v>647</v>
+        <v>620</v>
       </c>
       <c r="F1407" s="10" t="s">
-        <v>1609</v>
-      </c>
-      <c r="G1407" s="11"/>
-      <c r="H1407" s="12"/>
-      <c r="I1407" s="13"/>
+        <v>2055</v>
+      </c>
+      <c r="G1407" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1407" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1407" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="J1407" s="13"/>
     </row>
     <row r="1408" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1408" s="12">
-        <v>44159</v>
-      </c>
-      <c r="B1408" s="9"/>
+        <v>44378</v>
+      </c>
+      <c r="B1408" s="12">
+        <v>44378</v>
+      </c>
       <c r="C1408" s="14" t="s">
-        <v>13</v>
+        <v>387</v>
       </c>
       <c r="D1408" s="10" t="s">
-        <v>584</v>
+        <v>494</v>
       </c>
       <c r="E1408" s="11" t="s">
-        <v>647</v>
+        <v>620</v>
       </c>
       <c r="F1408" s="10" t="s">
-        <v>1617</v>
-      </c>
-      <c r="G1408" s="11"/>
-      <c r="H1408" s="12"/>
-      <c r="I1408" s="13"/>
+        <v>2042</v>
+      </c>
+      <c r="G1408" s="11" t="s">
+        <v>1648</v>
+      </c>
+      <c r="H1408" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1408" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1408" s="13"/>
     </row>
     <row r="1409" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1409" s="12"/>
+      <c r="A1409" s="12">
+        <v>44378</v>
+      </c>
       <c r="B1409" s="12">
-        <v>44309</v>
+        <v>44378</v>
       </c>
       <c r="C1409" s="14" t="s">
-        <v>13</v>
+        <v>559</v>
       </c>
       <c r="D1409" s="10" t="s">
-        <v>584</v>
+        <v>107</v>
       </c>
       <c r="E1409" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1409" s="10" t="s">
-        <v>1610</v>
-      </c>
-      <c r="G1409" s="11"/>
-      <c r="H1409" s="12"/>
-      <c r="I1409" s="13"/>
+        <v>2043</v>
+      </c>
+      <c r="G1409" s="11" t="s">
+        <v>1648</v>
+      </c>
+      <c r="H1409" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1409" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1409" s="13"/>
     </row>
     <row r="1410" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1410" s="12">
-        <v>44239</v>
-      </c>
-      <c r="B1410" s="9"/>
+        <v>44378</v>
+      </c>
+      <c r="B1410" s="12">
+        <v>44378</v>
+      </c>
       <c r="C1410" s="14" t="s">
-        <v>13</v>
+        <v>490</v>
       </c>
       <c r="D1410" s="10" t="s">
-        <v>584</v>
+        <v>491</v>
       </c>
       <c r="E1410" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1410" s="10" t="s">
-        <v>1607</v>
-      </c>
-      <c r="G1410" s="11"/>
-      <c r="H1410" s="12"/>
-      <c r="I1410" s="13"/>
+        <v>2044</v>
+      </c>
+      <c r="G1410" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1410" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1410" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="J1410" s="13"/>
     </row>
     <row r="1411" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1411" s="12"/>
-      <c r="B1411" s="9">
-        <v>44255</v>
+      <c r="A1411" s="12">
+        <v>44379</v>
+      </c>
+      <c r="B1411" s="12">
+        <v>44379</v>
       </c>
       <c r="C1411" s="14" t="s">
-        <v>13</v>
+        <v>1994</v>
       </c>
       <c r="D1411" s="10" t="s">
-        <v>584</v>
+        <v>89</v>
       </c>
       <c r="E1411" s="11" t="s">
-        <v>647</v>
+        <v>685</v>
       </c>
       <c r="F1411" s="10" t="s">
-        <v>1606</v>
-      </c>
-      <c r="G1411" s="11"/>
-      <c r="H1411" s="12"/>
-      <c r="I1411" s="13"/>
+        <v>2057</v>
+      </c>
+      <c r="G1411" s="11" t="s">
+        <v>1626</v>
+      </c>
+      <c r="H1411" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1411" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1411" s="13"/>
     </row>
-    <row r="1412" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1412" s="12"/>
-      <c r="B1412" s="9">
-        <v>44255</v>
+    <row r="1412" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1412" s="12">
+        <v>44379</v>
+      </c>
+      <c r="B1412" s="12">
+        <v>44379</v>
       </c>
       <c r="C1412" s="14" t="s">
-        <v>13</v>
+        <v>2058</v>
       </c>
       <c r="D1412" s="10" t="s">
-        <v>584</v>
+        <v>25</v>
       </c>
       <c r="E1412" s="11" t="s">
-        <v>647</v>
+        <v>620</v>
       </c>
       <c r="F1412" s="10" t="s">
-        <v>1611</v>
-      </c>
-      <c r="G1412" s="11"/>
-      <c r="H1412" s="12"/>
-      <c r="I1412" s="13"/>
-      <c r="J1412" s="13"/>
+        <v>2059</v>
+      </c>
+      <c r="G1412" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1412" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1412" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1412" s="13" t="s">
+        <v>2060</v>
+      </c>
     </row>
     <row r="1413" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1413" s="12"/>
-      <c r="B1413" s="12">
-        <v>44309</v>
-      </c>
-      <c r="C1413" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1413" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1413" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1413" s="10" t="s">
-        <v>1614</v>
-      </c>
+      <c r="B1413" s="12"/>
+      <c r="C1413" s="14"/>
+      <c r="D1413" s="10"/>
+      <c r="E1413" s="11"/>
+      <c r="F1413" s="10"/>
       <c r="G1413" s="11"/>
       <c r="H1413" s="12"/>
       <c r="I1413" s="13"/>
@@ -49157,43 +49383,23 @@
     </row>
     <row r="1414" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1414" s="12"/>
-      <c r="B1414" s="9">
-        <v>44235</v>
-      </c>
-      <c r="C1414" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1414" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1414" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1414" s="10" t="s">
-        <v>1615</v>
-      </c>
+      <c r="B1414" s="12"/>
+      <c r="C1414" s="14"/>
+      <c r="D1414" s="10"/>
+      <c r="E1414" s="11"/>
+      <c r="F1414" s="10"/>
       <c r="G1414" s="11"/>
       <c r="H1414" s="12"/>
       <c r="I1414" s="13"/>
       <c r="J1414" s="13"/>
     </row>
     <row r="1415" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1415" s="12">
-        <v>44245</v>
-      </c>
-      <c r="B1415" s="9"/>
-      <c r="C1415" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1415" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1415" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1415" s="10" t="s">
-        <v>1612</v>
-      </c>
+      <c r="A1415" s="12"/>
+      <c r="B1415" s="12"/>
+      <c r="C1415" s="14"/>
+      <c r="D1415" s="10"/>
+      <c r="E1415" s="11"/>
+      <c r="F1415" s="10"/>
       <c r="G1415" s="11"/>
       <c r="H1415" s="12"/>
       <c r="I1415" s="13"/>
@@ -49201,19 +49407,11 @@
     </row>
     <row r="1416" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1416" s="12"/>
-      <c r="B1416" s="9"/>
-      <c r="C1416" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1416" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1416" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1416" s="10" t="s">
-        <v>1583</v>
-      </c>
+      <c r="B1416" s="12"/>
+      <c r="C1416" s="14"/>
+      <c r="D1416" s="10"/>
+      <c r="E1416" s="11"/>
+      <c r="F1416" s="10"/>
       <c r="G1416" s="11"/>
       <c r="H1416" s="12"/>
       <c r="I1416" s="13"/>
@@ -49221,7 +49419,7 @@
     </row>
     <row r="1417" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1417" s="12"/>
-      <c r="B1417" s="9"/>
+      <c r="B1417" s="12"/>
       <c r="C1417" s="14"/>
       <c r="D1417" s="10"/>
       <c r="E1417" s="11"/>
@@ -49232,113 +49430,87 @@
       <c r="J1417" s="13"/>
     </row>
     <row r="1418" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1418" s="12">
-        <v>44176</v>
-      </c>
-      <c r="B1418" s="9"/>
-      <c r="C1418" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1418" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1418" s="11" t="s">
-        <v>1353</v>
-      </c>
-      <c r="F1418" s="10" t="s">
-        <v>1354</v>
-      </c>
+      <c r="A1418" s="12"/>
+      <c r="B1418" s="12"/>
+      <c r="C1418" s="14"/>
+      <c r="D1418" s="10"/>
+      <c r="E1418" s="11"/>
+      <c r="F1418" s="10"/>
       <c r="G1418" s="11"/>
       <c r="H1418" s="12"/>
       <c r="I1418" s="13"/>
       <c r="J1418" s="13"/>
     </row>
-    <row r="1419" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1419" s="12">
-        <v>44252</v>
-      </c>
+    <row r="1419" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1419" s="12"/>
       <c r="B1419" s="9"/>
-      <c r="C1419" s="14" t="s">
-        <v>898</v>
-      </c>
-      <c r="D1419" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="E1419" s="11" t="s">
-        <v>759</v>
-      </c>
-      <c r="F1419" s="10" t="s">
-        <v>1661</v>
-      </c>
+      <c r="C1419" s="14"/>
+      <c r="D1419" s="10"/>
+      <c r="E1419" s="11"/>
+      <c r="F1419" s="10"/>
       <c r="G1419" s="11"/>
       <c r="H1419" s="12"/>
       <c r="I1419" s="13"/>
-      <c r="J1419" s="13" t="s">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="1420" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1420" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1420" s="9"/>
-      <c r="C1420" s="14" t="s">
-        <v>898</v>
-      </c>
-      <c r="D1420" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="E1420" s="11" t="s">
-        <v>759</v>
-      </c>
-      <c r="F1420" s="10" t="s">
-        <v>1660</v>
-      </c>
-      <c r="G1420" s="11"/>
-      <c r="H1420" s="12"/>
-      <c r="I1420" s="13"/>
-      <c r="J1420" s="13"/>
-    </row>
-    <row r="1421" spans="1:10" ht="84" x14ac:dyDescent="0.2">
-      <c r="A1421" s="12">
-        <v>43864</v>
-      </c>
+      <c r="J1419" s="13"/>
+    </row>
+    <row r="1420" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1420" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B1420" s="2" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C1420" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1420" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1420" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1420" s="4" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G1420" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1420" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1420" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1420" s="36"/>
+    </row>
+    <row r="1421" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1421" s="12"/>
       <c r="B1421" s="9"/>
-      <c r="C1421" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1421" s="10" t="s">
-        <v>533</v>
-      </c>
-      <c r="E1421" s="11" t="s">
-        <v>1580</v>
-      </c>
-      <c r="F1421" s="10" t="s">
-        <v>534</v>
-      </c>
+      <c r="C1421" s="14"/>
+      <c r="D1421" s="10"/>
+      <c r="E1421" s="11"/>
+      <c r="F1421" s="10"/>
       <c r="G1421" s="11"/>
       <c r="H1421" s="12"/>
       <c r="I1421" s="13"/>
-      <c r="J1421" s="13" t="s">
-        <v>1707</v>
-      </c>
+      <c r="J1421" s="13"/>
     </row>
     <row r="1422" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1422" s="12">
-        <v>44112</v>
-      </c>
-      <c r="B1422" s="9"/>
+      <c r="A1422" s="12"/>
+      <c r="B1422" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1422" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1422" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1422" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1422" s="10" t="s">
-        <v>1097</v>
+        <v>1616</v>
       </c>
       <c r="G1422" s="11"/>
       <c r="H1422" s="12"/>
@@ -49346,21 +49518,21 @@
       <c r="J1422" s="13"/>
     </row>
     <row r="1423" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1423" s="12">
-        <v>44088</v>
-      </c>
-      <c r="B1423" s="9"/>
+      <c r="A1423" s="12"/>
+      <c r="B1423" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1423" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1423" s="10" t="s">
-        <v>906</v>
+        <v>584</v>
       </c>
       <c r="E1423" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1423" s="10" t="s">
-        <v>1011</v>
+        <v>1608</v>
       </c>
       <c r="G1423" s="11"/>
       <c r="H1423" s="12"/>
@@ -49368,21 +49540,21 @@
       <c r="J1423" s="13"/>
     </row>
     <row r="1424" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1424" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1424" s="9"/>
+      <c r="A1424" s="12"/>
+      <c r="B1424" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1424" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1424" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1424" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1424" s="10" t="s">
-        <v>903</v>
+        <v>1613</v>
       </c>
       <c r="G1424" s="11"/>
       <c r="H1424" s="12"/>
@@ -49390,21 +49562,21 @@
       <c r="J1424" s="13"/>
     </row>
     <row r="1425" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1425" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1425" s="9"/>
+      <c r="A1425" s="12"/>
+      <c r="B1425" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1425" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1425" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1425" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1425" s="10" t="s">
-        <v>902</v>
+        <v>1609</v>
       </c>
       <c r="G1425" s="11"/>
       <c r="H1425" s="12"/>
@@ -49413,372 +49585,760 @@
     </row>
     <row r="1426" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1426" s="12">
-        <v>44055</v>
+        <v>44159</v>
       </c>
       <c r="B1426" s="9"/>
       <c r="C1426" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1426" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1426" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1426" s="10" t="s">
-        <v>900</v>
+        <v>1617</v>
       </c>
       <c r="G1426" s="11"/>
       <c r="H1426" s="12"/>
       <c r="I1426" s="13"/>
       <c r="J1426" s="13"/>
     </row>
-    <row r="1427" spans="1:10" ht="108" x14ac:dyDescent="0.2">
-      <c r="A1427" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1427" s="9"/>
+    <row r="1427" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1427" s="12"/>
+      <c r="B1427" s="12">
+        <v>44309</v>
+      </c>
       <c r="C1427" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1427" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1427" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1427" s="10" t="s">
-        <v>901</v>
+        <v>1610</v>
       </c>
       <c r="G1427" s="11"/>
       <c r="H1427" s="12"/>
       <c r="I1427" s="13"/>
       <c r="J1427" s="13"/>
     </row>
-    <row r="1428" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1428" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1428" s="12">
-        <v>44055</v>
+        <v>44239</v>
       </c>
       <c r="B1428" s="9"/>
       <c r="C1428" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1428" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1428" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1428" s="10" t="s">
-        <v>904</v>
+        <v>1607</v>
       </c>
       <c r="G1428" s="11"/>
       <c r="H1428" s="12"/>
       <c r="I1428" s="13"/>
-      <c r="J1428" s="13" t="s">
-        <v>1590</v>
-      </c>
-    </row>
-    <row r="1429" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1429" s="12">
-        <v>44047</v>
-      </c>
-      <c r="B1429" s="9"/>
+      <c r="J1428" s="13"/>
+    </row>
+    <row r="1429" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1429" s="12"/>
+      <c r="B1429" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1429" s="14" t="s">
-        <v>537</v>
+        <v>13</v>
       </c>
       <c r="D1429" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1429" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1429" s="10" t="s">
-        <v>873</v>
-      </c>
-      <c r="G1429" s="11" t="s">
-        <v>1626</v>
-      </c>
+        <v>1606</v>
+      </c>
+      <c r="G1429" s="11"/>
       <c r="H1429" s="12"/>
       <c r="I1429" s="13"/>
       <c r="J1429" s="13"/>
     </row>
-    <row r="1430" spans="1:10" ht="168" x14ac:dyDescent="0.2">
-      <c r="A1430" s="12">
-        <v>43949</v>
-      </c>
-      <c r="B1430" s="9"/>
+    <row r="1430" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1430" s="12"/>
+      <c r="B1430" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1430" s="14" t="s">
-        <v>468</v>
+        <v>13</v>
       </c>
       <c r="D1430" s="10" t="s">
-        <v>89</v>
+        <v>584</v>
       </c>
       <c r="E1430" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1430" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1430" s="11" t="s">
-        <v>1641</v>
-      </c>
+        <v>1611</v>
+      </c>
+      <c r="G1430" s="11"/>
       <c r="H1430" s="12"/>
-      <c r="I1430" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1430" s="13"/>
       <c r="J1430" s="13"/>
     </row>
-    <row r="1431" spans="1:10" ht="168" x14ac:dyDescent="0.2">
-      <c r="A1431" s="12">
-        <v>43949</v>
-      </c>
-      <c r="B1431" s="9"/>
+    <row r="1431" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1431" s="12"/>
+      <c r="B1431" s="12">
+        <v>44309</v>
+      </c>
       <c r="C1431" s="14" t="s">
-        <v>468</v>
+        <v>13</v>
       </c>
       <c r="D1431" s="10" t="s">
-        <v>89</v>
+        <v>584</v>
       </c>
       <c r="E1431" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1431" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1431" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>1614</v>
+      </c>
+      <c r="G1431" s="11"/>
       <c r="H1431" s="12"/>
-      <c r="I1431" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1431" s="13" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="1432" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1432" s="12">
-        <v>43838</v>
-      </c>
-      <c r="B1432" s="9"/>
+      <c r="I1431" s="13"/>
+      <c r="J1431" s="13"/>
+    </row>
+    <row r="1432" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1432" s="12"/>
+      <c r="B1432" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1432" s="14" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="D1432" s="10" t="s">
-        <v>460</v>
+        <v>584</v>
       </c>
       <c r="E1432" s="11" t="s">
         <v>647</v>
       </c>
       <c r="F1432" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G1432" s="11" t="s">
-        <v>1642</v>
-      </c>
+        <v>1615</v>
+      </c>
+      <c r="G1432" s="11"/>
       <c r="H1432" s="12"/>
       <c r="I1432" s="13"/>
-      <c r="J1432" s="13" t="s">
-        <v>1534</v>
-      </c>
+      <c r="J1432" s="13"/>
     </row>
     <row r="1433" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1433" s="12">
-        <v>43816</v>
+        <v>44245</v>
       </c>
       <c r="B1433" s="9"/>
       <c r="C1433" s="14" t="s">
-        <v>475</v>
+        <v>13</v>
       </c>
       <c r="D1433" s="10" t="s">
-        <v>38</v>
+        <v>584</v>
       </c>
       <c r="E1433" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1433" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="G1433" s="11" t="s">
-        <v>1634</v>
-      </c>
+        <v>1612</v>
+      </c>
+      <c r="G1433" s="11"/>
       <c r="H1433" s="12"/>
       <c r="I1433" s="13"/>
-      <c r="J1433" s="13" t="s">
-        <v>1570</v>
-      </c>
-    </row>
-    <row r="1434" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1434" s="12">
-        <v>43762</v>
-      </c>
+      <c r="J1433" s="13"/>
+    </row>
+    <row r="1434" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1434" s="12"/>
       <c r="B1434" s="9"/>
       <c r="C1434" s="14" t="s">
-        <v>446</v>
+        <v>13</v>
       </c>
       <c r="D1434" s="10" t="s">
-        <v>17</v>
+        <v>584</v>
       </c>
       <c r="E1434" s="11" t="s">
-        <v>837</v>
+        <v>647</v>
       </c>
       <c r="F1434" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G1434" s="11" t="s">
-        <v>1631</v>
-      </c>
+        <v>1583</v>
+      </c>
+      <c r="G1434" s="11"/>
       <c r="H1434" s="12"/>
       <c r="I1434" s="13"/>
       <c r="J1434" s="13"/>
     </row>
     <row r="1435" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1435" s="12">
-        <v>44222</v>
-      </c>
+      <c r="A1435" s="12"/>
       <c r="B1435" s="9"/>
-      <c r="C1435" s="14" t="s">
-        <v>1495</v>
-      </c>
-      <c r="D1435" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1435" s="11" t="s">
-        <v>837</v>
-      </c>
-      <c r="F1435" s="10" t="s">
-        <v>1494</v>
-      </c>
-      <c r="G1435" s="11" t="s">
-        <v>309</v>
-      </c>
+      <c r="C1435" s="14"/>
+      <c r="D1435" s="10"/>
+      <c r="E1435" s="11"/>
+      <c r="F1435" s="10"/>
+      <c r="G1435" s="11"/>
       <c r="H1435" s="12"/>
       <c r="I1435" s="13"/>
       <c r="J1435" s="13"/>
     </row>
-    <row r="1436" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1436" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1436" s="12">
-        <v>44266</v>
+        <v>44176</v>
       </c>
       <c r="B1436" s="9"/>
       <c r="C1436" s="14" t="s">
-        <v>537</v>
+        <v>8</v>
       </c>
       <c r="D1436" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1436" s="11" t="s">
-        <v>570</v>
+        <v>1353</v>
       </c>
       <c r="F1436" s="10" t="s">
-        <v>1715</v>
+        <v>1354</v>
       </c>
       <c r="G1436" s="11"/>
       <c r="H1436" s="12"/>
       <c r="I1436" s="13"/>
-      <c r="J1436" s="13" t="s">
-        <v>1716</v>
-      </c>
-    </row>
-    <row r="1437" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1436" s="13"/>
+    </row>
+    <row r="1437" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1437" s="12">
-        <v>44286</v>
+        <v>44252</v>
       </c>
       <c r="B1437" s="9"/>
       <c r="C1437" s="14" t="s">
-        <v>288</v>
+        <v>898</v>
       </c>
       <c r="D1437" s="10" t="s">
-        <v>25</v>
+        <v>494</v>
       </c>
       <c r="E1437" s="11" t="s">
-        <v>1580</v>
+        <v>759</v>
       </c>
       <c r="F1437" s="10" t="s">
-        <v>1840</v>
+        <v>1661</v>
       </c>
       <c r="G1437" s="11"/>
       <c r="H1437" s="12"/>
       <c r="I1437" s="13"/>
-      <c r="J1437" s="13"/>
-    </row>
-    <row r="1438" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1438" s="12"/>
+      <c r="J1437" s="13" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1438" s="12">
+        <v>44252</v>
+      </c>
       <c r="B1438" s="9"/>
-      <c r="C1438" s="14"/>
-      <c r="D1438" s="10"/>
-      <c r="E1438" s="11"/>
-      <c r="F1438" s="10"/>
+      <c r="C1438" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1438" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1438" s="11" t="s">
+        <v>759</v>
+      </c>
+      <c r="F1438" s="10" t="s">
+        <v>1660</v>
+      </c>
       <c r="G1438" s="11"/>
       <c r="H1438" s="12"/>
       <c r="I1438" s="13"/>
       <c r="J1438" s="13"/>
     </row>
-    <row r="1439" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1439" s="12"/>
+    <row r="1439" spans="1:10" ht="84" x14ac:dyDescent="0.2">
+      <c r="A1439" s="12">
+        <v>43864</v>
+      </c>
       <c r="B1439" s="9"/>
-      <c r="C1439" s="14"/>
-      <c r="D1439" s="10"/>
-      <c r="E1439" s="11"/>
-      <c r="F1439" s="10"/>
+      <c r="C1439" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1439" s="10" t="s">
+        <v>533</v>
+      </c>
+      <c r="E1439" s="11" t="s">
+        <v>1580</v>
+      </c>
+      <c r="F1439" s="10" t="s">
+        <v>534</v>
+      </c>
       <c r="G1439" s="11"/>
       <c r="H1439" s="12"/>
       <c r="I1439" s="13"/>
-      <c r="J1439" s="13"/>
+      <c r="J1439" s="13" t="s">
+        <v>1707</v>
+      </c>
     </row>
     <row r="1440" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1440" s="12"/>
+      <c r="A1440" s="12">
+        <v>44112</v>
+      </c>
       <c r="B1440" s="9"/>
-      <c r="C1440" s="14"/>
-      <c r="D1440" s="10"/>
-      <c r="E1440" s="11"/>
-      <c r="F1440" s="10"/>
+      <c r="C1440" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1440" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1440" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1440" s="10" t="s">
+        <v>1097</v>
+      </c>
       <c r="G1440" s="11"/>
       <c r="H1440" s="12"/>
       <c r="I1440" s="13"/>
       <c r="J1440" s="13"/>
     </row>
     <row r="1441" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1441" s="12"/>
+      <c r="A1441" s="12">
+        <v>44088</v>
+      </c>
       <c r="B1441" s="9"/>
-      <c r="C1441" s="14"/>
-      <c r="D1441" s="10"/>
-      <c r="E1441" s="11"/>
-      <c r="F1441" s="10"/>
+      <c r="C1441" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1441" s="10" t="s">
+        <v>906</v>
+      </c>
+      <c r="E1441" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1441" s="10" t="s">
+        <v>1011</v>
+      </c>
       <c r="G1441" s="11"/>
       <c r="H1441" s="12"/>
       <c r="I1441" s="13"/>
       <c r="J1441" s="13"/>
     </row>
     <row r="1442" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1442" s="12"/>
+      <c r="A1442" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1442" s="9"/>
-      <c r="C1442" s="14"/>
-      <c r="D1442" s="10"/>
-      <c r="E1442" s="11"/>
-      <c r="F1442" s="10"/>
+      <c r="C1442" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1442" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1442" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1442" s="10" t="s">
+        <v>903</v>
+      </c>
       <c r="G1442" s="11"/>
       <c r="H1442" s="12"/>
       <c r="I1442" s="13"/>
       <c r="J1442" s="13"/>
     </row>
     <row r="1443" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1443" s="12"/>
+      <c r="A1443" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1443" s="9"/>
-      <c r="C1443" s="14"/>
-      <c r="D1443" s="10"/>
-      <c r="E1443" s="11"/>
-      <c r="F1443" s="10"/>
+      <c r="C1443" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1443" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1443" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1443" s="10" t="s">
+        <v>902</v>
+      </c>
       <c r="G1443" s="11"/>
       <c r="H1443" s="12"/>
       <c r="I1443" s="13"/>
       <c r="J1443" s="13"/>
     </row>
+    <row r="1444" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1444" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B1444" s="9"/>
+      <c r="C1444" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1444" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1444" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1444" s="10" t="s">
+        <v>900</v>
+      </c>
+      <c r="G1444" s="11"/>
+      <c r="H1444" s="12"/>
+      <c r="I1444" s="13"/>
+      <c r="J1444" s="13"/>
+    </row>
+    <row r="1445" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A1445" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B1445" s="9"/>
+      <c r="C1445" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1445" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1445" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1445" s="10" t="s">
+        <v>901</v>
+      </c>
+      <c r="G1445" s="11"/>
+      <c r="H1445" s="12"/>
+      <c r="I1445" s="13"/>
+      <c r="J1445" s="13"/>
+    </row>
+    <row r="1446" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1446" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B1446" s="9"/>
+      <c r="C1446" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1446" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1446" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1446" s="10" t="s">
+        <v>904</v>
+      </c>
+      <c r="G1446" s="11"/>
+      <c r="H1446" s="12"/>
+      <c r="I1446" s="13"/>
+      <c r="J1446" s="13" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1447" s="12">
+        <v>44047</v>
+      </c>
+      <c r="B1447" s="9"/>
+      <c r="C1447" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1447" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1447" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1447" s="10" t="s">
+        <v>873</v>
+      </c>
+      <c r="G1447" s="11" t="s">
+        <v>1626</v>
+      </c>
+      <c r="H1447" s="12"/>
+      <c r="I1447" s="13"/>
+      <c r="J1447" s="13"/>
+    </row>
+    <row r="1448" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1448" s="12">
+        <v>43949</v>
+      </c>
+      <c r="B1448" s="9"/>
+      <c r="C1448" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1448" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1448" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1448" s="10" t="s">
+        <v>686</v>
+      </c>
+      <c r="G1448" s="11" t="s">
+        <v>1641</v>
+      </c>
+      <c r="H1448" s="12"/>
+      <c r="I1448" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1448" s="13"/>
+    </row>
+    <row r="1449" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1449" s="12">
+        <v>43949</v>
+      </c>
+      <c r="B1449" s="9"/>
+      <c r="C1449" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1449" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1449" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1449" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="G1449" s="11" t="s">
+        <v>687</v>
+      </c>
+      <c r="H1449" s="12"/>
+      <c r="I1449" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1449" s="13" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1450" s="12">
+        <v>43838</v>
+      </c>
+      <c r="B1450" s="9"/>
+      <c r="C1450" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1450" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1450" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1450" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G1450" s="11" t="s">
+        <v>1642</v>
+      </c>
+      <c r="H1450" s="12"/>
+      <c r="I1450" s="13"/>
+      <c r="J1450" s="13" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1451" s="12">
+        <v>43816</v>
+      </c>
+      <c r="B1451" s="9"/>
+      <c r="C1451" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1451" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1451" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1451" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G1451" s="11" t="s">
+        <v>1634</v>
+      </c>
+      <c r="H1451" s="12"/>
+      <c r="I1451" s="13"/>
+      <c r="J1451" s="13" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1452" s="12">
+        <v>43762</v>
+      </c>
+      <c r="B1452" s="9"/>
+      <c r="C1452" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1452" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1452" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1452" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1452" s="11" t="s">
+        <v>1631</v>
+      </c>
+      <c r="H1452" s="12"/>
+      <c r="I1452" s="13"/>
+      <c r="J1452" s="13"/>
+    </row>
+    <row r="1453" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1453" s="12">
+        <v>44222</v>
+      </c>
+      <c r="B1453" s="9"/>
+      <c r="C1453" s="14" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D1453" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1453" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1453" s="10" t="s">
+        <v>1494</v>
+      </c>
+      <c r="G1453" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1453" s="12"/>
+      <c r="I1453" s="13"/>
+      <c r="J1453" s="13"/>
+    </row>
+    <row r="1454" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1454" s="12">
+        <v>44266</v>
+      </c>
+      <c r="B1454" s="9"/>
+      <c r="C1454" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1454" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1454" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1454" s="10" t="s">
+        <v>1715</v>
+      </c>
+      <c r="G1454" s="11"/>
+      <c r="H1454" s="12"/>
+      <c r="I1454" s="13"/>
+      <c r="J1454" s="13" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1455" s="12">
+        <v>44286</v>
+      </c>
+      <c r="B1455" s="9"/>
+      <c r="C1455" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1455" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1455" s="11" t="s">
+        <v>1580</v>
+      </c>
+      <c r="F1455" s="10" t="s">
+        <v>1840</v>
+      </c>
+      <c r="G1455" s="11"/>
+      <c r="H1455" s="12"/>
+      <c r="I1455" s="13"/>
+      <c r="J1455" s="13"/>
+    </row>
+    <row r="1456" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1456" s="12"/>
+      <c r="B1456" s="9"/>
+      <c r="C1456" s="14"/>
+      <c r="D1456" s="10"/>
+      <c r="E1456" s="11"/>
+      <c r="F1456" s="10"/>
+      <c r="G1456" s="11"/>
+      <c r="H1456" s="12"/>
+      <c r="I1456" s="13"/>
+      <c r="J1456" s="13"/>
+    </row>
+    <row r="1457" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1457" s="12"/>
+      <c r="B1457" s="9"/>
+      <c r="C1457" s="14"/>
+      <c r="D1457" s="10"/>
+      <c r="E1457" s="11"/>
+      <c r="F1457" s="10"/>
+      <c r="G1457" s="11"/>
+      <c r="H1457" s="12"/>
+      <c r="I1457" s="13"/>
+      <c r="J1457" s="13"/>
+    </row>
+    <row r="1458" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1458" s="12"/>
+      <c r="B1458" s="9"/>
+      <c r="C1458" s="14"/>
+      <c r="D1458" s="10"/>
+      <c r="E1458" s="11"/>
+      <c r="F1458" s="10"/>
+      <c r="G1458" s="11"/>
+      <c r="H1458" s="12"/>
+      <c r="I1458" s="13"/>
+      <c r="J1458" s="13"/>
+    </row>
+    <row r="1459" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1459" s="12"/>
+      <c r="B1459" s="9"/>
+      <c r="C1459" s="14"/>
+      <c r="D1459" s="10"/>
+      <c r="E1459" s="11"/>
+      <c r="F1459" s="10"/>
+      <c r="G1459" s="11"/>
+      <c r="H1459" s="12"/>
+      <c r="I1459" s="13"/>
+      <c r="J1459" s="13"/>
+    </row>
+    <row r="1460" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1460" s="12"/>
+      <c r="B1460" s="9"/>
+      <c r="C1460" s="14"/>
+      <c r="D1460" s="10"/>
+      <c r="E1460" s="11"/>
+      <c r="F1460" s="10"/>
+      <c r="G1460" s="11"/>
+      <c r="H1460" s="12"/>
+      <c r="I1460" s="13"/>
+      <c r="J1460" s="13"/>
+    </row>
+    <row r="1461" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1461" s="12"/>
+      <c r="B1461" s="9"/>
+      <c r="C1461" s="14"/>
+      <c r="D1461" s="10"/>
+      <c r="E1461" s="11"/>
+      <c r="F1461" s="10"/>
+      <c r="G1461" s="11"/>
+      <c r="H1461" s="12"/>
+      <c r="I1461" s="13"/>
+      <c r="J1461" s="13"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J1395" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1405:F1415">
-    <sortCondition ref="F1405:F1415"/>
+  <autoFilter ref="A1:J1402" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1423:F1433">
+    <sortCondition ref="F1423:F1433"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Acerto Rentabidade e filiais
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B2D0C1-FA15-4C22-AF63-3B0148CFF5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1409D9-7DC6-4DE4-962D-FB29C8070E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10025" uniqueCount="2061">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10057" uniqueCount="2068">
   <si>
     <t>Responsável</t>
   </si>
@@ -6551,6 +6551,28 @@
   </si>
   <si>
     <t>BKGCT06</t>
+  </si>
+  <si>
+    <t>Aplicação de patch 21-07-01-LIB_LABEL_01072021_P12_LOBO</t>
+  </si>
+  <si>
+    <t>Ontem a tarde o Anderson liberou o titulo em anexo, mas só pagamos hoje de manhã.
+Estava entrando em geração de cheques ontem e a rede travou quando eu estava no titulo....eu tive que dar um boot. Agora preciso entrar em geração de cheques com a data do dia 02/07/21 e não esta aparecendo o titulo.</t>
+  </si>
+  <si>
+    <t>Acerto das notas fiscais 2998 e 2997 para aliquota de 2% e faturamento por Barueri</t>
+  </si>
+  <si>
+    <t>Acerto na data de vencimento do título LF 361694PEN, favor ajustar para o dia 06/07/21</t>
+  </si>
+  <si>
+    <t>Nova Medição e  Filiais</t>
+  </si>
+  <si>
+    <t>Alteração no rdmake CNTA121_pe e CN120PED (chave do CNA : xFilial("CNA",cFilCtr))</t>
+  </si>
+  <si>
+    <t>Problemas com a Rentabilidade</t>
   </si>
 </sst>
 </file>
@@ -7316,11 +7338,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1461"/>
+  <dimension ref="A1:J1463"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1405" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1414" sqref="B1414"/>
+      <selection pane="bottomLeft" activeCell="F1418" sqref="F1418"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -49315,19 +49337,19 @@
         <v>44379</v>
       </c>
       <c r="C1411" s="14" t="s">
-        <v>1994</v>
+        <v>13</v>
       </c>
       <c r="D1411" s="10" t="s">
-        <v>89</v>
+        <v>584</v>
       </c>
       <c r="E1411" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1411" s="10" t="s">
-        <v>2057</v>
+        <v>2061</v>
       </c>
       <c r="G1411" s="11" t="s">
-        <v>1626</v>
+        <v>1623</v>
       </c>
       <c r="H1411" s="12" t="s">
         <v>112</v>
@@ -49337,7 +49359,7 @@
       </c>
       <c r="J1411" s="13"/>
     </row>
-    <row r="1412" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="1412" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1412" s="12">
         <v>44379</v>
       </c>
@@ -49345,97 +49367,185 @@
         <v>44379</v>
       </c>
       <c r="C1412" s="14" t="s">
+        <v>1994</v>
+      </c>
+      <c r="D1412" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1412" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1412" s="10" t="s">
+        <v>2057</v>
+      </c>
+      <c r="G1412" s="11" t="s">
+        <v>1626</v>
+      </c>
+      <c r="H1412" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1412" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1412" s="13"/>
+    </row>
+    <row r="1413" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1413" s="12">
+        <v>44379</v>
+      </c>
+      <c r="B1413" s="12">
+        <v>44379</v>
+      </c>
+      <c r="C1413" s="14" t="s">
         <v>2058</v>
       </c>
-      <c r="D1412" s="10" t="s">
+      <c r="D1413" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E1412" s="11" t="s">
+      <c r="E1413" s="11" t="s">
         <v>620</v>
       </c>
-      <c r="F1412" s="10" t="s">
+      <c r="F1413" s="10" t="s">
         <v>2059</v>
       </c>
-      <c r="G1412" s="11" t="s">
+      <c r="G1413" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="H1412" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1412" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1412" s="13" t="s">
+      <c r="H1413" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1413" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1413" s="13" t="s">
         <v>2060</v>
       </c>
     </row>
-    <row r="1413" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1413" s="12"/>
-      <c r="B1413" s="12"/>
-      <c r="C1413" s="14"/>
-      <c r="D1413" s="10"/>
-      <c r="E1413" s="11"/>
-      <c r="F1413" s="10"/>
-      <c r="G1413" s="11"/>
-      <c r="H1413" s="12"/>
-      <c r="I1413" s="13"/>
-      <c r="J1413" s="13"/>
-    </row>
-    <row r="1414" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1414" s="12"/>
-      <c r="B1414" s="12"/>
-      <c r="C1414" s="14"/>
-      <c r="D1414" s="10"/>
-      <c r="E1414" s="11"/>
-      <c r="F1414" s="10"/>
+    <row r="1414" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1414" s="12">
+        <v>44379</v>
+      </c>
+      <c r="B1414" s="12">
+        <v>44379</v>
+      </c>
+      <c r="C1414" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1414" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1414" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1414" s="10" t="s">
+        <v>2062</v>
+      </c>
       <c r="G1414" s="11"/>
       <c r="H1414" s="12"/>
-      <c r="I1414" s="13"/>
+      <c r="I1414" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="J1414" s="13"/>
     </row>
     <row r="1415" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1415" s="12"/>
-      <c r="B1415" s="12"/>
-      <c r="C1415" s="14"/>
-      <c r="D1415" s="10"/>
-      <c r="E1415" s="11"/>
-      <c r="F1415" s="10"/>
-      <c r="G1415" s="11"/>
-      <c r="H1415" s="12"/>
-      <c r="I1415" s="13"/>
+      <c r="A1415" s="12">
+        <v>44382</v>
+      </c>
+      <c r="B1415" s="12">
+        <v>44382</v>
+      </c>
+      <c r="C1415" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1415" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1415" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1415" s="10" t="s">
+        <v>2064</v>
+      </c>
+      <c r="G1415" s="11" t="s">
+        <v>1623</v>
+      </c>
+      <c r="H1415" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1415" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1415" s="13"/>
     </row>
     <row r="1416" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1416" s="12"/>
-      <c r="B1416" s="12"/>
-      <c r="C1416" s="14"/>
-      <c r="D1416" s="10"/>
-      <c r="E1416" s="11"/>
-      <c r="F1416" s="10"/>
-      <c r="G1416" s="11"/>
-      <c r="H1416" s="12"/>
-      <c r="I1416" s="13"/>
+      <c r="A1416" s="12">
+        <v>44382</v>
+      </c>
+      <c r="B1416" s="12">
+        <v>44382</v>
+      </c>
+      <c r="C1416" s="14" t="s">
+        <v>1994</v>
+      </c>
+      <c r="D1416" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1416" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1416" s="10" t="s">
+        <v>2063</v>
+      </c>
+      <c r="G1416" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1416" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1416" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1416" s="13"/>
     </row>
-    <row r="1417" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1417" s="12"/>
-      <c r="B1417" s="12"/>
-      <c r="C1417" s="14"/>
-      <c r="D1417" s="10"/>
-      <c r="E1417" s="11"/>
-      <c r="F1417" s="10"/>
+    <row r="1417" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1417" s="12">
+        <v>44382</v>
+      </c>
+      <c r="B1417" s="12">
+        <v>44382</v>
+      </c>
+      <c r="C1417" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1417" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1417" s="11" t="s">
+        <v>2065</v>
+      </c>
+      <c r="F1417" s="10" t="s">
+        <v>2066</v>
+      </c>
       <c r="G1417" s="11"/>
       <c r="H1417" s="12"/>
       <c r="I1417" s="13"/>
       <c r="J1417" s="13"/>
     </row>
     <row r="1418" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1418" s="12"/>
-      <c r="B1418" s="12"/>
-      <c r="C1418" s="14"/>
+      <c r="A1418" s="12">
+        <v>44382</v>
+      </c>
+      <c r="B1418" s="12">
+        <v>44382</v>
+      </c>
+      <c r="C1418" s="14" t="s">
+        <v>387</v>
+      </c>
       <c r="D1418" s="10"/>
       <c r="E1418" s="11"/>
-      <c r="F1418" s="10"/>
+      <c r="F1418" s="10" t="s">
+        <v>2067</v>
+      </c>
       <c r="G1418" s="11"/>
       <c r="H1418" s="12"/>
       <c r="I1418" s="13"/>
@@ -49443,7 +49553,7 @@
     </row>
     <row r="1419" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1419" s="12"/>
-      <c r="B1419" s="9"/>
+      <c r="B1419" s="12"/>
       <c r="C1419" s="14"/>
       <c r="D1419" s="10"/>
       <c r="E1419" s="11"/>
@@ -49454,34 +49564,16 @@
       <c r="J1419" s="13"/>
     </row>
     <row r="1420" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1420" s="1" t="s">
-        <v>1479</v>
-      </c>
-      <c r="B1420" s="2" t="s">
-        <v>1480</v>
-      </c>
-      <c r="C1420" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1420" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1420" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1420" s="4" t="s">
-        <v>1581</v>
-      </c>
-      <c r="G1420" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1420" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1420" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1420" s="36"/>
+      <c r="A1420" s="12"/>
+      <c r="B1420" s="12"/>
+      <c r="C1420" s="14"/>
+      <c r="D1420" s="10"/>
+      <c r="E1420" s="11"/>
+      <c r="F1420" s="10"/>
+      <c r="G1420" s="11"/>
+      <c r="H1420" s="12"/>
+      <c r="I1420" s="13"/>
+      <c r="J1420" s="13"/>
     </row>
     <row r="1421" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1421" s="12"/>
@@ -49496,44 +49588,42 @@
       <c r="J1421" s="13"/>
     </row>
     <row r="1422" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1422" s="12"/>
-      <c r="B1422" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1422" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1422" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1422" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1422" s="10" t="s">
-        <v>1616</v>
-      </c>
-      <c r="G1422" s="11"/>
-      <c r="H1422" s="12"/>
-      <c r="I1422" s="13"/>
-      <c r="J1422" s="13"/>
+      <c r="A1422" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B1422" s="2" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C1422" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1422" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1422" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1422" s="4" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G1422" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1422" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1422" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1422" s="36"/>
     </row>
     <row r="1423" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1423" s="12"/>
-      <c r="B1423" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1423" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1423" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1423" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1423" s="10" t="s">
-        <v>1608</v>
-      </c>
+      <c r="B1423" s="9"/>
+      <c r="C1423" s="14"/>
+      <c r="D1423" s="10"/>
+      <c r="E1423" s="11"/>
+      <c r="F1423" s="10"/>
       <c r="G1423" s="11"/>
       <c r="H1423" s="12"/>
       <c r="I1423" s="13"/>
@@ -49554,7 +49644,7 @@
         <v>647</v>
       </c>
       <c r="F1424" s="10" t="s">
-        <v>1613</v>
+        <v>1616</v>
       </c>
       <c r="G1424" s="11"/>
       <c r="H1424" s="12"/>
@@ -49576,7 +49666,7 @@
         <v>647</v>
       </c>
       <c r="F1425" s="10" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="G1425" s="11"/>
       <c r="H1425" s="12"/>
@@ -49584,10 +49674,10 @@
       <c r="J1425" s="13"/>
     </row>
     <row r="1426" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1426" s="12">
-        <v>44159</v>
-      </c>
-      <c r="B1426" s="9"/>
+      <c r="A1426" s="12"/>
+      <c r="B1426" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1426" s="14" t="s">
         <v>13</v>
       </c>
@@ -49598,7 +49688,7 @@
         <v>647</v>
       </c>
       <c r="F1426" s="10" t="s">
-        <v>1617</v>
+        <v>1613</v>
       </c>
       <c r="G1426" s="11"/>
       <c r="H1426" s="12"/>
@@ -49607,8 +49697,8 @@
     </row>
     <row r="1427" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1427" s="12"/>
-      <c r="B1427" s="12">
-        <v>44309</v>
+      <c r="B1427" s="9">
+        <v>44255</v>
       </c>
       <c r="C1427" s="14" t="s">
         <v>13</v>
@@ -49620,7 +49710,7 @@
         <v>647</v>
       </c>
       <c r="F1427" s="10" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="G1427" s="11"/>
       <c r="H1427" s="12"/>
@@ -49629,7 +49719,7 @@
     </row>
     <row r="1428" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1428" s="12">
-        <v>44239</v>
+        <v>44159</v>
       </c>
       <c r="B1428" s="9"/>
       <c r="C1428" s="14" t="s">
@@ -49642,7 +49732,7 @@
         <v>647</v>
       </c>
       <c r="F1428" s="10" t="s">
-        <v>1607</v>
+        <v>1617</v>
       </c>
       <c r="G1428" s="11"/>
       <c r="H1428" s="12"/>
@@ -49651,8 +49741,8 @@
     </row>
     <row r="1429" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1429" s="12"/>
-      <c r="B1429" s="9">
-        <v>44255</v>
+      <c r="B1429" s="12">
+        <v>44309</v>
       </c>
       <c r="C1429" s="14" t="s">
         <v>13</v>
@@ -49664,7 +49754,7 @@
         <v>647</v>
       </c>
       <c r="F1429" s="10" t="s">
-        <v>1606</v>
+        <v>1610</v>
       </c>
       <c r="G1429" s="11"/>
       <c r="H1429" s="12"/>
@@ -49672,10 +49762,10 @@
       <c r="J1429" s="13"/>
     </row>
     <row r="1430" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1430" s="12"/>
-      <c r="B1430" s="9">
-        <v>44255</v>
-      </c>
+      <c r="A1430" s="12">
+        <v>44239</v>
+      </c>
+      <c r="B1430" s="9"/>
       <c r="C1430" s="14" t="s">
         <v>13</v>
       </c>
@@ -49686,7 +49776,7 @@
         <v>647</v>
       </c>
       <c r="F1430" s="10" t="s">
-        <v>1611</v>
+        <v>1607</v>
       </c>
       <c r="G1430" s="11"/>
       <c r="H1430" s="12"/>
@@ -49695,8 +49785,8 @@
     </row>
     <row r="1431" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1431" s="12"/>
-      <c r="B1431" s="12">
-        <v>44309</v>
+      <c r="B1431" s="9">
+        <v>44255</v>
       </c>
       <c r="C1431" s="14" t="s">
         <v>13</v>
@@ -49708,7 +49798,7 @@
         <v>647</v>
       </c>
       <c r="F1431" s="10" t="s">
-        <v>1614</v>
+        <v>1606</v>
       </c>
       <c r="G1431" s="11"/>
       <c r="H1431" s="12"/>
@@ -49718,7 +49808,7 @@
     <row r="1432" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1432" s="12"/>
       <c r="B1432" s="9">
-        <v>44235</v>
+        <v>44255</v>
       </c>
       <c r="C1432" s="14" t="s">
         <v>13</v>
@@ -49730,7 +49820,7 @@
         <v>647</v>
       </c>
       <c r="F1432" s="10" t="s">
-        <v>1615</v>
+        <v>1611</v>
       </c>
       <c r="G1432" s="11"/>
       <c r="H1432" s="12"/>
@@ -49738,10 +49828,10 @@
       <c r="J1432" s="13"/>
     </row>
     <row r="1433" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1433" s="12">
-        <v>44245</v>
-      </c>
-      <c r="B1433" s="9"/>
+      <c r="A1433" s="12"/>
+      <c r="B1433" s="12">
+        <v>44309</v>
+      </c>
       <c r="C1433" s="14" t="s">
         <v>13</v>
       </c>
@@ -49752,7 +49842,7 @@
         <v>647</v>
       </c>
       <c r="F1433" s="10" t="s">
-        <v>1612</v>
+        <v>1614</v>
       </c>
       <c r="G1433" s="11"/>
       <c r="H1433" s="12"/>
@@ -49761,7 +49851,9 @@
     </row>
     <row r="1434" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1434" s="12"/>
-      <c r="B1434" s="9"/>
+      <c r="B1434" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1434" s="14" t="s">
         <v>13</v>
       </c>
@@ -49772,7 +49864,7 @@
         <v>647</v>
       </c>
       <c r="F1434" s="10" t="s">
-        <v>1583</v>
+        <v>1615</v>
       </c>
       <c r="G1434" s="11"/>
       <c r="H1434" s="12"/>
@@ -49780,156 +49872,154 @@
       <c r="J1434" s="13"/>
     </row>
     <row r="1435" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1435" s="12"/>
+      <c r="A1435" s="12">
+        <v>44245</v>
+      </c>
       <c r="B1435" s="9"/>
-      <c r="C1435" s="14"/>
-      <c r="D1435" s="10"/>
-      <c r="E1435" s="11"/>
-      <c r="F1435" s="10"/>
+      <c r="C1435" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1435" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1435" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1435" s="10" t="s">
+        <v>1612</v>
+      </c>
       <c r="G1435" s="11"/>
       <c r="H1435" s="12"/>
       <c r="I1435" s="13"/>
       <c r="J1435" s="13"/>
     </row>
     <row r="1436" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1436" s="12">
-        <v>44176</v>
-      </c>
+      <c r="A1436" s="12"/>
       <c r="B1436" s="9"/>
       <c r="C1436" s="14" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D1436" s="10" t="s">
         <v>584</v>
       </c>
       <c r="E1436" s="11" t="s">
-        <v>1353</v>
+        <v>647</v>
       </c>
       <c r="F1436" s="10" t="s">
-        <v>1354</v>
+        <v>1583</v>
       </c>
       <c r="G1436" s="11"/>
       <c r="H1436" s="12"/>
       <c r="I1436" s="13"/>
       <c r="J1436" s="13"/>
     </row>
-    <row r="1437" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1437" s="12">
-        <v>44252</v>
-      </c>
+    <row r="1437" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1437" s="12"/>
       <c r="B1437" s="9"/>
-      <c r="C1437" s="14" t="s">
-        <v>898</v>
-      </c>
-      <c r="D1437" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="E1437" s="11" t="s">
-        <v>759</v>
-      </c>
-      <c r="F1437" s="10" t="s">
-        <v>1661</v>
-      </c>
+      <c r="C1437" s="14"/>
+      <c r="D1437" s="10"/>
+      <c r="E1437" s="11"/>
+      <c r="F1437" s="10"/>
       <c r="G1437" s="11"/>
       <c r="H1437" s="12"/>
       <c r="I1437" s="13"/>
-      <c r="J1437" s="13" t="s">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="1438" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1437" s="13"/>
+    </row>
+    <row r="1438" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1438" s="12">
-        <v>44252</v>
+        <v>44176</v>
       </c>
       <c r="B1438" s="9"/>
       <c r="C1438" s="14" t="s">
-        <v>898</v>
+        <v>8</v>
       </c>
       <c r="D1438" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1438" s="11" t="s">
-        <v>759</v>
+        <v>1353</v>
       </c>
       <c r="F1438" s="10" t="s">
-        <v>1660</v>
+        <v>1354</v>
       </c>
       <c r="G1438" s="11"/>
       <c r="H1438" s="12"/>
       <c r="I1438" s="13"/>
       <c r="J1438" s="13"/>
     </row>
-    <row r="1439" spans="1:10" ht="84" x14ac:dyDescent="0.2">
+    <row r="1439" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1439" s="12">
-        <v>43864</v>
+        <v>44252</v>
       </c>
       <c r="B1439" s="9"/>
       <c r="C1439" s="14" t="s">
-        <v>19</v>
+        <v>898</v>
       </c>
       <c r="D1439" s="10" t="s">
-        <v>533</v>
+        <v>494</v>
       </c>
       <c r="E1439" s="11" t="s">
-        <v>1580</v>
+        <v>759</v>
       </c>
       <c r="F1439" s="10" t="s">
-        <v>534</v>
+        <v>1661</v>
       </c>
       <c r="G1439" s="11"/>
       <c r="H1439" s="12"/>
       <c r="I1439" s="13"/>
       <c r="J1439" s="13" t="s">
-        <v>1707</v>
-      </c>
-    </row>
-    <row r="1440" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1440" s="12">
-        <v>44112</v>
+        <v>44252</v>
       </c>
       <c r="B1440" s="9"/>
       <c r="C1440" s="14" t="s">
-        <v>623</v>
+        <v>898</v>
       </c>
       <c r="D1440" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1440" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1440" s="10" t="s">
-        <v>1097</v>
+        <v>1660</v>
       </c>
       <c r="G1440" s="11"/>
       <c r="H1440" s="12"/>
       <c r="I1440" s="13"/>
       <c r="J1440" s="13"/>
     </row>
-    <row r="1441" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1441" spans="1:10" ht="84" x14ac:dyDescent="0.2">
       <c r="A1441" s="12">
-        <v>44088</v>
+        <v>43864</v>
       </c>
       <c r="B1441" s="9"/>
       <c r="C1441" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D1441" s="10" t="s">
-        <v>906</v>
+        <v>533</v>
       </c>
       <c r="E1441" s="11" t="s">
-        <v>685</v>
+        <v>1580</v>
       </c>
       <c r="F1441" s="10" t="s">
-        <v>1011</v>
+        <v>534</v>
       </c>
       <c r="G1441" s="11"/>
       <c r="H1441" s="12"/>
       <c r="I1441" s="13"/>
-      <c r="J1441" s="13"/>
+      <c r="J1441" s="13" t="s">
+        <v>1707</v>
+      </c>
     </row>
     <row r="1442" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1442" s="12">
-        <v>44055</v>
+        <v>44112</v>
       </c>
       <c r="B1442" s="9"/>
       <c r="C1442" s="14" t="s">
@@ -49942,7 +50032,7 @@
         <v>570</v>
       </c>
       <c r="F1442" s="10" t="s">
-        <v>903</v>
+        <v>1097</v>
       </c>
       <c r="G1442" s="11"/>
       <c r="H1442" s="12"/>
@@ -49951,20 +50041,20 @@
     </row>
     <row r="1443" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1443" s="12">
-        <v>44055</v>
+        <v>44088</v>
       </c>
       <c r="B1443" s="9"/>
       <c r="C1443" s="14" t="s">
-        <v>623</v>
+        <v>19</v>
       </c>
       <c r="D1443" s="10" t="s">
-        <v>6</v>
+        <v>906</v>
       </c>
       <c r="E1443" s="11" t="s">
-        <v>570</v>
+        <v>685</v>
       </c>
       <c r="F1443" s="10" t="s">
-        <v>902</v>
+        <v>1011</v>
       </c>
       <c r="G1443" s="11"/>
       <c r="H1443" s="12"/>
@@ -49977,45 +50067,45 @@
       </c>
       <c r="B1444" s="9"/>
       <c r="C1444" s="14" t="s">
-        <v>898</v>
+        <v>623</v>
       </c>
       <c r="D1444" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1444" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1444" s="10" t="s">
-        <v>900</v>
+        <v>903</v>
       </c>
       <c r="G1444" s="11"/>
       <c r="H1444" s="12"/>
       <c r="I1444" s="13"/>
       <c r="J1444" s="13"/>
     </row>
-    <row r="1445" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="1445" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1445" s="12">
         <v>44055</v>
       </c>
       <c r="B1445" s="9"/>
       <c r="C1445" s="14" t="s">
-        <v>898</v>
+        <v>623</v>
       </c>
       <c r="D1445" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1445" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1445" s="10" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="G1445" s="11"/>
       <c r="H1445" s="12"/>
       <c r="I1445" s="13"/>
       <c r="J1445" s="13"/>
     </row>
-    <row r="1446" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1446" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1446" s="12">
         <v>44055</v>
       </c>
@@ -50030,258 +50120,278 @@
         <v>570</v>
       </c>
       <c r="F1446" s="10" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="G1446" s="11"/>
       <c r="H1446" s="12"/>
       <c r="I1446" s="13"/>
-      <c r="J1446" s="13" t="s">
-        <v>1590</v>
-      </c>
-    </row>
-    <row r="1447" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1446" s="13"/>
+    </row>
+    <row r="1447" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A1447" s="12">
-        <v>44047</v>
+        <v>44055</v>
       </c>
       <c r="B1447" s="9"/>
       <c r="C1447" s="14" t="s">
-        <v>537</v>
+        <v>898</v>
       </c>
       <c r="D1447" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1447" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1447" s="10" t="s">
-        <v>873</v>
-      </c>
-      <c r="G1447" s="11" t="s">
-        <v>1626</v>
-      </c>
+        <v>901</v>
+      </c>
+      <c r="G1447" s="11"/>
       <c r="H1447" s="12"/>
       <c r="I1447" s="13"/>
       <c r="J1447" s="13"/>
     </row>
-    <row r="1448" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1448" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1448" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1448" s="9"/>
       <c r="C1448" s="14" t="s">
-        <v>468</v>
+        <v>898</v>
       </c>
       <c r="D1448" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1448" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1448" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1448" s="11" t="s">
-        <v>1641</v>
-      </c>
+        <v>904</v>
+      </c>
+      <c r="G1448" s="11"/>
       <c r="H1448" s="12"/>
-      <c r="I1448" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1448" s="13"/>
-    </row>
-    <row r="1449" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="I1448" s="13"/>
+      <c r="J1448" s="13" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1449" s="12">
-        <v>43949</v>
+        <v>44047</v>
       </c>
       <c r="B1449" s="9"/>
       <c r="C1449" s="14" t="s">
-        <v>468</v>
+        <v>537</v>
       </c>
       <c r="D1449" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1449" s="11" t="s">
         <v>685</v>
       </c>
       <c r="F1449" s="10" t="s">
-        <v>705</v>
+        <v>873</v>
       </c>
       <c r="G1449" s="11" t="s">
-        <v>687</v>
+        <v>1626</v>
       </c>
       <c r="H1449" s="12"/>
-      <c r="I1449" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1449" s="13" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="1450" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1449" s="13"/>
+      <c r="J1449" s="13"/>
+    </row>
+    <row r="1450" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A1450" s="12">
-        <v>43838</v>
+        <v>43949</v>
       </c>
       <c r="B1450" s="9"/>
       <c r="C1450" s="14" t="s">
-        <v>103</v>
+        <v>468</v>
       </c>
       <c r="D1450" s="10" t="s">
-        <v>460</v>
+        <v>89</v>
       </c>
       <c r="E1450" s="11" t="s">
-        <v>647</v>
+        <v>685</v>
       </c>
       <c r="F1450" s="10" t="s">
-        <v>481</v>
+        <v>686</v>
       </c>
       <c r="G1450" s="11" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="H1450" s="12"/>
-      <c r="I1450" s="13"/>
-      <c r="J1450" s="13" t="s">
-        <v>1534</v>
-      </c>
-    </row>
-    <row r="1451" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I1450" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1450" s="13"/>
+    </row>
+    <row r="1451" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A1451" s="12">
-        <v>43816</v>
+        <v>43949</v>
       </c>
       <c r="B1451" s="9"/>
       <c r="C1451" s="14" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="D1451" s="10" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="E1451" s="11" t="s">
-        <v>570</v>
+        <v>685</v>
       </c>
       <c r="F1451" s="10" t="s">
-        <v>474</v>
+        <v>705</v>
       </c>
       <c r="G1451" s="11" t="s">
-        <v>1634</v>
+        <v>687</v>
       </c>
       <c r="H1451" s="12"/>
-      <c r="I1451" s="13"/>
+      <c r="I1451" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1451" s="13" t="s">
-        <v>1570</v>
-      </c>
-    </row>
-    <row r="1452" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1452" s="12">
-        <v>43762</v>
+        <v>43838</v>
       </c>
       <c r="B1452" s="9"/>
       <c r="C1452" s="14" t="s">
-        <v>446</v>
+        <v>103</v>
       </c>
       <c r="D1452" s="10" t="s">
-        <v>17</v>
+        <v>460</v>
       </c>
       <c r="E1452" s="11" t="s">
-        <v>837</v>
+        <v>647</v>
       </c>
       <c r="F1452" s="10" t="s">
-        <v>447</v>
+        <v>481</v>
       </c>
       <c r="G1452" s="11" t="s">
-        <v>1631</v>
+        <v>1642</v>
       </c>
       <c r="H1452" s="12"/>
       <c r="I1452" s="13"/>
-      <c r="J1452" s="13"/>
+      <c r="J1452" s="13" t="s">
+        <v>1534</v>
+      </c>
     </row>
     <row r="1453" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1453" s="12">
-        <v>44222</v>
+        <v>43816</v>
       </c>
       <c r="B1453" s="9"/>
       <c r="C1453" s="14" t="s">
-        <v>1495</v>
+        <v>475</v>
       </c>
       <c r="D1453" s="10" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="E1453" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1453" s="10" t="s">
-        <v>1494</v>
+        <v>474</v>
       </c>
       <c r="G1453" s="11" t="s">
-        <v>309</v>
+        <v>1634</v>
       </c>
       <c r="H1453" s="12"/>
       <c r="I1453" s="13"/>
-      <c r="J1453" s="13"/>
-    </row>
-    <row r="1454" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="J1453" s="13" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1454" s="12">
-        <v>44266</v>
+        <v>43762</v>
       </c>
       <c r="B1454" s="9"/>
       <c r="C1454" s="14" t="s">
-        <v>537</v>
+        <v>446</v>
       </c>
       <c r="D1454" s="10" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E1454" s="11" t="s">
-        <v>570</v>
+        <v>837</v>
       </c>
       <c r="F1454" s="10" t="s">
-        <v>1715</v>
-      </c>
-      <c r="G1454" s="11"/>
+        <v>447</v>
+      </c>
+      <c r="G1454" s="11" t="s">
+        <v>1631</v>
+      </c>
       <c r="H1454" s="12"/>
       <c r="I1454" s="13"/>
-      <c r="J1454" s="13" t="s">
-        <v>1716</v>
-      </c>
-    </row>
-    <row r="1455" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1454" s="13"/>
+    </row>
+    <row r="1455" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1455" s="12">
-        <v>44286</v>
+        <v>44222</v>
       </c>
       <c r="B1455" s="9"/>
       <c r="C1455" s="14" t="s">
-        <v>288</v>
+        <v>1495</v>
       </c>
       <c r="D1455" s="10" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="E1455" s="11" t="s">
-        <v>1580</v>
+        <v>837</v>
       </c>
       <c r="F1455" s="10" t="s">
-        <v>1840</v>
-      </c>
-      <c r="G1455" s="11"/>
+        <v>1494</v>
+      </c>
+      <c r="G1455" s="11" t="s">
+        <v>309</v>
+      </c>
       <c r="H1455" s="12"/>
       <c r="I1455" s="13"/>
       <c r="J1455" s="13"/>
     </row>
-    <row r="1456" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1456" s="12"/>
+    <row r="1456" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1456" s="12">
+        <v>44266</v>
+      </c>
       <c r="B1456" s="9"/>
-      <c r="C1456" s="14"/>
-      <c r="D1456" s="10"/>
-      <c r="E1456" s="11"/>
-      <c r="F1456" s="10"/>
+      <c r="C1456" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1456" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1456" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1456" s="10" t="s">
+        <v>1715</v>
+      </c>
       <c r="G1456" s="11"/>
       <c r="H1456" s="12"/>
       <c r="I1456" s="13"/>
-      <c r="J1456" s="13"/>
-    </row>
-    <row r="1457" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1457" s="12"/>
+      <c r="J1456" s="13" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1457" s="12">
+        <v>44286</v>
+      </c>
       <c r="B1457" s="9"/>
-      <c r="C1457" s="14"/>
-      <c r="D1457" s="10"/>
-      <c r="E1457" s="11"/>
-      <c r="F1457" s="10"/>
+      <c r="C1457" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1457" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1457" s="11" t="s">
+        <v>1580</v>
+      </c>
+      <c r="F1457" s="10" t="s">
+        <v>1840</v>
+      </c>
       <c r="G1457" s="11"/>
       <c r="H1457" s="12"/>
       <c r="I1457" s="13"/>
@@ -50335,10 +50445,34 @@
       <c r="I1461" s="13"/>
       <c r="J1461" s="13"/>
     </row>
+    <row r="1462" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1462" s="12"/>
+      <c r="B1462" s="9"/>
+      <c r="C1462" s="14"/>
+      <c r="D1462" s="10"/>
+      <c r="E1462" s="11"/>
+      <c r="F1462" s="10"/>
+      <c r="G1462" s="11"/>
+      <c r="H1462" s="12"/>
+      <c r="I1462" s="13"/>
+      <c r="J1462" s="13"/>
+    </row>
+    <row r="1463" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1463" s="12"/>
+      <c r="B1463" s="9"/>
+      <c r="C1463" s="14"/>
+      <c r="D1463" s="10"/>
+      <c r="E1463" s="11"/>
+      <c r="F1463" s="10"/>
+      <c r="G1463" s="11"/>
+      <c r="H1463" s="12"/>
+      <c r="I1463" s="13"/>
+      <c r="J1463" s="13"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1402" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1423:F1433">
-    <sortCondition ref="F1423:F1433"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1425:F1435">
+    <sortCondition ref="F1425:F1435"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -50354,7 +50488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE13D4C-C1F0-4B00-8A02-71F13D132F72}">
   <dimension ref="B1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Liberar João Cordeiro de Anexar Docs
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9ADF598-D1D1-4F43-B00C-AD29D185BBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273C7ABE-4098-47CE-BF3B-B7ECCDEA66DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10195" uniqueCount="2095">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10238" uniqueCount="2102">
   <si>
     <t>Responsável</t>
   </si>
@@ -6654,6 +6654,27 @@
   </si>
   <si>
     <t>Correção de diversos relatórios com problemas de performace</t>
+  </si>
+  <si>
+    <t>Acertos EFD</t>
+  </si>
+  <si>
+    <t>Auxiliar correção no procedimento de baixas</t>
+  </si>
+  <si>
+    <t>Pela segunda vez,no moment da medição ,apos erro de sistema um numero de medição desaparece,conforme segue. Por que acontece isso?</t>
+  </si>
+  <si>
+    <t>A explicação que vejo é que se alguém iniciou uma medição e não confirmou, enquanto havia outra medição sendo iniciada em outra tela ou por outro usuário, então o sistema reservou o número e não utilizou</t>
+  </si>
+  <si>
+    <t>Reunião a respeito da revisão de cadastros de Fornecedores e tabelas auxiliares</t>
+  </si>
+  <si>
+    <t>Desfazer as alterações da Balsa enviadas anteriormente</t>
+  </si>
+  <si>
+    <t>Acertos EFD Balsa</t>
   </si>
 </sst>
 </file>
@@ -7419,11 +7440,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1480"/>
+  <dimension ref="A1:J1489"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1423" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1436" sqref="A1436"/>
+      <pane ySplit="1" topLeftCell="A1430" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1442" sqref="A1442"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -50197,132 +50218,194 @@
       <c r="J1436" s="13"/>
     </row>
     <row r="1437" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1437" s="12"/>
-      <c r="B1437" s="12"/>
-      <c r="C1437" s="14"/>
-      <c r="D1437" s="10"/>
-      <c r="E1437" s="11"/>
-      <c r="F1437" s="10"/>
-      <c r="G1437" s="11"/>
-      <c r="H1437" s="12"/>
-      <c r="I1437" s="13"/>
+      <c r="A1437" s="12">
+        <v>44392</v>
+      </c>
+      <c r="B1437" s="12">
+        <v>44392</v>
+      </c>
+      <c r="C1437" s="14" t="s">
+        <v>1994</v>
+      </c>
+      <c r="D1437" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1437" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1437" s="10" t="s">
+        <v>2095</v>
+      </c>
+      <c r="G1437" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1437" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1437" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1437" s="13"/>
     </row>
     <row r="1438" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1438" s="12"/>
-      <c r="B1438" s="9"/>
-      <c r="C1438" s="14"/>
-      <c r="D1438" s="10"/>
-      <c r="E1438" s="11"/>
-      <c r="F1438" s="10"/>
-      <c r="G1438" s="11"/>
-      <c r="H1438" s="12"/>
-      <c r="I1438" s="13"/>
+      <c r="A1438" s="12">
+        <v>44392</v>
+      </c>
+      <c r="B1438" s="12">
+        <v>44392</v>
+      </c>
+      <c r="C1438" s="14" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D1438" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1438" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1438" s="10" t="s">
+        <v>2096</v>
+      </c>
+      <c r="G1438" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1438" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1438" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1438" s="13"/>
     </row>
-    <row r="1439" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1439" s="1" t="s">
-        <v>1479</v>
-      </c>
-      <c r="B1439" s="2" t="s">
-        <v>1480</v>
-      </c>
-      <c r="C1439" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1439" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1439" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1439" s="4" t="s">
-        <v>1581</v>
-      </c>
-      <c r="G1439" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1439" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1439" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1439" s="36"/>
+    <row r="1439" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1439" s="12">
+        <v>44392</v>
+      </c>
+      <c r="B1439" s="12">
+        <v>44392</v>
+      </c>
+      <c r="C1439" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1439" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1439" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1439" s="10" t="s">
+        <v>2097</v>
+      </c>
+      <c r="G1439" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1439" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1439" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1439" s="13" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="1440" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1440" s="12"/>
-      <c r="B1440" s="9"/>
-      <c r="C1440" s="14"/>
-      <c r="D1440" s="10"/>
-      <c r="E1440" s="11"/>
-      <c r="F1440" s="10"/>
-      <c r="G1440" s="11"/>
-      <c r="H1440" s="12"/>
-      <c r="I1440" s="13"/>
+      <c r="A1440" s="12">
+        <v>44392</v>
+      </c>
+      <c r="B1440" s="12">
+        <v>44392</v>
+      </c>
+      <c r="C1440" s="14" t="s">
+        <v>2036</v>
+      </c>
+      <c r="D1440" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1440" s="11" t="s">
+        <v>2092</v>
+      </c>
+      <c r="F1440" s="10" t="s">
+        <v>2099</v>
+      </c>
+      <c r="G1440" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1440" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1440" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1440" s="13"/>
     </row>
     <row r="1441" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1441" s="12"/>
-      <c r="B1441" s="9">
-        <v>44255</v>
+      <c r="A1441" s="12">
+        <v>44392</v>
+      </c>
+      <c r="B1441" s="12">
+        <v>44392</v>
       </c>
       <c r="C1441" s="14" t="s">
-        <v>13</v>
+        <v>1994</v>
       </c>
       <c r="D1441" s="10" t="s">
-        <v>584</v>
+        <v>89</v>
       </c>
       <c r="E1441" s="11" t="s">
-        <v>647</v>
+        <v>620</v>
       </c>
       <c r="F1441" s="10" t="s">
-        <v>1616</v>
-      </c>
-      <c r="G1441" s="11"/>
-      <c r="H1441" s="12"/>
-      <c r="I1441" s="13"/>
+        <v>2100</v>
+      </c>
+      <c r="G1441" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1441" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1441" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1441" s="13"/>
     </row>
     <row r="1442" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1442" s="12"/>
-      <c r="B1442" s="9">
-        <v>44255</v>
+      <c r="A1442" s="12">
+        <v>44392</v>
+      </c>
+      <c r="B1442" s="12">
+        <v>44392</v>
       </c>
       <c r="C1442" s="14" t="s">
-        <v>13</v>
+        <v>1994</v>
       </c>
       <c r="D1442" s="10" t="s">
-        <v>584</v>
+        <v>89</v>
       </c>
       <c r="E1442" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1442" s="10" t="s">
-        <v>1608</v>
-      </c>
-      <c r="G1442" s="11"/>
-      <c r="H1442" s="12"/>
-      <c r="I1442" s="13"/>
+        <v>2101</v>
+      </c>
+      <c r="G1442" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1442" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1442" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1442" s="13"/>
     </row>
     <row r="1443" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1443" s="12"/>
-      <c r="B1443" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1443" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1443" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1443" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1443" s="10" t="s">
-        <v>1613</v>
-      </c>
+      <c r="B1443" s="12"/>
+      <c r="C1443" s="14"/>
+      <c r="D1443" s="10"/>
+      <c r="E1443" s="11"/>
+      <c r="F1443" s="10"/>
       <c r="G1443" s="11"/>
       <c r="H1443" s="12"/>
       <c r="I1443" s="13"/>
@@ -50330,43 +50413,23 @@
     </row>
     <row r="1444" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1444" s="12"/>
-      <c r="B1444" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1444" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1444" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1444" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1444" s="10" t="s">
-        <v>1609</v>
-      </c>
+      <c r="B1444" s="12"/>
+      <c r="C1444" s="14"/>
+      <c r="D1444" s="10"/>
+      <c r="E1444" s="11"/>
+      <c r="F1444" s="10"/>
       <c r="G1444" s="11"/>
       <c r="H1444" s="12"/>
       <c r="I1444" s="13"/>
       <c r="J1444" s="13"/>
     </row>
     <row r="1445" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1445" s="12">
-        <v>44159</v>
-      </c>
-      <c r="B1445" s="9"/>
-      <c r="C1445" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1445" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1445" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1445" s="10" t="s">
-        <v>1617</v>
-      </c>
+      <c r="A1445" s="12"/>
+      <c r="B1445" s="12"/>
+      <c r="C1445" s="14"/>
+      <c r="D1445" s="10"/>
+      <c r="E1445" s="11"/>
+      <c r="F1445" s="10"/>
       <c r="G1445" s="11"/>
       <c r="H1445" s="12"/>
       <c r="I1445" s="13"/>
@@ -50374,87 +50437,65 @@
     </row>
     <row r="1446" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1446" s="12"/>
-      <c r="B1446" s="12">
-        <v>44309</v>
-      </c>
-      <c r="C1446" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1446" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1446" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1446" s="10" t="s">
-        <v>1610</v>
-      </c>
+      <c r="B1446" s="12"/>
+      <c r="C1446" s="14"/>
+      <c r="D1446" s="10"/>
+      <c r="E1446" s="11"/>
+      <c r="F1446" s="10"/>
       <c r="G1446" s="11"/>
       <c r="H1446" s="12"/>
       <c r="I1446" s="13"/>
       <c r="J1446" s="13"/>
     </row>
     <row r="1447" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1447" s="12">
-        <v>44239</v>
-      </c>
+      <c r="A1447" s="12"/>
       <c r="B1447" s="9"/>
-      <c r="C1447" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1447" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1447" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1447" s="10" t="s">
-        <v>1607</v>
-      </c>
+      <c r="C1447" s="14"/>
+      <c r="D1447" s="10"/>
+      <c r="E1447" s="11"/>
+      <c r="F1447" s="10"/>
       <c r="G1447" s="11"/>
       <c r="H1447" s="12"/>
       <c r="I1447" s="13"/>
       <c r="J1447" s="13"/>
     </row>
     <row r="1448" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1448" s="12"/>
-      <c r="B1448" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1448" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1448" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1448" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1448" s="10" t="s">
-        <v>1606</v>
-      </c>
-      <c r="G1448" s="11"/>
-      <c r="H1448" s="12"/>
-      <c r="I1448" s="13"/>
-      <c r="J1448" s="13"/>
+      <c r="A1448" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B1448" s="2" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C1448" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1448" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1448" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1448" s="4" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G1448" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1448" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1448" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1448" s="36"/>
     </row>
     <row r="1449" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1449" s="12"/>
-      <c r="B1449" s="9">
-        <v>44255</v>
-      </c>
-      <c r="C1449" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1449" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1449" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1449" s="10" t="s">
-        <v>1611</v>
-      </c>
+      <c r="B1449" s="9"/>
+      <c r="C1449" s="14"/>
+      <c r="D1449" s="10"/>
+      <c r="E1449" s="11"/>
+      <c r="F1449" s="10"/>
       <c r="G1449" s="11"/>
       <c r="H1449" s="12"/>
       <c r="I1449" s="13"/>
@@ -50462,8 +50503,8 @@
     </row>
     <row r="1450" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1450" s="12"/>
-      <c r="B1450" s="12">
-        <v>44309</v>
+      <c r="B1450" s="9">
+        <v>44255</v>
       </c>
       <c r="C1450" s="14" t="s">
         <v>13</v>
@@ -50475,7 +50516,7 @@
         <v>647</v>
       </c>
       <c r="F1450" s="10" t="s">
-        <v>1614</v>
+        <v>1616</v>
       </c>
       <c r="G1450" s="11"/>
       <c r="H1450" s="12"/>
@@ -50485,7 +50526,7 @@
     <row r="1451" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1451" s="12"/>
       <c r="B1451" s="9">
-        <v>44235</v>
+        <v>44255</v>
       </c>
       <c r="C1451" s="14" t="s">
         <v>13</v>
@@ -50497,7 +50538,7 @@
         <v>647</v>
       </c>
       <c r="F1451" s="10" t="s">
-        <v>1615</v>
+        <v>1608</v>
       </c>
       <c r="G1451" s="11"/>
       <c r="H1451" s="12"/>
@@ -50505,10 +50546,10 @@
       <c r="J1451" s="13"/>
     </row>
     <row r="1452" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1452" s="12">
-        <v>44245</v>
-      </c>
-      <c r="B1452" s="9"/>
+      <c r="A1452" s="12"/>
+      <c r="B1452" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1452" s="14" t="s">
         <v>13</v>
       </c>
@@ -50519,7 +50560,7 @@
         <v>647</v>
       </c>
       <c r="F1452" s="10" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="G1452" s="11"/>
       <c r="H1452" s="12"/>
@@ -50528,7 +50569,9 @@
     </row>
     <row r="1453" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1453" s="12"/>
-      <c r="B1453" s="9"/>
+      <c r="B1453" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1453" s="14" t="s">
         <v>13</v>
       </c>
@@ -50539,7 +50582,7 @@
         <v>647</v>
       </c>
       <c r="F1453" s="10" t="s">
-        <v>1583</v>
+        <v>1609</v>
       </c>
       <c r="G1453" s="11"/>
       <c r="H1453" s="12"/>
@@ -50547,125 +50590,131 @@
       <c r="J1453" s="13"/>
     </row>
     <row r="1454" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1454" s="12"/>
+      <c r="A1454" s="12">
+        <v>44159</v>
+      </c>
       <c r="B1454" s="9"/>
-      <c r="C1454" s="14"/>
-      <c r="D1454" s="10"/>
-      <c r="E1454" s="11"/>
-      <c r="F1454" s="10"/>
+      <c r="C1454" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1454" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1454" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1454" s="10" t="s">
+        <v>1617</v>
+      </c>
       <c r="G1454" s="11"/>
       <c r="H1454" s="12"/>
       <c r="I1454" s="13"/>
       <c r="J1454" s="13"/>
     </row>
     <row r="1455" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1455" s="12">
-        <v>44176</v>
-      </c>
-      <c r="B1455" s="9"/>
+      <c r="A1455" s="12"/>
+      <c r="B1455" s="12">
+        <v>44309</v>
+      </c>
       <c r="C1455" s="14" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D1455" s="10" t="s">
         <v>584</v>
       </c>
       <c r="E1455" s="11" t="s">
-        <v>1353</v>
+        <v>647</v>
       </c>
       <c r="F1455" s="10" t="s">
-        <v>1354</v>
+        <v>1610</v>
       </c>
       <c r="G1455" s="11"/>
       <c r="H1455" s="12"/>
       <c r="I1455" s="13"/>
       <c r="J1455" s="13"/>
     </row>
-    <row r="1456" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="1456" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1456" s="12">
-        <v>44252</v>
+        <v>44239</v>
       </c>
       <c r="B1456" s="9"/>
       <c r="C1456" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1456" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1456" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1456" s="10" t="s">
-        <v>1661</v>
+        <v>1607</v>
       </c>
       <c r="G1456" s="11"/>
       <c r="H1456" s="12"/>
       <c r="I1456" s="13"/>
-      <c r="J1456" s="13" t="s">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="1457" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1457" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1457" s="9"/>
+      <c r="J1456" s="13"/>
+    </row>
+    <row r="1457" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1457" s="12"/>
+      <c r="B1457" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1457" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1457" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1457" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1457" s="10" t="s">
-        <v>1660</v>
+        <v>1606</v>
       </c>
       <c r="G1457" s="11"/>
       <c r="H1457" s="12"/>
       <c r="I1457" s="13"/>
       <c r="J1457" s="13"/>
     </row>
-    <row r="1458" spans="1:10" ht="84" x14ac:dyDescent="0.2">
-      <c r="A1458" s="12">
-        <v>43864</v>
-      </c>
-      <c r="B1458" s="9"/>
+    <row r="1458" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1458" s="12"/>
+      <c r="B1458" s="9">
+        <v>44255</v>
+      </c>
       <c r="C1458" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1458" s="10" t="s">
-        <v>533</v>
+        <v>584</v>
       </c>
       <c r="E1458" s="11" t="s">
-        <v>1580</v>
+        <v>647</v>
       </c>
       <c r="F1458" s="10" t="s">
-        <v>534</v>
+        <v>1611</v>
       </c>
       <c r="G1458" s="11"/>
       <c r="H1458" s="12"/>
       <c r="I1458" s="13"/>
-      <c r="J1458" s="13" t="s">
-        <v>1707</v>
-      </c>
+      <c r="J1458" s="13"/>
     </row>
     <row r="1459" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1459" s="12">
-        <v>44112</v>
-      </c>
-      <c r="B1459" s="9"/>
+      <c r="A1459" s="12"/>
+      <c r="B1459" s="12">
+        <v>44309</v>
+      </c>
       <c r="C1459" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1459" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1459" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1459" s="10" t="s">
-        <v>1097</v>
+        <v>1614</v>
       </c>
       <c r="G1459" s="11"/>
       <c r="H1459" s="12"/>
@@ -50673,21 +50722,21 @@
       <c r="J1459" s="13"/>
     </row>
     <row r="1460" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1460" s="12">
-        <v>44088</v>
-      </c>
-      <c r="B1460" s="9"/>
+      <c r="A1460" s="12"/>
+      <c r="B1460" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1460" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1460" s="10" t="s">
-        <v>906</v>
+        <v>584</v>
       </c>
       <c r="E1460" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1460" s="10" t="s">
-        <v>1011</v>
+        <v>1615</v>
       </c>
       <c r="G1460" s="11"/>
       <c r="H1460" s="12"/>
@@ -50696,20 +50745,20 @@
     </row>
     <row r="1461" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1461" s="12">
-        <v>44055</v>
+        <v>44245</v>
       </c>
       <c r="B1461" s="9"/>
       <c r="C1461" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1461" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1461" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1461" s="10" t="s">
-        <v>903</v>
+        <v>1612</v>
       </c>
       <c r="G1461" s="11"/>
       <c r="H1461" s="12"/>
@@ -50717,21 +50766,19 @@
       <c r="J1461" s="13"/>
     </row>
     <row r="1462" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1462" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1462" s="12"/>
       <c r="B1462" s="9"/>
       <c r="C1462" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1462" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1462" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1462" s="10" t="s">
-        <v>902</v>
+        <v>1583</v>
       </c>
       <c r="G1462" s="11"/>
       <c r="H1462" s="12"/>
@@ -50739,52 +50786,42 @@
       <c r="J1462" s="13"/>
     </row>
     <row r="1463" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1463" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1463" s="12"/>
       <c r="B1463" s="9"/>
-      <c r="C1463" s="14" t="s">
-        <v>898</v>
-      </c>
-      <c r="D1463" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="E1463" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1463" s="10" t="s">
-        <v>900</v>
-      </c>
+      <c r="C1463" s="14"/>
+      <c r="D1463" s="10"/>
+      <c r="E1463" s="11"/>
+      <c r="F1463" s="10"/>
       <c r="G1463" s="11"/>
       <c r="H1463" s="12"/>
       <c r="I1463" s="13"/>
       <c r="J1463" s="13"/>
     </row>
-    <row r="1464" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="1464" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1464" s="12">
-        <v>44055</v>
+        <v>44176</v>
       </c>
       <c r="B1464" s="9"/>
       <c r="C1464" s="14" t="s">
-        <v>898</v>
+        <v>8</v>
       </c>
       <c r="D1464" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1464" s="11" t="s">
-        <v>570</v>
+        <v>1353</v>
       </c>
       <c r="F1464" s="10" t="s">
-        <v>901</v>
+        <v>1354</v>
       </c>
       <c r="G1464" s="11"/>
       <c r="H1464" s="12"/>
       <c r="I1464" s="13"/>
       <c r="J1464" s="13"/>
     </row>
-    <row r="1465" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1465" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1465" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1465" s="9"/>
       <c r="C1465" s="14" t="s">
@@ -50794,318 +50831,520 @@
         <v>494</v>
       </c>
       <c r="E1465" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1465" s="10" t="s">
-        <v>904</v>
+        <v>1661</v>
       </c>
       <c r="G1465" s="11"/>
       <c r="H1465" s="12"/>
       <c r="I1465" s="13"/>
       <c r="J1465" s="13" t="s">
-        <v>1590</v>
-      </c>
-    </row>
-    <row r="1466" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1466" s="12">
-        <v>44047</v>
+        <v>44252</v>
       </c>
       <c r="B1466" s="9"/>
       <c r="C1466" s="14" t="s">
-        <v>537</v>
+        <v>898</v>
       </c>
       <c r="D1466" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1466" s="11" t="s">
-        <v>685</v>
+        <v>759</v>
       </c>
       <c r="F1466" s="10" t="s">
-        <v>873</v>
-      </c>
-      <c r="G1466" s="11" t="s">
-        <v>1626</v>
-      </c>
+        <v>1660</v>
+      </c>
+      <c r="G1466" s="11"/>
       <c r="H1466" s="12"/>
       <c r="I1466" s="13"/>
       <c r="J1466" s="13"/>
     </row>
-    <row r="1467" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1467" spans="1:10" ht="84" x14ac:dyDescent="0.2">
       <c r="A1467" s="12">
-        <v>43949</v>
+        <v>43864</v>
       </c>
       <c r="B1467" s="9"/>
       <c r="C1467" s="14" t="s">
-        <v>468</v>
+        <v>19</v>
       </c>
       <c r="D1467" s="10" t="s">
-        <v>89</v>
+        <v>533</v>
       </c>
       <c r="E1467" s="11" t="s">
-        <v>685</v>
+        <v>1580</v>
       </c>
       <c r="F1467" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1467" s="11" t="s">
-        <v>1641</v>
-      </c>
+        <v>534</v>
+      </c>
+      <c r="G1467" s="11"/>
       <c r="H1467" s="12"/>
-      <c r="I1467" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1467" s="13"/>
-    </row>
-    <row r="1468" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="I1467" s="13"/>
+      <c r="J1467" s="13" t="s">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1468" s="12">
-        <v>43949</v>
+        <v>44112</v>
       </c>
       <c r="B1468" s="9"/>
       <c r="C1468" s="14" t="s">
-        <v>468</v>
+        <v>623</v>
       </c>
       <c r="D1468" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1468" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1468" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1468" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>1097</v>
+      </c>
+      <c r="G1468" s="11"/>
       <c r="H1468" s="12"/>
-      <c r="I1468" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1468" s="13" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="1469" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1468" s="13"/>
+      <c r="J1468" s="13"/>
+    </row>
+    <row r="1469" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1469" s="12">
-        <v>43838</v>
+        <v>44088</v>
       </c>
       <c r="B1469" s="9"/>
       <c r="C1469" s="14" t="s">
-        <v>103</v>
+        <v>19</v>
       </c>
       <c r="D1469" s="10" t="s">
-        <v>460</v>
+        <v>906</v>
       </c>
       <c r="E1469" s="11" t="s">
-        <v>647</v>
+        <v>685</v>
       </c>
       <c r="F1469" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G1469" s="11" t="s">
-        <v>1642</v>
-      </c>
+        <v>1011</v>
+      </c>
+      <c r="G1469" s="11"/>
       <c r="H1469" s="12"/>
       <c r="I1469" s="13"/>
-      <c r="J1469" s="13" t="s">
-        <v>1534</v>
-      </c>
+      <c r="J1469" s="13"/>
     </row>
     <row r="1470" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1470" s="12">
-        <v>43816</v>
+        <v>44055</v>
       </c>
       <c r="B1470" s="9"/>
       <c r="C1470" s="14" t="s">
-        <v>475</v>
+        <v>623</v>
       </c>
       <c r="D1470" s="10" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="E1470" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1470" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="G1470" s="11" t="s">
-        <v>1634</v>
-      </c>
+        <v>903</v>
+      </c>
+      <c r="G1470" s="11"/>
       <c r="H1470" s="12"/>
       <c r="I1470" s="13"/>
-      <c r="J1470" s="13" t="s">
-        <v>1570</v>
-      </c>
-    </row>
-    <row r="1471" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1470" s="13"/>
+    </row>
+    <row r="1471" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1471" s="12">
-        <v>43762</v>
+        <v>44055</v>
       </c>
       <c r="B1471" s="9"/>
       <c r="C1471" s="14" t="s">
-        <v>446</v>
+        <v>623</v>
       </c>
       <c r="D1471" s="10" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E1471" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1471" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G1471" s="11" t="s">
-        <v>1631</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="G1471" s="11"/>
       <c r="H1471" s="12"/>
       <c r="I1471" s="13"/>
       <c r="J1471" s="13"/>
     </row>
     <row r="1472" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1472" s="12">
-        <v>44222</v>
+        <v>44055</v>
       </c>
       <c r="B1472" s="9"/>
       <c r="C1472" s="14" t="s">
-        <v>1495</v>
+        <v>898</v>
       </c>
       <c r="D1472" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1472" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1472" s="10" t="s">
-        <v>1494</v>
-      </c>
-      <c r="G1472" s="11" t="s">
-        <v>309</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="G1472" s="11"/>
       <c r="H1472" s="12"/>
       <c r="I1472" s="13"/>
       <c r="J1472" s="13"/>
     </row>
-    <row r="1473" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1473" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A1473" s="12">
-        <v>44266</v>
+        <v>44055</v>
       </c>
       <c r="B1473" s="9"/>
       <c r="C1473" s="14" t="s">
-        <v>537</v>
+        <v>898</v>
       </c>
       <c r="D1473" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1473" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1473" s="10" t="s">
-        <v>1715</v>
+        <v>901</v>
       </c>
       <c r="G1473" s="11"/>
       <c r="H1473" s="12"/>
       <c r="I1473" s="13"/>
-      <c r="J1473" s="13" t="s">
-        <v>1716</v>
-      </c>
-    </row>
-    <row r="1474" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1473" s="13"/>
+    </row>
+    <row r="1474" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1474" s="12">
-        <v>44286</v>
+        <v>44055</v>
       </c>
       <c r="B1474" s="9"/>
       <c r="C1474" s="14" t="s">
-        <v>288</v>
+        <v>898</v>
       </c>
       <c r="D1474" s="10" t="s">
-        <v>25</v>
+        <v>494</v>
       </c>
       <c r="E1474" s="11" t="s">
-        <v>1580</v>
+        <v>570</v>
       </c>
       <c r="F1474" s="10" t="s">
-        <v>1840</v>
+        <v>904</v>
       </c>
       <c r="G1474" s="11"/>
       <c r="H1474" s="12"/>
       <c r="I1474" s="13"/>
-      <c r="J1474" s="13"/>
-    </row>
-    <row r="1475" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1475" s="12"/>
+      <c r="J1474" s="13" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1475" s="12">
+        <v>44047</v>
+      </c>
       <c r="B1475" s="9"/>
-      <c r="C1475" s="14"/>
-      <c r="D1475" s="10"/>
-      <c r="E1475" s="11"/>
-      <c r="F1475" s="10"/>
-      <c r="G1475" s="11"/>
+      <c r="C1475" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1475" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1475" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1475" s="10" t="s">
+        <v>873</v>
+      </c>
+      <c r="G1475" s="11" t="s">
+        <v>1626</v>
+      </c>
       <c r="H1475" s="12"/>
       <c r="I1475" s="13"/>
       <c r="J1475" s="13"/>
     </row>
-    <row r="1476" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1476" s="12"/>
+    <row r="1476" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1476" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1476" s="9"/>
-      <c r="C1476" s="14"/>
-      <c r="D1476" s="10"/>
-      <c r="E1476" s="11"/>
-      <c r="F1476" s="10"/>
-      <c r="G1476" s="11"/>
+      <c r="C1476" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1476" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1476" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1476" s="10" t="s">
+        <v>686</v>
+      </c>
+      <c r="G1476" s="11" t="s">
+        <v>1641</v>
+      </c>
       <c r="H1476" s="12"/>
-      <c r="I1476" s="13"/>
+      <c r="I1476" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1476" s="13"/>
     </row>
-    <row r="1477" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1477" s="12"/>
+    <row r="1477" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1477" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1477" s="9"/>
-      <c r="C1477" s="14"/>
-      <c r="D1477" s="10"/>
-      <c r="E1477" s="11"/>
-      <c r="F1477" s="10"/>
-      <c r="G1477" s="11"/>
+      <c r="C1477" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1477" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1477" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1477" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="G1477" s="11" t="s">
+        <v>687</v>
+      </c>
       <c r="H1477" s="12"/>
-      <c r="I1477" s="13"/>
-      <c r="J1477" s="13"/>
-    </row>
-    <row r="1478" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1478" s="12"/>
+      <c r="I1477" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1477" s="13" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1478" s="12">
+        <v>43838</v>
+      </c>
       <c r="B1478" s="9"/>
-      <c r="C1478" s="14"/>
-      <c r="D1478" s="10"/>
-      <c r="E1478" s="11"/>
-      <c r="F1478" s="10"/>
-      <c r="G1478" s="11"/>
+      <c r="C1478" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1478" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1478" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1478" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G1478" s="11" t="s">
+        <v>1642</v>
+      </c>
       <c r="H1478" s="12"/>
       <c r="I1478" s="13"/>
-      <c r="J1478" s="13"/>
+      <c r="J1478" s="13" t="s">
+        <v>1534</v>
+      </c>
     </row>
     <row r="1479" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1479" s="12"/>
+      <c r="A1479" s="12">
+        <v>43816</v>
+      </c>
       <c r="B1479" s="9"/>
-      <c r="C1479" s="14"/>
-      <c r="D1479" s="10"/>
-      <c r="E1479" s="11"/>
-      <c r="F1479" s="10"/>
-      <c r="G1479" s="11"/>
+      <c r="C1479" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1479" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1479" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1479" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G1479" s="11" t="s">
+        <v>1634</v>
+      </c>
       <c r="H1479" s="12"/>
       <c r="I1479" s="13"/>
-      <c r="J1479" s="13"/>
-    </row>
-    <row r="1480" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1480" s="12"/>
+      <c r="J1479" s="13" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1480" s="12">
+        <v>43762</v>
+      </c>
       <c r="B1480" s="9"/>
-      <c r="C1480" s="14"/>
-      <c r="D1480" s="10"/>
-      <c r="E1480" s="11"/>
-      <c r="F1480" s="10"/>
-      <c r="G1480" s="11"/>
+      <c r="C1480" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1480" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1480" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1480" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1480" s="11" t="s">
+        <v>1631</v>
+      </c>
       <c r="H1480" s="12"/>
       <c r="I1480" s="13"/>
       <c r="J1480" s="13"/>
     </row>
+    <row r="1481" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1481" s="12">
+        <v>44222</v>
+      </c>
+      <c r="B1481" s="9"/>
+      <c r="C1481" s="14" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D1481" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1481" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1481" s="10" t="s">
+        <v>1494</v>
+      </c>
+      <c r="G1481" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1481" s="12"/>
+      <c r="I1481" s="13"/>
+      <c r="J1481" s="13"/>
+    </row>
+    <row r="1482" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1482" s="12">
+        <v>44266</v>
+      </c>
+      <c r="B1482" s="9"/>
+      <c r="C1482" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1482" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1482" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1482" s="10" t="s">
+        <v>1715</v>
+      </c>
+      <c r="G1482" s="11"/>
+      <c r="H1482" s="12"/>
+      <c r="I1482" s="13"/>
+      <c r="J1482" s="13" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1483" s="12">
+        <v>44286</v>
+      </c>
+      <c r="B1483" s="9"/>
+      <c r="C1483" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1483" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1483" s="11" t="s">
+        <v>1580</v>
+      </c>
+      <c r="F1483" s="10" t="s">
+        <v>1840</v>
+      </c>
+      <c r="G1483" s="11"/>
+      <c r="H1483" s="12"/>
+      <c r="I1483" s="13"/>
+      <c r="J1483" s="13"/>
+    </row>
+    <row r="1484" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1484" s="12"/>
+      <c r="B1484" s="9"/>
+      <c r="C1484" s="14"/>
+      <c r="D1484" s="10"/>
+      <c r="E1484" s="11"/>
+      <c r="F1484" s="10"/>
+      <c r="G1484" s="11"/>
+      <c r="H1484" s="12"/>
+      <c r="I1484" s="13"/>
+      <c r="J1484" s="13"/>
+    </row>
+    <row r="1485" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1485" s="12"/>
+      <c r="B1485" s="9"/>
+      <c r="C1485" s="14"/>
+      <c r="D1485" s="10"/>
+      <c r="E1485" s="11"/>
+      <c r="F1485" s="10"/>
+      <c r="G1485" s="11"/>
+      <c r="H1485" s="12"/>
+      <c r="I1485" s="13"/>
+      <c r="J1485" s="13"/>
+    </row>
+    <row r="1486" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1486" s="12"/>
+      <c r="B1486" s="9"/>
+      <c r="C1486" s="14"/>
+      <c r="D1486" s="10"/>
+      <c r="E1486" s="11"/>
+      <c r="F1486" s="10"/>
+      <c r="G1486" s="11"/>
+      <c r="H1486" s="12"/>
+      <c r="I1486" s="13"/>
+      <c r="J1486" s="13"/>
+    </row>
+    <row r="1487" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1487" s="12"/>
+      <c r="B1487" s="9"/>
+      <c r="C1487" s="14"/>
+      <c r="D1487" s="10"/>
+      <c r="E1487" s="11"/>
+      <c r="F1487" s="10"/>
+      <c r="G1487" s="11"/>
+      <c r="H1487" s="12"/>
+      <c r="I1487" s="13"/>
+      <c r="J1487" s="13"/>
+    </row>
+    <row r="1488" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1488" s="12"/>
+      <c r="B1488" s="9"/>
+      <c r="C1488" s="14"/>
+      <c r="D1488" s="10"/>
+      <c r="E1488" s="11"/>
+      <c r="F1488" s="10"/>
+      <c r="G1488" s="11"/>
+      <c r="H1488" s="12"/>
+      <c r="I1488" s="13"/>
+      <c r="J1488" s="13"/>
+    </row>
+    <row r="1489" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1489" s="12"/>
+      <c r="B1489" s="9"/>
+      <c r="C1489" s="14"/>
+      <c r="D1489" s="10"/>
+      <c r="E1489" s="11"/>
+      <c r="F1489" s="10"/>
+      <c r="G1489" s="11"/>
+      <c r="H1489" s="12"/>
+      <c r="I1489" s="13"/>
+      <c r="J1489" s="13"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1402" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1442:F1452">
-    <sortCondition ref="F1442:F1452"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1451:F1461">
+    <sortCondition ref="F1451:F1461"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Ajustes Lib Ped Web
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901E7D6D-A50F-4D7E-A73B-684A2AB632D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8951DE06-5C24-4377-8BC0-80C8AF22AD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10523" uniqueCount="2152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10565" uniqueCount="2158">
   <si>
     <t>Responsável</t>
   </si>
@@ -6825,6 +6825,24 @@
   </si>
   <si>
     <t>Foram realizados diversos acertos de layout</t>
+  </si>
+  <si>
+    <t>Testes com a nova medição em área de produção</t>
+  </si>
+  <si>
+    <t>Campos descrição do contrato e nome do cliente não aparecem na nova medição</t>
+  </si>
+  <si>
+    <t>Relatorio Faturamento x Previsão de Faturamento não aparece numero cliente nova meidção</t>
+  </si>
+  <si>
+    <t>Reunião a respeito do fluxo do processos Financeiros e Contábeis</t>
+  </si>
+  <si>
+    <t>Melhoria de segurança no acesso a pedidos web</t>
+  </si>
+  <si>
+    <t>Correção de NFs para EFD 01-2017 - BK</t>
   </si>
 </sst>
 </file>
@@ -7593,11 +7611,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1533"/>
+  <dimension ref="A1:J1538"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1471" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1478" sqref="F1478"/>
+      <pane ySplit="1" topLeftCell="A1477" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1489" sqref="E1489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -51629,7 +51647,7 @@
         <v>19</v>
       </c>
       <c r="D1478" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1478" s="11" t="s">
         <v>837</v>
@@ -51659,7 +51677,7 @@
         <v>19</v>
       </c>
       <c r="D1479" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1479" s="11" t="s">
         <v>620</v>
@@ -51741,94 +51759,188 @@
       </c>
     </row>
     <row r="1482" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1482" s="12"/>
-      <c r="B1482" s="9"/>
-      <c r="C1482" s="14"/>
-      <c r="D1482" s="10"/>
-      <c r="E1482" s="11"/>
-      <c r="F1482" s="10"/>
-      <c r="G1482" s="11"/>
-      <c r="H1482" s="12"/>
-      <c r="I1482" s="13"/>
+      <c r="A1482" s="12">
+        <v>44413</v>
+      </c>
+      <c r="B1482" s="12">
+        <v>44419</v>
+      </c>
+      <c r="C1482" s="14" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D1482" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1482" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1482" s="10" t="s">
+        <v>2147</v>
+      </c>
+      <c r="G1482" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1482" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1482" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1482" s="13"/>
     </row>
     <row r="1483" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1483" s="12"/>
-      <c r="B1483" s="9"/>
-      <c r="C1483" s="14"/>
-      <c r="D1483" s="10"/>
-      <c r="E1483" s="11"/>
-      <c r="F1483" s="10"/>
-      <c r="G1483" s="11"/>
-      <c r="H1483" s="12"/>
-      <c r="I1483" s="13"/>
+      <c r="A1483" s="12">
+        <v>44420</v>
+      </c>
+      <c r="B1483" s="12">
+        <v>44420</v>
+      </c>
+      <c r="C1483" s="14" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D1483" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1483" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1483" s="10" t="s">
+        <v>2152</v>
+      </c>
+      <c r="G1483" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1483" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1483" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1483" s="13"/>
     </row>
     <row r="1484" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1484" s="12"/>
-      <c r="B1484" s="9"/>
-      <c r="C1484" s="14"/>
-      <c r="D1484" s="10"/>
-      <c r="E1484" s="11"/>
-      <c r="F1484" s="10"/>
-      <c r="G1484" s="11"/>
-      <c r="H1484" s="12"/>
-      <c r="I1484" s="13"/>
+      <c r="A1484" s="12">
+        <v>44420</v>
+      </c>
+      <c r="B1484" s="12">
+        <v>44420</v>
+      </c>
+      <c r="C1484" s="14" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D1484" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1484" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1484" s="10" t="s">
+        <v>2153</v>
+      </c>
+      <c r="G1484" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1484" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1484" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1484" s="13"/>
     </row>
-    <row r="1485" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1485" s="12"/>
-      <c r="B1485" s="12"/>
-      <c r="C1485" s="14"/>
-      <c r="D1485" s="10"/>
-      <c r="E1485" s="11"/>
-      <c r="F1485" s="10"/>
-      <c r="G1485" s="11"/>
-      <c r="H1485" s="12"/>
-      <c r="I1485" s="13"/>
-      <c r="J1485" s="13"/>
+    <row r="1485" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1485" s="12">
+        <v>44420</v>
+      </c>
+      <c r="B1485" s="12">
+        <v>44420</v>
+      </c>
+      <c r="C1485" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1485" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1485" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1485" s="10" t="s">
+        <v>2154</v>
+      </c>
+      <c r="G1485" s="11" t="s">
+        <v>1621</v>
+      </c>
+      <c r="H1485" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1485" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1485" s="13" t="s">
+        <v>1769</v>
+      </c>
     </row>
     <row r="1486" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1486" s="12"/>
-      <c r="B1486" s="12"/>
-      <c r="C1486" s="14"/>
-      <c r="D1486" s="10"/>
-      <c r="E1486" s="11"/>
-      <c r="F1486" s="10"/>
-      <c r="G1486" s="11"/>
-      <c r="H1486" s="12"/>
-      <c r="I1486" s="13"/>
+      <c r="A1486" s="12">
+        <v>44420</v>
+      </c>
+      <c r="B1486" s="12">
+        <v>44420</v>
+      </c>
+      <c r="C1486" s="14" t="s">
+        <v>2034</v>
+      </c>
+      <c r="D1486" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1486" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1486" s="10" t="s">
+        <v>2155</v>
+      </c>
+      <c r="G1486" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1486" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1486" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1486" s="13"/>
     </row>
     <row r="1487" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1487" s="12">
-        <v>44413</v>
-      </c>
-      <c r="B1487" s="12"/>
+        <v>44421</v>
+      </c>
+      <c r="B1487" s="12">
+        <v>44421</v>
+      </c>
       <c r="C1487" s="14" t="s">
-        <v>1056</v>
+        <v>13</v>
       </c>
       <c r="D1487" s="10" t="s">
-        <v>83</v>
+        <v>584</v>
       </c>
       <c r="E1487" s="11" t="s">
-        <v>837</v>
+        <v>698</v>
       </c>
       <c r="F1487" s="10" t="s">
-        <v>2147</v>
-      </c>
-      <c r="G1487" s="11" t="s">
-        <v>309</v>
-      </c>
+        <v>2156</v>
+      </c>
+      <c r="G1487" s="11"/>
       <c r="H1487" s="12"/>
       <c r="I1487" s="13"/>
       <c r="J1487" s="13"/>
     </row>
     <row r="1488" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1488" s="12">
-        <v>44399</v>
-      </c>
-      <c r="B1488" s="12"/>
+        <v>44421</v>
+      </c>
+      <c r="B1488" s="12">
+        <v>44421</v>
+      </c>
       <c r="C1488" s="14" t="s">
         <v>1992</v>
       </c>
@@ -51836,79 +51948,53 @@
         <v>89</v>
       </c>
       <c r="E1488" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1488" s="10" t="s">
-        <v>2115</v>
-      </c>
-      <c r="G1488" s="11"/>
-      <c r="H1488" s="12"/>
-      <c r="I1488" s="13"/>
+        <v>2157</v>
+      </c>
+      <c r="G1488" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1488" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1488" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1488" s="13"/>
     </row>
-    <row r="1489" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1489" s="12">
-        <v>44403</v>
-      </c>
+    <row r="1489" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1489" s="12"/>
       <c r="B1489" s="12"/>
-      <c r="C1489" s="14" t="s">
-        <v>1477</v>
-      </c>
-      <c r="D1489" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1489" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1489" s="10" t="s">
-        <v>2132</v>
-      </c>
+      <c r="C1489" s="14"/>
+      <c r="D1489" s="10"/>
+      <c r="E1489" s="11"/>
+      <c r="F1489" s="10"/>
       <c r="G1489" s="11"/>
       <c r="H1489" s="12"/>
       <c r="I1489" s="13"/>
       <c r="J1489" s="13"/>
     </row>
-    <row r="1490" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A1490" s="12">
-        <v>44266</v>
-      </c>
-      <c r="B1490" s="9"/>
-      <c r="C1490" s="14" t="s">
-        <v>537</v>
-      </c>
-      <c r="D1490" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1490" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1490" s="10" t="s">
-        <v>1713</v>
-      </c>
+    <row r="1490" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1490" s="12"/>
+      <c r="B1490" s="12"/>
+      <c r="C1490" s="14"/>
+      <c r="D1490" s="10"/>
+      <c r="E1490" s="11"/>
+      <c r="F1490" s="10"/>
       <c r="G1490" s="11"/>
       <c r="H1490" s="12"/>
       <c r="I1490" s="13"/>
-      <c r="J1490" s="13" t="s">
-        <v>1714</v>
-      </c>
-    </row>
-    <row r="1491" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1491" s="12">
-        <v>44286</v>
-      </c>
-      <c r="B1491" s="9"/>
-      <c r="C1491" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D1491" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1491" s="11" t="s">
-        <v>620</v>
-      </c>
-      <c r="F1491" s="10" t="s">
-        <v>1838</v>
-      </c>
+      <c r="J1490" s="13"/>
+    </row>
+    <row r="1491" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1491" s="12"/>
+      <c r="B1491" s="12"/>
+      <c r="C1491" s="14"/>
+      <c r="D1491" s="10"/>
+      <c r="E1491" s="11"/>
+      <c r="F1491" s="10"/>
       <c r="G1491" s="11"/>
       <c r="H1491" s="12"/>
       <c r="I1491" s="13"/>
@@ -51927,74 +52013,98 @@
       <c r="J1492" s="13"/>
     </row>
     <row r="1493" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1493" s="12"/>
+      <c r="A1493" s="12">
+        <v>44399</v>
+      </c>
       <c r="B1493" s="12"/>
-      <c r="C1493" s="14"/>
-      <c r="D1493" s="10"/>
-      <c r="E1493" s="11"/>
-      <c r="F1493" s="10"/>
+      <c r="C1493" s="14" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D1493" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1493" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1493" s="10" t="s">
+        <v>2115</v>
+      </c>
       <c r="G1493" s="11"/>
       <c r="H1493" s="12"/>
       <c r="I1493" s="13"/>
       <c r="J1493" s="13"/>
     </row>
-    <row r="1494" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1494" s="12"/>
+    <row r="1494" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1494" s="12">
+        <v>44403</v>
+      </c>
       <c r="B1494" s="12"/>
-      <c r="C1494" s="14"/>
-      <c r="D1494" s="10"/>
-      <c r="E1494" s="11"/>
-      <c r="F1494" s="10"/>
+      <c r="C1494" s="14" t="s">
+        <v>1477</v>
+      </c>
+      <c r="D1494" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1494" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1494" s="10" t="s">
+        <v>2132</v>
+      </c>
       <c r="G1494" s="11"/>
       <c r="H1494" s="12"/>
       <c r="I1494" s="13"/>
       <c r="J1494" s="13"/>
     </row>
-    <row r="1495" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1495" s="12"/>
+    <row r="1495" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1495" s="12">
+        <v>44266</v>
+      </c>
       <c r="B1495" s="9"/>
-      <c r="C1495" s="14"/>
-      <c r="D1495" s="10"/>
-      <c r="E1495" s="11"/>
-      <c r="F1495" s="10"/>
+      <c r="C1495" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1495" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1495" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1495" s="10" t="s">
+        <v>1713</v>
+      </c>
       <c r="G1495" s="11"/>
       <c r="H1495" s="12"/>
       <c r="I1495" s="13"/>
-      <c r="J1495" s="13"/>
-    </row>
-    <row r="1496" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1496" s="1" t="s">
-        <v>1479</v>
-      </c>
-      <c r="B1496" s="2" t="s">
-        <v>1480</v>
-      </c>
-      <c r="C1496" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1496" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1496" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1496" s="4" t="s">
-        <v>1579</v>
-      </c>
-      <c r="G1496" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1496" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1496" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1496" s="36"/>
+      <c r="J1495" s="13" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1496" s="12">
+        <v>44286</v>
+      </c>
+      <c r="B1496" s="9"/>
+      <c r="C1496" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1496" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1496" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1496" s="10" t="s">
+        <v>1838</v>
+      </c>
+      <c r="G1496" s="11"/>
+      <c r="H1496" s="12"/>
+      <c r="I1496" s="13"/>
+      <c r="J1496" s="13"/>
     </row>
     <row r="1497" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1497" s="12"/>
-      <c r="B1497" s="9"/>
+      <c r="B1497" s="12"/>
       <c r="C1497" s="14"/>
       <c r="D1497" s="10"/>
       <c r="E1497" s="11"/>
@@ -52006,21 +52116,11 @@
     </row>
     <row r="1498" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1498" s="12"/>
-      <c r="B1498" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1498" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1498" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1498" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1498" s="10" t="s">
-        <v>1614</v>
-      </c>
+      <c r="B1498" s="12"/>
+      <c r="C1498" s="14"/>
+      <c r="D1498" s="10"/>
+      <c r="E1498" s="11"/>
+      <c r="F1498" s="10"/>
       <c r="G1498" s="11"/>
       <c r="H1498" s="12"/>
       <c r="I1498" s="13"/>
@@ -52028,21 +52128,11 @@
     </row>
     <row r="1499" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1499" s="12"/>
-      <c r="B1499" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1499" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1499" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1499" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1499" s="10" t="s">
-        <v>1606</v>
-      </c>
+      <c r="B1499" s="12"/>
+      <c r="C1499" s="14"/>
+      <c r="D1499" s="10"/>
+      <c r="E1499" s="11"/>
+      <c r="F1499" s="10"/>
       <c r="G1499" s="11"/>
       <c r="H1499" s="12"/>
       <c r="I1499" s="13"/>
@@ -52050,63 +52140,53 @@
     </row>
     <row r="1500" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1500" s="12"/>
-      <c r="B1500" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1500" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1500" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1500" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1500" s="10" t="s">
-        <v>1611</v>
-      </c>
+      <c r="B1500" s="9"/>
+      <c r="C1500" s="14"/>
+      <c r="D1500" s="10"/>
+      <c r="E1500" s="11"/>
+      <c r="F1500" s="10"/>
       <c r="G1500" s="11"/>
       <c r="H1500" s="12"/>
       <c r="I1500" s="13"/>
       <c r="J1500" s="13"/>
     </row>
     <row r="1501" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1501" s="12"/>
-      <c r="B1501" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1501" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1501" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1501" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1501" s="10" t="s">
-        <v>1607</v>
-      </c>
-      <c r="G1501" s="11"/>
-      <c r="H1501" s="12"/>
-      <c r="I1501" s="13"/>
-      <c r="J1501" s="13"/>
+      <c r="A1501" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B1501" s="2" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C1501" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1501" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1501" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1501" s="4" t="s">
+        <v>1579</v>
+      </c>
+      <c r="G1501" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1501" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1501" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1501" s="36"/>
     </row>
     <row r="1502" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1502" s="12"/>
       <c r="B1502" s="9"/>
-      <c r="C1502" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1502" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1502" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1502" s="10" t="s">
-        <v>1615</v>
-      </c>
+      <c r="C1502" s="14"/>
+      <c r="D1502" s="10"/>
+      <c r="E1502" s="11"/>
+      <c r="F1502" s="10"/>
       <c r="G1502" s="11"/>
       <c r="H1502" s="12"/>
       <c r="I1502" s="13"/>
@@ -52127,7 +52207,7 @@
         <v>647</v>
       </c>
       <c r="F1503" s="10" t="s">
-        <v>1608</v>
+        <v>1614</v>
       </c>
       <c r="G1503" s="11"/>
       <c r="H1503" s="12"/>
@@ -52136,7 +52216,9 @@
     </row>
     <row r="1504" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1504" s="12"/>
-      <c r="B1504" s="9"/>
+      <c r="B1504" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1504" s="14" t="s">
         <v>13</v>
       </c>
@@ -52147,7 +52229,7 @@
         <v>647</v>
       </c>
       <c r="F1504" s="10" t="s">
-        <v>1605</v>
+        <v>1606</v>
       </c>
       <c r="G1504" s="11"/>
       <c r="H1504" s="12"/>
@@ -52169,7 +52251,7 @@
         <v>647</v>
       </c>
       <c r="F1505" s="10" t="s">
-        <v>1604</v>
+        <v>1611</v>
       </c>
       <c r="G1505" s="11"/>
       <c r="H1505" s="12"/>
@@ -52191,7 +52273,7 @@
         <v>647</v>
       </c>
       <c r="F1506" s="10" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="G1506" s="11"/>
       <c r="H1506" s="12"/>
@@ -52200,9 +52282,7 @@
     </row>
     <row r="1507" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1507" s="12"/>
-      <c r="B1507" s="12">
-        <v>44402</v>
-      </c>
+      <c r="B1507" s="9"/>
       <c r="C1507" s="14" t="s">
         <v>13</v>
       </c>
@@ -52213,7 +52293,7 @@
         <v>647</v>
       </c>
       <c r="F1507" s="10" t="s">
-        <v>1612</v>
+        <v>1615</v>
       </c>
       <c r="G1507" s="11"/>
       <c r="H1507" s="12"/>
@@ -52222,8 +52302,8 @@
     </row>
     <row r="1508" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1508" s="12"/>
-      <c r="B1508" s="9">
-        <v>44235</v>
+      <c r="B1508" s="12">
+        <v>44402</v>
       </c>
       <c r="C1508" s="14" t="s">
         <v>13</v>
@@ -52235,7 +52315,7 @@
         <v>647</v>
       </c>
       <c r="F1508" s="10" t="s">
-        <v>1613</v>
+        <v>1608</v>
       </c>
       <c r="G1508" s="11"/>
       <c r="H1508" s="12"/>
@@ -52255,7 +52335,7 @@
         <v>647</v>
       </c>
       <c r="F1509" s="10" t="s">
-        <v>1610</v>
+        <v>1605</v>
       </c>
       <c r="G1509" s="11"/>
       <c r="H1509" s="12"/>
@@ -52264,7 +52344,9 @@
     </row>
     <row r="1510" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1510" s="12"/>
-      <c r="B1510" s="9"/>
+      <c r="B1510" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1510" s="14" t="s">
         <v>13</v>
       </c>
@@ -52275,7 +52357,7 @@
         <v>647</v>
       </c>
       <c r="F1510" s="10" t="s">
-        <v>1581</v>
+        <v>1604</v>
       </c>
       <c r="G1510" s="11"/>
       <c r="H1510" s="12"/>
@@ -52284,78 +52366,84 @@
     </row>
     <row r="1511" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1511" s="12"/>
-      <c r="B1511" s="9"/>
-      <c r="C1511" s="14"/>
-      <c r="D1511" s="10"/>
-      <c r="E1511" s="11"/>
-      <c r="F1511" s="10"/>
+      <c r="B1511" s="12">
+        <v>44402</v>
+      </c>
+      <c r="C1511" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1511" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1511" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1511" s="10" t="s">
+        <v>1609</v>
+      </c>
       <c r="G1511" s="11"/>
       <c r="H1511" s="12"/>
       <c r="I1511" s="13"/>
       <c r="J1511" s="13"/>
     </row>
     <row r="1512" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1512" s="12">
-        <v>44176</v>
-      </c>
-      <c r="B1512" s="9"/>
+      <c r="A1512" s="12"/>
+      <c r="B1512" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1512" s="14" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D1512" s="10" t="s">
         <v>584</v>
       </c>
       <c r="E1512" s="11" t="s">
-        <v>1353</v>
+        <v>647</v>
       </c>
       <c r="F1512" s="10" t="s">
-        <v>1354</v>
+        <v>1612</v>
       </c>
       <c r="G1512" s="11"/>
       <c r="H1512" s="12"/>
       <c r="I1512" s="13"/>
       <c r="J1512" s="13"/>
     </row>
-    <row r="1513" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1513" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1513" s="9"/>
+    <row r="1513" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1513" s="12"/>
+      <c r="B1513" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1513" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1513" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1513" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1513" s="10" t="s">
-        <v>1659</v>
+        <v>1613</v>
       </c>
       <c r="G1513" s="11"/>
       <c r="H1513" s="12"/>
       <c r="I1513" s="13"/>
-      <c r="J1513" s="13" t="s">
-        <v>1682</v>
-      </c>
-    </row>
-    <row r="1514" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1514" s="12">
-        <v>44252</v>
-      </c>
+      <c r="J1513" s="13"/>
+    </row>
+    <row r="1514" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1514" s="12"/>
       <c r="B1514" s="9"/>
       <c r="C1514" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1514" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1514" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1514" s="10" t="s">
-        <v>1658</v>
+        <v>1610</v>
       </c>
       <c r="G1514" s="11"/>
       <c r="H1514" s="12"/>
@@ -52363,21 +52451,19 @@
       <c r="J1514" s="13"/>
     </row>
     <row r="1515" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1515" s="12">
-        <v>44112</v>
-      </c>
+      <c r="A1515" s="12"/>
       <c r="B1515" s="9"/>
       <c r="C1515" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1515" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1515" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1515" s="10" t="s">
-        <v>1097</v>
+        <v>1581</v>
       </c>
       <c r="G1515" s="11"/>
       <c r="H1515" s="12"/>
@@ -52385,22 +52471,12 @@
       <c r="J1515" s="13"/>
     </row>
     <row r="1516" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1516" s="12">
-        <v>44088</v>
-      </c>
+      <c r="A1516" s="12"/>
       <c r="B1516" s="9"/>
-      <c r="C1516" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1516" s="10" t="s">
-        <v>906</v>
-      </c>
-      <c r="E1516" s="11" t="s">
-        <v>685</v>
-      </c>
-      <c r="F1516" s="10" t="s">
-        <v>1011</v>
-      </c>
+      <c r="C1516" s="14"/>
+      <c r="D1516" s="10"/>
+      <c r="E1516" s="11"/>
+      <c r="F1516" s="10"/>
       <c r="G1516" s="11"/>
       <c r="H1516" s="12"/>
       <c r="I1516" s="13"/>
@@ -52408,51 +52484,53 @@
     </row>
     <row r="1517" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1517" s="12">
-        <v>44055</v>
+        <v>44176</v>
       </c>
       <c r="B1517" s="9"/>
       <c r="C1517" s="14" t="s">
-        <v>623</v>
+        <v>8</v>
       </c>
       <c r="D1517" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1517" s="11" t="s">
-        <v>570</v>
+        <v>1353</v>
       </c>
       <c r="F1517" s="10" t="s">
-        <v>903</v>
+        <v>1354</v>
       </c>
       <c r="G1517" s="11"/>
       <c r="H1517" s="12"/>
       <c r="I1517" s="13"/>
       <c r="J1517" s="13"/>
     </row>
-    <row r="1518" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1518" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1518" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1518" s="9"/>
       <c r="C1518" s="14" t="s">
-        <v>623</v>
+        <v>898</v>
       </c>
       <c r="D1518" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1518" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1518" s="10" t="s">
-        <v>902</v>
+        <v>1659</v>
       </c>
       <c r="G1518" s="11"/>
       <c r="H1518" s="12"/>
       <c r="I1518" s="13"/>
-      <c r="J1518" s="13"/>
-    </row>
-    <row r="1519" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1518" s="13" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="1519" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1519" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1519" s="9"/>
       <c r="C1519" s="14" t="s">
@@ -52462,272 +52540,322 @@
         <v>494</v>
       </c>
       <c r="E1519" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1519" s="10" t="s">
-        <v>900</v>
+        <v>1658</v>
       </c>
       <c r="G1519" s="11"/>
       <c r="H1519" s="12"/>
       <c r="I1519" s="13"/>
       <c r="J1519" s="13"/>
     </row>
-    <row r="1520" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="1520" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1520" s="12">
-        <v>44055</v>
+        <v>44112</v>
       </c>
       <c r="B1520" s="9"/>
       <c r="C1520" s="14" t="s">
-        <v>898</v>
+        <v>623</v>
       </c>
       <c r="D1520" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1520" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1520" s="10" t="s">
-        <v>901</v>
+        <v>1097</v>
       </c>
       <c r="G1520" s="11"/>
       <c r="H1520" s="12"/>
       <c r="I1520" s="13"/>
       <c r="J1520" s="13"/>
     </row>
-    <row r="1521" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1521" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1521" s="12">
-        <v>44055</v>
+        <v>44088</v>
       </c>
       <c r="B1521" s="9"/>
       <c r="C1521" s="14" t="s">
-        <v>898</v>
+        <v>19</v>
       </c>
       <c r="D1521" s="10" t="s">
-        <v>494</v>
+        <v>906</v>
       </c>
       <c r="E1521" s="11" t="s">
-        <v>570</v>
+        <v>685</v>
       </c>
       <c r="F1521" s="10" t="s">
-        <v>904</v>
+        <v>1011</v>
       </c>
       <c r="G1521" s="11"/>
       <c r="H1521" s="12"/>
       <c r="I1521" s="13"/>
-      <c r="J1521" s="13" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="1522" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1521" s="13"/>
+    </row>
+    <row r="1522" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1522" s="12">
-        <v>44047</v>
+        <v>44055</v>
       </c>
       <c r="B1522" s="9"/>
       <c r="C1522" s="14" t="s">
-        <v>537</v>
+        <v>623</v>
       </c>
       <c r="D1522" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E1522" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1522" s="10" t="s">
-        <v>873</v>
-      </c>
-      <c r="G1522" s="11" t="s">
-        <v>1624</v>
-      </c>
+        <v>903</v>
+      </c>
+      <c r="G1522" s="11"/>
       <c r="H1522" s="12"/>
       <c r="I1522" s="13"/>
       <c r="J1522" s="13"/>
     </row>
-    <row r="1523" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1523" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1523" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1523" s="9"/>
       <c r="C1523" s="14" t="s">
-        <v>468</v>
+        <v>623</v>
       </c>
       <c r="D1523" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1523" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1523" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1523" s="11" t="s">
-        <v>1639</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="G1523" s="11"/>
       <c r="H1523" s="12"/>
-      <c r="I1523" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1523" s="13"/>
       <c r="J1523" s="13"/>
     </row>
-    <row r="1524" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1524" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1524" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1524" s="9"/>
       <c r="C1524" s="14" t="s">
-        <v>468</v>
+        <v>898</v>
       </c>
       <c r="D1524" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1524" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1524" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1524" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="G1524" s="11"/>
       <c r="H1524" s="12"/>
-      <c r="I1524" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1524" s="13" t="s">
-        <v>1568</v>
-      </c>
-    </row>
-    <row r="1525" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1524" s="13"/>
+      <c r="J1524" s="13"/>
+    </row>
+    <row r="1525" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A1525" s="12">
-        <v>43838</v>
+        <v>44055</v>
       </c>
       <c r="B1525" s="9"/>
       <c r="C1525" s="14" t="s">
-        <v>103</v>
+        <v>898</v>
       </c>
       <c r="D1525" s="10" t="s">
-        <v>460</v>
+        <v>494</v>
       </c>
       <c r="E1525" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1525" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G1525" s="11" t="s">
-        <v>1640</v>
-      </c>
+        <v>901</v>
+      </c>
+      <c r="G1525" s="11"/>
       <c r="H1525" s="12"/>
       <c r="I1525" s="13"/>
-      <c r="J1525" s="13" t="s">
-        <v>1533</v>
-      </c>
-    </row>
-    <row r="1526" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1525" s="13"/>
+    </row>
+    <row r="1526" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1526" s="12">
-        <v>43816</v>
+        <v>44055</v>
       </c>
       <c r="B1526" s="9"/>
       <c r="C1526" s="14" t="s">
-        <v>475</v>
+        <v>898</v>
       </c>
       <c r="D1526" s="10" t="s">
-        <v>38</v>
+        <v>494</v>
       </c>
       <c r="E1526" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1526" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="G1526" s="11" t="s">
-        <v>1632</v>
-      </c>
+        <v>904</v>
+      </c>
+      <c r="G1526" s="11"/>
       <c r="H1526" s="12"/>
       <c r="I1526" s="13"/>
       <c r="J1526" s="13" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="1527" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="1527" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1527" s="12">
-        <v>43762</v>
+        <v>44047</v>
       </c>
       <c r="B1527" s="9"/>
       <c r="C1527" s="14" t="s">
-        <v>446</v>
+        <v>537</v>
       </c>
       <c r="D1527" s="10" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E1527" s="11" t="s">
-        <v>837</v>
+        <v>685</v>
       </c>
       <c r="F1527" s="10" t="s">
-        <v>447</v>
+        <v>873</v>
       </c>
       <c r="G1527" s="11" t="s">
-        <v>1629</v>
+        <v>1624</v>
       </c>
       <c r="H1527" s="12"/>
       <c r="I1527" s="13"/>
       <c r="J1527" s="13"/>
     </row>
-    <row r="1528" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1528" s="12"/>
+    <row r="1528" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1528" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1528" s="9"/>
-      <c r="C1528" s="14"/>
-      <c r="D1528" s="10"/>
-      <c r="E1528" s="11"/>
-      <c r="F1528" s="10"/>
-      <c r="G1528" s="11"/>
+      <c r="C1528" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1528" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1528" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1528" s="10" t="s">
+        <v>686</v>
+      </c>
+      <c r="G1528" s="11" t="s">
+        <v>1639</v>
+      </c>
       <c r="H1528" s="12"/>
-      <c r="I1528" s="13"/>
+      <c r="I1528" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1528" s="13"/>
     </row>
-    <row r="1529" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1529" s="12"/>
+    <row r="1529" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1529" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1529" s="9"/>
-      <c r="C1529" s="14"/>
-      <c r="D1529" s="10"/>
-      <c r="E1529" s="11"/>
-      <c r="F1529" s="10"/>
-      <c r="G1529" s="11"/>
+      <c r="C1529" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1529" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1529" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1529" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="G1529" s="11" t="s">
+        <v>687</v>
+      </c>
       <c r="H1529" s="12"/>
-      <c r="I1529" s="13"/>
-      <c r="J1529" s="13"/>
-    </row>
-    <row r="1530" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1530" s="12"/>
+      <c r="I1529" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1529" s="13" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="1530" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1530" s="12">
+        <v>43838</v>
+      </c>
       <c r="B1530" s="9"/>
-      <c r="C1530" s="14"/>
-      <c r="D1530" s="10"/>
-      <c r="E1530" s="11"/>
-      <c r="F1530" s="10"/>
-      <c r="G1530" s="11"/>
+      <c r="C1530" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1530" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1530" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1530" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G1530" s="11" t="s">
+        <v>1640</v>
+      </c>
       <c r="H1530" s="12"/>
       <c r="I1530" s="13"/>
-      <c r="J1530" s="13"/>
+      <c r="J1530" s="13" t="s">
+        <v>1533</v>
+      </c>
     </row>
     <row r="1531" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1531" s="12"/>
+      <c r="A1531" s="12">
+        <v>43816</v>
+      </c>
       <c r="B1531" s="9"/>
-      <c r="C1531" s="14"/>
-      <c r="D1531" s="10"/>
-      <c r="E1531" s="11"/>
-      <c r="F1531" s="10"/>
-      <c r="G1531" s="11"/>
+      <c r="C1531" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1531" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1531" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1531" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G1531" s="11" t="s">
+        <v>1632</v>
+      </c>
       <c r="H1531" s="12"/>
       <c r="I1531" s="13"/>
-      <c r="J1531" s="13"/>
-    </row>
-    <row r="1532" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1532" s="12"/>
+      <c r="J1531" s="13" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="1532" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1532" s="12">
+        <v>43762</v>
+      </c>
       <c r="B1532" s="9"/>
-      <c r="C1532" s="14"/>
-      <c r="D1532" s="10"/>
-      <c r="E1532" s="11"/>
-      <c r="F1532" s="10"/>
-      <c r="G1532" s="11"/>
+      <c r="C1532" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1532" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1532" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1532" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1532" s="11" t="s">
+        <v>1629</v>
+      </c>
       <c r="H1532" s="12"/>
       <c r="I1532" s="13"/>
       <c r="J1532" s="13"/>
@@ -52744,10 +52872,70 @@
       <c r="I1533" s="13"/>
       <c r="J1533" s="13"/>
     </row>
+    <row r="1534" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1534" s="12"/>
+      <c r="B1534" s="9"/>
+      <c r="C1534" s="14"/>
+      <c r="D1534" s="10"/>
+      <c r="E1534" s="11"/>
+      <c r="F1534" s="10"/>
+      <c r="G1534" s="11"/>
+      <c r="H1534" s="12"/>
+      <c r="I1534" s="13"/>
+      <c r="J1534" s="13"/>
+    </row>
+    <row r="1535" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1535" s="12"/>
+      <c r="B1535" s="9"/>
+      <c r="C1535" s="14"/>
+      <c r="D1535" s="10"/>
+      <c r="E1535" s="11"/>
+      <c r="F1535" s="10"/>
+      <c r="G1535" s="11"/>
+      <c r="H1535" s="12"/>
+      <c r="I1535" s="13"/>
+      <c r="J1535" s="13"/>
+    </row>
+    <row r="1536" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1536" s="12"/>
+      <c r="B1536" s="9"/>
+      <c r="C1536" s="14"/>
+      <c r="D1536" s="10"/>
+      <c r="E1536" s="11"/>
+      <c r="F1536" s="10"/>
+      <c r="G1536" s="11"/>
+      <c r="H1536" s="12"/>
+      <c r="I1536" s="13"/>
+      <c r="J1536" s="13"/>
+    </row>
+    <row r="1537" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1537" s="12"/>
+      <c r="B1537" s="9"/>
+      <c r="C1537" s="14"/>
+      <c r="D1537" s="10"/>
+      <c r="E1537" s="11"/>
+      <c r="F1537" s="10"/>
+      <c r="G1537" s="11"/>
+      <c r="H1537" s="12"/>
+      <c r="I1537" s="13"/>
+      <c r="J1537" s="13"/>
+    </row>
+    <row r="1538" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1538" s="12"/>
+      <c r="B1538" s="9"/>
+      <c r="C1538" s="14"/>
+      <c r="D1538" s="10"/>
+      <c r="E1538" s="11"/>
+      <c r="F1538" s="10"/>
+      <c r="G1538" s="11"/>
+      <c r="H1538" s="12"/>
+      <c r="I1538" s="13"/>
+      <c r="J1538" s="13"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1479" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1499:F1509">
-    <sortCondition ref="F1499:F1509"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1504:F1514">
+    <sortCondition ref="F1504:F1514"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Início Lib Doc de Entrada
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8951DE06-5C24-4377-8BC0-80C8AF22AD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36F20AE-202A-431A-BB46-0452E2C3C612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10565" uniqueCount="2158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10582" uniqueCount="2160">
   <si>
     <t>Responsável</t>
   </si>
@@ -6843,6 +6843,12 @@
   </si>
   <si>
     <t>Correção de NFs para EFD 01-2017 - BK</t>
+  </si>
+  <si>
+    <t>Atualização: 21-08-09-LIB_LABEL_09082021_P12_LOBO</t>
+  </si>
+  <si>
+    <t>Atualização Gestão de Contratos 21-08-05_ATUALIZACAO_12.1.25_GCT_EXPEDICAO_CONTINUA</t>
   </si>
 </sst>
 </file>
@@ -7611,11 +7617,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1538"/>
+  <dimension ref="A1:J1542"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1477" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1489" sqref="E1489"/>
+      <pane ySplit="1" topLeftCell="A1483" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1490" sqref="B1490"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -51929,9 +51935,15 @@
       <c r="F1487" s="10" t="s">
         <v>2156</v>
       </c>
-      <c r="G1487" s="11"/>
-      <c r="H1487" s="12"/>
-      <c r="I1487" s="13"/>
+      <c r="G1487" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H1487" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1487" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1487" s="13"/>
     </row>
     <row r="1488" spans="1:10" x14ac:dyDescent="0.2">
@@ -51965,27 +51977,63 @@
       <c r="J1488" s="13"/>
     </row>
     <row r="1489" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1489" s="12"/>
-      <c r="B1489" s="12"/>
-      <c r="C1489" s="14"/>
-      <c r="D1489" s="10"/>
-      <c r="E1489" s="11"/>
-      <c r="F1489" s="10"/>
-      <c r="G1489" s="11"/>
-      <c r="H1489" s="12"/>
-      <c r="I1489" s="13"/>
+      <c r="A1489" s="12">
+        <v>44417</v>
+      </c>
+      <c r="B1489" s="12">
+        <v>44423</v>
+      </c>
+      <c r="C1489" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1489" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1489" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1489" s="10" t="s">
+        <v>2158</v>
+      </c>
+      <c r="G1489" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1489" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1489" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1489" s="13"/>
     </row>
-    <row r="1490" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1490" s="12"/>
-      <c r="B1490" s="12"/>
-      <c r="C1490" s="14"/>
-      <c r="D1490" s="10"/>
-      <c r="E1490" s="11"/>
-      <c r="F1490" s="10"/>
-      <c r="G1490" s="11"/>
-      <c r="H1490" s="12"/>
-      <c r="I1490" s="13"/>
+    <row r="1490" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1490" s="12">
+        <v>44413</v>
+      </c>
+      <c r="B1490" s="12">
+        <v>44423</v>
+      </c>
+      <c r="C1490" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1490" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1490" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1490" s="10" t="s">
+        <v>2159</v>
+      </c>
+      <c r="G1490" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1490" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1490" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1490" s="13"/>
     </row>
     <row r="1491" spans="1:10" x14ac:dyDescent="0.2">
@@ -52013,176 +52061,158 @@
       <c r="J1492" s="13"/>
     </row>
     <row r="1493" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1493" s="12">
-        <v>44399</v>
-      </c>
+      <c r="A1493" s="12"/>
       <c r="B1493" s="12"/>
-      <c r="C1493" s="14" t="s">
-        <v>1992</v>
-      </c>
-      <c r="D1493" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1493" s="11" t="s">
-        <v>837</v>
-      </c>
-      <c r="F1493" s="10" t="s">
-        <v>2115</v>
-      </c>
+      <c r="C1493" s="14"/>
+      <c r="D1493" s="10"/>
+      <c r="E1493" s="11"/>
+      <c r="F1493" s="10"/>
       <c r="G1493" s="11"/>
       <c r="H1493" s="12"/>
       <c r="I1493" s="13"/>
       <c r="J1493" s="13"/>
     </row>
-    <row r="1494" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1494" s="12">
-        <v>44403</v>
-      </c>
+    <row r="1494" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1494" s="12"/>
       <c r="B1494" s="12"/>
-      <c r="C1494" s="14" t="s">
-        <v>1477</v>
-      </c>
-      <c r="D1494" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1494" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1494" s="10" t="s">
-        <v>2132</v>
-      </c>
+      <c r="C1494" s="14"/>
+      <c r="D1494" s="10"/>
+      <c r="E1494" s="11"/>
+      <c r="F1494" s="10"/>
       <c r="G1494" s="11"/>
       <c r="H1494" s="12"/>
       <c r="I1494" s="13"/>
       <c r="J1494" s="13"/>
     </row>
-    <row r="1495" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A1495" s="12">
-        <v>44266</v>
-      </c>
-      <c r="B1495" s="9"/>
-      <c r="C1495" s="14" t="s">
-        <v>537</v>
-      </c>
-      <c r="D1495" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1495" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1495" s="10" t="s">
-        <v>1713</v>
-      </c>
+    <row r="1495" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1495" s="12"/>
+      <c r="B1495" s="12"/>
+      <c r="C1495" s="14"/>
+      <c r="D1495" s="10"/>
+      <c r="E1495" s="11"/>
+      <c r="F1495" s="10"/>
       <c r="G1495" s="11"/>
       <c r="H1495" s="12"/>
       <c r="I1495" s="13"/>
-      <c r="J1495" s="13" t="s">
-        <v>1714</v>
-      </c>
-    </row>
-    <row r="1496" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1496" s="12">
-        <v>44286</v>
-      </c>
-      <c r="B1496" s="9"/>
-      <c r="C1496" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D1496" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1496" s="11" t="s">
-        <v>620</v>
-      </c>
-      <c r="F1496" s="10" t="s">
-        <v>1838</v>
-      </c>
+      <c r="J1495" s="13"/>
+    </row>
+    <row r="1496" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1496" s="12"/>
+      <c r="B1496" s="12"/>
+      <c r="C1496" s="14"/>
+      <c r="D1496" s="10"/>
+      <c r="E1496" s="11"/>
+      <c r="F1496" s="10"/>
       <c r="G1496" s="11"/>
       <c r="H1496" s="12"/>
       <c r="I1496" s="13"/>
       <c r="J1496" s="13"/>
     </row>
     <row r="1497" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1497" s="12"/>
+      <c r="A1497" s="12">
+        <v>44399</v>
+      </c>
       <c r="B1497" s="12"/>
-      <c r="C1497" s="14"/>
-      <c r="D1497" s="10"/>
-      <c r="E1497" s="11"/>
-      <c r="F1497" s="10"/>
+      <c r="C1497" s="14" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D1497" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1497" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1497" s="10" t="s">
+        <v>2115</v>
+      </c>
       <c r="G1497" s="11"/>
       <c r="H1497" s="12"/>
       <c r="I1497" s="13"/>
       <c r="J1497" s="13"/>
     </row>
-    <row r="1498" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1498" s="12"/>
+    <row r="1498" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1498" s="12">
+        <v>44403</v>
+      </c>
       <c r="B1498" s="12"/>
-      <c r="C1498" s="14"/>
-      <c r="D1498" s="10"/>
-      <c r="E1498" s="11"/>
-      <c r="F1498" s="10"/>
+      <c r="C1498" s="14" t="s">
+        <v>1477</v>
+      </c>
+      <c r="D1498" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1498" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1498" s="10" t="s">
+        <v>2132</v>
+      </c>
       <c r="G1498" s="11"/>
       <c r="H1498" s="12"/>
       <c r="I1498" s="13"/>
       <c r="J1498" s="13"/>
     </row>
-    <row r="1499" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1499" s="12"/>
-      <c r="B1499" s="12"/>
-      <c r="C1499" s="14"/>
-      <c r="D1499" s="10"/>
-      <c r="E1499" s="11"/>
-      <c r="F1499" s="10"/>
+    <row r="1499" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1499" s="12">
+        <v>44266</v>
+      </c>
+      <c r="B1499" s="9"/>
+      <c r="C1499" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1499" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1499" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1499" s="10" t="s">
+        <v>1713</v>
+      </c>
       <c r="G1499" s="11"/>
       <c r="H1499" s="12"/>
       <c r="I1499" s="13"/>
-      <c r="J1499" s="13"/>
-    </row>
-    <row r="1500" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1500" s="12"/>
+      <c r="J1499" s="13" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="1500" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1500" s="12">
+        <v>44286</v>
+      </c>
       <c r="B1500" s="9"/>
-      <c r="C1500" s="14"/>
-      <c r="D1500" s="10"/>
-      <c r="E1500" s="11"/>
-      <c r="F1500" s="10"/>
+      <c r="C1500" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1500" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1500" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1500" s="10" t="s">
+        <v>1838</v>
+      </c>
       <c r="G1500" s="11"/>
       <c r="H1500" s="12"/>
       <c r="I1500" s="13"/>
       <c r="J1500" s="13"/>
     </row>
     <row r="1501" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1501" s="1" t="s">
-        <v>1479</v>
-      </c>
-      <c r="B1501" s="2" t="s">
-        <v>1480</v>
-      </c>
-      <c r="C1501" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1501" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1501" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1501" s="4" t="s">
-        <v>1579</v>
-      </c>
-      <c r="G1501" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1501" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1501" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1501" s="36"/>
+      <c r="A1501" s="12"/>
+      <c r="B1501" s="12"/>
+      <c r="C1501" s="14"/>
+      <c r="D1501" s="10"/>
+      <c r="E1501" s="11"/>
+      <c r="F1501" s="10"/>
+      <c r="G1501" s="11"/>
+      <c r="H1501" s="12"/>
+      <c r="I1501" s="13"/>
+      <c r="J1501" s="13"/>
     </row>
     <row r="1502" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1502" s="12"/>
-      <c r="B1502" s="9"/>
+      <c r="B1502" s="12"/>
       <c r="C1502" s="14"/>
       <c r="D1502" s="10"/>
       <c r="E1502" s="11"/>
@@ -52194,21 +52224,11 @@
     </row>
     <row r="1503" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1503" s="12"/>
-      <c r="B1503" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1503" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1503" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1503" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1503" s="10" t="s">
-        <v>1614</v>
-      </c>
+      <c r="B1503" s="12"/>
+      <c r="C1503" s="14"/>
+      <c r="D1503" s="10"/>
+      <c r="E1503" s="11"/>
+      <c r="F1503" s="10"/>
       <c r="G1503" s="11"/>
       <c r="H1503" s="12"/>
       <c r="I1503" s="13"/>
@@ -52216,65 +52236,53 @@
     </row>
     <row r="1504" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1504" s="12"/>
-      <c r="B1504" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1504" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1504" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1504" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1504" s="10" t="s">
-        <v>1606</v>
-      </c>
+      <c r="B1504" s="9"/>
+      <c r="C1504" s="14"/>
+      <c r="D1504" s="10"/>
+      <c r="E1504" s="11"/>
+      <c r="F1504" s="10"/>
       <c r="G1504" s="11"/>
       <c r="H1504" s="12"/>
       <c r="I1504" s="13"/>
       <c r="J1504" s="13"/>
     </row>
     <row r="1505" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1505" s="12"/>
-      <c r="B1505" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1505" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1505" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1505" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1505" s="10" t="s">
-        <v>1611</v>
-      </c>
-      <c r="G1505" s="11"/>
-      <c r="H1505" s="12"/>
-      <c r="I1505" s="13"/>
-      <c r="J1505" s="13"/>
+      <c r="A1505" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B1505" s="2" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C1505" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1505" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1505" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1505" s="4" t="s">
+        <v>1579</v>
+      </c>
+      <c r="G1505" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1505" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1505" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1505" s="36"/>
     </row>
     <row r="1506" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1506" s="12"/>
-      <c r="B1506" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1506" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1506" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1506" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1506" s="10" t="s">
-        <v>1607</v>
-      </c>
+      <c r="B1506" s="9"/>
+      <c r="C1506" s="14"/>
+      <c r="D1506" s="10"/>
+      <c r="E1506" s="11"/>
+      <c r="F1506" s="10"/>
       <c r="G1506" s="11"/>
       <c r="H1506" s="12"/>
       <c r="I1506" s="13"/>
@@ -52282,7 +52290,9 @@
     </row>
     <row r="1507" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1507" s="12"/>
-      <c r="B1507" s="9"/>
+      <c r="B1507" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1507" s="14" t="s">
         <v>13</v>
       </c>
@@ -52293,7 +52303,7 @@
         <v>647</v>
       </c>
       <c r="F1507" s="10" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="G1507" s="11"/>
       <c r="H1507" s="12"/>
@@ -52315,7 +52325,7 @@
         <v>647</v>
       </c>
       <c r="F1508" s="10" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
       <c r="G1508" s="11"/>
       <c r="H1508" s="12"/>
@@ -52324,7 +52334,9 @@
     </row>
     <row r="1509" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1509" s="12"/>
-      <c r="B1509" s="9"/>
+      <c r="B1509" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1509" s="14" t="s">
         <v>13</v>
       </c>
@@ -52335,7 +52347,7 @@
         <v>647</v>
       </c>
       <c r="F1509" s="10" t="s">
-        <v>1605</v>
+        <v>1611</v>
       </c>
       <c r="G1509" s="11"/>
       <c r="H1509" s="12"/>
@@ -52357,7 +52369,7 @@
         <v>647</v>
       </c>
       <c r="F1510" s="10" t="s">
-        <v>1604</v>
+        <v>1607</v>
       </c>
       <c r="G1510" s="11"/>
       <c r="H1510" s="12"/>
@@ -52366,9 +52378,7 @@
     </row>
     <row r="1511" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1511" s="12"/>
-      <c r="B1511" s="12">
-        <v>44402</v>
-      </c>
+      <c r="B1511" s="9"/>
       <c r="C1511" s="14" t="s">
         <v>13</v>
       </c>
@@ -52379,7 +52389,7 @@
         <v>647</v>
       </c>
       <c r="F1511" s="10" t="s">
-        <v>1609</v>
+        <v>1615</v>
       </c>
       <c r="G1511" s="11"/>
       <c r="H1511" s="12"/>
@@ -52401,7 +52411,7 @@
         <v>647</v>
       </c>
       <c r="F1512" s="10" t="s">
-        <v>1612</v>
+        <v>1608</v>
       </c>
       <c r="G1512" s="11"/>
       <c r="H1512" s="12"/>
@@ -52410,9 +52420,7 @@
     </row>
     <row r="1513" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1513" s="12"/>
-      <c r="B1513" s="9">
-        <v>44235</v>
-      </c>
+      <c r="B1513" s="9"/>
       <c r="C1513" s="14" t="s">
         <v>13</v>
       </c>
@@ -52423,7 +52431,7 @@
         <v>647</v>
       </c>
       <c r="F1513" s="10" t="s">
-        <v>1613</v>
+        <v>1605</v>
       </c>
       <c r="G1513" s="11"/>
       <c r="H1513" s="12"/>
@@ -52432,7 +52440,9 @@
     </row>
     <row r="1514" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1514" s="12"/>
-      <c r="B1514" s="9"/>
+      <c r="B1514" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1514" s="14" t="s">
         <v>13</v>
       </c>
@@ -52443,7 +52453,7 @@
         <v>647</v>
       </c>
       <c r="F1514" s="10" t="s">
-        <v>1610</v>
+        <v>1604</v>
       </c>
       <c r="G1514" s="11"/>
       <c r="H1514" s="12"/>
@@ -52452,7 +52462,9 @@
     </row>
     <row r="1515" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1515" s="12"/>
-      <c r="B1515" s="9"/>
+      <c r="B1515" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1515" s="14" t="s">
         <v>13</v>
       </c>
@@ -52463,7 +52475,7 @@
         <v>647</v>
       </c>
       <c r="F1515" s="10" t="s">
-        <v>1581</v>
+        <v>1609</v>
       </c>
       <c r="G1515" s="11"/>
       <c r="H1515" s="12"/>
@@ -52472,78 +52484,82 @@
     </row>
     <row r="1516" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1516" s="12"/>
-      <c r="B1516" s="9"/>
-      <c r="C1516" s="14"/>
-      <c r="D1516" s="10"/>
-      <c r="E1516" s="11"/>
-      <c r="F1516" s="10"/>
+      <c r="B1516" s="12">
+        <v>44402</v>
+      </c>
+      <c r="C1516" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1516" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1516" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1516" s="10" t="s">
+        <v>1612</v>
+      </c>
       <c r="G1516" s="11"/>
       <c r="H1516" s="12"/>
       <c r="I1516" s="13"/>
       <c r="J1516" s="13"/>
     </row>
     <row r="1517" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1517" s="12">
-        <v>44176</v>
-      </c>
-      <c r="B1517" s="9"/>
+      <c r="A1517" s="12"/>
+      <c r="B1517" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1517" s="14" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D1517" s="10" t="s">
         <v>584</v>
       </c>
       <c r="E1517" s="11" t="s">
-        <v>1353</v>
+        <v>647</v>
       </c>
       <c r="F1517" s="10" t="s">
-        <v>1354</v>
+        <v>1613</v>
       </c>
       <c r="G1517" s="11"/>
       <c r="H1517" s="12"/>
       <c r="I1517" s="13"/>
       <c r="J1517" s="13"/>
     </row>
-    <row r="1518" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1518" s="12">
-        <v>44252</v>
-      </c>
+    <row r="1518" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1518" s="12"/>
       <c r="B1518" s="9"/>
       <c r="C1518" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1518" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1518" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1518" s="10" t="s">
-        <v>1659</v>
+        <v>1610</v>
       </c>
       <c r="G1518" s="11"/>
       <c r="H1518" s="12"/>
       <c r="I1518" s="13"/>
-      <c r="J1518" s="13" t="s">
-        <v>1682</v>
-      </c>
-    </row>
-    <row r="1519" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1519" s="12">
-        <v>44252</v>
-      </c>
+      <c r="J1518" s="13"/>
+    </row>
+    <row r="1519" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1519" s="12"/>
       <c r="B1519" s="9"/>
       <c r="C1519" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1519" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1519" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1519" s="10" t="s">
-        <v>1658</v>
+        <v>1581</v>
       </c>
       <c r="G1519" s="11"/>
       <c r="H1519" s="12"/>
@@ -52551,22 +52567,12 @@
       <c r="J1519" s="13"/>
     </row>
     <row r="1520" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1520" s="12">
-        <v>44112</v>
-      </c>
+      <c r="A1520" s="12"/>
       <c r="B1520" s="9"/>
-      <c r="C1520" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="D1520" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1520" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1520" s="10" t="s">
-        <v>1097</v>
-      </c>
+      <c r="C1520" s="14"/>
+      <c r="D1520" s="10"/>
+      <c r="E1520" s="11"/>
+      <c r="F1520" s="10"/>
       <c r="G1520" s="11"/>
       <c r="H1520" s="12"/>
       <c r="I1520" s="13"/>
@@ -52574,64 +52580,66 @@
     </row>
     <row r="1521" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1521" s="12">
-        <v>44088</v>
+        <v>44176</v>
       </c>
       <c r="B1521" s="9"/>
       <c r="C1521" s="14" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D1521" s="10" t="s">
-        <v>906</v>
+        <v>584</v>
       </c>
       <c r="E1521" s="11" t="s">
-        <v>685</v>
+        <v>1353</v>
       </c>
       <c r="F1521" s="10" t="s">
-        <v>1011</v>
+        <v>1354</v>
       </c>
       <c r="G1521" s="11"/>
       <c r="H1521" s="12"/>
       <c r="I1521" s="13"/>
       <c r="J1521" s="13"/>
     </row>
-    <row r="1522" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1522" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1522" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1522" s="9"/>
       <c r="C1522" s="14" t="s">
-        <v>623</v>
+        <v>898</v>
       </c>
       <c r="D1522" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1522" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1522" s="10" t="s">
-        <v>903</v>
+        <v>1659</v>
       </c>
       <c r="G1522" s="11"/>
       <c r="H1522" s="12"/>
       <c r="I1522" s="13"/>
-      <c r="J1522" s="13"/>
-    </row>
-    <row r="1523" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1522" s="13" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="1523" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1523" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1523" s="9"/>
       <c r="C1523" s="14" t="s">
-        <v>623</v>
+        <v>898</v>
       </c>
       <c r="D1523" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1523" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1523" s="10" t="s">
-        <v>902</v>
+        <v>1658</v>
       </c>
       <c r="G1523" s="11"/>
       <c r="H1523" s="12"/>
@@ -52640,270 +52648,310 @@
     </row>
     <row r="1524" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1524" s="12">
-        <v>44055</v>
+        <v>44112</v>
       </c>
       <c r="B1524" s="9"/>
       <c r="C1524" s="14" t="s">
-        <v>898</v>
+        <v>623</v>
       </c>
       <c r="D1524" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1524" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1524" s="10" t="s">
-        <v>900</v>
+        <v>1097</v>
       </c>
       <c r="G1524" s="11"/>
       <c r="H1524" s="12"/>
       <c r="I1524" s="13"/>
       <c r="J1524" s="13"/>
     </row>
-    <row r="1525" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="1525" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1525" s="12">
-        <v>44055</v>
+        <v>44088</v>
       </c>
       <c r="B1525" s="9"/>
       <c r="C1525" s="14" t="s">
-        <v>898</v>
+        <v>19</v>
       </c>
       <c r="D1525" s="10" t="s">
-        <v>494</v>
+        <v>906</v>
       </c>
       <c r="E1525" s="11" t="s">
-        <v>570</v>
+        <v>685</v>
       </c>
       <c r="F1525" s="10" t="s">
-        <v>901</v>
+        <v>1011</v>
       </c>
       <c r="G1525" s="11"/>
       <c r="H1525" s="12"/>
       <c r="I1525" s="13"/>
       <c r="J1525" s="13"/>
     </row>
-    <row r="1526" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1526" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1526" s="12">
         <v>44055</v>
       </c>
       <c r="B1526" s="9"/>
       <c r="C1526" s="14" t="s">
-        <v>898</v>
+        <v>623</v>
       </c>
       <c r="D1526" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1526" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1526" s="10" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="G1526" s="11"/>
       <c r="H1526" s="12"/>
       <c r="I1526" s="13"/>
-      <c r="J1526" s="13" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="1527" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1526" s="13"/>
+    </row>
+    <row r="1527" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1527" s="12">
-        <v>44047</v>
+        <v>44055</v>
       </c>
       <c r="B1527" s="9"/>
       <c r="C1527" s="14" t="s">
-        <v>537</v>
+        <v>623</v>
       </c>
       <c r="D1527" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E1527" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1527" s="10" t="s">
-        <v>873</v>
-      </c>
-      <c r="G1527" s="11" t="s">
-        <v>1624</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="G1527" s="11"/>
       <c r="H1527" s="12"/>
       <c r="I1527" s="13"/>
       <c r="J1527" s="13"/>
     </row>
-    <row r="1528" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1528" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1528" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1528" s="9"/>
       <c r="C1528" s="14" t="s">
-        <v>468</v>
+        <v>898</v>
       </c>
       <c r="D1528" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1528" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1528" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1528" s="11" t="s">
-        <v>1639</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="G1528" s="11"/>
       <c r="H1528" s="12"/>
-      <c r="I1528" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1528" s="13"/>
       <c r="J1528" s="13"/>
     </row>
-    <row r="1529" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1529" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A1529" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1529" s="9"/>
       <c r="C1529" s="14" t="s">
-        <v>468</v>
+        <v>898</v>
       </c>
       <c r="D1529" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1529" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1529" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1529" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>901</v>
+      </c>
+      <c r="G1529" s="11"/>
       <c r="H1529" s="12"/>
-      <c r="I1529" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1529" s="13" t="s">
-        <v>1568</v>
-      </c>
-    </row>
-    <row r="1530" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1529" s="13"/>
+      <c r="J1529" s="13"/>
+    </row>
+    <row r="1530" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1530" s="12">
-        <v>43838</v>
+        <v>44055</v>
       </c>
       <c r="B1530" s="9"/>
       <c r="C1530" s="14" t="s">
-        <v>103</v>
+        <v>898</v>
       </c>
       <c r="D1530" s="10" t="s">
-        <v>460</v>
+        <v>494</v>
       </c>
       <c r="E1530" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1530" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G1530" s="11" t="s">
-        <v>1640</v>
-      </c>
+        <v>904</v>
+      </c>
+      <c r="G1530" s="11"/>
       <c r="H1530" s="12"/>
       <c r="I1530" s="13"/>
       <c r="J1530" s="13" t="s">
-        <v>1533</v>
-      </c>
-    </row>
-    <row r="1531" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="1531" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1531" s="12">
-        <v>43816</v>
+        <v>44047</v>
       </c>
       <c r="B1531" s="9"/>
       <c r="C1531" s="14" t="s">
-        <v>475</v>
+        <v>537</v>
       </c>
       <c r="D1531" s="10" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="E1531" s="11" t="s">
-        <v>570</v>
+        <v>685</v>
       </c>
       <c r="F1531" s="10" t="s">
-        <v>474</v>
+        <v>873</v>
       </c>
       <c r="G1531" s="11" t="s">
-        <v>1632</v>
+        <v>1624</v>
       </c>
       <c r="H1531" s="12"/>
       <c r="I1531" s="13"/>
-      <c r="J1531" s="13" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="1532" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1531" s="13"/>
+    </row>
+    <row r="1532" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A1532" s="12">
-        <v>43762</v>
+        <v>43949</v>
       </c>
       <c r="B1532" s="9"/>
       <c r="C1532" s="14" t="s">
-        <v>446</v>
+        <v>468</v>
       </c>
       <c r="D1532" s="10" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="E1532" s="11" t="s">
-        <v>837</v>
+        <v>685</v>
       </c>
       <c r="F1532" s="10" t="s">
-        <v>447</v>
+        <v>686</v>
       </c>
       <c r="G1532" s="11" t="s">
-        <v>1629</v>
+        <v>1639</v>
       </c>
       <c r="H1532" s="12"/>
-      <c r="I1532" s="13"/>
+      <c r="I1532" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1532" s="13"/>
     </row>
-    <row r="1533" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1533" s="12"/>
+    <row r="1533" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1533" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1533" s="9"/>
-      <c r="C1533" s="14"/>
-      <c r="D1533" s="10"/>
-      <c r="E1533" s="11"/>
-      <c r="F1533" s="10"/>
-      <c r="G1533" s="11"/>
+      <c r="C1533" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1533" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1533" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1533" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="G1533" s="11" t="s">
+        <v>687</v>
+      </c>
       <c r="H1533" s="12"/>
-      <c r="I1533" s="13"/>
-      <c r="J1533" s="13"/>
-    </row>
-    <row r="1534" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1534" s="12"/>
+      <c r="I1533" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1533" s="13" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="1534" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1534" s="12">
+        <v>43838</v>
+      </c>
       <c r="B1534" s="9"/>
-      <c r="C1534" s="14"/>
-      <c r="D1534" s="10"/>
-      <c r="E1534" s="11"/>
-      <c r="F1534" s="10"/>
-      <c r="G1534" s="11"/>
+      <c r="C1534" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1534" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1534" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1534" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G1534" s="11" t="s">
+        <v>1640</v>
+      </c>
       <c r="H1534" s="12"/>
       <c r="I1534" s="13"/>
-      <c r="J1534" s="13"/>
+      <c r="J1534" s="13" t="s">
+        <v>1533</v>
+      </c>
     </row>
     <row r="1535" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1535" s="12"/>
+      <c r="A1535" s="12">
+        <v>43816</v>
+      </c>
       <c r="B1535" s="9"/>
-      <c r="C1535" s="14"/>
-      <c r="D1535" s="10"/>
-      <c r="E1535" s="11"/>
-      <c r="F1535" s="10"/>
-      <c r="G1535" s="11"/>
+      <c r="C1535" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1535" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1535" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1535" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G1535" s="11" t="s">
+        <v>1632</v>
+      </c>
       <c r="H1535" s="12"/>
       <c r="I1535" s="13"/>
-      <c r="J1535" s="13"/>
-    </row>
-    <row r="1536" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1536" s="12"/>
+      <c r="J1535" s="13" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="1536" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1536" s="12">
+        <v>43762</v>
+      </c>
       <c r="B1536" s="9"/>
-      <c r="C1536" s="14"/>
-      <c r="D1536" s="10"/>
-      <c r="E1536" s="11"/>
-      <c r="F1536" s="10"/>
-      <c r="G1536" s="11"/>
+      <c r="C1536" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1536" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1536" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1536" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1536" s="11" t="s">
+        <v>1629</v>
+      </c>
       <c r="H1536" s="12"/>
       <c r="I1536" s="13"/>
       <c r="J1536" s="13"/>
@@ -52932,10 +52980,58 @@
       <c r="I1538" s="13"/>
       <c r="J1538" s="13"/>
     </row>
+    <row r="1539" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1539" s="12"/>
+      <c r="B1539" s="9"/>
+      <c r="C1539" s="14"/>
+      <c r="D1539" s="10"/>
+      <c r="E1539" s="11"/>
+      <c r="F1539" s="10"/>
+      <c r="G1539" s="11"/>
+      <c r="H1539" s="12"/>
+      <c r="I1539" s="13"/>
+      <c r="J1539" s="13"/>
+    </row>
+    <row r="1540" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1540" s="12"/>
+      <c r="B1540" s="9"/>
+      <c r="C1540" s="14"/>
+      <c r="D1540" s="10"/>
+      <c r="E1540" s="11"/>
+      <c r="F1540" s="10"/>
+      <c r="G1540" s="11"/>
+      <c r="H1540" s="12"/>
+      <c r="I1540" s="13"/>
+      <c r="J1540" s="13"/>
+    </row>
+    <row r="1541" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1541" s="12"/>
+      <c r="B1541" s="9"/>
+      <c r="C1541" s="14"/>
+      <c r="D1541" s="10"/>
+      <c r="E1541" s="11"/>
+      <c r="F1541" s="10"/>
+      <c r="G1541" s="11"/>
+      <c r="H1541" s="12"/>
+      <c r="I1541" s="13"/>
+      <c r="J1541" s="13"/>
+    </row>
+    <row r="1542" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1542" s="12"/>
+      <c r="B1542" s="9"/>
+      <c r="C1542" s="14"/>
+      <c r="D1542" s="10"/>
+      <c r="E1542" s="11"/>
+      <c r="F1542" s="10"/>
+      <c r="G1542" s="11"/>
+      <c r="H1542" s="12"/>
+      <c r="I1542" s="13"/>
+      <c r="J1542" s="13"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1479" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1504:F1514">
-    <sortCondition ref="F1504:F1514"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1508:F1518">
+    <sortCondition ref="F1508:F1518"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Lib PV/PN REST 2.0
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F807C6C3-7C71-4D28-A273-D74E8B8FEFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E301E6E8-1D6E-4D8B-A1B8-DE103E3A061A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_FilterDatabase_0" localSheetId="0">'Demandas BK - Protheus'!$A$1:$I$53</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Demandas BK - Protheus'!$A$1:$J$1479</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Demandas BK - Protheus'!$A$1:$J$1480</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10589" uniqueCount="2161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10758" uniqueCount="2187">
   <si>
     <t>Responsável</t>
   </si>
@@ -6716,9 +6716,6 @@
     <t>EFD acertos</t>
   </si>
   <si>
-    <t>BCC não subiu planilha</t>
-  </si>
-  <si>
     <t>21-06-21_ATUALIZACAO_12.1.25_ATF_EXPEDICAO_CONTINUA</t>
   </si>
   <si>
@@ -6852,6 +6849,100 @@
   </si>
   <si>
     <t>Auxilio compensação de RA com valor maior que a NF</t>
+  </si>
+  <si>
+    <t>Acerto pedidos da Petrobrás com divergência no pagamento (ISS)</t>
+  </si>
+  <si>
+    <t>Dúvidas a respeito de pagamento antecipado (não era isso, pagamento normal que deve ter um produto atrelado para os relatórios)</t>
+  </si>
+  <si>
+    <t>Pergunta de abrir liberação de pedidos estava abrindo em todos os módulos</t>
+  </si>
+  <si>
+    <t>Gravar informações de motivo de estorno no documento de entrada</t>
+  </si>
+  <si>
+    <t>Ajustes EFD 07/2021</t>
+  </si>
+  <si>
+    <t>Correção da aliquota de ISS das NFs da Petrobras: 218,219,220,221 (RJ)</t>
+  </si>
+  <si>
+    <t>Implantação Liberação Pré Nota WEB</t>
+  </si>
+  <si>
+    <t>Acerto problema na liberação de Pedidos de Venda WEB
+Anexos do documento na Pré-Nota WEB
+Pedidos de venda estão sendo liberados em duplicidade
+Ajustes EFD 07-2021</t>
+  </si>
+  <si>
+    <t>Problemas com pedidos de vendas que são liberados e continuam com saldo a liberar (probelma com casas decimais do campo C6_QTDEMP)
+Suportes diversos fiscal e contabiidade
+Testes com várias opções de tipos de planilhas e medições para evitar o fracionamento de quantidade</t>
+  </si>
+  <si>
+    <t>Acerto no campo C6_QTDEMP e B2_QEMP (para 9 casas decimais)
+Estorno da medição 047620 e reemissão com valor alterado (nova medição)
+Acerto performace Mapa de INSS Retido
+Suportes diversos contabilidade
+Acerto nos pedidos: 048355,6,7,79,78,560,563 referentes a divergencias com entendimento da Petrobras</t>
+  </si>
+  <si>
+    <t>Correção dos títulos de pensão sobre férias, conforme solicitado pelo RH. "Adilson/Marcão!!!
+Precisamos atualizar o pagamento da pensão abaixo, saiu pra 30/07/2021 Gentileza atualizar para 04/08/2021."Criado titulo de pensão, conforme solicitado. "Adilson!!!
+Precisamos incluir titulo abaixo, como temos o pagamento da pensão das férias para o mesmo dia, o sistema não está puxando."</t>
+  </si>
+  <si>
+    <t>REINF empresa BK Julho/2020 e Balsa Nova/Bk e consolidação dos DADOS para envio e fechamento do período do REINF</t>
+  </si>
+  <si>
+    <t>Correção da rotina de integração erro de vencimento, verificado erro na inclusão do titulo, o mesmo foi corrigido e integrado normalmente.</t>
+  </si>
+  <si>
+    <t>Ajuste nos valores dos titulo informado errado, conforme solicitado pelo RH. "Adilson
+Obrigado pela inclusão, e me perdoe gentileza ajustar apenas os valores, me atentei as observações e datas e o principal o valor errei, me perdoe..</t>
+  </si>
+  <si>
+    <t>Geração do ECF das empresas BKTER, BK Seguros, CMOG e TERO.</t>
+  </si>
+  <si>
+    <t>Correção no pedido de venda bitributação, "048529 o cliente nos bi tributou, precisa colocar ISS CPOM de 5% por favor".</t>
+  </si>
+  <si>
+    <t>Correção do lançamento da nota fiscal de entrada, conforme solicitado. "Nota 2319 O item 74 reais e tes 104 CFOP 1556".</t>
+  </si>
+  <si>
+    <t>Finalizado a geração do ECF das empresas BKTER, BK Seguros, CMOG e TERO, iniciado a assinatura e transmissão dos mesmos, transmitido CMOG e TERO, as demais aguardando a assinatura da contadora.</t>
+  </si>
+  <si>
+    <t>Permitir o depsto fiscal classificar Doc de Entrada Estornado e Classificar Documentos de entrada lançados pelo Depto Fiscal sem liberação</t>
+  </si>
+  <si>
+    <t>Aprovada a alteração pelo Xavier e pelo Bruno</t>
+  </si>
+  <si>
+    <t>Rodolfo</t>
+  </si>
+  <si>
+    <t>Conforme conversa agora pela manhã por gentileza modifique os padrões de históricos que sobem para contabilidade de “ENTRADAS” e “SAIDAS”.
+Para que eles contenham um caráter especial entre as informações passadas no histórico que no caso foi o “:”.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consulta pedido na tela da nova medição mostra pedido repetido com medição de mais de um item </t>
+  </si>
+  <si>
+    <t>Atualização do artefato Smartclient</t>
+  </si>
+  <si>
+    <t>Tela web da Pré-nota - opção para filtro e ordenação de colunas</t>
+  </si>
+  <si>
+    <t>Lista dos principais clientes por tempo médio de relacionamento (podemos listar nossos 20 principais clientes por tempo médio de relacionamento)</t>
+  </si>
+  <si>
+    <t>BKFATR06 - Relação de Clientes (primeira e ultima compra)</t>
   </si>
 </sst>
 </file>
@@ -7620,11 +7711,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1542"/>
+  <dimension ref="A1:J1567"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1480" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1492" sqref="A1492"/>
+      <pane ySplit="1" topLeftCell="A1505" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1515" sqref="F1515"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -50930,7 +51021,7 @@
         <v>647</v>
       </c>
       <c r="F1454" s="10" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
       <c r="G1454" s="11" t="s">
         <v>295</v>
@@ -50960,7 +51051,7 @@
         <v>647</v>
       </c>
       <c r="F1455" s="10" t="s">
-        <v>2116</v>
+        <v>2115</v>
       </c>
       <c r="G1455" s="11" t="s">
         <v>1622</v>
@@ -50990,7 +51081,7 @@
         <v>647</v>
       </c>
       <c r="F1456" s="10" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="G1456" s="11" t="s">
         <v>1622</v>
@@ -51020,7 +51111,7 @@
         <v>647</v>
       </c>
       <c r="F1457" s="10" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="G1457" s="11" t="s">
         <v>1622</v>
@@ -51050,7 +51141,7 @@
         <v>647</v>
       </c>
       <c r="F1458" s="10" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="G1458" s="11" t="s">
         <v>1622</v>
@@ -51080,7 +51171,7 @@
         <v>647</v>
       </c>
       <c r="F1459" s="10" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="G1459" s="11" t="s">
         <v>1666</v>
@@ -51110,7 +51201,7 @@
         <v>647</v>
       </c>
       <c r="F1460" s="10" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
       <c r="G1460" s="11" t="s">
         <v>1622</v>
@@ -51140,10 +51231,10 @@
         <v>647</v>
       </c>
       <c r="F1461" s="10" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="G1461" s="41" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
       <c r="H1461" s="12" t="s">
         <v>112</v>
@@ -51170,10 +51261,10 @@
         <v>647</v>
       </c>
       <c r="F1462" s="10" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
       <c r="G1462" s="41" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
       <c r="H1462" s="12" t="s">
         <v>112</v>
@@ -51200,7 +51291,7 @@
         <v>647</v>
       </c>
       <c r="F1463" s="10" t="s">
-        <v>2125</v>
+        <v>2124</v>
       </c>
       <c r="G1463" s="11" t="s">
         <v>1621</v>
@@ -51230,7 +51321,7 @@
         <v>647</v>
       </c>
       <c r="F1464" s="10" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
       <c r="G1464" s="11" t="s">
         <v>1621</v>
@@ -51272,7 +51363,7 @@
         <v>13</v>
       </c>
       <c r="J1465" s="13" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="1466" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -51292,7 +51383,7 @@
         <v>570</v>
       </c>
       <c r="F1466" s="10" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
       <c r="G1466" s="11" t="s">
         <v>295</v>
@@ -51304,7 +51395,7 @@
         <v>13</v>
       </c>
       <c r="J1466" s="13" t="s">
-        <v>2133</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="1467" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -51324,7 +51415,7 @@
         <v>570</v>
       </c>
       <c r="F1467" s="10" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
       <c r="G1467" s="11" t="s">
         <v>1621</v>
@@ -51336,7 +51427,7 @@
         <v>13</v>
       </c>
       <c r="J1467" s="13" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="1468" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -51368,7 +51459,7 @@
         <v>13</v>
       </c>
       <c r="J1468" s="13" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="1469" spans="1:10" x14ac:dyDescent="0.2">
@@ -51388,7 +51479,7 @@
         <v>570</v>
       </c>
       <c r="F1469" s="10" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="G1469" s="11" t="s">
         <v>295</v>
@@ -51430,7 +51521,7 @@
         <v>13</v>
       </c>
       <c r="J1470" s="13" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="1471" spans="1:10" x14ac:dyDescent="0.2">
@@ -51450,7 +51541,7 @@
         <v>1832</v>
       </c>
       <c r="F1471" s="10" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
       <c r="G1471" s="11" t="s">
         <v>1626</v>
@@ -51480,7 +51571,7 @@
         <v>837</v>
       </c>
       <c r="F1472" s="10" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
       <c r="G1472" s="11" t="s">
         <v>309</v>
@@ -51492,7 +51583,7 @@
         <v>13</v>
       </c>
       <c r="J1472" s="13" t="s">
-        <v>2139</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="1473" spans="1:10" ht="84" x14ac:dyDescent="0.2">
@@ -51514,9 +51605,15 @@
       <c r="F1473" s="10" t="s">
         <v>534</v>
       </c>
-      <c r="G1473" s="11"/>
-      <c r="H1473" s="12"/>
-      <c r="I1473" s="13"/>
+      <c r="G1473" s="11" t="s">
+        <v>1632</v>
+      </c>
+      <c r="H1473" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1473" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1473" s="13" t="s">
         <v>1705</v>
       </c>
@@ -51538,7 +51635,7 @@
         <v>570</v>
       </c>
       <c r="F1474" s="10" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="G1474" s="11" t="s">
         <v>295</v>
@@ -51568,7 +51665,7 @@
         <v>570</v>
       </c>
       <c r="F1475" s="10" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="G1475" s="11" t="s">
         <v>295</v>
@@ -51580,7 +51677,7 @@
         <v>13</v>
       </c>
       <c r="J1475" s="13" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="1476" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -51600,7 +51697,7 @@
         <v>570</v>
       </c>
       <c r="F1476" s="10" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
       <c r="G1476" s="11" t="s">
         <v>1621</v>
@@ -51612,60 +51709,60 @@
         <v>13</v>
       </c>
       <c r="J1476" s="13" t="s">
-        <v>2144</v>
-      </c>
-    </row>
-    <row r="1477" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2143</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:10" ht="72" x14ac:dyDescent="0.2">
       <c r="A1477" s="12">
-        <v>44413</v>
+        <v>44412</v>
       </c>
       <c r="B1477" s="12">
-        <v>44413</v>
+        <v>44412</v>
       </c>
       <c r="C1477" s="14" t="s">
-        <v>2034</v>
+        <v>490</v>
       </c>
       <c r="D1477" s="10" t="s">
-        <v>83</v>
+        <v>491</v>
       </c>
       <c r="E1477" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1477" s="10" t="s">
-        <v>2145</v>
+        <v>2170</v>
       </c>
       <c r="G1477" s="11" t="s">
-        <v>2146</v>
+        <v>1629</v>
       </c>
       <c r="H1477" s="12" t="s">
         <v>112</v>
       </c>
       <c r="I1477" s="13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J1477" s="13"/>
     </row>
     <row r="1478" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1478" s="12">
-        <v>44222</v>
-      </c>
-      <c r="B1478" s="9">
         <v>44413</v>
       </c>
+      <c r="B1478" s="12">
+        <v>44413</v>
+      </c>
       <c r="C1478" s="14" t="s">
-        <v>19</v>
+        <v>2034</v>
       </c>
       <c r="D1478" s="10" t="s">
-        <v>494</v>
+        <v>83</v>
       </c>
       <c r="E1478" s="11" t="s">
         <v>837</v>
       </c>
       <c r="F1478" s="10" t="s">
-        <v>1494</v>
+        <v>2144</v>
       </c>
       <c r="G1478" s="11" t="s">
-        <v>309</v>
+        <v>2145</v>
       </c>
       <c r="H1478" s="12" t="s">
         <v>112</v>
@@ -51677,10 +51774,10 @@
     </row>
     <row r="1479" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1479" s="12">
-        <v>44418</v>
+        <v>44222</v>
       </c>
       <c r="B1479" s="9">
-        <v>44418</v>
+        <v>44413</v>
       </c>
       <c r="C1479" s="14" t="s">
         <v>19</v>
@@ -51689,10 +51786,10 @@
         <v>494</v>
       </c>
       <c r="E1479" s="11" t="s">
-        <v>620</v>
+        <v>837</v>
       </c>
       <c r="F1479" s="10" t="s">
-        <v>2148</v>
+        <v>1494</v>
       </c>
       <c r="G1479" s="11" t="s">
         <v>309</v>
@@ -51707,25 +51804,25 @@
     </row>
     <row r="1480" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1480" s="12">
-        <v>44410</v>
+        <v>44418</v>
       </c>
       <c r="B1480" s="9">
         <v>44418</v>
       </c>
       <c r="C1480" s="14" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D1480" s="10" t="s">
-        <v>584</v>
+        <v>494</v>
       </c>
       <c r="E1480" s="11" t="s">
-        <v>698</v>
+        <v>620</v>
       </c>
       <c r="F1480" s="10" t="s">
-        <v>2149</v>
+        <v>2147</v>
       </c>
       <c r="G1480" s="11" t="s">
-        <v>1626</v>
+        <v>309</v>
       </c>
       <c r="H1480" s="12" t="s">
         <v>112</v>
@@ -51737,25 +51834,25 @@
     </row>
     <row r="1481" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1481" s="12">
+        <v>44410</v>
+      </c>
+      <c r="B1481" s="9">
         <v>44418</v>
       </c>
-      <c r="B1481" s="9">
-        <v>44419</v>
-      </c>
       <c r="C1481" s="14" t="s">
-        <v>932</v>
+        <v>13</v>
       </c>
       <c r="D1481" s="10" t="s">
-        <v>17</v>
+        <v>584</v>
       </c>
       <c r="E1481" s="11" t="s">
-        <v>620</v>
+        <v>698</v>
       </c>
       <c r="F1481" s="10" t="s">
-        <v>2150</v>
+        <v>2148</v>
       </c>
       <c r="G1481" s="11" t="s">
-        <v>309</v>
+        <v>1626</v>
       </c>
       <c r="H1481" s="12" t="s">
         <v>112</v>
@@ -51763,28 +51860,26 @@
       <c r="I1481" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1481" s="13" t="s">
-        <v>2151</v>
-      </c>
+      <c r="J1481" s="13"/>
     </row>
     <row r="1482" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1482" s="12">
-        <v>44413</v>
-      </c>
-      <c r="B1482" s="12">
+        <v>44418</v>
+      </c>
+      <c r="B1482" s="9">
         <v>44419</v>
       </c>
       <c r="C1482" s="14" t="s">
-        <v>1056</v>
+        <v>932</v>
       </c>
       <c r="D1482" s="10" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="E1482" s="11" t="s">
-        <v>837</v>
+        <v>620</v>
       </c>
       <c r="F1482" s="10" t="s">
-        <v>2147</v>
+        <v>2149</v>
       </c>
       <c r="G1482" s="11" t="s">
         <v>309</v>
@@ -51795,26 +51890,28 @@
       <c r="I1482" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1482" s="13"/>
+      <c r="J1482" s="13" t="s">
+        <v>2150</v>
+      </c>
     </row>
     <row r="1483" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1483" s="12">
-        <v>44420</v>
+        <v>44413</v>
       </c>
       <c r="B1483" s="12">
-        <v>44420</v>
+        <v>44419</v>
       </c>
       <c r="C1483" s="14" t="s">
-        <v>1283</v>
+        <v>1056</v>
       </c>
       <c r="D1483" s="10" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="E1483" s="11" t="s">
         <v>837</v>
       </c>
       <c r="F1483" s="10" t="s">
-        <v>2152</v>
+        <v>2146</v>
       </c>
       <c r="G1483" s="11" t="s">
         <v>309</v>
@@ -51827,67 +51924,65 @@
       </c>
       <c r="J1483" s="13"/>
     </row>
-    <row r="1484" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1484" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1484" s="12">
-        <v>44420</v>
+        <v>44419</v>
       </c>
       <c r="B1484" s="12">
-        <v>44420</v>
+        <v>44419</v>
       </c>
       <c r="C1484" s="14" t="s">
-        <v>1283</v>
+        <v>2034</v>
       </c>
       <c r="D1484" s="10" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="E1484" s="11" t="s">
-        <v>837</v>
+        <v>620</v>
       </c>
       <c r="F1484" s="10" t="s">
-        <v>2153</v>
+        <v>2171</v>
       </c>
       <c r="G1484" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H1484" s="12" t="s">
         <v>112</v>
       </c>
       <c r="I1484" s="13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J1484" s="13"/>
     </row>
     <row r="1485" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1485" s="12">
-        <v>44420</v>
+        <v>44419</v>
       </c>
       <c r="B1485" s="12">
-        <v>44420</v>
+        <v>44419</v>
       </c>
       <c r="C1485" s="14" t="s">
-        <v>13</v>
+        <v>490</v>
       </c>
       <c r="D1485" s="10" t="s">
-        <v>584</v>
+        <v>491</v>
       </c>
       <c r="E1485" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1485" s="10" t="s">
-        <v>2154</v>
+        <v>2172</v>
       </c>
       <c r="G1485" s="11" t="s">
-        <v>1621</v>
+        <v>308</v>
       </c>
       <c r="H1485" s="12" t="s">
         <v>112</v>
       </c>
       <c r="I1485" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1485" s="13" t="s">
-        <v>1769</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J1485" s="13"/>
     </row>
     <row r="1486" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1486" s="12">
@@ -51897,16 +51992,16 @@
         <v>44420</v>
       </c>
       <c r="C1486" s="14" t="s">
-        <v>2034</v>
+        <v>1283</v>
       </c>
       <c r="D1486" s="10" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="E1486" s="11" t="s">
         <v>837</v>
       </c>
       <c r="F1486" s="10" t="s">
-        <v>2155</v>
+        <v>2151</v>
       </c>
       <c r="G1486" s="11" t="s">
         <v>309</v>
@@ -51921,55 +52016,55 @@
     </row>
     <row r="1487" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1487" s="12">
-        <v>44421</v>
+        <v>44420</v>
       </c>
       <c r="B1487" s="12">
-        <v>44421</v>
+        <v>44420</v>
       </c>
       <c r="C1487" s="14" t="s">
-        <v>13</v>
+        <v>1283</v>
       </c>
       <c r="D1487" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1487" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1487" s="10" t="s">
+        <v>2152</v>
+      </c>
+      <c r="G1487" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1487" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1487" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1487" s="13"/>
+    </row>
+    <row r="1488" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1488" s="12">
+        <v>44420</v>
+      </c>
+      <c r="B1488" s="12">
+        <v>44420</v>
+      </c>
+      <c r="C1488" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1488" s="10" t="s">
         <v>584</v>
       </c>
-      <c r="E1487" s="11" t="s">
-        <v>698</v>
-      </c>
-      <c r="F1487" s="10" t="s">
-        <v>2156</v>
-      </c>
-      <c r="G1487" s="11" t="s">
-        <v>308</v>
-      </c>
-      <c r="H1487" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1487" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1487" s="13"/>
-    </row>
-    <row r="1488" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1488" s="12">
-        <v>44421</v>
-      </c>
-      <c r="B1488" s="12">
-        <v>44421</v>
-      </c>
-      <c r="C1488" s="14" t="s">
-        <v>1992</v>
-      </c>
-      <c r="D1488" s="10" t="s">
-        <v>89</v>
-      </c>
       <c r="E1488" s="11" t="s">
-        <v>570</v>
+        <v>837</v>
       </c>
       <c r="F1488" s="10" t="s">
-        <v>2157</v>
+        <v>2153</v>
       </c>
       <c r="G1488" s="11" t="s">
-        <v>295</v>
+        <v>1621</v>
       </c>
       <c r="H1488" s="12" t="s">
         <v>112</v>
@@ -51977,29 +52072,31 @@
       <c r="I1488" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1488" s="13"/>
+      <c r="J1488" s="13" t="s">
+        <v>1769</v>
+      </c>
     </row>
     <row r="1489" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1489" s="12">
-        <v>44417</v>
+        <v>44420</v>
       </c>
       <c r="B1489" s="12">
-        <v>44423</v>
+        <v>44420</v>
       </c>
       <c r="C1489" s="14" t="s">
-        <v>13</v>
+        <v>2034</v>
       </c>
       <c r="D1489" s="10" t="s">
-        <v>584</v>
+        <v>83</v>
       </c>
       <c r="E1489" s="11" t="s">
-        <v>647</v>
+        <v>837</v>
       </c>
       <c r="F1489" s="10" t="s">
-        <v>2158</v>
+        <v>2154</v>
       </c>
       <c r="G1489" s="11" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="H1489" s="12" t="s">
         <v>112</v>
@@ -52009,12 +52106,12 @@
       </c>
       <c r="J1489" s="13"/>
     </row>
-    <row r="1490" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="1490" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1490" s="12">
-        <v>44413</v>
+        <v>44421</v>
       </c>
       <c r="B1490" s="12">
-        <v>44423</v>
+        <v>44421</v>
       </c>
       <c r="C1490" s="14" t="s">
         <v>13</v>
@@ -52023,13 +52120,13 @@
         <v>584</v>
       </c>
       <c r="E1490" s="11" t="s">
-        <v>647</v>
+        <v>698</v>
       </c>
       <c r="F1490" s="10" t="s">
-        <v>2159</v>
+        <v>2155</v>
       </c>
       <c r="G1490" s="11" t="s">
-        <v>295</v>
+        <v>308</v>
       </c>
       <c r="H1490" s="12" t="s">
         <v>112</v>
@@ -52041,22 +52138,22 @@
     </row>
     <row r="1491" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1491" s="12">
-        <v>44436</v>
+        <v>44421</v>
       </c>
       <c r="B1491" s="12">
-        <v>44436</v>
+        <v>44421</v>
       </c>
       <c r="C1491" s="14" t="s">
-        <v>559</v>
+        <v>1992</v>
       </c>
       <c r="D1491" s="10" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="E1491" s="11" t="s">
-        <v>620</v>
+        <v>570</v>
       </c>
       <c r="F1491" s="10" t="s">
-        <v>2160</v>
+        <v>2156</v>
       </c>
       <c r="G1491" s="11" t="s">
         <v>295</v>
@@ -52070,315 +52167,551 @@
       <c r="J1491" s="13"/>
     </row>
     <row r="1492" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1492" s="12"/>
-      <c r="B1492" s="12"/>
-      <c r="C1492" s="14"/>
-      <c r="D1492" s="10"/>
-      <c r="E1492" s="11"/>
-      <c r="F1492" s="10"/>
-      <c r="G1492" s="11"/>
-      <c r="H1492" s="12"/>
-      <c r="I1492" s="13"/>
+      <c r="A1492" s="12">
+        <v>44417</v>
+      </c>
+      <c r="B1492" s="12">
+        <v>44423</v>
+      </c>
+      <c r="C1492" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1492" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1492" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1492" s="10" t="s">
+        <v>2157</v>
+      </c>
+      <c r="G1492" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1492" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1492" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1492" s="13"/>
     </row>
-    <row r="1493" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1493" s="12"/>
-      <c r="B1493" s="12"/>
-      <c r="C1493" s="14"/>
-      <c r="D1493" s="10"/>
-      <c r="E1493" s="11"/>
-      <c r="F1493" s="10"/>
-      <c r="G1493" s="11"/>
-      <c r="H1493" s="12"/>
-      <c r="I1493" s="13"/>
+    <row r="1493" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1493" s="12">
+        <v>44413</v>
+      </c>
+      <c r="B1493" s="12">
+        <v>44423</v>
+      </c>
+      <c r="C1493" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1493" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1493" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1493" s="10" t="s">
+        <v>2158</v>
+      </c>
+      <c r="G1493" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1493" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1493" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1493" s="13"/>
     </row>
     <row r="1494" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1494" s="12"/>
-      <c r="B1494" s="12"/>
-      <c r="C1494" s="14"/>
-      <c r="D1494" s="10"/>
-      <c r="E1494" s="11"/>
-      <c r="F1494" s="10"/>
-      <c r="G1494" s="11"/>
-      <c r="H1494" s="12"/>
-      <c r="I1494" s="13"/>
+      <c r="A1494" s="12">
+        <v>44424</v>
+      </c>
+      <c r="B1494" s="12">
+        <v>44424</v>
+      </c>
+      <c r="C1494" s="14" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D1494" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1494" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1494" s="10" t="s">
+        <v>2164</v>
+      </c>
+      <c r="G1494" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H1494" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1494" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1494" s="13"/>
     </row>
-    <row r="1495" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1495" s="12"/>
-      <c r="B1495" s="12"/>
-      <c r="C1495" s="14"/>
-      <c r="D1495" s="10"/>
-      <c r="E1495" s="11"/>
-      <c r="F1495" s="10"/>
-      <c r="G1495" s="11"/>
-      <c r="H1495" s="12"/>
-      <c r="I1495" s="13"/>
+    <row r="1495" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1495" s="12">
+        <v>44426</v>
+      </c>
+      <c r="B1495" s="12">
+        <v>44426</v>
+      </c>
+      <c r="C1495" s="14" t="s">
+        <v>490</v>
+      </c>
+      <c r="D1495" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="E1495" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1495" s="10" t="s">
+        <v>2173</v>
+      </c>
+      <c r="G1495" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1495" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1495" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="J1495" s="13"/>
     </row>
     <row r="1496" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1496" s="12"/>
-      <c r="B1496" s="12"/>
-      <c r="C1496" s="14"/>
-      <c r="D1496" s="10"/>
-      <c r="E1496" s="11"/>
-      <c r="F1496" s="10"/>
-      <c r="G1496" s="11"/>
-      <c r="H1496" s="12"/>
-      <c r="I1496" s="13"/>
+      <c r="A1496" s="12">
+        <v>44426</v>
+      </c>
+      <c r="B1496" s="12">
+        <v>44426</v>
+      </c>
+      <c r="C1496" s="14" t="s">
+        <v>2034</v>
+      </c>
+      <c r="D1496" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1496" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1496" s="10" t="s">
+        <v>2174</v>
+      </c>
+      <c r="G1496" s="11" t="s">
+        <v>1626</v>
+      </c>
+      <c r="H1496" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1496" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="J1496" s="13"/>
     </row>
-    <row r="1497" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1497" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A1497" s="12">
-        <v>44399</v>
-      </c>
-      <c r="B1497" s="12"/>
+        <v>44427</v>
+      </c>
+      <c r="B1497" s="12">
+        <v>44427</v>
+      </c>
       <c r="C1497" s="14" t="s">
-        <v>1992</v>
+        <v>13</v>
       </c>
       <c r="D1497" s="10" t="s">
-        <v>89</v>
+        <v>584</v>
       </c>
       <c r="E1497" s="11" t="s">
-        <v>837</v>
+        <v>698</v>
       </c>
       <c r="F1497" s="10" t="s">
-        <v>2115</v>
-      </c>
-      <c r="G1497" s="11"/>
-      <c r="H1497" s="12"/>
-      <c r="I1497" s="13"/>
+        <v>2168</v>
+      </c>
+      <c r="G1497" s="11" t="s">
+        <v>1629</v>
+      </c>
+      <c r="H1497" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1497" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1497" s="13"/>
     </row>
-    <row r="1498" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="1498" spans="1:10" ht="72" x14ac:dyDescent="0.2">
       <c r="A1498" s="12">
-        <v>44403</v>
-      </c>
-      <c r="B1498" s="12"/>
+        <v>44428</v>
+      </c>
+      <c r="B1498" s="12">
+        <v>44428</v>
+      </c>
       <c r="C1498" s="14" t="s">
-        <v>1477</v>
+        <v>13</v>
       </c>
       <c r="D1498" s="10" t="s">
-        <v>38</v>
+        <v>584</v>
       </c>
       <c r="E1498" s="11" t="s">
-        <v>570</v>
+        <v>698</v>
       </c>
       <c r="F1498" s="10" t="s">
-        <v>2132</v>
-      </c>
-      <c r="G1498" s="11"/>
-      <c r="H1498" s="12"/>
-      <c r="I1498" s="13"/>
+        <v>2169</v>
+      </c>
+      <c r="G1498" s="11" t="s">
+        <v>1629</v>
+      </c>
+      <c r="H1498" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1498" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1498" s="13"/>
     </row>
     <row r="1499" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1499" s="12">
-        <v>44266</v>
-      </c>
-      <c r="B1499" s="9"/>
+        <v>44434</v>
+      </c>
+      <c r="B1499" s="12">
+        <v>44434</v>
+      </c>
       <c r="C1499" s="14" t="s">
-        <v>537</v>
+        <v>1992</v>
       </c>
       <c r="D1499" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1499" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1499" s="10" t="s">
+        <v>2167</v>
+      </c>
+      <c r="G1499" s="11" t="s">
+        <v>1629</v>
+      </c>
+      <c r="H1499" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1499" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1499" s="13"/>
+    </row>
+    <row r="1500" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1500" s="12">
+        <v>44435</v>
+      </c>
+      <c r="B1500" s="12">
+        <v>44435</v>
+      </c>
+      <c r="C1500" s="14" t="s">
+        <v>559</v>
+      </c>
+      <c r="D1500" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="E1499" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1499" s="10" t="s">
-        <v>1713</v>
-      </c>
-      <c r="G1499" s="11"/>
-      <c r="H1499" s="12"/>
-      <c r="I1499" s="13"/>
-      <c r="J1499" s="13" t="s">
-        <v>1714</v>
-      </c>
-    </row>
-    <row r="1500" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1500" s="12">
-        <v>44286</v>
-      </c>
-      <c r="B1500" s="9"/>
-      <c r="C1500" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D1500" s="10" t="s">
-        <v>25</v>
       </c>
       <c r="E1500" s="11" t="s">
         <v>620</v>
       </c>
       <c r="F1500" s="10" t="s">
-        <v>1838</v>
-      </c>
-      <c r="G1500" s="11"/>
-      <c r="H1500" s="12"/>
-      <c r="I1500" s="13"/>
+        <v>2159</v>
+      </c>
+      <c r="G1500" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1500" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1500" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1500" s="13"/>
     </row>
-    <row r="1501" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1501" s="12"/>
-      <c r="B1501" s="12"/>
-      <c r="C1501" s="14"/>
-      <c r="D1501" s="10"/>
-      <c r="E1501" s="11"/>
-      <c r="F1501" s="10"/>
-      <c r="G1501" s="11"/>
-      <c r="H1501" s="12"/>
-      <c r="I1501" s="13"/>
+    <row r="1501" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1501" s="12">
+        <v>44436</v>
+      </c>
+      <c r="B1501" s="12">
+        <v>44436</v>
+      </c>
+      <c r="C1501" s="14" t="s">
+        <v>462</v>
+      </c>
+      <c r="D1501" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1501" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1501" s="10" t="s">
+        <v>2175</v>
+      </c>
+      <c r="G1501" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1501" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1501" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="J1501" s="13"/>
     </row>
-    <row r="1502" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1502" s="12"/>
-      <c r="B1502" s="12"/>
-      <c r="C1502" s="14"/>
-      <c r="D1502" s="10"/>
-      <c r="E1502" s="11"/>
-      <c r="F1502" s="10"/>
-      <c r="G1502" s="11"/>
-      <c r="H1502" s="12"/>
-      <c r="I1502" s="13"/>
+    <row r="1502" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1502" s="12">
+        <v>44436</v>
+      </c>
+      <c r="B1502" s="12">
+        <v>44436</v>
+      </c>
+      <c r="C1502" s="14" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D1502" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1502" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1502" s="10" t="s">
+        <v>2176</v>
+      </c>
+      <c r="G1502" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1502" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1502" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="J1502" s="13"/>
     </row>
-    <row r="1503" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1503" s="12"/>
-      <c r="B1503" s="12"/>
-      <c r="C1503" s="14"/>
-      <c r="D1503" s="10"/>
-      <c r="E1503" s="11"/>
-      <c r="F1503" s="10"/>
-      <c r="G1503" s="11"/>
-      <c r="H1503" s="12"/>
-      <c r="I1503" s="13"/>
+    <row r="1503" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1503" s="12">
+        <v>44436</v>
+      </c>
+      <c r="B1503" s="12">
+        <v>44436</v>
+      </c>
+      <c r="C1503" s="14" t="s">
+        <v>2034</v>
+      </c>
+      <c r="D1503" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1503" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1503" s="10" t="s">
+        <v>2177</v>
+      </c>
+      <c r="G1503" s="11" t="s">
+        <v>1625</v>
+      </c>
+      <c r="H1503" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1503" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="J1503" s="13"/>
     </row>
-    <row r="1504" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1504" s="12"/>
-      <c r="B1504" s="9"/>
-      <c r="C1504" s="14"/>
-      <c r="D1504" s="10"/>
-      <c r="E1504" s="11"/>
-      <c r="F1504" s="10"/>
-      <c r="G1504" s="11"/>
-      <c r="H1504" s="12"/>
-      <c r="I1504" s="13"/>
+    <row r="1504" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1504" s="12">
+        <v>44438</v>
+      </c>
+      <c r="B1504" s="12">
+        <v>44438</v>
+      </c>
+      <c r="C1504" s="14" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D1504" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1504" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1504" s="10" t="s">
+        <v>2161</v>
+      </c>
+      <c r="G1504" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1504" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1504" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1504" s="13"/>
     </row>
     <row r="1505" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1505" s="1" t="s">
-        <v>1479</v>
-      </c>
-      <c r="B1505" s="2" t="s">
-        <v>1480</v>
-      </c>
-      <c r="C1505" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1505" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1505" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1505" s="4" t="s">
-        <v>1579</v>
-      </c>
-      <c r="G1505" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1505" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1505" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1505" s="36"/>
+      <c r="A1505" s="12">
+        <v>44438</v>
+      </c>
+      <c r="B1505" s="12">
+        <v>44438</v>
+      </c>
+      <c r="C1505" s="14" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D1505" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1505" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1505" s="10" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1505" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1505" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1505" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1505" s="13"/>
     </row>
     <row r="1506" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1506" s="12"/>
-      <c r="B1506" s="9"/>
-      <c r="C1506" s="14"/>
-      <c r="D1506" s="10"/>
-      <c r="E1506" s="11"/>
-      <c r="F1506" s="10"/>
-      <c r="G1506" s="11"/>
-      <c r="H1506" s="12"/>
-      <c r="I1506" s="13"/>
+      <c r="A1506" s="12">
+        <v>44439</v>
+      </c>
+      <c r="B1506" s="12">
+        <v>44439</v>
+      </c>
+      <c r="C1506" s="14" t="s">
+        <v>462</v>
+      </c>
+      <c r="D1506" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1506" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1506" s="10" t="s">
+        <v>2160</v>
+      </c>
+      <c r="G1506" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1506" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1506" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1506" s="13"/>
     </row>
     <row r="1507" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1507" s="12"/>
+      <c r="A1507" s="12">
+        <v>44439</v>
+      </c>
       <c r="B1507" s="12">
-        <v>44402</v>
+        <v>44439</v>
       </c>
       <c r="C1507" s="14" t="s">
-        <v>13</v>
+        <v>462</v>
       </c>
       <c r="D1507" s="10" t="s">
-        <v>584</v>
+        <v>107</v>
       </c>
       <c r="E1507" s="11" t="s">
-        <v>647</v>
+        <v>620</v>
       </c>
       <c r="F1507" s="10" t="s">
-        <v>1614</v>
-      </c>
-      <c r="G1507" s="11"/>
-      <c r="H1507" s="12"/>
-      <c r="I1507" s="13"/>
+        <v>2162</v>
+      </c>
+      <c r="G1507" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1507" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1507" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1507" s="13"/>
     </row>
     <row r="1508" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1508" s="12"/>
+      <c r="A1508" s="12">
+        <v>44439</v>
+      </c>
       <c r="B1508" s="12">
-        <v>44402</v>
+        <v>44439</v>
       </c>
       <c r="C1508" s="14" t="s">
-        <v>13</v>
+        <v>2034</v>
       </c>
       <c r="D1508" s="10" t="s">
-        <v>584</v>
+        <v>83</v>
       </c>
       <c r="E1508" s="11" t="s">
-        <v>647</v>
+        <v>759</v>
       </c>
       <c r="F1508" s="10" t="s">
-        <v>1606</v>
-      </c>
-      <c r="G1508" s="11"/>
-      <c r="H1508" s="12"/>
-      <c r="I1508" s="13"/>
+        <v>2166</v>
+      </c>
+      <c r="G1508" s="11" t="s">
+        <v>1632</v>
+      </c>
+      <c r="H1508" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1508" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1508" s="13"/>
     </row>
     <row r="1509" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1509" s="12"/>
+      <c r="A1509" s="12">
+        <v>44440</v>
+      </c>
       <c r="B1509" s="12">
-        <v>44402</v>
+        <v>44440</v>
       </c>
       <c r="C1509" s="14" t="s">
-        <v>13</v>
+        <v>1992</v>
       </c>
       <c r="D1509" s="10" t="s">
-        <v>584</v>
+        <v>89</v>
       </c>
       <c r="E1509" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1509" s="10" t="s">
-        <v>1611</v>
-      </c>
-      <c r="G1509" s="11"/>
-      <c r="H1509" s="12"/>
-      <c r="I1509" s="13"/>
+        <v>2165</v>
+      </c>
+      <c r="G1509" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1509" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1509" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1509" s="13"/>
     </row>
     <row r="1510" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1510" s="12"/>
+      <c r="A1510" s="12">
+        <v>44440</v>
+      </c>
       <c r="B1510" s="12">
-        <v>44402</v>
+        <v>44440</v>
       </c>
       <c r="C1510" s="14" t="s">
         <v>13</v>
@@ -52390,136 +52723,180 @@
         <v>647</v>
       </c>
       <c r="F1510" s="10" t="s">
-        <v>1607</v>
-      </c>
-      <c r="G1510" s="11"/>
-      <c r="H1510" s="12"/>
-      <c r="I1510" s="13"/>
+        <v>2183</v>
+      </c>
+      <c r="G1510" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1510" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1510" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1510" s="13"/>
     </row>
-    <row r="1511" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1511" s="12"/>
-      <c r="B1511" s="9"/>
+    <row r="1511" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1511" s="12">
+        <v>44441</v>
+      </c>
+      <c r="B1511" s="12">
+        <v>44441</v>
+      </c>
       <c r="C1511" s="14" t="s">
-        <v>13</v>
+        <v>1992</v>
       </c>
       <c r="D1511" s="10" t="s">
-        <v>584</v>
+        <v>89</v>
       </c>
       <c r="E1511" s="11" t="s">
-        <v>647</v>
+        <v>837</v>
       </c>
       <c r="F1511" s="10" t="s">
-        <v>1615</v>
-      </c>
-      <c r="G1511" s="11"/>
-      <c r="H1511" s="12"/>
-      <c r="I1511" s="13"/>
-      <c r="J1511" s="13"/>
-    </row>
-    <row r="1512" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1512" s="12"/>
+        <v>2178</v>
+      </c>
+      <c r="G1511" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1511" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1511" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1511" s="13" t="s">
+        <v>2179</v>
+      </c>
+    </row>
+    <row r="1512" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1512" s="12">
+        <v>44441</v>
+      </c>
       <c r="B1512" s="12">
-        <v>44402</v>
+        <v>44441</v>
       </c>
       <c r="C1512" s="14" t="s">
-        <v>13</v>
+        <v>2180</v>
       </c>
       <c r="D1512" s="10" t="s">
-        <v>584</v>
+        <v>83</v>
       </c>
       <c r="E1512" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1512" s="10" t="s">
-        <v>1608</v>
-      </c>
-      <c r="G1512" s="11"/>
-      <c r="H1512" s="12"/>
-      <c r="I1512" s="13"/>
+        <v>2181</v>
+      </c>
+      <c r="G1512" s="11" t="s">
+        <v>1624</v>
+      </c>
+      <c r="H1512" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1512" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1512" s="13"/>
     </row>
-    <row r="1513" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1513" s="12"/>
-      <c r="B1513" s="9"/>
+    <row r="1513" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1513" s="12">
+        <v>44441</v>
+      </c>
+      <c r="B1513" s="12">
+        <v>44441</v>
+      </c>
       <c r="C1513" s="14" t="s">
-        <v>13</v>
+        <v>527</v>
       </c>
       <c r="D1513" s="10" t="s">
-        <v>584</v>
+        <v>17</v>
       </c>
       <c r="E1513" s="11" t="s">
-        <v>647</v>
+        <v>837</v>
       </c>
       <c r="F1513" s="10" t="s">
-        <v>1605</v>
-      </c>
-      <c r="G1513" s="11"/>
-      <c r="H1513" s="12"/>
-      <c r="I1513" s="13"/>
+        <v>2182</v>
+      </c>
+      <c r="G1513" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1513" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1513" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1513" s="13"/>
     </row>
     <row r="1514" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1514" s="12"/>
+      <c r="A1514" s="12">
+        <v>44445</v>
+      </c>
       <c r="B1514" s="12">
-        <v>44402</v>
+        <v>44448</v>
       </c>
       <c r="C1514" s="14" t="s">
-        <v>13</v>
+        <v>1992</v>
       </c>
       <c r="D1514" s="10" t="s">
-        <v>584</v>
+        <v>89</v>
       </c>
       <c r="E1514" s="11" t="s">
-        <v>647</v>
+        <v>837</v>
       </c>
       <c r="F1514" s="10" t="s">
-        <v>1604</v>
-      </c>
-      <c r="G1514" s="11"/>
-      <c r="H1514" s="12"/>
-      <c r="I1514" s="13"/>
+        <v>2184</v>
+      </c>
+      <c r="G1514" s="11" t="s">
+        <v>1625</v>
+      </c>
+      <c r="H1514" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1514" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1514" s="13"/>
     </row>
-    <row r="1515" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1515" s="12"/>
+    <row r="1515" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1515" s="12">
+        <v>44448</v>
+      </c>
       <c r="B1515" s="12">
-        <v>44402</v>
+        <v>44448</v>
       </c>
       <c r="C1515" s="14" t="s">
-        <v>13</v>
+        <v>898</v>
       </c>
       <c r="D1515" s="10" t="s">
-        <v>584</v>
+        <v>494</v>
       </c>
       <c r="E1515" s="11" t="s">
-        <v>647</v>
+        <v>620</v>
       </c>
       <c r="F1515" s="10" t="s">
-        <v>1609</v>
-      </c>
-      <c r="G1515" s="11"/>
-      <c r="H1515" s="12"/>
-      <c r="I1515" s="13"/>
-      <c r="J1515" s="13"/>
+        <v>2185</v>
+      </c>
+      <c r="G1515" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1515" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1515" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1515" s="13" t="s">
+        <v>2186</v>
+      </c>
     </row>
     <row r="1516" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1516" s="12"/>
-      <c r="B1516" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1516" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1516" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1516" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1516" s="10" t="s">
-        <v>1612</v>
-      </c>
+      <c r="B1516" s="12"/>
+      <c r="C1516" s="14"/>
+      <c r="D1516" s="10"/>
+      <c r="E1516" s="11"/>
+      <c r="F1516" s="10"/>
       <c r="G1516" s="11"/>
       <c r="H1516" s="12"/>
       <c r="I1516" s="13"/>
@@ -52527,21 +52904,11 @@
     </row>
     <row r="1517" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1517" s="12"/>
-      <c r="B1517" s="9">
-        <v>44235</v>
-      </c>
-      <c r="C1517" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1517" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1517" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1517" s="10" t="s">
-        <v>1613</v>
-      </c>
+      <c r="B1517" s="12"/>
+      <c r="C1517" s="14"/>
+      <c r="D1517" s="10"/>
+      <c r="E1517" s="11"/>
+      <c r="F1517" s="10"/>
       <c r="G1517" s="11"/>
       <c r="H1517" s="12"/>
       <c r="I1517" s="13"/>
@@ -52549,19 +52916,11 @@
     </row>
     <row r="1518" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1518" s="12"/>
-      <c r="B1518" s="9"/>
-      <c r="C1518" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1518" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1518" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1518" s="10" t="s">
-        <v>1610</v>
-      </c>
+      <c r="B1518" s="12"/>
+      <c r="C1518" s="14"/>
+      <c r="D1518" s="10"/>
+      <c r="E1518" s="11"/>
+      <c r="F1518" s="10"/>
       <c r="G1518" s="11"/>
       <c r="H1518" s="12"/>
       <c r="I1518" s="13"/>
@@ -52569,19 +52928,11 @@
     </row>
     <row r="1519" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1519" s="12"/>
-      <c r="B1519" s="9"/>
-      <c r="C1519" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1519" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1519" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1519" s="10" t="s">
-        <v>1581</v>
-      </c>
+      <c r="B1519" s="12"/>
+      <c r="C1519" s="14"/>
+      <c r="D1519" s="10"/>
+      <c r="E1519" s="11"/>
+      <c r="F1519" s="10"/>
       <c r="G1519" s="11"/>
       <c r="H1519" s="12"/>
       <c r="I1519" s="13"/>
@@ -52589,7 +52940,7 @@
     </row>
     <row r="1520" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1520" s="12"/>
-      <c r="B1520" s="9"/>
+      <c r="B1520" s="12"/>
       <c r="C1520" s="14"/>
       <c r="D1520" s="10"/>
       <c r="E1520" s="11"/>
@@ -52600,80 +52951,58 @@
       <c r="J1520" s="13"/>
     </row>
     <row r="1521" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1521" s="12">
-        <v>44176</v>
-      </c>
-      <c r="B1521" s="9"/>
-      <c r="C1521" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1521" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1521" s="11" t="s">
-        <v>1353</v>
-      </c>
-      <c r="F1521" s="10" t="s">
-        <v>1354</v>
-      </c>
+      <c r="A1521" s="12"/>
+      <c r="B1521" s="12"/>
+      <c r="C1521" s="14"/>
+      <c r="D1521" s="10"/>
+      <c r="E1521" s="11"/>
+      <c r="F1521" s="10"/>
       <c r="G1521" s="11"/>
       <c r="H1521" s="12"/>
       <c r="I1521" s="13"/>
       <c r="J1521" s="13"/>
     </row>
-    <row r="1522" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1522" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1522" s="9"/>
-      <c r="C1522" s="14" t="s">
-        <v>898</v>
-      </c>
-      <c r="D1522" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="E1522" s="11" t="s">
-        <v>759</v>
-      </c>
-      <c r="F1522" s="10" t="s">
-        <v>1659</v>
-      </c>
+    <row r="1522" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1522" s="12"/>
+      <c r="B1522" s="12"/>
+      <c r="C1522" s="14"/>
+      <c r="D1522" s="10"/>
+      <c r="E1522" s="11"/>
+      <c r="F1522" s="10"/>
       <c r="G1522" s="11"/>
       <c r="H1522" s="12"/>
       <c r="I1522" s="13"/>
-      <c r="J1522" s="13" t="s">
-        <v>1682</v>
-      </c>
+      <c r="J1522" s="13"/>
     </row>
     <row r="1523" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1523" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1523" s="9"/>
+        <v>44403</v>
+      </c>
+      <c r="B1523" s="12"/>
       <c r="C1523" s="14" t="s">
-        <v>898</v>
+        <v>1477</v>
       </c>
       <c r="D1523" s="10" t="s">
-        <v>494</v>
+        <v>38</v>
       </c>
       <c r="E1523" s="11" t="s">
-        <v>759</v>
+        <v>570</v>
       </c>
       <c r="F1523" s="10" t="s">
-        <v>1658</v>
+        <v>2131</v>
       </c>
       <c r="G1523" s="11"/>
       <c r="H1523" s="12"/>
       <c r="I1523" s="13"/>
       <c r="J1523" s="13"/>
     </row>
-    <row r="1524" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1524" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1524" s="12">
-        <v>44112</v>
+        <v>44266</v>
       </c>
       <c r="B1524" s="9"/>
       <c r="C1524" s="14" t="s">
-        <v>623</v>
+        <v>537</v>
       </c>
       <c r="D1524" s="10" t="s">
         <v>6</v>
@@ -52682,29 +53011,31 @@
         <v>570</v>
       </c>
       <c r="F1524" s="10" t="s">
-        <v>1097</v>
+        <v>1713</v>
       </c>
       <c r="G1524" s="11"/>
       <c r="H1524" s="12"/>
       <c r="I1524" s="13"/>
-      <c r="J1524" s="13"/>
-    </row>
-    <row r="1525" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1524" s="13" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="1525" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1525" s="12">
-        <v>44088</v>
+        <v>44286</v>
       </c>
       <c r="B1525" s="9"/>
       <c r="C1525" s="14" t="s">
-        <v>19</v>
+        <v>288</v>
       </c>
       <c r="D1525" s="10" t="s">
-        <v>906</v>
+        <v>25</v>
       </c>
       <c r="E1525" s="11" t="s">
-        <v>685</v>
+        <v>620</v>
       </c>
       <c r="F1525" s="10" t="s">
-        <v>1011</v>
+        <v>1838</v>
       </c>
       <c r="G1525" s="11"/>
       <c r="H1525" s="12"/>
@@ -52712,278 +53043,220 @@
       <c r="J1525" s="13"/>
     </row>
     <row r="1526" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1526" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1526" s="9"/>
-      <c r="C1526" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="D1526" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1526" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1526" s="10" t="s">
-        <v>903</v>
-      </c>
+      <c r="A1526" s="12"/>
+      <c r="B1526" s="12"/>
+      <c r="C1526" s="14"/>
+      <c r="D1526" s="10"/>
+      <c r="E1526" s="11"/>
+      <c r="F1526" s="10"/>
       <c r="G1526" s="11"/>
       <c r="H1526" s="12"/>
       <c r="I1526" s="13"/>
       <c r="J1526" s="13"/>
     </row>
     <row r="1527" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1527" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1527" s="9"/>
-      <c r="C1527" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="D1527" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1527" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1527" s="10" t="s">
-        <v>902</v>
-      </c>
+      <c r="A1527" s="12"/>
+      <c r="B1527" s="12"/>
+      <c r="C1527" s="14"/>
+      <c r="D1527" s="10"/>
+      <c r="E1527" s="11"/>
+      <c r="F1527" s="10"/>
       <c r="G1527" s="11"/>
       <c r="H1527" s="12"/>
       <c r="I1527" s="13"/>
       <c r="J1527" s="13"/>
     </row>
     <row r="1528" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1528" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1528" s="9"/>
-      <c r="C1528" s="14" t="s">
-        <v>898</v>
-      </c>
-      <c r="D1528" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="E1528" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1528" s="10" t="s">
-        <v>900</v>
-      </c>
+      <c r="A1528" s="12"/>
+      <c r="B1528" s="12"/>
+      <c r="C1528" s="14"/>
+      <c r="D1528" s="10"/>
+      <c r="E1528" s="11"/>
+      <c r="F1528" s="10"/>
       <c r="G1528" s="11"/>
       <c r="H1528" s="12"/>
       <c r="I1528" s="13"/>
       <c r="J1528" s="13"/>
     </row>
-    <row r="1529" spans="1:10" ht="108" x14ac:dyDescent="0.2">
-      <c r="A1529" s="12">
-        <v>44055</v>
-      </c>
+    <row r="1529" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1529" s="12"/>
       <c r="B1529" s="9"/>
-      <c r="C1529" s="14" t="s">
-        <v>898</v>
-      </c>
-      <c r="D1529" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="E1529" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1529" s="10" t="s">
-        <v>901</v>
-      </c>
+      <c r="C1529" s="14"/>
+      <c r="D1529" s="10"/>
+      <c r="E1529" s="11"/>
+      <c r="F1529" s="10"/>
       <c r="G1529" s="11"/>
       <c r="H1529" s="12"/>
       <c r="I1529" s="13"/>
       <c r="J1529" s="13"/>
     </row>
-    <row r="1530" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A1530" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1530" s="9"/>
-      <c r="C1530" s="14" t="s">
-        <v>898</v>
-      </c>
-      <c r="D1530" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="E1530" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1530" s="10" t="s">
-        <v>904</v>
-      </c>
-      <c r="G1530" s="11"/>
-      <c r="H1530" s="12"/>
-      <c r="I1530" s="13"/>
-      <c r="J1530" s="13" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="1531" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1531" s="12">
-        <v>44047</v>
-      </c>
+    <row r="1530" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1530" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B1530" s="2" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C1530" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1530" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1530" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1530" s="4" t="s">
+        <v>1579</v>
+      </c>
+      <c r="G1530" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1530" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1530" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1530" s="36"/>
+    </row>
+    <row r="1531" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1531" s="12"/>
       <c r="B1531" s="9"/>
-      <c r="C1531" s="14" t="s">
-        <v>537</v>
-      </c>
-      <c r="D1531" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1531" s="11" t="s">
-        <v>685</v>
-      </c>
-      <c r="F1531" s="10" t="s">
-        <v>873</v>
-      </c>
-      <c r="G1531" s="11" t="s">
-        <v>1624</v>
-      </c>
+      <c r="C1531" s="14"/>
+      <c r="D1531" s="10"/>
+      <c r="E1531" s="11"/>
+      <c r="F1531" s="10"/>
+      <c r="G1531" s="11"/>
       <c r="H1531" s="12"/>
       <c r="I1531" s="13"/>
       <c r="J1531" s="13"/>
     </row>
-    <row r="1532" spans="1:10" ht="168" x14ac:dyDescent="0.2">
-      <c r="A1532" s="12">
-        <v>43949</v>
-      </c>
-      <c r="B1532" s="9"/>
+    <row r="1532" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1532" s="12"/>
+      <c r="B1532" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1532" s="14" t="s">
-        <v>468</v>
+        <v>13</v>
       </c>
       <c r="D1532" s="10" t="s">
-        <v>89</v>
+        <v>584</v>
       </c>
       <c r="E1532" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1532" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1532" s="11" t="s">
-        <v>1639</v>
-      </c>
+        <v>1614</v>
+      </c>
+      <c r="G1532" s="11"/>
       <c r="H1532" s="12"/>
-      <c r="I1532" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1532" s="13"/>
       <c r="J1532" s="13"/>
     </row>
-    <row r="1533" spans="1:10" ht="168" x14ac:dyDescent="0.2">
-      <c r="A1533" s="12">
-        <v>43949</v>
-      </c>
-      <c r="B1533" s="9"/>
+    <row r="1533" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1533" s="12"/>
+      <c r="B1533" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1533" s="14" t="s">
-        <v>468</v>
+        <v>13</v>
       </c>
       <c r="D1533" s="10" t="s">
-        <v>89</v>
+        <v>584</v>
       </c>
       <c r="E1533" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1533" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1533" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>1606</v>
+      </c>
+      <c r="G1533" s="11"/>
       <c r="H1533" s="12"/>
-      <c r="I1533" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1533" s="13" t="s">
-        <v>1568</v>
-      </c>
-    </row>
-    <row r="1534" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1534" s="12">
-        <v>43838</v>
-      </c>
-      <c r="B1534" s="9"/>
+      <c r="I1533" s="13"/>
+      <c r="J1533" s="13"/>
+    </row>
+    <row r="1534" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1534" s="12"/>
+      <c r="B1534" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1534" s="14" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="D1534" s="10" t="s">
-        <v>460</v>
+        <v>584</v>
       </c>
       <c r="E1534" s="11" t="s">
         <v>647</v>
       </c>
       <c r="F1534" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G1534" s="11" t="s">
-        <v>1640</v>
-      </c>
+        <v>1611</v>
+      </c>
+      <c r="G1534" s="11"/>
       <c r="H1534" s="12"/>
       <c r="I1534" s="13"/>
-      <c r="J1534" s="13" t="s">
-        <v>1533</v>
-      </c>
+      <c r="J1534" s="13"/>
     </row>
     <row r="1535" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1535" s="12">
-        <v>43816</v>
-      </c>
-      <c r="B1535" s="9"/>
+      <c r="A1535" s="12"/>
+      <c r="B1535" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1535" s="14" t="s">
-        <v>475</v>
+        <v>13</v>
       </c>
       <c r="D1535" s="10" t="s">
-        <v>38</v>
+        <v>584</v>
       </c>
       <c r="E1535" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1535" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="G1535" s="11" t="s">
-        <v>1632</v>
-      </c>
+        <v>1607</v>
+      </c>
+      <c r="G1535" s="11"/>
       <c r="H1535" s="12"/>
       <c r="I1535" s="13"/>
-      <c r="J1535" s="13" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="1536" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1536" s="12">
-        <v>43762</v>
-      </c>
+      <c r="J1535" s="13"/>
+    </row>
+    <row r="1536" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1536" s="12"/>
       <c r="B1536" s="9"/>
       <c r="C1536" s="14" t="s">
-        <v>446</v>
+        <v>13</v>
       </c>
       <c r="D1536" s="10" t="s">
-        <v>17</v>
+        <v>584</v>
       </c>
       <c r="E1536" s="11" t="s">
-        <v>837</v>
+        <v>647</v>
       </c>
       <c r="F1536" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G1536" s="11" t="s">
-        <v>1629</v>
-      </c>
+        <v>1615</v>
+      </c>
+      <c r="G1536" s="11"/>
       <c r="H1536" s="12"/>
       <c r="I1536" s="13"/>
       <c r="J1536" s="13"/>
     </row>
     <row r="1537" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1537" s="12"/>
-      <c r="B1537" s="9"/>
-      <c r="C1537" s="14"/>
-      <c r="D1537" s="10"/>
-      <c r="E1537" s="11"/>
-      <c r="F1537" s="10"/>
+      <c r="B1537" s="12">
+        <v>44402</v>
+      </c>
+      <c r="C1537" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1537" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1537" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1537" s="10" t="s">
+        <v>1608</v>
+      </c>
       <c r="G1537" s="11"/>
       <c r="H1537" s="12"/>
       <c r="I1537" s="13"/>
@@ -52992,10 +53265,18 @@
     <row r="1538" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1538" s="12"/>
       <c r="B1538" s="9"/>
-      <c r="C1538" s="14"/>
-      <c r="D1538" s="10"/>
-      <c r="E1538" s="11"/>
-      <c r="F1538" s="10"/>
+      <c r="C1538" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1538" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1538" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1538" s="10" t="s">
+        <v>1605</v>
+      </c>
       <c r="G1538" s="11"/>
       <c r="H1538" s="12"/>
       <c r="I1538" s="13"/>
@@ -53003,11 +53284,21 @@
     </row>
     <row r="1539" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1539" s="12"/>
-      <c r="B1539" s="9"/>
-      <c r="C1539" s="14"/>
-      <c r="D1539" s="10"/>
-      <c r="E1539" s="11"/>
-      <c r="F1539" s="10"/>
+      <c r="B1539" s="12">
+        <v>44402</v>
+      </c>
+      <c r="C1539" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1539" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1539" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1539" s="10" t="s">
+        <v>1604</v>
+      </c>
       <c r="G1539" s="11"/>
       <c r="H1539" s="12"/>
       <c r="I1539" s="13"/>
@@ -53015,11 +53306,21 @@
     </row>
     <row r="1540" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1540" s="12"/>
-      <c r="B1540" s="9"/>
-      <c r="C1540" s="14"/>
-      <c r="D1540" s="10"/>
-      <c r="E1540" s="11"/>
-      <c r="F1540" s="10"/>
+      <c r="B1540" s="12">
+        <v>44402</v>
+      </c>
+      <c r="C1540" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1540" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1540" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1540" s="10" t="s">
+        <v>1609</v>
+      </c>
       <c r="G1540" s="11"/>
       <c r="H1540" s="12"/>
       <c r="I1540" s="13"/>
@@ -53027,11 +53328,21 @@
     </row>
     <row r="1541" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1541" s="12"/>
-      <c r="B1541" s="9"/>
-      <c r="C1541" s="14"/>
-      <c r="D1541" s="10"/>
-      <c r="E1541" s="11"/>
-      <c r="F1541" s="10"/>
+      <c r="B1541" s="12">
+        <v>44402</v>
+      </c>
+      <c r="C1541" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1541" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1541" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1541" s="10" t="s">
+        <v>1612</v>
+      </c>
       <c r="G1541" s="11"/>
       <c r="H1541" s="12"/>
       <c r="I1541" s="13"/>
@@ -53039,20 +53350,532 @@
     </row>
     <row r="1542" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1542" s="12"/>
-      <c r="B1542" s="9"/>
-      <c r="C1542" s="14"/>
-      <c r="D1542" s="10"/>
-      <c r="E1542" s="11"/>
-      <c r="F1542" s="10"/>
+      <c r="B1542" s="9">
+        <v>44235</v>
+      </c>
+      <c r="C1542" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1542" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1542" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1542" s="10" t="s">
+        <v>1613</v>
+      </c>
       <c r="G1542" s="11"/>
       <c r="H1542" s="12"/>
       <c r="I1542" s="13"/>
       <c r="J1542" s="13"/>
     </row>
+    <row r="1543" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1543" s="12"/>
+      <c r="B1543" s="9"/>
+      <c r="C1543" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1543" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1543" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1543" s="10" t="s">
+        <v>1610</v>
+      </c>
+      <c r="G1543" s="11"/>
+      <c r="H1543" s="12"/>
+      <c r="I1543" s="13"/>
+      <c r="J1543" s="13"/>
+    </row>
+    <row r="1544" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1544" s="12"/>
+      <c r="B1544" s="9"/>
+      <c r="C1544" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1544" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1544" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1544" s="10" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G1544" s="11"/>
+      <c r="H1544" s="12"/>
+      <c r="I1544" s="13"/>
+      <c r="J1544" s="13"/>
+    </row>
+    <row r="1545" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1545" s="12"/>
+      <c r="B1545" s="9"/>
+      <c r="C1545" s="14"/>
+      <c r="D1545" s="10"/>
+      <c r="E1545" s="11"/>
+      <c r="F1545" s="10"/>
+      <c r="G1545" s="11"/>
+      <c r="H1545" s="12"/>
+      <c r="I1545" s="13"/>
+      <c r="J1545" s="13"/>
+    </row>
+    <row r="1546" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1546" s="12">
+        <v>44176</v>
+      </c>
+      <c r="B1546" s="9"/>
+      <c r="C1546" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1546" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1546" s="11" t="s">
+        <v>1353</v>
+      </c>
+      <c r="F1546" s="10" t="s">
+        <v>1354</v>
+      </c>
+      <c r="G1546" s="11"/>
+      <c r="H1546" s="12"/>
+      <c r="I1546" s="13"/>
+      <c r="J1546" s="13"/>
+    </row>
+    <row r="1547" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+      <c r="A1547" s="12">
+        <v>44252</v>
+      </c>
+      <c r="B1547" s="9"/>
+      <c r="C1547" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1547" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1547" s="11" t="s">
+        <v>759</v>
+      </c>
+      <c r="F1547" s="10" t="s">
+        <v>1659</v>
+      </c>
+      <c r="G1547" s="11"/>
+      <c r="H1547" s="12"/>
+      <c r="I1547" s="13"/>
+      <c r="J1547" s="13" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="1548" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1548" s="12">
+        <v>44252</v>
+      </c>
+      <c r="B1548" s="9"/>
+      <c r="C1548" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1548" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1548" s="11" t="s">
+        <v>759</v>
+      </c>
+      <c r="F1548" s="10" t="s">
+        <v>1658</v>
+      </c>
+      <c r="G1548" s="11"/>
+      <c r="H1548" s="12"/>
+      <c r="I1548" s="13"/>
+      <c r="J1548" s="13"/>
+    </row>
+    <row r="1549" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1549" s="12">
+        <v>44112</v>
+      </c>
+      <c r="B1549" s="9"/>
+      <c r="C1549" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1549" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1549" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1549" s="10" t="s">
+        <v>1097</v>
+      </c>
+      <c r="G1549" s="11"/>
+      <c r="H1549" s="12"/>
+      <c r="I1549" s="13"/>
+      <c r="J1549" s="13"/>
+    </row>
+    <row r="1550" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1550" s="12">
+        <v>44088</v>
+      </c>
+      <c r="B1550" s="9"/>
+      <c r="C1550" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1550" s="10" t="s">
+        <v>906</v>
+      </c>
+      <c r="E1550" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1550" s="10" t="s">
+        <v>1011</v>
+      </c>
+      <c r="G1550" s="11"/>
+      <c r="H1550" s="12"/>
+      <c r="I1550" s="13"/>
+      <c r="J1550" s="13"/>
+    </row>
+    <row r="1551" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1551" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B1551" s="9"/>
+      <c r="C1551" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1551" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1551" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1551" s="10" t="s">
+        <v>903</v>
+      </c>
+      <c r="G1551" s="11"/>
+      <c r="H1551" s="12"/>
+      <c r="I1551" s="13"/>
+      <c r="J1551" s="13"/>
+    </row>
+    <row r="1552" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1552" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B1552" s="9"/>
+      <c r="C1552" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1552" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1552" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1552" s="10" t="s">
+        <v>902</v>
+      </c>
+      <c r="G1552" s="11"/>
+      <c r="H1552" s="12"/>
+      <c r="I1552" s="13"/>
+      <c r="J1552" s="13"/>
+    </row>
+    <row r="1553" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1553" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B1553" s="9"/>
+      <c r="C1553" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1553" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1553" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1553" s="10" t="s">
+        <v>900</v>
+      </c>
+      <c r="G1553" s="11"/>
+      <c r="H1553" s="12"/>
+      <c r="I1553" s="13"/>
+      <c r="J1553" s="13"/>
+    </row>
+    <row r="1554" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A1554" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B1554" s="9"/>
+      <c r="C1554" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1554" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1554" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1554" s="10" t="s">
+        <v>901</v>
+      </c>
+      <c r="G1554" s="11"/>
+      <c r="H1554" s="12"/>
+      <c r="I1554" s="13"/>
+      <c r="J1554" s="13"/>
+    </row>
+    <row r="1555" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1555" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B1555" s="9"/>
+      <c r="C1555" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1555" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1555" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1555" s="10" t="s">
+        <v>904</v>
+      </c>
+      <c r="G1555" s="11"/>
+      <c r="H1555" s="12"/>
+      <c r="I1555" s="13"/>
+      <c r="J1555" s="13" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="1556" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1556" s="12">
+        <v>44047</v>
+      </c>
+      <c r="B1556" s="9"/>
+      <c r="C1556" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1556" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1556" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1556" s="10" t="s">
+        <v>873</v>
+      </c>
+      <c r="G1556" s="11" t="s">
+        <v>1624</v>
+      </c>
+      <c r="H1556" s="12"/>
+      <c r="I1556" s="13"/>
+      <c r="J1556" s="13"/>
+    </row>
+    <row r="1557" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1557" s="12">
+        <v>43949</v>
+      </c>
+      <c r="B1557" s="9"/>
+      <c r="C1557" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1557" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1557" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1557" s="10" t="s">
+        <v>686</v>
+      </c>
+      <c r="G1557" s="11" t="s">
+        <v>1639</v>
+      </c>
+      <c r="H1557" s="12"/>
+      <c r="I1557" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1557" s="13"/>
+    </row>
+    <row r="1558" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1558" s="12">
+        <v>43949</v>
+      </c>
+      <c r="B1558" s="9"/>
+      <c r="C1558" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1558" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1558" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1558" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="G1558" s="11" t="s">
+        <v>687</v>
+      </c>
+      <c r="H1558" s="12"/>
+      <c r="I1558" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1558" s="13" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="1559" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1559" s="12">
+        <v>43838</v>
+      </c>
+      <c r="B1559" s="9"/>
+      <c r="C1559" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1559" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1559" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1559" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G1559" s="11" t="s">
+        <v>1640</v>
+      </c>
+      <c r="H1559" s="12"/>
+      <c r="I1559" s="13"/>
+      <c r="J1559" s="13" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1560" s="12">
+        <v>43816</v>
+      </c>
+      <c r="B1560" s="9"/>
+      <c r="C1560" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1560" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1560" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1560" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G1560" s="11" t="s">
+        <v>1632</v>
+      </c>
+      <c r="H1560" s="12"/>
+      <c r="I1560" s="13"/>
+      <c r="J1560" s="13" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1561" s="12">
+        <v>43762</v>
+      </c>
+      <c r="B1561" s="9"/>
+      <c r="C1561" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1561" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1561" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1561" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1561" s="11" t="s">
+        <v>1629</v>
+      </c>
+      <c r="H1561" s="12"/>
+      <c r="I1561" s="13"/>
+      <c r="J1561" s="13"/>
+    </row>
+    <row r="1562" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1562" s="12"/>
+      <c r="B1562" s="9"/>
+      <c r="C1562" s="14"/>
+      <c r="D1562" s="10"/>
+      <c r="E1562" s="11"/>
+      <c r="F1562" s="10"/>
+      <c r="G1562" s="11"/>
+      <c r="H1562" s="12"/>
+      <c r="I1562" s="13"/>
+      <c r="J1562" s="13"/>
+    </row>
+    <row r="1563" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1563" s="12"/>
+      <c r="B1563" s="9"/>
+      <c r="C1563" s="14"/>
+      <c r="D1563" s="10"/>
+      <c r="E1563" s="11"/>
+      <c r="F1563" s="10"/>
+      <c r="G1563" s="11"/>
+      <c r="H1563" s="12"/>
+      <c r="I1563" s="13"/>
+      <c r="J1563" s="13"/>
+    </row>
+    <row r="1564" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1564" s="12"/>
+      <c r="B1564" s="9"/>
+      <c r="C1564" s="14"/>
+      <c r="D1564" s="10"/>
+      <c r="E1564" s="11"/>
+      <c r="F1564" s="10"/>
+      <c r="G1564" s="11"/>
+      <c r="H1564" s="12"/>
+      <c r="I1564" s="13"/>
+      <c r="J1564" s="13"/>
+    </row>
+    <row r="1565" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1565" s="12"/>
+      <c r="B1565" s="9"/>
+      <c r="C1565" s="14"/>
+      <c r="D1565" s="10"/>
+      <c r="E1565" s="11"/>
+      <c r="F1565" s="10"/>
+      <c r="G1565" s="11"/>
+      <c r="H1565" s="12"/>
+      <c r="I1565" s="13"/>
+      <c r="J1565" s="13"/>
+    </row>
+    <row r="1566" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1566" s="12"/>
+      <c r="B1566" s="9"/>
+      <c r="C1566" s="14"/>
+      <c r="D1566" s="10"/>
+      <c r="E1566" s="11"/>
+      <c r="F1566" s="10"/>
+      <c r="G1566" s="11"/>
+      <c r="H1566" s="12"/>
+      <c r="I1566" s="13"/>
+      <c r="J1566" s="13"/>
+    </row>
+    <row r="1567" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1567" s="12"/>
+      <c r="B1567" s="9"/>
+      <c r="C1567" s="14"/>
+      <c r="D1567" s="10"/>
+      <c r="E1567" s="11"/>
+      <c r="F1567" s="10"/>
+      <c r="G1567" s="11"/>
+      <c r="H1567" s="12"/>
+      <c r="I1567" s="13"/>
+      <c r="J1567" s="13"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J1479" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1508:F1518">
-    <sortCondition ref="F1508:F1518"/>
+  <autoFilter ref="A1:J1480" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1533:F1543">
+    <sortCondition ref="F1533:F1543"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Filtro lib de pedido de venda WEB
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E301E6E8-1D6E-4D8B-A1B8-DE103E3A061A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5F000C-33F5-4DD7-850E-9BE72D954C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10758" uniqueCount="2187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10772" uniqueCount="2189">
   <si>
     <t>Responsável</t>
   </si>
@@ -6943,6 +6943,12 @@
   </si>
   <si>
     <t>BKFATR06 - Relação de Clientes (primeira e ultima compra)</t>
+  </si>
+  <si>
+    <t>Atualizações: 21-08-30-LIB_LABEL_09082021_P12_LOBO, 21-09-03-CENTRAL_DE_ATUALIZACOES_V1_3_2, TOTVSLICENSE_WINDOWS, 21-09-08-TOTVS_DBACCESS_WINDOWS_X64-BUILD_20.1.1.5, 21-09-02_ATUALIZACAO_12.1.25_GCT_EXPEDICAO_CONTINUA, 21-08-26_ATUALIZACAO_12.1.25_BACKOFFICE_EXPEDICAO_CONTINUA e 21-08-28_ATUALIZACAO_12.1.25_TAF_EXPEDICAO_CONTINUA</t>
+  </si>
+  <si>
+    <t>Atualização dos serviços REST para a versão 2.0 e conversão dos programas</t>
   </si>
 </sst>
 </file>
@@ -7711,11 +7717,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1567"/>
+  <dimension ref="A1:J1568"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1505" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1515" sqref="F1515"/>
+      <pane ySplit="1" topLeftCell="A1547" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1553" sqref="F1553"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -52891,27 +52897,63 @@
       </c>
     </row>
     <row r="1516" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1516" s="12"/>
-      <c r="B1516" s="12"/>
-      <c r="C1516" s="14"/>
-      <c r="D1516" s="10"/>
-      <c r="E1516" s="11"/>
-      <c r="F1516" s="10"/>
-      <c r="G1516" s="11"/>
-      <c r="H1516" s="12"/>
-      <c r="I1516" s="13"/>
+      <c r="A1516" s="12">
+        <v>44449</v>
+      </c>
+      <c r="B1516" s="12">
+        <v>44449</v>
+      </c>
+      <c r="C1516" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1516" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1516" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1516" s="10" t="s">
+        <v>2188</v>
+      </c>
+      <c r="G1516" s="11" t="s">
+        <v>1629</v>
+      </c>
+      <c r="H1516" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1516" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1516" s="13"/>
     </row>
-    <row r="1517" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1517" s="12"/>
-      <c r="B1517" s="12"/>
-      <c r="C1517" s="14"/>
-      <c r="D1517" s="10"/>
-      <c r="E1517" s="11"/>
-      <c r="F1517" s="10"/>
-      <c r="G1517" s="11"/>
-      <c r="H1517" s="12"/>
-      <c r="I1517" s="13"/>
+    <row r="1517" spans="1:10" ht="72" x14ac:dyDescent="0.2">
+      <c r="A1517" s="12">
+        <v>44450</v>
+      </c>
+      <c r="B1517" s="12">
+        <v>44450</v>
+      </c>
+      <c r="C1517" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1517" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1517" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1517" s="10" t="s">
+        <v>2187</v>
+      </c>
+      <c r="G1517" s="11" t="s">
+        <v>1626</v>
+      </c>
+      <c r="H1517" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1517" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1517" s="13"/>
     </row>
     <row r="1518" spans="1:10" x14ac:dyDescent="0.2">
@@ -52974,81 +53016,81 @@
       <c r="I1522" s="13"/>
       <c r="J1522" s="13"/>
     </row>
-    <row r="1523" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1523" s="12">
-        <v>44403</v>
-      </c>
+    <row r="1523" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1523" s="12"/>
       <c r="B1523" s="12"/>
-      <c r="C1523" s="14" t="s">
-        <v>1477</v>
-      </c>
-      <c r="D1523" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1523" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1523" s="10" t="s">
-        <v>2131</v>
-      </c>
+      <c r="C1523" s="14"/>
+      <c r="D1523" s="10"/>
+      <c r="E1523" s="11"/>
+      <c r="F1523" s="10"/>
       <c r="G1523" s="11"/>
       <c r="H1523" s="12"/>
       <c r="I1523" s="13"/>
       <c r="J1523" s="13"/>
     </row>
-    <row r="1524" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1524" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1524" s="12">
-        <v>44266</v>
-      </c>
-      <c r="B1524" s="9"/>
+        <v>44403</v>
+      </c>
+      <c r="B1524" s="12"/>
       <c r="C1524" s="14" t="s">
-        <v>537</v>
+        <v>1477</v>
       </c>
       <c r="D1524" s="10" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="E1524" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1524" s="10" t="s">
-        <v>1713</v>
+        <v>2131</v>
       </c>
       <c r="G1524" s="11"/>
       <c r="H1524" s="12"/>
       <c r="I1524" s="13"/>
-      <c r="J1524" s="13" t="s">
-        <v>1714</v>
-      </c>
-    </row>
-    <row r="1525" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1524" s="13"/>
+    </row>
+    <row r="1525" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1525" s="12">
-        <v>44286</v>
+        <v>44266</v>
       </c>
       <c r="B1525" s="9"/>
       <c r="C1525" s="14" t="s">
-        <v>288</v>
+        <v>537</v>
       </c>
       <c r="D1525" s="10" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E1525" s="11" t="s">
-        <v>620</v>
+        <v>570</v>
       </c>
       <c r="F1525" s="10" t="s">
-        <v>1838</v>
+        <v>1713</v>
       </c>
       <c r="G1525" s="11"/>
       <c r="H1525" s="12"/>
       <c r="I1525" s="13"/>
-      <c r="J1525" s="13"/>
-    </row>
-    <row r="1526" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1526" s="12"/>
-      <c r="B1526" s="12"/>
-      <c r="C1526" s="14"/>
-      <c r="D1526" s="10"/>
-      <c r="E1526" s="11"/>
-      <c r="F1526" s="10"/>
+      <c r="J1525" s="13" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="1526" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1526" s="12">
+        <v>44286</v>
+      </c>
+      <c r="B1526" s="9"/>
+      <c r="C1526" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1526" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1526" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1526" s="10" t="s">
+        <v>1838</v>
+      </c>
       <c r="G1526" s="11"/>
       <c r="H1526" s="12"/>
       <c r="I1526" s="13"/>
@@ -53080,7 +53122,7 @@
     </row>
     <row r="1529" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1529" s="12"/>
-      <c r="B1529" s="9"/>
+      <c r="B1529" s="12"/>
       <c r="C1529" s="14"/>
       <c r="D1529" s="10"/>
       <c r="E1529" s="11"/>
@@ -53091,64 +53133,54 @@
       <c r="J1529" s="13"/>
     </row>
     <row r="1530" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1530" s="1" t="s">
+      <c r="A1530" s="12"/>
+      <c r="B1530" s="9"/>
+      <c r="C1530" s="14"/>
+      <c r="D1530" s="10"/>
+      <c r="E1530" s="11"/>
+      <c r="F1530" s="10"/>
+      <c r="G1530" s="11"/>
+      <c r="H1530" s="12"/>
+      <c r="I1530" s="13"/>
+      <c r="J1530" s="13"/>
+    </row>
+    <row r="1531" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1531" s="1" t="s">
         <v>1479</v>
       </c>
-      <c r="B1530" s="2" t="s">
+      <c r="B1531" s="2" t="s">
         <v>1480</v>
       </c>
-      <c r="C1530" s="3" t="s">
+      <c r="C1531" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1530" s="3" t="s">
+      <c r="D1531" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1530" s="3" t="s">
+      <c r="E1531" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="F1530" s="4" t="s">
+      <c r="F1531" s="4" t="s">
         <v>1579</v>
       </c>
-      <c r="G1530" s="5" t="s">
+      <c r="G1531" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H1530" s="6" t="s">
+      <c r="H1531" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I1530" s="7" t="s">
+      <c r="I1531" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1530" s="36"/>
-    </row>
-    <row r="1531" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1531" s="12"/>
-      <c r="B1531" s="9"/>
-      <c r="C1531" s="14"/>
-      <c r="D1531" s="10"/>
-      <c r="E1531" s="11"/>
-      <c r="F1531" s="10"/>
-      <c r="G1531" s="11"/>
-      <c r="H1531" s="12"/>
-      <c r="I1531" s="13"/>
-      <c r="J1531" s="13"/>
+      <c r="J1531" s="36"/>
     </row>
     <row r="1532" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1532" s="12"/>
-      <c r="B1532" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1532" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1532" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1532" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1532" s="10" t="s">
-        <v>1614</v>
-      </c>
+      <c r="B1532" s="9"/>
+      <c r="C1532" s="14"/>
+      <c r="D1532" s="10"/>
+      <c r="E1532" s="11"/>
+      <c r="F1532" s="10"/>
       <c r="G1532" s="11"/>
       <c r="H1532" s="12"/>
       <c r="I1532" s="13"/>
@@ -53169,7 +53201,7 @@
         <v>647</v>
       </c>
       <c r="F1533" s="10" t="s">
-        <v>1606</v>
+        <v>1614</v>
       </c>
       <c r="G1533" s="11"/>
       <c r="H1533" s="12"/>
@@ -53191,7 +53223,7 @@
         <v>647</v>
       </c>
       <c r="F1534" s="10" t="s">
-        <v>1611</v>
+        <v>1606</v>
       </c>
       <c r="G1534" s="11"/>
       <c r="H1534" s="12"/>
@@ -53213,7 +53245,7 @@
         <v>647</v>
       </c>
       <c r="F1535" s="10" t="s">
-        <v>1607</v>
+        <v>1611</v>
       </c>
       <c r="G1535" s="11"/>
       <c r="H1535" s="12"/>
@@ -53222,7 +53254,9 @@
     </row>
     <row r="1536" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1536" s="12"/>
-      <c r="B1536" s="9"/>
+      <c r="B1536" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1536" s="14" t="s">
         <v>13</v>
       </c>
@@ -53233,7 +53267,7 @@
         <v>647</v>
       </c>
       <c r="F1536" s="10" t="s">
-        <v>1615</v>
+        <v>1607</v>
       </c>
       <c r="G1536" s="11"/>
       <c r="H1536" s="12"/>
@@ -53242,9 +53276,7 @@
     </row>
     <row r="1537" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1537" s="12"/>
-      <c r="B1537" s="12">
-        <v>44402</v>
-      </c>
+      <c r="B1537" s="9"/>
       <c r="C1537" s="14" t="s">
         <v>13</v>
       </c>
@@ -53255,7 +53287,7 @@
         <v>647</v>
       </c>
       <c r="F1537" s="10" t="s">
-        <v>1608</v>
+        <v>1615</v>
       </c>
       <c r="G1537" s="11"/>
       <c r="H1537" s="12"/>
@@ -53264,7 +53296,9 @@
     </row>
     <row r="1538" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1538" s="12"/>
-      <c r="B1538" s="9"/>
+      <c r="B1538" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1538" s="14" t="s">
         <v>13</v>
       </c>
@@ -53275,7 +53309,7 @@
         <v>647</v>
       </c>
       <c r="F1538" s="10" t="s">
-        <v>1605</v>
+        <v>1608</v>
       </c>
       <c r="G1538" s="11"/>
       <c r="H1538" s="12"/>
@@ -53284,9 +53318,7 @@
     </row>
     <row r="1539" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1539" s="12"/>
-      <c r="B1539" s="12">
-        <v>44402</v>
-      </c>
+      <c r="B1539" s="9"/>
       <c r="C1539" s="14" t="s">
         <v>13</v>
       </c>
@@ -53297,7 +53329,7 @@
         <v>647</v>
       </c>
       <c r="F1539" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
       <c r="G1539" s="11"/>
       <c r="H1539" s="12"/>
@@ -53319,7 +53351,7 @@
         <v>647</v>
       </c>
       <c r="F1540" s="10" t="s">
-        <v>1609</v>
+        <v>1604</v>
       </c>
       <c r="G1540" s="11"/>
       <c r="H1540" s="12"/>
@@ -53341,7 +53373,7 @@
         <v>647</v>
       </c>
       <c r="F1541" s="10" t="s">
-        <v>1612</v>
+        <v>1609</v>
       </c>
       <c r="G1541" s="11"/>
       <c r="H1541" s="12"/>
@@ -53350,8 +53382,8 @@
     </row>
     <row r="1542" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1542" s="12"/>
-      <c r="B1542" s="9">
-        <v>44235</v>
+      <c r="B1542" s="12">
+        <v>44402</v>
       </c>
       <c r="C1542" s="14" t="s">
         <v>13</v>
@@ -53363,7 +53395,7 @@
         <v>647</v>
       </c>
       <c r="F1542" s="10" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="G1542" s="11"/>
       <c r="H1542" s="12"/>
@@ -53372,7 +53404,9 @@
     </row>
     <row r="1543" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1543" s="12"/>
-      <c r="B1543" s="9"/>
+      <c r="B1543" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1543" s="14" t="s">
         <v>13</v>
       </c>
@@ -53383,7 +53417,7 @@
         <v>647</v>
       </c>
       <c r="F1543" s="10" t="s">
-        <v>1610</v>
+        <v>1613</v>
       </c>
       <c r="G1543" s="11"/>
       <c r="H1543" s="12"/>
@@ -53403,7 +53437,7 @@
         <v>647</v>
       </c>
       <c r="F1544" s="10" t="s">
-        <v>1581</v>
+        <v>1610</v>
       </c>
       <c r="G1544" s="11"/>
       <c r="H1544" s="12"/>
@@ -53413,62 +53447,58 @@
     <row r="1545" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1545" s="12"/>
       <c r="B1545" s="9"/>
-      <c r="C1545" s="14"/>
-      <c r="D1545" s="10"/>
-      <c r="E1545" s="11"/>
-      <c r="F1545" s="10"/>
+      <c r="C1545" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1545" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1545" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1545" s="10" t="s">
+        <v>1581</v>
+      </c>
       <c r="G1545" s="11"/>
       <c r="H1545" s="12"/>
       <c r="I1545" s="13"/>
       <c r="J1545" s="13"/>
     </row>
     <row r="1546" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1546" s="12">
-        <v>44176</v>
-      </c>
+      <c r="A1546" s="12"/>
       <c r="B1546" s="9"/>
-      <c r="C1546" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1546" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1546" s="11" t="s">
-        <v>1353</v>
-      </c>
-      <c r="F1546" s="10" t="s">
-        <v>1354</v>
-      </c>
+      <c r="C1546" s="14"/>
+      <c r="D1546" s="10"/>
+      <c r="E1546" s="11"/>
+      <c r="F1546" s="10"/>
       <c r="G1546" s="11"/>
       <c r="H1546" s="12"/>
       <c r="I1546" s="13"/>
       <c r="J1546" s="13"/>
     </row>
-    <row r="1547" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="1547" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1547" s="12">
-        <v>44252</v>
+        <v>44176</v>
       </c>
       <c r="B1547" s="9"/>
       <c r="C1547" s="14" t="s">
-        <v>898</v>
+        <v>8</v>
       </c>
       <c r="D1547" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1547" s="11" t="s">
-        <v>759</v>
+        <v>1353</v>
       </c>
       <c r="F1547" s="10" t="s">
-        <v>1659</v>
+        <v>1354</v>
       </c>
       <c r="G1547" s="11"/>
       <c r="H1547" s="12"/>
       <c r="I1547" s="13"/>
-      <c r="J1547" s="13" t="s">
-        <v>1682</v>
-      </c>
-    </row>
-    <row r="1548" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1547" s="13"/>
+    </row>
+    <row r="1548" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1548" s="12">
         <v>44252</v>
       </c>
@@ -53483,29 +53513,31 @@
         <v>759</v>
       </c>
       <c r="F1548" s="10" t="s">
-        <v>1658</v>
+        <v>1659</v>
       </c>
       <c r="G1548" s="11"/>
       <c r="H1548" s="12"/>
       <c r="I1548" s="13"/>
-      <c r="J1548" s="13"/>
-    </row>
-    <row r="1549" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1548" s="13" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="1549" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1549" s="12">
-        <v>44112</v>
+        <v>44252</v>
       </c>
       <c r="B1549" s="9"/>
       <c r="C1549" s="14" t="s">
-        <v>623</v>
+        <v>898</v>
       </c>
       <c r="D1549" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1549" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1549" s="10" t="s">
-        <v>1097</v>
+        <v>1658</v>
       </c>
       <c r="G1549" s="11"/>
       <c r="H1549" s="12"/>
@@ -53514,20 +53546,20 @@
     </row>
     <row r="1550" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1550" s="12">
-        <v>44088</v>
+        <v>44112</v>
       </c>
       <c r="B1550" s="9"/>
       <c r="C1550" s="14" t="s">
-        <v>19</v>
+        <v>623</v>
       </c>
       <c r="D1550" s="10" t="s">
-        <v>906</v>
+        <v>6</v>
       </c>
       <c r="E1550" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1550" s="10" t="s">
-        <v>1011</v>
+        <v>1097</v>
       </c>
       <c r="G1550" s="11"/>
       <c r="H1550" s="12"/>
@@ -53536,20 +53568,20 @@
     </row>
     <row r="1551" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1551" s="12">
-        <v>44055</v>
+        <v>44088</v>
       </c>
       <c r="B1551" s="9"/>
       <c r="C1551" s="14" t="s">
-        <v>623</v>
+        <v>19</v>
       </c>
       <c r="D1551" s="10" t="s">
-        <v>6</v>
+        <v>906</v>
       </c>
       <c r="E1551" s="11" t="s">
-        <v>570</v>
+        <v>685</v>
       </c>
       <c r="F1551" s="10" t="s">
-        <v>903</v>
+        <v>1011</v>
       </c>
       <c r="G1551" s="11"/>
       <c r="H1551" s="12"/>
@@ -53571,7 +53603,7 @@
         <v>570</v>
       </c>
       <c r="F1552" s="10" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="G1552" s="11"/>
       <c r="H1552" s="12"/>
@@ -53584,23 +53616,23 @@
       </c>
       <c r="B1553" s="9"/>
       <c r="C1553" s="14" t="s">
-        <v>898</v>
+        <v>623</v>
       </c>
       <c r="D1553" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1553" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1553" s="10" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="G1553" s="11"/>
       <c r="H1553" s="12"/>
       <c r="I1553" s="13"/>
       <c r="J1553" s="13"/>
     </row>
-    <row r="1554" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="1554" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1554" s="12">
         <v>44055</v>
       </c>
@@ -53615,14 +53647,14 @@
         <v>570</v>
       </c>
       <c r="F1554" s="10" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="G1554" s="11"/>
       <c r="H1554" s="12"/>
       <c r="I1554" s="13"/>
       <c r="J1554" s="13"/>
     </row>
-    <row r="1555" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1555" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A1555" s="12">
         <v>44055</v>
       </c>
@@ -53637,63 +53669,59 @@
         <v>570</v>
       </c>
       <c r="F1555" s="10" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="G1555" s="11"/>
       <c r="H1555" s="12"/>
       <c r="I1555" s="13"/>
-      <c r="J1555" s="13" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="1556" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1555" s="13"/>
+    </row>
+    <row r="1556" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1556" s="12">
-        <v>44047</v>
+        <v>44055</v>
       </c>
       <c r="B1556" s="9"/>
       <c r="C1556" s="14" t="s">
-        <v>537</v>
+        <v>898</v>
       </c>
       <c r="D1556" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1556" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1556" s="10" t="s">
-        <v>873</v>
-      </c>
-      <c r="G1556" s="11" t="s">
-        <v>1624</v>
-      </c>
+        <v>904</v>
+      </c>
+      <c r="G1556" s="11"/>
       <c r="H1556" s="12"/>
       <c r="I1556" s="13"/>
-      <c r="J1556" s="13"/>
-    </row>
-    <row r="1557" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="J1556" s="13" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="1557" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1557" s="12">
-        <v>43949</v>
+        <v>44047</v>
       </c>
       <c r="B1557" s="9"/>
       <c r="C1557" s="14" t="s">
-        <v>468</v>
+        <v>537</v>
       </c>
       <c r="D1557" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1557" s="11" t="s">
         <v>685</v>
       </c>
       <c r="F1557" s="10" t="s">
-        <v>686</v>
+        <v>873</v>
       </c>
       <c r="G1557" s="11" t="s">
-        <v>1639</v>
+        <v>1624</v>
       </c>
       <c r="H1557" s="12"/>
-      <c r="I1557" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1557" s="13"/>
       <c r="J1557" s="13"/>
     </row>
     <row r="1558" spans="1:10" ht="168" x14ac:dyDescent="0.2">
@@ -53711,103 +53739,117 @@
         <v>685</v>
       </c>
       <c r="F1558" s="10" t="s">
-        <v>705</v>
+        <v>686</v>
       </c>
       <c r="G1558" s="11" t="s">
-        <v>687</v>
+        <v>1639</v>
       </c>
       <c r="H1558" s="12"/>
       <c r="I1558" s="13" t="s">
         <v>284</v>
       </c>
-      <c r="J1558" s="13" t="s">
-        <v>1568</v>
-      </c>
-    </row>
-    <row r="1559" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1558" s="13"/>
+    </row>
+    <row r="1559" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A1559" s="12">
-        <v>43838</v>
+        <v>43949</v>
       </c>
       <c r="B1559" s="9"/>
       <c r="C1559" s="14" t="s">
-        <v>103</v>
+        <v>468</v>
       </c>
       <c r="D1559" s="10" t="s">
-        <v>460</v>
+        <v>89</v>
       </c>
       <c r="E1559" s="11" t="s">
-        <v>647</v>
+        <v>685</v>
       </c>
       <c r="F1559" s="10" t="s">
-        <v>481</v>
+        <v>705</v>
       </c>
       <c r="G1559" s="11" t="s">
-        <v>1640</v>
+        <v>687</v>
       </c>
       <c r="H1559" s="12"/>
-      <c r="I1559" s="13"/>
+      <c r="I1559" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1559" s="13" t="s">
-        <v>1533</v>
-      </c>
-    </row>
-    <row r="1560" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1560" s="12">
-        <v>43816</v>
+        <v>43838</v>
       </c>
       <c r="B1560" s="9"/>
       <c r="C1560" s="14" t="s">
-        <v>475</v>
+        <v>103</v>
       </c>
       <c r="D1560" s="10" t="s">
-        <v>38</v>
+        <v>460</v>
       </c>
       <c r="E1560" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1560" s="10" t="s">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="G1560" s="11" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
       <c r="H1560" s="12"/>
       <c r="I1560" s="13"/>
       <c r="J1560" s="13" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="1561" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1561" s="12">
-        <v>43762</v>
+        <v>43816</v>
       </c>
       <c r="B1561" s="9"/>
       <c r="C1561" s="14" t="s">
-        <v>446</v>
+        <v>475</v>
       </c>
       <c r="D1561" s="10" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="E1561" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1561" s="10" t="s">
-        <v>447</v>
+        <v>474</v>
       </c>
       <c r="G1561" s="11" t="s">
-        <v>1629</v>
+        <v>1632</v>
       </c>
       <c r="H1561" s="12"/>
       <c r="I1561" s="13"/>
-      <c r="J1561" s="13"/>
-    </row>
-    <row r="1562" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1562" s="12"/>
+      <c r="J1561" s="13" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1562" s="12">
+        <v>43762</v>
+      </c>
       <c r="B1562" s="9"/>
-      <c r="C1562" s="14"/>
-      <c r="D1562" s="10"/>
-      <c r="E1562" s="11"/>
-      <c r="F1562" s="10"/>
-      <c r="G1562" s="11"/>
+      <c r="C1562" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1562" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1562" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1562" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1562" s="11" t="s">
+        <v>1629</v>
+      </c>
       <c r="H1562" s="12"/>
       <c r="I1562" s="13"/>
       <c r="J1562" s="13"/>
@@ -53872,10 +53914,22 @@
       <c r="I1567" s="13"/>
       <c r="J1567" s="13"/>
     </row>
+    <row r="1568" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1568" s="12"/>
+      <c r="B1568" s="9"/>
+      <c r="C1568" s="14"/>
+      <c r="D1568" s="10"/>
+      <c r="E1568" s="11"/>
+      <c r="F1568" s="10"/>
+      <c r="G1568" s="11"/>
+      <c r="H1568" s="12"/>
+      <c r="I1568" s="13"/>
+      <c r="J1568" s="13"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1480" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1533:F1543">
-    <sortCondition ref="F1533:F1543"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1534:F1544">
+    <sortCondition ref="F1534:F1544"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Substituição do ConOut por xxConOut
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06370A18-10EF-4E7E-8EE5-356B084185D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA478A90-BE0C-4CB4-B39B-22D3B4F3455E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10815" uniqueCount="2196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10829" uniqueCount="2197">
   <si>
     <t>Responsável</t>
   </si>
@@ -6970,6 +6970,9 @@
   </si>
   <si>
     <t>Ponto de Entrada MS520VLD()</t>
+  </si>
+  <si>
+    <t>Migração 12.1.27 Correção de 230 avisos de erros em programas</t>
   </si>
 </sst>
 </file>
@@ -7738,11 +7741,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1570"/>
+  <dimension ref="A1:J1573"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1514" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1524" sqref="A1524"/>
+      <pane ySplit="1" topLeftCell="A1517" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1525" sqref="F1525"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -53160,128 +53163,164 @@
       </c>
     </row>
     <row r="1524" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1524" s="12"/>
-      <c r="B1524" s="12"/>
-      <c r="C1524" s="14"/>
-      <c r="D1524" s="10"/>
-      <c r="E1524" s="11"/>
-      <c r="F1524" s="10"/>
-      <c r="G1524" s="11"/>
-      <c r="H1524" s="12"/>
-      <c r="I1524" s="13"/>
+      <c r="A1524" s="12">
+        <v>44459</v>
+      </c>
+      <c r="B1524" s="12">
+        <v>44459</v>
+      </c>
+      <c r="C1524" s="14" t="s">
+        <v>2019</v>
+      </c>
+      <c r="D1524" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1524" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1524" s="10" t="s">
+        <v>2193</v>
+      </c>
+      <c r="G1524" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1524" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1524" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1524" s="13"/>
     </row>
     <row r="1525" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1525" s="12"/>
-      <c r="B1525" s="12"/>
-      <c r="C1525" s="14"/>
-      <c r="D1525" s="10"/>
-      <c r="E1525" s="11"/>
-      <c r="F1525" s="10"/>
-      <c r="G1525" s="11"/>
-      <c r="H1525" s="12"/>
-      <c r="I1525" s="13"/>
+      <c r="A1525" s="12">
+        <v>44459</v>
+      </c>
+      <c r="B1525" s="12">
+        <v>44459</v>
+      </c>
+      <c r="C1525" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1525" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1525" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1525" s="10" t="s">
+        <v>2196</v>
+      </c>
+      <c r="G1525" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H1525" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1525" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1525" s="13"/>
     </row>
-    <row r="1526" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1526" s="12">
-        <v>44403</v>
-      </c>
+    <row r="1526" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1526" s="12"/>
       <c r="B1526" s="12"/>
-      <c r="C1526" s="14" t="s">
-        <v>1477</v>
-      </c>
-      <c r="D1526" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1526" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1526" s="10" t="s">
-        <v>2131</v>
-      </c>
+      <c r="C1526" s="14"/>
+      <c r="D1526" s="10"/>
+      <c r="E1526" s="11"/>
+      <c r="F1526" s="10"/>
       <c r="G1526" s="11"/>
       <c r="H1526" s="12"/>
       <c r="I1526" s="13"/>
       <c r="J1526" s="13"/>
     </row>
-    <row r="1527" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A1527" s="12">
-        <v>44266</v>
-      </c>
-      <c r="B1527" s="9"/>
-      <c r="C1527" s="14" t="s">
-        <v>537</v>
-      </c>
-      <c r="D1527" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1527" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1527" s="10" t="s">
-        <v>1713</v>
-      </c>
+    <row r="1527" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1527" s="12"/>
+      <c r="B1527" s="12"/>
+      <c r="C1527" s="14"/>
+      <c r="D1527" s="10"/>
+      <c r="E1527" s="11"/>
+      <c r="F1527" s="10"/>
       <c r="G1527" s="11"/>
       <c r="H1527" s="12"/>
       <c r="I1527" s="13"/>
-      <c r="J1527" s="13" t="s">
-        <v>1714</v>
-      </c>
-    </row>
-    <row r="1528" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1528" s="12">
-        <v>44286</v>
-      </c>
-      <c r="B1528" s="9"/>
-      <c r="C1528" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D1528" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1528" s="11" t="s">
-        <v>620</v>
-      </c>
-      <c r="F1528" s="10" t="s">
-        <v>1838</v>
-      </c>
+      <c r="J1527" s="13"/>
+    </row>
+    <row r="1528" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1528" s="12"/>
+      <c r="B1528" s="12"/>
+      <c r="C1528" s="14"/>
+      <c r="D1528" s="10"/>
+      <c r="E1528" s="11"/>
+      <c r="F1528" s="10"/>
       <c r="G1528" s="11"/>
       <c r="H1528" s="12"/>
       <c r="I1528" s="13"/>
       <c r="J1528" s="13"/>
     </row>
-    <row r="1529" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1529" s="12"/>
+    <row r="1529" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1529" s="12">
+        <v>44403</v>
+      </c>
       <c r="B1529" s="12"/>
-      <c r="C1529" s="14"/>
-      <c r="D1529" s="10"/>
-      <c r="E1529" s="11"/>
-      <c r="F1529" s="10"/>
+      <c r="C1529" s="14" t="s">
+        <v>1477</v>
+      </c>
+      <c r="D1529" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1529" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1529" s="10" t="s">
+        <v>2131</v>
+      </c>
       <c r="G1529" s="11"/>
       <c r="H1529" s="12"/>
       <c r="I1529" s="13"/>
       <c r="J1529" s="13"/>
     </row>
-    <row r="1530" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1530" s="12"/>
-      <c r="B1530" s="12"/>
-      <c r="C1530" s="14"/>
-      <c r="D1530" s="10"/>
-      <c r="E1530" s="11"/>
-      <c r="F1530" s="10"/>
+    <row r="1530" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1530" s="12">
+        <v>44266</v>
+      </c>
+      <c r="B1530" s="9"/>
+      <c r="C1530" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1530" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1530" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1530" s="10" t="s">
+        <v>1713</v>
+      </c>
       <c r="G1530" s="11"/>
       <c r="H1530" s="12"/>
       <c r="I1530" s="13"/>
-      <c r="J1530" s="13"/>
-    </row>
-    <row r="1531" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1531" s="12"/>
-      <c r="B1531" s="12"/>
-      <c r="C1531" s="14"/>
-      <c r="D1531" s="10"/>
-      <c r="E1531" s="11"/>
-      <c r="F1531" s="10"/>
+      <c r="J1530" s="13" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="1531" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1531" s="12">
+        <v>44286</v>
+      </c>
+      <c r="B1531" s="9"/>
+      <c r="C1531" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1531" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1531" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1531" s="10" t="s">
+        <v>1838</v>
+      </c>
       <c r="G1531" s="11"/>
       <c r="H1531" s="12"/>
       <c r="I1531" s="13"/>
@@ -53289,7 +53328,7 @@
     </row>
     <row r="1532" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1532" s="12"/>
-      <c r="B1532" s="9"/>
+      <c r="B1532" s="12"/>
       <c r="C1532" s="14"/>
       <c r="D1532" s="10"/>
       <c r="E1532" s="11"/>
@@ -53300,38 +53339,20 @@
       <c r="J1532" s="13"/>
     </row>
     <row r="1533" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1533" s="1" t="s">
-        <v>1479</v>
-      </c>
-      <c r="B1533" s="2" t="s">
-        <v>1480</v>
-      </c>
-      <c r="C1533" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1533" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1533" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1533" s="4" t="s">
-        <v>1579</v>
-      </c>
-      <c r="G1533" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1533" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1533" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1533" s="36"/>
+      <c r="A1533" s="12"/>
+      <c r="B1533" s="12"/>
+      <c r="C1533" s="14"/>
+      <c r="D1533" s="10"/>
+      <c r="E1533" s="11"/>
+      <c r="F1533" s="10"/>
+      <c r="G1533" s="11"/>
+      <c r="H1533" s="12"/>
+      <c r="I1533" s="13"/>
+      <c r="J1533" s="13"/>
     </row>
     <row r="1534" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1534" s="12"/>
-      <c r="B1534" s="9"/>
+      <c r="B1534" s="12"/>
       <c r="C1534" s="14"/>
       <c r="D1534" s="10"/>
       <c r="E1534" s="11"/>
@@ -53343,65 +53364,53 @@
     </row>
     <row r="1535" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1535" s="12"/>
-      <c r="B1535" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1535" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1535" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1535" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1535" s="10" t="s">
-        <v>1614</v>
-      </c>
+      <c r="B1535" s="9"/>
+      <c r="C1535" s="14"/>
+      <c r="D1535" s="10"/>
+      <c r="E1535" s="11"/>
+      <c r="F1535" s="10"/>
       <c r="G1535" s="11"/>
       <c r="H1535" s="12"/>
       <c r="I1535" s="13"/>
       <c r="J1535" s="13"/>
     </row>
     <row r="1536" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1536" s="12"/>
-      <c r="B1536" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1536" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1536" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1536" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1536" s="10" t="s">
-        <v>1606</v>
-      </c>
-      <c r="G1536" s="11"/>
-      <c r="H1536" s="12"/>
-      <c r="I1536" s="13"/>
-      <c r="J1536" s="13"/>
+      <c r="A1536" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B1536" s="2" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C1536" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1536" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1536" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1536" s="4" t="s">
+        <v>1579</v>
+      </c>
+      <c r="G1536" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1536" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1536" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1536" s="36"/>
     </row>
     <row r="1537" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1537" s="12"/>
-      <c r="B1537" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1537" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1537" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1537" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1537" s="10" t="s">
-        <v>1611</v>
-      </c>
+      <c r="B1537" s="9"/>
+      <c r="C1537" s="14"/>
+      <c r="D1537" s="10"/>
+      <c r="E1537" s="11"/>
+      <c r="F1537" s="10"/>
       <c r="G1537" s="11"/>
       <c r="H1537" s="12"/>
       <c r="I1537" s="13"/>
@@ -53422,7 +53431,7 @@
         <v>647</v>
       </c>
       <c r="F1538" s="10" t="s">
-        <v>1607</v>
+        <v>1614</v>
       </c>
       <c r="G1538" s="11"/>
       <c r="H1538" s="12"/>
@@ -53431,7 +53440,9 @@
     </row>
     <row r="1539" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1539" s="12"/>
-      <c r="B1539" s="9"/>
+      <c r="B1539" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1539" s="14" t="s">
         <v>13</v>
       </c>
@@ -53442,7 +53453,7 @@
         <v>647</v>
       </c>
       <c r="F1539" s="10" t="s">
-        <v>1615</v>
+        <v>1606</v>
       </c>
       <c r="G1539" s="11"/>
       <c r="H1539" s="12"/>
@@ -53464,7 +53475,7 @@
         <v>647</v>
       </c>
       <c r="F1540" s="10" t="s">
-        <v>1608</v>
+        <v>1611</v>
       </c>
       <c r="G1540" s="11"/>
       <c r="H1540" s="12"/>
@@ -53473,7 +53484,9 @@
     </row>
     <row r="1541" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1541" s="12"/>
-      <c r="B1541" s="9"/>
+      <c r="B1541" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1541" s="14" t="s">
         <v>13</v>
       </c>
@@ -53484,7 +53497,7 @@
         <v>647</v>
       </c>
       <c r="F1541" s="10" t="s">
-        <v>1605</v>
+        <v>1607</v>
       </c>
       <c r="G1541" s="11"/>
       <c r="H1541" s="12"/>
@@ -53493,9 +53506,7 @@
     </row>
     <row r="1542" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1542" s="12"/>
-      <c r="B1542" s="12">
-        <v>44402</v>
-      </c>
+      <c r="B1542" s="9"/>
       <c r="C1542" s="14" t="s">
         <v>13</v>
       </c>
@@ -53506,7 +53517,7 @@
         <v>647</v>
       </c>
       <c r="F1542" s="10" t="s">
-        <v>1604</v>
+        <v>1615</v>
       </c>
       <c r="G1542" s="11"/>
       <c r="H1542" s="12"/>
@@ -53528,7 +53539,7 @@
         <v>647</v>
       </c>
       <c r="F1543" s="10" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="G1543" s="11"/>
       <c r="H1543" s="12"/>
@@ -53537,9 +53548,7 @@
     </row>
     <row r="1544" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1544" s="12"/>
-      <c r="B1544" s="12">
-        <v>44402</v>
-      </c>
+      <c r="B1544" s="9"/>
       <c r="C1544" s="14" t="s">
         <v>13</v>
       </c>
@@ -53550,7 +53559,7 @@
         <v>647</v>
       </c>
       <c r="F1544" s="10" t="s">
-        <v>1612</v>
+        <v>1605</v>
       </c>
       <c r="G1544" s="11"/>
       <c r="H1544" s="12"/>
@@ -53559,8 +53568,8 @@
     </row>
     <row r="1545" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1545" s="12"/>
-      <c r="B1545" s="9">
-        <v>44235</v>
+      <c r="B1545" s="12">
+        <v>44402</v>
       </c>
       <c r="C1545" s="14" t="s">
         <v>13</v>
@@ -53572,7 +53581,7 @@
         <v>647</v>
       </c>
       <c r="F1545" s="10" t="s">
-        <v>1613</v>
+        <v>1604</v>
       </c>
       <c r="G1545" s="11"/>
       <c r="H1545" s="12"/>
@@ -53581,7 +53590,9 @@
     </row>
     <row r="1546" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1546" s="12"/>
-      <c r="B1546" s="9"/>
+      <c r="B1546" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1546" s="14" t="s">
         <v>13</v>
       </c>
@@ -53592,7 +53603,7 @@
         <v>647</v>
       </c>
       <c r="F1546" s="10" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="G1546" s="11"/>
       <c r="H1546" s="12"/>
@@ -53601,7 +53612,9 @@
     </row>
     <row r="1547" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1547" s="12"/>
-      <c r="B1547" s="9"/>
+      <c r="B1547" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1547" s="14" t="s">
         <v>13</v>
       </c>
@@ -53612,7 +53625,7 @@
         <v>647</v>
       </c>
       <c r="F1547" s="10" t="s">
-        <v>1581</v>
+        <v>1612</v>
       </c>
       <c r="G1547" s="11"/>
       <c r="H1547" s="12"/>
@@ -53621,79 +53634,73 @@
     </row>
     <row r="1548" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1548" s="12"/>
-      <c r="B1548" s="9"/>
-      <c r="C1548" s="14"/>
-      <c r="D1548" s="10"/>
-      <c r="E1548" s="11"/>
-      <c r="F1548" s="10"/>
+      <c r="B1548" s="9">
+        <v>44235</v>
+      </c>
+      <c r="C1548" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1548" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1548" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1548" s="10" t="s">
+        <v>1613</v>
+      </c>
       <c r="G1548" s="11"/>
       <c r="H1548" s="12"/>
       <c r="I1548" s="13"/>
       <c r="J1548" s="13"/>
     </row>
     <row r="1549" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1549" s="12">
-        <v>44176</v>
-      </c>
+      <c r="A1549" s="12"/>
       <c r="B1549" s="9"/>
       <c r="C1549" s="14" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D1549" s="10" t="s">
         <v>584</v>
       </c>
       <c r="E1549" s="11" t="s">
-        <v>1353</v>
+        <v>647</v>
       </c>
       <c r="F1549" s="10" t="s">
-        <v>1354</v>
+        <v>1610</v>
       </c>
       <c r="G1549" s="11"/>
       <c r="H1549" s="12"/>
       <c r="I1549" s="13"/>
       <c r="J1549" s="13"/>
     </row>
-    <row r="1550" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1550" s="12">
-        <v>44252</v>
-      </c>
+    <row r="1550" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1550" s="12"/>
       <c r="B1550" s="9"/>
       <c r="C1550" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1550" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1550" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1550" s="10" t="s">
-        <v>1659</v>
+        <v>1581</v>
       </c>
       <c r="G1550" s="11"/>
       <c r="H1550" s="12"/>
       <c r="I1550" s="13"/>
-      <c r="J1550" s="13" t="s">
-        <v>1682</v>
-      </c>
-    </row>
-    <row r="1551" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1551" s="12">
-        <v>44252</v>
-      </c>
+      <c r="J1550" s="13"/>
+    </row>
+    <row r="1551" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1551" s="12"/>
       <c r="B1551" s="9"/>
-      <c r="C1551" s="14" t="s">
-        <v>898</v>
-      </c>
-      <c r="D1551" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="E1551" s="11" t="s">
-        <v>759</v>
-      </c>
-      <c r="F1551" s="10" t="s">
-        <v>1658</v>
-      </c>
+      <c r="C1551" s="14"/>
+      <c r="D1551" s="10"/>
+      <c r="E1551" s="11"/>
+      <c r="F1551" s="10"/>
       <c r="G1551" s="11"/>
       <c r="H1551" s="12"/>
       <c r="I1551" s="13"/>
@@ -53701,64 +53708,66 @@
     </row>
     <row r="1552" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1552" s="12">
-        <v>44112</v>
+        <v>44176</v>
       </c>
       <c r="B1552" s="9"/>
       <c r="C1552" s="14" t="s">
-        <v>623</v>
+        <v>8</v>
       </c>
       <c r="D1552" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1552" s="11" t="s">
-        <v>570</v>
+        <v>1353</v>
       </c>
       <c r="F1552" s="10" t="s">
-        <v>1097</v>
+        <v>1354</v>
       </c>
       <c r="G1552" s="11"/>
       <c r="H1552" s="12"/>
       <c r="I1552" s="13"/>
       <c r="J1552" s="13"/>
     </row>
-    <row r="1553" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1553" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1553" s="12">
-        <v>44088</v>
+        <v>44252</v>
       </c>
       <c r="B1553" s="9"/>
       <c r="C1553" s="14" t="s">
-        <v>19</v>
+        <v>898</v>
       </c>
       <c r="D1553" s="10" t="s">
-        <v>906</v>
+        <v>494</v>
       </c>
       <c r="E1553" s="11" t="s">
-        <v>685</v>
+        <v>759</v>
       </c>
       <c r="F1553" s="10" t="s">
-        <v>1011</v>
+        <v>1659</v>
       </c>
       <c r="G1553" s="11"/>
       <c r="H1553" s="12"/>
       <c r="I1553" s="13"/>
-      <c r="J1553" s="13"/>
-    </row>
-    <row r="1554" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1553" s="13" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="1554" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1554" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1554" s="9"/>
       <c r="C1554" s="14" t="s">
-        <v>623</v>
+        <v>898</v>
       </c>
       <c r="D1554" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1554" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1554" s="10" t="s">
-        <v>903</v>
+        <v>1658</v>
       </c>
       <c r="G1554" s="11"/>
       <c r="H1554" s="12"/>
@@ -53767,7 +53776,7 @@
     </row>
     <row r="1555" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1555" s="12">
-        <v>44055</v>
+        <v>44112</v>
       </c>
       <c r="B1555" s="9"/>
       <c r="C1555" s="14" t="s">
@@ -53780,7 +53789,7 @@
         <v>570</v>
       </c>
       <c r="F1555" s="10" t="s">
-        <v>902</v>
+        <v>1097</v>
       </c>
       <c r="G1555" s="11"/>
       <c r="H1555" s="12"/>
@@ -53789,258 +53798,288 @@
     </row>
     <row r="1556" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1556" s="12">
-        <v>44055</v>
+        <v>44088</v>
       </c>
       <c r="B1556" s="9"/>
       <c r="C1556" s="14" t="s">
-        <v>898</v>
+        <v>19</v>
       </c>
       <c r="D1556" s="10" t="s">
-        <v>494</v>
+        <v>906</v>
       </c>
       <c r="E1556" s="11" t="s">
-        <v>570</v>
+        <v>685</v>
       </c>
       <c r="F1556" s="10" t="s">
-        <v>900</v>
+        <v>1011</v>
       </c>
       <c r="G1556" s="11"/>
       <c r="H1556" s="12"/>
       <c r="I1556" s="13"/>
       <c r="J1556" s="13"/>
     </row>
-    <row r="1557" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="1557" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1557" s="12">
         <v>44055</v>
       </c>
       <c r="B1557" s="9"/>
       <c r="C1557" s="14" t="s">
-        <v>898</v>
+        <v>623</v>
       </c>
       <c r="D1557" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1557" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1557" s="10" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="G1557" s="11"/>
       <c r="H1557" s="12"/>
       <c r="I1557" s="13"/>
       <c r="J1557" s="13"/>
     </row>
-    <row r="1558" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1558" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1558" s="12">
         <v>44055</v>
       </c>
       <c r="B1558" s="9"/>
       <c r="C1558" s="14" t="s">
-        <v>898</v>
+        <v>623</v>
       </c>
       <c r="D1558" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1558" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1558" s="10" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="G1558" s="11"/>
       <c r="H1558" s="12"/>
       <c r="I1558" s="13"/>
-      <c r="J1558" s="13" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="1559" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="J1558" s="13"/>
+    </row>
+    <row r="1559" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1559" s="12">
-        <v>44047</v>
+        <v>44055</v>
       </c>
       <c r="B1559" s="9"/>
       <c r="C1559" s="14" t="s">
-        <v>537</v>
+        <v>898</v>
       </c>
       <c r="D1559" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1559" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1559" s="10" t="s">
-        <v>873</v>
-      </c>
-      <c r="G1559" s="11" t="s">
-        <v>1624</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="G1559" s="11"/>
       <c r="H1559" s="12"/>
       <c r="I1559" s="13"/>
       <c r="J1559" s="13"/>
     </row>
-    <row r="1560" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1560" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A1560" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1560" s="9"/>
       <c r="C1560" s="14" t="s">
-        <v>468</v>
+        <v>898</v>
       </c>
       <c r="D1560" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1560" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1560" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1560" s="11" t="s">
-        <v>1639</v>
-      </c>
+        <v>901</v>
+      </c>
+      <c r="G1560" s="11"/>
       <c r="H1560" s="12"/>
-      <c r="I1560" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1560" s="13"/>
       <c r="J1560" s="13"/>
     </row>
-    <row r="1561" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1561" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1561" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1561" s="9"/>
       <c r="C1561" s="14" t="s">
-        <v>468</v>
+        <v>898</v>
       </c>
       <c r="D1561" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1561" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1561" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1561" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>904</v>
+      </c>
+      <c r="G1561" s="11"/>
       <c r="H1561" s="12"/>
-      <c r="I1561" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1561" s="13"/>
       <c r="J1561" s="13" t="s">
-        <v>1568</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="1562" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1562" s="12">
-        <v>43838</v>
+        <v>44047</v>
       </c>
       <c r="B1562" s="9"/>
       <c r="C1562" s="14" t="s">
-        <v>103</v>
+        <v>537</v>
       </c>
       <c r="D1562" s="10" t="s">
-        <v>460</v>
+        <v>6</v>
       </c>
       <c r="E1562" s="11" t="s">
-        <v>647</v>
+        <v>685</v>
       </c>
       <c r="F1562" s="10" t="s">
-        <v>481</v>
+        <v>873</v>
       </c>
       <c r="G1562" s="11" t="s">
-        <v>1640</v>
+        <v>1624</v>
       </c>
       <c r="H1562" s="12"/>
       <c r="I1562" s="13"/>
-      <c r="J1562" s="13" t="s">
-        <v>1533</v>
-      </c>
-    </row>
-    <row r="1563" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1562" s="13"/>
+    </row>
+    <row r="1563" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A1563" s="12">
-        <v>43816</v>
+        <v>43949</v>
       </c>
       <c r="B1563" s="9"/>
       <c r="C1563" s="14" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="D1563" s="10" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="E1563" s="11" t="s">
-        <v>570</v>
+        <v>685</v>
       </c>
       <c r="F1563" s="10" t="s">
-        <v>474</v>
+        <v>686</v>
       </c>
       <c r="G1563" s="11" t="s">
-        <v>1632</v>
+        <v>1639</v>
       </c>
       <c r="H1563" s="12"/>
-      <c r="I1563" s="13"/>
-      <c r="J1563" s="13" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="1564" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="I1563" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1563" s="13"/>
+    </row>
+    <row r="1564" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A1564" s="12">
-        <v>43762</v>
+        <v>43949</v>
       </c>
       <c r="B1564" s="9"/>
       <c r="C1564" s="14" t="s">
-        <v>446</v>
+        <v>468</v>
       </c>
       <c r="D1564" s="10" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="E1564" s="11" t="s">
-        <v>837</v>
+        <v>685</v>
       </c>
       <c r="F1564" s="10" t="s">
-        <v>447</v>
+        <v>705</v>
       </c>
       <c r="G1564" s="11" t="s">
-        <v>1629</v>
+        <v>687</v>
       </c>
       <c r="H1564" s="12"/>
-      <c r="I1564" s="13"/>
-      <c r="J1564" s="13"/>
-    </row>
-    <row r="1565" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1565" s="12"/>
+      <c r="I1564" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1564" s="13" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="1565" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1565" s="12">
+        <v>43838</v>
+      </c>
       <c r="B1565" s="9"/>
-      <c r="C1565" s="14"/>
-      <c r="D1565" s="10"/>
-      <c r="E1565" s="11"/>
-      <c r="F1565" s="10"/>
-      <c r="G1565" s="11"/>
+      <c r="C1565" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1565" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1565" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1565" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G1565" s="11" t="s">
+        <v>1640</v>
+      </c>
       <c r="H1565" s="12"/>
       <c r="I1565" s="13"/>
-      <c r="J1565" s="13"/>
+      <c r="J1565" s="13" t="s">
+        <v>1533</v>
+      </c>
     </row>
     <row r="1566" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1566" s="12"/>
+      <c r="A1566" s="12">
+        <v>43816</v>
+      </c>
       <c r="B1566" s="9"/>
-      <c r="C1566" s="14"/>
-      <c r="D1566" s="10"/>
-      <c r="E1566" s="11"/>
-      <c r="F1566" s="10"/>
-      <c r="G1566" s="11"/>
+      <c r="C1566" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1566" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1566" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1566" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G1566" s="11" t="s">
+        <v>1632</v>
+      </c>
       <c r="H1566" s="12"/>
       <c r="I1566" s="13"/>
-      <c r="J1566" s="13"/>
-    </row>
-    <row r="1567" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1567" s="12"/>
+      <c r="J1566" s="13" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="1567" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1567" s="12">
+        <v>43762</v>
+      </c>
       <c r="B1567" s="9"/>
-      <c r="C1567" s="14"/>
-      <c r="D1567" s="10"/>
-      <c r="E1567" s="11"/>
-      <c r="F1567" s="10"/>
-      <c r="G1567" s="11"/>
+      <c r="C1567" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1567" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1567" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1567" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1567" s="11" t="s">
+        <v>1629</v>
+      </c>
       <c r="H1567" s="12"/>
       <c r="I1567" s="13"/>
       <c r="J1567" s="13"/>
@@ -54081,10 +54120,46 @@
       <c r="I1570" s="13"/>
       <c r="J1570" s="13"/>
     </row>
+    <row r="1571" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1571" s="12"/>
+      <c r="B1571" s="9"/>
+      <c r="C1571" s="14"/>
+      <c r="D1571" s="10"/>
+      <c r="E1571" s="11"/>
+      <c r="F1571" s="10"/>
+      <c r="G1571" s="11"/>
+      <c r="H1571" s="12"/>
+      <c r="I1571" s="13"/>
+      <c r="J1571" s="13"/>
+    </row>
+    <row r="1572" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1572" s="12"/>
+      <c r="B1572" s="9"/>
+      <c r="C1572" s="14"/>
+      <c r="D1572" s="10"/>
+      <c r="E1572" s="11"/>
+      <c r="F1572" s="10"/>
+      <c r="G1572" s="11"/>
+      <c r="H1572" s="12"/>
+      <c r="I1572" s="13"/>
+      <c r="J1572" s="13"/>
+    </row>
+    <row r="1573" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1573" s="12"/>
+      <c r="B1573" s="9"/>
+      <c r="C1573" s="14"/>
+      <c r="D1573" s="10"/>
+      <c r="E1573" s="11"/>
+      <c r="F1573" s="10"/>
+      <c r="G1573" s="11"/>
+      <c r="H1573" s="12"/>
+      <c r="I1573" s="13"/>
+      <c r="J1573" s="13"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1480" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1536:F1546">
-    <sortCondition ref="F1536:F1546"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1539:F1549">
+    <sortCondition ref="F1539:F1549"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Validação MEI / Aval Forn
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19425A3D-1981-4939-8CBD-D4B378F53AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC2760F-A498-4DBC-91D2-A4684AEF37A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10885" uniqueCount="2208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10953" uniqueCount="2222">
   <si>
     <t>Responsável</t>
   </si>
@@ -6981,9 +6981,6 @@
     <t>Bloquear tes com credito de Pis/Cofins para fornecedores do MEI (a2_tpj)</t>
   </si>
   <si>
-    <t>Contabilizar acrescimos financeiros D-(despesas Serv P PJ 34202009) C-Fornecedores</t>
-  </si>
-  <si>
     <t>Liberação de Documentos via WEB para a Diretoria</t>
   </si>
   <si>
@@ -7000,13 +6997,58 @@
 Ponto de Entrada: MT103NAT</t>
   </si>
   <si>
-    <t xml:space="preserve">Refazer lançamentos automaticos da baixa a pagar </t>
-  </si>
-  <si>
     <t>Verificar porque não aparecem avaliação de fornecedores</t>
   </si>
   <si>
     <t>Bloquear alteração de Natureza para fornecedores com bloqueio de Natureza preenchida, no Doc de Entrada</t>
+  </si>
+  <si>
+    <t>Implantar NF do Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>Opçao de filtro por Tipo Bk na impressão de titulos (BKGCTR06)</t>
+  </si>
+  <si>
+    <t>BKGCTR06</t>
+  </si>
+  <si>
+    <t>Incluir usuária Michele nas avaliações de Fornecedores</t>
+  </si>
+  <si>
+    <t>GQREENTR e MT103INC</t>
+  </si>
+  <si>
+    <t>Emissão do relatório de Rentabilidade Consorcios geral</t>
+  </si>
+  <si>
+    <t>Tabela de glosas não aparece com conteudo na empresa BKTER</t>
+  </si>
+  <si>
+    <t>Compartilhada a tabela SZR para todas as Empresas</t>
+  </si>
+  <si>
+    <t>Criado rdmake de validação BKVlTes</t>
+  </si>
+  <si>
+    <t>Quando do estorno de documento de entrada, mandar para o grupo todo o motivo do estorno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contabilizar acrescimos financeiros D-(despesas Serv P PJ 34202009-SERVICOS TOMADOS PESSOA JURIDICA) C-Fornecedores </t>
+  </si>
+  <si>
+    <t>Alterar as TES do facilitador de Doc de Entrada para os fornecedores MEI</t>
+  </si>
+  <si>
+    <t>Remover bitributação do pedido 048786 - RN Mossoró</t>
+  </si>
+  <si>
+    <t>Alterar pessoas que podem fazer avaliação de fornecedores</t>
+  </si>
+  <si>
+    <t>Acertar refresh na tela de avaliação de fornecedores</t>
+  </si>
+  <si>
+    <t>AvalForn (GCREENTR)</t>
   </si>
 </sst>
 </file>
@@ -7775,11 +7817,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1584"/>
+  <dimension ref="A1:J1592"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1520" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1532" sqref="H1532"/>
+      <pane ySplit="1" topLeftCell="A1532" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1540" sqref="A1540"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -53303,7 +53345,7 @@
         <v>620</v>
       </c>
       <c r="F1527" s="10" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="G1527" s="11" t="s">
         <v>295</v>
@@ -53333,7 +53375,7 @@
         <v>620</v>
       </c>
       <c r="F1528" s="10" t="s">
-        <v>2201</v>
+        <v>2200</v>
       </c>
       <c r="G1528" s="11" t="s">
         <v>295</v>
@@ -53363,7 +53405,7 @@
         <v>620</v>
       </c>
       <c r="F1529" s="10" t="s">
-        <v>2203</v>
+        <v>2202</v>
       </c>
       <c r="G1529" s="11" t="s">
         <v>295</v>
@@ -53376,71 +53418,91 @@
       </c>
       <c r="J1529" s="13"/>
     </row>
-    <row r="1530" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1530" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1530" s="12">
         <v>44460</v>
       </c>
-      <c r="B1530" s="12"/>
+      <c r="B1530" s="12">
+        <v>44465</v>
+      </c>
       <c r="C1530" s="14" t="s">
-        <v>2019</v>
+        <v>19</v>
       </c>
       <c r="D1530" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1530" s="11" t="s">
         <v>837</v>
       </c>
       <c r="F1530" s="10" t="s">
-        <v>2198</v>
-      </c>
-      <c r="G1530" s="11"/>
-      <c r="H1530" s="12"/>
-      <c r="I1530" s="13"/>
-      <c r="J1530" s="13"/>
+        <v>2205</v>
+      </c>
+      <c r="G1530" s="11" t="s">
+        <v>1624</v>
+      </c>
+      <c r="H1530" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1530" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1530" s="13" t="s">
+        <v>2203</v>
+      </c>
     </row>
     <row r="1531" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1531" s="12">
-        <v>44460</v>
-      </c>
-      <c r="B1531" s="12"/>
+        <v>44466</v>
+      </c>
+      <c r="B1531" s="12">
+        <v>44466</v>
+      </c>
       <c r="C1531" s="14" t="s">
-        <v>19</v>
+        <v>462</v>
       </c>
       <c r="D1531" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1531" s="11" t="s">
         <v>837</v>
       </c>
       <c r="F1531" s="10" t="s">
-        <v>2199</v>
-      </c>
-      <c r="G1531" s="11"/>
-      <c r="H1531" s="12"/>
-      <c r="I1531" s="13"/>
-      <c r="J1531" s="13"/>
-    </row>
-    <row r="1532" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>2207</v>
+      </c>
+      <c r="G1531" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1531" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1531" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1531" s="13" t="s">
+        <v>2208</v>
+      </c>
+    </row>
+    <row r="1532" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1532" s="12">
-        <v>44460</v>
+        <v>44466</v>
       </c>
       <c r="B1532" s="12">
-        <v>44465</v>
+        <v>44466</v>
       </c>
       <c r="C1532" s="14" t="s">
-        <v>19</v>
+        <v>400</v>
       </c>
       <c r="D1532" s="10" t="s">
-        <v>494</v>
+        <v>518</v>
       </c>
       <c r="E1532" s="11" t="s">
         <v>837</v>
       </c>
       <c r="F1532" s="10" t="s">
-        <v>2207</v>
+        <v>2209</v>
       </c>
       <c r="G1532" s="11" t="s">
-        <v>1624</v>
+        <v>295</v>
       </c>
       <c r="H1532" s="12" t="s">
         <v>112</v>
@@ -53449,16 +53511,18 @@
         <v>13</v>
       </c>
       <c r="J1532" s="13" t="s">
-        <v>2204</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="1533" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1533" s="12">
-        <v>44460</v>
-      </c>
-      <c r="B1533" s="12"/>
+        <v>44466</v>
+      </c>
+      <c r="B1533" s="12">
+        <v>44466</v>
+      </c>
       <c r="C1533" s="14" t="s">
-        <v>19</v>
+        <v>898</v>
       </c>
       <c r="D1533" s="10" t="s">
         <v>494</v>
@@ -53467,301 +53531,413 @@
         <v>837</v>
       </c>
       <c r="F1533" s="10" t="s">
-        <v>2200</v>
-      </c>
-      <c r="G1533" s="11"/>
-      <c r="H1533" s="12"/>
-      <c r="I1533" s="13"/>
+        <v>2211</v>
+      </c>
+      <c r="G1533" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1533" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1533" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1533" s="13"/>
     </row>
     <row r="1534" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1534" s="12">
-        <v>44460</v>
-      </c>
-      <c r="B1534" s="12"/>
+        <v>44466</v>
+      </c>
+      <c r="B1534" s="12">
+        <v>44467</v>
+      </c>
       <c r="C1534" s="14" t="s">
-        <v>19</v>
+        <v>1283</v>
       </c>
       <c r="D1534" s="10" t="s">
-        <v>494</v>
+        <v>17</v>
       </c>
       <c r="E1534" s="11" t="s">
-        <v>837</v>
+        <v>620</v>
       </c>
       <c r="F1534" s="10" t="s">
-        <v>2205</v>
-      </c>
-      <c r="G1534" s="11"/>
-      <c r="H1534" s="12"/>
-      <c r="I1534" s="13"/>
-      <c r="J1534" s="13"/>
+        <v>2212</v>
+      </c>
+      <c r="G1534" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1534" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1534" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1534" s="13" t="s">
+        <v>2213</v>
+      </c>
     </row>
     <row r="1535" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1535" s="12">
-        <v>44462</v>
-      </c>
-      <c r="B1535" s="12"/>
+        <v>44460</v>
+      </c>
+      <c r="B1535" s="12">
+        <v>44467</v>
+      </c>
       <c r="C1535" s="14" t="s">
-        <v>400</v>
+        <v>2019</v>
       </c>
       <c r="D1535" s="10" t="s">
-        <v>518</v>
+        <v>89</v>
       </c>
       <c r="E1535" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1535" s="10" t="s">
+        <v>2198</v>
+      </c>
+      <c r="G1535" s="11" t="s">
+        <v>1624</v>
+      </c>
+      <c r="H1535" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1535" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1535" s="13" t="s">
+        <v>2214</v>
+      </c>
+    </row>
+    <row r="1536" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1536" s="12">
+        <v>44467</v>
+      </c>
+      <c r="B1536" s="12">
+        <v>44467</v>
+      </c>
+      <c r="C1536" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1536" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1536" s="11" t="s">
         <v>620</v>
       </c>
-      <c r="F1535" s="10" t="s">
-        <v>2206</v>
-      </c>
-      <c r="G1535" s="11"/>
-      <c r="H1535" s="12"/>
-      <c r="I1535" s="13"/>
-      <c r="J1535" s="13"/>
-    </row>
-    <row r="1536" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1536" s="12"/>
-      <c r="B1536" s="12"/>
-      <c r="C1536" s="14"/>
-      <c r="D1536" s="10"/>
-      <c r="E1536" s="11"/>
-      <c r="F1536" s="10"/>
-      <c r="G1536" s="11"/>
-      <c r="H1536" s="12"/>
-      <c r="I1536" s="13"/>
+      <c r="F1536" s="10" t="s">
+        <v>2217</v>
+      </c>
+      <c r="G1536" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1536" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1536" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1536" s="13"/>
     </row>
     <row r="1537" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1537" s="12"/>
-      <c r="B1537" s="12"/>
-      <c r="C1537" s="14"/>
-      <c r="D1537" s="10"/>
-      <c r="E1537" s="11"/>
-      <c r="F1537" s="10"/>
-      <c r="G1537" s="11"/>
-      <c r="H1537" s="12"/>
-      <c r="I1537" s="13"/>
+      <c r="A1537" s="12">
+        <v>44467</v>
+      </c>
+      <c r="B1537" s="12">
+        <v>44467</v>
+      </c>
+      <c r="C1537" s="14" t="s">
+        <v>575</v>
+      </c>
+      <c r="D1537" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1537" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1537" s="10" t="s">
+        <v>2218</v>
+      </c>
+      <c r="G1537" s="11" t="s">
+        <v>1621</v>
+      </c>
+      <c r="H1537" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1537" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1537" s="13"/>
     </row>
     <row r="1538" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1538" s="12"/>
-      <c r="B1538" s="12"/>
-      <c r="C1538" s="14"/>
-      <c r="D1538" s="10"/>
-      <c r="E1538" s="11"/>
-      <c r="F1538" s="10"/>
-      <c r="G1538" s="11"/>
-      <c r="H1538" s="12"/>
-      <c r="I1538" s="13"/>
+      <c r="A1538" s="12">
+        <v>44467</v>
+      </c>
+      <c r="B1538" s="12">
+        <v>44467</v>
+      </c>
+      <c r="C1538" s="14" t="s">
+        <v>1477</v>
+      </c>
+      <c r="D1538" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1538" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1538" s="10" t="s">
+        <v>2219</v>
+      </c>
+      <c r="G1538" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1538" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1538" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1538" s="13"/>
     </row>
     <row r="1539" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1539" s="12"/>
-      <c r="B1539" s="12"/>
-      <c r="C1539" s="14"/>
-      <c r="D1539" s="10"/>
-      <c r="E1539" s="11"/>
-      <c r="F1539" s="10"/>
-      <c r="G1539" s="11"/>
-      <c r="H1539" s="12"/>
-      <c r="I1539" s="13"/>
-      <c r="J1539" s="13"/>
-    </row>
-    <row r="1540" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1540" s="12">
-        <v>44403</v>
-      </c>
+      <c r="A1539" s="12">
+        <v>44467</v>
+      </c>
+      <c r="B1539" s="12">
+        <v>44467</v>
+      </c>
+      <c r="C1539" s="14" t="s">
+        <v>1477</v>
+      </c>
+      <c r="D1539" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1539" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1539" s="10" t="s">
+        <v>2220</v>
+      </c>
+      <c r="G1539" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1539" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1539" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1539" s="13" t="s">
+        <v>2221</v>
+      </c>
+    </row>
+    <row r="1540" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1540" s="12"/>
       <c r="B1540" s="12"/>
-      <c r="C1540" s="14" t="s">
-        <v>1477</v>
-      </c>
-      <c r="D1540" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1540" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1540" s="10" t="s">
-        <v>2131</v>
-      </c>
+      <c r="C1540" s="14"/>
+      <c r="D1540" s="10"/>
+      <c r="E1540" s="11"/>
+      <c r="F1540" s="10"/>
       <c r="G1540" s="11"/>
       <c r="H1540" s="12"/>
       <c r="I1540" s="13"/>
       <c r="J1540" s="13"/>
     </row>
-    <row r="1541" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A1541" s="12">
-        <v>44266</v>
-      </c>
-      <c r="B1541" s="9"/>
-      <c r="C1541" s="14" t="s">
-        <v>537</v>
-      </c>
-      <c r="D1541" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1541" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1541" s="10" t="s">
-        <v>1713</v>
-      </c>
+    <row r="1541" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1541" s="12"/>
+      <c r="B1541" s="12"/>
+      <c r="C1541" s="14"/>
+      <c r="D1541" s="10"/>
+      <c r="E1541" s="11"/>
+      <c r="F1541" s="10"/>
       <c r="G1541" s="11"/>
       <c r="H1541" s="12"/>
       <c r="I1541" s="13"/>
-      <c r="J1541" s="13" t="s">
-        <v>1714</v>
-      </c>
-    </row>
-    <row r="1542" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1542" s="12">
-        <v>44286</v>
-      </c>
-      <c r="B1542" s="9"/>
-      <c r="C1542" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D1542" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1542" s="11" t="s">
-        <v>620</v>
-      </c>
-      <c r="F1542" s="10" t="s">
-        <v>1838</v>
-      </c>
+      <c r="J1541" s="13"/>
+    </row>
+    <row r="1542" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1542" s="12"/>
+      <c r="B1542" s="12"/>
+      <c r="C1542" s="14"/>
+      <c r="D1542" s="10"/>
+      <c r="E1542" s="11"/>
+      <c r="F1542" s="10"/>
       <c r="G1542" s="11"/>
       <c r="H1542" s="12"/>
       <c r="I1542" s="13"/>
       <c r="J1542" s="13"/>
     </row>
-    <row r="1543" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1543" s="12"/>
+    <row r="1543" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1543" s="12">
+        <v>44467</v>
+      </c>
       <c r="B1543" s="12"/>
-      <c r="C1543" s="14"/>
-      <c r="D1543" s="10"/>
-      <c r="E1543" s="11"/>
-      <c r="F1543" s="10"/>
+      <c r="C1543" s="14" t="s">
+        <v>1477</v>
+      </c>
+      <c r="D1543" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1543" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1543" s="10" t="s">
+        <v>2215</v>
+      </c>
       <c r="G1543" s="11"/>
       <c r="H1543" s="12"/>
       <c r="I1543" s="13"/>
       <c r="J1543" s="13"/>
     </row>
-    <row r="1544" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1544" s="12"/>
+    <row r="1544" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1544" s="12">
+        <v>44460</v>
+      </c>
       <c r="B1544" s="12"/>
-      <c r="C1544" s="14"/>
-      <c r="D1544" s="10"/>
-      <c r="E1544" s="11"/>
-      <c r="F1544" s="10"/>
+      <c r="C1544" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1544" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1544" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1544" s="10" t="s">
+        <v>2216</v>
+      </c>
       <c r="G1544" s="11"/>
       <c r="H1544" s="12"/>
       <c r="I1544" s="13"/>
       <c r="J1544" s="13"/>
     </row>
     <row r="1545" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1545" s="12"/>
+      <c r="A1545" s="12">
+        <v>44460</v>
+      </c>
       <c r="B1545" s="12"/>
-      <c r="C1545" s="14"/>
-      <c r="D1545" s="10"/>
-      <c r="E1545" s="11"/>
-      <c r="F1545" s="10"/>
+      <c r="C1545" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1545" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1545" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1545" s="10" t="s">
+        <v>2199</v>
+      </c>
       <c r="G1545" s="11"/>
       <c r="H1545" s="12"/>
       <c r="I1545" s="13"/>
       <c r="J1545" s="13"/>
     </row>
     <row r="1546" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1546" s="12"/>
-      <c r="B1546" s="9"/>
-      <c r="C1546" s="14"/>
-      <c r="D1546" s="10"/>
-      <c r="E1546" s="11"/>
-      <c r="F1546" s="10"/>
+      <c r="A1546" s="12">
+        <v>44462</v>
+      </c>
+      <c r="B1546" s="12"/>
+      <c r="C1546" s="14" t="s">
+        <v>400</v>
+      </c>
+      <c r="D1546" s="10" t="s">
+        <v>518</v>
+      </c>
+      <c r="E1546" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1546" s="10" t="s">
+        <v>2204</v>
+      </c>
       <c r="G1546" s="11"/>
       <c r="H1546" s="12"/>
       <c r="I1546" s="13"/>
       <c r="J1546" s="13"/>
     </row>
     <row r="1547" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1547" s="1" t="s">
-        <v>1479</v>
-      </c>
-      <c r="B1547" s="2" t="s">
-        <v>1480</v>
-      </c>
-      <c r="C1547" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1547" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1547" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1547" s="4" t="s">
-        <v>1579</v>
-      </c>
-      <c r="G1547" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1547" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1547" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1547" s="36"/>
-    </row>
-    <row r="1548" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1548" s="12"/>
-      <c r="B1548" s="9"/>
-      <c r="C1548" s="14"/>
-      <c r="D1548" s="10"/>
-      <c r="E1548" s="11"/>
-      <c r="F1548" s="10"/>
+      <c r="A1547" s="12">
+        <v>44466</v>
+      </c>
+      <c r="B1547" s="12"/>
+      <c r="C1547" s="14" t="s">
+        <v>462</v>
+      </c>
+      <c r="D1547" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1547" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1547" s="10" t="s">
+        <v>2206</v>
+      </c>
+      <c r="G1547" s="11"/>
+      <c r="H1547" s="12"/>
+      <c r="I1547" s="13"/>
+      <c r="J1547" s="13"/>
+    </row>
+    <row r="1548" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1548" s="12">
+        <v>44403</v>
+      </c>
+      <c r="B1548" s="12"/>
+      <c r="C1548" s="14" t="s">
+        <v>1477</v>
+      </c>
+      <c r="D1548" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1548" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1548" s="10" t="s">
+        <v>2131</v>
+      </c>
       <c r="G1548" s="11"/>
       <c r="H1548" s="12"/>
       <c r="I1548" s="13"/>
       <c r="J1548" s="13"/>
     </row>
-    <row r="1549" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1549" s="12"/>
-      <c r="B1549" s="12">
-        <v>44402</v>
-      </c>
+    <row r="1549" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1549" s="12">
+        <v>44266</v>
+      </c>
+      <c r="B1549" s="9"/>
       <c r="C1549" s="14" t="s">
-        <v>13</v>
+        <v>537</v>
       </c>
       <c r="D1549" s="10" t="s">
-        <v>584</v>
+        <v>6</v>
       </c>
       <c r="E1549" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1549" s="10" t="s">
-        <v>1614</v>
+        <v>1713</v>
       </c>
       <c r="G1549" s="11"/>
       <c r="H1549" s="12"/>
       <c r="I1549" s="13"/>
-      <c r="J1549" s="13"/>
-    </row>
-    <row r="1550" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1550" s="12"/>
-      <c r="B1550" s="12">
-        <v>44402</v>
-      </c>
+      <c r="J1549" s="13" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="1550" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1550" s="12">
+        <v>44286</v>
+      </c>
+      <c r="B1550" s="9"/>
       <c r="C1550" s="14" t="s">
-        <v>13</v>
+        <v>288</v>
       </c>
       <c r="D1550" s="10" t="s">
-        <v>584</v>
+        <v>25</v>
       </c>
       <c r="E1550" s="11" t="s">
-        <v>647</v>
+        <v>620</v>
       </c>
       <c r="F1550" s="10" t="s">
-        <v>1606</v>
+        <v>1838</v>
       </c>
       <c r="G1550" s="11"/>
       <c r="H1550" s="12"/>
@@ -53770,21 +53946,11 @@
     </row>
     <row r="1551" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1551" s="12"/>
-      <c r="B1551" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1551" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1551" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1551" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1551" s="10" t="s">
-        <v>1611</v>
-      </c>
+      <c r="B1551" s="12"/>
+      <c r="C1551" s="14"/>
+      <c r="D1551" s="10"/>
+      <c r="E1551" s="11"/>
+      <c r="F1551" s="10"/>
       <c r="G1551" s="11"/>
       <c r="H1551" s="12"/>
       <c r="I1551" s="13"/>
@@ -53792,21 +53958,11 @@
     </row>
     <row r="1552" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1552" s="12"/>
-      <c r="B1552" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1552" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1552" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1552" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1552" s="10" t="s">
-        <v>1607</v>
-      </c>
+      <c r="B1552" s="12"/>
+      <c r="C1552" s="14"/>
+      <c r="D1552" s="10"/>
+      <c r="E1552" s="11"/>
+      <c r="F1552" s="10"/>
       <c r="G1552" s="11"/>
       <c r="H1552" s="12"/>
       <c r="I1552" s="13"/>
@@ -53814,19 +53970,11 @@
     </row>
     <row r="1553" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1553" s="12"/>
-      <c r="B1553" s="9"/>
-      <c r="C1553" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1553" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1553" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1553" s="10" t="s">
-        <v>1615</v>
-      </c>
+      <c r="B1553" s="12"/>
+      <c r="C1553" s="14"/>
+      <c r="D1553" s="10"/>
+      <c r="E1553" s="11"/>
+      <c r="F1553" s="10"/>
       <c r="G1553" s="11"/>
       <c r="H1553" s="12"/>
       <c r="I1553" s="13"/>
@@ -53834,63 +53982,53 @@
     </row>
     <row r="1554" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1554" s="12"/>
-      <c r="B1554" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1554" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1554" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1554" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1554" s="10" t="s">
-        <v>1608</v>
-      </c>
+      <c r="B1554" s="9"/>
+      <c r="C1554" s="14"/>
+      <c r="D1554" s="10"/>
+      <c r="E1554" s="11"/>
+      <c r="F1554" s="10"/>
       <c r="G1554" s="11"/>
       <c r="H1554" s="12"/>
       <c r="I1554" s="13"/>
       <c r="J1554" s="13"/>
     </row>
     <row r="1555" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1555" s="12"/>
-      <c r="B1555" s="9"/>
-      <c r="C1555" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1555" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1555" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1555" s="10" t="s">
-        <v>1605</v>
-      </c>
-      <c r="G1555" s="11"/>
-      <c r="H1555" s="12"/>
-      <c r="I1555" s="13"/>
-      <c r="J1555" s="13"/>
+      <c r="A1555" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B1555" s="2" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C1555" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1555" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1555" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1555" s="4" t="s">
+        <v>1579</v>
+      </c>
+      <c r="G1555" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1555" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1555" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1555" s="36"/>
     </row>
     <row r="1556" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1556" s="12"/>
-      <c r="B1556" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1556" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1556" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1556" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1556" s="10" t="s">
-        <v>1604</v>
-      </c>
+      <c r="B1556" s="9"/>
+      <c r="C1556" s="14"/>
+      <c r="D1556" s="10"/>
+      <c r="E1556" s="11"/>
+      <c r="F1556" s="10"/>
       <c r="G1556" s="11"/>
       <c r="H1556" s="12"/>
       <c r="I1556" s="13"/>
@@ -53911,7 +54049,7 @@
         <v>647</v>
       </c>
       <c r="F1557" s="10" t="s">
-        <v>1609</v>
+        <v>1614</v>
       </c>
       <c r="G1557" s="11"/>
       <c r="H1557" s="12"/>
@@ -53933,7 +54071,7 @@
         <v>647</v>
       </c>
       <c r="F1558" s="10" t="s">
-        <v>1612</v>
+        <v>1606</v>
       </c>
       <c r="G1558" s="11"/>
       <c r="H1558" s="12"/>
@@ -53942,8 +54080,8 @@
     </row>
     <row r="1559" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1559" s="12"/>
-      <c r="B1559" s="9">
-        <v>44235</v>
+      <c r="B1559" s="12">
+        <v>44402</v>
       </c>
       <c r="C1559" s="14" t="s">
         <v>13</v>
@@ -53955,7 +54093,7 @@
         <v>647</v>
       </c>
       <c r="F1559" s="10" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
       <c r="G1559" s="11"/>
       <c r="H1559" s="12"/>
@@ -53964,7 +54102,9 @@
     </row>
     <row r="1560" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1560" s="12"/>
-      <c r="B1560" s="9"/>
+      <c r="B1560" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1560" s="14" t="s">
         <v>13</v>
       </c>
@@ -53975,7 +54115,7 @@
         <v>647</v>
       </c>
       <c r="F1560" s="10" t="s">
-        <v>1610</v>
+        <v>1607</v>
       </c>
       <c r="G1560" s="11"/>
       <c r="H1560" s="12"/>
@@ -53995,7 +54135,7 @@
         <v>647</v>
       </c>
       <c r="F1561" s="10" t="s">
-        <v>1581</v>
+        <v>1615</v>
       </c>
       <c r="G1561" s="11"/>
       <c r="H1561" s="12"/>
@@ -54004,78 +54144,84 @@
     </row>
     <row r="1562" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1562" s="12"/>
-      <c r="B1562" s="9"/>
-      <c r="C1562" s="14"/>
-      <c r="D1562" s="10"/>
-      <c r="E1562" s="11"/>
-      <c r="F1562" s="10"/>
+      <c r="B1562" s="12">
+        <v>44402</v>
+      </c>
+      <c r="C1562" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1562" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1562" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1562" s="10" t="s">
+        <v>1608</v>
+      </c>
       <c r="G1562" s="11"/>
       <c r="H1562" s="12"/>
       <c r="I1562" s="13"/>
       <c r="J1562" s="13"/>
     </row>
     <row r="1563" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1563" s="12">
-        <v>44176</v>
-      </c>
+      <c r="A1563" s="12"/>
       <c r="B1563" s="9"/>
       <c r="C1563" s="14" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D1563" s="10" t="s">
         <v>584</v>
       </c>
       <c r="E1563" s="11" t="s">
-        <v>1353</v>
+        <v>647</v>
       </c>
       <c r="F1563" s="10" t="s">
-        <v>1354</v>
+        <v>1605</v>
       </c>
       <c r="G1563" s="11"/>
       <c r="H1563" s="12"/>
       <c r="I1563" s="13"/>
       <c r="J1563" s="13"/>
     </row>
-    <row r="1564" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1564" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1564" s="9"/>
+    <row r="1564" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1564" s="12"/>
+      <c r="B1564" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1564" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1564" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1564" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1564" s="10" t="s">
-        <v>1659</v>
+        <v>1604</v>
       </c>
       <c r="G1564" s="11"/>
       <c r="H1564" s="12"/>
       <c r="I1564" s="13"/>
-      <c r="J1564" s="13" t="s">
-        <v>1682</v>
-      </c>
-    </row>
-    <row r="1565" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1565" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1565" s="9"/>
+      <c r="J1564" s="13"/>
+    </row>
+    <row r="1565" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1565" s="12"/>
+      <c r="B1565" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1565" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1565" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1565" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1565" s="10" t="s">
-        <v>1658</v>
+        <v>1609</v>
       </c>
       <c r="G1565" s="11"/>
       <c r="H1565" s="12"/>
@@ -54083,21 +54229,21 @@
       <c r="J1565" s="13"/>
     </row>
     <row r="1566" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1566" s="12">
-        <v>44112</v>
-      </c>
-      <c r="B1566" s="9"/>
+      <c r="A1566" s="12"/>
+      <c r="B1566" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1566" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1566" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1566" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1566" s="10" t="s">
-        <v>1097</v>
+        <v>1612</v>
       </c>
       <c r="G1566" s="11"/>
       <c r="H1566" s="12"/>
@@ -54105,21 +54251,21 @@
       <c r="J1566" s="13"/>
     </row>
     <row r="1567" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1567" s="12">
-        <v>44088</v>
-      </c>
-      <c r="B1567" s="9"/>
+      <c r="A1567" s="12"/>
+      <c r="B1567" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1567" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1567" s="10" t="s">
-        <v>906</v>
+        <v>584</v>
       </c>
       <c r="E1567" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1567" s="10" t="s">
-        <v>1011</v>
+        <v>1613</v>
       </c>
       <c r="G1567" s="11"/>
       <c r="H1567" s="12"/>
@@ -54127,21 +54273,19 @@
       <c r="J1567" s="13"/>
     </row>
     <row r="1568" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1568" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1568" s="12"/>
       <c r="B1568" s="9"/>
       <c r="C1568" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1568" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1568" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1568" s="10" t="s">
-        <v>903</v>
+        <v>1610</v>
       </c>
       <c r="G1568" s="11"/>
       <c r="H1568" s="12"/>
@@ -54149,21 +54293,19 @@
       <c r="J1568" s="13"/>
     </row>
     <row r="1569" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1569" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1569" s="12"/>
       <c r="B1569" s="9"/>
       <c r="C1569" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1569" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1569" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1569" s="10" t="s">
-        <v>902</v>
+        <v>1581</v>
       </c>
       <c r="G1569" s="11"/>
       <c r="H1569" s="12"/>
@@ -54171,52 +54313,42 @@
       <c r="J1569" s="13"/>
     </row>
     <row r="1570" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1570" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1570" s="12"/>
       <c r="B1570" s="9"/>
-      <c r="C1570" s="14" t="s">
-        <v>898</v>
-      </c>
-      <c r="D1570" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="E1570" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1570" s="10" t="s">
-        <v>900</v>
-      </c>
+      <c r="C1570" s="14"/>
+      <c r="D1570" s="10"/>
+      <c r="E1570" s="11"/>
+      <c r="F1570" s="10"/>
       <c r="G1570" s="11"/>
       <c r="H1570" s="12"/>
       <c r="I1570" s="13"/>
       <c r="J1570" s="13"/>
     </row>
-    <row r="1571" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="1571" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1571" s="12">
-        <v>44055</v>
+        <v>44176</v>
       </c>
       <c r="B1571" s="9"/>
       <c r="C1571" s="14" t="s">
-        <v>898</v>
+        <v>8</v>
       </c>
       <c r="D1571" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1571" s="11" t="s">
-        <v>570</v>
+        <v>1353</v>
       </c>
       <c r="F1571" s="10" t="s">
-        <v>901</v>
+        <v>1354</v>
       </c>
       <c r="G1571" s="11"/>
       <c r="H1571" s="12"/>
       <c r="I1571" s="13"/>
       <c r="J1571" s="13"/>
     </row>
-    <row r="1572" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1572" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1572" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1572" s="9"/>
       <c r="C1572" s="14" t="s">
@@ -54226,248 +54358,426 @@
         <v>494</v>
       </c>
       <c r="E1572" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1572" s="10" t="s">
-        <v>904</v>
+        <v>1659</v>
       </c>
       <c r="G1572" s="11"/>
       <c r="H1572" s="12"/>
       <c r="I1572" s="13"/>
       <c r="J1572" s="13" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="1573" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="1573" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1573" s="12">
-        <v>44047</v>
+        <v>44252</v>
       </c>
       <c r="B1573" s="9"/>
       <c r="C1573" s="14" t="s">
-        <v>537</v>
+        <v>898</v>
       </c>
       <c r="D1573" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1573" s="11" t="s">
-        <v>685</v>
+        <v>759</v>
       </c>
       <c r="F1573" s="10" t="s">
-        <v>873</v>
-      </c>
-      <c r="G1573" s="11" t="s">
-        <v>1624</v>
-      </c>
+        <v>1658</v>
+      </c>
+      <c r="G1573" s="11"/>
       <c r="H1573" s="12"/>
       <c r="I1573" s="13"/>
       <c r="J1573" s="13"/>
     </row>
-    <row r="1574" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1574" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1574" s="12">
-        <v>43949</v>
+        <v>44112</v>
       </c>
       <c r="B1574" s="9"/>
       <c r="C1574" s="14" t="s">
-        <v>468</v>
+        <v>623</v>
       </c>
       <c r="D1574" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1574" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1574" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1574" s="11" t="s">
-        <v>1639</v>
-      </c>
+        <v>1097</v>
+      </c>
+      <c r="G1574" s="11"/>
       <c r="H1574" s="12"/>
-      <c r="I1574" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1574" s="13"/>
       <c r="J1574" s="13"/>
     </row>
-    <row r="1575" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1575" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1575" s="12">
-        <v>43949</v>
+        <v>44088</v>
       </c>
       <c r="B1575" s="9"/>
       <c r="C1575" s="14" t="s">
-        <v>468</v>
+        <v>19</v>
       </c>
       <c r="D1575" s="10" t="s">
-        <v>89</v>
+        <v>906</v>
       </c>
       <c r="E1575" s="11" t="s">
         <v>685</v>
       </c>
       <c r="F1575" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1575" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>1011</v>
+      </c>
+      <c r="G1575" s="11"/>
       <c r="H1575" s="12"/>
-      <c r="I1575" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1575" s="13" t="s">
-        <v>1568</v>
-      </c>
-    </row>
-    <row r="1576" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1575" s="13"/>
+      <c r="J1575" s="13"/>
+    </row>
+    <row r="1576" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1576" s="12">
-        <v>43838</v>
+        <v>44055</v>
       </c>
       <c r="B1576" s="9"/>
       <c r="C1576" s="14" t="s">
-        <v>103</v>
+        <v>623</v>
       </c>
       <c r="D1576" s="10" t="s">
-        <v>460</v>
+        <v>6</v>
       </c>
       <c r="E1576" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1576" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G1576" s="11" t="s">
-        <v>1640</v>
-      </c>
+        <v>903</v>
+      </c>
+      <c r="G1576" s="11"/>
       <c r="H1576" s="12"/>
       <c r="I1576" s="13"/>
-      <c r="J1576" s="13" t="s">
-        <v>1533</v>
-      </c>
+      <c r="J1576" s="13"/>
     </row>
     <row r="1577" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1577" s="12">
-        <v>43816</v>
+        <v>44055</v>
       </c>
       <c r="B1577" s="9"/>
       <c r="C1577" s="14" t="s">
-        <v>475</v>
+        <v>623</v>
       </c>
       <c r="D1577" s="10" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="E1577" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1577" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="G1577" s="11" t="s">
-        <v>1632</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="G1577" s="11"/>
       <c r="H1577" s="12"/>
       <c r="I1577" s="13"/>
-      <c r="J1577" s="13" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="1578" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1577" s="13"/>
+    </row>
+    <row r="1578" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1578" s="12">
-        <v>43762</v>
+        <v>44055</v>
       </c>
       <c r="B1578" s="9"/>
       <c r="C1578" s="14" t="s">
-        <v>446</v>
+        <v>898</v>
       </c>
       <c r="D1578" s="10" t="s">
-        <v>17</v>
+        <v>494</v>
       </c>
       <c r="E1578" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1578" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G1578" s="11" t="s">
-        <v>1629</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="G1578" s="11"/>
       <c r="H1578" s="12"/>
       <c r="I1578" s="13"/>
       <c r="J1578" s="13"/>
     </row>
-    <row r="1579" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1579" s="12"/>
+    <row r="1579" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A1579" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1579" s="9"/>
-      <c r="C1579" s="14"/>
-      <c r="D1579" s="10"/>
-      <c r="E1579" s="11"/>
-      <c r="F1579" s="10"/>
+      <c r="C1579" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1579" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1579" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1579" s="10" t="s">
+        <v>901</v>
+      </c>
       <c r="G1579" s="11"/>
       <c r="H1579" s="12"/>
       <c r="I1579" s="13"/>
       <c r="J1579" s="13"/>
     </row>
-    <row r="1580" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1580" s="12"/>
+    <row r="1580" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1580" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1580" s="9"/>
-      <c r="C1580" s="14"/>
-      <c r="D1580" s="10"/>
-      <c r="E1580" s="11"/>
-      <c r="F1580" s="10"/>
+      <c r="C1580" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1580" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1580" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1580" s="10" t="s">
+        <v>904</v>
+      </c>
       <c r="G1580" s="11"/>
       <c r="H1580" s="12"/>
       <c r="I1580" s="13"/>
-      <c r="J1580" s="13"/>
-    </row>
-    <row r="1581" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1581" s="12"/>
+      <c r="J1580" s="13" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1581" s="12">
+        <v>44047</v>
+      </c>
       <c r="B1581" s="9"/>
-      <c r="C1581" s="14"/>
-      <c r="D1581" s="10"/>
-      <c r="E1581" s="11"/>
-      <c r="F1581" s="10"/>
-      <c r="G1581" s="11"/>
+      <c r="C1581" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1581" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1581" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1581" s="10" t="s">
+        <v>873</v>
+      </c>
+      <c r="G1581" s="11" t="s">
+        <v>1624</v>
+      </c>
       <c r="H1581" s="12"/>
       <c r="I1581" s="13"/>
       <c r="J1581" s="13"/>
     </row>
-    <row r="1582" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1582" s="12"/>
+    <row r="1582" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1582" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1582" s="9"/>
-      <c r="C1582" s="14"/>
-      <c r="D1582" s="10"/>
-      <c r="E1582" s="11"/>
-      <c r="F1582" s="10"/>
-      <c r="G1582" s="11"/>
+      <c r="C1582" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1582" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1582" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1582" s="10" t="s">
+        <v>686</v>
+      </c>
+      <c r="G1582" s="11" t="s">
+        <v>1639</v>
+      </c>
       <c r="H1582" s="12"/>
-      <c r="I1582" s="13"/>
+      <c r="I1582" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1582" s="13"/>
     </row>
-    <row r="1583" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1583" s="12"/>
+    <row r="1583" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1583" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1583" s="9"/>
-      <c r="C1583" s="14"/>
-      <c r="D1583" s="10"/>
-      <c r="E1583" s="11"/>
-      <c r="F1583" s="10"/>
-      <c r="G1583" s="11"/>
+      <c r="C1583" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1583" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1583" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1583" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="G1583" s="11" t="s">
+        <v>687</v>
+      </c>
       <c r="H1583" s="12"/>
-      <c r="I1583" s="13"/>
-      <c r="J1583" s="13"/>
-    </row>
-    <row r="1584" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1584" s="12"/>
+      <c r="I1583" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1583" s="13" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="1584" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1584" s="12">
+        <v>43838</v>
+      </c>
       <c r="B1584" s="9"/>
-      <c r="C1584" s="14"/>
-      <c r="D1584" s="10"/>
-      <c r="E1584" s="11"/>
-      <c r="F1584" s="10"/>
-      <c r="G1584" s="11"/>
+      <c r="C1584" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1584" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1584" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1584" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G1584" s="11" t="s">
+        <v>1640</v>
+      </c>
       <c r="H1584" s="12"/>
       <c r="I1584" s="13"/>
-      <c r="J1584" s="13"/>
+      <c r="J1584" s="13" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1585" s="12">
+        <v>43816</v>
+      </c>
+      <c r="B1585" s="9"/>
+      <c r="C1585" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1585" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1585" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1585" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G1585" s="11" t="s">
+        <v>1632</v>
+      </c>
+      <c r="H1585" s="12"/>
+      <c r="I1585" s="13"/>
+      <c r="J1585" s="13" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1586" s="12">
+        <v>43762</v>
+      </c>
+      <c r="B1586" s="9"/>
+      <c r="C1586" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1586" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1586" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1586" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1586" s="11" t="s">
+        <v>1629</v>
+      </c>
+      <c r="H1586" s="12"/>
+      <c r="I1586" s="13"/>
+      <c r="J1586" s="13"/>
+    </row>
+    <row r="1587" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1587" s="12"/>
+      <c r="B1587" s="9"/>
+      <c r="C1587" s="14"/>
+      <c r="D1587" s="10"/>
+      <c r="E1587" s="11"/>
+      <c r="F1587" s="10"/>
+      <c r="G1587" s="11"/>
+      <c r="H1587" s="12"/>
+      <c r="I1587" s="13"/>
+      <c r="J1587" s="13"/>
+    </row>
+    <row r="1588" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1588" s="12"/>
+      <c r="B1588" s="9"/>
+      <c r="C1588" s="14"/>
+      <c r="D1588" s="10"/>
+      <c r="E1588" s="11"/>
+      <c r="F1588" s="10"/>
+      <c r="G1588" s="11"/>
+      <c r="H1588" s="12"/>
+      <c r="I1588" s="13"/>
+      <c r="J1588" s="13"/>
+    </row>
+    <row r="1589" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1589" s="12"/>
+      <c r="B1589" s="9"/>
+      <c r="C1589" s="14"/>
+      <c r="D1589" s="10"/>
+      <c r="E1589" s="11"/>
+      <c r="F1589" s="10"/>
+      <c r="G1589" s="11"/>
+      <c r="H1589" s="12"/>
+      <c r="I1589" s="13"/>
+      <c r="J1589" s="13"/>
+    </row>
+    <row r="1590" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1590" s="12"/>
+      <c r="B1590" s="9"/>
+      <c r="C1590" s="14"/>
+      <c r="D1590" s="10"/>
+      <c r="E1590" s="11"/>
+      <c r="F1590" s="10"/>
+      <c r="G1590" s="11"/>
+      <c r="H1590" s="12"/>
+      <c r="I1590" s="13"/>
+      <c r="J1590" s="13"/>
+    </row>
+    <row r="1591" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1591" s="12"/>
+      <c r="B1591" s="9"/>
+      <c r="C1591" s="14"/>
+      <c r="D1591" s="10"/>
+      <c r="E1591" s="11"/>
+      <c r="F1591" s="10"/>
+      <c r="G1591" s="11"/>
+      <c r="H1591" s="12"/>
+      <c r="I1591" s="13"/>
+      <c r="J1591" s="13"/>
+    </row>
+    <row r="1592" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1592" s="12"/>
+      <c r="B1592" s="9"/>
+      <c r="C1592" s="14"/>
+      <c r="D1592" s="10"/>
+      <c r="E1592" s="11"/>
+      <c r="F1592" s="10"/>
+      <c r="G1592" s="11"/>
+      <c r="H1592" s="12"/>
+      <c r="I1592" s="13"/>
+      <c r="J1592" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1480" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1550:F1560">
-    <sortCondition ref="F1550:F1560"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1558:F1568">
+    <sortCondition ref="F1558:F1568"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Incluir coluna espécie no rel XFISR101
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47031AD-B858-48F8-B211-06FF6D743A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE93B94-A760-4B91-B096-11BC6F23523B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11310" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11209" uniqueCount="2261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11245" uniqueCount="2266">
   <si>
     <t>Responsável</t>
   </si>
@@ -7171,6 +7171,24 @@
   </si>
   <si>
     <t>Acerto portador do titulo 353920LFE para 341</t>
+  </si>
+  <si>
+    <t>Acerto BCC de diversas TES de entrada</t>
+  </si>
+  <si>
+    <t>Reunião Ativo Imobilizado:
+1 - Gerar planilha a partir dos itens de compras no formato da planilha de carga
+2 - Implantar o sistema a partir dos lançamentos de compras atuais
+3 - Verificar a possibilidade de se incluir bens não patrimoniaveis no sistema para controles de localização</t>
+  </si>
+  <si>
+    <t>Alinhamento sobre revisão de cadastros de fornecedores e base fiscal</t>
+  </si>
+  <si>
+    <t>Liberação do Pedido 049205 duplicada</t>
+  </si>
+  <si>
+    <t>Incluir coluna Especie no relatório de conferencia EFD Personalizado</t>
   </si>
 </sst>
 </file>
@@ -7939,11 +7957,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1624"/>
+  <dimension ref="A1:J1631"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1567" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1580" sqref="A1580"/>
+      <pane ySplit="1" topLeftCell="A1576" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1585" sqref="A1585"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -55057,131 +55075,177 @@
       <c r="J1579" s="13"/>
     </row>
     <row r="1580" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1580" s="12"/>
-      <c r="B1580" s="12"/>
-      <c r="C1580" s="14"/>
-      <c r="D1580" s="10"/>
-      <c r="E1580" s="11"/>
-      <c r="F1580" s="10"/>
-      <c r="G1580" s="11"/>
-      <c r="H1580" s="12"/>
-      <c r="I1580" s="13"/>
+      <c r="A1580" s="12">
+        <v>44514</v>
+      </c>
+      <c r="B1580" s="12">
+        <v>44514</v>
+      </c>
+      <c r="C1580" s="14" t="s">
+        <v>1988</v>
+      </c>
+      <c r="D1580" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1580" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1580" s="10" t="s">
+        <v>2263</v>
+      </c>
+      <c r="G1580" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1580" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1580" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1580" s="13"/>
     </row>
     <row r="1581" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1581" s="12"/>
-      <c r="B1581" s="12"/>
-      <c r="C1581" s="14"/>
-      <c r="D1581" s="10"/>
-      <c r="E1581" s="11"/>
-      <c r="F1581" s="10"/>
-      <c r="G1581" s="11"/>
-      <c r="H1581" s="12"/>
-      <c r="I1581" s="13"/>
+      <c r="A1581" s="12">
+        <v>44514</v>
+      </c>
+      <c r="B1581" s="12">
+        <v>44514</v>
+      </c>
+      <c r="C1581" s="14" t="s">
+        <v>1988</v>
+      </c>
+      <c r="D1581" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1581" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1581" s="10" t="s">
+        <v>2261</v>
+      </c>
+      <c r="G1581" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1581" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1581" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1581" s="13"/>
     </row>
-    <row r="1582" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1582" s="12"/>
-      <c r="B1582" s="12"/>
-      <c r="C1582" s="14"/>
-      <c r="D1582" s="10"/>
-      <c r="E1582" s="11"/>
-      <c r="F1582" s="10"/>
-      <c r="G1582" s="11"/>
-      <c r="H1582" s="12"/>
-      <c r="I1582" s="13"/>
+    <row r="1582" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="A1582" s="12">
+        <v>44514</v>
+      </c>
+      <c r="B1582" s="12">
+        <v>44514</v>
+      </c>
+      <c r="C1582" s="14" t="s">
+        <v>2030</v>
+      </c>
+      <c r="D1582" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1582" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1582" s="10" t="s">
+        <v>2262</v>
+      </c>
+      <c r="G1582" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1582" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1582" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1582" s="13"/>
     </row>
     <row r="1583" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1583" s="12">
-        <v>43816</v>
-      </c>
-      <c r="B1583" s="9"/>
+        <v>44514</v>
+      </c>
+      <c r="B1583" s="12">
+        <v>44514</v>
+      </c>
       <c r="C1583" s="14" t="s">
-        <v>475</v>
+        <v>1282</v>
       </c>
       <c r="D1583" s="10" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="E1583" s="11" t="s">
-        <v>570</v>
+        <v>837</v>
       </c>
       <c r="F1583" s="10" t="s">
-        <v>474</v>
+        <v>2264</v>
       </c>
       <c r="G1583" s="11" t="s">
-        <v>1629</v>
-      </c>
-      <c r="H1583" s="12"/>
-      <c r="I1583" s="13"/>
-      <c r="J1583" s="13" t="s">
-        <v>1566</v>
-      </c>
+        <v>1643</v>
+      </c>
+      <c r="H1583" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1583" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1583" s="13"/>
     </row>
     <row r="1584" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1584" s="12">
-        <v>44460</v>
-      </c>
-      <c r="B1584" s="12"/>
+        <v>44514</v>
+      </c>
+      <c r="B1584" s="12">
+        <v>44514</v>
+      </c>
       <c r="C1584" s="14" t="s">
-        <v>19</v>
+        <v>1988</v>
       </c>
       <c r="D1584" s="10" t="s">
-        <v>494</v>
+        <v>89</v>
       </c>
       <c r="E1584" s="11" t="s">
         <v>837</v>
       </c>
       <c r="F1584" s="10" t="s">
-        <v>2195</v>
-      </c>
-      <c r="G1584" s="11"/>
-      <c r="H1584" s="12"/>
-      <c r="I1584" s="13"/>
-      <c r="J1584" s="13"/>
+        <v>2265</v>
+      </c>
+      <c r="G1584" s="11" t="s">
+        <v>1644</v>
+      </c>
+      <c r="H1584" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1584" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1584" s="13" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="1585" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1585" s="12">
-        <v>44466</v>
-      </c>
+      <c r="A1585" s="12"/>
       <c r="B1585" s="12"/>
-      <c r="C1585" s="14" t="s">
-        <v>462</v>
-      </c>
-      <c r="D1585" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1585" s="11" t="s">
-        <v>837</v>
-      </c>
-      <c r="F1585" s="10" t="s">
-        <v>2202</v>
-      </c>
+      <c r="C1585" s="14"/>
+      <c r="D1585" s="10"/>
+      <c r="E1585" s="11"/>
+      <c r="F1585" s="10"/>
       <c r="G1585" s="11"/>
       <c r="H1585" s="12"/>
       <c r="I1585" s="13"/>
       <c r="J1585" s="13"/>
     </row>
     <row r="1586" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1586" s="12">
-        <v>44440</v>
-      </c>
-      <c r="B1586" s="9"/>
-      <c r="C1586" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1586" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1586" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1586" s="10" t="s">
-        <v>1578</v>
-      </c>
-      <c r="G1586" s="11" t="s">
-        <v>1636</v>
-      </c>
+      <c r="A1586" s="12"/>
+      <c r="B1586" s="12"/>
+      <c r="C1586" s="14"/>
+      <c r="D1586" s="10"/>
+      <c r="E1586" s="11"/>
+      <c r="F1586" s="10"/>
+      <c r="G1586" s="11"/>
       <c r="H1586" s="12"/>
       <c r="I1586" s="13"/>
       <c r="J1586" s="13"/>
@@ -55212,7 +55276,7 @@
     </row>
     <row r="1589" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1589" s="12"/>
-      <c r="B1589" s="9"/>
+      <c r="B1589" s="12"/>
       <c r="C1589" s="14"/>
       <c r="D1589" s="10"/>
       <c r="E1589" s="11"/>
@@ -55223,63 +55287,69 @@
       <c r="J1589" s="13"/>
     </row>
     <row r="1590" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1590" s="1" t="s">
-        <v>1476</v>
-      </c>
-      <c r="B1590" s="2" t="s">
-        <v>1477</v>
-      </c>
-      <c r="C1590" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1590" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1590" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1590" s="4" t="s">
-        <v>1576</v>
-      </c>
-      <c r="G1590" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1590" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1590" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1590" s="36"/>
+      <c r="A1590" s="12">
+        <v>43816</v>
+      </c>
+      <c r="B1590" s="9"/>
+      <c r="C1590" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1590" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1590" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1590" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G1590" s="11" t="s">
+        <v>1629</v>
+      </c>
+      <c r="H1590" s="12"/>
+      <c r="I1590" s="13"/>
+      <c r="J1590" s="13" t="s">
+        <v>1566</v>
+      </c>
     </row>
     <row r="1591" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1591" s="12"/>
-      <c r="B1591" s="9"/>
-      <c r="C1591" s="14"/>
-      <c r="D1591" s="10"/>
-      <c r="E1591" s="11"/>
-      <c r="F1591" s="10"/>
+      <c r="A1591" s="12">
+        <v>44460</v>
+      </c>
+      <c r="B1591" s="12"/>
+      <c r="C1591" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1591" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1591" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1591" s="10" t="s">
+        <v>2195</v>
+      </c>
       <c r="G1591" s="11"/>
       <c r="H1591" s="12"/>
       <c r="I1591" s="13"/>
       <c r="J1591" s="13"/>
     </row>
     <row r="1592" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1592" s="12"/>
-      <c r="B1592" s="12">
-        <v>44402</v>
-      </c>
+      <c r="A1592" s="12">
+        <v>44466</v>
+      </c>
+      <c r="B1592" s="12"/>
       <c r="C1592" s="14" t="s">
-        <v>13</v>
+        <v>462</v>
       </c>
       <c r="D1592" s="10" t="s">
-        <v>584</v>
+        <v>107</v>
       </c>
       <c r="E1592" s="11" t="s">
-        <v>647</v>
+        <v>837</v>
       </c>
       <c r="F1592" s="10" t="s">
-        <v>1611</v>
+        <v>2202</v>
       </c>
       <c r="G1592" s="11"/>
       <c r="H1592" s="12"/>
@@ -55287,10 +55357,10 @@
       <c r="J1592" s="13"/>
     </row>
     <row r="1593" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1593" s="12"/>
-      <c r="B1593" s="12">
-        <v>44402</v>
-      </c>
+      <c r="A1593" s="12">
+        <v>44440</v>
+      </c>
+      <c r="B1593" s="9"/>
       <c r="C1593" s="14" t="s">
         <v>13</v>
       </c>
@@ -55301,30 +55371,22 @@
         <v>647</v>
       </c>
       <c r="F1593" s="10" t="s">
-        <v>1603</v>
-      </c>
-      <c r="G1593" s="11"/>
+        <v>1578</v>
+      </c>
+      <c r="G1593" s="11" t="s">
+        <v>1636</v>
+      </c>
       <c r="H1593" s="12"/>
       <c r="I1593" s="13"/>
       <c r="J1593" s="13"/>
     </row>
     <row r="1594" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1594" s="12"/>
-      <c r="B1594" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1594" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1594" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1594" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1594" s="10" t="s">
-        <v>1608</v>
-      </c>
+      <c r="B1594" s="12"/>
+      <c r="C1594" s="14"/>
+      <c r="D1594" s="10"/>
+      <c r="E1594" s="11"/>
+      <c r="F1594" s="10"/>
       <c r="G1594" s="11"/>
       <c r="H1594" s="12"/>
       <c r="I1594" s="13"/>
@@ -55332,21 +55394,11 @@
     </row>
     <row r="1595" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1595" s="12"/>
-      <c r="B1595" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1595" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1595" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1595" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1595" s="10" t="s">
-        <v>1604</v>
-      </c>
+      <c r="B1595" s="12"/>
+      <c r="C1595" s="14"/>
+      <c r="D1595" s="10"/>
+      <c r="E1595" s="11"/>
+      <c r="F1595" s="10"/>
       <c r="G1595" s="11"/>
       <c r="H1595" s="12"/>
       <c r="I1595" s="13"/>
@@ -55355,60 +55407,52 @@
     <row r="1596" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1596" s="12"/>
       <c r="B1596" s="9"/>
-      <c r="C1596" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1596" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1596" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1596" s="10" t="s">
-        <v>1612</v>
-      </c>
+      <c r="C1596" s="14"/>
+      <c r="D1596" s="10"/>
+      <c r="E1596" s="11"/>
+      <c r="F1596" s="10"/>
       <c r="G1596" s="11"/>
       <c r="H1596" s="12"/>
       <c r="I1596" s="13"/>
       <c r="J1596" s="13"/>
     </row>
     <row r="1597" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1597" s="12"/>
-      <c r="B1597" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1597" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1597" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1597" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1597" s="10" t="s">
-        <v>1605</v>
-      </c>
-      <c r="G1597" s="11"/>
-      <c r="H1597" s="12"/>
-      <c r="I1597" s="13"/>
-      <c r="J1597" s="13"/>
+      <c r="A1597" s="1" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B1597" s="2" t="s">
+        <v>1477</v>
+      </c>
+      <c r="C1597" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1597" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1597" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1597" s="4" t="s">
+        <v>1576</v>
+      </c>
+      <c r="G1597" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1597" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1597" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1597" s="36"/>
     </row>
     <row r="1598" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1598" s="12"/>
       <c r="B1598" s="9"/>
-      <c r="C1598" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1598" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1598" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1598" s="10" t="s">
-        <v>1602</v>
-      </c>
+      <c r="C1598" s="14"/>
+      <c r="D1598" s="10"/>
+      <c r="E1598" s="11"/>
+      <c r="F1598" s="10"/>
       <c r="G1598" s="11"/>
       <c r="H1598" s="12"/>
       <c r="I1598" s="13"/>
@@ -55429,7 +55473,7 @@
         <v>647</v>
       </c>
       <c r="F1599" s="10" t="s">
-        <v>1601</v>
+        <v>1611</v>
       </c>
       <c r="G1599" s="11"/>
       <c r="H1599" s="12"/>
@@ -55451,7 +55495,7 @@
         <v>647</v>
       </c>
       <c r="F1600" s="10" t="s">
-        <v>1606</v>
+        <v>1603</v>
       </c>
       <c r="G1600" s="11"/>
       <c r="H1600" s="12"/>
@@ -55473,7 +55517,7 @@
         <v>647</v>
       </c>
       <c r="F1601" s="10" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="G1601" s="11"/>
       <c r="H1601" s="12"/>
@@ -55482,8 +55526,8 @@
     </row>
     <row r="1602" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1602" s="12"/>
-      <c r="B1602" s="9">
-        <v>44235</v>
+      <c r="B1602" s="12">
+        <v>44402</v>
       </c>
       <c r="C1602" s="14" t="s">
         <v>13</v>
@@ -55495,7 +55539,7 @@
         <v>647</v>
       </c>
       <c r="F1602" s="10" t="s">
-        <v>1610</v>
+        <v>1604</v>
       </c>
       <c r="G1602" s="11"/>
       <c r="H1602" s="12"/>
@@ -55515,7 +55559,7 @@
         <v>647</v>
       </c>
       <c r="F1603" s="10" t="s">
-        <v>1607</v>
+        <v>1612</v>
       </c>
       <c r="G1603" s="11"/>
       <c r="H1603" s="12"/>
@@ -55524,78 +55568,84 @@
     </row>
     <row r="1604" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1604" s="12"/>
-      <c r="B1604" s="9"/>
-      <c r="C1604" s="14"/>
-      <c r="D1604" s="10"/>
-      <c r="E1604" s="11"/>
-      <c r="F1604" s="10"/>
+      <c r="B1604" s="12">
+        <v>44402</v>
+      </c>
+      <c r="C1604" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1604" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1604" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1604" s="10" t="s">
+        <v>1605</v>
+      </c>
       <c r="G1604" s="11"/>
       <c r="H1604" s="12"/>
       <c r="I1604" s="13"/>
       <c r="J1604" s="13"/>
     </row>
-    <row r="1605" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1605" s="12">
-        <v>44252</v>
-      </c>
+    <row r="1605" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1605" s="12"/>
       <c r="B1605" s="9"/>
       <c r="C1605" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1605" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1605" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1605" s="10" t="s">
-        <v>1656</v>
+        <v>1602</v>
       </c>
       <c r="G1605" s="11"/>
       <c r="H1605" s="12"/>
       <c r="I1605" s="13"/>
-      <c r="J1605" s="13" t="s">
-        <v>1679</v>
-      </c>
-    </row>
-    <row r="1606" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1606" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1606" s="9"/>
+      <c r="J1605" s="13"/>
+    </row>
+    <row r="1606" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1606" s="12"/>
+      <c r="B1606" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1606" s="14" t="s">
-        <v>898</v>
+        <v>13</v>
       </c>
       <c r="D1606" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1606" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1606" s="10" t="s">
-        <v>1655</v>
+        <v>1601</v>
       </c>
       <c r="G1606" s="11"/>
       <c r="H1606" s="12"/>
       <c r="I1606" s="13"/>
       <c r="J1606" s="13"/>
     </row>
-    <row r="1607" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1607" s="12">
-        <v>44112</v>
-      </c>
-      <c r="B1607" s="9"/>
+    <row r="1607" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1607" s="12"/>
+      <c r="B1607" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1607" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1607" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1607" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1607" s="10" t="s">
-        <v>2243</v>
+        <v>1606</v>
       </c>
       <c r="G1607" s="11"/>
       <c r="H1607" s="12"/>
@@ -55603,21 +55653,21 @@
       <c r="J1607" s="13"/>
     </row>
     <row r="1608" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1608" s="12">
-        <v>44088</v>
-      </c>
-      <c r="B1608" s="9"/>
+      <c r="A1608" s="12"/>
+      <c r="B1608" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1608" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1608" s="10" t="s">
-        <v>906</v>
+        <v>584</v>
       </c>
       <c r="E1608" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1608" s="10" t="s">
-        <v>1011</v>
+        <v>1609</v>
       </c>
       <c r="G1608" s="11"/>
       <c r="H1608" s="12"/>
@@ -55625,21 +55675,21 @@
       <c r="J1608" s="13"/>
     </row>
     <row r="1609" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1609" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1609" s="9"/>
+      <c r="A1609" s="12"/>
+      <c r="B1609" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1609" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1609" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1609" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1609" s="10" t="s">
-        <v>903</v>
+        <v>1610</v>
       </c>
       <c r="G1609" s="11"/>
       <c r="H1609" s="12"/>
@@ -55647,21 +55697,19 @@
       <c r="J1609" s="13"/>
     </row>
     <row r="1610" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1610" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1610" s="12"/>
       <c r="B1610" s="9"/>
       <c r="C1610" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1610" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1610" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1610" s="10" t="s">
-        <v>902</v>
+        <v>1607</v>
       </c>
       <c r="G1610" s="11"/>
       <c r="H1610" s="12"/>
@@ -55669,30 +55717,20 @@
       <c r="J1610" s="13"/>
     </row>
     <row r="1611" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1611" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1611" s="12"/>
       <c r="B1611" s="9"/>
-      <c r="C1611" s="14" t="s">
-        <v>898</v>
-      </c>
-      <c r="D1611" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="E1611" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1611" s="10" t="s">
-        <v>900</v>
-      </c>
+      <c r="C1611" s="14"/>
+      <c r="D1611" s="10"/>
+      <c r="E1611" s="11"/>
+      <c r="F1611" s="10"/>
       <c r="G1611" s="11"/>
       <c r="H1611" s="12"/>
       <c r="I1611" s="13"/>
       <c r="J1611" s="13"/>
     </row>
-    <row r="1612" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="1612" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1612" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1612" s="9"/>
       <c r="C1612" s="14" t="s">
@@ -55702,19 +55740,21 @@
         <v>494</v>
       </c>
       <c r="E1612" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1612" s="10" t="s">
-        <v>901</v>
+        <v>1656</v>
       </c>
       <c r="G1612" s="11"/>
       <c r="H1612" s="12"/>
       <c r="I1612" s="13"/>
-      <c r="J1612" s="13"/>
-    </row>
-    <row r="1613" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="J1612" s="13" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="1613" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1613" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1613" s="9"/>
       <c r="C1613" s="14" t="s">
@@ -55724,222 +55764,376 @@
         <v>494</v>
       </c>
       <c r="E1613" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1613" s="10" t="s">
-        <v>904</v>
+        <v>1655</v>
       </c>
       <c r="G1613" s="11"/>
       <c r="H1613" s="12"/>
       <c r="I1613" s="13"/>
-      <c r="J1613" s="13" t="s">
-        <v>1585</v>
-      </c>
+      <c r="J1613" s="13"/>
     </row>
     <row r="1614" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1614" s="12">
-        <v>44047</v>
+        <v>44112</v>
       </c>
       <c r="B1614" s="9"/>
       <c r="C1614" s="14" t="s">
-        <v>537</v>
+        <v>623</v>
       </c>
       <c r="D1614" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E1614" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1614" s="10" t="s">
-        <v>873</v>
-      </c>
-      <c r="G1614" s="11" t="s">
-        <v>1621</v>
-      </c>
+        <v>2243</v>
+      </c>
+      <c r="G1614" s="11"/>
       <c r="H1614" s="12"/>
       <c r="I1614" s="13"/>
       <c r="J1614" s="13"/>
     </row>
-    <row r="1615" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1615" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1615" s="12">
-        <v>43949</v>
+        <v>44088</v>
       </c>
       <c r="B1615" s="9"/>
       <c r="C1615" s="14" t="s">
-        <v>468</v>
+        <v>19</v>
       </c>
       <c r="D1615" s="10" t="s">
-        <v>89</v>
+        <v>906</v>
       </c>
       <c r="E1615" s="11" t="s">
         <v>685</v>
       </c>
       <c r="F1615" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1615" s="11" t="s">
-        <v>1636</v>
-      </c>
+        <v>1011</v>
+      </c>
+      <c r="G1615" s="11"/>
       <c r="H1615" s="12"/>
-      <c r="I1615" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1615" s="13"/>
       <c r="J1615" s="13"/>
     </row>
-    <row r="1616" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1616" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1616" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1616" s="9"/>
       <c r="C1616" s="14" t="s">
-        <v>468</v>
+        <v>623</v>
       </c>
       <c r="D1616" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1616" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1616" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1616" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>903</v>
+      </c>
+      <c r="G1616" s="11"/>
       <c r="H1616" s="12"/>
-      <c r="I1616" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1616" s="13" t="s">
-        <v>1565</v>
-      </c>
-    </row>
-    <row r="1617" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1616" s="13"/>
+      <c r="J1616" s="13"/>
+    </row>
+    <row r="1617" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1617" s="12">
-        <v>43838</v>
+        <v>44055</v>
       </c>
       <c r="B1617" s="9"/>
       <c r="C1617" s="14" t="s">
-        <v>103</v>
+        <v>623</v>
       </c>
       <c r="D1617" s="10" t="s">
-        <v>460</v>
+        <v>6</v>
       </c>
       <c r="E1617" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1617" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G1617" s="11" t="s">
-        <v>1637</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="G1617" s="11"/>
       <c r="H1617" s="12"/>
       <c r="I1617" s="13"/>
-      <c r="J1617" s="13" t="s">
-        <v>1530</v>
-      </c>
-    </row>
-    <row r="1618" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1617" s="13"/>
+    </row>
+    <row r="1618" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1618" s="12">
-        <v>43762</v>
+        <v>44055</v>
       </c>
       <c r="B1618" s="9"/>
       <c r="C1618" s="14" t="s">
-        <v>446</v>
+        <v>898</v>
       </c>
       <c r="D1618" s="10" t="s">
-        <v>17</v>
+        <v>494</v>
       </c>
       <c r="E1618" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1618" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G1618" s="11" t="s">
-        <v>1626</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="G1618" s="11"/>
       <c r="H1618" s="12"/>
       <c r="I1618" s="13"/>
       <c r="J1618" s="13"/>
     </row>
-    <row r="1619" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1619" s="12"/>
+    <row r="1619" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A1619" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1619" s="9"/>
-      <c r="C1619" s="14"/>
-      <c r="D1619" s="10"/>
-      <c r="E1619" s="11"/>
-      <c r="F1619" s="10"/>
+      <c r="C1619" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1619" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1619" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1619" s="10" t="s">
+        <v>901</v>
+      </c>
       <c r="G1619" s="11"/>
       <c r="H1619" s="12"/>
       <c r="I1619" s="13"/>
       <c r="J1619" s="13"/>
     </row>
-    <row r="1620" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1620" s="12"/>
+    <row r="1620" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1620" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1620" s="9"/>
-      <c r="C1620" s="14"/>
-      <c r="D1620" s="10"/>
-      <c r="E1620" s="11"/>
-      <c r="F1620" s="10"/>
+      <c r="C1620" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1620" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1620" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1620" s="10" t="s">
+        <v>904</v>
+      </c>
       <c r="G1620" s="11"/>
       <c r="H1620" s="12"/>
       <c r="I1620" s="13"/>
-      <c r="J1620" s="13"/>
-    </row>
-    <row r="1621" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1621" s="12"/>
+      <c r="J1620" s="13" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="1621" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1621" s="12">
+        <v>44047</v>
+      </c>
       <c r="B1621" s="9"/>
-      <c r="C1621" s="14"/>
-      <c r="D1621" s="10"/>
-      <c r="E1621" s="11"/>
-      <c r="F1621" s="10"/>
-      <c r="G1621" s="11"/>
+      <c r="C1621" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1621" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1621" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1621" s="10" t="s">
+        <v>873</v>
+      </c>
+      <c r="G1621" s="11" t="s">
+        <v>1621</v>
+      </c>
       <c r="H1621" s="12"/>
       <c r="I1621" s="13"/>
       <c r="J1621" s="13"/>
     </row>
-    <row r="1622" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1622" s="12"/>
+    <row r="1622" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1622" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1622" s="9"/>
-      <c r="C1622" s="14"/>
-      <c r="D1622" s="10"/>
-      <c r="E1622" s="11"/>
-      <c r="F1622" s="10"/>
-      <c r="G1622" s="11"/>
+      <c r="C1622" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1622" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1622" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1622" s="10" t="s">
+        <v>686</v>
+      </c>
+      <c r="G1622" s="11" t="s">
+        <v>1636</v>
+      </c>
       <c r="H1622" s="12"/>
-      <c r="I1622" s="13"/>
+      <c r="I1622" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1622" s="13"/>
     </row>
-    <row r="1623" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1623" s="12"/>
+    <row r="1623" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1623" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1623" s="9"/>
-      <c r="C1623" s="14"/>
-      <c r="D1623" s="10"/>
-      <c r="E1623" s="11"/>
-      <c r="F1623" s="10"/>
-      <c r="G1623" s="11"/>
+      <c r="C1623" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1623" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1623" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1623" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="G1623" s="11" t="s">
+        <v>687</v>
+      </c>
       <c r="H1623" s="12"/>
-      <c r="I1623" s="13"/>
-      <c r="J1623" s="13"/>
-    </row>
-    <row r="1624" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1624" s="12"/>
+      <c r="I1623" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1623" s="13" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="1624" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1624" s="12">
+        <v>43838</v>
+      </c>
       <c r="B1624" s="9"/>
-      <c r="C1624" s="14"/>
-      <c r="D1624" s="10"/>
-      <c r="E1624" s="11"/>
-      <c r="F1624" s="10"/>
-      <c r="G1624" s="11"/>
+      <c r="C1624" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1624" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1624" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1624" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G1624" s="11" t="s">
+        <v>1637</v>
+      </c>
       <c r="H1624" s="12"/>
       <c r="I1624" s="13"/>
-      <c r="J1624" s="13"/>
+      <c r="J1624" s="13" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="1625" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1625" s="12">
+        <v>43762</v>
+      </c>
+      <c r="B1625" s="9"/>
+      <c r="C1625" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1625" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1625" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1625" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1625" s="11" t="s">
+        <v>1626</v>
+      </c>
+      <c r="H1625" s="12"/>
+      <c r="I1625" s="13"/>
+      <c r="J1625" s="13"/>
+    </row>
+    <row r="1626" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1626" s="12"/>
+      <c r="B1626" s="9"/>
+      <c r="C1626" s="14"/>
+      <c r="D1626" s="10"/>
+      <c r="E1626" s="11"/>
+      <c r="F1626" s="10"/>
+      <c r="G1626" s="11"/>
+      <c r="H1626" s="12"/>
+      <c r="I1626" s="13"/>
+      <c r="J1626" s="13"/>
+    </row>
+    <row r="1627" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1627" s="12"/>
+      <c r="B1627" s="9"/>
+      <c r="C1627" s="14"/>
+      <c r="D1627" s="10"/>
+      <c r="E1627" s="11"/>
+      <c r="F1627" s="10"/>
+      <c r="G1627" s="11"/>
+      <c r="H1627" s="12"/>
+      <c r="I1627" s="13"/>
+      <c r="J1627" s="13"/>
+    </row>
+    <row r="1628" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1628" s="12"/>
+      <c r="B1628" s="9"/>
+      <c r="C1628" s="14"/>
+      <c r="D1628" s="10"/>
+      <c r="E1628" s="11"/>
+      <c r="F1628" s="10"/>
+      <c r="G1628" s="11"/>
+      <c r="H1628" s="12"/>
+      <c r="I1628" s="13"/>
+      <c r="J1628" s="13"/>
+    </row>
+    <row r="1629" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1629" s="12"/>
+      <c r="B1629" s="9"/>
+      <c r="C1629" s="14"/>
+      <c r="D1629" s="10"/>
+      <c r="E1629" s="11"/>
+      <c r="F1629" s="10"/>
+      <c r="G1629" s="11"/>
+      <c r="H1629" s="12"/>
+      <c r="I1629" s="13"/>
+      <c r="J1629" s="13"/>
+    </row>
+    <row r="1630" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1630" s="12"/>
+      <c r="B1630" s="9"/>
+      <c r="C1630" s="14"/>
+      <c r="D1630" s="10"/>
+      <c r="E1630" s="11"/>
+      <c r="F1630" s="10"/>
+      <c r="G1630" s="11"/>
+      <c r="H1630" s="12"/>
+      <c r="I1630" s="13"/>
+      <c r="J1630" s="13"/>
+    </row>
+    <row r="1631" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1631" s="12"/>
+      <c r="B1631" s="9"/>
+      <c r="C1631" s="14"/>
+      <c r="D1631" s="10"/>
+      <c r="E1631" s="11"/>
+      <c r="F1631" s="10"/>
+      <c r="G1631" s="11"/>
+      <c r="H1631" s="12"/>
+      <c r="I1631" s="13"/>
+      <c r="J1631" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1480" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1593:F1603">
-    <sortCondition ref="F1593:F1603"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1600:F1610">
+    <sortCondition ref="F1600:F1610"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Correção BKGCTR15 para somente o mês atual
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB1A58B-398C-4644-ACBF-E44ACA5A7DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E034B533-4E1D-4AE5-A760-20E5957BDA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12133" uniqueCount="2406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12141" uniqueCount="2408">
   <si>
     <t>Responsável</t>
   </si>
@@ -7630,6 +7630,13 @@
   </si>
   <si>
     <t>Reconstituição do ambiente e base de testes para a versão 12.1.33 e limpeza de arquivos temporarios gerados na migração de versão</t>
+  </si>
+  <si>
+    <t>Proventos do contrato 179000580 não apareceram no mês de outubro/2021</t>
+  </si>
+  <si>
+    <t>UPDATE  CUSTOSIGA SET ccSIGA='179000580'
+ where ccSIGA='Er:000580'</t>
   </si>
 </sst>
 </file>
@@ -8401,8 +8408,8 @@
   <dimension ref="A1:J1756"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1695" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1708" sqref="F1708"/>
+      <pane ySplit="1" topLeftCell="A1698" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1709" sqref="A1709"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -59409,17 +59416,37 @@
       </c>
       <c r="J1707" s="13"/>
     </row>
-    <row r="1708" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1708" s="12"/>
-      <c r="B1708" s="12"/>
-      <c r="C1708" s="14"/>
-      <c r="D1708" s="10"/>
-      <c r="E1708" s="11"/>
-      <c r="F1708" s="10"/>
-      <c r="G1708" s="11"/>
-      <c r="H1708" s="12"/>
-      <c r="I1708" s="13"/>
-      <c r="J1708" s="13"/>
+    <row r="1708" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1708" s="12">
+        <v>44540</v>
+      </c>
+      <c r="B1708" s="12">
+        <v>44540</v>
+      </c>
+      <c r="C1708" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="D1708" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1708" s="11" t="s">
+        <v>494</v>
+      </c>
+      <c r="F1708" s="10" t="s">
+        <v>2406</v>
+      </c>
+      <c r="G1708" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1708" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1708" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1708" s="13" t="s">
+        <v>2407</v>
+      </c>
     </row>
     <row r="1709" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1709" s="12"/>

</xml_diff>

<commit_message>
Alterações lib Docs de Entrada - Compras
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE9EE2C-E691-44BE-887B-82B0303E1F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1A7717-88F4-4040-A7D0-3FDD3783E1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12374" uniqueCount="2446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12452" uniqueCount="2457">
   <si>
     <t>Responsável</t>
   </si>
@@ -7752,6 +7752,40 @@
   </si>
   <si>
     <t>Alteração dos produtos (aliq ISS = 2% e TES=505), Planilhas (Rec INSS=N, Emissaõ Normal), Itens de Planilhas (TES=505), referentes aos pedidos de vendas: 50137, 50138, 50140, 50142, 50143, 50144, 50149 e 50151 (evitando-se a bitributação pela Petrobras)</t>
+  </si>
+  <si>
+    <t>Excluir o titulo 000002601 LILIAN CRISTIANE MORAES da BHG lançado em duplicidade</t>
+  </si>
+  <si>
+    <t>Corrigir contrato com nome de cliente em branco</t>
+  </si>
+  <si>
+    <t>Dúvidas sobre relatorio de titulos em aberto</t>
+  </si>
+  <si>
+    <t>Alterar campo no layout do cnab a pagar Itau para não consistir CPF quando for título de pensão</t>
+  </si>
+  <si>
+    <t>Recuperar registros deletados de ISS das NFs 4632 de 151,17, 4634 de 151,17, 4634 de 454,65, 4523 de 751,32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Por gentileza, alterar no sistema as notas fiscais 000003876 e 000003877,  estão com o valor de ISS a maior no sistema.  Conforme analisado o ISS delas é 2 %, porém o sistema está puxando 5%, causando assim uma diferença entre meu sistema e prefeitura.
+Nota Fiscal 3876 : 55.628,46 * 2 % = 1.112,57  Valor Correto – Valor na planilha Incorreto  = 2.781,42 Valor faturado  3877 : 67.336,20 * 2% = 1.346,72 Valor Correto – Valor na Planilha Incorreto = 3.336,81     </t>
+  </si>
+  <si>
+    <t>Liquidação e compensação de alguns titulos de ISS</t>
+  </si>
+  <si>
+    <t>Problemas com revisão de contratos - campo loja desabilitado</t>
+  </si>
+  <si>
+    <t>Verificação de diferença entre o sistema e o EFD Contribuições</t>
+  </si>
+  <si>
+    <t>Exclusãod de diversas pré-notas não aprovadas no sistema</t>
+  </si>
+  <si>
+    <t>Problemas no estorno da NF 000021531</t>
   </si>
 </sst>
 </file>
@@ -8520,11 +8554,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1786"/>
+  <dimension ref="A1:J1799"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1731" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1737" sqref="C1737"/>
+      <pane ySplit="1" topLeftCell="A1746" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1754" sqref="A1754:XFD1756"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -60600,192 +60634,340 @@
       <c r="J1742" s="13"/>
     </row>
     <row r="1743" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1743" s="12"/>
-      <c r="B1743" s="12"/>
-      <c r="C1743" s="14"/>
-      <c r="D1743" s="10"/>
-      <c r="E1743" s="11"/>
-      <c r="F1743" s="10"/>
-      <c r="G1743" s="11"/>
-      <c r="H1743" s="12"/>
-      <c r="I1743" s="13"/>
+      <c r="A1743" s="12">
+        <v>44567</v>
+      </c>
+      <c r="B1743" s="12">
+        <v>44567</v>
+      </c>
+      <c r="C1743" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1743" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1743" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1743" s="10" t="s">
+        <v>2446</v>
+      </c>
+      <c r="G1743" s="11" t="s">
+        <v>1641</v>
+      </c>
+      <c r="H1743" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1743" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1743" s="13"/>
     </row>
     <row r="1744" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1744" s="12"/>
-      <c r="B1744" s="12"/>
-      <c r="C1744" s="14"/>
-      <c r="D1744" s="10"/>
-      <c r="E1744" s="11"/>
-      <c r="F1744" s="10"/>
-      <c r="G1744" s="11"/>
-      <c r="H1744" s="12"/>
-      <c r="I1744" s="13"/>
+      <c r="A1744" s="12">
+        <v>44567</v>
+      </c>
+      <c r="B1744" s="12">
+        <v>44567</v>
+      </c>
+      <c r="C1744" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1744" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1744" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1744" s="10" t="s">
+        <v>2447</v>
+      </c>
+      <c r="G1744" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1744" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1744" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1744" s="13"/>
     </row>
     <row r="1745" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1745" s="12"/>
-      <c r="B1745" s="12"/>
-      <c r="C1745" s="14"/>
-      <c r="D1745" s="10"/>
-      <c r="E1745" s="11"/>
-      <c r="F1745" s="10"/>
-      <c r="G1745" s="11"/>
-      <c r="H1745" s="12"/>
-      <c r="I1745" s="13"/>
+      <c r="A1745" s="12">
+        <v>44567</v>
+      </c>
+      <c r="B1745" s="12">
+        <v>44567</v>
+      </c>
+      <c r="C1745" s="14" t="s">
+        <v>2173</v>
+      </c>
+      <c r="D1745" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1745" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1745" s="10" t="s">
+        <v>2448</v>
+      </c>
+      <c r="G1745" s="11" t="s">
+        <v>1616</v>
+      </c>
+      <c r="H1745" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1745" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1745" s="13"/>
     </row>
-    <row r="1746" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1746" s="12"/>
-      <c r="B1746" s="12"/>
-      <c r="C1746" s="14"/>
-      <c r="D1746" s="10"/>
-      <c r="E1746" s="11"/>
-      <c r="F1746" s="10"/>
-      <c r="G1746" s="11"/>
-      <c r="H1746" s="12"/>
-      <c r="I1746" s="13"/>
-      <c r="J1746" s="13"/>
-    </row>
-    <row r="1747" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1746" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1746" s="12">
+        <v>44567</v>
+      </c>
+      <c r="B1746" s="12">
+        <v>44567</v>
+      </c>
+      <c r="C1746" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1746" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1746" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1746" s="10" t="s">
+        <v>2449</v>
+      </c>
+      <c r="G1746" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1746" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1746" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1746" s="13" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1747" s="12">
-        <v>44522</v>
-      </c>
-      <c r="B1747" s="12"/>
+        <v>44567</v>
+      </c>
+      <c r="B1747" s="12">
+        <v>44567</v>
+      </c>
       <c r="C1747" s="14" t="s">
-        <v>46</v>
+        <v>462</v>
       </c>
       <c r="D1747" s="10" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="E1747" s="11" t="s">
-        <v>570</v>
+        <v>620</v>
       </c>
       <c r="F1747" s="10" t="s">
-        <v>2369</v>
-      </c>
-      <c r="G1747" s="11"/>
-      <c r="H1747" s="12"/>
-      <c r="I1747" s="13"/>
+        <v>2450</v>
+      </c>
+      <c r="G1747" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1747" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1747" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1747" s="13"/>
     </row>
-    <row r="1748" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1748" spans="1:10" ht="84" x14ac:dyDescent="0.2">
       <c r="A1748" s="12">
-        <v>43816</v>
-      </c>
-      <c r="B1748" s="9"/>
+        <v>44568</v>
+      </c>
+      <c r="B1748" s="12">
+        <v>44568</v>
+      </c>
       <c r="C1748" s="14" t="s">
-        <v>475</v>
+        <v>1986</v>
       </c>
       <c r="D1748" s="10" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="E1748" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1748" s="10" t="s">
-        <v>474</v>
+        <v>2451</v>
       </c>
       <c r="G1748" s="11" t="s">
-        <v>1627</v>
-      </c>
-      <c r="H1748" s="12"/>
-      <c r="I1748" s="13"/>
-      <c r="J1748" s="13" t="s">
-        <v>1565</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="H1748" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1748" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1748" s="13"/>
     </row>
     <row r="1749" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1749" s="12">
-        <v>44460</v>
-      </c>
-      <c r="B1749" s="12"/>
+        <v>44568</v>
+      </c>
+      <c r="B1749" s="12">
+        <v>44568</v>
+      </c>
       <c r="C1749" s="14" t="s">
-        <v>19</v>
+        <v>623</v>
       </c>
       <c r="D1749" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1749" s="11" t="s">
         <v>837</v>
       </c>
       <c r="F1749" s="10" t="s">
-        <v>2193</v>
-      </c>
-      <c r="G1749" s="11"/>
-      <c r="H1749" s="12"/>
-      <c r="I1749" s="13"/>
+        <v>2452</v>
+      </c>
+      <c r="G1749" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1749" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1749" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1749" s="13"/>
     </row>
     <row r="1750" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1750" s="12"/>
-      <c r="B1750" s="12"/>
-      <c r="C1750" s="14"/>
-      <c r="D1750" s="10"/>
-      <c r="E1750" s="11"/>
-      <c r="F1750" s="10"/>
-      <c r="G1750" s="11"/>
-      <c r="H1750" s="12"/>
-      <c r="I1750" s="13"/>
+      <c r="A1750" s="12">
+        <v>44568</v>
+      </c>
+      <c r="B1750" s="12">
+        <v>44568</v>
+      </c>
+      <c r="C1750" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1750" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1750" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1750" s="10" t="s">
+        <v>2453</v>
+      </c>
+      <c r="G1750" s="11" t="s">
+        <v>1616</v>
+      </c>
+      <c r="H1750" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1750" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="J1750" s="13"/>
     </row>
     <row r="1751" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1751" s="12"/>
-      <c r="B1751" s="12"/>
-      <c r="C1751" s="14"/>
-      <c r="D1751" s="10"/>
-      <c r="E1751" s="11"/>
-      <c r="F1751" s="10"/>
-      <c r="G1751" s="11"/>
-      <c r="H1751" s="12"/>
-      <c r="I1751" s="13"/>
+      <c r="A1751" s="12">
+        <v>44571</v>
+      </c>
+      <c r="B1751" s="12">
+        <v>44571</v>
+      </c>
+      <c r="C1751" s="14" t="s">
+        <v>1986</v>
+      </c>
+      <c r="D1751" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1751" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1751" s="10" t="s">
+        <v>2454</v>
+      </c>
+      <c r="G1751" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1751" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1751" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1751" s="13"/>
     </row>
     <row r="1752" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1752" s="12"/>
-      <c r="B1752" s="9"/>
-      <c r="C1752" s="14"/>
-      <c r="D1752" s="10"/>
-      <c r="E1752" s="11"/>
-      <c r="F1752" s="10"/>
-      <c r="G1752" s="11"/>
-      <c r="H1752" s="12"/>
-      <c r="I1752" s="13"/>
+      <c r="A1752" s="12">
+        <v>44571</v>
+      </c>
+      <c r="B1752" s="12">
+        <v>44572</v>
+      </c>
+      <c r="C1752" s="14" t="s">
+        <v>2269</v>
+      </c>
+      <c r="D1752" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1752" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1752" s="10" t="s">
+        <v>2455</v>
+      </c>
+      <c r="G1752" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1752" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1752" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1752" s="13"/>
     </row>
     <row r="1753" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1753" s="1" t="s">
-        <v>1475</v>
-      </c>
-      <c r="B1753" s="2" t="s">
-        <v>1476</v>
-      </c>
-      <c r="C1753" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1753" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1753" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1753" s="4" t="s">
-        <v>1575</v>
-      </c>
-      <c r="G1753" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1753" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1753" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1753" s="36"/>
+      <c r="A1753" s="12">
+        <v>44572</v>
+      </c>
+      <c r="B1753" s="12">
+        <v>44572</v>
+      </c>
+      <c r="C1753" s="14" t="s">
+        <v>2269</v>
+      </c>
+      <c r="D1753" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1753" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1753" s="10" t="s">
+        <v>2456</v>
+      </c>
+      <c r="G1753" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1753" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1753" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1753" s="13"/>
     </row>
     <row r="1754" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1754" s="12"/>
-      <c r="B1754" s="9"/>
+      <c r="B1754" s="12"/>
       <c r="C1754" s="14"/>
       <c r="D1754" s="10"/>
       <c r="E1754" s="11"/>
@@ -60797,21 +60979,11 @@
     </row>
     <row r="1755" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1755" s="12"/>
-      <c r="B1755" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1755" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1755" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1755" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1755" s="10" t="s">
-        <v>1609</v>
-      </c>
+      <c r="B1755" s="12"/>
+      <c r="C1755" s="14"/>
+      <c r="D1755" s="10"/>
+      <c r="E1755" s="11"/>
+      <c r="F1755" s="10"/>
       <c r="G1755" s="11"/>
       <c r="H1755" s="12"/>
       <c r="I1755" s="13"/>
@@ -60819,21 +60991,11 @@
     </row>
     <row r="1756" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1756" s="12"/>
-      <c r="B1756" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1756" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1756" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1756" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1756" s="10" t="s">
-        <v>1601</v>
-      </c>
+      <c r="B1756" s="12"/>
+      <c r="C1756" s="14"/>
+      <c r="D1756" s="10"/>
+      <c r="E1756" s="11"/>
+      <c r="F1756" s="10"/>
       <c r="G1756" s="11"/>
       <c r="H1756" s="12"/>
       <c r="I1756" s="13"/>
@@ -60841,21 +61003,11 @@
     </row>
     <row r="1757" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1757" s="12"/>
-      <c r="B1757" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1757" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1757" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1757" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1757" s="10" t="s">
-        <v>1606</v>
-      </c>
+      <c r="B1757" s="12"/>
+      <c r="C1757" s="14"/>
+      <c r="D1757" s="10"/>
+      <c r="E1757" s="11"/>
+      <c r="F1757" s="10"/>
       <c r="G1757" s="11"/>
       <c r="H1757" s="12"/>
       <c r="I1757" s="13"/>
@@ -60863,21 +61015,11 @@
     </row>
     <row r="1758" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1758" s="12"/>
-      <c r="B1758" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1758" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1758" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1758" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1758" s="10" t="s">
-        <v>1602</v>
-      </c>
+      <c r="B1758" s="12"/>
+      <c r="C1758" s="14"/>
+      <c r="D1758" s="10"/>
+      <c r="E1758" s="11"/>
+      <c r="F1758" s="10"/>
       <c r="G1758" s="11"/>
       <c r="H1758" s="12"/>
       <c r="I1758" s="13"/>
@@ -60885,40 +61027,32 @@
     </row>
     <row r="1759" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1759" s="12"/>
-      <c r="B1759" s="9"/>
-      <c r="C1759" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1759" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1759" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1759" s="10" t="s">
-        <v>1610</v>
-      </c>
+      <c r="B1759" s="12"/>
+      <c r="C1759" s="14"/>
+      <c r="D1759" s="10"/>
+      <c r="E1759" s="11"/>
+      <c r="F1759" s="10"/>
       <c r="G1759" s="11"/>
       <c r="H1759" s="12"/>
       <c r="I1759" s="13"/>
       <c r="J1759" s="13"/>
     </row>
-    <row r="1760" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1760" s="12"/>
-      <c r="B1760" s="12">
-        <v>44402</v>
-      </c>
+    <row r="1760" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1760" s="12">
+        <v>44522</v>
+      </c>
+      <c r="B1760" s="12"/>
       <c r="C1760" s="14" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="D1760" s="10" t="s">
-        <v>584</v>
+        <v>6</v>
       </c>
       <c r="E1760" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1760" s="10" t="s">
-        <v>1603</v>
+        <v>2369</v>
       </c>
       <c r="G1760" s="11"/>
       <c r="H1760" s="12"/>
@@ -60926,41 +61060,47 @@
       <c r="J1760" s="13"/>
     </row>
     <row r="1761" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1761" s="12"/>
+      <c r="A1761" s="12">
+        <v>43816</v>
+      </c>
       <c r="B1761" s="9"/>
       <c r="C1761" s="14" t="s">
-        <v>13</v>
+        <v>475</v>
       </c>
       <c r="D1761" s="10" t="s">
-        <v>584</v>
+        <v>38</v>
       </c>
       <c r="E1761" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1761" s="10" t="s">
-        <v>1600</v>
-      </c>
-      <c r="G1761" s="11"/>
+        <v>474</v>
+      </c>
+      <c r="G1761" s="11" t="s">
+        <v>1627</v>
+      </c>
       <c r="H1761" s="12"/>
       <c r="I1761" s="13"/>
-      <c r="J1761" s="13"/>
+      <c r="J1761" s="13" t="s">
+        <v>1565</v>
+      </c>
     </row>
     <row r="1762" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1762" s="12"/>
-      <c r="B1762" s="12">
-        <v>44402</v>
-      </c>
+      <c r="A1762" s="12">
+        <v>44460</v>
+      </c>
+      <c r="B1762" s="12"/>
       <c r="C1762" s="14" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D1762" s="10" t="s">
-        <v>584</v>
+        <v>494</v>
       </c>
       <c r="E1762" s="11" t="s">
-        <v>647</v>
+        <v>837</v>
       </c>
       <c r="F1762" s="10" t="s">
-        <v>1599</v>
+        <v>2193</v>
       </c>
       <c r="G1762" s="11"/>
       <c r="H1762" s="12"/>
@@ -60969,21 +61109,11 @@
     </row>
     <row r="1763" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1763" s="12"/>
-      <c r="B1763" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1763" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1763" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1763" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1763" s="10" t="s">
-        <v>1604</v>
-      </c>
+      <c r="B1763" s="12"/>
+      <c r="C1763" s="14"/>
+      <c r="D1763" s="10"/>
+      <c r="E1763" s="11"/>
+      <c r="F1763" s="10"/>
       <c r="G1763" s="11"/>
       <c r="H1763" s="12"/>
       <c r="I1763" s="13"/>
@@ -60991,21 +61121,11 @@
     </row>
     <row r="1764" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1764" s="12"/>
-      <c r="B1764" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1764" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1764" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1764" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1764" s="10" t="s">
-        <v>1607</v>
-      </c>
+      <c r="B1764" s="12"/>
+      <c r="C1764" s="14"/>
+      <c r="D1764" s="10"/>
+      <c r="E1764" s="11"/>
+      <c r="F1764" s="10"/>
       <c r="G1764" s="11"/>
       <c r="H1764" s="12"/>
       <c r="I1764" s="13"/>
@@ -61013,45 +61133,45 @@
     </row>
     <row r="1765" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1765" s="12"/>
-      <c r="B1765" s="9">
-        <v>44235</v>
-      </c>
-      <c r="C1765" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1765" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1765" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1765" s="10" t="s">
-        <v>1608</v>
-      </c>
+      <c r="B1765" s="9"/>
+      <c r="C1765" s="14"/>
+      <c r="D1765" s="10"/>
+      <c r="E1765" s="11"/>
+      <c r="F1765" s="10"/>
       <c r="G1765" s="11"/>
       <c r="H1765" s="12"/>
       <c r="I1765" s="13"/>
       <c r="J1765" s="13"/>
     </row>
     <row r="1766" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1766" s="12"/>
-      <c r="B1766" s="9"/>
-      <c r="C1766" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1766" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1766" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1766" s="10" t="s">
-        <v>1605</v>
-      </c>
-      <c r="G1766" s="11"/>
-      <c r="H1766" s="12"/>
-      <c r="I1766" s="13"/>
-      <c r="J1766" s="13"/>
+      <c r="A1766" s="1" t="s">
+        <v>1475</v>
+      </c>
+      <c r="B1766" s="2" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C1766" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1766" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1766" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1766" s="4" t="s">
+        <v>1575</v>
+      </c>
+      <c r="G1766" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1766" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1766" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1766" s="36"/>
     </row>
     <row r="1767" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1767" s="12"/>
@@ -61065,68 +61185,66 @@
       <c r="I1767" s="13"/>
       <c r="J1767" s="13"/>
     </row>
-    <row r="1768" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1768" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1768" s="9"/>
+    <row r="1768" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1768" s="12"/>
+      <c r="B1768" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1768" s="14" t="s">
-        <v>897</v>
+        <v>13</v>
       </c>
       <c r="D1768" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1768" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1768" s="10" t="s">
-        <v>1654</v>
+        <v>1609</v>
       </c>
       <c r="G1768" s="11"/>
       <c r="H1768" s="12"/>
       <c r="I1768" s="13"/>
-      <c r="J1768" s="13" t="s">
-        <v>1677</v>
-      </c>
-    </row>
-    <row r="1769" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1769" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1769" s="9"/>
+      <c r="J1768" s="13"/>
+    </row>
+    <row r="1769" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1769" s="12"/>
+      <c r="B1769" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1769" s="14" t="s">
-        <v>897</v>
+        <v>13</v>
       </c>
       <c r="D1769" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1769" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1769" s="10" t="s">
-        <v>1653</v>
+        <v>1601</v>
       </c>
       <c r="G1769" s="11"/>
       <c r="H1769" s="12"/>
       <c r="I1769" s="13"/>
       <c r="J1769" s="13"/>
     </row>
-    <row r="1770" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1770" s="12">
-        <v>44112</v>
-      </c>
-      <c r="B1770" s="9"/>
+    <row r="1770" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1770" s="12"/>
+      <c r="B1770" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1770" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1770" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1770" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1770" s="10" t="s">
-        <v>2241</v>
+        <v>1606</v>
       </c>
       <c r="G1770" s="11"/>
       <c r="H1770" s="12"/>
@@ -61134,21 +61252,21 @@
       <c r="J1770" s="13"/>
     </row>
     <row r="1771" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1771" s="12">
-        <v>44088</v>
-      </c>
-      <c r="B1771" s="9"/>
+      <c r="A1771" s="12"/>
+      <c r="B1771" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1771" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1771" s="10" t="s">
-        <v>905</v>
+        <v>584</v>
       </c>
       <c r="E1771" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1771" s="10" t="s">
-        <v>1010</v>
+        <v>1602</v>
       </c>
       <c r="G1771" s="11"/>
       <c r="H1771" s="12"/>
@@ -61156,21 +61274,19 @@
       <c r="J1771" s="13"/>
     </row>
     <row r="1772" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1772" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1772" s="12"/>
       <c r="B1772" s="9"/>
       <c r="C1772" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1772" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1772" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1772" s="10" t="s">
-        <v>902</v>
+        <v>1610</v>
       </c>
       <c r="G1772" s="11"/>
       <c r="H1772" s="12"/>
@@ -61178,21 +61294,21 @@
       <c r="J1772" s="13"/>
     </row>
     <row r="1773" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1773" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1773" s="9"/>
+      <c r="A1773" s="12"/>
+      <c r="B1773" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1773" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1773" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1773" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1773" s="10" t="s">
-        <v>901</v>
+        <v>1603</v>
       </c>
       <c r="G1773" s="11"/>
       <c r="H1773" s="12"/>
@@ -61200,253 +61316,527 @@
       <c r="J1773" s="13"/>
     </row>
     <row r="1774" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1774" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1774" s="12"/>
       <c r="B1774" s="9"/>
       <c r="C1774" s="14" t="s">
-        <v>897</v>
+        <v>13</v>
       </c>
       <c r="D1774" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1774" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1774" s="10" t="s">
-        <v>899</v>
+        <v>1600</v>
       </c>
       <c r="G1774" s="11"/>
       <c r="H1774" s="12"/>
       <c r="I1774" s="13"/>
       <c r="J1774" s="13"/>
     </row>
-    <row r="1775" spans="1:10" ht="108" x14ac:dyDescent="0.2">
-      <c r="A1775" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1775" s="9"/>
+    <row r="1775" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1775" s="12"/>
+      <c r="B1775" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1775" s="14" t="s">
-        <v>897</v>
+        <v>13</v>
       </c>
       <c r="D1775" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1775" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1775" s="10" t="s">
-        <v>900</v>
+        <v>1599</v>
       </c>
       <c r="G1775" s="11"/>
       <c r="H1775" s="12"/>
       <c r="I1775" s="13"/>
       <c r="J1775" s="13"/>
     </row>
-    <row r="1776" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A1776" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1776" s="9"/>
+    <row r="1776" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1776" s="12"/>
+      <c r="B1776" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1776" s="14" t="s">
-        <v>897</v>
+        <v>13</v>
       </c>
       <c r="D1776" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1776" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1776" s="10" t="s">
-        <v>903</v>
+        <v>1604</v>
       </c>
       <c r="G1776" s="11"/>
       <c r="H1776" s="12"/>
       <c r="I1776" s="13"/>
-      <c r="J1776" s="13" t="s">
-        <v>1583</v>
-      </c>
-    </row>
-    <row r="1777" spans="1:10" ht="168" x14ac:dyDescent="0.2">
-      <c r="A1777" s="12">
-        <v>43949</v>
-      </c>
-      <c r="B1777" s="9"/>
+      <c r="J1776" s="13"/>
+    </row>
+    <row r="1777" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1777" s="12"/>
+      <c r="B1777" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1777" s="14" t="s">
-        <v>468</v>
+        <v>13</v>
       </c>
       <c r="D1777" s="10" t="s">
-        <v>89</v>
+        <v>584</v>
       </c>
       <c r="E1777" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1777" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1777" s="11" t="s">
-        <v>1634</v>
-      </c>
+        <v>1607</v>
+      </c>
+      <c r="G1777" s="11"/>
       <c r="H1777" s="12"/>
-      <c r="I1777" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1777" s="13"/>
       <c r="J1777" s="13"/>
     </row>
-    <row r="1778" spans="1:10" ht="168" x14ac:dyDescent="0.2">
-      <c r="A1778" s="12">
-        <v>43949</v>
-      </c>
-      <c r="B1778" s="9"/>
+    <row r="1778" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1778" s="12"/>
+      <c r="B1778" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1778" s="14" t="s">
-        <v>468</v>
+        <v>13</v>
       </c>
       <c r="D1778" s="10" t="s">
-        <v>89</v>
+        <v>584</v>
       </c>
       <c r="E1778" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1778" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1778" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>1608</v>
+      </c>
+      <c r="G1778" s="11"/>
       <c r="H1778" s="12"/>
-      <c r="I1778" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1778" s="13" t="s">
-        <v>1564</v>
-      </c>
-    </row>
-    <row r="1779" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1779" s="12">
-        <v>43838</v>
-      </c>
+      <c r="I1778" s="13"/>
+      <c r="J1778" s="13"/>
+    </row>
+    <row r="1779" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1779" s="12"/>
       <c r="B1779" s="9"/>
       <c r="C1779" s="14" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="D1779" s="10" t="s">
-        <v>460</v>
+        <v>584</v>
       </c>
       <c r="E1779" s="11" t="s">
         <v>647</v>
       </c>
       <c r="F1779" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G1779" s="11" t="s">
-        <v>1635</v>
-      </c>
+        <v>1605</v>
+      </c>
+      <c r="G1779" s="11"/>
       <c r="H1779" s="12"/>
       <c r="I1779" s="13"/>
-      <c r="J1779" s="13" t="s">
-        <v>1529</v>
-      </c>
-    </row>
-    <row r="1780" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1780" s="12">
-        <v>43762</v>
-      </c>
+      <c r="J1779" s="13"/>
+    </row>
+    <row r="1780" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1780" s="12"/>
       <c r="B1780" s="9"/>
-      <c r="C1780" s="14" t="s">
-        <v>446</v>
-      </c>
-      <c r="D1780" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1780" s="11" t="s">
-        <v>837</v>
-      </c>
-      <c r="F1780" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G1780" s="11" t="s">
-        <v>1624</v>
-      </c>
+      <c r="C1780" s="14"/>
+      <c r="D1780" s="10"/>
+      <c r="E1780" s="11"/>
+      <c r="F1780" s="10"/>
+      <c r="G1780" s="11"/>
       <c r="H1780" s="12"/>
       <c r="I1780" s="13"/>
       <c r="J1780" s="13"/>
     </row>
-    <row r="1781" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1781" s="12"/>
+    <row r="1781" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+      <c r="A1781" s="12">
+        <v>44252</v>
+      </c>
       <c r="B1781" s="9"/>
-      <c r="C1781" s="14"/>
-      <c r="D1781" s="10"/>
-      <c r="E1781" s="11"/>
-      <c r="F1781" s="10"/>
+      <c r="C1781" s="14" t="s">
+        <v>897</v>
+      </c>
+      <c r="D1781" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1781" s="11" t="s">
+        <v>759</v>
+      </c>
+      <c r="F1781" s="10" t="s">
+        <v>1654</v>
+      </c>
       <c r="G1781" s="11"/>
       <c r="H1781" s="12"/>
       <c r="I1781" s="13"/>
-      <c r="J1781" s="13"/>
-    </row>
-    <row r="1782" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1782" s="12"/>
+      <c r="J1781" s="13" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1782" s="12">
+        <v>44252</v>
+      </c>
       <c r="B1782" s="9"/>
-      <c r="C1782" s="14"/>
-      <c r="D1782" s="10"/>
-      <c r="E1782" s="11"/>
-      <c r="F1782" s="10"/>
+      <c r="C1782" s="14" t="s">
+        <v>897</v>
+      </c>
+      <c r="D1782" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1782" s="11" t="s">
+        <v>759</v>
+      </c>
+      <c r="F1782" s="10" t="s">
+        <v>1653</v>
+      </c>
       <c r="G1782" s="11"/>
       <c r="H1782" s="12"/>
       <c r="I1782" s="13"/>
       <c r="J1782" s="13"/>
     </row>
-    <row r="1783" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1783" s="12"/>
+    <row r="1783" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1783" s="12">
+        <v>44112</v>
+      </c>
       <c r="B1783" s="9"/>
-      <c r="C1783" s="14"/>
-      <c r="D1783" s="10"/>
-      <c r="E1783" s="11"/>
-      <c r="F1783" s="10"/>
+      <c r="C1783" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1783" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1783" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1783" s="10" t="s">
+        <v>2241</v>
+      </c>
       <c r="G1783" s="11"/>
       <c r="H1783" s="12"/>
       <c r="I1783" s="13"/>
       <c r="J1783" s="13"/>
     </row>
     <row r="1784" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1784" s="12"/>
+      <c r="A1784" s="12">
+        <v>44088</v>
+      </c>
       <c r="B1784" s="9"/>
-      <c r="C1784" s="14"/>
-      <c r="D1784" s="10"/>
-      <c r="E1784" s="11"/>
-      <c r="F1784" s="10"/>
+      <c r="C1784" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1784" s="10" t="s">
+        <v>905</v>
+      </c>
+      <c r="E1784" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1784" s="10" t="s">
+        <v>1010</v>
+      </c>
       <c r="G1784" s="11"/>
       <c r="H1784" s="12"/>
       <c r="I1784" s="13"/>
       <c r="J1784" s="13"/>
     </row>
     <row r="1785" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1785" s="12"/>
+      <c r="A1785" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1785" s="9"/>
-      <c r="C1785" s="14"/>
-      <c r="D1785" s="10"/>
-      <c r="E1785" s="11"/>
-      <c r="F1785" s="10"/>
+      <c r="C1785" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1785" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1785" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1785" s="10" t="s">
+        <v>902</v>
+      </c>
       <c r="G1785" s="11"/>
       <c r="H1785" s="12"/>
       <c r="I1785" s="13"/>
       <c r="J1785" s="13"/>
     </row>
     <row r="1786" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1786" s="12"/>
+      <c r="A1786" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1786" s="9"/>
-      <c r="C1786" s="14"/>
-      <c r="D1786" s="10"/>
-      <c r="E1786" s="11"/>
-      <c r="F1786" s="10"/>
+      <c r="C1786" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1786" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1786" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1786" s="10" t="s">
+        <v>901</v>
+      </c>
       <c r="G1786" s="11"/>
       <c r="H1786" s="12"/>
       <c r="I1786" s="13"/>
       <c r="J1786" s="13"/>
     </row>
+    <row r="1787" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1787" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B1787" s="9"/>
+      <c r="C1787" s="14" t="s">
+        <v>897</v>
+      </c>
+      <c r="D1787" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1787" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1787" s="10" t="s">
+        <v>899</v>
+      </c>
+      <c r="G1787" s="11"/>
+      <c r="H1787" s="12"/>
+      <c r="I1787" s="13"/>
+      <c r="J1787" s="13"/>
+    </row>
+    <row r="1788" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A1788" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B1788" s="9"/>
+      <c r="C1788" s="14" t="s">
+        <v>897</v>
+      </c>
+      <c r="D1788" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1788" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1788" s="10" t="s">
+        <v>900</v>
+      </c>
+      <c r="G1788" s="11"/>
+      <c r="H1788" s="12"/>
+      <c r="I1788" s="13"/>
+      <c r="J1788" s="13"/>
+    </row>
+    <row r="1789" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1789" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B1789" s="9"/>
+      <c r="C1789" s="14" t="s">
+        <v>897</v>
+      </c>
+      <c r="D1789" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1789" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1789" s="10" t="s">
+        <v>903</v>
+      </c>
+      <c r="G1789" s="11"/>
+      <c r="H1789" s="12"/>
+      <c r="I1789" s="13"/>
+      <c r="J1789" s="13" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="1790" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1790" s="12">
+        <v>43949</v>
+      </c>
+      <c r="B1790" s="9"/>
+      <c r="C1790" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1790" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1790" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1790" s="10" t="s">
+        <v>686</v>
+      </c>
+      <c r="G1790" s="11" t="s">
+        <v>1634</v>
+      </c>
+      <c r="H1790" s="12"/>
+      <c r="I1790" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1790" s="13"/>
+    </row>
+    <row r="1791" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1791" s="12">
+        <v>43949</v>
+      </c>
+      <c r="B1791" s="9"/>
+      <c r="C1791" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1791" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1791" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1791" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="G1791" s="11" t="s">
+        <v>687</v>
+      </c>
+      <c r="H1791" s="12"/>
+      <c r="I1791" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1791" s="13" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="1792" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1792" s="12">
+        <v>43838</v>
+      </c>
+      <c r="B1792" s="9"/>
+      <c r="C1792" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1792" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1792" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1792" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G1792" s="11" t="s">
+        <v>1635</v>
+      </c>
+      <c r="H1792" s="12"/>
+      <c r="I1792" s="13"/>
+      <c r="J1792" s="13" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="1793" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1793" s="12">
+        <v>43762</v>
+      </c>
+      <c r="B1793" s="9"/>
+      <c r="C1793" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1793" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1793" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1793" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1793" s="11" t="s">
+        <v>1624</v>
+      </c>
+      <c r="H1793" s="12"/>
+      <c r="I1793" s="13"/>
+      <c r="J1793" s="13"/>
+    </row>
+    <row r="1794" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1794" s="12"/>
+      <c r="B1794" s="9"/>
+      <c r="C1794" s="14"/>
+      <c r="D1794" s="10"/>
+      <c r="E1794" s="11"/>
+      <c r="F1794" s="10"/>
+      <c r="G1794" s="11"/>
+      <c r="H1794" s="12"/>
+      <c r="I1794" s="13"/>
+      <c r="J1794" s="13"/>
+    </row>
+    <row r="1795" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1795" s="12"/>
+      <c r="B1795" s="9"/>
+      <c r="C1795" s="14"/>
+      <c r="D1795" s="10"/>
+      <c r="E1795" s="11"/>
+      <c r="F1795" s="10"/>
+      <c r="G1795" s="11"/>
+      <c r="H1795" s="12"/>
+      <c r="I1795" s="13"/>
+      <c r="J1795" s="13"/>
+    </row>
+    <row r="1796" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1796" s="12"/>
+      <c r="B1796" s="9"/>
+      <c r="C1796" s="14"/>
+      <c r="D1796" s="10"/>
+      <c r="E1796" s="11"/>
+      <c r="F1796" s="10"/>
+      <c r="G1796" s="11"/>
+      <c r="H1796" s="12"/>
+      <c r="I1796" s="13"/>
+      <c r="J1796" s="13"/>
+    </row>
+    <row r="1797" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1797" s="12"/>
+      <c r="B1797" s="9"/>
+      <c r="C1797" s="14"/>
+      <c r="D1797" s="10"/>
+      <c r="E1797" s="11"/>
+      <c r="F1797" s="10"/>
+      <c r="G1797" s="11"/>
+      <c r="H1797" s="12"/>
+      <c r="I1797" s="13"/>
+      <c r="J1797" s="13"/>
+    </row>
+    <row r="1798" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1798" s="12"/>
+      <c r="B1798" s="9"/>
+      <c r="C1798" s="14"/>
+      <c r="D1798" s="10"/>
+      <c r="E1798" s="11"/>
+      <c r="F1798" s="10"/>
+      <c r="G1798" s="11"/>
+      <c r="H1798" s="12"/>
+      <c r="I1798" s="13"/>
+      <c r="J1798" s="13"/>
+    </row>
+    <row r="1799" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1799" s="12"/>
+      <c r="B1799" s="9"/>
+      <c r="C1799" s="14"/>
+      <c r="D1799" s="10"/>
+      <c r="E1799" s="11"/>
+      <c r="F1799" s="10"/>
+      <c r="G1799" s="11"/>
+      <c r="H1799" s="12"/>
+      <c r="I1799" s="13"/>
+      <c r="J1799" s="13"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1480" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1756:F1766">
-    <sortCondition ref="F1756:F1766"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1769:F1779">
+    <sortCondition ref="F1769:F1779"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Exportar planilhas e cron excel
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1A7717-88F4-4040-A7D0-3FDD3783E1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499B0028-00F1-4B32-932D-55CA09EFD1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12452" uniqueCount="2457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12491" uniqueCount="2465">
   <si>
     <t>Responsável</t>
   </si>
@@ -7786,6 +7786,32 @@
   </si>
   <si>
     <t>Problemas no estorno da NF 000021531</t>
+  </si>
+  <si>
+    <t>Criar usuária juliana.villega no Protheus</t>
+  </si>
+  <si>
+    <t>Alterados os vencimentos das primeiras parcelas dos títulos 585612202 e 691210202 de 31/01/2022 para 05/01/2022.
+Alteradas as datas de emissão e digitação de todos os 60 títulos e também dos documentos de entradas correspondentes de 12/01/2022 para 05/01/2022.
+Obs: a TES do Doc de Entrada 585612202 foi alterada para 115, para não gerar livros fiscais.</t>
+  </si>
+  <si>
+    <t>Alterar vencimento de titulos com data anterior a emissão</t>
+  </si>
+  <si>
+    <t>Compensação Diego</t>
+  </si>
+  <si>
+    <t>Alteração de diversas configurações em diversas situações de Notas Fiscais para ajuste de acordo com o cliente / fiscal</t>
+  </si>
+  <si>
+    <t>Novo relatório de exportação de planilhas e cronogramas</t>
+  </si>
+  <si>
+    <t>BKGCTR27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alterar o e-mail do cliente DH da Balsa para financeiro@dh.sp.gov.br                                                                             </t>
   </si>
 </sst>
 </file>
@@ -8554,11 +8580,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1799"/>
+  <dimension ref="A1:J1805"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1746" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1754" sqref="A1754:XFD1756"/>
+      <pane ySplit="1" topLeftCell="A1758" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1761" sqref="A1761"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -60965,143 +60991,215 @@
       </c>
       <c r="J1753" s="13"/>
     </row>
-    <row r="1754" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1754" s="12"/>
-      <c r="B1754" s="12"/>
-      <c r="C1754" s="14"/>
-      <c r="D1754" s="10"/>
-      <c r="E1754" s="11"/>
-      <c r="F1754" s="10"/>
-      <c r="G1754" s="11"/>
-      <c r="H1754" s="12"/>
-      <c r="I1754" s="13"/>
-      <c r="J1754" s="13"/>
+    <row r="1754" spans="1:10" ht="84" x14ac:dyDescent="0.2">
+      <c r="A1754" s="12">
+        <v>44573</v>
+      </c>
+      <c r="B1754" s="12">
+        <v>44573</v>
+      </c>
+      <c r="C1754" s="14" t="s">
+        <v>1986</v>
+      </c>
+      <c r="D1754" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1754" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1754" s="10" t="s">
+        <v>2459</v>
+      </c>
+      <c r="G1754" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1754" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1754" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1754" s="13" t="s">
+        <v>2458</v>
+      </c>
     </row>
     <row r="1755" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1755" s="12"/>
-      <c r="B1755" s="12"/>
-      <c r="C1755" s="14"/>
-      <c r="D1755" s="10"/>
-      <c r="E1755" s="11"/>
-      <c r="F1755" s="10"/>
-      <c r="G1755" s="11"/>
-      <c r="H1755" s="12"/>
-      <c r="I1755" s="13"/>
+      <c r="A1755" s="12">
+        <v>44574</v>
+      </c>
+      <c r="B1755" s="12">
+        <v>44574</v>
+      </c>
+      <c r="C1755" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1755" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1755" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1755" s="10" t="s">
+        <v>2457</v>
+      </c>
+      <c r="G1755" s="11" t="s">
+        <v>1616</v>
+      </c>
+      <c r="H1755" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1755" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="J1755" s="13"/>
     </row>
     <row r="1756" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1756" s="12"/>
-      <c r="B1756" s="12"/>
+      <c r="A1756" s="12">
+        <v>44574</v>
+      </c>
+      <c r="B1756" s="12">
+        <v>44574</v>
+      </c>
       <c r="C1756" s="14"/>
       <c r="D1756" s="10"/>
       <c r="E1756" s="11"/>
-      <c r="F1756" s="10"/>
+      <c r="F1756" s="10" t="s">
+        <v>759</v>
+      </c>
       <c r="G1756" s="11"/>
       <c r="H1756" s="12"/>
       <c r="I1756" s="13"/>
       <c r="J1756" s="13"/>
     </row>
     <row r="1757" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1757" s="12"/>
-      <c r="B1757" s="12"/>
+      <c r="A1757" s="12">
+        <v>44574</v>
+      </c>
+      <c r="B1757" s="12">
+        <v>44574</v>
+      </c>
       <c r="C1757" s="14"/>
       <c r="D1757" s="10"/>
       <c r="E1757" s="11"/>
-      <c r="F1757" s="10"/>
+      <c r="F1757" s="10" t="s">
+        <v>2460</v>
+      </c>
       <c r="G1757" s="11"/>
       <c r="H1757" s="12"/>
       <c r="I1757" s="13"/>
       <c r="J1757" s="13"/>
     </row>
-    <row r="1758" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1758" s="12"/>
-      <c r="B1758" s="12"/>
-      <c r="C1758" s="14"/>
-      <c r="D1758" s="10"/>
-      <c r="E1758" s="11"/>
-      <c r="F1758" s="10"/>
-      <c r="G1758" s="11"/>
-      <c r="H1758" s="12"/>
-      <c r="I1758" s="13"/>
+    <row r="1758" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1758" s="12">
+        <v>44575</v>
+      </c>
+      <c r="B1758" s="12">
+        <v>44575</v>
+      </c>
+      <c r="C1758" s="14" t="s">
+        <v>462</v>
+      </c>
+      <c r="D1758" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1758" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1758" s="10" t="s">
+        <v>2461</v>
+      </c>
+      <c r="G1758" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H1758" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1758" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1758" s="13"/>
     </row>
     <row r="1759" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1759" s="12"/>
-      <c r="B1759" s="12"/>
-      <c r="C1759" s="14"/>
-      <c r="D1759" s="10"/>
-      <c r="E1759" s="11"/>
-      <c r="F1759" s="10"/>
-      <c r="G1759" s="11"/>
-      <c r="H1759" s="12"/>
-      <c r="I1759" s="13"/>
-      <c r="J1759" s="13"/>
-    </row>
-    <row r="1760" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1759" s="12">
+        <v>44575</v>
+      </c>
+      <c r="B1759" s="12">
+        <v>44575</v>
+      </c>
+      <c r="C1759" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1759" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1759" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1759" s="10" t="s">
+        <v>2462</v>
+      </c>
+      <c r="G1759" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H1759" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1759" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1759" s="13" t="s">
+        <v>2463</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1760" s="12">
-        <v>44522</v>
-      </c>
-      <c r="B1760" s="12"/>
+        <v>44578</v>
+      </c>
+      <c r="B1760" s="12">
+        <v>44578</v>
+      </c>
       <c r="C1760" s="14" t="s">
-        <v>46</v>
+        <v>575</v>
       </c>
       <c r="D1760" s="10" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="E1760" s="11" t="s">
-        <v>570</v>
+        <v>620</v>
       </c>
       <c r="F1760" s="10" t="s">
-        <v>2369</v>
-      </c>
-      <c r="G1760" s="11"/>
-      <c r="H1760" s="12"/>
-      <c r="I1760" s="13"/>
+        <v>2464</v>
+      </c>
+      <c r="G1760" s="11" t="s">
+        <v>1641</v>
+      </c>
+      <c r="H1760" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1760" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1760" s="13"/>
     </row>
     <row r="1761" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1761" s="12">
-        <v>43816</v>
-      </c>
-      <c r="B1761" s="9"/>
-      <c r="C1761" s="14" t="s">
-        <v>475</v>
-      </c>
-      <c r="D1761" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1761" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1761" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="G1761" s="11" t="s">
-        <v>1627</v>
-      </c>
+      <c r="A1761" s="12"/>
+      <c r="B1761" s="12"/>
+      <c r="C1761" s="14"/>
+      <c r="D1761" s="10"/>
+      <c r="E1761" s="11"/>
+      <c r="F1761" s="10"/>
+      <c r="G1761" s="11"/>
       <c r="H1761" s="12"/>
       <c r="I1761" s="13"/>
-      <c r="J1761" s="13" t="s">
-        <v>1565</v>
-      </c>
+      <c r="J1761" s="13"/>
     </row>
     <row r="1762" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1762" s="12">
-        <v>44460</v>
-      </c>
+      <c r="A1762" s="12"/>
       <c r="B1762" s="12"/>
-      <c r="C1762" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1762" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="E1762" s="11" t="s">
-        <v>837</v>
-      </c>
-      <c r="F1762" s="10" t="s">
-        <v>2193</v>
-      </c>
+      <c r="C1762" s="14"/>
+      <c r="D1762" s="10"/>
+      <c r="E1762" s="11"/>
+      <c r="F1762" s="10"/>
       <c r="G1762" s="11"/>
       <c r="H1762" s="12"/>
       <c r="I1762" s="13"/>
@@ -61133,7 +61231,7 @@
     </row>
     <row r="1765" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1765" s="12"/>
-      <c r="B1765" s="9"/>
+      <c r="B1765" s="12"/>
       <c r="C1765" s="14"/>
       <c r="D1765" s="10"/>
       <c r="E1765" s="11"/>
@@ -61143,64 +61241,70 @@
       <c r="I1765" s="13"/>
       <c r="J1765" s="13"/>
     </row>
-    <row r="1766" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1766" s="1" t="s">
-        <v>1475</v>
-      </c>
-      <c r="B1766" s="2" t="s">
-        <v>1476</v>
-      </c>
-      <c r="C1766" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1766" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1766" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1766" s="4" t="s">
-        <v>1575</v>
-      </c>
-      <c r="G1766" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1766" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1766" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1766" s="36"/>
+    <row r="1766" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1766" s="12">
+        <v>44522</v>
+      </c>
+      <c r="B1766" s="12"/>
+      <c r="C1766" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1766" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1766" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1766" s="10" t="s">
+        <v>2369</v>
+      </c>
+      <c r="G1766" s="11"/>
+      <c r="H1766" s="12"/>
+      <c r="I1766" s="13"/>
+      <c r="J1766" s="13"/>
     </row>
     <row r="1767" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1767" s="12"/>
+      <c r="A1767" s="12">
+        <v>43816</v>
+      </c>
       <c r="B1767" s="9"/>
-      <c r="C1767" s="14"/>
-      <c r="D1767" s="10"/>
-      <c r="E1767" s="11"/>
-      <c r="F1767" s="10"/>
-      <c r="G1767" s="11"/>
+      <c r="C1767" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1767" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1767" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1767" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G1767" s="11" t="s">
+        <v>1627</v>
+      </c>
       <c r="H1767" s="12"/>
       <c r="I1767" s="13"/>
-      <c r="J1767" s="13"/>
+      <c r="J1767" s="13" t="s">
+        <v>1565</v>
+      </c>
     </row>
     <row r="1768" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1768" s="12"/>
-      <c r="B1768" s="12">
-        <v>44402</v>
-      </c>
+      <c r="A1768" s="12">
+        <v>44460</v>
+      </c>
+      <c r="B1768" s="12"/>
       <c r="C1768" s="14" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D1768" s="10" t="s">
-        <v>584</v>
+        <v>494</v>
       </c>
       <c r="E1768" s="11" t="s">
-        <v>647</v>
+        <v>837</v>
       </c>
       <c r="F1768" s="10" t="s">
-        <v>1609</v>
+        <v>2193</v>
       </c>
       <c r="G1768" s="11"/>
       <c r="H1768" s="12"/>
@@ -61209,21 +61313,11 @@
     </row>
     <row r="1769" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1769" s="12"/>
-      <c r="B1769" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1769" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1769" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1769" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1769" s="10" t="s">
-        <v>1601</v>
-      </c>
+      <c r="B1769" s="12"/>
+      <c r="C1769" s="14"/>
+      <c r="D1769" s="10"/>
+      <c r="E1769" s="11"/>
+      <c r="F1769" s="10"/>
       <c r="G1769" s="11"/>
       <c r="H1769" s="12"/>
       <c r="I1769" s="13"/>
@@ -61231,21 +61325,11 @@
     </row>
     <row r="1770" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1770" s="12"/>
-      <c r="B1770" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1770" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1770" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1770" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1770" s="10" t="s">
-        <v>1606</v>
-      </c>
+      <c r="B1770" s="12"/>
+      <c r="C1770" s="14"/>
+      <c r="D1770" s="10"/>
+      <c r="E1770" s="11"/>
+      <c r="F1770" s="10"/>
       <c r="G1770" s="11"/>
       <c r="H1770" s="12"/>
       <c r="I1770" s="13"/>
@@ -61253,63 +61337,53 @@
     </row>
     <row r="1771" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1771" s="12"/>
-      <c r="B1771" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1771" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1771" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1771" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1771" s="10" t="s">
-        <v>1602</v>
-      </c>
+      <c r="B1771" s="9"/>
+      <c r="C1771" s="14"/>
+      <c r="D1771" s="10"/>
+      <c r="E1771" s="11"/>
+      <c r="F1771" s="10"/>
       <c r="G1771" s="11"/>
       <c r="H1771" s="12"/>
       <c r="I1771" s="13"/>
       <c r="J1771" s="13"/>
     </row>
     <row r="1772" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1772" s="12"/>
-      <c r="B1772" s="9"/>
-      <c r="C1772" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1772" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1772" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1772" s="10" t="s">
-        <v>1610</v>
-      </c>
-      <c r="G1772" s="11"/>
-      <c r="H1772" s="12"/>
-      <c r="I1772" s="13"/>
-      <c r="J1772" s="13"/>
+      <c r="A1772" s="1" t="s">
+        <v>1475</v>
+      </c>
+      <c r="B1772" s="2" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C1772" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1772" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1772" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1772" s="4" t="s">
+        <v>1575</v>
+      </c>
+      <c r="G1772" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1772" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1772" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1772" s="36"/>
     </row>
     <row r="1773" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1773" s="12"/>
-      <c r="B1773" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1773" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1773" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1773" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1773" s="10" t="s">
-        <v>1603</v>
-      </c>
+      <c r="B1773" s="9"/>
+      <c r="C1773" s="14"/>
+      <c r="D1773" s="10"/>
+      <c r="E1773" s="11"/>
+      <c r="F1773" s="10"/>
       <c r="G1773" s="11"/>
       <c r="H1773" s="12"/>
       <c r="I1773" s="13"/>
@@ -61317,7 +61391,9 @@
     </row>
     <row r="1774" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1774" s="12"/>
-      <c r="B1774" s="9"/>
+      <c r="B1774" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1774" s="14" t="s">
         <v>13</v>
       </c>
@@ -61328,7 +61404,7 @@
         <v>647</v>
       </c>
       <c r="F1774" s="10" t="s">
-        <v>1600</v>
+        <v>1609</v>
       </c>
       <c r="G1774" s="11"/>
       <c r="H1774" s="12"/>
@@ -61350,7 +61426,7 @@
         <v>647</v>
       </c>
       <c r="F1775" s="10" t="s">
-        <v>1599</v>
+        <v>1601</v>
       </c>
       <c r="G1775" s="11"/>
       <c r="H1775" s="12"/>
@@ -61372,7 +61448,7 @@
         <v>647</v>
       </c>
       <c r="F1776" s="10" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="G1776" s="11"/>
       <c r="H1776" s="12"/>
@@ -61394,7 +61470,7 @@
         <v>647</v>
       </c>
       <c r="F1777" s="10" t="s">
-        <v>1607</v>
+        <v>1602</v>
       </c>
       <c r="G1777" s="11"/>
       <c r="H1777" s="12"/>
@@ -61403,9 +61479,7 @@
     </row>
     <row r="1778" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1778" s="12"/>
-      <c r="B1778" s="9">
-        <v>44235</v>
-      </c>
+      <c r="B1778" s="9"/>
       <c r="C1778" s="14" t="s">
         <v>13</v>
       </c>
@@ -61416,7 +61490,7 @@
         <v>647</v>
       </c>
       <c r="F1778" s="10" t="s">
-        <v>1608</v>
+        <v>1610</v>
       </c>
       <c r="G1778" s="11"/>
       <c r="H1778" s="12"/>
@@ -61425,7 +61499,9 @@
     </row>
     <row r="1779" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1779" s="12"/>
-      <c r="B1779" s="9"/>
+      <c r="B1779" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1779" s="14" t="s">
         <v>13</v>
       </c>
@@ -61436,7 +61512,7 @@
         <v>647</v>
       </c>
       <c r="F1779" s="10" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
       <c r="G1779" s="11"/>
       <c r="H1779" s="12"/>
@@ -61446,77 +61522,83 @@
     <row r="1780" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1780" s="12"/>
       <c r="B1780" s="9"/>
-      <c r="C1780" s="14"/>
-      <c r="D1780" s="10"/>
-      <c r="E1780" s="11"/>
-      <c r="F1780" s="10"/>
+      <c r="C1780" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1780" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1780" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1780" s="10" t="s">
+        <v>1600</v>
+      </c>
       <c r="G1780" s="11"/>
       <c r="H1780" s="12"/>
       <c r="I1780" s="13"/>
       <c r="J1780" s="13"/>
     </row>
-    <row r="1781" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1781" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1781" s="9"/>
+    <row r="1781" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1781" s="12"/>
+      <c r="B1781" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1781" s="14" t="s">
-        <v>897</v>
+        <v>13</v>
       </c>
       <c r="D1781" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1781" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1781" s="10" t="s">
-        <v>1654</v>
+        <v>1599</v>
       </c>
       <c r="G1781" s="11"/>
       <c r="H1781" s="12"/>
       <c r="I1781" s="13"/>
-      <c r="J1781" s="13" t="s">
-        <v>1677</v>
-      </c>
-    </row>
-    <row r="1782" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1782" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1782" s="9"/>
+      <c r="J1781" s="13"/>
+    </row>
+    <row r="1782" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1782" s="12"/>
+      <c r="B1782" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1782" s="14" t="s">
-        <v>897</v>
+        <v>13</v>
       </c>
       <c r="D1782" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1782" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1782" s="10" t="s">
-        <v>1653</v>
+        <v>1604</v>
       </c>
       <c r="G1782" s="11"/>
       <c r="H1782" s="12"/>
       <c r="I1782" s="13"/>
       <c r="J1782" s="13"/>
     </row>
-    <row r="1783" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1783" s="12">
-        <v>44112</v>
-      </c>
-      <c r="B1783" s="9"/>
+    <row r="1783" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1783" s="12"/>
+      <c r="B1783" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1783" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1783" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1783" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1783" s="10" t="s">
-        <v>2241</v>
+        <v>1607</v>
       </c>
       <c r="G1783" s="11"/>
       <c r="H1783" s="12"/>
@@ -61524,21 +61606,21 @@
       <c r="J1783" s="13"/>
     </row>
     <row r="1784" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1784" s="12">
-        <v>44088</v>
-      </c>
-      <c r="B1784" s="9"/>
+      <c r="A1784" s="12"/>
+      <c r="B1784" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1784" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1784" s="10" t="s">
-        <v>905</v>
+        <v>584</v>
       </c>
       <c r="E1784" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1784" s="10" t="s">
-        <v>1010</v>
+        <v>1608</v>
       </c>
       <c r="G1784" s="11"/>
       <c r="H1784" s="12"/>
@@ -61546,21 +61628,19 @@
       <c r="J1784" s="13"/>
     </row>
     <row r="1785" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1785" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1785" s="12"/>
       <c r="B1785" s="9"/>
       <c r="C1785" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1785" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1785" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1785" s="10" t="s">
-        <v>902</v>
+        <v>1605</v>
       </c>
       <c r="G1785" s="11"/>
       <c r="H1785" s="12"/>
@@ -61568,30 +61648,20 @@
       <c r="J1785" s="13"/>
     </row>
     <row r="1786" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1786" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1786" s="12"/>
       <c r="B1786" s="9"/>
-      <c r="C1786" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="D1786" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1786" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1786" s="10" t="s">
-        <v>901</v>
-      </c>
+      <c r="C1786" s="14"/>
+      <c r="D1786" s="10"/>
+      <c r="E1786" s="11"/>
+      <c r="F1786" s="10"/>
       <c r="G1786" s="11"/>
       <c r="H1786" s="12"/>
       <c r="I1786" s="13"/>
       <c r="J1786" s="13"/>
     </row>
-    <row r="1787" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1787" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1787" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1787" s="9"/>
       <c r="C1787" s="14" t="s">
@@ -61601,19 +61671,21 @@
         <v>494</v>
       </c>
       <c r="E1787" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1787" s="10" t="s">
-        <v>899</v>
+        <v>1654</v>
       </c>
       <c r="G1787" s="11"/>
       <c r="H1787" s="12"/>
       <c r="I1787" s="13"/>
-      <c r="J1787" s="13"/>
-    </row>
-    <row r="1788" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="J1787" s="13" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="1788" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1788" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1788" s="9"/>
       <c r="C1788" s="14" t="s">
@@ -61623,220 +61695,352 @@
         <v>494</v>
       </c>
       <c r="E1788" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1788" s="10" t="s">
-        <v>900</v>
+        <v>1653</v>
       </c>
       <c r="G1788" s="11"/>
       <c r="H1788" s="12"/>
       <c r="I1788" s="13"/>
       <c r="J1788" s="13"/>
     </row>
-    <row r="1789" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1789" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1789" s="12">
-        <v>44055</v>
+        <v>44112</v>
       </c>
       <c r="B1789" s="9"/>
       <c r="C1789" s="14" t="s">
-        <v>897</v>
+        <v>623</v>
       </c>
       <c r="D1789" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1789" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1789" s="10" t="s">
-        <v>903</v>
+        <v>2241</v>
       </c>
       <c r="G1789" s="11"/>
       <c r="H1789" s="12"/>
       <c r="I1789" s="13"/>
-      <c r="J1789" s="13" t="s">
-        <v>1583</v>
-      </c>
-    </row>
-    <row r="1790" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="J1789" s="13"/>
+    </row>
+    <row r="1790" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1790" s="12">
-        <v>43949</v>
+        <v>44088</v>
       </c>
       <c r="B1790" s="9"/>
       <c r="C1790" s="14" t="s">
-        <v>468</v>
+        <v>19</v>
       </c>
       <c r="D1790" s="10" t="s">
-        <v>89</v>
+        <v>905</v>
       </c>
       <c r="E1790" s="11" t="s">
         <v>685</v>
       </c>
       <c r="F1790" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1790" s="11" t="s">
-        <v>1634</v>
-      </c>
+        <v>1010</v>
+      </c>
+      <c r="G1790" s="11"/>
       <c r="H1790" s="12"/>
-      <c r="I1790" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1790" s="13"/>
       <c r="J1790" s="13"/>
     </row>
-    <row r="1791" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1791" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1791" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1791" s="9"/>
       <c r="C1791" s="14" t="s">
-        <v>468</v>
+        <v>623</v>
       </c>
       <c r="D1791" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1791" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1791" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1791" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="G1791" s="11"/>
       <c r="H1791" s="12"/>
-      <c r="I1791" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1791" s="13" t="s">
-        <v>1564</v>
-      </c>
-    </row>
-    <row r="1792" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1791" s="13"/>
+      <c r="J1791" s="13"/>
+    </row>
+    <row r="1792" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1792" s="12">
-        <v>43838</v>
+        <v>44055</v>
       </c>
       <c r="B1792" s="9"/>
       <c r="C1792" s="14" t="s">
-        <v>103</v>
+        <v>623</v>
       </c>
       <c r="D1792" s="10" t="s">
-        <v>460</v>
+        <v>6</v>
       </c>
       <c r="E1792" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1792" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G1792" s="11" t="s">
-        <v>1635</v>
-      </c>
+        <v>901</v>
+      </c>
+      <c r="G1792" s="11"/>
       <c r="H1792" s="12"/>
       <c r="I1792" s="13"/>
-      <c r="J1792" s="13" t="s">
-        <v>1529</v>
-      </c>
-    </row>
-    <row r="1793" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1792" s="13"/>
+    </row>
+    <row r="1793" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1793" s="12">
-        <v>43762</v>
+        <v>44055</v>
       </c>
       <c r="B1793" s="9"/>
       <c r="C1793" s="14" t="s">
-        <v>446</v>
+        <v>897</v>
       </c>
       <c r="D1793" s="10" t="s">
-        <v>17</v>
+        <v>494</v>
       </c>
       <c r="E1793" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1793" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G1793" s="11" t="s">
-        <v>1624</v>
-      </c>
+        <v>899</v>
+      </c>
+      <c r="G1793" s="11"/>
       <c r="H1793" s="12"/>
       <c r="I1793" s="13"/>
       <c r="J1793" s="13"/>
     </row>
-    <row r="1794" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1794" s="12"/>
+    <row r="1794" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A1794" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1794" s="9"/>
-      <c r="C1794" s="14"/>
-      <c r="D1794" s="10"/>
-      <c r="E1794" s="11"/>
-      <c r="F1794" s="10"/>
+      <c r="C1794" s="14" t="s">
+        <v>897</v>
+      </c>
+      <c r="D1794" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1794" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1794" s="10" t="s">
+        <v>900</v>
+      </c>
       <c r="G1794" s="11"/>
       <c r="H1794" s="12"/>
       <c r="I1794" s="13"/>
       <c r="J1794" s="13"/>
     </row>
-    <row r="1795" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1795" s="12"/>
+    <row r="1795" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1795" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1795" s="9"/>
-      <c r="C1795" s="14"/>
-      <c r="D1795" s="10"/>
-      <c r="E1795" s="11"/>
-      <c r="F1795" s="10"/>
+      <c r="C1795" s="14" t="s">
+        <v>897</v>
+      </c>
+      <c r="D1795" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1795" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1795" s="10" t="s">
+        <v>903</v>
+      </c>
       <c r="G1795" s="11"/>
       <c r="H1795" s="12"/>
       <c r="I1795" s="13"/>
-      <c r="J1795" s="13"/>
-    </row>
-    <row r="1796" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1796" s="12"/>
+      <c r="J1795" s="13" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="1796" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1796" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1796" s="9"/>
-      <c r="C1796" s="14"/>
-      <c r="D1796" s="10"/>
-      <c r="E1796" s="11"/>
-      <c r="F1796" s="10"/>
-      <c r="G1796" s="11"/>
+      <c r="C1796" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1796" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1796" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1796" s="10" t="s">
+        <v>686</v>
+      </c>
+      <c r="G1796" s="11" t="s">
+        <v>1634</v>
+      </c>
       <c r="H1796" s="12"/>
-      <c r="I1796" s="13"/>
+      <c r="I1796" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1796" s="13"/>
     </row>
-    <row r="1797" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1797" s="12"/>
+    <row r="1797" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1797" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1797" s="9"/>
-      <c r="C1797" s="14"/>
-      <c r="D1797" s="10"/>
-      <c r="E1797" s="11"/>
-      <c r="F1797" s="10"/>
-      <c r="G1797" s="11"/>
+      <c r="C1797" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1797" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1797" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1797" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="G1797" s="11" t="s">
+        <v>687</v>
+      </c>
       <c r="H1797" s="12"/>
-      <c r="I1797" s="13"/>
-      <c r="J1797" s="13"/>
-    </row>
-    <row r="1798" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1798" s="12"/>
+      <c r="I1797" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1797" s="13" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="1798" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1798" s="12">
+        <v>43838</v>
+      </c>
       <c r="B1798" s="9"/>
-      <c r="C1798" s="14"/>
-      <c r="D1798" s="10"/>
-      <c r="E1798" s="11"/>
-      <c r="F1798" s="10"/>
-      <c r="G1798" s="11"/>
+      <c r="C1798" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1798" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1798" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1798" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G1798" s="11" t="s">
+        <v>1635</v>
+      </c>
       <c r="H1798" s="12"/>
       <c r="I1798" s="13"/>
-      <c r="J1798" s="13"/>
-    </row>
-    <row r="1799" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1799" s="12"/>
+      <c r="J1798" s="13" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="1799" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1799" s="12">
+        <v>43762</v>
+      </c>
       <c r="B1799" s="9"/>
-      <c r="C1799" s="14"/>
-      <c r="D1799" s="10"/>
-      <c r="E1799" s="11"/>
-      <c r="F1799" s="10"/>
-      <c r="G1799" s="11"/>
+      <c r="C1799" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1799" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1799" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1799" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1799" s="11" t="s">
+        <v>1624</v>
+      </c>
       <c r="H1799" s="12"/>
       <c r="I1799" s="13"/>
       <c r="J1799" s="13"/>
     </row>
+    <row r="1800" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1800" s="12"/>
+      <c r="B1800" s="9"/>
+      <c r="C1800" s="14"/>
+      <c r="D1800" s="10"/>
+      <c r="E1800" s="11"/>
+      <c r="F1800" s="10"/>
+      <c r="G1800" s="11"/>
+      <c r="H1800" s="12"/>
+      <c r="I1800" s="13"/>
+      <c r="J1800" s="13"/>
+    </row>
+    <row r="1801" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1801" s="12"/>
+      <c r="B1801" s="9"/>
+      <c r="C1801" s="14"/>
+      <c r="D1801" s="10"/>
+      <c r="E1801" s="11"/>
+      <c r="F1801" s="10"/>
+      <c r="G1801" s="11"/>
+      <c r="H1801" s="12"/>
+      <c r="I1801" s="13"/>
+      <c r="J1801" s="13"/>
+    </row>
+    <row r="1802" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1802" s="12"/>
+      <c r="B1802" s="9"/>
+      <c r="C1802" s="14"/>
+      <c r="D1802" s="10"/>
+      <c r="E1802" s="11"/>
+      <c r="F1802" s="10"/>
+      <c r="G1802" s="11"/>
+      <c r="H1802" s="12"/>
+      <c r="I1802" s="13"/>
+      <c r="J1802" s="13"/>
+    </row>
+    <row r="1803" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1803" s="12"/>
+      <c r="B1803" s="9"/>
+      <c r="C1803" s="14"/>
+      <c r="D1803" s="10"/>
+      <c r="E1803" s="11"/>
+      <c r="F1803" s="10"/>
+      <c r="G1803" s="11"/>
+      <c r="H1803" s="12"/>
+      <c r="I1803" s="13"/>
+      <c r="J1803" s="13"/>
+    </row>
+    <row r="1804" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1804" s="12"/>
+      <c r="B1804" s="9"/>
+      <c r="C1804" s="14"/>
+      <c r="D1804" s="10"/>
+      <c r="E1804" s="11"/>
+      <c r="F1804" s="10"/>
+      <c r="G1804" s="11"/>
+      <c r="H1804" s="12"/>
+      <c r="I1804" s="13"/>
+      <c r="J1804" s="13"/>
+    </row>
+    <row r="1805" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1805" s="12"/>
+      <c r="B1805" s="9"/>
+      <c r="C1805" s="14"/>
+      <c r="D1805" s="10"/>
+      <c r="E1805" s="11"/>
+      <c r="F1805" s="10"/>
+      <c r="G1805" s="11"/>
+      <c r="H1805" s="12"/>
+      <c r="I1805" s="13"/>
+      <c r="J1805" s="13"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1480" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1769:F1779">
-    <sortCondition ref="F1769:F1779"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1775:F1785">
+    <sortCondition ref="F1775:F1785"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Acerto BKFINR26 a BKAJUDIRF
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBA360D-C531-4C62-A41B-DB16A83F0567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F410A79E-66F0-4518-9F3D-C00D8FF1D687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Demandas BK - Protheus'!$A$1:$J$1480</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -79,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12511" uniqueCount="2466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12556" uniqueCount="2475">
   <si>
     <t>Responsável</t>
   </si>
@@ -7816,6 +7815,33 @@
   </si>
   <si>
     <t>Incluir campo Item no relatório BKGCTR27</t>
+  </si>
+  <si>
+    <t>Organizar campos do browse do cadastro de fornecedores em todas as empresas</t>
+  </si>
+  <si>
+    <t>Emissão de relatorio de contas a receber em aberto 2021</t>
+  </si>
+  <si>
+    <t>Problemas com Doc de Entrada que não estava retendo os impostos (acertada a Natureza que estava sem as alíqotas de PCC)</t>
+  </si>
+  <si>
+    <t>Por favor pode verificar porque o faturamento dos correios filtrado na planilha em anexo está duplicado as medições e notas fiscais?</t>
+  </si>
+  <si>
+    <t>BKGCRT26 estava duplicndo linhas quando eram referentes a medições canceladas e reentradas com revisão diferente</t>
+  </si>
+  <si>
+    <t>Precisamos conversar sobre a DIRF 2021, você propõe algum dia, precisamos alinhar isso o quanto antes. Referente aos relatórios e o que o sistema e capaz de puxar para validação DIRF</t>
+  </si>
+  <si>
+    <t>Revisão na rotina de acerto de códigos da DIRF BKAJUDIRF, para não sobrepor códigos digitados</t>
+  </si>
+  <si>
+    <t>Estou efetuado a apuração do lucro ´presumido da corretora, e temos uma nota fiscal na prefeitura cancelada e ativa no sistema. Por gentileza, excluir ou cancelar a mesma do sistema, segue o número da nota fiscal 2806 valor de  289,33.</t>
+  </si>
+  <si>
+    <t>Alterado o parâmetro MV_EXCNFS para 20 temporariamente e voltado para 10 após a exclusão da NF</t>
   </si>
 </sst>
 </file>
@@ -8584,11 +8610,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1805"/>
+  <dimension ref="A1:J1811"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1752" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1763" sqref="A1763"/>
+      <pane ySplit="1" topLeftCell="A1764" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1768" sqref="A1768"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -61242,118 +61268,198 @@
       </c>
     </row>
     <row r="1762" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1762" s="12"/>
-      <c r="B1762" s="12"/>
-      <c r="C1762" s="14"/>
-      <c r="D1762" s="10"/>
-      <c r="E1762" s="11"/>
-      <c r="F1762" s="10"/>
-      <c r="G1762" s="11"/>
-      <c r="H1762" s="12"/>
-      <c r="I1762" s="13"/>
+      <c r="A1762" s="12">
+        <v>44579</v>
+      </c>
+      <c r="B1762" s="12">
+        <v>44579</v>
+      </c>
+      <c r="C1762" s="14" t="s">
+        <v>2269</v>
+      </c>
+      <c r="D1762" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1762" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1762" s="10" t="s">
+        <v>2466</v>
+      </c>
+      <c r="G1762" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1762" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1762" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1762" s="13"/>
     </row>
     <row r="1763" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1763" s="12"/>
-      <c r="B1763" s="12"/>
-      <c r="C1763" s="14"/>
-      <c r="D1763" s="10"/>
-      <c r="E1763" s="11"/>
-      <c r="F1763" s="10"/>
-      <c r="G1763" s="11"/>
-      <c r="H1763" s="12"/>
-      <c r="I1763" s="13"/>
+      <c r="A1763" s="12">
+        <v>44579</v>
+      </c>
+      <c r="B1763" s="12">
+        <v>44579</v>
+      </c>
+      <c r="C1763" s="14" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D1763" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1763" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1763" s="10" t="s">
+        <v>2467</v>
+      </c>
+      <c r="G1763" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1763" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1763" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1763" s="13"/>
     </row>
-    <row r="1764" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1764" s="12"/>
-      <c r="B1764" s="12"/>
-      <c r="C1764" s="14"/>
-      <c r="D1764" s="10"/>
-      <c r="E1764" s="11"/>
-      <c r="F1764" s="10"/>
-      <c r="G1764" s="11"/>
-      <c r="H1764" s="12"/>
-      <c r="I1764" s="13"/>
+    <row r="1764" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1764" s="12">
+        <v>44580</v>
+      </c>
+      <c r="B1764" s="12">
+        <v>44580</v>
+      </c>
+      <c r="C1764" s="14" t="s">
+        <v>2269</v>
+      </c>
+      <c r="D1764" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1764" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1764" s="10" t="s">
+        <v>2468</v>
+      </c>
+      <c r="G1764" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1764" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1764" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1764" s="13"/>
     </row>
-    <row r="1765" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1765" s="12"/>
-      <c r="B1765" s="12"/>
-      <c r="C1765" s="14"/>
-      <c r="D1765" s="10"/>
-      <c r="E1765" s="11"/>
-      <c r="F1765" s="10"/>
-      <c r="G1765" s="11"/>
-      <c r="H1765" s="12"/>
-      <c r="I1765" s="13"/>
-      <c r="J1765" s="13"/>
-    </row>
-    <row r="1766" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1765" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1765" s="12">
+        <v>44580</v>
+      </c>
+      <c r="B1765" s="12">
+        <v>44580</v>
+      </c>
+      <c r="C1765" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="D1765" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1765" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1765" s="10" t="s">
+        <v>2469</v>
+      </c>
+      <c r="G1765" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H1765" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1765" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1765" s="13" t="s">
+        <v>2470</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1766" s="12">
-        <v>44522</v>
-      </c>
-      <c r="B1766" s="12"/>
+        <v>44580</v>
+      </c>
+      <c r="B1766" s="12">
+        <v>44580</v>
+      </c>
       <c r="C1766" s="14" t="s">
-        <v>46</v>
+        <v>1986</v>
       </c>
       <c r="D1766" s="10" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="E1766" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1766" s="10" t="s">
-        <v>2369</v>
-      </c>
-      <c r="G1766" s="11"/>
-      <c r="H1766" s="12"/>
-      <c r="I1766" s="13"/>
-      <c r="J1766" s="13"/>
-    </row>
-    <row r="1767" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2471</v>
+      </c>
+      <c r="G1766" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1766" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1766" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1766" s="13" t="s">
+        <v>2472</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1767" s="12">
-        <v>43816</v>
-      </c>
-      <c r="B1767" s="9"/>
+        <v>44580</v>
+      </c>
+      <c r="B1767" s="12">
+        <v>44580</v>
+      </c>
       <c r="C1767" s="14" t="s">
-        <v>475</v>
+        <v>1986</v>
       </c>
       <c r="D1767" s="10" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="E1767" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1767" s="10" t="s">
-        <v>474</v>
+        <v>2473</v>
       </c>
       <c r="G1767" s="11" t="s">
-        <v>1627</v>
-      </c>
-      <c r="H1767" s="12"/>
-      <c r="I1767" s="13"/>
+        <v>295</v>
+      </c>
+      <c r="H1767" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1767" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1767" s="13" t="s">
-        <v>1565</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="1768" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1768" s="12">
-        <v>44460</v>
-      </c>
+      <c r="A1768" s="12"/>
       <c r="B1768" s="12"/>
-      <c r="C1768" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1768" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="E1768" s="11" t="s">
-        <v>837</v>
-      </c>
-      <c r="F1768" s="10" t="s">
-        <v>2193</v>
-      </c>
+      <c r="C1768" s="14"/>
+      <c r="D1768" s="10"/>
+      <c r="E1768" s="11"/>
+      <c r="F1768" s="10"/>
       <c r="G1768" s="11"/>
       <c r="H1768" s="12"/>
       <c r="I1768" s="13"/>
@@ -61385,7 +61491,7 @@
     </row>
     <row r="1771" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1771" s="12"/>
-      <c r="B1771" s="9"/>
+      <c r="B1771" s="12"/>
       <c r="C1771" s="14"/>
       <c r="D1771" s="10"/>
       <c r="E1771" s="11"/>
@@ -61395,64 +61501,70 @@
       <c r="I1771" s="13"/>
       <c r="J1771" s="13"/>
     </row>
-    <row r="1772" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1772" s="1" t="s">
-        <v>1475</v>
-      </c>
-      <c r="B1772" s="2" t="s">
-        <v>1476</v>
-      </c>
-      <c r="C1772" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1772" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1772" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1772" s="4" t="s">
-        <v>1575</v>
-      </c>
-      <c r="G1772" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1772" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1772" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1772" s="36"/>
+    <row r="1772" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1772" s="12">
+        <v>44522</v>
+      </c>
+      <c r="B1772" s="12"/>
+      <c r="C1772" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1772" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1772" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1772" s="10" t="s">
+        <v>2369</v>
+      </c>
+      <c r="G1772" s="11"/>
+      <c r="H1772" s="12"/>
+      <c r="I1772" s="13"/>
+      <c r="J1772" s="13"/>
     </row>
     <row r="1773" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1773" s="12"/>
+      <c r="A1773" s="12">
+        <v>43816</v>
+      </c>
       <c r="B1773" s="9"/>
-      <c r="C1773" s="14"/>
-      <c r="D1773" s="10"/>
-      <c r="E1773" s="11"/>
-      <c r="F1773" s="10"/>
-      <c r="G1773" s="11"/>
+      <c r="C1773" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1773" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1773" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1773" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G1773" s="11" t="s">
+        <v>1627</v>
+      </c>
       <c r="H1773" s="12"/>
       <c r="I1773" s="13"/>
-      <c r="J1773" s="13"/>
+      <c r="J1773" s="13" t="s">
+        <v>1565</v>
+      </c>
     </row>
     <row r="1774" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1774" s="12"/>
-      <c r="B1774" s="12">
-        <v>44402</v>
-      </c>
+      <c r="A1774" s="12">
+        <v>44460</v>
+      </c>
+      <c r="B1774" s="12"/>
       <c r="C1774" s="14" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D1774" s="10" t="s">
-        <v>584</v>
+        <v>494</v>
       </c>
       <c r="E1774" s="11" t="s">
-        <v>647</v>
+        <v>837</v>
       </c>
       <c r="F1774" s="10" t="s">
-        <v>1609</v>
+        <v>2193</v>
       </c>
       <c r="G1774" s="11"/>
       <c r="H1774" s="12"/>
@@ -61461,21 +61573,11 @@
     </row>
     <row r="1775" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1775" s="12"/>
-      <c r="B1775" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1775" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1775" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1775" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1775" s="10" t="s">
-        <v>1601</v>
-      </c>
+      <c r="B1775" s="12"/>
+      <c r="C1775" s="14"/>
+      <c r="D1775" s="10"/>
+      <c r="E1775" s="11"/>
+      <c r="F1775" s="10"/>
       <c r="G1775" s="11"/>
       <c r="H1775" s="12"/>
       <c r="I1775" s="13"/>
@@ -61483,21 +61585,11 @@
     </row>
     <row r="1776" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1776" s="12"/>
-      <c r="B1776" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1776" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1776" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1776" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1776" s="10" t="s">
-        <v>1606</v>
-      </c>
+      <c r="B1776" s="12"/>
+      <c r="C1776" s="14"/>
+      <c r="D1776" s="10"/>
+      <c r="E1776" s="11"/>
+      <c r="F1776" s="10"/>
       <c r="G1776" s="11"/>
       <c r="H1776" s="12"/>
       <c r="I1776" s="13"/>
@@ -61505,63 +61597,53 @@
     </row>
     <row r="1777" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1777" s="12"/>
-      <c r="B1777" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1777" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1777" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1777" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1777" s="10" t="s">
-        <v>1602</v>
-      </c>
+      <c r="B1777" s="9"/>
+      <c r="C1777" s="14"/>
+      <c r="D1777" s="10"/>
+      <c r="E1777" s="11"/>
+      <c r="F1777" s="10"/>
       <c r="G1777" s="11"/>
       <c r="H1777" s="12"/>
       <c r="I1777" s="13"/>
       <c r="J1777" s="13"/>
     </row>
     <row r="1778" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1778" s="12"/>
-      <c r="B1778" s="9"/>
-      <c r="C1778" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1778" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1778" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1778" s="10" t="s">
-        <v>1610</v>
-      </c>
-      <c r="G1778" s="11"/>
-      <c r="H1778" s="12"/>
-      <c r="I1778" s="13"/>
-      <c r="J1778" s="13"/>
+      <c r="A1778" s="1" t="s">
+        <v>1475</v>
+      </c>
+      <c r="B1778" s="2" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C1778" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1778" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1778" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1778" s="4" t="s">
+        <v>1575</v>
+      </c>
+      <c r="G1778" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1778" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1778" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1778" s="36"/>
     </row>
     <row r="1779" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1779" s="12"/>
-      <c r="B1779" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1779" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1779" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1779" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1779" s="10" t="s">
-        <v>1603</v>
-      </c>
+      <c r="B1779" s="9"/>
+      <c r="C1779" s="14"/>
+      <c r="D1779" s="10"/>
+      <c r="E1779" s="11"/>
+      <c r="F1779" s="10"/>
       <c r="G1779" s="11"/>
       <c r="H1779" s="12"/>
       <c r="I1779" s="13"/>
@@ -61569,7 +61651,9 @@
     </row>
     <row r="1780" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1780" s="12"/>
-      <c r="B1780" s="9"/>
+      <c r="B1780" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1780" s="14" t="s">
         <v>13</v>
       </c>
@@ -61580,7 +61664,7 @@
         <v>647</v>
       </c>
       <c r="F1780" s="10" t="s">
-        <v>1600</v>
+        <v>1609</v>
       </c>
       <c r="G1780" s="11"/>
       <c r="H1780" s="12"/>
@@ -61602,7 +61686,7 @@
         <v>647</v>
       </c>
       <c r="F1781" s="10" t="s">
-        <v>1599</v>
+        <v>1601</v>
       </c>
       <c r="G1781" s="11"/>
       <c r="H1781" s="12"/>
@@ -61624,7 +61708,7 @@
         <v>647</v>
       </c>
       <c r="F1782" s="10" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="G1782" s="11"/>
       <c r="H1782" s="12"/>
@@ -61646,7 +61730,7 @@
         <v>647</v>
       </c>
       <c r="F1783" s="10" t="s">
-        <v>1607</v>
+        <v>1602</v>
       </c>
       <c r="G1783" s="11"/>
       <c r="H1783" s="12"/>
@@ -61655,9 +61739,7 @@
     </row>
     <row r="1784" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1784" s="12"/>
-      <c r="B1784" s="9">
-        <v>44235</v>
-      </c>
+      <c r="B1784" s="9"/>
       <c r="C1784" s="14" t="s">
         <v>13</v>
       </c>
@@ -61668,7 +61750,7 @@
         <v>647</v>
       </c>
       <c r="F1784" s="10" t="s">
-        <v>1608</v>
+        <v>1610</v>
       </c>
       <c r="G1784" s="11"/>
       <c r="H1784" s="12"/>
@@ -61677,7 +61759,9 @@
     </row>
     <row r="1785" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1785" s="12"/>
-      <c r="B1785" s="9"/>
+      <c r="B1785" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1785" s="14" t="s">
         <v>13</v>
       </c>
@@ -61688,7 +61772,7 @@
         <v>647</v>
       </c>
       <c r="F1785" s="10" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
       <c r="G1785" s="11"/>
       <c r="H1785" s="12"/>
@@ -61698,77 +61782,83 @@
     <row r="1786" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1786" s="12"/>
       <c r="B1786" s="9"/>
-      <c r="C1786" s="14"/>
-      <c r="D1786" s="10"/>
-      <c r="E1786" s="11"/>
-      <c r="F1786" s="10"/>
+      <c r="C1786" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1786" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1786" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1786" s="10" t="s">
+        <v>1600</v>
+      </c>
       <c r="G1786" s="11"/>
       <c r="H1786" s="12"/>
       <c r="I1786" s="13"/>
       <c r="J1786" s="13"/>
     </row>
-    <row r="1787" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1787" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1787" s="9"/>
+    <row r="1787" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1787" s="12"/>
+      <c r="B1787" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1787" s="14" t="s">
-        <v>897</v>
+        <v>13</v>
       </c>
       <c r="D1787" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1787" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1787" s="10" t="s">
-        <v>1654</v>
+        <v>1599</v>
       </c>
       <c r="G1787" s="11"/>
       <c r="H1787" s="12"/>
       <c r="I1787" s="13"/>
-      <c r="J1787" s="13" t="s">
-        <v>1677</v>
-      </c>
-    </row>
-    <row r="1788" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1788" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1788" s="9"/>
+      <c r="J1787" s="13"/>
+    </row>
+    <row r="1788" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1788" s="12"/>
+      <c r="B1788" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1788" s="14" t="s">
-        <v>897</v>
+        <v>13</v>
       </c>
       <c r="D1788" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1788" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1788" s="10" t="s">
-        <v>1653</v>
+        <v>1604</v>
       </c>
       <c r="G1788" s="11"/>
       <c r="H1788" s="12"/>
       <c r="I1788" s="13"/>
       <c r="J1788" s="13"/>
     </row>
-    <row r="1789" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1789" s="12">
-        <v>44112</v>
-      </c>
-      <c r="B1789" s="9"/>
+    <row r="1789" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1789" s="12"/>
+      <c r="B1789" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1789" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1789" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1789" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1789" s="10" t="s">
-        <v>2241</v>
+        <v>1607</v>
       </c>
       <c r="G1789" s="11"/>
       <c r="H1789" s="12"/>
@@ -61776,21 +61866,21 @@
       <c r="J1789" s="13"/>
     </row>
     <row r="1790" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1790" s="12">
-        <v>44088</v>
-      </c>
-      <c r="B1790" s="9"/>
+      <c r="A1790" s="12"/>
+      <c r="B1790" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1790" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1790" s="10" t="s">
-        <v>905</v>
+        <v>584</v>
       </c>
       <c r="E1790" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1790" s="10" t="s">
-        <v>1010</v>
+        <v>1608</v>
       </c>
       <c r="G1790" s="11"/>
       <c r="H1790" s="12"/>
@@ -61798,21 +61888,19 @@
       <c r="J1790" s="13"/>
     </row>
     <row r="1791" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1791" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1791" s="12"/>
       <c r="B1791" s="9"/>
       <c r="C1791" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1791" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1791" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1791" s="10" t="s">
-        <v>902</v>
+        <v>1605</v>
       </c>
       <c r="G1791" s="11"/>
       <c r="H1791" s="12"/>
@@ -61820,30 +61908,20 @@
       <c r="J1791" s="13"/>
     </row>
     <row r="1792" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1792" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1792" s="12"/>
       <c r="B1792" s="9"/>
-      <c r="C1792" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="D1792" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1792" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1792" s="10" t="s">
-        <v>901</v>
-      </c>
+      <c r="C1792" s="14"/>
+      <c r="D1792" s="10"/>
+      <c r="E1792" s="11"/>
+      <c r="F1792" s="10"/>
       <c r="G1792" s="11"/>
       <c r="H1792" s="12"/>
       <c r="I1792" s="13"/>
       <c r="J1792" s="13"/>
     </row>
-    <row r="1793" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1793" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1793" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1793" s="9"/>
       <c r="C1793" s="14" t="s">
@@ -61853,19 +61931,21 @@
         <v>494</v>
       </c>
       <c r="E1793" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1793" s="10" t="s">
-        <v>899</v>
+        <v>1654</v>
       </c>
       <c r="G1793" s="11"/>
       <c r="H1793" s="12"/>
       <c r="I1793" s="13"/>
-      <c r="J1793" s="13"/>
-    </row>
-    <row r="1794" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="J1793" s="13" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="1794" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1794" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1794" s="9"/>
       <c r="C1794" s="14" t="s">
@@ -61875,220 +61955,352 @@
         <v>494</v>
       </c>
       <c r="E1794" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1794" s="10" t="s">
-        <v>900</v>
+        <v>1653</v>
       </c>
       <c r="G1794" s="11"/>
       <c r="H1794" s="12"/>
       <c r="I1794" s="13"/>
       <c r="J1794" s="13"/>
     </row>
-    <row r="1795" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1795" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1795" s="12">
-        <v>44055</v>
+        <v>44112</v>
       </c>
       <c r="B1795" s="9"/>
       <c r="C1795" s="14" t="s">
-        <v>897</v>
+        <v>623</v>
       </c>
       <c r="D1795" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1795" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1795" s="10" t="s">
-        <v>903</v>
+        <v>2241</v>
       </c>
       <c r="G1795" s="11"/>
       <c r="H1795" s="12"/>
       <c r="I1795" s="13"/>
-      <c r="J1795" s="13" t="s">
-        <v>1583</v>
-      </c>
-    </row>
-    <row r="1796" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="J1795" s="13"/>
+    </row>
+    <row r="1796" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1796" s="12">
-        <v>43949</v>
+        <v>44088</v>
       </c>
       <c r="B1796" s="9"/>
       <c r="C1796" s="14" t="s">
-        <v>468</v>
+        <v>19</v>
       </c>
       <c r="D1796" s="10" t="s">
-        <v>89</v>
+        <v>905</v>
       </c>
       <c r="E1796" s="11" t="s">
         <v>685</v>
       </c>
       <c r="F1796" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1796" s="11" t="s">
-        <v>1634</v>
-      </c>
+        <v>1010</v>
+      </c>
+      <c r="G1796" s="11"/>
       <c r="H1796" s="12"/>
-      <c r="I1796" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1796" s="13"/>
       <c r="J1796" s="13"/>
     </row>
-    <row r="1797" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1797" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1797" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1797" s="9"/>
       <c r="C1797" s="14" t="s">
-        <v>468</v>
+        <v>623</v>
       </c>
       <c r="D1797" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1797" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1797" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1797" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="G1797" s="11"/>
       <c r="H1797" s="12"/>
-      <c r="I1797" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1797" s="13" t="s">
-        <v>1564</v>
-      </c>
-    </row>
-    <row r="1798" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1797" s="13"/>
+      <c r="J1797" s="13"/>
+    </row>
+    <row r="1798" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1798" s="12">
-        <v>43838</v>
+        <v>44055</v>
       </c>
       <c r="B1798" s="9"/>
       <c r="C1798" s="14" t="s">
-        <v>103</v>
+        <v>623</v>
       </c>
       <c r="D1798" s="10" t="s">
-        <v>460</v>
+        <v>6</v>
       </c>
       <c r="E1798" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1798" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G1798" s="11" t="s">
-        <v>1635</v>
-      </c>
+        <v>901</v>
+      </c>
+      <c r="G1798" s="11"/>
       <c r="H1798" s="12"/>
       <c r="I1798" s="13"/>
-      <c r="J1798" s="13" t="s">
-        <v>1529</v>
-      </c>
-    </row>
-    <row r="1799" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1798" s="13"/>
+    </row>
+    <row r="1799" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1799" s="12">
-        <v>43762</v>
+        <v>44055</v>
       </c>
       <c r="B1799" s="9"/>
       <c r="C1799" s="14" t="s">
-        <v>446</v>
+        <v>897</v>
       </c>
       <c r="D1799" s="10" t="s">
-        <v>17</v>
+        <v>494</v>
       </c>
       <c r="E1799" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1799" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G1799" s="11" t="s">
-        <v>1624</v>
-      </c>
+        <v>899</v>
+      </c>
+      <c r="G1799" s="11"/>
       <c r="H1799" s="12"/>
       <c r="I1799" s="13"/>
       <c r="J1799" s="13"/>
     </row>
-    <row r="1800" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1800" s="12"/>
+    <row r="1800" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A1800" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1800" s="9"/>
-      <c r="C1800" s="14"/>
-      <c r="D1800" s="10"/>
-      <c r="E1800" s="11"/>
-      <c r="F1800" s="10"/>
+      <c r="C1800" s="14" t="s">
+        <v>897</v>
+      </c>
+      <c r="D1800" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1800" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1800" s="10" t="s">
+        <v>900</v>
+      </c>
       <c r="G1800" s="11"/>
       <c r="H1800" s="12"/>
       <c r="I1800" s="13"/>
       <c r="J1800" s="13"/>
     </row>
-    <row r="1801" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1801" s="12"/>
+    <row r="1801" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1801" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1801" s="9"/>
-      <c r="C1801" s="14"/>
-      <c r="D1801" s="10"/>
-      <c r="E1801" s="11"/>
-      <c r="F1801" s="10"/>
+      <c r="C1801" s="14" t="s">
+        <v>897</v>
+      </c>
+      <c r="D1801" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1801" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1801" s="10" t="s">
+        <v>903</v>
+      </c>
       <c r="G1801" s="11"/>
       <c r="H1801" s="12"/>
       <c r="I1801" s="13"/>
-      <c r="J1801" s="13"/>
-    </row>
-    <row r="1802" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1802" s="12"/>
+      <c r="J1801" s="13" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="1802" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1802" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1802" s="9"/>
-      <c r="C1802" s="14"/>
-      <c r="D1802" s="10"/>
-      <c r="E1802" s="11"/>
-      <c r="F1802" s="10"/>
-      <c r="G1802" s="11"/>
+      <c r="C1802" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1802" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1802" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1802" s="10" t="s">
+        <v>686</v>
+      </c>
+      <c r="G1802" s="11" t="s">
+        <v>1634</v>
+      </c>
       <c r="H1802" s="12"/>
-      <c r="I1802" s="13"/>
+      <c r="I1802" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1802" s="13"/>
     </row>
-    <row r="1803" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1803" s="12"/>
+    <row r="1803" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1803" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1803" s="9"/>
-      <c r="C1803" s="14"/>
-      <c r="D1803" s="10"/>
-      <c r="E1803" s="11"/>
-      <c r="F1803" s="10"/>
-      <c r="G1803" s="11"/>
+      <c r="C1803" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1803" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1803" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1803" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="G1803" s="11" t="s">
+        <v>687</v>
+      </c>
       <c r="H1803" s="12"/>
-      <c r="I1803" s="13"/>
-      <c r="J1803" s="13"/>
-    </row>
-    <row r="1804" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1804" s="12"/>
+      <c r="I1803" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1803" s="13" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="1804" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1804" s="12">
+        <v>43838</v>
+      </c>
       <c r="B1804" s="9"/>
-      <c r="C1804" s="14"/>
-      <c r="D1804" s="10"/>
-      <c r="E1804" s="11"/>
-      <c r="F1804" s="10"/>
-      <c r="G1804" s="11"/>
+      <c r="C1804" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1804" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1804" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1804" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G1804" s="11" t="s">
+        <v>1635</v>
+      </c>
       <c r="H1804" s="12"/>
       <c r="I1804" s="13"/>
-      <c r="J1804" s="13"/>
-    </row>
-    <row r="1805" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1805" s="12"/>
+      <c r="J1804" s="13" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="1805" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1805" s="12">
+        <v>43762</v>
+      </c>
       <c r="B1805" s="9"/>
-      <c r="C1805" s="14"/>
-      <c r="D1805" s="10"/>
-      <c r="E1805" s="11"/>
-      <c r="F1805" s="10"/>
-      <c r="G1805" s="11"/>
+      <c r="C1805" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1805" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1805" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1805" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1805" s="11" t="s">
+        <v>1624</v>
+      </c>
       <c r="H1805" s="12"/>
       <c r="I1805" s="13"/>
       <c r="J1805" s="13"/>
     </row>
+    <row r="1806" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1806" s="12"/>
+      <c r="B1806" s="9"/>
+      <c r="C1806" s="14"/>
+      <c r="D1806" s="10"/>
+      <c r="E1806" s="11"/>
+      <c r="F1806" s="10"/>
+      <c r="G1806" s="11"/>
+      <c r="H1806" s="12"/>
+      <c r="I1806" s="13"/>
+      <c r="J1806" s="13"/>
+    </row>
+    <row r="1807" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1807" s="12"/>
+      <c r="B1807" s="9"/>
+      <c r="C1807" s="14"/>
+      <c r="D1807" s="10"/>
+      <c r="E1807" s="11"/>
+      <c r="F1807" s="10"/>
+      <c r="G1807" s="11"/>
+      <c r="H1807" s="12"/>
+      <c r="I1807" s="13"/>
+      <c r="J1807" s="13"/>
+    </row>
+    <row r="1808" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1808" s="12"/>
+      <c r="B1808" s="9"/>
+      <c r="C1808" s="14"/>
+      <c r="D1808" s="10"/>
+      <c r="E1808" s="11"/>
+      <c r="F1808" s="10"/>
+      <c r="G1808" s="11"/>
+      <c r="H1808" s="12"/>
+      <c r="I1808" s="13"/>
+      <c r="J1808" s="13"/>
+    </row>
+    <row r="1809" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1809" s="12"/>
+      <c r="B1809" s="9"/>
+      <c r="C1809" s="14"/>
+      <c r="D1809" s="10"/>
+      <c r="E1809" s="11"/>
+      <c r="F1809" s="10"/>
+      <c r="G1809" s="11"/>
+      <c r="H1809" s="12"/>
+      <c r="I1809" s="13"/>
+      <c r="J1809" s="13"/>
+    </row>
+    <row r="1810" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1810" s="12"/>
+      <c r="B1810" s="9"/>
+      <c r="C1810" s="14"/>
+      <c r="D1810" s="10"/>
+      <c r="E1810" s="11"/>
+      <c r="F1810" s="10"/>
+      <c r="G1810" s="11"/>
+      <c r="H1810" s="12"/>
+      <c r="I1810" s="13"/>
+      <c r="J1810" s="13"/>
+    </row>
+    <row r="1811" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1811" s="12"/>
+      <c r="B1811" s="9"/>
+      <c r="C1811" s="14"/>
+      <c r="D1811" s="10"/>
+      <c r="E1811" s="11"/>
+      <c r="F1811" s="10"/>
+      <c r="G1811" s="11"/>
+      <c r="H1811" s="12"/>
+      <c r="I1811" s="13"/>
+      <c r="J1811" s="13"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1480" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1775:F1785">
-    <sortCondition ref="F1775:F1785"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1781:F1791">
+    <sortCondition ref="F1781:F1791"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Mostrar CNPJ no Doc de Entrada
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F410A79E-66F0-4518-9F3D-C00D8FF1D687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6C15E9-4268-4E46-903F-2675FA44196C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12556" uniqueCount="2475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12599" uniqueCount="2480">
   <si>
     <t>Responsável</t>
   </si>
@@ -7838,10 +7838,25 @@
     <t>Revisão na rotina de acerto de códigos da DIRF BKAJUDIRF, para não sobrepor códigos digitados</t>
   </si>
   <si>
-    <t>Estou efetuado a apuração do lucro ´presumido da corretora, e temos uma nota fiscal na prefeitura cancelada e ativa no sistema. Por gentileza, excluir ou cancelar a mesma do sistema, segue o número da nota fiscal 2806 valor de  289,33.</t>
-  </si>
-  <si>
     <t>Alterado o parâmetro MV_EXCNFS para 20 temporariamente e voltado para 10 após a exclusão da NF</t>
+  </si>
+  <si>
+    <t>Ajustes EFD Balsa Nova de dezembro/2020</t>
+  </si>
+  <si>
+    <t>Reunião a respeito de titulos em aberto em 31/12/2021</t>
+  </si>
+  <si>
+    <t>Mostrar CNPJ/CPF na tela inicial do Doc de Entrada</t>
+  </si>
+  <si>
+    <t>Estou efetuado a apuração do lucro presumido da corretora, e temos uma nota fiscal na prefeitura cancelada e ativa no sistema. Por gentileza, excluir ou cancelar a mesma do sistema, segue o número da nota fiscal 2806 valor de  289,33.</t>
+  </si>
+  <si>
+    <t>Por favor acertar também as datas de emissões e vencimentos dos títulos abaixo para data do dia 05/01/2022 003546895 000245781</t>
+  </si>
+  <si>
+    <t>Por favor mudar a data de vencimentos de todos os títulos de todas as empresa que consiste na data 25/01/2022 conforme abaixo uma que peguei no BHG INT 3. Preciso que isso seja feito com urgência pois já estamos colocando todos os títulos no banco!</t>
   </si>
 </sst>
 </file>
@@ -8610,11 +8625,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1811"/>
+  <dimension ref="A1:J1817"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1764" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1768" sqref="A1768"/>
+      <selection pane="bottomLeft" activeCell="A1774" sqref="A1774"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -61053,27 +61068,27 @@
         <v>2458</v>
       </c>
     </row>
-    <row r="1755" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1755" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1755" s="12">
-        <v>44574</v>
+        <v>44573</v>
       </c>
       <c r="B1755" s="12">
-        <v>44574</v>
+        <v>44573</v>
       </c>
       <c r="C1755" s="14" t="s">
-        <v>537</v>
+        <v>1986</v>
       </c>
       <c r="D1755" s="10" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="E1755" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1755" s="10" t="s">
-        <v>2457</v>
+        <v>2478</v>
       </c>
       <c r="G1755" s="11" t="s">
-        <v>1616</v>
+        <v>295</v>
       </c>
       <c r="H1755" s="12" t="s">
         <v>112</v>
@@ -61091,25 +61106,25 @@
         <v>44574</v>
       </c>
       <c r="C1756" s="14" t="s">
-        <v>2028</v>
+        <v>537</v>
       </c>
       <c r="D1756" s="10" t="s">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="E1756" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1756" s="10" t="s">
-        <v>759</v>
+        <v>2457</v>
       </c>
       <c r="G1756" s="11" t="s">
-        <v>309</v>
+        <v>1616</v>
       </c>
       <c r="H1756" s="12" t="s">
         <v>112</v>
       </c>
       <c r="I1756" s="13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J1756" s="13"/>
     </row>
@@ -61121,50 +61136,50 @@
         <v>44574</v>
       </c>
       <c r="C1757" s="14" t="s">
-        <v>623</v>
+        <v>2028</v>
       </c>
       <c r="D1757" s="10" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
       <c r="E1757" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1757" s="10" t="s">
+        <v>759</v>
+      </c>
+      <c r="G1757" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1757" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1757" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1757" s="13"/>
+    </row>
+    <row r="1758" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1758" s="12">
+        <v>44574</v>
+      </c>
+      <c r="B1758" s="12">
+        <v>44574</v>
+      </c>
+      <c r="C1758" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1758" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1758" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1758" s="10" t="s">
         <v>2464</v>
       </c>
-      <c r="G1757" s="11" t="s">
+      <c r="G1758" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="H1757" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1757" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1757" s="13"/>
-    </row>
-    <row r="1758" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1758" s="12">
-        <v>44575</v>
-      </c>
-      <c r="B1758" s="12">
-        <v>44575</v>
-      </c>
-      <c r="C1758" s="14" t="s">
-        <v>462</v>
-      </c>
-      <c r="D1758" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1758" s="11" t="s">
-        <v>620</v>
-      </c>
-      <c r="F1758" s="10" t="s">
-        <v>2460</v>
-      </c>
-      <c r="G1758" s="11" t="s">
-        <v>308</v>
-      </c>
       <c r="H1758" s="12" t="s">
         <v>112</v>
       </c>
@@ -61173,7 +61188,7 @@
       </c>
       <c r="J1758" s="13"/>
     </row>
-    <row r="1759" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1759" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1759" s="12">
         <v>44575</v>
       </c>
@@ -61181,16 +61196,16 @@
         <v>44575</v>
       </c>
       <c r="C1759" s="14" t="s">
-        <v>387</v>
+        <v>462</v>
       </c>
       <c r="D1759" s="10" t="s">
-        <v>494</v>
+        <v>107</v>
       </c>
       <c r="E1759" s="11" t="s">
         <v>620</v>
       </c>
       <c r="F1759" s="10" t="s">
-        <v>2461</v>
+        <v>2460</v>
       </c>
       <c r="G1759" s="11" t="s">
         <v>308</v>
@@ -61201,31 +61216,29 @@
       <c r="I1759" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1759" s="13" t="s">
-        <v>2462</v>
-      </c>
+      <c r="J1759" s="13"/>
     </row>
     <row r="1760" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1760" s="12">
-        <v>44578</v>
+        <v>44575</v>
       </c>
       <c r="B1760" s="12">
-        <v>44578</v>
+        <v>44575</v>
       </c>
       <c r="C1760" s="14" t="s">
-        <v>575</v>
+        <v>387</v>
       </c>
       <c r="D1760" s="10" t="s">
-        <v>107</v>
+        <v>494</v>
       </c>
       <c r="E1760" s="11" t="s">
         <v>620</v>
       </c>
       <c r="F1760" s="10" t="s">
-        <v>2463</v>
+        <v>2461</v>
       </c>
       <c r="G1760" s="11" t="s">
-        <v>1641</v>
+        <v>308</v>
       </c>
       <c r="H1760" s="12" t="s">
         <v>112</v>
@@ -61233,7 +61246,9 @@
       <c r="I1760" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1760" s="13"/>
+      <c r="J1760" s="13" t="s">
+        <v>2462</v>
+      </c>
     </row>
     <row r="1761" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1761" s="12">
@@ -61243,16 +61258,16 @@
         <v>44578</v>
       </c>
       <c r="C1761" s="14" t="s">
-        <v>387</v>
+        <v>575</v>
       </c>
       <c r="D1761" s="10" t="s">
-        <v>494</v>
+        <v>107</v>
       </c>
       <c r="E1761" s="11" t="s">
         <v>620</v>
       </c>
       <c r="F1761" s="10" t="s">
-        <v>2465</v>
+        <v>2463</v>
       </c>
       <c r="G1761" s="11" t="s">
         <v>1641</v>
@@ -61263,31 +61278,29 @@
       <c r="I1761" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1761" s="13" t="s">
-        <v>2462</v>
-      </c>
+      <c r="J1761" s="13"/>
     </row>
     <row r="1762" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1762" s="12">
-        <v>44579</v>
+        <v>44578</v>
       </c>
       <c r="B1762" s="12">
-        <v>44579</v>
+        <v>44578</v>
       </c>
       <c r="C1762" s="14" t="s">
-        <v>2269</v>
+        <v>387</v>
       </c>
       <c r="D1762" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1762" s="11" t="s">
         <v>620</v>
       </c>
       <c r="F1762" s="10" t="s">
-        <v>2466</v>
+        <v>2465</v>
       </c>
       <c r="G1762" s="11" t="s">
-        <v>309</v>
+        <v>1641</v>
       </c>
       <c r="H1762" s="12" t="s">
         <v>112</v>
@@ -61295,7 +61308,9 @@
       <c r="I1762" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1762" s="13"/>
+      <c r="J1762" s="13" t="s">
+        <v>2462</v>
+      </c>
     </row>
     <row r="1763" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1763" s="12">
@@ -61305,19 +61320,19 @@
         <v>44579</v>
       </c>
       <c r="C1763" s="14" t="s">
-        <v>1157</v>
+        <v>2269</v>
       </c>
       <c r="D1763" s="10" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="E1763" s="11" t="s">
         <v>620</v>
       </c>
       <c r="F1763" s="10" t="s">
-        <v>2467</v>
+        <v>2466</v>
       </c>
       <c r="G1763" s="11" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="H1763" s="12" t="s">
         <v>112</v>
@@ -61327,24 +61342,24 @@
       </c>
       <c r="J1763" s="13"/>
     </row>
-    <row r="1764" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="1764" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1764" s="12">
-        <v>44580</v>
+        <v>44579</v>
       </c>
       <c r="B1764" s="12">
-        <v>44580</v>
+        <v>44579</v>
       </c>
       <c r="C1764" s="14" t="s">
-        <v>2269</v>
+        <v>1157</v>
       </c>
       <c r="D1764" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1764" s="11" t="s">
         <v>620</v>
       </c>
       <c r="F1764" s="10" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="G1764" s="11" t="s">
         <v>295</v>
@@ -61365,19 +61380,19 @@
         <v>44580</v>
       </c>
       <c r="C1765" s="14" t="s">
-        <v>537</v>
+        <v>2269</v>
       </c>
       <c r="D1765" s="10" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="E1765" s="11" t="s">
-        <v>570</v>
+        <v>620</v>
       </c>
       <c r="F1765" s="10" t="s">
-        <v>2469</v>
+        <v>2468</v>
       </c>
       <c r="G1765" s="11" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="H1765" s="12" t="s">
         <v>112</v>
@@ -61385,11 +61400,9 @@
       <c r="I1765" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1765" s="13" t="s">
-        <v>2470</v>
-      </c>
-    </row>
-    <row r="1766" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1765" s="13"/>
+    </row>
+    <row r="1766" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1766" s="12">
         <v>44580</v>
       </c>
@@ -61397,19 +61410,19 @@
         <v>44580</v>
       </c>
       <c r="C1766" s="14" t="s">
-        <v>1986</v>
+        <v>537</v>
       </c>
       <c r="D1766" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1766" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1766" s="10" t="s">
-        <v>2471</v>
+        <v>2469</v>
       </c>
       <c r="G1766" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H1766" s="12" t="s">
         <v>112</v>
@@ -61418,7 +61431,7 @@
         <v>13</v>
       </c>
       <c r="J1766" s="13" t="s">
-        <v>2472</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="1767" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -61438,134 +61451,212 @@
         <v>570</v>
       </c>
       <c r="F1767" s="10" t="s">
+        <v>2471</v>
+      </c>
+      <c r="G1767" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1767" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1767" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1767" s="13" t="s">
+        <v>2472</v>
+      </c>
+    </row>
+    <row r="1768" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1768" s="12">
+        <v>44580</v>
+      </c>
+      <c r="B1768" s="12">
+        <v>44580</v>
+      </c>
+      <c r="C1768" s="14" t="s">
+        <v>1986</v>
+      </c>
+      <c r="D1768" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1768" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1768" s="10" t="s">
+        <v>2477</v>
+      </c>
+      <c r="G1768" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1768" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1768" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1768" s="13" t="s">
         <v>2473</v>
       </c>
-      <c r="G1767" s="11" t="s">
+    </row>
+    <row r="1769" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1769" s="12">
+        <v>44581</v>
+      </c>
+      <c r="B1769" s="12">
+        <v>44581</v>
+      </c>
+      <c r="C1769" s="14" t="s">
+        <v>1986</v>
+      </c>
+      <c r="D1769" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1769" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1769" s="10" t="s">
+        <v>1463</v>
+      </c>
+      <c r="G1769" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1769" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1769" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1769" s="13"/>
+    </row>
+    <row r="1770" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1770" s="12">
+        <v>44581</v>
+      </c>
+      <c r="B1770" s="12">
+        <v>44581</v>
+      </c>
+      <c r="C1770" s="14" t="s">
+        <v>1986</v>
+      </c>
+      <c r="D1770" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1770" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1770" s="10" t="s">
+        <v>2474</v>
+      </c>
+      <c r="G1770" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="H1767" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1767" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1767" s="13" t="s">
-        <v>2474</v>
-      </c>
-    </row>
-    <row r="1768" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1768" s="12"/>
-      <c r="B1768" s="12"/>
-      <c r="C1768" s="14"/>
-      <c r="D1768" s="10"/>
-      <c r="E1768" s="11"/>
-      <c r="F1768" s="10"/>
-      <c r="G1768" s="11"/>
-      <c r="H1768" s="12"/>
-      <c r="I1768" s="13"/>
-      <c r="J1768" s="13"/>
-    </row>
-    <row r="1769" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1769" s="12"/>
-      <c r="B1769" s="12"/>
-      <c r="C1769" s="14"/>
-      <c r="D1769" s="10"/>
-      <c r="E1769" s="11"/>
-      <c r="F1769" s="10"/>
-      <c r="G1769" s="11"/>
-      <c r="H1769" s="12"/>
-      <c r="I1769" s="13"/>
-      <c r="J1769" s="13"/>
-    </row>
-    <row r="1770" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1770" s="12"/>
-      <c r="B1770" s="12"/>
-      <c r="C1770" s="14"/>
-      <c r="D1770" s="10"/>
-      <c r="E1770" s="11"/>
-      <c r="F1770" s="10"/>
-      <c r="G1770" s="11"/>
-      <c r="H1770" s="12"/>
-      <c r="I1770" s="13"/>
+      <c r="H1770" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1770" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1770" s="13"/>
     </row>
     <row r="1771" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1771" s="12"/>
-      <c r="B1771" s="12"/>
-      <c r="C1771" s="14"/>
-      <c r="D1771" s="10"/>
-      <c r="E1771" s="11"/>
-      <c r="F1771" s="10"/>
-      <c r="G1771" s="11"/>
-      <c r="H1771" s="12"/>
-      <c r="I1771" s="13"/>
+      <c r="A1771" s="12">
+        <v>44581</v>
+      </c>
+      <c r="B1771" s="12">
+        <v>44581</v>
+      </c>
+      <c r="C1771" s="14" t="s">
+        <v>2173</v>
+      </c>
+      <c r="D1771" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1771" s="11" t="s">
+        <v>759</v>
+      </c>
+      <c r="F1771" s="10" t="s">
+        <v>2475</v>
+      </c>
+      <c r="G1771" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1771" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1771" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1771" s="13"/>
     </row>
-    <row r="1772" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1772" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1772" s="12">
-        <v>44522</v>
-      </c>
-      <c r="B1772" s="12"/>
+        <v>44581</v>
+      </c>
+      <c r="B1772" s="12">
+        <v>44581</v>
+      </c>
       <c r="C1772" s="14" t="s">
-        <v>46</v>
+        <v>2269</v>
       </c>
       <c r="D1772" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1772" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1772" s="10" t="s">
+        <v>2476</v>
+      </c>
+      <c r="G1772" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1772" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1772" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1772" s="13" t="s">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="1773" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1773" s="12">
+        <v>44582</v>
+      </c>
+      <c r="B1773" s="12">
+        <v>44582</v>
+      </c>
+      <c r="C1773" s="14" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D1773" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="E1772" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1772" s="10" t="s">
-        <v>2369</v>
-      </c>
-      <c r="G1772" s="11"/>
-      <c r="H1772" s="12"/>
-      <c r="I1772" s="13"/>
-      <c r="J1772" s="13"/>
-    </row>
-    <row r="1773" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1773" s="12">
-        <v>43816</v>
-      </c>
-      <c r="B1773" s="9"/>
-      <c r="C1773" s="14" t="s">
-        <v>475</v>
-      </c>
-      <c r="D1773" s="10" t="s">
-        <v>38</v>
       </c>
       <c r="E1773" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1773" s="10" t="s">
-        <v>474</v>
+        <v>2479</v>
       </c>
       <c r="G1773" s="11" t="s">
-        <v>1627</v>
-      </c>
-      <c r="H1773" s="12"/>
-      <c r="I1773" s="13"/>
-      <c r="J1773" s="13" t="s">
-        <v>1565</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="H1773" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1773" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1773" s="13"/>
     </row>
     <row r="1774" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1774" s="12">
-        <v>44460</v>
-      </c>
+      <c r="A1774" s="12"/>
       <c r="B1774" s="12"/>
-      <c r="C1774" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1774" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="E1774" s="11" t="s">
-        <v>837</v>
-      </c>
-      <c r="F1774" s="10" t="s">
-        <v>2193</v>
-      </c>
+      <c r="C1774" s="14"/>
+      <c r="D1774" s="10"/>
+      <c r="E1774" s="11"/>
+      <c r="F1774" s="10"/>
       <c r="G1774" s="11"/>
       <c r="H1774" s="12"/>
       <c r="I1774" s="13"/>
@@ -61597,7 +61688,7 @@
     </row>
     <row r="1777" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1777" s="12"/>
-      <c r="B1777" s="9"/>
+      <c r="B1777" s="12"/>
       <c r="C1777" s="14"/>
       <c r="D1777" s="10"/>
       <c r="E1777" s="11"/>
@@ -61607,64 +61698,70 @@
       <c r="I1777" s="13"/>
       <c r="J1777" s="13"/>
     </row>
-    <row r="1778" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1778" s="1" t="s">
-        <v>1475</v>
-      </c>
-      <c r="B1778" s="2" t="s">
-        <v>1476</v>
-      </c>
-      <c r="C1778" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1778" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1778" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1778" s="4" t="s">
-        <v>1575</v>
-      </c>
-      <c r="G1778" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1778" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1778" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1778" s="36"/>
+    <row r="1778" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1778" s="12">
+        <v>44522</v>
+      </c>
+      <c r="B1778" s="12"/>
+      <c r="C1778" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1778" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1778" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1778" s="10" t="s">
+        <v>2369</v>
+      </c>
+      <c r="G1778" s="11"/>
+      <c r="H1778" s="12"/>
+      <c r="I1778" s="13"/>
+      <c r="J1778" s="13"/>
     </row>
     <row r="1779" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1779" s="12"/>
+      <c r="A1779" s="12">
+        <v>43816</v>
+      </c>
       <c r="B1779" s="9"/>
-      <c r="C1779" s="14"/>
-      <c r="D1779" s="10"/>
-      <c r="E1779" s="11"/>
-      <c r="F1779" s="10"/>
-      <c r="G1779" s="11"/>
+      <c r="C1779" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1779" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1779" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1779" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="G1779" s="11" t="s">
+        <v>1627</v>
+      </c>
       <c r="H1779" s="12"/>
       <c r="I1779" s="13"/>
-      <c r="J1779" s="13"/>
+      <c r="J1779" s="13" t="s">
+        <v>1565</v>
+      </c>
     </row>
     <row r="1780" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1780" s="12"/>
-      <c r="B1780" s="12">
-        <v>44402</v>
-      </c>
+      <c r="A1780" s="12">
+        <v>44460</v>
+      </c>
+      <c r="B1780" s="12"/>
       <c r="C1780" s="14" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D1780" s="10" t="s">
-        <v>584</v>
+        <v>494</v>
       </c>
       <c r="E1780" s="11" t="s">
-        <v>647</v>
+        <v>837</v>
       </c>
       <c r="F1780" s="10" t="s">
-        <v>1609</v>
+        <v>2193</v>
       </c>
       <c r="G1780" s="11"/>
       <c r="H1780" s="12"/>
@@ -61673,21 +61770,11 @@
     </row>
     <row r="1781" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1781" s="12"/>
-      <c r="B1781" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1781" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1781" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1781" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1781" s="10" t="s">
-        <v>1601</v>
-      </c>
+      <c r="B1781" s="12"/>
+      <c r="C1781" s="14"/>
+      <c r="D1781" s="10"/>
+      <c r="E1781" s="11"/>
+      <c r="F1781" s="10"/>
       <c r="G1781" s="11"/>
       <c r="H1781" s="12"/>
       <c r="I1781" s="13"/>
@@ -61695,21 +61782,11 @@
     </row>
     <row r="1782" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1782" s="12"/>
-      <c r="B1782" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1782" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1782" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1782" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1782" s="10" t="s">
-        <v>1606</v>
-      </c>
+      <c r="B1782" s="12"/>
+      <c r="C1782" s="14"/>
+      <c r="D1782" s="10"/>
+      <c r="E1782" s="11"/>
+      <c r="F1782" s="10"/>
       <c r="G1782" s="11"/>
       <c r="H1782" s="12"/>
       <c r="I1782" s="13"/>
@@ -61717,63 +61794,53 @@
     </row>
     <row r="1783" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1783" s="12"/>
-      <c r="B1783" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1783" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1783" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1783" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1783" s="10" t="s">
-        <v>1602</v>
-      </c>
+      <c r="B1783" s="9"/>
+      <c r="C1783" s="14"/>
+      <c r="D1783" s="10"/>
+      <c r="E1783" s="11"/>
+      <c r="F1783" s="10"/>
       <c r="G1783" s="11"/>
       <c r="H1783" s="12"/>
       <c r="I1783" s="13"/>
       <c r="J1783" s="13"/>
     </row>
     <row r="1784" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1784" s="12"/>
-      <c r="B1784" s="9"/>
-      <c r="C1784" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1784" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1784" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1784" s="10" t="s">
-        <v>1610</v>
-      </c>
-      <c r="G1784" s="11"/>
-      <c r="H1784" s="12"/>
-      <c r="I1784" s="13"/>
-      <c r="J1784" s="13"/>
+      <c r="A1784" s="1" t="s">
+        <v>1475</v>
+      </c>
+      <c r="B1784" s="2" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C1784" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1784" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1784" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1784" s="4" t="s">
+        <v>1575</v>
+      </c>
+      <c r="G1784" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1784" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1784" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1784" s="36"/>
     </row>
     <row r="1785" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1785" s="12"/>
-      <c r="B1785" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1785" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1785" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1785" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1785" s="10" t="s">
-        <v>1603</v>
-      </c>
+      <c r="B1785" s="9"/>
+      <c r="C1785" s="14"/>
+      <c r="D1785" s="10"/>
+      <c r="E1785" s="11"/>
+      <c r="F1785" s="10"/>
       <c r="G1785" s="11"/>
       <c r="H1785" s="12"/>
       <c r="I1785" s="13"/>
@@ -61781,7 +61848,9 @@
     </row>
     <row r="1786" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1786" s="12"/>
-      <c r="B1786" s="9"/>
+      <c r="B1786" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1786" s="14" t="s">
         <v>13</v>
       </c>
@@ -61792,7 +61861,7 @@
         <v>647</v>
       </c>
       <c r="F1786" s="10" t="s">
-        <v>1600</v>
+        <v>1609</v>
       </c>
       <c r="G1786" s="11"/>
       <c r="H1786" s="12"/>
@@ -61814,7 +61883,7 @@
         <v>647</v>
       </c>
       <c r="F1787" s="10" t="s">
-        <v>1599</v>
+        <v>1601</v>
       </c>
       <c r="G1787" s="11"/>
       <c r="H1787" s="12"/>
@@ -61836,7 +61905,7 @@
         <v>647</v>
       </c>
       <c r="F1788" s="10" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="G1788" s="11"/>
       <c r="H1788" s="12"/>
@@ -61858,7 +61927,7 @@
         <v>647</v>
       </c>
       <c r="F1789" s="10" t="s">
-        <v>1607</v>
+        <v>1602</v>
       </c>
       <c r="G1789" s="11"/>
       <c r="H1789" s="12"/>
@@ -61867,9 +61936,7 @@
     </row>
     <row r="1790" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1790" s="12"/>
-      <c r="B1790" s="9">
-        <v>44235</v>
-      </c>
+      <c r="B1790" s="9"/>
       <c r="C1790" s="14" t="s">
         <v>13</v>
       </c>
@@ -61880,7 +61947,7 @@
         <v>647</v>
       </c>
       <c r="F1790" s="10" t="s">
-        <v>1608</v>
+        <v>1610</v>
       </c>
       <c r="G1790" s="11"/>
       <c r="H1790" s="12"/>
@@ -61889,7 +61956,9 @@
     </row>
     <row r="1791" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1791" s="12"/>
-      <c r="B1791" s="9"/>
+      <c r="B1791" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1791" s="14" t="s">
         <v>13</v>
       </c>
@@ -61900,7 +61969,7 @@
         <v>647</v>
       </c>
       <c r="F1791" s="10" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
       <c r="G1791" s="11"/>
       <c r="H1791" s="12"/>
@@ -61910,77 +61979,83 @@
     <row r="1792" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1792" s="12"/>
       <c r="B1792" s="9"/>
-      <c r="C1792" s="14"/>
-      <c r="D1792" s="10"/>
-      <c r="E1792" s="11"/>
-      <c r="F1792" s="10"/>
+      <c r="C1792" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1792" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1792" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1792" s="10" t="s">
+        <v>1600</v>
+      </c>
       <c r="G1792" s="11"/>
       <c r="H1792" s="12"/>
       <c r="I1792" s="13"/>
       <c r="J1792" s="13"/>
     </row>
-    <row r="1793" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1793" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1793" s="9"/>
+    <row r="1793" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1793" s="12"/>
+      <c r="B1793" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1793" s="14" t="s">
-        <v>897</v>
+        <v>13</v>
       </c>
       <c r="D1793" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1793" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1793" s="10" t="s">
-        <v>1654</v>
+        <v>1599</v>
       </c>
       <c r="G1793" s="11"/>
       <c r="H1793" s="12"/>
       <c r="I1793" s="13"/>
-      <c r="J1793" s="13" t="s">
-        <v>1677</v>
-      </c>
-    </row>
-    <row r="1794" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1794" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1794" s="9"/>
+      <c r="J1793" s="13"/>
+    </row>
+    <row r="1794" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1794" s="12"/>
+      <c r="B1794" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1794" s="14" t="s">
-        <v>897</v>
+        <v>13</v>
       </c>
       <c r="D1794" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1794" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1794" s="10" t="s">
-        <v>1653</v>
+        <v>1604</v>
       </c>
       <c r="G1794" s="11"/>
       <c r="H1794" s="12"/>
       <c r="I1794" s="13"/>
       <c r="J1794" s="13"/>
     </row>
-    <row r="1795" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1795" s="12">
-        <v>44112</v>
-      </c>
-      <c r="B1795" s="9"/>
+    <row r="1795" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1795" s="12"/>
+      <c r="B1795" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1795" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1795" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1795" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1795" s="10" t="s">
-        <v>2241</v>
+        <v>1607</v>
       </c>
       <c r="G1795" s="11"/>
       <c r="H1795" s="12"/>
@@ -61988,21 +62063,21 @@
       <c r="J1795" s="13"/>
     </row>
     <row r="1796" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1796" s="12">
-        <v>44088</v>
-      </c>
-      <c r="B1796" s="9"/>
+      <c r="A1796" s="12"/>
+      <c r="B1796" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1796" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1796" s="10" t="s">
-        <v>905</v>
+        <v>584</v>
       </c>
       <c r="E1796" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1796" s="10" t="s">
-        <v>1010</v>
+        <v>1608</v>
       </c>
       <c r="G1796" s="11"/>
       <c r="H1796" s="12"/>
@@ -62010,21 +62085,19 @@
       <c r="J1796" s="13"/>
     </row>
     <row r="1797" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1797" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1797" s="12"/>
       <c r="B1797" s="9"/>
       <c r="C1797" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1797" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1797" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1797" s="10" t="s">
-        <v>902</v>
+        <v>1605</v>
       </c>
       <c r="G1797" s="11"/>
       <c r="H1797" s="12"/>
@@ -62032,30 +62105,20 @@
       <c r="J1797" s="13"/>
     </row>
     <row r="1798" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1798" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1798" s="12"/>
       <c r="B1798" s="9"/>
-      <c r="C1798" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="D1798" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1798" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1798" s="10" t="s">
-        <v>901</v>
-      </c>
+      <c r="C1798" s="14"/>
+      <c r="D1798" s="10"/>
+      <c r="E1798" s="11"/>
+      <c r="F1798" s="10"/>
       <c r="G1798" s="11"/>
       <c r="H1798" s="12"/>
       <c r="I1798" s="13"/>
       <c r="J1798" s="13"/>
     </row>
-    <row r="1799" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1799" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1799" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1799" s="9"/>
       <c r="C1799" s="14" t="s">
@@ -62065,19 +62128,21 @@
         <v>494</v>
       </c>
       <c r="E1799" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1799" s="10" t="s">
-        <v>899</v>
+        <v>1654</v>
       </c>
       <c r="G1799" s="11"/>
       <c r="H1799" s="12"/>
       <c r="I1799" s="13"/>
-      <c r="J1799" s="13"/>
-    </row>
-    <row r="1800" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="J1799" s="13" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="1800" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1800" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1800" s="9"/>
       <c r="C1800" s="14" t="s">
@@ -62087,220 +62152,352 @@
         <v>494</v>
       </c>
       <c r="E1800" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1800" s="10" t="s">
-        <v>900</v>
+        <v>1653</v>
       </c>
       <c r="G1800" s="11"/>
       <c r="H1800" s="12"/>
       <c r="I1800" s="13"/>
       <c r="J1800" s="13"/>
     </row>
-    <row r="1801" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1801" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1801" s="12">
-        <v>44055</v>
+        <v>44112</v>
       </c>
       <c r="B1801" s="9"/>
       <c r="C1801" s="14" t="s">
-        <v>897</v>
+        <v>623</v>
       </c>
       <c r="D1801" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1801" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F1801" s="10" t="s">
-        <v>903</v>
+        <v>2241</v>
       </c>
       <c r="G1801" s="11"/>
       <c r="H1801" s="12"/>
       <c r="I1801" s="13"/>
-      <c r="J1801" s="13" t="s">
-        <v>1583</v>
-      </c>
-    </row>
-    <row r="1802" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="J1801" s="13"/>
+    </row>
+    <row r="1802" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1802" s="12">
-        <v>43949</v>
+        <v>44088</v>
       </c>
       <c r="B1802" s="9"/>
       <c r="C1802" s="14" t="s">
-        <v>468</v>
+        <v>19</v>
       </c>
       <c r="D1802" s="10" t="s">
-        <v>89</v>
+        <v>905</v>
       </c>
       <c r="E1802" s="11" t="s">
         <v>685</v>
       </c>
       <c r="F1802" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1802" s="11" t="s">
-        <v>1634</v>
-      </c>
+        <v>1010</v>
+      </c>
+      <c r="G1802" s="11"/>
       <c r="H1802" s="12"/>
-      <c r="I1802" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1802" s="13"/>
       <c r="J1802" s="13"/>
     </row>
-    <row r="1803" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1803" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1803" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1803" s="9"/>
       <c r="C1803" s="14" t="s">
-        <v>468</v>
+        <v>623</v>
       </c>
       <c r="D1803" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1803" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1803" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1803" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="G1803" s="11"/>
       <c r="H1803" s="12"/>
-      <c r="I1803" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1803" s="13" t="s">
-        <v>1564</v>
-      </c>
-    </row>
-    <row r="1804" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1803" s="13"/>
+      <c r="J1803" s="13"/>
+    </row>
+    <row r="1804" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1804" s="12">
-        <v>43838</v>
+        <v>44055</v>
       </c>
       <c r="B1804" s="9"/>
       <c r="C1804" s="14" t="s">
-        <v>103</v>
+        <v>623</v>
       </c>
       <c r="D1804" s="10" t="s">
-        <v>460</v>
+        <v>6</v>
       </c>
       <c r="E1804" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1804" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G1804" s="11" t="s">
-        <v>1635</v>
-      </c>
+        <v>901</v>
+      </c>
+      <c r="G1804" s="11"/>
       <c r="H1804" s="12"/>
       <c r="I1804" s="13"/>
-      <c r="J1804" s="13" t="s">
-        <v>1529</v>
-      </c>
-    </row>
-    <row r="1805" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1804" s="13"/>
+    </row>
+    <row r="1805" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1805" s="12">
-        <v>43762</v>
+        <v>44055</v>
       </c>
       <c r="B1805" s="9"/>
       <c r="C1805" s="14" t="s">
-        <v>446</v>
+        <v>897</v>
       </c>
       <c r="D1805" s="10" t="s">
-        <v>17</v>
+        <v>494</v>
       </c>
       <c r="E1805" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1805" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G1805" s="11" t="s">
-        <v>1624</v>
-      </c>
+        <v>899</v>
+      </c>
+      <c r="G1805" s="11"/>
       <c r="H1805" s="12"/>
       <c r="I1805" s="13"/>
       <c r="J1805" s="13"/>
     </row>
-    <row r="1806" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1806" s="12"/>
+    <row r="1806" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A1806" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1806" s="9"/>
-      <c r="C1806" s="14"/>
-      <c r="D1806" s="10"/>
-      <c r="E1806" s="11"/>
-      <c r="F1806" s="10"/>
+      <c r="C1806" s="14" t="s">
+        <v>897</v>
+      </c>
+      <c r="D1806" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1806" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1806" s="10" t="s">
+        <v>900</v>
+      </c>
       <c r="G1806" s="11"/>
       <c r="H1806" s="12"/>
       <c r="I1806" s="13"/>
       <c r="J1806" s="13"/>
     </row>
-    <row r="1807" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1807" s="12"/>
+    <row r="1807" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1807" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1807" s="9"/>
-      <c r="C1807" s="14"/>
-      <c r="D1807" s="10"/>
-      <c r="E1807" s="11"/>
-      <c r="F1807" s="10"/>
+      <c r="C1807" s="14" t="s">
+        <v>897</v>
+      </c>
+      <c r="D1807" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1807" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1807" s="10" t="s">
+        <v>903</v>
+      </c>
       <c r="G1807" s="11"/>
       <c r="H1807" s="12"/>
       <c r="I1807" s="13"/>
-      <c r="J1807" s="13"/>
-    </row>
-    <row r="1808" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1808" s="12"/>
+      <c r="J1807" s="13" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="1808" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1808" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1808" s="9"/>
-      <c r="C1808" s="14"/>
-      <c r="D1808" s="10"/>
-      <c r="E1808" s="11"/>
-      <c r="F1808" s="10"/>
-      <c r="G1808" s="11"/>
+      <c r="C1808" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1808" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1808" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1808" s="10" t="s">
+        <v>686</v>
+      </c>
+      <c r="G1808" s="11" t="s">
+        <v>1634</v>
+      </c>
       <c r="H1808" s="12"/>
-      <c r="I1808" s="13"/>
+      <c r="I1808" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1808" s="13"/>
     </row>
-    <row r="1809" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1809" s="12"/>
+    <row r="1809" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1809" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1809" s="9"/>
-      <c r="C1809" s="14"/>
-      <c r="D1809" s="10"/>
-      <c r="E1809" s="11"/>
-      <c r="F1809" s="10"/>
-      <c r="G1809" s="11"/>
+      <c r="C1809" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1809" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1809" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1809" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="G1809" s="11" t="s">
+        <v>687</v>
+      </c>
       <c r="H1809" s="12"/>
-      <c r="I1809" s="13"/>
-      <c r="J1809" s="13"/>
-    </row>
-    <row r="1810" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1810" s="12"/>
+      <c r="I1809" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1809" s="13" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="1810" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1810" s="12">
+        <v>43838</v>
+      </c>
       <c r="B1810" s="9"/>
-      <c r="C1810" s="14"/>
-      <c r="D1810" s="10"/>
-      <c r="E1810" s="11"/>
-      <c r="F1810" s="10"/>
-      <c r="G1810" s="11"/>
+      <c r="C1810" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1810" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1810" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1810" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G1810" s="11" t="s">
+        <v>1635</v>
+      </c>
       <c r="H1810" s="12"/>
       <c r="I1810" s="13"/>
-      <c r="J1810" s="13"/>
-    </row>
-    <row r="1811" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1811" s="12"/>
+      <c r="J1810" s="13" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="1811" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1811" s="12">
+        <v>43762</v>
+      </c>
       <c r="B1811" s="9"/>
-      <c r="C1811" s="14"/>
-      <c r="D1811" s="10"/>
-      <c r="E1811" s="11"/>
-      <c r="F1811" s="10"/>
-      <c r="G1811" s="11"/>
+      <c r="C1811" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1811" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1811" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1811" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1811" s="11" t="s">
+        <v>1624</v>
+      </c>
       <c r="H1811" s="12"/>
       <c r="I1811" s="13"/>
       <c r="J1811" s="13"/>
     </row>
+    <row r="1812" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1812" s="12"/>
+      <c r="B1812" s="9"/>
+      <c r="C1812" s="14"/>
+      <c r="D1812" s="10"/>
+      <c r="E1812" s="11"/>
+      <c r="F1812" s="10"/>
+      <c r="G1812" s="11"/>
+      <c r="H1812" s="12"/>
+      <c r="I1812" s="13"/>
+      <c r="J1812" s="13"/>
+    </row>
+    <row r="1813" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1813" s="12"/>
+      <c r="B1813" s="9"/>
+      <c r="C1813" s="14"/>
+      <c r="D1813" s="10"/>
+      <c r="E1813" s="11"/>
+      <c r="F1813" s="10"/>
+      <c r="G1813" s="11"/>
+      <c r="H1813" s="12"/>
+      <c r="I1813" s="13"/>
+      <c r="J1813" s="13"/>
+    </row>
+    <row r="1814" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1814" s="12"/>
+      <c r="B1814" s="9"/>
+      <c r="C1814" s="14"/>
+      <c r="D1814" s="10"/>
+      <c r="E1814" s="11"/>
+      <c r="F1814" s="10"/>
+      <c r="G1814" s="11"/>
+      <c r="H1814" s="12"/>
+      <c r="I1814" s="13"/>
+      <c r="J1814" s="13"/>
+    </row>
+    <row r="1815" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1815" s="12"/>
+      <c r="B1815" s="9"/>
+      <c r="C1815" s="14"/>
+      <c r="D1815" s="10"/>
+      <c r="E1815" s="11"/>
+      <c r="F1815" s="10"/>
+      <c r="G1815" s="11"/>
+      <c r="H1815" s="12"/>
+      <c r="I1815" s="13"/>
+      <c r="J1815" s="13"/>
+    </row>
+    <row r="1816" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1816" s="12"/>
+      <c r="B1816" s="9"/>
+      <c r="C1816" s="14"/>
+      <c r="D1816" s="10"/>
+      <c r="E1816" s="11"/>
+      <c r="F1816" s="10"/>
+      <c r="G1816" s="11"/>
+      <c r="H1816" s="12"/>
+      <c r="I1816" s="13"/>
+      <c r="J1816" s="13"/>
+    </row>
+    <row r="1817" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1817" s="12"/>
+      <c r="B1817" s="9"/>
+      <c r="C1817" s="14"/>
+      <c r="D1817" s="10"/>
+      <c r="E1817" s="11"/>
+      <c r="F1817" s="10"/>
+      <c r="G1817" s="11"/>
+      <c r="H1817" s="12"/>
+      <c r="I1817" s="13"/>
+      <c r="J1817" s="13"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1480" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1781:F1791">
-    <sortCondition ref="F1781:F1791"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1787:F1797">
+    <sortCondition ref="F1787:F1797"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Dirf e Lib alt E@_VALOR
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6C15E9-4268-4E46-903F-2675FA44196C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAD9C12-704C-4D99-AC43-7B27D0651E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12599" uniqueCount="2480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12653" uniqueCount="2487">
   <si>
     <t>Responsável</t>
   </si>
@@ -7857,6 +7857,27 @@
   </si>
   <si>
     <t>Por favor mudar a data de vencimentos de todos os títulos de todas as empresa que consiste na data 25/01/2022 conforme abaixo uma que peguei no BHG INT 3. Preciso que isso seja feito com urgência pois já estamos colocando todos os títulos no banco!</t>
+  </si>
+  <si>
+    <t>Suporte emissão de relatório de faturamento</t>
+  </si>
+  <si>
+    <t>Logotipo BK Financeiro</t>
+  </si>
+  <si>
+    <t>Corrigir vencimento de Liquido de Folha na integração</t>
+  </si>
+  <si>
+    <t>Suporte abertura de período fiscal</t>
+  </si>
+  <si>
+    <t>Acerto baixa de RA efetuada no ano de 2021 e o correto é 2022</t>
+  </si>
+  <si>
+    <t>Verificar titulos com saldo a receber conforme relatório do Leandro BKFINR26</t>
+  </si>
+  <si>
+    <t>DIRF 2021 - Geração dos arquivos e conferencia</t>
   </si>
 </sst>
 </file>
@@ -8625,11 +8646,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1817"/>
+  <dimension ref="A1:J1825"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1764" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1774" sqref="A1774"/>
+      <pane ySplit="1" topLeftCell="A1772" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1782" sqref="A1782"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -61651,133 +61672,239 @@
       <c r="J1773" s="13"/>
     </row>
     <row r="1774" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1774" s="12"/>
-      <c r="B1774" s="12"/>
-      <c r="C1774" s="14"/>
-      <c r="D1774" s="10"/>
-      <c r="E1774" s="11"/>
-      <c r="F1774" s="10"/>
-      <c r="G1774" s="11"/>
-      <c r="H1774" s="12"/>
-      <c r="I1774" s="13"/>
+      <c r="A1774" s="12">
+        <v>44582</v>
+      </c>
+      <c r="B1774" s="12">
+        <v>44582</v>
+      </c>
+      <c r="C1774" s="14" t="s">
+        <v>1986</v>
+      </c>
+      <c r="D1774" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1774" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1774" s="10" t="s">
+        <v>1463</v>
+      </c>
+      <c r="G1774" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1774" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1774" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1774" s="13"/>
     </row>
     <row r="1775" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1775" s="12"/>
-      <c r="B1775" s="12"/>
-      <c r="C1775" s="14"/>
-      <c r="D1775" s="10"/>
-      <c r="E1775" s="11"/>
-      <c r="F1775" s="10"/>
-      <c r="G1775" s="11"/>
-      <c r="H1775" s="12"/>
-      <c r="I1775" s="13"/>
+      <c r="A1775" s="12">
+        <v>44582</v>
+      </c>
+      <c r="B1775" s="12">
+        <v>44582</v>
+      </c>
+      <c r="C1775" s="14" t="s">
+        <v>490</v>
+      </c>
+      <c r="D1775" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="E1775" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1775" s="10" t="s">
+        <v>2482</v>
+      </c>
+      <c r="G1775" s="11" t="s">
+        <v>1616</v>
+      </c>
+      <c r="H1775" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1775" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1775" s="13"/>
     </row>
     <row r="1776" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1776" s="12"/>
-      <c r="B1776" s="12"/>
-      <c r="C1776" s="14"/>
-      <c r="D1776" s="10"/>
-      <c r="E1776" s="11"/>
-      <c r="F1776" s="10"/>
-      <c r="G1776" s="11"/>
-      <c r="H1776" s="12"/>
-      <c r="I1776" s="13"/>
+      <c r="A1776" s="12">
+        <v>44585</v>
+      </c>
+      <c r="B1776" s="12">
+        <v>44585</v>
+      </c>
+      <c r="C1776" s="14" t="s">
+        <v>559</v>
+      </c>
+      <c r="D1776" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1776" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1776" s="10" t="s">
+        <v>2480</v>
+      </c>
+      <c r="G1776" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1776" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1776" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1776" s="13"/>
     </row>
     <row r="1777" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1777" s="12"/>
-      <c r="B1777" s="12"/>
-      <c r="C1777" s="14"/>
-      <c r="D1777" s="10"/>
-      <c r="E1777" s="11"/>
-      <c r="F1777" s="10"/>
-      <c r="G1777" s="11"/>
-      <c r="H1777" s="12"/>
-      <c r="I1777" s="13"/>
+      <c r="A1777" s="12">
+        <v>44585</v>
+      </c>
+      <c r="B1777" s="12">
+        <v>44585</v>
+      </c>
+      <c r="C1777" s="14" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D1777" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1777" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1777" s="10" t="s">
+        <v>2481</v>
+      </c>
+      <c r="G1777" s="11" t="s">
+        <v>1641</v>
+      </c>
+      <c r="H1777" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1777" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1777" s="13"/>
     </row>
-    <row r="1778" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1778" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1778" s="12">
-        <v>44522</v>
-      </c>
-      <c r="B1778" s="12"/>
+        <v>44585</v>
+      </c>
+      <c r="B1778" s="12">
+        <v>44585</v>
+      </c>
       <c r="C1778" s="14" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="D1778" s="10" t="s">
-        <v>6</v>
+        <v>494</v>
       </c>
       <c r="E1778" s="11" t="s">
-        <v>570</v>
+        <v>620</v>
       </c>
       <c r="F1778" s="10" t="s">
-        <v>2369</v>
-      </c>
-      <c r="G1778" s="11"/>
-      <c r="H1778" s="12"/>
-      <c r="I1778" s="13"/>
+        <v>2483</v>
+      </c>
+      <c r="G1778" s="11" t="s">
+        <v>1616</v>
+      </c>
+      <c r="H1778" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1778" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1778" s="13"/>
     </row>
     <row r="1779" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1779" s="12">
-        <v>43816</v>
-      </c>
-      <c r="B1779" s="9"/>
+        <v>44585</v>
+      </c>
+      <c r="B1779" s="12">
+        <v>44585</v>
+      </c>
       <c r="C1779" s="14" t="s">
-        <v>475</v>
+        <v>999</v>
       </c>
       <c r="D1779" s="10" t="s">
-        <v>38</v>
+        <v>1000</v>
       </c>
       <c r="E1779" s="11" t="s">
-        <v>570</v>
+        <v>620</v>
       </c>
       <c r="F1779" s="10" t="s">
-        <v>474</v>
+        <v>2484</v>
       </c>
       <c r="G1779" s="11" t="s">
-        <v>1627</v>
-      </c>
-      <c r="H1779" s="12"/>
-      <c r="I1779" s="13"/>
-      <c r="J1779" s="13" t="s">
-        <v>1565</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="H1779" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1779" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1779" s="13"/>
     </row>
     <row r="1780" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1780" s="12">
-        <v>44460</v>
-      </c>
-      <c r="B1780" s="12"/>
+        <v>44586</v>
+      </c>
+      <c r="B1780" s="12">
+        <v>44586</v>
+      </c>
       <c r="C1780" s="14" t="s">
-        <v>19</v>
+        <v>559</v>
       </c>
       <c r="D1780" s="10" t="s">
-        <v>494</v>
+        <v>6</v>
       </c>
       <c r="E1780" s="11" t="s">
         <v>837</v>
       </c>
       <c r="F1780" s="10" t="s">
-        <v>2193</v>
-      </c>
-      <c r="G1780" s="11"/>
+        <v>2485</v>
+      </c>
+      <c r="G1780" s="11" t="s">
+        <v>308</v>
+      </c>
       <c r="H1780" s="12"/>
       <c r="I1780" s="13"/>
       <c r="J1780" s="13"/>
     </row>
     <row r="1781" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1781" s="12"/>
-      <c r="B1781" s="12"/>
-      <c r="C1781" s="14"/>
-      <c r="D1781" s="10"/>
-      <c r="E1781" s="11"/>
-      <c r="F1781" s="10"/>
-      <c r="G1781" s="11"/>
-      <c r="H1781" s="12"/>
-      <c r="I1781" s="13"/>
+      <c r="A1781" s="12">
+        <v>44586</v>
+      </c>
+      <c r="B1781" s="12">
+        <v>44586</v>
+      </c>
+      <c r="C1781" s="14" t="s">
+        <v>1986</v>
+      </c>
+      <c r="D1781" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1781" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1781" s="10" t="s">
+        <v>2486</v>
+      </c>
+      <c r="G1781" s="11" t="s">
+        <v>1620</v>
+      </c>
+      <c r="H1781" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1781" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1781" s="13"/>
     </row>
     <row r="1782" spans="1:10" x14ac:dyDescent="0.2">
@@ -61794,7 +61921,7 @@
     </row>
     <row r="1783" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1783" s="12"/>
-      <c r="B1783" s="9"/>
+      <c r="B1783" s="12"/>
       <c r="C1783" s="14"/>
       <c r="D1783" s="10"/>
       <c r="E1783" s="11"/>
@@ -61805,38 +61932,20 @@
       <c r="J1783" s="13"/>
     </row>
     <row r="1784" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1784" s="1" t="s">
-        <v>1475</v>
-      </c>
-      <c r="B1784" s="2" t="s">
-        <v>1476</v>
-      </c>
-      <c r="C1784" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1784" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1784" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1784" s="4" t="s">
-        <v>1575</v>
-      </c>
-      <c r="G1784" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1784" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1784" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1784" s="36"/>
+      <c r="A1784" s="12"/>
+      <c r="B1784" s="12"/>
+      <c r="C1784" s="14"/>
+      <c r="D1784" s="10"/>
+      <c r="E1784" s="11"/>
+      <c r="F1784" s="10"/>
+      <c r="G1784" s="11"/>
+      <c r="H1784" s="12"/>
+      <c r="I1784" s="13"/>
+      <c r="J1784" s="13"/>
     </row>
     <row r="1785" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1785" s="12"/>
-      <c r="B1785" s="9"/>
+      <c r="B1785" s="12"/>
       <c r="C1785" s="14"/>
       <c r="D1785" s="10"/>
       <c r="E1785" s="11"/>
@@ -61846,22 +61955,22 @@
       <c r="I1785" s="13"/>
       <c r="J1785" s="13"/>
     </row>
-    <row r="1786" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1786" s="12"/>
-      <c r="B1786" s="12">
-        <v>44402</v>
-      </c>
+    <row r="1786" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1786" s="12">
+        <v>44522</v>
+      </c>
+      <c r="B1786" s="12"/>
       <c r="C1786" s="14" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="D1786" s="10" t="s">
-        <v>584</v>
+        <v>6</v>
       </c>
       <c r="E1786" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1786" s="10" t="s">
-        <v>1609</v>
+        <v>2369</v>
       </c>
       <c r="G1786" s="11"/>
       <c r="H1786" s="12"/>
@@ -61869,43 +61978,47 @@
       <c r="J1786" s="13"/>
     </row>
     <row r="1787" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1787" s="12"/>
-      <c r="B1787" s="12">
-        <v>44402</v>
-      </c>
+      <c r="A1787" s="12">
+        <v>43816</v>
+      </c>
+      <c r="B1787" s="9"/>
       <c r="C1787" s="14" t="s">
-        <v>13</v>
+        <v>475</v>
       </c>
       <c r="D1787" s="10" t="s">
-        <v>584</v>
+        <v>38</v>
       </c>
       <c r="E1787" s="11" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
       <c r="F1787" s="10" t="s">
-        <v>1601</v>
-      </c>
-      <c r="G1787" s="11"/>
+        <v>474</v>
+      </c>
+      <c r="G1787" s="11" t="s">
+        <v>1627</v>
+      </c>
       <c r="H1787" s="12"/>
       <c r="I1787" s="13"/>
-      <c r="J1787" s="13"/>
+      <c r="J1787" s="13" t="s">
+        <v>1565</v>
+      </c>
     </row>
     <row r="1788" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1788" s="12"/>
-      <c r="B1788" s="12">
-        <v>44402</v>
-      </c>
+      <c r="A1788" s="12">
+        <v>44460</v>
+      </c>
+      <c r="B1788" s="12"/>
       <c r="C1788" s="14" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D1788" s="10" t="s">
-        <v>584</v>
+        <v>494</v>
       </c>
       <c r="E1788" s="11" t="s">
-        <v>647</v>
+        <v>837</v>
       </c>
       <c r="F1788" s="10" t="s">
-        <v>1606</v>
+        <v>2193</v>
       </c>
       <c r="G1788" s="11"/>
       <c r="H1788" s="12"/>
@@ -61914,21 +62027,11 @@
     </row>
     <row r="1789" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1789" s="12"/>
-      <c r="B1789" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1789" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1789" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1789" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1789" s="10" t="s">
-        <v>1602</v>
-      </c>
+      <c r="B1789" s="12"/>
+      <c r="C1789" s="14"/>
+      <c r="D1789" s="10"/>
+      <c r="E1789" s="11"/>
+      <c r="F1789" s="10"/>
       <c r="G1789" s="11"/>
       <c r="H1789" s="12"/>
       <c r="I1789" s="13"/>
@@ -61936,19 +62039,11 @@
     </row>
     <row r="1790" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1790" s="12"/>
-      <c r="B1790" s="9"/>
-      <c r="C1790" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1790" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1790" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1790" s="10" t="s">
-        <v>1610</v>
-      </c>
+      <c r="B1790" s="12"/>
+      <c r="C1790" s="14"/>
+      <c r="D1790" s="10"/>
+      <c r="E1790" s="11"/>
+      <c r="F1790" s="10"/>
       <c r="G1790" s="11"/>
       <c r="H1790" s="12"/>
       <c r="I1790" s="13"/>
@@ -61956,63 +62051,53 @@
     </row>
     <row r="1791" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1791" s="12"/>
-      <c r="B1791" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1791" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1791" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1791" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1791" s="10" t="s">
-        <v>1603</v>
-      </c>
+      <c r="B1791" s="9"/>
+      <c r="C1791" s="14"/>
+      <c r="D1791" s="10"/>
+      <c r="E1791" s="11"/>
+      <c r="F1791" s="10"/>
       <c r="G1791" s="11"/>
       <c r="H1791" s="12"/>
       <c r="I1791" s="13"/>
       <c r="J1791" s="13"/>
     </row>
     <row r="1792" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1792" s="12"/>
-      <c r="B1792" s="9"/>
-      <c r="C1792" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1792" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1792" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1792" s="10" t="s">
-        <v>1600</v>
-      </c>
-      <c r="G1792" s="11"/>
-      <c r="H1792" s="12"/>
-      <c r="I1792" s="13"/>
-      <c r="J1792" s="13"/>
+      <c r="A1792" s="1" t="s">
+        <v>1475</v>
+      </c>
+      <c r="B1792" s="2" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C1792" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1792" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1792" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1792" s="4" t="s">
+        <v>1575</v>
+      </c>
+      <c r="G1792" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1792" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1792" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1792" s="36"/>
     </row>
     <row r="1793" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1793" s="12"/>
-      <c r="B1793" s="12">
-        <v>44402</v>
-      </c>
-      <c r="C1793" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1793" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1793" s="11" t="s">
-        <v>647</v>
-      </c>
-      <c r="F1793" s="10" t="s">
-        <v>1599</v>
-      </c>
+      <c r="B1793" s="9"/>
+      <c r="C1793" s="14"/>
+      <c r="D1793" s="10"/>
+      <c r="E1793" s="11"/>
+      <c r="F1793" s="10"/>
       <c r="G1793" s="11"/>
       <c r="H1793" s="12"/>
       <c r="I1793" s="13"/>
@@ -62033,7 +62118,7 @@
         <v>647</v>
       </c>
       <c r="F1794" s="10" t="s">
-        <v>1604</v>
+        <v>1609</v>
       </c>
       <c r="G1794" s="11"/>
       <c r="H1794" s="12"/>
@@ -62055,7 +62140,7 @@
         <v>647</v>
       </c>
       <c r="F1795" s="10" t="s">
-        <v>1607</v>
+        <v>1601</v>
       </c>
       <c r="G1795" s="11"/>
       <c r="H1795" s="12"/>
@@ -62064,8 +62149,8 @@
     </row>
     <row r="1796" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1796" s="12"/>
-      <c r="B1796" s="9">
-        <v>44235</v>
+      <c r="B1796" s="12">
+        <v>44402</v>
       </c>
       <c r="C1796" s="14" t="s">
         <v>13</v>
@@ -62077,7 +62162,7 @@
         <v>647</v>
       </c>
       <c r="F1796" s="10" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
       <c r="G1796" s="11"/>
       <c r="H1796" s="12"/>
@@ -62086,7 +62171,9 @@
     </row>
     <row r="1797" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1797" s="12"/>
-      <c r="B1797" s="9"/>
+      <c r="B1797" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1797" s="14" t="s">
         <v>13</v>
       </c>
@@ -62097,7 +62184,7 @@
         <v>647</v>
       </c>
       <c r="F1797" s="10" t="s">
-        <v>1605</v>
+        <v>1602</v>
       </c>
       <c r="G1797" s="11"/>
       <c r="H1797" s="12"/>
@@ -62107,77 +62194,81 @@
     <row r="1798" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1798" s="12"/>
       <c r="B1798" s="9"/>
-      <c r="C1798" s="14"/>
-      <c r="D1798" s="10"/>
-      <c r="E1798" s="11"/>
-      <c r="F1798" s="10"/>
+      <c r="C1798" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1798" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1798" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1798" s="10" t="s">
+        <v>1610</v>
+      </c>
       <c r="G1798" s="11"/>
       <c r="H1798" s="12"/>
       <c r="I1798" s="13"/>
       <c r="J1798" s="13"/>
     </row>
-    <row r="1799" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1799" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1799" s="9"/>
+    <row r="1799" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1799" s="12"/>
+      <c r="B1799" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1799" s="14" t="s">
-        <v>897</v>
+        <v>13</v>
       </c>
       <c r="D1799" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1799" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1799" s="10" t="s">
-        <v>1654</v>
+        <v>1603</v>
       </c>
       <c r="G1799" s="11"/>
       <c r="H1799" s="12"/>
       <c r="I1799" s="13"/>
-      <c r="J1799" s="13" t="s">
-        <v>1677</v>
-      </c>
-    </row>
-    <row r="1800" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1800" s="12">
-        <v>44252</v>
-      </c>
+      <c r="J1799" s="13"/>
+    </row>
+    <row r="1800" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1800" s="12"/>
       <c r="B1800" s="9"/>
       <c r="C1800" s="14" t="s">
-        <v>897</v>
+        <v>13</v>
       </c>
       <c r="D1800" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1800" s="11" t="s">
-        <v>759</v>
+        <v>647</v>
       </c>
       <c r="F1800" s="10" t="s">
-        <v>1653</v>
+        <v>1600</v>
       </c>
       <c r="G1800" s="11"/>
       <c r="H1800" s="12"/>
       <c r="I1800" s="13"/>
       <c r="J1800" s="13"/>
     </row>
-    <row r="1801" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1801" s="12">
-        <v>44112</v>
-      </c>
-      <c r="B1801" s="9"/>
+    <row r="1801" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1801" s="12"/>
+      <c r="B1801" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1801" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1801" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1801" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1801" s="10" t="s">
-        <v>2241</v>
+        <v>1599</v>
       </c>
       <c r="G1801" s="11"/>
       <c r="H1801" s="12"/>
@@ -62185,21 +62276,21 @@
       <c r="J1801" s="13"/>
     </row>
     <row r="1802" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1802" s="12">
-        <v>44088</v>
-      </c>
-      <c r="B1802" s="9"/>
+      <c r="A1802" s="12"/>
+      <c r="B1802" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1802" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1802" s="10" t="s">
-        <v>905</v>
+        <v>584</v>
       </c>
       <c r="E1802" s="11" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
       <c r="F1802" s="10" t="s">
-        <v>1010</v>
+        <v>1604</v>
       </c>
       <c r="G1802" s="11"/>
       <c r="H1802" s="12"/>
@@ -62207,21 +62298,21 @@
       <c r="J1802" s="13"/>
     </row>
     <row r="1803" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1803" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1803" s="9"/>
+      <c r="A1803" s="12"/>
+      <c r="B1803" s="12">
+        <v>44402</v>
+      </c>
       <c r="C1803" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1803" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1803" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1803" s="10" t="s">
-        <v>902</v>
+        <v>1607</v>
       </c>
       <c r="G1803" s="11"/>
       <c r="H1803" s="12"/>
@@ -62229,21 +62320,21 @@
       <c r="J1803" s="13"/>
     </row>
     <row r="1804" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1804" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1804" s="9"/>
+      <c r="A1804" s="12"/>
+      <c r="B1804" s="9">
+        <v>44235</v>
+      </c>
       <c r="C1804" s="14" t="s">
-        <v>623</v>
+        <v>13</v>
       </c>
       <c r="D1804" s="10" t="s">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="E1804" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1804" s="10" t="s">
-        <v>901</v>
+        <v>1608</v>
       </c>
       <c r="G1804" s="11"/>
       <c r="H1804" s="12"/>
@@ -62251,52 +62342,40 @@
       <c r="J1804" s="13"/>
     </row>
     <row r="1805" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1805" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A1805" s="12"/>
       <c r="B1805" s="9"/>
       <c r="C1805" s="14" t="s">
-        <v>897</v>
+        <v>13</v>
       </c>
       <c r="D1805" s="10" t="s">
-        <v>494</v>
+        <v>584</v>
       </c>
       <c r="E1805" s="11" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="F1805" s="10" t="s">
-        <v>899</v>
+        <v>1605</v>
       </c>
       <c r="G1805" s="11"/>
       <c r="H1805" s="12"/>
       <c r="I1805" s="13"/>
       <c r="J1805" s="13"/>
     </row>
-    <row r="1806" spans="1:10" ht="108" x14ac:dyDescent="0.2">
-      <c r="A1806" s="12">
-        <v>44055</v>
-      </c>
+    <row r="1806" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1806" s="12"/>
       <c r="B1806" s="9"/>
-      <c r="C1806" s="14" t="s">
-        <v>897</v>
-      </c>
-      <c r="D1806" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="E1806" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="F1806" s="10" t="s">
-        <v>900</v>
-      </c>
+      <c r="C1806" s="14"/>
+      <c r="D1806" s="10"/>
+      <c r="E1806" s="11"/>
+      <c r="F1806" s="10"/>
       <c r="G1806" s="11"/>
       <c r="H1806" s="12"/>
       <c r="I1806" s="13"/>
       <c r="J1806" s="13"/>
     </row>
-    <row r="1807" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1807" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1807" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1807" s="9"/>
       <c r="C1807" s="14" t="s">
@@ -62306,198 +62385,376 @@
         <v>494</v>
       </c>
       <c r="E1807" s="11" t="s">
-        <v>570</v>
+        <v>759</v>
       </c>
       <c r="F1807" s="10" t="s">
-        <v>903</v>
+        <v>1654</v>
       </c>
       <c r="G1807" s="11"/>
       <c r="H1807" s="12"/>
       <c r="I1807" s="13"/>
       <c r="J1807" s="13" t="s">
-        <v>1583</v>
-      </c>
-    </row>
-    <row r="1808" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="1808" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1808" s="12">
-        <v>43949</v>
+        <v>44252</v>
       </c>
       <c r="B1808" s="9"/>
       <c r="C1808" s="14" t="s">
-        <v>468</v>
+        <v>897</v>
       </c>
       <c r="D1808" s="10" t="s">
-        <v>89</v>
+        <v>494</v>
       </c>
       <c r="E1808" s="11" t="s">
-        <v>685</v>
+        <v>759</v>
       </c>
       <c r="F1808" s="10" t="s">
-        <v>686</v>
-      </c>
-      <c r="G1808" s="11" t="s">
-        <v>1634</v>
-      </c>
+        <v>1653</v>
+      </c>
+      <c r="G1808" s="11"/>
       <c r="H1808" s="12"/>
-      <c r="I1808" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1808" s="13"/>
       <c r="J1808" s="13"/>
     </row>
-    <row r="1809" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1809" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1809" s="12">
-        <v>43949</v>
+        <v>44112</v>
       </c>
       <c r="B1809" s="9"/>
       <c r="C1809" s="14" t="s">
-        <v>468</v>
+        <v>623</v>
       </c>
       <c r="D1809" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1809" s="11" t="s">
-        <v>685</v>
+        <v>570</v>
       </c>
       <c r="F1809" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="G1809" s="11" t="s">
-        <v>687</v>
-      </c>
+        <v>2241</v>
+      </c>
+      <c r="G1809" s="11"/>
       <c r="H1809" s="12"/>
-      <c r="I1809" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1809" s="13" t="s">
-        <v>1564</v>
-      </c>
-    </row>
-    <row r="1810" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1809" s="13"/>
+      <c r="J1809" s="13"/>
+    </row>
+    <row r="1810" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1810" s="12">
-        <v>43838</v>
+        <v>44088</v>
       </c>
       <c r="B1810" s="9"/>
       <c r="C1810" s="14" t="s">
-        <v>103</v>
+        <v>19</v>
       </c>
       <c r="D1810" s="10" t="s">
-        <v>460</v>
+        <v>905</v>
       </c>
       <c r="E1810" s="11" t="s">
-        <v>647</v>
+        <v>685</v>
       </c>
       <c r="F1810" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="G1810" s="11" t="s">
-        <v>1635</v>
-      </c>
+        <v>1010</v>
+      </c>
+      <c r="G1810" s="11"/>
       <c r="H1810" s="12"/>
       <c r="I1810" s="13"/>
-      <c r="J1810" s="13" t="s">
-        <v>1529</v>
-      </c>
-    </row>
-    <row r="1811" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1810" s="13"/>
+    </row>
+    <row r="1811" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1811" s="12">
-        <v>43762</v>
+        <v>44055</v>
       </c>
       <c r="B1811" s="9"/>
       <c r="C1811" s="14" t="s">
-        <v>446</v>
+        <v>623</v>
       </c>
       <c r="D1811" s="10" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E1811" s="11" t="s">
-        <v>837</v>
+        <v>570</v>
       </c>
       <c r="F1811" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G1811" s="11" t="s">
-        <v>1624</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="G1811" s="11"/>
       <c r="H1811" s="12"/>
       <c r="I1811" s="13"/>
       <c r="J1811" s="13"/>
     </row>
     <row r="1812" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1812" s="12"/>
+      <c r="A1812" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1812" s="9"/>
-      <c r="C1812" s="14"/>
-      <c r="D1812" s="10"/>
-      <c r="E1812" s="11"/>
-      <c r="F1812" s="10"/>
+      <c r="C1812" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1812" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1812" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1812" s="10" t="s">
+        <v>901</v>
+      </c>
       <c r="G1812" s="11"/>
       <c r="H1812" s="12"/>
       <c r="I1812" s="13"/>
       <c r="J1812" s="13"/>
     </row>
     <row r="1813" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1813" s="12"/>
+      <c r="A1813" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1813" s="9"/>
-      <c r="C1813" s="14"/>
-      <c r="D1813" s="10"/>
-      <c r="E1813" s="11"/>
-      <c r="F1813" s="10"/>
+      <c r="C1813" s="14" t="s">
+        <v>897</v>
+      </c>
+      <c r="D1813" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1813" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1813" s="10" t="s">
+        <v>899</v>
+      </c>
       <c r="G1813" s="11"/>
       <c r="H1813" s="12"/>
       <c r="I1813" s="13"/>
       <c r="J1813" s="13"/>
     </row>
-    <row r="1814" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1814" s="12"/>
+    <row r="1814" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A1814" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1814" s="9"/>
-      <c r="C1814" s="14"/>
-      <c r="D1814" s="10"/>
-      <c r="E1814" s="11"/>
-      <c r="F1814" s="10"/>
+      <c r="C1814" s="14" t="s">
+        <v>897</v>
+      </c>
+      <c r="D1814" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1814" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1814" s="10" t="s">
+        <v>900</v>
+      </c>
       <c r="G1814" s="11"/>
       <c r="H1814" s="12"/>
       <c r="I1814" s="13"/>
       <c r="J1814" s="13"/>
     </row>
-    <row r="1815" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1815" s="12"/>
+    <row r="1815" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1815" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1815" s="9"/>
-      <c r="C1815" s="14"/>
-      <c r="D1815" s="10"/>
-      <c r="E1815" s="11"/>
-      <c r="F1815" s="10"/>
+      <c r="C1815" s="14" t="s">
+        <v>897</v>
+      </c>
+      <c r="D1815" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1815" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1815" s="10" t="s">
+        <v>903</v>
+      </c>
       <c r="G1815" s="11"/>
       <c r="H1815" s="12"/>
       <c r="I1815" s="13"/>
-      <c r="J1815" s="13"/>
-    </row>
-    <row r="1816" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1816" s="12"/>
+      <c r="J1815" s="13" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="1816" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1816" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1816" s="9"/>
-      <c r="C1816" s="14"/>
-      <c r="D1816" s="10"/>
-      <c r="E1816" s="11"/>
-      <c r="F1816" s="10"/>
-      <c r="G1816" s="11"/>
+      <c r="C1816" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1816" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1816" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1816" s="10" t="s">
+        <v>686</v>
+      </c>
+      <c r="G1816" s="11" t="s">
+        <v>1634</v>
+      </c>
       <c r="H1816" s="12"/>
-      <c r="I1816" s="13"/>
+      <c r="I1816" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1816" s="13"/>
     </row>
-    <row r="1817" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1817" s="12"/>
+    <row r="1817" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1817" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1817" s="9"/>
-      <c r="C1817" s="14"/>
-      <c r="D1817" s="10"/>
-      <c r="E1817" s="11"/>
-      <c r="F1817" s="10"/>
-      <c r="G1817" s="11"/>
+      <c r="C1817" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1817" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1817" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="F1817" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="G1817" s="11" t="s">
+        <v>687</v>
+      </c>
       <c r="H1817" s="12"/>
-      <c r="I1817" s="13"/>
-      <c r="J1817" s="13"/>
+      <c r="I1817" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1817" s="13" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="1818" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1818" s="12">
+        <v>43838</v>
+      </c>
+      <c r="B1818" s="9"/>
+      <c r="C1818" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1818" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1818" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1818" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="G1818" s="11" t="s">
+        <v>1635</v>
+      </c>
+      <c r="H1818" s="12"/>
+      <c r="I1818" s="13"/>
+      <c r="J1818" s="13" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="1819" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1819" s="12">
+        <v>43762</v>
+      </c>
+      <c r="B1819" s="9"/>
+      <c r="C1819" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1819" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1819" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="F1819" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1819" s="11" t="s">
+        <v>1624</v>
+      </c>
+      <c r="H1819" s="12"/>
+      <c r="I1819" s="13"/>
+      <c r="J1819" s="13"/>
+    </row>
+    <row r="1820" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1820" s="12"/>
+      <c r="B1820" s="9"/>
+      <c r="C1820" s="14"/>
+      <c r="D1820" s="10"/>
+      <c r="E1820" s="11"/>
+      <c r="F1820" s="10"/>
+      <c r="G1820" s="11"/>
+      <c r="H1820" s="12"/>
+      <c r="I1820" s="13"/>
+      <c r="J1820" s="13"/>
+    </row>
+    <row r="1821" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1821" s="12"/>
+      <c r="B1821" s="9"/>
+      <c r="C1821" s="14"/>
+      <c r="D1821" s="10"/>
+      <c r="E1821" s="11"/>
+      <c r="F1821" s="10"/>
+      <c r="G1821" s="11"/>
+      <c r="H1821" s="12"/>
+      <c r="I1821" s="13"/>
+      <c r="J1821" s="13"/>
+    </row>
+    <row r="1822" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1822" s="12"/>
+      <c r="B1822" s="9"/>
+      <c r="C1822" s="14"/>
+      <c r="D1822" s="10"/>
+      <c r="E1822" s="11"/>
+      <c r="F1822" s="10"/>
+      <c r="G1822" s="11"/>
+      <c r="H1822" s="12"/>
+      <c r="I1822" s="13"/>
+      <c r="J1822" s="13"/>
+    </row>
+    <row r="1823" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1823" s="12"/>
+      <c r="B1823" s="9"/>
+      <c r="C1823" s="14"/>
+      <c r="D1823" s="10"/>
+      <c r="E1823" s="11"/>
+      <c r="F1823" s="10"/>
+      <c r="G1823" s="11"/>
+      <c r="H1823" s="12"/>
+      <c r="I1823" s="13"/>
+      <c r="J1823" s="13"/>
+    </row>
+    <row r="1824" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1824" s="12"/>
+      <c r="B1824" s="9"/>
+      <c r="C1824" s="14"/>
+      <c r="D1824" s="10"/>
+      <c r="E1824" s="11"/>
+      <c r="F1824" s="10"/>
+      <c r="G1824" s="11"/>
+      <c r="H1824" s="12"/>
+      <c r="I1824" s="13"/>
+      <c r="J1824" s="13"/>
+    </row>
+    <row r="1825" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1825" s="12"/>
+      <c r="B1825" s="9"/>
+      <c r="C1825" s="14"/>
+      <c r="D1825" s="10"/>
+      <c r="E1825" s="11"/>
+      <c r="F1825" s="10"/>
+      <c r="G1825" s="11"/>
+      <c r="H1825" s="12"/>
+      <c r="I1825" s="13"/>
+      <c r="J1825" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1480" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1787:F1797">
-    <sortCondition ref="F1787:F1797"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1795:F1805">
+    <sortCondition ref="F1795:F1805"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Retorno Hist Multas / Lib Doc Web
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BE6FE4-E907-4279-AF93-567A22B75BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92055668-10BE-4792-84D9-4102BA4AB657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha1" sheetId="3" r:id="rId2"/>
-    <sheet name="Nova Medição" sheetId="2" r:id="rId3"/>
+    <sheet name="Nova Medição" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_FilterDatabase_0" localSheetId="0">'Demandas BK - Protheus'!$A$1:$I$53</definedName>
@@ -78,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13003" uniqueCount="2547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13031" uniqueCount="2550">
   <si>
     <t>Responsável</t>
   </si>
@@ -8066,6 +8065,15 @@
   </si>
   <si>
     <t>Poderia por gentileza lançar esses 02 títulos, não consigo pois ele saiu em 2019.</t>
+  </si>
+  <si>
+    <t>Voltou em 21/02/22</t>
+  </si>
+  <si>
+    <t>Retornar programa excluido de Historico de Multas e Bonificações</t>
+  </si>
+  <si>
+    <t>Acertos EFD BK Jan/22</t>
   </si>
 </sst>
 </file>
@@ -8837,11 +8845,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1871"/>
+  <dimension ref="A1:J1875"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1827" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1836" sqref="A1836"/>
+      <pane ySplit="1" topLeftCell="A1833" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1840" sqref="A1840"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -63708,7 +63716,7 @@
         <v>489</v>
       </c>
       <c r="E1834" s="11" t="s">
-        <v>568</v>
+        <v>683</v>
       </c>
       <c r="F1834" s="10" t="s">
         <v>2546</v>
@@ -63755,114 +63763,156 @@
       <c r="J1835" s="13"/>
     </row>
     <row r="1836" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1836" s="12"/>
-      <c r="B1836" s="12"/>
-      <c r="C1836" s="14"/>
-      <c r="D1836" s="10"/>
-      <c r="E1836" s="11"/>
-      <c r="F1836" s="10"/>
-      <c r="G1836" s="11"/>
-      <c r="H1836" s="12"/>
-      <c r="I1836" s="13"/>
+      <c r="A1836" s="12">
+        <v>44610</v>
+      </c>
+      <c r="B1836" s="12">
+        <v>44610</v>
+      </c>
+      <c r="C1836" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1836" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E1836" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F1836" s="10" t="s">
+        <v>2532</v>
+      </c>
+      <c r="G1836" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H1836" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1836" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1836" s="13"/>
     </row>
     <row r="1837" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1837" s="12"/>
-      <c r="B1837" s="12"/>
-      <c r="C1837" s="14"/>
-      <c r="D1837" s="10"/>
-      <c r="E1837" s="11"/>
-      <c r="F1837" s="10"/>
-      <c r="G1837" s="11"/>
-      <c r="H1837" s="12"/>
-      <c r="I1837" s="13"/>
+      <c r="A1837" s="12">
+        <v>44613</v>
+      </c>
+      <c r="B1837" s="12">
+        <v>44613</v>
+      </c>
+      <c r="C1837" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D1837" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E1837" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F1837" s="10" t="s">
+        <v>2548</v>
+      </c>
+      <c r="G1837" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1837" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1837" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1837" s="13"/>
     </row>
     <row r="1838" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1838" s="12"/>
-      <c r="B1838" s="12"/>
-      <c r="C1838" s="14"/>
-      <c r="D1838" s="10"/>
-      <c r="E1838" s="11"/>
-      <c r="F1838" s="10"/>
-      <c r="G1838" s="11"/>
-      <c r="H1838" s="12"/>
-      <c r="I1838" s="13"/>
+      <c r="A1838" s="12">
+        <v>44613</v>
+      </c>
+      <c r="B1838" s="12">
+        <v>44613</v>
+      </c>
+      <c r="C1838" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1838" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E1838" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F1838" s="10" t="s">
+        <v>2532</v>
+      </c>
+      <c r="G1838" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H1838" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1838" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1838" s="13"/>
     </row>
     <row r="1839" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1839" s="12"/>
-      <c r="B1839" s="12"/>
-      <c r="C1839" s="14"/>
-      <c r="D1839" s="10"/>
-      <c r="E1839" s="11"/>
-      <c r="F1839" s="10"/>
-      <c r="G1839" s="11"/>
-      <c r="H1839" s="12"/>
-      <c r="I1839" s="13"/>
+      <c r="A1839" s="12">
+        <v>44613</v>
+      </c>
+      <c r="B1839" s="12">
+        <v>44613</v>
+      </c>
+      <c r="C1839" s="14" t="s">
+        <v>1971</v>
+      </c>
+      <c r="D1839" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1839" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1839" s="10" t="s">
+        <v>2549</v>
+      </c>
+      <c r="G1839" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1839" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1839" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1839" s="13"/>
     </row>
     <row r="1840" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1840" s="12">
-        <v>44607</v>
-      </c>
+      <c r="A1840" s="12"/>
       <c r="B1840" s="12"/>
-      <c r="C1840" s="14" t="s">
-        <v>462</v>
-      </c>
-      <c r="D1840" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1840" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F1840" s="10" t="s">
-        <v>2530</v>
-      </c>
+      <c r="C1840" s="14"/>
+      <c r="D1840" s="10"/>
+      <c r="E1840" s="11"/>
+      <c r="F1840" s="10"/>
       <c r="G1840" s="11"/>
       <c r="H1840" s="12"/>
       <c r="I1840" s="13"/>
       <c r="J1840" s="13"/>
     </row>
     <row r="1841" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1841" s="12">
-        <v>44607</v>
-      </c>
+      <c r="A1841" s="12"/>
       <c r="B1841" s="12"/>
-      <c r="C1841" s="14" t="s">
-        <v>557</v>
-      </c>
-      <c r="D1841" s="10" t="s">
-        <v>2531</v>
-      </c>
-      <c r="E1841" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F1841" s="10" t="s">
-        <v>2537</v>
-      </c>
+      <c r="C1841" s="14"/>
+      <c r="D1841" s="10"/>
+      <c r="E1841" s="11"/>
+      <c r="F1841" s="10"/>
       <c r="G1841" s="11"/>
       <c r="H1841" s="12"/>
       <c r="I1841" s="13"/>
       <c r="J1841" s="13"/>
     </row>
     <row r="1842" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1842" s="12">
-        <v>44607</v>
-      </c>
+      <c r="A1842" s="12"/>
       <c r="B1842" s="12"/>
-      <c r="C1842" s="14" t="s">
-        <v>1194</v>
-      </c>
-      <c r="D1842" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1842" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F1842" s="10" t="s">
-        <v>2538</v>
-      </c>
+      <c r="C1842" s="14"/>
+      <c r="D1842" s="10"/>
+      <c r="E1842" s="11"/>
+      <c r="F1842" s="10"/>
       <c r="G1842" s="11"/>
       <c r="H1842" s="12"/>
       <c r="I1842" s="13"/>
@@ -63881,45 +63931,65 @@
       <c r="J1843" s="13"/>
     </row>
     <row r="1844" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1844" s="12"/>
+      <c r="A1844" s="12">
+        <v>44607</v>
+      </c>
       <c r="B1844" s="12"/>
-      <c r="C1844" s="14"/>
-      <c r="D1844" s="10"/>
-      <c r="E1844" s="11"/>
-      <c r="F1844" s="10"/>
+      <c r="C1844" s="14" t="s">
+        <v>462</v>
+      </c>
+      <c r="D1844" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1844" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F1844" s="10" t="s">
+        <v>2530</v>
+      </c>
       <c r="G1844" s="11"/>
       <c r="H1844" s="12"/>
       <c r="I1844" s="13"/>
       <c r="J1844" s="13"/>
     </row>
     <row r="1845" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1845" s="12"/>
+      <c r="A1845" s="12">
+        <v>44607</v>
+      </c>
       <c r="B1845" s="12"/>
-      <c r="C1845" s="14"/>
-      <c r="D1845" s="10"/>
-      <c r="E1845" s="11"/>
-      <c r="F1845" s="10"/>
+      <c r="C1845" s="14" t="s">
+        <v>557</v>
+      </c>
+      <c r="D1845" s="10" t="s">
+        <v>2531</v>
+      </c>
+      <c r="E1845" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F1845" s="10" t="s">
+        <v>2537</v>
+      </c>
       <c r="G1845" s="11"/>
       <c r="H1845" s="12"/>
       <c r="I1845" s="13"/>
       <c r="J1845" s="13"/>
     </row>
-    <row r="1846" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1846" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1846" s="12">
-        <v>44522</v>
+        <v>44607</v>
       </c>
       <c r="B1846" s="12"/>
       <c r="C1846" s="14" t="s">
-        <v>46</v>
+        <v>1194</v>
       </c>
       <c r="D1846" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E1846" s="11" t="s">
-        <v>568</v>
+        <v>835</v>
       </c>
       <c r="F1846" s="10" t="s">
-        <v>2353</v>
+        <v>2538</v>
       </c>
       <c r="G1846" s="11"/>
       <c r="H1846" s="12"/>
@@ -63952,7 +64022,7 @@
     </row>
     <row r="1849" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1849" s="12"/>
-      <c r="B1849" s="9"/>
+      <c r="B1849" s="12"/>
       <c r="C1849" s="14"/>
       <c r="D1849" s="10"/>
       <c r="E1849" s="11"/>
@@ -63962,39 +64032,31 @@
       <c r="I1849" s="13"/>
       <c r="J1849" s="13"/>
     </row>
-    <row r="1850" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1850" s="1" t="s">
-        <v>1473</v>
-      </c>
-      <c r="B1850" s="2" t="s">
-        <v>1474</v>
-      </c>
-      <c r="C1850" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1850" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1850" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="F1850" s="4" t="s">
-        <v>1572</v>
-      </c>
-      <c r="G1850" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1850" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1850" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1850" s="36"/>
+    <row r="1850" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1850" s="12">
+        <v>44522</v>
+      </c>
+      <c r="B1850" s="12"/>
+      <c r="C1850" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1850" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1850" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1850" s="10" t="s">
+        <v>2353</v>
+      </c>
+      <c r="G1850" s="11"/>
+      <c r="H1850" s="12"/>
+      <c r="I1850" s="13"/>
+      <c r="J1850" s="13"/>
     </row>
     <row r="1851" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1851" s="12"/>
-      <c r="B1851" s="9"/>
+      <c r="B1851" s="12"/>
       <c r="C1851" s="14"/>
       <c r="D1851" s="10"/>
       <c r="E1851" s="11"/>
@@ -64006,7 +64068,7 @@
     </row>
     <row r="1852" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1852" s="12"/>
-      <c r="B1852" s="9"/>
+      <c r="B1852" s="12"/>
       <c r="C1852" s="14"/>
       <c r="D1852" s="10"/>
       <c r="E1852" s="11"/>
@@ -64016,356 +64078,374 @@
       <c r="I1852" s="13"/>
       <c r="J1852" s="13"/>
     </row>
-    <row r="1853" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1853" s="12">
-        <v>44252</v>
-      </c>
+    <row r="1853" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1853" s="12"/>
       <c r="B1853" s="9"/>
-      <c r="C1853" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D1853" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E1853" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F1853" s="10" t="s">
-        <v>1639</v>
-      </c>
+      <c r="C1853" s="14"/>
+      <c r="D1853" s="10"/>
+      <c r="E1853" s="11"/>
+      <c r="F1853" s="10"/>
       <c r="G1853" s="11"/>
       <c r="H1853" s="12"/>
       <c r="I1853" s="13"/>
-      <c r="J1853" s="13" t="s">
-        <v>1662</v>
-      </c>
-    </row>
-    <row r="1854" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1854" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1854" s="9"/>
-      <c r="C1854" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D1854" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E1854" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F1854" s="10" t="s">
-        <v>1638</v>
-      </c>
-      <c r="G1854" s="11"/>
-      <c r="H1854" s="12"/>
-      <c r="I1854" s="13"/>
-      <c r="J1854" s="13"/>
-    </row>
-    <row r="1855" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1855" s="12">
-        <v>44112</v>
-      </c>
+      <c r="J1853" s="13"/>
+    </row>
+    <row r="1854" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1854" s="1" t="s">
+        <v>1473</v>
+      </c>
+      <c r="B1854" s="2" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C1854" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1854" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1854" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F1854" s="4" t="s">
+        <v>1572</v>
+      </c>
+      <c r="G1854" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1854" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1854" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1854" s="36"/>
+    </row>
+    <row r="1855" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1855" s="12"/>
       <c r="B1855" s="9"/>
-      <c r="C1855" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D1855" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1855" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1855" s="10" t="s">
-        <v>2225</v>
-      </c>
+      <c r="C1855" s="14"/>
+      <c r="D1855" s="10"/>
+      <c r="E1855" s="11"/>
+      <c r="F1855" s="10"/>
       <c r="G1855" s="11"/>
       <c r="H1855" s="12"/>
       <c r="I1855" s="13"/>
       <c r="J1855" s="13"/>
     </row>
     <row r="1856" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1856" s="12">
-        <v>44088</v>
-      </c>
+      <c r="A1856" s="12"/>
       <c r="B1856" s="9"/>
-      <c r="C1856" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1856" s="10" t="s">
-        <v>903</v>
-      </c>
-      <c r="E1856" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="F1856" s="10" t="s">
-        <v>1008</v>
-      </c>
+      <c r="C1856" s="14"/>
+      <c r="D1856" s="10"/>
+      <c r="E1856" s="11"/>
+      <c r="F1856" s="10"/>
       <c r="G1856" s="11"/>
       <c r="H1856" s="12"/>
       <c r="I1856" s="13"/>
       <c r="J1856" s="13"/>
     </row>
-    <row r="1857" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1857" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1857" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1857" s="9"/>
       <c r="C1857" s="14" t="s">
-        <v>621</v>
+        <v>895</v>
       </c>
       <c r="D1857" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E1857" s="11" t="s">
-        <v>568</v>
+        <v>757</v>
       </c>
       <c r="F1857" s="10" t="s">
-        <v>900</v>
+        <v>1639</v>
       </c>
       <c r="G1857" s="11"/>
       <c r="H1857" s="12"/>
       <c r="I1857" s="13"/>
-      <c r="J1857" s="13"/>
-    </row>
-    <row r="1858" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1857" s="13" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="1858" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1858" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B1858" s="9"/>
       <c r="C1858" s="14" t="s">
-        <v>621</v>
+        <v>895</v>
       </c>
       <c r="D1858" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E1858" s="11" t="s">
-        <v>568</v>
+        <v>757</v>
       </c>
       <c r="F1858" s="10" t="s">
-        <v>899</v>
+        <v>1638</v>
       </c>
       <c r="G1858" s="11"/>
       <c r="H1858" s="12"/>
       <c r="I1858" s="13"/>
       <c r="J1858" s="13"/>
     </row>
-    <row r="1859" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1859" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1859" s="12">
-        <v>44055</v>
+        <v>44112</v>
       </c>
       <c r="B1859" s="9"/>
       <c r="C1859" s="14" t="s">
-        <v>895</v>
+        <v>621</v>
       </c>
       <c r="D1859" s="10" t="s">
-        <v>492</v>
+        <v>6</v>
       </c>
       <c r="E1859" s="11" t="s">
         <v>568</v>
       </c>
       <c r="F1859" s="10" t="s">
-        <v>897</v>
+        <v>2225</v>
       </c>
       <c r="G1859" s="11"/>
       <c r="H1859" s="12"/>
       <c r="I1859" s="13"/>
       <c r="J1859" s="13"/>
     </row>
-    <row r="1860" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="1860" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1860" s="12">
-        <v>44055</v>
+        <v>44088</v>
       </c>
       <c r="B1860" s="9"/>
       <c r="C1860" s="14" t="s">
-        <v>895</v>
+        <v>19</v>
       </c>
       <c r="D1860" s="10" t="s">
-        <v>492</v>
+        <v>903</v>
       </c>
       <c r="E1860" s="11" t="s">
-        <v>568</v>
+        <v>683</v>
       </c>
       <c r="F1860" s="10" t="s">
-        <v>898</v>
+        <v>1008</v>
       </c>
       <c r="G1860" s="11"/>
       <c r="H1860" s="12"/>
       <c r="I1860" s="13"/>
       <c r="J1860" s="13"/>
     </row>
-    <row r="1861" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1861" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1861" s="12">
         <v>44055</v>
       </c>
       <c r="B1861" s="9"/>
       <c r="C1861" s="14" t="s">
-        <v>895</v>
+        <v>621</v>
       </c>
       <c r="D1861" s="10" t="s">
-        <v>492</v>
+        <v>6</v>
       </c>
       <c r="E1861" s="11" t="s">
         <v>568</v>
       </c>
       <c r="F1861" s="10" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="G1861" s="11"/>
       <c r="H1861" s="12"/>
       <c r="I1861" s="13"/>
-      <c r="J1861" s="13" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="1862" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="J1861" s="13"/>
+    </row>
+    <row r="1862" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1862" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1862" s="9"/>
       <c r="C1862" s="14" t="s">
-        <v>468</v>
+        <v>621</v>
       </c>
       <c r="D1862" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E1862" s="11" t="s">
-        <v>683</v>
+        <v>568</v>
       </c>
       <c r="F1862" s="10" t="s">
-        <v>684</v>
-      </c>
-      <c r="G1862" s="11" t="s">
-        <v>1619</v>
-      </c>
+        <v>899</v>
+      </c>
+      <c r="G1862" s="11"/>
       <c r="H1862" s="12"/>
-      <c r="I1862" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1862" s="13"/>
       <c r="J1862" s="13"/>
     </row>
-    <row r="1863" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1863" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1863" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1863" s="9"/>
       <c r="C1863" s="14" t="s">
-        <v>468</v>
+        <v>895</v>
       </c>
       <c r="D1863" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E1863" s="11" t="s">
-        <v>683</v>
+        <v>568</v>
       </c>
       <c r="F1863" s="10" t="s">
-        <v>703</v>
-      </c>
-      <c r="G1863" s="11" t="s">
-        <v>685</v>
-      </c>
+        <v>897</v>
+      </c>
+      <c r="G1863" s="11"/>
       <c r="H1863" s="12"/>
-      <c r="I1863" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1863" s="13" t="s">
-        <v>1562</v>
-      </c>
-    </row>
-    <row r="1864" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1863" s="13"/>
+      <c r="J1863" s="13"/>
+    </row>
+    <row r="1864" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A1864" s="12">
-        <v>43838</v>
+        <v>44055</v>
       </c>
       <c r="B1864" s="9"/>
       <c r="C1864" s="14" t="s">
-        <v>103</v>
+        <v>895</v>
       </c>
       <c r="D1864" s="10" t="s">
-        <v>460</v>
+        <v>492</v>
       </c>
       <c r="E1864" s="11" t="s">
-        <v>645</v>
+        <v>568</v>
       </c>
       <c r="F1864" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="G1864" s="11" t="s">
-        <v>1620</v>
-      </c>
+        <v>898</v>
+      </c>
+      <c r="G1864" s="11"/>
       <c r="H1864" s="12"/>
       <c r="I1864" s="13"/>
-      <c r="J1864" s="13" t="s">
-        <v>1527</v>
-      </c>
-    </row>
-    <row r="1865" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1864" s="13"/>
+    </row>
+    <row r="1865" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1865" s="12">
-        <v>43762</v>
+        <v>44055</v>
       </c>
       <c r="B1865" s="9"/>
       <c r="C1865" s="14" t="s">
-        <v>446</v>
+        <v>895</v>
       </c>
       <c r="D1865" s="10" t="s">
-        <v>17</v>
+        <v>492</v>
       </c>
       <c r="E1865" s="11" t="s">
-        <v>835</v>
+        <v>568</v>
       </c>
       <c r="F1865" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G1865" s="11" t="s">
-        <v>1609</v>
-      </c>
+        <v>901</v>
+      </c>
+      <c r="G1865" s="11"/>
       <c r="H1865" s="12"/>
       <c r="I1865" s="13"/>
-      <c r="J1865" s="13"/>
-    </row>
-    <row r="1866" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1866" s="12"/>
+      <c r="J1865" s="13" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="1866" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1866" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1866" s="9"/>
-      <c r="C1866" s="14"/>
-      <c r="D1866" s="10"/>
-      <c r="E1866" s="11"/>
-      <c r="F1866" s="10"/>
-      <c r="G1866" s="11"/>
+      <c r="C1866" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1866" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1866" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F1866" s="10" t="s">
+        <v>684</v>
+      </c>
+      <c r="G1866" s="11" t="s">
+        <v>1619</v>
+      </c>
       <c r="H1866" s="12"/>
-      <c r="I1866" s="13"/>
+      <c r="I1866" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J1866" s="13"/>
     </row>
-    <row r="1867" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1867" s="12"/>
+    <row r="1867" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1867" s="12">
+        <v>43949</v>
+      </c>
       <c r="B1867" s="9"/>
-      <c r="C1867" s="14"/>
-      <c r="D1867" s="10"/>
-      <c r="E1867" s="11"/>
-      <c r="F1867" s="10"/>
-      <c r="G1867" s="11"/>
+      <c r="C1867" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1867" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1867" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F1867" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="G1867" s="11" t="s">
+        <v>685</v>
+      </c>
       <c r="H1867" s="12"/>
-      <c r="I1867" s="13"/>
-      <c r="J1867" s="13"/>
-    </row>
-    <row r="1868" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1868" s="12"/>
+      <c r="I1867" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1867" s="13" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="1868" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1868" s="12">
+        <v>43838</v>
+      </c>
       <c r="B1868" s="9"/>
-      <c r="C1868" s="14"/>
-      <c r="D1868" s="10"/>
-      <c r="E1868" s="11"/>
-      <c r="F1868" s="10"/>
-      <c r="G1868" s="11"/>
+      <c r="C1868" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1868" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1868" s="11" t="s">
+        <v>645</v>
+      </c>
+      <c r="F1868" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="G1868" s="11" t="s">
+        <v>1620</v>
+      </c>
       <c r="H1868" s="12"/>
       <c r="I1868" s="13"/>
-      <c r="J1868" s="13"/>
-    </row>
-    <row r="1869" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1869" s="12"/>
+      <c r="J1868" s="13" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="1869" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1869" s="12">
+        <v>43762</v>
+      </c>
       <c r="B1869" s="9"/>
-      <c r="C1869" s="14"/>
-      <c r="D1869" s="10"/>
-      <c r="E1869" s="11"/>
-      <c r="F1869" s="10"/>
-      <c r="G1869" s="11"/>
+      <c r="C1869" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1869" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1869" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F1869" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1869" s="11" t="s">
+        <v>1609</v>
+      </c>
       <c r="H1869" s="12"/>
       <c r="I1869" s="13"/>
       <c r="J1869" s="13"/>
@@ -64393,6 +64473,54 @@
       <c r="H1871" s="12"/>
       <c r="I1871" s="13"/>
       <c r="J1871" s="13"/>
+    </row>
+    <row r="1872" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1872" s="12"/>
+      <c r="B1872" s="9"/>
+      <c r="C1872" s="14"/>
+      <c r="D1872" s="10"/>
+      <c r="E1872" s="11"/>
+      <c r="F1872" s="10"/>
+      <c r="G1872" s="11"/>
+      <c r="H1872" s="12"/>
+      <c r="I1872" s="13"/>
+      <c r="J1872" s="13"/>
+    </row>
+    <row r="1873" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1873" s="12"/>
+      <c r="B1873" s="9"/>
+      <c r="C1873" s="14"/>
+      <c r="D1873" s="10"/>
+      <c r="E1873" s="11"/>
+      <c r="F1873" s="10"/>
+      <c r="G1873" s="11"/>
+      <c r="H1873" s="12"/>
+      <c r="I1873" s="13"/>
+      <c r="J1873" s="13"/>
+    </row>
+    <row r="1874" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1874" s="12"/>
+      <c r="B1874" s="9"/>
+      <c r="C1874" s="14"/>
+      <c r="D1874" s="10"/>
+      <c r="E1874" s="11"/>
+      <c r="F1874" s="10"/>
+      <c r="G1874" s="11"/>
+      <c r="H1874" s="12"/>
+      <c r="I1874" s="13"/>
+      <c r="J1874" s="13"/>
+    </row>
+    <row r="1875" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1875" s="12"/>
+      <c r="B1875" s="9"/>
+      <c r="C1875" s="14"/>
+      <c r="D1875" s="10"/>
+      <c r="E1875" s="11"/>
+      <c r="F1875" s="10"/>
+      <c r="G1875" s="11"/>
+      <c r="H1875" s="12"/>
+      <c r="I1875" s="13"/>
+      <c r="J1875" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1480" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -64407,25 +64535,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3653A101-0AA1-4A4A-8B2D-1DFD6A3AA321}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:N13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE13D4C-C1F0-4B00-8A02-71F13D132F72}">
   <dimension ref="B1:G35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64433,7 +64547,7 @@
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="87.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="79.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -64757,7 +64871,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>1733</v>
+        <v>2547</v>
       </c>
       <c r="F19" s="39" t="s">
         <v>1754</v>

</xml_diff>

<commit_message>
Alterações até 17/03/22 12:00
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7497E3-B2DC-422D-83E1-E887847B29FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A9AF73-4084-4639-BD71-B0ED079EC8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
-    <sheet name="Nova Medição" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha1" sheetId="3" r:id="rId2"/>
+    <sheet name="Nova Medição" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_FilterDatabase_0" localSheetId="0">'Demandas BK - Protheus'!$A$1:$I$53</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Demandas BK - Protheus'!$A$1:$J$1480</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Demandas BK - Protheus'!$A$1:$J$1881</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13328" uniqueCount="2602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13421" uniqueCount="2617">
   <si>
     <t>Responsável</t>
   </si>
@@ -8212,9 +8213,6 @@
     <t>Era necessario reprocessar a EFD</t>
   </si>
   <si>
-    <t>Relatorio de baixas de pagamento com usuarios (criar opção analitica por cc e na sintetica colocar "Diversas" caso tenha mais de um cc GCTR028</t>
-  </si>
-  <si>
     <t>Relatório BKFATR04 com linha duplicada</t>
   </si>
   <si>
@@ -8235,6 +8233,56 @@
   <si>
     <t xml:space="preserve">Testes na baixa "Portal Petrobras"
 Alterar o padrão de saldo "1 Real" para "Zero" </t>
+  </si>
+  <si>
+    <t>Relatorio de baixas de pagamento com usuarios (criar opção analitica por cc e na sintetica colocar "Diversas" caso tenha mais de um cc GCTR028)</t>
+  </si>
+  <si>
+    <t>BKGCTR28</t>
+  </si>
+  <si>
+    <t>Atualização dos programas GIT e VS-CODE do VMSIGA12</t>
+  </si>
+  <si>
+    <t>Suporte emissao de relatório comparativo de saldos de contas em 12 meses</t>
+  </si>
+  <si>
+    <t>Suporte emissão de posição de fornecedores</t>
+  </si>
+  <si>
+    <t>Testar nova medição</t>
+  </si>
+  <si>
+    <t>Alterar os acessos do usuário fernando.sampaio</t>
+  </si>
+  <si>
+    <t>Grupos: 29-Master Contabilidade e 8-Master Repac (iguais ao seu usuário). Superior: Antes era Vanderleia agora é Bruno Bueno
+Departamento: Controladoria</t>
+  </si>
+  <si>
+    <t>SF1140I e BKCOMA08
+Na digitação da pré-nota, vou ver apenas o CNPJ e o mes de emissao e na classificação, o sistema vai consultar a validade da chave no site do SEFAZ</t>
+  </si>
+  <si>
+    <t>Alterar os fornecedores das NFs 000036482 (Claro) e 012875633 (Kabum) ambas digitadas incorretamente pelo Tiago da TI</t>
+  </si>
+  <si>
+    <t>Suporte diferença EFD BK</t>
+  </si>
+  <si>
+    <t>NF 000005296 Pedido 050610 emitida sem retenção de PCC</t>
+  </si>
+  <si>
+    <t>Verificação de log referente a cancelamento e reemissão de NF de saída</t>
+  </si>
+  <si>
+    <t>BKGCTR28 listando apv pgto incorreto</t>
+  </si>
+  <si>
+    <t>Criar camo tipo Memo para historico do contas a Receber</t>
+  </si>
+  <si>
+    <t>Auxilio assinatura digital no site da SEFAZ</t>
   </si>
 </sst>
 </file>
@@ -9006,11 +9054,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1914"/>
+  <dimension ref="A1:J1928"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1875" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1879" sqref="A1879"/>
+      <pane ySplit="1" topLeftCell="A1886" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1892" sqref="A1892"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -65072,7 +65120,7 @@
         <v>835</v>
       </c>
       <c r="F1873" s="10" t="s">
-        <v>2598</v>
+        <v>2597</v>
       </c>
       <c r="G1873" s="11" t="s">
         <v>1604</v>
@@ -65102,7 +65150,7 @@
         <v>618</v>
       </c>
       <c r="F1874" s="10" t="s">
-        <v>2595</v>
+        <v>2594</v>
       </c>
       <c r="G1874" s="11" t="s">
         <v>295</v>
@@ -65114,7 +65162,7 @@
         <v>13</v>
       </c>
       <c r="J1874" s="13" t="s">
-        <v>2600</v>
+        <v>2599</v>
       </c>
     </row>
     <row r="1875" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -65134,7 +65182,7 @@
         <v>618</v>
       </c>
       <c r="F1875" s="10" t="s">
-        <v>2597</v>
+        <v>2596</v>
       </c>
       <c r="G1875" s="11" t="s">
         <v>295</v>
@@ -65164,7 +65212,7 @@
         <v>2589</v>
       </c>
       <c r="F1876" s="10" t="s">
-        <v>2599</v>
+        <v>2598</v>
       </c>
       <c r="G1876" s="11" t="s">
         <v>295</v>
@@ -65194,7 +65242,7 @@
         <v>618</v>
       </c>
       <c r="F1877" s="10" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="G1877" s="11" t="s">
         <v>295</v>
@@ -65224,7 +65272,7 @@
         <v>835</v>
       </c>
       <c r="F1878" s="10" t="s">
-        <v>2594</v>
+        <v>2601</v>
       </c>
       <c r="G1878" s="11" t="s">
         <v>1605</v>
@@ -65235,107 +65283,203 @@
       <c r="I1878" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1878" s="13"/>
+      <c r="J1878" s="13" t="s">
+        <v>2602</v>
+      </c>
     </row>
     <row r="1879" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1879" s="12"/>
-      <c r="B1879" s="12"/>
-      <c r="C1879" s="14"/>
-      <c r="D1879" s="10"/>
-      <c r="E1879" s="11"/>
-      <c r="F1879" s="10"/>
-      <c r="G1879" s="11"/>
-      <c r="H1879" s="12"/>
-      <c r="I1879" s="13"/>
+      <c r="A1879" s="12">
+        <v>44630</v>
+      </c>
+      <c r="B1879" s="12">
+        <v>44630</v>
+      </c>
+      <c r="C1879" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1879" s="10" t="s">
+        <v>696</v>
+      </c>
+      <c r="E1879" s="11" t="s">
+        <v>2589</v>
+      </c>
+      <c r="F1879" s="10" t="s">
+        <v>2603</v>
+      </c>
+      <c r="G1879" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1879" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1879" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1879" s="13"/>
     </row>
     <row r="1880" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1880" s="12"/>
-      <c r="B1880" s="12"/>
-      <c r="C1880" s="14"/>
-      <c r="D1880" s="10"/>
-      <c r="E1880" s="11"/>
-      <c r="F1880" s="10"/>
-      <c r="G1880" s="11"/>
-      <c r="H1880" s="12"/>
-      <c r="I1880" s="13"/>
+      <c r="A1880" s="12">
+        <v>44630</v>
+      </c>
+      <c r="B1880" s="12">
+        <v>44630</v>
+      </c>
+      <c r="C1880" s="14" t="s">
+        <v>2158</v>
+      </c>
+      <c r="D1880" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1880" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F1880" s="10" t="s">
+        <v>2604</v>
+      </c>
+      <c r="G1880" s="11" t="s">
+        <v>1626</v>
+      </c>
+      <c r="H1880" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1880" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1880" s="13"/>
     </row>
     <row r="1881" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1881" s="12"/>
-      <c r="B1881" s="12"/>
-      <c r="C1881" s="14"/>
-      <c r="D1881" s="10"/>
-      <c r="E1881" s="11"/>
-      <c r="F1881" s="10"/>
-      <c r="G1881" s="11"/>
-      <c r="H1881" s="12"/>
-      <c r="I1881" s="13"/>
+      <c r="A1881" s="12">
+        <v>44630</v>
+      </c>
+      <c r="B1881" s="12">
+        <v>44630</v>
+      </c>
+      <c r="C1881" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1881" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E1881" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F1881" s="10" t="s">
+        <v>2605</v>
+      </c>
+      <c r="G1881" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1881" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1881" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1881" s="13"/>
     </row>
-    <row r="1882" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1882" s="12"/>
-      <c r="B1882" s="12"/>
-      <c r="C1882" s="14"/>
-      <c r="D1882" s="10"/>
-      <c r="E1882" s="11"/>
-      <c r="F1882" s="10"/>
-      <c r="G1882" s="11"/>
-      <c r="H1882" s="12"/>
-      <c r="I1882" s="13"/>
-      <c r="J1882" s="13"/>
-    </row>
-    <row r="1883" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1882" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1882" s="12">
+        <v>44631</v>
+      </c>
+      <c r="B1882" s="12">
+        <v>44631</v>
+      </c>
+      <c r="C1882" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D1882" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E1882" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F1882" s="10" t="s">
+        <v>2607</v>
+      </c>
+      <c r="G1882" s="11" t="s">
+        <v>1601</v>
+      </c>
+      <c r="H1882" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1882" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1882" s="13" t="s">
+        <v>2608</v>
+      </c>
+    </row>
+    <row r="1883" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1883" s="12">
-        <v>44607</v>
-      </c>
-      <c r="B1883" s="12"/>
+        <v>44263</v>
+      </c>
+      <c r="B1883" s="12">
+        <v>44634</v>
+      </c>
       <c r="C1883" s="14" t="s">
-        <v>1194</v>
+        <v>2253</v>
       </c>
       <c r="D1883" s="10" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="E1883" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F1883" s="10" t="s">
-        <v>2537</v>
-      </c>
-      <c r="G1883" s="11"/>
-      <c r="H1883" s="12"/>
-      <c r="I1883" s="13"/>
-      <c r="J1883" s="13"/>
-    </row>
-    <row r="1884" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2595</v>
+      </c>
+      <c r="G1883" s="11" t="s">
+        <v>1604</v>
+      </c>
+      <c r="H1883" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1883" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1883" s="13" t="s">
+        <v>2609</v>
+      </c>
+    </row>
+    <row r="1884" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1884" s="12">
-        <v>44614</v>
-      </c>
-      <c r="B1884" s="12"/>
+        <v>44634</v>
+      </c>
+      <c r="B1884" s="12">
+        <v>44634</v>
+      </c>
       <c r="C1884" s="14" t="s">
-        <v>19</v>
+        <v>1971</v>
       </c>
       <c r="D1884" s="10" t="s">
-        <v>492</v>
+        <v>89</v>
       </c>
       <c r="E1884" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F1884" s="10" t="s">
-        <v>2551</v>
-      </c>
-      <c r="G1884" s="11"/>
-      <c r="H1884" s="12"/>
-      <c r="I1884" s="13"/>
+        <v>2610</v>
+      </c>
+      <c r="G1884" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1884" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1884" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1884" s="13"/>
     </row>
     <row r="1885" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1885" s="12">
-        <v>44614</v>
-      </c>
-      <c r="B1885" s="12"/>
+        <v>44634</v>
+      </c>
+      <c r="B1885" s="12">
+        <v>44634</v>
+      </c>
       <c r="C1885" s="14" t="s">
-        <v>895</v>
+        <v>19</v>
       </c>
       <c r="D1885" s="10" t="s">
         <v>492</v>
@@ -65344,95 +65488,125 @@
         <v>835</v>
       </c>
       <c r="F1885" s="10" t="s">
-        <v>2557</v>
-      </c>
-      <c r="G1885" s="11"/>
-      <c r="H1885" s="12"/>
-      <c r="I1885" s="13"/>
+        <v>2531</v>
+      </c>
+      <c r="G1885" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H1885" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1885" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1885" s="13"/>
     </row>
     <row r="1886" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1886" s="12">
-        <v>44616</v>
-      </c>
-      <c r="B1886" s="12"/>
+        <v>44635</v>
+      </c>
+      <c r="B1886" s="12">
+        <v>44635</v>
+      </c>
       <c r="C1886" s="14" t="s">
-        <v>2253</v>
+        <v>1971</v>
       </c>
       <c r="D1886" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E1886" s="11" t="s">
-        <v>618</v>
+        <v>835</v>
       </c>
       <c r="F1886" s="10" t="s">
-        <v>2558</v>
-      </c>
-      <c r="G1886" s="11"/>
-      <c r="H1886" s="12"/>
-      <c r="I1886" s="13"/>
+        <v>2611</v>
+      </c>
+      <c r="G1886" s="11" t="s">
+        <v>1604</v>
+      </c>
+      <c r="H1886" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1886" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1886" s="13"/>
     </row>
     <row r="1887" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1887" s="12">
-        <v>44623</v>
-      </c>
-      <c r="B1887" s="12"/>
+        <v>44635</v>
+      </c>
+      <c r="B1887" s="12">
+        <v>44635</v>
+      </c>
       <c r="C1887" s="14" t="s">
-        <v>535</v>
+        <v>557</v>
       </c>
       <c r="D1887" s="10" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="E1887" s="11" t="s">
         <v>835</v>
       </c>
       <c r="F1887" s="10" t="s">
-        <v>2576</v>
-      </c>
-      <c r="G1887" s="11"/>
-      <c r="H1887" s="12"/>
-      <c r="I1887" s="13"/>
+        <v>2612</v>
+      </c>
+      <c r="G1887" s="11" t="s">
+        <v>1601</v>
+      </c>
+      <c r="H1887" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1887" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1887" s="13"/>
     </row>
     <row r="1888" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1888" s="12">
-        <v>44263</v>
-      </c>
-      <c r="B1888" s="12"/>
+        <v>44635</v>
+      </c>
+      <c r="B1888" s="12">
+        <v>44635</v>
+      </c>
       <c r="C1888" s="14" t="s">
-        <v>2253</v>
+        <v>573</v>
       </c>
       <c r="D1888" s="10" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="E1888" s="11" t="s">
-        <v>618</v>
+        <v>835</v>
       </c>
       <c r="F1888" s="10" t="s">
-        <v>2596</v>
-      </c>
-      <c r="G1888" s="11"/>
-      <c r="H1888" s="12"/>
-      <c r="I1888" s="13"/>
+        <v>2613</v>
+      </c>
+      <c r="G1888" s="11" t="s">
+        <v>1601</v>
+      </c>
+      <c r="H1888" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1888" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1888" s="13"/>
     </row>
-    <row r="1889" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1889" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1889" s="12">
-        <v>44522</v>
+        <v>44635</v>
       </c>
       <c r="B1889" s="12"/>
       <c r="C1889" s="14" t="s">
-        <v>46</v>
+        <v>535</v>
       </c>
       <c r="D1889" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E1889" s="11" t="s">
-        <v>568</v>
+        <v>835</v>
       </c>
       <c r="F1889" s="10" t="s">
-        <v>2353</v>
+        <v>2614</v>
       </c>
       <c r="G1889" s="11"/>
       <c r="H1889" s="12"/>
@@ -65440,32 +65614,68 @@
       <c r="J1889" s="13"/>
     </row>
     <row r="1890" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1890" s="12"/>
-      <c r="B1890" s="12"/>
-      <c r="C1890" s="14"/>
-      <c r="D1890" s="10"/>
-      <c r="E1890" s="11"/>
-      <c r="F1890" s="10"/>
-      <c r="G1890" s="11"/>
-      <c r="H1890" s="12"/>
-      <c r="I1890" s="13"/>
+      <c r="A1890" s="12">
+        <v>44635</v>
+      </c>
+      <c r="B1890" s="12">
+        <v>44636</v>
+      </c>
+      <c r="C1890" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="D1890" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1890" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F1890" s="10" t="s">
+        <v>2615</v>
+      </c>
+      <c r="G1890" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1890" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1890" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1890" s="13"/>
     </row>
     <row r="1891" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1891" s="12"/>
-      <c r="B1891" s="12"/>
-      <c r="C1891" s="14"/>
-      <c r="D1891" s="10"/>
-      <c r="E1891" s="11"/>
-      <c r="F1891" s="10"/>
-      <c r="G1891" s="11"/>
-      <c r="H1891" s="12"/>
-      <c r="I1891" s="13"/>
+      <c r="A1891" s="12">
+        <v>44636</v>
+      </c>
+      <c r="B1891" s="12">
+        <v>44636</v>
+      </c>
+      <c r="C1891" s="14" t="s">
+        <v>2253</v>
+      </c>
+      <c r="D1891" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1891" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F1891" s="10" t="s">
+        <v>2616</v>
+      </c>
+      <c r="G1891" s="11" t="s">
+        <v>1626</v>
+      </c>
+      <c r="H1891" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1891" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1891" s="13"/>
     </row>
     <row r="1892" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1892" s="12"/>
-      <c r="B1892" s="9"/>
+      <c r="B1892" s="12"/>
       <c r="C1892" s="14"/>
       <c r="D1892" s="10"/>
       <c r="E1892" s="11"/>
@@ -65476,38 +65686,20 @@
       <c r="J1892" s="13"/>
     </row>
     <row r="1893" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1893" s="1" t="s">
-        <v>1473</v>
-      </c>
-      <c r="B1893" s="2" t="s">
-        <v>1474</v>
-      </c>
-      <c r="C1893" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1893" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1893" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="F1893" s="4" t="s">
-        <v>1572</v>
-      </c>
-      <c r="G1893" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1893" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1893" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1893" s="36"/>
+      <c r="A1893" s="12"/>
+      <c r="B1893" s="12"/>
+      <c r="C1893" s="14"/>
+      <c r="D1893" s="10"/>
+      <c r="E1893" s="11"/>
+      <c r="F1893" s="10"/>
+      <c r="G1893" s="11"/>
+      <c r="H1893" s="12"/>
+      <c r="I1893" s="13"/>
+      <c r="J1893" s="13"/>
     </row>
     <row r="1894" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1894" s="12"/>
-      <c r="B1894" s="9"/>
+      <c r="B1894" s="12"/>
       <c r="C1894" s="14"/>
       <c r="D1894" s="10"/>
       <c r="E1894" s="11"/>
@@ -65519,7 +65711,7 @@
     </row>
     <row r="1895" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1895" s="12"/>
-      <c r="B1895" s="9"/>
+      <c r="B1895" s="12"/>
       <c r="C1895" s="14"/>
       <c r="D1895" s="10"/>
       <c r="E1895" s="11"/>
@@ -65529,68 +65721,64 @@
       <c r="I1895" s="13"/>
       <c r="J1895" s="13"/>
     </row>
-    <row r="1896" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="1896" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1896" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1896" s="9"/>
+        <v>44630</v>
+      </c>
+      <c r="B1896" s="12"/>
       <c r="C1896" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D1896" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E1896" s="11" t="s">
-        <v>757</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D1896" s="10"/>
+      <c r="E1896" s="11"/>
       <c r="F1896" s="10" t="s">
-        <v>1639</v>
+        <v>2606</v>
       </c>
       <c r="G1896" s="11"/>
       <c r="H1896" s="12"/>
       <c r="I1896" s="13"/>
-      <c r="J1896" s="13" t="s">
-        <v>1662</v>
-      </c>
-    </row>
-    <row r="1897" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J1896" s="13"/>
+    </row>
+    <row r="1897" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1897" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B1897" s="9"/>
+        <v>44614</v>
+      </c>
+      <c r="B1897" s="12">
+        <v>44614</v>
+      </c>
       <c r="C1897" s="14" t="s">
-        <v>895</v>
+        <v>19</v>
       </c>
       <c r="D1897" s="10" t="s">
         <v>492</v>
       </c>
       <c r="E1897" s="11" t="s">
-        <v>757</v>
+        <v>835</v>
       </c>
       <c r="F1897" s="10" t="s">
-        <v>1638</v>
+        <v>2531</v>
       </c>
       <c r="G1897" s="11"/>
       <c r="H1897" s="12"/>
       <c r="I1897" s="13"/>
       <c r="J1897" s="13"/>
     </row>
-    <row r="1898" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="1898" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1898" s="12">
-        <v>44112</v>
-      </c>
-      <c r="B1898" s="9"/>
+        <v>44607</v>
+      </c>
+      <c r="B1898" s="12"/>
       <c r="C1898" s="14" t="s">
-        <v>621</v>
+        <v>1194</v>
       </c>
       <c r="D1898" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E1898" s="11" t="s">
-        <v>568</v>
+        <v>835</v>
       </c>
       <c r="F1898" s="10" t="s">
-        <v>2225</v>
+        <v>2537</v>
       </c>
       <c r="G1898" s="11"/>
       <c r="H1898" s="12"/>
@@ -65599,20 +65787,20 @@
     </row>
     <row r="1899" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1899" s="12">
-        <v>44088</v>
-      </c>
-      <c r="B1899" s="9"/>
+        <v>44614</v>
+      </c>
+      <c r="B1899" s="12"/>
       <c r="C1899" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D1899" s="10" t="s">
-        <v>903</v>
+        <v>492</v>
       </c>
       <c r="E1899" s="11" t="s">
-        <v>683</v>
+        <v>835</v>
       </c>
       <c r="F1899" s="10" t="s">
-        <v>1008</v>
+        <v>2551</v>
       </c>
       <c r="G1899" s="11"/>
       <c r="H1899" s="12"/>
@@ -65621,20 +65809,20 @@
     </row>
     <row r="1900" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1900" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1900" s="9"/>
+        <v>44614</v>
+      </c>
+      <c r="B1900" s="12"/>
       <c r="C1900" s="14" t="s">
-        <v>621</v>
+        <v>895</v>
       </c>
       <c r="D1900" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E1900" s="11" t="s">
-        <v>568</v>
+        <v>835</v>
       </c>
       <c r="F1900" s="10" t="s">
-        <v>900</v>
+        <v>2557</v>
       </c>
       <c r="G1900" s="11"/>
       <c r="H1900" s="12"/>
@@ -65643,20 +65831,20 @@
     </row>
     <row r="1901" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1901" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1901" s="9"/>
+        <v>44616</v>
+      </c>
+      <c r="B1901" s="12"/>
       <c r="C1901" s="14" t="s">
-        <v>621</v>
+        <v>2253</v>
       </c>
       <c r="D1901" s="10" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="E1901" s="11" t="s">
-        <v>568</v>
+        <v>618</v>
       </c>
       <c r="F1901" s="10" t="s">
-        <v>899</v>
+        <v>2558</v>
       </c>
       <c r="G1901" s="11"/>
       <c r="H1901" s="12"/>
@@ -65665,172 +65853,122 @@
     </row>
     <row r="1902" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1902" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1902" s="9"/>
+        <v>44623</v>
+      </c>
+      <c r="B1902" s="12"/>
       <c r="C1902" s="14" t="s">
-        <v>895</v>
+        <v>535</v>
       </c>
       <c r="D1902" s="10" t="s">
-        <v>492</v>
+        <v>6</v>
       </c>
       <c r="E1902" s="11" t="s">
-        <v>568</v>
+        <v>835</v>
       </c>
       <c r="F1902" s="10" t="s">
-        <v>897</v>
+        <v>2576</v>
       </c>
       <c r="G1902" s="11"/>
       <c r="H1902" s="12"/>
       <c r="I1902" s="13"/>
       <c r="J1902" s="13"/>
     </row>
-    <row r="1903" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="1903" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A1903" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1903" s="9"/>
+        <v>44522</v>
+      </c>
+      <c r="B1903" s="12"/>
       <c r="C1903" s="14" t="s">
-        <v>895</v>
+        <v>46</v>
       </c>
       <c r="D1903" s="10" t="s">
-        <v>492</v>
+        <v>6</v>
       </c>
       <c r="E1903" s="11" t="s">
         <v>568</v>
       </c>
       <c r="F1903" s="10" t="s">
-        <v>898</v>
+        <v>2353</v>
       </c>
       <c r="G1903" s="11"/>
       <c r="H1903" s="12"/>
       <c r="I1903" s="13"/>
       <c r="J1903" s="13"/>
     </row>
-    <row r="1904" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A1904" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B1904" s="9"/>
-      <c r="C1904" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D1904" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E1904" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F1904" s="10" t="s">
-        <v>901</v>
-      </c>
+    <row r="1904" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1904" s="12"/>
+      <c r="B1904" s="12"/>
+      <c r="C1904" s="14"/>
+      <c r="D1904" s="10"/>
+      <c r="E1904" s="11"/>
+      <c r="F1904" s="10"/>
       <c r="G1904" s="11"/>
       <c r="H1904" s="12"/>
       <c r="I1904" s="13"/>
-      <c r="J1904" s="13" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="1905" spans="1:10" ht="168" x14ac:dyDescent="0.2">
-      <c r="A1905" s="12">
-        <v>43949</v>
-      </c>
-      <c r="B1905" s="9"/>
-      <c r="C1905" s="14" t="s">
-        <v>468</v>
-      </c>
-      <c r="D1905" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1905" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="F1905" s="10" t="s">
-        <v>684</v>
-      </c>
-      <c r="G1905" s="11" t="s">
-        <v>1619</v>
-      </c>
+      <c r="J1904" s="13"/>
+    </row>
+    <row r="1905" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1905" s="12"/>
+      <c r="B1905" s="12"/>
+      <c r="C1905" s="14"/>
+      <c r="D1905" s="10"/>
+      <c r="E1905" s="11"/>
+      <c r="F1905" s="10"/>
+      <c r="G1905" s="11"/>
       <c r="H1905" s="12"/>
-      <c r="I1905" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1905" s="13"/>
       <c r="J1905" s="13"/>
     </row>
-    <row r="1906" spans="1:10" ht="168" x14ac:dyDescent="0.2">
-      <c r="A1906" s="12">
-        <v>43949</v>
-      </c>
+    <row r="1906" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1906" s="12"/>
       <c r="B1906" s="9"/>
-      <c r="C1906" s="14" t="s">
-        <v>468</v>
-      </c>
-      <c r="D1906" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1906" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="F1906" s="10" t="s">
-        <v>703</v>
-      </c>
-      <c r="G1906" s="11" t="s">
-        <v>685</v>
-      </c>
+      <c r="C1906" s="14"/>
+      <c r="D1906" s="10"/>
+      <c r="E1906" s="11"/>
+      <c r="F1906" s="10"/>
+      <c r="G1906" s="11"/>
       <c r="H1906" s="12"/>
-      <c r="I1906" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1906" s="13" t="s">
-        <v>1562</v>
-      </c>
-    </row>
-    <row r="1907" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1907" s="12">
-        <v>43838</v>
-      </c>
-      <c r="B1907" s="9"/>
-      <c r="C1907" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1907" s="10" t="s">
-        <v>460</v>
-      </c>
-      <c r="E1907" s="11" t="s">
-        <v>645</v>
-      </c>
-      <c r="F1907" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="G1907" s="11" t="s">
-        <v>1620</v>
-      </c>
-      <c r="H1907" s="12"/>
-      <c r="I1907" s="13"/>
-      <c r="J1907" s="13" t="s">
-        <v>1527</v>
-      </c>
-    </row>
-    <row r="1908" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1908" s="12">
-        <v>43762</v>
-      </c>
+      <c r="I1906" s="13"/>
+      <c r="J1906" s="13"/>
+    </row>
+    <row r="1907" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1907" s="1" t="s">
+        <v>1473</v>
+      </c>
+      <c r="B1907" s="2" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C1907" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1907" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1907" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F1907" s="4" t="s">
+        <v>1572</v>
+      </c>
+      <c r="G1907" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1907" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1907" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1907" s="36"/>
+    </row>
+    <row r="1908" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1908" s="12"/>
       <c r="B1908" s="9"/>
-      <c r="C1908" s="14" t="s">
-        <v>446</v>
-      </c>
-      <c r="D1908" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1908" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F1908" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G1908" s="11" t="s">
-        <v>1609</v>
-      </c>
+      <c r="C1908" s="14"/>
+      <c r="D1908" s="10"/>
+      <c r="E1908" s="11"/>
+      <c r="F1908" s="10"/>
+      <c r="G1908" s="11"/>
       <c r="H1908" s="12"/>
       <c r="I1908" s="13"/>
       <c r="J1908" s="13"/>
@@ -65847,68 +65985,386 @@
       <c r="I1909" s="13"/>
       <c r="J1909" s="13"/>
     </row>
-    <row r="1910" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1910" s="12"/>
+    <row r="1910" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+      <c r="A1910" s="12">
+        <v>44252</v>
+      </c>
       <c r="B1910" s="9"/>
-      <c r="C1910" s="14"/>
-      <c r="D1910" s="10"/>
-      <c r="E1910" s="11"/>
-      <c r="F1910" s="10"/>
+      <c r="C1910" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D1910" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E1910" s="11" t="s">
+        <v>757</v>
+      </c>
+      <c r="F1910" s="10" t="s">
+        <v>1639</v>
+      </c>
       <c r="G1910" s="11"/>
       <c r="H1910" s="12"/>
       <c r="I1910" s="13"/>
-      <c r="J1910" s="13"/>
-    </row>
-    <row r="1911" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1911" s="12"/>
+      <c r="J1910" s="13" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="1911" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1911" s="12">
+        <v>44252</v>
+      </c>
       <c r="B1911" s="9"/>
-      <c r="C1911" s="14"/>
-      <c r="D1911" s="10"/>
-      <c r="E1911" s="11"/>
-      <c r="F1911" s="10"/>
+      <c r="C1911" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D1911" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E1911" s="11" t="s">
+        <v>757</v>
+      </c>
+      <c r="F1911" s="10" t="s">
+        <v>1638</v>
+      </c>
       <c r="G1911" s="11"/>
       <c r="H1911" s="12"/>
       <c r="I1911" s="13"/>
       <c r="J1911" s="13"/>
     </row>
-    <row r="1912" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1912" s="12"/>
+    <row r="1912" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1912" s="12">
+        <v>44112</v>
+      </c>
       <c r="B1912" s="9"/>
-      <c r="C1912" s="14"/>
-      <c r="D1912" s="10"/>
-      <c r="E1912" s="11"/>
-      <c r="F1912" s="10"/>
+      <c r="C1912" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="D1912" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1912" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1912" s="10" t="s">
+        <v>2225</v>
+      </c>
       <c r="G1912" s="11"/>
       <c r="H1912" s="12"/>
       <c r="I1912" s="13"/>
       <c r="J1912" s="13"/>
     </row>
     <row r="1913" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1913" s="12"/>
+      <c r="A1913" s="12">
+        <v>44088</v>
+      </c>
       <c r="B1913" s="9"/>
-      <c r="C1913" s="14"/>
-      <c r="D1913" s="10"/>
-      <c r="E1913" s="11"/>
-      <c r="F1913" s="10"/>
+      <c r="C1913" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1913" s="10" t="s">
+        <v>903</v>
+      </c>
+      <c r="E1913" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F1913" s="10" t="s">
+        <v>1008</v>
+      </c>
       <c r="G1913" s="11"/>
       <c r="H1913" s="12"/>
       <c r="I1913" s="13"/>
       <c r="J1913" s="13"/>
     </row>
     <row r="1914" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1914" s="12"/>
+      <c r="A1914" s="12">
+        <v>44055</v>
+      </c>
       <c r="B1914" s="9"/>
-      <c r="C1914" s="14"/>
-      <c r="D1914" s="10"/>
-      <c r="E1914" s="11"/>
-      <c r="F1914" s="10"/>
+      <c r="C1914" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="D1914" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1914" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1914" s="10" t="s">
+        <v>900</v>
+      </c>
       <c r="G1914" s="11"/>
       <c r="H1914" s="12"/>
       <c r="I1914" s="13"/>
       <c r="J1914" s="13"/>
     </row>
+    <row r="1915" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1915" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B1915" s="9"/>
+      <c r="C1915" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="D1915" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1915" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1915" s="10" t="s">
+        <v>899</v>
+      </c>
+      <c r="G1915" s="11"/>
+      <c r="H1915" s="12"/>
+      <c r="I1915" s="13"/>
+      <c r="J1915" s="13"/>
+    </row>
+    <row r="1916" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1916" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B1916" s="9"/>
+      <c r="C1916" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D1916" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E1916" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1916" s="10" t="s">
+        <v>897</v>
+      </c>
+      <c r="G1916" s="11"/>
+      <c r="H1916" s="12"/>
+      <c r="I1916" s="13"/>
+      <c r="J1916" s="13"/>
+    </row>
+    <row r="1917" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A1917" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B1917" s="9"/>
+      <c r="C1917" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D1917" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E1917" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1917" s="10" t="s">
+        <v>898</v>
+      </c>
+      <c r="G1917" s="11"/>
+      <c r="H1917" s="12"/>
+      <c r="I1917" s="13"/>
+      <c r="J1917" s="13"/>
+    </row>
+    <row r="1918" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1918" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B1918" s="9"/>
+      <c r="C1918" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D1918" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E1918" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1918" s="10" t="s">
+        <v>901</v>
+      </c>
+      <c r="G1918" s="11"/>
+      <c r="H1918" s="12"/>
+      <c r="I1918" s="13"/>
+      <c r="J1918" s="13" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="1919" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1919" s="12">
+        <v>43949</v>
+      </c>
+      <c r="B1919" s="9"/>
+      <c r="C1919" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1919" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1919" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F1919" s="10" t="s">
+        <v>684</v>
+      </c>
+      <c r="G1919" s="11" t="s">
+        <v>1619</v>
+      </c>
+      <c r="H1919" s="12"/>
+      <c r="I1919" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1919" s="13"/>
+    </row>
+    <row r="1920" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A1920" s="12">
+        <v>43949</v>
+      </c>
+      <c r="B1920" s="9"/>
+      <c r="C1920" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1920" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1920" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F1920" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="G1920" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="H1920" s="12"/>
+      <c r="I1920" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1920" s="13" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="1921" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1921" s="12">
+        <v>43838</v>
+      </c>
+      <c r="B1921" s="9"/>
+      <c r="C1921" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1921" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1921" s="11" t="s">
+        <v>645</v>
+      </c>
+      <c r="F1921" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="G1921" s="11" t="s">
+        <v>1620</v>
+      </c>
+      <c r="H1921" s="12"/>
+      <c r="I1921" s="13"/>
+      <c r="J1921" s="13" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="1922" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1922" s="12">
+        <v>43762</v>
+      </c>
+      <c r="B1922" s="9"/>
+      <c r="C1922" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1922" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1922" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F1922" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1922" s="11" t="s">
+        <v>1609</v>
+      </c>
+      <c r="H1922" s="12"/>
+      <c r="I1922" s="13"/>
+      <c r="J1922" s="13"/>
+    </row>
+    <row r="1923" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1923" s="12"/>
+      <c r="B1923" s="9"/>
+      <c r="C1923" s="14"/>
+      <c r="D1923" s="10"/>
+      <c r="E1923" s="11"/>
+      <c r="F1923" s="10"/>
+      <c r="G1923" s="11"/>
+      <c r="H1923" s="12"/>
+      <c r="I1923" s="13"/>
+      <c r="J1923" s="13"/>
+    </row>
+    <row r="1924" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1924" s="12"/>
+      <c r="B1924" s="9"/>
+      <c r="C1924" s="14"/>
+      <c r="D1924" s="10"/>
+      <c r="E1924" s="11"/>
+      <c r="F1924" s="10"/>
+      <c r="G1924" s="11"/>
+      <c r="H1924" s="12"/>
+      <c r="I1924" s="13"/>
+      <c r="J1924" s="13"/>
+    </row>
+    <row r="1925" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1925" s="12"/>
+      <c r="B1925" s="9"/>
+      <c r="C1925" s="14"/>
+      <c r="D1925" s="10"/>
+      <c r="E1925" s="11"/>
+      <c r="F1925" s="10"/>
+      <c r="G1925" s="11"/>
+      <c r="H1925" s="12"/>
+      <c r="I1925" s="13"/>
+      <c r="J1925" s="13"/>
+    </row>
+    <row r="1926" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1926" s="12"/>
+      <c r="B1926" s="9"/>
+      <c r="C1926" s="14"/>
+      <c r="D1926" s="10"/>
+      <c r="E1926" s="11"/>
+      <c r="F1926" s="10"/>
+      <c r="G1926" s="11"/>
+      <c r="H1926" s="12"/>
+      <c r="I1926" s="13"/>
+      <c r="J1926" s="13"/>
+    </row>
+    <row r="1927" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1927" s="12"/>
+      <c r="B1927" s="9"/>
+      <c r="C1927" s="14"/>
+      <c r="D1927" s="10"/>
+      <c r="E1927" s="11"/>
+      <c r="F1927" s="10"/>
+      <c r="G1927" s="11"/>
+      <c r="H1927" s="12"/>
+      <c r="I1927" s="13"/>
+      <c r="J1927" s="13"/>
+    </row>
+    <row r="1928" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1928" s="12"/>
+      <c r="B1928" s="9"/>
+      <c r="C1928" s="14"/>
+      <c r="D1928" s="10"/>
+      <c r="E1928" s="11"/>
+      <c r="F1928" s="10"/>
+      <c r="G1928" s="11"/>
+      <c r="H1928" s="12"/>
+      <c r="I1928" s="13"/>
+      <c r="J1928" s="13"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J1480" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J1881" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J1281" r:id="rId1" xr:uid="{B64A69E0-7BE4-4C80-936B-0B004BD04638}"/>
@@ -65920,6 +66376,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E16FADF7-6C4C-4356-9576-380717A61E1D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE13D4C-C1F0-4B00-8A02-71F13D132F72}">
   <dimension ref="B1:G35"/>
   <sheetViews>

</xml_diff>

<commit_message>
Relação de Doc de Entrada
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED3B3A9-0A85-4F62-8621-32D561971B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB1B4B6-FF3A-4F33-AE85-4C29D67D0A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13588" uniqueCount="2640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13621" uniqueCount="2646">
   <si>
     <t>Responsável</t>
   </si>
@@ -8353,6 +8353,33 @@
   </si>
   <si>
     <t>Correção de diversas NF de entrada e saída para correção do EFD de fev/2022</t>
+  </si>
+  <si>
+    <t>Dashboard Compras:
+Número de scs
+Sc atendidas no prazo de 5 dias
+Números  de pedidos d compras
+Pedidos de compras em atraso
+Qt nota fiscal
+Número de fornecedores novos
+Avaliação d fornecedor
+Pedidos urgentes</t>
+  </si>
+  <si>
+    <t>Alterar a opção de Livre para Parciel e corrigir valor do saldo quando se usa esta opção no Portal Petrobras</t>
+  </si>
+  <si>
+    <t>Auxilio emissão de Relatorio de Movimentação Bancária</t>
+  </si>
+  <si>
+    <t>Contabilização financeiro de folha de pgto - dúvidas</t>
+  </si>
+  <si>
+    <t>Criar novo relatório para estatísticas de digitação de Doc de Entrada: 
+Número de nota,  Valor,  Emissão, Qtd por mês,  De todas as plataformas no acesso da Bárbara.</t>
+  </si>
+  <si>
+    <t>BKCOMR14</t>
   </si>
 </sst>
 </file>
@@ -8855,7 +8882,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8869,7 +8896,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -8881,7 +8908,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -8893,14 +8920,14 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -8928,14 +8955,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -8963,9 +9007,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -9127,11 +9188,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1952"/>
+  <dimension ref="A1:J1954"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1902" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1914" sqref="A1914"/>
+      <pane ySplit="1" topLeftCell="A1912" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1918" sqref="A1918"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -66436,56 +66497,130 @@
       </c>
       <c r="J1913" s="13"/>
     </row>
-    <row r="1914" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1914" s="12"/>
-      <c r="B1914" s="12"/>
-      <c r="C1914" s="14"/>
-      <c r="D1914" s="10"/>
-      <c r="E1914" s="11"/>
-      <c r="F1914" s="10"/>
-      <c r="G1914" s="11"/>
-      <c r="H1914" s="12"/>
-      <c r="I1914" s="13"/>
+    <row r="1914" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1914" s="12">
+        <v>44645</v>
+      </c>
+      <c r="B1914" s="12">
+        <v>44645</v>
+      </c>
+      <c r="C1914" s="14" t="s">
+        <v>557</v>
+      </c>
+      <c r="D1914" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1914" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F1914" s="10" t="s">
+        <v>2641</v>
+      </c>
+      <c r="G1914" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1914" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1914" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1914" s="13"/>
     </row>
     <row r="1915" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1915" s="12"/>
-      <c r="B1915" s="12"/>
-      <c r="C1915" s="14"/>
-      <c r="D1915" s="10"/>
-      <c r="E1915" s="11"/>
-      <c r="F1915" s="10"/>
-      <c r="G1915" s="11"/>
-      <c r="H1915" s="12"/>
-      <c r="I1915" s="13"/>
+      <c r="A1915" s="12">
+        <v>44645</v>
+      </c>
+      <c r="B1915" s="12">
+        <v>44645</v>
+      </c>
+      <c r="C1915" s="14" t="s">
+        <v>1193</v>
+      </c>
+      <c r="D1915" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1915" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F1915" s="10" t="s">
+        <v>2642</v>
+      </c>
+      <c r="G1915" s="11" t="s">
+        <v>1599</v>
+      </c>
+      <c r="H1915" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1915" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1915" s="13"/>
     </row>
     <row r="1916" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1916" s="12"/>
-      <c r="B1916" s="12"/>
-      <c r="C1916" s="14"/>
-      <c r="D1916" s="10"/>
-      <c r="E1916" s="11"/>
-      <c r="F1916" s="10"/>
-      <c r="G1916" s="11"/>
-      <c r="H1916" s="12"/>
-      <c r="I1916" s="13"/>
+      <c r="A1916" s="12">
+        <v>44645</v>
+      </c>
+      <c r="B1916" s="12">
+        <v>44645</v>
+      </c>
+      <c r="C1916" s="14" t="s">
+        <v>2156</v>
+      </c>
+      <c r="D1916" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1916" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F1916" s="10" t="s">
+        <v>2643</v>
+      </c>
+      <c r="G1916" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1916" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1916" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1916" s="13"/>
     </row>
-    <row r="1917" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1917" s="12"/>
-      <c r="B1917" s="12"/>
-      <c r="C1917" s="14"/>
-      <c r="D1917" s="10"/>
-      <c r="E1917" s="11"/>
-      <c r="F1917" s="10"/>
-      <c r="G1917" s="11"/>
-      <c r="H1917" s="12"/>
-      <c r="I1917" s="13"/>
-      <c r="J1917" s="13"/>
+    <row r="1917" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1917" s="12">
+        <v>44645</v>
+      </c>
+      <c r="B1917" s="12">
+        <v>44645</v>
+      </c>
+      <c r="C1917" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1917" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1917" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F1917" s="10" t="s">
+        <v>2644</v>
+      </c>
+      <c r="G1917" s="11" t="s">
+        <v>1602</v>
+      </c>
+      <c r="H1917" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1917" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1917" s="13" t="s">
+        <v>2645</v>
+      </c>
     </row>
     <row r="1918" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1918" s="43"/>
+      <c r="A1918" s="12"/>
       <c r="B1918" s="12"/>
       <c r="C1918" s="14"/>
       <c r="D1918" s="10"/>
@@ -66509,65 +66644,55 @@
       <c r="J1919" s="13"/>
     </row>
     <row r="1920" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1920" s="12">
-        <v>44642</v>
-      </c>
+      <c r="A1920" s="43"/>
       <c r="B1920" s="12"/>
-      <c r="C1920" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="D1920" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E1920" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F1920" s="10" t="s">
-        <v>2628</v>
-      </c>
+      <c r="C1920" s="14"/>
+      <c r="D1920" s="10"/>
+      <c r="E1920" s="11"/>
+      <c r="F1920" s="10"/>
       <c r="G1920" s="11"/>
       <c r="H1920" s="12"/>
       <c r="I1920" s="13"/>
       <c r="J1920" s="13"/>
     </row>
-    <row r="1921" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1921" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A1921" s="12">
-        <v>44642</v>
+        <v>44645</v>
       </c>
       <c r="B1921" s="12"/>
       <c r="C1921" s="14" t="s">
-        <v>387</v>
+        <v>288</v>
       </c>
       <c r="D1921" s="10" t="s">
-        <v>492</v>
+        <v>25</v>
       </c>
       <c r="E1921" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F1921" s="10" t="s">
-        <v>2627</v>
+        <v>2640</v>
       </c>
       <c r="G1921" s="11"/>
       <c r="H1921" s="12"/>
       <c r="I1921" s="13"/>
       <c r="J1921" s="13"/>
     </row>
-    <row r="1922" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="1922" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1922" s="12">
-        <v>44641</v>
+        <v>44642</v>
       </c>
       <c r="B1922" s="12"/>
       <c r="C1922" s="14" t="s">
-        <v>13</v>
+        <v>387</v>
       </c>
       <c r="D1922" s="10" t="s">
-        <v>582</v>
+        <v>492</v>
       </c>
       <c r="E1922" s="11" t="s">
-        <v>645</v>
+        <v>835</v>
       </c>
       <c r="F1922" s="10" t="s">
-        <v>2623</v>
+        <v>2628</v>
       </c>
       <c r="G1922" s="11"/>
       <c r="H1922" s="12"/>
@@ -66576,40 +66701,42 @@
     </row>
     <row r="1923" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1923" s="12">
-        <v>44630</v>
+        <v>44642</v>
       </c>
       <c r="B1923" s="12"/>
       <c r="C1923" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1923" s="10"/>
-      <c r="E1923" s="11"/>
+        <v>387</v>
+      </c>
+      <c r="D1923" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E1923" s="11" t="s">
+        <v>835</v>
+      </c>
       <c r="F1923" s="10" t="s">
-        <v>2604</v>
+        <v>2627</v>
       </c>
       <c r="G1923" s="11"/>
       <c r="H1923" s="12"/>
       <c r="I1923" s="13"/>
       <c r="J1923" s="13"/>
     </row>
-    <row r="1924" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1924" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1924" s="12">
-        <v>44614</v>
-      </c>
-      <c r="B1924" s="12">
-        <v>44614</v>
-      </c>
+        <v>44641</v>
+      </c>
+      <c r="B1924" s="12"/>
       <c r="C1924" s="14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1924" s="10" t="s">
-        <v>492</v>
+        <v>582</v>
       </c>
       <c r="E1924" s="11" t="s">
-        <v>835</v>
+        <v>645</v>
       </c>
       <c r="F1924" s="10" t="s">
-        <v>2529</v>
+        <v>2623</v>
       </c>
       <c r="G1924" s="11"/>
       <c r="H1924" s="12"/>
@@ -66618,20 +66745,16 @@
     </row>
     <row r="1925" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1925" s="12">
-        <v>44614</v>
+        <v>44630</v>
       </c>
       <c r="B1925" s="12"/>
       <c r="C1925" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1925" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E1925" s="11" t="s">
-        <v>835</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D1925" s="10"/>
+      <c r="E1925" s="11"/>
       <c r="F1925" s="10" t="s">
-        <v>2549</v>
+        <v>2604</v>
       </c>
       <c r="G1925" s="11"/>
       <c r="H1925" s="12"/>
@@ -66642,9 +66765,11 @@
       <c r="A1926" s="12">
         <v>44614</v>
       </c>
-      <c r="B1926" s="12"/>
+      <c r="B1926" s="12">
+        <v>44614</v>
+      </c>
       <c r="C1926" s="14" t="s">
-        <v>895</v>
+        <v>19</v>
       </c>
       <c r="D1926" s="10" t="s">
         <v>492</v>
@@ -66653,7 +66778,7 @@
         <v>835</v>
       </c>
       <c r="F1926" s="10" t="s">
-        <v>2555</v>
+        <v>2529</v>
       </c>
       <c r="G1926" s="11"/>
       <c r="H1926" s="12"/>
@@ -66662,20 +66787,20 @@
     </row>
     <row r="1927" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1927" s="12">
-        <v>44616</v>
+        <v>44614</v>
       </c>
       <c r="B1927" s="12"/>
       <c r="C1927" s="14" t="s">
-        <v>2251</v>
+        <v>19</v>
       </c>
       <c r="D1927" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E1927" s="11" t="s">
-        <v>618</v>
+        <v>835</v>
       </c>
       <c r="F1927" s="10" t="s">
-        <v>2556</v>
+        <v>2549</v>
       </c>
       <c r="G1927" s="11"/>
       <c r="H1927" s="12"/>
@@ -66684,42 +66809,42 @@
     </row>
     <row r="1928" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1928" s="12">
-        <v>44623</v>
+        <v>44614</v>
       </c>
       <c r="B1928" s="12"/>
       <c r="C1928" s="14" t="s">
-        <v>535</v>
+        <v>895</v>
       </c>
       <c r="D1928" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E1928" s="11" t="s">
         <v>835</v>
       </c>
       <c r="F1928" s="10" t="s">
-        <v>2574</v>
+        <v>2555</v>
       </c>
       <c r="G1928" s="11"/>
       <c r="H1928" s="12"/>
       <c r="I1928" s="13"/>
       <c r="J1928" s="13"/>
     </row>
-    <row r="1929" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1929" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1929" s="12">
-        <v>44522</v>
+        <v>44616</v>
       </c>
       <c r="B1929" s="12"/>
       <c r="C1929" s="14" t="s">
-        <v>46</v>
+        <v>2251</v>
       </c>
       <c r="D1929" s="10" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="E1929" s="11" t="s">
-        <v>568</v>
+        <v>618</v>
       </c>
       <c r="F1929" s="10" t="s">
-        <v>2351</v>
+        <v>2556</v>
       </c>
       <c r="G1929" s="11"/>
       <c r="H1929" s="12"/>
@@ -66727,24 +66852,44 @@
       <c r="J1929" s="13"/>
     </row>
     <row r="1930" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1930" s="12"/>
+      <c r="A1930" s="12">
+        <v>44623</v>
+      </c>
       <c r="B1930" s="12"/>
-      <c r="C1930" s="14"/>
-      <c r="D1930" s="10"/>
-      <c r="E1930" s="11"/>
-      <c r="F1930" s="10"/>
+      <c r="C1930" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="D1930" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1930" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F1930" s="10" t="s">
+        <v>2574</v>
+      </c>
       <c r="G1930" s="11"/>
       <c r="H1930" s="12"/>
       <c r="I1930" s="13"/>
       <c r="J1930" s="13"/>
     </row>
-    <row r="1931" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1931" s="12"/>
+    <row r="1931" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1931" s="12">
+        <v>44522</v>
+      </c>
       <c r="B1931" s="12"/>
-      <c r="C1931" s="14"/>
-      <c r="D1931" s="10"/>
-      <c r="E1931" s="11"/>
-      <c r="F1931" s="10"/>
+      <c r="C1931" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1931" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1931" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1931" s="10" t="s">
+        <v>2351</v>
+      </c>
       <c r="G1931" s="11"/>
       <c r="H1931" s="12"/>
       <c r="I1931" s="13"/>
@@ -66752,7 +66897,7 @@
     </row>
     <row r="1932" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1932" s="12"/>
-      <c r="B1932" s="9"/>
+      <c r="B1932" s="12"/>
       <c r="C1932" s="14"/>
       <c r="D1932" s="10"/>
       <c r="E1932" s="11"/>
@@ -66763,34 +66908,16 @@
       <c r="J1932" s="13"/>
     </row>
     <row r="1933" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1933" s="1" t="s">
-        <v>1472</v>
-      </c>
-      <c r="B1933" s="2" t="s">
-        <v>1473</v>
-      </c>
-      <c r="C1933" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1933" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1933" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="F1933" s="4" t="s">
-        <v>1571</v>
-      </c>
-      <c r="G1933" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1933" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1933" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1933" s="36"/>
+      <c r="A1933" s="12"/>
+      <c r="B1933" s="12"/>
+      <c r="C1933" s="14"/>
+      <c r="D1933" s="10"/>
+      <c r="E1933" s="11"/>
+      <c r="F1933" s="10"/>
+      <c r="G1933" s="11"/>
+      <c r="H1933" s="12"/>
+      <c r="I1933" s="13"/>
+      <c r="J1933" s="13"/>
     </row>
     <row r="1934" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1934" s="12"/>
@@ -66805,110 +66932,108 @@
       <c r="J1934" s="13"/>
     </row>
     <row r="1935" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1935" s="12"/>
-      <c r="B1935" s="9"/>
-      <c r="C1935" s="14"/>
-      <c r="D1935" s="10"/>
-      <c r="E1935" s="11"/>
-      <c r="F1935" s="10"/>
-      <c r="G1935" s="11"/>
-      <c r="H1935" s="12"/>
-      <c r="I1935" s="13"/>
-      <c r="J1935" s="13"/>
-    </row>
-    <row r="1936" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A1936" s="12">
-        <v>44252</v>
-      </c>
+      <c r="A1935" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B1935" s="2" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C1935" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1935" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1935" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F1935" s="4" t="s">
+        <v>1571</v>
+      </c>
+      <c r="G1935" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1935" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1935" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1935" s="36"/>
+    </row>
+    <row r="1936" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1936" s="12"/>
       <c r="B1936" s="9"/>
-      <c r="C1936" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D1936" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E1936" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F1936" s="10" t="s">
-        <v>1637</v>
-      </c>
+      <c r="C1936" s="14"/>
+      <c r="D1936" s="10"/>
+      <c r="E1936" s="11"/>
+      <c r="F1936" s="10"/>
       <c r="G1936" s="11"/>
       <c r="H1936" s="12"/>
       <c r="I1936" s="13"/>
-      <c r="J1936" s="13" t="s">
-        <v>1660</v>
-      </c>
-    </row>
-    <row r="1937" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1937" s="12">
-        <v>44252</v>
-      </c>
+      <c r="J1936" s="13"/>
+    </row>
+    <row r="1937" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1937" s="12"/>
       <c r="B1937" s="9"/>
-      <c r="C1937" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D1937" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E1937" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F1937" s="10" t="s">
-        <v>1636</v>
-      </c>
+      <c r="C1937" s="14"/>
+      <c r="D1937" s="10"/>
+      <c r="E1937" s="11"/>
+      <c r="F1937" s="10"/>
       <c r="G1937" s="11"/>
       <c r="H1937" s="12"/>
       <c r="I1937" s="13"/>
       <c r="J1937" s="13"/>
     </row>
-    <row r="1938" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="1938" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A1938" s="12">
-        <v>44112</v>
+        <v>44252</v>
       </c>
       <c r="B1938" s="9"/>
       <c r="C1938" s="14" t="s">
-        <v>621</v>
+        <v>895</v>
       </c>
       <c r="D1938" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E1938" s="11" t="s">
-        <v>568</v>
+        <v>757</v>
       </c>
       <c r="F1938" s="10" t="s">
-        <v>2223</v>
+        <v>1637</v>
       </c>
       <c r="G1938" s="11"/>
       <c r="H1938" s="12"/>
       <c r="I1938" s="13"/>
-      <c r="J1938" s="13"/>
-    </row>
-    <row r="1939" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J1938" s="13" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="1939" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1939" s="12">
-        <v>44088</v>
+        <v>44252</v>
       </c>
       <c r="B1939" s="9"/>
       <c r="C1939" s="14" t="s">
-        <v>19</v>
+        <v>895</v>
       </c>
       <c r="D1939" s="10" t="s">
-        <v>902</v>
+        <v>492</v>
       </c>
       <c r="E1939" s="11" t="s">
-        <v>683</v>
+        <v>757</v>
       </c>
       <c r="F1939" s="10" t="s">
-        <v>1007</v>
+        <v>1636</v>
       </c>
       <c r="G1939" s="11"/>
       <c r="H1939" s="12"/>
       <c r="I1939" s="13"/>
       <c r="J1939" s="13"/>
     </row>
-    <row r="1940" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1940" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1940" s="12">
-        <v>44055</v>
+        <v>44112</v>
       </c>
       <c r="B1940" s="9"/>
       <c r="C1940" s="14" t="s">
@@ -66921,7 +67046,7 @@
         <v>568</v>
       </c>
       <c r="F1940" s="10" t="s">
-        <v>900</v>
+        <v>2223</v>
       </c>
       <c r="G1940" s="11"/>
       <c r="H1940" s="12"/>
@@ -66930,172 +67055,192 @@
     </row>
     <row r="1941" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1941" s="12">
-        <v>44055</v>
+        <v>44088</v>
       </c>
       <c r="B1941" s="9"/>
       <c r="C1941" s="14" t="s">
-        <v>895</v>
+        <v>19</v>
       </c>
       <c r="D1941" s="10" t="s">
-        <v>492</v>
+        <v>902</v>
       </c>
       <c r="E1941" s="11" t="s">
-        <v>568</v>
+        <v>683</v>
       </c>
       <c r="F1941" s="10" t="s">
-        <v>897</v>
+        <v>1007</v>
       </c>
       <c r="G1941" s="11"/>
       <c r="H1941" s="12"/>
       <c r="I1941" s="13"/>
       <c r="J1941" s="13"/>
     </row>
-    <row r="1942" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="1942" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1942" s="12">
         <v>44055</v>
       </c>
       <c r="B1942" s="9"/>
       <c r="C1942" s="14" t="s">
-        <v>895</v>
+        <v>621</v>
       </c>
       <c r="D1942" s="10" t="s">
-        <v>492</v>
+        <v>6</v>
       </c>
       <c r="E1942" s="11" t="s">
         <v>568</v>
       </c>
       <c r="F1942" s="10" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="G1942" s="11"/>
       <c r="H1942" s="12"/>
       <c r="I1942" s="13"/>
       <c r="J1942" s="13"/>
     </row>
-    <row r="1943" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1943" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1943" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1943" s="9"/>
       <c r="C1943" s="14" t="s">
-        <v>468</v>
+        <v>895</v>
       </c>
       <c r="D1943" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E1943" s="11" t="s">
-        <v>683</v>
+        <v>568</v>
       </c>
       <c r="F1943" s="10" t="s">
-        <v>684</v>
-      </c>
-      <c r="G1943" s="11" t="s">
-        <v>1617</v>
-      </c>
+        <v>897</v>
+      </c>
+      <c r="G1943" s="11"/>
       <c r="H1943" s="12"/>
-      <c r="I1943" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I1943" s="13"/>
       <c r="J1943" s="13"/>
     </row>
-    <row r="1944" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="1944" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A1944" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B1944" s="9"/>
       <c r="C1944" s="14" t="s">
-        <v>468</v>
+        <v>895</v>
       </c>
       <c r="D1944" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E1944" s="11" t="s">
-        <v>683</v>
+        <v>568</v>
       </c>
       <c r="F1944" s="10" t="s">
-        <v>703</v>
-      </c>
-      <c r="G1944" s="11" t="s">
-        <v>685</v>
-      </c>
+        <v>898</v>
+      </c>
+      <c r="G1944" s="11"/>
       <c r="H1944" s="12"/>
-      <c r="I1944" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1944" s="13" t="s">
-        <v>1561</v>
-      </c>
-    </row>
-    <row r="1945" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I1944" s="13"/>
+      <c r="J1944" s="13"/>
+    </row>
+    <row r="1945" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A1945" s="12">
-        <v>43838</v>
+        <v>43949</v>
       </c>
       <c r="B1945" s="9"/>
       <c r="C1945" s="14" t="s">
-        <v>103</v>
+        <v>468</v>
       </c>
       <c r="D1945" s="10" t="s">
-        <v>460</v>
+        <v>89</v>
       </c>
       <c r="E1945" s="11" t="s">
-        <v>645</v>
+        <v>683</v>
       </c>
       <c r="F1945" s="10" t="s">
-        <v>479</v>
+        <v>684</v>
       </c>
       <c r="G1945" s="11" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="H1945" s="12"/>
-      <c r="I1945" s="13"/>
-      <c r="J1945" s="13" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="1946" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="I1945" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1945" s="13"/>
+    </row>
+    <row r="1946" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A1946" s="12">
-        <v>43762</v>
+        <v>43949</v>
       </c>
       <c r="B1946" s="9"/>
       <c r="C1946" s="14" t="s">
-        <v>446</v>
+        <v>468</v>
       </c>
       <c r="D1946" s="10" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="E1946" s="11" t="s">
-        <v>835</v>
+        <v>683</v>
       </c>
       <c r="F1946" s="10" t="s">
-        <v>447</v>
+        <v>703</v>
       </c>
       <c r="G1946" s="11" t="s">
-        <v>1607</v>
+        <v>685</v>
       </c>
       <c r="H1946" s="12"/>
-      <c r="I1946" s="13"/>
-      <c r="J1946" s="13"/>
-    </row>
-    <row r="1947" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1947" s="12"/>
+      <c r="I1946" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1946" s="13" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="1947" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1947" s="12">
+        <v>43838</v>
+      </c>
       <c r="B1947" s="9"/>
-      <c r="C1947" s="14"/>
-      <c r="D1947" s="10"/>
-      <c r="E1947" s="11"/>
-      <c r="F1947" s="10"/>
-      <c r="G1947" s="11"/>
+      <c r="C1947" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1947" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E1947" s="11" t="s">
+        <v>645</v>
+      </c>
+      <c r="F1947" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="G1947" s="11" t="s">
+        <v>1618</v>
+      </c>
       <c r="H1947" s="12"/>
       <c r="I1947" s="13"/>
-      <c r="J1947" s="13"/>
-    </row>
-    <row r="1948" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1948" s="12"/>
+      <c r="J1947" s="13" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1948" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1948" s="12">
+        <v>43762</v>
+      </c>
       <c r="B1948" s="9"/>
-      <c r="C1948" s="14"/>
-      <c r="D1948" s="10"/>
-      <c r="E1948" s="11"/>
-      <c r="F1948" s="10"/>
-      <c r="G1948" s="11"/>
+      <c r="C1948" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1948" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1948" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F1948" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1948" s="11" t="s">
+        <v>1607</v>
+      </c>
       <c r="H1948" s="12"/>
       <c r="I1948" s="13"/>
       <c r="J1948" s="13"/>
@@ -67147,6 +67292,30 @@
       <c r="H1952" s="12"/>
       <c r="I1952" s="13"/>
       <c r="J1952" s="13"/>
+    </row>
+    <row r="1953" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1953" s="12"/>
+      <c r="B1953" s="9"/>
+      <c r="C1953" s="14"/>
+      <c r="D1953" s="10"/>
+      <c r="E1953" s="11"/>
+      <c r="F1953" s="10"/>
+      <c r="G1953" s="11"/>
+      <c r="H1953" s="12"/>
+      <c r="I1953" s="13"/>
+      <c r="J1953" s="13"/>
+    </row>
+    <row r="1954" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1954" s="12"/>
+      <c r="B1954" s="9"/>
+      <c r="C1954" s="14"/>
+      <c r="D1954" s="10"/>
+      <c r="E1954" s="11"/>
+      <c r="F1954" s="10"/>
+      <c r="G1954" s="11"/>
+      <c r="H1954" s="12"/>
+      <c r="I1954" s="13"/>
+      <c r="J1954" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1881" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Alteração pasta de TMP para LOG
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7284A4EE-C9BE-4881-8685-83D363081C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1675EE9-0508-46AA-8D84-CF245796FA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14094" uniqueCount="2726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14241" uniqueCount="2757">
   <si>
     <t>Responsável</t>
   </si>
@@ -8628,6 +8628,101 @@
   <si>
     <t>LP 530-006
 LP-531-006</t>
+  </si>
+  <si>
+    <t>Permitir liberar pré-notas de todas as áreas</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>Administração</t>
+  </si>
+  <si>
+    <t>Solicitação de suporte para apuração de resultados</t>
+  </si>
+  <si>
+    <t>Envio de Passo a Passo para apuração de resultados.docx</t>
+  </si>
+  <si>
+    <t>Inclusão de item "Despesas de Campo" nas rentabilidades (eventos +703 e -706) - remover "SOL" do item "DESPESAS DIARIAS"</t>
+  </si>
+  <si>
+    <t>Configurar condição de pagamento 101 para não postegar pagamentos em feriados e finais de semana</t>
+  </si>
+  <si>
+    <t>Ponto de entrada A103CND2</t>
+  </si>
+  <si>
+    <t>Conta 12109001 não estava somando na conta analitica 12109</t>
+  </si>
+  <si>
+    <t>Corrigida a conta superior da conta 12109001 para 12109</t>
+  </si>
+  <si>
+    <t>Gentileza ajustar esse titulo para 02/05/2022, terminei colocando para 30/04 (sábado).</t>
+  </si>
+  <si>
+    <t>Corrigido via query</t>
+  </si>
+  <si>
+    <t>Ajustes EFD BK 03/2022 (Acerto de cadastros de clientes e outros que geram erros recorrentes de importação)</t>
+  </si>
+  <si>
+    <t>Geração da EFD em base testes, após todas as correções, alterando o vencimento e baixas dos titulos a receber para a data de emissão</t>
+  </si>
+  <si>
+    <t>Não estou conseguindo integrar o rubi pelo TOTVS. Toda vez que eu clico em importar aparece isso</t>
+  </si>
+  <si>
+    <t>Função mostraerro() substituida por GetAutoGRLog()
+Removido o campo CDOC do cabeçalho</t>
+  </si>
+  <si>
+    <t>Faturamento VOA SE SPE (Cadastro de clientes e correção de 7 pedidos)</t>
+  </si>
+  <si>
+    <t>Erro ao incluir NDC via Nova Medição</t>
+  </si>
+  <si>
+    <t>Corrigidos os programas CNTA121 e FIN040INC</t>
+  </si>
+  <si>
+    <t>Treinar Chris e João Golvea na nova medição</t>
+  </si>
+  <si>
+    <t>Encerrar contratos com status "Solicitação de Encerramento"</t>
+  </si>
+  <si>
+    <t>Acerto diversos pedidos Petrobras  - substituição de CNPJ</t>
+  </si>
+  <si>
+    <t>Dúvidas a respeito dos relatórios BKFINR12 e BKFINR30</t>
+  </si>
+  <si>
+    <t>Alterado CN9_FLGCAU para = '2'</t>
+  </si>
+  <si>
+    <t>Lincoln</t>
+  </si>
+  <si>
+    <t>Medição com problema: TES não informada</t>
+  </si>
+  <si>
+    <t>Havia um item no contrato 281000577 sem TES cadastrada</t>
+  </si>
+  <si>
+    <t>Não imprimir o D / C nos relatorios comparativos da contabilidade</t>
+  </si>
+  <si>
+    <t>BKGCT06 - 15</t>
+  </si>
+  <si>
+    <t>Precisamos que alterem o nome do CC 385000596,para inclusão do número do contrato , que só recebemos agora.  CC 385000596 DE: VOA SP CT XXX/XXXX-SERVIÇOS DE RAIO X 
+PARA: VOA SP Nº 0021/PS/SEDE/2022</t>
+  </si>
+  <si>
+    <t>03/05/2022 - 8:00 12:00 14:00 19:30</t>
   </si>
 </sst>
 </file>
@@ -9442,19 +9537,19 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J2024"/>
+  <dimension ref="A1:J2043"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1973" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1982" sqref="F1982"/>
+      <pane ySplit="1" topLeftCell="A1991" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2002" sqref="F2002"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="8" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="33" customWidth="1"/>
     <col min="6" max="6" width="72.7109375" style="34" customWidth="1"/>
     <col min="7" max="7" width="10.140625" style="8" bestFit="1" customWidth="1"/>
@@ -68795,21 +68890,33 @@
       <c r="A1981" s="12">
         <v>44677</v>
       </c>
-      <c r="B1981" s="12"/>
+      <c r="B1981" s="12">
+        <v>44678</v>
+      </c>
       <c r="C1981" s="14" t="s">
         <v>628</v>
       </c>
       <c r="D1981" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E1981" s="11"/>
+      <c r="E1981" s="11" t="s">
+        <v>835</v>
+      </c>
       <c r="F1981" s="10" t="s">
         <v>2723</v>
       </c>
-      <c r="G1981" s="11"/>
-      <c r="H1981" s="12"/>
-      <c r="I1981" s="13"/>
-      <c r="J1981" s="13"/>
+      <c r="G1981" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1981" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1981" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1981" s="13" t="s">
+        <v>1201</v>
+      </c>
     </row>
     <row r="1982" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1982" s="12">
@@ -68844,354 +68951,572 @@
       </c>
     </row>
     <row r="1983" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1983" s="12"/>
-      <c r="B1983" s="12"/>
-      <c r="C1983" s="14"/>
-      <c r="D1983" s="10"/>
-      <c r="E1983" s="11"/>
-      <c r="F1983" s="10"/>
-      <c r="G1983" s="11"/>
-      <c r="H1983" s="12"/>
-      <c r="I1983" s="13"/>
+      <c r="A1983" s="12">
+        <v>44678</v>
+      </c>
+      <c r="B1983" s="12">
+        <v>44678</v>
+      </c>
+      <c r="C1983" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1983" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1983" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F1983" s="10" t="s">
+        <v>2726</v>
+      </c>
+      <c r="G1983" s="11" t="s">
+        <v>1624</v>
+      </c>
+      <c r="H1983" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1983" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1983" s="13"/>
     </row>
     <row r="1984" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1984" s="12"/>
-      <c r="B1984" s="12"/>
-      <c r="C1984" s="14"/>
-      <c r="D1984" s="10"/>
-      <c r="E1984" s="11"/>
-      <c r="F1984" s="10"/>
-      <c r="G1984" s="11"/>
-      <c r="H1984" s="12"/>
-      <c r="I1984" s="13"/>
+      <c r="A1984" s="12">
+        <v>44678</v>
+      </c>
+      <c r="B1984" s="12">
+        <v>44678</v>
+      </c>
+      <c r="C1984" s="14" t="s">
+        <v>2727</v>
+      </c>
+      <c r="D1984" s="10" t="s">
+        <v>2728</v>
+      </c>
+      <c r="E1984" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F1984" s="10" t="s">
+        <v>2726</v>
+      </c>
+      <c r="G1984" s="11" t="s">
+        <v>1624</v>
+      </c>
+      <c r="H1984" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1984" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1984" s="13"/>
     </row>
-    <row r="1985" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1985" s="12"/>
-      <c r="B1985" s="12"/>
-      <c r="C1985" s="14"/>
-      <c r="D1985" s="10"/>
-      <c r="E1985" s="11"/>
-      <c r="F1985" s="10"/>
-      <c r="G1985" s="11"/>
-      <c r="H1985" s="12"/>
-      <c r="I1985" s="13"/>
+    <row r="1985" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1985" s="12">
+        <v>44679</v>
+      </c>
+      <c r="B1985" s="12">
+        <v>44679</v>
+      </c>
+      <c r="C1985" s="14" t="s">
+        <v>1969</v>
+      </c>
+      <c r="D1985" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1985" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F1985" s="10" t="s">
+        <v>2738</v>
+      </c>
+      <c r="G1985" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1985" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1985" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1985" s="13"/>
     </row>
-    <row r="1986" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1986" s="12"/>
-      <c r="B1986" s="12"/>
-      <c r="C1986" s="14"/>
-      <c r="D1986" s="10"/>
-      <c r="E1986" s="11"/>
-      <c r="F1986" s="10"/>
-      <c r="G1986" s="11"/>
-      <c r="H1986" s="12"/>
-      <c r="I1986" s="13"/>
+    <row r="1986" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1986" s="12">
+        <v>44679</v>
+      </c>
+      <c r="B1986" s="12">
+        <v>44679</v>
+      </c>
+      <c r="C1986" s="14" t="s">
+        <v>1969</v>
+      </c>
+      <c r="D1986" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1986" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F1986" s="10" t="s">
+        <v>2739</v>
+      </c>
+      <c r="G1986" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1986" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1986" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1986" s="13"/>
     </row>
     <row r="1987" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1987" s="12">
-        <v>44649</v>
-      </c>
-      <c r="B1987" s="12"/>
+        <v>44679</v>
+      </c>
+      <c r="B1987" s="12">
+        <v>44679</v>
+      </c>
       <c r="C1987" s="14" t="s">
-        <v>1969</v>
+        <v>2296</v>
       </c>
       <c r="D1987" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E1987" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F1987" s="10" t="s">
-        <v>2655</v>
-      </c>
-      <c r="G1987" s="11"/>
-      <c r="H1987" s="12"/>
+        <v>2729</v>
+      </c>
+      <c r="G1987" s="11" t="s">
+        <v>1599</v>
+      </c>
+      <c r="H1987" s="12" t="s">
+        <v>112</v>
+      </c>
       <c r="I1987" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J1987" s="13"/>
+      <c r="J1987" s="13" t="s">
+        <v>2730</v>
+      </c>
     </row>
     <row r="1988" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1988" s="12">
-        <v>44670</v>
-      </c>
-      <c r="B1988" s="12"/>
+        <v>44679</v>
+      </c>
+      <c r="B1988" s="12">
+        <v>44679</v>
+      </c>
       <c r="C1988" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D1988" s="10"/>
-      <c r="E1988" s="11"/>
+        <v>1969</v>
+      </c>
+      <c r="D1988" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1988" s="11" t="s">
+        <v>618</v>
+      </c>
       <c r="F1988" s="10" t="s">
-        <v>2695</v>
-      </c>
-      <c r="G1988" s="11"/>
-      <c r="H1988" s="12"/>
-      <c r="I1988" s="13"/>
-      <c r="J1988" s="13"/>
-    </row>
-    <row r="1989" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+        <v>2732</v>
+      </c>
+      <c r="G1988" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1988" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1988" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1988" s="13" t="s">
+        <v>2733</v>
+      </c>
+    </row>
+    <row r="1989" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1989" s="12">
-        <v>44670</v>
-      </c>
-      <c r="B1989" s="12"/>
+        <v>44680</v>
+      </c>
+      <c r="B1989" s="12">
+        <v>44680</v>
+      </c>
       <c r="C1989" s="14" t="s">
-        <v>66</v>
+        <v>2156</v>
       </c>
       <c r="D1989" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1989" s="11" t="s">
+        <v>667</v>
+      </c>
+      <c r="F1989" s="10" t="s">
+        <v>2734</v>
+      </c>
+      <c r="G1989" s="11" t="s">
+        <v>1624</v>
+      </c>
+      <c r="H1989" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1989" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1989" s="13" t="s">
+        <v>2735</v>
+      </c>
+    </row>
+    <row r="1990" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1990" s="12">
+        <v>44680</v>
+      </c>
+      <c r="B1990" s="12">
+        <v>44680</v>
+      </c>
+      <c r="C1990" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="D1990" s="10" t="s">
         <v>489</v>
       </c>
-      <c r="E1989" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F1989" s="10" t="s">
-        <v>2694</v>
-      </c>
-      <c r="G1989" s="11"/>
-      <c r="H1989" s="12"/>
-      <c r="I1989" s="13"/>
-      <c r="J1989" s="13"/>
-    </row>
-    <row r="1990" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1990" s="12">
-        <v>44670</v>
-      </c>
-      <c r="B1990" s="12"/>
-      <c r="C1990" s="14" t="s">
-        <v>573</v>
-      </c>
-      <c r="D1990" s="10" t="s">
-        <v>6</v>
-      </c>
       <c r="E1990" s="11" t="s">
-        <v>835</v>
+        <v>683</v>
       </c>
       <c r="F1990" s="10" t="s">
-        <v>2693</v>
-      </c>
-      <c r="G1990" s="11"/>
-      <c r="H1990" s="12"/>
-      <c r="I1990" s="13"/>
-      <c r="J1990" s="13"/>
-    </row>
-    <row r="1991" spans="1:10" ht="132" x14ac:dyDescent="0.2">
+        <v>2736</v>
+      </c>
+      <c r="G1990" s="11" t="s">
+        <v>1624</v>
+      </c>
+      <c r="H1990" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1990" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1990" s="13" t="s">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="1991" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A1991" s="12">
-        <v>44645</v>
-      </c>
-      <c r="B1991" s="12"/>
+        <v>44680</v>
+      </c>
+      <c r="B1991" s="12">
+        <v>44680</v>
+      </c>
       <c r="C1991" s="14" t="s">
-        <v>288</v>
+        <v>2156</v>
       </c>
       <c r="D1991" s="10" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="E1991" s="11" t="s">
-        <v>618</v>
+        <v>683</v>
       </c>
       <c r="F1991" s="10" t="s">
-        <v>2666</v>
-      </c>
-      <c r="G1991" s="11"/>
-      <c r="H1991" s="12"/>
-      <c r="I1991" s="13"/>
-      <c r="J1991" s="13"/>
+        <v>2740</v>
+      </c>
+      <c r="G1991" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1991" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1991" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1991" s="13" t="s">
+        <v>2741</v>
+      </c>
     </row>
     <row r="1992" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1992" s="12">
-        <v>44642</v>
-      </c>
-      <c r="B1992" s="12"/>
+        <v>44680</v>
+      </c>
+      <c r="B1992" s="12">
+        <v>44680</v>
+      </c>
       <c r="C1992" s="14" t="s">
-        <v>387</v>
+        <v>462</v>
       </c>
       <c r="D1992" s="10" t="s">
-        <v>492</v>
+        <v>107</v>
       </c>
       <c r="E1992" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F1992" s="10" t="s">
-        <v>2627</v>
-      </c>
-      <c r="G1992" s="11"/>
-      <c r="H1992" s="12"/>
-      <c r="I1992" s="13"/>
+        <v>2742</v>
+      </c>
+      <c r="G1992" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1992" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1992" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1992" s="13"/>
     </row>
     <row r="1993" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1993" s="12">
-        <v>44642</v>
-      </c>
-      <c r="B1993" s="12"/>
+        <v>44683</v>
+      </c>
+      <c r="B1993" s="12">
+        <v>44683</v>
+      </c>
       <c r="C1993" s="14" t="s">
-        <v>387</v>
+        <v>628</v>
       </c>
       <c r="D1993" s="10" t="s">
-        <v>492</v>
+        <v>17</v>
       </c>
       <c r="E1993" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F1993" s="10" t="s">
-        <v>2626</v>
-      </c>
-      <c r="G1993" s="11"/>
-      <c r="H1993" s="12"/>
-      <c r="I1993" s="13"/>
-      <c r="J1993" s="13"/>
+        <v>2743</v>
+      </c>
+      <c r="G1993" s="11" t="s">
+        <v>1602</v>
+      </c>
+      <c r="H1993" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1993" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1993" s="13" t="s">
+        <v>2744</v>
+      </c>
     </row>
     <row r="1994" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1994" s="12">
-        <v>44630</v>
-      </c>
-      <c r="B1994" s="12"/>
+        <v>44683</v>
+      </c>
+      <c r="B1994" s="12">
+        <v>44683</v>
+      </c>
       <c r="C1994" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1994" s="10"/>
-      <c r="E1994" s="11"/>
+        <v>895</v>
+      </c>
+      <c r="D1994" s="10" t="s">
+        <v>1851</v>
+      </c>
+      <c r="E1994" s="11" t="s">
+        <v>618</v>
+      </c>
       <c r="F1994" s="10" t="s">
-        <v>2603</v>
-      </c>
-      <c r="G1994" s="11"/>
-      <c r="H1994" s="12"/>
-      <c r="I1994" s="13"/>
+        <v>2745</v>
+      </c>
+      <c r="G1994" s="11" t="s">
+        <v>1602</v>
+      </c>
+      <c r="H1994" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1994" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1994" s="13"/>
     </row>
     <row r="1995" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1995" s="12">
-        <v>44614</v>
+        <v>44683</v>
       </c>
       <c r="B1995" s="12">
-        <v>44614</v>
+        <v>44683</v>
       </c>
       <c r="C1995" s="14" t="s">
-        <v>19</v>
+        <v>462</v>
       </c>
       <c r="D1995" s="10" t="s">
-        <v>492</v>
+        <v>107</v>
       </c>
       <c r="E1995" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F1995" s="10" t="s">
-        <v>2529</v>
-      </c>
-      <c r="G1995" s="11"/>
-      <c r="H1995" s="12"/>
-      <c r="I1995" s="13"/>
+        <v>2747</v>
+      </c>
+      <c r="G1995" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1995" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1995" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1995" s="13"/>
     </row>
     <row r="1996" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1996" s="12">
-        <v>44614</v>
-      </c>
-      <c r="B1996" s="12"/>
-      <c r="C1996" s="14" t="s">
-        <v>19</v>
+        <v>44684</v>
+      </c>
+      <c r="B1996" s="12">
+        <v>44684</v>
+      </c>
+      <c r="C1996" s="10" t="s">
+        <v>621</v>
       </c>
       <c r="D1996" s="10" t="s">
-        <v>492</v>
+        <v>6</v>
       </c>
       <c r="E1996" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F1996" s="10" t="s">
-        <v>2549</v>
-      </c>
-      <c r="G1996" s="11"/>
-      <c r="H1996" s="12"/>
-      <c r="I1996" s="13"/>
+        <v>2748</v>
+      </c>
+      <c r="G1996" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1996" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1996" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J1996" s="13"/>
     </row>
     <row r="1997" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1997" s="12">
-        <v>44616</v>
-      </c>
-      <c r="B1997" s="12"/>
+        <v>44678</v>
+      </c>
+      <c r="B1997" s="12">
+        <v>44684</v>
+      </c>
       <c r="C1997" s="14" t="s">
-        <v>2251</v>
+        <v>2682</v>
       </c>
       <c r="D1997" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E1997" s="11" t="s">
-        <v>618</v>
+        <v>835</v>
       </c>
       <c r="F1997" s="10" t="s">
-        <v>2556</v>
-      </c>
-      <c r="G1997" s="11"/>
-      <c r="H1997" s="12"/>
-      <c r="I1997" s="13"/>
-      <c r="J1997" s="13"/>
+        <v>2746</v>
+      </c>
+      <c r="G1997" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1997" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1997" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1997" s="13" t="s">
+        <v>2749</v>
+      </c>
     </row>
     <row r="1998" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1998" s="12">
-        <v>44623</v>
-      </c>
-      <c r="B1998" s="12"/>
-      <c r="C1998" s="14" t="s">
-        <v>535</v>
+        <v>44684</v>
+      </c>
+      <c r="B1998" s="12">
+        <v>44684</v>
+      </c>
+      <c r="C1998" s="10" t="s">
+        <v>2750</v>
       </c>
       <c r="D1998" s="10" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E1998" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F1998" s="10" t="s">
+        <v>2751</v>
+      </c>
+      <c r="G1998" s="11" t="s">
+        <v>1624</v>
+      </c>
+      <c r="H1998" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1998" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1998" s="13" t="s">
+        <v>2752</v>
+      </c>
+    </row>
+    <row r="1999" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1999" s="12">
+        <v>44670</v>
+      </c>
+      <c r="B1999" s="12">
+        <v>44684</v>
+      </c>
+      <c r="C1999" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D1999" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E1999" s="11" t="s">
         <v>835</v>
       </c>
-      <c r="F1998" s="10" t="s">
-        <v>2574</v>
-      </c>
-      <c r="G1998" s="11"/>
-      <c r="H1998" s="12"/>
-      <c r="I1998" s="13"/>
-      <c r="J1998" s="13"/>
-    </row>
-    <row r="1999" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A1999" s="12">
-        <v>44522</v>
-      </c>
-      <c r="B1999" s="12"/>
-      <c r="C1999" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1999" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1999" s="11" t="s">
+      <c r="F1999" s="10" t="s">
+        <v>2695</v>
+      </c>
+      <c r="G1999" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1999" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1999" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1999" s="13" t="s">
+        <v>2754</v>
+      </c>
+    </row>
+    <row r="2000" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2000" s="12">
+        <v>44684</v>
+      </c>
+      <c r="B2000" s="12">
+        <v>44684</v>
+      </c>
+      <c r="C2000" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2000" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2000" s="11" t="s">
         <v>568</v>
       </c>
-      <c r="F1999" s="10" t="s">
-        <v>2351</v>
-      </c>
-      <c r="G1999" s="11"/>
-      <c r="H1999" s="12"/>
-      <c r="I1999" s="13"/>
-      <c r="J1999" s="13"/>
-    </row>
-    <row r="2000" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2000" s="12"/>
-      <c r="B2000" s="12"/>
-      <c r="C2000" s="14"/>
-      <c r="D2000" s="10"/>
-      <c r="E2000" s="11"/>
-      <c r="F2000" s="10"/>
-      <c r="G2000" s="11"/>
-      <c r="H2000" s="12"/>
-      <c r="I2000" s="13"/>
+      <c r="F2000" s="10" t="s">
+        <v>2755</v>
+      </c>
+      <c r="G2000" s="11" t="s">
+        <v>1624</v>
+      </c>
+      <c r="H2000" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2000" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2000" s="13"/>
     </row>
     <row r="2001" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2001" s="12"/>
       <c r="B2001" s="12"/>
-      <c r="C2001" s="14"/>
+      <c r="C2001" s="10"/>
       <c r="D2001" s="10"/>
       <c r="E2001" s="11"/>
-      <c r="F2001" s="10"/>
+      <c r="F2001" s="30" t="s">
+        <v>2756</v>
+      </c>
       <c r="G2001" s="11"/>
       <c r="H2001" s="12"/>
       <c r="I2001" s="13"/>
@@ -69200,7 +69525,7 @@
     <row r="2002" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2002" s="12"/>
       <c r="B2002" s="12"/>
-      <c r="C2002" s="14"/>
+      <c r="C2002" s="10"/>
       <c r="D2002" s="10"/>
       <c r="E2002" s="11"/>
       <c r="F2002" s="10"/>
@@ -69223,7 +69548,7 @@
     </row>
     <row r="2004" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2004" s="12"/>
-      <c r="B2004" s="9"/>
+      <c r="B2004" s="12"/>
       <c r="C2004" s="14"/>
       <c r="D2004" s="10"/>
       <c r="E2004" s="11"/>
@@ -69234,121 +69559,133 @@
       <c r="J2004" s="13"/>
     </row>
     <row r="2005" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2005" s="1" t="s">
-        <v>1472</v>
-      </c>
-      <c r="B2005" s="2" t="s">
-        <v>1473</v>
-      </c>
-      <c r="C2005" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2005" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2005" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="F2005" s="4" t="s">
-        <v>1571</v>
-      </c>
-      <c r="G2005" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2005" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2005" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2005" s="36"/>
-    </row>
-    <row r="2006" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2006" s="12"/>
-      <c r="B2006" s="9"/>
-      <c r="C2006" s="14"/>
-      <c r="D2006" s="10"/>
-      <c r="E2006" s="11"/>
-      <c r="F2006" s="10"/>
+      <c r="A2005" s="12">
+        <v>44684</v>
+      </c>
+      <c r="B2005" s="12"/>
+      <c r="C2005" s="14" t="s">
+        <v>2156</v>
+      </c>
+      <c r="D2005" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2005" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2005" s="10" t="s">
+        <v>2753</v>
+      </c>
+      <c r="G2005" s="11"/>
+      <c r="H2005" s="12"/>
+      <c r="I2005" s="13"/>
+      <c r="J2005" s="13"/>
+    </row>
+    <row r="2006" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2006" s="12">
+        <v>44677</v>
+      </c>
+      <c r="B2006" s="12"/>
+      <c r="C2006" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2006" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2006" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2006" s="10" t="s">
+        <v>2731</v>
+      </c>
       <c r="G2006" s="11"/>
       <c r="H2006" s="12"/>
       <c r="I2006" s="13"/>
       <c r="J2006" s="13"/>
     </row>
     <row r="2007" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2007" s="12"/>
-      <c r="B2007" s="9"/>
-      <c r="C2007" s="14"/>
-      <c r="D2007" s="10"/>
-      <c r="E2007" s="11"/>
-      <c r="F2007" s="10"/>
+      <c r="A2007" s="12">
+        <v>44649</v>
+      </c>
+      <c r="B2007" s="12"/>
+      <c r="C2007" s="14" t="s">
+        <v>1969</v>
+      </c>
+      <c r="D2007" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2007" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2007" s="10" t="s">
+        <v>2655</v>
+      </c>
       <c r="G2007" s="11"/>
       <c r="H2007" s="12"/>
-      <c r="I2007" s="13"/>
+      <c r="I2007" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2007" s="13"/>
     </row>
-    <row r="2008" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="2008" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A2008" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2008" s="9"/>
+        <v>44670</v>
+      </c>
+      <c r="B2008" s="12"/>
       <c r="C2008" s="14" t="s">
-        <v>895</v>
+        <v>66</v>
       </c>
       <c r="D2008" s="10" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="E2008" s="11" t="s">
-        <v>757</v>
+        <v>835</v>
       </c>
       <c r="F2008" s="10" t="s">
-        <v>1637</v>
+        <v>2694</v>
       </c>
       <c r="G2008" s="11"/>
       <c r="H2008" s="12"/>
       <c r="I2008" s="13"/>
-      <c r="J2008" s="13" t="s">
-        <v>1660</v>
-      </c>
-    </row>
-    <row r="2009" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J2008" s="13"/>
+    </row>
+    <row r="2009" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2009" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2009" s="9"/>
+        <v>44670</v>
+      </c>
+      <c r="B2009" s="12"/>
       <c r="C2009" s="14" t="s">
-        <v>895</v>
+        <v>573</v>
       </c>
       <c r="D2009" s="10" t="s">
-        <v>492</v>
+        <v>6</v>
       </c>
       <c r="E2009" s="11" t="s">
-        <v>757</v>
+        <v>835</v>
       </c>
       <c r="F2009" s="10" t="s">
-        <v>1636</v>
+        <v>2693</v>
       </c>
       <c r="G2009" s="11"/>
       <c r="H2009" s="12"/>
       <c r="I2009" s="13"/>
       <c r="J2009" s="13"/>
     </row>
-    <row r="2010" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="2010" spans="1:10" ht="132" x14ac:dyDescent="0.2">
       <c r="A2010" s="12">
-        <v>44112</v>
-      </c>
-      <c r="B2010" s="9"/>
+        <v>44645</v>
+      </c>
+      <c r="B2010" s="12"/>
       <c r="C2010" s="14" t="s">
-        <v>621</v>
+        <v>288</v>
       </c>
       <c r="D2010" s="10" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E2010" s="11" t="s">
-        <v>568</v>
+        <v>618</v>
       </c>
       <c r="F2010" s="10" t="s">
-        <v>2223</v>
+        <v>2666</v>
       </c>
       <c r="G2010" s="11"/>
       <c r="H2010" s="12"/>
@@ -69357,20 +69694,20 @@
     </row>
     <row r="2011" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2011" s="12">
-        <v>44088</v>
-      </c>
-      <c r="B2011" s="9"/>
+        <v>44642</v>
+      </c>
+      <c r="B2011" s="12"/>
       <c r="C2011" s="14" t="s">
-        <v>19</v>
+        <v>387</v>
       </c>
       <c r="D2011" s="10" t="s">
-        <v>902</v>
+        <v>492</v>
       </c>
       <c r="E2011" s="11" t="s">
-        <v>683</v>
+        <v>835</v>
       </c>
       <c r="F2011" s="10" t="s">
-        <v>1007</v>
+        <v>2627</v>
       </c>
       <c r="G2011" s="11"/>
       <c r="H2011" s="12"/>
@@ -69379,20 +69716,20 @@
     </row>
     <row r="2012" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2012" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B2012" s="9"/>
+        <v>44642</v>
+      </c>
+      <c r="B2012" s="12"/>
       <c r="C2012" s="14" t="s">
-        <v>621</v>
+        <v>387</v>
       </c>
       <c r="D2012" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2012" s="11" t="s">
-        <v>568</v>
+        <v>835</v>
       </c>
       <c r="F2012" s="10" t="s">
-        <v>900</v>
+        <v>2626</v>
       </c>
       <c r="G2012" s="11"/>
       <c r="H2012" s="12"/>
@@ -69401,155 +69738,137 @@
     </row>
     <row r="2013" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2013" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B2013" s="9"/>
+        <v>44630</v>
+      </c>
+      <c r="B2013" s="12"/>
       <c r="C2013" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2013" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2013" s="11" t="s">
-        <v>568</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D2013" s="10"/>
+      <c r="E2013" s="11"/>
       <c r="F2013" s="10" t="s">
-        <v>897</v>
+        <v>2603</v>
       </c>
       <c r="G2013" s="11"/>
       <c r="H2013" s="12"/>
       <c r="I2013" s="13"/>
       <c r="J2013" s="13"/>
     </row>
-    <row r="2014" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="2014" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2014" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B2014" s="9"/>
+        <v>44614</v>
+      </c>
+      <c r="B2014" s="12">
+        <v>44614</v>
+      </c>
       <c r="C2014" s="14" t="s">
-        <v>895</v>
+        <v>19</v>
       </c>
       <c r="D2014" s="10" t="s">
         <v>492</v>
       </c>
       <c r="E2014" s="11" t="s">
-        <v>568</v>
+        <v>835</v>
       </c>
       <c r="F2014" s="10" t="s">
-        <v>898</v>
+        <v>2529</v>
       </c>
       <c r="G2014" s="11"/>
       <c r="H2014" s="12"/>
       <c r="I2014" s="13"/>
       <c r="J2014" s="13"/>
     </row>
-    <row r="2015" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="2015" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2015" s="12">
-        <v>43949</v>
-      </c>
-      <c r="B2015" s="9"/>
+        <v>44614</v>
+      </c>
+      <c r="B2015" s="12"/>
       <c r="C2015" s="14" t="s">
-        <v>468</v>
+        <v>19</v>
       </c>
       <c r="D2015" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E2015" s="11" t="s">
-        <v>683</v>
+        <v>835</v>
       </c>
       <c r="F2015" s="10" t="s">
-        <v>684</v>
-      </c>
-      <c r="G2015" s="11" t="s">
-        <v>1617</v>
-      </c>
+        <v>2549</v>
+      </c>
+      <c r="G2015" s="11"/>
       <c r="H2015" s="12"/>
-      <c r="I2015" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I2015" s="13"/>
       <c r="J2015" s="13"/>
     </row>
-    <row r="2016" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="2016" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2016" s="12">
-        <v>43949</v>
-      </c>
-      <c r="B2016" s="9"/>
+        <v>44616</v>
+      </c>
+      <c r="B2016" s="12"/>
       <c r="C2016" s="14" t="s">
-        <v>468</v>
+        <v>2251</v>
       </c>
       <c r="D2016" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E2016" s="11" t="s">
-        <v>683</v>
+        <v>618</v>
       </c>
       <c r="F2016" s="10" t="s">
-        <v>703</v>
-      </c>
-      <c r="G2016" s="11" t="s">
-        <v>685</v>
-      </c>
+        <v>2556</v>
+      </c>
+      <c r="G2016" s="11"/>
       <c r="H2016" s="12"/>
-      <c r="I2016" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J2016" s="13" t="s">
-        <v>1561</v>
-      </c>
-    </row>
-    <row r="2017" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I2016" s="13"/>
+      <c r="J2016" s="13"/>
+    </row>
+    <row r="2017" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2017" s="12">
-        <v>43838</v>
-      </c>
-      <c r="B2017" s="9"/>
+        <v>44623</v>
+      </c>
+      <c r="B2017" s="12"/>
       <c r="C2017" s="14" t="s">
-        <v>103</v>
+        <v>535</v>
       </c>
       <c r="D2017" s="10" t="s">
-        <v>460</v>
+        <v>6</v>
       </c>
       <c r="E2017" s="11" t="s">
-        <v>645</v>
+        <v>835</v>
       </c>
       <c r="F2017" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="G2017" s="11" t="s">
-        <v>1618</v>
-      </c>
+        <v>2574</v>
+      </c>
+      <c r="G2017" s="11"/>
       <c r="H2017" s="12"/>
       <c r="I2017" s="13"/>
-      <c r="J2017" s="13" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="2018" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J2017" s="13"/>
+    </row>
+    <row r="2018" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A2018" s="12">
-        <v>43762</v>
-      </c>
-      <c r="B2018" s="9"/>
+        <v>44522</v>
+      </c>
+      <c r="B2018" s="12"/>
       <c r="C2018" s="14" t="s">
-        <v>446</v>
+        <v>46</v>
       </c>
       <c r="D2018" s="10" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E2018" s="11" t="s">
-        <v>835</v>
+        <v>568</v>
       </c>
       <c r="F2018" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G2018" s="11" t="s">
-        <v>1607</v>
-      </c>
+        <v>2351</v>
+      </c>
+      <c r="G2018" s="11"/>
       <c r="H2018" s="12"/>
       <c r="I2018" s="13"/>
       <c r="J2018" s="13"/>
     </row>
     <row r="2019" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2019" s="12"/>
-      <c r="B2019" s="9"/>
+      <c r="B2019" s="12"/>
       <c r="C2019" s="14"/>
       <c r="D2019" s="10"/>
       <c r="E2019" s="11"/>
@@ -69561,7 +69880,7 @@
     </row>
     <row r="2020" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2020" s="12"/>
-      <c r="B2020" s="9"/>
+      <c r="B2020" s="12"/>
       <c r="C2020" s="14"/>
       <c r="D2020" s="10"/>
       <c r="E2020" s="11"/>
@@ -69573,7 +69892,7 @@
     </row>
     <row r="2021" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2021" s="12"/>
-      <c r="B2021" s="9"/>
+      <c r="B2021" s="12"/>
       <c r="C2021" s="14"/>
       <c r="D2021" s="10"/>
       <c r="E2021" s="11"/>
@@ -69585,7 +69904,7 @@
     </row>
     <row r="2022" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2022" s="12"/>
-      <c r="B2022" s="9"/>
+      <c r="B2022" s="12"/>
       <c r="C2022" s="14"/>
       <c r="D2022" s="10"/>
       <c r="E2022" s="11"/>
@@ -69608,16 +69927,390 @@
       <c r="J2023" s="13"/>
     </row>
     <row r="2024" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2024" s="12"/>
-      <c r="B2024" s="9"/>
-      <c r="C2024" s="14"/>
-      <c r="D2024" s="10"/>
-      <c r="E2024" s="11"/>
-      <c r="F2024" s="10"/>
-      <c r="G2024" s="11"/>
-      <c r="H2024" s="12"/>
-      <c r="I2024" s="13"/>
-      <c r="J2024" s="13"/>
+      <c r="A2024" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B2024" s="2" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C2024" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2024" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2024" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F2024" s="4" t="s">
+        <v>1571</v>
+      </c>
+      <c r="G2024" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2024" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2024" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2024" s="36"/>
+    </row>
+    <row r="2025" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2025" s="12"/>
+      <c r="B2025" s="9"/>
+      <c r="C2025" s="14"/>
+      <c r="D2025" s="10"/>
+      <c r="E2025" s="11"/>
+      <c r="F2025" s="10"/>
+      <c r="G2025" s="11"/>
+      <c r="H2025" s="12"/>
+      <c r="I2025" s="13"/>
+      <c r="J2025" s="13"/>
+    </row>
+    <row r="2026" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2026" s="12"/>
+      <c r="B2026" s="9"/>
+      <c r="C2026" s="14"/>
+      <c r="D2026" s="10"/>
+      <c r="E2026" s="11"/>
+      <c r="F2026" s="10"/>
+      <c r="G2026" s="11"/>
+      <c r="H2026" s="12"/>
+      <c r="I2026" s="13"/>
+      <c r="J2026" s="13"/>
+    </row>
+    <row r="2027" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+      <c r="A2027" s="12">
+        <v>44252</v>
+      </c>
+      <c r="B2027" s="9"/>
+      <c r="C2027" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2027" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2027" s="11" t="s">
+        <v>757</v>
+      </c>
+      <c r="F2027" s="10" t="s">
+        <v>1637</v>
+      </c>
+      <c r="G2027" s="11"/>
+      <c r="H2027" s="12"/>
+      <c r="I2027" s="13"/>
+      <c r="J2027" s="13" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="2028" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2028" s="12">
+        <v>44252</v>
+      </c>
+      <c r="B2028" s="9"/>
+      <c r="C2028" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2028" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2028" s="11" t="s">
+        <v>757</v>
+      </c>
+      <c r="F2028" s="10" t="s">
+        <v>1636</v>
+      </c>
+      <c r="G2028" s="11"/>
+      <c r="H2028" s="12"/>
+      <c r="I2028" s="13"/>
+      <c r="J2028" s="13"/>
+    </row>
+    <row r="2029" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2029" s="12">
+        <v>44112</v>
+      </c>
+      <c r="B2029" s="9"/>
+      <c r="C2029" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="D2029" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2029" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2029" s="10" t="s">
+        <v>2223</v>
+      </c>
+      <c r="G2029" s="11"/>
+      <c r="H2029" s="12"/>
+      <c r="I2029" s="13"/>
+      <c r="J2029" s="13"/>
+    </row>
+    <row r="2030" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2030" s="12">
+        <v>44088</v>
+      </c>
+      <c r="B2030" s="9"/>
+      <c r="C2030" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2030" s="10" t="s">
+        <v>902</v>
+      </c>
+      <c r="E2030" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2030" s="10" t="s">
+        <v>1007</v>
+      </c>
+      <c r="G2030" s="11"/>
+      <c r="H2030" s="12"/>
+      <c r="I2030" s="13"/>
+      <c r="J2030" s="13"/>
+    </row>
+    <row r="2031" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2031" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B2031" s="9"/>
+      <c r="C2031" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="D2031" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2031" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2031" s="10" t="s">
+        <v>900</v>
+      </c>
+      <c r="G2031" s="11"/>
+      <c r="H2031" s="12"/>
+      <c r="I2031" s="13"/>
+      <c r="J2031" s="13"/>
+    </row>
+    <row r="2032" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2032" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B2032" s="9"/>
+      <c r="C2032" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2032" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2032" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2032" s="10" t="s">
+        <v>897</v>
+      </c>
+      <c r="G2032" s="11"/>
+      <c r="H2032" s="12"/>
+      <c r="I2032" s="13"/>
+      <c r="J2032" s="13"/>
+    </row>
+    <row r="2033" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A2033" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B2033" s="9"/>
+      <c r="C2033" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2033" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2033" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2033" s="10" t="s">
+        <v>898</v>
+      </c>
+      <c r="G2033" s="11"/>
+      <c r="H2033" s="12"/>
+      <c r="I2033" s="13"/>
+      <c r="J2033" s="13"/>
+    </row>
+    <row r="2034" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2034" s="12">
+        <v>43949</v>
+      </c>
+      <c r="B2034" s="9"/>
+      <c r="C2034" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2034" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2034" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2034" s="10" t="s">
+        <v>684</v>
+      </c>
+      <c r="G2034" s="11" t="s">
+        <v>1617</v>
+      </c>
+      <c r="H2034" s="12"/>
+      <c r="I2034" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J2034" s="13"/>
+    </row>
+    <row r="2035" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2035" s="12">
+        <v>43949</v>
+      </c>
+      <c r="B2035" s="9"/>
+      <c r="C2035" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2035" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2035" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2035" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="G2035" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="H2035" s="12"/>
+      <c r="I2035" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J2035" s="13" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="2036" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2036" s="12">
+        <v>43838</v>
+      </c>
+      <c r="B2036" s="9"/>
+      <c r="C2036" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2036" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2036" s="11" t="s">
+        <v>645</v>
+      </c>
+      <c r="F2036" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="G2036" s="11" t="s">
+        <v>1618</v>
+      </c>
+      <c r="H2036" s="12"/>
+      <c r="I2036" s="13"/>
+      <c r="J2036" s="13" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="2037" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2037" s="12">
+        <v>43762</v>
+      </c>
+      <c r="B2037" s="9"/>
+      <c r="C2037" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D2037" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2037" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2037" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G2037" s="11" t="s">
+        <v>1607</v>
+      </c>
+      <c r="H2037" s="12"/>
+      <c r="I2037" s="13"/>
+      <c r="J2037" s="13"/>
+    </row>
+    <row r="2038" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2038" s="12"/>
+      <c r="B2038" s="9"/>
+      <c r="C2038" s="14"/>
+      <c r="D2038" s="10"/>
+      <c r="E2038" s="11"/>
+      <c r="F2038" s="10"/>
+      <c r="G2038" s="11"/>
+      <c r="H2038" s="12"/>
+      <c r="I2038" s="13"/>
+      <c r="J2038" s="13"/>
+    </row>
+    <row r="2039" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2039" s="12"/>
+      <c r="B2039" s="9"/>
+      <c r="C2039" s="14"/>
+      <c r="D2039" s="10"/>
+      <c r="E2039" s="11"/>
+      <c r="F2039" s="10"/>
+      <c r="G2039" s="11"/>
+      <c r="H2039" s="12"/>
+      <c r="I2039" s="13"/>
+      <c r="J2039" s="13"/>
+    </row>
+    <row r="2040" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2040" s="12"/>
+      <c r="B2040" s="9"/>
+      <c r="C2040" s="14"/>
+      <c r="D2040" s="10"/>
+      <c r="E2040" s="11"/>
+      <c r="F2040" s="10"/>
+      <c r="G2040" s="11"/>
+      <c r="H2040" s="12"/>
+      <c r="I2040" s="13"/>
+      <c r="J2040" s="13"/>
+    </row>
+    <row r="2041" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2041" s="12"/>
+      <c r="B2041" s="9"/>
+      <c r="C2041" s="14"/>
+      <c r="D2041" s="10"/>
+      <c r="E2041" s="11"/>
+      <c r="F2041" s="10"/>
+      <c r="G2041" s="11"/>
+      <c r="H2041" s="12"/>
+      <c r="I2041" s="13"/>
+      <c r="J2041" s="13"/>
+    </row>
+    <row r="2042" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2042" s="12"/>
+      <c r="B2042" s="9"/>
+      <c r="C2042" s="14"/>
+      <c r="D2042" s="10"/>
+      <c r="E2042" s="11"/>
+      <c r="F2042" s="10"/>
+      <c r="G2042" s="11"/>
+      <c r="H2042" s="12"/>
+      <c r="I2042" s="13"/>
+      <c r="J2042" s="13"/>
+    </row>
+    <row r="2043" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2043" s="12"/>
+      <c r="B2043" s="9"/>
+      <c r="C2043" s="14"/>
+      <c r="D2043" s="10"/>
+      <c r="E2043" s="11"/>
+      <c r="F2043" s="10"/>
+      <c r="G2043" s="11"/>
+      <c r="H2043" s="12"/>
+      <c r="I2043" s="13"/>
+      <c r="J2043" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1881" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Motivo na lib de Pre nota web
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B752147D-86EB-414C-A98A-DA16ABB41F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8554A8-4A32-4BB2-B2E3-5CE484E9B5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14581" uniqueCount="2841">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14609" uniqueCount="2845">
   <si>
     <t>Responsável</t>
   </si>
@@ -8831,9 +8831,6 @@
     <t>Excluir pré-nota 000056008</t>
   </si>
   <si>
-    <t>Rejeitar Pr-e-Nota</t>
-  </si>
-  <si>
     <t>Valor total</t>
   </si>
   <si>
@@ -8979,6 +8976,21 @@
   </si>
   <si>
     <t>Alterar data do cancelamento da baixa do titulo a receber 5712</t>
+  </si>
+  <si>
+    <t>Acertar competência do pedido 051388</t>
+  </si>
+  <si>
+    <t>Auxilio medição com duas NFs</t>
+  </si>
+  <si>
+    <t>Rejeitar Pré-Nota e abrir campo para digitação de motivo (Web)</t>
+  </si>
+  <si>
+    <t>Enviar e-mail ao Rejeitar Pré-Nota via Web</t>
+  </si>
+  <si>
+    <t>Suporte nova medição (campo obs)</t>
   </si>
 </sst>
 </file>
@@ -9793,11 +9805,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J2069"/>
+  <dimension ref="A1:J2077"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2023" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2030" sqref="A2030"/>
+      <pane ySplit="1" topLeftCell="A2026" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2034" sqref="A2034"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -70615,7 +70627,7 @@
         <v>683</v>
       </c>
       <c r="F2028" s="30" t="s">
-        <v>2839</v>
+        <v>2838</v>
       </c>
       <c r="G2028" s="11" t="s">
         <v>1624</v>
@@ -70645,7 +70657,7 @@
         <v>683</v>
       </c>
       <c r="F2029" s="30" t="s">
-        <v>2840</v>
+        <v>2839</v>
       </c>
       <c r="G2029" s="11" t="s">
         <v>1624</v>
@@ -70659,216 +70671,204 @@
       <c r="J2029" s="13"/>
     </row>
     <row r="2030" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2030" s="12"/>
-      <c r="B2030" s="12"/>
-      <c r="C2030" s="10"/>
-      <c r="D2030" s="10"/>
-      <c r="E2030" s="11"/>
-      <c r="F2030" s="30"/>
-      <c r="G2030" s="11"/>
-      <c r="H2030" s="12"/>
-      <c r="I2030" s="13"/>
+      <c r="A2030" s="12">
+        <v>44697</v>
+      </c>
+      <c r="B2030" s="12">
+        <v>44697</v>
+      </c>
+      <c r="C2030" s="10" t="s">
+        <v>2681</v>
+      </c>
+      <c r="D2030" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2030" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2030" s="30" t="s">
+        <v>2840</v>
+      </c>
+      <c r="G2030" s="11" t="s">
+        <v>1624</v>
+      </c>
+      <c r="H2030" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2030" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2030" s="13"/>
     </row>
     <row r="2031" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2031" s="12"/>
-      <c r="B2031" s="12"/>
-      <c r="C2031" s="10"/>
-      <c r="D2031" s="10"/>
-      <c r="E2031" s="11"/>
-      <c r="F2031" s="30"/>
-      <c r="G2031" s="11"/>
-      <c r="H2031" s="12"/>
-      <c r="I2031" s="13"/>
+      <c r="A2031" s="12">
+        <v>44697</v>
+      </c>
+      <c r="B2031" s="12">
+        <v>44697</v>
+      </c>
+      <c r="C2031" s="10" t="s">
+        <v>638</v>
+      </c>
+      <c r="D2031" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2031" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2031" s="30" t="s">
+        <v>2841</v>
+      </c>
+      <c r="G2031" s="11" t="s">
+        <v>1599</v>
+      </c>
+      <c r="H2031" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2031" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2031" s="13"/>
     </row>
     <row r="2032" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2032" s="12"/>
-      <c r="B2032" s="12"/>
-      <c r="C2032" s="10"/>
-      <c r="D2032" s="10"/>
-      <c r="E2032" s="11"/>
-      <c r="F2032" s="10"/>
-      <c r="G2032" s="11"/>
-      <c r="H2032" s="12"/>
-      <c r="I2032" s="13"/>
+      <c r="A2032" s="12">
+        <v>41041</v>
+      </c>
+      <c r="B2032" s="12">
+        <v>44697</v>
+      </c>
+      <c r="C2032" s="10" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2032" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2032" s="11" t="s">
+        <v>667</v>
+      </c>
+      <c r="F2032" s="10" t="s">
+        <v>2842</v>
+      </c>
+      <c r="G2032" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H2032" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2032" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2032" s="13"/>
     </row>
     <row r="2033" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2033" s="12">
-        <v>41041</v>
-      </c>
-      <c r="B2033" s="12"/>
-      <c r="C2033" s="14" t="s">
-        <v>706</v>
+        <v>44697</v>
+      </c>
+      <c r="B2033" s="12">
+        <v>44697</v>
+      </c>
+      <c r="C2033" s="10" t="s">
+        <v>638</v>
       </c>
       <c r="D2033" s="10" t="s">
-        <v>492</v>
+        <v>17</v>
       </c>
       <c r="E2033" s="11" t="s">
-        <v>667</v>
-      </c>
-      <c r="F2033" s="10" t="s">
-        <v>2791</v>
-      </c>
-      <c r="G2033" s="11"/>
-      <c r="H2033" s="12"/>
-      <c r="I2033" s="13"/>
+        <v>618</v>
+      </c>
+      <c r="F2033" s="30" t="s">
+        <v>2844</v>
+      </c>
+      <c r="G2033" s="11" t="s">
+        <v>1624</v>
+      </c>
+      <c r="H2033" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2033" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2033" s="13"/>
     </row>
     <row r="2034" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2034" s="12">
-        <v>44684</v>
-      </c>
+      <c r="A2034" s="12"/>
       <c r="B2034" s="12"/>
-      <c r="C2034" s="14" t="s">
-        <v>2156</v>
-      </c>
-      <c r="D2034" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2034" s="11" t="s">
-        <v>618</v>
-      </c>
-      <c r="F2034" s="10" t="s">
-        <v>2752</v>
-      </c>
+      <c r="C2034" s="10"/>
+      <c r="D2034" s="10"/>
+      <c r="E2034" s="11"/>
+      <c r="F2034" s="30"/>
       <c r="G2034" s="11"/>
       <c r="H2034" s="12"/>
       <c r="I2034" s="13"/>
       <c r="J2034" s="13"/>
     </row>
-    <row r="2035" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2035" s="12">
-        <v>44677</v>
-      </c>
+    <row r="2035" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2035" s="12"/>
       <c r="B2035" s="12"/>
-      <c r="C2035" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="D2035" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2035" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2035" s="10" t="s">
-        <v>2730</v>
-      </c>
+      <c r="C2035" s="10"/>
+      <c r="D2035" s="10"/>
+      <c r="E2035" s="11"/>
+      <c r="F2035" s="30"/>
       <c r="G2035" s="11"/>
       <c r="H2035" s="12"/>
       <c r="I2035" s="13"/>
       <c r="J2035" s="13"/>
     </row>
     <row r="2036" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2036" s="12">
-        <v>44649</v>
-      </c>
+      <c r="A2036" s="12"/>
       <c r="B2036" s="12"/>
-      <c r="C2036" s="14" t="s">
-        <v>1969</v>
-      </c>
-      <c r="D2036" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2036" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2036" s="10" t="s">
-        <v>2654</v>
-      </c>
+      <c r="C2036" s="10"/>
+      <c r="D2036" s="10"/>
+      <c r="E2036" s="11"/>
+      <c r="F2036" s="30"/>
       <c r="G2036" s="11"/>
       <c r="H2036" s="12"/>
-      <c r="I2036" s="13" t="s">
-        <v>13</v>
-      </c>
+      <c r="I2036" s="13"/>
       <c r="J2036" s="13"/>
     </row>
-    <row r="2037" spans="1:10" ht="132" x14ac:dyDescent="0.2">
-      <c r="A2037" s="12">
-        <v>44645</v>
-      </c>
+    <row r="2037" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2037" s="12"/>
       <c r="B2037" s="12"/>
-      <c r="C2037" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D2037" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2037" s="11" t="s">
-        <v>618</v>
-      </c>
-      <c r="F2037" s="10" t="s">
-        <v>2665</v>
-      </c>
+      <c r="C2037" s="10"/>
+      <c r="D2037" s="10"/>
+      <c r="E2037" s="11"/>
+      <c r="F2037" s="10"/>
       <c r="G2037" s="11"/>
       <c r="H2037" s="12"/>
       <c r="I2037" s="13"/>
       <c r="J2037" s="13"/>
     </row>
     <row r="2038" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2038" s="12">
-        <v>44642</v>
-      </c>
+      <c r="A2038" s="12"/>
       <c r="B2038" s="12"/>
-      <c r="C2038" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="D2038" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2038" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2038" s="10" t="s">
-        <v>2626</v>
-      </c>
+      <c r="C2038" s="10"/>
+      <c r="D2038" s="10"/>
+      <c r="E2038" s="11"/>
+      <c r="F2038" s="10"/>
       <c r="G2038" s="11"/>
       <c r="H2038" s="12"/>
       <c r="I2038" s="13"/>
       <c r="J2038" s="13"/>
     </row>
     <row r="2039" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2039" s="12">
-        <v>44642</v>
-      </c>
+      <c r="A2039" s="12"/>
       <c r="B2039" s="12"/>
-      <c r="C2039" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="D2039" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2039" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2039" s="10" t="s">
-        <v>2625</v>
-      </c>
+      <c r="C2039" s="10"/>
+      <c r="D2039" s="10"/>
+      <c r="E2039" s="11"/>
+      <c r="F2039" s="10"/>
       <c r="G2039" s="11"/>
       <c r="H2039" s="12"/>
       <c r="I2039" s="13"/>
       <c r="J2039" s="13"/>
     </row>
     <row r="2040" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2040" s="12">
-        <v>44614</v>
-      </c>
-      <c r="B2040" s="12">
-        <v>44614</v>
-      </c>
-      <c r="C2040" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2040" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2040" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2040" s="10" t="s">
-        <v>2529</v>
-      </c>
+      <c r="A2040" s="12"/>
+      <c r="B2040" s="12"/>
+      <c r="C2040" s="10"/>
+      <c r="D2040" s="10"/>
+      <c r="E2040" s="11"/>
+      <c r="F2040" s="30"/>
       <c r="G2040" s="11"/>
       <c r="H2040" s="12"/>
       <c r="I2040" s="13"/>
@@ -70876,20 +70876,20 @@
     </row>
     <row r="2041" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2041" s="12">
-        <v>44614</v>
+        <v>41041</v>
       </c>
       <c r="B2041" s="12"/>
-      <c r="C2041" s="14" t="s">
-        <v>19</v>
+      <c r="C2041" s="10" t="s">
+        <v>895</v>
       </c>
       <c r="D2041" s="10" t="s">
         <v>492</v>
       </c>
       <c r="E2041" s="11" t="s">
-        <v>835</v>
+        <v>667</v>
       </c>
       <c r="F2041" s="10" t="s">
-        <v>2549</v>
+        <v>2843</v>
       </c>
       <c r="G2041" s="11"/>
       <c r="H2041" s="12"/>
@@ -70898,515 +70898,695 @@
     </row>
     <row r="2042" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2042" s="12">
-        <v>44616</v>
+        <v>44684</v>
       </c>
       <c r="B2042" s="12"/>
       <c r="C2042" s="14" t="s">
-        <v>2251</v>
+        <v>2156</v>
       </c>
       <c r="D2042" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E2042" s="11" t="s">
         <v>618</v>
       </c>
       <c r="F2042" s="10" t="s">
-        <v>2556</v>
+        <v>2752</v>
       </c>
       <c r="G2042" s="11"/>
       <c r="H2042" s="12"/>
       <c r="I2042" s="13"/>
       <c r="J2042" s="13"/>
     </row>
-    <row r="2043" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2043" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2043" s="12">
-        <v>44623</v>
+        <v>44677</v>
       </c>
       <c r="B2043" s="12"/>
       <c r="C2043" s="14" t="s">
-        <v>535</v>
+        <v>387</v>
       </c>
       <c r="D2043" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2043" s="11" t="s">
         <v>835</v>
       </c>
       <c r="F2043" s="10" t="s">
-        <v>2574</v>
+        <v>2730</v>
       </c>
       <c r="G2043" s="11"/>
       <c r="H2043" s="12"/>
       <c r="I2043" s="13"/>
       <c r="J2043" s="13"/>
     </row>
-    <row r="2044" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="2044" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2044" s="12">
-        <v>44522</v>
+        <v>44649</v>
       </c>
       <c r="B2044" s="12"/>
       <c r="C2044" s="14" t="s">
-        <v>46</v>
+        <v>1969</v>
       </c>
       <c r="D2044" s="10" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="E2044" s="11" t="s">
-        <v>568</v>
+        <v>835</v>
       </c>
       <c r="F2044" s="10" t="s">
-        <v>2351</v>
+        <v>2654</v>
       </c>
       <c r="G2044" s="11"/>
       <c r="H2044" s="12"/>
-      <c r="I2044" s="13"/>
+      <c r="I2044" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2044" s="13"/>
     </row>
-    <row r="2045" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2045" s="12"/>
+    <row r="2045" spans="1:10" ht="132" x14ac:dyDescent="0.2">
+      <c r="A2045" s="12">
+        <v>44645</v>
+      </c>
       <c r="B2045" s="12"/>
-      <c r="C2045" s="14"/>
-      <c r="D2045" s="10"/>
-      <c r="E2045" s="11"/>
-      <c r="F2045" s="10"/>
+      <c r="C2045" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D2045" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2045" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2045" s="10" t="s">
+        <v>2665</v>
+      </c>
       <c r="G2045" s="11"/>
       <c r="H2045" s="12"/>
       <c r="I2045" s="13"/>
       <c r="J2045" s="13"/>
     </row>
     <row r="2046" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2046" s="12"/>
+      <c r="A2046" s="12">
+        <v>44642</v>
+      </c>
       <c r="B2046" s="12"/>
-      <c r="C2046" s="14"/>
-      <c r="D2046" s="10"/>
-      <c r="E2046" s="11"/>
-      <c r="F2046" s="10"/>
+      <c r="C2046" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2046" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2046" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2046" s="10" t="s">
+        <v>2626</v>
+      </c>
       <c r="G2046" s="11"/>
       <c r="H2046" s="12"/>
       <c r="I2046" s="13"/>
       <c r="J2046" s="13"/>
     </row>
     <row r="2047" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2047" s="12"/>
+      <c r="A2047" s="12">
+        <v>44642</v>
+      </c>
       <c r="B2047" s="12"/>
-      <c r="C2047" s="14"/>
-      <c r="D2047" s="10"/>
-      <c r="E2047" s="11"/>
-      <c r="F2047" s="10"/>
+      <c r="C2047" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2047" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2047" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2047" s="10" t="s">
+        <v>2625</v>
+      </c>
       <c r="G2047" s="11"/>
       <c r="H2047" s="12"/>
       <c r="I2047" s="13"/>
       <c r="J2047" s="13"/>
     </row>
     <row r="2048" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2048" s="12"/>
-      <c r="B2048" s="12"/>
-      <c r="C2048" s="14"/>
-      <c r="D2048" s="10"/>
-      <c r="E2048" s="11"/>
-      <c r="F2048" s="10"/>
+      <c r="A2048" s="12">
+        <v>44614</v>
+      </c>
+      <c r="B2048" s="12">
+        <v>44614</v>
+      </c>
+      <c r="C2048" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2048" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2048" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2048" s="10" t="s">
+        <v>2529</v>
+      </c>
       <c r="G2048" s="11"/>
       <c r="H2048" s="12"/>
       <c r="I2048" s="13"/>
       <c r="J2048" s="13"/>
     </row>
     <row r="2049" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2049" s="12"/>
-      <c r="B2049" s="9"/>
-      <c r="C2049" s="14"/>
-      <c r="D2049" s="10"/>
-      <c r="E2049" s="11"/>
-      <c r="F2049" s="10"/>
+      <c r="A2049" s="12">
+        <v>44614</v>
+      </c>
+      <c r="B2049" s="12"/>
+      <c r="C2049" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2049" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2049" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2049" s="10" t="s">
+        <v>2549</v>
+      </c>
       <c r="G2049" s="11"/>
       <c r="H2049" s="12"/>
       <c r="I2049" s="13"/>
       <c r="J2049" s="13"/>
     </row>
     <row r="2050" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2050" s="1" t="s">
-        <v>1472</v>
-      </c>
-      <c r="B2050" s="2" t="s">
-        <v>1473</v>
-      </c>
-      <c r="C2050" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2050" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2050" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="F2050" s="4" t="s">
-        <v>1571</v>
-      </c>
-      <c r="G2050" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2050" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2050" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2050" s="36"/>
+      <c r="A2050" s="12">
+        <v>44616</v>
+      </c>
+      <c r="B2050" s="12"/>
+      <c r="C2050" s="14" t="s">
+        <v>2251</v>
+      </c>
+      <c r="D2050" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2050" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2050" s="10" t="s">
+        <v>2556</v>
+      </c>
+      <c r="G2050" s="11"/>
+      <c r="H2050" s="12"/>
+      <c r="I2050" s="13"/>
+      <c r="J2050" s="13"/>
     </row>
     <row r="2051" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2051" s="12"/>
-      <c r="B2051" s="9"/>
-      <c r="C2051" s="14"/>
-      <c r="D2051" s="10"/>
-      <c r="E2051" s="11"/>
-      <c r="F2051" s="10"/>
+      <c r="A2051" s="12">
+        <v>44623</v>
+      </c>
+      <c r="B2051" s="12"/>
+      <c r="C2051" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="D2051" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2051" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2051" s="10" t="s">
+        <v>2574</v>
+      </c>
       <c r="G2051" s="11"/>
       <c r="H2051" s="12"/>
       <c r="I2051" s="13"/>
       <c r="J2051" s="13"/>
     </row>
-    <row r="2052" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2052" s="12"/>
-      <c r="B2052" s="9"/>
-      <c r="C2052" s="14"/>
-      <c r="D2052" s="10"/>
-      <c r="E2052" s="11"/>
-      <c r="F2052" s="10"/>
+    <row r="2052" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2052" s="12">
+        <v>44522</v>
+      </c>
+      <c r="B2052" s="12"/>
+      <c r="C2052" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2052" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2052" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2052" s="10" t="s">
+        <v>2351</v>
+      </c>
       <c r="G2052" s="11"/>
       <c r="H2052" s="12"/>
       <c r="I2052" s="13"/>
       <c r="J2052" s="13"/>
     </row>
-    <row r="2053" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A2053" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2053" s="9"/>
-      <c r="C2053" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2053" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2053" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2053" s="10" t="s">
-        <v>1637</v>
-      </c>
+    <row r="2053" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2053" s="12"/>
+      <c r="B2053" s="12"/>
+      <c r="C2053" s="14"/>
+      <c r="D2053" s="10"/>
+      <c r="E2053" s="11"/>
+      <c r="F2053" s="10"/>
       <c r="G2053" s="11"/>
       <c r="H2053" s="12"/>
       <c r="I2053" s="13"/>
-      <c r="J2053" s="13" t="s">
-        <v>1660</v>
-      </c>
-    </row>
-    <row r="2054" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A2054" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2054" s="9"/>
-      <c r="C2054" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2054" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2054" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2054" s="10" t="s">
-        <v>1636</v>
-      </c>
+      <c r="J2053" s="13"/>
+    </row>
+    <row r="2054" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2054" s="12"/>
+      <c r="B2054" s="12"/>
+      <c r="C2054" s="14"/>
+      <c r="D2054" s="10"/>
+      <c r="E2054" s="11"/>
+      <c r="F2054" s="10"/>
       <c r="G2054" s="11"/>
       <c r="H2054" s="12"/>
       <c r="I2054" s="13"/>
       <c r="J2054" s="13"/>
     </row>
-    <row r="2055" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2055" s="12">
-        <v>44112</v>
-      </c>
-      <c r="B2055" s="9"/>
-      <c r="C2055" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D2055" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2055" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2055" s="10" t="s">
-        <v>2223</v>
-      </c>
+    <row r="2055" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2055" s="12"/>
+      <c r="B2055" s="12"/>
+      <c r="C2055" s="14"/>
+      <c r="D2055" s="10"/>
+      <c r="E2055" s="11"/>
+      <c r="F2055" s="10"/>
       <c r="G2055" s="11"/>
       <c r="H2055" s="12"/>
       <c r="I2055" s="13"/>
       <c r="J2055" s="13"/>
     </row>
     <row r="2056" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2056" s="12">
-        <v>44088</v>
-      </c>
-      <c r="B2056" s="9"/>
-      <c r="C2056" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2056" s="10" t="s">
-        <v>902</v>
-      </c>
-      <c r="E2056" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="F2056" s="10" t="s">
-        <v>1007</v>
-      </c>
+      <c r="A2056" s="12"/>
+      <c r="B2056" s="12"/>
+      <c r="C2056" s="14"/>
+      <c r="D2056" s="10"/>
+      <c r="E2056" s="11"/>
+      <c r="F2056" s="10"/>
       <c r="G2056" s="11"/>
       <c r="H2056" s="12"/>
       <c r="I2056" s="13"/>
       <c r="J2056" s="13"/>
     </row>
     <row r="2057" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2057" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A2057" s="12"/>
       <c r="B2057" s="9"/>
-      <c r="C2057" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D2057" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2057" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2057" s="10" t="s">
-        <v>900</v>
-      </c>
+      <c r="C2057" s="14"/>
+      <c r="D2057" s="10"/>
+      <c r="E2057" s="11"/>
+      <c r="F2057" s="10"/>
       <c r="G2057" s="11"/>
       <c r="H2057" s="12"/>
       <c r="I2057" s="13"/>
       <c r="J2057" s="13"/>
     </row>
     <row r="2058" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2058" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B2058" s="9"/>
-      <c r="C2058" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2058" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2058" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2058" s="10" t="s">
-        <v>897</v>
-      </c>
-      <c r="G2058" s="11"/>
-      <c r="H2058" s="12"/>
-      <c r="I2058" s="13"/>
-      <c r="J2058" s="13"/>
-    </row>
-    <row r="2059" spans="1:10" ht="108" x14ac:dyDescent="0.2">
-      <c r="A2059" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A2058" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B2058" s="2" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C2058" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2058" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2058" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F2058" s="4" t="s">
+        <v>1571</v>
+      </c>
+      <c r="G2058" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2058" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2058" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2058" s="36"/>
+    </row>
+    <row r="2059" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2059" s="12"/>
       <c r="B2059" s="9"/>
-      <c r="C2059" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2059" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2059" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2059" s="10" t="s">
-        <v>898</v>
-      </c>
+      <c r="C2059" s="14"/>
+      <c r="D2059" s="10"/>
+      <c r="E2059" s="11"/>
+      <c r="F2059" s="10"/>
       <c r="G2059" s="11"/>
       <c r="H2059" s="12"/>
       <c r="I2059" s="13"/>
       <c r="J2059" s="13"/>
     </row>
-    <row r="2060" spans="1:10" ht="168" x14ac:dyDescent="0.2">
-      <c r="A2060" s="12">
-        <v>43949</v>
-      </c>
+    <row r="2060" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2060" s="12"/>
       <c r="B2060" s="9"/>
-      <c r="C2060" s="14" t="s">
-        <v>468</v>
-      </c>
-      <c r="D2060" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2060" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="F2060" s="10" t="s">
-        <v>684</v>
-      </c>
-      <c r="G2060" s="11" t="s">
-        <v>1617</v>
-      </c>
+      <c r="C2060" s="14"/>
+      <c r="D2060" s="10"/>
+      <c r="E2060" s="11"/>
+      <c r="F2060" s="10"/>
+      <c r="G2060" s="11"/>
       <c r="H2060" s="12"/>
-      <c r="I2060" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I2060" s="13"/>
       <c r="J2060" s="13"/>
     </row>
-    <row r="2061" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="2061" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A2061" s="12">
-        <v>43949</v>
+        <v>44252</v>
       </c>
       <c r="B2061" s="9"/>
       <c r="C2061" s="14" t="s">
-        <v>468</v>
+        <v>895</v>
       </c>
       <c r="D2061" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E2061" s="11" t="s">
-        <v>683</v>
+        <v>757</v>
       </c>
       <c r="F2061" s="10" t="s">
-        <v>703</v>
-      </c>
-      <c r="G2061" s="11" t="s">
-        <v>685</v>
-      </c>
+        <v>1637</v>
+      </c>
+      <c r="G2061" s="11"/>
       <c r="H2061" s="12"/>
-      <c r="I2061" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I2061" s="13"/>
       <c r="J2061" s="13" t="s">
-        <v>1561</v>
-      </c>
-    </row>
-    <row r="2062" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="2062" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A2062" s="12">
-        <v>43838</v>
+        <v>44252</v>
       </c>
       <c r="B2062" s="9"/>
       <c r="C2062" s="14" t="s">
-        <v>103</v>
+        <v>895</v>
       </c>
       <c r="D2062" s="10" t="s">
-        <v>460</v>
+        <v>492</v>
       </c>
       <c r="E2062" s="11" t="s">
-        <v>645</v>
+        <v>757</v>
       </c>
       <c r="F2062" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="G2062" s="11" t="s">
-        <v>1618</v>
-      </c>
+        <v>1636</v>
+      </c>
+      <c r="G2062" s="11"/>
       <c r="H2062" s="12"/>
       <c r="I2062" s="13"/>
-      <c r="J2062" s="13" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="2063" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J2062" s="13"/>
+    </row>
+    <row r="2063" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2063" s="12">
-        <v>43762</v>
+        <v>44112</v>
       </c>
       <c r="B2063" s="9"/>
       <c r="C2063" s="14" t="s">
-        <v>446</v>
+        <v>621</v>
       </c>
       <c r="D2063" s="10" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E2063" s="11" t="s">
-        <v>835</v>
+        <v>568</v>
       </c>
       <c r="F2063" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G2063" s="11" t="s">
-        <v>1607</v>
-      </c>
+        <v>2223</v>
+      </c>
+      <c r="G2063" s="11"/>
       <c r="H2063" s="12"/>
       <c r="I2063" s="13"/>
       <c r="J2063" s="13"/>
     </row>
     <row r="2064" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2064" s="12"/>
+      <c r="A2064" s="12">
+        <v>44088</v>
+      </c>
       <c r="B2064" s="9"/>
-      <c r="C2064" s="14"/>
-      <c r="D2064" s="10"/>
-      <c r="E2064" s="11"/>
-      <c r="F2064" s="10"/>
+      <c r="C2064" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2064" s="10" t="s">
+        <v>902</v>
+      </c>
+      <c r="E2064" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2064" s="10" t="s">
+        <v>1007</v>
+      </c>
       <c r="G2064" s="11"/>
       <c r="H2064" s="12"/>
       <c r="I2064" s="13"/>
       <c r="J2064" s="13"/>
     </row>
     <row r="2065" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2065" s="12"/>
+      <c r="A2065" s="12">
+        <v>44055</v>
+      </c>
       <c r="B2065" s="9"/>
-      <c r="C2065" s="14"/>
-      <c r="D2065" s="10"/>
-      <c r="E2065" s="11"/>
-      <c r="F2065" s="10"/>
+      <c r="C2065" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="D2065" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2065" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2065" s="10" t="s">
+        <v>900</v>
+      </c>
       <c r="G2065" s="11"/>
       <c r="H2065" s="12"/>
       <c r="I2065" s="13"/>
       <c r="J2065" s="13"/>
     </row>
     <row r="2066" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2066" s="12"/>
+      <c r="A2066" s="12">
+        <v>44055</v>
+      </c>
       <c r="B2066" s="9"/>
-      <c r="C2066" s="14"/>
-      <c r="D2066" s="10"/>
-      <c r="E2066" s="11"/>
-      <c r="F2066" s="10"/>
+      <c r="C2066" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2066" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2066" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2066" s="10" t="s">
+        <v>897</v>
+      </c>
       <c r="G2066" s="11"/>
       <c r="H2066" s="12"/>
       <c r="I2066" s="13"/>
       <c r="J2066" s="13"/>
     </row>
-    <row r="2067" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2067" s="12"/>
+    <row r="2067" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A2067" s="12">
+        <v>44055</v>
+      </c>
       <c r="B2067" s="9"/>
-      <c r="C2067" s="14"/>
-      <c r="D2067" s="10"/>
-      <c r="E2067" s="11"/>
-      <c r="F2067" s="10"/>
+      <c r="C2067" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2067" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2067" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2067" s="10" t="s">
+        <v>898</v>
+      </c>
       <c r="G2067" s="11"/>
       <c r="H2067" s="12"/>
       <c r="I2067" s="13"/>
       <c r="J2067" s="13"/>
     </row>
-    <row r="2068" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2068" s="12"/>
+    <row r="2068" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2068" s="12">
+        <v>43949</v>
+      </c>
       <c r="B2068" s="9"/>
-      <c r="C2068" s="14"/>
-      <c r="D2068" s="10"/>
-      <c r="E2068" s="11"/>
-      <c r="F2068" s="10"/>
-      <c r="G2068" s="11"/>
+      <c r="C2068" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2068" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2068" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2068" s="10" t="s">
+        <v>684</v>
+      </c>
+      <c r="G2068" s="11" t="s">
+        <v>1617</v>
+      </c>
       <c r="H2068" s="12"/>
-      <c r="I2068" s="13"/>
+      <c r="I2068" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J2068" s="13"/>
     </row>
-    <row r="2069" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2069" s="12"/>
+    <row r="2069" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2069" s="12">
+        <v>43949</v>
+      </c>
       <c r="B2069" s="9"/>
-      <c r="C2069" s="14"/>
-      <c r="D2069" s="10"/>
-      <c r="E2069" s="11"/>
-      <c r="F2069" s="10"/>
-      <c r="G2069" s="11"/>
+      <c r="C2069" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2069" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2069" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2069" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="G2069" s="11" t="s">
+        <v>685</v>
+      </c>
       <c r="H2069" s="12"/>
-      <c r="I2069" s="13"/>
-      <c r="J2069" s="13"/>
+      <c r="I2069" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J2069" s="13" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="2070" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2070" s="12">
+        <v>43838</v>
+      </c>
+      <c r="B2070" s="9"/>
+      <c r="C2070" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2070" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2070" s="11" t="s">
+        <v>645</v>
+      </c>
+      <c r="F2070" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="G2070" s="11" t="s">
+        <v>1618</v>
+      </c>
+      <c r="H2070" s="12"/>
+      <c r="I2070" s="13"/>
+      <c r="J2070" s="13" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="2071" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2071" s="12">
+        <v>43762</v>
+      </c>
+      <c r="B2071" s="9"/>
+      <c r="C2071" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D2071" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2071" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2071" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G2071" s="11" t="s">
+        <v>1607</v>
+      </c>
+      <c r="H2071" s="12"/>
+      <c r="I2071" s="13"/>
+      <c r="J2071" s="13"/>
+    </row>
+    <row r="2072" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2072" s="12"/>
+      <c r="B2072" s="9"/>
+      <c r="C2072" s="14"/>
+      <c r="D2072" s="10"/>
+      <c r="E2072" s="11"/>
+      <c r="F2072" s="10"/>
+      <c r="G2072" s="11"/>
+      <c r="H2072" s="12"/>
+      <c r="I2072" s="13"/>
+      <c r="J2072" s="13"/>
+    </row>
+    <row r="2073" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2073" s="12"/>
+      <c r="B2073" s="9"/>
+      <c r="C2073" s="14"/>
+      <c r="D2073" s="10"/>
+      <c r="E2073" s="11"/>
+      <c r="F2073" s="10"/>
+      <c r="G2073" s="11"/>
+      <c r="H2073" s="12"/>
+      <c r="I2073" s="13"/>
+      <c r="J2073" s="13"/>
+    </row>
+    <row r="2074" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2074" s="12"/>
+      <c r="B2074" s="9"/>
+      <c r="C2074" s="14"/>
+      <c r="D2074" s="10"/>
+      <c r="E2074" s="11"/>
+      <c r="F2074" s="10"/>
+      <c r="G2074" s="11"/>
+      <c r="H2074" s="12"/>
+      <c r="I2074" s="13"/>
+      <c r="J2074" s="13"/>
+    </row>
+    <row r="2075" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2075" s="12"/>
+      <c r="B2075" s="9"/>
+      <c r="C2075" s="14"/>
+      <c r="D2075" s="10"/>
+      <c r="E2075" s="11"/>
+      <c r="F2075" s="10"/>
+      <c r="G2075" s="11"/>
+      <c r="H2075" s="12"/>
+      <c r="I2075" s="13"/>
+      <c r="J2075" s="13"/>
+    </row>
+    <row r="2076" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2076" s="12"/>
+      <c r="B2076" s="9"/>
+      <c r="C2076" s="14"/>
+      <c r="D2076" s="10"/>
+      <c r="E2076" s="11"/>
+      <c r="F2076" s="10"/>
+      <c r="G2076" s="11"/>
+      <c r="H2076" s="12"/>
+      <c r="I2076" s="13"/>
+      <c r="J2076" s="13"/>
+    </row>
+    <row r="2077" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2077" s="12"/>
+      <c r="B2077" s="9"/>
+      <c r="C2077" s="14"/>
+      <c r="D2077" s="10"/>
+      <c r="E2077" s="11"/>
+      <c r="F2077" s="10"/>
+      <c r="G2077" s="11"/>
+      <c r="H2077" s="12"/>
+      <c r="I2077" s="13"/>
+      <c r="J2077" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1881" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -71441,129 +71621,129 @@
       <c r="H3" s="43"/>
       <c r="I3" s="43"/>
       <c r="L3" t="s">
+        <v>2799</v>
+      </c>
+      <c r="M3" t="s">
         <v>2800</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>2801</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>2802</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>2803</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>2804</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>2805</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>2806</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>2807</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
+        <v>2799</v>
+      </c>
+      <c r="V3" t="s">
+        <v>2800</v>
+      </c>
+      <c r="W3" t="s">
         <v>2808</v>
       </c>
-      <c r="U3" t="s">
-        <v>2800</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="X3" t="s">
+        <v>2809</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>2810</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>2802</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>2811</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>2812</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>2813</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>2814</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>2815</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>2816</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>2818</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>2819</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>2834</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>2820</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>2821</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>2822</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>2823</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>2824</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>2825</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>2826</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>2827</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>2828</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>2829</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>2830</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>2831</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>2832</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>2833</v>
+      </c>
+      <c r="AY3" t="s">
         <v>2801</v>
-      </c>
-      <c r="W3" t="s">
-        <v>2809</v>
-      </c>
-      <c r="X3" t="s">
-        <v>2810</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>2811</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>2803</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>2812</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>2813</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>2814</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>2815</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>2816</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>2817</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>2818</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>2819</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>2820</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>2835</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>2821</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>2822</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>2823</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>2824</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>2825</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>2826</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>2827</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>2828</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>2829</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>2830</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>2831</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>2832</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>2833</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>2834</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>2802</v>
       </c>
     </row>
     <row r="4" spans="5:51" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
-        <v>2792</v>
+        <v>2791</v>
       </c>
       <c r="F4">
         <v>6000</v>
@@ -71571,7 +71751,7 @@
       <c r="G4" s="43"/>
       <c r="H4" s="43"/>
       <c r="I4" s="43" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="J4">
         <v>1500</v>
@@ -71625,7 +71805,7 @@
         <v>1</v>
       </c>
       <c r="AB4" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC4">
         <v>2047079</v>
@@ -71640,10 +71820,10 @@
         <v>320200527</v>
       </c>
       <c r="AG4" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH4" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>2838</v>
       </c>
       <c r="AI4">
         <v>316000507</v>
@@ -71701,7 +71881,7 @@
       <c r="G5" s="44"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43" t="s">
-        <v>2797</v>
+        <v>2796</v>
       </c>
       <c r="J5">
         <v>1500</v>
@@ -71755,7 +71935,7 @@
         <v>1</v>
       </c>
       <c r="AB5" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC5">
         <v>2047079</v>
@@ -71770,10 +71950,10 @@
         <v>320200527</v>
       </c>
       <c r="AG5" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH5" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>2838</v>
       </c>
       <c r="AI5">
         <v>316000507</v>
@@ -71829,7 +72009,7 @@
     </row>
     <row r="6" spans="5:51" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>2793</v>
+        <v>2792</v>
       </c>
       <c r="F6">
         <v>1000</v>
@@ -71839,7 +72019,7 @@
         <v>250</v>
       </c>
       <c r="I6" s="43" t="s">
-        <v>2798</v>
+        <v>2797</v>
       </c>
       <c r="J6">
         <v>1500</v>
@@ -71893,7 +72073,7 @@
         <v>1</v>
       </c>
       <c r="AB6" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC6">
         <v>2047079</v>
@@ -71908,10 +72088,10 @@
         <v>320200527</v>
       </c>
       <c r="AG6" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH6" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>2838</v>
       </c>
       <c r="AI6">
         <v>316000507</v>
@@ -71967,7 +72147,7 @@
     </row>
     <row r="7" spans="5:51" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
       <c r="F7">
         <v>2000</v>
@@ -71977,7 +72157,7 @@
         <v>500</v>
       </c>
       <c r="I7" s="43" t="s">
-        <v>2799</v>
+        <v>2798</v>
       </c>
       <c r="J7">
         <v>1500</v>
@@ -72031,7 +72211,7 @@
         <v>1</v>
       </c>
       <c r="AB7" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC7">
         <v>2047079</v>
@@ -72046,10 +72226,10 @@
         <v>320200527</v>
       </c>
       <c r="AG7" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH7" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>2838</v>
       </c>
       <c r="AI7">
         <v>316000507</v>
@@ -72105,7 +72285,7 @@
     </row>
     <row r="8" spans="5:51" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>2795</v>
+        <v>2794</v>
       </c>
       <c r="F8">
         <v>3000</v>
@@ -72163,7 +72343,7 @@
         <v>1</v>
       </c>
       <c r="AB8" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC8">
         <v>2047079</v>
@@ -72178,10 +72358,10 @@
         <v>320200527</v>
       </c>
       <c r="AG8" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH8" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>2838</v>
       </c>
       <c r="AI8">
         <v>316000507</v>
@@ -72289,7 +72469,7 @@
         <v>1</v>
       </c>
       <c r="AB9" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC9">
         <v>2047079</v>
@@ -72304,10 +72484,10 @@
         <v>320200527</v>
       </c>
       <c r="AG9" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH9" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>2838</v>
       </c>
       <c r="AI9">
         <v>316000507</v>
@@ -72411,7 +72591,7 @@
         <v>1</v>
       </c>
       <c r="AB10" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC10">
         <v>2047079</v>
@@ -72426,10 +72606,10 @@
         <v>320200527</v>
       </c>
       <c r="AG10" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH10" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>2838</v>
       </c>
       <c r="AI10">
         <v>291000469</v>
@@ -72533,7 +72713,7 @@
         <v>1</v>
       </c>
       <c r="AB11" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC11">
         <v>2047079</v>
@@ -72548,10 +72728,10 @@
         <v>320200527</v>
       </c>
       <c r="AG11" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH11" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>2838</v>
       </c>
       <c r="AI11">
         <v>319000507</v>
@@ -72655,7 +72835,7 @@
         <v>1</v>
       </c>
       <c r="AB12" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC12">
         <v>2047079</v>
@@ -72670,10 +72850,10 @@
         <v>320200527</v>
       </c>
       <c r="AG12" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH12" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>2838</v>
       </c>
       <c r="AI12">
         <v>319000507</v>
@@ -72777,7 +72957,7 @@
         <v>1</v>
       </c>
       <c r="AB13" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC13">
         <v>2047079</v>
@@ -72792,10 +72972,10 @@
         <v>320200527</v>
       </c>
       <c r="AG13" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH13" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>2838</v>
       </c>
       <c r="AI13">
         <v>291000469</v>
@@ -72899,7 +73079,7 @@
         <v>1</v>
       </c>
       <c r="AB14" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC14">
         <v>2047079</v>
@@ -72914,10 +73094,10 @@
         <v>320200527</v>
       </c>
       <c r="AG14" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH14" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>2838</v>
       </c>
       <c r="AI14">
         <v>291000469</v>
@@ -73021,7 +73201,7 @@
         <v>1</v>
       </c>
       <c r="AB15" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC15">
         <v>2047079</v>
@@ -73036,10 +73216,10 @@
         <v>320200527</v>
       </c>
       <c r="AG15" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH15" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>2838</v>
       </c>
       <c r="AI15">
         <v>316000507</v>
@@ -73143,7 +73323,7 @@
         <v>1</v>
       </c>
       <c r="AB16" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC16">
         <v>2047079</v>
@@ -73158,10 +73338,10 @@
         <v>320200527</v>
       </c>
       <c r="AG16" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH16" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH16" t="s">
-        <v>2838</v>
       </c>
       <c r="AI16">
         <v>316000507</v>
@@ -73265,7 +73445,7 @@
         <v>1</v>
       </c>
       <c r="AB17" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC17">
         <v>2047079</v>
@@ -73280,10 +73460,10 @@
         <v>320200527</v>
       </c>
       <c r="AG17" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH17" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>2838</v>
       </c>
       <c r="AI17">
         <v>291000469</v>
@@ -73387,7 +73567,7 @@
         <v>1</v>
       </c>
       <c r="AB18" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC18">
         <v>2047079</v>
@@ -73402,10 +73582,10 @@
         <v>320200527</v>
       </c>
       <c r="AG18" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH18" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH18" t="s">
-        <v>2838</v>
       </c>
       <c r="AI18">
         <v>316000507</v>
@@ -73509,7 +73689,7 @@
         <v>1</v>
       </c>
       <c r="AB19" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC19">
         <v>2047079</v>
@@ -73524,10 +73704,10 @@
         <v>320200527</v>
       </c>
       <c r="AG19" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH19" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH19" t="s">
-        <v>2838</v>
       </c>
       <c r="AI19">
         <v>318000507</v>
@@ -73631,7 +73811,7 @@
         <v>1</v>
       </c>
       <c r="AB20" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC20">
         <v>2047079</v>
@@ -73646,10 +73826,10 @@
         <v>320200527</v>
       </c>
       <c r="AG20" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH20" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH20" t="s">
-        <v>2838</v>
       </c>
       <c r="AI20">
         <v>318000507</v>
@@ -73753,7 +73933,7 @@
         <v>1</v>
       </c>
       <c r="AB21" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC21">
         <v>2047079</v>
@@ -73768,10 +73948,10 @@
         <v>320200527</v>
       </c>
       <c r="AG21" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH21" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH21" t="s">
-        <v>2838</v>
       </c>
       <c r="AI21">
         <v>318000507</v>
@@ -73875,7 +74055,7 @@
         <v>1</v>
       </c>
       <c r="AB22" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC22">
         <v>2047079</v>
@@ -73890,10 +74070,10 @@
         <v>320200527</v>
       </c>
       <c r="AG22" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH22" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH22" t="s">
-        <v>2838</v>
       </c>
       <c r="AI22">
         <v>318000507</v>
@@ -73997,7 +74177,7 @@
         <v>1</v>
       </c>
       <c r="AB23" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC23">
         <v>2047079</v>
@@ -74012,10 +74192,10 @@
         <v>320200527</v>
       </c>
       <c r="AG23" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH23" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH23" t="s">
-        <v>2838</v>
       </c>
       <c r="AI23">
         <v>316000507</v>
@@ -74119,7 +74299,7 @@
         <v>1</v>
       </c>
       <c r="AB24" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC24">
         <v>2047079</v>
@@ -74134,10 +74314,10 @@
         <v>320200527</v>
       </c>
       <c r="AG24" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH24" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH24" t="s">
-        <v>2838</v>
       </c>
       <c r="AI24">
         <v>316000507</v>
@@ -74241,7 +74421,7 @@
         <v>1</v>
       </c>
       <c r="AB25" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC25">
         <v>2047079</v>
@@ -74256,10 +74436,10 @@
         <v>320200527</v>
       </c>
       <c r="AG25" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH25" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH25" t="s">
-        <v>2838</v>
       </c>
       <c r="AI25">
         <v>318000507</v>
@@ -74363,7 +74543,7 @@
         <v>1</v>
       </c>
       <c r="AB26" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC26">
         <v>2047079</v>
@@ -74378,10 +74558,10 @@
         <v>320200527</v>
       </c>
       <c r="AG26" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH26" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH26" t="s">
-        <v>2838</v>
       </c>
       <c r="AI26">
         <v>318000507</v>
@@ -74485,7 +74665,7 @@
         <v>1</v>
       </c>
       <c r="AB27" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC27">
         <v>2047079</v>
@@ -74500,10 +74680,10 @@
         <v>320200527</v>
       </c>
       <c r="AG27" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH27" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH27" t="s">
-        <v>2838</v>
       </c>
       <c r="AI27">
         <v>319000507</v>
@@ -74607,7 +74787,7 @@
         <v>1</v>
       </c>
       <c r="AB28" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC28">
         <v>2047079</v>
@@ -74622,10 +74802,10 @@
         <v>320200527</v>
       </c>
       <c r="AG28" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH28" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH28" t="s">
-        <v>2838</v>
       </c>
       <c r="AI28">
         <v>319000507</v>
@@ -74729,7 +74909,7 @@
         <v>1</v>
       </c>
       <c r="AB29" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC29">
         <v>2047079</v>
@@ -74744,10 +74924,10 @@
         <v>320200527</v>
       </c>
       <c r="AG29" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH29" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH29" t="s">
-        <v>2838</v>
       </c>
       <c r="AI29">
         <v>318000507</v>
@@ -74851,7 +75031,7 @@
         <v>1</v>
       </c>
       <c r="AB30" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC30">
         <v>2047079</v>
@@ -74866,10 +75046,10 @@
         <v>320200527</v>
       </c>
       <c r="AG30" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH30" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH30" t="s">
-        <v>2838</v>
       </c>
       <c r="AI30">
         <v>318000507</v>
@@ -74973,7 +75153,7 @@
         <v>1</v>
       </c>
       <c r="AB31" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="AC31">
         <v>2047079</v>
@@ -74988,10 +75168,10 @@
         <v>320200527</v>
       </c>
       <c r="AG31" t="s">
+        <v>2836</v>
+      </c>
+      <c r="AH31" t="s">
         <v>2837</v>
-      </c>
-      <c r="AH31" t="s">
-        <v>2838</v>
       </c>
       <c r="AI31">
         <v>316000507</v>

</xml_diff>

<commit_message>
Acerto gravação glosas dashboard antigo
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8554A8-4A32-4BB2-B2E3-5CE484E9B5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A68119B-C511-4489-994F-0C62A2CDAAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14609" uniqueCount="2845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14673" uniqueCount="2855">
   <si>
     <t>Responsável</t>
   </si>
@@ -8709,9 +8709,6 @@
     <t>Havia um item no contrato 281000577 sem TES cadastrada</t>
   </si>
   <si>
-    <t>Não imprimir o D / C nos relatorios comparativos da contabilidade</t>
-  </si>
-  <si>
     <t>BKGCT06 - 15</t>
   </si>
   <si>
@@ -8991,6 +8988,39 @@
   </si>
   <si>
     <t>Suporte nova medição (campo obs)</t>
+  </si>
+  <si>
+    <t>Criar filtro na tela de solicitação de compras, apenas com as solicitações bloqueadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1_QUJE == 0 .And. (C1_COTACAO == Space(Len(C1_COTACAO)) .Or. C1_COTACAO == "IMPORT") .And. C1_APROV == "B" .AND. Empty(C1_RESIDUO)                                                                                                                            </t>
+  </si>
+  <si>
+    <t>Incluir eventos do SZ5 no BKGCTR26 e também PIS/COFINS de entradas com crédito e saídas</t>
+  </si>
+  <si>
+    <t>Não imprimir o D / C nos relatorios comparativos da contabilidade (PERSONALIZAR FONTE)</t>
+  </si>
+  <si>
+    <t>Reunião - Ativo Imobilizado</t>
+  </si>
+  <si>
+    <t>Reunião - Dashboard e outros assuntos</t>
+  </si>
+  <si>
+    <t>Remoção IR retido na NF 6041</t>
+  </si>
+  <si>
+    <t>Verificação de lançamentos contábeis do faturamento não encontrados</t>
+  </si>
+  <si>
+    <t>Acertar valores de glosas e bonificações no dashboard antigo</t>
+  </si>
+  <si>
+    <t>Problemas com o estorno de uma medição onde os valores estavam incorretos nas planilhas e cronograma</t>
+  </si>
+  <si>
+    <t>Titulo a pagar 532512222 com decrescimo informado nos titulos de abatimento de impostos</t>
   </si>
 </sst>
 </file>
@@ -9801,15 +9831,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Planilha1">
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J2077"/>
+  <dimension ref="A1:J2085"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2026" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2034" sqref="A2034"/>
+      <pane ySplit="1" topLeftCell="A2034" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2043" sqref="A2043"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -68519,7 +68549,7 @@
         <v>13</v>
       </c>
       <c r="J1959" s="13" t="s">
-        <v>2783</v>
+        <v>2782</v>
       </c>
     </row>
     <row r="1960" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -69669,7 +69699,7 @@
         <v>683</v>
       </c>
       <c r="F1997" s="10" t="s">
-        <v>2787</v>
+        <v>2786</v>
       </c>
       <c r="G1997" s="11" t="s">
         <v>1599</v>
@@ -69805,7 +69835,7 @@
         <v>13</v>
       </c>
       <c r="J2001" s="13" t="s">
-        <v>2753</v>
+        <v>2752</v>
       </c>
     </row>
     <row r="2002" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -69825,7 +69855,7 @@
         <v>568</v>
       </c>
       <c r="F2002" s="10" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="G2002" s="11" t="s">
         <v>1624</v>
@@ -69855,7 +69885,7 @@
         <v>618</v>
       </c>
       <c r="F2003" s="30" t="s">
-        <v>2763</v>
+        <v>2762</v>
       </c>
       <c r="G2003" s="11" t="s">
         <v>1604</v>
@@ -69887,7 +69917,7 @@
         <v>618</v>
       </c>
       <c r="F2004" s="30" t="s">
-        <v>2755</v>
+        <v>2754</v>
       </c>
       <c r="G2004" s="11" t="s">
         <v>295</v>
@@ -69899,7 +69929,7 @@
         <v>13</v>
       </c>
       <c r="J2004" s="13" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
     </row>
     <row r="2005" spans="1:10" x14ac:dyDescent="0.2">
@@ -69919,7 +69949,7 @@
         <v>568</v>
       </c>
       <c r="F2005" s="30" t="s">
-        <v>2759</v>
+        <v>2758</v>
       </c>
       <c r="G2005" s="11" t="s">
         <v>309</v>
@@ -69931,7 +69961,7 @@
         <v>13</v>
       </c>
       <c r="J2005" s="13" t="s">
-        <v>2760</v>
+        <v>2759</v>
       </c>
     </row>
     <row r="2006" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -69951,7 +69981,7 @@
         <v>568</v>
       </c>
       <c r="F2006" s="30" t="s">
-        <v>2758</v>
+        <v>2757</v>
       </c>
       <c r="G2006" s="11" t="s">
         <v>1599</v>
@@ -69963,7 +69993,7 @@
         <v>13</v>
       </c>
       <c r="J2006" s="13" t="s">
-        <v>2761</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="2007" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -69983,7 +70013,7 @@
         <v>618</v>
       </c>
       <c r="F2007" s="30" t="s">
-        <v>2762</v>
+        <v>2761</v>
       </c>
       <c r="G2007" s="11" t="s">
         <v>1604</v>
@@ -70015,7 +70045,7 @@
         <v>618</v>
       </c>
       <c r="F2008" s="30" t="s">
-        <v>2773</v>
+        <v>2772</v>
       </c>
       <c r="G2008" s="11" t="s">
         <v>1599</v>
@@ -70027,7 +70057,7 @@
         <v>13</v>
       </c>
       <c r="J2008" s="13" t="s">
-        <v>2764</v>
+        <v>2763</v>
       </c>
     </row>
     <row r="2009" spans="1:10" x14ac:dyDescent="0.2">
@@ -70047,7 +70077,7 @@
         <v>618</v>
       </c>
       <c r="F2009" s="30" t="s">
-        <v>2765</v>
+        <v>2764</v>
       </c>
       <c r="G2009" s="11" t="s">
         <v>1624</v>
@@ -70059,7 +70089,7 @@
         <v>13</v>
       </c>
       <c r="J2009" s="13" t="s">
-        <v>2766</v>
+        <v>2765</v>
       </c>
     </row>
     <row r="2010" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -70079,7 +70109,7 @@
         <v>568</v>
       </c>
       <c r="F2010" s="30" t="s">
-        <v>2767</v>
+        <v>2766</v>
       </c>
       <c r="G2010" s="11" t="s">
         <v>309</v>
@@ -70091,7 +70121,7 @@
         <v>13</v>
       </c>
       <c r="J2010" s="13" t="s">
-        <v>2768</v>
+        <v>2767</v>
       </c>
     </row>
     <row r="2011" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -70111,7 +70141,7 @@
         <v>618</v>
       </c>
       <c r="F2011" s="30" t="s">
-        <v>2769</v>
+        <v>2768</v>
       </c>
       <c r="G2011" s="11" t="s">
         <v>1599</v>
@@ -70123,7 +70153,7 @@
         <v>13</v>
       </c>
       <c r="J2011" s="13" t="s">
-        <v>2770</v>
+        <v>2769</v>
       </c>
     </row>
     <row r="2012" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -70143,7 +70173,7 @@
         <v>835</v>
       </c>
       <c r="F2012" s="10" t="s">
-        <v>2772</v>
+        <v>2771</v>
       </c>
       <c r="G2012" s="11" t="s">
         <v>1599</v>
@@ -70155,7 +70185,7 @@
         <v>13</v>
       </c>
       <c r="J2012" s="13" t="s">
-        <v>2771</v>
+        <v>2770</v>
       </c>
     </row>
     <row r="2013" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -70205,7 +70235,7 @@
         <v>645</v>
       </c>
       <c r="F2014" s="10" t="s">
-        <v>2778</v>
+        <v>2777</v>
       </c>
       <c r="G2014" s="11" t="s">
         <v>1599</v>
@@ -70235,7 +70265,7 @@
         <v>683</v>
       </c>
       <c r="F2015" s="10" t="s">
-        <v>2784</v>
+        <v>2783</v>
       </c>
       <c r="G2015" s="11" t="s">
         <v>1599</v>
@@ -70265,7 +70295,7 @@
         <v>618</v>
       </c>
       <c r="F2016" s="10" t="s">
-        <v>2785</v>
+        <v>2784</v>
       </c>
       <c r="G2016" s="11" t="s">
         <v>295</v>
@@ -70295,7 +70325,7 @@
         <v>618</v>
       </c>
       <c r="F2017" s="10" t="s">
-        <v>2786</v>
+        <v>2785</v>
       </c>
       <c r="G2017" s="11" t="s">
         <v>1828</v>
@@ -70325,10 +70355,10 @@
         <v>618</v>
       </c>
       <c r="F2018" s="10" t="s">
+        <v>2773</v>
+      </c>
+      <c r="G2018" s="11" t="s">
         <v>2774</v>
-      </c>
-      <c r="G2018" s="11" t="s">
-        <v>2775</v>
       </c>
       <c r="H2018" s="12" t="s">
         <v>112</v>
@@ -70355,7 +70385,7 @@
         <v>683</v>
       </c>
       <c r="F2019" s="10" t="s">
-        <v>2782</v>
+        <v>2781</v>
       </c>
       <c r="G2019" s="11" t="s">
         <v>1599</v>
@@ -70385,7 +70415,7 @@
         <v>618</v>
       </c>
       <c r="F2020" s="30" t="s">
-        <v>2776</v>
+        <v>2775</v>
       </c>
       <c r="G2020" s="11" t="s">
         <v>295</v>
@@ -70415,7 +70445,7 @@
         <v>696</v>
       </c>
       <c r="F2021" s="30" t="s">
-        <v>2777</v>
+        <v>2776</v>
       </c>
       <c r="G2021" s="11" t="s">
         <v>295</v>
@@ -70445,7 +70475,7 @@
         <v>618</v>
       </c>
       <c r="F2022" s="30" t="s">
-        <v>2779</v>
+        <v>2778</v>
       </c>
       <c r="G2022" s="11" t="s">
         <v>295</v>
@@ -70475,7 +70505,7 @@
         <v>683</v>
       </c>
       <c r="F2023" s="30" t="s">
-        <v>2780</v>
+        <v>2779</v>
       </c>
       <c r="G2023" s="11" t="s">
         <v>309</v>
@@ -70505,7 +70535,7 @@
         <v>835</v>
       </c>
       <c r="F2024" s="10" t="s">
-        <v>2757</v>
+        <v>2756</v>
       </c>
       <c r="G2024" s="11" t="s">
         <v>295</v>
@@ -70517,7 +70547,7 @@
         <v>13</v>
       </c>
       <c r="J2024" s="13" t="s">
-        <v>2781</v>
+        <v>2780</v>
       </c>
     </row>
     <row r="2025" spans="1:10" x14ac:dyDescent="0.2">
@@ -70537,7 +70567,7 @@
         <v>683</v>
       </c>
       <c r="F2025" s="30" t="s">
-        <v>2788</v>
+        <v>2787</v>
       </c>
       <c r="G2025" s="11" t="s">
         <v>1601</v>
@@ -70567,7 +70597,7 @@
         <v>618</v>
       </c>
       <c r="F2026" s="30" t="s">
-        <v>2789</v>
+        <v>2788</v>
       </c>
       <c r="G2026" s="11" t="s">
         <v>1624</v>
@@ -70597,7 +70627,7 @@
         <v>618</v>
       </c>
       <c r="F2027" s="30" t="s">
-        <v>2790</v>
+        <v>2789</v>
       </c>
       <c r="G2027" s="11" t="s">
         <v>1624</v>
@@ -70627,7 +70657,7 @@
         <v>683</v>
       </c>
       <c r="F2028" s="30" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="G2028" s="11" t="s">
         <v>1624</v>
@@ -70657,7 +70687,7 @@
         <v>683</v>
       </c>
       <c r="F2029" s="30" t="s">
-        <v>2839</v>
+        <v>2838</v>
       </c>
       <c r="G2029" s="11" t="s">
         <v>1624</v>
@@ -70687,7 +70717,7 @@
         <v>618</v>
       </c>
       <c r="F2030" s="30" t="s">
-        <v>2840</v>
+        <v>2839</v>
       </c>
       <c r="G2030" s="11" t="s">
         <v>1624</v>
@@ -70717,7 +70747,7 @@
         <v>618</v>
       </c>
       <c r="F2031" s="30" t="s">
-        <v>2841</v>
+        <v>2840</v>
       </c>
       <c r="G2031" s="11" t="s">
         <v>1599</v>
@@ -70747,7 +70777,7 @@
         <v>667</v>
       </c>
       <c r="F2032" s="10" t="s">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="G2032" s="11" t="s">
         <v>308</v>
@@ -70777,7 +70807,7 @@
         <v>618</v>
       </c>
       <c r="F2033" s="30" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="G2033" s="11" t="s">
         <v>1624</v>
@@ -70791,276 +70821,356 @@
       <c r="J2033" s="13"/>
     </row>
     <row r="2034" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2034" s="12"/>
-      <c r="B2034" s="12"/>
-      <c r="C2034" s="10"/>
-      <c r="D2034" s="10"/>
-      <c r="E2034" s="11"/>
-      <c r="F2034" s="30"/>
-      <c r="G2034" s="11"/>
-      <c r="H2034" s="12"/>
-      <c r="I2034" s="13"/>
+      <c r="A2034" s="12">
+        <v>41041</v>
+      </c>
+      <c r="B2034" s="12">
+        <v>44697</v>
+      </c>
+      <c r="C2034" s="10" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2034" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2034" s="11" t="s">
+        <v>667</v>
+      </c>
+      <c r="F2034" s="10" t="s">
+        <v>2842</v>
+      </c>
+      <c r="G2034" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H2034" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2034" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2034" s="13"/>
     </row>
-    <row r="2035" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2035" s="12"/>
-      <c r="B2035" s="12"/>
-      <c r="C2035" s="10"/>
-      <c r="D2035" s="10"/>
-      <c r="E2035" s="11"/>
-      <c r="F2035" s="30"/>
-      <c r="G2035" s="11"/>
-      <c r="H2035" s="12"/>
-      <c r="I2035" s="13"/>
-      <c r="J2035" s="13"/>
+    <row r="2035" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2035" s="12">
+        <v>44698</v>
+      </c>
+      <c r="B2035" s="12">
+        <v>44698</v>
+      </c>
+      <c r="C2035" s="10" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2035" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2035" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2035" s="30" t="s">
+        <v>2844</v>
+      </c>
+      <c r="G2035" s="11" t="s">
+        <v>1599</v>
+      </c>
+      <c r="H2035" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2035" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2035" s="13" t="s">
+        <v>2845</v>
+      </c>
     </row>
     <row r="2036" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2036" s="12"/>
-      <c r="B2036" s="12"/>
-      <c r="C2036" s="10"/>
-      <c r="D2036" s="10"/>
-      <c r="E2036" s="11"/>
-      <c r="F2036" s="30"/>
-      <c r="G2036" s="11"/>
-      <c r="H2036" s="12"/>
-      <c r="I2036" s="13"/>
+      <c r="A2036" s="12">
+        <v>44698</v>
+      </c>
+      <c r="B2036" s="12">
+        <v>44698</v>
+      </c>
+      <c r="C2036" s="10" t="s">
+        <v>2011</v>
+      </c>
+      <c r="D2036" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2036" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2036" s="30" t="s">
+        <v>2848</v>
+      </c>
+      <c r="G2036" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H2036" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2036" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2036" s="13"/>
     </row>
     <row r="2037" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2037" s="12"/>
-      <c r="B2037" s="12"/>
-      <c r="C2037" s="10"/>
-      <c r="D2037" s="10"/>
-      <c r="E2037" s="11"/>
-      <c r="F2037" s="10"/>
-      <c r="G2037" s="11"/>
-      <c r="H2037" s="12"/>
-      <c r="I2037" s="13"/>
+      <c r="A2037" s="12">
+        <v>44698</v>
+      </c>
+      <c r="B2037" s="12">
+        <v>44698</v>
+      </c>
+      <c r="C2037" s="10" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2037" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2037" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2037" s="30" t="s">
+        <v>2849</v>
+      </c>
+      <c r="G2037" s="11" t="s">
+        <v>1602</v>
+      </c>
+      <c r="H2037" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2037" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2037" s="13"/>
     </row>
     <row r="2038" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2038" s="12"/>
-      <c r="B2038" s="12"/>
-      <c r="C2038" s="10"/>
-      <c r="D2038" s="10"/>
-      <c r="E2038" s="11"/>
-      <c r="F2038" s="10"/>
-      <c r="G2038" s="11"/>
-      <c r="H2038" s="12"/>
-      <c r="I2038" s="13"/>
+      <c r="A2038" s="12">
+        <v>44700</v>
+      </c>
+      <c r="B2038" s="12">
+        <v>44700</v>
+      </c>
+      <c r="C2038" s="10" t="s">
+        <v>557</v>
+      </c>
+      <c r="D2038" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2038" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2038" s="10" t="s">
+        <v>2850</v>
+      </c>
+      <c r="G2038" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H2038" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2038" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2038" s="13"/>
     </row>
     <row r="2039" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2039" s="12"/>
-      <c r="B2039" s="12"/>
-      <c r="C2039" s="10"/>
-      <c r="D2039" s="10"/>
-      <c r="E2039" s="11"/>
-      <c r="F2039" s="10"/>
-      <c r="G2039" s="11"/>
-      <c r="H2039" s="12"/>
-      <c r="I2039" s="13"/>
+      <c r="A2039" s="12">
+        <v>44700</v>
+      </c>
+      <c r="B2039" s="12">
+        <v>44700</v>
+      </c>
+      <c r="C2039" s="10" t="s">
+        <v>2156</v>
+      </c>
+      <c r="D2039" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2039" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2039" s="10" t="s">
+        <v>2851</v>
+      </c>
+      <c r="G2039" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H2039" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2039" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2039" s="13"/>
     </row>
-    <row r="2040" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2040" s="12"/>
-      <c r="B2040" s="12"/>
-      <c r="C2040" s="10"/>
-      <c r="D2040" s="10"/>
-      <c r="E2040" s="11"/>
-      <c r="F2040" s="30"/>
-      <c r="G2040" s="11"/>
-      <c r="H2040" s="12"/>
-      <c r="I2040" s="13"/>
+    <row r="2040" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2040" s="12">
+        <v>44700</v>
+      </c>
+      <c r="B2040" s="12">
+        <v>44700</v>
+      </c>
+      <c r="C2040" s="10" t="s">
+        <v>525</v>
+      </c>
+      <c r="D2040" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2040" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2040" s="10" t="s">
+        <v>2853</v>
+      </c>
+      <c r="G2040" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H2040" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2040" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2040" s="13"/>
     </row>
-    <row r="2041" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2041" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2041" s="12">
-        <v>41041</v>
-      </c>
-      <c r="B2041" s="12"/>
+        <v>44700</v>
+      </c>
+      <c r="B2041" s="12">
+        <v>44700</v>
+      </c>
       <c r="C2041" s="10" t="s">
-        <v>895</v>
+        <v>557</v>
       </c>
       <c r="D2041" s="10" t="s">
-        <v>492</v>
+        <v>6</v>
       </c>
       <c r="E2041" s="11" t="s">
-        <v>667</v>
+        <v>683</v>
       </c>
       <c r="F2041" s="10" t="s">
-        <v>2843</v>
-      </c>
-      <c r="G2041" s="11"/>
-      <c r="H2041" s="12"/>
-      <c r="I2041" s="13"/>
+        <v>2854</v>
+      </c>
+      <c r="G2041" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H2041" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2041" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2041" s="13"/>
     </row>
     <row r="2042" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2042" s="12">
-        <v>44684</v>
-      </c>
-      <c r="B2042" s="12"/>
-      <c r="C2042" s="14" t="s">
-        <v>2156</v>
+        <v>44698</v>
+      </c>
+      <c r="B2042" s="12">
+        <v>44700</v>
+      </c>
+      <c r="C2042" s="10" t="s">
+        <v>895</v>
       </c>
       <c r="D2042" s="10" t="s">
-        <v>83</v>
+        <v>492</v>
       </c>
       <c r="E2042" s="11" t="s">
-        <v>618</v>
+        <v>835</v>
       </c>
       <c r="F2042" s="10" t="s">
-        <v>2752</v>
-      </c>
-      <c r="G2042" s="11"/>
-      <c r="H2042" s="12"/>
-      <c r="I2042" s="13"/>
+        <v>2852</v>
+      </c>
+      <c r="G2042" s="11" t="s">
+        <v>1602</v>
+      </c>
+      <c r="H2042" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2042" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2042" s="13"/>
     </row>
-    <row r="2043" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2043" s="12">
-        <v>44677</v>
-      </c>
+    <row r="2043" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2043" s="12"/>
       <c r="B2043" s="12"/>
-      <c r="C2043" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="D2043" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2043" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2043" s="10" t="s">
-        <v>2730</v>
-      </c>
+      <c r="C2043" s="10"/>
+      <c r="D2043" s="10"/>
+      <c r="E2043" s="11"/>
+      <c r="F2043" s="10"/>
       <c r="G2043" s="11"/>
       <c r="H2043" s="12"/>
       <c r="I2043" s="13"/>
       <c r="J2043" s="13"/>
     </row>
     <row r="2044" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2044" s="12">
-        <v>44649</v>
-      </c>
+      <c r="A2044" s="12"/>
       <c r="B2044" s="12"/>
-      <c r="C2044" s="14" t="s">
-        <v>1969</v>
-      </c>
-      <c r="D2044" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2044" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2044" s="10" t="s">
-        <v>2654</v>
-      </c>
+      <c r="C2044" s="10"/>
+      <c r="D2044" s="10"/>
+      <c r="E2044" s="11"/>
+      <c r="F2044" s="10"/>
       <c r="G2044" s="11"/>
       <c r="H2044" s="12"/>
-      <c r="I2044" s="13" t="s">
-        <v>13</v>
-      </c>
+      <c r="I2044" s="13"/>
       <c r="J2044" s="13"/>
     </row>
-    <row r="2045" spans="1:10" ht="132" x14ac:dyDescent="0.2">
-      <c r="A2045" s="12">
-        <v>44645</v>
-      </c>
+    <row r="2045" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2045" s="12"/>
       <c r="B2045" s="12"/>
-      <c r="C2045" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D2045" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2045" s="11" t="s">
-        <v>618</v>
-      </c>
-      <c r="F2045" s="10" t="s">
-        <v>2665</v>
-      </c>
+      <c r="C2045" s="10"/>
+      <c r="D2045" s="10"/>
+      <c r="E2045" s="11"/>
+      <c r="F2045" s="10"/>
       <c r="G2045" s="11"/>
       <c r="H2045" s="12"/>
       <c r="I2045" s="13"/>
       <c r="J2045" s="13"/>
     </row>
     <row r="2046" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2046" s="12">
-        <v>44642</v>
-      </c>
+      <c r="A2046" s="12"/>
       <c r="B2046" s="12"/>
-      <c r="C2046" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="D2046" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2046" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2046" s="10" t="s">
-        <v>2626</v>
-      </c>
+      <c r="C2046" s="10"/>
+      <c r="D2046" s="10"/>
+      <c r="E2046" s="11"/>
+      <c r="F2046" s="10"/>
       <c r="G2046" s="11"/>
       <c r="H2046" s="12"/>
       <c r="I2046" s="13"/>
       <c r="J2046" s="13"/>
     </row>
     <row r="2047" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2047" s="12">
-        <v>44642</v>
-      </c>
+      <c r="A2047" s="12"/>
       <c r="B2047" s="12"/>
-      <c r="C2047" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="D2047" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2047" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2047" s="10" t="s">
-        <v>2625</v>
-      </c>
+      <c r="C2047" s="10"/>
+      <c r="D2047" s="10"/>
+      <c r="E2047" s="11"/>
+      <c r="F2047" s="10"/>
       <c r="G2047" s="11"/>
       <c r="H2047" s="12"/>
       <c r="I2047" s="13"/>
       <c r="J2047" s="13"/>
     </row>
     <row r="2048" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2048" s="12">
-        <v>44614</v>
-      </c>
-      <c r="B2048" s="12">
-        <v>44614</v>
-      </c>
-      <c r="C2048" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2048" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2048" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2048" s="10" t="s">
-        <v>2529</v>
-      </c>
+      <c r="A2048" s="12"/>
+      <c r="B2048" s="12"/>
+      <c r="C2048" s="10"/>
+      <c r="D2048" s="10"/>
+      <c r="E2048" s="11"/>
+      <c r="F2048" s="10"/>
       <c r="G2048" s="11"/>
       <c r="H2048" s="12"/>
       <c r="I2048" s="13"/>
       <c r="J2048" s="13"/>
     </row>
-    <row r="2049" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2049" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2049" s="12">
-        <v>44614</v>
+        <v>44698</v>
       </c>
       <c r="B2049" s="12"/>
-      <c r="C2049" s="14" t="s">
-        <v>19</v>
+      <c r="C2049" s="10" t="s">
+        <v>895</v>
       </c>
       <c r="D2049" s="10" t="s">
         <v>492</v>
@@ -71068,525 +71178,705 @@
       <c r="E2049" s="11" t="s">
         <v>835</v>
       </c>
-      <c r="F2049" s="10" t="s">
-        <v>2549</v>
+      <c r="F2049" s="30" t="s">
+        <v>2846</v>
       </c>
       <c r="G2049" s="11"/>
       <c r="H2049" s="12"/>
       <c r="I2049" s="13"/>
       <c r="J2049" s="13"/>
     </row>
-    <row r="2050" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2050" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2050" s="12">
-        <v>44616</v>
+        <v>44684</v>
       </c>
       <c r="B2050" s="12"/>
       <c r="C2050" s="14" t="s">
-        <v>2251</v>
+        <v>2156</v>
       </c>
       <c r="D2050" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E2050" s="11" t="s">
         <v>618</v>
       </c>
       <c r="F2050" s="10" t="s">
-        <v>2556</v>
+        <v>2847</v>
       </c>
       <c r="G2050" s="11"/>
       <c r="H2050" s="12"/>
       <c r="I2050" s="13"/>
       <c r="J2050" s="13"/>
     </row>
-    <row r="2051" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2051" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2051" s="12">
-        <v>44623</v>
+        <v>44677</v>
       </c>
       <c r="B2051" s="12"/>
       <c r="C2051" s="14" t="s">
-        <v>535</v>
+        <v>387</v>
       </c>
       <c r="D2051" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2051" s="11" t="s">
         <v>835</v>
       </c>
       <c r="F2051" s="10" t="s">
-        <v>2574</v>
+        <v>2730</v>
       </c>
       <c r="G2051" s="11"/>
       <c r="H2051" s="12"/>
       <c r="I2051" s="13"/>
       <c r="J2051" s="13"/>
     </row>
-    <row r="2052" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="2052" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2052" s="12">
-        <v>44522</v>
+        <v>44649</v>
       </c>
       <c r="B2052" s="12"/>
       <c r="C2052" s="14" t="s">
-        <v>46</v>
+        <v>1969</v>
       </c>
       <c r="D2052" s="10" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="E2052" s="11" t="s">
-        <v>568</v>
+        <v>835</v>
       </c>
       <c r="F2052" s="10" t="s">
-        <v>2351</v>
+        <v>2654</v>
       </c>
       <c r="G2052" s="11"/>
       <c r="H2052" s="12"/>
-      <c r="I2052" s="13"/>
+      <c r="I2052" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2052" s="13"/>
     </row>
-    <row r="2053" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2053" s="12"/>
+    <row r="2053" spans="1:10" ht="132" x14ac:dyDescent="0.2">
+      <c r="A2053" s="12">
+        <v>44645</v>
+      </c>
       <c r="B2053" s="12"/>
-      <c r="C2053" s="14"/>
-      <c r="D2053" s="10"/>
-      <c r="E2053" s="11"/>
-      <c r="F2053" s="10"/>
+      <c r="C2053" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D2053" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2053" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2053" s="10" t="s">
+        <v>2665</v>
+      </c>
       <c r="G2053" s="11"/>
       <c r="H2053" s="12"/>
       <c r="I2053" s="13"/>
       <c r="J2053" s="13"/>
     </row>
     <row r="2054" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2054" s="12"/>
+      <c r="A2054" s="12">
+        <v>44642</v>
+      </c>
       <c r="B2054" s="12"/>
-      <c r="C2054" s="14"/>
-      <c r="D2054" s="10"/>
-      <c r="E2054" s="11"/>
-      <c r="F2054" s="10"/>
+      <c r="C2054" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2054" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2054" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2054" s="10" t="s">
+        <v>2626</v>
+      </c>
       <c r="G2054" s="11"/>
       <c r="H2054" s="12"/>
       <c r="I2054" s="13"/>
       <c r="J2054" s="13"/>
     </row>
     <row r="2055" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2055" s="12"/>
+      <c r="A2055" s="12">
+        <v>44642</v>
+      </c>
       <c r="B2055" s="12"/>
-      <c r="C2055" s="14"/>
-      <c r="D2055" s="10"/>
-      <c r="E2055" s="11"/>
-      <c r="F2055" s="10"/>
+      <c r="C2055" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2055" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2055" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2055" s="10" t="s">
+        <v>2625</v>
+      </c>
       <c r="G2055" s="11"/>
       <c r="H2055" s="12"/>
       <c r="I2055" s="13"/>
       <c r="J2055" s="13"/>
     </row>
     <row r="2056" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2056" s="12"/>
-      <c r="B2056" s="12"/>
-      <c r="C2056" s="14"/>
-      <c r="D2056" s="10"/>
-      <c r="E2056" s="11"/>
-      <c r="F2056" s="10"/>
+      <c r="A2056" s="12">
+        <v>44614</v>
+      </c>
+      <c r="B2056" s="12">
+        <v>44614</v>
+      </c>
+      <c r="C2056" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2056" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2056" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2056" s="10" t="s">
+        <v>2529</v>
+      </c>
       <c r="G2056" s="11"/>
       <c r="H2056" s="12"/>
       <c r="I2056" s="13"/>
       <c r="J2056" s="13"/>
     </row>
     <row r="2057" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2057" s="12"/>
-      <c r="B2057" s="9"/>
-      <c r="C2057" s="14"/>
-      <c r="D2057" s="10"/>
-      <c r="E2057" s="11"/>
-      <c r="F2057" s="10"/>
+      <c r="A2057" s="12">
+        <v>44614</v>
+      </c>
+      <c r="B2057" s="12"/>
+      <c r="C2057" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2057" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2057" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2057" s="10" t="s">
+        <v>2549</v>
+      </c>
       <c r="G2057" s="11"/>
       <c r="H2057" s="12"/>
       <c r="I2057" s="13"/>
       <c r="J2057" s="13"/>
     </row>
     <row r="2058" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2058" s="1" t="s">
-        <v>1472</v>
-      </c>
-      <c r="B2058" s="2" t="s">
-        <v>1473</v>
-      </c>
-      <c r="C2058" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2058" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2058" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="F2058" s="4" t="s">
-        <v>1571</v>
-      </c>
-      <c r="G2058" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2058" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2058" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2058" s="36"/>
+      <c r="A2058" s="12">
+        <v>44616</v>
+      </c>
+      <c r="B2058" s="12"/>
+      <c r="C2058" s="14" t="s">
+        <v>2251</v>
+      </c>
+      <c r="D2058" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2058" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2058" s="10" t="s">
+        <v>2556</v>
+      </c>
+      <c r="G2058" s="11"/>
+      <c r="H2058" s="12"/>
+      <c r="I2058" s="13"/>
+      <c r="J2058" s="13"/>
     </row>
     <row r="2059" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2059" s="12"/>
-      <c r="B2059" s="9"/>
-      <c r="C2059" s="14"/>
-      <c r="D2059" s="10"/>
-      <c r="E2059" s="11"/>
-      <c r="F2059" s="10"/>
+      <c r="A2059" s="12">
+        <v>44623</v>
+      </c>
+      <c r="B2059" s="12"/>
+      <c r="C2059" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="D2059" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2059" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2059" s="10" t="s">
+        <v>2574</v>
+      </c>
       <c r="G2059" s="11"/>
       <c r="H2059" s="12"/>
       <c r="I2059" s="13"/>
       <c r="J2059" s="13"/>
     </row>
-    <row r="2060" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2060" s="12"/>
-      <c r="B2060" s="9"/>
-      <c r="C2060" s="14"/>
-      <c r="D2060" s="10"/>
-      <c r="E2060" s="11"/>
-      <c r="F2060" s="10"/>
+    <row r="2060" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2060" s="12">
+        <v>44522</v>
+      </c>
+      <c r="B2060" s="12"/>
+      <c r="C2060" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2060" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2060" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2060" s="10" t="s">
+        <v>2351</v>
+      </c>
       <c r="G2060" s="11"/>
       <c r="H2060" s="12"/>
       <c r="I2060" s="13"/>
       <c r="J2060" s="13"/>
     </row>
-    <row r="2061" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A2061" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2061" s="9"/>
-      <c r="C2061" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2061" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2061" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2061" s="10" t="s">
-        <v>1637</v>
-      </c>
+    <row r="2061" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2061" s="12"/>
+      <c r="B2061" s="12"/>
+      <c r="C2061" s="14"/>
+      <c r="D2061" s="10"/>
+      <c r="E2061" s="11"/>
+      <c r="F2061" s="10"/>
       <c r="G2061" s="11"/>
       <c r="H2061" s="12"/>
       <c r="I2061" s="13"/>
-      <c r="J2061" s="13" t="s">
-        <v>1660</v>
-      </c>
-    </row>
-    <row r="2062" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A2062" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2062" s="9"/>
-      <c r="C2062" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2062" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2062" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2062" s="10" t="s">
-        <v>1636</v>
-      </c>
+      <c r="J2061" s="13"/>
+    </row>
+    <row r="2062" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2062" s="12"/>
+      <c r="B2062" s="12"/>
+      <c r="C2062" s="14"/>
+      <c r="D2062" s="10"/>
+      <c r="E2062" s="11"/>
+      <c r="F2062" s="10"/>
       <c r="G2062" s="11"/>
       <c r="H2062" s="12"/>
       <c r="I2062" s="13"/>
       <c r="J2062" s="13"/>
     </row>
-    <row r="2063" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2063" s="12">
-        <v>44112</v>
-      </c>
-      <c r="B2063" s="9"/>
-      <c r="C2063" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D2063" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2063" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2063" s="10" t="s">
-        <v>2223</v>
-      </c>
+    <row r="2063" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2063" s="12"/>
+      <c r="B2063" s="12"/>
+      <c r="C2063" s="14"/>
+      <c r="D2063" s="10"/>
+      <c r="E2063" s="11"/>
+      <c r="F2063" s="10"/>
       <c r="G2063" s="11"/>
       <c r="H2063" s="12"/>
       <c r="I2063" s="13"/>
       <c r="J2063" s="13"/>
     </row>
     <row r="2064" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2064" s="12">
-        <v>44088</v>
-      </c>
-      <c r="B2064" s="9"/>
-      <c r="C2064" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2064" s="10" t="s">
-        <v>902</v>
-      </c>
-      <c r="E2064" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="F2064" s="10" t="s">
-        <v>1007</v>
-      </c>
+      <c r="A2064" s="12"/>
+      <c r="B2064" s="12"/>
+      <c r="C2064" s="14"/>
+      <c r="D2064" s="10"/>
+      <c r="E2064" s="11"/>
+      <c r="F2064" s="10"/>
       <c r="G2064" s="11"/>
       <c r="H2064" s="12"/>
       <c r="I2064" s="13"/>
       <c r="J2064" s="13"/>
     </row>
     <row r="2065" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2065" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A2065" s="12"/>
       <c r="B2065" s="9"/>
-      <c r="C2065" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D2065" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2065" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2065" s="10" t="s">
-        <v>900</v>
-      </c>
+      <c r="C2065" s="14"/>
+      <c r="D2065" s="10"/>
+      <c r="E2065" s="11"/>
+      <c r="F2065" s="10"/>
       <c r="G2065" s="11"/>
       <c r="H2065" s="12"/>
       <c r="I2065" s="13"/>
       <c r="J2065" s="13"/>
     </row>
     <row r="2066" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2066" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B2066" s="9"/>
-      <c r="C2066" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2066" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2066" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2066" s="10" t="s">
-        <v>897</v>
-      </c>
-      <c r="G2066" s="11"/>
-      <c r="H2066" s="12"/>
-      <c r="I2066" s="13"/>
-      <c r="J2066" s="13"/>
-    </row>
-    <row r="2067" spans="1:10" ht="108" x14ac:dyDescent="0.2">
-      <c r="A2067" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A2066" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B2066" s="2" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C2066" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2066" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2066" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F2066" s="4" t="s">
+        <v>1571</v>
+      </c>
+      <c r="G2066" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2066" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2066" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2066" s="36"/>
+    </row>
+    <row r="2067" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2067" s="12"/>
       <c r="B2067" s="9"/>
-      <c r="C2067" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2067" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2067" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2067" s="10" t="s">
-        <v>898</v>
-      </c>
+      <c r="C2067" s="14"/>
+      <c r="D2067" s="10"/>
+      <c r="E2067" s="11"/>
+      <c r="F2067" s="10"/>
       <c r="G2067" s="11"/>
       <c r="H2067" s="12"/>
       <c r="I2067" s="13"/>
       <c r="J2067" s="13"/>
     </row>
-    <row r="2068" spans="1:10" ht="168" x14ac:dyDescent="0.2">
-      <c r="A2068" s="12">
-        <v>43949</v>
-      </c>
+    <row r="2068" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2068" s="12"/>
       <c r="B2068" s="9"/>
-      <c r="C2068" s="14" t="s">
-        <v>468</v>
-      </c>
-      <c r="D2068" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2068" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="F2068" s="10" t="s">
-        <v>684</v>
-      </c>
-      <c r="G2068" s="11" t="s">
-        <v>1617</v>
-      </c>
+      <c r="C2068" s="14"/>
+      <c r="D2068" s="10"/>
+      <c r="E2068" s="11"/>
+      <c r="F2068" s="10"/>
+      <c r="G2068" s="11"/>
       <c r="H2068" s="12"/>
-      <c r="I2068" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I2068" s="13"/>
       <c r="J2068" s="13"/>
     </row>
-    <row r="2069" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="2069" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A2069" s="12">
-        <v>43949</v>
+        <v>44252</v>
       </c>
       <c r="B2069" s="9"/>
       <c r="C2069" s="14" t="s">
-        <v>468</v>
+        <v>895</v>
       </c>
       <c r="D2069" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E2069" s="11" t="s">
-        <v>683</v>
+        <v>757</v>
       </c>
       <c r="F2069" s="10" t="s">
-        <v>703</v>
-      </c>
-      <c r="G2069" s="11" t="s">
-        <v>685</v>
-      </c>
+        <v>1637</v>
+      </c>
+      <c r="G2069" s="11"/>
       <c r="H2069" s="12"/>
-      <c r="I2069" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I2069" s="13"/>
       <c r="J2069" s="13" t="s">
-        <v>1561</v>
-      </c>
-    </row>
-    <row r="2070" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="2070" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A2070" s="12">
-        <v>43838</v>
+        <v>44252</v>
       </c>
       <c r="B2070" s="9"/>
       <c r="C2070" s="14" t="s">
-        <v>103</v>
+        <v>895</v>
       </c>
       <c r="D2070" s="10" t="s">
-        <v>460</v>
+        <v>492</v>
       </c>
       <c r="E2070" s="11" t="s">
-        <v>645</v>
+        <v>757</v>
       </c>
       <c r="F2070" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="G2070" s="11" t="s">
-        <v>1618</v>
-      </c>
+        <v>1636</v>
+      </c>
+      <c r="G2070" s="11"/>
       <c r="H2070" s="12"/>
       <c r="I2070" s="13"/>
-      <c r="J2070" s="13" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="2071" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J2070" s="13"/>
+    </row>
+    <row r="2071" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2071" s="12">
-        <v>43762</v>
+        <v>44112</v>
       </c>
       <c r="B2071" s="9"/>
       <c r="C2071" s="14" t="s">
-        <v>446</v>
+        <v>621</v>
       </c>
       <c r="D2071" s="10" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E2071" s="11" t="s">
-        <v>835</v>
+        <v>568</v>
       </c>
       <c r="F2071" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G2071" s="11" t="s">
-        <v>1607</v>
-      </c>
+        <v>2223</v>
+      </c>
+      <c r="G2071" s="11"/>
       <c r="H2071" s="12"/>
       <c r="I2071" s="13"/>
       <c r="J2071" s="13"/>
     </row>
     <row r="2072" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2072" s="12"/>
+      <c r="A2072" s="12">
+        <v>44088</v>
+      </c>
       <c r="B2072" s="9"/>
-      <c r="C2072" s="14"/>
-      <c r="D2072" s="10"/>
-      <c r="E2072" s="11"/>
-      <c r="F2072" s="10"/>
+      <c r="C2072" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2072" s="10" t="s">
+        <v>902</v>
+      </c>
+      <c r="E2072" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2072" s="10" t="s">
+        <v>1007</v>
+      </c>
       <c r="G2072" s="11"/>
       <c r="H2072" s="12"/>
       <c r="I2072" s="13"/>
       <c r="J2072" s="13"/>
     </row>
     <row r="2073" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2073" s="12"/>
+      <c r="A2073" s="12">
+        <v>44055</v>
+      </c>
       <c r="B2073" s="9"/>
-      <c r="C2073" s="14"/>
-      <c r="D2073" s="10"/>
-      <c r="E2073" s="11"/>
-      <c r="F2073" s="10"/>
+      <c r="C2073" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="D2073" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2073" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2073" s="10" t="s">
+        <v>900</v>
+      </c>
       <c r="G2073" s="11"/>
       <c r="H2073" s="12"/>
       <c r="I2073" s="13"/>
       <c r="J2073" s="13"/>
     </row>
     <row r="2074" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2074" s="12"/>
+      <c r="A2074" s="12">
+        <v>44055</v>
+      </c>
       <c r="B2074" s="9"/>
-      <c r="C2074" s="14"/>
-      <c r="D2074" s="10"/>
-      <c r="E2074" s="11"/>
-      <c r="F2074" s="10"/>
+      <c r="C2074" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2074" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2074" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2074" s="10" t="s">
+        <v>897</v>
+      </c>
       <c r="G2074" s="11"/>
       <c r="H2074" s="12"/>
       <c r="I2074" s="13"/>
       <c r="J2074" s="13"/>
     </row>
-    <row r="2075" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2075" s="12"/>
+    <row r="2075" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A2075" s="12">
+        <v>44055</v>
+      </c>
       <c r="B2075" s="9"/>
-      <c r="C2075" s="14"/>
-      <c r="D2075" s="10"/>
-      <c r="E2075" s="11"/>
-      <c r="F2075" s="10"/>
+      <c r="C2075" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2075" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2075" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2075" s="10" t="s">
+        <v>898</v>
+      </c>
       <c r="G2075" s="11"/>
       <c r="H2075" s="12"/>
       <c r="I2075" s="13"/>
       <c r="J2075" s="13"/>
     </row>
-    <row r="2076" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2076" s="12"/>
+    <row r="2076" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2076" s="12">
+        <v>43949</v>
+      </c>
       <c r="B2076" s="9"/>
-      <c r="C2076" s="14"/>
-      <c r="D2076" s="10"/>
-      <c r="E2076" s="11"/>
-      <c r="F2076" s="10"/>
-      <c r="G2076" s="11"/>
+      <c r="C2076" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2076" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2076" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2076" s="10" t="s">
+        <v>684</v>
+      </c>
+      <c r="G2076" s="11" t="s">
+        <v>1617</v>
+      </c>
       <c r="H2076" s="12"/>
-      <c r="I2076" s="13"/>
+      <c r="I2076" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J2076" s="13"/>
     </row>
-    <row r="2077" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2077" s="12"/>
+    <row r="2077" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2077" s="12">
+        <v>43949</v>
+      </c>
       <c r="B2077" s="9"/>
-      <c r="C2077" s="14"/>
-      <c r="D2077" s="10"/>
-      <c r="E2077" s="11"/>
-      <c r="F2077" s="10"/>
-      <c r="G2077" s="11"/>
+      <c r="C2077" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2077" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2077" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2077" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="G2077" s="11" t="s">
+        <v>685</v>
+      </c>
       <c r="H2077" s="12"/>
-      <c r="I2077" s="13"/>
-      <c r="J2077" s="13"/>
+      <c r="I2077" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J2077" s="13" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="2078" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2078" s="12">
+        <v>43838</v>
+      </c>
+      <c r="B2078" s="9"/>
+      <c r="C2078" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2078" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2078" s="11" t="s">
+        <v>645</v>
+      </c>
+      <c r="F2078" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="G2078" s="11" t="s">
+        <v>1618</v>
+      </c>
+      <c r="H2078" s="12"/>
+      <c r="I2078" s="13"/>
+      <c r="J2078" s="13" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="2079" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2079" s="12">
+        <v>43762</v>
+      </c>
+      <c r="B2079" s="9"/>
+      <c r="C2079" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D2079" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2079" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2079" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G2079" s="11" t="s">
+        <v>1607</v>
+      </c>
+      <c r="H2079" s="12"/>
+      <c r="I2079" s="13"/>
+      <c r="J2079" s="13"/>
+    </row>
+    <row r="2080" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2080" s="12"/>
+      <c r="B2080" s="9"/>
+      <c r="C2080" s="14"/>
+      <c r="D2080" s="10"/>
+      <c r="E2080" s="11"/>
+      <c r="F2080" s="10"/>
+      <c r="G2080" s="11"/>
+      <c r="H2080" s="12"/>
+      <c r="I2080" s="13"/>
+      <c r="J2080" s="13"/>
+    </row>
+    <row r="2081" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2081" s="12"/>
+      <c r="B2081" s="9"/>
+      <c r="C2081" s="14"/>
+      <c r="D2081" s="10"/>
+      <c r="E2081" s="11"/>
+      <c r="F2081" s="10"/>
+      <c r="G2081" s="11"/>
+      <c r="H2081" s="12"/>
+      <c r="I2081" s="13"/>
+      <c r="J2081" s="13"/>
+    </row>
+    <row r="2082" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2082" s="12"/>
+      <c r="B2082" s="9"/>
+      <c r="C2082" s="14"/>
+      <c r="D2082" s="10"/>
+      <c r="E2082" s="11"/>
+      <c r="F2082" s="10"/>
+      <c r="G2082" s="11"/>
+      <c r="H2082" s="12"/>
+      <c r="I2082" s="13"/>
+      <c r="J2082" s="13"/>
+    </row>
+    <row r="2083" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2083" s="12"/>
+      <c r="B2083" s="9"/>
+      <c r="C2083" s="14"/>
+      <c r="D2083" s="10"/>
+      <c r="E2083" s="11"/>
+      <c r="F2083" s="10"/>
+      <c r="G2083" s="11"/>
+      <c r="H2083" s="12"/>
+      <c r="I2083" s="13"/>
+      <c r="J2083" s="13"/>
+    </row>
+    <row r="2084" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2084" s="12"/>
+      <c r="B2084" s="9"/>
+      <c r="C2084" s="14"/>
+      <c r="D2084" s="10"/>
+      <c r="E2084" s="11"/>
+      <c r="F2084" s="10"/>
+      <c r="G2084" s="11"/>
+      <c r="H2084" s="12"/>
+      <c r="I2084" s="13"/>
+      <c r="J2084" s="13"/>
+    </row>
+    <row r="2085" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2085" s="12"/>
+      <c r="B2085" s="9"/>
+      <c r="C2085" s="14"/>
+      <c r="D2085" s="10"/>
+      <c r="E2085" s="11"/>
+      <c r="F2085" s="10"/>
+      <c r="G2085" s="11"/>
+      <c r="H2085" s="12"/>
+      <c r="I2085" s="13"/>
+      <c r="J2085" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1881" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -71602,6 +71892,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9BB448-231A-4961-B838-50885C350BA8}">
+  <sheetPr codeName="Planilha2"/>
   <dimension ref="E3:AY32"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -71621,129 +71912,129 @@
       <c r="H3" s="43"/>
       <c r="I3" s="43"/>
       <c r="L3" t="s">
+        <v>2798</v>
+      </c>
+      <c r="M3" t="s">
         <v>2799</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>2800</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>2801</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>2802</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>2803</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>2804</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>2805</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>2806</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
+        <v>2798</v>
+      </c>
+      <c r="V3" t="s">
+        <v>2799</v>
+      </c>
+      <c r="W3" t="s">
         <v>2807</v>
       </c>
-      <c r="U3" t="s">
-        <v>2799</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="X3" t="s">
+        <v>2808</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>2809</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>2801</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>2810</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>2811</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>2812</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>2813</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>2814</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>2815</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>2816</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>2818</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>2833</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>2819</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>2820</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>2821</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>2822</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>2823</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>2824</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>2825</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>2826</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>2827</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>2828</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>2829</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>2830</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>2831</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>2832</v>
+      </c>
+      <c r="AY3" t="s">
         <v>2800</v>
-      </c>
-      <c r="W3" t="s">
-        <v>2808</v>
-      </c>
-      <c r="X3" t="s">
-        <v>2809</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>2810</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>2802</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>2811</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>2812</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>2813</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>2814</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>2815</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>2816</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>2817</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>2818</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>2819</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>2834</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>2820</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>2821</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>2822</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>2823</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>2824</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>2825</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>2826</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>2827</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>2828</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>2829</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>2830</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>2831</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>2832</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>2833</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>2801</v>
       </c>
     </row>
     <row r="4" spans="5:51" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
-        <v>2791</v>
+        <v>2790</v>
       </c>
       <c r="F4">
         <v>6000</v>
@@ -71751,7 +72042,7 @@
       <c r="G4" s="43"/>
       <c r="H4" s="43"/>
       <c r="I4" s="43" t="s">
-        <v>2795</v>
+        <v>2794</v>
       </c>
       <c r="J4">
         <v>1500</v>
@@ -71805,7 +72096,7 @@
         <v>1</v>
       </c>
       <c r="AB4" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC4">
         <v>2047079</v>
@@ -71820,10 +72111,10 @@
         <v>320200527</v>
       </c>
       <c r="AG4" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH4" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>2837</v>
       </c>
       <c r="AI4">
         <v>316000507</v>
@@ -71881,7 +72172,7 @@
       <c r="G5" s="44"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="J5">
         <v>1500</v>
@@ -71935,7 +72226,7 @@
         <v>1</v>
       </c>
       <c r="AB5" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC5">
         <v>2047079</v>
@@ -71950,10 +72241,10 @@
         <v>320200527</v>
       </c>
       <c r="AG5" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH5" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>2837</v>
       </c>
       <c r="AI5">
         <v>316000507</v>
@@ -72009,7 +72300,7 @@
     </row>
     <row r="6" spans="5:51" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>2792</v>
+        <v>2791</v>
       </c>
       <c r="F6">
         <v>1000</v>
@@ -72019,7 +72310,7 @@
         <v>250</v>
       </c>
       <c r="I6" s="43" t="s">
-        <v>2797</v>
+        <v>2796</v>
       </c>
       <c r="J6">
         <v>1500</v>
@@ -72073,7 +72364,7 @@
         <v>1</v>
       </c>
       <c r="AB6" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC6">
         <v>2047079</v>
@@ -72088,10 +72379,10 @@
         <v>320200527</v>
       </c>
       <c r="AG6" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH6" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>2837</v>
       </c>
       <c r="AI6">
         <v>316000507</v>
@@ -72147,7 +72438,7 @@
     </row>
     <row r="7" spans="5:51" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>2793</v>
+        <v>2792</v>
       </c>
       <c r="F7">
         <v>2000</v>
@@ -72157,7 +72448,7 @@
         <v>500</v>
       </c>
       <c r="I7" s="43" t="s">
-        <v>2798</v>
+        <v>2797</v>
       </c>
       <c r="J7">
         <v>1500</v>
@@ -72211,7 +72502,7 @@
         <v>1</v>
       </c>
       <c r="AB7" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC7">
         <v>2047079</v>
@@ -72226,10 +72517,10 @@
         <v>320200527</v>
       </c>
       <c r="AG7" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH7" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>2837</v>
       </c>
       <c r="AI7">
         <v>316000507</v>
@@ -72285,7 +72576,7 @@
     </row>
     <row r="8" spans="5:51" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
       <c r="F8">
         <v>3000</v>
@@ -72343,7 +72634,7 @@
         <v>1</v>
       </c>
       <c r="AB8" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC8">
         <v>2047079</v>
@@ -72358,10 +72649,10 @@
         <v>320200527</v>
       </c>
       <c r="AG8" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH8" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>2837</v>
       </c>
       <c r="AI8">
         <v>316000507</v>
@@ -72469,7 +72760,7 @@
         <v>1</v>
       </c>
       <c r="AB9" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC9">
         <v>2047079</v>
@@ -72484,10 +72775,10 @@
         <v>320200527</v>
       </c>
       <c r="AG9" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH9" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>2837</v>
       </c>
       <c r="AI9">
         <v>316000507</v>
@@ -72591,7 +72882,7 @@
         <v>1</v>
       </c>
       <c r="AB10" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC10">
         <v>2047079</v>
@@ -72606,10 +72897,10 @@
         <v>320200527</v>
       </c>
       <c r="AG10" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH10" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>2837</v>
       </c>
       <c r="AI10">
         <v>291000469</v>
@@ -72713,7 +73004,7 @@
         <v>1</v>
       </c>
       <c r="AB11" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC11">
         <v>2047079</v>
@@ -72728,10 +73019,10 @@
         <v>320200527</v>
       </c>
       <c r="AG11" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH11" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>2837</v>
       </c>
       <c r="AI11">
         <v>319000507</v>
@@ -72835,7 +73126,7 @@
         <v>1</v>
       </c>
       <c r="AB12" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC12">
         <v>2047079</v>
@@ -72850,10 +73141,10 @@
         <v>320200527</v>
       </c>
       <c r="AG12" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH12" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>2837</v>
       </c>
       <c r="AI12">
         <v>319000507</v>
@@ -72957,7 +73248,7 @@
         <v>1</v>
       </c>
       <c r="AB13" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC13">
         <v>2047079</v>
@@ -72972,10 +73263,10 @@
         <v>320200527</v>
       </c>
       <c r="AG13" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH13" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>2837</v>
       </c>
       <c r="AI13">
         <v>291000469</v>
@@ -73079,7 +73370,7 @@
         <v>1</v>
       </c>
       <c r="AB14" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC14">
         <v>2047079</v>
@@ -73094,10 +73385,10 @@
         <v>320200527</v>
       </c>
       <c r="AG14" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH14" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>2837</v>
       </c>
       <c r="AI14">
         <v>291000469</v>
@@ -73201,7 +73492,7 @@
         <v>1</v>
       </c>
       <c r="AB15" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC15">
         <v>2047079</v>
@@ -73216,10 +73507,10 @@
         <v>320200527</v>
       </c>
       <c r="AG15" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH15" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>2837</v>
       </c>
       <c r="AI15">
         <v>316000507</v>
@@ -73323,7 +73614,7 @@
         <v>1</v>
       </c>
       <c r="AB16" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC16">
         <v>2047079</v>
@@ -73338,10 +73629,10 @@
         <v>320200527</v>
       </c>
       <c r="AG16" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH16" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH16" t="s">
-        <v>2837</v>
       </c>
       <c r="AI16">
         <v>316000507</v>
@@ -73445,7 +73736,7 @@
         <v>1</v>
       </c>
       <c r="AB17" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC17">
         <v>2047079</v>
@@ -73460,10 +73751,10 @@
         <v>320200527</v>
       </c>
       <c r="AG17" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH17" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>2837</v>
       </c>
       <c r="AI17">
         <v>291000469</v>
@@ -73567,7 +73858,7 @@
         <v>1</v>
       </c>
       <c r="AB18" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC18">
         <v>2047079</v>
@@ -73582,10 +73873,10 @@
         <v>320200527</v>
       </c>
       <c r="AG18" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH18" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH18" t="s">
-        <v>2837</v>
       </c>
       <c r="AI18">
         <v>316000507</v>
@@ -73689,7 +73980,7 @@
         <v>1</v>
       </c>
       <c r="AB19" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC19">
         <v>2047079</v>
@@ -73704,10 +73995,10 @@
         <v>320200527</v>
       </c>
       <c r="AG19" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH19" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH19" t="s">
-        <v>2837</v>
       </c>
       <c r="AI19">
         <v>318000507</v>
@@ -73811,7 +74102,7 @@
         <v>1</v>
       </c>
       <c r="AB20" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC20">
         <v>2047079</v>
@@ -73826,10 +74117,10 @@
         <v>320200527</v>
       </c>
       <c r="AG20" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH20" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH20" t="s">
-        <v>2837</v>
       </c>
       <c r="AI20">
         <v>318000507</v>
@@ -73933,7 +74224,7 @@
         <v>1</v>
       </c>
       <c r="AB21" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC21">
         <v>2047079</v>
@@ -73948,10 +74239,10 @@
         <v>320200527</v>
       </c>
       <c r="AG21" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH21" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH21" t="s">
-        <v>2837</v>
       </c>
       <c r="AI21">
         <v>318000507</v>
@@ -74055,7 +74346,7 @@
         <v>1</v>
       </c>
       <c r="AB22" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC22">
         <v>2047079</v>
@@ -74070,10 +74361,10 @@
         <v>320200527</v>
       </c>
       <c r="AG22" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH22" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH22" t="s">
-        <v>2837</v>
       </c>
       <c r="AI22">
         <v>318000507</v>
@@ -74177,7 +74468,7 @@
         <v>1</v>
       </c>
       <c r="AB23" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC23">
         <v>2047079</v>
@@ -74192,10 +74483,10 @@
         <v>320200527</v>
       </c>
       <c r="AG23" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH23" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH23" t="s">
-        <v>2837</v>
       </c>
       <c r="AI23">
         <v>316000507</v>
@@ -74299,7 +74590,7 @@
         <v>1</v>
       </c>
       <c r="AB24" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC24">
         <v>2047079</v>
@@ -74314,10 +74605,10 @@
         <v>320200527</v>
       </c>
       <c r="AG24" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH24" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH24" t="s">
-        <v>2837</v>
       </c>
       <c r="AI24">
         <v>316000507</v>
@@ -74421,7 +74712,7 @@
         <v>1</v>
       </c>
       <c r="AB25" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC25">
         <v>2047079</v>
@@ -74436,10 +74727,10 @@
         <v>320200527</v>
       </c>
       <c r="AG25" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH25" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH25" t="s">
-        <v>2837</v>
       </c>
       <c r="AI25">
         <v>318000507</v>
@@ -74543,7 +74834,7 @@
         <v>1</v>
       </c>
       <c r="AB26" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC26">
         <v>2047079</v>
@@ -74558,10 +74849,10 @@
         <v>320200527</v>
       </c>
       <c r="AG26" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH26" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH26" t="s">
-        <v>2837</v>
       </c>
       <c r="AI26">
         <v>318000507</v>
@@ -74665,7 +74956,7 @@
         <v>1</v>
       </c>
       <c r="AB27" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC27">
         <v>2047079</v>
@@ -74680,10 +74971,10 @@
         <v>320200527</v>
       </c>
       <c r="AG27" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH27" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH27" t="s">
-        <v>2837</v>
       </c>
       <c r="AI27">
         <v>319000507</v>
@@ -74787,7 +75078,7 @@
         <v>1</v>
       </c>
       <c r="AB28" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC28">
         <v>2047079</v>
@@ -74802,10 +75093,10 @@
         <v>320200527</v>
       </c>
       <c r="AG28" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH28" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH28" t="s">
-        <v>2837</v>
       </c>
       <c r="AI28">
         <v>319000507</v>
@@ -74909,7 +75200,7 @@
         <v>1</v>
       </c>
       <c r="AB29" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC29">
         <v>2047079</v>
@@ -74924,10 +75215,10 @@
         <v>320200527</v>
       </c>
       <c r="AG29" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH29" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH29" t="s">
-        <v>2837</v>
       </c>
       <c r="AI29">
         <v>318000507</v>
@@ -75031,7 +75322,7 @@
         <v>1</v>
       </c>
       <c r="AB30" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC30">
         <v>2047079</v>
@@ -75046,10 +75337,10 @@
         <v>320200527</v>
       </c>
       <c r="AG30" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH30" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH30" t="s">
-        <v>2837</v>
       </c>
       <c r="AI30">
         <v>318000507</v>
@@ -75153,7 +75444,7 @@
         <v>1</v>
       </c>
       <c r="AB31" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="AC31">
         <v>2047079</v>
@@ -75168,10 +75459,10 @@
         <v>320200527</v>
       </c>
       <c r="AG31" t="s">
+        <v>2835</v>
+      </c>
+      <c r="AH31" t="s">
         <v>2836</v>
-      </c>
-      <c r="AH31" t="s">
-        <v>2837</v>
       </c>
       <c r="AI31">
         <v>316000507</v>
@@ -75243,6 +75534,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E16FADF7-6C4C-4356-9576-380717A61E1D}">
+  <sheetPr codeName="Planilha3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -75260,6 +75552,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE13D4C-C1F0-4B00-8A02-71F13D132F72}">
+  <sheetPr codeName="Planilha4"/>
   <dimension ref="B1:G35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">

</xml_diff>

<commit_message>
Alterações 25 e 26/05/22 glosas e reajustes
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490E87E6-3A50-4A93-9953-F19E5328E5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12B1AE5-D0DB-41BF-B260-C6E4772DB430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14706" uniqueCount="2832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14751" uniqueCount="2841">
   <si>
     <t>Responsável</t>
   </si>
@@ -8951,6 +8951,35 @@
   </si>
   <si>
     <t>Por gentileza, cadastrar os dados bancários abaixo para as notas fiscais emitidas ao cliente: 385000595 VOASE CT 0005/PS/SEDE/2022 001 – BANCO DO BRASIL AG: 3320-0 C/C: 177676-2</t>
+  </si>
+  <si>
+    <t>Geração automática da tabela GLOSAS para o banco de dados PowerBk</t>
+  </si>
+  <si>
+    <t>Devido a um erro identificado, foi necessário alterar diversos relatórios que estavam com divergências na soma de valores de multas e bonificações</t>
+  </si>
+  <si>
+    <t>Reunião a respeito da base do Pis/Cofins sem o Iss</t>
+  </si>
+  <si>
+    <t>Recriação da area de testes - banco e metadados</t>
+  </si>
+  <si>
+    <t>Criação do campo CTT_XCONTRAT para indicar se o Centro de Custo é de contrato (s/n)</t>
+  </si>
+  <si>
+    <t>Relatório faturamento de reajustes, repactuação e retroativo não está filtrando as planilhas com reajuste</t>
+  </si>
+  <si>
+    <t>Alterei via banco de dados todas as planilhas do sistema constantes na planilha excel enviada pela Fábia para Tipo = 2 - Reajuste.
+Alterei também o relatório "BKFINR21 - Relatório faturamento de reajustes, repactuação e retroativo", incluindo opção de se filtrar ou não as planilhas marcadas com "Reajuste"</t>
+  </si>
+  <si>
+    <t>As aprovações da BK seguros não aparcem para mim
+E tirar o acesso de aprovação da Simone e qualquer pessoa do seguro!</t>
+  </si>
+  <si>
+    <t>Alterado o programa BKGrupos para considerar a empresa 12 e a usuária financeiro.seguros com superior o usuário 000153 - Bruno Bueno</t>
   </si>
 </sst>
 </file>
@@ -9756,11 +9785,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J2108"/>
+  <dimension ref="A1:J2111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2055" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2065" sqref="A2065"/>
+      <pane ySplit="1" topLeftCell="A2068" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2072" sqref="A2072"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -9774,7 +9803,7 @@
     <col min="7" max="7" width="10.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="35" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="54.140625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="55.7109375" style="8" customWidth="1"/>
     <col min="11" max="1017" width="8.7109375" style="8"/>
     <col min="1018" max="16384" width="9.140625" style="8"/>
   </cols>
@@ -71711,193 +71740,275 @@
       </c>
       <c r="J2065" s="13"/>
     </row>
-    <row r="2066" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2066" s="12"/>
-      <c r="B2066" s="12"/>
-      <c r="C2066" s="10"/>
-      <c r="D2066" s="10"/>
-      <c r="E2066" s="11"/>
-      <c r="F2066" s="10"/>
-      <c r="G2066" s="11"/>
-      <c r="H2066" s="12"/>
-      <c r="I2066" s="13"/>
-      <c r="J2066" s="13"/>
+    <row r="2066" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2066" s="12">
+        <v>44705</v>
+      </c>
+      <c r="B2066" s="12">
+        <v>44705</v>
+      </c>
+      <c r="C2066" s="10" t="s">
+        <v>2681</v>
+      </c>
+      <c r="D2066" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2066" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2066" s="10" t="s">
+        <v>2832</v>
+      </c>
+      <c r="G2066" s="11" t="s">
+        <v>1607</v>
+      </c>
+      <c r="H2066" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2066" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2066" s="13" t="s">
+        <v>2833</v>
+      </c>
     </row>
     <row r="2067" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2067" s="12"/>
-      <c r="B2067" s="12"/>
-      <c r="C2067" s="10"/>
-      <c r="D2067" s="10"/>
-      <c r="E2067" s="11"/>
-      <c r="F2067" s="10"/>
-      <c r="G2067" s="11"/>
-      <c r="H2067" s="12"/>
-      <c r="I2067" s="13"/>
+      <c r="A2067" s="12">
+        <v>44706</v>
+      </c>
+      <c r="B2067" s="12">
+        <v>44706</v>
+      </c>
+      <c r="C2067" s="10" t="s">
+        <v>2011</v>
+      </c>
+      <c r="D2067" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2067" s="11" t="s">
+        <v>2067</v>
+      </c>
+      <c r="F2067" s="10" t="s">
+        <v>2834</v>
+      </c>
+      <c r="G2067" s="11" t="s">
+        <v>1599</v>
+      </c>
+      <c r="H2067" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2067" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2067" s="13"/>
     </row>
-    <row r="2068" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2068" s="12"/>
-      <c r="B2068" s="12"/>
-      <c r="C2068" s="10"/>
-      <c r="D2068" s="10"/>
-      <c r="E2068" s="11"/>
-      <c r="F2068" s="10"/>
-      <c r="G2068" s="11"/>
-      <c r="H2068" s="12"/>
-      <c r="I2068" s="13"/>
+    <row r="2068" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2068" s="12">
+        <v>44706</v>
+      </c>
+      <c r="B2068" s="12">
+        <v>44706</v>
+      </c>
+      <c r="C2068" s="10" t="s">
+        <v>2681</v>
+      </c>
+      <c r="D2068" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2068" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2068" s="10" t="s">
+        <v>2836</v>
+      </c>
+      <c r="G2068" s="11" t="s">
+        <v>1599</v>
+      </c>
+      <c r="H2068" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2068" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2068" s="13"/>
     </row>
     <row r="2069" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2069" s="12"/>
-      <c r="B2069" s="12"/>
-      <c r="C2069" s="10"/>
-      <c r="D2069" s="10"/>
-      <c r="E2069" s="11"/>
-      <c r="F2069" s="10"/>
-      <c r="G2069" s="11"/>
-      <c r="H2069" s="12"/>
-      <c r="I2069" s="13"/>
+      <c r="A2069" s="12">
+        <v>44706</v>
+      </c>
+      <c r="B2069" s="12">
+        <v>44706</v>
+      </c>
+      <c r="C2069" s="10" t="s">
+        <v>2011</v>
+      </c>
+      <c r="D2069" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2069" s="11" t="s">
+        <v>2067</v>
+      </c>
+      <c r="F2069" s="10" t="s">
+        <v>2835</v>
+      </c>
+      <c r="G2069" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H2069" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2069" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2069" s="13"/>
     </row>
-    <row r="2070" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2070" s="12"/>
-      <c r="B2070" s="12"/>
-      <c r="C2070" s="10"/>
-      <c r="D2070" s="10"/>
-      <c r="E2070" s="11"/>
-      <c r="F2070" s="10"/>
-      <c r="G2070" s="11"/>
-      <c r="H2070" s="12"/>
-      <c r="I2070" s="13"/>
-      <c r="J2070" s="13"/>
-    </row>
-    <row r="2071" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2071" s="12"/>
-      <c r="B2071" s="12"/>
-      <c r="C2071" s="10"/>
-      <c r="D2071" s="10"/>
-      <c r="E2071" s="11"/>
-      <c r="F2071" s="10"/>
-      <c r="G2071" s="11"/>
-      <c r="H2071" s="12"/>
-      <c r="I2071" s="13"/>
-      <c r="J2071" s="13"/>
-    </row>
-    <row r="2072" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2072" s="12">
-        <v>44698</v>
-      </c>
+    <row r="2070" spans="1:10" ht="72" x14ac:dyDescent="0.2">
+      <c r="A2070" s="12">
+        <v>44707</v>
+      </c>
+      <c r="B2070" s="12">
+        <v>44707</v>
+      </c>
+      <c r="C2070" s="10" t="s">
+        <v>621</v>
+      </c>
+      <c r="D2070" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2070" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2070" s="10" t="s">
+        <v>2837</v>
+      </c>
+      <c r="G2070" s="11" t="s">
+        <v>1602</v>
+      </c>
+      <c r="H2070" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2070" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2070" s="13" t="s">
+        <v>2838</v>
+      </c>
+    </row>
+    <row r="2071" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2071" s="12">
+        <v>44707</v>
+      </c>
+      <c r="B2071" s="12">
+        <v>44707</v>
+      </c>
+      <c r="C2071" s="10" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2071" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2071" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2071" s="10" t="s">
+        <v>2839</v>
+      </c>
+      <c r="G2071" s="11" t="s">
+        <v>1599</v>
+      </c>
+      <c r="H2071" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2071" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2071" s="13" t="s">
+        <v>2840</v>
+      </c>
+    </row>
+    <row r="2072" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2072" s="12"/>
       <c r="B2072" s="12"/>
-      <c r="C2072" s="10" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2072" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2072" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2072" s="30" t="s">
-        <v>2799</v>
-      </c>
+      <c r="C2072" s="10"/>
+      <c r="D2072" s="10"/>
+      <c r="E2072" s="11"/>
+      <c r="F2072" s="10"/>
       <c r="G2072" s="11"/>
       <c r="H2072" s="12"/>
       <c r="I2072" s="13"/>
       <c r="J2072" s="13"/>
     </row>
-    <row r="2073" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2073" s="12">
-        <v>44684</v>
-      </c>
+    <row r="2073" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2073" s="12"/>
       <c r="B2073" s="12"/>
-      <c r="C2073" s="14" t="s">
-        <v>2156</v>
-      </c>
-      <c r="D2073" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2073" s="11" t="s">
-        <v>618</v>
-      </c>
-      <c r="F2073" s="10" t="s">
-        <v>2800</v>
-      </c>
+      <c r="C2073" s="10"/>
+      <c r="D2073" s="10"/>
+      <c r="E2073" s="11"/>
+      <c r="F2073" s="10"/>
       <c r="G2073" s="11"/>
       <c r="H2073" s="12"/>
       <c r="I2073" s="13"/>
       <c r="J2073" s="13"/>
     </row>
-    <row r="2074" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2074" s="12">
-        <v>44677</v>
-      </c>
+    <row r="2074" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2074" s="12"/>
       <c r="B2074" s="12"/>
-      <c r="C2074" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="D2074" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2074" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2074" s="10" t="s">
-        <v>2730</v>
-      </c>
+      <c r="C2074" s="10"/>
+      <c r="D2074" s="10"/>
+      <c r="E2074" s="11"/>
+      <c r="F2074" s="10"/>
       <c r="G2074" s="11"/>
       <c r="H2074" s="12"/>
       <c r="I2074" s="13"/>
       <c r="J2074" s="13"/>
     </row>
-    <row r="2075" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2075" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2075" s="12">
-        <v>44649</v>
+        <v>44698</v>
       </c>
       <c r="B2075" s="12"/>
-      <c r="C2075" s="14" t="s">
-        <v>1969</v>
+      <c r="C2075" s="10" t="s">
+        <v>895</v>
       </c>
       <c r="D2075" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E2075" s="11" t="s">
         <v>835</v>
       </c>
-      <c r="F2075" s="10" t="s">
-        <v>2654</v>
+      <c r="F2075" s="30" t="s">
+        <v>2799</v>
       </c>
       <c r="G2075" s="11"/>
       <c r="H2075" s="12"/>
-      <c r="I2075" s="13" t="s">
-        <v>13</v>
-      </c>
+      <c r="I2075" s="13"/>
       <c r="J2075" s="13"/>
     </row>
-    <row r="2076" spans="1:10" ht="132" x14ac:dyDescent="0.2">
+    <row r="2076" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2076" s="12">
-        <v>44645</v>
+        <v>44684</v>
       </c>
       <c r="B2076" s="12"/>
       <c r="C2076" s="14" t="s">
-        <v>288</v>
+        <v>2156</v>
       </c>
       <c r="D2076" s="10" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="E2076" s="11" t="s">
         <v>618</v>
       </c>
       <c r="F2076" s="10" t="s">
-        <v>2665</v>
+        <v>2800</v>
       </c>
       <c r="G2076" s="11"/>
       <c r="H2076" s="12"/>
       <c r="I2076" s="13"/>
       <c r="J2076" s="13"/>
     </row>
-    <row r="2077" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2077" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2077" s="12">
-        <v>44642</v>
+        <v>44677</v>
       </c>
       <c r="B2077" s="12"/>
       <c r="C2077" s="14" t="s">
@@ -71910,7 +72021,7 @@
         <v>835</v>
       </c>
       <c r="F2077" s="10" t="s">
-        <v>2626</v>
+        <v>2730</v>
       </c>
       <c r="G2077" s="11"/>
       <c r="H2077" s="12"/>
@@ -71919,44 +72030,44 @@
     </row>
     <row r="2078" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2078" s="12">
-        <v>44642</v>
+        <v>44649</v>
       </c>
       <c r="B2078" s="12"/>
       <c r="C2078" s="14" t="s">
-        <v>387</v>
+        <v>1969</v>
       </c>
       <c r="D2078" s="10" t="s">
-        <v>492</v>
+        <v>89</v>
       </c>
       <c r="E2078" s="11" t="s">
         <v>835</v>
       </c>
       <c r="F2078" s="10" t="s">
-        <v>2625</v>
+        <v>2654</v>
       </c>
       <c r="G2078" s="11"/>
       <c r="H2078" s="12"/>
-      <c r="I2078" s="13"/>
+      <c r="I2078" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2078" s="13"/>
     </row>
-    <row r="2079" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2079" spans="1:10" ht="132" x14ac:dyDescent="0.2">
       <c r="A2079" s="12">
-        <v>44614</v>
-      </c>
-      <c r="B2079" s="12">
-        <v>44614</v>
-      </c>
+        <v>44645</v>
+      </c>
+      <c r="B2079" s="12"/>
       <c r="C2079" s="14" t="s">
-        <v>19</v>
+        <v>288</v>
       </c>
       <c r="D2079" s="10" t="s">
-        <v>492</v>
+        <v>25</v>
       </c>
       <c r="E2079" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F2079" s="10" t="s">
-        <v>2529</v>
+        <v>2665</v>
       </c>
       <c r="G2079" s="11"/>
       <c r="H2079" s="12"/>
@@ -71965,11 +72076,11 @@
     </row>
     <row r="2080" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2080" s="12">
-        <v>44614</v>
+        <v>44642</v>
       </c>
       <c r="B2080" s="12"/>
       <c r="C2080" s="14" t="s">
-        <v>19</v>
+        <v>387</v>
       </c>
       <c r="D2080" s="10" t="s">
         <v>492</v>
@@ -71978,7 +72089,7 @@
         <v>835</v>
       </c>
       <c r="F2080" s="10" t="s">
-        <v>2549</v>
+        <v>2626</v>
       </c>
       <c r="G2080" s="11"/>
       <c r="H2080" s="12"/>
@@ -71987,20 +72098,20 @@
     </row>
     <row r="2081" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2081" s="12">
-        <v>44616</v>
+        <v>44642</v>
       </c>
       <c r="B2081" s="12"/>
       <c r="C2081" s="14" t="s">
-        <v>2251</v>
+        <v>387</v>
       </c>
       <c r="D2081" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E2081" s="11" t="s">
-        <v>618</v>
+        <v>835</v>
       </c>
       <c r="F2081" s="10" t="s">
-        <v>2556</v>
+        <v>2625</v>
       </c>
       <c r="G2081" s="11"/>
       <c r="H2081" s="12"/>
@@ -72009,42 +72120,44 @@
     </row>
     <row r="2082" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2082" s="12">
-        <v>44623</v>
-      </c>
-      <c r="B2082" s="12"/>
+        <v>44614</v>
+      </c>
+      <c r="B2082" s="12">
+        <v>44614</v>
+      </c>
       <c r="C2082" s="14" t="s">
-        <v>535</v>
+        <v>19</v>
       </c>
       <c r="D2082" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2082" s="11" t="s">
         <v>835</v>
       </c>
       <c r="F2082" s="10" t="s">
-        <v>2574</v>
+        <v>2529</v>
       </c>
       <c r="G2082" s="11"/>
       <c r="H2082" s="12"/>
       <c r="I2082" s="13"/>
       <c r="J2082" s="13"/>
     </row>
-    <row r="2083" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="2083" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2083" s="12">
-        <v>44522</v>
+        <v>44614</v>
       </c>
       <c r="B2083" s="12"/>
       <c r="C2083" s="14" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="D2083" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2083" s="11" t="s">
-        <v>568</v>
+        <v>835</v>
       </c>
       <c r="F2083" s="10" t="s">
-        <v>2351</v>
+        <v>2549</v>
       </c>
       <c r="G2083" s="11"/>
       <c r="H2083" s="12"/>
@@ -72052,36 +72165,66 @@
       <c r="J2083" s="13"/>
     </row>
     <row r="2084" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2084" s="12"/>
+      <c r="A2084" s="12">
+        <v>44616</v>
+      </c>
       <c r="B2084" s="12"/>
-      <c r="C2084" s="14"/>
-      <c r="D2084" s="10"/>
-      <c r="E2084" s="11"/>
-      <c r="F2084" s="10"/>
+      <c r="C2084" s="14" t="s">
+        <v>2251</v>
+      </c>
+      <c r="D2084" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2084" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2084" s="10" t="s">
+        <v>2556</v>
+      </c>
       <c r="G2084" s="11"/>
       <c r="H2084" s="12"/>
       <c r="I2084" s="13"/>
       <c r="J2084" s="13"/>
     </row>
     <row r="2085" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2085" s="12"/>
+      <c r="A2085" s="12">
+        <v>44623</v>
+      </c>
       <c r="B2085" s="12"/>
-      <c r="C2085" s="14"/>
-      <c r="D2085" s="10"/>
-      <c r="E2085" s="11"/>
-      <c r="F2085" s="10"/>
+      <c r="C2085" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="D2085" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2085" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2085" s="10" t="s">
+        <v>2574</v>
+      </c>
       <c r="G2085" s="11"/>
       <c r="H2085" s="12"/>
       <c r="I2085" s="13"/>
       <c r="J2085" s="13"/>
     </row>
-    <row r="2086" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2086" s="12"/>
+    <row r="2086" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2086" s="12">
+        <v>44522</v>
+      </c>
       <c r="B2086" s="12"/>
-      <c r="C2086" s="14"/>
-      <c r="D2086" s="10"/>
-      <c r="E2086" s="11"/>
-      <c r="F2086" s="10"/>
+      <c r="C2086" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2086" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2086" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2086" s="10" t="s">
+        <v>2351</v>
+      </c>
       <c r="G2086" s="11"/>
       <c r="H2086" s="12"/>
       <c r="I2086" s="13"/>
@@ -72101,7 +72244,7 @@
     </row>
     <row r="2088" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2088" s="12"/>
-      <c r="B2088" s="9"/>
+      <c r="B2088" s="12"/>
       <c r="C2088" s="14"/>
       <c r="D2088" s="10"/>
       <c r="E2088" s="11"/>
@@ -72112,38 +72255,20 @@
       <c r="J2088" s="13"/>
     </row>
     <row r="2089" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2089" s="1" t="s">
-        <v>1472</v>
-      </c>
-      <c r="B2089" s="2" t="s">
-        <v>1473</v>
-      </c>
-      <c r="C2089" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2089" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2089" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="F2089" s="4" t="s">
-        <v>1571</v>
-      </c>
-      <c r="G2089" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2089" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2089" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2089" s="36"/>
+      <c r="A2089" s="12"/>
+      <c r="B2089" s="12"/>
+      <c r="C2089" s="14"/>
+      <c r="D2089" s="10"/>
+      <c r="E2089" s="11"/>
+      <c r="F2089" s="10"/>
+      <c r="G2089" s="11"/>
+      <c r="H2089" s="12"/>
+      <c r="I2089" s="13"/>
+      <c r="J2089" s="13"/>
     </row>
     <row r="2090" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2090" s="12"/>
-      <c r="B2090" s="9"/>
+      <c r="B2090" s="12"/>
       <c r="C2090" s="14"/>
       <c r="D2090" s="10"/>
       <c r="E2090" s="11"/>
@@ -72165,298 +72290,316 @@
       <c r="I2091" s="13"/>
       <c r="J2091" s="13"/>
     </row>
-    <row r="2092" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A2092" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2092" s="9"/>
-      <c r="C2092" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2092" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2092" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2092" s="10" t="s">
-        <v>1637</v>
-      </c>
-      <c r="G2092" s="11"/>
-      <c r="H2092" s="12"/>
-      <c r="I2092" s="13"/>
-      <c r="J2092" s="13" t="s">
-        <v>1660</v>
-      </c>
-    </row>
-    <row r="2093" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A2093" s="12">
-        <v>44252</v>
-      </c>
+    <row r="2092" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2092" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B2092" s="2" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C2092" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2092" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2092" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F2092" s="4" t="s">
+        <v>1571</v>
+      </c>
+      <c r="G2092" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2092" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2092" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2092" s="36"/>
+    </row>
+    <row r="2093" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2093" s="12"/>
       <c r="B2093" s="9"/>
-      <c r="C2093" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2093" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2093" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2093" s="10" t="s">
-        <v>1636</v>
-      </c>
+      <c r="C2093" s="14"/>
+      <c r="D2093" s="10"/>
+      <c r="E2093" s="11"/>
+      <c r="F2093" s="10"/>
       <c r="G2093" s="11"/>
       <c r="H2093" s="12"/>
       <c r="I2093" s="13"/>
       <c r="J2093" s="13"/>
     </row>
-    <row r="2094" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2094" s="12">
-        <v>44112</v>
-      </c>
+    <row r="2094" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2094" s="12"/>
       <c r="B2094" s="9"/>
-      <c r="C2094" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D2094" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2094" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2094" s="10" t="s">
-        <v>2223</v>
-      </c>
+      <c r="C2094" s="14"/>
+      <c r="D2094" s="10"/>
+      <c r="E2094" s="11"/>
+      <c r="F2094" s="10"/>
       <c r="G2094" s="11"/>
       <c r="H2094" s="12"/>
       <c r="I2094" s="13"/>
       <c r="J2094" s="13"/>
     </row>
-    <row r="2095" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2095" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A2095" s="12">
-        <v>44088</v>
+        <v>44252</v>
       </c>
       <c r="B2095" s="9"/>
       <c r="C2095" s="14" t="s">
-        <v>19</v>
+        <v>895</v>
       </c>
       <c r="D2095" s="10" t="s">
-        <v>902</v>
+        <v>492</v>
       </c>
       <c r="E2095" s="11" t="s">
-        <v>683</v>
+        <v>757</v>
       </c>
       <c r="F2095" s="10" t="s">
-        <v>1007</v>
+        <v>1637</v>
       </c>
       <c r="G2095" s="11"/>
       <c r="H2095" s="12"/>
       <c r="I2095" s="13"/>
-      <c r="J2095" s="13"/>
-    </row>
-    <row r="2096" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J2095" s="13" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="2096" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A2096" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B2096" s="9"/>
       <c r="C2096" s="14" t="s">
-        <v>621</v>
+        <v>895</v>
       </c>
       <c r="D2096" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2096" s="11" t="s">
-        <v>568</v>
+        <v>757</v>
       </c>
       <c r="F2096" s="10" t="s">
-        <v>900</v>
+        <v>1636</v>
       </c>
       <c r="G2096" s="11"/>
       <c r="H2096" s="12"/>
       <c r="I2096" s="13"/>
       <c r="J2096" s="13"/>
     </row>
-    <row r="2097" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2097" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2097" s="12">
-        <v>44055</v>
+        <v>44112</v>
       </c>
       <c r="B2097" s="9"/>
       <c r="C2097" s="14" t="s">
-        <v>895</v>
+        <v>621</v>
       </c>
       <c r="D2097" s="10" t="s">
-        <v>492</v>
+        <v>6</v>
       </c>
       <c r="E2097" s="11" t="s">
         <v>568</v>
       </c>
       <c r="F2097" s="10" t="s">
-        <v>897</v>
+        <v>2223</v>
       </c>
       <c r="G2097" s="11"/>
       <c r="H2097" s="12"/>
       <c r="I2097" s="13"/>
       <c r="J2097" s="13"/>
     </row>
-    <row r="2098" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="2098" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2098" s="12">
-        <v>44055</v>
+        <v>44088</v>
       </c>
       <c r="B2098" s="9"/>
       <c r="C2098" s="14" t="s">
-        <v>895</v>
+        <v>19</v>
       </c>
       <c r="D2098" s="10" t="s">
-        <v>492</v>
+        <v>902</v>
       </c>
       <c r="E2098" s="11" t="s">
-        <v>568</v>
+        <v>683</v>
       </c>
       <c r="F2098" s="10" t="s">
-        <v>898</v>
+        <v>1007</v>
       </c>
       <c r="G2098" s="11"/>
       <c r="H2098" s="12"/>
       <c r="I2098" s="13"/>
       <c r="J2098" s="13"/>
     </row>
-    <row r="2099" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="2099" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2099" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B2099" s="9"/>
       <c r="C2099" s="14" t="s">
-        <v>468</v>
+        <v>621</v>
       </c>
       <c r="D2099" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E2099" s="11" t="s">
-        <v>683</v>
+        <v>568</v>
       </c>
       <c r="F2099" s="10" t="s">
-        <v>684</v>
-      </c>
-      <c r="G2099" s="11" t="s">
-        <v>1617</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="G2099" s="11"/>
       <c r="H2099" s="12"/>
-      <c r="I2099" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I2099" s="13"/>
       <c r="J2099" s="13"/>
     </row>
-    <row r="2100" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="2100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2100" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B2100" s="9"/>
       <c r="C2100" s="14" t="s">
-        <v>468</v>
+        <v>895</v>
       </c>
       <c r="D2100" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E2100" s="11" t="s">
-        <v>683</v>
+        <v>568</v>
       </c>
       <c r="F2100" s="10" t="s">
-        <v>703</v>
-      </c>
-      <c r="G2100" s="11" t="s">
-        <v>685</v>
-      </c>
+        <v>897</v>
+      </c>
+      <c r="G2100" s="11"/>
       <c r="H2100" s="12"/>
-      <c r="I2100" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J2100" s="13" t="s">
-        <v>1561</v>
-      </c>
-    </row>
-    <row r="2101" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I2100" s="13"/>
+      <c r="J2100" s="13"/>
+    </row>
+    <row r="2101" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A2101" s="12">
-        <v>43838</v>
+        <v>44055</v>
       </c>
       <c r="B2101" s="9"/>
       <c r="C2101" s="14" t="s">
-        <v>103</v>
+        <v>895</v>
       </c>
       <c r="D2101" s="10" t="s">
-        <v>460</v>
+        <v>492</v>
       </c>
       <c r="E2101" s="11" t="s">
-        <v>645</v>
+        <v>568</v>
       </c>
       <c r="F2101" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="G2101" s="11" t="s">
-        <v>1618</v>
-      </c>
+        <v>898</v>
+      </c>
+      <c r="G2101" s="11"/>
       <c r="H2101" s="12"/>
       <c r="I2101" s="13"/>
-      <c r="J2101" s="13" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="2102" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J2101" s="13"/>
+    </row>
+    <row r="2102" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A2102" s="12">
-        <v>43762</v>
+        <v>43949</v>
       </c>
       <c r="B2102" s="9"/>
       <c r="C2102" s="14" t="s">
-        <v>446</v>
+        <v>468</v>
       </c>
       <c r="D2102" s="10" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="E2102" s="11" t="s">
-        <v>835</v>
+        <v>683</v>
       </c>
       <c r="F2102" s="10" t="s">
-        <v>447</v>
+        <v>684</v>
       </c>
       <c r="G2102" s="11" t="s">
-        <v>1607</v>
+        <v>1617</v>
       </c>
       <c r="H2102" s="12"/>
-      <c r="I2102" s="13"/>
+      <c r="I2102" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J2102" s="13"/>
     </row>
-    <row r="2103" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2103" s="12"/>
+    <row r="2103" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2103" s="12">
+        <v>43949</v>
+      </c>
       <c r="B2103" s="9"/>
-      <c r="C2103" s="14"/>
-      <c r="D2103" s="10"/>
-      <c r="E2103" s="11"/>
-      <c r="F2103" s="10"/>
-      <c r="G2103" s="11"/>
+      <c r="C2103" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2103" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2103" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2103" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="G2103" s="11" t="s">
+        <v>685</v>
+      </c>
       <c r="H2103" s="12"/>
-      <c r="I2103" s="13"/>
-      <c r="J2103" s="13"/>
-    </row>
-    <row r="2104" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2104" s="12"/>
+      <c r="I2103" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J2103" s="13" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="2104" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2104" s="12">
+        <v>43838</v>
+      </c>
       <c r="B2104" s="9"/>
-      <c r="C2104" s="14"/>
-      <c r="D2104" s="10"/>
-      <c r="E2104" s="11"/>
-      <c r="F2104" s="10"/>
-      <c r="G2104" s="11"/>
+      <c r="C2104" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2104" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2104" s="11" t="s">
+        <v>645</v>
+      </c>
+      <c r="F2104" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="G2104" s="11" t="s">
+        <v>1618</v>
+      </c>
       <c r="H2104" s="12"/>
       <c r="I2104" s="13"/>
-      <c r="J2104" s="13"/>
-    </row>
-    <row r="2105" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2105" s="12"/>
+      <c r="J2104" s="13" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="2105" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2105" s="12">
+        <v>43762</v>
+      </c>
       <c r="B2105" s="9"/>
-      <c r="C2105" s="14"/>
-      <c r="D2105" s="10"/>
-      <c r="E2105" s="11"/>
-      <c r="F2105" s="10"/>
-      <c r="G2105" s="11"/>
+      <c r="C2105" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D2105" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2105" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2105" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G2105" s="11" t="s">
+        <v>1607</v>
+      </c>
       <c r="H2105" s="12"/>
       <c r="I2105" s="13"/>
       <c r="J2105" s="13"/>
@@ -72496,6 +72639,42 @@
       <c r="H2108" s="12"/>
       <c r="I2108" s="13"/>
       <c r="J2108" s="13"/>
+    </row>
+    <row r="2109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2109" s="12"/>
+      <c r="B2109" s="9"/>
+      <c r="C2109" s="14"/>
+      <c r="D2109" s="10"/>
+      <c r="E2109" s="11"/>
+      <c r="F2109" s="10"/>
+      <c r="G2109" s="11"/>
+      <c r="H2109" s="12"/>
+      <c r="I2109" s="13"/>
+      <c r="J2109" s="13"/>
+    </row>
+    <row r="2110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2110" s="12"/>
+      <c r="B2110" s="9"/>
+      <c r="C2110" s="14"/>
+      <c r="D2110" s="10"/>
+      <c r="E2110" s="11"/>
+      <c r="F2110" s="10"/>
+      <c r="G2110" s="11"/>
+      <c r="H2110" s="12"/>
+      <c r="I2110" s="13"/>
+      <c r="J2110" s="13"/>
+    </row>
+    <row r="2111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2111" s="12"/>
+      <c r="B2111" s="9"/>
+      <c r="C2111" s="14"/>
+      <c r="D2111" s="10"/>
+      <c r="E2111" s="11"/>
+      <c r="F2111" s="10"/>
+      <c r="G2111" s="11"/>
+      <c r="H2111" s="12"/>
+      <c r="I2111" s="13"/>
+      <c r="J2111" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1881" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Gravar campos C5_XXREV e C5_XXPARC
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12B1AE5-D0DB-41BF-B260-C6E4772DB430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8385F21A-5CA2-46AD-B500-178EE1BE0A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14751" uniqueCount="2841">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14784" uniqueCount="2847">
   <si>
     <t>Responsável</t>
   </si>
@@ -8980,6 +8980,25 @@
   </si>
   <si>
     <t>Alterado o programa BKGrupos para considerar a empresa 12 e a usuária financeiro.seguros com superior o usuário 000153 - Bruno Bueno</t>
+  </si>
+  <si>
+    <t>CN121PED</t>
+  </si>
+  <si>
+    <t>Correção via banco de dados de inconsistências na tabela CND das empresas 01, 02 e 14 causadas em falha de gravação na versão 11 e medição antiga.
+Gravação dos campos C5_XXREV e C5_XXPARC para gerar informações a serem utilizadas pelos relatórios, gerando maior performace (será necessário alterar os relatórios existentes).</t>
+  </si>
+  <si>
+    <t>Criação do usuário noe.braga</t>
+  </si>
+  <si>
+    <t>Criar novo grupo para o usuário noe.braga apenas com consultas</t>
+  </si>
+  <si>
+    <t>Problemas com a baixa da PA 392807LPM</t>
+  </si>
+  <si>
+    <t>Gerar arquivo ECD (foram realizadas diversas correções: Inclusão de contas referenciais e contas contabeis (não foram cadastradas corretamente), campos não preenchidos no plano de contas e alteração de centro de custo excluído)</t>
   </si>
 </sst>
 </file>
@@ -9785,11 +9804,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J2111"/>
+  <dimension ref="A1:J2117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2068" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2072" sqref="A2072"/>
+      <pane ySplit="1" topLeftCell="A2071" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2077" sqref="B2077"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -18780,7 +18799,7 @@
       </c>
       <c r="J324" s="13"/>
     </row>
-    <row r="325" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A325" s="12">
         <v>43760</v>
       </c>
@@ -45732,7 +45751,7 @@
       </c>
       <c r="J1212" s="13"/>
     </row>
-    <row r="1213" spans="1:10" ht="72" x14ac:dyDescent="0.2">
+    <row r="1213" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A1213" s="12">
         <v>44271</v>
       </c>
@@ -48236,7 +48255,7 @@
       </c>
       <c r="J1294" s="13"/>
     </row>
-    <row r="1295" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1295" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1295" s="12">
         <v>44315</v>
       </c>
@@ -53504,7 +53523,7 @@
         <v>2107</v>
       </c>
     </row>
-    <row r="1468" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="1468" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1468" s="12">
         <v>44399</v>
       </c>
@@ -59582,7 +59601,7 @@
       </c>
       <c r="J1667" s="13"/>
     </row>
-    <row r="1668" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="1668" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1668" s="12">
         <v>44518</v>
       </c>
@@ -66108,7 +66127,7 @@
       </c>
       <c r="J1881" s="13"/>
     </row>
-    <row r="1882" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1882" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A1882" s="12">
         <v>44631</v>
       </c>
@@ -71926,183 +71945,205 @@
         <v>2840</v>
       </c>
     </row>
-    <row r="2072" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2072" s="12"/>
-      <c r="B2072" s="12"/>
-      <c r="C2072" s="10"/>
-      <c r="D2072" s="10"/>
-      <c r="E2072" s="11"/>
-      <c r="F2072" s="10"/>
-      <c r="G2072" s="11"/>
-      <c r="H2072" s="12"/>
-      <c r="I2072" s="13"/>
-      <c r="J2072" s="13"/>
-    </row>
-    <row r="2073" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2073" s="12"/>
-      <c r="B2073" s="12"/>
-      <c r="C2073" s="10"/>
-      <c r="D2073" s="10"/>
-      <c r="E2073" s="11"/>
-      <c r="F2073" s="10"/>
-      <c r="G2073" s="11"/>
-      <c r="H2073" s="12"/>
-      <c r="I2073" s="13"/>
+    <row r="2072" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="A2072" s="12">
+        <v>44708</v>
+      </c>
+      <c r="B2072" s="12">
+        <v>44708</v>
+      </c>
+      <c r="C2072" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2072" s="10" t="s">
+        <v>582</v>
+      </c>
+      <c r="E2072" s="11" t="s">
+        <v>696</v>
+      </c>
+      <c r="F2072" s="10" t="s">
+        <v>2842</v>
+      </c>
+      <c r="G2072" s="11" t="s">
+        <v>1602</v>
+      </c>
+      <c r="H2072" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2072" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2072" s="13" t="s">
+        <v>2841</v>
+      </c>
+    </row>
+    <row r="2073" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2073" s="12">
+        <v>44708</v>
+      </c>
+      <c r="B2073" s="12">
+        <v>44708</v>
+      </c>
+      <c r="C2073" s="10" t="s">
+        <v>2156</v>
+      </c>
+      <c r="D2073" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2073" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2073" s="10" t="s">
+        <v>2846</v>
+      </c>
+      <c r="G2073" s="11" t="s">
+        <v>1602</v>
+      </c>
+      <c r="H2073" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2073" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2073" s="13"/>
     </row>
     <row r="2074" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2074" s="12"/>
-      <c r="B2074" s="12"/>
-      <c r="C2074" s="10"/>
-      <c r="D2074" s="10"/>
-      <c r="E2074" s="11"/>
-      <c r="F2074" s="10"/>
-      <c r="G2074" s="11"/>
-      <c r="H2074" s="12"/>
-      <c r="I2074" s="13"/>
+      <c r="A2074" s="12">
+        <v>44708</v>
+      </c>
+      <c r="B2074" s="12">
+        <v>44708</v>
+      </c>
+      <c r="C2074" s="10" t="s">
+        <v>1925</v>
+      </c>
+      <c r="D2074" s="10" t="s">
+        <v>749</v>
+      </c>
+      <c r="E2074" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2074" s="10" t="s">
+        <v>2843</v>
+      </c>
+      <c r="G2074" s="11" t="s">
+        <v>1624</v>
+      </c>
+      <c r="H2074" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2074" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2074" s="13"/>
     </row>
-    <row r="2075" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="2075" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2075" s="12">
-        <v>44698</v>
+        <v>44708</v>
       </c>
       <c r="B2075" s="12"/>
       <c r="C2075" s="10" t="s">
-        <v>895</v>
+        <v>446</v>
       </c>
       <c r="D2075" s="10" t="s">
-        <v>492</v>
+        <v>166</v>
       </c>
       <c r="E2075" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2075" s="30" t="s">
-        <v>2799</v>
+        <v>683</v>
+      </c>
+      <c r="F2075" s="10" t="s">
+        <v>2844</v>
       </c>
       <c r="G2075" s="11"/>
       <c r="H2075" s="12"/>
       <c r="I2075" s="13"/>
       <c r="J2075" s="13"/>
     </row>
-    <row r="2076" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="2076" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2076" s="12">
-        <v>44684</v>
-      </c>
-      <c r="B2076" s="12"/>
-      <c r="C2076" s="14" t="s">
-        <v>2156</v>
+        <v>44708</v>
+      </c>
+      <c r="B2076" s="12">
+        <v>44708</v>
+      </c>
+      <c r="C2076" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="D2076" s="10" t="s">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="E2076" s="11" t="s">
         <v>618</v>
       </c>
       <c r="F2076" s="10" t="s">
-        <v>2800</v>
-      </c>
-      <c r="G2076" s="11"/>
-      <c r="H2076" s="12"/>
-      <c r="I2076" s="13"/>
+        <v>2845</v>
+      </c>
+      <c r="G2076" s="11" t="s">
+        <v>1599</v>
+      </c>
+      <c r="H2076" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2076" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2076" s="13"/>
     </row>
-    <row r="2077" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2077" s="12">
-        <v>44677</v>
-      </c>
+    <row r="2077" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2077" s="12"/>
       <c r="B2077" s="12"/>
-      <c r="C2077" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="D2077" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2077" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2077" s="10" t="s">
-        <v>2730</v>
-      </c>
+      <c r="C2077" s="10"/>
+      <c r="D2077" s="10"/>
+      <c r="E2077" s="11"/>
+      <c r="F2077" s="10"/>
       <c r="G2077" s="11"/>
       <c r="H2077" s="12"/>
       <c r="I2077" s="13"/>
       <c r="J2077" s="13"/>
     </row>
     <row r="2078" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2078" s="12">
-        <v>44649</v>
-      </c>
+      <c r="A2078" s="12"/>
       <c r="B2078" s="12"/>
-      <c r="C2078" s="14" t="s">
-        <v>1969</v>
-      </c>
-      <c r="D2078" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2078" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2078" s="10" t="s">
-        <v>2654</v>
-      </c>
+      <c r="C2078" s="10"/>
+      <c r="D2078" s="10"/>
+      <c r="E2078" s="11"/>
+      <c r="F2078" s="10"/>
       <c r="G2078" s="11"/>
       <c r="H2078" s="12"/>
-      <c r="I2078" s="13" t="s">
-        <v>13</v>
-      </c>
+      <c r="I2078" s="13"/>
       <c r="J2078" s="13"/>
     </row>
-    <row r="2079" spans="1:10" ht="132" x14ac:dyDescent="0.2">
-      <c r="A2079" s="12">
-        <v>44645</v>
-      </c>
+    <row r="2079" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2079" s="12"/>
       <c r="B2079" s="12"/>
-      <c r="C2079" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D2079" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2079" s="11" t="s">
-        <v>618</v>
-      </c>
-      <c r="F2079" s="10" t="s">
-        <v>2665</v>
-      </c>
+      <c r="C2079" s="10"/>
+      <c r="D2079" s="10"/>
+      <c r="E2079" s="11"/>
+      <c r="F2079" s="10"/>
       <c r="G2079" s="11"/>
       <c r="H2079" s="12"/>
       <c r="I2079" s="13"/>
       <c r="J2079" s="13"/>
     </row>
     <row r="2080" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2080" s="12">
-        <v>44642</v>
-      </c>
+      <c r="A2080" s="12"/>
       <c r="B2080" s="12"/>
-      <c r="C2080" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="D2080" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2080" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2080" s="10" t="s">
-        <v>2626</v>
-      </c>
+      <c r="C2080" s="10"/>
+      <c r="D2080" s="10"/>
+      <c r="E2080" s="11"/>
+      <c r="F2080" s="10"/>
       <c r="G2080" s="11"/>
       <c r="H2080" s="12"/>
       <c r="I2080" s="13"/>
       <c r="J2080" s="13"/>
     </row>
-    <row r="2081" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2081" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2081" s="12">
-        <v>44642</v>
+        <v>44698</v>
       </c>
       <c r="B2081" s="12"/>
-      <c r="C2081" s="14" t="s">
-        <v>387</v>
+      <c r="C2081" s="10" t="s">
+        <v>895</v>
       </c>
       <c r="D2081" s="10" t="s">
         <v>492</v>
@@ -72110,45 +72151,43 @@
       <c r="E2081" s="11" t="s">
         <v>835</v>
       </c>
-      <c r="F2081" s="10" t="s">
-        <v>2625</v>
+      <c r="F2081" s="30" t="s">
+        <v>2799</v>
       </c>
       <c r="G2081" s="11"/>
       <c r="H2081" s="12"/>
       <c r="I2081" s="13"/>
       <c r="J2081" s="13"/>
     </row>
-    <row r="2082" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2082" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2082" s="12">
-        <v>44614</v>
-      </c>
-      <c r="B2082" s="12">
-        <v>44614</v>
-      </c>
+        <v>44684</v>
+      </c>
+      <c r="B2082" s="12"/>
       <c r="C2082" s="14" t="s">
-        <v>19</v>
+        <v>2156</v>
       </c>
       <c r="D2082" s="10" t="s">
-        <v>492</v>
+        <v>83</v>
       </c>
       <c r="E2082" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F2082" s="10" t="s">
-        <v>2529</v>
+        <v>2800</v>
       </c>
       <c r="G2082" s="11"/>
       <c r="H2082" s="12"/>
       <c r="I2082" s="13"/>
       <c r="J2082" s="13"/>
     </row>
-    <row r="2083" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2083" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2083" s="12">
-        <v>44614</v>
+        <v>44677</v>
       </c>
       <c r="B2083" s="12"/>
       <c r="C2083" s="14" t="s">
-        <v>19</v>
+        <v>387</v>
       </c>
       <c r="D2083" s="10" t="s">
         <v>492</v>
@@ -72157,7 +72196,7 @@
         <v>835</v>
       </c>
       <c r="F2083" s="10" t="s">
-        <v>2549</v>
+        <v>2730</v>
       </c>
       <c r="G2083" s="11"/>
       <c r="H2083" s="12"/>
@@ -72166,64 +72205,66 @@
     </row>
     <row r="2084" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2084" s="12">
-        <v>44616</v>
+        <v>44649</v>
       </c>
       <c r="B2084" s="12"/>
       <c r="C2084" s="14" t="s">
-        <v>2251</v>
+        <v>1969</v>
       </c>
       <c r="D2084" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E2084" s="11" t="s">
-        <v>618</v>
+        <v>835</v>
       </c>
       <c r="F2084" s="10" t="s">
-        <v>2556</v>
+        <v>2654</v>
       </c>
       <c r="G2084" s="11"/>
       <c r="H2084" s="12"/>
-      <c r="I2084" s="13"/>
+      <c r="I2084" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2084" s="13"/>
     </row>
-    <row r="2085" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2085" spans="1:10" ht="132" x14ac:dyDescent="0.2">
       <c r="A2085" s="12">
-        <v>44623</v>
+        <v>44645</v>
       </c>
       <c r="B2085" s="12"/>
       <c r="C2085" s="14" t="s">
-        <v>535</v>
+        <v>288</v>
       </c>
       <c r="D2085" s="10" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E2085" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F2085" s="10" t="s">
-        <v>2574</v>
+        <v>2665</v>
       </c>
       <c r="G2085" s="11"/>
       <c r="H2085" s="12"/>
       <c r="I2085" s="13"/>
       <c r="J2085" s="13"/>
     </row>
-    <row r="2086" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="2086" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2086" s="12">
-        <v>44522</v>
+        <v>44642</v>
       </c>
       <c r="B2086" s="12"/>
       <c r="C2086" s="14" t="s">
-        <v>46</v>
+        <v>387</v>
       </c>
       <c r="D2086" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2086" s="11" t="s">
-        <v>568</v>
+        <v>835</v>
       </c>
       <c r="F2086" s="10" t="s">
-        <v>2351</v>
+        <v>2626</v>
       </c>
       <c r="G2086" s="11"/>
       <c r="H2086" s="12"/>
@@ -72231,98 +72272,142 @@
       <c r="J2086" s="13"/>
     </row>
     <row r="2087" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2087" s="12"/>
+      <c r="A2087" s="12">
+        <v>44642</v>
+      </c>
       <c r="B2087" s="12"/>
-      <c r="C2087" s="14"/>
-      <c r="D2087" s="10"/>
-      <c r="E2087" s="11"/>
-      <c r="F2087" s="10"/>
+      <c r="C2087" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2087" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2087" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2087" s="10" t="s">
+        <v>2625</v>
+      </c>
       <c r="G2087" s="11"/>
       <c r="H2087" s="12"/>
       <c r="I2087" s="13"/>
       <c r="J2087" s="13"/>
     </row>
     <row r="2088" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2088" s="12"/>
-      <c r="B2088" s="12"/>
-      <c r="C2088" s="14"/>
-      <c r="D2088" s="10"/>
-      <c r="E2088" s="11"/>
-      <c r="F2088" s="10"/>
+      <c r="A2088" s="12">
+        <v>44614</v>
+      </c>
+      <c r="B2088" s="12">
+        <v>44614</v>
+      </c>
+      <c r="C2088" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2088" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2088" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2088" s="10" t="s">
+        <v>2529</v>
+      </c>
       <c r="G2088" s="11"/>
       <c r="H2088" s="12"/>
       <c r="I2088" s="13"/>
       <c r="J2088" s="13"/>
     </row>
     <row r="2089" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2089" s="12"/>
+      <c r="A2089" s="12">
+        <v>44614</v>
+      </c>
       <c r="B2089" s="12"/>
-      <c r="C2089" s="14"/>
-      <c r="D2089" s="10"/>
-      <c r="E2089" s="11"/>
-      <c r="F2089" s="10"/>
+      <c r="C2089" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2089" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2089" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2089" s="10" t="s">
+        <v>2549</v>
+      </c>
       <c r="G2089" s="11"/>
       <c r="H2089" s="12"/>
       <c r="I2089" s="13"/>
       <c r="J2089" s="13"/>
     </row>
     <row r="2090" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2090" s="12"/>
+      <c r="A2090" s="12">
+        <v>44616</v>
+      </c>
       <c r="B2090" s="12"/>
-      <c r="C2090" s="14"/>
-      <c r="D2090" s="10"/>
-      <c r="E2090" s="11"/>
-      <c r="F2090" s="10"/>
+      <c r="C2090" s="14" t="s">
+        <v>2251</v>
+      </c>
+      <c r="D2090" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2090" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2090" s="10" t="s">
+        <v>2556</v>
+      </c>
       <c r="G2090" s="11"/>
       <c r="H2090" s="12"/>
       <c r="I2090" s="13"/>
       <c r="J2090" s="13"/>
     </row>
     <row r="2091" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2091" s="12"/>
-      <c r="B2091" s="9"/>
-      <c r="C2091" s="14"/>
-      <c r="D2091" s="10"/>
-      <c r="E2091" s="11"/>
-      <c r="F2091" s="10"/>
+      <c r="A2091" s="12">
+        <v>44623</v>
+      </c>
+      <c r="B2091" s="12"/>
+      <c r="C2091" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="D2091" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2091" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2091" s="10" t="s">
+        <v>2574</v>
+      </c>
       <c r="G2091" s="11"/>
       <c r="H2091" s="12"/>
       <c r="I2091" s="13"/>
       <c r="J2091" s="13"/>
     </row>
-    <row r="2092" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2092" s="1" t="s">
-        <v>1472</v>
-      </c>
-      <c r="B2092" s="2" t="s">
-        <v>1473</v>
-      </c>
-      <c r="C2092" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2092" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2092" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="F2092" s="4" t="s">
-        <v>1571</v>
-      </c>
-      <c r="G2092" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2092" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2092" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2092" s="36"/>
+    <row r="2092" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2092" s="12">
+        <v>44522</v>
+      </c>
+      <c r="B2092" s="12"/>
+      <c r="C2092" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2092" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2092" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2092" s="10" t="s">
+        <v>2351</v>
+      </c>
+      <c r="G2092" s="11"/>
+      <c r="H2092" s="12"/>
+      <c r="I2092" s="13"/>
+      <c r="J2092" s="13"/>
     </row>
     <row r="2093" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2093" s="12"/>
-      <c r="B2093" s="9"/>
+      <c r="B2093" s="12"/>
       <c r="C2093" s="14"/>
       <c r="D2093" s="10"/>
       <c r="E2093" s="11"/>
@@ -72334,7 +72419,7 @@
     </row>
     <row r="2094" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2094" s="12"/>
-      <c r="B2094" s="9"/>
+      <c r="B2094" s="12"/>
       <c r="C2094" s="14"/>
       <c r="D2094" s="10"/>
       <c r="E2094" s="11"/>
@@ -72344,143 +72429,99 @@
       <c r="I2094" s="13"/>
       <c r="J2094" s="13"/>
     </row>
-    <row r="2095" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A2095" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2095" s="9"/>
-      <c r="C2095" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2095" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2095" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2095" s="10" t="s">
-        <v>1637</v>
-      </c>
+    <row r="2095" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2095" s="12"/>
+      <c r="B2095" s="12"/>
+      <c r="C2095" s="14"/>
+      <c r="D2095" s="10"/>
+      <c r="E2095" s="11"/>
+      <c r="F2095" s="10"/>
       <c r="G2095" s="11"/>
       <c r="H2095" s="12"/>
       <c r="I2095" s="13"/>
-      <c r="J2095" s="13" t="s">
-        <v>1660</v>
-      </c>
-    </row>
-    <row r="2096" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A2096" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2096" s="9"/>
-      <c r="C2096" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2096" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2096" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2096" s="10" t="s">
-        <v>1636</v>
-      </c>
+      <c r="J2095" s="13"/>
+    </row>
+    <row r="2096" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2096" s="12"/>
+      <c r="B2096" s="12"/>
+      <c r="C2096" s="14"/>
+      <c r="D2096" s="10"/>
+      <c r="E2096" s="11"/>
+      <c r="F2096" s="10"/>
       <c r="G2096" s="11"/>
       <c r="H2096" s="12"/>
       <c r="I2096" s="13"/>
       <c r="J2096" s="13"/>
     </row>
-    <row r="2097" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2097" s="12">
-        <v>44112</v>
-      </c>
+    <row r="2097" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2097" s="12"/>
       <c r="B2097" s="9"/>
-      <c r="C2097" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D2097" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2097" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2097" s="10" t="s">
-        <v>2223</v>
-      </c>
+      <c r="C2097" s="14"/>
+      <c r="D2097" s="10"/>
+      <c r="E2097" s="11"/>
+      <c r="F2097" s="10"/>
       <c r="G2097" s="11"/>
       <c r="H2097" s="12"/>
       <c r="I2097" s="13"/>
       <c r="J2097" s="13"/>
     </row>
     <row r="2098" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2098" s="12">
-        <v>44088</v>
-      </c>
-      <c r="B2098" s="9"/>
-      <c r="C2098" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2098" s="10" t="s">
-        <v>902</v>
-      </c>
-      <c r="E2098" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="F2098" s="10" t="s">
-        <v>1007</v>
-      </c>
-      <c r="G2098" s="11"/>
-      <c r="H2098" s="12"/>
-      <c r="I2098" s="13"/>
-      <c r="J2098" s="13"/>
+      <c r="A2098" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B2098" s="2" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C2098" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2098" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2098" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F2098" s="4" t="s">
+        <v>1571</v>
+      </c>
+      <c r="G2098" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2098" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2098" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2098" s="36"/>
     </row>
     <row r="2099" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2099" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A2099" s="12"/>
       <c r="B2099" s="9"/>
-      <c r="C2099" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D2099" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2099" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2099" s="10" t="s">
-        <v>900</v>
-      </c>
+      <c r="C2099" s="14"/>
+      <c r="D2099" s="10"/>
+      <c r="E2099" s="11"/>
+      <c r="F2099" s="10"/>
       <c r="G2099" s="11"/>
       <c r="H2099" s="12"/>
       <c r="I2099" s="13"/>
       <c r="J2099" s="13"/>
     </row>
     <row r="2100" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2100" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A2100" s="12"/>
       <c r="B2100" s="9"/>
-      <c r="C2100" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2100" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2100" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2100" s="10" t="s">
-        <v>897</v>
-      </c>
+      <c r="C2100" s="14"/>
+      <c r="D2100" s="10"/>
+      <c r="E2100" s="11"/>
+      <c r="F2100" s="10"/>
       <c r="G2100" s="11"/>
       <c r="H2100" s="12"/>
       <c r="I2100" s="13"/>
       <c r="J2100" s="13"/>
     </row>
-    <row r="2101" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="2101" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A2101" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B2101" s="9"/>
       <c r="C2101" s="14" t="s">
@@ -72490,191 +72531,325 @@
         <v>492</v>
       </c>
       <c r="E2101" s="11" t="s">
-        <v>568</v>
+        <v>757</v>
       </c>
       <c r="F2101" s="10" t="s">
-        <v>898</v>
+        <v>1637</v>
       </c>
       <c r="G2101" s="11"/>
       <c r="H2101" s="12"/>
       <c r="I2101" s="13"/>
-      <c r="J2101" s="13"/>
-    </row>
-    <row r="2102" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="J2101" s="13" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="2102" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A2102" s="12">
-        <v>43949</v>
+        <v>44252</v>
       </c>
       <c r="B2102" s="9"/>
       <c r="C2102" s="14" t="s">
-        <v>468</v>
+        <v>895</v>
       </c>
       <c r="D2102" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E2102" s="11" t="s">
-        <v>683</v>
+        <v>757</v>
       </c>
       <c r="F2102" s="10" t="s">
-        <v>684</v>
-      </c>
-      <c r="G2102" s="11" t="s">
-        <v>1617</v>
-      </c>
+        <v>1636</v>
+      </c>
+      <c r="G2102" s="11"/>
       <c r="H2102" s="12"/>
-      <c r="I2102" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I2102" s="13"/>
       <c r="J2102" s="13"/>
     </row>
-    <row r="2103" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="2103" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2103" s="12">
-        <v>43949</v>
+        <v>44112</v>
       </c>
       <c r="B2103" s="9"/>
       <c r="C2103" s="14" t="s">
-        <v>468</v>
+        <v>621</v>
       </c>
       <c r="D2103" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E2103" s="11" t="s">
-        <v>683</v>
+        <v>568</v>
       </c>
       <c r="F2103" s="10" t="s">
-        <v>703</v>
-      </c>
-      <c r="G2103" s="11" t="s">
-        <v>685</v>
-      </c>
+        <v>2223</v>
+      </c>
+      <c r="G2103" s="11"/>
       <c r="H2103" s="12"/>
-      <c r="I2103" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J2103" s="13" t="s">
-        <v>1561</v>
-      </c>
-    </row>
-    <row r="2104" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I2103" s="13"/>
+      <c r="J2103" s="13"/>
+    </row>
+    <row r="2104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2104" s="12">
-        <v>43838</v>
+        <v>44088</v>
       </c>
       <c r="B2104" s="9"/>
       <c r="C2104" s="14" t="s">
-        <v>103</v>
+        <v>19</v>
       </c>
       <c r="D2104" s="10" t="s">
-        <v>460</v>
+        <v>902</v>
       </c>
       <c r="E2104" s="11" t="s">
-        <v>645</v>
+        <v>683</v>
       </c>
       <c r="F2104" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="G2104" s="11" t="s">
-        <v>1618</v>
-      </c>
+        <v>1007</v>
+      </c>
+      <c r="G2104" s="11"/>
       <c r="H2104" s="12"/>
       <c r="I2104" s="13"/>
-      <c r="J2104" s="13" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="2105" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J2104" s="13"/>
+    </row>
+    <row r="2105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2105" s="12">
-        <v>43762</v>
+        <v>44055</v>
       </c>
       <c r="B2105" s="9"/>
       <c r="C2105" s="14" t="s">
-        <v>446</v>
+        <v>621</v>
       </c>
       <c r="D2105" s="10" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E2105" s="11" t="s">
-        <v>835</v>
+        <v>568</v>
       </c>
       <c r="F2105" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G2105" s="11" t="s">
-        <v>1607</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="G2105" s="11"/>
       <c r="H2105" s="12"/>
       <c r="I2105" s="13"/>
       <c r="J2105" s="13"/>
     </row>
     <row r="2106" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2106" s="12"/>
+      <c r="A2106" s="12">
+        <v>44055</v>
+      </c>
       <c r="B2106" s="9"/>
-      <c r="C2106" s="14"/>
-      <c r="D2106" s="10"/>
-      <c r="E2106" s="11"/>
-      <c r="F2106" s="10"/>
+      <c r="C2106" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2106" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2106" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2106" s="10" t="s">
+        <v>897</v>
+      </c>
       <c r="G2106" s="11"/>
       <c r="H2106" s="12"/>
       <c r="I2106" s="13"/>
       <c r="J2106" s="13"/>
     </row>
-    <row r="2107" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2107" s="12"/>
+    <row r="2107" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A2107" s="12">
+        <v>44055</v>
+      </c>
       <c r="B2107" s="9"/>
-      <c r="C2107" s="14"/>
-      <c r="D2107" s="10"/>
-      <c r="E2107" s="11"/>
-      <c r="F2107" s="10"/>
+      <c r="C2107" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2107" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2107" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2107" s="10" t="s">
+        <v>898</v>
+      </c>
       <c r="G2107" s="11"/>
       <c r="H2107" s="12"/>
       <c r="I2107" s="13"/>
       <c r="J2107" s="13"/>
     </row>
-    <row r="2108" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2108" s="12"/>
+    <row r="2108" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2108" s="12">
+        <v>43949</v>
+      </c>
       <c r="B2108" s="9"/>
-      <c r="C2108" s="14"/>
-      <c r="D2108" s="10"/>
-      <c r="E2108" s="11"/>
-      <c r="F2108" s="10"/>
-      <c r="G2108" s="11"/>
+      <c r="C2108" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2108" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2108" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2108" s="10" t="s">
+        <v>684</v>
+      </c>
+      <c r="G2108" s="11" t="s">
+        <v>1617</v>
+      </c>
       <c r="H2108" s="12"/>
-      <c r="I2108" s="13"/>
+      <c r="I2108" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J2108" s="13"/>
     </row>
-    <row r="2109" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2109" s="12"/>
+    <row r="2109" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2109" s="12">
+        <v>43949</v>
+      </c>
       <c r="B2109" s="9"/>
-      <c r="C2109" s="14"/>
-      <c r="D2109" s="10"/>
-      <c r="E2109" s="11"/>
-      <c r="F2109" s="10"/>
-      <c r="G2109" s="11"/>
+      <c r="C2109" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2109" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2109" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2109" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="G2109" s="11" t="s">
+        <v>685</v>
+      </c>
       <c r="H2109" s="12"/>
-      <c r="I2109" s="13"/>
-      <c r="J2109" s="13"/>
-    </row>
-    <row r="2110" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2110" s="12"/>
+      <c r="I2109" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J2109" s="13" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="2110" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2110" s="12">
+        <v>43838</v>
+      </c>
       <c r="B2110" s="9"/>
-      <c r="C2110" s="14"/>
-      <c r="D2110" s="10"/>
-      <c r="E2110" s="11"/>
-      <c r="F2110" s="10"/>
-      <c r="G2110" s="11"/>
+      <c r="C2110" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2110" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2110" s="11" t="s">
+        <v>645</v>
+      </c>
+      <c r="F2110" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="G2110" s="11" t="s">
+        <v>1618</v>
+      </c>
       <c r="H2110" s="12"/>
       <c r="I2110" s="13"/>
-      <c r="J2110" s="13"/>
-    </row>
-    <row r="2111" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2111" s="12"/>
+      <c r="J2110" s="13" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="2111" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2111" s="12">
+        <v>43762</v>
+      </c>
       <c r="B2111" s="9"/>
-      <c r="C2111" s="14"/>
-      <c r="D2111" s="10"/>
-      <c r="E2111" s="11"/>
-      <c r="F2111" s="10"/>
-      <c r="G2111" s="11"/>
+      <c r="C2111" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D2111" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2111" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2111" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G2111" s="11" t="s">
+        <v>1607</v>
+      </c>
       <c r="H2111" s="12"/>
       <c r="I2111" s="13"/>
       <c r="J2111" s="13"/>
+    </row>
+    <row r="2112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2112" s="12"/>
+      <c r="B2112" s="9"/>
+      <c r="C2112" s="14"/>
+      <c r="D2112" s="10"/>
+      <c r="E2112" s="11"/>
+      <c r="F2112" s="10"/>
+      <c r="G2112" s="11"/>
+      <c r="H2112" s="12"/>
+      <c r="I2112" s="13"/>
+      <c r="J2112" s="13"/>
+    </row>
+    <row r="2113" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2113" s="12"/>
+      <c r="B2113" s="9"/>
+      <c r="C2113" s="14"/>
+      <c r="D2113" s="10"/>
+      <c r="E2113" s="11"/>
+      <c r="F2113" s="10"/>
+      <c r="G2113" s="11"/>
+      <c r="H2113" s="12"/>
+      <c r="I2113" s="13"/>
+      <c r="J2113" s="13"/>
+    </row>
+    <row r="2114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2114" s="12"/>
+      <c r="B2114" s="9"/>
+      <c r="C2114" s="14"/>
+      <c r="D2114" s="10"/>
+      <c r="E2114" s="11"/>
+      <c r="F2114" s="10"/>
+      <c r="G2114" s="11"/>
+      <c r="H2114" s="12"/>
+      <c r="I2114" s="13"/>
+      <c r="J2114" s="13"/>
+    </row>
+    <row r="2115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2115" s="12"/>
+      <c r="B2115" s="9"/>
+      <c r="C2115" s="14"/>
+      <c r="D2115" s="10"/>
+      <c r="E2115" s="11"/>
+      <c r="F2115" s="10"/>
+      <c r="G2115" s="11"/>
+      <c r="H2115" s="12"/>
+      <c r="I2115" s="13"/>
+      <c r="J2115" s="13"/>
+    </row>
+    <row r="2116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2116" s="12"/>
+      <c r="B2116" s="9"/>
+      <c r="C2116" s="14"/>
+      <c r="D2116" s="10"/>
+      <c r="E2116" s="11"/>
+      <c r="F2116" s="10"/>
+      <c r="G2116" s="11"/>
+      <c r="H2116" s="12"/>
+      <c r="I2116" s="13"/>
+      <c r="J2116" s="13"/>
+    </row>
+    <row r="2117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2117" s="12"/>
+      <c r="B2117" s="9"/>
+      <c r="C2117" s="14"/>
+      <c r="D2117" s="10"/>
+      <c r="E2117" s="11"/>
+      <c r="F2117" s="10"/>
+      <c r="G2117" s="11"/>
+      <c r="H2117" s="12"/>
+      <c r="I2117" s="13"/>
+      <c r="J2117" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1881" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Tabela GERAL e GASTOSGERAIS Dashboard
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8385F21A-5CA2-46AD-B500-178EE1BE0A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFB9A46-43C8-42E8-A003-E2321EB9A9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha1" sheetId="3" r:id="rId2"/>
-    <sheet name="Nova Medição" sheetId="2" r:id="rId3"/>
+    <sheet name="Nova Medição" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_FilterDatabase_0" localSheetId="0">'Demandas BK - Protheus'!$A$1:$I$53</definedName>
@@ -78,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14784" uniqueCount="2847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14841" uniqueCount="2856">
   <si>
     <t>Responsável</t>
   </si>
@@ -8999,6 +8998,37 @@
   </si>
   <si>
     <t>Gerar arquivo ECD (foram realizadas diversas correções: Inclusão de contas referenciais e contas contabeis (não foram cadastradas corretamente), campos não preenchidos no plano de contas e alteração de centro de custo excluído)</t>
+  </si>
+  <si>
+    <t>MV_DEISSBS - Indica se o valor do ISS deve ser retirado da base de cálculo do PIS/COFINS/CSLL.
+MV_DEISSBS = .F. - o ISS será descontado na base do PIS/COF/CSLL
+MV_DEISSBS = .T. - o ISS não será descontado na base do PIS/COF/CSLL
+Importante: O parâmetro MV_DEISSBS é exclusivo para operações de saída.</t>
+  </si>
+  <si>
+    <t>Terminei lançando o valor errado , a menor. Gentileza ajustar para o Jardel/Andresa integrar novamente: Titulo 069096MFG da Balsa - de 12,6 para 126,90</t>
+  </si>
+  <si>
+    <t>Auxilio baixas portal petrobras com valor a maior</t>
+  </si>
+  <si>
+    <t>Alterar os formatos de data na geração das tabelas do PowerBk</t>
+  </si>
+  <si>
+    <t>Testes na redução de ISS da Base do Pis/Cofins</t>
+  </si>
+  <si>
+    <t>Alteração das aliquotas de ISS e outros do contrato 153000560</t>
+  </si>
+  <si>
+    <t>Atualização 22-05-27-CENTRAL_DE_ATUALIZACOES_V1_4_3
+Atualização PACOTE_DE_ATUALIZACAO_STORED_PROCEDURES</t>
+  </si>
+  <si>
+    <t>Acerto EFD BK 04/2022: uma NF saída estava com redução de ISS na base</t>
+  </si>
+  <si>
+    <t>Criar grupo igual ao User Gestão apenas para consultas (Basic Gestão)</t>
   </si>
 </sst>
 </file>
@@ -9804,11 +9834,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J2117"/>
+  <dimension ref="A1:J2124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2071" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2077" sqref="B2077"/>
+      <pane ySplit="1" topLeftCell="A2075" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2087" sqref="C2087"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -72089,241 +72119,315 @@
       </c>
       <c r="J2076" s="13"/>
     </row>
-    <row r="2077" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2077" s="12"/>
-      <c r="B2077" s="12"/>
-      <c r="C2077" s="10"/>
-      <c r="D2077" s="10"/>
-      <c r="E2077" s="11"/>
-      <c r="F2077" s="10"/>
-      <c r="G2077" s="11"/>
-      <c r="H2077" s="12"/>
-      <c r="I2077" s="13"/>
+    <row r="2077" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2077" s="12">
+        <v>44711</v>
+      </c>
+      <c r="B2077" s="12">
+        <v>44711</v>
+      </c>
+      <c r="C2077" s="10" t="s">
+        <v>2364</v>
+      </c>
+      <c r="D2077" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="E2077" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2077" s="10" t="s">
+        <v>2848</v>
+      </c>
+      <c r="G2077" s="11" t="s">
+        <v>1599</v>
+      </c>
+      <c r="H2077" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2077" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2077" s="13"/>
     </row>
     <row r="2078" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2078" s="12"/>
-      <c r="B2078" s="12"/>
-      <c r="C2078" s="10"/>
-      <c r="D2078" s="10"/>
-      <c r="E2078" s="11"/>
-      <c r="F2078" s="10"/>
-      <c r="G2078" s="11"/>
-      <c r="H2078" s="12"/>
-      <c r="I2078" s="13"/>
+      <c r="A2078" s="12">
+        <v>44711</v>
+      </c>
+      <c r="B2078" s="12">
+        <v>44711</v>
+      </c>
+      <c r="C2078" s="10" t="s">
+        <v>2677</v>
+      </c>
+      <c r="D2078" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2078" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2078" s="10" t="s">
+        <v>2849</v>
+      </c>
+      <c r="G2078" s="11" t="s">
+        <v>1599</v>
+      </c>
+      <c r="H2078" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2078" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2078" s="13"/>
     </row>
     <row r="2079" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2079" s="12"/>
-      <c r="B2079" s="12"/>
-      <c r="C2079" s="10"/>
-      <c r="D2079" s="10"/>
-      <c r="E2079" s="11"/>
-      <c r="F2079" s="10"/>
-      <c r="G2079" s="11"/>
-      <c r="H2079" s="12"/>
-      <c r="I2079" s="13"/>
+      <c r="A2079" s="12">
+        <v>44711</v>
+      </c>
+      <c r="B2079" s="12">
+        <v>44711</v>
+      </c>
+      <c r="C2079" s="10" t="s">
+        <v>2681</v>
+      </c>
+      <c r="D2079" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2079" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2079" s="10" t="s">
+        <v>2850</v>
+      </c>
+      <c r="G2079" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H2079" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2079" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2079" s="13"/>
     </row>
     <row r="2080" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2080" s="12"/>
-      <c r="B2080" s="12"/>
-      <c r="C2080" s="10"/>
-      <c r="D2080" s="10"/>
-      <c r="E2080" s="11"/>
-      <c r="F2080" s="10"/>
-      <c r="G2080" s="11"/>
-      <c r="H2080" s="12"/>
-      <c r="I2080" s="13"/>
+      <c r="A2080" s="12">
+        <v>44711</v>
+      </c>
+      <c r="B2080" s="12">
+        <v>44711</v>
+      </c>
+      <c r="C2080" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="D2080" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2080" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2080" s="10" t="s">
+        <v>2851</v>
+      </c>
+      <c r="G2080" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H2080" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2080" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2080" s="13"/>
     </row>
-    <row r="2081" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="2081" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2081" s="12">
-        <v>44698</v>
-      </c>
-      <c r="B2081" s="12"/>
+        <v>44711</v>
+      </c>
+      <c r="B2081" s="12">
+        <v>44711</v>
+      </c>
       <c r="C2081" s="10" t="s">
-        <v>895</v>
+        <v>462</v>
       </c>
       <c r="D2081" s="10" t="s">
-        <v>492</v>
+        <v>107</v>
       </c>
       <c r="E2081" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2081" s="30" t="s">
-        <v>2799</v>
-      </c>
-      <c r="G2081" s="11"/>
-      <c r="H2081" s="12"/>
-      <c r="I2081" s="13"/>
+        <v>618</v>
+      </c>
+      <c r="F2081" s="10" t="s">
+        <v>2852</v>
+      </c>
+      <c r="G2081" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H2081" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2081" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2081" s="13"/>
     </row>
-    <row r="2082" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="2082" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2082" s="12">
-        <v>44684</v>
-      </c>
-      <c r="B2082" s="12"/>
-      <c r="C2082" s="14" t="s">
-        <v>2156</v>
+        <v>44711</v>
+      </c>
+      <c r="B2082" s="12">
+        <v>44711</v>
+      </c>
+      <c r="C2082" s="10" t="s">
+        <v>1969</v>
       </c>
       <c r="D2082" s="10" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E2082" s="11" t="s">
         <v>618</v>
       </c>
       <c r="F2082" s="10" t="s">
-        <v>2800</v>
-      </c>
-      <c r="G2082" s="11"/>
-      <c r="H2082" s="12"/>
-      <c r="I2082" s="13"/>
+        <v>2854</v>
+      </c>
+      <c r="G2082" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H2082" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2082" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2082" s="13"/>
     </row>
     <row r="2083" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2083" s="12">
-        <v>44677</v>
-      </c>
-      <c r="B2083" s="12"/>
-      <c r="C2083" s="14" t="s">
-        <v>387</v>
+        <v>44712</v>
+      </c>
+      <c r="B2083" s="12">
+        <v>44712</v>
+      </c>
+      <c r="C2083" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="D2083" s="10" t="s">
-        <v>492</v>
+        <v>582</v>
       </c>
       <c r="E2083" s="11" t="s">
-        <v>835</v>
+        <v>645</v>
       </c>
       <c r="F2083" s="10" t="s">
-        <v>2730</v>
-      </c>
-      <c r="G2083" s="11"/>
-      <c r="H2083" s="12"/>
-      <c r="I2083" s="13"/>
+        <v>2853</v>
+      </c>
+      <c r="G2083" s="11" t="s">
+        <v>1599</v>
+      </c>
+      <c r="H2083" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2083" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2083" s="13"/>
     </row>
     <row r="2084" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2084" s="12">
-        <v>44649</v>
-      </c>
-      <c r="B2084" s="12"/>
-      <c r="C2084" s="14" t="s">
-        <v>1969</v>
+        <v>44708</v>
+      </c>
+      <c r="B2084" s="12">
+        <v>44712</v>
+      </c>
+      <c r="C2084" s="10" t="s">
+        <v>446</v>
       </c>
       <c r="D2084" s="10" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="E2084" s="11" t="s">
-        <v>835</v>
+        <v>667</v>
       </c>
       <c r="F2084" s="10" t="s">
-        <v>2654</v>
-      </c>
-      <c r="G2084" s="11"/>
-      <c r="H2084" s="12"/>
+        <v>2855</v>
+      </c>
+      <c r="G2084" s="11" t="s">
+        <v>1625</v>
+      </c>
+      <c r="H2084" s="12" t="s">
+        <v>112</v>
+      </c>
       <c r="I2084" s="13" t="s">
         <v>13</v>
       </c>
       <c r="J2084" s="13"/>
     </row>
-    <row r="2085" spans="1:10" ht="132" x14ac:dyDescent="0.2">
-      <c r="A2085" s="12">
-        <v>44645</v>
-      </c>
+    <row r="2085" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2085" s="12"/>
       <c r="B2085" s="12"/>
-      <c r="C2085" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D2085" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2085" s="11" t="s">
-        <v>618</v>
-      </c>
-      <c r="F2085" s="10" t="s">
-        <v>2665</v>
-      </c>
+      <c r="C2085" s="10"/>
+      <c r="D2085" s="10"/>
+      <c r="E2085" s="11"/>
+      <c r="F2085" s="10"/>
       <c r="G2085" s="11"/>
       <c r="H2085" s="12"/>
       <c r="I2085" s="13"/>
       <c r="J2085" s="13"/>
     </row>
     <row r="2086" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2086" s="12">
-        <v>44642</v>
-      </c>
+      <c r="A2086" s="12"/>
       <c r="B2086" s="12"/>
-      <c r="C2086" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="D2086" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2086" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2086" s="10" t="s">
-        <v>2626</v>
-      </c>
+      <c r="C2086" s="10"/>
+      <c r="D2086" s="10"/>
+      <c r="E2086" s="11"/>
+      <c r="F2086" s="10"/>
       <c r="G2086" s="11"/>
       <c r="H2086" s="12"/>
       <c r="I2086" s="13"/>
       <c r="J2086" s="13"/>
     </row>
     <row r="2087" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2087" s="12">
-        <v>44642</v>
-      </c>
+      <c r="A2087" s="12"/>
       <c r="B2087" s="12"/>
-      <c r="C2087" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="D2087" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2087" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2087" s="10" t="s">
-        <v>2625</v>
-      </c>
+      <c r="C2087" s="10"/>
+      <c r="D2087" s="10"/>
+      <c r="E2087" s="11"/>
+      <c r="F2087" s="10"/>
       <c r="G2087" s="11"/>
       <c r="H2087" s="12"/>
       <c r="I2087" s="13"/>
       <c r="J2087" s="13"/>
     </row>
-    <row r="2088" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2088" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A2088" s="12">
-        <v>44614</v>
-      </c>
-      <c r="B2088" s="12">
-        <v>44614</v>
-      </c>
+        <v>44649</v>
+      </c>
+      <c r="B2088" s="12"/>
       <c r="C2088" s="14" t="s">
-        <v>19</v>
+        <v>1969</v>
       </c>
       <c r="D2088" s="10" t="s">
-        <v>492</v>
+        <v>89</v>
       </c>
       <c r="E2088" s="11" t="s">
         <v>835</v>
       </c>
       <c r="F2088" s="10" t="s">
-        <v>2529</v>
+        <v>2654</v>
       </c>
       <c r="G2088" s="11"/>
       <c r="H2088" s="12"/>
-      <c r="I2088" s="13"/>
-      <c r="J2088" s="13"/>
-    </row>
-    <row r="2089" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I2088" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2088" s="13" t="s">
+        <v>2847</v>
+      </c>
+    </row>
+    <row r="2089" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2089" s="12">
-        <v>44614</v>
+        <v>44698</v>
       </c>
       <c r="B2089" s="12"/>
-      <c r="C2089" s="14" t="s">
-        <v>19</v>
+      <c r="C2089" s="10" t="s">
+        <v>895</v>
       </c>
       <c r="D2089" s="10" t="s">
         <v>492</v>
@@ -72331,74 +72435,74 @@
       <c r="E2089" s="11" t="s">
         <v>835</v>
       </c>
-      <c r="F2089" s="10" t="s">
-        <v>2549</v>
+      <c r="F2089" s="30" t="s">
+        <v>2799</v>
       </c>
       <c r="G2089" s="11"/>
       <c r="H2089" s="12"/>
       <c r="I2089" s="13"/>
       <c r="J2089" s="13"/>
     </row>
-    <row r="2090" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2090" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2090" s="12">
-        <v>44616</v>
+        <v>44684</v>
       </c>
       <c r="B2090" s="12"/>
       <c r="C2090" s="14" t="s">
-        <v>2251</v>
+        <v>2156</v>
       </c>
       <c r="D2090" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E2090" s="11" t="s">
         <v>618</v>
       </c>
       <c r="F2090" s="10" t="s">
-        <v>2556</v>
+        <v>2800</v>
       </c>
       <c r="G2090" s="11"/>
       <c r="H2090" s="12"/>
       <c r="I2090" s="13"/>
       <c r="J2090" s="13"/>
     </row>
-    <row r="2091" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2091" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2091" s="12">
-        <v>44623</v>
+        <v>44677</v>
       </c>
       <c r="B2091" s="12"/>
       <c r="C2091" s="14" t="s">
-        <v>535</v>
+        <v>387</v>
       </c>
       <c r="D2091" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2091" s="11" t="s">
         <v>835</v>
       </c>
       <c r="F2091" s="10" t="s">
-        <v>2574</v>
+        <v>2730</v>
       </c>
       <c r="G2091" s="11"/>
       <c r="H2091" s="12"/>
       <c r="I2091" s="13"/>
       <c r="J2091" s="13"/>
     </row>
-    <row r="2092" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="2092" spans="1:10" ht="132" x14ac:dyDescent="0.2">
       <c r="A2092" s="12">
-        <v>44522</v>
+        <v>44645</v>
       </c>
       <c r="B2092" s="12"/>
       <c r="C2092" s="14" t="s">
-        <v>46</v>
+        <v>288</v>
       </c>
       <c r="D2092" s="10" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E2092" s="11" t="s">
-        <v>568</v>
+        <v>618</v>
       </c>
       <c r="F2092" s="10" t="s">
-        <v>2351</v>
+        <v>2665</v>
       </c>
       <c r="G2092" s="11"/>
       <c r="H2092" s="12"/>
@@ -72406,102 +72510,156 @@
       <c r="J2092" s="13"/>
     </row>
     <row r="2093" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2093" s="12"/>
+      <c r="A2093" s="12">
+        <v>44642</v>
+      </c>
       <c r="B2093" s="12"/>
-      <c r="C2093" s="14"/>
-      <c r="D2093" s="10"/>
-      <c r="E2093" s="11"/>
-      <c r="F2093" s="10"/>
+      <c r="C2093" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2093" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2093" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2093" s="10" t="s">
+        <v>2626</v>
+      </c>
       <c r="G2093" s="11"/>
       <c r="H2093" s="12"/>
       <c r="I2093" s="13"/>
       <c r="J2093" s="13"/>
     </row>
     <row r="2094" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2094" s="12"/>
+      <c r="A2094" s="12">
+        <v>44642</v>
+      </c>
       <c r="B2094" s="12"/>
-      <c r="C2094" s="14"/>
-      <c r="D2094" s="10"/>
-      <c r="E2094" s="11"/>
-      <c r="F2094" s="10"/>
+      <c r="C2094" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2094" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2094" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2094" s="10" t="s">
+        <v>2625</v>
+      </c>
       <c r="G2094" s="11"/>
       <c r="H2094" s="12"/>
       <c r="I2094" s="13"/>
       <c r="J2094" s="13"/>
     </row>
     <row r="2095" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2095" s="12"/>
-      <c r="B2095" s="12"/>
-      <c r="C2095" s="14"/>
-      <c r="D2095" s="10"/>
-      <c r="E2095" s="11"/>
-      <c r="F2095" s="10"/>
+      <c r="A2095" s="12">
+        <v>44614</v>
+      </c>
+      <c r="B2095" s="12">
+        <v>44614</v>
+      </c>
+      <c r="C2095" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2095" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2095" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2095" s="10" t="s">
+        <v>2529</v>
+      </c>
       <c r="G2095" s="11"/>
       <c r="H2095" s="12"/>
       <c r="I2095" s="13"/>
       <c r="J2095" s="13"/>
     </row>
     <row r="2096" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2096" s="12"/>
+      <c r="A2096" s="12">
+        <v>44614</v>
+      </c>
       <c r="B2096" s="12"/>
-      <c r="C2096" s="14"/>
-      <c r="D2096" s="10"/>
-      <c r="E2096" s="11"/>
-      <c r="F2096" s="10"/>
+      <c r="C2096" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2096" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2096" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2096" s="10" t="s">
+        <v>2549</v>
+      </c>
       <c r="G2096" s="11"/>
       <c r="H2096" s="12"/>
       <c r="I2096" s="13"/>
       <c r="J2096" s="13"/>
     </row>
     <row r="2097" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2097" s="12"/>
-      <c r="B2097" s="9"/>
-      <c r="C2097" s="14"/>
-      <c r="D2097" s="10"/>
-      <c r="E2097" s="11"/>
-      <c r="F2097" s="10"/>
+      <c r="A2097" s="12">
+        <v>44616</v>
+      </c>
+      <c r="B2097" s="12"/>
+      <c r="C2097" s="14" t="s">
+        <v>2251</v>
+      </c>
+      <c r="D2097" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2097" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2097" s="10" t="s">
+        <v>2556</v>
+      </c>
       <c r="G2097" s="11"/>
       <c r="H2097" s="12"/>
       <c r="I2097" s="13"/>
       <c r="J2097" s="13"/>
     </row>
     <row r="2098" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2098" s="1" t="s">
-        <v>1472</v>
-      </c>
-      <c r="B2098" s="2" t="s">
-        <v>1473</v>
-      </c>
-      <c r="C2098" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2098" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2098" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="F2098" s="4" t="s">
-        <v>1571</v>
-      </c>
-      <c r="G2098" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2098" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2098" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2098" s="36"/>
-    </row>
-    <row r="2099" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2099" s="12"/>
-      <c r="B2099" s="9"/>
-      <c r="C2099" s="14"/>
-      <c r="D2099" s="10"/>
-      <c r="E2099" s="11"/>
-      <c r="F2099" s="10"/>
+      <c r="A2098" s="12">
+        <v>44623</v>
+      </c>
+      <c r="B2098" s="12"/>
+      <c r="C2098" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="D2098" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2098" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2098" s="10" t="s">
+        <v>2574</v>
+      </c>
+      <c r="G2098" s="11"/>
+      <c r="H2098" s="12"/>
+      <c r="I2098" s="13"/>
+      <c r="J2098" s="13"/>
+    </row>
+    <row r="2099" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2099" s="12">
+        <v>44522</v>
+      </c>
+      <c r="B2099" s="12"/>
+      <c r="C2099" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2099" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2099" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2099" s="10" t="s">
+        <v>2351</v>
+      </c>
       <c r="G2099" s="11"/>
       <c r="H2099" s="12"/>
       <c r="I2099" s="13"/>
@@ -72509,7 +72667,7 @@
     </row>
     <row r="2100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2100" s="12"/>
-      <c r="B2100" s="9"/>
+      <c r="B2100" s="12"/>
       <c r="C2100" s="14"/>
       <c r="D2100" s="10"/>
       <c r="E2100" s="11"/>
@@ -72519,337 +72677,439 @@
       <c r="I2100" s="13"/>
       <c r="J2100" s="13"/>
     </row>
-    <row r="2101" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A2101" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2101" s="9"/>
-      <c r="C2101" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2101" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2101" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2101" s="10" t="s">
-        <v>1637</v>
-      </c>
+    <row r="2101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2101" s="12"/>
+      <c r="B2101" s="12"/>
+      <c r="C2101" s="14"/>
+      <c r="D2101" s="10"/>
+      <c r="E2101" s="11"/>
+      <c r="F2101" s="10"/>
       <c r="G2101" s="11"/>
       <c r="H2101" s="12"/>
       <c r="I2101" s="13"/>
-      <c r="J2101" s="13" t="s">
-        <v>1660</v>
-      </c>
-    </row>
-    <row r="2102" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A2102" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2102" s="9"/>
-      <c r="C2102" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2102" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2102" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2102" s="10" t="s">
-        <v>1636</v>
-      </c>
+      <c r="J2101" s="13"/>
+    </row>
+    <row r="2102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2102" s="12"/>
+      <c r="B2102" s="12"/>
+      <c r="C2102" s="14"/>
+      <c r="D2102" s="10"/>
+      <c r="E2102" s="11"/>
+      <c r="F2102" s="10"/>
       <c r="G2102" s="11"/>
       <c r="H2102" s="12"/>
       <c r="I2102" s="13"/>
       <c r="J2102" s="13"/>
     </row>
-    <row r="2103" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2103" s="12">
-        <v>44112</v>
-      </c>
-      <c r="B2103" s="9"/>
-      <c r="C2103" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D2103" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2103" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2103" s="10" t="s">
-        <v>2223</v>
-      </c>
+    <row r="2103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2103" s="12"/>
+      <c r="B2103" s="12"/>
+      <c r="C2103" s="14"/>
+      <c r="D2103" s="10"/>
+      <c r="E2103" s="11"/>
+      <c r="F2103" s="10"/>
       <c r="G2103" s="11"/>
       <c r="H2103" s="12"/>
       <c r="I2103" s="13"/>
       <c r="J2103" s="13"/>
     </row>
     <row r="2104" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2104" s="12">
-        <v>44088</v>
-      </c>
+      <c r="A2104" s="12"/>
       <c r="B2104" s="9"/>
-      <c r="C2104" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2104" s="10" t="s">
-        <v>902</v>
-      </c>
-      <c r="E2104" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="F2104" s="10" t="s">
-        <v>1007</v>
-      </c>
+      <c r="C2104" s="14"/>
+      <c r="D2104" s="10"/>
+      <c r="E2104" s="11"/>
+      <c r="F2104" s="10"/>
       <c r="G2104" s="11"/>
       <c r="H2104" s="12"/>
       <c r="I2104" s="13"/>
       <c r="J2104" s="13"/>
     </row>
     <row r="2105" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2105" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B2105" s="9"/>
-      <c r="C2105" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D2105" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2105" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2105" s="10" t="s">
-        <v>900</v>
-      </c>
-      <c r="G2105" s="11"/>
-      <c r="H2105" s="12"/>
-      <c r="I2105" s="13"/>
-      <c r="J2105" s="13"/>
+      <c r="A2105" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B2105" s="2" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C2105" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2105" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2105" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F2105" s="4" t="s">
+        <v>1571</v>
+      </c>
+      <c r="G2105" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2105" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2105" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2105" s="36"/>
     </row>
     <row r="2106" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2106" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A2106" s="12"/>
       <c r="B2106" s="9"/>
-      <c r="C2106" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2106" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2106" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2106" s="10" t="s">
-        <v>897</v>
-      </c>
+      <c r="C2106" s="14"/>
+      <c r="D2106" s="10"/>
+      <c r="E2106" s="11"/>
+      <c r="F2106" s="10"/>
       <c r="G2106" s="11"/>
       <c r="H2106" s="12"/>
       <c r="I2106" s="13"/>
       <c r="J2106" s="13"/>
     </row>
-    <row r="2107" spans="1:10" ht="108" x14ac:dyDescent="0.2">
-      <c r="A2107" s="12">
-        <v>44055</v>
-      </c>
+    <row r="2107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2107" s="12"/>
       <c r="B2107" s="9"/>
-      <c r="C2107" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2107" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2107" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2107" s="10" t="s">
-        <v>898</v>
-      </c>
+      <c r="C2107" s="14"/>
+      <c r="D2107" s="10"/>
+      <c r="E2107" s="11"/>
+      <c r="F2107" s="10"/>
       <c r="G2107" s="11"/>
       <c r="H2107" s="12"/>
       <c r="I2107" s="13"/>
       <c r="J2107" s="13"/>
     </row>
-    <row r="2108" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="2108" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A2108" s="12">
-        <v>43949</v>
+        <v>44252</v>
       </c>
       <c r="B2108" s="9"/>
       <c r="C2108" s="14" t="s">
-        <v>468</v>
+        <v>895</v>
       </c>
       <c r="D2108" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E2108" s="11" t="s">
-        <v>683</v>
+        <v>757</v>
       </c>
       <c r="F2108" s="10" t="s">
-        <v>684</v>
-      </c>
-      <c r="G2108" s="11" t="s">
-        <v>1617</v>
-      </c>
+        <v>1637</v>
+      </c>
+      <c r="G2108" s="11"/>
       <c r="H2108" s="12"/>
-      <c r="I2108" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J2108" s="13"/>
-    </row>
-    <row r="2109" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="I2108" s="13"/>
+      <c r="J2108" s="13" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="2109" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A2109" s="12">
-        <v>43949</v>
+        <v>44252</v>
       </c>
       <c r="B2109" s="9"/>
       <c r="C2109" s="14" t="s">
-        <v>468</v>
+        <v>895</v>
       </c>
       <c r="D2109" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E2109" s="11" t="s">
-        <v>683</v>
+        <v>757</v>
       </c>
       <c r="F2109" s="10" t="s">
-        <v>703</v>
-      </c>
-      <c r="G2109" s="11" t="s">
-        <v>685</v>
-      </c>
+        <v>1636</v>
+      </c>
+      <c r="G2109" s="11"/>
       <c r="H2109" s="12"/>
-      <c r="I2109" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J2109" s="13" t="s">
-        <v>1561</v>
-      </c>
+      <c r="I2109" s="13"/>
+      <c r="J2109" s="13"/>
     </row>
     <row r="2110" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2110" s="12">
-        <v>43838</v>
+        <v>44112</v>
       </c>
       <c r="B2110" s="9"/>
       <c r="C2110" s="14" t="s">
-        <v>103</v>
+        <v>621</v>
       </c>
       <c r="D2110" s="10" t="s">
-        <v>460</v>
+        <v>6</v>
       </c>
       <c r="E2110" s="11" t="s">
-        <v>645</v>
+        <v>568</v>
       </c>
       <c r="F2110" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="G2110" s="11" t="s">
-        <v>1618</v>
-      </c>
+        <v>2223</v>
+      </c>
+      <c r="G2110" s="11"/>
       <c r="H2110" s="12"/>
       <c r="I2110" s="13"/>
-      <c r="J2110" s="13" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="2111" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J2110" s="13"/>
+    </row>
+    <row r="2111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2111" s="12">
-        <v>43762</v>
+        <v>44088</v>
       </c>
       <c r="B2111" s="9"/>
       <c r="C2111" s="14" t="s">
-        <v>446</v>
+        <v>19</v>
       </c>
       <c r="D2111" s="10" t="s">
-        <v>17</v>
+        <v>902</v>
       </c>
       <c r="E2111" s="11" t="s">
-        <v>835</v>
+        <v>683</v>
       </c>
       <c r="F2111" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G2111" s="11" t="s">
-        <v>1607</v>
-      </c>
+        <v>1007</v>
+      </c>
+      <c r="G2111" s="11"/>
       <c r="H2111" s="12"/>
       <c r="I2111" s="13"/>
       <c r="J2111" s="13"/>
     </row>
     <row r="2112" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2112" s="12"/>
+      <c r="A2112" s="12">
+        <v>44055</v>
+      </c>
       <c r="B2112" s="9"/>
-      <c r="C2112" s="14"/>
-      <c r="D2112" s="10"/>
-      <c r="E2112" s="11"/>
-      <c r="F2112" s="10"/>
+      <c r="C2112" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="D2112" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2112" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2112" s="10" t="s">
+        <v>900</v>
+      </c>
       <c r="G2112" s="11"/>
       <c r="H2112" s="12"/>
       <c r="I2112" s="13"/>
       <c r="J2112" s="13"/>
     </row>
     <row r="2113" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2113" s="12"/>
+      <c r="A2113" s="12">
+        <v>44055</v>
+      </c>
       <c r="B2113" s="9"/>
-      <c r="C2113" s="14"/>
-      <c r="D2113" s="10"/>
-      <c r="E2113" s="11"/>
-      <c r="F2113" s="10"/>
+      <c r="C2113" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2113" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2113" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2113" s="10" t="s">
+        <v>897</v>
+      </c>
       <c r="G2113" s="11"/>
       <c r="H2113" s="12"/>
       <c r="I2113" s="13"/>
       <c r="J2113" s="13"/>
     </row>
-    <row r="2114" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2114" s="12"/>
+    <row r="2114" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A2114" s="12">
+        <v>44055</v>
+      </c>
       <c r="B2114" s="9"/>
-      <c r="C2114" s="14"/>
-      <c r="D2114" s="10"/>
-      <c r="E2114" s="11"/>
-      <c r="F2114" s="10"/>
+      <c r="C2114" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2114" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2114" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2114" s="10" t="s">
+        <v>898</v>
+      </c>
       <c r="G2114" s="11"/>
       <c r="H2114" s="12"/>
       <c r="I2114" s="13"/>
       <c r="J2114" s="13"/>
     </row>
-    <row r="2115" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2115" s="12"/>
+    <row r="2115" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2115" s="12">
+        <v>43949</v>
+      </c>
       <c r="B2115" s="9"/>
-      <c r="C2115" s="14"/>
-      <c r="D2115" s="10"/>
-      <c r="E2115" s="11"/>
-      <c r="F2115" s="10"/>
-      <c r="G2115" s="11"/>
+      <c r="C2115" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2115" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2115" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2115" s="10" t="s">
+        <v>684</v>
+      </c>
+      <c r="G2115" s="11" t="s">
+        <v>1617</v>
+      </c>
       <c r="H2115" s="12"/>
-      <c r="I2115" s="13"/>
+      <c r="I2115" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J2115" s="13"/>
     </row>
-    <row r="2116" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2116" s="12"/>
+    <row r="2116" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2116" s="12">
+        <v>43949</v>
+      </c>
       <c r="B2116" s="9"/>
-      <c r="C2116" s="14"/>
-      <c r="D2116" s="10"/>
-      <c r="E2116" s="11"/>
-      <c r="F2116" s="10"/>
-      <c r="G2116" s="11"/>
+      <c r="C2116" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2116" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2116" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2116" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="G2116" s="11" t="s">
+        <v>685</v>
+      </c>
       <c r="H2116" s="12"/>
-      <c r="I2116" s="13"/>
-      <c r="J2116" s="13"/>
-    </row>
-    <row r="2117" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2117" s="12"/>
+      <c r="I2116" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J2116" s="13" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="2117" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2117" s="12">
+        <v>43838</v>
+      </c>
       <c r="B2117" s="9"/>
-      <c r="C2117" s="14"/>
-      <c r="D2117" s="10"/>
-      <c r="E2117" s="11"/>
-      <c r="F2117" s="10"/>
-      <c r="G2117" s="11"/>
+      <c r="C2117" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2117" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2117" s="11" t="s">
+        <v>645</v>
+      </c>
+      <c r="F2117" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="G2117" s="11" t="s">
+        <v>1618</v>
+      </c>
       <c r="H2117" s="12"/>
       <c r="I2117" s="13"/>
-      <c r="J2117" s="13"/>
+      <c r="J2117" s="13" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="2118" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2118" s="12">
+        <v>43762</v>
+      </c>
+      <c r="B2118" s="9"/>
+      <c r="C2118" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D2118" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2118" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2118" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G2118" s="11" t="s">
+        <v>1607</v>
+      </c>
+      <c r="H2118" s="12"/>
+      <c r="I2118" s="13"/>
+      <c r="J2118" s="13"/>
+    </row>
+    <row r="2119" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2119" s="12"/>
+      <c r="B2119" s="9"/>
+      <c r="C2119" s="14"/>
+      <c r="D2119" s="10"/>
+      <c r="E2119" s="11"/>
+      <c r="F2119" s="10"/>
+      <c r="G2119" s="11"/>
+      <c r="H2119" s="12"/>
+      <c r="I2119" s="13"/>
+      <c r="J2119" s="13"/>
+    </row>
+    <row r="2120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2120" s="12"/>
+      <c r="B2120" s="9"/>
+      <c r="C2120" s="14"/>
+      <c r="D2120" s="10"/>
+      <c r="E2120" s="11"/>
+      <c r="F2120" s="10"/>
+      <c r="G2120" s="11"/>
+      <c r="H2120" s="12"/>
+      <c r="I2120" s="13"/>
+      <c r="J2120" s="13"/>
+    </row>
+    <row r="2121" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2121" s="12"/>
+      <c r="B2121" s="9"/>
+      <c r="C2121" s="14"/>
+      <c r="D2121" s="10"/>
+      <c r="E2121" s="11"/>
+      <c r="F2121" s="10"/>
+      <c r="G2121" s="11"/>
+      <c r="H2121" s="12"/>
+      <c r="I2121" s="13"/>
+      <c r="J2121" s="13"/>
+    </row>
+    <row r="2122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2122" s="12"/>
+      <c r="B2122" s="9"/>
+      <c r="C2122" s="14"/>
+      <c r="D2122" s="10"/>
+      <c r="E2122" s="11"/>
+      <c r="F2122" s="10"/>
+      <c r="G2122" s="11"/>
+      <c r="H2122" s="12"/>
+      <c r="I2122" s="13"/>
+      <c r="J2122" s="13"/>
+    </row>
+    <row r="2123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2123" s="12"/>
+      <c r="B2123" s="9"/>
+      <c r="C2123" s="14"/>
+      <c r="D2123" s="10"/>
+      <c r="E2123" s="11"/>
+      <c r="F2123" s="10"/>
+      <c r="G2123" s="11"/>
+      <c r="H2123" s="12"/>
+      <c r="I2123" s="13"/>
+      <c r="J2123" s="13"/>
+    </row>
+    <row r="2124" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2124" s="12"/>
+      <c r="B2124" s="9"/>
+      <c r="C2124" s="14"/>
+      <c r="D2124" s="10"/>
+      <c r="E2124" s="11"/>
+      <c r="F2124" s="10"/>
+      <c r="G2124" s="11"/>
+      <c r="H2124" s="12"/>
+      <c r="I2124" s="13"/>
+      <c r="J2124" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1881" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -72864,79 +73124,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E16FADF7-6C4C-4356-9576-380717A61E1D}">
-  <sheetPr codeName="Planilha3"/>
-  <dimension ref="C3:F10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>134</v>
-      </c>
-      <c r="D4">
-        <f>+C4/C3</f>
-        <v>0.72826086956521741</v>
-      </c>
-      <c r="E4">
-        <f>+C3*D7</f>
-        <v>130.09375</v>
-      </c>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>1280</v>
-      </c>
-      <c r="F6">
-        <f>+C3/C6</f>
-        <v>0.14374999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>905</v>
-      </c>
-      <c r="D7">
-        <f>+C7/C6</f>
-        <v>0.70703125</v>
-      </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>790</v>
-      </c>
-      <c r="F9">
-        <f>+C3/C9</f>
-        <v>0.23291139240506328</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <v>409</v>
-      </c>
-      <c r="D10">
-        <f>+C10/C9</f>
-        <v>0.51772151898734176</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE13D4C-C1F0-4B00-8A02-71F13D132F72}">
   <sheetPr codeName="Planilha4"/>
   <dimension ref="B1:G35"/>

</xml_diff>

<commit_message>
Inclusao de previsoes na tabela GERAL Dashboard
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B6FB33-726B-4CC9-8B6E-37ACD412BF17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12232EAC-5AFF-4EC3-B7FF-45C146C728A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15031" uniqueCount="2888">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15053" uniqueCount="2891">
   <si>
     <t>Responsável</t>
   </si>
@@ -9126,6 +9126,16 @@
   </si>
   <si>
     <t>Continuação do desenvolvimento - Dashboard</t>
+  </si>
+  <si>
+    <t>Reinstalação do git (não estava atualizando a pasta remote)</t>
+  </si>
+  <si>
+    <t>Relatorio BKGCTR21 não está listando os reajustes</t>
+  </si>
+  <si>
+    <t>Planilhas não estavam preenchidas corretamente
+Feito reajuste via query</t>
   </si>
 </sst>
 </file>
@@ -9935,7 +9945,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2113" sqref="F2113"/>
+      <selection pane="bottomLeft" activeCell="A2116" sqref="A2116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -73295,40 +73305,96 @@
       <c r="J2112" s="13"/>
     </row>
     <row r="2113" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2113" s="12"/>
-      <c r="B2113" s="12"/>
-      <c r="C2113" s="10"/>
-      <c r="D2113" s="10"/>
-      <c r="E2113" s="11"/>
-      <c r="F2113" s="10"/>
-      <c r="G2113" s="11"/>
-      <c r="H2113" s="12"/>
-      <c r="I2113" s="13"/>
+      <c r="A2113" s="12">
+        <v>44725</v>
+      </c>
+      <c r="B2113" s="12">
+        <v>44725</v>
+      </c>
+      <c r="C2113" s="10" t="s">
+        <v>2680</v>
+      </c>
+      <c r="D2113" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2113" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2113" s="10" t="s">
+        <v>2887</v>
+      </c>
+      <c r="G2113" s="11" t="s">
+        <v>1603</v>
+      </c>
+      <c r="H2113" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2113" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2113" s="13"/>
     </row>
     <row r="2114" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2114" s="12"/>
-      <c r="B2114" s="12"/>
-      <c r="C2114" s="10"/>
-      <c r="D2114" s="10"/>
-      <c r="E2114" s="11"/>
-      <c r="F2114" s="10"/>
-      <c r="G2114" s="11"/>
-      <c r="H2114" s="12"/>
-      <c r="I2114" s="13"/>
+      <c r="A2114" s="12">
+        <v>44725</v>
+      </c>
+      <c r="B2114" s="12">
+        <v>44725</v>
+      </c>
+      <c r="C2114" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2114" s="10" t="s">
+        <v>582</v>
+      </c>
+      <c r="E2114" s="11" t="s">
+        <v>696</v>
+      </c>
+      <c r="F2114" s="10" t="s">
+        <v>2888</v>
+      </c>
+      <c r="G2114" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H2114" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2114" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2114" s="13"/>
     </row>
-    <row r="2115" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2115" s="12"/>
-      <c r="B2115" s="12"/>
-      <c r="C2115" s="10"/>
-      <c r="D2115" s="10"/>
-      <c r="E2115" s="11"/>
-      <c r="F2115" s="10"/>
-      <c r="G2115" s="11"/>
-      <c r="H2115" s="12"/>
-      <c r="I2115" s="13"/>
-      <c r="J2115" s="13"/>
+    <row r="2115" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2115" s="12">
+        <v>44726</v>
+      </c>
+      <c r="B2115" s="12">
+        <v>44726</v>
+      </c>
+      <c r="C2115" s="10" t="s">
+        <v>621</v>
+      </c>
+      <c r="D2115" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2115" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2115" s="10" t="s">
+        <v>2889</v>
+      </c>
+      <c r="G2115" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H2115" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2115" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2115" s="13" t="s">
+        <v>2890</v>
+      </c>
     </row>
     <row r="2116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2116" s="12"/>

</xml_diff>

<commit_message>
Acerto RM no mapa de inss ret
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B14541-E7C1-464C-B79E-03D03DC7E970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5053F473-1D97-462A-8B61-7AD97C55D1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15300" uniqueCount="2932">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15325" uniqueCount="2936">
   <si>
     <t>Responsável</t>
   </si>
@@ -9278,6 +9278,18 @@
   </si>
   <si>
     <t>Normatização de códigos Rentabilidade/Prev x Realizado e Dashboard</t>
+  </si>
+  <si>
+    <t>Acerto data de movimento bancario da PA PAGFOR170622  e outros suportes</t>
+  </si>
+  <si>
+    <t>Quando da exclusão de titulos do RH, o sistema não está enviando e-mail avisando</t>
+  </si>
+  <si>
+    <t>Suportes diversos referentes a revisão de contratos e nova medição</t>
+  </si>
+  <si>
+    <t>Criação de registro de log de envio de e-mails para detecção de erro</t>
   </si>
 </sst>
 </file>
@@ -10083,11 +10095,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J2192"/>
+  <dimension ref="A1:J2195"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2149" sqref="G2149"/>
+      <pane ySplit="1" topLeftCell="A2145" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2154" sqref="A2154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -74577,166 +74589,202 @@
       <c r="J2149" s="13"/>
     </row>
     <row r="2150" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2150" s="12"/>
-      <c r="B2150" s="12"/>
-      <c r="C2150" s="10"/>
-      <c r="D2150" s="10"/>
-      <c r="E2150" s="11"/>
-      <c r="F2150" s="10"/>
-      <c r="G2150" s="11"/>
-      <c r="H2150" s="12"/>
-      <c r="I2150" s="13"/>
+      <c r="A2150" s="12">
+        <v>44743</v>
+      </c>
+      <c r="B2150" s="12">
+        <v>44743</v>
+      </c>
+      <c r="C2150" s="10" t="s">
+        <v>557</v>
+      </c>
+      <c r="D2150" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2150" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2150" s="10" t="s">
+        <v>2932</v>
+      </c>
+      <c r="G2150" s="11" t="s">
+        <v>1598</v>
+      </c>
+      <c r="H2150" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2150" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2150" s="13"/>
     </row>
     <row r="2151" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2151" s="12"/>
-      <c r="B2151" s="12"/>
-      <c r="C2151" s="10"/>
-      <c r="D2151" s="10"/>
-      <c r="E2151" s="11"/>
-      <c r="F2151" s="10"/>
+      <c r="A2151" s="12">
+        <v>44743</v>
+      </c>
+      <c r="B2151" s="12">
+        <v>44743</v>
+      </c>
+      <c r="C2151" s="10" t="s">
+        <v>557</v>
+      </c>
+      <c r="D2151" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2151" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2151" s="10" t="s">
+        <v>2933</v>
+      </c>
       <c r="G2151" s="11"/>
       <c r="H2151" s="12"/>
       <c r="I2151" s="13"/>
       <c r="J2151" s="13"/>
     </row>
     <row r="2152" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2152" s="12"/>
-      <c r="B2152" s="12"/>
-      <c r="C2152" s="10"/>
-      <c r="D2152" s="10"/>
-      <c r="E2152" s="11"/>
-      <c r="F2152" s="10"/>
-      <c r="G2152" s="11"/>
-      <c r="H2152" s="12"/>
-      <c r="I2152" s="13"/>
+      <c r="A2152" s="12">
+        <v>44743</v>
+      </c>
+      <c r="B2152" s="12">
+        <v>44743</v>
+      </c>
+      <c r="C2152" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2152" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2152" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2152" s="10" t="s">
+        <v>2934</v>
+      </c>
+      <c r="G2152" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H2152" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2152" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2152" s="13"/>
     </row>
     <row r="2153" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2153" s="12"/>
-      <c r="B2153" s="12"/>
-      <c r="C2153" s="10"/>
-      <c r="D2153" s="10"/>
-      <c r="E2153" s="11"/>
-      <c r="F2153" s="10"/>
-      <c r="G2153" s="11"/>
-      <c r="H2153" s="12"/>
-      <c r="I2153" s="13"/>
+      <c r="A2153" s="12">
+        <v>44743</v>
+      </c>
+      <c r="B2153" s="12">
+        <v>44743</v>
+      </c>
+      <c r="C2153" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2153" s="10" t="s">
+        <v>582</v>
+      </c>
+      <c r="E2153" s="11" t="s">
+        <v>645</v>
+      </c>
+      <c r="F2153" s="10" t="s">
+        <v>2935</v>
+      </c>
+      <c r="G2153" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H2153" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2153" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2153" s="13"/>
     </row>
-    <row r="2154" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2154" s="12">
-        <v>44698</v>
-      </c>
+    <row r="2154" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2154" s="12"/>
       <c r="B2154" s="12"/>
-      <c r="C2154" s="10" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2154" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2154" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2154" s="30" t="s">
-        <v>2798</v>
-      </c>
+      <c r="C2154" s="10"/>
+      <c r="D2154" s="10"/>
+      <c r="E2154" s="11"/>
+      <c r="F2154" s="10"/>
       <c r="G2154" s="11"/>
       <c r="H2154" s="12"/>
       <c r="I2154" s="13"/>
       <c r="J2154" s="13"/>
     </row>
-    <row r="2155" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2155" s="12">
-        <v>44684</v>
-      </c>
+    <row r="2155" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2155" s="12"/>
       <c r="B2155" s="12"/>
-      <c r="C2155" s="14" t="s">
-        <v>2155</v>
-      </c>
-      <c r="D2155" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2155" s="11" t="s">
-        <v>618</v>
-      </c>
-      <c r="F2155" s="10" t="s">
-        <v>2799</v>
-      </c>
+      <c r="C2155" s="10"/>
+      <c r="D2155" s="10"/>
+      <c r="E2155" s="11"/>
+      <c r="F2155" s="10"/>
       <c r="G2155" s="11"/>
       <c r="H2155" s="12"/>
       <c r="I2155" s="13"/>
       <c r="J2155" s="13"/>
     </row>
-    <row r="2156" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2156" s="12">
-        <v>44677</v>
-      </c>
+    <row r="2156" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2156" s="12"/>
       <c r="B2156" s="12"/>
-      <c r="C2156" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="D2156" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2156" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2156" s="10" t="s">
-        <v>2729</v>
-      </c>
+      <c r="C2156" s="10"/>
+      <c r="D2156" s="10"/>
+      <c r="E2156" s="11"/>
+      <c r="F2156" s="10"/>
       <c r="G2156" s="11"/>
       <c r="H2156" s="12"/>
       <c r="I2156" s="13"/>
       <c r="J2156" s="13"/>
     </row>
-    <row r="2157" spans="1:10" ht="132" x14ac:dyDescent="0.2">
+    <row r="2157" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2157" s="12">
-        <v>44645</v>
+        <v>44698</v>
       </c>
       <c r="B2157" s="12"/>
-      <c r="C2157" s="14" t="s">
-        <v>288</v>
+      <c r="C2157" s="10" t="s">
+        <v>895</v>
       </c>
       <c r="D2157" s="10" t="s">
-        <v>25</v>
+        <v>492</v>
       </c>
       <c r="E2157" s="11" t="s">
-        <v>618</v>
-      </c>
-      <c r="F2157" s="10" t="s">
-        <v>2664</v>
+        <v>835</v>
+      </c>
+      <c r="F2157" s="30" t="s">
+        <v>2798</v>
       </c>
       <c r="G2157" s="11"/>
       <c r="H2157" s="12"/>
       <c r="I2157" s="13"/>
       <c r="J2157" s="13"/>
     </row>
-    <row r="2158" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2158" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2158" s="12">
-        <v>44642</v>
+        <v>44684</v>
       </c>
       <c r="B2158" s="12"/>
       <c r="C2158" s="14" t="s">
-        <v>387</v>
+        <v>2155</v>
       </c>
       <c r="D2158" s="10" t="s">
-        <v>492</v>
+        <v>83</v>
       </c>
       <c r="E2158" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F2158" s="10" t="s">
-        <v>2625</v>
+        <v>2799</v>
       </c>
       <c r="G2158" s="11"/>
       <c r="H2158" s="12"/>
       <c r="I2158" s="13"/>
       <c r="J2158" s="13"/>
     </row>
-    <row r="2159" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2159" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2159" s="12">
-        <v>44642</v>
+        <v>44677</v>
       </c>
       <c r="B2159" s="12"/>
       <c r="C2159" s="14" t="s">
@@ -74749,31 +74797,29 @@
         <v>835</v>
       </c>
       <c r="F2159" s="10" t="s">
-        <v>2624</v>
+        <v>2729</v>
       </c>
       <c r="G2159" s="11"/>
       <c r="H2159" s="12"/>
       <c r="I2159" s="13"/>
       <c r="J2159" s="13"/>
     </row>
-    <row r="2160" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2160" spans="1:10" ht="132" x14ac:dyDescent="0.2">
       <c r="A2160" s="12">
-        <v>44614</v>
-      </c>
-      <c r="B2160" s="12">
-        <v>44614</v>
-      </c>
+        <v>44645</v>
+      </c>
+      <c r="B2160" s="12"/>
       <c r="C2160" s="14" t="s">
-        <v>19</v>
+        <v>288</v>
       </c>
       <c r="D2160" s="10" t="s">
-        <v>492</v>
+        <v>25</v>
       </c>
       <c r="E2160" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F2160" s="10" t="s">
-        <v>2528</v>
+        <v>2664</v>
       </c>
       <c r="G2160" s="11"/>
       <c r="H2160" s="12"/>
@@ -74782,11 +74828,11 @@
     </row>
     <row r="2161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2161" s="12">
-        <v>44614</v>
+        <v>44642</v>
       </c>
       <c r="B2161" s="12"/>
       <c r="C2161" s="14" t="s">
-        <v>19</v>
+        <v>387</v>
       </c>
       <c r="D2161" s="10" t="s">
         <v>492</v>
@@ -74795,7 +74841,7 @@
         <v>835</v>
       </c>
       <c r="F2161" s="10" t="s">
-        <v>2548</v>
+        <v>2625</v>
       </c>
       <c r="G2161" s="11"/>
       <c r="H2161" s="12"/>
@@ -74804,20 +74850,20 @@
     </row>
     <row r="2162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2162" s="12">
-        <v>44616</v>
+        <v>44642</v>
       </c>
       <c r="B2162" s="12"/>
       <c r="C2162" s="14" t="s">
-        <v>2250</v>
+        <v>387</v>
       </c>
       <c r="D2162" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E2162" s="11" t="s">
-        <v>618</v>
+        <v>835</v>
       </c>
       <c r="F2162" s="10" t="s">
-        <v>2555</v>
+        <v>2624</v>
       </c>
       <c r="G2162" s="11"/>
       <c r="H2162" s="12"/>
@@ -74826,42 +74872,44 @@
     </row>
     <row r="2163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2163" s="12">
-        <v>44623</v>
-      </c>
-      <c r="B2163" s="12"/>
+        <v>44614</v>
+      </c>
+      <c r="B2163" s="12">
+        <v>44614</v>
+      </c>
       <c r="C2163" s="14" t="s">
-        <v>535</v>
+        <v>19</v>
       </c>
       <c r="D2163" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2163" s="11" t="s">
         <v>835</v>
       </c>
       <c r="F2163" s="10" t="s">
-        <v>2573</v>
+        <v>2528</v>
       </c>
       <c r="G2163" s="11"/>
       <c r="H2163" s="12"/>
       <c r="I2163" s="13"/>
       <c r="J2163" s="13"/>
     </row>
-    <row r="2164" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="2164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2164" s="12">
-        <v>44522</v>
+        <v>44614</v>
       </c>
       <c r="B2164" s="12"/>
       <c r="C2164" s="14" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="D2164" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2164" s="11" t="s">
-        <v>568</v>
+        <v>835</v>
       </c>
       <c r="F2164" s="10" t="s">
-        <v>2350</v>
+        <v>2548</v>
       </c>
       <c r="G2164" s="11"/>
       <c r="H2164" s="12"/>
@@ -74869,36 +74917,66 @@
       <c r="J2164" s="13"/>
     </row>
     <row r="2165" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2165" s="12"/>
+      <c r="A2165" s="12">
+        <v>44616</v>
+      </c>
       <c r="B2165" s="12"/>
-      <c r="C2165" s="14"/>
-      <c r="D2165" s="10"/>
-      <c r="E2165" s="11"/>
-      <c r="F2165" s="10"/>
+      <c r="C2165" s="14" t="s">
+        <v>2250</v>
+      </c>
+      <c r="D2165" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2165" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2165" s="10" t="s">
+        <v>2555</v>
+      </c>
       <c r="G2165" s="11"/>
       <c r="H2165" s="12"/>
       <c r="I2165" s="13"/>
       <c r="J2165" s="13"/>
     </row>
     <row r="2166" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2166" s="12"/>
+      <c r="A2166" s="12">
+        <v>44623</v>
+      </c>
       <c r="B2166" s="12"/>
-      <c r="C2166" s="14"/>
-      <c r="D2166" s="10"/>
-      <c r="E2166" s="11"/>
-      <c r="F2166" s="10"/>
+      <c r="C2166" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="D2166" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2166" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2166" s="10" t="s">
+        <v>2573</v>
+      </c>
       <c r="G2166" s="11"/>
       <c r="H2166" s="12"/>
       <c r="I2166" s="13"/>
       <c r="J2166" s="13"/>
     </row>
-    <row r="2167" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2167" s="12"/>
+    <row r="2167" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2167" s="12">
+        <v>44522</v>
+      </c>
       <c r="B2167" s="12"/>
-      <c r="C2167" s="14"/>
-      <c r="D2167" s="10"/>
-      <c r="E2167" s="11"/>
-      <c r="F2167" s="10"/>
+      <c r="C2167" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2167" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2167" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2167" s="10" t="s">
+        <v>2350</v>
+      </c>
       <c r="G2167" s="11"/>
       <c r="H2167" s="12"/>
       <c r="I2167" s="13"/>
@@ -74954,7 +75032,7 @@
     </row>
     <row r="2172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2172" s="12"/>
-      <c r="B2172" s="9"/>
+      <c r="B2172" s="12"/>
       <c r="C2172" s="14"/>
       <c r="D2172" s="10"/>
       <c r="E2172" s="11"/>
@@ -74965,38 +75043,20 @@
       <c r="J2172" s="13"/>
     </row>
     <row r="2173" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2173" s="1" t="s">
-        <v>1472</v>
-      </c>
-      <c r="B2173" s="2" t="s">
-        <v>1473</v>
-      </c>
-      <c r="C2173" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2173" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2173" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="F2173" s="4" t="s">
-        <v>1571</v>
-      </c>
-      <c r="G2173" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2173" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2173" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2173" s="36"/>
+      <c r="A2173" s="12"/>
+      <c r="B2173" s="12"/>
+      <c r="C2173" s="14"/>
+      <c r="D2173" s="10"/>
+      <c r="E2173" s="11"/>
+      <c r="F2173" s="10"/>
+      <c r="G2173" s="11"/>
+      <c r="H2173" s="12"/>
+      <c r="I2173" s="13"/>
+      <c r="J2173" s="13"/>
     </row>
     <row r="2174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2174" s="12"/>
-      <c r="B2174" s="9"/>
+      <c r="B2174" s="12"/>
       <c r="C2174" s="14"/>
       <c r="D2174" s="10"/>
       <c r="E2174" s="11"/>
@@ -75018,298 +75078,316 @@
       <c r="I2175" s="13"/>
       <c r="J2175" s="13"/>
     </row>
-    <row r="2176" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A2176" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2176" s="9"/>
-      <c r="C2176" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2176" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2176" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2176" s="10" t="s">
-        <v>1636</v>
-      </c>
-      <c r="G2176" s="11"/>
-      <c r="H2176" s="12"/>
-      <c r="I2176" s="13"/>
-      <c r="J2176" s="13" t="s">
-        <v>1659</v>
-      </c>
-    </row>
-    <row r="2177" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A2177" s="12">
-        <v>44252</v>
-      </c>
+    <row r="2176" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2176" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B2176" s="2" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C2176" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2176" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2176" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F2176" s="4" t="s">
+        <v>1571</v>
+      </c>
+      <c r="G2176" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2176" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2176" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2176" s="36"/>
+    </row>
+    <row r="2177" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2177" s="12"/>
       <c r="B2177" s="9"/>
-      <c r="C2177" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2177" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2177" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2177" s="10" t="s">
-        <v>1635</v>
-      </c>
+      <c r="C2177" s="14"/>
+      <c r="D2177" s="10"/>
+      <c r="E2177" s="11"/>
+      <c r="F2177" s="10"/>
       <c r="G2177" s="11"/>
       <c r="H2177" s="12"/>
       <c r="I2177" s="13"/>
       <c r="J2177" s="13"/>
     </row>
-    <row r="2178" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2178" s="12">
-        <v>44112</v>
-      </c>
+    <row r="2178" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2178" s="12"/>
       <c r="B2178" s="9"/>
-      <c r="C2178" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D2178" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2178" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2178" s="10" t="s">
-        <v>2222</v>
-      </c>
+      <c r="C2178" s="14"/>
+      <c r="D2178" s="10"/>
+      <c r="E2178" s="11"/>
+      <c r="F2178" s="10"/>
       <c r="G2178" s="11"/>
       <c r="H2178" s="12"/>
       <c r="I2178" s="13"/>
       <c r="J2178" s="13"/>
     </row>
-    <row r="2179" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2179" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A2179" s="12">
-        <v>44088</v>
+        <v>44252</v>
       </c>
       <c r="B2179" s="9"/>
       <c r="C2179" s="14" t="s">
-        <v>19</v>
+        <v>895</v>
       </c>
       <c r="D2179" s="10" t="s">
-        <v>902</v>
+        <v>492</v>
       </c>
       <c r="E2179" s="11" t="s">
-        <v>683</v>
+        <v>757</v>
       </c>
       <c r="F2179" s="10" t="s">
-        <v>1007</v>
+        <v>1636</v>
       </c>
       <c r="G2179" s="11"/>
       <c r="H2179" s="12"/>
       <c r="I2179" s="13"/>
-      <c r="J2179" s="13"/>
-    </row>
-    <row r="2180" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J2179" s="13" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="2180" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A2180" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B2180" s="9"/>
       <c r="C2180" s="14" t="s">
-        <v>621</v>
+        <v>895</v>
       </c>
       <c r="D2180" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2180" s="11" t="s">
-        <v>568</v>
+        <v>757</v>
       </c>
       <c r="F2180" s="10" t="s">
-        <v>900</v>
+        <v>1635</v>
       </c>
       <c r="G2180" s="11"/>
       <c r="H2180" s="12"/>
       <c r="I2180" s="13"/>
       <c r="J2180" s="13"/>
     </row>
-    <row r="2181" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2181" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2181" s="12">
-        <v>44055</v>
+        <v>44112</v>
       </c>
       <c r="B2181" s="9"/>
       <c r="C2181" s="14" t="s">
-        <v>895</v>
+        <v>621</v>
       </c>
       <c r="D2181" s="10" t="s">
-        <v>492</v>
+        <v>6</v>
       </c>
       <c r="E2181" s="11" t="s">
         <v>568</v>
       </c>
       <c r="F2181" s="10" t="s">
-        <v>897</v>
+        <v>2222</v>
       </c>
       <c r="G2181" s="11"/>
       <c r="H2181" s="12"/>
       <c r="I2181" s="13"/>
       <c r="J2181" s="13"/>
     </row>
-    <row r="2182" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="2182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2182" s="12">
-        <v>44055</v>
+        <v>44088</v>
       </c>
       <c r="B2182" s="9"/>
       <c r="C2182" s="14" t="s">
-        <v>895</v>
+        <v>19</v>
       </c>
       <c r="D2182" s="10" t="s">
-        <v>492</v>
+        <v>902</v>
       </c>
       <c r="E2182" s="11" t="s">
-        <v>568</v>
+        <v>683</v>
       </c>
       <c r="F2182" s="10" t="s">
-        <v>898</v>
+        <v>1007</v>
       </c>
       <c r="G2182" s="11"/>
       <c r="H2182" s="12"/>
       <c r="I2182" s="13"/>
       <c r="J2182" s="13"/>
     </row>
-    <row r="2183" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="2183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2183" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B2183" s="9"/>
       <c r="C2183" s="14" t="s">
-        <v>468</v>
+        <v>621</v>
       </c>
       <c r="D2183" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E2183" s="11" t="s">
-        <v>683</v>
+        <v>568</v>
       </c>
       <c r="F2183" s="10" t="s">
-        <v>684</v>
-      </c>
-      <c r="G2183" s="11" t="s">
-        <v>1616</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="G2183" s="11"/>
       <c r="H2183" s="12"/>
-      <c r="I2183" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I2183" s="13"/>
       <c r="J2183" s="13"/>
     </row>
-    <row r="2184" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="2184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2184" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B2184" s="9"/>
       <c r="C2184" s="14" t="s">
-        <v>468</v>
+        <v>895</v>
       </c>
       <c r="D2184" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E2184" s="11" t="s">
-        <v>683</v>
+        <v>568</v>
       </c>
       <c r="F2184" s="10" t="s">
-        <v>703</v>
-      </c>
-      <c r="G2184" s="11" t="s">
-        <v>685</v>
-      </c>
+        <v>897</v>
+      </c>
+      <c r="G2184" s="11"/>
       <c r="H2184" s="12"/>
-      <c r="I2184" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J2184" s="13" t="s">
-        <v>1561</v>
-      </c>
-    </row>
-    <row r="2185" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I2184" s="13"/>
+      <c r="J2184" s="13"/>
+    </row>
+    <row r="2185" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A2185" s="12">
-        <v>43838</v>
+        <v>44055</v>
       </c>
       <c r="B2185" s="9"/>
       <c r="C2185" s="14" t="s">
-        <v>103</v>
+        <v>895</v>
       </c>
       <c r="D2185" s="10" t="s">
-        <v>460</v>
+        <v>492</v>
       </c>
       <c r="E2185" s="11" t="s">
-        <v>645</v>
+        <v>568</v>
       </c>
       <c r="F2185" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="G2185" s="11" t="s">
-        <v>1617</v>
-      </c>
+        <v>898</v>
+      </c>
+      <c r="G2185" s="11"/>
       <c r="H2185" s="12"/>
       <c r="I2185" s="13"/>
-      <c r="J2185" s="13" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="2186" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J2185" s="13"/>
+    </row>
+    <row r="2186" spans="1:10" ht="168" x14ac:dyDescent="0.2">
       <c r="A2186" s="12">
-        <v>43762</v>
+        <v>43949</v>
       </c>
       <c r="B2186" s="9"/>
       <c r="C2186" s="14" t="s">
-        <v>446</v>
+        <v>468</v>
       </c>
       <c r="D2186" s="10" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="E2186" s="11" t="s">
-        <v>835</v>
+        <v>683</v>
       </c>
       <c r="F2186" s="10" t="s">
-        <v>447</v>
+        <v>684</v>
       </c>
       <c r="G2186" s="11" t="s">
-        <v>1606</v>
+        <v>1616</v>
       </c>
       <c r="H2186" s="12"/>
-      <c r="I2186" s="13"/>
+      <c r="I2186" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J2186" s="13"/>
     </row>
-    <row r="2187" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2187" s="12"/>
+    <row r="2187" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2187" s="12">
+        <v>43949</v>
+      </c>
       <c r="B2187" s="9"/>
-      <c r="C2187" s="14"/>
-      <c r="D2187" s="10"/>
-      <c r="E2187" s="11"/>
-      <c r="F2187" s="10"/>
-      <c r="G2187" s="11"/>
+      <c r="C2187" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2187" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2187" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2187" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="G2187" s="11" t="s">
+        <v>685</v>
+      </c>
       <c r="H2187" s="12"/>
-      <c r="I2187" s="13"/>
-      <c r="J2187" s="13"/>
-    </row>
-    <row r="2188" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2188" s="12"/>
+      <c r="I2187" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J2187" s="13" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="2188" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2188" s="12">
+        <v>43838</v>
+      </c>
       <c r="B2188" s="9"/>
-      <c r="C2188" s="14"/>
-      <c r="D2188" s="10"/>
-      <c r="E2188" s="11"/>
-      <c r="F2188" s="10"/>
-      <c r="G2188" s="11"/>
+      <c r="C2188" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2188" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2188" s="11" t="s">
+        <v>645</v>
+      </c>
+      <c r="F2188" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="G2188" s="11" t="s">
+        <v>1617</v>
+      </c>
       <c r="H2188" s="12"/>
       <c r="I2188" s="13"/>
-      <c r="J2188" s="13"/>
-    </row>
-    <row r="2189" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2189" s="12"/>
+      <c r="J2188" s="13" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="2189" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2189" s="12">
+        <v>43762</v>
+      </c>
       <c r="B2189" s="9"/>
-      <c r="C2189" s="14"/>
-      <c r="D2189" s="10"/>
-      <c r="E2189" s="11"/>
-      <c r="F2189" s="10"/>
-      <c r="G2189" s="11"/>
+      <c r="C2189" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D2189" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2189" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2189" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G2189" s="11" t="s">
+        <v>1606</v>
+      </c>
       <c r="H2189" s="12"/>
       <c r="I2189" s="13"/>
       <c r="J2189" s="13"/>
@@ -75349,6 +75427,42 @@
       <c r="H2192" s="12"/>
       <c r="I2192" s="13"/>
       <c r="J2192" s="13"/>
+    </row>
+    <row r="2193" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2193" s="12"/>
+      <c r="B2193" s="9"/>
+      <c r="C2193" s="14"/>
+      <c r="D2193" s="10"/>
+      <c r="E2193" s="11"/>
+      <c r="F2193" s="10"/>
+      <c r="G2193" s="11"/>
+      <c r="H2193" s="12"/>
+      <c r="I2193" s="13"/>
+      <c r="J2193" s="13"/>
+    </row>
+    <row r="2194" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2194" s="12"/>
+      <c r="B2194" s="9"/>
+      <c r="C2194" s="14"/>
+      <c r="D2194" s="10"/>
+      <c r="E2194" s="11"/>
+      <c r="F2194" s="10"/>
+      <c r="G2194" s="11"/>
+      <c r="H2194" s="12"/>
+      <c r="I2194" s="13"/>
+      <c r="J2194" s="13"/>
+    </row>
+    <row r="2195" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2195" s="12"/>
+      <c r="B2195" s="9"/>
+      <c r="C2195" s="14"/>
+      <c r="D2195" s="10"/>
+      <c r="E2195" s="11"/>
+      <c r="F2195" s="10"/>
+      <c r="G2195" s="11"/>
+      <c r="H2195" s="12"/>
+      <c r="I2195" s="13"/>
+      <c r="J2195" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1881" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Tabela FOLHA no DashBoard
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF93242-6C06-462A-8D38-5C0AC5A6E6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B62978-894C-42F7-A245-4B5120654A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15565" uniqueCount="2982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15595" uniqueCount="2988">
   <si>
     <t>Responsável</t>
   </si>
@@ -9434,6 +9434,27 @@
   </si>
   <si>
     <t>Relatorio de emprestimo0s não aparece todos os titulos</t>
+  </si>
+  <si>
+    <t>Divergencia entre o valor líquido dos relatórios "BKFINR30-Clientes em Aberto"  e "BKGCTR07-Mapa de INSS Retido"</t>
+  </si>
+  <si>
+    <t>No Mapa de Inss Retido não considerava a Conta Vinculada</t>
+  </si>
+  <si>
+    <t>Erro na chave da tabela FATURAMENTO do Dashboard</t>
+  </si>
+  <si>
+    <t>Erro na apuração da EFD: valores retidos de Notas de Saida incorretos.</t>
+  </si>
+  <si>
+    <t>Foram identificados 3 problemas:
+1- Baixa financeira da NF FA0000030 não foi gravada corretamente.
+2-Cliente 000281-46 estava como Não recolhe ISS no cad de cliente e Sim no pedido, a EFD desconta o valor do ISS Bitributado da base do PIS/COFINS retido
+3-Quando NF é Bitributada e o pedido esta com C5_RETISS = '2'  A EFD desconta o valor do ISS Bitributado da base do PIS/COFINS retido</t>
+  </si>
+  <si>
+    <t>Geração da tabela FOLHA</t>
   </si>
 </sst>
 </file>
@@ -10239,11 +10260,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J2228"/>
+  <dimension ref="A1:J2232"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2193" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2202" sqref="A2202"/>
+      <pane ySplit="1" topLeftCell="A2184" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2189" sqref="A2189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -75830,11 +75851,13 @@
         <v>2980</v>
       </c>
     </row>
-    <row r="2186" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2186" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2186" s="12">
-        <v>44754</v>
-      </c>
-      <c r="B2186" s="12"/>
+        <v>44755</v>
+      </c>
+      <c r="B2186" s="12">
+        <v>44755</v>
+      </c>
       <c r="C2186" s="10" t="s">
         <v>621</v>
       </c>
@@ -75845,144 +75868,178 @@
         <v>618</v>
       </c>
       <c r="F2186" s="10" t="s">
-        <v>2981</v>
-      </c>
-      <c r="G2186" s="11"/>
-      <c r="H2186" s="12"/>
-      <c r="I2186" s="13"/>
-      <c r="J2186" s="13"/>
+        <v>2982</v>
+      </c>
+      <c r="G2186" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H2186" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2186" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2186" s="13" t="s">
+        <v>2983</v>
+      </c>
     </row>
     <row r="2187" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2187" s="12"/>
-      <c r="B2187" s="12"/>
-      <c r="C2187" s="10"/>
-      <c r="D2187" s="10"/>
-      <c r="E2187" s="11"/>
-      <c r="F2187" s="10"/>
-      <c r="G2187" s="11"/>
-      <c r="H2187" s="12"/>
-      <c r="I2187" s="13"/>
+      <c r="A2187" s="12">
+        <v>44755</v>
+      </c>
+      <c r="B2187" s="12">
+        <v>44755</v>
+      </c>
+      <c r="C2187" s="10" t="s">
+        <v>2680</v>
+      </c>
+      <c r="D2187" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2187" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2187" s="10" t="s">
+        <v>2984</v>
+      </c>
+      <c r="G2187" s="11" t="s">
+        <v>1598</v>
+      </c>
+      <c r="H2187" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2187" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2187" s="13"/>
     </row>
-    <row r="2188" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2188" s="12"/>
-      <c r="B2188" s="12"/>
-      <c r="C2188" s="10"/>
-      <c r="D2188" s="10"/>
-      <c r="E2188" s="11"/>
-      <c r="F2188" s="10"/>
-      <c r="G2188" s="11"/>
-      <c r="H2188" s="12"/>
-      <c r="I2188" s="13"/>
-      <c r="J2188" s="13"/>
+    <row r="2188" spans="1:10" ht="84" x14ac:dyDescent="0.2">
+      <c r="A2188" s="12">
+        <v>44755</v>
+      </c>
+      <c r="B2188" s="12">
+        <v>44755</v>
+      </c>
+      <c r="C2188" s="10" t="s">
+        <v>1968</v>
+      </c>
+      <c r="D2188" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2188" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2188" s="10" t="s">
+        <v>2985</v>
+      </c>
+      <c r="G2188" s="11" t="s">
+        <v>1827</v>
+      </c>
+      <c r="H2188" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2188" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2188" s="13" t="s">
+        <v>2986</v>
+      </c>
     </row>
     <row r="2189" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2189" s="12"/>
-      <c r="B2189" s="12"/>
-      <c r="C2189" s="10"/>
-      <c r="D2189" s="10"/>
-      <c r="E2189" s="11"/>
-      <c r="F2189" s="10"/>
-      <c r="G2189" s="11"/>
-      <c r="H2189" s="12"/>
-      <c r="I2189" s="13"/>
+      <c r="A2189" s="12">
+        <v>44755</v>
+      </c>
+      <c r="B2189" s="12">
+        <v>44755</v>
+      </c>
+      <c r="C2189" s="10" t="s">
+        <v>2680</v>
+      </c>
+      <c r="D2189" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2189" s="11" t="s">
+        <v>2943</v>
+      </c>
+      <c r="F2189" s="10" t="s">
+        <v>2987</v>
+      </c>
+      <c r="G2189" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H2189" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2189" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2189" s="13"/>
     </row>
-    <row r="2190" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="2190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2190" s="12">
-        <v>44698</v>
+        <v>44754</v>
       </c>
       <c r="B2190" s="12"/>
       <c r="C2190" s="10" t="s">
-        <v>895</v>
+        <v>621</v>
       </c>
       <c r="D2190" s="10" t="s">
-        <v>492</v>
+        <v>6</v>
       </c>
       <c r="E2190" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2190" s="30" t="s">
-        <v>2798</v>
+        <v>618</v>
+      </c>
+      <c r="F2190" s="10" t="s">
+        <v>2981</v>
       </c>
       <c r="G2190" s="11"/>
       <c r="H2190" s="12"/>
       <c r="I2190" s="13"/>
       <c r="J2190" s="13"/>
     </row>
-    <row r="2191" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2191" s="12">
-        <v>44684</v>
-      </c>
+    <row r="2191" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2191" s="12"/>
       <c r="B2191" s="12"/>
-      <c r="C2191" s="14" t="s">
-        <v>2155</v>
-      </c>
-      <c r="D2191" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2191" s="11" t="s">
-        <v>618</v>
-      </c>
-      <c r="F2191" s="10" t="s">
-        <v>2799</v>
-      </c>
+      <c r="C2191" s="10"/>
+      <c r="D2191" s="10"/>
+      <c r="E2191" s="11"/>
+      <c r="F2191" s="10"/>
       <c r="G2191" s="11"/>
       <c r="H2191" s="12"/>
       <c r="I2191" s="13"/>
       <c r="J2191" s="13"/>
     </row>
-    <row r="2192" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2192" s="12">
-        <v>44677</v>
-      </c>
+    <row r="2192" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2192" s="12"/>
       <c r="B2192" s="12"/>
-      <c r="C2192" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="D2192" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2192" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2192" s="10" t="s">
-        <v>2729</v>
-      </c>
+      <c r="C2192" s="10"/>
+      <c r="D2192" s="10"/>
+      <c r="E2192" s="11"/>
+      <c r="F2192" s="10"/>
       <c r="G2192" s="11"/>
       <c r="H2192" s="12"/>
       <c r="I2192" s="13"/>
       <c r="J2192" s="13"/>
     </row>
-    <row r="2193" spans="1:10" ht="132" x14ac:dyDescent="0.2">
-      <c r="A2193" s="12">
-        <v>44645</v>
-      </c>
+    <row r="2193" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2193" s="12"/>
       <c r="B2193" s="12"/>
-      <c r="C2193" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D2193" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2193" s="11" t="s">
-        <v>618</v>
-      </c>
-      <c r="F2193" s="10" t="s">
-        <v>2664</v>
-      </c>
+      <c r="C2193" s="10"/>
+      <c r="D2193" s="10"/>
+      <c r="E2193" s="11"/>
+      <c r="F2193" s="10"/>
       <c r="G2193" s="11"/>
       <c r="H2193" s="12"/>
       <c r="I2193" s="13"/>
       <c r="J2193" s="13"/>
     </row>
-    <row r="2194" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2194" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2194" s="12">
-        <v>44642</v>
+        <v>44698</v>
       </c>
       <c r="B2194" s="12"/>
-      <c r="C2194" s="14" t="s">
-        <v>387</v>
+      <c r="C2194" s="10" t="s">
+        <v>895</v>
       </c>
       <c r="D2194" s="10" t="s">
         <v>492</v>
@@ -75990,45 +76047,43 @@
       <c r="E2194" s="11" t="s">
         <v>835</v>
       </c>
-      <c r="F2194" s="10" t="s">
-        <v>2625</v>
+      <c r="F2194" s="30" t="s">
+        <v>2798</v>
       </c>
       <c r="G2194" s="11"/>
       <c r="H2194" s="12"/>
       <c r="I2194" s="13"/>
       <c r="J2194" s="13"/>
     </row>
-    <row r="2195" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2195" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2195" s="12">
-        <v>44642</v>
+        <v>44684</v>
       </c>
       <c r="B2195" s="12"/>
       <c r="C2195" s="14" t="s">
-        <v>387</v>
+        <v>2155</v>
       </c>
       <c r="D2195" s="10" t="s">
-        <v>492</v>
+        <v>83</v>
       </c>
       <c r="E2195" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F2195" s="10" t="s">
-        <v>2624</v>
+        <v>2799</v>
       </c>
       <c r="G2195" s="11"/>
       <c r="H2195" s="12"/>
       <c r="I2195" s="13"/>
       <c r="J2195" s="13"/>
     </row>
-    <row r="2196" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2196" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2196" s="12">
-        <v>44614</v>
-      </c>
-      <c r="B2196" s="12">
-        <v>44614</v>
-      </c>
+        <v>44677</v>
+      </c>
+      <c r="B2196" s="12"/>
       <c r="C2196" s="14" t="s">
-        <v>19</v>
+        <v>387</v>
       </c>
       <c r="D2196" s="10" t="s">
         <v>492</v>
@@ -76037,29 +76092,29 @@
         <v>835</v>
       </c>
       <c r="F2196" s="10" t="s">
-        <v>2528</v>
+        <v>2729</v>
       </c>
       <c r="G2196" s="11"/>
       <c r="H2196" s="12"/>
       <c r="I2196" s="13"/>
       <c r="J2196" s="13"/>
     </row>
-    <row r="2197" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2197" spans="1:10" ht="132" x14ac:dyDescent="0.2">
       <c r="A2197" s="12">
-        <v>44614</v>
+        <v>44645</v>
       </c>
       <c r="B2197" s="12"/>
       <c r="C2197" s="14" t="s">
-        <v>19</v>
+        <v>288</v>
       </c>
       <c r="D2197" s="10" t="s">
-        <v>492</v>
+        <v>25</v>
       </c>
       <c r="E2197" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F2197" s="10" t="s">
-        <v>2548</v>
+        <v>2664</v>
       </c>
       <c r="G2197" s="11"/>
       <c r="H2197" s="12"/>
@@ -76068,20 +76123,20 @@
     </row>
     <row r="2198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2198" s="12">
-        <v>44616</v>
+        <v>44642</v>
       </c>
       <c r="B2198" s="12"/>
       <c r="C2198" s="14" t="s">
-        <v>2250</v>
+        <v>387</v>
       </c>
       <c r="D2198" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E2198" s="11" t="s">
-        <v>618</v>
+        <v>835</v>
       </c>
       <c r="F2198" s="10" t="s">
-        <v>2555</v>
+        <v>2625</v>
       </c>
       <c r="G2198" s="11"/>
       <c r="H2198" s="12"/>
@@ -76090,42 +76145,44 @@
     </row>
     <row r="2199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2199" s="12">
-        <v>44623</v>
+        <v>44642</v>
       </c>
       <c r="B2199" s="12"/>
       <c r="C2199" s="14" t="s">
-        <v>535</v>
+        <v>387</v>
       </c>
       <c r="D2199" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2199" s="11" t="s">
         <v>835</v>
       </c>
       <c r="F2199" s="10" t="s">
-        <v>2573</v>
+        <v>2624</v>
       </c>
       <c r="G2199" s="11"/>
       <c r="H2199" s="12"/>
       <c r="I2199" s="13"/>
       <c r="J2199" s="13"/>
     </row>
-    <row r="2200" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="2200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2200" s="12">
-        <v>44522</v>
-      </c>
-      <c r="B2200" s="12"/>
+        <v>44614</v>
+      </c>
+      <c r="B2200" s="12">
+        <v>44614</v>
+      </c>
       <c r="C2200" s="14" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="D2200" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2200" s="11" t="s">
-        <v>568</v>
+        <v>835</v>
       </c>
       <c r="F2200" s="10" t="s">
-        <v>2350</v>
+        <v>2528</v>
       </c>
       <c r="G2200" s="11"/>
       <c r="H2200" s="12"/>
@@ -76133,48 +76190,88 @@
       <c r="J2200" s="13"/>
     </row>
     <row r="2201" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2201" s="12"/>
+      <c r="A2201" s="12">
+        <v>44614</v>
+      </c>
       <c r="B2201" s="12"/>
-      <c r="C2201" s="14"/>
-      <c r="D2201" s="10"/>
-      <c r="E2201" s="11"/>
-      <c r="F2201" s="10"/>
+      <c r="C2201" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2201" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2201" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2201" s="10" t="s">
+        <v>2548</v>
+      </c>
       <c r="G2201" s="11"/>
       <c r="H2201" s="12"/>
       <c r="I2201" s="13"/>
       <c r="J2201" s="13"/>
     </row>
     <row r="2202" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2202" s="12"/>
+      <c r="A2202" s="12">
+        <v>44616</v>
+      </c>
       <c r="B2202" s="12"/>
-      <c r="C2202" s="14"/>
-      <c r="D2202" s="10"/>
-      <c r="E2202" s="11"/>
-      <c r="F2202" s="10"/>
+      <c r="C2202" s="14" t="s">
+        <v>2250</v>
+      </c>
+      <c r="D2202" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2202" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2202" s="10" t="s">
+        <v>2555</v>
+      </c>
       <c r="G2202" s="11"/>
       <c r="H2202" s="12"/>
       <c r="I2202" s="13"/>
       <c r="J2202" s="13"/>
     </row>
     <row r="2203" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2203" s="12"/>
+      <c r="A2203" s="12">
+        <v>44623</v>
+      </c>
       <c r="B2203" s="12"/>
-      <c r="C2203" s="14"/>
-      <c r="D2203" s="10"/>
-      <c r="E2203" s="11"/>
-      <c r="F2203" s="10"/>
+      <c r="C2203" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="D2203" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2203" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2203" s="10" t="s">
+        <v>2573</v>
+      </c>
       <c r="G2203" s="11"/>
       <c r="H2203" s="12"/>
       <c r="I2203" s="13"/>
       <c r="J2203" s="13"/>
     </row>
-    <row r="2204" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2204" s="12"/>
+    <row r="2204" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2204" s="12">
+        <v>44522</v>
+      </c>
       <c r="B2204" s="12"/>
-      <c r="C2204" s="14"/>
-      <c r="D2204" s="10"/>
-      <c r="E2204" s="11"/>
-      <c r="F2204" s="10"/>
+      <c r="C2204" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2204" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2204" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2204" s="10" t="s">
+        <v>2350</v>
+      </c>
       <c r="G2204" s="11"/>
       <c r="H2204" s="12"/>
       <c r="I2204" s="13"/>
@@ -76218,7 +76315,7 @@
     </row>
     <row r="2208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2208" s="12"/>
-      <c r="B2208" s="9"/>
+      <c r="B2208" s="12"/>
       <c r="C2208" s="14"/>
       <c r="D2208" s="10"/>
       <c r="E2208" s="11"/>
@@ -76229,38 +76326,20 @@
       <c r="J2208" s="13"/>
     </row>
     <row r="2209" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2209" s="1" t="s">
-        <v>1472</v>
-      </c>
-      <c r="B2209" s="2" t="s">
-        <v>1473</v>
-      </c>
-      <c r="C2209" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2209" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2209" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="F2209" s="4" t="s">
-        <v>1571</v>
-      </c>
-      <c r="G2209" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2209" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2209" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2209" s="36"/>
+      <c r="A2209" s="12"/>
+      <c r="B2209" s="12"/>
+      <c r="C2209" s="14"/>
+      <c r="D2209" s="10"/>
+      <c r="E2209" s="11"/>
+      <c r="F2209" s="10"/>
+      <c r="G2209" s="11"/>
+      <c r="H2209" s="12"/>
+      <c r="I2209" s="13"/>
+      <c r="J2209" s="13"/>
     </row>
     <row r="2210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2210" s="12"/>
-      <c r="B2210" s="9"/>
+      <c r="B2210" s="12"/>
       <c r="C2210" s="14"/>
       <c r="D2210" s="10"/>
       <c r="E2210" s="11"/>
@@ -76272,7 +76351,7 @@
     </row>
     <row r="2211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2211" s="12"/>
-      <c r="B2211" s="9"/>
+      <c r="B2211" s="12"/>
       <c r="C2211" s="14"/>
       <c r="D2211" s="10"/>
       <c r="E2211" s="11"/>
@@ -76282,121 +76361,99 @@
       <c r="I2211" s="13"/>
       <c r="J2211" s="13"/>
     </row>
-    <row r="2212" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A2212" s="12">
-        <v>44252</v>
-      </c>
+    <row r="2212" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2212" s="12"/>
       <c r="B2212" s="9"/>
-      <c r="C2212" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2212" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2212" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2212" s="10" t="s">
-        <v>1636</v>
-      </c>
+      <c r="C2212" s="14"/>
+      <c r="D2212" s="10"/>
+      <c r="E2212" s="11"/>
+      <c r="F2212" s="10"/>
       <c r="G2212" s="11"/>
       <c r="H2212" s="12"/>
       <c r="I2212" s="13"/>
-      <c r="J2212" s="13" t="s">
-        <v>1659</v>
-      </c>
-    </row>
-    <row r="2213" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A2213" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2213" s="9"/>
-      <c r="C2213" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2213" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2213" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2213" s="10" t="s">
-        <v>1635</v>
-      </c>
-      <c r="G2213" s="11"/>
-      <c r="H2213" s="12"/>
-      <c r="I2213" s="13"/>
-      <c r="J2213" s="13"/>
-    </row>
-    <row r="2214" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2214" s="12">
-        <v>44112</v>
-      </c>
+      <c r="J2212" s="13"/>
+    </row>
+    <row r="2213" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2213" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B2213" s="2" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C2213" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2213" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2213" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F2213" s="4" t="s">
+        <v>1571</v>
+      </c>
+      <c r="G2213" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2213" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2213" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2213" s="36"/>
+    </row>
+    <row r="2214" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2214" s="12"/>
       <c r="B2214" s="9"/>
-      <c r="C2214" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D2214" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2214" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2214" s="10" t="s">
-        <v>2222</v>
-      </c>
+      <c r="C2214" s="14"/>
+      <c r="D2214" s="10"/>
+      <c r="E2214" s="11"/>
+      <c r="F2214" s="10"/>
       <c r="G2214" s="11"/>
       <c r="H2214" s="12"/>
       <c r="I2214" s="13"/>
       <c r="J2214" s="13"/>
     </row>
     <row r="2215" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2215" s="12">
-        <v>44088</v>
-      </c>
+      <c r="A2215" s="12"/>
       <c r="B2215" s="9"/>
-      <c r="C2215" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2215" s="10" t="s">
-        <v>902</v>
-      </c>
-      <c r="E2215" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="F2215" s="10" t="s">
-        <v>1007</v>
-      </c>
+      <c r="C2215" s="14"/>
+      <c r="D2215" s="10"/>
+      <c r="E2215" s="11"/>
+      <c r="F2215" s="10"/>
       <c r="G2215" s="11"/>
       <c r="H2215" s="12"/>
       <c r="I2215" s="13"/>
       <c r="J2215" s="13"/>
     </row>
-    <row r="2216" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2216" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A2216" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B2216" s="9"/>
       <c r="C2216" s="14" t="s">
-        <v>621</v>
+        <v>895</v>
       </c>
       <c r="D2216" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2216" s="11" t="s">
-        <v>568</v>
+        <v>757</v>
       </c>
       <c r="F2216" s="10" t="s">
-        <v>900</v>
+        <v>1636</v>
       </c>
       <c r="G2216" s="11"/>
       <c r="H2216" s="12"/>
       <c r="I2216" s="13"/>
-      <c r="J2216" s="13"/>
-    </row>
-    <row r="2217" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J2216" s="13" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="2217" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A2217" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B2217" s="9"/>
       <c r="C2217" s="14" t="s">
@@ -76406,186 +76463,226 @@
         <v>492</v>
       </c>
       <c r="E2217" s="11" t="s">
-        <v>568</v>
+        <v>757</v>
       </c>
       <c r="F2217" s="10" t="s">
-        <v>897</v>
+        <v>1635</v>
       </c>
       <c r="G2217" s="11"/>
       <c r="H2217" s="12"/>
       <c r="I2217" s="13"/>
       <c r="J2217" s="13"/>
     </row>
-    <row r="2218" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="2218" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2218" s="12">
-        <v>44055</v>
+        <v>44112</v>
       </c>
       <c r="B2218" s="9"/>
       <c r="C2218" s="14" t="s">
-        <v>895</v>
+        <v>621</v>
       </c>
       <c r="D2218" s="10" t="s">
-        <v>492</v>
+        <v>6</v>
       </c>
       <c r="E2218" s="11" t="s">
         <v>568</v>
       </c>
       <c r="F2218" s="10" t="s">
-        <v>898</v>
+        <v>2222</v>
       </c>
       <c r="G2218" s="11"/>
       <c r="H2218" s="12"/>
       <c r="I2218" s="13"/>
       <c r="J2218" s="13"/>
     </row>
-    <row r="2219" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="2219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2219" s="12">
-        <v>43949</v>
+        <v>44088</v>
       </c>
       <c r="B2219" s="9"/>
       <c r="C2219" s="14" t="s">
-        <v>468</v>
+        <v>19</v>
       </c>
       <c r="D2219" s="10" t="s">
-        <v>89</v>
+        <v>902</v>
       </c>
       <c r="E2219" s="11" t="s">
         <v>683</v>
       </c>
       <c r="F2219" s="10" t="s">
-        <v>684</v>
-      </c>
-      <c r="G2219" s="11" t="s">
-        <v>1616</v>
-      </c>
+        <v>1007</v>
+      </c>
+      <c r="G2219" s="11"/>
       <c r="H2219" s="12"/>
-      <c r="I2219" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I2219" s="13"/>
       <c r="J2219" s="13"/>
     </row>
-    <row r="2220" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="2220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2220" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B2220" s="9"/>
       <c r="C2220" s="14" t="s">
-        <v>468</v>
+        <v>621</v>
       </c>
       <c r="D2220" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E2220" s="11" t="s">
-        <v>683</v>
+        <v>568</v>
       </c>
       <c r="F2220" s="10" t="s">
-        <v>703</v>
-      </c>
-      <c r="G2220" s="11" t="s">
-        <v>685</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="G2220" s="11"/>
       <c r="H2220" s="12"/>
-      <c r="I2220" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J2220" s="13" t="s">
-        <v>1561</v>
-      </c>
-    </row>
-    <row r="2221" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I2220" s="13"/>
+      <c r="J2220" s="13"/>
+    </row>
+    <row r="2221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2221" s="12">
-        <v>43838</v>
+        <v>44055</v>
       </c>
       <c r="B2221" s="9"/>
       <c r="C2221" s="14" t="s">
-        <v>103</v>
+        <v>895</v>
       </c>
       <c r="D2221" s="10" t="s">
-        <v>460</v>
+        <v>492</v>
       </c>
       <c r="E2221" s="11" t="s">
-        <v>645</v>
+        <v>568</v>
       </c>
       <c r="F2221" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="G2221" s="11" t="s">
-        <v>1617</v>
-      </c>
+        <v>897</v>
+      </c>
+      <c r="G2221" s="11"/>
       <c r="H2221" s="12"/>
       <c r="I2221" s="13"/>
-      <c r="J2221" s="13" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="2222" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J2221" s="13"/>
+    </row>
+    <row r="2222" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A2222" s="12">
-        <v>43762</v>
+        <v>44055</v>
       </c>
       <c r="B2222" s="9"/>
       <c r="C2222" s="14" t="s">
-        <v>446</v>
+        <v>895</v>
       </c>
       <c r="D2222" s="10" t="s">
-        <v>17</v>
+        <v>492</v>
       </c>
       <c r="E2222" s="11" t="s">
-        <v>835</v>
+        <v>568</v>
       </c>
       <c r="F2222" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G2222" s="11" t="s">
-        <v>1606</v>
-      </c>
+        <v>898</v>
+      </c>
+      <c r="G2222" s="11"/>
       <c r="H2222" s="12"/>
       <c r="I2222" s="13"/>
       <c r="J2222" s="13"/>
     </row>
-    <row r="2223" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2223" s="12"/>
+    <row r="2223" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2223" s="12">
+        <v>43949</v>
+      </c>
       <c r="B2223" s="9"/>
-      <c r="C2223" s="14"/>
-      <c r="D2223" s="10"/>
-      <c r="E2223" s="11"/>
-      <c r="F2223" s="10"/>
-      <c r="G2223" s="11"/>
+      <c r="C2223" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2223" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2223" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2223" s="10" t="s">
+        <v>684</v>
+      </c>
+      <c r="G2223" s="11" t="s">
+        <v>1616</v>
+      </c>
       <c r="H2223" s="12"/>
-      <c r="I2223" s="13"/>
+      <c r="I2223" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J2223" s="13"/>
     </row>
-    <row r="2224" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2224" s="12"/>
+    <row r="2224" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2224" s="12">
+        <v>43949</v>
+      </c>
       <c r="B2224" s="9"/>
-      <c r="C2224" s="14"/>
-      <c r="D2224" s="10"/>
-      <c r="E2224" s="11"/>
-      <c r="F2224" s="10"/>
-      <c r="G2224" s="11"/>
+      <c r="C2224" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2224" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2224" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2224" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="G2224" s="11" t="s">
+        <v>685</v>
+      </c>
       <c r="H2224" s="12"/>
-      <c r="I2224" s="13"/>
-      <c r="J2224" s="13"/>
-    </row>
-    <row r="2225" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2225" s="12"/>
+      <c r="I2224" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J2224" s="13" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="2225" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2225" s="12">
+        <v>43838</v>
+      </c>
       <c r="B2225" s="9"/>
-      <c r="C2225" s="14"/>
-      <c r="D2225" s="10"/>
-      <c r="E2225" s="11"/>
-      <c r="F2225" s="10"/>
-      <c r="G2225" s="11"/>
+      <c r="C2225" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2225" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2225" s="11" t="s">
+        <v>645</v>
+      </c>
+      <c r="F2225" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="G2225" s="11" t="s">
+        <v>1617</v>
+      </c>
       <c r="H2225" s="12"/>
       <c r="I2225" s="13"/>
-      <c r="J2225" s="13"/>
-    </row>
-    <row r="2226" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2226" s="12"/>
+      <c r="J2225" s="13" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="2226" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2226" s="12">
+        <v>43762</v>
+      </c>
       <c r="B2226" s="9"/>
-      <c r="C2226" s="14"/>
-      <c r="D2226" s="10"/>
-      <c r="E2226" s="11"/>
-      <c r="F2226" s="10"/>
-      <c r="G2226" s="11"/>
+      <c r="C2226" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D2226" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2226" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2226" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G2226" s="11" t="s">
+        <v>1606</v>
+      </c>
       <c r="H2226" s="12"/>
       <c r="I2226" s="13"/>
       <c r="J2226" s="13"/>
@@ -76613,6 +76710,54 @@
       <c r="H2228" s="12"/>
       <c r="I2228" s="13"/>
       <c r="J2228" s="13"/>
+    </row>
+    <row r="2229" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2229" s="12"/>
+      <c r="B2229" s="9"/>
+      <c r="C2229" s="14"/>
+      <c r="D2229" s="10"/>
+      <c r="E2229" s="11"/>
+      <c r="F2229" s="10"/>
+      <c r="G2229" s="11"/>
+      <c r="H2229" s="12"/>
+      <c r="I2229" s="13"/>
+      <c r="J2229" s="13"/>
+    </row>
+    <row r="2230" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2230" s="12"/>
+      <c r="B2230" s="9"/>
+      <c r="C2230" s="14"/>
+      <c r="D2230" s="10"/>
+      <c r="E2230" s="11"/>
+      <c r="F2230" s="10"/>
+      <c r="G2230" s="11"/>
+      <c r="H2230" s="12"/>
+      <c r="I2230" s="13"/>
+      <c r="J2230" s="13"/>
+    </row>
+    <row r="2231" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2231" s="12"/>
+      <c r="B2231" s="9"/>
+      <c r="C2231" s="14"/>
+      <c r="D2231" s="10"/>
+      <c r="E2231" s="11"/>
+      <c r="F2231" s="10"/>
+      <c r="G2231" s="11"/>
+      <c r="H2231" s="12"/>
+      <c r="I2231" s="13"/>
+      <c r="J2231" s="13"/>
+    </row>
+    <row r="2232" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2232" s="12"/>
+      <c r="B2232" s="9"/>
+      <c r="C2232" s="14"/>
+      <c r="D2232" s="10"/>
+      <c r="E2232" s="11"/>
+      <c r="F2232" s="10"/>
+      <c r="G2232" s="11"/>
+      <c r="H2232" s="12"/>
+      <c r="I2232" s="13"/>
+      <c r="J2232" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1881" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Acerto Mapa de INSS Retido
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1355097-FD93-46EB-A99A-E91BC7172937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F070B5E0-5425-46D8-A3FD-DCE5D2ECCE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandas BK - Protheus" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15749" uniqueCount="3013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15846" uniqueCount="3028">
   <si>
     <t>Responsável</t>
   </si>
@@ -9433,9 +9433,6 @@
     <t>BKFINR32</t>
   </si>
   <si>
-    <t>Relatorio de emprestimo0s não aparece todos os titulos</t>
-  </si>
-  <si>
     <t>Divergencia entre o valor líquido dos relatórios "BKFINR30-Clientes em Aberto"  e "BKGCTR07-Mapa de INSS Retido"</t>
   </si>
   <si>
@@ -9533,6 +9530,62 @@
   </si>
   <si>
     <t>Encargos e incidencias de folha no dasboard</t>
+  </si>
+  <si>
+    <t>As vezes, não é possível escoclher entre Multa e Bonificação da planilha selecionada na Nova Medição</t>
+  </si>
+  <si>
+    <t>Erika</t>
+  </si>
+  <si>
+    <t>Problemas com dízimas na nova medição</t>
+  </si>
+  <si>
+    <t>NFs não estão aparecendo para liberar no meu usuário</t>
+  </si>
+  <si>
+    <t>Foi orientado acertar as dizimas da quantidade</t>
+  </si>
+  <si>
+    <t>NF foi relançada pelo Depto Fiscal, indo para a Vanderleia liberar</t>
+  </si>
+  <si>
+    <t>Alimentar a tabela GERAL com o campo custo da tabela FOLHA</t>
+  </si>
+  <si>
+    <t>Alimentar a tabela GERAL com o campo custo da tabela FOLHA e criação das tabelas EMPRESAS e CCUSTOS</t>
+  </si>
+  <si>
+    <t>Alterar os municípios das planilhas 6 a 21 de Macae para Rio de Janeiro do contrato 335000521</t>
+  </si>
+  <si>
+    <t>Alterar os municípios das planilhas 4 e 5 de Macae para Rio de Janeiro do contrato 335000521 e verificar os demais contratos deste cliente se estavam neste municípo</t>
+  </si>
+  <si>
+    <t>Conforme ocorreu em meses anteriores,temos municípios novos no contrato BHG 305000554.
+FAVOR VERIFICAR A TRIBUTAÇÃO E CRIAR PRODUTO PARA JARINU E SANTA GERTRUDES</t>
+  </si>
+  <si>
+    <t>Criados os produtos</t>
+  </si>
+  <si>
+    <t>Baseado em erro verificado na aprovação do mes passado .
+Note que as planilhas tem dois codigos de serviço,17.02 e 23.01.
+Me parece que o produto para 17.02 é igual para os dois municipios e nao precisa ser alterado.(335000521-001)
+Ja o de desenho industrial esta diferente ,rio com 335000521-002 e macae 335000521-003.Precisamos alterar para o produto do Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>Os produtos são identicos, não há necessidade de se alterar</t>
+  </si>
+  <si>
+    <t>Ajustes no DashBoard
+Criar campo RESULTADO na tabela GERAL (descontar a conta vinculada) do liquido.
+BHG X2 Faturamento ( dado o fato que as despesas e custos representam 100% do consorcio)
+Tabela geral com valores duplicados
+O ISS Retido e Apurado precisam entrar dentro da conta de faturamento líquido e a retenção e conta vinculada precisam sair</t>
+  </si>
+  <si>
+    <t>Relatorio de emprestimos não aparece todos os titulos</t>
   </si>
 </sst>
 </file>
@@ -10338,11 +10391,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J2256"/>
+  <dimension ref="A1:J2268"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2208" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2213" sqref="A2213"/>
+      <pane ySplit="1" topLeftCell="A2234" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2241" sqref="F2241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -75946,7 +75999,7 @@
         <v>618</v>
       </c>
       <c r="F2186" s="10" t="s">
-        <v>2982</v>
+        <v>2981</v>
       </c>
       <c r="G2186" s="11" t="s">
         <v>295</v>
@@ -75958,7 +76011,7 @@
         <v>13</v>
       </c>
       <c r="J2186" s="13" t="s">
-        <v>2983</v>
+        <v>2982</v>
       </c>
     </row>
     <row r="2187" spans="1:10" x14ac:dyDescent="0.2">
@@ -75978,7 +76031,7 @@
         <v>618</v>
       </c>
       <c r="F2187" s="10" t="s">
-        <v>2984</v>
+        <v>2983</v>
       </c>
       <c r="G2187" s="11" t="s">
         <v>1598</v>
@@ -76008,7 +76061,7 @@
         <v>618</v>
       </c>
       <c r="F2188" s="10" t="s">
-        <v>2985</v>
+        <v>2984</v>
       </c>
       <c r="G2188" s="11" t="s">
         <v>1827</v>
@@ -76020,7 +76073,7 @@
         <v>13</v>
       </c>
       <c r="J2188" s="13" t="s">
-        <v>2986</v>
+        <v>2985</v>
       </c>
     </row>
     <row r="2189" spans="1:10" x14ac:dyDescent="0.2">
@@ -76040,7 +76093,7 @@
         <v>2943</v>
       </c>
       <c r="F2189" s="10" t="s">
-        <v>2987</v>
+        <v>2986</v>
       </c>
       <c r="G2189" s="11" t="s">
         <v>308</v>
@@ -76070,7 +76123,7 @@
         <v>618</v>
       </c>
       <c r="F2190" s="10" t="s">
-        <v>2989</v>
+        <v>2988</v>
       </c>
       <c r="G2190" s="11" t="s">
         <v>309</v>
@@ -76100,7 +76153,7 @@
         <v>2943</v>
       </c>
       <c r="F2191" s="10" t="s">
-        <v>2988</v>
+        <v>2987</v>
       </c>
       <c r="G2191" s="11" t="s">
         <v>309</v>
@@ -76130,7 +76183,7 @@
         <v>618</v>
       </c>
       <c r="F2192" s="10" t="s">
-        <v>2990</v>
+        <v>2989</v>
       </c>
       <c r="G2192" s="11" t="s">
         <v>1623</v>
@@ -76160,7 +76213,7 @@
         <v>2943</v>
       </c>
       <c r="F2193" s="10" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="G2193" s="11" t="s">
         <v>295</v>
@@ -76172,19 +76225,31 @@
         <v>13</v>
       </c>
       <c r="J2193" s="13" t="s">
-        <v>2992</v>
+        <v>2991</v>
       </c>
     </row>
     <row r="2194" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2194" s="12"/>
-      <c r="B2194" s="12"/>
-      <c r="C2194" s="10"/>
-      <c r="D2194" s="10"/>
-      <c r="E2194" s="11"/>
+      <c r="A2194" s="12">
+        <v>44760</v>
+      </c>
+      <c r="B2194" s="12">
+        <v>44760</v>
+      </c>
+      <c r="C2194" s="10" t="s">
+        <v>1924</v>
+      </c>
+      <c r="D2194" s="10" t="s">
+        <v>749</v>
+      </c>
+      <c r="E2194" s="11" t="s">
+        <v>618</v>
+      </c>
       <c r="F2194" s="10" t="s">
-        <v>2995</v>
-      </c>
-      <c r="G2194" s="11"/>
+        <v>2994</v>
+      </c>
+      <c r="G2194" s="11" t="s">
+        <v>1598</v>
+      </c>
       <c r="H2194" s="12"/>
       <c r="I2194" s="13"/>
       <c r="J2194" s="13"/>
@@ -76193,7 +76258,9 @@
       <c r="A2195" s="12">
         <v>44754</v>
       </c>
-      <c r="B2195" s="12"/>
+      <c r="B2195" s="12">
+        <v>44760</v>
+      </c>
       <c r="C2195" s="10" t="s">
         <v>621</v>
       </c>
@@ -76204,18 +76271,26 @@
         <v>618</v>
       </c>
       <c r="F2195" s="10" t="s">
-        <v>2981</v>
-      </c>
-      <c r="G2195" s="11"/>
-      <c r="H2195" s="12"/>
-      <c r="I2195" s="13"/>
+        <v>3027</v>
+      </c>
+      <c r="G2195" s="11" t="s">
+        <v>1601</v>
+      </c>
+      <c r="H2195" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2195" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2195" s="13"/>
     </row>
     <row r="2196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2196" s="12">
         <v>44761</v>
       </c>
-      <c r="B2196" s="12"/>
+      <c r="B2196" s="12">
+        <v>44761</v>
+      </c>
       <c r="C2196" s="10" t="s">
         <v>387</v>
       </c>
@@ -76226,7 +76301,7 @@
         <v>835</v>
       </c>
       <c r="F2196" s="10" t="s">
-        <v>2993</v>
+        <v>2992</v>
       </c>
       <c r="G2196" s="11"/>
       <c r="H2196" s="12"/>
@@ -76250,7 +76325,7 @@
         <v>2943</v>
       </c>
       <c r="F2197" s="10" t="s">
-        <v>2994</v>
+        <v>2993</v>
       </c>
       <c r="G2197" s="11" t="s">
         <v>309</v>
@@ -76280,7 +76355,7 @@
         <v>618</v>
       </c>
       <c r="F2198" s="10" t="s">
-        <v>2998</v>
+        <v>2997</v>
       </c>
       <c r="G2198" s="11" t="s">
         <v>1602</v>
@@ -76310,7 +76385,7 @@
         <v>835</v>
       </c>
       <c r="F2199" s="10" t="s">
-        <v>2997</v>
+        <v>2996</v>
       </c>
       <c r="G2199" s="11" t="s">
         <v>295</v>
@@ -76340,7 +76415,7 @@
         <v>618</v>
       </c>
       <c r="F2200" s="10" t="s">
-        <v>2999</v>
+        <v>2998</v>
       </c>
       <c r="G2200" s="11" t="s">
         <v>295</v>
@@ -76370,7 +76445,7 @@
         <v>618</v>
       </c>
       <c r="F2201" s="10" t="s">
-        <v>3000</v>
+        <v>2999</v>
       </c>
       <c r="G2201" s="11" t="s">
         <v>1623</v>
@@ -76400,7 +76475,7 @@
         <v>683</v>
       </c>
       <c r="F2202" s="10" t="s">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="G2202" s="11" t="s">
         <v>295</v>
@@ -76430,7 +76505,7 @@
         <v>683</v>
       </c>
       <c r="F2203" s="10" t="s">
-        <v>3002</v>
+        <v>3001</v>
       </c>
       <c r="G2203" s="11" t="s">
         <v>295</v>
@@ -76460,7 +76535,7 @@
         <v>683</v>
       </c>
       <c r="F2204" s="10" t="s">
-        <v>3003</v>
+        <v>3002</v>
       </c>
       <c r="G2204" s="11" t="s">
         <v>309</v>
@@ -76490,7 +76565,7 @@
         <v>645</v>
       </c>
       <c r="F2205" s="10" t="s">
-        <v>3004</v>
+        <v>3003</v>
       </c>
       <c r="G2205" s="11" t="s">
         <v>1601</v>
@@ -76520,7 +76595,7 @@
         <v>696</v>
       </c>
       <c r="F2206" s="10" t="s">
-        <v>3005</v>
+        <v>3004</v>
       </c>
       <c r="G2206" s="11" t="s">
         <v>295</v>
@@ -76550,7 +76625,7 @@
         <v>2943</v>
       </c>
       <c r="F2207" s="10" t="s">
-        <v>3006</v>
+        <v>3005</v>
       </c>
       <c r="G2207" s="11" t="s">
         <v>309</v>
@@ -76580,7 +76655,7 @@
         <v>618</v>
       </c>
       <c r="F2208" s="10" t="s">
-        <v>3007</v>
+        <v>3006</v>
       </c>
       <c r="G2208" s="11" t="s">
         <v>295</v>
@@ -76610,7 +76685,7 @@
         <v>683</v>
       </c>
       <c r="F2209" s="10" t="s">
-        <v>3008</v>
+        <v>3007</v>
       </c>
       <c r="G2209" s="11" t="s">
         <v>1623</v>
@@ -76640,7 +76715,7 @@
         <v>683</v>
       </c>
       <c r="F2210" s="10" t="s">
-        <v>3009</v>
+        <v>3008</v>
       </c>
       <c r="G2210" s="11" t="s">
         <v>1598</v>
@@ -76670,7 +76745,7 @@
         <v>835</v>
       </c>
       <c r="F2211" s="10" t="s">
-        <v>3010</v>
+        <v>3009</v>
       </c>
       <c r="G2211" s="11" t="s">
         <v>308</v>
@@ -76700,7 +76775,7 @@
         <v>835</v>
       </c>
       <c r="F2212" s="10" t="s">
-        <v>3011</v>
+        <v>3010</v>
       </c>
       <c r="G2212" s="11" t="s">
         <v>1598</v>
@@ -76720,11 +76795,17 @@
       <c r="B2213" s="12">
         <v>44768</v>
       </c>
-      <c r="C2213" s="10"/>
-      <c r="D2213" s="10"/>
-      <c r="E2213" s="11"/>
+      <c r="C2213" s="10" t="s">
+        <v>2680</v>
+      </c>
+      <c r="D2213" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2213" s="11" t="s">
+        <v>835</v>
+      </c>
       <c r="F2213" s="10" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="G2213" s="11" t="s">
         <v>308</v>
@@ -76738,236 +76819,334 @@
       <c r="J2213" s="13"/>
     </row>
     <row r="2214" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2214" s="12"/>
-      <c r="B2214" s="12"/>
-      <c r="C2214" s="10"/>
-      <c r="D2214" s="10"/>
-      <c r="E2214" s="11"/>
-      <c r="F2214" s="10"/>
-      <c r="G2214" s="11"/>
-      <c r="H2214" s="12"/>
-      <c r="I2214" s="13"/>
+      <c r="A2214" s="12">
+        <v>44769</v>
+      </c>
+      <c r="B2214" s="12">
+        <v>44769</v>
+      </c>
+      <c r="C2214" s="10" t="s">
+        <v>2680</v>
+      </c>
+      <c r="D2214" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2214" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2214" s="10" t="s">
+        <v>3011</v>
+      </c>
+      <c r="G2214" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H2214" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2214" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2214" s="13"/>
     </row>
     <row r="2215" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2215" s="12"/>
-      <c r="B2215" s="12"/>
-      <c r="C2215" s="10"/>
-      <c r="D2215" s="10"/>
-      <c r="E2215" s="11"/>
-      <c r="F2215" s="10"/>
-      <c r="G2215" s="11"/>
-      <c r="H2215" s="12"/>
-      <c r="I2215" s="13"/>
-      <c r="J2215" s="13"/>
+      <c r="A2215" s="12">
+        <v>44770</v>
+      </c>
+      <c r="B2215" s="12">
+        <v>44770</v>
+      </c>
+      <c r="C2215" s="10" t="s">
+        <v>3013</v>
+      </c>
+      <c r="D2215" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2215" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2215" s="10" t="s">
+        <v>3014</v>
+      </c>
+      <c r="G2215" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H2215" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2215" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2215" s="13" t="s">
+        <v>3016</v>
+      </c>
     </row>
     <row r="2216" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2216" s="12"/>
-      <c r="B2216" s="12"/>
-      <c r="C2216" s="10"/>
-      <c r="D2216" s="10"/>
-      <c r="E2216" s="11"/>
-      <c r="F2216" s="10"/>
-      <c r="G2216" s="11"/>
-      <c r="H2216" s="12"/>
-      <c r="I2216" s="13"/>
-      <c r="J2216" s="13"/>
+      <c r="A2216" s="12">
+        <v>44770</v>
+      </c>
+      <c r="B2216" s="12">
+        <v>44770</v>
+      </c>
+      <c r="C2216" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D2216" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2216" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2216" s="10" t="s">
+        <v>3015</v>
+      </c>
+      <c r="G2216" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H2216" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2216" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2216" s="13" t="s">
+        <v>3017</v>
+      </c>
     </row>
     <row r="2217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2217" s="12">
-        <v>44761</v>
-      </c>
-      <c r="B2217" s="12"/>
+        <v>44770</v>
+      </c>
+      <c r="B2217" s="12">
+        <v>44770</v>
+      </c>
       <c r="C2217" s="10" t="s">
-        <v>557</v>
+        <v>2680</v>
       </c>
       <c r="D2217" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2217" s="11" t="s">
         <v>835</v>
       </c>
       <c r="F2217" s="10" t="s">
-        <v>2996</v>
-      </c>
-      <c r="G2217" s="11"/>
-      <c r="H2217" s="12"/>
-      <c r="I2217" s="13"/>
+        <v>3018</v>
+      </c>
+      <c r="G2217" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H2217" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2217" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2217" s="13"/>
     </row>
     <row r="2218" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2218" s="12">
-        <v>44698</v>
-      </c>
-      <c r="B2218" s="12"/>
+        <v>44770</v>
+      </c>
+      <c r="B2218" s="12">
+        <v>44770</v>
+      </c>
       <c r="C2218" s="10" t="s">
-        <v>895</v>
+        <v>387</v>
       </c>
       <c r="D2218" s="10" t="s">
         <v>492</v>
       </c>
       <c r="E2218" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2218" s="30" t="s">
-        <v>2798</v>
-      </c>
-      <c r="G2218" s="11"/>
-      <c r="H2218" s="12"/>
-      <c r="I2218" s="13"/>
+        <v>683</v>
+      </c>
+      <c r="F2218" s="10" t="s">
+        <v>3020</v>
+      </c>
+      <c r="G2218" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H2218" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2218" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2218" s="13"/>
     </row>
     <row r="2219" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2219" s="12">
-        <v>44684</v>
-      </c>
-      <c r="B2219" s="12"/>
-      <c r="C2219" s="14" t="s">
-        <v>2155</v>
+        <v>44771</v>
+      </c>
+      <c r="B2219" s="12">
+        <v>44771</v>
+      </c>
+      <c r="C2219" s="10" t="s">
+        <v>2680</v>
       </c>
       <c r="D2219" s="10" t="s">
-        <v>83</v>
+        <v>492</v>
       </c>
       <c r="E2219" s="11" t="s">
-        <v>618</v>
+        <v>835</v>
       </c>
       <c r="F2219" s="10" t="s">
-        <v>2799</v>
-      </c>
-      <c r="G2219" s="11"/>
-      <c r="H2219" s="12"/>
-      <c r="I2219" s="13"/>
+        <v>3019</v>
+      </c>
+      <c r="G2219" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H2219" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2219" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2219" s="13"/>
     </row>
     <row r="2220" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2220" s="12">
-        <v>44677</v>
-      </c>
-      <c r="B2220" s="12"/>
-      <c r="C2220" s="14" t="s">
+        <v>44771</v>
+      </c>
+      <c r="B2220" s="12">
+        <v>44771</v>
+      </c>
+      <c r="C2220" s="10" t="s">
+        <v>638</v>
+      </c>
+      <c r="D2220" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2220" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2220" s="10" t="s">
+        <v>3021</v>
+      </c>
+      <c r="G2220" s="11" t="s">
+        <v>1598</v>
+      </c>
+      <c r="H2220" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2220" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2220" s="13"/>
+    </row>
+    <row r="2221" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2221" s="12">
+        <v>44770</v>
+      </c>
+      <c r="B2221" s="12">
+        <v>44771</v>
+      </c>
+      <c r="C2221" s="10" t="s">
         <v>387</v>
       </c>
-      <c r="D2220" s="10" t="s">
+      <c r="D2221" s="10" t="s">
         <v>492</v>
       </c>
-      <c r="E2220" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2220" s="10" t="s">
-        <v>2729</v>
-      </c>
-      <c r="G2220" s="11"/>
-      <c r="H2220" s="12"/>
-      <c r="I2220" s="13"/>
-      <c r="J2220" s="13"/>
-    </row>
-    <row r="2221" spans="1:10" ht="132" x14ac:dyDescent="0.2">
-      <c r="A2221" s="12">
-        <v>44645</v>
-      </c>
-      <c r="B2221" s="12"/>
-      <c r="C2221" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D2221" s="10" t="s">
-        <v>25</v>
-      </c>
       <c r="E2221" s="11" t="s">
-        <v>618</v>
+        <v>683</v>
       </c>
       <c r="F2221" s="10" t="s">
-        <v>2664</v>
-      </c>
-      <c r="G2221" s="11"/>
-      <c r="H2221" s="12"/>
-      <c r="I2221" s="13"/>
-      <c r="J2221" s="13"/>
-    </row>
-    <row r="2222" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3022</v>
+      </c>
+      <c r="G2221" s="11" t="s">
+        <v>1598</v>
+      </c>
+      <c r="H2221" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2221" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2221" s="13" t="s">
+        <v>3023</v>
+      </c>
+    </row>
+    <row r="2222" spans="1:10" ht="72" x14ac:dyDescent="0.2">
       <c r="A2222" s="12">
-        <v>44642</v>
-      </c>
-      <c r="B2222" s="12"/>
-      <c r="C2222" s="14" t="s">
+        <v>44770</v>
+      </c>
+      <c r="B2222" s="12">
+        <v>44771</v>
+      </c>
+      <c r="C2222" s="10" t="s">
         <v>387</v>
       </c>
       <c r="D2222" s="10" t="s">
         <v>492</v>
       </c>
       <c r="E2222" s="11" t="s">
-        <v>835</v>
+        <v>683</v>
       </c>
       <c r="F2222" s="10" t="s">
-        <v>2625</v>
-      </c>
-      <c r="G2222" s="11"/>
-      <c r="H2222" s="12"/>
-      <c r="I2222" s="13"/>
-      <c r="J2222" s="13"/>
-    </row>
-    <row r="2223" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3024</v>
+      </c>
+      <c r="G2222" s="11" t="s">
+        <v>1598</v>
+      </c>
+      <c r="H2222" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2222" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2222" s="13" t="s">
+        <v>3025</v>
+      </c>
+    </row>
+    <row r="2223" spans="1:10" ht="84" x14ac:dyDescent="0.2">
       <c r="A2223" s="12">
-        <v>44642</v>
-      </c>
-      <c r="B2223" s="12"/>
-      <c r="C2223" s="14" t="s">
-        <v>387</v>
+        <v>44774</v>
+      </c>
+      <c r="B2223" s="12">
+        <v>44774</v>
+      </c>
+      <c r="C2223" s="10" t="s">
+        <v>2680</v>
       </c>
       <c r="D2223" s="10" t="s">
         <v>492</v>
       </c>
       <c r="E2223" s="11" t="s">
-        <v>835</v>
+        <v>2943</v>
       </c>
       <c r="F2223" s="10" t="s">
-        <v>2624</v>
-      </c>
-      <c r="G2223" s="11"/>
-      <c r="H2223" s="12"/>
-      <c r="I2223" s="13"/>
-      <c r="J2223" s="13"/>
+        <v>3026</v>
+      </c>
+      <c r="G2223" s="11" t="s">
+        <v>1606</v>
+      </c>
+      <c r="H2223" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2223" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2223" s="13" t="s">
+        <v>2829</v>
+      </c>
     </row>
     <row r="2224" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2224" s="12">
-        <v>44614</v>
-      </c>
-      <c r="B2224" s="12">
-        <v>44614</v>
-      </c>
-      <c r="C2224" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2224" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2224" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2224" s="10" t="s">
-        <v>2528</v>
-      </c>
+      <c r="A2224" s="12"/>
+      <c r="B2224" s="12"/>
+      <c r="C2224" s="10"/>
+      <c r="D2224" s="10"/>
+      <c r="E2224" s="11"/>
+      <c r="F2224" s="10"/>
       <c r="G2224" s="11"/>
       <c r="H2224" s="12"/>
       <c r="I2224" s="13"/>
       <c r="J2224" s="13"/>
     </row>
     <row r="2225" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2225" s="12">
-        <v>44614</v>
-      </c>
+      <c r="A2225" s="12"/>
       <c r="B2225" s="12"/>
-      <c r="C2225" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2225" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2225" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2225" s="10" t="s">
-        <v>2548</v>
-      </c>
+      <c r="C2225" s="10"/>
+      <c r="D2225" s="10"/>
+      <c r="E2225" s="11"/>
+      <c r="F2225" s="10"/>
       <c r="G2225" s="11"/>
       <c r="H2225" s="12"/>
       <c r="I2225" s="13"/>
@@ -76975,20 +77154,20 @@
     </row>
     <row r="2226" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2226" s="12">
-        <v>44616</v>
+        <v>44754</v>
       </c>
       <c r="B2226" s="12"/>
-      <c r="C2226" s="14" t="s">
-        <v>2250</v>
+      <c r="C2226" s="10" t="s">
+        <v>621</v>
       </c>
       <c r="D2226" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E2226" s="11" t="s">
         <v>618</v>
       </c>
       <c r="F2226" s="10" t="s">
-        <v>2555</v>
+        <v>3027</v>
       </c>
       <c r="G2226" s="11"/>
       <c r="H2226" s="12"/>
@@ -76997,42 +77176,42 @@
     </row>
     <row r="2227" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2227" s="12">
-        <v>44623</v>
+        <v>44761</v>
       </c>
       <c r="B2227" s="12"/>
-      <c r="C2227" s="14" t="s">
-        <v>535</v>
+      <c r="C2227" s="10" t="s">
+        <v>387</v>
       </c>
       <c r="D2227" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2227" s="11" t="s">
         <v>835</v>
       </c>
       <c r="F2227" s="10" t="s">
-        <v>2573</v>
+        <v>2992</v>
       </c>
       <c r="G2227" s="11"/>
       <c r="H2227" s="12"/>
       <c r="I2227" s="13"/>
       <c r="J2227" s="13"/>
     </row>
-    <row r="2228" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="2228" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2228" s="12">
-        <v>44522</v>
+        <v>44770</v>
       </c>
       <c r="B2228" s="12"/>
-      <c r="C2228" s="14" t="s">
-        <v>46</v>
+      <c r="C2228" s="10" t="s">
+        <v>628</v>
       </c>
       <c r="D2228" s="10" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E2228" s="11" t="s">
-        <v>568</v>
+        <v>618</v>
       </c>
       <c r="F2228" s="10" t="s">
-        <v>2350</v>
+        <v>3012</v>
       </c>
       <c r="G2228" s="11"/>
       <c r="H2228" s="12"/>
@@ -77040,411 +77219,405 @@
       <c r="J2228" s="13"/>
     </row>
     <row r="2229" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2229" s="12"/>
+      <c r="A2229" s="12">
+        <v>44761</v>
+      </c>
       <c r="B2229" s="12"/>
-      <c r="C2229" s="14"/>
-      <c r="D2229" s="10"/>
-      <c r="E2229" s="11"/>
-      <c r="F2229" s="10"/>
+      <c r="C2229" s="10" t="s">
+        <v>557</v>
+      </c>
+      <c r="D2229" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2229" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2229" s="10" t="s">
+        <v>2995</v>
+      </c>
       <c r="G2229" s="11"/>
       <c r="H2229" s="12"/>
       <c r="I2229" s="13"/>
       <c r="J2229" s="13"/>
     </row>
-    <row r="2230" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2230" s="12"/>
+    <row r="2230" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2230" s="12">
+        <v>44698</v>
+      </c>
       <c r="B2230" s="12"/>
-      <c r="C2230" s="14"/>
-      <c r="D2230" s="10"/>
-      <c r="E2230" s="11"/>
-      <c r="F2230" s="10"/>
+      <c r="C2230" s="10" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2230" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2230" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2230" s="30" t="s">
+        <v>2798</v>
+      </c>
       <c r="G2230" s="11"/>
       <c r="H2230" s="12"/>
       <c r="I2230" s="13"/>
       <c r="J2230" s="13"/>
     </row>
-    <row r="2231" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2231" s="12"/>
+    <row r="2231" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2231" s="12">
+        <v>44684</v>
+      </c>
       <c r="B2231" s="12"/>
-      <c r="C2231" s="14"/>
-      <c r="D2231" s="10"/>
-      <c r="E2231" s="11"/>
-      <c r="F2231" s="10"/>
+      <c r="C2231" s="14" t="s">
+        <v>2155</v>
+      </c>
+      <c r="D2231" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2231" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2231" s="10" t="s">
+        <v>2799</v>
+      </c>
       <c r="G2231" s="11"/>
       <c r="H2231" s="12"/>
       <c r="I2231" s="13"/>
       <c r="J2231" s="13"/>
     </row>
-    <row r="2232" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2232" s="12"/>
+    <row r="2232" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2232" s="12">
+        <v>44677</v>
+      </c>
       <c r="B2232" s="12"/>
-      <c r="C2232" s="14"/>
-      <c r="D2232" s="10"/>
-      <c r="E2232" s="11"/>
-      <c r="F2232" s="10"/>
+      <c r="C2232" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2232" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2232" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2232" s="10" t="s">
+        <v>2729</v>
+      </c>
       <c r="G2232" s="11"/>
       <c r="H2232" s="12"/>
       <c r="I2232" s="13"/>
       <c r="J2232" s="13"/>
     </row>
-    <row r="2233" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2233" s="12"/>
+    <row r="2233" spans="1:10" ht="132" x14ac:dyDescent="0.2">
+      <c r="A2233" s="12">
+        <v>44645</v>
+      </c>
       <c r="B2233" s="12"/>
-      <c r="C2233" s="14"/>
-      <c r="D2233" s="10"/>
-      <c r="E2233" s="11"/>
-      <c r="F2233" s="10"/>
+      <c r="C2233" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D2233" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2233" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2233" s="10" t="s">
+        <v>2664</v>
+      </c>
       <c r="G2233" s="11"/>
       <c r="H2233" s="12"/>
       <c r="I2233" s="13"/>
       <c r="J2233" s="13"/>
     </row>
     <row r="2234" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2234" s="12"/>
+      <c r="A2234" s="12">
+        <v>44642</v>
+      </c>
       <c r="B2234" s="12"/>
-      <c r="C2234" s="14"/>
-      <c r="D2234" s="10"/>
-      <c r="E2234" s="11"/>
-      <c r="F2234" s="10"/>
+      <c r="C2234" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2234" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2234" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2234" s="10" t="s">
+        <v>2625</v>
+      </c>
       <c r="G2234" s="11"/>
       <c r="H2234" s="12"/>
       <c r="I2234" s="13"/>
       <c r="J2234" s="13"/>
     </row>
     <row r="2235" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2235" s="12"/>
+      <c r="A2235" s="12">
+        <v>44642</v>
+      </c>
       <c r="B2235" s="12"/>
-      <c r="C2235" s="14"/>
-      <c r="D2235" s="10"/>
-      <c r="E2235" s="11"/>
-      <c r="F2235" s="10"/>
+      <c r="C2235" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2235" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2235" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2235" s="10" t="s">
+        <v>2624</v>
+      </c>
       <c r="G2235" s="11"/>
       <c r="H2235" s="12"/>
       <c r="I2235" s="13"/>
       <c r="J2235" s="13"/>
     </row>
     <row r="2236" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2236" s="12"/>
-      <c r="B2236" s="9"/>
-      <c r="C2236" s="14"/>
-      <c r="D2236" s="10"/>
-      <c r="E2236" s="11"/>
-      <c r="F2236" s="10"/>
+      <c r="A2236" s="12">
+        <v>44614</v>
+      </c>
+      <c r="B2236" s="12">
+        <v>44614</v>
+      </c>
+      <c r="C2236" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2236" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2236" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2236" s="10" t="s">
+        <v>2528</v>
+      </c>
       <c r="G2236" s="11"/>
       <c r="H2236" s="12"/>
       <c r="I2236" s="13"/>
       <c r="J2236" s="13"/>
     </row>
     <row r="2237" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2237" s="1" t="s">
-        <v>1472</v>
-      </c>
-      <c r="B2237" s="2" t="s">
-        <v>1473</v>
-      </c>
-      <c r="C2237" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2237" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2237" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="F2237" s="4" t="s">
-        <v>1571</v>
-      </c>
-      <c r="G2237" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2237" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2237" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2237" s="36"/>
+      <c r="A2237" s="12">
+        <v>44614</v>
+      </c>
+      <c r="B2237" s="12"/>
+      <c r="C2237" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2237" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2237" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2237" s="10" t="s">
+        <v>2548</v>
+      </c>
+      <c r="G2237" s="11"/>
+      <c r="H2237" s="12"/>
+      <c r="I2237" s="13"/>
+      <c r="J2237" s="13"/>
     </row>
     <row r="2238" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2238" s="12"/>
-      <c r="B2238" s="9"/>
-      <c r="C2238" s="14"/>
-      <c r="D2238" s="10"/>
-      <c r="E2238" s="11"/>
-      <c r="F2238" s="10"/>
+      <c r="A2238" s="12">
+        <v>44616</v>
+      </c>
+      <c r="B2238" s="12"/>
+      <c r="C2238" s="14" t="s">
+        <v>2250</v>
+      </c>
+      <c r="D2238" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2238" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2238" s="10" t="s">
+        <v>2555</v>
+      </c>
       <c r="G2238" s="11"/>
       <c r="H2238" s="12"/>
       <c r="I2238" s="13"/>
       <c r="J2238" s="13"/>
     </row>
     <row r="2239" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2239" s="12"/>
-      <c r="B2239" s="9"/>
-      <c r="C2239" s="14"/>
-      <c r="D2239" s="10"/>
-      <c r="E2239" s="11"/>
-      <c r="F2239" s="10"/>
+      <c r="A2239" s="12">
+        <v>44623</v>
+      </c>
+      <c r="B2239" s="12"/>
+      <c r="C2239" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="D2239" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2239" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2239" s="10" t="s">
+        <v>2573</v>
+      </c>
       <c r="G2239" s="11"/>
       <c r="H2239" s="12"/>
       <c r="I2239" s="13"/>
       <c r="J2239" s="13"/>
     </row>
-    <row r="2240" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="2240" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A2240" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2240" s="9"/>
+        <v>44522</v>
+      </c>
+      <c r="B2240" s="12"/>
       <c r="C2240" s="14" t="s">
-        <v>895</v>
+        <v>46</v>
       </c>
       <c r="D2240" s="10" t="s">
-        <v>492</v>
+        <v>6</v>
       </c>
       <c r="E2240" s="11" t="s">
-        <v>757</v>
+        <v>568</v>
       </c>
       <c r="F2240" s="10" t="s">
-        <v>1636</v>
+        <v>2350</v>
       </c>
       <c r="G2240" s="11"/>
       <c r="H2240" s="12"/>
       <c r="I2240" s="13"/>
-      <c r="J2240" s="13" t="s">
-        <v>1659</v>
-      </c>
-    </row>
-    <row r="2241" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A2241" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2241" s="9"/>
-      <c r="C2241" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2241" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2241" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2241" s="10" t="s">
-        <v>1635</v>
-      </c>
+      <c r="J2240" s="13"/>
+    </row>
+    <row r="2241" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2241" s="12"/>
+      <c r="B2241" s="12"/>
+      <c r="C2241" s="14"/>
+      <c r="D2241" s="10"/>
+      <c r="E2241" s="11"/>
+      <c r="F2241" s="10"/>
       <c r="G2241" s="11"/>
       <c r="H2241" s="12"/>
       <c r="I2241" s="13"/>
       <c r="J2241" s="13"/>
     </row>
-    <row r="2242" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2242" s="12">
-        <v>44112</v>
-      </c>
-      <c r="B2242" s="9"/>
-      <c r="C2242" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D2242" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2242" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2242" s="10" t="s">
-        <v>2222</v>
-      </c>
+    <row r="2242" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2242" s="12"/>
+      <c r="B2242" s="12"/>
+      <c r="C2242" s="14"/>
+      <c r="D2242" s="10"/>
+      <c r="E2242" s="11"/>
+      <c r="F2242" s="10"/>
       <c r="G2242" s="11"/>
       <c r="H2242" s="12"/>
       <c r="I2242" s="13"/>
       <c r="J2242" s="13"/>
     </row>
     <row r="2243" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2243" s="12">
-        <v>44088</v>
-      </c>
-      <c r="B2243" s="9"/>
-      <c r="C2243" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2243" s="10" t="s">
-        <v>902</v>
-      </c>
-      <c r="E2243" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="F2243" s="10" t="s">
-        <v>1007</v>
-      </c>
+      <c r="A2243" s="12"/>
+      <c r="B2243" s="12"/>
+      <c r="C2243" s="14"/>
+      <c r="D2243" s="10"/>
+      <c r="E2243" s="11"/>
+      <c r="F2243" s="10"/>
       <c r="G2243" s="11"/>
       <c r="H2243" s="12"/>
       <c r="I2243" s="13"/>
       <c r="J2243" s="13"/>
     </row>
     <row r="2244" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2244" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B2244" s="9"/>
-      <c r="C2244" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D2244" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2244" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2244" s="10" t="s">
-        <v>900</v>
-      </c>
+      <c r="A2244" s="12"/>
+      <c r="B2244" s="12"/>
+      <c r="C2244" s="14"/>
+      <c r="D2244" s="10"/>
+      <c r="E2244" s="11"/>
+      <c r="F2244" s="10"/>
       <c r="G2244" s="11"/>
       <c r="H2244" s="12"/>
       <c r="I2244" s="13"/>
       <c r="J2244" s="13"/>
     </row>
     <row r="2245" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2245" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B2245" s="9"/>
-      <c r="C2245" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2245" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2245" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2245" s="10" t="s">
-        <v>897</v>
-      </c>
+      <c r="A2245" s="12"/>
+      <c r="B2245" s="12"/>
+      <c r="C2245" s="14"/>
+      <c r="D2245" s="10"/>
+      <c r="E2245" s="11"/>
+      <c r="F2245" s="10"/>
       <c r="G2245" s="11"/>
       <c r="H2245" s="12"/>
       <c r="I2245" s="13"/>
       <c r="J2245" s="13"/>
     </row>
-    <row r="2246" spans="1:10" ht="108" x14ac:dyDescent="0.2">
-      <c r="A2246" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B2246" s="9"/>
-      <c r="C2246" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2246" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2246" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2246" s="10" t="s">
-        <v>898</v>
-      </c>
+    <row r="2246" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2246" s="12"/>
+      <c r="B2246" s="12"/>
+      <c r="C2246" s="14"/>
+      <c r="D2246" s="10"/>
+      <c r="E2246" s="11"/>
+      <c r="F2246" s="10"/>
       <c r="G2246" s="11"/>
       <c r="H2246" s="12"/>
       <c r="I2246" s="13"/>
       <c r="J2246" s="13"/>
     </row>
-    <row r="2247" spans="1:10" ht="168" x14ac:dyDescent="0.2">
-      <c r="A2247" s="12">
-        <v>43949</v>
-      </c>
-      <c r="B2247" s="9"/>
-      <c r="C2247" s="14" t="s">
-        <v>468</v>
-      </c>
-      <c r="D2247" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2247" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="F2247" s="10" t="s">
-        <v>684</v>
-      </c>
-      <c r="G2247" s="11" t="s">
-        <v>1616</v>
-      </c>
+    <row r="2247" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2247" s="12"/>
+      <c r="B2247" s="12"/>
+      <c r="C2247" s="14"/>
+      <c r="D2247" s="10"/>
+      <c r="E2247" s="11"/>
+      <c r="F2247" s="10"/>
+      <c r="G2247" s="11"/>
       <c r="H2247" s="12"/>
-      <c r="I2247" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I2247" s="13"/>
       <c r="J2247" s="13"/>
     </row>
-    <row r="2248" spans="1:10" ht="168" x14ac:dyDescent="0.2">
-      <c r="A2248" s="12">
-        <v>43949</v>
-      </c>
+    <row r="2248" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2248" s="12"/>
       <c r="B2248" s="9"/>
-      <c r="C2248" s="14" t="s">
-        <v>468</v>
-      </c>
-      <c r="D2248" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2248" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="F2248" s="10" t="s">
-        <v>703</v>
-      </c>
-      <c r="G2248" s="11" t="s">
-        <v>685</v>
-      </c>
+      <c r="C2248" s="14"/>
+      <c r="D2248" s="10"/>
+      <c r="E2248" s="11"/>
+      <c r="F2248" s="10"/>
+      <c r="G2248" s="11"/>
       <c r="H2248" s="12"/>
-      <c r="I2248" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J2248" s="13" t="s">
-        <v>1561</v>
-      </c>
-    </row>
-    <row r="2249" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2249" s="12">
-        <v>43838</v>
-      </c>
-      <c r="B2249" s="9"/>
-      <c r="C2249" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2249" s="10" t="s">
-        <v>460</v>
-      </c>
-      <c r="E2249" s="11" t="s">
-        <v>645</v>
-      </c>
-      <c r="F2249" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="G2249" s="11" t="s">
-        <v>1617</v>
-      </c>
-      <c r="H2249" s="12"/>
-      <c r="I2249" s="13"/>
-      <c r="J2249" s="13" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="2250" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A2250" s="12">
-        <v>43762</v>
-      </c>
+      <c r="I2248" s="13"/>
+      <c r="J2248" s="13"/>
+    </row>
+    <row r="2249" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2249" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B2249" s="2" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C2249" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2249" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2249" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F2249" s="4" t="s">
+        <v>1571</v>
+      </c>
+      <c r="G2249" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2249" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2249" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2249" s="36"/>
+    </row>
+    <row r="2250" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2250" s="12"/>
       <c r="B2250" s="9"/>
-      <c r="C2250" s="14" t="s">
-        <v>446</v>
-      </c>
-      <c r="D2250" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2250" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2250" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G2250" s="11" t="s">
-        <v>1606</v>
-      </c>
+      <c r="C2250" s="14"/>
+      <c r="D2250" s="10"/>
+      <c r="E2250" s="11"/>
+      <c r="F2250" s="10"/>
+      <c r="G2250" s="11"/>
       <c r="H2250" s="12"/>
       <c r="I2250" s="13"/>
       <c r="J2250" s="13"/>
@@ -77461,65 +77634,337 @@
       <c r="I2251" s="13"/>
       <c r="J2251" s="13"/>
     </row>
-    <row r="2252" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2252" s="12"/>
+    <row r="2252" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+      <c r="A2252" s="12">
+        <v>44252</v>
+      </c>
       <c r="B2252" s="9"/>
-      <c r="C2252" s="14"/>
-      <c r="D2252" s="10"/>
-      <c r="E2252" s="11"/>
-      <c r="F2252" s="10"/>
+      <c r="C2252" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2252" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2252" s="11" t="s">
+        <v>757</v>
+      </c>
+      <c r="F2252" s="10" t="s">
+        <v>1636</v>
+      </c>
       <c r="G2252" s="11"/>
       <c r="H2252" s="12"/>
       <c r="I2252" s="13"/>
-      <c r="J2252" s="13"/>
-    </row>
-    <row r="2253" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2253" s="12"/>
+      <c r="J2252" s="13" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="2253" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2253" s="12">
+        <v>44252</v>
+      </c>
       <c r="B2253" s="9"/>
-      <c r="C2253" s="14"/>
-      <c r="D2253" s="10"/>
-      <c r="E2253" s="11"/>
-      <c r="F2253" s="10"/>
+      <c r="C2253" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2253" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2253" s="11" t="s">
+        <v>757</v>
+      </c>
+      <c r="F2253" s="10" t="s">
+        <v>1635</v>
+      </c>
       <c r="G2253" s="11"/>
       <c r="H2253" s="12"/>
       <c r="I2253" s="13"/>
       <c r="J2253" s="13"/>
     </row>
-    <row r="2254" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2254" s="12"/>
+    <row r="2254" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2254" s="12">
+        <v>44112</v>
+      </c>
       <c r="B2254" s="9"/>
-      <c r="C2254" s="14"/>
-      <c r="D2254" s="10"/>
-      <c r="E2254" s="11"/>
-      <c r="F2254" s="10"/>
+      <c r="C2254" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="D2254" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2254" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2254" s="10" t="s">
+        <v>2222</v>
+      </c>
       <c r="G2254" s="11"/>
       <c r="H2254" s="12"/>
       <c r="I2254" s="13"/>
       <c r="J2254" s="13"/>
     </row>
     <row r="2255" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2255" s="12"/>
+      <c r="A2255" s="12">
+        <v>44088</v>
+      </c>
       <c r="B2255" s="9"/>
-      <c r="C2255" s="14"/>
-      <c r="D2255" s="10"/>
-      <c r="E2255" s="11"/>
-      <c r="F2255" s="10"/>
+      <c r="C2255" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2255" s="10" t="s">
+        <v>902</v>
+      </c>
+      <c r="E2255" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2255" s="10" t="s">
+        <v>1007</v>
+      </c>
       <c r="G2255" s="11"/>
       <c r="H2255" s="12"/>
       <c r="I2255" s="13"/>
       <c r="J2255" s="13"/>
     </row>
     <row r="2256" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2256" s="12"/>
+      <c r="A2256" s="12">
+        <v>44055</v>
+      </c>
       <c r="B2256" s="9"/>
-      <c r="C2256" s="14"/>
-      <c r="D2256" s="10"/>
-      <c r="E2256" s="11"/>
-      <c r="F2256" s="10"/>
+      <c r="C2256" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="D2256" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2256" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2256" s="10" t="s">
+        <v>900</v>
+      </c>
       <c r="G2256" s="11"/>
       <c r="H2256" s="12"/>
       <c r="I2256" s="13"/>
       <c r="J2256" s="13"/>
+    </row>
+    <row r="2257" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2257" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B2257" s="9"/>
+      <c r="C2257" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2257" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2257" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2257" s="10" t="s">
+        <v>897</v>
+      </c>
+      <c r="G2257" s="11"/>
+      <c r="H2257" s="12"/>
+      <c r="I2257" s="13"/>
+      <c r="J2257" s="13"/>
+    </row>
+    <row r="2258" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A2258" s="12">
+        <v>44055</v>
+      </c>
+      <c r="B2258" s="9"/>
+      <c r="C2258" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2258" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2258" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2258" s="10" t="s">
+        <v>898</v>
+      </c>
+      <c r="G2258" s="11"/>
+      <c r="H2258" s="12"/>
+      <c r="I2258" s="13"/>
+      <c r="J2258" s="13"/>
+    </row>
+    <row r="2259" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2259" s="12">
+        <v>43949</v>
+      </c>
+      <c r="B2259" s="9"/>
+      <c r="C2259" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2259" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2259" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2259" s="10" t="s">
+        <v>684</v>
+      </c>
+      <c r="G2259" s="11" t="s">
+        <v>1616</v>
+      </c>
+      <c r="H2259" s="12"/>
+      <c r="I2259" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J2259" s="13"/>
+    </row>
+    <row r="2260" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2260" s="12">
+        <v>43949</v>
+      </c>
+      <c r="B2260" s="9"/>
+      <c r="C2260" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2260" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2260" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2260" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="G2260" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="H2260" s="12"/>
+      <c r="I2260" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J2260" s="13" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="2261" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2261" s="12">
+        <v>43838</v>
+      </c>
+      <c r="B2261" s="9"/>
+      <c r="C2261" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2261" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2261" s="11" t="s">
+        <v>645</v>
+      </c>
+      <c r="F2261" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="G2261" s="11" t="s">
+        <v>1617</v>
+      </c>
+      <c r="H2261" s="12"/>
+      <c r="I2261" s="13"/>
+      <c r="J2261" s="13" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="2262" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2262" s="12">
+        <v>43762</v>
+      </c>
+      <c r="B2262" s="9"/>
+      <c r="C2262" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D2262" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2262" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2262" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G2262" s="11" t="s">
+        <v>1606</v>
+      </c>
+      <c r="H2262" s="12"/>
+      <c r="I2262" s="13"/>
+      <c r="J2262" s="13"/>
+    </row>
+    <row r="2263" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2263" s="12"/>
+      <c r="B2263" s="9"/>
+      <c r="C2263" s="14"/>
+      <c r="D2263" s="10"/>
+      <c r="E2263" s="11"/>
+      <c r="F2263" s="10"/>
+      <c r="G2263" s="11"/>
+      <c r="H2263" s="12"/>
+      <c r="I2263" s="13"/>
+      <c r="J2263" s="13"/>
+    </row>
+    <row r="2264" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2264" s="12"/>
+      <c r="B2264" s="9"/>
+      <c r="C2264" s="14"/>
+      <c r="D2264" s="10"/>
+      <c r="E2264" s="11"/>
+      <c r="F2264" s="10"/>
+      <c r="G2264" s="11"/>
+      <c r="H2264" s="12"/>
+      <c r="I2264" s="13"/>
+      <c r="J2264" s="13"/>
+    </row>
+    <row r="2265" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2265" s="12"/>
+      <c r="B2265" s="9"/>
+      <c r="C2265" s="14"/>
+      <c r="D2265" s="10"/>
+      <c r="E2265" s="11"/>
+      <c r="F2265" s="10"/>
+      <c r="G2265" s="11"/>
+      <c r="H2265" s="12"/>
+      <c r="I2265" s="13"/>
+      <c r="J2265" s="13"/>
+    </row>
+    <row r="2266" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2266" s="12"/>
+      <c r="B2266" s="9"/>
+      <c r="C2266" s="14"/>
+      <c r="D2266" s="10"/>
+      <c r="E2266" s="11"/>
+      <c r="F2266" s="10"/>
+      <c r="G2266" s="11"/>
+      <c r="H2266" s="12"/>
+      <c r="I2266" s="13"/>
+      <c r="J2266" s="13"/>
+    </row>
+    <row r="2267" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2267" s="12"/>
+      <c r="B2267" s="9"/>
+      <c r="C2267" s="14"/>
+      <c r="D2267" s="10"/>
+      <c r="E2267" s="11"/>
+      <c r="F2267" s="10"/>
+      <c r="G2267" s="11"/>
+      <c r="H2267" s="12"/>
+      <c r="I2267" s="13"/>
+      <c r="J2267" s="13"/>
+    </row>
+    <row r="2268" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2268" s="12"/>
+      <c r="B2268" s="9"/>
+      <c r="C2268" s="14"/>
+      <c r="D2268" s="10"/>
+      <c r="E2268" s="11"/>
+      <c r="F2268" s="10"/>
+      <c r="G2268" s="11"/>
+      <c r="H2268" s="12"/>
+      <c r="I2268" s="13"/>
+      <c r="J2268" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1881" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Alterações Dashboard e evento 720 inc proventos
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F496C3A6-73BC-42F4-BD1B-C118FC85E755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0579CC-E521-4080-801C-4D3FEB74C596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15930" uniqueCount="3040">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15952" uniqueCount="3044">
   <si>
     <t>Responsável</t>
   </si>
@@ -9640,6 +9640,19 @@
   </si>
   <si>
     <t>Incluir o codigo 695 nos eventos de proventos rentabilidade e dashboard e gerar tabelas e agendar prov. X realizado.</t>
+  </si>
+  <si>
+    <t>Fui liberar as pensões da folha de 07/2022, não verifiquei que o cálculo no rubi estava para 02/08/2022 , e terminei liberando ai fui conferir e verifiquei que estava dia 02/08/2022.
+Tinha que ser alterado no RUBI para saírem 05/08/2022, e para não ter que devolve-los o Lau ainda não integrou, gentileza ajusta-los para 05/08/2022</t>
+  </si>
+  <si>
+    <t>Documento de entrada em 60 parcelas com divergência de valores</t>
+  </si>
+  <si>
+    <t>Instruido colocar a diferença de centavos na última parcela</t>
+  </si>
+  <si>
+    <t>Tive que recalcular uma rescisão, para não devolvermos porque depois teríamos que liberar com o mesmo tipo e o sistema não acataria porque o pagamento é amanha. Gentileza alterar o título abaixo para o valor que segue.</t>
   </si>
 </sst>
 </file>
@@ -10445,11 +10458,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J2281"/>
+  <dimension ref="A1:J2285"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2230" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2236" sqref="G2236"/>
+      <pane ySplit="1" topLeftCell="A2232" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2239" sqref="A2239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -77542,168 +77555,184 @@
       </c>
       <c r="J2235" s="13"/>
     </row>
-    <row r="2236" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2236" s="12"/>
-      <c r="B2236" s="12"/>
-      <c r="C2236" s="10"/>
-      <c r="D2236" s="10"/>
-      <c r="E2236" s="11"/>
-      <c r="F2236" s="10"/>
-      <c r="G2236" s="11"/>
-      <c r="H2236" s="12"/>
-      <c r="I2236" s="13"/>
+    <row r="2236" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="A2236" s="12">
+        <v>44776</v>
+      </c>
+      <c r="B2236" s="12">
+        <v>44776</v>
+      </c>
+      <c r="C2236" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="D2236" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="E2236" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2236" s="10" t="s">
+        <v>3040</v>
+      </c>
+      <c r="G2236" s="11" t="s">
+        <v>1598</v>
+      </c>
+      <c r="H2236" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2236" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2236" s="13"/>
     </row>
     <row r="2237" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2237" s="12"/>
-      <c r="B2237" s="12"/>
-      <c r="C2237" s="10"/>
-      <c r="D2237" s="10"/>
-      <c r="E2237" s="11"/>
-      <c r="F2237" s="10"/>
-      <c r="G2237" s="11"/>
-      <c r="H2237" s="12"/>
-      <c r="I2237" s="13"/>
-      <c r="J2237" s="13"/>
-    </row>
-    <row r="2238" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2238" s="12"/>
-      <c r="B2238" s="12"/>
-      <c r="C2238" s="10"/>
-      <c r="D2238" s="10"/>
-      <c r="E2238" s="11"/>
-      <c r="F2238" s="10"/>
-      <c r="G2238" s="11"/>
-      <c r="H2238" s="12"/>
-      <c r="I2238" s="13"/>
+      <c r="A2237" s="12">
+        <v>44776</v>
+      </c>
+      <c r="B2237" s="12">
+        <v>44776</v>
+      </c>
+      <c r="C2237" s="10" t="s">
+        <v>1968</v>
+      </c>
+      <c r="D2237" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2237" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2237" s="10" t="s">
+        <v>3041</v>
+      </c>
+      <c r="G2237" s="11" t="s">
+        <v>1598</v>
+      </c>
+      <c r="H2237" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2237" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2237" s="13" t="s">
+        <v>3042</v>
+      </c>
+    </row>
+    <row r="2238" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2238" s="12">
+        <v>44776</v>
+      </c>
+      <c r="B2238" s="12">
+        <v>44776</v>
+      </c>
+      <c r="C2238" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="D2238" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="E2238" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2238" s="10" t="s">
+        <v>3043</v>
+      </c>
+      <c r="G2238" s="11" t="s">
+        <v>1598</v>
+      </c>
+      <c r="H2238" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2238" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="J2238" s="13"/>
     </row>
     <row r="2239" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2239" s="12">
-        <v>44754</v>
-      </c>
+      <c r="A2239" s="12"/>
       <c r="B2239" s="12"/>
-      <c r="C2239" s="10" t="s">
-        <v>621</v>
-      </c>
-      <c r="D2239" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2239" s="11" t="s">
-        <v>618</v>
-      </c>
-      <c r="F2239" s="10" t="s">
-        <v>3027</v>
-      </c>
+      <c r="C2239" s="10"/>
+      <c r="D2239" s="10"/>
+      <c r="E2239" s="11"/>
+      <c r="F2239" s="10"/>
       <c r="G2239" s="11"/>
       <c r="H2239" s="12"/>
       <c r="I2239" s="13"/>
       <c r="J2239" s="13"/>
     </row>
     <row r="2240" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2240" s="12">
-        <v>44761</v>
-      </c>
+      <c r="A2240" s="12"/>
       <c r="B2240" s="12"/>
-      <c r="C2240" s="10" t="s">
-        <v>387</v>
-      </c>
-      <c r="D2240" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2240" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2240" s="10" t="s">
-        <v>2992</v>
-      </c>
+      <c r="C2240" s="10"/>
+      <c r="D2240" s="10"/>
+      <c r="E2240" s="11"/>
+      <c r="F2240" s="10"/>
       <c r="G2240" s="11"/>
       <c r="H2240" s="12"/>
       <c r="I2240" s="13"/>
       <c r="J2240" s="13"/>
     </row>
-    <row r="2241" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2241" s="12">
-        <v>44770</v>
-      </c>
+    <row r="2241" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2241" s="12"/>
       <c r="B2241" s="12"/>
-      <c r="C2241" s="10" t="s">
-        <v>628</v>
-      </c>
-      <c r="D2241" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2241" s="11" t="s">
-        <v>618</v>
-      </c>
-      <c r="F2241" s="10" t="s">
-        <v>3012</v>
-      </c>
+      <c r="C2241" s="10"/>
+      <c r="D2241" s="10"/>
+      <c r="E2241" s="11"/>
+      <c r="F2241" s="10"/>
       <c r="G2241" s="11"/>
       <c r="H2241" s="12"/>
       <c r="I2241" s="13"/>
       <c r="J2241" s="13"/>
     </row>
     <row r="2242" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2242" s="12">
-        <v>44761</v>
-      </c>
+      <c r="A2242" s="12"/>
       <c r="B2242" s="12"/>
-      <c r="C2242" s="10" t="s">
-        <v>557</v>
-      </c>
-      <c r="D2242" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2242" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2242" s="10" t="s">
-        <v>2995</v>
-      </c>
+      <c r="C2242" s="10"/>
+      <c r="D2242" s="10"/>
+      <c r="E2242" s="11"/>
+      <c r="F2242" s="10"/>
       <c r="G2242" s="11"/>
       <c r="H2242" s="12"/>
       <c r="I2242" s="13"/>
       <c r="J2242" s="13"/>
     </row>
-    <row r="2243" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="2243" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2243" s="12">
-        <v>44698</v>
+        <v>44754</v>
       </c>
       <c r="B2243" s="12"/>
       <c r="C2243" s="10" t="s">
-        <v>895</v>
+        <v>621</v>
       </c>
       <c r="D2243" s="10" t="s">
-        <v>492</v>
+        <v>6</v>
       </c>
       <c r="E2243" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2243" s="30" t="s">
-        <v>2798</v>
+        <v>618</v>
+      </c>
+      <c r="F2243" s="10" t="s">
+        <v>3027</v>
       </c>
       <c r="G2243" s="11"/>
       <c r="H2243" s="12"/>
       <c r="I2243" s="13"/>
       <c r="J2243" s="13"/>
     </row>
-    <row r="2244" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="2244" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2244" s="12">
-        <v>44684</v>
+        <v>44761</v>
       </c>
       <c r="B2244" s="12"/>
-      <c r="C2244" s="14" t="s">
-        <v>2155</v>
+      <c r="C2244" s="10" t="s">
+        <v>387</v>
       </c>
       <c r="D2244" s="10" t="s">
-        <v>83</v>
+        <v>492</v>
       </c>
       <c r="E2244" s="11" t="s">
-        <v>618</v>
+        <v>835</v>
       </c>
       <c r="F2244" s="10" t="s">
-        <v>2799</v>
+        <v>2992</v>
       </c>
       <c r="G2244" s="11"/>
       <c r="H2244" s="12"/>
@@ -77712,55 +77741,55 @@
     </row>
     <row r="2245" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2245" s="12">
-        <v>44677</v>
+        <v>44770</v>
       </c>
       <c r="B2245" s="12"/>
-      <c r="C2245" s="14" t="s">
-        <v>387</v>
+      <c r="C2245" s="10" t="s">
+        <v>628</v>
       </c>
       <c r="D2245" s="10" t="s">
-        <v>492</v>
+        <v>17</v>
       </c>
       <c r="E2245" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F2245" s="10" t="s">
-        <v>2729</v>
+        <v>3012</v>
       </c>
       <c r="G2245" s="11"/>
       <c r="H2245" s="12"/>
       <c r="I2245" s="13"/>
       <c r="J2245" s="13"/>
     </row>
-    <row r="2246" spans="1:10" ht="132" x14ac:dyDescent="0.2">
+    <row r="2246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2246" s="12">
-        <v>44645</v>
+        <v>44761</v>
       </c>
       <c r="B2246" s="12"/>
-      <c r="C2246" s="14" t="s">
-        <v>288</v>
+      <c r="C2246" s="10" t="s">
+        <v>557</v>
       </c>
       <c r="D2246" s="10" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E2246" s="11" t="s">
-        <v>618</v>
+        <v>835</v>
       </c>
       <c r="F2246" s="10" t="s">
-        <v>2664</v>
+        <v>2995</v>
       </c>
       <c r="G2246" s="11"/>
       <c r="H2246" s="12"/>
       <c r="I2246" s="13"/>
       <c r="J2246" s="13"/>
     </row>
-    <row r="2247" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2247" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2247" s="12">
-        <v>44642</v>
+        <v>44698</v>
       </c>
       <c r="B2247" s="12"/>
-      <c r="C2247" s="14" t="s">
-        <v>387</v>
+      <c r="C2247" s="10" t="s">
+        <v>895</v>
       </c>
       <c r="D2247" s="10" t="s">
         <v>492</v>
@@ -77768,45 +77797,43 @@
       <c r="E2247" s="11" t="s">
         <v>835</v>
       </c>
-      <c r="F2247" s="10" t="s">
-        <v>2625</v>
+      <c r="F2247" s="30" t="s">
+        <v>2798</v>
       </c>
       <c r="G2247" s="11"/>
       <c r="H2247" s="12"/>
       <c r="I2247" s="13"/>
       <c r="J2247" s="13"/>
     </row>
-    <row r="2248" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2248" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2248" s="12">
-        <v>44642</v>
+        <v>44684</v>
       </c>
       <c r="B2248" s="12"/>
       <c r="C2248" s="14" t="s">
-        <v>387</v>
+        <v>2155</v>
       </c>
       <c r="D2248" s="10" t="s">
-        <v>492</v>
+        <v>83</v>
       </c>
       <c r="E2248" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F2248" s="10" t="s">
-        <v>2624</v>
+        <v>2799</v>
       </c>
       <c r="G2248" s="11"/>
       <c r="H2248" s="12"/>
       <c r="I2248" s="13"/>
       <c r="J2248" s="13"/>
     </row>
-    <row r="2249" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2249" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2249" s="12">
-        <v>44614</v>
-      </c>
-      <c r="B2249" s="12">
-        <v>44614</v>
-      </c>
+        <v>44677</v>
+      </c>
+      <c r="B2249" s="12"/>
       <c r="C2249" s="14" t="s">
-        <v>19</v>
+        <v>387</v>
       </c>
       <c r="D2249" s="10" t="s">
         <v>492</v>
@@ -77815,29 +77842,29 @@
         <v>835</v>
       </c>
       <c r="F2249" s="10" t="s">
-        <v>2528</v>
+        <v>2729</v>
       </c>
       <c r="G2249" s="11"/>
       <c r="H2249" s="12"/>
       <c r="I2249" s="13"/>
       <c r="J2249" s="13"/>
     </row>
-    <row r="2250" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2250" spans="1:10" ht="132" x14ac:dyDescent="0.2">
       <c r="A2250" s="12">
-        <v>44614</v>
+        <v>44645</v>
       </c>
       <c r="B2250" s="12"/>
       <c r="C2250" s="14" t="s">
-        <v>19</v>
+        <v>288</v>
       </c>
       <c r="D2250" s="10" t="s">
-        <v>492</v>
+        <v>25</v>
       </c>
       <c r="E2250" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F2250" s="10" t="s">
-        <v>2548</v>
+        <v>2664</v>
       </c>
       <c r="G2250" s="11"/>
       <c r="H2250" s="12"/>
@@ -77846,20 +77873,20 @@
     </row>
     <row r="2251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2251" s="12">
-        <v>44616</v>
+        <v>44642</v>
       </c>
       <c r="B2251" s="12"/>
       <c r="C2251" s="14" t="s">
-        <v>2250</v>
+        <v>387</v>
       </c>
       <c r="D2251" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E2251" s="11" t="s">
-        <v>618</v>
+        <v>835</v>
       </c>
       <c r="F2251" s="10" t="s">
-        <v>2555</v>
+        <v>2625</v>
       </c>
       <c r="G2251" s="11"/>
       <c r="H2251" s="12"/>
@@ -77868,42 +77895,44 @@
     </row>
     <row r="2252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2252" s="12">
-        <v>44623</v>
+        <v>44642</v>
       </c>
       <c r="B2252" s="12"/>
       <c r="C2252" s="14" t="s">
-        <v>535</v>
+        <v>387</v>
       </c>
       <c r="D2252" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2252" s="11" t="s">
         <v>835</v>
       </c>
       <c r="F2252" s="10" t="s">
-        <v>2573</v>
+        <v>2624</v>
       </c>
       <c r="G2252" s="11"/>
       <c r="H2252" s="12"/>
       <c r="I2252" s="13"/>
       <c r="J2252" s="13"/>
     </row>
-    <row r="2253" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="2253" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2253" s="12">
-        <v>44522</v>
-      </c>
-      <c r="B2253" s="12"/>
+        <v>44614</v>
+      </c>
+      <c r="B2253" s="12">
+        <v>44614</v>
+      </c>
       <c r="C2253" s="14" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="D2253" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2253" s="11" t="s">
-        <v>568</v>
+        <v>835</v>
       </c>
       <c r="F2253" s="10" t="s">
-        <v>2350</v>
+        <v>2528</v>
       </c>
       <c r="G2253" s="11"/>
       <c r="H2253" s="12"/>
@@ -77911,48 +77940,88 @@
       <c r="J2253" s="13"/>
     </row>
     <row r="2254" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2254" s="12"/>
+      <c r="A2254" s="12">
+        <v>44614</v>
+      </c>
       <c r="B2254" s="12"/>
-      <c r="C2254" s="14"/>
-      <c r="D2254" s="10"/>
-      <c r="E2254" s="11"/>
-      <c r="F2254" s="10"/>
+      <c r="C2254" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2254" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2254" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2254" s="10" t="s">
+        <v>2548</v>
+      </c>
       <c r="G2254" s="11"/>
       <c r="H2254" s="12"/>
       <c r="I2254" s="13"/>
       <c r="J2254" s="13"/>
     </row>
     <row r="2255" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2255" s="12"/>
+      <c r="A2255" s="12">
+        <v>44616</v>
+      </c>
       <c r="B2255" s="12"/>
-      <c r="C2255" s="14"/>
-      <c r="D2255" s="10"/>
-      <c r="E2255" s="11"/>
-      <c r="F2255" s="10"/>
+      <c r="C2255" s="14" t="s">
+        <v>2250</v>
+      </c>
+      <c r="D2255" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2255" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2255" s="10" t="s">
+        <v>2555</v>
+      </c>
       <c r="G2255" s="11"/>
       <c r="H2255" s="12"/>
       <c r="I2255" s="13"/>
       <c r="J2255" s="13"/>
     </row>
     <row r="2256" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2256" s="12"/>
+      <c r="A2256" s="12">
+        <v>44623</v>
+      </c>
       <c r="B2256" s="12"/>
-      <c r="C2256" s="14"/>
-      <c r="D2256" s="10"/>
-      <c r="E2256" s="11"/>
-      <c r="F2256" s="10"/>
+      <c r="C2256" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="D2256" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2256" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2256" s="10" t="s">
+        <v>2573</v>
+      </c>
       <c r="G2256" s="11"/>
       <c r="H2256" s="12"/>
       <c r="I2256" s="13"/>
       <c r="J2256" s="13"/>
     </row>
-    <row r="2257" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2257" s="12"/>
+    <row r="2257" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2257" s="12">
+        <v>44522</v>
+      </c>
       <c r="B2257" s="12"/>
-      <c r="C2257" s="14"/>
-      <c r="D2257" s="10"/>
-      <c r="E2257" s="11"/>
-      <c r="F2257" s="10"/>
+      <c r="C2257" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2257" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2257" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2257" s="10" t="s">
+        <v>2350</v>
+      </c>
       <c r="G2257" s="11"/>
       <c r="H2257" s="12"/>
       <c r="I2257" s="13"/>
@@ -77996,7 +78065,7 @@
     </row>
     <row r="2261" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2261" s="12"/>
-      <c r="B2261" s="9"/>
+      <c r="B2261" s="12"/>
       <c r="C2261" s="14"/>
       <c r="D2261" s="10"/>
       <c r="E2261" s="11"/>
@@ -78007,38 +78076,20 @@
       <c r="J2261" s="13"/>
     </row>
     <row r="2262" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2262" s="1" t="s">
-        <v>1472</v>
-      </c>
-      <c r="B2262" s="2" t="s">
-        <v>1473</v>
-      </c>
-      <c r="C2262" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2262" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2262" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="F2262" s="4" t="s">
-        <v>1571</v>
-      </c>
-      <c r="G2262" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2262" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2262" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2262" s="36"/>
+      <c r="A2262" s="12"/>
+      <c r="B2262" s="12"/>
+      <c r="C2262" s="14"/>
+      <c r="D2262" s="10"/>
+      <c r="E2262" s="11"/>
+      <c r="F2262" s="10"/>
+      <c r="G2262" s="11"/>
+      <c r="H2262" s="12"/>
+      <c r="I2262" s="13"/>
+      <c r="J2262" s="13"/>
     </row>
     <row r="2263" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2263" s="12"/>
-      <c r="B2263" s="9"/>
+      <c r="B2263" s="12"/>
       <c r="C2263" s="14"/>
       <c r="D2263" s="10"/>
       <c r="E2263" s="11"/>
@@ -78050,7 +78101,7 @@
     </row>
     <row r="2264" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2264" s="12"/>
-      <c r="B2264" s="9"/>
+      <c r="B2264" s="12"/>
       <c r="C2264" s="14"/>
       <c r="D2264" s="10"/>
       <c r="E2264" s="11"/>
@@ -78060,121 +78111,99 @@
       <c r="I2264" s="13"/>
       <c r="J2264" s="13"/>
     </row>
-    <row r="2265" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A2265" s="12">
-        <v>44252</v>
-      </c>
+    <row r="2265" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2265" s="12"/>
       <c r="B2265" s="9"/>
-      <c r="C2265" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2265" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2265" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2265" s="10" t="s">
-        <v>1636</v>
-      </c>
+      <c r="C2265" s="14"/>
+      <c r="D2265" s="10"/>
+      <c r="E2265" s="11"/>
+      <c r="F2265" s="10"/>
       <c r="G2265" s="11"/>
       <c r="H2265" s="12"/>
       <c r="I2265" s="13"/>
-      <c r="J2265" s="13" t="s">
-        <v>1659</v>
-      </c>
-    </row>
-    <row r="2266" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A2266" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2266" s="9"/>
-      <c r="C2266" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2266" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2266" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2266" s="10" t="s">
-        <v>1635</v>
-      </c>
-      <c r="G2266" s="11"/>
-      <c r="H2266" s="12"/>
-      <c r="I2266" s="13"/>
-      <c r="J2266" s="13"/>
-    </row>
-    <row r="2267" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2267" s="12">
-        <v>44112</v>
-      </c>
+      <c r="J2265" s="13"/>
+    </row>
+    <row r="2266" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2266" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B2266" s="2" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C2266" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2266" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2266" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F2266" s="4" t="s">
+        <v>1571</v>
+      </c>
+      <c r="G2266" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2266" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2266" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2266" s="36"/>
+    </row>
+    <row r="2267" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2267" s="12"/>
       <c r="B2267" s="9"/>
-      <c r="C2267" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D2267" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2267" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2267" s="10" t="s">
-        <v>2222</v>
-      </c>
+      <c r="C2267" s="14"/>
+      <c r="D2267" s="10"/>
+      <c r="E2267" s="11"/>
+      <c r="F2267" s="10"/>
       <c r="G2267" s="11"/>
       <c r="H2267" s="12"/>
       <c r="I2267" s="13"/>
       <c r="J2267" s="13"/>
     </row>
     <row r="2268" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2268" s="12">
-        <v>44088</v>
-      </c>
+      <c r="A2268" s="12"/>
       <c r="B2268" s="9"/>
-      <c r="C2268" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2268" s="10" t="s">
-        <v>902</v>
-      </c>
-      <c r="E2268" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="F2268" s="10" t="s">
-        <v>1007</v>
-      </c>
+      <c r="C2268" s="14"/>
+      <c r="D2268" s="10"/>
+      <c r="E2268" s="11"/>
+      <c r="F2268" s="10"/>
       <c r="G2268" s="11"/>
       <c r="H2268" s="12"/>
       <c r="I2268" s="13"/>
       <c r="J2268" s="13"/>
     </row>
-    <row r="2269" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2269" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A2269" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B2269" s="9"/>
       <c r="C2269" s="14" t="s">
-        <v>621</v>
+        <v>895</v>
       </c>
       <c r="D2269" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2269" s="11" t="s">
-        <v>568</v>
+        <v>757</v>
       </c>
       <c r="F2269" s="10" t="s">
-        <v>900</v>
+        <v>1636</v>
       </c>
       <c r="G2269" s="11"/>
       <c r="H2269" s="12"/>
       <c r="I2269" s="13"/>
-      <c r="J2269" s="13"/>
-    </row>
-    <row r="2270" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J2269" s="13" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="2270" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A2270" s="12">
-        <v>44055</v>
+        <v>44252</v>
       </c>
       <c r="B2270" s="9"/>
       <c r="C2270" s="14" t="s">
@@ -78184,186 +78213,226 @@
         <v>492</v>
       </c>
       <c r="E2270" s="11" t="s">
-        <v>568</v>
+        <v>757</v>
       </c>
       <c r="F2270" s="10" t="s">
-        <v>897</v>
+        <v>1635</v>
       </c>
       <c r="G2270" s="11"/>
       <c r="H2270" s="12"/>
       <c r="I2270" s="13"/>
       <c r="J2270" s="13"/>
     </row>
-    <row r="2271" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+    <row r="2271" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2271" s="12">
-        <v>44055</v>
+        <v>44112</v>
       </c>
       <c r="B2271" s="9"/>
       <c r="C2271" s="14" t="s">
-        <v>895</v>
+        <v>621</v>
       </c>
       <c r="D2271" s="10" t="s">
-        <v>492</v>
+        <v>6</v>
       </c>
       <c r="E2271" s="11" t="s">
         <v>568</v>
       </c>
       <c r="F2271" s="10" t="s">
-        <v>898</v>
+        <v>2222</v>
       </c>
       <c r="G2271" s="11"/>
       <c r="H2271" s="12"/>
       <c r="I2271" s="13"/>
       <c r="J2271" s="13"/>
     </row>
-    <row r="2272" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="2272" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2272" s="12">
-        <v>43949</v>
+        <v>44088</v>
       </c>
       <c r="B2272" s="9"/>
       <c r="C2272" s="14" t="s">
-        <v>468</v>
+        <v>19</v>
       </c>
       <c r="D2272" s="10" t="s">
-        <v>89</v>
+        <v>902</v>
       </c>
       <c r="E2272" s="11" t="s">
         <v>683</v>
       </c>
       <c r="F2272" s="10" t="s">
-        <v>684</v>
-      </c>
-      <c r="G2272" s="11" t="s">
-        <v>1616</v>
-      </c>
+        <v>1007</v>
+      </c>
+      <c r="G2272" s="11"/>
       <c r="H2272" s="12"/>
-      <c r="I2272" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I2272" s="13"/>
       <c r="J2272" s="13"/>
     </row>
-    <row r="2273" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="2273" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2273" s="12">
-        <v>43949</v>
+        <v>44055</v>
       </c>
       <c r="B2273" s="9"/>
       <c r="C2273" s="14" t="s">
-        <v>468</v>
+        <v>621</v>
       </c>
       <c r="D2273" s="10" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E2273" s="11" t="s">
-        <v>683</v>
+        <v>568</v>
       </c>
       <c r="F2273" s="10" t="s">
-        <v>703</v>
-      </c>
-      <c r="G2273" s="11" t="s">
-        <v>685</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="G2273" s="11"/>
       <c r="H2273" s="12"/>
-      <c r="I2273" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="J2273" s="13" t="s">
-        <v>1561</v>
-      </c>
-    </row>
-    <row r="2274" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="I2273" s="13"/>
+      <c r="J2273" s="13"/>
+    </row>
+    <row r="2274" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2274" s="12">
-        <v>43838</v>
+        <v>44055</v>
       </c>
       <c r="B2274" s="9"/>
       <c r="C2274" s="14" t="s">
-        <v>103</v>
+        <v>895</v>
       </c>
       <c r="D2274" s="10" t="s">
-        <v>460</v>
+        <v>492</v>
       </c>
       <c r="E2274" s="11" t="s">
-        <v>645</v>
+        <v>568</v>
       </c>
       <c r="F2274" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="G2274" s="11" t="s">
-        <v>1617</v>
-      </c>
+        <v>897</v>
+      </c>
+      <c r="G2274" s="11"/>
       <c r="H2274" s="12"/>
       <c r="I2274" s="13"/>
-      <c r="J2274" s="13" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="2275" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J2274" s="13"/>
+    </row>
+    <row r="2275" spans="1:10" ht="108" x14ac:dyDescent="0.2">
       <c r="A2275" s="12">
-        <v>43762</v>
+        <v>44055</v>
       </c>
       <c r="B2275" s="9"/>
       <c r="C2275" s="14" t="s">
-        <v>446</v>
+        <v>895</v>
       </c>
       <c r="D2275" s="10" t="s">
-        <v>17</v>
+        <v>492</v>
       </c>
       <c r="E2275" s="11" t="s">
-        <v>835</v>
+        <v>568</v>
       </c>
       <c r="F2275" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G2275" s="11" t="s">
-        <v>1606</v>
-      </c>
+        <v>898</v>
+      </c>
+      <c r="G2275" s="11"/>
       <c r="H2275" s="12"/>
       <c r="I2275" s="13"/>
       <c r="J2275" s="13"/>
     </row>
-    <row r="2276" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2276" s="12"/>
+    <row r="2276" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2276" s="12">
+        <v>43949</v>
+      </c>
       <c r="B2276" s="9"/>
-      <c r="C2276" s="14"/>
-      <c r="D2276" s="10"/>
-      <c r="E2276" s="11"/>
-      <c r="F2276" s="10"/>
-      <c r="G2276" s="11"/>
+      <c r="C2276" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2276" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2276" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2276" s="10" t="s">
+        <v>684</v>
+      </c>
+      <c r="G2276" s="11" t="s">
+        <v>1616</v>
+      </c>
       <c r="H2276" s="12"/>
-      <c r="I2276" s="13"/>
+      <c r="I2276" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J2276" s="13"/>
     </row>
-    <row r="2277" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2277" s="12"/>
+    <row r="2277" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2277" s="12">
+        <v>43949</v>
+      </c>
       <c r="B2277" s="9"/>
-      <c r="C2277" s="14"/>
-      <c r="D2277" s="10"/>
-      <c r="E2277" s="11"/>
-      <c r="F2277" s="10"/>
-      <c r="G2277" s="11"/>
+      <c r="C2277" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2277" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2277" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2277" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="G2277" s="11" t="s">
+        <v>685</v>
+      </c>
       <c r="H2277" s="12"/>
-      <c r="I2277" s="13"/>
-      <c r="J2277" s="13"/>
-    </row>
-    <row r="2278" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2278" s="12"/>
+      <c r="I2277" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J2277" s="13" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="2278" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2278" s="12">
+        <v>43838</v>
+      </c>
       <c r="B2278" s="9"/>
-      <c r="C2278" s="14"/>
-      <c r="D2278" s="10"/>
-      <c r="E2278" s="11"/>
-      <c r="F2278" s="10"/>
-      <c r="G2278" s="11"/>
+      <c r="C2278" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2278" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2278" s="11" t="s">
+        <v>645</v>
+      </c>
+      <c r="F2278" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="G2278" s="11" t="s">
+        <v>1617</v>
+      </c>
       <c r="H2278" s="12"/>
       <c r="I2278" s="13"/>
-      <c r="J2278" s="13"/>
-    </row>
-    <row r="2279" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2279" s="12"/>
+      <c r="J2278" s="13" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="2279" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2279" s="12">
+        <v>43762</v>
+      </c>
       <c r="B2279" s="9"/>
-      <c r="C2279" s="14"/>
-      <c r="D2279" s="10"/>
-      <c r="E2279" s="11"/>
-      <c r="F2279" s="10"/>
-      <c r="G2279" s="11"/>
+      <c r="C2279" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D2279" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2279" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2279" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G2279" s="11" t="s">
+        <v>1606</v>
+      </c>
       <c r="H2279" s="12"/>
       <c r="I2279" s="13"/>
       <c r="J2279" s="13"/>
@@ -78391,6 +78460,54 @@
       <c r="H2281" s="12"/>
       <c r="I2281" s="13"/>
       <c r="J2281" s="13"/>
+    </row>
+    <row r="2282" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2282" s="12"/>
+      <c r="B2282" s="9"/>
+      <c r="C2282" s="14"/>
+      <c r="D2282" s="10"/>
+      <c r="E2282" s="11"/>
+      <c r="F2282" s="10"/>
+      <c r="G2282" s="11"/>
+      <c r="H2282" s="12"/>
+      <c r="I2282" s="13"/>
+      <c r="J2282" s="13"/>
+    </row>
+    <row r="2283" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2283" s="12"/>
+      <c r="B2283" s="9"/>
+      <c r="C2283" s="14"/>
+      <c r="D2283" s="10"/>
+      <c r="E2283" s="11"/>
+      <c r="F2283" s="10"/>
+      <c r="G2283" s="11"/>
+      <c r="H2283" s="12"/>
+      <c r="I2283" s="13"/>
+      <c r="J2283" s="13"/>
+    </row>
+    <row r="2284" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2284" s="12"/>
+      <c r="B2284" s="9"/>
+      <c r="C2284" s="14"/>
+      <c r="D2284" s="10"/>
+      <c r="E2284" s="11"/>
+      <c r="F2284" s="10"/>
+      <c r="G2284" s="11"/>
+      <c r="H2284" s="12"/>
+      <c r="I2284" s="13"/>
+      <c r="J2284" s="13"/>
+    </row>
+    <row r="2285" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2285" s="12"/>
+      <c r="B2285" s="9"/>
+      <c r="C2285" s="14"/>
+      <c r="D2285" s="10"/>
+      <c r="E2285" s="11"/>
+      <c r="F2285" s="10"/>
+      <c r="G2285" s="11"/>
+      <c r="H2285" s="12"/>
+      <c r="I2285" s="13"/>
+      <c r="J2285" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1881" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Alteração Pedido de Compra
</commit_message>
<xml_diff>
--- a/demanda_Siga _BK.xlsx
+++ b/demanda_Siga _BK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.139.0.30\Protheus12\BK\Advpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0579CC-E521-4080-801C-4D3FEB74C596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7360471C-A0CA-418F-84AF-4AA7D8769A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="347" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15952" uniqueCount="3044">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16001" uniqueCount="3051">
   <si>
     <t>Responsável</t>
   </si>
@@ -9653,6 +9653,27 @@
   </si>
   <si>
     <t>Tive que recalcular uma rescisão, para não devolvermos porque depois teríamos que liberar com o mesmo tipo e o sistema não acataria porque o pagamento é amanha. Gentileza alterar o título abaixo para o valor que segue.</t>
+  </si>
+  <si>
+    <t>Incluir o codigo 720 nos eventos de proventos rentabilidade e dashboard e gerar tabelas e agendar prov. X realizado.</t>
+  </si>
+  <si>
+    <t>Alteração no calculo do faturamento líquido da tabela FATURAMENTO e outras melhorias</t>
+  </si>
+  <si>
+    <t>Aviso na geração do Bordero quando o pagamento a CLT for superior a 15000</t>
+  </si>
+  <si>
+    <t>Alterar a ordem de liberação de pedidos de venda WEB para mostrar primeiro os pedidos a liberar e os liberados embaixo</t>
+  </si>
+  <si>
+    <t>Diversos ajustes no Dashboard</t>
+  </si>
+  <si>
+    <t>Configuração da nova interface de usuário</t>
+  </si>
+  <si>
+    <t>Inserir frase fixa na impressão do pedido de compras e na obs atual, colocar na frente a que item se refere e melhorar o layout</t>
   </si>
 </sst>
 </file>
@@ -10458,11 +10479,11 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J2285"/>
+  <dimension ref="A1:J2293"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2232" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2239" sqref="A2239"/>
+      <pane ySplit="1" topLeftCell="A2239" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2245" sqref="A2245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -77647,71 +77668,143 @@
       </c>
       <c r="J2238" s="13"/>
     </row>
-    <row r="2239" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2239" s="12"/>
-      <c r="B2239" s="12"/>
-      <c r="C2239" s="10"/>
-      <c r="D2239" s="10"/>
-      <c r="E2239" s="11"/>
-      <c r="F2239" s="10"/>
-      <c r="G2239" s="11"/>
-      <c r="H2239" s="12"/>
-      <c r="I2239" s="13"/>
+    <row r="2239" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2239" s="12">
+        <v>44776</v>
+      </c>
+      <c r="B2239" s="12">
+        <v>44776</v>
+      </c>
+      <c r="C2239" s="10" t="s">
+        <v>2680</v>
+      </c>
+      <c r="D2239" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2239" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2239" s="10" t="s">
+        <v>3044</v>
+      </c>
+      <c r="G2239" s="11" t="s">
+        <v>1598</v>
+      </c>
+      <c r="H2239" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2239" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2239" s="13"/>
     </row>
-    <row r="2240" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2240" s="12"/>
-      <c r="B2240" s="12"/>
-      <c r="C2240" s="10"/>
-      <c r="D2240" s="10"/>
-      <c r="E2240" s="11"/>
-      <c r="F2240" s="10"/>
-      <c r="G2240" s="11"/>
-      <c r="H2240" s="12"/>
-      <c r="I2240" s="13"/>
+    <row r="2240" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2240" s="12">
+        <v>44776</v>
+      </c>
+      <c r="B2240" s="12">
+        <v>44776</v>
+      </c>
+      <c r="C2240" s="10" t="s">
+        <v>2680</v>
+      </c>
+      <c r="D2240" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2240" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2240" s="10" t="s">
+        <v>3045</v>
+      </c>
+      <c r="G2240" s="11" t="s">
+        <v>1603</v>
+      </c>
+      <c r="H2240" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2240" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2240" s="13"/>
     </row>
-    <row r="2241" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2241" s="12"/>
-      <c r="B2241" s="12"/>
-      <c r="C2241" s="10"/>
-      <c r="D2241" s="10"/>
-      <c r="E2241" s="11"/>
-      <c r="F2241" s="10"/>
-      <c r="G2241" s="11"/>
-      <c r="H2241" s="12"/>
-      <c r="I2241" s="13"/>
+    <row r="2241" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2241" s="12">
+        <v>44777</v>
+      </c>
+      <c r="B2241" s="12">
+        <v>44777</v>
+      </c>
+      <c r="C2241" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="D2241" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2241" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2241" s="10" t="s">
+        <v>3047</v>
+      </c>
+      <c r="G2241" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H2241" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2241" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2241" s="13"/>
     </row>
     <row r="2242" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2242" s="12"/>
-      <c r="B2242" s="12"/>
-      <c r="C2242" s="10"/>
-      <c r="D2242" s="10"/>
-      <c r="E2242" s="11"/>
-      <c r="F2242" s="10"/>
-      <c r="G2242" s="11"/>
-      <c r="H2242" s="12"/>
-      <c r="I2242" s="13"/>
+      <c r="A2242" s="12">
+        <v>44777</v>
+      </c>
+      <c r="B2242" s="12">
+        <v>44777</v>
+      </c>
+      <c r="C2242" s="10" t="s">
+        <v>2680</v>
+      </c>
+      <c r="D2242" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2242" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2242" s="10" t="s">
+        <v>3048</v>
+      </c>
+      <c r="G2242" s="11" t="s">
+        <v>1827</v>
+      </c>
+      <c r="H2242" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2242" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2242" s="13"/>
     </row>
     <row r="2243" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2243" s="12">
-        <v>44754</v>
-      </c>
-      <c r="B2243" s="12"/>
+        <v>44780</v>
+      </c>
+      <c r="B2243" s="12">
+        <v>44780</v>
+      </c>
       <c r="C2243" s="10" t="s">
-        <v>621</v>
+        <v>13</v>
       </c>
       <c r="D2243" s="10" t="s">
-        <v>6</v>
+        <v>582</v>
       </c>
       <c r="E2243" s="11" t="s">
-        <v>618</v>
-      </c>
-      <c r="F2243" s="10" t="s">
-        <v>3027</v>
-      </c>
+        <v>645</v>
+      </c>
+      <c r="F2243" s="10"/>
       <c r="G2243" s="11"/>
       <c r="H2243" s="12"/>
       <c r="I2243" s="13"/>
@@ -77719,152 +77812,128 @@
     </row>
     <row r="2244" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2244" s="12">
-        <v>44761</v>
-      </c>
-      <c r="B2244" s="12"/>
+        <v>44781</v>
+      </c>
+      <c r="B2244" s="12">
+        <v>44781</v>
+      </c>
       <c r="C2244" s="10" t="s">
-        <v>387</v>
+        <v>13</v>
       </c>
       <c r="D2244" s="10" t="s">
-        <v>492</v>
+        <v>582</v>
       </c>
       <c r="E2244" s="11" t="s">
-        <v>835</v>
+        <v>645</v>
       </c>
       <c r="F2244" s="10" t="s">
-        <v>2992</v>
-      </c>
-      <c r="G2244" s="11"/>
-      <c r="H2244" s="12"/>
-      <c r="I2244" s="13"/>
+        <v>3049</v>
+      </c>
+      <c r="G2244" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H2244" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2244" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2244" s="13"/>
     </row>
     <row r="2245" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2245" s="12">
-        <v>44770</v>
-      </c>
-      <c r="B2245" s="12"/>
+        <v>44781</v>
+      </c>
+      <c r="B2245" s="12">
+        <v>44781</v>
+      </c>
       <c r="C2245" s="10" t="s">
-        <v>628</v>
+        <v>288</v>
       </c>
       <c r="D2245" s="10" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E2245" s="11" t="s">
         <v>618</v>
       </c>
       <c r="F2245" s="10" t="s">
-        <v>3012</v>
-      </c>
-      <c r="G2245" s="11"/>
-      <c r="H2245" s="12"/>
-      <c r="I2245" s="13"/>
+        <v>3050</v>
+      </c>
+      <c r="G2245" s="11" t="s">
+        <v>1827</v>
+      </c>
+      <c r="H2245" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2245" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J2245" s="13"/>
     </row>
     <row r="2246" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2246" s="12">
-        <v>44761</v>
-      </c>
+      <c r="A2246" s="12"/>
       <c r="B2246" s="12"/>
-      <c r="C2246" s="10" t="s">
-        <v>557</v>
-      </c>
-      <c r="D2246" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2246" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2246" s="10" t="s">
-        <v>2995</v>
-      </c>
+      <c r="C2246" s="10"/>
+      <c r="D2246" s="10"/>
+      <c r="E2246" s="11"/>
+      <c r="F2246" s="10"/>
       <c r="G2246" s="11"/>
       <c r="H2246" s="12"/>
       <c r="I2246" s="13"/>
       <c r="J2246" s="13"/>
     </row>
-    <row r="2247" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2247" s="12">
-        <v>44698</v>
-      </c>
+    <row r="2247" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2247" s="12"/>
       <c r="B2247" s="12"/>
-      <c r="C2247" s="10" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2247" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2247" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2247" s="30" t="s">
-        <v>2798</v>
-      </c>
+      <c r="C2247" s="10"/>
+      <c r="D2247" s="10"/>
+      <c r="E2247" s="11"/>
+      <c r="F2247" s="10"/>
       <c r="G2247" s="11"/>
       <c r="H2247" s="12"/>
       <c r="I2247" s="13"/>
       <c r="J2247" s="13"/>
     </row>
-    <row r="2248" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2248" s="12">
-        <v>44684</v>
-      </c>
+    <row r="2248" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2248" s="12"/>
       <c r="B2248" s="12"/>
-      <c r="C2248" s="14" t="s">
-        <v>2155</v>
-      </c>
-      <c r="D2248" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2248" s="11" t="s">
-        <v>618</v>
-      </c>
-      <c r="F2248" s="10" t="s">
-        <v>2799</v>
-      </c>
+      <c r="C2248" s="10"/>
+      <c r="D2248" s="10"/>
+      <c r="E2248" s="11"/>
+      <c r="F2248" s="10"/>
       <c r="G2248" s="11"/>
       <c r="H2248" s="12"/>
       <c r="I2248" s="13"/>
       <c r="J2248" s="13"/>
     </row>
-    <row r="2249" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2249" s="12">
-        <v>44677</v>
-      </c>
+    <row r="2249" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2249" s="12"/>
       <c r="B2249" s="12"/>
-      <c r="C2249" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="D2249" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2249" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F2249" s="10" t="s">
-        <v>2729</v>
-      </c>
+      <c r="C2249" s="10"/>
+      <c r="D2249" s="10"/>
+      <c r="E2249" s="11"/>
+      <c r="F2249" s="10"/>
       <c r="G2249" s="11"/>
       <c r="H2249" s="12"/>
       <c r="I2249" s="13"/>
       <c r="J2249" s="13"/>
     </row>
-    <row r="2250" spans="1:10" ht="132" x14ac:dyDescent="0.2">
+    <row r="2250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2250" s="12">
-        <v>44645</v>
+        <v>44777</v>
       </c>
       <c r="B2250" s="12"/>
-      <c r="C2250" s="14" t="s">
-        <v>288</v>
+      <c r="C2250" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="D2250" s="10" t="s">
-        <v>25</v>
+        <v>489</v>
       </c>
       <c r="E2250" s="11" t="s">
-        <v>618</v>
+        <v>835</v>
       </c>
       <c r="F2250" s="10" t="s">
-        <v>2664</v>
+        <v>3046</v>
       </c>
       <c r="G2250" s="11"/>
       <c r="H2250" s="12"/>
@@ -77873,20 +77942,20 @@
     </row>
     <row r="2251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2251" s="12">
-        <v>44642</v>
+        <v>44754</v>
       </c>
       <c r="B2251" s="12"/>
-      <c r="C2251" s="14" t="s">
-        <v>387</v>
+      <c r="C2251" s="10" t="s">
+        <v>621</v>
       </c>
       <c r="D2251" s="10" t="s">
-        <v>492</v>
+        <v>6</v>
       </c>
       <c r="E2251" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F2251" s="10" t="s">
-        <v>2625</v>
+        <v>3027</v>
       </c>
       <c r="G2251" s="11"/>
       <c r="H2251" s="12"/>
@@ -77895,10 +77964,10 @@
     </row>
     <row r="2252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2252" s="12">
-        <v>44642</v>
+        <v>44761</v>
       </c>
       <c r="B2252" s="12"/>
-      <c r="C2252" s="14" t="s">
+      <c r="C2252" s="10" t="s">
         <v>387</v>
       </c>
       <c r="D2252" s="10" t="s">
@@ -77908,31 +77977,29 @@
         <v>835</v>
       </c>
       <c r="F2252" s="10" t="s">
-        <v>2624</v>
+        <v>2992</v>
       </c>
       <c r="G2252" s="11"/>
       <c r="H2252" s="12"/>
       <c r="I2252" s="13"/>
       <c r="J2252" s="13"/>
     </row>
-    <row r="2253" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2253" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2253" s="12">
-        <v>44614</v>
-      </c>
-      <c r="B2253" s="12">
-        <v>44614</v>
-      </c>
-      <c r="C2253" s="14" t="s">
-        <v>19</v>
+        <v>44770</v>
+      </c>
+      <c r="B2253" s="12"/>
+      <c r="C2253" s="10" t="s">
+        <v>628</v>
       </c>
       <c r="D2253" s="10" t="s">
-        <v>492</v>
+        <v>17</v>
       </c>
       <c r="E2253" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F2253" s="10" t="s">
-        <v>2528</v>
+        <v>3012</v>
       </c>
       <c r="G2253" s="11"/>
       <c r="H2253" s="12"/>
@@ -77941,221 +78008,285 @@
     </row>
     <row r="2254" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2254" s="12">
-        <v>44614</v>
+        <v>44761</v>
       </c>
       <c r="B2254" s="12"/>
-      <c r="C2254" s="14" t="s">
-        <v>19</v>
+      <c r="C2254" s="10" t="s">
+        <v>557</v>
       </c>
       <c r="D2254" s="10" t="s">
-        <v>492</v>
+        <v>6</v>
       </c>
       <c r="E2254" s="11" t="s">
         <v>835</v>
       </c>
       <c r="F2254" s="10" t="s">
-        <v>2548</v>
+        <v>2995</v>
       </c>
       <c r="G2254" s="11"/>
       <c r="H2254" s="12"/>
       <c r="I2254" s="13"/>
       <c r="J2254" s="13"/>
     </row>
-    <row r="2255" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2255" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2255" s="12">
-        <v>44616</v>
+        <v>44698</v>
       </c>
       <c r="B2255" s="12"/>
-      <c r="C2255" s="14" t="s">
-        <v>2250</v>
+      <c r="C2255" s="10" t="s">
+        <v>895</v>
       </c>
       <c r="D2255" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E2255" s="11" t="s">
-        <v>618</v>
-      </c>
-      <c r="F2255" s="10" t="s">
-        <v>2555</v>
+        <v>835</v>
+      </c>
+      <c r="F2255" s="30" t="s">
+        <v>2798</v>
       </c>
       <c r="G2255" s="11"/>
       <c r="H2255" s="12"/>
       <c r="I2255" s="13"/>
       <c r="J2255" s="13"/>
     </row>
-    <row r="2256" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2256" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2256" s="12">
-        <v>44623</v>
+        <v>44684</v>
       </c>
       <c r="B2256" s="12"/>
       <c r="C2256" s="14" t="s">
-        <v>535</v>
+        <v>2155</v>
       </c>
       <c r="D2256" s="10" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
       <c r="E2256" s="11" t="s">
-        <v>835</v>
+        <v>618</v>
       </c>
       <c r="F2256" s="10" t="s">
-        <v>2573</v>
+        <v>2799</v>
       </c>
       <c r="G2256" s="11"/>
       <c r="H2256" s="12"/>
       <c r="I2256" s="13"/>
       <c r="J2256" s="13"/>
     </row>
-    <row r="2257" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="2257" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2257" s="12">
-        <v>44522</v>
+        <v>44677</v>
       </c>
       <c r="B2257" s="12"/>
       <c r="C2257" s="14" t="s">
-        <v>46</v>
+        <v>387</v>
       </c>
       <c r="D2257" s="10" t="s">
-        <v>6</v>
+        <v>492</v>
       </c>
       <c r="E2257" s="11" t="s">
-        <v>568</v>
+        <v>835</v>
       </c>
       <c r="F2257" s="10" t="s">
-        <v>2350</v>
+        <v>2729</v>
       </c>
       <c r="G2257" s="11"/>
       <c r="H2257" s="12"/>
       <c r="I2257" s="13"/>
       <c r="J2257" s="13"/>
     </row>
-    <row r="2258" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2258" s="12"/>
+    <row r="2258" spans="1:10" ht="132" x14ac:dyDescent="0.2">
+      <c r="A2258" s="12">
+        <v>44645</v>
+      </c>
       <c r="B2258" s="12"/>
-      <c r="C2258" s="14"/>
-      <c r="D2258" s="10"/>
-      <c r="E2258" s="11"/>
-      <c r="F2258" s="10"/>
+      <c r="C2258" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D2258" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2258" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2258" s="10" t="s">
+        <v>2664</v>
+      </c>
       <c r="G2258" s="11"/>
       <c r="H2258" s="12"/>
       <c r="I2258" s="13"/>
       <c r="J2258" s="13"/>
     </row>
     <row r="2259" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2259" s="12"/>
+      <c r="A2259" s="12">
+        <v>44642</v>
+      </c>
       <c r="B2259" s="12"/>
-      <c r="C2259" s="14"/>
-      <c r="D2259" s="10"/>
-      <c r="E2259" s="11"/>
-      <c r="F2259" s="10"/>
+      <c r="C2259" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2259" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2259" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2259" s="10" t="s">
+        <v>2625</v>
+      </c>
       <c r="G2259" s="11"/>
       <c r="H2259" s="12"/>
       <c r="I2259" s="13"/>
       <c r="J2259" s="13"/>
     </row>
     <row r="2260" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2260" s="12"/>
+      <c r="A2260" s="12">
+        <v>44642</v>
+      </c>
       <c r="B2260" s="12"/>
-      <c r="C2260" s="14"/>
-      <c r="D2260" s="10"/>
-      <c r="E2260" s="11"/>
-      <c r="F2260" s="10"/>
+      <c r="C2260" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2260" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2260" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2260" s="10" t="s">
+        <v>2624</v>
+      </c>
       <c r="G2260" s="11"/>
       <c r="H2260" s="12"/>
       <c r="I2260" s="13"/>
       <c r="J2260" s="13"/>
     </row>
     <row r="2261" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2261" s="12"/>
-      <c r="B2261" s="12"/>
-      <c r="C2261" s="14"/>
-      <c r="D2261" s="10"/>
-      <c r="E2261" s="11"/>
-      <c r="F2261" s="10"/>
+      <c r="A2261" s="12">
+        <v>44614</v>
+      </c>
+      <c r="B2261" s="12">
+        <v>44614</v>
+      </c>
+      <c r="C2261" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2261" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2261" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2261" s="10" t="s">
+        <v>2528</v>
+      </c>
       <c r="G2261" s="11"/>
       <c r="H2261" s="12"/>
       <c r="I2261" s="13"/>
       <c r="J2261" s="13"/>
     </row>
     <row r="2262" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2262" s="12"/>
+      <c r="A2262" s="12">
+        <v>44614</v>
+      </c>
       <c r="B2262" s="12"/>
-      <c r="C2262" s="14"/>
-      <c r="D2262" s="10"/>
-      <c r="E2262" s="11"/>
-      <c r="F2262" s="10"/>
+      <c r="C2262" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2262" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2262" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2262" s="10" t="s">
+        <v>2548</v>
+      </c>
       <c r="G2262" s="11"/>
       <c r="H2262" s="12"/>
       <c r="I2262" s="13"/>
       <c r="J2262" s="13"/>
     </row>
     <row r="2263" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2263" s="12"/>
+      <c r="A2263" s="12">
+        <v>44616</v>
+      </c>
       <c r="B2263" s="12"/>
-      <c r="C2263" s="14"/>
-      <c r="D2263" s="10"/>
-      <c r="E2263" s="11"/>
-      <c r="F2263" s="10"/>
+      <c r="C2263" s="14" t="s">
+        <v>2250</v>
+      </c>
+      <c r="D2263" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2263" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2263" s="10" t="s">
+        <v>2555</v>
+      </c>
       <c r="G2263" s="11"/>
       <c r="H2263" s="12"/>
       <c r="I2263" s="13"/>
       <c r="J2263" s="13"/>
     </row>
     <row r="2264" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2264" s="12"/>
+      <c r="A2264" s="12">
+        <v>44623</v>
+      </c>
       <c r="B2264" s="12"/>
-      <c r="C2264" s="14"/>
-      <c r="D2264" s="10"/>
-      <c r="E2264" s="11"/>
-      <c r="F2264" s="10"/>
+      <c r="C2264" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="D2264" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2264" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2264" s="10" t="s">
+        <v>2573</v>
+      </c>
       <c r="G2264" s="11"/>
       <c r="H2264" s="12"/>
       <c r="I2264" s="13"/>
       <c r="J2264" s="13"/>
     </row>
-    <row r="2265" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2265" s="12"/>
-      <c r="B2265" s="9"/>
-      <c r="C2265" s="14"/>
-      <c r="D2265" s="10"/>
-      <c r="E2265" s="11"/>
-      <c r="F2265" s="10"/>
+    <row r="2265" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2265" s="12">
+        <v>44522</v>
+      </c>
+      <c r="B2265" s="12"/>
+      <c r="C2265" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2265" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2265" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2265" s="10" t="s">
+        <v>2350</v>
+      </c>
       <c r="G2265" s="11"/>
       <c r="H2265" s="12"/>
       <c r="I2265" s="13"/>
       <c r="J2265" s="13"/>
     </row>
     <row r="2266" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2266" s="1" t="s">
-        <v>1472</v>
-      </c>
-      <c r="B2266" s="2" t="s">
-        <v>1473</v>
-      </c>
-      <c r="C2266" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2266" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2266" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="F2266" s="4" t="s">
-        <v>1571</v>
-      </c>
-      <c r="G2266" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2266" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2266" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2266" s="36"/>
+      <c r="A2266" s="12"/>
+      <c r="B2266" s="12"/>
+      <c r="C2266" s="14"/>
+      <c r="D2266" s="10"/>
+      <c r="E2266" s="11"/>
+      <c r="F2266" s="10"/>
+      <c r="G2266" s="11"/>
+      <c r="H2266" s="12"/>
+      <c r="I2266" s="13"/>
+      <c r="J2266" s="13"/>
     </row>
     <row r="2267" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2267" s="12"/>
-      <c r="B2267" s="9"/>
+      <c r="B2267" s="12"/>
       <c r="C2267" s="14"/>
       <c r="D2267" s="10"/>
       <c r="E2267" s="11"/>
@@ -78167,7 +78298,7 @@
     </row>
     <row r="2268" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2268" s="12"/>
-      <c r="B2268" s="9"/>
+      <c r="B2268" s="12"/>
       <c r="C2268" s="14"/>
       <c r="D2268" s="10"/>
       <c r="E2268" s="11"/>
@@ -78177,337 +78308,451 @@
       <c r="I2268" s="13"/>
       <c r="J2268" s="13"/>
     </row>
-    <row r="2269" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A2269" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2269" s="9"/>
-      <c r="C2269" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2269" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2269" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2269" s="10" t="s">
-        <v>1636</v>
-      </c>
+    <row r="2269" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2269" s="12"/>
+      <c r="B2269" s="12"/>
+      <c r="C2269" s="14"/>
+      <c r="D2269" s="10"/>
+      <c r="E2269" s="11"/>
+      <c r="F2269" s="10"/>
       <c r="G2269" s="11"/>
       <c r="H2269" s="12"/>
       <c r="I2269" s="13"/>
-      <c r="J2269" s="13" t="s">
-        <v>1659</v>
-      </c>
-    </row>
-    <row r="2270" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A2270" s="12">
-        <v>44252</v>
-      </c>
-      <c r="B2270" s="9"/>
-      <c r="C2270" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2270" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2270" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="F2270" s="10" t="s">
-        <v>1635</v>
-      </c>
+      <c r="J2269" s="13"/>
+    </row>
+    <row r="2270" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2270" s="12"/>
+      <c r="B2270" s="12"/>
+      <c r="C2270" s="14"/>
+      <c r="D2270" s="10"/>
+      <c r="E2270" s="11"/>
+      <c r="F2270" s="10"/>
       <c r="G2270" s="11"/>
       <c r="H2270" s="12"/>
       <c r="I2270" s="13"/>
       <c r="J2270" s="13"/>
     </row>
-    <row r="2271" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2271" s="12">
-        <v>44112</v>
-      </c>
-      <c r="B2271" s="9"/>
-      <c r="C2271" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D2271" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2271" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2271" s="10" t="s">
-        <v>2222</v>
-      </c>
+    <row r="2271" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2271" s="12"/>
+      <c r="B2271" s="12"/>
+      <c r="C2271" s="14"/>
+      <c r="D2271" s="10"/>
+      <c r="E2271" s="11"/>
+      <c r="F2271" s="10"/>
       <c r="G2271" s="11"/>
       <c r="H2271" s="12"/>
       <c r="I2271" s="13"/>
       <c r="J2271" s="13"/>
     </row>
     <row r="2272" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2272" s="12">
-        <v>44088</v>
-      </c>
-      <c r="B2272" s="9"/>
-      <c r="C2272" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2272" s="10" t="s">
-        <v>902</v>
-      </c>
-      <c r="E2272" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="F2272" s="10" t="s">
-        <v>1007</v>
-      </c>
+      <c r="A2272" s="12"/>
+      <c r="B2272" s="12"/>
+      <c r="C2272" s="14"/>
+      <c r="D2272" s="10"/>
+      <c r="E2272" s="11"/>
+      <c r="F2272" s="10"/>
       <c r="G2272" s="11"/>
       <c r="H2272" s="12"/>
       <c r="I2272" s="13"/>
       <c r="J2272" s="13"/>
     </row>
     <row r="2273" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2273" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A2273" s="12"/>
       <c r="B2273" s="9"/>
-      <c r="C2273" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="D2273" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2273" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2273" s="10" t="s">
-        <v>900</v>
-      </c>
+      <c r="C2273" s="14"/>
+      <c r="D2273" s="10"/>
+      <c r="E2273" s="11"/>
+      <c r="F2273" s="10"/>
       <c r="G2273" s="11"/>
       <c r="H2273" s="12"/>
       <c r="I2273" s="13"/>
       <c r="J2273" s="13"/>
     </row>
     <row r="2274" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2274" s="12">
-        <v>44055</v>
-      </c>
-      <c r="B2274" s="9"/>
-      <c r="C2274" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2274" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2274" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2274" s="10" t="s">
-        <v>897</v>
-      </c>
-      <c r="G2274" s="11"/>
-      <c r="H2274" s="12"/>
-      <c r="I2274" s="13"/>
-      <c r="J2274" s="13"/>
-    </row>
-    <row r="2275" spans="1:10" ht="108" x14ac:dyDescent="0.2">
-      <c r="A2275" s="12">
-        <v>44055</v>
-      </c>
+      <c r="A2274" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B2274" s="2" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C2274" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2274" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2274" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F2274" s="4" t="s">
+        <v>1571</v>
+      </c>
+      <c r="G2274" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2274" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2274" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2274" s="36"/>
+    </row>
+    <row r="2275" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2275" s="12"/>
       <c r="B2275" s="9"/>
-      <c r="C2275" s="14" t="s">
-        <v>895</v>
-      </c>
-      <c r="D2275" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2275" s="11" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2275" s="10" t="s">
-        <v>898</v>
-      </c>
+      <c r="C2275" s="14"/>
+      <c r="D2275" s="10"/>
+      <c r="E2275" s="11"/>
+      <c r="F2275" s="10"/>
       <c r="G2275" s="11"/>
       <c r="H2275" s="12"/>
       <c r="I2275" s="13"/>
       <c r="J2275" s="13"/>
     </row>
-    <row r="2276" spans="1:10" ht="168" x14ac:dyDescent="0.2">
-      <c r="A2276" s="12">
-        <v>43949</v>
-      </c>
+    <row r="2276" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2276" s="12"/>
       <c r="B2276" s="9"/>
-      <c r="C2276" s="14" t="s">
-        <v>468</v>
-      </c>
-      <c r="D2276" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2276" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="F2276" s="10" t="s">
-        <v>684</v>
-      </c>
-      <c r="G2276" s="11" t="s">
-        <v>1616</v>
-      </c>
+      <c r="C2276" s="14"/>
+      <c r="D2276" s="10"/>
+      <c r="E2276" s="11"/>
+      <c r="F2276" s="10"/>
+      <c r="G2276" s="11"/>
       <c r="H2276" s="12"/>
-      <c r="I2276" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I2276" s="13"/>
       <c r="J2276" s="13"/>
     </row>
-    <row r="2277" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+    <row r="2277" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A2277" s="12">
-        <v>43949</v>
+        <v>44252</v>
       </c>
       <c r="B2277" s="9"/>
       <c r="C2277" s="14" t="s">
-        <v>468</v>
+        <v>895</v>
       </c>
       <c r="D2277" s="10" t="s">
-        <v>89</v>
+        <v>492</v>
       </c>
       <c r="E2277" s="11" t="s">
-        <v>683</v>
+        <v>757</v>
       </c>
       <c r="F2277" s="10" t="s">
-        <v>703</v>
-      </c>
-      <c r="G2277" s="11" t="s">
-        <v>685</v>
-      </c>
+        <v>1636</v>
+      </c>
+      <c r="G2277" s="11"/>
       <c r="H2277" s="12"/>
-      <c r="I2277" s="13" t="s">
-        <v>284</v>
-      </c>
+      <c r="I2277" s="13"/>
       <c r="J2277" s="13" t="s">
-        <v>1561</v>
-      </c>
-    </row>
-    <row r="2278" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="2278" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A2278" s="12">
-        <v>43838</v>
+        <v>44252</v>
       </c>
       <c r="B2278" s="9"/>
       <c r="C2278" s="14" t="s">
-        <v>103</v>
+        <v>895</v>
       </c>
       <c r="D2278" s="10" t="s">
-        <v>460</v>
+        <v>492</v>
       </c>
       <c r="E2278" s="11" t="s">
-        <v>645</v>
+        <v>757</v>
       </c>
       <c r="F2278" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="G2278" s="11" t="s">
-        <v>1617</v>
-      </c>
+        <v>1635</v>
+      </c>
+      <c r="G2278" s="11"/>
       <c r="H2278" s="12"/>
       <c r="I2278" s="13"/>
-      <c r="J2278" s="13" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="2279" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J2278" s="13"/>
+    </row>
+    <row r="2279" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A2279" s="12">
-        <v>43762</v>
+        <v>44112</v>
       </c>
       <c r="B2279" s="9"/>
       <c r="C2279" s="14" t="s">
-        <v>446</v>
+        <v>621</v>
       </c>
       <c r="D2279" s="10" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E2279" s="11" t="s">
-        <v>835</v>
+        <v>568</v>
       </c>
       <c r="F2279" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="G2279" s="11" t="s">
-        <v>1606</v>
-      </c>
+        <v>2222</v>
+      </c>
+      <c r="G2279" s="11"/>
       <c r="H2279" s="12"/>
       <c r="I2279" s="13"/>
       <c r="J2279" s="13"/>
     </row>
     <row r="2280" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2280" s="12"/>
+      <c r="A2280" s="12">
+        <v>44088</v>
+      </c>
       <c r="B2280" s="9"/>
-      <c r="C2280" s="14"/>
-      <c r="D2280" s="10"/>
-      <c r="E2280" s="11"/>
-      <c r="F2280" s="10"/>
+      <c r="C2280" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2280" s="10" t="s">
+        <v>902</v>
+      </c>
+      <c r="E2280" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2280" s="10" t="s">
+        <v>1007</v>
+      </c>
       <c r="G2280" s="11"/>
       <c r="H2280" s="12"/>
       <c r="I2280" s="13"/>
       <c r="J2280" s="13"/>
     </row>
     <row r="2281" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2281" s="12"/>
+      <c r="A2281" s="12">
+        <v>44055</v>
+      </c>
       <c r="B2281" s="9"/>
-      <c r="C2281" s="14"/>
-      <c r="D2281" s="10"/>
-      <c r="E2281" s="11"/>
-      <c r="F2281" s="10"/>
+      <c r="C2281" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="D2281" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2281" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2281" s="10" t="s">
+        <v>900</v>
+      </c>
       <c r="G2281" s="11"/>
       <c r="H2281" s="12"/>
       <c r="I2281" s="13"/>
       <c r="J2281" s="13"/>
     </row>
     <row r="2282" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2282" s="12"/>
+      <c r="A2282" s="12">
+        <v>44055</v>
+      </c>
       <c r="B2282" s="9"/>
-      <c r="C2282" s="14"/>
-      <c r="D2282" s="10"/>
-      <c r="E2282" s="11"/>
-      <c r="F2282" s="10"/>
+      <c r="C2282" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2282" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2282" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2282" s="10" t="s">
+        <v>897</v>
+      </c>
       <c r="G2282" s="11"/>
       <c r="H2282" s="12"/>
       <c r="I2282" s="13"/>
       <c r="J2282" s="13"/>
     </row>
-    <row r="2283" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2283" s="12"/>
+    <row r="2283" spans="1:10" ht="108" x14ac:dyDescent="0.2">
+      <c r="A2283" s="12">
+        <v>44055</v>
+      </c>
       <c r="B2283" s="9"/>
-      <c r="C2283" s="14"/>
-      <c r="D2283" s="10"/>
-      <c r="E2283" s="11"/>
-      <c r="F2283" s="10"/>
+      <c r="C2283" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="D2283" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2283" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2283" s="10" t="s">
+        <v>898</v>
+      </c>
       <c r="G2283" s="11"/>
       <c r="H2283" s="12"/>
       <c r="I2283" s="13"/>
       <c r="J2283" s="13"/>
     </row>
-    <row r="2284" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2284" s="12"/>
+    <row r="2284" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2284" s="12">
+        <v>43949</v>
+      </c>
       <c r="B2284" s="9"/>
-      <c r="C2284" s="14"/>
-      <c r="D2284" s="10"/>
-      <c r="E2284" s="11"/>
-      <c r="F2284" s="10"/>
-      <c r="G2284" s="11"/>
+      <c r="C2284" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2284" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2284" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2284" s="10" t="s">
+        <v>684</v>
+      </c>
+      <c r="G2284" s="11" t="s">
+        <v>1616</v>
+      </c>
       <c r="H2284" s="12"/>
-      <c r="I2284" s="13"/>
+      <c r="I2284" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="J2284" s="13"/>
     </row>
-    <row r="2285" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2285" s="12"/>
+    <row r="2285" spans="1:10" ht="168" x14ac:dyDescent="0.2">
+      <c r="A2285" s="12">
+        <v>43949</v>
+      </c>
       <c r="B2285" s="9"/>
-      <c r="C2285" s="14"/>
-      <c r="D2285" s="10"/>
-      <c r="E2285" s="11"/>
-      <c r="F2285" s="10"/>
-      <c r="G2285" s="11"/>
+      <c r="C2285" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="D2285" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2285" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2285" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="G2285" s="11" t="s">
+        <v>685</v>
+      </c>
       <c r="H2285" s="12"/>
-      <c r="I2285" s="13"/>
-      <c r="J2285" s="13"/>
+      <c r="I2285" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J2285" s="13" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="2286" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2286" s="12">
+        <v>43838</v>
+      </c>
+      <c r="B2286" s="9"/>
+      <c r="C2286" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2286" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2286" s="11" t="s">
+        <v>645</v>
+      </c>
+      <c r="F2286" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="G2286" s="11" t="s">
+        <v>1617</v>
+      </c>
+      <c r="H2286" s="12"/>
+      <c r="I2286" s="13"/>
+      <c r="J2286" s="13" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="2287" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2287" s="12">
+        <v>43762</v>
+      </c>
+      <c r="B2287" s="9"/>
+      <c r="C2287" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="D2287" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2287" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F2287" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G2287" s="11" t="s">
+        <v>1606</v>
+      </c>
+      <c r="H2287" s="12"/>
+      <c r="I2287" s="13"/>
+      <c r="J2287" s="13"/>
+    </row>
+    <row r="2288" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2288" s="12"/>
+      <c r="B2288" s="9"/>
+      <c r="C2288" s="14"/>
+      <c r="D2288" s="10"/>
+      <c r="E2288" s="11"/>
+      <c r="F2288" s="10"/>
+      <c r="G2288" s="11"/>
+      <c r="H2288" s="12"/>
+      <c r="I2288" s="13"/>
+      <c r="J2288" s="13"/>
+    </row>
+    <row r="2289" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2289" s="12"/>
+      <c r="B2289" s="9"/>
+      <c r="C2289" s="14"/>
+      <c r="D2289" s="10"/>
+      <c r="E2289" s="11"/>
+      <c r="F2289" s="10"/>
+      <c r="G2289" s="11"/>
+      <c r="H2289" s="12"/>
+      <c r="I2289" s="13"/>
+      <c r="J2289" s="13"/>
+    </row>
+    <row r="2290" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2290" s="12"/>
+      <c r="B2290" s="9"/>
+      <c r="C2290" s="14"/>
+      <c r="D2290" s="10"/>
+      <c r="E2290" s="11"/>
+      <c r="F2290" s="10"/>
+      <c r="G2290" s="11"/>
+      <c r="H2290" s="12"/>
+      <c r="I2290" s="13"/>
+      <c r="J2290" s="13"/>
+    </row>
+    <row r="2291" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2291" s="12"/>
+      <c r="B2291" s="9"/>
+      <c r="C2291" s="14"/>
+      <c r="D2291" s="10"/>
+      <c r="E2291" s="11"/>
+      <c r="F2291" s="10"/>
+      <c r="G2291" s="11"/>
+      <c r="H2291" s="12"/>
+      <c r="I2291" s="13"/>
+      <c r="J2291" s="13"/>
+    </row>
+    <row r="2292" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2292" s="12"/>
+      <c r="B2292" s="9"/>
+      <c r="C2292" s="14"/>
+      <c r="D2292" s="10"/>
+      <c r="E2292" s="11"/>
+      <c r="F2292" s="10"/>
+      <c r="G2292" s="11"/>
+      <c r="H2292" s="12"/>
+      <c r="I2292" s="13"/>
+      <c r="J2292" s="13"/>
+    </row>
+    <row r="2293" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2293" s="12"/>
+      <c r="B2293" s="9"/>
+      <c r="C2293" s="14"/>
+      <c r="D2293" s="10"/>
+      <c r="E2293" s="11"/>
+      <c r="F2293" s="10"/>
+      <c r="G2293" s="11"/>
+      <c r="H2293" s="12"/>
+      <c r="I2293" s="13"/>
+      <c r="J2293" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1881" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>